<commit_message>
Add dropdowns to form and fix Excel backend integration
</commit_message>
<xml_diff>
--- a/data/defects.xlsx
+++ b/data/defects.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -175,16 +175,13 @@
     <t>Problem1</t>
   </si>
   <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAB4AAAAQ4CAYAAADo08FDAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAP+6SURBVHhe7N15fBT1/T/w1+Y+N+QAlnCYhFMuQY5wCsQTxVZpbWnlR63i0aoULQq16tfWfi0qVqt+v62Wr1W+2sNWaQuVSxf4BiGBBEIIEAgkAUKykHs39/n7I5lh57PXbHY3e+T1fDzmAfnM7OzMZz7zmdl5z+fz0RgulXWDApNGTCB348njKf5QeHn0iYjIGn+4hol4TSN/5I/nGnkCazBP8p/cVdYIvl4/+E++EhFR//PlqxivYET9zbUaIUhMICIiIiIiIiIiIiIiIiIi/8QAMBERERERERERERERERFRgGAAmIiIiIiIiIiIiIiIiIgoQDAATEREREREREREREREREQUIBgAJiIiIiIiIiIiIiIiIiIKEAwAExEREREREREREREREREFCAaAiYiIiIiIiIiIiIiIiIgChMZwqaxbTKQAoRETyN148niKPxReHn0iIrLGH65hIs9f07q7Pf8dNND447lGnsDaxZP8J3eVNYKv1w/d0Gh8fRuJiMhbfPkK4T93BkSBwrUagQHgQOZa2SAVePJ4ij8UXh59IiKyxh+uYSLPXNO6u7vR3d2Nzq4udHd1oaurS1yEyAX+eK6RJ3imBqMe/pO7/hQADgrSICgoCEFBQdBoNAwGExGRgi9fFfznzoAoULhWIzAAHMhcKxukAk8eT/GHwsujT0RE1vjDNUzk/mtad3c3urq60NHZicioKDS3tKCzsxOtra3iokRERANGaGgoQkNDERkZiebGRoQEB8uBYCIiIvj4L0r3/3IkIvtcqxEYAA5krpUNUoEnj6f4Q+Hl0SciImv84Romcv81raurCx0dHYiIjkZTUxOio6Oh1WoRFBQkLkpERDRgdHV1obm5GVVVVdBqtWhubERoSAivj0REJPPlX5Tu/+VIRPa5ViPwDpOIiIiIiNyqs7MTEVFRaGhowLBhwzBo0CA+3CYiogEvKCgI0dHRGDlyJBoaGhAZFYXOzk5xMSIiIiIil/EpDBERERERuU13dzc6OjrQ1NyMuLg4Bn6JiIgEQUFBiIuLQ1NzMzo6OtDdzTZVRERERORefBpDRD7GtW4NiIiIvIfXMElnZyc6OjoQGRkpziIiIiIAMTExaG1tRWdnJwPAREREROR2HAM4EPHZY7/hyeMJvl6AedSJiEjk69cuR9x7bevq6kJDQwM6AYwZM0acTURERL3OnTuH4N5gMHvMICIi+PivS/f+cuzR1d2NnAvF2HE6H/llF2Ew1eOKqR4AMDQ2DrrYOEwdMQpLr5+KmdelIUjjyzlE5Al9L/MMAAeavpcF6gOePJ7gy4WYR5yIiES+fN1Sy73Xt66uLphMJnRpNAwAExER2XHu3DkEdXcjNjaWAWAiIgJ8/BemO385tnZ0YPPXe/H7r/WoajCJs61KionFY/MzsHr+EoSHhIiziQKc87UDA8CBxPnjTy7iyeNuvlyIebSJiMgaX752qeXeaxwDwEREROowAExERCJf/oXprl+O/z6Zhxe3f4by+lpxlirJcfH45bJv4a5J08RZRAHOuRqCd5dERERERH3i3I03ERERERER0UDV3d2Njbu3YfUnm/sc/AWA8vparP5kMzbu3obubneFpck1fD7iixgADgQanl9EntPtxvfbiIgoMPDmi4iIiIiIiEit7u5u/OivH+K3+3aJs/rst/t24Ud//ZBBYBpAnCvrHu0Cuqy5Bo8d+yOq2xrFWbK4IYkIjo4QkwEAEyOG4vWhy8RklxzIOnStQtBoEBIcDI1GXRy8u7sLHZ2dQO/nNRoNFsyZKy7mlC/36hE/KB4zpk8XZ6Gquhrni4tRVV2F5pYWAEBMdDSG6YZhdFoaYqKjferZY0NjI84XF6OiogINjT3HPDIiAklJSRidloakxETxI8g9dgy1tbW4JSNDnOUXPHbyDFg+VKABHmEiIrLC165V7uDe6x27gCYiIlKHXUATEZHIl39xuvLLcePubW4N/pr7yeLbseG2u8Vk6lcaF0sIOc9xbeHRAPA/yo/i1bPbxWSF6MHxCI+JEpNl/77uITHJJZmHDiIuLg5hYWFoa2uDqaEB48aOFRez6mxREWJjYuTP1tfXY+HceeJiTrEVAD55+jROnynEoLg4DE4ajNjYWABAbW0tDFcMaO/owMwbb8SI4cMVn/OWssuXkXP0KEJDQqDT6RAfHw8AMJlMqKysRF19Pa6fMAGTrr9e8TkGgEnJcaXVf3h0iYjIGl+6VrmLe695/RkAPnToEA4dOoQzZ84AAOLi4nDdddfh9ttv9/h3ExERuYoBYCIiEvnyL86+/nL898k8rP5ks5jsVpvvX80xgb1KLLl9LS3kHDHflQbk3WVYWBji4+MRHtHT8lin06maACA8IgLx8fEICwsT1uo+UvD3+vETcMuSDNwwZQrSUlKQlpKCGdOn4647liIpMRE5R4+i7PJl8eP9Tgr+JiUm4q6lSzFj+nR5e2+YMgW3ZGTg+gkTcLqwECdPnxY/TkREROQn7N9YU//6r//6L2zduhXjx4/Hf/7nf+K9997DI488gkGDBuH999/Hv//9b/EjA4Jer8fbb7+NtrY2cRYREREREVG/au3owIvbPxOT3e7F7Z+htaNDTCav4fMTX+D2AHC5qQrbzx3C9nOHkHf5DNqMJptTR0OT+PEBzzz4K7aWlWmABfPmISkxEcfz88W5/e54fj6SEhOxYJ7t1tCTrr+eQWDyE918Q4mIiAQc89fXfPLJJ7hy5QqeffZZ3HXXXUhKSgIAjBkzBvfffz9WrlyJ3bt349ChQ+JHXVZWVoannnoKjz76qDwx4EpERERERGRp89d7UV5fKya7XXl9LTZ/vVdMJh9SUlqKrOxsi6mktFRc1G+dKCgQk2xyZlnb7Mcx3B4A/t4/f4l1X/031n313/jL0S/QWGGwOZkuX4axrFxcxYClNvgrmXbDDWjv6MCZoiLzJfrVmaIitHd0YNoNN4izLDAITL7PfoVJREQDEQO/vubcuXM4fPgw1qxZIwd+RVOnTsVtt92GvXvd+wBAr9fjjTfewE9/+lO89957eO+99/DOO+8gNTVVXJSIiIiIiGhA6+ruxu+/1ovJHvP7r/Xo6ubzXV/0lV6PVQ88gGfWr7eYVj3wAJ57/nlU19SIH/MrJwoK8OMnnsC27faHxQWAbdu348dPPOHGILD1cu/2APCVRufe5jAeLUaF/jhqSi5bnQYKZ4O/ABATHY1BcXGorKxUzuhHlZWVGBQXh5joaHGWVQwC2/bKxo1YuHixPK1Zu1ZcxGKZhYsXi4tY2PzBBxafWbh4MTZ/8IG4aJ/dt2KF3Yptzdq1bv0+V23+4H+wZu1PhFTrlaS5NWvXWuSjtN/SsXGXVzZuxCsbN4rJQO922Jr3ysaNVsuOK9y9b2rdt2IFsrKzxWSZo/kSR+XTnm3bt+O+FSvEZLfLys5WlCvx+IrzrS1jjbXyYF6OpX2ztpw9tpYXj4mt5TzFVn3n6TcJ7Z2v5szzw1p94qnt3PzBB/16HMzdt2KF284hT9dFnl4/AKxZ+xMsXLxIMW3bvk1czMIrG3+NhYsXickD1vHjxzFu3DibwV/JXXfdhbq6Opw7d06c1ScNDQ3YvXs37r77bowYMUJODwsLw9133+3RIWKIiIiIiIj8Tc6FYlQ1mMRkj6lqMCHnQrGYTF4j9aamwc0ZGcjct8/q9Pqrr6KiogJv/OY34gr8ypTJk/HsunV4bdMmu8+it23fjtc2bcKz69ZhyuTJ4mwXWMY33B4ANven+3+FnLVbMHLQUADAo3OXI2ftFjw6d7liufZy54LGgaayqtJx8NeG2NhYtLS0iMn9pqWlBbGxsWKyXeZBYG8Gr33JmrVrYTAYFBWfNO605L4VK3AsL0+xzLPr1mHh4sUOg2DTp02zqFg/2rLF4w+6A9EPVq1S5OPdy5YBAJ7bsAGZ+/aJi3vErbfcgh07d4rJAIAdO3fi1ltuEZNd0p/7BrMgjMFgEGcBDuZv277da4EuV+j37lWUq2N5eYqXJiorKy3O4+c2bFCsQyTdaLz91lty2n0rVkCn08nr+Ntf/gL0HuOpU6eqelHD2nptHRNn1usuYj5l7tuH1JQUcbF+Zy3fzOuTH6xahVUPPOCxILC7OHOOmV+bHF2nRNa+x511kfr1u7/1b89x3y9Pdy+7W1zEwnMbfobMffvF5AHLYDAgReV5PWjQIK/cb4rdRH/88ceK+W1tbXj77bcV3UiLy3z88cd4++23cezYMTz66KPYsGEDGhoagN5g9IYNG+TPPvXUUygrK1N8/vLly4pt0Ov77817IiIiIiKiHafVDV8579vvonvjSigHmEzBWxs34BGzlEd+shXdP7H/crTa76T+8ZVejzVrf4I1a9danV7ZuBFjx47Fo488gswDB3z+uZgjdy9bZjcIbB78leIKnuTRAPDf87/C6MQRePWuJwEAaxZ8FwDw3qHPhSW96+zZIlWTpzQ0NiImOhotLS3IPXbMYnLXsHOV1dViElpaWlBnNIrJbiXuT+6xY2hpaUFMdDQaGhvFxW3qj+1fsHix3elJlQ+9nVFSWopjeXl4ysqDaInUskwK1kikCuWZ9esV6Wpk9gaZ1bRaC2y2u0jwVdLFQQyoSH/3x8XDU7Zt3y6/6CC+BKFmvr8Sg7mrVq7Ert275b+vXL3q9P5u+fhjfM+s5eXmDz7AMJ3O4rskqx98EB9t2SImWxDX6+iYqF1voBPzTbT6wQeh0+nwVQAFaPR79+L2227D9GnToHdzN7ye56abLwooMTExmDx5Mv7617/ixIkT4mxZWVkZ3njjDTz44IN477338MYbb6CgoEAR4D1z5gyWLFkidyP9wgsvIDc31yJIe/LkSZw8eRLvvfceNm7ciJiYGJSVleGFF17AbbfdJn/+scces/jctm3b8Oqrr+K9997DE0884XC7iYiIiIiI3Cm/7KKYZEUKvjMTOIc5+M4ocd418779Lp65/BQ0v7X/crS676T+UFJagpd++QuMGT0GU6dOtToVFRXhvfffx5z0dADAlStXxNX4HVtB4P4J/irjHB4NAH9+Yi/2Fx/F4tEz8N63f4Zk7WA8ufV1cTGvCQ4ORmhoKGpra1RNoaGhCA4OFlfjktiYWAyKi0NISAhq62qtTvbU1taqaoHb0tKCq1VVOFt8rQuElpYWnL9wAVerqhTLOiM2Nha1tY630doUEhKCQXFxXt1+0YF9++xO75i13HIXqWVagZ3+3nfs3ImfPvWUmAyYBfusvVHiyKqVKxUtSUtKSxXdkYrddord0Ipv5Ny3YoU8TwxOwqyVoLV1o7drZvNuMV/Z+GvF/JLSEsX8+1b0vFQiuW/Fd7Ft+zZ5vkTqOtPyM+4L/IpdwErdDpvniXl+OcprR6wFVPR792LpHXfIf4vd4Zp/v7R90jzYOb7ivsHKusX5jvbflruXLbN40cGcvflr1q7Fa5s24Vhens1tkrbFWvlUQ9wPKc8kfd1vd8vKzsYwnU7R8nXX7t34/ve+p1hO9INVq+y21rW2XnvHROJovf3BWve+961YoSgn5ufEQrMu3mGlzDtzXK3lmzXDzALo1s5RWNkOsZxDRV0rbr9YjmEjLxydY6IdO3fi5owMZCxZYrPXAme+x7wukt4SNbf5gw/k/bVXxzpe/7XAr6PrknTduW/Fd+VlSkpLFMuo4ej69srGX1t890Cm0+lQqvIcrKurw+DBg8XkPlu5ciUWLlyId999F48++qhFQLWtrQ2ff/45ZsyYgSlTpgC9geP7778fBQUFcgveKVOmyPMBYMSIEZgxYwbKy8vlNACIj4/HPffco0jbt28fZsyYgYyMDDlt/Pjxim6po6KisHz5crlb6vHjx2PSpEk4fvy4vAwREREREZEnGUz1YpKluSvwk4q/Yew/y3DXbOvPTeZ9+118PfxvGPt3x78DVX2nF2VlZzs1+TMpmLvmySex+sGHsPrBBy2m+fPnW/QoGAjEIHD/BH8lUoO3bs8GgAHIAd/v3HArdhQexKELvvPWeWxMDK4bNQojR45UNV03ahRiY2LE1bgkfdYs3LIkw/qU0TPZUlVdjbr6egxPThZnWYiIiMCk8eMBAGeLi+XgaWxMDMalpYmLqzY8ORl19fWostI6VyLth60pfdYs8SMWPLX9vuIHq1bhtU2bLB5mw6xVp/QWjDXTp03r04Dhk3v7mJe+4yu9Hls+/FDuknSYWQvhktJSPLN+vTz/9VdfVazrtU2b8NrGjcjctw9L77gDb7z5pmL+R1u2YMrkyYp1m3e/+crGjfhoyxZFt5jH8vIUD7yvbV/P/J7tUz4Qf23TJnkZ9D4072md2POZnz71VL+1RhTz5Fmzlpf28lqNW2+5Bcfy8hRpx/Ly5HEDXtm4Efn5+fL6n123DqseeECx/LW82ufw+Jq7dqyUXRaL229v/z3h7bfewrPr1sldAJu3dBW3RSyf7iR+V1/2e8+XX2L6tGny31evXsWOnTvlYJaY1yL93r2KrsBLSkthMBhQWVmpCIqJN5KTJ01Cfr7trnLE9arlaL394bkNGzB92jQ5EC0Fd6VysvmDD/Dapk1ymd7y4YfyZ9WcT/aozbcKgwFDhwyR/zY/R6Hy3Htl40bFcAF9qfNs5YW9c0y0bft26HqD3nPS06HT6SxeVHLle6zVgbt278aqlSsBB3WsmvWj9/rh6LoExTm/v8/nvJrrG11zww034OzZs6hy8BLgV199hUGDBmHMmDHiLJesXLkS77zzDiZNmoR3331X0TXz1atXUVJSghtuuEHxmfj4eAQHB6Ourk5OE7uBzszMRE1NDdra2uRlkpOTFWMLNzQ0oKCgwGL9otTUVAwxq0/CwsKQkJCgWIaIiIiIiMiTrqgIxj4yOx07Du8HDh1C0cwFQjfQAOZuwNfD/+aw5a9EzXd6y4mCAjyzfr1TU1+e+fuua2MCDwTmQeD+C/4qeTwAbC4qLEJMQkdLCxorrqD2TJHViaxraGxETm4uBsXFYcTw4eJsm6RgqRQ8HeXEZ60ZMXw4BsXFISc316nunPvK3dtvzb+stKQtKS21CJS40+oHH8SWDz+UAzz91VJObI22+sEHFWm33nKL/AaO9MaONH9Oerpi2R+sWiX/nbFkicWbO9OnTVNUcE+tXYtjeXlyK7QdO3daBB1/+tRT2LFzp9yaavWDDyE1JVWeb759kp7tuLaM2Hp6TvocRStZZ0ljJ0uTvVaA9vLEXl6rcfeyZTAYDHK5zMrOhsFgkPN4x86dim7F7162zCIAY759jo6vOfvH6lp+2Nv//taf2+Lqd23+4AMcy8tTBKWksUmlacfOnXaDwAaDwWqLty0ffyyv4werVuGZ9esVx2zo0KGosLO9ttbriKP1upPUqtNay8/vf+97cjD0tU2bFHXDR1u2KMp1akqKU+eTPWryTTqe5vWkeVmCynPPss5Ld7rOs5cXau358kvcfttt8t+333Yb9nz5pWIZV75HrAOllxykz7tax8Jhfl9r5Wt+3VFzzvdcR6619i0pLVF1faNrxowZg9mzZ+Ptt9+2GQTOz8/Hv/71LyxZskSc5RZhYWFYs2YN3njjDQDABx98oAjcSi2Epenll19GVVWV3HPOxx9/jCeffBKTJ0+Wu3FeuHCh/Hlb6urqEBwcjPj4eHEWERERERGRn1mEe27Mxj8OAcB+/KPiW3h+rvn8dLz3GPCoyuAvAGh8OLho3jhK7SQ19gk8vnucAonHA8B/vv8/0dzeij9k/wOL0m7E8imeeQjj18xffFDxEkRDYyMOfP014KBVqC3j0tIQHxfntuCptA0Hvv6634LA7tx+cyWlpXht0yZ82yxgUFJaiv/3wAPY5MEWg+h98J3Z2/Lyoy1bFK1j1TBv5aGWFDAYOnSonGbevehrmzbJQRupBddCoVtUiXmrNWl95oGlqVOnyv+HWaDxypUrZq2c5yiWkf427/vfvDtO8+2TmG9HVnYWIJfRa10f9CWvJD9YtUpxEbYVJIWKPLGV12pNnzYNBSdPAgAKTp6UgzxSfq564AFFIEwMJphvn6PjK7HVIt3aOA329t98uxwF0t2hP7fFle9as3at3MLTnmfXrbPZpa410nExDwxKY87a637eWxzlkz1Sq05pMu+eWgqGLly8GEvvuEMut7bKtfk8R+dTX5i/UHIsL8+iK21lfWZ9G83PPVvLOFPn2VqHM0p6x7a/2awXk8mTJile+nHH9yy94w65DvxKr7cIdKurY63feF27fji+Llk/5213A91zHbnWqlgK/Dq6vpHS7bffjvr6erz22mv497//LQeCz507h08++QQff/wxbrvtNsydq3h64HZS984lJSW4evWqnP7EE0/IgV3zacqUKSgrK0Nubi6eeOIJRTfOajU1NTkcgoWIiIiIiMjbhsbGiUlKc+di6dFDeL/3z/cPZ2Pp7GvD+gHZePSFMjzz0QY8YpZqz5BYrZhE5BXm3T5bGxO4P3g0APzczT/EJF0aXtu3Bc9ufxs1TUY8d/MPxcW8SqPRoLyiQtWk0diJyvaVk6s0D/4umD8fMdHR4iKqJJuNM+iqmOhoLJg/H+jHILA7t99cakoKDvQGXr69YoUc/F16xx34u4MxLt1lTno6tnz4IY7l5SErO1t+mGyvBfKxvDzFA2i1CgoK5C460TvmpNjNqbm//eUv2PLhh3ht0yangzLucN+K7/ZuX89Dc3H7/ImjvFbj1ltuwa7du4Herk8zhFZO4htjmfv22W1d15/HV9wue4F0T+vPbbH3XVJL1UwHwV8ADluTiqR6xPxlD/SOOXvFLGDhK+zlk6ukYKgzQVFY2aZMB+eTGuYvlIjBX3/2lV4PCEHzZ9avV8xzhymTJ8t1YH5+vqIOtF/HOnnz1Q8C6frWH6qqqvD2229j3LhxuPfee3HmzBn8/Oc/x6OPPor3338fdXV1eOSRR3DXXXeJH/W4IUOGIDU1FZWVleIshaioKEUr3ra2NtTU1CiWsUZaP8fyJSIiIiIiX6ezGwBOwVvfTAduXIvuj7b2TI+lAzfOVQZ7L36Msb8H3tu40rJ7aCvsfyf5OvHZpb8Sx/w17w66P4PAHg0A3zlhPnIuncJ7hz4HALy2r6fbxUfnLheW9C6TyYSuri6gu9vq1NXVBZPJJH7MdU4+f3RX8NcTvBEE9iQp2CsFf3/eh/H8XGEe7EhNScHSO+7An/78Z8Uyks0ffACdTtenQMRrmzbJ4yVKXQi//dZb8nxrgSGppfL0adOcepBv3ioGQuuva0HunhZX15a51gIrKzurd/t+K8+3tn3XdFu0vpR4eyxStXntiNQF6uYPPoDBYJBb0ql5acAWR8fX1rrd0ZrPF125ehXDhBdOzFv+OXrAr9aatWsxfdo0RZmwp7KyEjo7L8LodDrFtqWmpFht7SuOOXvlyhWL/TUnrlctR+vtLyWlpfhoyxZs+fBDfLRli1w32KorzOeJZd4Zfc03c7a2w1pdKu6HtTrPVjm2tQ5n7Nq9G8+uW2cRMP/BqlVywNYd32PeDfSxvDxFi25X61g11yV3cf76NrBJwd+hQ4fi8ccfx9y5c/H000/LLWxfe+01PP74424f9xe94+9+9NFHiq6e29rasHfvXnnM3bCwMCxZsgR//etfceLECcVnt23bBgAYNGgQOjs7sc/shZ9PP/0UJ3tbtNsjrT8zMxN6s+v0mTNnUFZWpliWiIiIiIjIm6aOGCUmXTNqAe7CZ5j/g3uhMZsePZqOZ74tNAQ4tBGaf47A1yqCwDeMuE5MIp+lDJC99OKLbm0E4i1i8FfijSCwRwPAC/5rNW59/wn57/cOfY6Zb62SA8K+IigoCKNGjsTMmTOtTqNGjkRQkEezyiFfDv5KAjEI/MCqVR4P/paUllqM5SmNASw9zH5uwwYcy8uz6BZ68wcf4KMtWxTduqqRlZ0td4EqVUJicEEKlJh/xjzwIAaOHNmxc6fi82+8+SZ+sGoVYBbkllqIWVtGfBhfUlqi2D5rUlNSMH3aNDxrdgy3bd+OY3l5iuX6m6O8dsb0adOwa/duRden0n6L+SmWM3Nqj6+aY+Vt7jy+u3bvxq233CL/PX3aNOj37pX/3vLxx/L/+0rqLvd7Zl3Pi8zP/ZLerurNx1cVTZk82WK81dtvuw2vbdok/y3VM+Y3IgUnT1p0127O2nrVcLTe/vLshg3yuLo/WLUKb/YGCKVybV5XlJSWYtv27X06n0R9zTdzas49tXWevXJsLy8k4vrMScHXyVbGqLk5I0MO2Lr6PZKld9yBN958U1EH2q9jr/24sLf+1JRUh/ntLn25vt234rvY/MH/AL2fW7h4kfz5Vzb+Gvet+K7wicAgBn+94fTp03jyySflsX2ffPJJJCQkYM2aNQgLCwMATJkyBU888YRiHOAXXngB06dPB3q7jX7iiSeQm5srz09OTlY1BjB61//CCy9g27Zt8uf/+Mc/YtCgQeKiREREREREXrP0etvPgh6591tAzgEcFNLf3/oZMHOBZaD30EbMz5mDrx10B33H9VPEJPKy6ppqMUnW1NjU+z8Nbs642eZQXf7CVvBX0t9BYLdHNYdGX+vKTA1NfRvCatsRUdpkdQoI4ti+TpZffwj+SgItCLz6wQfFJLdLTUnBjp07FWNL7tq9G5lCN7CZ+/bJY7RKk/SAWHp4bMuxvDzF555Zvx6Z+/bhObMH71JA5Jn167Fw8WI8u2GDRReU0ryFixdj+rRpVisxW36wahX+9Oc/Kz5vnr/P9QZmpPEPFy5ehNtvuw2rH3wI6H0Yf237Flndvmu65f9JLcCk7z1RUOD2h/fOUpPXat16yy0wGAwW3T+//dZbmD5tmuK4T7ESkDGn9vheO1bX1t1zrDx/vjhy97Jl8nniTIBOZCsfnlq7VnG+Si3oXSG1xBTHmF24eLEiKC9/5wMP4Nl16+zm993LlqHCYFC0rlz94IOK47Zr926Lboc/2rJFMW6ryNp61XC0XncS67uFveNaS0F0Kd9WP/ggjuXlyeXkuQ0bFOfMqgcekIOYfTmfzPU130Rqzj01dZ6jcmwvLxydY3/6858xfdo0q29sSgFqqUcLV75HkrFkiUUdqKaOvXvZ3b3rX4RXNv5aMU/y3Iaf2b0uuYtz17eByxeCvzExMdi4caPFuL4rrVwLpkyZoljmzTffxIgRI+T5I0aMwJtvvinPz8jIwMqVKxWBZPFvc+LnN27ciJiYGABARkaG1c+tXLnS6rYSERERERF5wszr0pAUEysmAwDe/+29GPt3K89JLn6MsRs+xkGUYu2GjfL4wABw8O9PQPMDZZq5pJhYzLwuTUwmL5mTPgdjRo/GPcuXK56tmE9/++zv+OY3vil+1C+dKCiwG/yVmAeBTwi9NbqbxnCp7FqkxA3KTVU4eqUIAJB18ig+/eIf4iLXtHWh62ojIkcPRnC05YMNAMj79WdikksyDx1CXJxWDphpNBqcLSrC+HHjbHanaTAYcObsWYwbOxbd3T3ZVVtbi8rKSiyca/EuipITgV5r/Cn4a85ft9tZbj15+khqBQzAYeXi+1w8YXziiBD5hm3bt+NEQYHiRQ97pBbB9gLL8OB6A52z+Ubu5Oq1ZSBw7/VTGj6lS6NxS1fMvhD8JSIi8oRz584hqLsbsbGxXu95joiIfIMv/4Ltyy/H/9q/B7/a9U8x2SOev/2beHzRrWIy9QvbJVccXsvc0KFDkZqSKib36kuJ864TBQWqG404s2xfuT0AbO6fh77Ez/7nNTFZISQuEkFhIWKyzN0B4EtlZbhQdgnx8fFISkrybADYdplXxd+DqP6+/Wp47OQZsFw5afp2NBYuXiwmAQBef/XVgBvPlgaeVzZutBgL1Rq1y0nULq92uYGC+eEtrlxbBoq+XUNtcWcAmMFfIiIKZAwAExGRyJd/wfbll2NrRwfmvfELlNfXirPcKjkuHgd/+h8ID7EdayJP8nTJ7UvpI48GgL88cQjr/nRtvMG+cHcAGGZBYK1Wi/DwcFRWVWHkiBGIiooSFwUANDU14VJZGQYnJckB4La2NtTX13ssABwowdNA2Q9bPHbyDFgunDQ8GkREZMGV68pA4t5rqDsDwF999RUKCwsZ/CUiooDEADAREYl8+VdsX385/vtkHlZ/sllMdqvN96/GXZOmicnUb7xRcvtaIgeO4HVPP/2SmOgu0eGR2HMyC40tfRvLd/64abhr+iIx2WVxWi000ODK1Uo0NjVBo9GgqbERtbW1VqeGhgZ0dXejsbERTY2NaGpqQmtrKzQaDUaNGCmuvqesu1jer1ZWoqa2FvPmzvXroGlYWBh0Oh3KKyoQExMDrVYrLkJkpi8nDit6IiKSbr7Eibyhu7sbbW1t6NZokJCQIM52SlpaGmbPni0mExERBYSamhpoAISHh0Oj4b0LEREF5i/ZcUN06OjsRHbpeXGWW/xk8e14cK7740jkjEAsuf7Poy2ABySW8wGFJ4+7OXsC8QgQEZGz1w6y5N7rqTtbABMREQUytgAmIiKRL//CdeWXY3d3N3701w/xz/xccZZLvjl1Bn733Qf4IpXXeSP/XSmRAwPvLt3JG2WcaMBiBU9ERERERERERETk6zQaDX733Qfwk8W3i7P67CeLb2fwd0BjD3COMABMREREREREREREREREHqPRaLDhtrux+f7VSI6LF2erlhwXj833r8aG2+5m8Jd6sRxYwy6g3YFla8DiyeNuak4m5joREZlTc+0g+9x7bWUX0EREROqwC2giIhL58i9cd/5ybO3owOav9+L3X+tR1WASZ1uVFBOLx+ZnYPX8JQgPCRFnk1f5Qsl1ZwkNDAwAu8oXyjV5DU8ed3N0QjHHiYhI5OjaQY659/rKADAREZE6DAATEZHIl3/huveXY4+u7m7kXCjGjtP5yC+7CIOpHldM9QCAobFx0MXGYeqIUVh6/VTMvC4NQWzx66N84bh4ooT6NwaAXeELZZq8iiePu9k7qZjbRERkjb1rB6nj3musFAAODgvDyJEj+UCbiIjIhuLiYqCzkwFgIiKS+fIvXPf+cqTA4msll6UVHAOYiIiIiPyXr/3AIElQUBDCwsLQ0NAgziIiIiIAjY2NCAsLY+CXiIiIiDyCd5lE5OO6+cYOEREJNAz++jCNRoPg4GCEhoaitrZWnE1ERDTgdXV1oa6uDuFhYQgODoaG3VkSERERkZsxAExEPoyBXyIiEvEBqa/TaDQICQlBXXU1YmJicOnSJRiNRnExIiKiAaerqwvNzc24fPkywsLCYKyrQ0hICAPAREREROR2HAPYFbw/H/B48rib+UnF3CUiImt4A+Z+7r/mdnZ2oqW1Fc3NzUhMSkJLayva2trQ1dUlLkpERDRgSEMkhIaEoK62FpEREYiIiEBwcLC4KBERDVC+/IvX/b8cKXD4WsllaQUDwC7ytTJN/Y4nj7sxAExERPbw5ssz3H/N7QbQ2dGBtrY2NDc3o6WlBZ2dnejq7ga63f99NBCxPqAe1msU66n9h+Wzf1w7ztdy3IfzXqNBkEaD4OAgREREIDIyEmFhYQgOCfHlrSYion7my9cEb99hkS/zxZLLEssAsDN8sQyTV/HkISIi6g+8CfMsz9zRdHd3o7u7G52dnWhvb0dXVxe6Gfwlt2G9QPZqL9tz+gfLZ//pOdY9Oe77+a7RaBAUpEFoaKg89i+7fyYiInO+fFXw9h0W+TJfLLkssQwAO8MXyzB5FU8eIiIiT+MNmOd59o5GCgRL/ydyD9YNZK/2sj2nf7B89jd/yfGeYG83A79ERGSTL18dvH2HRb7MF0suSywDwGr5Yvklr+PJQ0RE5Gm8CfM83tGQP2LdQLZqL+up/Y9ltD/5V277ShklIiJf5MvXNF7ByDZfLrkYsKU3SEwgInUGZpVBRERERETka7rNJl/hi9sUuJjLRERERN7E+15fxAAwUR+wKiMiIiIiIiIiIiIiIpIwcuJLGAAmchKrMCIiIiIiIiLf4j/tTny9i0QiIiIiV/jHHdlAwAAwkRNYdREREREREZFz+EuyP/lHbjMITERERESexQCwIxrel1MP//gRSUREROQM3uEQkX/yv9pLap/qf1vuj/wjl/nAiYiILPnHNYzI3wzMey4GgO0ZmGWCrOCFl4iIiAIP73CIyD+x9iIiIqJAxtfGiMgdGAC2hcFf6sULLREREQUe3uEQkX+yrL0sU4jgVw/O+QCKiIhs849rGRH5IgaAiezgBZaIiIgCD+9wiMg/WdZelilEIv8oJQwCExEREXmWNPzGwLnvYgBYNLCOPxERERENKP7xGJyISKSsvfynbSf5Bv8oLXwgRURE1vnHdYzInK/frw+Mey4GgM0NjGNORERERAOSL//4IiKyjbUXERERDXS+Hk4jso6l1ps0hktlPAJg8Jes48lBRETkbbxJcw/e1VCgYd0wUFjWXpYp/ofl15v8I/cDoZwTEZGneOtaxqsT2bKn5AjeOvx3XDJeRXtnhzibVAoNCsbIuKF4evZ9uDl1pjjbaQwAS7xVa5JP48lBRETkbbxJcx3vaCgQsW4YCCxrL8sU/8Uy7E3+kfuBVN6JiMidvHUd45WJrNmgfw//PHtATCYX3T12Hl67+UdislPYBTSHWCEbeEEjIiIi/8c7GiLyT8raq9sixf9J+xRo++Uf/CPX+cCKiIis84/rGA0EO85nMfjrIduKDuKLc1lislMGdgCY99FkAy+iRERE5P94R0NE/om1FxEREZF9fI2MfMF/5/xDTCI3+l2ua/k7cAPADP6SDbxwEhERkf/jHQ0R+SfL2ssyhcgd/OfBOR9gERGRbf5xLaNAddF4VUwiN7pgvCImOWXgBoCJrOAFk4iIiPwf72iIyD9Z1l6WKYFpoOynb/KP3GcQmIiIiHxPW2e7mERu1N7ZISY5ZeAFgDmECtngHz/6iIiIiOzhHQ0R+Sdl7eU/bTPdR9rngbbfvsE/cp0PtIiIyDr/uI4RUX8bWAFg3ieTDbxIEhERkf/jHQ0R+SfWXkRERESu4Wtk5G8enbtcTCI3GzgBYAZ/qZf5e9W8MBIREVFg4B0NEfkny9rLMoWoP/jP8wE+4CIiItv841pGBHx7Sgb2PPKumOySnLVbkLN2i5g8YPlcAPi3776DB1Y/JP/95FNr8eRTaxXLEPUVL4BEtq1ZuxZr1rK+JeDtd97BDx+6di0eCAbiPqvBesFf8A6HiPyTZe1lmTIwMR+8yT9yn0FgIiIi8n8zR050Kgj82rI1yFm7BbUv61H7sh7lL+7An+7/lbgY9er3APDmDz7AgiWLLSYpyNvQ2Ch+xHnSsCjmUz/a/MEHWLB4MTZ/8IE4CwCwYPFiLFi8WEwOeFK+eIu1H3ElpaVYs3YtsrKzxVketfmDD7Bw8WLF9Nzzz/f7djgibac/8aVjunDxYh8NnIgVpFhRiunWJlvE5Tw3Wcvz+1aswCsbN/Yef8vP9Ey2eav8qGFtf3/40EP4Sq8XF3WZW67FXvbKxo24b8UKMVl2oqAACxcvlo91IOyzozp7oZ17E/Jn1u5wiAYCln1/Z/0IivdtA3kib7JePn0NywoREVnnH9cxGoheW7ZGDt7OHDkRf8j+B+KjtKqCwH+6/1dYeeNSlNVfxYYv3sWGL97FtlP/h8HRg8RFqVe/B4Almza+qpgeeWg1AODn6zfgw83/Iy6uDu99yQZbF70rV67gWF6emNxvXn/1Vbz+6qt46cUX0dDQgGfWr8eJggJxMXKCrxxTaXp4dU/d5l2eeJgkrtOd63aOeX4vv+deGAwGPLN+PTZ/YOtaYnt7vV1+1DCvN4YNG4aXfvlLtweBn9uwAX/8H1v55x/SZ8+GwWCwGczftn07dDod5qSnAwGyz4HL1lV8IOq2MhENZDwP/BWPGhEREZFnib8ceedM3lb7sh4ZY2Yi/oUMeXp2+9uY+dYqVUHgxaNnYN/5XNzzx3V479DneO/Q53j077/Gre8/IS5KvbwWAJ6Tnq6YpkyeLC5C1CfiRc2XL2xS+b85IwNvv/UWdDodtm3fLi5GfsS1uk0Mprpr8gxfOc/mpM+Rp++tWIG33/otfrBqFT7asgVZ2Vni4n7PvN545Ve/wpjRo90eAA4EN2dkQKfTQb93rzgLAHDgwAEsnD9fTCbyUd6uaYl8nXhXonYiTxNznDlP/sR/yqvnfvMREVHg8Y9rGwWa8z/7BzZ88S5mvrVKnAUA0J/LwcyREzH3uiniLFlkaDhMrep68Hvu5h/i/M/+gdqX9Tj/s3/guZt/qJi/fMoSHHh8M8pf3CEv89qyNYplpPGEX1u2Rl5O8ujc5Tj5zF99vhtqrwWAbVEz5m9WdjYeWP0QFixZjKV3LwuY7gyzsrPxs+efl7uI/vaKFRb79uTatViweDG+0uvlZZcuW4Z/9QYNf/vOO1i6bBkWLF6Mnz3/PKprahSfz8rOxgMPPSR/x8+ef96rLU6fXLsWT65di6/0enx7xQp5v8VgRklpqSJvHnjoIZSUlsrzzffrzmWWZUIaw3Db9u24c9kyuWveZ9avBwA8s369oitQbxmm08FgMAC93ZM+9/zz8vbet2KF1eDwV3o9fvjQQ1jYu+/btm/HmrVrLfIgKztbsZw4vy8cbeNzzz9vdUxN6ThI5TMrOxvPPf+83W5tbe2T+XHzxWNqTt1+/gRr1v4E27Zvw53L7sLCxYss0u9b8V0sXLwIa9b+BNU11fhKr5fT7lvxXYtzes3an1i0hs3KzsLCxYvsBkh7ju/P5e24b8V3sW37NsDsZrGktATPPf9z3LR4ERYuXoQfPvQgSkpLFOvxhtUPPoTp06bhX9t6thc29+daebVXfhyVdW+aPm0aGhoaFGn2zndb5+Xb77wjd5lsbdxXR+sUl//zX/6ChYsXK65D27Zvx0I7XRS728L583HgwAExGV/p9TA1NODuu++W0wJln51lbx+tkfLpREGBU59z3UD+iTqQ952I/JX/BM6IHPOPsswgMBEREfkO82Dpn+7/FbIvFuC9Q58rlpG8tmwNvjWlp0XwoQsnxNmy/cVHcffEmywCtaL4SC3uv/EOvLZvCzZ88S5qm414Yv53MHLQUHmZ28fPwcU6A36x5w/Y8MW7+LIoGw+n32MRgI6P1GJ68jikv/0A4l/IAHqDvxvvfALHy4uw4Yt38e7Xn2Lx6Bmqg8DWtn/udVPw6NzlYrLLfC4A7EhWdjbWbViPBfPmY9PGV7Hu6afx2dbP++HBo2d9pddj3fr1yMvLw9I77sB93/oWAODDLVvw23feERfHpt/8BjExMVh6xx0wNTTgtU2b8LPnn8exvDx8a/ly6HQ6ZB44gN+//778Gek7YmNj8cCqVbjvW99CXl4ent2wwSJQ3J8qDAb87yefYN1TT2HTq69imE6HTb/5jWKbntmwAQCw6dVXe5YZNgxXrlwBpDKxfj3mz5+P1199FT99+ml8/rllmagwGHCioAD/u2ULMvftw8OrV+PHjz0GAPjxY4/h9VdfxdixYxWf6W8mkwk6nQ4AUFBQgLS0NLz4wgu9Xdveg9c2bVIEvr/S6/HSL38p7/uLL7yAz7duxblz58zW2pNHz6jII2c52sabMzJw7vx5xTYDwKGsLCxYsACJCQnytumGDpW7tp0/f36furX1xWMqcbyf136wK8vqfjn93LlzOFFQgJ8+9RReevE/cO7cOfzil7/E799/D4898ihef/VVxERH45e/eln+jCssj++9vcf3WoB3fe+5+dqrr+I14dz0tqlTpyLTLPhne39KAWjw8OqH8ePHfgRYKT+Wn7U8H70l8+uvMXXqVPlvR+f73DlzrJ6XmV9/jdtvu02RJlGzTrHr7ENZPS8X5JmlnygowMIFC8yW8qwlS5bA1NBgUZdkHz6MMaNHIzUlRZFuzl/32RmO9tGWCoMBf9i8GSvvvx+vv/oq/t/KlfhoyxaHn6O+8I9HzkT+Tmydysn1iSjQ+Ee59mwPUEREFDj847pGgSJ91GS8c6Cntaw45azdgm9NycDoX98jfszCPX9ch8OXTuLh9HusttiVJERpcccf1sjdRD+59XVEhobj/824U17m0b//Gt//5HlFV9IA8MCsZWZr6lnXg5++jEt11553P7t4FXIunZI//8pXf8S2U/+HxaNnKD5rzdzrpsjbb572xerf4tnF1ltHu8JrAeAFSxYrJrWt9Da9+SaW3nEHVj/0IObM6ekC8/+tXInPtlp/e8CbPtyyRW6xaj5Zs+k3vwEAvLZxI36+YQN+8uSTeO+//xuxMTH422efWTyov+P22/HzDRvw8w0bsPSOO4DeB85vvP46Vj/4INY99RQAKB5O/+799zFm9Gi889ZbWP3gg/jJk0/iW8uXw9TQgF27d8vL9TeDwYA3Xn9d7tb06bVrYWpoUDxANxgM+Obdd8vL/PpXv5IDM3KZePBBuVvU/7dyJT7/XFkmDAYDHn3kESQmJAAApkyejNTUVABAamoq5qSny/P6W0lpKV7ZuBHnzp/H3ct6KpnvrVgh79Oc9HR8r7dlXlZvgAEAPv7kE8W+z0lPx6bXX5fnS95QmUfOcrSNN2dkIDYmRrHNJaWlyDxwABlLlgC927ZwwQKsefJJeT2rH3wQS++4Q/ECgxq+cEyl1r3SJNVtzuzntbKaqEgHgEcfeQRz0ufg5owM3HH7HTiWl4fHHnkUN2dkYE76HKy8fyUMvQFkV31vxQo89OBDSE+fg/T0OVjRe3wPZV2rrw0GA75x991yF8z/+av/xJixY33iIeDkSZMUf/eU14cU3UUDQFbv/vSUn56AYE/5mSOXH0dlvT9lZWcjKzsbX+n1WLN2LWKio3HvPddukhyd73cvW2ZxXp4oKIDBYMDNGT1vsokcrXNyb1fnUqC1uqYGx/LysHDBApw8eVJez7G8PCe7RXfNlMmTodPpkH34sJxWXVODAwcOYPm99yqWFfnrPsNKPSRNIkf7aIvBYMBTa9f21js958MPVq1y+DmyR6w1vVl7Eg0E14IkPNOIyDW8dhMRkX/ilYv6w9zrpiAhSouPv/+yYuzf+BcykHPpFOIjtaqCv5J7/rgOd27+CYqry/Bw+j3IWbtF0bIXAM5XlykCtlKr4sm60WZL9bTE/ccPNyFn7RaUv7gDABAbHq1YRlzXyEFDkRClxd9PKBubHL18BpGh4RYtiEWHLpyQWxKf/9k/5OBvzqVTTuWDWl4LAG/a+KpiUtNKr7qmBoYrBtzcGziSpKWmwtTQYBEk9TadTofp06ZZTKKs7GyYGhowfdo0xUPixIQE3HH77UDvw3lz6bNny/8fOmQIAMgtKtE7RiR6H9Ki9zsMBgPOnT+vCEZ/uGULAKCpqUleX3+bPm2aIkgntcgyP546nQ6/f/99xYsCiQkJPWXCYJCDiZJUK2VC/B5fID2UX/XAAziWl4eXXnxRUQa2bd+Ot995B2vWrsWdvYHhxt5jVV1Tg3Pnz1vse2JCAsaMGSP/7Uwe9YW9bURvudy9Z4/8d1ZWFnQ6Heakp8vb9g2zblglGUuWwGAweLV1el9IrXulaezYscJ+Ksfnvbaf1fI6esqqZfB3zJgxivSo6CigN9Auie5Na2xUdgncF90Atm3fhrffeQc/WfsT3LnsLgBAU9O1sRZ0Oh3ee/99RVfS1rbdGzeUjY2W9Zq0P2vM9qfRbH/scVTW+8sz69fjmfXr8dIvfwmdToc//s//yHWb2vNdPC/37t2L6dOmWW0Rq2adqSkpGDN6tBz4zMvLw/Rp0zB3zhxkfv010FunGwwGzJkzR7EeT1t+zz2KbqAPHjwIU0MD5s2bp1jOnL/vs1gPSZM5Nftoi7WyMnnSJIefI1u8UUMSDWTXWsfx7CMiZ1g+KPfVWoStgImISD1fvZpRYJiaPBY7Cg9aDW5WNtZh9K97grjOdH986MIJ3Pr+E3jo05cRGRqOrQ9YNohzZM8j72LljUsBAJ+f2Itf7PmDuIhVd14/HwCw8c4nFC2ZN975BNC7v2pI+SEFf299v+fz7ua1ALDUikqa1ATmis4VAQDWrV+vCGKu6x2z0Ve6HZXccdtteOettywmZ0RH97xxcPXqVXGWBSkQbM+Y0aPlbpTNJ1utvnzF6xs3YuzYsVi3fr1ijOCzRT1lQhqvU5qkcTx9rUyIpIfy//3uu/jbX/6iOA6vbNyI3/3+9wCAb37jG3jxhRfMPgkU9e67I9JynsgjR9uI3taG5t3N7t6zR+5mVs0+qFnGl1ir29Tsg5pl+lM3gF9v/LXZ8f2m1eP76saNGDd2LJ5dvx7fWfFd6O10293fN5QlpSVyl+oA8IqK/bFFTVnvL5n79iFz3z78+LHHsGPnTsWLMWrP9/TZsxXnZebXX+PWW26R12NO7TqnT5sm9zqRffgw5s6Zg3nz5sFgMKCktBQFBQXQ6XQWgUNPmzNnDkwNDfKYzYeysrDQ7IUpa/x+n4V6SJrMqd1HZ/X1c0RE/eNaq9/+vi8hosAh1SG+XZcwCExERETe996hz/H9T54XkwHAZrpan5/Yi0+O7sToxBFYPkXZwMGe5VOWYObIiXj3609xzx/X4ZWv/mhzfGJRfnnP87RPj+/Bhi/etZi+ON3TKESN0b++BzsKD3os+AtvBoD7YujQnqbcP37sMYsA5iYfGuvTnRobe1qmufPhsfhAeE56ulvX7wmpKSn4+YYN+N8PP8T0adPwH7/8JQ5lZyvKhNjSSWp96cuk/Be7Bz1RUIAdO3fip08/jTVPPil3s2lOejnAEU/lkZpthFkXrFlZWSgpLcW58+flQLe0bfb0dft8iT/uZ0Hv8V339E+x5sknkdHbxbQoNSUVP9vwM3zUe26+9MtfKFoDe9Ou3buxcH7P2KvXymvP/khdZjumUV3W+9v3VqzAwgUL8Mabb8ot5dWe7zdnZMjn5Vd6PRrttIhVu87ZvUFlqYvlyZMn9/RIMHo0CgoKesbCnd/zllx/Sk1JwfRp03AoKwvVNTXIPHDA4UtP/r7PaqjdR7Wk+xVnP0e++9iYiIiI1PHdVsEcE5iIiNTxpasXUV9UGKvEJJsGx8QDAPaey5HT1AaQD104gZomI2LDo+Xxg80n8+6i1XA1CO6I/wSANT0PcXU6HZqamiwCmHNUtiL2RXPS0xEbE4NjeXmKrp6ra2qwc9cuAMA0K11HO2Ps2LGIjYnBufPnLcZb/s+NGxV/+xrzLoClQDAAFJw8KZeJxgArE9KD9LS0NDlN7AZ8yuTJiI2JwWGzsS3R2+Wo+djPnsojNdsoWX7PPdi9Zw+yelveSS8cSNum37tX/Aj0e/dizOjRiu37urdbVUllZaXib1+VmpKqYj8tu012J2fyrhtAQ28X0qlpPWMqozcobM6822opEAxAMf6pqL/ekn9l46/R2NCA++//PmDWJXaa2f7YKq8iZ8p6f/vp00+jsaEBn3zyCeDk+b5w/nzs3rMH2YcPK4YQEKld55zea9nWf/wD0TEx8ost06dNw4mCAhzLy8MkYVzm/nLrLbcg88ABbP3HPxAbE+MwABwI++yI2n205ty5cxbd82cfPmxRZ5M9/VUbElEPjvlLRJ5gq0t5328fTEREJOKVi3xdztot+NP9v8Kjc5fj0bnL8dqyNXhi/ndwvrpMHudXjS9Of43m9lb88vZH8ejc5Xju5h/iuZt/KC5m02cn9Fg6YZ7Ftux55F1xUa/znwBwr1UrV+LDLVuw+YMPkJWdjazsbPxr+3afD2I68qPHHgMAPLthA/5z40b89p138OiPfwxTQwOeXbfO5QeqiQkJ+Nbynn7Uf/Hyy/jtO+9g8wcf4Mm1a7Fj505xcZ9SVFSEnz3/vHy8//SXvwC94w2it0x8JJSJbdu34xUVZUJqqXT48GGfCejALGD/57/8BVnZ2fhKr8cfNm8WF8Py5cvxt88+Uyz3y5dfVnR7CxfzCL1jSJtPJwoKVG8jertgPXf+PHbv2YO5wliYjz3yCHbs3Im333lHXv/mDz7Ajp078egjj8jL3XrLLTh3/rz8fdu2b8eWjz9WrAs+d0yvPWx87JFHzfYzC1nZWdj8wf9Y7KcnKPMuC9u2b7Oad+bGjh2LmJgY/KX3M3q9Hn/YrBwLoaioCM89/3N5f/7ce26qCXi584ZS+n4pT+9b8V0cOHAAr258VQ6sK8trT6tXcX+k5QDg8OEjcvlxpqz3t8SEBPy/lSvxt88+k7dX7fm+ZMkSnDt/HkVFRRbjwIrUrnPatGn4/PPPFa1eZ8+ejWN5eTAYDA4Dr54itW7+/PPPsWBBT6twR/x9n9VQu4/WrHvmGYs6e+X994uLkVXurAGJyDFbARoiInfwhxdM2AqYiIjU893rGRGwePQMbLzzCWy88wncdf187Dufi3s/fEZczK5LdVfw7tefIi1xBDbe+QQemv1NvPLVH8XFbHp2+9t4fd//In3UZHlb5l03FXvP54qLep1vB4Ct3KN+Y9ky/OLFF7Fz926sW78e69avx6GsLMyZPVtc1K9I+zV06FDs2LkTf/vsM8RER+MXL76IbyxbJi7eJ6sffBA/fuwxRMfE4G+ffYYPt2wBAPzixRfFRX2K1E2ldLx379mDl158EXN6u2C9e9kyvPTii9i1ezeeWb8ez/SWiXQVZSIxIQHPrluHnbt24cdPPOEDAcMeiQkJ+OnTT+NYXh6eWb8ev3//fTy8erW4GFY/+CB+sGoV/vfjj/HM+vX4+JNP8Ogjj2CYEAB2JY/QO0ak+fSHzZtVbyN6W5otXLAAV65cwd1Ceb45IwMvvfiivJ5n1q9HcXExXn/1VfkYo3cf7vvWt+R93fPll1i1cqViXfDhY9qzn/+BY3nHrOynmq6I++7uZXfjvm99G//78f/azDvx5i4xIRHrnv4pjuXl4dn16/H799/Dw6sfViwjnZvPrl+PZ9evx+49u/HSi/+hen/E7+wr87L59ddf4/bbbsP/btmi6Fo9MSERP+3dn57yark/0nI95WcnfvzE4zhRUGDls7bLujd8b8UKjBk9Gr95803AifNd6p69obFRca5Zo3adc3vH2zV/CWBOejoMBgMWqgy8ekJiQgIWLlgAU0ODRR1ki7/vsxpq91E0ZswYLL/3Xrzx5pvyeffSiy/6dLCbiAYqjvlLRP2FQWAiIiIic7Uv61VNoxNHiB+1auZbq5D8y6WIfyED8S9kYNLr38X3P3le0e3yzLdWYeZbqxSfA4D4FzIU3S2/8tUfMfrX9yD+hQyM/vU9+PzEXotlbK0LwufjX8jAgv9a7VQQub9oDJfKeH9KfsF3C6rvuW/FCtx+221Y/eCD4iyvWbN2LXQ6HZ7r7cI78PlXBeat88u/cknirdwi8r41a9cCAN5+6y1xVj/wzxpDifUHUf/y9YAMEQWWa7XNtbsWX7x/Ya1IRESOWbuC8QpCout////EJHKz04/9r5ikmm+2AL7Wgw4RwIuLU7Kys2EwGBy24OpP0rjEalve+T//qcC83SLG29/fN9JFyn+OMxF5m3/WdkT+69p1mmceEfUf8feB+DcREZH/4K9YIv/newFg3h+TgBca2/78l79YjN34y5dfxvRp0xTd33pLdU0NsrKz8cuXX8bCBQt8Yps8y7+Cgr50bvnSthARuRdrOKL+de1ejGcfEfU/f3hZ1Je3jYiIfA3vqYn8l28FgHkPSgJeYOxLTU3F119/LY/duOXjj7F8+XL8h4+M67z1H//AM+vXY9iwYfjp00+Ls8mLfPHc8sVtIiIiIn9yrdUv7yuIiOzhAzgiIiJyXVhwqJhEbhQaHCImOcW3xgDm/SeZ8Z2CSaSW/1Rivnp++U8OmvPV3CQKNP5ZQ7COIOpP1wLARETe5j93Lqw1iYiIqG++8enPUFRTJiaTm1wXp8PO770uJqvmWy2AiXrx5wfRwMQWO0REROS8a92t8j6CiIiIiIiof/zoxm+KSeRGj8+8R0xyClsAu9maf/0Gu85mi8l+4fZx6Xj7G97vptd3CiSRs/ynEvOH84y5SURK/lMrKLGOIPI8Bn+JyHf5xx0Ma1AiIiLqm5/u+S98cT5LTCYX3Zo2C2/ftkZMdgoDwG42ftN3xSS/cmbdX8WkfuU7hZGoL/ynEvOXc80/ctRfcpPI3/lHjWCJdQSRZzH4S0S+zz/uYliTEhERUd98VZKD17P+ijLTVXR2dYmzSaXgoCCMiB2CtbO/jTtGp4uzncYAsJuxBbBrfKcwEjnLvyowfznX/CNX/SU3ifydf9QISqwfiDyPAWAi8g/+cyfDGpWIiIgClS/fkbn/Hsw3AsC+nOfUr7xfGIn6wr8qMX86z/wrZ+FnuUvkb/ypRmBdQNR/GAAmIv/gP3cyrFGJiIgokPnqXZn778HcFgDu7u5Gd3cfVuWreU1e0YcSRORF/leB+ds5xhwmomv8pUZgPUDUvxgAJiL/4h93NKxViYiIKJD54h1Z7/2XRoMgjXu2z6UAcHd3Nzo7O9HV1SUHgLt7ZoiLWueefaAAorLkEPkI/6vE/O0cYw4T0TX+UiOwHiDqXwwAE5H/8Y+7GtasREREFKh8825Mo9H0TkBQUJA89VWfAsBdXV3o6upCR2cn4pMSERkVhZCQEGjcFJUmIiIiIiIiIiIiIiIiIhoouru70dHRgaamJtRVVyM4OLjPgWCnA8BdXV1ob29HzKA4DIqP79OXEhERERERERERERERERGRpa6uLtTV1sJUX4/Q0FCn47Gql+7u7kZXVxfa2tsxOHkYEhITnf4yIiIiIiIiIiIiIiIiIiKyLSgoCAmJiRgybBja2tvR1dUlLmKX6ghud3c32tvbMTR5GCIjI8XZRERERERERERERERERETkJpGRkdANG4a2tjZ0dXWhu1tdx86qAsBSn9PRcXGIYPCXiIiIiIiIiIiIiIiIiMjjIiIjETtoEDo7O8VZNjkMAEtdP3d3dyM+IV6cTUREREREREREREREREREHhIfHw9oNOjs7ISaNsCqAsCdnZ2IS0jgmL9EHpCfny8mERF5BesjIqLAwTqdyDaeH0SBgecyBRKWZyJSg3WF8wIpz4KCghAntQLu7nbYFbTdiG53N9ANoKOrC5HRUeJsIiIiIiIiIiIiIiIiIiLysMjISHR0dDgM/sJRABjo6f65q6MDoaGh4kwiIiIiIiIiIiIiIp+xZ88elJWViclOKysrw549e8RkIiIirwkJDe2J23Z1ibMs2AwAS9Hj7q4udHZ1QaPRiIuQE0pKSsQkmb15RERERERERERERKTehQsXcOjQIZemCxcuiKslIiLyKo1Gg66uLnSr6AJaY7hUZnUJ6YNt7e1oamrEhMmTxUV8Qk1NDQwGAzo7OxEeHo4RI0YgKsr3uqvOz89HSkoKtFqtIt1oNKK0tBRTp05VpNPAkZ+fz+NPRD6B9RERUeBgnU5kG88PosDAc5ls2bNnD5KSkhAWFibOckpbWxuqqqpw6623irPczl3lOTc3FxcvXhSTVRk1ahRmzJghJhMNSLm5OSguLsbVq1fltNTUVIwZMxbjxo1TLNuf3FVXmDt//jyqq6vFZK9ITEzE6NGjxWSXeCLPvO3UiQLExsYiODgIQUE22/naDwB3d3ejvb0djY2NuH7qFHERrzt79ixKSkoQHByM0NBQNDU1ITg4GFOnToVOpxMX9yqDwYCioiIsXLhQkZ6ZmYmxY8f63PZS/wnECoiI/BPrIyKiwME6ncg2nh9EgYHnMtly6NAhpKWlYejQoeIsp1y5cgXFxcWYO3euOMvt3FWeS0pK8H//938AgLS0NHG2TZcuXcLIkSMtnl1T4CsrK0N0dDTi4+PFWQPO2bNn8c9//gN79uxGY2MjYmJikJp67TwqKSlGQ0MDhg4dim9845u48867MGTIEMU6PM1ddYW5w4cP4/Lly4iNjRVn9SuTyYThw4dj9uzZ4iyXeCLPvO1k/gk5ABwcHCzOljkMALe1taGxqQkTfSwAfPHiRRQUFECn02Hs2LEAgJaWFpw7dw4mkwkLFizwuZbAn376Ke644w65FbDRaMTOnTvxne98R1yUBpBArICIyD+xPiIiChys04ls4/lBFBh4LlMgcWd5loLAOp0Ot99+uzjbKr1ej7i4OLYAHmCuXLmC/Px8DBo0CLNmzRJnDxhXr17F3/72Kf70p0+QmpqKZcvuxtSpN8hxJ3NHj+bi8OHD0Ou/QlNTE773ve/jgQd+KC7mMe6sKySHDx+G0WjELbfcIs7qV19++SW0Wi0DwCpcCwAHIyg4CLYG8LXdNticg36kvaGiogLx8fGKkzAiIgKTJ09GUFAQSktLFcv7gri4OBw/flz++/jx44iLi1MsQ0RERESuyc/PF5OIiIiIiIgGhNTUVNx0000wGAzYtWuXONuqjIwMBn8HIIPBgLCwMNTV1aG2tlacPSCcPXsWTz+9Fl9+uQcbNvwMf/zjR/jWt75tNfgLADfeOAOPPfYjfPrp37Fs2d3485//hHXrfqroKprI09SM/wvVLYAbGzHxBu9GyI8dO4bGxkb57/r6eowZMwbJycmK5QDgzJkzqKmpUbQAHjJkiFf7ZgeAwsJCZGdn49577wUAbN26Fenp6ZgwYYK4qGqlpaUoLi5WpGVkZCj+Jt/WlzdQurq6YDKZ0NLSgpaWFnE2EcLCwhAVFQWtVguNxvo7QIFcjtTsP1nqS31E3sFjZR/zh6hv50Eg3xtQYOrrPV9fzo/+kpuba/WF9qamJjQ2Ntod48uerq4uDB48WEyGyWRCREQEQkNDxVlISUnx62CArby0pr29HS0tLaq7PrSXb9Z4Ky+dyQNP80QeuPNcdmbcVE+XF3eOw+pMGfD0frmzDKjZr6amJgQFBSEiIkKcpUpLSwu6uroc9jDprv1yZ3mW9KUlsDMOHjwIAJg3b544y6Py8/NRVVUl/63VajFz5kzFMqSOXq/HyJEjUV5ejqFDh7oUp/BHubk5eO65nyElJRX/8R8vWb1XcuTo0Vxs3PhrxMTE4I033vR4l9CeqCvEFsCHDh1SxOIciY6OlrvKd+WzbAGsXsHxfMTGxiIkJKS3BbD0W0gZ7vXJAHBhYaHFA4fS0lLEx8cjOjpaTtPpdFZb0JaXl8NkMsl/X7lyBcHBwRbj7A4aNAgpKSmKNE/bunUrkpKSAABVVVVyMLgvrF1kpZsfNftVWlqKqqoqXiC9zNkKqK2tDbW1tQgPD0doaCi6urrQ1dUlLkYDWFBQz+Dv3d3dqK+vR1JSEsLDwxXLBHI5UrP/ZJ2z9RF5D4+VfcwfIufPg0C+N6DA5Mo9n7PnR3/KzMxESUkJhg0bpkivr69HVVWV1WcgjnR0dKChoQFjxowRZ+H8+fMYPHiwPFSVpKKiAqmpqX49FqStvLTGaDSisrISo0ePFmdZZSvfrPFmXtrKg5aWFhiNRrc/pL569Sq0Wq1FwM1TeeDOc9lWXlnjT+VlIO9XWVkZwsLC+lzOr169ira2NowYMUKcJXPnfrmzPJvzVBDYYDDIjZLS0tIsnrs70tfn0jk5OQCg+Jyn8i7QSQ3LMjIycPz4cdTV1WHRokXiYgHr6tWrePrptRg6VIeNG18VZzulsrISjz/+I4wePQabNr0hznYrT5R3MQD85ZdfAr0vVzhiNBoBwG2fZQBYHb8OAO/fvx9VVVUICwuT0+rr6zFhwgSMHz9esawaBw4cgNFoRExMjJzW2tqKtLQ0TJs2TbGsp0mtgAG41Po3Pz8fDQ0NLr1h1dcLLbmXMxVQZ2cnqqqqoNVq0dbWJs4mshAWFob6+noMHjxYHhB+IJUja/tPtjlTH5F38VjZx/whcu48GEj3BhSYnL3nc+b86G+ZmZmoqKjA0qVLFekXLlzAkSNHcOONNyrS1bh69SrKy8uxfPlycRb279+PsWPHWvSutmPHDgwbNswtQQ1vsZWX1pSXl6OoqEj1g29b+WaNN/PSVh44u79q2coXT+WBO89la3ml0WgQFBSEzs5OxbLO5p+tfLHG3Xllbb9sCbT9Onr0KKKjo/v0LBm9PUw2NjbarXfduV/uLM8iTwSB8/PzERYWJt87OrvtfXkubTKZcOTIEcyaNUt1S3Wy7ciRIwgJCcH06dNRW1uLnJwcTJ06FUOHDhUXDUjr1v0UBkMFXnttU59a/oqOHs3Fiy++4PExgT1RV1gLAKsNxHrrs87wRJ55m+0AMBRB4L71HdQPtFotxo8fL08JCQniIqpFRUVh8ODBGDt2rDypfTPY3SZMmIDIyEhERkb2OfiL3tbDaWlpYrKCXq9XtIQ2GAzQ6/VA79tSxcXFMBqN0Ov1yOdYeX6hsbERkZGRfDBHqrW1tSEqKkrR9cZAKkfW9p+IiIiUBtK9AQUm3vMRkbtpNBpEREQgKioKISEh4mwiv9KXMYEdqaqqwvDhwzFkyBBFd8ySvj6XLiwshF6vlyfzeVLQt7q6Wk4T2fte9H53YWEhcnJy5O8wGAwwmUyK7/U0a12Ym0wmGAwGMdkjmpubUVdXh/j4eABAfHw8oqKiUF5eLi4akPbv349Dhw7iwQdXuyX4i96xgaUxgTkeMHmXRp58NgAcqIxGI5qbm9Hc3Cw3cXeWdCFwtmsNczNnzkRaWhq0Wi0yMjIC7g2IQNXc3OzU2FZEABAcHIympib574FWjsT9JyIiIqWBdm9AgYn3fETkLlLwVwr8RkZGMghshdjVN/k2dwaBS0tLERERgdjYWOh0OkRERFgNaNpi67l0fn4+ysvLkZGRIU8NDQ2KIHBycjKKi4tdasxUXl6OESNGICMjA8nJyTh16hROnDghf6dWq3Vp/Y6YTCYUFxfLwztKaUeOHJG71fa0CxcuIDg4WDGMZGJiImpraxXLBapt2/6Fm2++2S2t98099tiPEBUVhS+++Lc4i8gr/CIAPGjQIISFhaG2thZHjx51empqakJERISiC2hvOX78OLRaLbRaLY4fPy7OVkUcH5kGDh576ouuri60trbKfw+0ciTuv7P+9Kc/YfPmzX1+aWeg2bp1KzZv3uzStHXrVnG11EfW3h4uLCzE9u3bsX37dhQWFoqzSYWtW7cy7yigDLR7AwpMrt7zERFBCP5euXIFhw4dQnNzM4PAgpCQENxyyy1OtZzryxjm5JuqqqoUvXUmJCRYbQXsrKqqKkycOFGRlpaWhqqqKrlV74QJEzBr1ixUVVVBr9f36XdZUlKS3LBq+PDhQG9g2Xx+Q0OD/Le7xcbGIiMjAwBw8OBBOfiblJTk0nCPzqiurpZb/0qGDh2Kzs5Oq8H83NxcfPbZZ26bcnNzxa/oN2fPnsWhQwexeHHPMXC3jIyb8a9//VNMJvIKvwgAR0ZGYsiQIYiPj0d0dLTT0+DBg5GYmOj1GzWj0Yji4mJcf/31uP766+WuLoic0dXVJSYR2WWtzFhLC1Su7GthYaHckqSoqEicLTt27Jjd+Z5y8uRJNDc3y39fuXLFK9thbtq0aViwYIFL07Rp08TVUh/p9XrF2935+fnIzs5GVFQUQkNDceDAAZff/iaiwODK9ZLIF7AME1nX2tqKM2fOKKaLFy+iqqoKeXl5bp2qqqpw8eJFi+/zp5czzIO/J0+eREREBCIjI8XFBrSQkBA5TxISElQ9b502bRp7H/Qyd40DbDKZYDQa5cApehtvGY1GRdfLzrLV46X0t/kwD1IAdeLEiSgvL0dOTo7ZJxwLCwuT/y91K+2NFu1SsFcK/vbXOVJbW4umpiZ0dHTg5MmT8lReXo7g4GBUVlaKH0FTUxMaGxvlhm2uTI2NjV7tteX48TzExMS4vfWvZPbs2bhy5QrOnj0rziLqd0Fm3UHbn7wsNTVVMSaws5P5WzzeIrX+nTBhAiZMmABtH1sBJyYmAjZa9RARkftcuHABWq0WOp0O58+fF2cDvcHf2tpalJaW9mvwVRqv5ejRo2hubpYfUHjyLVU1UlNT5etcX6fU1FRxtdRHc+fOVXTxVVhYiJtuugkZGRm4/fbbcfPNN8NgMCAzM1P8KPU+JCksLLT7wl5hYSHvyYiIiMimyMhIp1pJultnZycaGxstptbWVly+fNmtU2trq8X3NDY2IjQ01Kt5oEZoaChuvPFGRfA3Pj4e06dPB3p/f3V0dIgfG3Ck4G9TUxNOnDgBqOgiOywsDOPGjVN8hvqXu4K/AHD58mWgN2gpjZd76tQpxbz+otPpMGvWLBiNRr/9TTZv3jwkJyf3W/AXAC5evIjg4GB0dHTAaDQqpvDwcNTV1SkaG0giIiIwZ84clydvBNvNlZaWYvLkKWKy29x44wzExMTg3Ln+e0ZIA1G32ST+fW3yixbAgcC89a+kr62AY2NjodVqUVZWJs6yYP52FLt2IyJST/oBMWrUKAwbNszqDwop+Dtp0iSkpKR4LAhsLcAUGRmJG2+8EQBw9OhRiwcUA5UUsHNlKikpEVfrt8RxnqKiohQB9tTUVEyePLlP9yOB7k9/+hPy8vJw+vRpbN261aJc1NXV4dNPP8Xp06exa9cu6PV6xXwiIiIa2DQaDUJDQ3H33XdjwoQJ4ux+ExUVhRtvvFExjRkzBuHh4Zg4caJbp/DwcIwZM0b+nhkzZmDOnDlYsWKFV/NAjTlz5mDMmDEM/joQGhoKmP1elrpxtRUEDgsLQ3h4OJqampCbm4u6ujqvtvwbiNwZ/AWAmpoapKWlKcbplcbSrampUSzrzHPp6OhowEqDJ1stgyVSC15zznyvL+jv+rGurg6JiYmYO3euxSQ9Z7pw4YL4sYBRXFysGPvYE1JT0yyeIRB5g8ZQViaFiBW6u7vR3d2NtrY2NDY2YmI/voWyf/9+tLW14brrrgMADBs2TFykT6TWUujtynP48OH91s1kZmYmqqqqcO+99yrSt27diqSkJKe7HJDGBtBqtZg5c6acLvXRn5KSgpycHISFhclvEB08eBAtLS3yGAOlpaUoLi6W/ybvyM/PV/2W14ULFzBo0CAxmcihuro6uU4diOXIfP/Vys3NxbFjx7Bs2TJERUXh008/lX/koPeakpeXh7S0NAwdOhTovbY0NDS4NQibn5+Pw4cPQ6vV4jvf+Y44G83NzTh69CiioqJc/l5n6iNftXXrVlRXV4vJTklMTLS4XvsaZ4+V9KM/NDQU3//+98XZ2Lx5MxYsWNDvPzw9xdn8saakpEQOluv1ejQ1NWHZsmVAbzlrb2/HHXfcAa1WC6PRiK1btyI9PT1g8pD8nzPnwUC8N6DApPaez5nzo79lZmbiyJEjGDdunCL9ypUraGxsRFCQ4/f4u7u7LQIxXV1dqvJGcvbsWcyaNcvpZxW+xFZeWmMymVBfX4+oqChxllUtLS0IDQ1FcHCwOAvoDWTMmDEDKSkpMBqNOHToEMrLyxEZGYkVK1aIi3tMZmYmKioqsHTpUkX6hQsXkJOTIz/od5ejR49i5syZuO6666DRaBAZGYng4GCP5YG7z2Vrwd9///vfFr8vOjs70d7erroVW1NTE0JDQ+XgqT0NDQ0ICQlBdHQ0goODXc6rzMxMnDx5UpHW2tqKtrY2RRp6646uri6b5Rq9LzbMmjULixYtgsFgwIkTJ5CQkIAZM2YAQrBcDP4CwIwZM1SfZ/aoOb8NBoPLgfuQkBCbgUe4ua50d3mGB4K/BoMBp06dwqxZsywCr9Kz6okTJ0Kn0/XpuXR+fj6qqqoUaQcPHkRCQgImTJgAk8mEkpISRT4VFhaivLxc/oyj783JyUFMTIzid5ter5e3G73bVl5e3m/j8fYnqeHCzJkzLcYAlhw7dgxNTU2YP3++nJafn4+srCxMmjTJpXKan5+PkydPYs6cOS6txxU/+tFjmDhxIh577EfiLLd58sknMGXKFDz++BPiLJd5oq44fPgwjEYjbrnlFgDAl19+Ca1Wi9mzZ4uLWvDWZ53hiTzztoLjxxEbG4uQkBAEBQfb7MQ54ALA9m7AOzs75bd+qqqqEB8fL3en7CmlpaW4cOECTCYToqOjMWfOHHmcjObmZhw4cAAmkwmJiYm47rrrnH77JCcnR9FiJyIiQr44SRdeSVpamsWFVboI9uc4A6TkTAVk6+Fcc8UpnCo375ojAWkzUmH9Mq5UW5KLioiJmDisp1zWluSiuOba58X5aonrIe9SFwBuRsWpU2gZNgOptg5abQlyi5uRPHEinCwSXqX2YaC5rVu3AoAcCNy1axcMBgN+8IMfCEt61vbt22E0GuXgk7Ufn83NzW4Zl8qZ+siRwsJCHDhwQEy2K5ACkJ7Wl2Nl68e/0WjEp59+KpevPXv2KD4HALfeequY5NP6kj/WFBYWorGxEVVVVWhqapLrg61bt2LYsGGYM2eOvKzUwtrewx/xYYQkPz8fDQ0NFg8Y8vPzAcBieU8R7yvN8V7R/zhzHti+NyDyL2rv+Zw5P/pbZmYmioqKFA9d0dtd47lz55CQkKBIF7W2tqKhoQGTJk0SZ1m9jywqKkJycrLc8kry9ddfY+zYsXava77OVl5aYzAYcP78eYwaNUqcZdXFixcxePBgq/fg4eHhmDx5MuLj45Gfn4+jR48iNDQUQ4YMQXFxMR599FHxIx7jrQDw6NGjERERAY1G49E8cOe5bC34W1hYiIqKCnFRBYPBgLCwMAwaNAjd3VYfscJkMiEiIgKNjY1oa2vDkCFDxEVkRqMRISEhCAkJQW1tLe6//35xEacYDAa5MYyksLAQlZWV0Gq1ivSOjg60t7crynVbW5v83FISERGBxYsXIy4uzmYQOCgoyGPBX6g8vw8ePIjw8HCbQS5Hamtr0draanGPbs6ddaU7yzPs/P5zhTTWrnljJHPm8/v6XFoK6EqSk5MtgrXmzJ+FQ8Xz8IEeALYW3BXZChLn5uYiJycHkydP7lNZzc/PR0FBAWbOnCnXF97AALAlVwKx3vqsMzyRZ942YAPAEREROH/+vNXByp3l6sW7ubkZhw4dQmJiIuLi4nDhwgUkJSXJP8ROnjyJqqoqXHfddaivr0d1dTXmzp1r9QcEBS5nKiDLh3M9AbvyZiHQWluCEqTaDuKZcRTgdTSf/IOjAHBPwL7n/wlptgLAUnmLDPgAsMFgwPbt2zF9+nT5pjS/tyXu7NmzVZ+zrjLfjoKCAowcOdKjvTY4Ux85YjQaFT/a1EhOTrZ4CEHWqTlWubm5KCgoQHt7u9x63fwhwNy5c9HU1IScnByEhobKDwWkISYqKytRVVUFDMAAcElJCQ4dOgStVou4uDi0t7ejvr5eEQC+/vrrFQ8NpHGU7d0/WnvLHWYPPsQ36Q8ePIjk5GSnXxB0B3cHn0tLS1FVVWXzYRG5nzPngbV7AyJ/pPaez5nzo7+5GrC7evUqysvLVfdmsn//fowdOxbJycmK9B07dmDYsGF2r2u+zlZeWqM2fyU5OTkYNWqURSAvNjZW7kEkMzMTp06dQlpaGubMmYOsrCy0tLTg7rvvVnzGk2zlgbP7q9bRo0eRnp4uD3/m6Txw17lsLfjb0NAAk8kkLmrh/PnzCAoKQlxcHDo7O8XZAIDq6mpER0ejoqICzc3NmDhxoriIrLKyEuHh4ejo6MDly5ddDgBb8/XXX+PSpUsW29HS0oLGxkZFsPfq1au4ePGixT1ccHAwRowYYTMIjN6Wz54I/sJO2Tb3+eefIzIyss8vGRcWFqK5uRnLly8XZ8ncWVe6qzyjj8FfvV6PuLg4rwbmyLOkxmgjR450eF7o9XokJibihhtuUKRLQWCpXlcrKysLxcXFXg/+AsBLL70Ik6kBGze+Ks5ym2XL7sTq1Q/jvvsse/JzlTvrCom1QCwAVc/opJfI3fVZBoDVURsAdtx3kB+qrKzE2bNnUVFR0afp4sWLOH36tLhap1VXV6OzsxM33HADUlJSkJSUpGhVYTQakZSUhJSUFNxwww3o7Oy06FaGyJ7mihKUIxkTxVa28eqCv0RAzwsDPa2102CvPUFzRQnKIxPsLhMoTp06BQAYO3asnDZ16lRERUXh4sWLZkt6VmlpKUJDQzF27FiMHDkSly5dEhfxWVqtFhMmTHBqUnNzSOoUFhaioKAA06dPx+zZs+UxgM3HBP70009x6NAhxMXFKR4KjBgxAs3NzaiqqkJSUpJivQPF2bNnodPpsGzZMixcuBBxcXHiIhYtKaqqqhx26yc9TDMf18pkMqGlpQURERGK+0Ap3dO91RAREZF7mAd/d+7ciaKiIsyePRtz5sxBQ0MDysrKFL8vAlFSUpIc/PWXPJCCv+Hh4Rg8eDDKyspQVlaGuro6dHZ2OpxmzJghH/eBpLOzE2VlZaivr4dOp8OUKVNQU1MjB3w9Gfwl+6TgL3rHAM/MzFQ1GQwGjs8c4KqrqxETEyMPY2bP0KFD0dXVJSZjxowZmDlzJi5duoS9e/eKs63au3cvLl265BPBXwBISUlFcfF5MdltpOHh0tLSxFl+Q+oZxmg0OpzMl3f1s+R+ARkARu+N99KlS/s0iW/A9VViYiKCg4Nx/PhxudWD+cNtrVaLqqoqlJaW4vjx4wgODuZDPnJCLQzlzUgYNgx2G2I2V+BUbi5ypelUBcw7ixbVluTiVIXlEs0Vp2ysoxkVp3JRUluLktxc5OaWoNbOesi9Kqx0R9XU1OTcyyTxqZghvkQgaq5ASXkk0lJ9q3WQW/bfCoPBgJEjR1oEJHU6HQwGg3yT4mnFxcXQ6XTQarVITU1Fe3u73CqP7DMajSgsLHRqcsdxLSkpsVivs1NJSYm4WqedPn0a06dPx9SpU+WWKfX19YogcGhoKK6//nqLt9WLiopQWlqKlJQUDB48WDHPltLSUjEJJpNJEej0N9LDD6PRaPXFj4sXL8r7l5ubC6PR6PAeMjY2FhEREYrgcXV1NbRaLWJiYhRlsLq6GhEREXKL4IMHD6K0tBR6vV7u9sxkMsl/6/V6HDx4UP48elsnFRYWIj8/3+YyziosLFR8p9QyRvoOcwcPHkR+fj5ycnJQXFwMo9EIvV7PeoyInOapez4id5GCv8beoTUuX76M9PR0jBkzBgDknkUctbjyZ7GxsVi2bJnf5UFxcTE6OzvR1NSE06dPOz0N5HrIXhCYwV/vqampgVarlZ87q50iIyN5rALciBEjMHfuXFXdok+aNEnuEUE0Y8YMLFmyBFVVVQ6DwHv37kVVVRWWLFniE8FfAJgyZQquXr2KoqIicZZb5OcfR3R0NGbM8N/er+bOnYtbbrlF9TR37ly3fJbcL2ADwL4gMjISaWlpqKurQ1FREbRareLNj7S0NGi1WhQVFaGurg5paWns/pnUq61DDRIwyME1u7muBfETZ2DGjBmYMWMiklGOUyW14mJ2NZefQglS7a6juaIOERNnOA4kkts0NTWhvLwcJ06cUKSdPn3a6a537WtGRUk5ItN869h6av/z8/PR1NRkdfgB6c1uqYWwJ5WUlKCpqUnuxjA1NbXfWyD7s/Lychw4cMCpyZVyI8nLy7NYr7NTXl6euFqnRUVFyd3b/N///R/Gjx8vt/yVgsD33nuvxQM48+Cv2tYZJpMJxcXFisCiNO5ScXGxYll/MW7cODQ1NWHz5s346quvMGrUKEUr4Li4OIwePRp6vR6bN2/G+fPncdNNN1m8NGJNQkICGhoa5L+rqqoQExMDrVarSDcajYiJiZH/Ru8DylmzZsldSF++fFn+OyMjA2FhYRbB1fLycmi1WsUy0thczsrvHatYWldaWpo8vtbUqVOh1WpRWFgImL0UMHXqVMycOVO+783IyAi4rpeIyLM8dc9H5C7mwd+dO3eivb0dixcvlscTPn36NCorK93e3bIv8ec8mDZtGqKiohAVFYUFCxbg1ltvdWoaMWKEuMoBRQoCt7e3Q6fTYfz48aisrERLSwuDv14yY8YM3HvvvX2afCVAR74vNTUVS5YsQU1NDfbt2yfOBgDs27cPNTU1WLJkiU/1lDBjxkykpqZi27Z/ibPcYvv2bbj11tvEZCKvCMgxgLOyslDhYBwIe86dO4cjR47gkUceEWcRuZ0zfdArxmerLUFuMZRj/6pRW4LcighMnNjTclgc49fa38VIwwzzPqWbK3DqVC3iJ07EsMiecWFr45XjBIvrIc+RHoaNHj0ap0+fRlxcnPyWtcTRGMA9alHSU6gUXYgry0AtSnIrEOFDYwA7u/+O7Nq1y2FXy1qtFt/5jvvH8TC3a9cuVFdX4/vf/76clpWVhYKCAixbtgw6nU6xvDs4Ux/ZsnXrVpffgk9MTFQ9bt1ApfZYZWVloaqqCsuWLQN6j097ezumTp3qluCvOSkAPGXKFBw5cgRJSUmqttET1OaPJxw7dgwtLS0232I1GAw4deqUHMTV6/WYNWsWAODIkSPyOMDi+L8HDx5EQkKCxXEzJ46zKwV6zcdsk4Lz4njDIimQbJ6P0rbaGqfYfN/0ej0mTpwo11XitpHnOXMe2L43IPId7rznc+b86G+2xrVUO2YrxwC+xlZeWqM2fyXSGMCjR4+WA59ffPEFOjs7kZGRIb/E1dDQgB07dmDs2LFeyUtbeeDs/tpjHvzt7zxw17nc3NyMo0ePAgBuvPFGREZGoqGhAZWVleKiFk6dOoWwsDAkJyejcwCNAWxu8ODBGDZsmKLb55aWFosxgd3JVtk2N5DHACayRa/Xo76+Xky2kJSUpKpcl5SUYP/+/YiKisLChQsRExODhoYGZGZmoqmpCYsWLfKp4K/kb3/7FH/4w/t46623+/T8w5adO3dg48Zf449//Ajjxo0TZ7uFJ+oKcQzgQ4cOobGxUVzMpujoaPkZiCuf5RjA6g3oMYCJSEnRfXNxjTjbociICDHBotvpyAgxhfrLlClTgN63qq09CHNJbQmKm5Mx0YcHlXbn/huNRly6dAmJiYkYP3681Umn08FoNLqlm15bjEYjDAYD2tvbsXXrVnmSWv9a627XV0ybNg0LFixwaZo2bZq4WuqjiooKxTi+zc3N+M53vmPxEMTV4C8AzJs3D+gNYnoz+OtO+fn58phY1s755uZmnDx5UpE2ePBgRUtekRQQNRgMMBgMcjfPsbGx0Gq1qK6ulsf/lYK/kgjxeix0yVxcXIy2tjbFfLEVsRS8deYHGczGLT5y5IiiC+iWlhZ5GZ1Oh6SkJOj1eiQlJXnkRRUiGrjcec9H5A5RUVF2A5/oDVJFR0ereojujxwFf+EneRAZGSkHw48ePYrm5mbExMQgNjYWzc3NdqfGxkbF/dBAYy34O2PGDIsxgYnIN8TFxSEpKcnm1N7ejurqatW9G6SmpmLRokWoq6uTfzMaDAbU1dX5bPAXAO677zsYPXoM/ud/Nouz+qyyshIffPA/+P737/dY8Le/SM8LpO7k7U3my7v6WXK/4HVPP/2SmGius7MT7e3tGKxicHB3uXDhAjo7O+W30O21ThCFhISgrKwMDQ0NfX6AWVNTg/Lyco+9pUZk7sqVKxiq8vyqr683e/jbgrpKE0LjByM2VFhQVouS3FO42DEEE28Yh1HJyUiObEVFQwgGD45FKICWugo0hAzG4N6VOPq7RwvqKhoQMngwYkM70FBZiY7YZMSbxYCtf448ZejQoWhvb1d0M2+upaVFrlOV5chcC+oqaoF46Vg2o6LkIkzNJlRWVKCiogIVFbVoRgdMlRWoaI1EsvlB9yJn9t+eY8eO4erVq5g3bx5uuOEGXHfddRaTTqfDyZMn0dHR4bEHjwUFBbh8+TLGjh0rd0cWFRWF2NhY+WZcegjqTs7UR7bEx8db/IBwdlIzHs1Ap/ZYVVVV4dy5czCZTDh69CiSkpIsfoC5I/grGTlyJFpbWzFp0iRxVr9Smz/27Nq1C5cvX8bQoUMRGhqK5uZmResoqaVIS0sLBg8ejNDQnutdTU0NampqMHr0aLO1KVVXV6OrqwstLS0IDg6Wt9VoNKKpqQldXV3o7OxUfN+lS5cQGxurqMsOHjyIzs5OzJ8/H6mpqdBoNDCZTBg5ciTQ2/1zWFgYksxeAkDvW9qDBw+2CA6bu3LlCtBbv6K39U5lZSUyMjKQmpqqmMy3qba2FiaTCYMGDVJ8b11dHZqamixamJHnOHMe2L43IPIt7rrnc+b86G/SGPPx8fEwmUzydPnyZVy9ehWNjY0W4zaaT3V1dWhoaEBnZ2fv/bvlVFdXh/b2dphMJtTU1CAiIgKtra2K7zt//jwSExNVtaj2Vbby0tpUWVmJmpoahISEoLGx0eEUGhqKW265Re7yuKOjwyLwmZWVherqatxyyy12r7medPHiRavPx+rr61FeXu5Uj3sisdtnb+SBO8/l0NBQDB48WD5PBg8ejLi4OGg0GhQXF1uUAWkymUwAgI6ODot50mQ0GtHe3o6WlhZ0dHQAvQ+8rU1GoxGtra3o7OxES0uLyy9VGgwGlJWVKeqJixcvyvdsYh1SU1ODuro6+e/6+no0NTWh0UrdM3HiRKvB36ioKMTExCA6OhoXLlxAXV2d2+8B1ZzfFy9eRFBQkFzfOTs1NTWho6MDgwYNspgnTe6sK91ZnolsSU5OtnjOJU3h4eEoLCzExIkTnXrmFB8fj9zcXAwfPhwJCQlybEVqTeqrxo0bhw8//AAmkwkzZ/b0yuWK9eufBQA8/fRPER0dLc52G0/UFZcvX0Zra6t8j11cXAxtb0vc4cOH252qqqrc+tnw8HAMHz5csX2u8kSeedvVK1cQHh6OoKAgaIKCbLYAZgDYCgaAqT85UwEpHs6FhqCjrgLl9oJwzXWoqAzFqBtGQjqLmusqUNkS6VQAuLIjVvkdtQYU14Zi8Kh4RIIBYF9h72FX3wLAoYgdnIzkZPMpEq0VLYifeAPGDbZR7rxE7f7bc/DgQYSHh2PBggXiLFl4eDjKy8tRWVnpsZaq2dnZCA0NxZ133mlxQ97S0oJLly4hKirKIqjjKmfqI19VUlKCK1euWDyccGYymUwuB6GlVuLiuu1NYWFhCA8PF1dlldpjdd1118HU+2AnKSkJixcvVsx3Z/BX4u5y2Rdq88eW/Px8XLhwAXfeeSdSU1PlOlBirZtAyenTpxEVFWX3B0tbWxvq6urQ1taG+Ph4uX7q6OjAhQsXEBwcjMjISEVeigFgg8GAiooKzJ8/X17GYDCgublZEQCGWRBXWqaystLhD3oxANzd3Y3y8nJERkbafIBrMplw5swZzJo1C2fOnEFSUpJcphkA7n/OnAe27w2IfI+9ezq193zOnB/97eLFiyguLoZGo5FfKpKeUbS0tKC5uRlNTU02p9bWVnR1daG6uhqVlZVWp7q6OrS0tKCmpqd3KFNvINh8unz5MoYPH+6WoIa32MpLa1N1dbUcBK+vr7c7hYaG4hvf+IZivFsx8Hn69GkUFhZi9uzZGD16NEwmk+r7PHfyVABYDP6qyQNPcOe5bDQaERMTYzUIXF5ejtLSUhiNRhiNRtTW1qKyslJ+cc9RgFG6D+rq6kJXV5fFfPOppqYGTU1N6OzsRHBwMCZPnixuqlOOHTuGI0eOoLS0VJ6qq6vR2NhoUbaNRqO8HVJaQ0MD2tvbLZaNj49Henq61eBva2sr0Nv6y1NBYDXnt8lkQnNzs8W2q51aW1uh0WjQ1tZmsW5pcmdd6c7yTNQXe/bsQXh4OG699VZxlkPWAsC+HltJTEyEwWDA3//+N7S0tPQ5CFxZWYmXX/4lzp49g1dffR2jRo0SF3ErT9QV1gLAagOx3vqsMzyRZ96mNgDMMYCt4BjA1J+c6YPecny2njFbayKT5TF9e5JLUIJUpEaYj9Urjd1bjmaz5cWxeq39XVwDJMjjwvZ8Z3OytEzPGMAtwyzHjeUYwL7DlTGAlXxvDGA11IwHV1JSgq+++gqTJ0/GnDlzxNkK+fn5OHz4MKZPn+72G1qDwYDt27fb3Y6PPvoIOp0Ot99+uzjLJc7UR77KV8YgLiwsxIEDB8RkuxYsWGDRNbMt7jhWngj++gpX8yczM1N+kCmyFfytra2VW1tPmjTJ7o8LU+84vAAsxtTV6/UAoBg/F8JYuzBbh7Sc9HdERITcHXdOTg6MRqNiXWrGEoaNMYCl9Znni3lem6+7sLAQDQ0N8nhxpaWlKC4utpqn5BnOnAe27w2I/Iuaez44eX70N1vjWl64cAFHjhxxeczWkydPYuTIkfKLjBwDuIfaMXGlwCcAbNu2DbW1tbj11lsVgc+LFy8iKysL48aNw8KFC3H27Fk0NDQ4XLcn2MoDtftrTV/ywFPceS5nZmYiLCwM6enpVu/3Wltb5aE2ysvLUVRUhEWLFglrsc7WeWaNu889W2XAGrX7Jb24aiv429bWBo1Gg4iICISEhMBgMODEiRNuHRNYzX4dPXoU0dHRGD9+vDhLlTNnzqCxsdHueeLO4+XO8kzkrMzMTBQXF+P222/v01A+77//PmbNmoUxY8b4TWzlb3/7FG+99Sbuuede7NmzG1OmTMVDD6126vlIZmYmPvigpxvpp556GjNm2B4v3V08UVeIYwA7Mxavtz7rDE/kmbdxDGCiASEeqTMmIhnlOCWN8Zubi9yKCOjiAUQOQ2oyUH6qN70ESE1LEFfiUGRyGiIqpPUXoyYhjYFdCjjS+J7imJvWTJ06FaGhoaioqBBnuezUqVOAg+3Q6XS4dOkSjEajOGvAu/fee7F69WqXJleDvwAwYcIEi/U6mhwF5NwpkIO/7lDf27rHmry8PLmV1YEDB7Bnzx7s2bMHOTk5aGpqchj8Re+D04iICHn8X3PSODiOfnTHxsYiOTkZp06dgl6vx4kTJ6x2iZqcnIyysjJ5zN6YmJg+l7WZM2dCq9UqxgCWtjcnJwfoLfvSv0ajUQ4kp6SkICIiAnq9Xk4jIiLyJ+aBz507d+Lq1auYMWOGIvDZ0NCAvLw8DB8+HAsXLkRHRwcKCgrkbn+9oampCUePHlVM586dQ2trK06dOuXUVF1d7XQe+JMLFy6gtbXVYkxg9PYEZev+cCBRE/xFb8MiqctrnU7HMYGJfFhJSQnOnDmD8ePHO/wdGiik4O/atU/hmWeexbvv/jeampqwdu0a/OY3b6CoqEj8iEJmZiZefvkXeOGFn0OnG4bf/Oatfgn+EjmLAWAivxeJYRNnYMYMs8msNXDksInK9PhUxfz41BmKYK71v+OV36FoHtrz/WKLUXE95A/ikTrD8lgq9bx0EIiHNjU1FTfffLPqm92bbrrJI2MAq9mOuXPn2u2mmsgeBn8dS0pKQlVVlZgMAEhLS0NwcDCioqJw/fXXy9PUqVOxaNEih8Ffybx58+SWuuZmzpxptZXsvHnzLF4MmTBhAjIyMpCRkSHPt7fOjIwM1W+9Tp061eqy5uvKyMiQt2nmzJkW3y1+37x58yzSiIiI/EFERIQi8Hn58mXMmTNH0c1jQ0MD9Ho9QkJC5GtiWVmZV4O/ABAcHIzo6GiLSepiUe00YsQILFmyBHAyD/xNW1ubIggs9ZDR3d3t9WPpS4xGI4KDg60GfyXWgsCtra1oampSLEdE3nXkyBEkJiba7IUu0JgHf++77ztA73jAv/vd7/Hww4/gxIl8PPzwQ/jOd76Nl1/+BX7/+9/J04YN67Fs2Z144YWfo6mpGa+8shGbNr2BIUOGiF9D5BMYACYiIuoNvEoPddRITU3tcys6e9Rsh1arxYQJE+SWd0RqMfirzsSJE2E0GqHX61FYWIj8/Hy51erQoUMxadIktLa2orKyEiNGjMCIESNUB36JiIjIf8TGxmL48OHy/fmuXbtQXl5uEfhEb28YwcHBWLp0KbRaLS5fvuwTga7w8HCMHz9eMY0aNQpJSUmYNm2aw2nmzJmYM2cO5s+fDziZB/7KPAg8adIkdHd3o7GxEd3dVkfRG1CkvNHpdJg3b57N4K9ECgLX1tYqPkNEviEzMxPNzc2YO3euOCsgWQv+mrvvvu/g44//hLfffgff/OY9CAoKUvSEodPpsHr1w/jjHz/Cpk1vOOwyn8jbGAAmIiIicpOSkhIUFha6NEndkXuCVqtl8FcFrVYrdwV++vRpXLx4UdFVsxQErq2txbFjx8w+SURERIEgODgY1113HVJTU5GYmIjQ0FDo9XqUl5cjPT3dIvC5b98+VFdXIz09HVqtFlVVVaivr1cs4280Gg0iIyMRGRmJ0NBQaDQap/LA30mBTgZ/LUl5A8Bu8FfS3d2NvXv3evR3DhE5T+r6efr06XZ7oQsUjoK/5mbMmIkHHvghXnrpl/jd734vT8888yzuu+87GDdunPgRIp/EADCRnwkK4mlLzrFWZqylBaqBtK/kfXl5eThw4IBLU15enrhatxk6dCiDvypptVpkZGTg3nvvxbJlyyxa5ktB4JaWFjQ3Nyvm+YqZM2d6pKcCCky8XpK/YxkmdwkODsaIESMQFxeH8+fP49///jc+/vhjnDlzBlFRURaBQCnwuWjRIqSmpqKqqgpXr15VLONvNBoNIiIiEBIS0qc8CBRtbW0M/trQ1taG7OxslJaWirOs6ujoQFlZmZhMRF505MgR6HQ6twzR093djezsbHzyySfIzs72uXrTmeAvUSDhLyQiPxIREcEHG+S04OBghIeHy38PtHIk7j+RJ917771YvXq1S5PU8pR839ChQzF37lxERgbgwOg0oAy0ewMKTLznI3eJi4tDXFwcTp8+jezsbLS2tmLEiBG4/vrrERoaiuPHj6OoqAiwEvhsaGjw++AvAISEhCAkJKRPeRBofC2I4UsqKyvFJCLyE3q9Hs3NzbjpppvEWX2yaNEiLF68WJ58qWtkBn9pINMYysqs3sl0d3eju7tbftttohveBFFr//79aGtrw3XXXQcAGDZsmLiITREREcjKykJFRQWWLl0qzlbl3LlzOHLkCB555BFxFpHb5efnq37TymQyyecmkVrBwcHo6OjAoEGDgAFYjsT9J9ucqY/Iu3is7GP+EDl3Hgy0ewMKTM7c8zlzfvS3zMxMlJSUWDwHqa+vR1VVFeLi4hTpzmpqakJ4eLg8dv358+cxePBgiy57KyoqkJqaioULFyrS/YmtvLSmqalJHqP0jjvugMlkwo4dOxAZGYnRo0crlj1//jwaGxvR2dmJ9vZ2OfB58uRJlJSUWNSldXV1GD9+PGbPnq1I7w+28qClpQVGoxFDhgxRpANAVFQU5s+f36c86G/uPJdt5ZU1RqMRlZWVFvlii63zzBp3n3sDeb/KysoQFhZmtZyrcfXqVbS1tWHEiBHiLJk798ud5ZnInsLCQhw4cACzZ88O+DIXiMFfT9QVhw8fhtFoxC233AIA+PLLL4HentEcMRqNAOC2z2q1WrffM3kiz7yt4PhxxMbGIiQkBEHBwdCIC/QKXvf00y+Jieakm7nBvT8O+sOFCxfQ2dkp/3ALCQlBR0eHqiksLAzl5eVoaGjocxeHNTU1KC8vx4wZM8RZDv3hD39Abm6u1en8+fMYOXIk30omhStXrsg/vh0JCQlBXV0dYmJi0NnZKc4mshAWFobGxkbExcXJLXsGUjmytv9kmzP1EXkXj5V9zB8i586DgXRvQIHJ2Xs+Z86P/lZVVYWmpia0trYqpubmZrS3t6O9vR1tbW19nsyDk62trejq6kJQUBA6OjoU3xcWFobBgwcjOTlZsX3+xFZeWpukZ1CjR49GYmIijh49ipqaGkycOFFcLSIjI1FaWgqNRoPly5dDp9Ph0qVLOHv2LDQaDYKCghRTVFQUEhMTvVLmbOVBZ2cnQkJCLNJbW1sxevRoJCQkOJ0H3uDOc9lWXlmb2tvb5c+J86xNts4za5O7z72BvF+dnZ3QaDTo7Oy0mKdm6ujogEajQVdXl8U8aXLnfrmzPBPZYjQasX//fiQmJrrlxQVfFojBX3iorrh8+TJaW1uRlpYG9H5He3u7RZ1nbQKA6OhojBw50uXPFhcXIzw8HMOHD5e3zR08kWfedvXKFYSHhyMoKAiaoCCbAWC/aAHsjCFDhuDEiRNeawH8/vvvY9y4cVbfyj116hRCQ0Nxxx13qHoDggYGZ99AaW1tRU1NDaKjoxESEoLOzk50dXWJi9EAJj1oQO+NXXx8PCIiIhTLBHI5UrP/ZJ2z9RF5D4+VfcwfIufPg0C+N6DA5Mo9n7PnBw0sly5dwv/93/9hyJAhNh9AHj58GDNmzMCUKVPEWQHBX/KA5zIFElfL82effSYmueRb3/qWmEQBQK/Xw2AwYNmyZQEdnwjU4C/cUFdYI7YA9ha2AFZPbQtgBoCtcDUAPGvWLIwZM0aRHhISgoaGBpw8eRIJCQkBV+Co7/pSAXV3d6O+vh6NjY3o6OgQZxMhJCQE0dHR0Gq1NltBBHI5UrP/ZKkv9RF5B4+Vfcwfor6dB4F8b0CBqa/3fH05P2hgOHHiBE6ePInIyEibvcpdvXoVly9fxq233trnrmV9mT/lAc9lCiSuluf3338fOp0OkZGR4iynNDc3w2Aw9Om5OPk2qetnNcaPH++3LYQDOfgLN9QV1jAA7H/8PgBcVVWFsLAwcZZDEyZMgMFg8LkAcEREBKqrq1FXV6dIN5ecnBzQb96QdYFYARGRf2J9RIGCZZmI5wGRPTw/SHL69GnU1NSgubkZdXV1aGpqQnx8vM0xUJubm3Hu3DnodDosWrRInO2X/DkPeC5TIHG1PNvrldIZ9fX1OHv2bJ+ei5NvMxgMdmMT5gYNGuS17v1dEejBX7ihrrDm8OHDuHz5MmJjY8VZ/cpkMmH48OEMAKvg1wHgwsJCtLS0iMmqjBw5EqdOnfLJAHBWVhZOnjypSJdoNBrEx8eze+gBKBArICLyT6yPKFCwLBPxPCCyh+cHmdu/fz8uXLgAjUaDMWPG2Aye1NTU4PLly4iKisLixYu9/pDUnfw1D3guUyBxtTy/9957YpJLHn30UTGJyKcNhOAv3FBXWHP+/HlUV1eLyV6RmJho8yW0vvJEnnmbXweAXZWZmYmLFy9i4sSJ4ixVXHnTyVEA2Fpg+ty5c8jOzkZ4eDiio6OdCgKXlpaiuLhYkZaRkaH4m3xbIFZAROSfWB9RoGBZJuJ5QGQPzw8SHT16FOfOnUN7ezuio6MREREhjynd1NSExsZGtLW1QafTYfbs2V4PfHqCP+YBz2UKJK6WZ1vPpJ3lqGFUTk4OjEajIi0tLQ0pKSnIz89HVVWV/Gw6Pz8fAOT9Ev8mcqf/+q93MWTIkIAO/sINdcVAFIh5pjYArH6QHD/T2NiII0eO9Gk6e/YsNBpbWeY5s2fPRmNjI3bu3GlxIbXm4MGDKC8vR0ZGhjylpaWhtLRUXJSIiIiIiIiIiKy48cYbsXTpUkydOhVxcXFoamqCwWCAwWBAZ2cndDodbrrpJtx8880+Efj0BOYBUWCrqqrCsWPHxOQ+SU5OVjyPTklJAXoDu2yYRN7y+ONPBHzwl8hZAdkC2JtsvW2lpgXw/fffj4sXL+Lw4cMOWwLn5+ejoaEB8+bNE2eRnwnEN1CIyD+xPqJAwbJMxPOAyB6eH0SBgecyBRJXy7OtZ9KSiooKnD9/HgsWLBBnKahpARwTE4MJEyaIsyyILX7Fv0WlpaVyMFliMpnQ2Njol+PREnmCq3XFQBSIeTbgWwD7o3PnzqGtrQ2pqamoqanBzp07xUVkVVVVSEtLE5MtFBYWQq/Xy5N0oZXk5OSgsLAQ+fn58jIHDx5UzBc/U1hYiJycHEWaO1lrwWwymWAwGMRkIiIiIiIiIiIiIvKy/Px8i+fIaplMJhQXFyueS5tMJhw5csRi+EMiIlKHAWAfkp2djezsbBQWFgIA6urqxEUAQA6EOnrzKT8/36KL6IaGBosLcXl5ObRarbxMWFiYHOBNSkpCQ0ODYvmGhgYkJSUp0tyFF3siIiIiIiIiIiKigSM2NlbuPvrgwYPy8+CkpCT2gElE1EcMAPuAMWPG4P7771dM6enp4mKylpYWMcmqqqoqTJw4UZGWlpaGqqoqmEwmOU2r1Sq61xg/fjyMRiNMJhNSUlLQ0tIiB51NJhOMRqNFdxzuwos9ERERERERERERkW8qLy9X9Dhp/pzZVdLzX+l5cKB120pE1J8YAA5QtloJS383NjbKaTExMWZL9ARhYbZMUlKS3Br58uXLHmv9a44XeyIiIiIiIiIiIqK+OXXqlNWh9uBgniPJycmKHielZ8nuMm/ePCQnJ/N5MBGRixgA9qKSkhKcOXNGMdXX14uLWUhMTATMgryeNmTIENTU1AC93T9rtVpxEY/gxZ6IiIiIiIiIiIjIeVFRUSgrK7MI9J46dQp1dXUWjYJ8yYQJE8QkIiJyEgPAXtTU1ITGxkbF1NbWJi5mITY2FlqtFmVlZeIsWXR0NGAlSGytZbD4neIyOp1O7gbak90/W8OLPQUqcSzuQBGo+0Xka3iuERGRNbw+EBERkSQlJQUjRoxAWVkZamtrAbPg77hx4/qll0ciIvIeBoC9aNKkSbjxxhsV0+DBg8XFrJLG6c3JyVGkl5aWorS0FLGxsUhKSsKpU6cU84uLi5GcnKxIq6qqUgSKrS2TlJSEsrIy3hgQERERERERCUpLSxXjIer1enERtyssLFQ8E8jPz3f4vWqWcbf8/HyXXk7IycmxyFuxNRv1nStlVzy24t9E7sA6wDVSEFjq3ZHB34FHuvZLkxhP8DRPn7srV67E2LFjFdNf//pXAMD69esxduxY8SNOeeutt7By5Uox2YK17/dVBw8exMGDB8Vkm8R7TmvULAMv3YsOZAwAe9HRo0exf/9+xVReXi4uZlVsbCwyMjIAoRItLy+XW+hOnToVycnJivkJCQkWrWqTk5NRVlYmLxMTE2OxzJAhQ2A0GjFkyBBFOhEREREREdFAdvDgQZSXlyvGQ0xLS/PIQ057pk6dKj8nQG9gT3wQJy7jL8TxJvuzZzK1rOW3r/OVskvkCOsA10hB4KCgIAZ/B5icnBy0tbUpzp+wsDBxMaepLe85OTny+Ttr1iwUFxfDZDKJi7ns8ccfR1FRkTx997vfBQC8+uqrKCoqEhd3u5UrV8rb8MUXX+D555/vl+/tC/OGgGLvsf3BX+9F/ZVPBYCtvdHliQrB006dOoUdO3YoJms3zyNHjrR4OyUhIUFczK6ZM2cqKvB58+Yp5k+YMEExXwzsSszXY23M3ZaWFkRERCi6jiYiIiIiIiIayKTWjuJv8ZSUFJ8MUBBJWHYtBUoL5sLCQovnq3q9HoWFheKiDgVKnlDPuX3jjTe6HPydOXOmzefLU6dOVTxXdvQ3eZbJZILRaMT48eMV6f15DNra2jB8+HDAbFjLxsZGcTG/V1ZWhrvuugvobQmcnp6uuqFff7t69SoSEhIQExODq1evirMpwGgMZWXdYiIAdHd3o7u7G21tbWhsbMTEfqgYcnJyFK1PCwsLUV5ejlmzZiE2NlZcXJXS0lJUVVVh5syZ4iyPyMzMFJOA3hO/qKgIFRUVWLp0qTjbwrlz53DkyBE88sgj4iy3EvPcloMHD1ptPUyuy8/P79cLL/mGQD3ugbpfAwWPn//gsbKP+UPE82Cg4nFXx535pNfrMXHiRIcvS0vPNyRJSUmKbTh48CCSk5NRXl6OlpYWALB4FpKfn4+qqioAQEREBBISEtDQ0CA/75CCNFOnTkVOTg6MRqP8Wen7zJeRuLptJpMJR44ckZePiIhQBBWtfaczHD23ULv9xcXFAICMjAx5nQ0NDXI+TZw4EdHR0Yp9MW+hYm8/beW3yN460NsSx3woL7EMuFNfy675NonHVvzb09x5LsML22/Onc8vCwsLFXWDRN/b5aYzLa+czRN37ockkOoAe1wtz++//z50Oh0iIyPFWU5pbm6GwWDw+DNp6h96vR5paWl2X+xx9hzSarWqy3t+fj7CwsIwYcIE+RonnVfSSym2zm21Vq5ciZkzZ2Lt2rXiLKxfvx7obQkMAIsXL8aPfvQj/O53v8Ply5cBAF988YWim+j169fj888/BwAMHz4c99xzD3JycvDxxx/Ly4jWr1+PYcOGYe3atdi/fz9Wr14ttwB+6623AMDq9vWFq3WFXq/HrFmz0NjYqDge5hzdc6pdxhrxuuLoPtMd90au5pkvKjh+HLGxsQgJCUFQcDA04gK9gtc9/fRLYqK5zs5OtLe3Y/DQoeIstysvL0dYWJj8JlJSUhIqKirQ0dHR57eT6urq0NTUZDGmradcd911VqeYmBhcvHgRtbW1CA4ORk1Njd2pvr4e1dXVmDFjhvgVbiXmuSg/Px8nT57EoEGDMGnSJHE2ucGVK1cwtB/OL/Itjo7773//ewQHB6OgoAC5ubkYNWoU/vjHP/YprT/PXUf7pYZer8dXX32FCxcuYPjw4QgPDxcX8Ru7du3Cvn37kJycjJiYGHG2z3HH8aP+wWNlX1/y5w9/+ANyc3NdnkpLSzFx4kRx9UT9ri/nAfk/Tx33kpIS7NixA9nZ2airq0Nqaqq4iFvk5uZiz549OH78ODo7O+Xf8e7+fnflk8FgQGVlJaZMmSLOUsjPz8eVK1eQkZGB1NRUpKam4vz586itrZW349KlS6isrMT06dMxYcIEmEwmlJWVYeTIkfI6GhoacNNNNyE1NRWhoaEoLi5GeHi4nE9XrlwBAAwdOhTJycnQaDTo7OzE/Pnz5e8xX8Zd21ZSUoIJEyZgwoQJSE1NxZUrV1BVVWXzO51l77mFM9s/a9Ys+SFzeXk5qqqqMHr0aEyZMgWtra0oLi5GTU2NnMfV1dWK/bC3n7byW2RvHSaTCcePH5e3MzIyEmFhYR75PeRM2W1ubsb8+fORmpoKjUaDkydPyuegeGzFvz3NXeeypL+335w7n19WVVWhra3NYl2pqamoqKhQnB+OOJsn7twPSSDVAfa4Wp5LS0vR1dWF1tZWl6auri5ERUXxN02AaG1txcWLF2EymayWr76cQ86U96FDh+Ls2bMoKiqCyWTCTTfdJM+TgofWzm1nfP7550hOTsacOXPEWfjyyy8BALfeeisA4MMPP8Q///lP/PWvf8VLL72Ey5cv43e/+x0eeOABoDeQm52djaNHj2LNmjVITU3FCy+8gBEjRmD58uWKdZu79dZbsWHDBvznf/4ncnNzcfToUXleVlYWAFjdvr5wpa4oLS1Fc3MzxowZg5iYGFRUVKCzsxODBg2Sl1Fzz6lmGVvE64q9+0x33Ru5kme+6uqVKwgPD0dQUBA0QUE2A8A+3QLYPG348OE237KCjTcBzpw5Y/NtFPHNlr68OeCszMxMnD59Wky2SaPR4OGHHxaTKcAE4hso5Jij437s2DHodDo0NTWhpaUFo0aNwrlz55xOa2trw/XXXy+u3mMc7ZcjJSUl+OqrrzB79mwUFBQgLS3NbTdI3vDRRx8BAMaPH+8X++Hq8UNvAL++vl5MdkpcXJzVNxDVGCjfr+ZY9de22OLN71eTP6L3338f48aNQ1xcnDgLAFBfX4/KykqMGTNGnCW7dOkS2tvb8a1vfUucRdTv+nIeBDqj0YhTp06hoqIC6K1j7LV+y83NRUVFBZYtWybO8lnOHPfm5mYUFxerellw69atGDZsGCZOnIjt27dj/Pjxbn9Z2Wg0YuvWrfKDwa+++grLli2DTqdz+/c7k0/2lJaWori42OG1ylpLS+kZhvQsQux1S2wlY20d+fn5aGtrs9oCGDZa4onLWFuvs9smEr9X/E5niS3rYPYMpy/bj951hoWFydsktewzbyVVWlqK8vJyiy6SJeJ+in+rYf4ZR/nqTs6UXfF5mdRSJyUlxeLYin97mrvOZYm4/a60SrL33NGV1nRq2GoBDBvH3t62inlib3nxXHXXc1hxvQigOsCcu8szkcS89XpycrLiXOjrOaS2vOv1emi1WowYMQKnTp1S1As5OTkYMWKEzXtxtVauXIns7GxFmtSq11oL4HvuuUdujSu21h07diw2b96MRYsWyetav349Ll++bLcFsNTt88MPP4zVq1dj+fLl8neuXLkSDz/8sGKdrnClrhDjb9auF9bKhHjPqWYZW8Trili+zO+H3HVv5Eqe+Sq1LYB9agxga9ra2hAREYHLly9j1qxZyDAbrFwqLCaTSa6UMjIy5DeUZs6cibS0NGi1WmSYjW2b3/uGgrSutLQ0RXDZUxYuXIhHHnlE9cTgL7kiNzcXmZmZiik3N9fiprk/ZGVlWWyLJ7cjMzNT7kZEJLXQ8nVVVVVoamrCkCFDMGrUKACQ384aMmQIIiIikJWVpUgTlzMajaitrRXW7NtMJhM6Ozsxfvx4REZGor29XVzEb+Tm5iI0NBTjx4+Xf9gPBHFxcUhKSnJpshWAU2Ogf785b2+Lt7+/L+Li4jBmzBir07BhwxAZGWmRbj652t0aEXmO0WjEzp07UVxcLNcx9fX12LVrFwwGg7g4DAYDCgoKkORiiwQ1DAaDfL8s/cb1tObmZhw9ehR1dXVobm4WZysYjUYYjUbMmTMHWq0WaWlpcosNdyotLUViYqLc+kSn0+Hy5cv99v2eIpUv8eGm9Lf5OHgRERHy/6Ojo4He+2Nb6wgLC1P87Sxb63Vm2ySFZmOOFhcXo62tTZ7nDsnJyfIznIyMDMTGxvZ5+yXm+ScFoqwtZ84d+2lrHTqdDhEREdDr9SgtLRU/1u+k/D1y5Ii8vXq9Xg6EDhTFxcWYMmUKMjIykJSUhBMnTgB2nkVC5XPH4uJi+bO2nl96QmJiImB2fNVsqzl7y9vaD3ufUSuQ6gCi/hYbGyvXU+Xl5cjJyQFcuA9QS3rZZebMmdDpdMjIyEBDQ4N8v2s0Gi2+u68ef/xxFBUVyZN5l86iYcOGyf+XWqsWFRVh//79AGARqDVf3prFixfj8ccfx8cff4xFixahqKgI2dnZcvA5OzvbYp3eYOodE1oakxkABg0aBKPRKN/T2SoT5vWlmmXQGyQ2n8zvG0W27jN97d7IH/l0AFiqDFJSUjBhwgTFm2FJSUnyRVaqjKT5Op3O7ltkVVVVisHPU1JSEBERwUJEAeXixYs4c+aMYjp27Bi2bt3abw+WYNZy4tKlSyguLkZVVRWioqKg1WrFRd3mzJkzqKysFJOB3ny5ePGimOxzamtr7f6wbmlpcRjcbWpq8mig3d1KSkqQk5ODYcOGoa2tDZ2dneIifqWiogI6nQ4pKSloampCSUmJuEhAmjFjBhYuXOjS5EqLnoH+/ea8vS3e/n5naTQaGI1GVFRUWJ2MRiOCg4Mt0s2nlpYWv6+7iCSFhYVunbzt0KFD6OjowLJly+Q65t5770VkZKT8EMxcTk4OtFqtx3vwyM3Nxfbt21FQUIAzZ87g8OHD+PTTTz163yAFfwHgxhtvdPjySnl5ueLefdCgQWhqalIs4w719fWKF3/i4uLQ1NTUb9/fF2IgZaA6ePCgRXAnELljPx2tY968eZg1axaKi4sdPix1hTNl1zzoJk32xpIMNMnJyfIzxiFDhsi/0+09i1Tz3NF8vf1J/E4122rO2eXRx8/4IkfnL5Gv0+l0mDVrFoxGo6r63xUmkwktLS2KYCN6r3NVVVVycNjfFRUV4fLly7jrrrsU6fv27cPnn38uB4d9gTTmsfmLXVIvFtI8dxLvHcTrj1r9dW8UqHwuAFxeXi4XwIaGBkU3G4U23rJy5k0AvsFIA8348eOxevVqufu09vZ2HDt2TFzMY2bMmCE/XEtMTMS9997brw/0/dXSpUvlFr3WjBo1CkuXLhWTFaZOnYqFCxeKyT6ppKQEe/fuRVJSEpYsWQIA6OrqQkdHBwDgxIkTOHz4MK5evSp80jcZDAYYDAa59YpWq8XZs2fFxYjIh2g0GlRWVuL8+fNWJ6m1mZhuPjU0NLAVAAWM/fv3Y9++fW6ZpLfpvclgMMitksyNGjXK4gFYfn4+DAYDpk2bpkh3t8LCQqv35UajEYcOHfLIi3zOBn/JvtjYWGi1WpSVlYmzZFIrBrGc2Wo9YY21FrcA0NDQoPjbWe7YNoPBgJaWFkV3f/31fMUd26+WO/ZT7TqkllpardYjD2ThYtkdaJxtlaT2uWNfWtO5g1SPREdHq95WibPLo4+fUctWGfXVOoDIF5gH4frzHDInvTxh3qW0LzBvDWzO2suiavzqV78CALm7aW+rqalBWlqaRWA2OTkZNTU1gMp7TjXLuFt/3BsFKp8LAJt36WEe/HX0lpWzbwKIBT1jgL3BSAOPTqfDmN5xC73Rra7RaOyXLvQCxSeffIJz586JybJz587hk08+EZMVsrKy8O9//1tM9jnWgr+Sjo4OZGdn49ChQ7h48SK+/vprXLp0SbGMLyoqKkJUVBRSU1MBs4fLnniQS0TuM3jwYCxYsKDPU3h4uLhKCzk5OQ7vVfV6fZ9/ZPYH84d3jl6+tKa0tFSxDr1eLy5CPkCj0SA9PR3333+/S1N6ejo0GlsjEvWf9vZ2DBo0SEy2SDMajSgoKMD48ePl67inXLhwQUySNTU14fjx42Kyy/Ly8tDU1ISmpiYcOHAAe/bssTnZCwzRNePHj4fRaLSot0tLS1FaWorY2FgkJSUpxglFb/evalu+SME6qetZ9K5fzb2lvWXcsW3iw2OTyaQY59OT3LH9aqndT3v57Wgdht6XSCXSkGieoqbsarVai/ztzx7FfJ29Z5HiM0dfee5YXV2NiIgIRRBI3E5H2you62h59PEzjvhbHUDU30wmk0WdLfXMI/Va4Mo5ZK+8S9eQM2fOKNLz8/NRXFysGN7TV5iP4yv561//ajG+sDnpM7/4xS8U6evXr8fzzz+PESNGyF1Be5P0EovUA4i54cOHo6WlBQaDQdU9p5pl3KW/740Ckc8FgK1R+5aVmjcBxAs20UAidYscFRUlzvKokpISmw/dyLr09HS7b9rpdDqkp6eLyQppaWmYMmWKmOxT7AV/JTExMWhpaUFNTQ06OzvtBsZ9xaVLlzBy5Ej574kTJ6K9vd3iLcJApNfrsXXrVtWTpwI/JSUlFt/laPJUd5vezpPm5macPHlSTJbZ2z53bsvJkyetjjPZX9/fF0VFRVbvOdHblV1fgp8SW/eqrqyzP+Tk5MgvbEoPPO0Fs0UHDx5EeXm54uFfWlqa2/a7tLTU4kE2ue7cuXPYsWMHduzYIQ+lcfXqVezevRu7d++We+i4ePGivJwvXq/NxzGzlSaVnxtuuEGR7gmOujGuqKgQk1yWlpaG4OBgREVF4frrr7c7SQ+IkpOTFQ90ysvLPfJiZ1xcHOrr6+W/KyoqMHjw4H77/r6SnkNAeEGmvLxcDm5MnToVycnJivkJCQlOtXyRnodInzcajQ4fzkrdrOr1epsPWV3dttjYWCQnJ+PUqVPQ6/U4ceKExQv7nuTq9qulZj8d5beadUjz9Ho9YmJiXA6Q2aOm7M6cORNarVYxX+xJYaATn0X6+nNH88COs9vq7PLo42ec4U91AFF/i42NRVVVleL8qKmpket+uHAOqSnv4r2Lvvf3/f9n797Do6jyfeF/Q8IdolzkknQSiAQVEQe5RS5qdAMbxpwtyAAO7h32e0ROtmfEyWYObnAzjFvYMvJG4RxPRmHeQ96RERnG+E4UZmAgys2AQcaICCR2bp0QMNxCuMgt7x9dValaXdVd3dXXyvfjsx5JVXV1rVWrVlfVr9aqx6V3n7e0tGB3lD38/N577wFSYDcjIwNffvmlzyGcxc/I7x+uqKjAe++9h4MHDyIjIwPPPvus8MnwcblcSExM1Dz8I5MDuvLDn+J+0zvnNLNMsITz3MiO4hpdrlZxIgC0traitbUV169fx+XLlzFsxAhxkaArKytDjx49PBqYS5cu4YsvvsCwYcMwYMAA5e8uXbpg/PjxykmEHCyRx5AfNGgQqqur4XQ6NQ1bWVkZmpubNdPKy8sxIgx5JBKFqu4VFRXh7Nmz6NOnD/r27YuLFy+isbERHTt2xCOPPBLyHg1qhw8fxpEjR/Dcc8+Js0Jiw4YNuOeee3SHPy4qKgIAzJgxQ5wVVr72+86dO5Geno5+/fqJswDppqvT6fT6XrrKykpcvXpVM5pCqPnKl5qv4G95eTm6deuGIUOGYPv27Th//jzuvPNO9OnTB3/3d38nLh41jh8/jn379inDrss+/vhj3LhxI+J1zxt/9p+Rw4cP+7yhrdatW7eQDAvf2Njod8A9IyPD64MXgQpFmZjdV2aG+vS2fWa2xQxv2xGK7zdbPmobNmxARkYGHnroIUC6yLhw4QKGDh2qG2iorq6Gy+WCw+FQLkB27tyJK1eueL2wky9uxXNR2YEDB9CpUydAdVEVTQ4cOIAHHnhAuXAsKyuDw+EwdeyUl5d7vOIl2Kqrq9HU1BSVZRdugRwHau+++y7GjBkDSK9i6NKlC3r16qWcn/zpT3/SLP/UU0+hqakJ3333HQCga9euGDBgAC5evIhDhw7h+eef1ywfbkbngEVFRejYsSOefPJJVFVVYdeuXZg4caLHNWko7JZebeSNv+fPZvb76dOn8c0336BXr14YOXKkOBuQRpIZNmyYEuj5+OOP0bFjRwwcOBBHjhzB1KlTTR333jQ3N+PYsWOa89nCwkLlPZFOpxM//elPgRB8v5lyIqLoF+xjWQ5iyOtU31+E6v7kmDFjlAeI9O5F+rrvKK4X0jmMeP8yUMePH0dLS4vmfKixsRHHjh1D3759NWXma1vFMvG1vF4+fH2G3FgmRGQG2wr/2bHMjn71FXr27ImEhAR0iI+H0Zhb8Yvz8laIE9Vu3bqFGzdu4K7+/cVZQdfQ0IBOnTp53GTr3LkzfvjhBzidTlRVVeHcuXNITU3FpUuXkJKSgpaWFhw7dgxVVVWoqqrCnXfeqVw03nnnnTh16hQqKipw6dIl9O/fH0lJSTh79iyOHz+ufGbAgAHsnUgRcfr0afQPwfF1/PhxXL16FVevXsXZs2eVcfiTk5PhcDjQo0cP8SMhc/z4cdy6dQv333+/OCskvvzyS/Tt2xdpaWniLGWok/vuu0+c5Zfq6mqPNuPSpUs4f/68qbL1td8PHz6M3r1744cffsDZs2dxxx13oLKyEp06dcKFCxfQ2NiIM2fOIC4uTpkmLnfmzBlcunRJGfrbjFDnS9bc3Iw///nP6N69OyZPnizOBgD0798fvXv3RklJCS5cuIC/+7u/Q2trK27duuXxpK0vVvPlj8OHD+PmzZvo1asXmpqalHTt2jU0NDQgKSnJ0neGMi9m9583SUlJSEtLM51C9YRgjx49PL7LV7JafkZCUSZm9pUcdP3hhx+QlpaGH374Ac3NzWhubsbVq1eV/HrbPjPbYuT06dO4cOGC5vuamprw/fff46677kLHjh2BEH2/mfIRffnll+jTpw8GDhyIY8eO4dy5cxgwYADi4+PR0tLikRISEhAXF4fTp0/j9u3buPPOO+F0OnHjxg2vFxYNDQ3o0aMHbty4gVu3bmmO58bGRpw/fx533HEHrl+/rsn/8ePHUV5erpy79u3bVxly+sCBA7h16xa+/PJLVFVVKQ95lZeX45tvvkFVVRVOnTqFy5cvo7q62vR69Zw/fx5XrlxB37590djYCJfLpYw2cfz4cTQ1NXmcy8u++eYbDB061Oex5m2b5LweO3YMFRUVmvllZWVobGzEDz/8gKqqKuXc3+w6xfILtlC233oCOQ7UDh8+jOTkZDQ1NeHq1at47LHHkJ6eju7du+Pbb79FTU0Npk2bhqFDhyIzMxOdOnXC1atXkZiYiF69eqFv375ISUnBgAEDcPv2bSQnJ4tfoeuDDz7A8OHDNdMqKipw9OhRS097x8XF4cSJE7hw4QJ++OEHNDU14fDhwzh79izGjBmDXr16YefOnejVq1dIH1JQ69OnD06ePInbt2+LsxTyQylmmdnvPXr0QLdu3VBbW4sLFy5g4MCB4iL429/+hrvuukupmwMGDIDL5cKZM2cwbNgw3H333eJH/Hb+/HlUVlZi6NChyrQ77rgDNTU1uHLlCh566CH06tULCMH3myknIop+wT6WT58+DUjXopBGdurZs6fy+339+nU0NDQgOTkZN27cMLwX6eu+o7heGNy/DJR8DSp/d1VVFb7//ns8/vjjHuv1ta1imfhaXi8fvj5DbsGuz0RkT2wr/GfHMjtz+jQ6d+6MDh06IK5DB8MAcFT1ACZqj0L1BIrYAxjSRcaVK1fQsWNHy0/N+6OoqAh33HFHUJ5kNSPUPYDFUQiMpnnja79fkobTLC0txfnz5zFt2jRs2rQJ48aNQ1NTk6lpQ4YMQYcOHZQhl3zRy4PeNG985Uvt8OHDKCsrw/Dhww0/U1JSgqamJmRlZWHw4ME4dOgQmpub/eoBrJcHvWnB0NzcjKKiIq/v2Taqm2bobbfetED5s/8osszsq2+++Ub3vVSQbv4//PDD4uSg+vzzz5WHj0RJSUkhfSjITPmI5B7AAwcOVHowmtWhQwc89NBD2Lt3r6kewHJAReyZUV5ervT+Vc8rLy/H9evXlb/FnhUHDhzAtWvXMGbMGKVnbrnQ21bu9ZGYmGh6vUbk7xPbHfkhK72ek/L3+1q3r20S8yrmU68HsL/rDAW9tlpvWjAFchyoyT2A1ecYMvn8ZObMmfj+++/x3Xff4cyZM2ht1V5axsXFoV+/frj77rt1g4yiiooKTJ8+HcnJyfj0008NpwXq+PHj+Pbbb3H27FlACiref//9GDx4MEpLS3HixAnMmDEjrMObNjY24quvvkJjYyMSExMxcOBAnDhxAjdu3EDHjh2Rk5MjfsQrf/b76dOn4XQ68aMf/Uh3hAg786eciCh68VgmO2F9JiIz2Fb4z45lZrYHcEy8A5iIAte3b19MmjQJkyZNwpNPPolu3bopT6qGi9wz1S7U70o6cOCAcgO3b9++QbuBu2nTJlRWViIzM1O54Tpv3jwMGTIEmZmZyMjIwKZNmzTTxOVKS0vxySefCGs2Fo58qY0aNQqjR4/G0aNHUa7zvhAx+AtpG/0VznxVVFTgxo0bmD17Np577jmPlJKSgrq6OvFjpoUzLxT77r//fvTt2xfx8fEYMWIEJk+erKRQB38B4OGHH9Z854gRIxAfH4++ffuGNPhr1cCBA+FwOAAADocDEydONEy9e/dGhw4dMHToUHTp0kVclVf33nsvmpublQd+Ll26hKamJt1ekk1NTUqPEqjet1Stem9uUlKSpo1samrSjJYwYMAAj565ZtYr2r17Nzp16oRhw4bh2rVrmva7paXFsCeH0buURWa2SZ3Xfv36+Vy3v+sMBbu23wkJCTh06BDOnDmD3r1745577sEDDzyABx54APfccw969+6NM2fO4NChQ+JHdWVkZCjD9z/22GNK8HfmzJmWg7+QjrsZM2Yov8tPPvkkBg8ejObmZpw4cQL33HMPEhMTUVVVhY8//hgbNmzAhg0bsGXLFt1zlWAYMGAApk6dipycHMyYMQOZmZlKADrUgej+/fvj4Ycf9hiWv7CwEIWFhTh8+LAyvaqqCr///e+xYcMG5f1twXTkyBGvr24I9fcTERERERHZTVQNAU3UHoVqCAJ5COi+qqGQO3furLwXtnPnzprh1kLl+PHjqK2txf33368M4RZqlZWViI+P1x36+MiRIxg4cKBSJlbIwbza2lr0Fd6j44uv/R4fH48BAwYoPcFEnTp1wp133onevXuLsxTykPp33XWXOMurUOZLlJSUhLi4OPztb39Da2ur8lm94C+kHrYdOnQw1YtIZCVfZu3btw/9+vUzDG7Fx8fj5MmT6Natm0cgxh+hyou/+0/P7t278be//Q3Hjx8POJ06dSrgIVjby/eb3VcDBw7EhQsXUFtbiwEDBijDLqt522Yz22KGPBy13vsmQ/H9ZstHTT0E9J133onbt2/D5XKhY8eOuoHBiooKnDt3TvOOYLNDQMvt86VLl5ThlKuqqtC5c2ekpqaiqalJGQK6sbER33//PRoaGjTD+MlDzd95552oq6tT/g2pR+H333+vDM0sO3/+vF/rFR04cAD9+vXDiBEj0KNHDwwePBjfffcdzp8/j/79++P48eMe3ym7cOECzp8/73V/mtkmMa+tra1oaGhAX2lI5wsXLuDKlSvKMNeBrDOUQtV+6wnkOFCTh4C+cuUKLl26hOTkZOW85NKlS7hw4QLuv/9+ZQjjlpYWXJKGtD537hzOnTun/G7Hx8drgvC+zJ8/Hxs3bsRvfvMbzJw5E6tXrxYXCaqdO3cCAKZOnYqqqirs2bMH3bp1w49+9COkpqaiQ4cOKC8vt/z7bdb+/fsBAHfffbfyQIpZVvZ7c3Mz9uzZg0ceeQRpaWnKOyp79OiBTz/9FKmpqXjsscfw5ZdfegxTb1VLSwuqq6tx+/Zt9OnTR5wd9O+3Uk5EFD14LJOdsD4TkRlsK/xnxzIzOwQ0ewATtSPyux8h9QwOhwsXLqBjx45eb/gGW2pqKurq6jS9FgDgL3/5C65cuYKMjAzNdCvGjx+PpKSkoN/AbWpqwpUrV8TJiitXrqCpqUmcrNHc3Izz58+Lk00JVb70iD2BjYK/kG6E+hvQVgtlvhobG9Hc3Ow1OD148GAkJiaipqZGnOW3UObFijvuuAN9+/a1lKyMGNDev1/PyJEjMXToUMPhPb1tc7C2pWvXrhg6dKhH8Bdh+v5ADBo0yOuwtSkpKZrgbyD69eunDNN97tw59OvXT1xE8fjjj3skK+9DlYnrNFrvpUuXcO3aNY8eyuPHj0dTU5MSKDIiB3QaGxvFWR7E7THaJn+I6wvGOgMVre23kb59++LWrVvYu3cvSktLcebMGdx3332a3qn33Xcfhg8fjqSkJPTp0wd9+vRBUlIShg8fjvvuu0+zPrM+/fRTvPDCCyEP/h4/fhyNjY0YM2YMIA2fn5iYiCeffBL33nsv7r33XkyaNAkDBgwIWS9gNfk7OnbsiGHDhomzQ6q6uhp9+vTB4MGDMXjwYAwYMAD19fXKNYTcOzk9Pd3neai/MjIyMGjQIFRXV3v0BA7H9xMREREREdkNewATRVionkA5LvUAvnr1KiorK3H8+HF89dVXuHHjBhITE/Hwww+jc+fO4seCprm5GVVVVXC5XIDU87GpqcnSjXKzHA4Hvv/+e5w4cQLHjx9HZWUlDh06hJaWFjz44INB7/kcSJ587ffDhw+jd+/ehsGPs2fPora21msw2+Vy4dKlS7o9oc0IRb6MqHsC//DDD7rBX5lRmZgVSL7MOHHiBAD4fL/vrVu3cP78+aDUw2DnJdD9p5aUlIS0tDRLyVsQyZf28v3+7itvw4h622Yz22KW0TaE4vv9LR9IPYB79uyJ+Ph4tLS0KO8vlv8tpmvXrim9HuXU2NiImzdveg3sqXsA9+jRA2fPnlV6/MqBMnUPYLmHa9euXZV3B4vq6urQs2dPw16xMnnIY7PrVbt+/ToaGhqQnJzscf4QFxeHS5cu6Qb4ZZ07d8bZs2fR3NxsuF/NbJOYV3G7xB7AgawzHILdfusJ5DhQk3sADxkyBB07dsS5c+dw7do15fxk0KBB6NSpE06cOIE+ffrA4XCgb9++6NevH/r164e+ffsiMTERzc3NOHfunF89gGWZmZnipKBqbm7GZ599hpSUFDz00EMAgD179uDee+/1qKeXLl1CTU2NslyoHDhwAFevXsWwYcNw9913i7N9srLfT548iS5duiBNGinn9OnTuHHjBm7fvo1Lly4pbVRLSwtOnToVUHDf5XIpAV0xyaNUNDQ0aHoCV1VVBe37ZVbKiYiiB49lshPWZyIyg22F/+xYZuwBHKOqqqqwadMmFBcXo1nqqUlkxZUrV3D27FmcPXsWHTt2REpKCv7+7//e8EZ8MDQ3N+PPf/4z9u3bp/SK3LdvHy5fviwuGjJTp07FE088gfT0dPTt2xfDhw/HjBkzMGrUKHHRqDRt2jSkpqaKkxWpqanKO3+NjBgxwmcwMprIPYG9BX+j2ahRo/Dkk0+Kkz2MGDHC1HJEFH4XL17Ed999F3C6ceOGuEqf+vbti6amJo9gk6xnz55ITEzEsWPHNNO99USUP/P1118r06qrqzXnlv6uV15efthFVl5eDqfTiU6dOhl+VnbPPfegubkZZWVlmunV1dWorq72e5uMWMkn6RsyZAimTZtmeH7S2NiImpoaXLhwQZl27do1uFwunD17VrNsNPnqq68AAKNHj9ZM7969u+Zvo2nB9pe//AVnz55FSkpKyIPfkfLtt996TXLP3rq6Oly9elX8OBEREQXBlStXeD5MRNQOxDW6XK3iREhPy7e2tuL69eu4fPkyhnnpyUDBUVVVhZKSEvSV3gnXpUsXPP300+JiZDPl5eVeewqRPfna77/5zW8wbtw4w967lZWVOHjwIObNmyfOUpSWluL8+fOYPXu2OCtkfOVr9+7d4iRLHn/8cXFS2NgpLzJf+4+iB/eVd4GUz7vvvosxY8YYtrsNDQ2oqKjAo48+Ks5SlJaWorm52ev5W1lZGXr06IF7771XmbZ7925NG3D8+HG0tLRoglJlZWWawGZ6eroyhLE8/LI4pPGBAwdw7do1QAo0d+rUCdevX9eUjbf16hGX76t6j638fYmJiR4BNTVxHV26dMH48eMN53vL66VLl/DFF19gzJgxyrua5e1Qb5s/67SLQI4DtXfeeQetrbqXioA0rPdPfvIT/OlPf0KXLl0MX13RrVs3XLt2Df/lv/wXcVZEVVVVYdeuXRg7dqymnDZs2IDhw4d7BGBLS0tx4sQJ5OTkaKYHQ3NzMz7//HPU1dUhJSUFU6dOFRcxzcp+37t3L6AazUT++6677sK3336LGTNmAFIbpf47mI4cOYLz58/j/vvvV57SF79P/DsQVsqJiKIHj2Wyk3DV5ytXrqCsrAyXLl1Cv379lNdgEFFsCFdbYSd2LLOjX32Fnj17IiEhAR3i4w17ADMAHAHNzc346quvcNdddyk3/9TB36ysLBw+fBjV1dWYP3+++HGyGTs2QJFSVVWFv/3tb+JkQ1ZuGlnla78fOXIEAwYMMByuUh5q1ChQAQBnzpzRDCkaDr7yZaegqZ3yIvO1/8zYvXs3Ll68KE42dMcdd4Qk7/62BwDwox/9KCS9z0NRJmb2lb/fq8fMthiJ5PebKR9RuALAkVReXo5OnTppgs9kX4EcB2rHjx8XJ2l07twZgwcPxp/+9CdkZGTA4XAo5x4A0KlTJ/Tr1w8ulwsVFRVRFwAuKipCx44dPUblkHvh/vSnP1WmNTc34+OPP0afPn0sBWdF8nWh0+lEx44d8dBDD1k+Pq3s9/LyctTW1iplsmXLFowYMQJJSUkoKipSgt+7d+9Gx44dgz7SjF7wF1I5Bfv7Ay0n8WESmHhwJpqVl5ejqakpoN/aaKG3T2TqB4H06D2UJSqXesh5W080kPelzNfDWN7ESp5h4VgmikbhqM9y8PfGjRtwOByoqqpCnz59GAS2Ib3fR/mcRfz9j6V2HwCWLFmCDz/8UPl73LhxeO+99zTLGFmyZAkAYPXq1eKsmBGOtsJu7FhmDABHqaqqKnz22Wfo0KEDrl27hlGjRqF3796a4G95eTm++eYbjBo1KmaGq6XA2bEBipTGxkZUVFSIkw1ZuWlkla/9/qc//UmcFJCePXsiKytLnBwyvvJlp6CpnfIi87X/zDh8+LBhLzA93bp1C8lvnb/tAQBkZGRgwIAB4mTLQlEmZvaVv9+rx8y2GInk95spH9G7776LAQMGoGvXruIsQBrOtrm5Gf369RNnKc6fP4/4+PioDABXV1fD6XRqesqSvQVyHARCHQDWE40BYLk379SpUz3a/cbGRvzlL39B165dMXDgQADAqVOnACDor1GpqqrCyZMnkZaW5jUA5Q9/9ntzczOOHTum6e1cWFiovK/Z6XQqgfCPP/4YHTt2xMCBA3HkyBHdsrNCDP6WlpZi2LBhSnkH+/v9KSc1MwHDaFBdXY2mpiZNAFBvmt34ewPbzP70d52RIL9aQb1v1XXc330fC3mWBXosE0WjUNdndfB3xIgR6NKlC77//nucPHmSQWAbMvMbJxPbfX9/N8Lp2WefBQBNwHfJkiWmA7rBDAB/8MEHKC4uNh18DpZQtxV2ZMcyYwA4Cp0+fRqffPIJEhISMHnyZDidTnzzzTdISEhg8Lcds2MDRL752u8bNmwQJwXkrrvuwj/8wz+Ik0PGV77sFDS1U15kvvYfRQ/uK+8CKZ8//vGP4qSA9OrVKyqOZ70nvqNhuyh8AjkOArFr1y788MMPuPPOO5GYmIj4+HgAwK1bt9DS0oJz586hc+fOeOKJJ8SPRszHH3+MgQMHGl5vyT1z5d50AwcO1AQjo5k/+72xsRFlZWWaXtBVVVX45ptvAAD333+/MjKGPEz1lStXcPfdd5v+DrMqKiqQmJio9Pz9+OOPMXr0aCXIG+zv96ec1Py5mRpJejdu9aaFQ3V1tUcP6UuXLuHy5cuWgvh6xBvYvpjZn/6uUxTq/Ou9CkHk7763mmcjoSiLQI9lar9CUQ+DJZT1WS/4K2MQ2J7M/MbJxHbf398Ns6wefxUVFZg+fTq2bduGjIwMcbYp4Q4Af/DBB5gzZ45mWkVFBRoaGryOLuZNKNsKu7JjmTEAHGWuXLmCgwcP4tSpU2hubsYDDzyAESNGoLy8HGfPnvU7+Kt3Uy9Wh57Sy4u3ixe1chsMWWXHBoh8s+t+95UvOwVN7ZQXma/9R9GD+8o7lg9R+I6DK1eu4LvvvsO5c+dw+fJl3Lp1CwAQHx+P7t27o3fv3rj77rvRrVs38aMUAuHa77Eu0HLydTP1+PHjaGhoUP4WhyCW3znudDoB6fxPXmdLS4tyXTxs2DB0794dX3zxhfJZ9bmiHPSTqd+lLl5f9+3bF9evX/eYJt+PgOqGr7x9DQ0NyjvkxWtz+Roc0vf27t3b4731Mnk71dunNy1YxPx4Kyeo9uf169c1eVIvI64TOvtZLCOZXl71plm1e/duw/tBRvWhU6dOHnmS96O/eW5sbMSxY8d058n08q03zV+BHsvUPunVOb1pkRKq+uwt+CsLJAgsjzCkFqtDCtuRt3MWcf+o/9b73ZCX8/ZboHeOo6Z3rOlN8yUjIwOvvfaaR1BV7a233sLbb7+t/K0OGOsFgL0tDymI+8orryh/v/baayguLsbBgweVaTNnzvQIKssB6+TkZHz66aeG0/wVqrbCzuxYZu0iAGz1qZFwqa6uxsmTJwEAI0eOxMmTJ/H1118rQWBIldBs8Bc+GvFoYuaJITEv8o+J3kWDVWa2J9zs2ACRb3bd73bNV3vB/Rc7uK+8Y/kQ8Thor7jfzQm0nMRrV7VynYeTDxw4gB49eijfdeDAAVy7dk1zrSvfaB02bBgGDBigXA+LQV11wO748eNITk7WrEM9X++6V2+aeANY3L7y8nK0tLQo2yH+LQf+fL1v9sCBAwCABx54AF988YVHYDxYxPz4Kie57NXB0zJhOGVxneXl5bh+/boyXw6AiDe61UKdf7nOGK1X3PfV1dVoaGjwCIb37dtXeTckTOZZvnkv15nGxkZ0797d8F5OsMsi0GM5mGLl3qS/7JovhKAeBkso6rOZ4K/MnyCwXIbqdqS6uhoAdNsRCj9f5ywwCABD53dDXsbotwA65xBGrB5/crBWL+AKKcBbX1+v9MqVg7fyK8LEALCv5eXvk/+uqKjAl19+iTlz5pjqAQwAjz32GABg/fr1mD59uuG2mxWKtsLu7FhmZgPAHcQJseLSpUtwOp1KoyFP++KLLzyePoqU48eP47PPPkN5eTkSExPx8MMPo0uXLhgxYgQeeOABfP3110oDS23uvfdedOnSBfX19eIsIiIiIiIioohpaGjA7t27lXTp0iUAQFNTE4YNG6ZZNj09HU1NTcoyAJCUlORxY7Rv375KQCU5OVlZTj2/paVF+fvee+/VrEPu1RkM6u3r16+f0hMYUh7T09OVvwcMGIC+ffsqfxuRAwSB3Oi1wkw5JSYmaoJc99xzD5qbmzX7TK2pqUl5TzakQEeXLl2UwIeeUOf/3nvvxZgxY9DU1ITdu3fj+PHj4iIagwYNwrVr19DY2AhI99Kam5s9gn0yb3m+fPkyACjlPGDAAI/6rRbqsgi3WLg3GQi75ktmt3poxJ/gL6RXiPXu3Rvff/89amtrxdkK+V622GNz0KBBhu1IOOi1w5cuXVLauvbI6JwlEN5+C2R65zgiq8ffSy+9hG3btuHDDz9ERkYG3nrrLc38Dz/8EL/85S+Vv+fMmYPk5GR88MEHmuVkvpZ/++23Na/py8jI8Nr7WI/c0zcYwV8if8VsALhnz56aJ0zkE5G+fft6/ACF09dff419+/bhk08+wXfffYf4+HiMHDkS999/v2Y5MQg8YsQI3H///SgrKwtKUPj48eOaBl5c54EDB1BdXa3Mh/Rk0PHjx1FWVqZMb2xsxKVLlzTrUhPnqU8Oy8rK4HQ60dzcrLsN3nTq1AnwsX5IJx3q9cr5OnDggPIZ+cfN2/aI5aX+QdQrKyIiIiIiImp/kpKS8PjjjytJ7vUIKfilJv8tB8kgDTEskq9/oQqk6S2npr6GdTqdHoHNQKm/t3v37oBwA13Mo3rbvRk/fjySkpL8vtFrla9y6tGjh+ZvufzV+0wml8EXX3yhuX+gDpIbCXX+5Xtkw4YNQ0NDg9KT2Ujfvn1x4cIFAEB9fb1hIN9XngcMGIAuXbpg9+7dusEXPaEui3CK1nuTVtk1X2p2qod6rly5gi+++AItLS2mgr8AUFVVhTNnzmDIkCFITU0VZyvEh4HM8nbv1df9X1/3Zu3+0EKg9M5ZAuHrt0Bmpp4hCMdfRkYGKioqsGHDBrz99tt49tlnAQCfffYZIAVaMzIylGTUyczX8vL8QN/Vq/bpp5/ihRdeYPCXwi5mA8Ayq0+NBFvPnj1x9uxZdOvWDWPHjsWDDz6IO++8U1wMMAgCDxw40OtTVmaUl5ejoaFB08C3tLR4BGCdTifGjBmjGaqooaEBDocDjz/+OJKSknDs2DF8/fXXynoSExM166mvr1fW8fjjj6NTp07K/NGjRyM9PR2JiYl4/PHH/do3169fV3oBG63fiNPpxAMPPIDHH38cffv2xddffw142Z5yaRgr+TvS09Pxheo9QfI6xbIiIiIiIiIiCrcDBw54XMPGAr1hKEMpVOUkr0+dzPR6C0f+BwwYgDFjxqC5udlrr7d+/frh3LlzAICWlhYkJiaKi2iI+VXnefz48RgzZgycTqdHUMdIOMoinKLt3mSw2DVfMrvVQ5kc/G1ubsYPP/ygvJbQm6qqKtTW1mLo0KEYOnSoOFth9DCQL77uvZq5/+vt3mx7eGghGoi/A2Z///QE4/h79NFHsW3bNhw8eFAJ1kIapllM3nrtisv6Wj5QL730kjiJKORiPgCMIDw1EkyDBg3CPffcg4sXL6KiogI1NTXiIhrqIHBpaSm+//573HHHHeJiuoyGcYj1oafkH/hBgwYFtH5vQ1bpCdYQFkRERERERNT+yD1lxYBboDfKvWlsbMS1a9c07+Xzdc0bDOrewGrq+wPRxGw5ifcXvO0zo/0cbczcuxgwYIAyDLS34Z/N5lkOviQmJhr2tLK7aLo3GUx2zZddqYO/DocDAwcOxJkzZzyCqWpmg78waEfN8HXv1cz9XzP3Zu3+0EKkmP0tiISMjAzl33IMQx0M9sbX8vJ8+f2/RLHIFgFgBOmpkWC59957kZKSgvr6enz77bf461//iq+++go1NTW6P5QjRoxAWloaKioqkJycjEmTJomL6NIbxsHoYiXah55SB7NbWlo0T2f5u36jIav0BHsICyKz7HoSatd8EUUbHmtERKSHvw+R0bNnT/Tt2xfHjh3TTHc6nZoHqoNBvAl76dIlNDQ0CEsBzc3N4iTdaWb17NkTiYmJyghbkN63aGWdoWS2nJqamjQ3tL3tM7kMxP3sLbASapcuXfL4fvkdwOr7Qnr7qW/fvnC5XIbDP8NEnhsbGzXlJ4/m1l5F073JYLJrvuxGDP526tQJPXv29BoE9if4Gyiz91593f8127bwoYXgUP9u+PotCJeKigosWbJEM01+B/Cjjz6KjIwMjBs3Ds8995xmGfEzMl/LZ2RkYObMmViwYIEyr6KiQvM+4YMHDyr/JopGtgkAR5tRo0YhJSUFra2t6NGjBy5evIgTJ05gz549+OKLL/Ddd98pP3TXrl3DzZs3kZaWhr//+78XVxXVgjWkkjqYrQ7+Bmv9vojDV1gZwoKIiIiIiIjalxEjRiApKUlzc7t3795BD5z07NkTSdLrmnbv3o2vv/7a4zpZ7lm1e/duzQhb4jR/yb1p5fw1NzcjKSnJ9HuAw8lMOUG6F+FyuZQ89ejRw+s+Gz16NBITEzX72dfwyaHUs2dPNDU1abbn3LlzeFw1RKrRvu/Xrx+am5vRr18/ZZoeX3mWy1guP95LIYqMI0eOoKmpSQn+yoyCwIEEf/v06QME2BNUvO+qvvca7Pu/3tpx8k3vd8PXb0E4ZGRk4MMPP9S8r/ejjz7S9NB97733MG7cOM0yDz30kGY9ar6WX716tWb+9OnTlflz5sxBcnIyMjIyDIPMRJEW1+hytYoTAaC1tRWtra24fv06Ll++jGF8aiYgu6Whme+++2506tQJjY2NuHz5Mq5evYrW1lZ069YN8fHx6Nq1q+mevwBQVlame2Eiv+Ng2LBhmqc9GxsbcezYMeUi4MCBA0hKStKcmOutc/fu3Zp1VVdXo6GhAePHj/dYJ6Sntc6dO6cEcaurq9HU1KQZdkmk973Q2WborF/+EZKf6hLzJZfHmDFj0LNnT4/tMSovNXGdwVYuvf+ZiCjS2B6RXbAuE/E4IPKGx0fwlJeXo1OnTh7X8xT91Pd3YhWPZbITq/W5sbERX3zxBTp06KB7D/PSpUs4deoU+vXrh549e/od/JWVlZUBqoeC9Kjv1/q692rm/m+o780SxRKrbUV7ZMcyO/rVV+jZsycSEhLQIT4eceICEvYADrHMzEx07doV3333HSANwXP33Xdj+PDh6NOnjzKcwqhRo4RPBiZWhp4yw+z6/RWNQ1gQERERERERxRL5Aevk5GRxFsWAhoYG9O7dW5xMRDFqwIABGDNmDG7fvq28W1dN3RM40OAvANxzzz1obm5WAsGy6upqw+/1du81VPd/iYiIAeCQ69atGyZOnIi4uDglCAwAFy5cQFNTE/r164eJEyeiW7dums9ZEe1DT5llZv3+0tueaBjCgoiIiIiIiCialZWVaa6bnU4nHn/8cfTs2VNclKJYeXk5dpsY7pqIYo+vIPDVq1cRFxcXcPAX0v1aubeu+jehoaHBsIeut3uvobj/S0REbhwCOkxOnTqFQ4cOoUuXLujcuTPOnTuHpKQkZGZmiotSO2PHIQiIKDaxPSK7YF0m4nFA5A2PDyJ74LFMdhLM+qw3HPSZM2dw8eJFDBs2LODgLxFFXjDbivbCjmXGIaCjzMCBA/Hggw/i8uXLOHv2LDIyMhj8JSIiIiIiIiIiIqKgEXsCM/hLRNQ+MQAcRoMGDcKIESMwfvx4PPDAA+JsIiIiIgoCuz3ZSURERERE5A91EJjBXyKi9okB4DAbMmQIBg4cKE4mIiIiIiIiIiIiIgoKOQjM4C8RUfvEADARERERERERERERkc0MGDCAwV8ionaKAWAiIiIiIiIiIiIiIiIiIptgAJiIiIiIiIiIiIiIiIiIyCYYACYiIiIiIiIiIiIiIiIisgkGgImIiIiIiIiIiIiIiIiIbIIBYCIiIiIiIiIiIiIiIiIim2AAmIiIiIiIiIiIiIiIiIjIJhgAJiIiIiIiIiIiIiIiIiKyCQaAiYiIiIiIiIiIiIiIiIhsggFgIiIiIiIiIiIiIiIiIiKbYACYiIiIiIiIiIiIiIiIiMgmGAAmIiIiIiIiIiIiIiIiIrKgoqICGRkZWLJkiTjLw2OPPYbHHntMnBw0DAATEREREREREREREREREVmQkZGBbdu24cMPP/QaBJYDv59++qk4K2gYAA6TjIwMVFRUKNH/zz77TFxEl/y5SIqGbSAiIiL7CfT8iIgomvH6iYiIiIiIqP3yFQQOR/AXDAAH32OPPYaMjAwlieSbAY8++qg4i2Lc7t27vaaysjLxI9ROqduIjIwMvPXWW+IifuONRlIT2x8xsT2icHv22Wfx7LPPipMVsXZ+xDaXwklsw8XENt23jIwMwzaIx3NsE48HMfH4IB7jRMGlPqZ4fBEFh3wseXsw2ts8onDw1eZ7m99e62+GQRA4XMFfMAAcPHIlfuqpp5QGe9u2bfjggw/ERcnGhg0bhscff1w3jR49Wlyc2rFt27YpbcVLL70kziayjO0RRYuKigq4XC64XC7DiwEi8o5tunUulysoD91R9OHxYV/yfRY5qR/k8HaTkYjM8dWJhYgCoz6u5GQm8CX/tskPRqt/68R5RMHg62H9YGnP9TdDCAKHM/gLBoCD51e/+hVeeOEFTSAnIyMDc+bM0SwnT1c33p999pnXE66Ghgav85csWaLME18Y/cEHH2g+qw5Iq79b/blnn31WWZ43SYjCy9vxLB/D6uNZvikCANOnTw/LjzYRkT8++eQTPPXUU3jqqafwySefiLMVGcKNXPF8RD1frz1Ur0ecJ/6tpv4e9UW53nrY5hLFrvXr1+Ptt9/2evNN3c6If+u1CeLfar6u4by1PXrXaETtTUVFBaZPn44NGzagQnpwlgF9ouCQz2nZiYUodNQdP9pr4IuiWwUf1g+bDFUQGGEM/oIB4OA5ePAgfvzjH4uTTfnlL3+p/Bi88MILHhf63uYvWbIE9fX1yvxx48ZpbkZ++eWXyrzXXnsNr7zyijIPqnXLlU7uii5/hgJXXV0tTiLyytfxDADFxcWa41l9Y3Lbtm147733NMsTge0RRdhHH32EH//4xxg5ciQ++ugjcbYu8Xzk1KlT4iIe7aG3efL50IYNGzTLLlmyBMnJyaiQbnr98pe/9LoetrkUDdimB+61117Dc889J042TWwTjNoWmLiG89b2iNdoZB6PD/toaGhAcnKy5ob5Sy+9hAqdh7GeffZZTeDqs88+87ivIjN6+MLXg/lEdmKmE4vRsWKExxCReeLDzmoZGRn461//6vFbJ8+Tr0czdB5OVBO/Q/1ZIph4WF+sQyJf80Vm669df0/k/If7Go8B4CBQV9xArF+/Xvn3Sy+9pASAzMz/8MMPsWDBAmX+c889h4MHDyp/r169Wvm3fCKnXvevfvUr5d+Q1qe+AcGhaQNTXl4Op9OpuQHR2NiI3bt3a5aj9mv69OnKD5l8MeXreIZ0QxAGxzORHrZHFEmfffYZHA4HMjIylBu4Zm4giecj6vMZmbf2UJwnB3zkbVCfR8nzMjIy4HA4vK6HbS5FGtt0a+bMmYOZM2d6PGBnltgmGLUtMHEN563tEa/RyBweH/YiH1fi8aq+eSg/jJWdnY3i4mJlmW3btiE3N1f1KTdvD18899xzqFD11CKyM1+dWLwdK0Z4DBGZIz7srCctLc3jt06P+HCiTPwOvQeqibw9rC/WIZGv+WYY1V/+ngQXA8BRKDk5WZykIc5PSkpS/i0HoeWDQz2crF6AWv1Zmd5y5J8RI0YgPT3d4wYEkUw9FIz6qXZvxzNRINgeUSRt27ZNM1zjU089hSNHjmiWMRLq8xG5bVU/kHPw4EE0NDSIixJFDbbp1q1evToi7wOWr+HMtD1612jkG48P+/n0008xevRoZAjv/xXNmTNH8+DswYMH8dBDD2mWgYmHL8w8pEYU6+Q67+1c29exYoTHEFEb9bme+ngTH3a20vlKfDhRPk7F79B7oJraN18P64t1SKyn3uZXSKO1yEnsnS4zqr/g70lQMQAcBBkZGUhOTjaszP6oqKhAfX29OFmhN1/vRmWG1KtQPZysmZM1CAeb2c+Qp0GDBvEGBPnN6HgmsoLtEUXKhx9+iLfffls58X/77bc9niw1EurzEblt5buZKNawTbfOzPuAg0l9Dce2J7R4fNiPPOxzcnKy1+uimTNn4rPPPtPc0FSTzyWMHr6oqKjAc8895/VGJVF74OtYMcJjiEhLPNdTE3+jQiEc30Gxy8zD+r7qkNH8DGm0FjmpXy9gBn9PgstUADguLk6cRIJf/epXeOWVVzzGKzdTSdVDfG3YsAHjxo3THEDe5s+cOVMzvNiSJUswc+ZMQBruSs3MU+7jxo3z+D4KnPoGxJkzZ8TZRBrejmczfF2QUfvG9ojC7YMPPsC4ceM0J/4VFRVwOBw+gy7hOh8ZN25cwOtmm0uRxDbdmoyMDOV9wOrRlZKTk5X3X5m5dvJGbMPU13BW2h7yjceHPa1evRrjxo0zvMfy0EMPYdu2bThy5Aiys7PF2crxJ96QVz98IU975ZVXfJ6rEMWqDB+dWMwcK0Z4DBGZUxHih50Rpu+g2GXmYX1fdcjXfCv4e+Kb2ZitqQAwALTevi1OIpVHH30U27ZtwyuvvKIcOL/85S9NPeGQnZ2tfObgwYMe4/p7my8P4SDPr6+vV6bJ3y3PM+O9996Dy+VSPqM3bBL5R74B0dTUJM4i0vB2PPsyc+ZMPPfcc16HRiNie0ThVFxcrHsDdvTo0ZqHXfSE63zkvffew8GDB5XvMduGss2laMA23Rr5fcDq0ZV+9atfKTdCrPJ2DRdo20Pm8fiIfXoP1B88eBADBgxQ/lY/jCUPA/3RRx8Z3ocx+/DFuHHjxElEtuKrE4vZY8UIjyEiY/4+7BzIg8f+fge1L2Ye1vdVh3zNDxb+nui77UesNq7R5WoVJwJAa2srWltbcePGDVy9dg2D774bnTp3FhcjizIyMrBt27ag3GSg6NHY2Ihjx46JkwEAjz/+uObv8vJyjBgxQjONiChY2B6RHVRUVGD69OlBf6qUKNawTScyxuPDfh577DHNQxqvvfaaEtxdsmQJPvzwQ4wbN055wGLJkiWA8K5D8Z6Lep3yZ+XzDNkLL7zg8a47ik48lgMn1vvk5GR8+umnyt96xwqEY0r+N6Qho2U8hgLD+mwfevf51b9h6uPrtddewyuvvOJxXGVkZHj81ukdf/J3iX97+w6KbVbbimeffRbZ2dkeD8y99dZbKCsrU9p7X3XI13yRmfqLEP2eWC2zaHP9+nU4KyrQvXt3dOjQAfHx8eIiCp8B4Js3b+LatWvo068fevfpIy5GFomVnYiIiIi0nn32WSQnJ5seFYGIiIjanyVLluChhx7yuKFJRETUnvGBaiJ7OX/uHM40NqJbt24+A8Deh4CWxpGOj4/H92fO4PatW+ISRERERERBtWTJEuWp0AzpPWUM/hIREZGRiooKHDx4kMFfIiIiwa9+9SvMnDlTnExEMej27dv4/swZxMfHIy4uzue7gL32AAaAmzdv4tatW7hy5Qru7N0bA5OTxUWJiIiIiIiIiIjCTh4ic8OGDXj00UfF2URERO2K/LsomzlzJh+oJrKJ06dO4WxTE7p06YJOnTqhQ4cO6NDBuJ+vYQAYUhD41q1buH37Nq798AOuXrmCu++5B927dxcXJSIiIiIiIiIiIiIiIiKiILp8+TIqTpxA927d0LFTJ3RMSECHDh289gI2Dg1L4uLiENehAxLi49G5c2dUffcdLre0iIsREREREREREREREREREVGQXL58Gc6KCnTp3BkJCQnoYGL4Z/gKAMtjSHeIi0N8fDwSOnZEfFwcTn77LRrq6/lOYCIiIiIiIiIiIiIiIiKiILp9+zYa6utx4tgxd4xW6vXrq+evzOsQ0JCGgZaHgr516xZu3LyJG9ev4/r167hx4wYGDRmCxMREdOzY0dQXEhERERERERERERERERFRm9bWVty4cQOXmptRXVWFDnFx6Ny5szLssxwEljvweuMzAHz79m0lCHz79m3cuHEDN2/dwpUrV3Dt2jVxcaJ2x+sBpMP7IRk+/m63N126dcO1K1fEyRRy0VKb2qtgHkVERGRv/M2OGtwVhsyd2egVoLlPRpbedpO+WNif0S8qahx3ZQR4K/SoqBUmecsHERERhVPXLl3QrVs3xMfHo2PHjprgb4cOXgd59h0AloO/ra2tuN3ails3b+LWrVu4du0art+4IS5ORERhFUsXkXbj9eeTiIhIxR6/17b45bPHrggJ8/tXXYjmPxV63LnBE037NbZFtFZyN4ZVRPd1SLACERERRYOOHTuiS5cuiI+PR7zq/b9B6QEMnSBwq6onMBERRRvvDT8Fm8+fUSIiavfs8dsc07949tgFIWV+/8qFaf4T4cGdHFzRtn9jU1TUSu7KsPG9v+Wd4XvJ6MDKQ0REFGlyz9+4Dh38Cv7CbAAYUhBY/v/t27fRCii9gYnaG28Hje/DLnK8bTfZTTTXRDvi0UVERN7Y43c5Zn/t7FH8IRez+1fBHR18sV8rokFU1EzuyojR7n/1joiKmmECKw8REVGkyL1+4wBl6GcApoK/8CcALNPrDUzUHhkdOOYOvfAz2l6ys2itjXbEI4yIiLyxx29yzP7a2aP4Qy5m9y/AnRxysV07ok3Eait3Y8S07XN5J0SsFgSIlYeIiCgSAun1q+Z3ABiqIDAApTcwUXujV+/9O/zCR29bqb2I1lppNzzKiIjIG3v8Hsfsr509ip+IyJqYbcTtIbZ/ilh5iIiIwi1O6vULuHv8+hv8RaABYJl6WGj530TtTTQ/v8mjksyJxtoba3i0ERGRN/b4rY3ZXzt7FH/IRf/+5Y6MDtFfU2JBRGszd2HERHS/W8aKQ0REFC7qgG8ggV+ZpQCwGoPARNGHRySZF/gPCYFHGxER+WCP39mY/bWzR/GHXPTvX+7I6BD9NSUWRLw2czdGVMT3f0BYaYiIiMIh0N6+eoIWACai6MODm/wTnB+W9otHHBERGbHHb2zM/tLZo/hDKvr3LXdidIn+GhMLIl6ruRujQsTrgd9YcYiIiGKFewBpIiIiXsgRERERtSutUXUGGOclUXQR9w/3FRERERFRtPG7B3BraysuXb6Mm7du4cbNm+JsinEdExKQEB+Pnt27B62buT8SOnXC5atX8cO1a7h67Zo4m8Ksa5cu6NylC7p37Yob16+Lsz3I7cMttg9EREREREREREREREQB65iQgPgAY3Z+BYC79OiBhoYG9OrVC3fccQe6du0qLkIx7urVq7h48SLOnz+PpKQkXGtpERcJnfh4nD13DgMHDkRiYiLi4+PFJSjMbt26hebmZpw6dQp9evdG661b4iKKH65fR8uVK+jcqROSHQ62D0RERERERERERERERAGSY3Znz55Fj27d0LlTJ3ERQ6YDwK2trTh/6RJSU1PRvXt3cTbZzOXLl1FbW4tePXv6/VRBIBI6dcLp779HRkYGOnbsKM6mCLtx4wYqKirQ/667dHsCt7a24tzFixg0aBDbByIiIiIiIiIiIiIioiCRY3Z3+hGzM/0O4EuXL6NXr14M7rQT3bt3R69evXDp8mVxVkhcvnoVAwcOZPA3SnXs2BEDBw7E5atXxVmA1D507tSJ7QMREREREREREREREVEQBRKzMx0AvnnrFu644w5xMtnYHXfcgZtehvwNph+uXUNiYqI4maJIYmIifrh2DXGAR7p16xaSHQ7xI0RERERERERERERERGTRHXfcgQ5+vDrVdAD4xs2bfKdnO9O1a1fcuHlTnBwSV69d4zt//fT22/8LM2c+hQkTHsYbb/xanB108fHxuHrtmjgZYPtAREREREREREREREQUMl27dsWVK1fEyYZMB4CJKDqcOXMG//iP81Ba+jlef/3X6N+/Pz76qAiHD5eJixIREREREREREREREVE7wwAwxYza2lpxkk+BfCaYWlpa4HK5xMmW/PrXq+F0OvHSSz/H0KFD8cwzP8VPfzoPo0aNFhclIiIiIiIiIiIiIiKidoYBYIoJtbW1OHbsGE6ePCnOMnTy5EkcO3YsYkHglpYWHDhwwK9t9uWzzz7D558fwOTJk5WA709+MhsvvPDfxUWJiIiIiIiIiIiIiIioHWIAmIJq2fJ/x8zZs7Bs+b+LsyxJTU1Feno6nE6nqYDqyZMn4XQ6kZ6ejtTUVHF2yMnBXwAYO3asODsgJ0+exIYN7wIAxo4dJ84mIiIiIiIiIiIiIiIiCl4AuGrDDGRkZAhpBjZUaRbCDI9l2tKS3apliQRDhw41FQRWB3+HDh0qzg45dfB3/Pjx6NGjh7iIX7Zt+wQTJjyMf/7nHDidTgDAypWvYebMp8RFY5ZH++HRGOzGEgvthe/1S3Yv8T5fl7lt870Nvteze4l2vtFyRERERERERERERETUfgUtAOw2E+9UVKBCSu/MPIrVU1RB4MHPoUg1X047lgwHMBNTHxdWRyTwFQS2W/AXAIYMycCqVa9j8uTJAID09HSsWvU6li17RVw0JlVtmIEpq4ElO+Q24R3M/HChJkC6e8lC4B112wJ8uFB4wMSAmfUDVdgwIwMZCz9UTTOjChtm6G2bNijrexvMrQcAMHwJdght6Gq2nUREREREREREREREUWvFiuWYMOFh3diW2h/+sAUTJjyMP/xhizjLL0EOAGs9/t+WYDiO4pNd3qI0u/Gb1UeBmVPBGEbsW/nqf+DDLVux8tX/EGcFjVEQ2I7BX0j5ffTRR9HSchkAkJn5MB599FHlHcCxzX38D1+Sj+cGy9Mex39bMhz48C+QY5+Pr9YGOc21LTC9/qoNeVh9dDiW7NiBJcPbPu3bYDxXpLdtwEmnvG1mtsHMeoiIiIiIiIiIiIiIKBatWPEqJk+ejH/+5xzDIPAf/rAFb731Jl566ef4yU9mi7P9EtIAsGxouhL18FC14X/iQwzHkv/G8C+ZJwaBgx38bWlpESd5Fargr9rXX5cDAIYPfwCQAt5vv/2/sGLFcuVJkJMnT2LFiuV4441faz6r1tjYiA0bNuAvf/mLOMvD73//e/z+978XJwdPlRMnddqIwelDAXyIv4i9XwXi5zyYXP/g54pQUVGkCtAGkcltICIiIiIiIiIiIiIi+/IWBA5m8BehDgDv/s1qHPU6tHMVdn1yFJj5s9AEXtqpkydPYsKEh7FixXJxloeZM58K6rtkly3/d8ycPQvLlv+7OCvo1EHgYAZ/AeDQoUPYv3+/OFlXOIK/hw+XKUHpRx99FABw6tQpAMDnn3+Ot956E4cPl+FnP3sBO3fuxF//ulPzebUBAwbgySefRF1dndcgsBz4/elPfyrOCp6qChzFcGSIx//gDBh3xK3ChrzVODp8CXw+NxLQ+i2qqsBRdcA30G0Q1yM7uhpTVO//nWFmHGwiIiIiIiIiIiIiIoo4vSBwsIO/CH4A+EMsVAUmFn4IDF/y34yHdt79G7hHfzZcggIwdOhQ/J//U4idO3d6DQLLgd8PP/xInNXuDR06FGfPnvUZBA5H8BcAvv76awDAiBEPKtMeffRRvPDCf8czz7gDtEuX/huee24B9u//HH/5i3EAGCaCwGEJ/vpFekdvRgYyMqZg9dGZeKfoOYgx1cjbjSXuhs93cNor/fU8vlr77t8dS4bj6OopDAITEREREREREREREcUIdRD47bf/V9CDvwh+AHgm3lEFJyp2LAFWT0HGjA3wDE9UYcP/9AxwUHD4CgLbIfirHvZZ753AVjgcDjz00ENeg8DhCv4CwNGjRwEAw4d79hl94AH3kND9+vXzq3EwCgJHX/AXyjty2wKfJ7FQ3ft19xLlwRN3WqK83zcoTK5/95KF7iHt860Fp82uZ/BzRXhnJnD0k106bSwREREREREREREREUUjOQj8+99vCnrwF8EPAAsGP4f8JcOBo59glxidkHv//sx7gIMCZxQEDmXwd+Wr/4EPt2zFylf/Q5wVVOI7f8V3AgeDtyBwOIO/0Hn/r1pKSioA4PLly+Isn8QgcNiDv4MzMBxHUSG2D0bDJksGP5ePJcOBo6t/4w7EPr5a0zO2omK1e+SBANfvwWj9KruXZGDhh8OxZIfwLmE/t8FwPd4crWAAmIiIiIiIiIiIiIgohqxY8Sr27/886MFfhDwA7MXuv3wIeH0/MAWDGAQOZfA3XMTgryxcQeBwB3/l9//26NFDef+vWmHhRgDA6dOncebMGXG2T+ogMMIZ/AWAwekYCuCkUxu+rHKeBDAU4utvPQzP8P4AidX1m+QO2gIz39EJ2vqxDV7Xo6sKzpMmyoGIiIiIiIiIiIiIiNqNEAeAd+M37m6+2mBG1Qa4R3/28n5gChp1EBghDv4uW/7vmDl7FpYt/3dxVlAYBX9l4QgChzP4C9X7fx9++GFl2pkzZ3Dy5El89tlnKC//Cj/96TwAQFnZF1i8+F9x+HCZsqwZAwYMwHPPPRfe4C8A4HFMnQkcXZ0H5TW2VRuQt/qoqn3YjSXikMvSCALDf/yEj8CnmfVbU7VhhhS0rcBq3RWa2waf66nagBnCcPpVG/I4kgIREREREREREREREWnENbpcreJEPafPnsWIESPEyYqqDTMwZbX7PaUaM99BhRDNcPdym4l3dIZRpehSXl6O/n36iJMNLVv+7/j2+Le47977/BoG2lf9gongr5o/y5rlcrnw5ZdfokuXLmEL/gLA4sX/is8/P4B16/4nRo0arUz7+utydO/eHcuWvYKWlstYuvRl9OjRAw8//DBWrHhVXE1QGNUHM/vPG7nnq2z4kh0oUj01ote+GAZKdQSyfjdf7dRuLMlYCNWqVbTDOHvfBjPrqcKGGVOg3Uxf20dERERERERERERERHZQXl6OfjoxGj1BCwCTPRkF/IyEKgBcW1uLY8eO+RXQlYPAw4YNQ2qq+z25VrlcLtx5551hC/4CwIQJD2PEiAdRUPAbZdof/rAFBw8exDPPPKMEhd9449fo1q0bXnjhv6s+HVxG9cHX/iMiIiIiIiIiIiIiIqLAMQBMQWMU8As2M/WrtrbW70BuIJ+JtM8++wwA8Oijj+IPf9iCt956U9P7N5KM6oOZ/UdERERERERERERERESB8ScAHOJ3ABMFTyCB3EA+E0knT57E0qUvY+3aN3H4cBk2bFiPl176eVQEf4mIiIiIiIiIiIiIiCj6MQBMFEWGDh2KESMexOnTp7Fy5WtYtOgl/OQns8XFiIiIiIiIiIiIiIiIiHSZHgL63MWLGDR4MLp27SrOIpu6evUqqquq0PuOO8RZQdd8+TLS774b8fHx4iyKErdu3YLzu++Q2L27OIvtAxERERERERERERERUYhcvXoV9fX16GEyDmO6B3BCfDwuXrwoTiYbu3jxIhLCFJDt3KULmpubxckURZqbm9G5SxdxMsD2gYiIiIiIiIiIiIiIKGQuXryILgYxGj2mA8A9u3fH+fPncfnyZXEW2dDly5dx/vx59NTp7RkK3bt2xalTp3Djxg1xFkWBGzdu4NSpU+hu8GRJz+7dcfbsWbYPREREREREREREREREQSTH7Pzpsml6CGgA6NKjBxoaGtCrVy/ccccdHO7Vhq5evYqLFy/i/PnzSEpKwrWWFnGR0ImPx9lz5zBw4EAkJiZyOOgocOvWLTQ3N+PUqVPo07s3cOuWuIjih+vXcfnaNbYPREREREREREREREREFokxu6t+xOz8CgADQGtrKy5dvoybt27hxs2b4myKcR0TEpAQH4+e3bsjLi5OnB1yCZ064fLVq/jh2jVcvXZNnE1h1rVLF3Tu0gXdu3bFzevXxdke5PYhLj4eV65cEWcTERERERERERERERGRCd26dUOXLl0QD/gds/M7AExEFM3YoBG18e+UIHjsdBxGqgzbI716w/IPHr3ylUWynL1tl73IpRzuHAdv74Z7y00LXhbDLvJlGsOFRxQxkT9yQymsrYK9i9I2wlcnWCGIiIiCzfQ7gImIYkEcU0CJ7ClSl9CsUxQI1pvQitbyjdbtIq1I/Z7YVSvLlCiGiVdS9rqiYvtEkWOf44iIiChaMABMRES81LKxSN3EYZ0iij7Reos6GreJ2kTiN8TOWJ5EdmWvX7OwtFXRemJCESQ+WMEKQkREZAUDwEREBPDSikJAvHTnJTwRGWH7EJ3CEgBoR1ieRHZnr1+ysLVZ4sWCvYqRLGOFICIiChQDwERERO1A2G7gEFnAe3/hwbKNBLbCFG3YEhBRFGMTRRqsEERERIFgAJiIiBRi8CVUiSIjWsIPsVQH5CG0o6XsiIIlWtvkaNue4IqdloTtnl1F65FPZCfilQ+POaLg4HFERETkLwaAiYgo7HjpFjnRclOfdYCIjLB9iKxo+I0gIrIf/rr5jbFz8iA+WMFKQkRE5A0DwEREFBG8TCPxsp2X70QkY3sQGQz+EhGFEn/ZAiJeLLAYyQMrBRERkZ64CxcuBHSdf/v2bXToEPvx4+rqavTq1Uuc3G6cP38egwYNEifHHLvUR+aDZCxDLZZHYFhu0Yv7RovlYW/cvxRpdqmDdskHRTe71DO75IPsyy511C75oNjE+kdEemKhbbja0iJO8pDQsSPi4+MRn5CADvHx6NChA27fvo3bt27h1s2buHXrFm7euCF+TCPgUrh165Y4KSbdvHlTnNSu2CX/dqmPzAfJWIZaLI/AsNyiF/eNFsvD3rh/KdLsUgftkg+KbnapZ3bJB9mXXeqoXfJBsYn1j4j0xHrbEB8fj+49e6Jbjx7o3LUrEjp2VALaHTp0QELHjujctSu69eiB7j17Ij4+XlyFIuAewD/88AM6d+4sTg6iehQt/iPw8xcxI1mcFzzHjx/HwIEDxcmh991v8Xxpvfvffcbg3/9+GlLEZcLg1KlTuPfee8XJQVN/qAh/3LIftQBSZ/8cL44Nzc4MaX08tA6Lt9S6/506AbOfnoEQZSN8+YA7Lz9/cQZCkZWQ5sMqoRxSJ/wcL4aykQlQVJRhfRHWvSkdv6mz8fSLY0NSX8yIivIQHVqHdXgRL46V/1yH+qdD+5vlr6gst0AdWod19U9H5fEaiKjaN0JdjoSoKo9QUpd1/SGse7MemWtmIIJFHxbtZv+GQhQcn3YQsjp4aB0Wl6aozqkPYd3iUmSueTEkx3XI8mFHh9Zhcf3TWCOdN0TjeVq0CnU909wjCOG1WKjz0a5orqFTMSHE9+nai1DX0fpD6/DHLbU81qJVjNybinasf+RWj0Pr3sQWd4OH2S/a/xqbvIuFtsGoB3CnLl3QpWtXcbJP165exfVr18TJUdwD+NAfUZcK7D8kBUlDJOT58CI9cznenbcc744F/uPPfxNnh0VI819fhDdLk/HimjVYs2YNMkvfRFGIdmdI8wEgdbY7D2teHIv6N9fhkLhAkIQtH2vWYE2Igr8IQz4sm/BzpRyi9QQ74mVYX4TFf0zG03I5ZZbizVAdwCZEvDxMUT1gESVio9zMi74SDpzd9o1V7a486g9h3Zul7SL4i/a4fynqhLQO1tZBuWQ9VBrS36qQ5sOGqjeprz9DuWfsJaT1TLpHIF9jPI03sThE1xghzUc71HYv4WkghPdE2pOQ1tFD6/BmaaZyP47HWnRS36PLrAvdPVM7Y/0jwB1HKs2UjqengS3r+CvV3sVq2xBo8BcAunTtik5duoiTzQeAr1+/rvk71IV4qBTIfPFpTNh/CKH8/YvkEMjOc3/Dge/+hgPfNSA940fi7LAIZf7rD9VhwtNttzXHvrgmZE+Jhro+tknG2Am1KA3R70jo81GP+nopibOCKPT5sKqtHKJVpMuw/tB+pGaqevyOfVHpQREJkS4PI7X1h3DokDvVR+F9xWgtN+K+EbWr8lCCv6HpIRiN2tX+pagUyjqYOiEFdVIE+FBpCiakiksETyjzYUeP/I/ZqHuzKKTXPXYUynpWf2g/Jjzddo2RPGM2UkN0zyeU+Wjf6lGHlJA9TN6ehLKOHiqt1dyP47EWreR7U4dQX5uKZB5YfmP9IwBAcgpqt6xD0aFDqE+egTUcPqndi8W2IT4+PuDgr6xL164ew0GbCgBfv34dly9f1ky7ffu25u/gOoTSWqD+UD2Quh9/DFGwDSEOgPrDWRGZHsDRkn+rQlsfwyfU+aiVg7/19Qhl7DPU+bCsLjyBcCsiX4apSJEuPg6tW4zFi2dhVgSfoIt8eehLTU5GspxCeMM3UNFabsR9I2pP5bFnfz0yJ9RiSzt6xL897V+KTiGtg8ljkVJ3CPU4hNKU0L4uI6T5sKWxeHF2XURHsYlFoaxn9XXilNAJZT7ao9ot67Bu3TqsW1ePzJ+HbjSx9sQuddQu+YiE2vp61B/6I958sxTJP28/D4cGE+sfAQCSZ2DNmhcxFvXue5gRvH9J0SEW24Yu3bqJkwIirsdnAFgv+IsQR9Hri7YAs5/G2ORkjH16AmpD1d0ywgHQ9N4/wvi7f4TxY6bjcZxCGK+FFKHMf3Kydgjv+qLFCFX7G8r6KKqvgxIYC7ZQ5yM1eSzGjpVSiPKAMOTDspS2cghhMVgS6TJUH79jX1yDNWv+Bx4RFwqjSJeHsbYAcDSK3nKjyO+behwqKoqa4fsiXx7h88jsGRg7Yw1mt6Nh3trT/qXoFNo6mIyxKXU4VFSKlFCeYIc8HzY19kXMrpPeCUemhLKejc1M1b7mq74etanJIbkmC2U+2qPU2S/ixRdfxIsvzgjpvYT2JJR1VH2s1R86hPpDpaidEJr7H6HMh92lJo/F2BkvYs3PU7AllL2fbIz1jwCgvmgdiuqB5LEzMOPFn2NCbWnU3OugyIi1tiGhY0fEJySIkzWqqqpQVFSEqqoqcZZGfEICEjp2VP72GQDu1KkTevXqhV69emmmh64Q63GoLhWZY+Wb6jMwG1tCdoMsdPnwzVn6W7z+59/i9U3rUd3nR0gRFwiDkOZfuthevG4d1q1bjDfrZiNUIzCENB+qp10XL16M0pSfx+xQ1m1P7a7DuqLQDP+DMOSjPYh4GY59ET/HH7F4sVz3twCZIar4JkS8PGIUyy16RX7fJCMZ+7Fl3Tos3hK6B5vMinx5hN/YF2ejrp28Q6897t9gajt/K2p71yz5JdR1MHlsCvbvTwl5UCTU+bCrsS/ORmq1OJWMhLSeae4RrMPiPwI/D9FNgpDmgygIQlpHVcfaH0u34M1f1yI1RL9RIc1HeyHd+w5Vpxk7Y/0jAEiekYm6Nxe7r5kWv4m6CU+zR307F2ttgzhss+jo0aPYsGEDysrK8Lvf/Q5Hjx4VF9FQry/uwoULrZq5Jp0+fRr9+/cXJ8ecPXv24MEHHxQntxtfffUVHnkkkv36gsMu9ZH5IBnLUIvlERiWW/TivtFiedgb9y9Fml3qoF3yQdHNLvXMLvkg+wp3Ha2vrw/JyFXhzgeRGusfEemJhbbhakuL8u9uPXpoeu2K8vPzcfbsWeXvPn36IC8vT7OM2s0bN3BFWn/AAeCGhgYkJSWJk2POyP+YLU5qd478+xZxUsyxS31kPkjGMtRieQSG5Ra9uG+0WB72xv1LkWaXOmiXfFB0s0s9s0s+yL7sUkftkg+KTax/RKQnFtoGdQC4xx13oEMH/cGai4qKUFZWJk7G6NGjMWPGDHEyIL0DueXiRQBA3MWLF1tv3bqF27dv+5W++eYbcb0x6X+UrhcntTu/zlwgTiIiIiIiIiIiIiIiIiKiIBozZgw6S+/9TRRevyv74osv8NFHH4mTFU899RTGjBkjTgYANJ8/D1jpAbxz506MGDFCnEwUEXd3j61x3YmIwuG7y97fIUFEREREREThZ5f7WLzmJCIi8l/nzp29BoDPnj2Ld999Fy2qnsKiHj164Pnnn0efPn3EWUoAWL9fsc3tWX4P7rnnHtxzz1wU1ohzPfm7fFSq2YPl90j5WL5HnGtrlRvmIcExDAmOeVhXLc4lIiIiIiIiIiIiIiIiiry//vWvXoO/ANDS0oK//vWv4mSN8AWA9xRirhyAFNPcuZi7vBB7YjW4GhOqcFKcZJkqqOwzLUf7CjsTERERERERERERERERmdfc3CxO0uVrufAFgPEdjoiTZEeO4MgHq7Bgyj2Yu3wPGAcmIiIiIiIiIiIiIiIiovZk5syZGD9+PEaPHm2Yxo8fj5kzZ4of1QhjAFhlznqcOHFCSjuwY/0cjJRmHflgAaa0syGKY9cjeFXZjydw4sR6zFHmzcF6zbxX8Yjms0REREREREREREREREQk69OnD3784x9jxowZhunHP/6x7vt/1SITANZIQ9ojr2KzOnj4wQIwBkxERERERERERERERERE5B/rAeAa1bt9LUVtH8Gr69v6j37wV+26avYUYvncuZr3ys6duxyFHuNF12BP4XLN+4bnzl3u5f3CNdizXLVe3XWqmV1e2o656vfgGr/r2Gz+9iyXv7cQNTV7sFxev3ro7Jo9mnXNXV4YNcNqm9l+s2Xh5i7nSf8wDAkOKf3DCqwrqRUXFNRi3ZK2z+SWaOdWlqzQrtMxD5OW7EWldjFsl9fxD79DZfVe5Mqf0VmWiIiIiIiIiIiIiIiIKNQsB4BrPt2uvNt35N1pwlw/pd2tDAWNk1VKQHDP8nswZcEqfHBE+xbhI0c+wKopczWBwT3Lp2DBqg807xs+cuQDLPitXnD6CFZNmYIFH6iW1llnG7PL16BwrrQdmk2W33UsbrP5/LXZjiVTFkDZlJNV0j/2YPmUBZp1HflgFaZMWWX8DuaI0N9+/8qirZw/P6yafHgL8v7x/8F21SRR5YZ/Q94m6Y9R/4Z/zWqbt33JMNz7j1u068QRfL5pIe51rDBY75/xzxMXYr38mePVwnwiIiIiIiIiIiIiIiKi0LMeAP5OCf9i2mNWA8CDMVT+95HvNL1WR46cg/U7dijvlN2h9BY+glVKcHcP/vqB9M8567FD/Y5hVUBZaySW7nAv19YB+Qi2f6q/NDASS9e7t2PHUuXNxVi1pK2XbU3hEqySimXk0rbtWK9eXghIm8ufypEjOAJgjrwtm3OQBmDP8gWQi2DkUmne+qVtgfVoYbD98KMs1OWMee/guOsYbrqO4fjvZuNhZSkd1b/DP6+QPjjq33D8//tHDJFmVW6Yh2wpMPzwCr11bkH2kr3S0iqHj+BzAAt+92f38qp1EhEREREREREREREREYWL1wDwoXVFOCRO1FAFXEdOg9X4L5CGu3UilY+8egKbN7+KR9LaviDtkb9re2ewrKYKJ8Vp8juGVQHGNiOxdMdm5KS5l3vkv7YFSo98px8AHrl0NXIeca8pLedf2rZBCVjvwW+VqOQc/EvOI9L3puGRnNVQYsAf/BVyKNN0/kRz1uNVeVsA7f7AHPyLO2NIeyQHm1XDa0cNj+33pyxq8On2tnIuXj1JCbgOyVqBva4VmKZaus1e5E78T3wOAJiNYk2gthbbitsCw//nOe06l86T/ti0S78X8Lx3UJCVCgAM/hIREREREREREREREVFEGASA61G0bjG21NaJM7T2/LWtt+m0x3QCrP6qgdKhWOD5Xti2nq6KtMcwTQmwLsCUe+Zi7vI9qNGP5XpS90DWJfZyVgesT6KqRghCz/k7PKIsCwBpGKx8gbS8xFT+NEZi6X/Vrt3rd6uH144KOtsvMVcWqroy8m5kCHON/GHRQqwHAIzEgt+JQeIafCsP4Xz4P3Gv8v5fd5J7BusbifzcSeJEIiIiIiIiIiIiIiIiorAyCAADY19cg9nuzoyG9rR1/7U+/DOEAObIu5WA8p7lc3XfC+spDTmr12OOEuk8giMfLMCUKXOxXP9FuhapA7r+OgK5k7H5/IXBnuWqwGtbWq4zCnUomC4L3d7evg2/t20Y7vV/FoZyrq7GUe0UIiIiIiIiIiIiIiIiorCqqKjAe++9h9WrV2PZsmVYvXo13nvvPVRUVIiL6jIIACcjWZykI7jDPwM1n26HEvYbOtgdAK4pxP/+oG2o3/U73O+FPXFivc6wwADSHsGrm09gx471mDOyLdj3waolCH4MuAZVgUQhAQAjcXdaAPmzM3/KwmdvbX335f43LJD/2LQQuSWqmYMGYbj871H/prz/1zOJPYeJiIiIiIiIiIiIiIiIrNu+fTs2btyIb7/9Fs3NzQCA5uZmfPvtt9i4cSO2b9d9UamGQQDYHDn+O+df9N6v6y/1u3P1hwceufS/QnplrE9paY/g1c2bsUN56W5bj9vAietQD1k9FIPThMDkySrpvcAydcBYWl7Fn/zpUn+36h3DAICa79qC69488qoUdNWmVz13R0j5LgvV8NtHvoO55x0AYBIKfjdb+Wv9P65Qvc83DfeNkv552J91EhEREREREREREREREVlTUVGBffv2iZM19u3b57MnsKUAsNsc/J2l4GANavYUYq76Pa9z/gU5OsG/I9s/lQKqNSicq/Ne2JpCzJ27HIV75LBrDWraXhTr7nFr0QcL5krrr8Gewv+t2mb5nbuP4O/k7qpHVmFJ4R5lm/cULoES4xbf0Wsmfz6pvhsf4H9LXZ5r9izH3AX+ry2SfJdFGh5re+EzspfsRaX0V2XJ75D7D+rAriBrBYrnyX9swaoNtdK/UzE9W17nFmT/w++wvVpeDqis3ovcf5iHScryRERERERERERERERERMFx8OBBcZIuX8t5DQCPffFFjBUninQCmT59sED1ftkpmLJgldI7deSc9Tih7m6a9hiUON+RVZgifUYJpIqOfIBVC6Yo61binsEYpnrkSIzEEWn9U7DAoMfyI/+1bcjiI6sWKNusLD9yKXbIefQ3fz488l+Xom117nKYsuADHMFIKCNiRys/yyIt51/ahobetBD3OoYhwTEM9/7jf2L9Ye2yommr31GGgv58xb9hnRToHfLcfyJf6QX8n8ie6F5ngmMY7p24EOsPG2wMERERERERERERERERkQX19fXiJF2+lvMaADZjjunuv3crgUnRyJEjMWfpUqzfcQKbPcYaTkPO5h1YOkf96ZGYs3QH1osvhk3Lwer1c4RA50jMWboeOzYHY5jqaVi9Y712W0bOwfodm7U9ltMewas7dmD9nJHaPI/U2xY/8mdGWg4271gK7SYuxY4Tm/Evgbw010/KsMwB8bcsHsGrJ9zl/LBq6sOjZiP/d/+Xj/f0TsK/rlCizcgr2Cv9OxUv/n9/RvGK2XhYDgRL3Ov9M/Y+l6qdQURERERERERERERERGSR/M5fX3wtF3fx4sXWW7du4fbt236lb775Bj/5yU/E9RERERERERERERERERERkaC6uhqdExIAAIm9eomzsWzZMnGSoZUrV4qT0Hz+PAAg7sKFC63iTDN27tyJqVOnipNjTmJios8ouZ3ZJf+JiYm46TomTo45CY5hzAcBLEMPLI/AJDiG2aKNtyO7/P4GC8vD3rh/KdLsUgftkg+KbnapZ3bJB9mXne5j8VijSGFbT0R6YqFtOHfuXFgCwJaHgCYiIiIiIiIiIiIiIiIioujAADARERERERERERERERERkU0wAExEREREREREREREREREZBMMABMRERERERERERERERER2QQDwERERERERERERERERERENsEAMBERERERERERERERERGRTTAATEREBACHN+KJebl4/bA4g4iIiIiIiIiIiIgodjAATERERERERERERERERERkEwwAExEReSjH6/Ny8YSU3L2CdaYd3ogn5q3C5lMATu3AQlUP4rriVcqyTyzdgTrhG4iIiIiIiIiIiIiI1BITE8VJunwtxwAwERGRoK74Y+xMm4GNmwqwa1MBXh6lP83Q4Y2YvzkJr24qwK5NuZhcU4TXik+LSxERERERERERERERKZKTk8VJunwtxwAwERGRICUpCagpwny5d6/BNCN1DQ0ADmL5vFw8Ma8AO8UFiIiIiIiIiIiIiIgE48aNEyfp8rUcA8BERESiUfOxa9MKLEirw/rFuVhYfFp/mlfjpB7A7vROdn9xASIiIiIiIiIiIiIiRUZGBiZOnChO1pg4cSIyMjLEyRoMABMREQnqijdi86n+mLtqBRakGU9TqysrQ6X075SkJAAHsVd6HzBRWJXmIzt7Eba6xBmBKc3PRvairQjS6oiIiIiIiIiIiMiLadOmYf78+bjvvvuUd/0mJibivvvuw/z58zFt2jTxIx4YACYiIhKkjE5CyeJcPDFvBdbXjMM/ZffXnYZR05QewfNdSZgsr2DUfLw6EdiZn4sn5rnT6wwGkyEXti7yDLL6DLwGGuh1bcWi7Gzkl4oz9JTiQAmQPikTDmmKa+siZGf72DaV0vxs9/LZ2cg296VERERERERERETtWkZGBp599lksWbIEK1euxJIlS/Dss8/67PkrYwCYiIgI8rDPBXh5FICBU/COMnzzfEyAwTT0x9xV0rTc+XhZ/jyACbltwz8r6yXS5UDmpHTAuRelSkTVM/BqWmYeiovXYpbfH9RRegAlSMekTCX8i9K9TqSni9troDQfK0vSkVNQjOLiYizD+/4HrImIiIiIiIiIiMgvDAATERERRZgjcxLS4cReOaLqcqEGQJrDHXhVet3q9Lzd+4YwXejh2/ZZ/d7C3tZd6o5Coy3+W4q9znRM+sUzyFJvr9yLWV5PdjYWbXXB5apRrQ3IzAtSYJqIiIiIiIiIiIgMMQBMREREFGmOTLg7AZfCBcBVuhdOZGF8prsXbW5hGpYVF6O4eBmynIV4Q4nkOpH2TDGKC3KQ7izEFnGE5dJ85BY6kbWsGMXFz6BWXMDruj17IbtK98KZPgmZjkyMz1Jt79Y3UIgcFBQXoyAnHUjPwS9mOeCY5Q4UF+YaB6CJiIiIiIiIiIgouBgAJiIiIoo49TDQ7mGWkTUemYDUi7YEK7OzkZ29EiWaz6Uj1UuPWvdnpUAyMpGXl6kz32DdBsM/I80BB4BMdwTYxzDQmciTg8JSIJivASYiIiIiIiIiIgotBoCJiIiIooA8DHRtaSnc8V91sDZL6qXrTmuDOo6y/rr1h38GULLSPczzyhJAGgba4UgDnIXIzc5GbiGQ84tZmncXO2atdfcwBlDj8hoxJiIiIiIiIiIiIosYACYiIiKKBtIw0CWFhW3DPwPu4CpKcCCAnrPuz9bAHXMtRb7Q/dZ43QbDP2uCxQXIkYat3nqgBMhaJk1ve89vab6qx6/wXmMiIiIiIiIiIiIKDQaAiYiIiKKCNAw0oAz/DADIzMOyLKBkZba75222H8MoZ+ZhWZb8Dt73kTpbOwS04bqNhn9OT1X17G0bthqpWW09g7OzkZ2dj1IAmXnLAHnduYVATgGEUaiJiIiIiIiIiIgoyOIuXLjQKk40Y+fOnZg6dao4OeYkJiaiublZnNxu2CX/iYmJuOk6Jk6OOQmOYcwHASxDD8Epj3K8Pq8AO6W/hsxdgXey+wvL2EuCY5gt2ng7ivbf39L8bKysyUHBWu1Qzvpc2LooF4Vpy1Cclwm4tmJRbiHSlhWbDvZGe3mQNdy/FGl2qYN2yQdFN7vUM7vkg+zL8n2swxvxRP5BTM4rwF09iWUAAP/0SURBVMuj4PV6t654FeZvrgPSZmDjqilIUa/HIl5zUiSxrSciPbHQNpw7dw6dExIAAIm9eomzLWs+fx5gD2AiImofpIvhtBnYuKkAuzatQNbn27FfXExRjtfn5WJh8WlxBlE74Dn8s3cOzHpG1QM4txDO9ByInY2JiIiIiCgUvF3vnsb+z+swJC0FqCnD/lPiZ4mIiMiuGAAmIiL7O/wldgKY/LT8tHN/zF01HxOkQO8Tclq6A3U4jc1L3U9OV25eIU1zPzWtXQ4ATmPzUtXnVUHj/QXieqWntOdtxOsFuXhi3iosXKpel/QZ1d9EkZGJvOJirJVf5GtGZp70/l8pmeo5TERERERElhle7wI49RVKalKQ9bMnMRl1KCnjQ85ERETtBQPARERke3UNDQDGYdIocc4IvLypALs2FWDXmhkYUlOETYf7Y+6qXEyWhs3atWoKUg5vxPzNSXh1UwF2bcrF5JoivFZ8GnXFv8V6uJ+y3jg3BUibgVey+wOHN2L5vhQsWNO23teU3sQHsRO52LVpKV55WP0Udjn27gOGPPxgUIfkIiIiIiIiIvsyvt4F6srKUJk2GhMGjsCkiUDl51/xgWMiIqJ2ggFgIiJqx1Q9eBcXoVKcLXFfUB/E8nm5eEL1XiUj+w8dBNJGY8JAAAMfRFYaUOmSA8ApWPDUCPe/Ro/GEOkp7Lrij7ETKcgabe/3EhMREREREVE4uId/RsoApACYMHYch4EmIiJqRxgAJiKidqIBdcKFbl3xb7G+Zpy7Z++aGRiinS2QlpPSO9n9kZKUBNQUYf68XMzfDCz4mTzklkkDp+CfJgKVn2/Hps/r2oLGRERERERERKZ5Xu+6h38GsK/A/dBz/kGAw0ATERG1GwwAExGR7aVku993tP5/qt+3uxH71Qs1NBj2AE5JSgJwEHsPa6fvP3QQmJgrBYWXYq4UvE11qIZ2li66J4919/oVuZ/CPoidNep3NhFFkdJ8ZGcvwlaXOIOIiIiIiCLN6Hp3c1kZKjUPMq/AgjQOA01ERNReMABMRETtwAi8LL2Ld/4895DP/69jGuZmP4nJ8tDO+Q0Ykta2/KSJQOXmFXhi6Q7UjZqPVycCO/Ol4aLn5eL1w1LwVn6ael4unpjnDiqnZC/FqxPrsH6xNLT0xFy8rPM+JgDAqIcwGTB8ZxO1U66tWJSdrQ28urZikV4gVllWlRZthbgYERG5sHWRZxtZmi9N02lP80tNtMk6nxO/Q/luZRlxXcLn80s1nyYiIjKmd737EPB5HZCWhFRluf6Y8LDqYWUiIqL2pp1dezEATERE7cPAKXhHGMIZGIGXlWlL8c6qAiVQOyFXmr7K3StX+VtKL486jc1/VPUAXjMDQ1S9hDXL50q9f0fN1/QU1pj4ECaI06idS0d6uhN7S82FctNzClBcXIzi4mXIchYi1yP4EKDMPBQXr8UshziDiCjWOJA5KR1w7kVb01qKAyVA+qRMyM1c1rJiqT0tRl6mvJzvNtm4HXZh66JcFCIHBdJ6l2U5UZirfahH+fyyLKDkfc8HfoiIiGSj5kvXpdLfHte7IzB3Vdv1rCwle6nxNSkREVE7EZlrr1LkZ2djUXi+DGAAmIiIKFD9MfdpVQ/gxUWoTJuBef724j38JXbCeIhoat8mPZMDFG6Bf88iZiJvWRbgLMSWUnkI53zk52cjOzsf7kk6vdRK85G9aCu2KvPcy8pPR+Z7rEvdw03s2RbeE1oiIrMcmZOQDlUg1+VCDYA0h++nXMy3yWI7vAWFTiDrmVlKkDlzdo52O1RcrhpxEhEREREREQWZeO3l2rrI/P0yo+WlQK92ugtbF61ECQBnYa76K0OKAWAiIqJASU9dK0l4utoU8cltIjVHJiall+CA72iDliMV6QBqXHJgoQQlWIbi4jxkluZjZUk6cgqKUVyQg3RnId6Qg7XOQuxNLXBPRwne1w3ilgDj2z67pRRwbX1D6dlWkJMOpOfgF+wyTETRyJEJdyfgUrgAuEr3woksjFd6+gIlK8ULePVnTbbJqnbYfVMhHanqZtHhQBoAZ23bNzgLc5GdnY3cQiCngCMvEBERERERhYLutVdpPnIL07BMNaqT1/tlhstnIk8a+ant3pkDs9YuQ5bU+zhcGAAmIiIiiloOzHomCyXvWx3OOR05s93RjVL3WKfIdKgCIUoAIh2TMh26gYk2QhCDiCimqIeBdqF0rxPIGg9V/LdtCOi1bT123YLVJrdJVzWo6TnyDQX9nsFERERERERknd61l/vB3RKszM5Gdra7t67qEx73y4yXV42Sl1sIp2Y94cUAMBEREVE0y5yNHKjfV2mCqxZOk0OaBoPDkQY4C5ErPz35CzFoQkQUPeRhoGtLS+GO/6rDvz6YbZNV7bDDkQbACc0zNUZDTztm4ZkswGlqqGkiIiIiIiIKiO61V5bUo9ed1voclslzedfWN1DolKYX5CBd/EgYMQBMREREFNUcmPVMGgrf3yvOMFCK/JUlQHoOpE6/Go5UuecbAJcY/JCefJQCE2aDIqUHSoCsZdIJL4ctJaIoJ41+UFJY6DH8s29m2mShHc4cjywAJaqxo0u3GH935vgsACaHmiYiIiIiIqKAqK+93A/uGl2Hed4v8768RHowOFIYACYiIgqlwxvxxLxV2HxKnEEBK81HdvYi6L6e1kggn4kmmeOR5XR6PWmU31+Snb0SJVnLdIYudXPMWotlWU4U5kpD0WQtQ54SgEgH9ua6pxsEkPVkjs8CSlZK35+N7Ox89lwjoigmDQMNeAz/DPU7gLOzka/XmBm0ycbtcCbyCnKQrmonV5ZkYVlxnsd3A/oBYyIiIiIiIgoy9bVXZh6WZRldD+rcLzNY3jHrGWTJQ0OvrEG60gU4E+Oz3NeN4RJ34cKFVnGiGTt37sTUqVPFyT6V5mdjpTwYdtYyFOdlAq6tWJRbiLRlxaobkFCmO5He9iJm11Ysyt2LSfLfFiUmJqK5uVmcHBhle1XSc1Ag3IB1bV2E3EKnap4LWxflolC8g5Ceg4JfAG8I68wSy8kCy/k3medQS0xMxE3XMXGyp8Mb8UT+QQDA5LwCvDxKmn5qBxYuLkKlOD1QhzfiifwGLFizFHMHijONJTiGmcuHh9PYvHQF1mMGNq6aghSPv8Mr8Hy02V+Qi+X7pD8m5mJX7ghlPw1W7aO64lWYvxnuskbbfpQNmbsC72T3V01p4/5sHZCmKidVXVAI36+ep64vuusLUDDK0IjudurkLRL5NhJweZzagYWLy5BlUD9Cuc2KANuDYEhwDGtr40vzka38AAe5rQ73b0FpPrJX1rSdG5gRyGdCyPLvbygEXEbSeUyaj/M6L0JaHj7qvud5mUGdzlqG4jyH8Tmbur77OoeFZxm5twPu5V1t26w571NtV9ayYuQ5PLczPafAPUSRTh6MPqOck4dISPdvlDF7rWO0vwFVfTKquzrrk+u50T42mh7qfR8t7FIHYycf4vWt2BYatFs+jiHzdVpqq6Ftm0vzs7Gypm2aZ/svbrckPQcFz9QiVz7GMmEyj+K04N3HCCXdembUHqnbnky4e7+r3n+WnrMMk/au1C9T6V6HYdso/VZ67l8vdULVnOnmg7zzuT/bjlXP44f8ZfY+lu69kSiiuea0C502JnTnTMbHGfnGtr6dMDoPcc80PIb4W9V+Bb1tCPh+mbFz586hc0ICACCxVy9xtmXN588DYe8BXJqPlSXpyClwj4e9DO+b6ImTjvT0thcxx4L0nAJpCMRlyHIWInfRVrRtvQule51IT1cNvwgHZq0tRnFxAXLSpUasuFjTcydrWds44iE537DIe56jTQqGpAE7D5UrU/Z/VITKtBQM0Sznj3K8Pi8XC4tPizPCpD/mPj0OqCnCpsMATn2Fkhpg8tMhDmyFyuGNWL4vBQvWFGDXpgK8io/96j05OU/63ESgcvN27BcXAACcxv7P6zAkLQWoKcN+Yf1D5q7Ark0F2JU3Dtin/X55/bs2qR8W8L6+6OF9O+2Wb/exPRoTVIFXJY+bcjG5pgjzl+5AnfpDwTZqPnZtCn/w10jWMun9E85CvOH7R1ilFPnZ2Vjk5TNh+y3IzDMxzLCwvaY+Q4FxYNYzqh7Auf71Hg4X/bqvd17WRqnTy7KAkvex1eX7nE31aYvnsOlIT9cZMjY93eP9MfJ54jKPd9cYn0N65k31IQpMQNc6bfTrqPF0X7jvKTKkwCik9rG4WBp1QjsKh2675eMYMl+npR7emna9FAdKgPRJmVJ7rdf+m23jzeTR6m9AdPLeHkk3YOVyKy7ApL0H4DBVpsY892/bPKM6QcGgtz/lcwy944dCwvDeiNl7UGaXIz3e2h/zvF1HezvOiEjkeR7i7RjibxURwh0AdrlqNH9n5pm7ETvpmRxAuJklK81v616dHaobzQHLRJ77ihZb5I13lWKvMx2TfvEMsuRxw21FzLP7REe7j1zYuki7v0rzw7v/sh4eB+z7UgoMlmPvPmDyw6M1y+wvyMUT86QkB4gOb8QT8zbidXne0h2ow2lsXlqAnQAqN69oWxZAyf8UPh9Ko6ZhgRTY3v9RESoxDpNUPTQ98iJdCHhM1+Rxo0HwNLTqGho0f0/IDUHw7NRXKKlJQdbPnsRk1KGkTP+CSNwWQybXF3Emt9Me+XYf20MeftDgQYgReDlP9eCETt03bAeW7sBmZZ50nBhNP7UDC+fl4nWP71Afj6exeanqu0J9ke5wIA2As1Y+YRbbafdN2OzsfOTnZyM7exEWLXI/UekszDXRXou/Be4nLz2+Q/hueViVtmWlG6mabclHqWsrFsnLl+Yje9FWbFXOB/JRChe2itur/ozR+YPme8L7uxQVrATJM/OUG7DFft7YDStN3Td/Xiaew5rl7RzWjEmTsoCSA9Ln3cGLrEmTxMUsCTRv5EksS7PXOhpiHfU13QJxe4mConQLCp1A1jNtvwOZs3OQ7qWNlYl10t9jSP15R+Yk7XdK7+pKc0grNNn+6zKZR6u/AVHLqD0qPYASqMvFgVlrDYY5D4BYPyjEvO1PK8cP+UW8LnffG9G7B6V3f0dnOfXridTXqcLn3dNIJrY/uteSutN1rks1KzI6zrxdo0vXyJrrW1/X1e3w2pbsS30eYngM8beKgszK/bIIC2sA2D32tfTOOX/ew+fIxKR0nZcpq58QNnwKNcIcqUgHUONyb5erdC+c6ZOQ6ZDG+95bauoHWBlHPBZ+sDV5zkSefDNY2kdbSsUnssWnscNg9EOYjIPYexjA4S+xE+MwSR3/VT9luWYGhtQU4TUlGHMQGNs2fdPh/pi7KheT5Z6FynCydRj8tHo51fpDoj8mPJwC7CvA8n3AkLnTMAHuvMzfnIRXVT0e3XkZgZel3pye23gQO5GLXZvmu9cRZinZ7mDi+sW5Ab07dWe++6JFUw6CurIyqWfoCEyaCFR+/pUmSF+5eQWemJfbNry0KgAtr18d2Pe1vmjhazttle9TjagCMDhJfwhwAEBSEoYAqGpoO76Vuu+tHagpQoljhXs6DuL/9TVdQ2xDgLri37qHbN9UgI1zU4C0GXjFYOjyoJBugqanOgzaaXnBEpRgGYqL12Lt2mXIkp+CNhPcU/8WlOYjtzANy4qLld7Bb2x1wbX1fdWTmlLPjdJ85BY6pR4dz6BW2Rh5W3RuJDoLsTe1wL39KMH7W4FZ3rbX6/lDCTBeryzIFjR13/d5mfw+T2U4Sp8VX2B0DmtW5nhkQfp86QGUIAvjPQ6AtvPElSVAes5szTFidA5pOW/kIeBrHTWhjvqc7gX3PUWC+yZ5OjRVVSdgqNdu+TqG/KrTjky4Lznd7bqrdC+cqjbUV/vvjdk8Wv4NiFYG7ZG7XPR/p6zQ3b8SozpB1nnbn1aOH/KP/r0RvXtQevd39JbTV1f8MXamua9HtSN+tW+67Y/RtaTudO/XpcbHmbdrdE/G19We1+BEMU91HmJ8DPG3ikgW1gCw/ANWkJMOSBd2bS9R9sY9tGDJ+9qT+lJ31BCZ6gs88SnUqOIeegBpDjgAZLpbH1NDEChDG4k3saOe1Ns3WxoSUpqqfiLbtfV9lCAdkzLDmbP+GCT3lj10EJj4kCZIuP/QQUAeNnbgg8hKAypdciAnBYOSVAsbMrtc8LgvDgBgHP5JCh65nxg9iOXzcvHEPPfTn26qHofie1GRggVPRfK9Mu6Ll41zUwDpYsefJ1CVoYrzxqFy8wqdz7qHLUbKAKQAmDB2nMfwxUPmykE8z16tyvqVCyjf64sOvrfTVvluaECl38dhW9331Q5kje4PDByAwTAzXc3fbQqukpVSe5y1THovin477ZaOnCCM4+s+KS/ByuxsZKvezeJwpAHOQuSqbvJqT+AzkaeM5+dtW6TfEL2brzq8nz8IN3TJNvTqvq/zsvQc+cGCQJ8Y1j+HNc+BVGkY6NIDJUDWeM8HINTnicuy4CzM1ZxfG51DWs8beQr0WsfNs456n+4L9z1FG3XAUL/d8n4M+Ven1Q8dS+290ob6bv8DpQ2KWv0NiD6BtkdW6O9fN6M6QaEUuuOH9Ji9N+Lt/o5vKUlJQE0R5gfwAL6d6bU/RteSRtMD4+0a3ZPxdbXnNThRLDN/HsLfKiJZmAPAbo5Za91PH6l6xvqUORs5iMED1VULpzzUlKsUe51oe0feyhJA5yIm5qny7Nr6BgqdWe4nzgpy2t5Z55iFZ7IA594t2LLX2XaSFDZCb1lHCHvahZU7sI20JKRqpo+TegC70zvZ/d09Dmuk6WtmWHj/ceikZC9191rW9NDU/turUQ95fBZoe0cy9hW4L5DyDwI6AU8MnIJ/8voeYYnZ9UWa2e20W769aWhApa9ewmHQdsEt9b7+mfHT2VYpN8qkwKphO22V+vcPACB9h5TWznJIQ6gUICfdfZNX/71IRMEh1n3T52XyOUugw3h6OYf1fR4sBTBKVrp7yfl6OiFzvH/n11bzRrqMrnV87RePOupjuiXc9xQiDkcaACc097zF4ZfVdNoto2PIK506LT90XFvqbu+z2rr/mmv/DfiVRy+/AbHId3tUA7O7TGZqH+vsXwoHnf1p8fihwBjdG5FZvr8zaj52bVqBBWnuIHNIX0cUa0Le/ngeZ35foxteV+tcgxPFMP3zEM9jiL9VRG3CGgAuzVc9wWt0gWTIgVnPpKHw/b1tU1JVwwhLB7ZyURcVSpHvHtMKszPbhp1q+/EtQI5qWCp70OZZQwoGyNxP35SgRHh/UrikjB4tnRRLPfZUUh0pbT0ZpSDX5LGR7BEbuJSkJEAe7tqIFASLFvsLVE+1qofxlXthKsMMSz1Q5V6aosNfYqdOcK+urAyVmqD4CizQrLfNhLHjfJafP+uLJH+20xb5TkrCENSh2vB1xuV4Pf8gkDYD83SGuPLeDkiBbql++p7unXskglypHEPwzmuzhHY6cNrfAveNUs8hEF1b87HV5cCste7fQyg3VeUT+FLkm+o+J53IS+cWvs4Fov/8gcLBn/OyzPFZunXYHM9zWHFoUuUJZZ0H4twBDLT1dPdGegeS+fNrq3kjNcNrHT/2dzhx31NISAHdElXFKt1SqBl+WUPVbhkeQyZ51Gnp2Csp1H6/P+2/Lr/yqPMbYFPKEN5vqN+HmW8cMPGzbfTYvxRSRvtzq9Xjh/xieG/EG5P3d9zX89K/izdi86n+mLvKfU1PWur2x+ha0mi6N0bHmaaZM7hGd/+WSf82vK5mm0n2ZnQM8beKqE1YA8CZecsA+R0t7hcouN9LYFbmeGQ5nW3DCM9ai2VZ0juCpO7/fq0vROR3RGRnr0RJ1jJpOCL5YiZVFegU34VrTHm3TbZ/Q8mFi36e5YZYGnJkZQ3S1Y+tSRfORmP1h5wUTNQLHqZkL8WrE6X3rCwuQuXEXB/vQJHef7p5heb9qFFh1Hy8OlH1/tZ57gsI93DR0tDQ+Q0YEkUn+RNycwF5excXAXNXSOUvvcNG6in5xLwV7qdchXfZKHnNP4ghymdlctBY3Uta6hFeU4b9YrBQ6kW881C5Mklblj7WFzXDJ/nYTjvmWxqGWXxCWn7P8RPzCrBzYq7hu5C8twMpwOcr3NM1AWSj6d5NGDuurSf1vFw8MW+j997XQeS1ndaQ3ptSmGv4njWj3wJk5mFZludvmSMzFXtzs5GdnYtCZxaekXoFK7/t2e8j1eNpIj3pwN5c97mA8gCS8fZG6/mDhmsrFkXpb749+HlepnOz3y/COSzgcL8PzFmI3Oy2Y2CZ3hCW0g1yoxviUJ8nrixBunB+LR53HqzmjRTG1zp+7G8/tO1b/QAL930wlCJfKsPsbHWPGtXQjNnZ2vfVSu132zzh/aQ683X3T8zKRF5BDtLlHhfZ2VhZkoVlxXn67ydXtVvGx5DwGaMy86jTUrsOeA7/bLb912UujwqP3wC7kspFaeuy8X6q9r30Wn62jR7710SdIAv09ud4wPLxQ/4wvjeivQcFw/s7wr2qUdOUXr7zXUnSK8SAlNFJKFncdo9FfqUYSVTtj9G1pNF0b9el+sfZbMwyukbPnK308s2tTZPuqXq7rmY7SXandwzxt4pILe7ChQut4kQzdu7cialTp4qTY05iYiKam5vFye1GZPNfinw5SGDxzntiYiJuuo6Jk2NOgmMY80EAy9BDoOWxvyAXy+tmYKNBkDcghzfiifwGLFgj9NQ1mu7TaWxeugLrU3KxK3cEcGoHFi4uwuC8Ah8PnviW4BgWwTY+TErzkb2yBjkFaxFLI1r5/P11bcWi3EKkLSuOvuC0Iffvek1Ogd/Di/ksD4pp3L8UaYHVQelaJT0HBdIDvVsXbYFj7Wy4FuWiEPJ0d+/vlSXp7t8iuNtvKG2hsB4L7Xtg+SDyj13qmV3yQfZlp/tYPNYoUtjWE5GeWGgbzp07h84JCQCAxF69xNmWNZ8/D4S7BzCRhjTcl68hUYiIAjXhqRkYEi09kg31x9ynVT2A/ew9TO1DaX7bk9ttT45re6a5n+jWm6bl2rpImt/WY013/aX5bcuoeySX5iM7Ox/58mcWbYULLmxdtBIlck9wj6fbiYhijHytoryqxoFZa/OQWboFhcIrbDJn5yDd8L1imchblgU4C7FFp00mIiIiIiIiCgUGgClyMvNQXOz/k+9ERKYNnIJ3gv1O3VHz9d/TazTdjFHzpff/SimYPZbtLjMPxcWx1fvXb6X5Us+yYhRLwxu9sdUF19b33T3KpPfa5GVCd5q4rtxCJ7KWFaO4+BnUbik1XL93JcD4tuW3lErDOAJIzyloG/6biChGuVw1uq+qcU9PR6q6kXM4kAbAWWvQdjpSkQ6gxv2Ce0A9dC0fmCEiIiIiIqIQYACYiIiIKIqVHihpe/+r9D5YZ60LDkca4CxErqonr940NW1AIxN5eZmG6/dOCH4QERHS/WgY3Q/iFPOBGSIiIiIiIgoJBoCJiIiIYlFmHoqLC5CT7kRhbjYWbXXpTyMiogDVQNVpF5AftIETmudkXC7UAEhzGIRyXbVweptPREREREREFGQMABMRERFFMUdqOuDci1IXAFcp9jqBrPGZcG3Nx1aXA7PWFiAn3b2s3jQ1d+BCDmiUIj+/1HD9aq7SvXBqphAR2Ztj1jPIghOFb7QN0Vyan4/SzPHIAlByoO2FvqVbCuHUGS7arRT5K0uA9BzM1p1PREREREREFHwMABMREenYX5CLJ5buQJ04IwpE87ZR8DlmrcWyLHeP3uzcQjizliEvE3BkpmJvbjays3NR6MzCM7McutM0MvPa1pX9PlJnZxquH5mzlZ7EubVpyNKuSUcmxmcBzsJcvtOSiGwgE3nSe85zs93v630/dTYy5eklK93v8M3OxsqSLCwrzoM6vusszJXmr0RJ1jKPoZ6VdwBnZyO/LZZMREQUEH+uEf1ZloiIiGJX3IULF1rFiWbs3LkTU6dOFSfHnMTERDQ3N4uT2w275D8xMRE3XcfEyTEnwTGM+SCAZehBtzxO7cDCxUUYnFeAl0dpZ1lXjtfnFaBq7gq8k90fAFBXvArzN9cBaTOwcdUUpIgf0WH0mf0FuVi+T/pjYi525Y5Q8lOJFCxYsxRzB8p5LEOW/Deg3bak7Xgi/yAmG5RBgmOYLdp4O7LL72+wsDzsjfuXIs0uddAu+aDoZpd6Zpd8kH15vY+lvg6EfJ2oIl9DKuRrxFxkfV6A9ZCvP09j89IVqr/Vy+pc68o016ji9agWrzkpktjWE5GeWGgbzp07h84JCQCAxF69xNmWNZ8/D7AHMBERkY7DX2InUpA12n1BDJzG/s/rMCQtBagpw/5TwvK6DD5zeCOW70vBgjUF2LWpAK/iY2xW1peCIWl1KCk73bYakce2ERERERERkV3s/6gIlWmjMUEVdB0ydwV2bSrArrxxwD71NaT6GnEE5j49DqgpwqbDAE59hZIaYPLTqgeYhevJ/QW5mL8ZyvWp5hp14IPISqvD+o/KVV9GREREsYIBYCIispX9Bbl4Yp6UlGGtyvG6PG1eLl4/bDRNWsehg4D6gvvUVyipSUHWz57EZKgDtKexeanq++blYmGxNM/gM3UNDdJn3Sbkap+mznp6BrB5O/arF1Lx2DYiIiIiIiKyiXLs3QcMefhB3VGnxOtJiNeIo6ZhQRqw81C5O5CMcZikGi1Ks+zhjVi+D5icp70mbbtG7Y8JD6cA+740vD4lIiKi6MUAMBER2Ye6d+2aGRhSU4TXik+jrvhj7EybgY3SE80vj4LuNDfPC+66sjLpCewRmDQRqPz8K9QBqCv+rXs4rU0F2Dg3BUibgVfkYbQMPpOS7Q4Ir1+ciyfmrdI+uQ0ASQ8iK+0g9qoC0m08t42IiIiIiIhs4lQjqgAMTtKO+FS5eQWemCf31tW+Ikh7jSgHbQuwfB8wZO40TFDWol3WHUxOwaAkadhp5cHmtuvUlKQkAA2oE69biYiIKOoxAExERLaheZp54IPISgMqXafdF601RZgvXsgK0wDPIbHkoZyRMgApACaMHWdiGGhvnxmBl+WAsRQIVvc+Bvpj7tPjsPOPcu9lFY9tIyIiIiIiIttoaEClHJRVGTJ3hfshZ82IVPrXiO6HjgFgHP5JekDZaFnFwCl4Rx5iWi0pCUNQh2rPjsdEREQU5RgAJiIi+xs1H7s2rcCCNHfAdWHxaf1pYhAZbe9Nwr4C99PQ+QcB6aK7LYgsPYn9M+ndSl4+I0vJXopdm3IxGUBVg/DO31HTsABl2C9cZHtsGxEREREREbUPA6fgnyYClapXBulfI/bHoDQAaUlIVU0Vl3X37mVwl4iIyK4YACYiIttIdaS09bSVgrCTx45AXfFGbD7VH3NXrcCCNPeyetPEIbEgD+WMcXhVGiraHTR2D+m8+dBBYGKuNL1tGC6vnylQ9fg1GN7L3Qs4Cev/WKaa5rltREREREREZCM+etxOGDsOgPzKIH+uEXWWld8XnL/R+B2/Bj2SiYiIKPoxAExERDFtZ778nqKNqM1eilcnSu/XXVyEyom5eHkUkDI6CSWLc/HEvBVYX+MeBktvmueQWNJQzponp6V3KtWUAY5xbb18pW3Y7+szT+UC8jYvLgLmrlC9f1hl1EOYXFOHSvlvj20j23NtxaLsRdjqkv+djWz5b3G+VaX52nUHQzC3j4iIiIioPRg4AIP1RomSjXoIkwHsPFTu3zWi7rL9MXdVAV6deBDL5Wva/IMAkpAiP9zc0KD5m4iIiGJH3IULF1rFiWbs3LkTU6dOFSeH1Mc7PhMnWfbTWdlobm4WJ0clu+Q/VPm46TomTg6pLaXfiZMsYz5iE8tQK5bLY39BLpbXzcDGVdJQzl6dxualK7A+JRe7ckcAp3Zg4eIiDM4r0A/o+hCqcgt3G29Hofrd8rVvSvOzsbImBwVrZ8Hh2opFuXuBdCcwqQBrZzncAdbcvZhUsBazHOKn/VSaj+yVNcgxsa5IlQeFB/cvRZpd6qBd8kHRzS71zC75IPsKVR01usY1e11qdjlIy9aPXCxOtozHGpkVquOI9Y8otrXXtuHcuXPonJAAAEjs1UucbVnz+fNALAaAn3n6SXFywN7/48cxURlkdsl/qPJhdOIcKltKv2M+dEQqH5HEMtSK3fIox+vzClA1dwXeyTbxBDUAHN4oPSEtSTN38a0nVOUW7jbejkL1u+V935QiP3slanKEYO+ySdi7shbPFOchUx0AdqkCuNiKRbmFSFtWjDzHVizKrcWknBoUFjoBAFnLlgErV6LE/QeK8zKVAHB6uhNOJ4B0KfAMwLV1EXKlzyI9Bwt/fFcEyoPCJTL1naiNXeqgXfJB0c0u9cwu+SD7ClUdNbzGPbUDCxeXIWtN22uGPPlz/epeNv1ni0OSDx5rZEaojiPWP6LY1l7bhnAFgGNuCOjW1tagpVgk5sFKiiRxW6ykSBK3xUqKJHFbrKT2SiwHK8kOxDxZSeEzAi9vKjBx8awyar70jl8pBRj8lYl5t5IouMTytZJMcblQAyDNIXTHdWRiUnoJDpRqJ3tXgsLaZ1BcXICcdKBk5ftILShG8bIsoOR91RDN7t7FxQU5SHcW4o2tLqA0H7mFaVhWXIzi4mXIchYCkSgPCitxH1lJRIEQ65GVFEnitlhJREbEumIlRZK4LVYSUSiI9cxK8mngFLyzyVvwF35ev7qXRbjzQSQQ65CVRET2IR7fVhJpxV4AOIgpFol5sJIiSdwWKymSxG2xkiJJ3BYrqb0Sy8FKsgMxT1ZSeyLm3Uqi4BLL10oyxVULJ9KR6jEcswOznslCyftb4c+rdbPGZwJwwJEGIH0SMh0AHKlIhxO1yorSMSnTATgcSAPgrHXB5aoBUIKV2dnIzpZ6DevkyUqi6CPuIyuJKBBiPbKSIkncFiuJyIhYV6ykSBK3xUoiCgWxnllJkSRui5VE5C+xDllJRGQf4vFtJZFWzAWAPfaolRSLxDxYSZEkbouVFEnitlhJkSRui5XUXonlYCXZgZgnK6k9EfNuJVFwieVrJVmVORs52ItSfyLAlmRJPYDdCdDJk5VE0UfcR1YSUSDEemQlRZK4LVYSkRGxrlhJkSRui5VEFApiPbOSIkncFiuJyF9iHbKSiMg+xOPbSiKNmAsAi126raRYJObBSookcVuspEgSt8VKiiRxW6yk9kosByvJDsQ8WUntiZh3K4mCSyxfK8kUj965ag7MeiYNhe/vFWcAAFyleyG9sddPTuwtdSnDT2eNz4TDkQbAc8hpMU9WEkUfcR9ZSUSBEOuRlRRJ4rZYSURGxLpiJUWSuC1WElEoiPXMSookcVusJCJ/iXXISiIi+xCPbyuJtGIvABzEFIvEPFhJkSRui5UUSeK2WEmRJG6LldReieVgJdmBmCcrKeYc3ogn5q3C5lPiDN/EvFtJFFxi+VpJpkjDMNe4dCPAQOZ4ZDmdbYHezNnISXeiMDcbubVpyNIubVIW0mpzkZ1bCGd6DmZnAsjMw7IsoGRlNrKz3Qk6ebKSKPqI+8hKIgqEWI+spEgSt8VKIjIi1hUrKZLEbbGSiEJBrGdWUiSJ22IlEflLrENWEhHZh3h8W0mkFXsBYJ2ofqApFol5sJIiSdwWKymSxG2xkiJJ3BYrqb0Sy8FKsgMxT1ZSeyLm3Uqi4BLL10oyJxPjswDn3lL3u34ds7C2eC1mKe8EzkRecTGKlWkOzForDdOcl4e84mLkZcqfk/4NIDOvGMVrZ8H9EdW8zDwUF+chL09ah7yM/BlhCGgxT1YSRR9xH1lJRIEQ65GVFEnitlhJREbEumIlRZK4LVYSUSiI9cxKiiRxW6wkIn+JdchKIiL7EI9vK4m0YjAAHLwUi8Q8WEmRJG6LlRRJ4rZYSZEkbouV1F6J5WAl2YGYJysp5oyaj12blmLuQHGGb2LerSQKLrF8rSSzMmfnIN0Zznf9mifmyUqi6CPuIyuJKBBiPbKSIkncFiuJyIhYV6ykSBK3xUoiCgWxnllJkSRui5VE5C+xDllJRGQf4vFtJZFW3IULFwIqlp07d2Lq1Kni5JD6eMdnmJn99+JkAMCv1/zfyr9v3byJGzdu4IfrP+D6Dz/gjV//WrOs7MPiP+Ons7LR3NwszopKdsl/qPJx03VMnBVSW0q/Yz50RCofkcQy1IrK8ji8EU/kA5MnHsTOfQDSZmDjqilIAVBXvArzN9cBSMGCNe7A7f6CXCzfJ31WXvbUDixc3ICsuQ1Yv7kOADA5LxfIL8BOAJiYi125I4BTO7BwcREG5xXgZRh972lsXroC62vaNnHhzxaHpNzC3cbbUah+t2J137A87I37lyLNLnXQLvmg6GaXemaXfJB9haqOWrrGDUCortV5rJEZoTqOWP+IYlt7bRvOnTuHzgkJAIDEXr3E2ZY1nz8P2KkH8C/+9V9x8+ZNXLt6FS2XW3DpUjMuXWzGr1f/2mPZWH4aQMxDrOZf3BbmQ1xzeInbEqv5iCSxHNp7GYp5io7yOAiMLcCuNTMwpKYImw67A8PzN9dhcl4Bdm16EtUflQOHN2L5vhQsWNO27GvFp5V1rHc9iV2bVmBBGrAz/2MMWlOAXXnjgH0fG7z31/N764p/i/WYgY2bCrBxbgqQNgOI2nIjcN94EPPU3svDbsR9xP1L4SbWo1itg+K2xGo+KLqJdSVW65m4LbGaD7IvsZ7Fah0VtyVW80GxSaxDrH9EBLYNIRV7AWAv/7285H/g0qVmNF+8iObmZry19i2PZdT/xSIxD+r/Yin/4rao/2M+wk/cFvV/sZSPSBLLQf1feyxDMU/q/yJXHikYlKSdUtfQAGAcJo0CgBF4OXcE9h86CKSNxoSBAAY+iKw0oNIlB4CByWNHAOiPlBS0LZeUhCGoQ3WDeu0yz+81IuZd/V/kyo3AfeNBzJP6v/ZYHnYj7iP1f9y/FA5iPVL/F0t1UNwW9X+xlA+KbmJdUf8XS/VM3Bb1f7GUD7IvsZ6p/4ulOipui/q/WMoHxSaxDqn/Y/0jar/E41v9H9sGa2IvAKwT1Ven119fjUvNzfjf/7vAY56YYpGYBzHFSv7FbRET8xFe4raIKVbyEUliOYipvZWhmCcxtbfyEKUkJQE1RZg/LxfzNwMLfjYFYLlFNbF8xdTe9o2YJzG1t/KwG3EfiYn7l0JNrEdiipU6KG6LmGIlHxTdxLoiplipZ+K2iClW8kH2JdYzMcVKHRW3RUyxkg+KTWIdEhPrH1H7JB7fYmLbELgYDAC3+kwbfvv/eEzTS7FIzINeioX8i9uil5iP8BG3RS/FQj4iSSwHvdSeylDMk16KhvJISUoC0IC6UwBQjtcLypHqSAFqyrD/FIBTX6GkRu71Gzz7Dx10vzN4UwF2bXK/dxgxVG7tkVi+eqk97RsxT3qpPZWH3Yj7SC9x/1IoifVIL8VCHRS3RS/FQj4ouol1RS/FQj0Tt0UvxUI+yL7EeqaXYqGOituil2IhHxSbxDqkl1j/iNof8fjWS2wbAmMQAK5H0brFWLxuHYoOifMiq1Unqh9oikViHqykSBK3xUqKJHFbrKRIErfFSmqvxHKwkuxAzJOVFFKj5uPViXVYvzgXT8z7GIOeGoGU7KVt0xYXoXJiLl4eJX7QmgljxwH7CvDEvFwpbQRiqdzaIbF8rSQ7EPNkJVH0EfeRlUQUCLEeWUmRJG6LlURkRKwrVlIkidtiJRGFgljPrKRIErfFSiLyl1iHrCQisg/x+LaSSEs3AFxf9Cbw9BqsefFpYMs6RFMMWIzoW0mxSMyDlRRJ4rZYSZEkbouVFEnitlhJ7ZVYDlaSHYh5spKCYtT8tp62A6fgnU0FSlB3Qm6BR0/ctmkF2JUr9f7V+9yqKUgR56n/rfu9p7H5j6oewGtmYAgOAtFYbqQQy9dKsgMxT1YSRR9xH1lJRIEQ65GVFEnitlhJREbEumIlRZK4LVYSUSiI9cxKiiRxW6wkIn+JdchKIiL7EI9vK4m0dAPAyTPWYEYyANSjDilIFheIoNYgplgk5sFKiiRxW6ykSBK3xUqKJHFbrKT2SiwHK8kOxDxZSfbTH3OfVvUAXlyEyrQZgE7erSQKLrF8rSQ7EPNkJVH0EfeRlUQUCLEeWUmRJG6LlURkRKwrVlIkidtiJRGFgljPrKRIErfFSiLyl1iHrCQisg/x+LaSSEs3AOxWj6LFW5Dy8xnRFQDWieoHmmKRmAcrKZLEbbGSIkncFispksRtsZLaK7EcrCQ7EPNkJdnSqPltPYw3uXsSg+UW1cTytZLsQMyTlUTRR9xHVhJRIMR6ZCVFkrgtVhKREbGuWEmRJG6LlUQUCmI9s5IiSdwWK4nIX2IdspKIyD7E49tKIi2DAPAhrFv8RyT/XO4JHEVag5hikZgHKymSxG2xkiJJ3BYrKZLEbbGS2iuxHKwkOxDzZCW1J2LerSQKLrF8rSQ7EPNkJVH0EfeRlUQUCLEeWUmRJG6LlURkRKwrVlIkidtiJRGFgljPrKRIErfFSiLyl1iHrCQisg/x+LaSSEM3AHxo3RbUpgKlf1yHdeuKUC8uEEHi/rSSYpGYByspksRtsZIiSdwWKymSxG2xktorsRysJDsQ82QltSdi3q0kCi6xfK0kOxDzZCVR9BH3kZVEFAixHllJkSRui5VEZESsK1ZSJInbYiURhYJYz6ykSBK3xUoi8pdYh6wkIrIP8fi2kkgr7sKFCwGVy86dOzF16lRxckh9vOMzcZJlP52VjebmZnFyVLJL/kOVj5uuY+LkkNpS+p04yTLmIzaxDLVYHoEJVbmFu423o1D9bsXqvmF52Bv3L0WaXeqgXfJB0c0u9cwu+SD7ClUdDfc1Lq85KZJCdRyx/hHFtvbaNpw7dw6dExIAAIm9eomzLWs+fx6ItQBwKCQmJkZ9ZQglu+Q/MTEx7CfOoZDgGMZ8EMAy9MDyCEyCY5gt2ng7ssvvb7CwPOyN+5cizS510C75oOhml3pml3yQfdnpPhaPNYoUtvVEpCcW2oawBYDXr18fUACYiIiIiIiIiIiIiIiIiIjMmTx5cngCwFZ6AM+aNUucHHPi4uLQ2hpQEdiCXfIfFxdnmycnmQ8Cy9ADyyMwCY5htmjj7cguv7/BwvKwN+5fijS71EG75IOim13qmV3yQfYVFxeHdX97Spwcc1780UeqY60Saydk4KUDqgWe34bWd6apJoTP9oVxeG1YBfYvGiLOCoLg5jW027odC+M+wlOt7yCwrQtEeL5Tt63fvhBx04/irYr9MC5O9fZtx8K41zDM6/LB4r1cKtdOQA4KQ1QP2oHtCxE3/V0Az2ObQRkHxvt+84/xuoLbDmzHwrjpeHf8W6jYvwhta5TbLnUZSdOgXbZy7QRkyI2chfYtEnTbhihTU1MTlgBwB3EGEREREREREREREZF/xuOtila0traitbUCbx2djriF28WFdFRi7YQJWFspTjfL8/PT3mkNUiDFSKB59RTcbfUsi/Zk+0fv4vnnh+OlN8zui2l4p9VK8Ld9l3c02f7Ru3h+WytadYKrsSC47QAAjMd4bMEn6rpZ+Qm2YDzGKxO2Y2FcDvDKW6ppACrXIuel4djW2orW1m14/t3XWMdjFAPARERERERERERERBREQ7BovxA4qFyLCXFxiJPShLWVqh5pB/BSRlxbEFV3WXnWBGV63MK1up+vXDtB8xlxfW2x2u1YOGEt1i40mKf524iY1+1YGLcQbR9T/V25FhMWrsXaCXGIm7AWlR7b6m17Kt2f082HPN+zLADgpKrMlMk62yKWk2a7VNPj4oSg5/aFbfMWfqSaEU7b8dG7z+Opd57C8+9+pCp/b9un3lde9hvcPTTb8r8Q23XL20c5CftCU0dFhvtCy3O74KMeedtG9+e2+9xGo7roY92G5Wu0PnPlsH1hHKa/C7w73bgN8VrvVbTti49jyP0Bw+0zWhcg18m28gheOyAbjtmzgS2qCHDlJ1sw/JVXMFyZIj0AkaFMAKTl8NYvpED6NPziLe16KHYwAExEREREREREREREQTYNTz1/AMcq4A5oZBzDK61tvWZnb8nB2sohWLS/Am+Nl3rUvjPNy7LuYEtbz7RWtL6zSOfzou1YmLEFs5Ueu9uA6arA1IGXsGVYhXtexVs4+pocFJqGd1pbobtKD+q8+vDuFqCwFa2aoVlVjLZn+xt4afg29/RtzwPPbxO2Ta8sAeBdbEGh5/ogbouXcpfKwj29Fa0Vs7ElR17PdiycflTpEV0x7CjeldcfTts/wrvPP4VpmIannn8XH6kDnla3b/tCTIdU9q1yL1O98vZWTtDui9ZtGP6SXL4ib/tCvZjedkmM6pGvbTzwEl7ztY2GddHHuo0Yrs9cOUx7pxXuj6nbEC/HvNEx6NG++DqGvGyf4bqkoPF0eB+q2mj/GZaVp6E/ng1s+UTa1kp8smU4njJYluyJAWAiIiIiIiIiIiIiCp3KkziKdzFd6bXm7jmpGzD1sqy2Z5pJ2z/Cu8+/ohrmVwzWPo9X5JlDhmL4gWPQ26ygGT8bP9aN/MqCvT1e1qfeFi/lDriDjUqvw4yXoLwCWSjfIYtewfPyvDDa/tG7eF6Kbk176nm8K0eAg7F9057C8+9O1+3R68GonADtvvCohyq+9oXM63Z52e/B2EYjXtftJ7PlIPJ1zBscg8bti0FZetk+43W9i+kZx/CKt+AvYPyd/hiyCK8MfwlvbJcDx0/5+E6yGwaAiYiIiIiIiIiIiCjItuOjd8djmDy86Pi3UKHuHeitd60/y0YFIa+hkDEM49+d7g40TT+Kt34RggIxKnelx6I0vUJ4Z2jEbcdH8hDAcXGIm/4uIA4DbYncs7UQyInTDN2rEcxyMtoXGia3Sy0Y22hUFwNdt9H6YLYcIsjv7Xseb711FNP1x232zVtZ6ZAfhlA/IEHtBwPARERERERERERERBRU2xdOb+uFN2Qohh/YAlOvkfSy7JAfzwZeesN3kEtt2lMe7yJ+7d3ngzoUqiavyMCw8UdxUvq+yrWv+T/ksI7KT7Zg+DY5yLRf1bsxSLyUOwBg/DDI8e3KT7a09ezMGIbxqmBrsPLrl+0f4d3n1UMhV+Ct8dIw0Ka3z8x+G4JF+1uxTTPEtMConAAA7+I1uSJ6q4e+9oUHE9ulZnEbvdZFw3Ubl6/h+vwuB0mAx7zf7YuX7fO2rqGL9mMbpuu+z9gXw7IyIvUSn24i/zLttm/HGy8Bs/W6TFPUYwCYiIiIiIiIiIiIiCw6gJcy5KFQ49zvJlW6wk3DOxWzsUU1v6234hD8eDbcn1243fuyQxbhledVQ64u3K7zedE0vLNteNu2ZWzB7Apfw68CwHYsjIuD7iq95nUIFr3S9n0Zx2bjLVPdIL0bMnR4Ww/XuDjETdB7t6qvsvDGe7kXzt6CDGl6xrHhbcMoD1mEwreOKvskB68EJb/+8OzdOAQ/nj3ePQy06e0z3m+VayeoysS9v927Wyhvb+UEd2/R2ccypHr4EoZvM6qHXvaFivF2eeFrG/E8hvvYRsO66HXdxuVruD6T5eApwGNet33xxsv2+VjXtHcM3q/sg3FZGZmGp54HxusOR+1u4+IyXsKBAy8hQ27vNNs+HUffKvQdaKaoFHfhwoVWcaIZO3fuxKxZs8TJMScuLg6trQEVgS3YJf9xcXG46TomTo45CY5hzAcBLEMPLI/AJDiG2aKNtyO7/P4GC8vD3rh/KdLsUgftkg+KbnapZ3bJB9lXXFwc1v3tKXFyzHnxRx/xWAuj7Qvj8NFT8vCylVg7IQcoNNED0KaC09Zvx8K4j/CUz/exthfmyiPYdTHY67MzlpVvwWkbQqumpgadExIAAIm9eomzLWs+fx5gD2AiIiIiIiIiIiIioug27Rdv4ajS8y8DLw2Xh5ymgFSuxYS46Xj3+ae8BjvJU7DrYrDXZ2csK/IHewDHwNMAoWSX/MexB3BUsUs+IollqMXyCAx7AEcvu/z+BgvLw964fynS7FIH7ZIPim52qWd2yQfZVxx7ABNZxraeiPTEQtvAHsBEREREREREREREREREROQXBoCJiIiIiIiIiIiIiIiIiGyCAWAiIiIiIiIiIiIiIiIiIptgADiCKtdOkF7WHYe4hdvF2UREREREREREZFkl1k6Q7r/ExSFuwlpUiotEke0L4zBhbfi2sHLtBM33iX9HE3/Kxms+ti+U6sNC8I4cERER2REDwJFSuRY5Lw3HttZWtLZuw/Pvvvb/s/fvsY5cd57g+Q0gXfXPTJW9O8B0l9OqVDviQuZwB3ap12iTyq3RytuVwTuSWKgUZ4FE9oWrLdIaYJIcV11oZBCNRINrrXBdbkYu0DIpjY3biQR2qC6YluYy0i1pBW/q0g1vq2Rg2HThMlzKlFXVNUDvOl3Tf6o69o948ETwnGDwcS8f+f0ACenG48Q5Jx4k43ceUH0nJSIiIiIiIiKieTiw8gY6pRFc14XruhiVOjDWJgjswMrnI++EzJaL46oubrRFJss7i2XVjd1to9xz4botmPGVdCbiAfr437ME+zfRepfPRmXjG0esogyneUwbFW3+Z6dcNL/LvyaXlL5jIS98ZtuVcYMudXo2KkGjryXXW5rji9uEjc5i5ZjExmq0fAwAr4hz1AGa+/6XTBP7TaBzxBuGiIiIiIiIiGhp7APU0MShEDTUq4doogPvNUz8hb34t/gCOfYS2bGQr1jey9q8BSdpW9io5C1YwgthbyA4Lzhd6/dRM8ajw0UDYap9fY6FvHBc+cvYpLzNIp6XCmzh+JE8S48nL6+yDBN1LKkb6XGS2RUNhTbQLqjzENaxJA90NpYV7F8Pkw0ftqt862CyjreLiZZ7jNO8ZE77mpw3feeog2y9Ch0A7AoKgyZGfqe6bG1Pcs4dWPkC0PMafbnSepvzeklzfMdCI9xmhCZqOLAB6FXUs8F3jzg2VqPTwQAwERERERERERFtJedkAGR3vBfHIR072T6Go8hCCRMt/0Ws67pwRyV09oSXse0OcOjCPa5Cn7Ztv4ZOxn+xO2pi0LDgQEf1eIRmLofmyIXbUvRFle4LLwBqDFEPjztCqSN5GT0tb7Po1zAseun0ym0UguOPmkDtwA+cq44nK++UMkTqOE51nGRmy0WvDK8HcJiHDkqjIK0eUBBedCfmgUKyYLkqsJ7CRLBf2RAi1mtOdRxlXry0bWGqvkhDitQNFFQNEuQNH+I9nuPHiedPXvYxuyIstytCg4VY4EZVHokToU4i+ZGWM5YH8bgzHHM+8jqGqgwT5y4pj+ryequD4eQ1aJWusEIUP4ezNp4J1gmNlVTXi6xsooT8TtxzyrwkWHr6Do46QMbw/zoZIFfa9Z/FJoplyWe5c4QOmthXfKQqrxdVnQpSHX9CLsy/kVF0AmRjNTolDAATERERERERERHJiC+zjRr64rpcCbtiRDBpW5RRD17s6jvI9oeY+s44pNjXOcEAbRTCl6reC1rpy+jEvM0gN36pbmRyyAWj2+k7yIrbpT3etDLE6zgu7XGS2F20y3Whh1jspf60PNBYJFg+JbA+K1VDCPsAtWzPW+5F9jHZlmJKXvo1NHAYrhv36pulgYKqQYKs4UPc9PxJyy4wi2W0u35g5gTIhYGjEYYIruEp5YlooxPUSeSYqnJG8+AF4UrY1Wc55rxUdawqQ/zcJeVRXV7ARqUw8I7puhhlBmgH6cct1Hgmbsr1omy0MkN+U+dFdBrpjzDsZ7EjFKQf+5AbnMT2Gg3R79dghJ8r8WG5ZdfLlDoVTD2+XsVhqeMf38CwPu6BrO+WgM7RRDnZWI1OCwPARERERERERES0lfSdLDA4ib1stdFtj3vkKDkWvFEkgxelTeTi2wRm2XaZcsEwk+N/E+9mzzpvsx4vTRlkZj0OnT4xWD4tsD4zRUOINKbmRUhbXDdrA4V5GyTMkj9V2c0iyu0ubL/HZL2e9fa3u2gHgaVp5YlIOKaqnGEe/OkPS7vQZzrmsiWUQTx30/KoKm/svOnVOsrBurhlNp6Zdr3Er8vALPlFyryITiN95wSDXAbBx7VePURzUAj3K7SBrBgdDpT9RiF+wL0xLdo4rU59aY8/GvaBcg+9MtCWNNhYuqS6jF8PSdsm3TNTKfaddn/RqWIAeEX03ZLQusfGQQ0oSZ/MREREREREREQ0F7OIct+ff89nVwrCi14DmdwAQQcex2pEeywJL56do478BXVglm2XQd9Btq+aTzDmrPOW9nizlEEm7XGSmEWU243IkJmNdhnFNEFoWj0jg1zbD8gUBmiqx32dT9oGCitvkBA8y0YYZoswjQwGXRt2t42yeDGnLY9KYjlNFMttdG0vCB2+6170mGdBlcfE8i7ZWR5rmtPOy9zp66gej89Rrzy9MZeRSZdyOtOP71h5NDIjuC0TZsuby3dvSgCajdXotDAAvCp6FfVy0PKhgEHzUDIZORERERERERERzc9Ey+0BhaDniddjB34vNUBHtZ715rXTNBjDEprB29DIMI4ajGFW3Ztplm0jdOyWMDFvZTomWqMSOn7evX/xoS4XyducEo8XL2/KMsgkHmcWJlq98TWgGR2URi2vdx7N74wC685RB9leEFQYD7UaMTUvQg9Bcd2sDRTmbZAwNX9pePdWZ6+BQcbw8j7oojsQ0pm1PCoJ5TSLZbQbe/7wz0s85mmalkdVeY0McuFniaQB0TxUxxLNe73Mmt80eRGdRvpJvVDtCgoDSW/nSD4cHHX60l66EfPUqer4sWGiR0NpyaLYWI1OCQPAK2S2xi0ejqXfToiIiIiIiIiIaDGxOe9cF+4og4bmz+9ntsbLW1VUj8fBP716LKxroRXMqahXcRybX1G5LUy0XDGgGP073M/vDqNXj4X3RMn7Qq/iOFI2eeBSnbf48Sb/HjMT9lOUSXE8sbzKMijqOJ7XpOPIy+G9k4v0PhKvATGIKMkDpXU2gXV9J4u20MBDy8uGW52WlzKyQ8NfV0O2F6yboYFCYoOEeMOHuGn5S0ffLQH9INhlophto50tRp8facujklhO+IGsvjf8s7dg8WOmMq2OkyTkMam8ehWHzUE4tO0e6uMGRPNIOlbEnNfLLPlNyotjIR98foqWlX5ENPDpHdsvdwHoBc9nMU+RfBioZWXzgsevl5R1muL4E8NED5o49D9UwqHRY/t4n6EPeGM1OhXa/fv33fjCNN58801cvnw5vnjjaJoG152rCrbCtpRf0zR8/NEwvnjjnDufYTkIYB1OYH3M59z5zFY847fRtnz+LgvrY7vx/NKqbcs1uC3loPW2LdfZtpSDtpemabjx02J88ca59vnuyu81u6KhWwwC+g6s/B5wqOgJLGWjonVRVDSeoPX1YD3rH9zr1LHy2MOhskHPJrEreZzsz/B8cizkjQ5Koxn2oY14Nty7dw+/fu4cAOA3PvWp+OqF/c0vfwmwBzARERERERERERERbSJzv4lB2GvOQC0bDJlKtCUcC3mtgHZZ7M394NB3S0DnSNKzf8M4FhqKIaOV9CqOVUPbE6XAADARERERERERERERbZ74EOKTY71OER9mnWjNBNf4zNf2ltiWofi3pRy0URgAJiIiIiIiIiIiIiIiIiLaEgwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIiIiIi2BAPAK2BXNGia9y9vbfz05US0BuznM7j46oeRZc6rV3Du+TuRZZPu4Lnz12HHF/tk6cY5r16Zug0REREREdHqOLDyGrS8BfEtjGPlw/czWmX8q0i63LGQ95cJm8Ku5CF/tWOjok0eM8yLVhF+h82WPzUblUi6Z+E0j2mjoqnqd17R/NoVvpsjIiKi7cQA8FlzLHQzI7iuC3fUBGoHp/QlmYgeJOalEn78xo+ElwUfovfG+3j20sXIdrMyXxrizlcfii8mIiIiIiLaEDYq2h5QbyInLnYs7NWy6LkuXLeHcrvhBRoVy52jDrI9713OoOu9yXGsPBqZQ1R1MWFRDjl0cBSJ6h6hg5yQlxnzF+HAyi87QLpOTLTc44T6XZzZcnF8mgd44C2zgcAy0lpGGlGOlV+gEcHy8zNd+mNuUwOJ+HmK/71OZqn3xHLYFb8RUbrzrTZbIyXpcjaiUjjNY65xIyrHQl44X+k6TPrXhKZBW3q5thcDwGdNr6IlfrHMZWCI64mI5vH4E3j2vdvo3Q0W3MPP3ivhqcf9P+/exMXzGZzz/8V77I5evRKue+6d8fJ4715H2E7Zu3jKsYiIiIiIiM6OH0SMvXxxjjpAcx+mv81+E+gcOcrlExwLe50SDhODh1mUStH9naMOsvU6suGS2fInbAErb6DW76NmRF9unwgvvcPFjoV8xYq+JBdeyEdfuoovWSUvWsOgggat0hVWiGxU8has8KVuBbZwvHTHir0Yj+U3sWyihPxGgydJeSFahs1qtMEGEvNa7Dwvq97tbhvlngvXbfmfJfOYsZGSYjkbUa3C+jai8r4LVaHD+4wuDJoY+ecqW9uTnBMHVr4A9FyvY+Upl2ubMAC8AmGLBmOI+rF/oRMRLeQinrryPl57yw+2vvM2XrnyhP8F7w6ee+zn+MZHQ3z80RAff3Qbz7zxAm6EweIOXsOL3rp3X8CgeXPyBzO8wO5Xrht4I0jnJVnv4mnHIiIiIiIi2jz6bgmDggbN6KC0b8DaS/dOZ2e3BHSO/N9YDo46WRTnfxMv0FE9HqGZy6E5cuG2gkTb6OAwHHlu0BACou0OcOjCPa5Ch42KMUTdDV6mjlDqBC9dTbTC5S7cUQmdvSAdG5XCwDum62KUGaAdpB/Xr2FY9LbrldsoBMeLjIiXdCyRjYrRQck/ruv2gILw4j5Stth+afObOi+koupxJ22U4O2gaISgTgsIgvrqxgGRHmQJDQAiVA0MJhozxMogsCviunhwac0bbUiON9FAQlkPQa9M2bqzMqUOUouXc9bGK4rzrDp3aepdepxkdkVDoQ20C+o8JF5rodkaKamWT2AjKu+f6n5c+DoM1qmfk4llEyXkd75r1cFRB8j458w5GSBX2vU/u00Uy30MR9E9vMB/E/tL+f70YGEAeAXMVvBFMoOGfyOIX2rO/gOSiLaBOAy0fbszHv757l0M0MGTYa/cS/j6e+/jZx8Ee5bwjWCY5wsXkH3v54h/zgKA89Zt4PofJrcanHosIiIiIiKiDaRXcez3Otk92sOw3gKCF7NJL3L0KurZGg5sAPYBatli8m+qhZVRD16o6zvI9ofj33e5EnaDd+3OCQZooxC+qPVehIcvXcUXvkYN/SANu4t2uR72vNGrdZSDdXG58ctaI5NDLngZr+8IL+8TjiWKHXfiJbFYNtEs+UXKvJBcpMddmkYJCY0QlGn5wYoC0At7NSakk7oBwJQGBv0aOsKUfpGGFQKzWEbb793oBSzE63IDGm0oG1L4VPVgH6CW7XnLe2Wg3IN4ys5GUh3MaKHGK7LznHTuptW76jjJzJYL71SIeUi4xhPzsDg2oprjflzoOoyb9/zPkN/UeRlh2M9iRzhQPxbxHZzE9hoN0e/XYITfWU5r2OztwwDwKulV1P0vq3r1OLw5zv4Dkoi2QjgM9B28fksY/hkAHn0Bfx72yvX+vSyuX6azPBYREREREdFZcizsDetoGRYagyZG7gjNgWxoybEgKGR32ygv5831cuSCIRfH/1qmGGALXuLGhtZcprM81jTrlJcNFO1xJ1I0SkhohKBOKwiCCEPaJqSTugHAtAYGqjLEmUWU213YQX2EvdqSJKR95o02FA0pQgl5XQeqOpjVMhuvIMW5m1bvaY+TZNo1Pi0Pi2IjKn/5LPfjEq/Dec//LPlFyrw4JxgI06Lq1UM0B4Vwv0IbyIrR4UDZb2TiB8QbSV+8KMQA8FmzK5EhRLrtXNjdnYhoMd4w0D97WRz+OejVK84PPB/9y5eA699NbmG1pGMRERERERGdJn23JPSgsXFQA0q7unK5x/F6LUVa7uvYibyJlTCLKLcLKLTLqXsuJedjCfQdZPuxuRVFwstZ56gzfolrZJDzA1wA4FiNhN5AKamOJTKL0TkcHQuNNPU5a37T5IWWR9UIQamMZnOAQjxgNHM6p8VEsdxG1/aGOF3qPYuEcq668YKRQa7tB3AKAzRXMU7rWdfBrMdTnbtpZj3OumMjquU6y2NNM3dedFSPx3XYK0+PlxmZdCkTA8BnzywChaBlSAHoccJqIloe81IJr9wShn8GAFzEy+9ewmuPBcMyZ3Du/PXkQK7Mhav4xhVheOfn78S3WN6xiIiIiIiIlsKfk86ohcMHVmy/V1E56L1TwKB56L2fUS0HYFcMDOt+z0O/V5KhaShA7FUjY6JYxrj3TsSM+YvQsVvCxPyF6ZhojUroGME7Km08pKJexWGpEw61aAyz4x4/ehWHzUHY62kPdTQXeQ+bdKwIE61e1iur5g8jOhJ6garMkt/UeSGZaKOFFBIaISSltVM9Rg+F8byTCemkbgAwbwMDCbNYRruxFxv+eQmSyomExgtp62ABzlEH2V4QwFnhu25VHZyWtMebdu6mSXucJEu8xjFxj7IR1QTVOTuN+1F1LNG853/W/KbJS7xntciuoDCQPDsj+XBw1OnLewnThPUNAPuTUo8nkd4W0bHQU7X02VB2OEn5Ks/jHTz39E3JWPPbxX5+HGy7+OqH4XLn1SvjIJwQrJNvfwfPhQG7DM6ddb29cx3nzl/BjVPtOXoHz0mCkfbz0XpbFnk9n7LHr8uHXL5wFXciwzJf938oX8TL4f9P/q1/9RbuBPMDAzBfEtJ4yQsyx7dRH2s1nFevnF39K5zWNTY7/+WSpkHz56BfR3ZllZ8bDwbHyo9f9M38snATide+Bi0/nodGVReq7zGzbq9aDjiw8tG8ICF92f0b2TZ2DHU68uOuB7+MkbzZqITz+4j/H1/vlytWH15asfMfef5N1qtXR/FnpI1KUp3ZFclzdd78YnyewnXxdAKxsoXnOr5/NG+OlQ+vFdkz17Hy0etmonzx9MX8J9V3IF43SelJ1i3tuTXtmlPdS+pniuyen+9e3TSyuoRwbiXnO/XzTxAOK6e6J5Ytfq2KyyfLICuveE1Mbk9nIzYnnfAuxmyNlx0LEYuk5eJ7nHA76csdEy1hmFqzJaYlrps9f6JwSrGWOXHMyN96Fcfxuf3CITmDf+N9xanK3FYLLWFfcd1x1UT1WBaINSf2kZc/+VgRZkvIqxBkkpVNkJTfaL5myMua+/e37uDa57vhv3926z/EN1m+SKOFhGd5KLkRQlJaZquHbE2YbzMhnXQNAOZsYCBjFlHu9xXDP29Bow0JfSeLdtjhaUWfd0l1cBoSjxc/zwnnbprE48xi3mvc/86TtpGSajnYiArBumXej0nHipjz/M+S39R5MZDJDRBO8+vHATVNg9df0v/cdSzkg9+SkXwYqGVXMc+4iux3geo3xNnT7t+/78YXpvHmm2/i8uXL8cVLY1fyOMlk0cG+8kvuMmiaBtedqwq2wqmV37FQOdpFq6p7N2t8fo4l0zQNH380jC/2A8B38Uc/uCr50rV+zp3PKMqR4O5NPPfW7+Llrz4E3L2Ji4/9HN/46DpM8f9xB8+d/w4+9+4tXINi+yXW1TzlsJ/P4HWU8AqeCAOLy3cHz51/G0+dRUBSdV7i2ynMU4fbbJH6cF69gq/gxWiQ+gFx7nxGeMY7sPIGhnVhSJqDHRwnfmNyYOX3gMPg5Ur8b5rXqX3+phH5XLZR0RrIjFZ7Tk+/PmxU8ifYj7/AU9UFFN9j5theujzYt1dCpwEcij9w4tuMjlHVY/evlHB/QpWO4rinLP359fI3yPWRDctqo6J1UQzLEvy/uE90mWPlsYdD4TfE5Db+lornoiF51imuoWBtRUMXZbRRFIIAsuNOLpvMr5evTmkULnOsPIxaFr2JMojpieWJPa/tCrRGBiM//5FjxtZN1IuyfJ7J/E+WcZJ6m8n04p89Xv5q2d5EXlTU1+CUa055TyquB+U9H9koxb0a2SGkLsc6COoSKIn3jmMhv9cB+tk5n3+xo1Q0dItJz8JlU12rKcvrWPBOdxW65N5aR+t9naW3LeV4oDkW8kYN/XL65/0m0TQNN35ajC9eimGji++c/B/wT/7FZ/GfAQD+A370j94H/m8X8bufiW+9mGuf7/Jem6D+HNtW0c/n+He308NnPVES1ffY1Zv8zbdcZ/tsmPKbMr657969e/j1c+cAAL/xqU/FVy/sb375S2BtewDbFa/lx058BW0Mveq9+AgI3f9XJ9bDNdLb1OspfEPosfncO+J+Yq9R8e+ENO/exMXnb+LG015v2hvPi2l+iBtPL6m364WrXpAR/vyrGGF0F3Deug1c/0P/IXMRf3QdeO2tD5Xbr9YdvH6rhKdeegLP3no70jpG7EUrDiUsW27PWcfRHqJJ14J/XoVzruzVuZb1TNPOr7TXfOycR54NkbSuwxa2jffGT3eNfeg9M6THW5B9gBqaCKfi0avj4K8jtLYLWksGL9j7fb81pBX7278bpfv6yyuWtIePF0ixYAs9feI9LMd/e9taQu+ZmRtmUoRz1AHClrMm9ptARzlu0XZT1oXie8ys20eW6zvIImjlaqLlHqMa+3KkTN85Qke8f2Wco3CYOWU6iuOulyzq9TLajfhz4xQkPRdnYqPbLqPYKqIsDI81Nz9fh8I1pVcP0cy10U1MXMduKYdB2JRaYBZRVg2zZRZRjgxfNsKwLw4HtuTyLUxH9bgXHcJsIeprTn0vKSjveUGqe3VTZVEqRcvgHHWQrdcxHtlP/hxKUxd2RUOhDa+H0bTvIbBjre7Fv6d8twh7GWvQKl1hRVya8sZNn9OMiHxB7+S5PpsfYL/4OX74Ly/ga2HwFwD+E/zuv1h+8JcU7C7a5Wk9GreLud/EIOwBbKCWfbDKT7R2HAt5rYB2uagMQK6SvlsCOkcTv782l/o3JZD0m+X0rWEA2IHVAHr8grfxwqGujCHq8dbxK3ERL4vD0r57Ca9VhWGO33sRrxm3/XUvYNBMMwTylDRv3QasIT7+wVVcu1TCK7eDgNKP8BouoXBBSGoZ7t7F4NEZ0o1v/96LeEQSvDp177yNV648ARMX8dSVDl4PAl7vXMeTaE0OJaxYbi6rjpXXwh0899jP8Y3wuLfxzBsvTA8yx+uZVkt1fu/exFeuG3gjOL8vXfTP+W08825wzlvAVaFhwXsv4meXvHVvXOngyeD6ePcF4Pp31S/JVXl457v4+iP+tX2zBFxpTQ7nPSfnZICcdAgqGxWjg9IoGEqtBxTysBwd1eMRmrkcmiMXbqsa+9tM2NdPut0BDl24ss+Afg0NHIb7jYfvkujX0MmMvG1HTQxUX6iIkvjDQcUbHKjM+j1m6vbOCQY5yVw2aYyG4XBW3g+GyaGE7IMasnXJcTeR2UIvW8NBvJALEYYQ9BulqJ+LAOA3dgnrvKCe68ju+j+sTRTL04K00zknAyC7E8tXirmxkuZCsrtoKxtkmiiW++MgVlge31zlm6zv5fLyPJRGtOcwzzU37ZmiuOe36l6V2Im8zHFw1MlOn1ssJbPlolcGyr2U30OSKL9b2KgUBt53HdfFKDNQ3/tpyhsZCs/AsH76vaGI6AF373/DB5f/LjLx5XR2zNaD13AhPpz8g1Z+onWz7o2opkzdsJGUvynlv1nOytoFgB1rD52SbDx32jThXDWjDBrSub9W4J3r4551j72IH0dWlvANscfmez+X95KIS0pTDPo9Pu7d6rx1G3jyd5f8kPsQN6q38YyVdgjn+PZiMLuF7PUUgc0lsW938Owlb9jnSBD38Sfw7K3K5NzAicuXUceKa+HuXQzQwZNh78xL+Pp77+NnH0R7jkZ7bMbrmVZPfn6jveZ977yNV658DdfC4P1FPHXFO+cAgEdfwB/5AVrD+AK+FOx/4UJCzw8o87ASE62TZ3ipPm1fyYvvsTLq4Y7Tjilsq+8gq+rFRqQkzq03pcGBb9bvMcnbO7D2OigdLvADp9wLX6j0ym00Igfwe2hu0Rdoc3/ZjT3K6AXXQKofmn5jF+G6kc9fBNjdNsp+5ZvFMtrpIqRLFARbvWGjx7/xhSB2t5hYbrNYRt8PYonlwdzlm7W+V2+2a27aM0V1z2/fvTrBn8/twIbXmz17ir0Opn0PSaT4bhFLU6/Wlfc+kK68o2EfKPfQK0PdK4CI6FT8r/ifwnmA7+BHv4ivJyIiomWR/qZU/GY5K2sWAPZarfdrhveiotD2/v8s+0TT8ulV1FP/ED9Fd2/i4lWMe/e9+wK+FN9mVjOlGfRu/RC9N4Bnvrzc+Ujt5y/htSdfFAJVyZK3jwW5TtUdvH4LeOWqH1S92gHCYaCDoPSLQNUfYnfK8tOsY8AL+P15GCj3/r38OKB/9Vbk70ByPRPFPPxZfOlWxb8XRvj2c8ubD1vfyaK/8gcx0TqYJUAwx/cYyfZ2xUCndLi0Xl9GJhf527EaGIRDp24JP6iyZ53EVkiG1J3Tcp6LNrrBkLT+7xdEhkmePb/6ThYYnMSCRA5OBqqhY8fB1ugcSkEQe4TmoJA8zFQ4DHQ8QDmtfKtio9tW1ceclNfcNJPPFNU9v5X3qkTQUCDemGBbJZXXsfJoZEZwWybMlotRqYO9aS2KiIgW8dv/KR7+l/8OQwDAf47/5qdF3Pjpl/EH/2V8QyIiIlqqmX9Tav6/0+ClvWYBYB3VY6Glfa+MXNP7sUQbxq5E5l9a+guatO7exUD8+9HPhkPfOW/djvUAVvltfO7R8fytzqvfwSvi6hnSNC+V8ErzhfmHJpby5gz9pnEbd4IehQD0L18ShqC9gz+5HgRE5dtH3L2Jb976Aj73cHzFKXjnbbxyRRzO+Ta+/agwDDQA4CFc+4E3xO605adTx74LF5B97zZ6qXpGp6hnWivRe8b3+BN49tZ3InN7f/NWCU8taVjmOOet28jeDO6FW8ttOGAWUW6LAQAblYrtLxfmUXQsNNL2TlpkXwg9GGfajxal75aA2kE4D+JBDSipu2pvH8dCw/9eoqwLxfeYWbf35tLW0MiMYoE5OWX6Rga5MOgWH+Z38hwq09kw5n4TqNWE4Ve9QFtNGFPJsRrzz2ukei7Owu6iLfTOdt2RMFfvnPk1iyj3o0NHOdYeav68sbPTUU2ajwgYBzEPZMM/q8q3OnalcCpz68WvuVT3kvBMSb7nJ/dPlf4m8u+twgyf7XPVReL3EAOZ3LgBhmM1EodyDkWetyn3m1JesaHJaHh2rf2J6AH1mc/i9y7fxXf+0c/x7+PriIiI6FTFf1OqfrOclTULAD8IbFROZR6sNWMWgaCngFYAemc919EdPOcPyRwOA3zhKr735O1wjttHRgaeje8m9RCu1Qx8/bFgv0v49qP+qlnTfPwJPPve+wsMTSzxznfx9feAH1+/FA5BfPHVD4ELV/GNK8FwxRUMrvu9UBXbi0MYn3vsRWRvLjn4pCAO/+x5CIUnv4BXbt+J5ul8Bk/Cmw9VtRxIU8fiEM5Bz+G0LuLldy/hNf9aSExDUc9nwws+j/MYGyqb5CL3TAbnnr/jnfOb4/v/3GO38cy7/lzUp0D/rDHuDX8+g3NPp5mLPC0TrVETg/DZ3EBm3/SW97LjYUKNDkqjll9GHbsleOsqtuTvpH2nKSM79Ef8MGrI9tLuRwvTq6iXgyFjCxg0J3upbRvHyo/ncjVqyAbfS1R1ofoeM+v29gFqfYxHtwnnCrVR8fMSzO3r3WKK9PUqDpuDcJjfWrY3HubX7qIdH25dlY7quOtKr+KwGe3tbLa83qxBfRqdEkapGosKc9KG5VY9F9Ob7PGnY7eUC4dJni+/JlpuT7im/P0WGUrZ3EcTHQTT/MqYxTLabfXwz55o+dRk9R0nbjM5r3VUdE7mAnqn00g4fs0p7iXlM0V5z896r246E8UykJP2dlY8h+aqi6TvITqq9fE6Y1hC7HEiF3neathDPcV+6vLq1cPIM6AwaOJwesHoNDgW8sK7GLsyfqZI5/EGxterpkGbmN5hMWmOL24TzqceK4ecjcrU52pa6rTsijrvq6PO73TJ+65neeUy9SK+tvO/4J+Gwz+/hT/Fb+G/+Ex8SyIiIlqq+G9KxW+Ws6Ldv3/fjS9M480338Tly5fjizeOpmlw3bmqYE42KvkT7C/yAmeJzr78p0PTNHz8kTfAzXq7g+fOfwefe1ceXD13PrMh5Ui22nIk1/GmWKwOP8SNp18ArEXrYFnpLG6x+tgc9vMZvH4pGEZ88fo/dz6zps94GxWti6L74AZ9t+Xzd1lYH9uN55dWbVuuwW0pB623bbnO4uVwrDwOdo69BlR2BVoj4zessVHRGsiM4o3WHVh5A8O6K8ytHufAyu8Bh/F9p0hzfMeCl3QVeiwvdiWPk/2kYy7zu/Yy0zoLi+R3ln3nPPcCTdNw46fF+OKNc+3z3fV+ZkTuJVqKKXVqV1SjoUyaZVuZ+LN+XnZFQ8HvrpdryvMjboNc03uGT6kLzyzPlmnUaS1al6dDnd/pkvc9nfImH3N1zjBfdsWb9gdl9M7ieKdkWc+G03Tv3j38+rlPAAB+41OfjK9e2N/88j7AHsCrZgutSZffopTW0Dtv45UrX5s7mEMpsI4T+D3jFT2DIz2rn7+JG09fwtffe9/r/fr8HW+juzdxUUjjuWBI7rs3cfH5m17P46dv4sbzwjp8iBtPsxdyGuZzL2AQ9gC+hK8/wmuZiIiIiGgxDo46CKelck4GyJV2/Zf1k/N4exsdoYMm1ANDeEHZWt8foSAY6sCxkBfe88hGQEh1/AnjabWMDNARhnSIjEogHPBEWB7JRyyPYq9WVVqA/1JY6CHrWHlhX2+0O0votTze3Rsef/zuS1YvSe/HktIO8hXkuSusGLMrwj52ZdyjGg6sfPRdnKrexuVNd+43pbfwtnOOOsjWk4JzNDO9inpWPbKM2XKFoNzkPSaKbruo5GMp2RUUBk2MXBeu20O2tjeZhmOhEW4zQhP+dC1T6uIsLbcu198s19nynfXxzo7dbaPcc+FucPCXohgAXikTrXA+LRfuqITO3rShfGijPX4dH78kDndMS8c69vmB2/MZYZjqi3g5nGt5iI/fvYTXqv4Qw3dv4ivXDbwRrHvpKq794Da+/egX8O13h36d3sFzj93GM+8GabSAq0Jg99ZtwBri4x9cxbVLJbxyOwga/+h05mTeRheu4o54jrb2WjbR4pdJIiIiIjoTIwz7WewI78XFuZkBYBBMGB0YDcNhyr2AXnxoYB3V4xGauRyaI9cflt5GxeigNAre8/SAgvwF8dTj61Ucljr+8Q0M6+OepvpuCegchUNC79Wy6AXvlcLuym10cOi/a2piEM4Db6NiDFEX5nYvdfxghzItP7hZQHJvoH4Nncxo8pj2AWpZfz75XhkoC1NZhKa8H1OlDRuVwsA7B66LUWYgnbfbLJbD6QucEyAXToswwhDi8PyqehOpzr2iXh8oqmD/lAB/5P4S/1allzbgHm38MUt6k40UML0xQqo0Fs2Dav+zreN4QxTR1MYS0m09kaHvJ567SRTHSlGnbJQjq5cp15My7SBfQZ43oFFOUn6l14/ieKF4/VRgC+lEzpGqjh0L+Yrlnaf4tA+x8x4hzS8keZKd83Ev93YhKFdCHlXXZ9p6pzPDAPCqiQ8Zo4Z+fD0R0Vz8wO1HQ3z8kTBn7TvXx718H3sRP/YXO2/dBq7/ofrHPGS9qy/iqSvv42cf+H8+KgR5H38Cz956G3aQtnJOZiIiIiIiolPknGCQyyCIAU3MzdwGsmJ0OFD2g5aui165jca0l5h2F+1yXRgSWB5ISHv80bAPlHvolYG2NBDp9W6EZP5poIx6GDHeQbY/xAh+XUTmYPdeYg9HSWm1UTCGqCcFfwH1MdNKfD+mSDtW53q1jrK4W8AsotzuwvYDgvV61jsvdhft7I7wW1VxnGkS6vWBogz2TwnwqyjTSxtwjzX+SEwvXeONxMYIadJYNA/K/c+2jiMNUZRkjSUS2BUUMH7uztYDUXaslHXKRjkPcKOcpPyqrh/Z8WL6NQyL3n69cvAZ6pUBtQM/eDuljtsd4NCFKw4vnnjeVfn1VyvP2ZjZcuFdEkG5EvIovT7T1judJQaAVym8aYObqAlxemgioqW6exMXr2Lcy/fdF/Cl+DZLcxFPXeng9Xc+RO8N4JkvPxTfgIiIiIiIaAV0VI/HLzR75XFPLhUjs8y3NdOP71h5NDIjuC0TZsvFqNTB3rLeoOaCYUzH/2Tvr8fKaDYHKMi6C6VhZJBr+wHvwgBN2bjap/5+zEAmN8CJM8IwW4RpZDDo2t5Ql0VJfuYxc70+YBID/DNKG3CPNf5QStl4w6NoJDBTGhKL7o8V1fEymUWU24WJXoZzS1mnbJSjkHg9KdLetEY5SflNef1I5cZTSBiZHHLBedR3kBW3S6rjnBgIx/TzPjW/c9alIo/S6zNtvdOZYgD4rDknGIh/C19EnKPOYh/ORETTPPrZ8TPnrdthD2D9y5eA69+VDyESePwJPHvrO+Mhn+/exDdvlfDU47HtfOalEl5pvsDhn4mIiIiIaHWSXnTaFRQG8ZesQdCyGw6RetTpSwMCEWYR5XYjMoRjo11GYnxRdfxYj7TRUP62SN8tCb2JUtB3kO3L56tMSmuneoweCnMN5egcdZDtBUHRca+5CfO8H4ucJ8CxGtLeZoCO3RLQ2WtgkDG8ehh00R1MOT9pJdTrA0UV7J83wK9KD3MG3JPSOyuL5kG1/7rU8UKC3oaHwJ6mHuZ26dgoZ8K811NqbJQzex0veN7nMXMeN6DeH0AMAJ8Zf8x0owYE8wpEho/QYAyz8lYxRETLcOEqvvfkbTziDwH9yMjAs8K6b1zp4MlgeOjn7wB4CIUn4c0l/Pwdbw7hm8Z4buHHbuOZd4XhpeMefwLPvvc+h38mIiIiIqIVCl40+3+K89MVgF4wvKJjIR/0PNOrOGwO/F4sBmpZ2RCZXlBxPAegiVYv6/2tadCMDkojSU+dFMef6JE2aOLQj5w6R53Ie6V6WehtM/XFsInWqIROkEdNCLJMScts9ZCtzT6Uo76T9eYTDNKNz2eIBd6PRc6Thj3U0VS8ndZ3S0A/COSbKGbbaGeLk+cnFcm5V9XrAyQx2K8M8EfvTzGIr0wvbcA91vhDmd48jTfiUqaxaB6U+2NFdXwqvIBsr9yGP0rwfFLWaQQb5Ywpr6cEm9YoJym/81w/s5qxjhPP+2nlV5FH6fWZtt7pTDEAfGbGY6YfC09WvXo8bhHRaqEljutORDSXh3DtB7eEuXrH9K/e8ucFHuLjl67j5R9cDZ855kvBnMFDfPzSxej2/t94/Pp4m4+EY1y4ijtCWmNf4PDPRERERES0Qv6L5uCNpF7FcdgzRQjQ6lUcCy/Do+9r5G9Qw22C9WZrvI/qxXqq40d7pIlzAI6GQEmITpgtYbtwzj4x8Bz7O3L8aB6S0zLRitXP+P2W+ph2t+3NJ+i6cN0RmuFcj1Hq92PqtOP7HVdNVI8lQXeMyz0+VfHzOv040vd5QRoJ9fqgUAb7EwP8Oqr1ccMJY1gKg/jK9FIH3KOBz8T00jTeSJQujUXzoNz/jOs40hAFNirKYZvjjSXUHCsvHEtDAbKGN0nix0pXp2yU8wA3yknMb9L1Ez/eHOasY/V5T8rvnJLyKL0+E+pdbGRHZ0q7f/++G1+YxptvvonLly/HF28cTdPgunNVwVbYlvJrmoaPPxrGF2+cc+czLAcB21KH71zHudtPjIPHC9iK+liBc+czW/GM30bb8vm7LKyP7cbzS6u2LdfgtpSD1tu2XGcT5XAs5PeAw01vdL+J5XAs5MW5Dcs9ZUD9QaJpGm78tBhfvHGufb4b3mt2RUO3GATZHVjexSpvCJHCMtJzrDz2cIjjqr6U9Ba1aB4W3T9u3vTsSh4n+/52K3wuTTzrVyBSFxtg3nNOtEnW4dkwzb179/Dr5z4BAPiNT30yvnphf/PL+wADwJtxMZymbSk/A8DrZVvKsUqswyjWx3wYAF5f2/L5uyysj+3G80urti3X4LaUg9bbtlxn21IO2l7bGABeerB/GemJwcllpLeoRfOw6P5x86QXC/iuMgC68mf9CoPfc5vnnBNtmJU/G1JgAPiMbMLFcJq2pfwMAK+XbSnHKrEOo1gf82EAeH1ty+fvsrA+thvPL63atlyD21IOWm/bcp1tSzloe21lAJjojPFZT0Qym/BsOKsAMOcAJiIiIiIiIiIiIiIiIiLaEgwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIiIiIi2BAPARERERERERET0gLBR0Sqw44tX7gzzZVegaRq0szoeEREREZ05BoCJiIiIiIiIiIgiHFj5PCwnvnzz2d02yj0XrtuCGV9JdCrSNXCwKxryC9906Y61XOmPuZwyboL0dbI8Dqy85jdweVAbufh1kLcQXmWOhbz4d4SNihbbfiXnbpJj5SP3Svzv072XonUw77Hm3S9JvB42k/oaO406e5AxALwSNip5C1Zl/IFUkV3tRERERERERES0mLDHqwat0o2ucyzkw2BB8H7GgZU3UOv3UTM0aBMvbeLvdSqwhXTGLy79F+vhPyGg7FjIV6zJF/UI8it/MSrPLyR5kr9rsisaCm2gXQjKlZBH/0XzuO78BGN54ItaWhaz5eK4qscXT7FZjTXmK+ODZN7z6T23O6URXNeF67oYNQcoqJ6lW8lGRdsD6k3kxMV6FfVsB0fKOs0hhxoONqyizvJemvdY8+63Gea9V5Ntd52dPQaAV6VfQyfjfyCNmhg0VK1wiIiIiIiIiIhoPjYqhQGaIz8gkBmgLa4zOij561y3BxTysBwd1eMRmrmct19L0k+2X8Ow6O3XK7dRMIao++94UDvwAw4mWn4gwnv/U0JnT3j/0+4Ahy7c4yrCV52OhXwB6El756ry669O8a7JbLnoleH1AG6ZyXl0LOzVsugF61qmnwe/rK4L1x2h1Nlb+gtg2lDKBgqChAYO0Z5taRo1qBtrnAiNF8LFsoYXygYNyY0jEhuWBCTHS1/GeG9WVfll2yTlPd7zTvxblV5SPSUTz0O0bmV5UJ/PqewD1NDEoRA40quHaOba6PrJyBq0TC5T5U1yPuN/B9tI6ynpXMvyMSUt6fVgouUeo2rElwNGBugoI8BZ1OtltCWfGYA6H3ZFyINdERozKQKDKeprskxqy72Xku/piV63ijqJS85jQuOxvAVbeu9IKPOS9nizpDGloZwyneT6FSXXmeLckRIDwCtTRj34QNJ3kO0PMYpvQkRERERERERE87O7aJfrCF/BVOsoK9YBJorlPoZpXtDkmtj3I7RGJodcc98L2Oo7yIrbiS88jRr64rpcCbuRTi5BIFkW/E2T3znfNSny6Bx1gKBcAecEA7RRCF/wei+AU9UZbbkpDRTgBweUDRwkpjZqUDXWaKODQ/l+kYYXSQ0aEhpHIKlhSYysoYdIVUb7ALVsz1vutdrARFsU5TZJeU+gTC+pnpII58HtIVubto/qfE7nnAyA7E6sjnXsBA9kWYMW2bJp4ucz9fWUcK6l+UhKyzu/abIb0HdLQOdIfQ2YLfSysl7A6nyYxTLafnTdOQFyCHoZjzBE/PPNN1FfU54Zs1DVr/K6Fs1wTyfUyVSpGo952zVS3TtT8pLqeNPTmKxX2b2alM4s9RsjPT6lxQAwERERERERERHRsoXBLv9l6Cg2LOeEMprNAQpn2b1l5jx6we9R+ILX+zf5Mp0eOFMbKExp4CA1Z6OGpP3EhhfTGjQoGkfEyxppWBI30dAjLiGvi1DlfR7T6klJKNvE9XC2ZA1aZMumip/PWa4nxbmW5mNqWstn7kuCa0n5MIsot7uw4eCoA9TrWW+53UV7IhjvE+tr6jNjVvL6TWWWezqpTqZJ23gs7b0zLS9pjjctjbT1mpTOLPU7IeXxSYoBYCIiIiIiIiIi2k5GBrl2N+xV41iNca8Ts4hyuzHu5eJYaLTLKM4UDZgil0EwGqdz1JkahNmpHqOHgny4x9PKryKP+m4p2iMJwcvXpLkkiVRW0MAhDVWDhnkaRyyTkUGuXfACKYUBmkEUJ8028+ZdlR4S6mlN6DtZYHAS6xno4GSQQ0YyJPKpWWY9LTOtNPQq6tka9qyT6HJlPgxkcgOcOCMMs0WYRgaDrg2720Z54Q+mJUq6ruelrJMVWEZelpEGlpgOLQ0DwEREREREREREtJ30Kg6bg7BHyh7qaIaREBOtXtabv07ToBkdlEZB70QduyXMPg+lSK/isNSB4R/bGGZT9XgxW6rhHpPyO6ekPOpV1MtCb56K7eVhVEInyIOmjedzdSzk4/Ok0oMjRQOFxAYOqzCtQYOicURiw5IlcY46yPaCIMqx0Esy5TaqvIdBO3+dkHdletPqSamNRnCuI9eDOg9zM4so96NDGDvWHmr+UMSyBi2yZQvlbc56kuZjzrQWZe43gVptXObEfHifk529BgYZw9t20EV3kLJhUopnxjIor2vRLPd0Yp0si+reiVlGXpaRBqakM0v90lIxALwSJlqR4U7ifxMRERERERER0TLo1eOwJ8px1UT1WHgHY7aEnirRF8PhfhPdV0y0hPk89eoxjoWhGsV3POKx3VZrvJ9exXFkTlBxPxMt1UtqZX7j75bif4+ZrWiPHGUe/W3H6/yd9CqOwzy4cIPj6FUcq/JND4B0DRTUDRzmtUhjjYQGDVMaR6gbliyHvpNFuyDkKz8576Vym6S8Q0e1Pj5PxrAU5l2ZXlI9wUZF1fAj10RpaPjXQw3Z3riBjSoP859PEy23Bwj5NzoljIRn7kSDFtmyxLxNk1RPCaT5SErLRkXTMFk93nLNqKHfr8EQtnGOOkBpVz4ss0iv4jBS4KR8+MHrfh/ZHR2AiWK2jXa2OHHfy6V7ZixKfV2LG81yTyfXyXKUkZXeO3HLyMu8acTv1YR0ZqpfWibt/v37bnxhGm+++SYuX74cX7xxNE2D685VBVthW8qvaRo+/mgYX7xxzp3PsBwEsA4nsD7mc+58Ziue8dtoWz5/l4X1sd14fmnVtuUa3JZy0HrblutsW8pB20vTNNz4aTG+eONc+3yX99opsSsausWgsYYDK78HHEYbWKTZZhZzpedY8DYTG7ScDT7r07MreZzsTzmXW2qu63qlbFS0LoqKRlw03SY8G+7du4dfP/cJAMBvfOqT8dUL+5tf3gfYA5iIiIiIiIiIiIiIaH2Y+00Mwl6LBmrZ+kTAKs02s5gnPfugg9Lh2Qd/aQaOhcbAGwr7QTTPdU20LdgDeANaA5ymbSm/xh7Aa2VbyrFKrMMo1sd82AN4fW3L5++ysD62G88vrdq2XIPbUg5ab9tynW1LOWh7aewBTLQwPuuJSGYTng3sAUxERERERERERERERERERDNhAJiIiIiIiIiIiIiIiIiIaEswAExEREREREREREREREREtCWUAeCffP8G/viPb+D7P4mvISIiIiIiIiIiIiIiIiKidSQNAP/l92/gX3/6Gr71rT8A/vL7+Mv4BkRERERERERERERES2ejolVgxxdvhWWWbRlpLSMNFRsVLQ/LiS/fJMn1Y1c05E+xgHZFg6Z5/8LjOBbyeQuJR7Ur0KbWvVi2szxXyXXqWPlTrdMHil3xrx91fZ+Ns7y+SCQPAP8C+Mxf3sAf//GfAl/8fXw6vgERERERERERERER0QPNgZVnYEPORMs9RlWPL98eZsvF8WkV0LHQzYzgui7cUROoHXhBPL2KeraDo4Rrzu62US5nUTtIG/Zb9FzxPlhHdreNcs+F67ZgxleeqUWvL5qXNAAM/L/xi6AH8D+7AY4CTUREREREREREREQydkVDJYg12RVoYQ/FWGDIsZD3ezRGejVKnFj5cLswbdioCPuLvRwjeRCPm+qYNip5C5bQ43Kc1mQa3joHVt5Ard9HzdCgRXYIdhuXQVwvL9vkccS8qtICgp5+Qi+/hHTGvQI1aJXueHlEvD4qsIU0x+mpz8dET09pHfrLKxasvCZcN7NaRn7Vdaw6X9HeqvE8pD+3UnoVrSBipu8giwFO/F2MDNBRRoBtdNtlFFtFlNvdaM9P5bmP9wYWe4xG/xZ7JXvXnOw+SK5nxOo0sS5S1ttkvjDlnCTl0dvPnppHx7tuhXS89KekraxfVXrp6yFgVzQU2kC7IFzLc92D8Tqc5946y2cBiRQB4Av4zKcB4NP49EPxdUREREREREREREREHrNYRrvrhzBOgByCHoojDFHCrg4vCGAMUXddr1ejO0KpszcRGPK00cFh2Ptx0AiCASZa4f4u3FEJnT1vnZgHOEfooIRdfYZj9mvoCD0ux8e0UTE6KI2CNHpAIQ/L0VE9HqGZy6E5cuG2Yn3sHAt7tSx6wbHD9aqyJeRVmZYfNCkAvbCXX0I6sFEpDLz8ui5GmQHa45Si+jUMi952vXIbhSBNsTdqwvmIUtWhv7rdAQ5duMdVzN1JcNH8KutYdb4kEq8h1TlJwTnBIBfcR4C+WwI6R/J82F20y0WYMFEstxHcEjOdexW7ggJ64/pzWzAhuw8S6hmI1qnbQ7amqouU9SbNl095TqbksV9DY1oe7QPUsv5xe2Wg3IN32UxJW0WZXsp6EJgtF14SwTlZ4B5c9N6KWCAfNDNpAPiLf5DHL/7ZDXz/xg108A/wxfgGREREREREREREREQAYAa9DR0cdYB6PYvhyA9GZXe8F/nOCQZooxD2/PJ6DQ5H8cQAoIy62PuxP0S4mdiL0aihHywP8wA4Rx2gtAt9Gce0u2iX68LwpSaKZVUaY85RB2juS4ZeVRwnIa/qtIJgjBDwSkgnXha9WkdZSC0i18S+n6iRySEXHF/fQVbcTnU+RNPqUAhuzm3B/KrrWHG+pBTbJp2TqRxYex2UDtMFxOxuG+WiV4pIo4hZzr2KWUS5XZD26J2gqGePUE/xa0GUtt4S86U4J1hSHlUS055R2npIssg9uOC9FbFIPmhm0gAwPv37uPata/j9a9fwrWsM/xIRERERERERERGRioFMboATZ4RhtgjTyGDQtSPBKMALJIzEXmKu6/dwSyns7Rr0MmsiF64Mejx6QehSEEVY9Jhnaea8ltFsDlCIDwk9czpzSjwfa2iV+Z3znNgVA53SYcr5U210g2F/NQ1aoQ3Eh4FeSNDL8xDY06LDjouWWc+p6i1lvkTLyKORQa5d8Ot6gGYQJZ03bVV6SFsPKzRvmelUyQPAD4i/98e/h4f/6B/i7/3x7z2w/4LyExEREREREREREc1Hx24J6Ow1MMgYXs+wQRfdQRlh/FffQbYfDA29gFwGhv+/zlEn0svMLJbRbuz5wz8v6ZhmEeV2Y9yz0LHQaAvlUtB3S8LwqCkk5DUprZ3qMXoojOfiTEjHCzCNA4KO1Zh9GOC4hPMRmrMOT4Uiv0l1vLCkc6LkzQfbyIxwnC766/euFIdCHqGZ84eBTn3ug8Yc3l/y7XRUj73hgMdDTMco6tnTRiO4GJKuhZnrLUW+RAvm0TnqINsL6vo4GqRXpq2uX2V6M9eDxFncg8oyC84iHxTSBoOB+7d/+7eY5d9/f+efAwA++JN/FU9vozz8R/8wvuiBtennkoiIiIiIiIiIiIiIiGid3b17F79+7hMAgN/41Cfjqxf2N7+8DwDQ7t2758ZXTvNf3XgWAPAX3/phfNVGCXq+bno5FrEtdaBpGj7+aBhfvHHOnc+wHASwDiewPuZz7nwGrjvzxzydAU3TeG4ErI/txvNLq7Yt1+C2lIPW27ZcZ9tSDtpemqZhG65QDeC9RivDZz0RyWzCs+HevXtnEgB+oIeAJiIiIiIiIiIiIiIiIiLaJgwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIiIiIjOgOv/Ow1B2gwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIiIiIi2BAPARERERERERERERERERERbggFgIiIiIiIiIiIiIiIiIqItwQAwEREREREREREREREREdGWYACYiIiIiIiIiIiIiIiIiGhLMABMRERERERERERERERERLQlGAAmIiIiIiIiIiIiIiIiItoSDAATEREREREREREREREREW0JBoCJiIiIiIiIiIiIiIiIiLYEA8Ar5Fh5aJrm/avY8dVERERERERERERERERERDNhAHhVHAt7tSx6rgvX7aHcbsBy4hsREREREREREREREREREaXHAPCKOEcdoLkPEwBgYr8JdI4YASYiIiIiIiIiIiIiIiKi+TEATERERERERERERERERES0JRgAJiIiIiIiIiIiIiIiIiLaEgwAExERERERERERERERERFtCQaAV0TfLQG1A9gAABsHNaC0q8c3IyIiIiIiIiIiIiIiIiJKjQHgVdGrqJfbKGgaNK2AQfMQVcZ/iYiIiIiIiIiIiIiIiGgBDACvkNly4brev2NGf4mIiIiIiIiIiIiIiIhoQQwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIiIiIi2BAPARERERERERERERERERERbggFgIiIiIiIiIiIiIiIiIqItwQAwEREREREREREREREREdGWYACYiIiIiIiIiIiIiIiIiGhLMAC8AnZFg6Z5//KWE19NRERERERERERERERERDQXBoDPmmOhmxnBdV24oyZQO4Ad34aIiIiIiIiIiIiIiIiIaA4MAJ81vYpWVR//ncvAENcTEREREREREREREREREc2JAeAVCIeANoaoH1chhIOJiIiIiIiIiIiIiIiIiObGAPAKmC3XHwI6g4aWh+UAjpUP5wWucExoIiIiIiIiIiIiIiIiIpoDA8CrpFdRL/cxHAF69dgLCrsuWmZ8QyIiIiIiIiIiIiIiIiKi6RgAPmt2Rejha6PbziHDSYCJiIiIiIiIiIiIiIiIaAkYAD5rZhEo+HMAawWgd4wqJwEmIiIiIiIiIiIiIiIioiVYwwCwjYo/F66madDyFpz4JhvNRMsf6nnbh3u2K+PzmLdWdRbv4Lmnb27ZNTTJfj6Dc+e9fxdf/TBc7rx6JVx+7vk7U7a/g+eCbc9ncG6N6k2e3w9x42khv+ev4MbdYA+xLOLyQHzfDJ57Z7zWefVKeBzx/wEA71zHufPXMZ6q20tL3H/5ziK/8WPI6m0zTdTJCtjPR+/NlbIr0Pz550/T7J8BNipaRbhW6TQ5Vn78XWs8NMlWU12TsrqILIvsk/Q9VVwn3mMOrHx8W/lx51muSt9bZSEfKW9S/rddrOzCOZq8Nvw6jWwf1Fd8Xfx5Gl+veq6p8uMvn7i2ounEr9H4NT1xzpXpTcnHxPJ4+aLln6zLTaAqq/q+k5dTfX/Jt1env37i512LjGolXp92RUPesie2j9fJtojeb3GT92468+5HapPX8Ez3nF3x9+N5oc1gAdCEf1Z8AyIiIlqSab+5V2sNA8AAck2MgiDpcRXsILuBHAvdzMg7h6MmUDtYiwt+K929ideN2/j4oyE+fvcF4Pp3vbq+exNfuW7gjY+G+PijFp699R0voKfaHgAefQF//tHQW/eDq+tx771zHU/++Thf3xgJ+cUX8O13/fx+dAvXLsAPZFaAm/7ydy/htZfHwe8xYd+bJbzSlAe89c8a+PEbPwrXOT8fARhhFAZH7+Fn75Xw1OPjfU7HWeRXVp+z+hA3nt6e4PGymC8NceerD8UXr4TdbaNczqJ2cIpPZbuCwmD8WV4fLvoZ4MDKx4Msi1h2ehvGsbBXy6LnunDdHsrtxvbXhep7iaIu9Opx2FjPdUdo5nIo7fqfitLvqQ6sfAHoBfsEI7zYqGh7QL2JXCw/suPOvFyVvs8+6KDULEcXSvP/oCj7dSicI+nzSkf12Pt71Mwh1/SvnbC+cmiO/HR6WdT2gh96Dqy8gU7J3951MWoOUFD+8JPkBwCQQw41qB7TdkWD0SmNz6M7Qqmzl3AfJ6enzodquaL80rrcFJKyqu471fMEivsrUi89ZGv+uVKlv7bE815GuyEJ5vplPayaU+6hwAP+eUxnTLiG3RGag0LqILDdbaPcc+G6LWxxG37aMk0Arv+vBkw+s4mIiGhJpv3mXp31DADT5tOraIljW+cyWP1Ux7EervEeo0/fxA2hp+m4h+QdPBfpQSn+nZDm3Zu4+PxNr1eln/Y4zSUGyS5cxctBYOnCBWT9YJ/z1m3g+h/6P1Av4o+uA6+99aFy+01hvnQ9+Uf3O9/F1/EC/igIcF64ijsvXYxtJPHIBflL8MefwLPv/RwjAMCH6L1h4NtBXQLAO2/jlStPJOfpNJxZfhOuccR7md/Ejacv4evvvY+vPyb0Or97ExdlvZfP6h6JSLrX4+WZkv+JtK7DFraN98aP9LZX5iHeE1vWW3sRNrrtMoqtIsrtbuTFvNg7SezdIFtuV8SeP9Nf3pqt4GVZvAVc/G/gROgNNe6JZ6DW76Nm+L01HAv5iiX0eoynE/072sPKmkwvaf+JY/nLhB4k6p4/68k56gDNff+cmNhvAp2jzSrDzMTvJfoOshjgxElZF84ROighiP9KOUfooIn9iYeriZZ7jGrsS5DquLMuV6UP+IEY1FHdia+gJOPnVUpmEeX+0PvctQ9QQxOHwndgvXqIZq6N7kw/BLOo1xUBNsdCo11GLxJI01E9TppWJiG9RYnlj6+atS7XjPK+m/F3jnMyQK60658vE8VyH8NRQvqbIrsT/S7qWMgXELs2k0g+3+O9qCM9zG1U8hbsie8JQXKKz2bZ57gv8n3GrgjrY99tVGnLhD1FNWiVbnRdUjpJ+9Ep0FE9jjW8UJwfu6Kh0AbaBaHXsGLb4Dq1hO/PYoxZ9r06OT2i5SgD0s9qIiIiWoYpv7lj3/VStkFcivUMAPdrMPjFd+OFP26MIeqpXwScpot4OejdGvQMrQq9KN97Ea8JPWMHih6WUVPSvHUbsLzetNculfDK7SCg9CO8hksozNXDMsHduxg8OkO68e3fexGPSIJXK/X4dbzxiJevyTz5gcYg+Aavx+uXnvzdFNebsO/VDp69pAoSX8RTVzp4/R14vWfxWRQ+a+DHo3tAcDzjt+M7nYKzyO9kfSZe45Fe5kN8/NJVXPvBbXz7Ub8n8UsXvWDnY7fxTNizuAVcFQK7Z32PIOFenyhPivy/9yJ+dslb98aVDp587Of4hp9upHd9nCoP73wXX3+k5S2/WQKutPCytLf2nOwu2uUiTJgoloWAhF1BAb2wx1rYu0Gx3CyW0Q52lgXHzBZ6We+zfLbP8TY6OPSPFfSS0lE99npgNkcu3GDuhHYHOJT1JoqJ9LBy4baq8vSSRI5lo2IMUQ/rZFrPO1o7zgkGuSkBXYF9UEO2Llxnsu+poyH6wvLVDxHpwGoAPdn1Lcv/A6ONQnCOgkDP3M8rn91F2w8AOieDyaAYdOxkIwsEkvwE/HxNtCAeDdEvF2cPrKrSAxLyoVouEMq/cF2uVIqyCpS/cxT3V38Yfe0+OJl2hHXkB2o1DVqhjXJRvArbKBgdlEazBP1ln+/R6ZLcUQmdsIe9V7+Nie8J8IJuSZ/Niu8M4vcZ5wTIoQMvBj/CMPxuMyXtCBuVwiDsZTrKDNAW1ynTSdqPTs+4QUbS+TFbLnpleD2AW2bitoB3nXaEUQIGwYtAxffqqekRLUEbSGysRERERAtS/ua2UTE6KIUj0fSAQj6+0alZwwCw+KNP/FFHm8Zs+edxlEFjYn60FXnn+rhn3WMv4seRlSV8Q+wZG/ainCIpTTG4+vgTePbW216Q8q3bQKog5Sw+xI3qbTxjpR26Ob69GOhrIXv9hVPofTkf8yUvX98YXYr1QBWHLJ7SM3iCuG8sqBdjGF/A4Ocfer1nH7kAPTyXH6L3BvDMl89iaN+zyK+iPhXXeLSXucI7b+OVK18ThpO+iKeuvI+ffeD/eab3SEB+r0vLMzX/497mhvEFfCnY/8IFKN/3A8o8nDa7O35hGwnimkWU24WJuRyTl3s9iJ2jDhD2bBI28T8D6kNjcn+lMuphryrxpZxEygBetIfVnMRjOScYiIECzeu9pMwnrRkH1l4HpcMpDQdCfq/58AJK+J5aHr/U7ZXbaKS76E+FY+2hU5Jd9wn5fyAIw/wKgaDZn1dCIKxbnAgqpSfPT8DcFwIHUmJvyen5Vqenyodqubr8s9flulCVVU7+O0d+f+nVQ2+oWf9cFdpAdmfaEdaROHyu99JifH7LKJf7y+nBLPaENWroR1YqvidM+2xWfWcIv884OOoA9XrW28fuoh005piWtsjuol2uh73x9Wod4SD8Sekk7UdnI+n8xE3dVrhO9R1kg1ESVN+rp6ZHNJ+aMAewC0z9bCMiIqLFSH9zx77rB79jzsoaBoBFU17+0mbQq6ivw3m8exMXr2Lcu+/dF/Cl+DazminNoGfmtCDcfOznL+G1J19MPW9r8vaxINeaMF8a4s/F4YwldKG3a3rJ5dW/fAl440ewfz7ye94G5/IefnZavVQTnWF+Z7rGF3W698hGePiz+NKtit/Te4RvP6fq6T0PG91g+DrN672DcBjo4KX1IbCnCb0X1cu9HsTeC9NwblQJs+VitGnDWk4jzvHo/5N1tKT1Y1cMdEqHCUPlRjlWAwNlAwL191QjI5uR96w4OOr00a8Z4b3erxmSeQ7V+X9QpX9eBYEwbw7JoGr1nSwwOIkFWB2cDHLIzNPtRq+inq1hzzoZLzMyyE08u0doprnkZOnNRV5+Ufq63HDK3zni/TWeU9prIDLn9bBWJp8fxdYIpY4hvR5SC4aRDj5fR/L5zaXm+mw2kMkNcOKMMMwWYRoZDLp2pMEcMG/aEstKh5bERrct3I+znJ9Ztg2pvlfPmx5RsmAO4CaASnwlERERLd/SfnMvz3oHgB0LDfELOW0OuyL8+I/9sDpLd+9iIP796GfDYW+ct27HegCr/DY+9+h4nlzn1e/gFXH1DGmal0p4pfnCkoe29eYM/aZxG3eCHoVBEDAcgvYO/uR6EFCTbx9x9ya+eesL+NzD8RVnz3n1SmQO1NHofWQ/q8g3gl6kleg8rcFcrkp38HpSeS9cQPa92/jmGwi3MYwvYND8jtfDNr79qTvj/Cqu8eg1pvD4E3j21ncic2N/81YJTymGNT6deyQdaXlmzP+inLduI3sz6IV9S9FAY052F22hh6IXMIjPS+m9pO6Jw0MrlpvFMtqNvcnhnwE4Vj7yAng07Pu9nYIXrcF2jdgQh0KvSX+ey8gIk0rqdPXdElA7SL5OE/afoO8g2w+GiNxM0TqxcVBLDuJvBwdWXkMjM8KxOD9rYl3E/44Rv6dGgnJeADaph5/quLMul4sGm9xeGbnmaHK4c37PBhKfV2noqIrz/JhFlPvRIZ8caw81yXMyLXO/CdRq42eSXkW93EYhxTDFMhPpLSRa/sXqcv0o77s0v3NU95ddQWHgXQ/K9DeCrNw6qodNDAoLDoEvzKnsHHViPYAV3xPm/mzWsVsCOnsNDDKGl86gi+5A+P4xS9qRz4LY94mkdJL2o1NjVwrj3hhJ5ydulm2lYt+rF06PKFnVHwKalxgREdHpm/jNbRZRbjfGI8D4v2POytoFgB0rHxnyKds7Tt1LYzPYqMz5wmajmEUg6GWmFYAzP4938Jw/XG04jOyFq/jek7fDOW4fGRl4Nr6b1EO4VjPCuVEfGV3Ctx/1V82a5uNP4Nn33l/u0LbvfBdffw/48fVL4TC9F1/9ELhwFd+40sGT5zM4d76CwXW/t69ie+fVK5FhfrM3lxx8mpP+1a8BV4N5aTN4EtPmRL2Il999AYNwn+/gc9JelOJ8t0L9SHk9bn8sBCX1L18C3ns/YS7eZVtRfpOu8cg1lsG55+8AeAiFJ+Hl9fk73vm4Ob5/zj12G8+8mzBc92ncI2lJyzNj/hekf9bAK8L1fu7pNHORpzPRmwU6dks5tLt29LNX01BADy0z9pksLAeCQEdfOvyzXq0LnwHifjqq9Ww4dKgxLEV7reWaKA39XotGDdleMDea94K2ZmiSXozeemW6QbAkKEfFlqSXsP8EE61RCZ1g+FMt1oNjE0TqpIBBM32P2I1lH6DWx7hXbDA/Z1Jd2F20Y8OGKr+n6lUcNgd+OgZq2eCa94foNWrhHMHeJac47qzLVekrKPP/wBCH2PTqSv28SsncRzOcN9REy+1F0jM6JYyUQwpP5meCXsVh7IFkttxwrl1vXyN9kFmSnjofquUCofwL1+VKScqquu8Uv3OU95djIR8sLwC94HpQpb+2hKG/VfkNnoXSi0Um9nmsV3FY6oTXtjHMxoZCLiMr/Z4w/2ezvlsC+kFjBRPFbBvtrDjP9gxpRz4LNOyhLnyfSEgncT9aHvEa9p5R48ZRCednwizbjqm/V8+XHtEsmgCO4guJiIho+SZ+c5to9cbvHDWjg9KoJaw/Xdq9e/fc+MJp/qsb3uv/v/jWD+OrNsrf++PfA868HDYq+RPsK18Ena3V1MHyaZqGjz8axhevoTt47vx38Ll35cHVc+czG1KOZNtSjlV6cOtQfo88KPVhP5/B65eGfiOHD3Hj6RcAS/68SOPc+Qxcd+aP+ZRsVLQGMqMHLYC0HJqmneK52Tysj+3G80urti3X4LaUYz42KloXRTcI+tJp2ZbrbFvKQdtL0zRswxWqAbzXaGX4rCcimU14Nty7dw+/du4TAIDf/NQn46sX9qtf3gfWsQfwg8XvtRH+y4+7gtN2eudtvHLla3MHc4i23gN+j5jPib3XL+Hrj6xxXdjd8bB5RERERERERERERLQ2GABeKROtcC5GF+6ohM7eAzA89IPs8ev4+KUZh+AlepA86PfIhau481EwB/BwvevCbE3OKUpERER0Kky02PuXiIiIiIgoNQaAV82ujHsAGzX04+uJiIiIiIiIiIiIiIiIiFJiAHiVHAv5AtALewA3IU4PTUREREREREREREREREQ0CwaAz5pzgoH4dy4DI1h11GEPYCIiIiIiIiIiIiIiIiKaGwPAZ8ZGxR/mGaVd6ACgV3FY6sDwh4A2hlmU47sREREREREREREREREREaXEAPCZMdHyh3o+rurhUr167A3/7LpwWy20jqtecJiIiIiIiIiIiIiIiIiIaEYMABMRERERERERERERERERbQkGgImIiIiIiIiIiIiIiIiItgQDwEREREREREREREREREREW4IBYCIiIiIiIiIiIiIiIiKiLcEAMBERERERERERERERERHRlmAAmIiIiIiIiIiIiIiIiIhoSzAATERERERERERERERERES0JRgAJiIiIiIiIiIiIiIiIiLaEgwAr4SNSt6CVdGgad6/ih3fhoiIiIiIiIiIiIiIiIhoNgwAr0q/hk5mBNd14Y6aGDQsOPFtiIiIiIiIiIiIiIiIiIhmwADwypRRr+re/+o7yPaHGMU3ISIiIiIiIiIiIiIiIiKaAQPARERERERERERERERERERbggFgIiIiIiIiIiIiIiIiIqItwQAwEREREREREREREREREdGWYAB4JUy03BZM5d9ERERERERERERERERERLNjAJiIiIiIiIiIiIiIiIiIaEswAExEREREREREREREREREtCUYACYiIiIiIiIiIiIiIiIi2hIMABMRERERERERERERERERbQkGgImIiIiIiIiIiIiIiIiItgQDwEREREREREREREREREREW0IaAP7F/+d/xP/9dvDPRv//F9+CiIiIiIiIiIiIiIiIiIjWjTQA/Jn/4z/G/3DpH+N/+OJvAfi7yP3v4lsQEREREREREREREREREdG6kQaAPf8O/8+f/BX+T5c+H19BRERERERERERERERERERrSB0A/nkPd//3BeTiy4mIiIiIiIiIiIiIiIiIaC0pA8D90V/iwmf/bnwxERERERERERERERERERGtKUUA+N/hw//vp/EQ5/7den/xrR/iL771w/hiIiIiIiIiIiIiIiIiItpAigDw38X/9co/5vDPW+zv/fHvTfwjIiIiIiIiIiIiIiIios2mCAATEREREREREREREREREdGm0QaDgfu3f/u3mOXff3/nnwMAPviTfxVPb6M8/Ef/ML7ogfAX3/qhtMfvpp9PIiIiIiIiIiIiIiIionV19+5d/Nq5TwAAfvNTn4yvXtivfnkfAKDdv3/fja9M480338Tly5fjizeKLAj6IFAFgDd5LmBN0/DxR8P44o1z7nyG5SCAdTiB9TGfc+czcN25PubplGmaxnMjYH1sN55fWrVtuQa3pRy03rblOtuWctD20jQNN35ajC/eONc+3+W9RivDZz0RyWzCs+HevXsMAJ+FTbgYTgMDwOtpW4Jc21KOVWIdRrE+5sMA8Pp6UL9/qLA+thvPL63atlyD21IOWm/bcp1tSzloezEATLQ4PuuJSGYTng1nFQDmHMAPqL/41g/xF9/6IT74k38V/j8RERERERERERER0SayKxq0ih1ffLocBw4A2BXkLSe+djrHQl7ToPn/wuzHlmuahrxloRJbpmkVLKXE8+Zf5FjIBwWwK0Ie84gnnfpcRdKZr7yOlR/Xq4rqPCCeh3FZ7MpkuZKE+ZixrqP5d2Dl/bzkLe/aE6VNO+12EK7xaWZJk84EA8BERERERERERERERLTBbHQHZZQH3ZkDhPOzUdk7ii+cgY2KMUTddeG6Lly3BxSEoGK55y/3/h1Xq2j525VzTYxcF67bghlLdS5mC8dVPb50JvbBEPWW6QVTC0AvyPuohI4hBm5nO1e55mhcDz2gsfQgY8J5SCiL2apjeJCmBDEz1LVd0WDU+sKCA3RKXn2MSh3Mc/jZLHqN0yoxAExERERERERERERERJvL7mJQ2sd+aYBuGBSzhR6zkp6jdgX5SsXv+RmsF/YJeljaFeTz+Yk0HKuBdr8GI+ieOTyYnpbI7mLQ3BcCuCZa7jFSxgblInmVHd9GJfx/B1bez2vYezO+z3gbx8qPt4mXx7HQQBEmAOeog2xPCEzrVRw2hfMiPVczipRT1it2XI69TnznmITzkFwWE0U0pvQCluQjqOtIr2NZb2IbKLoYNXPxFckmrkNZ/QTi5zsqeo0npePr7MXut+T06XQxAExERERERERERERERBvKgdUYoLSrQ98tYdDwAk2O1QB6Qa/OfRiS6FN/kMGh0LM0sk99iD0/KtfP1id62+rVutcTt+UtDdIa+QFCVVoB52SA7E5CtLdd8INpYkBtuiCvhvT4JorZDo4cAM4ROlkvaBuYzDOwWwJOHGCELLLDIzjOCVDaRSTnoyGQMeL/G9J3shicOMpzlaRfM8b1UADqfoR8XM69SK/Yvdh5rGeFHrQSSechuSyAkQGGo+h6UXI+dr1rz3UxasrSMWHGu3ebLRzCC7Lu4RD+pRcxeR1O1k9g8nxHz4Z4jSelE/DOyfT7ic4GA8BERERERERERERERLSZnCN0+n3UDA2aUUO/7wU49WodKAQB1D3IBrLNBYFMP5I3GvbRDvYptNH3o3K5eBRQIkzLp0orIAYSQ7Y9DvRGhoBOP9RzkFfV8c1iFp0jx+vdWoymKttH3wE6RzZOUEQRQ4xGQyAWMBWDqKqgaHZHV56rJJEhoIV6GJcTKO16x9Z3S/55HAdujUxyD9qk85BYFtW+gsR86MCR36M2MsxzAsfKYw+HcF0Xh9iTzrk7eR1O1s943eT5VklKJxDeJ1PuJzobDAATEREREREREREREdFGsg9qyIY9fV24PS/A6Q3lG18WFQak/EidkcmhLKYl62KZ0tS0zCKytT1h6F8HVqMw/7DIMcrjm0VkOwc46GQRi//K9zGLyHYaGMKAkQEaDUzsJwZC9d0SBoXxsNFaxYbd9fZRn6v5GRmEaThHHf88juOTo+GU4GrCeUgqC6b0HkYsgBzPh13ZAw69euiVI6sSicHnNAFVWf2M10nOt0JSOoHTvJ9odgwAExERERERERERERHRBrLRbZejAUmziGztAJaVlw4dLMoNGpH10V7DmrSH5ZiBDIQ5gGOmp2WiNSqhYwTbGBjWXemwvvNQH99EMdtGOzb8s3ofE8VsH9jRoe8AfWQwEfoTI516FcejDBpBz9Z2AYV2G4VKRXmubNm8winp1UOUOt4w0UanhMPYeWwMgp63qmMknAdlWbxzPu7hK09bng+PWcx6PaE1DV2UE3sSByLnpwD0UlwssvoZr5Odb9H4Gk9KJ7DY/UTLpt2/f9+NL0zjzTffxOXLl+OLN46maXDduapgK2xL+TVNw8cfDeOLN8658xmWgwDW4QTWx3zOnc9sxTN+G23L5++ysD62G88vrdq2XIPbUg5ab9tynW1LOWh7aZqGGz8txhdvnGuf7/Jeo5VZyrPeriB/so9jSSCLZmdXKkAr/VDVUQ6syhF2W9Xo3MJLtexj2PCKbJ5C2jSvpTwbTtm9e/fwa+c+AQD4zU99Mr56Yb/65X2APYCJiIiIiIiIiIiIiIhoEeZ+Bg1Fb+jpdFRPPXi63GPYlQYy+0G4e7lpEy0DA8BERERERERERERERPRgMVvs/btMehXHKYYk3hZm6xi8fGidMQBMRERERERERERERERERLQlGAAmIiIiIiIiIiIiIiIiItoSDACvkGPloWma92/usfGJiIiIiIiIiIiIiOhMOQ6c+DIJx8pj4vW/XUHeStg7ZdqAjUoQY9AqiBzGsZDPW3DiebArkXhENH8OrLyfnr/vqZlWB8sQ1OOsx5p1e8y5z7TzPG/+4xwLeU1bLI2zskl5XXMMAK+KY2GvlkXPdeG6PZTbDfB6JiIiIiIiIiIiIiJadzYqe0fxheklzj+cPm3HagA9F67rYtQcoBEGGRxYezX0/b/06iEyjQpsOLAaQM+fq9euaDBqwVYA7AN0SiMvvVIHB/HA9TIl1sEyCPV46sea5xjTzvPy8u8cdZDtuQulcVY2Ka/rjgHgFXGOOkBzH95j1sR+E+gcMQJMRERERERERERERJSe0Gs17AUr6clqV8Yjcobb2aiEPV0dWHlhebCtsH8+n4emVWBZDbT7NRgVW76tsGyv42dTFPTolOTJiaQtKYdArx7Dj+VC38kiu+MFzRxrD51SE+XxlqjWgUZ+D8N6y49L2EDRxaiZC7eayq4gX6kgH+Q3zL9fb9PWx9NS1EFsw8XPUdiDVnKt+D1OvWX5hI56knMhHM8OjyHPV7yMkfMsyUNkvSz/CWlHs21hr9ZHuxCUTZ5GWI7IzpKySPIq74ku2TdCko+JvNIiGAAmIiIiIiIiIiIiIqLNJPRadXtAoWL7AdBxT9a9IJpU7oW9Zbs2AJgoZjs4cgA4R+hkizD94FzQs9atD8P9+9k6XLeFarWOcq6JUcuUbisuq2eFHrYysTzpkbQV5Zhgo9LIYN/LPPY6JRxWd6KbmEVk+1kU/YAxYMIM/z9Y1MIh9qBpGvZwGAaXRf1BBod+fgvdYqw+p6+XmjgvosXPUUhyrQC7OHSDXtTAcDTeXKQ6F8HxgqOo8hUvo3ieZXmIrk/OQzztCL2Kw2YO5d4xqro6jXg5oCzLZF4j27n7MPwA9uS+YtqSfMTySothAJiIiIiIiIiIiIiIiDaSczIIe77CbMFtmRgNgdKut0zfLYVRvVzGEHcFAJjFLDpHjjf0rB8dHQ37aBf83omFNvoJ+8u2HQ2BYFMjk9zDVpZmQFWOKBsVrYvicRU6vNFH+/0aDK2Adr8WBt4cqwGUIQwTPcmx8tjDIVzXxSH2pPOw5kq70P0ex7K8T1svM227Rc9RQHatQAeO/J6okeGwY1TnIn68efK17DwkmSUNaVkkedWrdSDYTtvDkWrfSNryfNDyMABMREREREREREREREQbSd/JYnDiByodC/m8BWTGUy46R51xNFbGLCLbOcBBZ9w71sjkUA57NLpeoFBBtq2RGcezRkN1QG8aY1o5HAt5rYui0HNTrx77eemhnGvi0Ov2ib1hHa1WC/XhXuLwukGAVN/JTgTtVmbBcxSQXStWZQ849NLojcfMnjD1XPjmyZe95DwkmSUNWVnkeTXRCrbpecF62b7RtNPng+bDAPCK6LsloHYQjoV+UBu3diAiIiIiIiIiIiIiohTMFupDw+tpaHRQOqzCrB6i1PGWGZ2SFwRVMlHMttH2hxbGRI9GTdIT1kAG3vyssm3FZY1Bcg/gSWLayeWwD2roo42CMp8A4MDa66C075XO3C+hsyebkzVW7gLQSxG8PBuLnaOQ5FqpFrOoGV4aXZTHAeKYaeciMD1fgXH+TGkeJvOfNg9JZklDVhZZXh0rH26jFYB6VZfuG007fT5oPtr9+/fd+MI03nzzTVy+fDm+eONomgbXnasKFmZXNBTa3v/nmiMcr+ACX2X5l0nTNHz80TC+eOOcO59hOQhgHU5gfczn3PnMVjzjt9G2fP4uC+tju/H80qptyzW4LeWg9bYt19m2lIO2l6ZpuPHTYnzxxrn2+S7vNVoZPuuJSGYTng337t3Dr537BADgNz/1yfjqhf3ql/cB9gBeLbM17v6+iuAvEREREREREREREREREW0XBoCJiIiIiIiIiIiIiIiIiLYEA8BERERERERERERERERERFuCAWAiIiIiIiIiIiIiIiIioi3BADAREREREREREREREW0ux0Je05C3HMCueP8FAMeB/3/Lo0pTzMOsgjTFvJ82VTmWYeFy2KhoGjRNg6ZVYAMAHFh5f1ne8vM+ZVnF21O+nXCMcDt/ayuP8aIp6c28b7gh8mFeZMQ6iNdFsElCPavWJZ131T60kRgAJiIiIiIiIiIiIiKijeUcdZDtuTiu6oDZ8v4LG5W9o/imC1KnGcnDTNRpnp5VHDM9x2oAPReu62LUHKBhOXCsPQzr/rJSBwc2APsAndJIuayHgheMlWwnHsMtdsOgrV3RYNT648xMSS9cNnXfBsaxVQfWXg3ClhImWq4L1+2hnGti5Lpw3RbMyCbBtZ7Wep93Wi4GgImIiIiIiIiIiIiIaDM5FvZqfbQLeS/A5vdidKwG2v0ajIrtLatUkA96UdqVWI9Kobdl0Csz3Ga8XSTNpDzIepzaFeTz+YlenBNpDg/G+QTkeRPFywa/d2mYd6Fe/ONb8WMKacXLLPYKDXu3xo85UZ8AOnup6lhWJ3r1GC0/0qnvZJHd0TEaZoGut7/RKWE/Egkdc06A0q4XFDWLZQxOJmpMqt21AdhA0cWomQuXy9KTLZPtOw7QOjgZZLHjx2odaw+dUhPl8ZbpiXUWnBvZ+ZaIXGuJ+3jXr3fe5edt4jqJkF//yfvQsjEAvAJ2JbjI5xwOgogoxn4+g4uvfhhZ5rx6BeeevxNZNukOnjt/XfmBK0s3znn1ytRtVuND3Hg6g3PnhX9T62P50tQhERERERERERHNSa/isJlDuXcMsTOkXq17PSf9SGJ/kMGh36O00C2GvUu78d6g9SH2gvf25V5ku3iawsEiefACfOMep0F6/Wx9ohdnPE0xn4l5EwT7uD2gYTkAdr2/XRejJjAc+dv5x6+qyoHJMqsk1SfCY43zpCqHrE7GbFQaGT/Y2waKsf3NFg7hBZr3cIiWCYyGg3gi0u30ah0o+LGaxgBe2NaEGcuILD3ZMtm+HhsVzUAtW/TK6FjY65RwWN2Jb5jaZJ3Jz3dc9FpT7XOEirYHHHq92VXnLek6UV3/SfvQ8jEAfNYcC92Md+G7oyZQO1AGXoiI0jIvlfDjN34ktAD8EL033sezly5GtpuV+dIQd776UHzxBvkCvv3uEB9/NMTHH93Gt/+8cuZB4M2vQyIiIiIiIiKizZcr7UL3e5TmMkZk3WjYRzsIBhba6PvRsPh2aY2G4x6i+m4pjK6lSS/IZ0CVN1G4j5HxjqUDR34PTHFI4lTHT7ENptQnxHT8PKnKIdvXY6OidVE8rvr1UUYxFmB1rDz2cAjXdXGIPeQtB0YmG91Isd14iGUXbj0LKPIhS0+2TM0/TrHr9Uw/6qDfr8HQCmj3a9KA/jQTdaY434kU+/RrNbSFzWY/b4td/7Q8DACfNb2KltgMKZcBL3kiWtjjT+DZ926jdzdYcA8/e6+Epx73/7x7ExeFnrDxHqmjV6+E6557Z7w83rvXEbZTBlKnHGt1HsK1H7Tw7K3v4MZdP5/P3/R6CT990wuex/I+ros7eO7pm7CF8o/LlbQuXofetjeelx1jsseyeC6IiIiIiGh+dkWDFh/mMokw3CUcRz7c5owvbMNhM9Oa4xihafvKyrSoIM1px06yyL5ERAswMjmUg16OrgtX1jN2BkYG6Bx5zzPnqKMMLqaRJm9hUHg0BDIG7IrXg9N1XfTmGmdYbjRMGVyU5ClNOUKOhbzWRVHo5Wpkor1Gs/54ysF/9Z0s+sMR9J1x3dvdtnI78XNZ3C5Olp5smYzss1+vHvt14M3tezjTHL5y85xv1T655giuW8dwzxu6eabz5lvm9U/zYwB4BcIhoI0h6mHrFSKiRVzEU1fex2tv+YHGd97GK1ee8L8g3cFzj/0c3/ho3BP2mTde8IKgAIAOXsOL3rp3X8Cg6QdD4+7exFeuG3gjSOclWe/iacdaNa+efvaB/+et24A1xMc/uAodd/DcY7fxTNhjuAVcvTLO+3sv4ptBPX3UQva6UK6kdXHvvYjXjNuT9f3Od/H1R1re8psl4EoLLwcBfCIiIiIiWoCN7qCM8qCbfhS2cM4+G5W9o/haYf0pWuQYifsqyrQQIc3EY0+xyL5ERBMMZCCZ51YiMhxw4tSN6dLUq4codQyvd2WnNCXIl5xmmrzlBg2/hyZQr+owi1nUDG/7LmTz4CYfM8IsIlvzytIYCPPbThHPU5pyBOyDGvpooyBsq1cPkWn4+/vDQkfSLAC9lgmY+2HdF9CbHO7Z305ML9hOSpKedJlEPM/q68BGRTa/c0rTz3dgfN6T9zHRqg9hVOyZzltgtuufTot2//59N74wjTfffBOXL1+OL944mqbBdeeqgsU5FvJGB6XRMXaP8mE3+3LPVT4wlm2l5V8iTdPw8UfD+OKNc+58huUgYN46fOc6zjU/iz//wVWMns/g9UtDL4B49yYuPvYifhzb/NmbQ7z8+B08d/5tPPXR9XGwWPjbefUKvoIXceerD0X+XxRZnnis2MIZzFUf+BA3nn4BsG7h2oXxUjuom4dv4mIV+N4PrnoNcd65jnO3n4gEtsNtJ+op7bpY/cTqN/K3eHxJXuZx7nxmK57x22hbPn+XhfWx3Xh+adW25RrclnLQetuW62yiHHYF+ZN9HGIPBzvH/jsXGxWt4A9xWEYvPvegsI9R63tz1okva/z1x9VRcjrCcXK5HLL1Y7RM4di5JkbHVeiy/EwcI4dyGUDxGC1UoBWCARolxw323TmY2M6w/HdQ5R7cFhLyEj1evjFAv59Fb5RBw6jBe4uVQ1N8r1XueUNcnuzjuApYeQO1vpC2nTLf0npNqiMdjpX3z6+sflUkacKZzHd8twVpmoYbPy3GF2+ca5/vbsUzgzbTxLP+QSY8C4kedJvwbLh37x5+7dwnAAC/+alPxlcv7Fe/vA+wB/CK6VXUy31vSP6w2//ZBX+JaMuEw0Dfweu3hOGfAeDRF/DnYa9c798iAdlEZ3msmd3B67e+gM89HF++Bh7+LL50q+IN/3x1hG8/t1jwl4iIiIiIAMCB1RigtKtD3y1h0PB61zhWAwiHM9yHoejMolfrKOeaGCle1kxLR1xfz3oh08g+9SH2LCcxnfG6Q2QGwtCb5R5c18WoGR0Sc0JsO7FMyXmJHq+frcN1WzCxi0P/Hdao6U81Kaknx9pDpzTytit1xnMcpsi3rD5ky2RkZVKRpanMNxEREdEGYQD4rNkVYcx3G912jsOfE9GS+MMbvywO/wzgwgVkI/MDz0f/8iXg+neTh0xb0rFOi/18Ba9c+VqkR3Do8SfG8wPD6zn9zUggvYNvBnP5zrQuHeet28jeDILm0V7LREREREQ0J+cInX7fG+LQqKHf7+DIiQ+nuYd5B0Selo4/7SHgz6HnLeujHQ5D2fbmK0xIZ5yGjt3SeOjNXMoXSknbyfIy9Xg6cJT39glGs5MZDYHSrtcbTd8teZHiKfkJyOpDtkxGViYVWZqqfBMRrS0On09EEgwAnzWzKHyxLAC9Y/DZTETLYl4q4ZVbHTx7Sew9ehEvv3sJrz2W8XqXns/g3PnryYFcmQtX8Y0rHTwZpPH8nfgWyzvW0ryPrwt5eRKthGGVL+Llm8Z4+8du45l3x8M6AyVkR5f8dS8iezPtunT0zxp45apQb08r5mImIiIiIqLU7IMasmEPTxduL4vOkePNbTexbB7J6RiZcfxwNPSCpUYmh7KYJ28yQWU6sjSWRZaXacezK3vAobd9rxxfO2ZkEJbDOeqMI+GpyOpDtmwsuX5VJtNcLN9ERERE62FNA8A2Kv6E0pqWx3aNtCJ8sdzy4Z7tSnAO000Mfjru4LkHIIhiPz8OGl0MeiH6c7OGwSQhWCff/g6eCwN2Kwg+vXMd585fGfe+PBV38JwkGGk/H6235fkQN54+47p8/Lp8yOULV3EnMixzEKC8iJeFuWvjf+tfvRWZ89d8SUjDD6TGt1Ef66w9hGs/iA5FHQn+XriKO8H8vwG//lS9cJ8Syh+vY9W6aP2o69u+3cGzYQ/g2/g2TqMn9el8vjpWfoXP+fTsyio/j9bN6VwLRPPxr8e8NyTnmAMrr0HTKhOf3QuzK/71Py1tG5Wp23jmfxamP8a8lvv8E58fGrTx8EYLmKcO5tmHZnc6nxfz3y+LmP+aWU1+aTlsdNtlFMUfJGYR2doBLCs/fpYVgLqydb6BDGowFM87Z0o6Yg/TxsDrTRvtdeo9o5PSkaWxmHGZZHmZdjyzmPV6VGsauihjcOJI60mvHqLUMaBpGoxOCYfKOp4kqw/ZMu98esdIql/ARmXiu4b8OIvke138+1t3cO3z3fDfP7v1H+KbEBER0cKC9xbBv+X9ZlqGNQwAO7DyBWH+DfaQ3UiOhW7Gmy/FHTWB2sFcP7Qphbs38bpx2wsavfvCeIjeuzfxlesG3vhoiI8/ao2HtlVtj9jcrfHA2Cmzb3fw7BUDX39Z1qv0dJkvDaMBzKW4g+fOvwDUXsCX4quIJMznXsAg7AF8CV9/RDFU9dxin6+jEjoH2/xkdmDlo1+6zJbLIZGAyWuB37VoLeSQgzckZ8g5Qgc5TL52lpm855PY3bbfM6i1okZKyzS97Mt//pXRc1247gjNQUGY4iZuet7UFtmXlmOdvzts8/WxzWVbBROtiWe9t6xaPR73EJ3YBsJwmjqqx5JepP56fVo6QkeA4+NjvyNAtHOAMh3/GLJ5hMXhPvVqkK4gWC/dTizTZF6mHQ9mK9y+1ZLUU7zuXBfucdV7xyDNjyChXmXL0tYvYCCTjR1LmaYk3xtk2Ojin/7wt/BPflrEjZ8WceOnX8bv/PB9/OgX8S2JKBW7Mn9DsFn2dRyvkcos+wSCfebZN8my01MRjzNLPYQNe+WBN7uSssFqJB0tRUPhSY6VT/hd5MVL8pFj+A2UZGVfJlWafn6m1vEMlHUQKbtwnmLn2LHy6c7X2smhOfK/N/SyqO1NNjhblfULADtH6KCJ/fgXQNosehUt8SVTLoPVD5gT6+Ea6W3q9RS+IfSMfe4dcT+x16j4d0Kad2/i4vM3wx6gN54X0/wQN55eUm/XC1fxchC8vHABWYwwuuvNJ4rrfxj28vyj68Brb32o3H617uD1WyU89dITePbW25EPWLG3sjiUsGy5PWcdO69eifaEVl4L/nkVzrm65/BFvPzRLVx7OL6cNlO8564oad0M4j2nlUNVz8k+QE38fNWrOA7etsS+hAbftezK+P9hV4TeeWlfTHqt7K1wRIgKbOFYkS+ZijxM9tYR/46nH+znwMobqAVzvfmJRXvvqPYN9o9+Kd/I758q/K5FaymLUmk83CLgDbmYrdcReVcbe1Z497Tsno/1UhV+ZNoVDYU2vLkBp2wbOBF6B6X7gZz0jPGfqcHxKt3ofspnnv8CI8xnBbas7I6FfMXynmP+c3ui96K0HlXHSOLNDTk4caKfGeFzNH5e0pKUC0n1Rqdibb87yK6P9J/d4v0c2UZRJqmEeyhCmabqXpeVjSjao7UwOP3vcWd9vLOho9ravGDuzH7xc/zwX17A1/7FZ/GfhQv/E/zuv7iI3/1MZEsiOgup5+a1UdlTzWw+g9THWzNhvmeoB8eC11bRD7yNSugY0e9X3UEZ5UF3ym8aT67pd2ZzXbg9oKH6freIck9odOQ3UJqn7Kmp03SOOsj2lt1QWMKxkDeGqIflrmNoSH4X2BXs4XCywd2mMYso94fwZ9KY+D2g/N1wStYvADwaot+vwQgrZdpLB1pX4csjY4j6WrSYvIiXxeDKu5fwWlUYmve9F/Ga0DN20EwzbO+UNG/dBiyvN+21SyW8ctvv3Xr3R3gNl1BYau8+AHfvYvDoDOnGt3/vRTwyNbB5Ct55G69ceQImLuKpKx28HgRc37nuzdka1rEfZFMsN5dVx8pr4Q6ee+zn+EZ43Nt45o0XUgWZiVbNORkgV9qVPIttVIwOSkFLNbcHFLwvYmaxjHbX+xR2TiD0zhthiBJ2JxOb1K9hWPTS7pXbKARf+iKjQ6jzMFW/ho4w4sSgYcGBjurxCM2c3wJP9eVRuq//wjvrfynvlYFyb7Jnwibjdy1aUzu7JaBzFAaLjjrZ6JCdsFGJ/HAcodTZg+XI7vlozx93VELHb4Vrtrz5Csu96dt62ujgMHw+ZWt7Czyf4JWjMAhbCI8yA7Tj+8rYFRQgvjBowVQ979odb25G6XdwVT2qjpHEwVGnj+yOHvnMCBqajFxJ3lKRlWvOeqO5re93B8n1kfqzW7if4/elokyTEu6hie3SphmQlI0IiH5WSZ/ty3bWx6Olufe/4YPLfxeZ+HKirSc26vR/48p6HdoV5CsVf3kFdnxqmPh61THCRm6S40Z2GffMDQJAsu0cq4F2XxhGf3gQy4Ps2BKJx5uShqy+xivHje2CfROPkUelEu8N6sDKe9uNG6j6w/P7+Z5eD0JqRx1ke8LvFb2Kw+YAwU8S2F0MSvvYLwnLZmVXkM/nhca38fob1+leJ75zSrKyx6/D+HUqO5eS8zFRnwHHwl6tj3b43VRSNqF3btizV3KMaXUwcZ5gotXLRhp/w7GQ7xZPPxh9Fuwu2mFnyLS/G07P+gWAEW0J0Su3T6e1BZ06s+Vf2KMMGhMfGivyzvVxr9HHXsSPIytL+IbYM/a9n49baiRJSlMMrj4+7t3qvHUbePJ3l/wj6kPcqN7GM1baoZvj24vB7Bay188usGnf7uDZS15vx0gQ9/En8OytyuTcwInLl1HHimvh7l0M0MGTYQ/gS/j6e+/jZx9E51uO9BgmWnd2F+1yXRgC2ESx3Mdw5Ldaa3dhw8FRB6jXs95yu4t2difd/ZUb9xgwMjnkmvvelz59Z9yrLykPU5XH86PpO8iKreymWmTfDcfvWrSO9Crq2RoObPjBnGI0+OicYIA2CuEPTq+XnPJZIf44NWrwB7CUS9xWeFYs4/kUe+bp1TrK4m4qZhHldkHyMkYilxBoS6rH1McI9jfQKY28QFv4meH9yIc0cLiAeeuNli/pc/usvjvMLd19mXivJ91DolnSJCI6Ff8r/qdwHuA7HAKatpo4dL3r7sNwAGAXh/7v3lET4Wdwf5DBoeti1Byg0C3668dBwmB9vBdo5Bj1Ifb8oN3kcRX83+HisQJ6tY5yromR3/hLzGPXlh97qtjxpqchry8AcKw9dEpe49ZRqTPeV3mMQ2QG8V9gOnZLwIkDjJBFdngExzmJ/G6YVg+i0RDIxIYc1Xey/rz0DqzGAKVdHfpuSWj0p9b355PXNGGeeQD9bB2u24IhqQPplAlJ2gVJANWTVPb4dao8l7HzEU9TOBgOmzmUe96UYMrzK6M85ynrYMIRKkZt8mRuFH/0Hk2D1i2OG8+l/d1witYzACwwMulm/aI1pldRX4cfundv4uJV+HPiej07F56bdaY0g96tH6L3BvDMl5c756z9/CW89uSLqecMTd7+Ip664gU2T98dvH4LeCWY+/RqBwiHgQ6C0i8CVXEIaPXy06xjIDZPsv/v5ccB/au3In8TrRt9J4v+zA9iA5ncACfOCMNsEaaRwaBre3NnRrvlbRcjg1zwpbwwQHM7xrxT4nctWidB70HlcybXxChsPev9i/+WBfwWxJHhwJrquYRn2Xalgt5Yh8De5AuDmSjrMe0xgjmAxSHDTBTLbXRtL/BXUkagaVNs1HeHs/7sVt5DREQr9tv/KR7+l/8OQwDAf47/xp8D+A/+y/iGRNtFHLpe0/ZwBAA6cOT3ajRq48BUMMKJvpNFThJ0CkdAMTKRKOho2PemkdE0aIU2+sOR/LgKsmOpxEdhkR17mvjxpqahqC/4wdbg+72+WwrrZfIYQRzPmyomTt8BOkc2TlBEEUOMRkNgR/27IV4PotjpCWV3dG9EomBKDaOGfj8YlUYtMgS0MBJSUEZZHYhB6FTvViJDQCePtpR0narOZXy7tGRlU4kfY+Y6iOnXhiiuoGfscgVzAI/QHBSiPd9X/Lth/QLARgY5v+W4OKQYbRi7EpnfqNvOraYRx927GIh/P/rZcC5i563bsR7AKr+Nzz06nifXefU7eEVcPUOa5qUSXmm+MP/QxFIf4sbTGXzTuI07Qa9VAPqXLwHXv+vfS3fwJ9eDgKh8+4i7N/HNW1/A585i/tp33sYrV8ThnG/j248Kw0ADAB7CtR8M8YY4PLRi+enUse/CBWTfu43eGfWMJloqv1dXZO65iu0vb4y/ZDkWGu2yP+yq1zqzs9fAIGN4PWUGXXQHwfolScxD8CI5WNU49SE/g3lQvC9mXmvIrcLvWrTO/GdVIXwGCPQdZFP8cA+Fwy5593ViW+TEbYVe8pHn05wi92D8uZbmmaejeuz13o+3gk8lVT3OdwyzWEa7sYdO2qF+Z5FYb3Qq1vm7Q8zCn92JZYpJdQ9NSzPNvU5L5TgTwxkuzWmkGfKHxgz+VM4r7W9d4dzRD7zPfBa/d/kuvvOPfo5/H19HtNWEoev94WXtyp43LYrrTQGTVhgYjXUxNTI5bxqZ4Djx6WTiw9oukfzYs5mWRlJ9GRmEZXOOOsremmJQdjSU/AIzi8h2GhjCgJEBGg3Iv2+loO+WMCiMh5TWKjbsrpeefVATvhsu59zI6mBqeU/JtHM5K1nZREllm1YH4nnyeFP7BAFnb7QfHdXjOoaROZw3kY5qvYx20OM87e+GU7R+AWB/rPZgSLFaVjV3z6aKfXnfVmZRaP1UAPzhBM7OHTznD8kcDgN84Sq+9+TtcI7bR0YGno3vJvUQrtUMfP2xYL9L+Paj/qpZ03z8CTz73vsLDE0s8c538fX3gB9fvxQOQXzx1Q+BC1fxjSvBcMUVDK77vX0V24tDGJ977EVkb95S9A5eLnH4Z89DKDz5Bbxy+040T+czeBItvPx4dLhlcTmQpo7FIZyDnsNpXcTL717Ca/61kJzG+Br8sT+38tkNDe0F+cd5jA2VTSncwXPKc7upTLRGTQzCZ3MDmX3/x0ovOx6qxOigNBq3QtR3S0A/CBCaKGbbaMeHZV1YUh50VOvjdcawhGaqBoXeC+iaMftLMH0nO25JqSnmxtlkW/9dizabiWI5+BEYZ6I1KqETPCs0TeihGrvn9SoOS51wrmtjmFUPFzxt21wTpaE/HJhRi81fNIfIPahhD3XhuaZ+5jlWXii3hgKCe3fW5526HtXHSMksotzvC8O4xfLmWMgrh5cWh8aqwI7vm1hvdDrW+btD9PpY/LM7uUxR6ntoYjtlmup7PV42WgYblb2kPlkLMltnNGddfB65+LzSNrqDMsqDcWMZejBl6kV8bed/wT8Nh39+C3+K38J/8Zn4lkTbI/I91h++1yyOP2u7KPtDA0+XGzQi6QSivX01f97WyePOx0AGkrlafbJjz2paGkn1pVcPUep4v4mMTgmHinKKx2gMZF/WTRSzfWBHh74D9DFuiOtJrocIvYrjUQaNoMdyu4BCu41CpYJuvCGfWUS2dgB7gdiMrA7k5Z33GOnLPu1cjqVLU1Y2r868ZfJz6ZHXQWSD8Dx5+W0gM5LFiky0ekAhb8GZuw7XgLmPJoKgb9rfDadHu3//vhtfmMabb76Jy5cvxxdvHE3T4LpzVcGcbFTyJ9gPxgFfsbMv/+nQNA0ff+QNcLPe7uC589/B596VB1fPnc9sSDmSrbYcyXW8KRarww9x4+kXAGvROlhWOotbrD7mcQfPnX8bT310XfHibzOcO5/Zimf8WbMrGrrFYEgWB1Z+DziUfTmd37Z8/i4L62O78fzSqm3LNbgt5TgNZ/HZ/aDYlutMLIdj5b0Xw+Ue3GIX+S6Adht9lNFzWzBho6IVvF7YuSZGx1XodgX5xgD9fhY9t4hufL14MLuC/Mk+jqujcTph2tHttELQ1ztY78DKG6j1FWmL75DC4ygubH/9IfZwsHM8WwMeOnOapuHGT4vxxRvn2ue7W/HMoM10Kp9Z0561lMix8uFnUPT72bpwYFWOsNuKf97SNjmVZ8OS3bt3D7927hMAgN/81Cfjqxf2q1/eB9ayB/ADxUYljPxr0JSt4WlrvPM2XrnytZUH07Ya6ziB3ytZ0TM40rP6+Zu48fQlfP29973e78/f8Ta6exMXhTTCXs13b+Li8ze9nsdP38SN58Uezx/ixtNb0gtZVX4A9vPynuGq5bS+zH2xt5OBWrbOF8hERERrjJ/dlESv1lHONTHy30D3Bxkcui5GzQG6tjcEN4JhFOtD7PkvZvrZOly3BUOxPi6SjrsPQ7aZP/ff+Nh76JS8OQdHpY4ybQBwTgYJ03Y4sBrecIr6bgmDYOhBIiKiMyT2Bi0Mmthfq+AvvFFYGPylBwgDwCslzBHgunBHJXT2+CV9qz1+HR+/JA53TEvHOvb5gdtI0PEiXg7nWh7i43cv4bXqTe+Zc/cmvnLdwBvBupeu4toPbuPbj34B33536NfpHTz32G08826QRgu4KgR2b90GrCE+/sFVXLtUwiu3g6Dxj05nTuYzl1D+d67jSYhzWfs9h1XLab3pVRyLn8/r1VyViIiI4vjZTTPIhcPUe0bD/ngI8UI7nPsx589/p1ofFx2OcQ+yQaeDNAOjIcI58PTd0ngSPQl9Jzs5fKlte7/1nCN0+n1v6E6jhv6K55sjItpYZzas/7YS4h0To1oQ0VljAHjV7Mq4B7BRw+Q02URE8/ADt/Gg4zvXx71RH3sRP/YXO2/dBq7/YXJwcqJ39UU8deV9/OwD/89HhSDv40/g2Vtve/MJvnU7YU7mDZJU/sefwLO3KhO9qpXLiYiIiIhoLRiZHMphz93JBgTT1o8JL717WXRSRGCNDMLtnKMOEAsQR5hFZGt7wshxDqxGAV0bsA9qyIp5THl8IiIiItpeDACvkmMhXwB6wRf0UROSabKJiJbj7k1cvIpxL993X8CX4tsszUU8daWD19/5EL03gGe+/FB8gy0T9K5+EajKel3HlxMRERER0dkwkEENRkX+TTzac1dDPjYM87T1AcfKjxv4F4B6ih5kevUQpY4BTdNgdEo4TNzHRGtUQscYD3c+rLtomTa67TKKYlzaLCJbO4ANG5U8R5ojIiIiehAxAHzWnBMMxL9zGQTtO52jDnsAE9HpevSz42fOW7fDHsD6ly8B17+bHJx8/Ak8e+s7456sd2/im7dKeOrx2HY+81IJrzRf2JLhn9OW/yFc+8EQb1zp4HVhfmD1ciIiIiIiOl06qsd+z11haE+9egyvM290eq7jqh4bAlSyXuRvq1ePxz1w3dbk6ErSY/t5c1VDZZpoictjw52P8x8/XrAstj8R0VayUQka4IT/KsnvuER2Rdm4Z504Vh4VO5Zfx0I+aJyUshxhOgtzYOX9+g4TlC0Tqder8yWe3+C8ytKZsp2WF0bRmJ86n/Nbv3MLwHFOvwFZynLR/BgAPjP+A8ioAcF8M3oVh6UODP/BZAyzKMd3IyJalgtX8b0nb+MRfwjoR0YGnhXWfeNKB08Gw0M/fwfAQyg8CW8u4efveL1ZbxrjuYUfu41n3k2Y0/bxJ/Dse+9v8PDPQn2cvw47ofzOq1fGQ2ufz+BJtPDy4+rlRERERERERES0DEFDnR7KuSZGqoY420JoUOQcdZDtyRovnQH7AJ3SCK7rooeCH8AUlzUmA66yfQDYFQ1GTd41zrEagD/Nwag5QMNypOlIt8MIw2zPbzh1jLOsnrmsy7mFjcreUXwhLZvm/zsNftoMAJ+ZcYtR8WaNtBBttdgyk4iW4CFc+8EtYa7aMf2rt/x5gYf4+KXrePkHV8NnjvlSMGfwEB+/dDG6vf83Hr8+3uYj4RgXruKOkNbYFzZ0+Odg6ObYPMqK8kfqVVZ/seVERERERERERHSahN6f4XD4smUBWQ9Sgd8jM9Kb1K4gn8/72wv7T6Ttb1up+GlUYNsVdW/VcP9xmnsdIR3LARwLe7U+2gUhL97/SPIhSSdCcuwwf/L6cE6A0q73JtAsljE4cYRApYOTQRY7sReF0n1gA0UXo6Z8cszxqBmAvpNFdkeXpiPbDs4JBu2C+pwozulkuafU3zqf23jeoC53cC1bVgPtvmz6DMk9IvTijfRkjh9TtixItRKbYsOuTPQQ30au/+80BGkzAExERKfjnbfxypWvSQPRREREREREREREp8Wx9sJeoqNSB3uWI1023n7cg9R192FMRAt3ceh35Bo1geHIW9rP1uG6LRji/vVhJO1Af5DBod9DtdAthr1Vu7Yqv+M069lYD1m9isNmDuVetGdrpBx+PhLTUdQVAKDs9Z4N8igaDSMTXQpsVDQDtWxxohe2fB8TZnxDKRuVRgb7piqdwHg7jIZA0yuXewgcTJwT+TmNl3ta/WGNzy2EvLk9+D2j5eUOruVqte71pg8i6r7p98jY5DHlywDAbPWQrR2Mg+WNAZr7qS6KDXf6XYAZACYiotPx+HX2eCUiIiIiIiIiojM3Go57ieq7JWA4ki4L6NU6UAh6N+5hYgBcHTjye3GKwxXnMgYAYDTsox3sX2ijL6QdbutPDanvZMP9ArK8jYZAsJmRkfeQjZPlY1o6smNDKJuMkcnGF/n8kVCL3Yn5XdX7TGOjonVR9EdPVacT3S4ydPJoiImw8ZRzGphWf1jjcwshbzAy3rlNWe64qfeIYOKYimUeE8Vy22tk4Byhk62v/3DdG4IBYCIiIiIiIiIiIiIi2hpGBugc+UPTHnWAjCFdNjaewtHtZcPtAnZlDzj01vfKkVWAH3wrh70jXbix3pPTyPImxslGQ3nvzjhZPqalIzv2NPrOeB+72/aGZg6GAFaQ7TOVYyGvdVEU5nWWpiPZLp6f+PGmndPAtPqbRla/86Q5z7kFMG6M4EeL05Z7UvI9Ih4/fkzVsoC538Sga8M+6KD0QPT+PRsMABMRERERERERERER0dbQq4codQyvl2OnhMOqLl0WcKy837NRg1YA6rEuiGYxi5rhre8imL92LNo7MjanaQqyvIlpNgby3p1xsnxMS0d27KnM/XCfAnpomV46mYZ/7EbGT8dGJZivVrKP3Hgf+6CGPtooiPUqSUe2XSQ/3eLE8aad08C0+ptGVr/zpDnPuQWA3KDh7eNf19PLbSCDyTmApfeIWUS25pVNPH78mKplIb2KOhpooAS/szQtgXb//v255hl+8803cfny5fjijaNpGlx3rirYCttSfk3T8PFHw/jijXPufIblIIB1OIH1MZ9z5zNb8YzfRtvy+bssrI/txvNLq7Yt1+C2lIPW27ZcZ9tSDtpemqbhxk+L8cUb59rnu7zXaGX4rCdKwa4gf7I/Hgr7LMiOKVsW4cDKGxjW3YlA/aw24dlw7949fOITvwYA+OQnfzO+emH37/8KYA9gIiIiIiIiIiIiIiIiIjpzdgWaZqCWTeoVTvNgAJiIiIiIiIiIiIiIiIhom5ithF63p0R2TNmygNkK5zSm5WIAmIiIiIiIiIiIiIiIiIhoSzAAvBLeJOZWZTxhd2w+bSIiIiIiIiIiIiIiIiKimTEAvCr9GjqZkde1fdTEoGHBiW9DRERERERERERERESzc5z079xTbutYeXlnLsdCXtOQt9KkMgsHVt7vSBY/sGMhn5fFFdT7KPMPGxW/s5qmVeBtIktnynZaHkuvAiKaCwPAK1NGPRjzXN9Btj/EKL4JERERERERERERERHNyEZl7yi+UGGWbeWcow6yPVc9z+m87AN0Sl5Hsh4KQvDWgbVXQz+6tUexj13RYNSke8CxGkDPheu6GDUHaFiONB3pdhhhmO15nd3cYyy7CohoPgwAExERERERERERERHRhprslepYDbT7NRhe1BL5cL3fQ9WuIJ/PQ9MqsMRtxbTC3rXjZXud+LG9nrh7tT7ahcm0bbF3bJCeXUG+UvHzVIFtV2I9aoWkT4DSrhdRNYtlDE68HDnWHjqlJsqx7aHcxwaKLkbNXHxzAIBePUbL9P9/J4vsji5NR7YdnBMM2oVYnRHRqjEATEREREREREREREREG0nsleq6+zAcQK/WUc41MWqZAHZx6Aa9VoGhPxRnP1uH67ZQFbaNpFUfYs9yIsvqWUkPWr2Kw2YO5d6492uQtmHthb1oR6UO9vzxkfuDDA79XrSFbjHsUduNRYBHw0F0AfyAc6eEw+pOfA2g2gcmTD9wm8xGpZHBvqlKJzDeDqMh0PSnuzwEDjgGNNFaYACYiIiIiIiIiIiIiIg2kl6tA4Wgh+8eJgZz1oEjvxeuOARyLmNENgOA0bCPdpBWoY3+cITREAg2NTLyHrRxQdqj4bgXrb5bCqPPudIudL8XrSwfASOTjS+Cc9RBv1+DoRXQ7tfCoHJAtk86NipaF8XjKvTEdKLbwWyNh74eDZEUNiais8MA8EqYaLktjBvcxP8mIiIiIiIiIiIiIqLpTLT8Hr5uL4vOUTQgalf2gENvfU82ZrLAyORQDnsTu3BbJozMuNfwaCjpAZzAyCDMj3PUGUeSU9J3xvvb3TayOzr06rGfvx7KuSYOY5PuyvaZyrGQ17ooCnEKaTqS7RwrL8xNjHTHI6JTxwAwERERERERERERERFtJMfK+71/NWgFoF7VARjIwJvX1yxmUTO89V2M59EdG28b7U2sIW85kWWNQboewAG9eohSx/B6H3dKE8Haqcz9cP8CeuH8u5NsVIL5d+fYxz6ooY82CkK5ZenIttOrh8g0/DrrFv3jCfkhopXQ7t+/78YXpvHmm2/i8uXL8cUbR9M0uO5cVbAVtqX8mqbh44+G8cUb59z5DMtBAOtwAutjPufOZ7biGb+NtuXzd1lYH9uN55dWbVuuwW0pB623bbnOtqUctL00TcONnxbjizfOtc93ea/RyvBZT0Qym/BsuHfvHj7xiV8DAHzyk78ZX72w+/d/BbAHMBERERERERERERERERHR9mAAmIiIiIiIiIiIiIiIiIhoSzAATERERERERERERERERES0JRgAJiIiIiIiIiIiIiIiIiLaEooA8F/iJzf+GH984wa+/5fxdURERERERERERERERGvAsZDXNGjhvzwsR72+YsuXa5qGfGTHlOzKfPsBcKz8OD8JpNs5FvJ5C46/Pl4O2TIpIR2Z6LEdWHk/zXAfG5XwOBV4mwrbTWSciM6CNAD8l9//Z/jX/+Bb+Na1PwD+9PtgDJiIiIiIiIiIiIiIiNZSuQfXdf1/dQyNIBBpo2IMUQ/X9YCCECCO7DdCqbMXDR6nYbZwXNXjS5fGrmgwav3YUgfWXg3BUr16HJajVy6jXtWlyyZF04mLH9ux9jCse2mOSh0c2IBjNYCev6w5QMNyAPsAndLIOzYKk8FrIjp10gDwp7+YB/719/GT7/8pfvGZL+LT8Q2IiIiIiIiIiIiIiIjWjon95gBdG4DdxaC5D1NY13KPIY2FqtgV5PN5r3drpNewH0gOewDLesIKyyQ9Zvc6sWNNsIGii1EzF1nqWHvolJooR5Z6eWlkxPIqlvmU6QDSY4+GWaDr5d3olLBvesHnlp+4vpNFdkeHcwKUdr1KNotlDE5mjaoT0aKkAeC//MkvgM98EZ/+4j8AfvET9gAmIiIiIiIiIiIiIqKNoO9kMThx4JwMkN1JiPa2C8IwyQY6pUNpcLifrcN1WzCxi0O/V+2oCQxH423EnrCuuw/DiS2rD7FnOZFl9ayq723AhBmP3DoW9jolHFZ3YisAu4uJnr6yZUByOh7JsdEGitHyjNmoNDLYN4HRcCAsJ6JVkAeAfwH8g9//ND796S/iH+AYP2EEmIiIiIiIiIiIiIiINkAQ+A0CwRG27ffOFYaAHjWRg2qYZCCXMbz/0YEjf27b+LDMerUOFIJg8h6OAIyGfbSDZYU2+sMRRkMgSM7IeL1r7Uq8l7Cac9RBv1+DoRXQ7tfGQVjHQgPFaE/f2DLxOLYknen5KKM4ERSG36u5i+JxFToAI5ONb0BEZ0waAP7iH3wG//qPb+D737+BDkr4fY4BTUREREREREREREREa8/GQS3rBSrNIrI1cV5fB1aj4A0PLdKrOO4BhSmT1dqVPeAwmFc3vtZEK5hPuJdF58iBkcmhHPYKduG2TBiZcc/h0dALIpstf70fQE0yntu3h3KuicMgaC1GlgOxZeJxTEk60/JhZPyhtX3ZHR1wLOS1LopuKww06ztA58gf8LrbTu6FTUSnQhoAxqd/H9e+dQ2///vX8K1rX4yvJSIiIiIiIiIiIiIiWg+RoZwbyIyCYKSJ1qiEjjEe5nlYd8M5ayPMFnoo+PP5ypnFLGp+Wl1E57Z1rPw4DwVv2OVor2ANecuJLGsMonP7LkI23LVs2SL06iEyDb88/nDP9kENfbRREMoIcx+ljgFN01BAT17fRHSqtPv377vxhWm8+eabuHz5cnzxxtE0Da47VxVshW0pv6Zp+PijYXzxxjl3PsNyEMA6nMD6mM+585mteMZvo235/F0W1sd24/mlVduWa3BbykHrbVuus20pB20vTdNw46fF+OKNc+3zXd5rtDJ81hORzCY8G+7du4dPfOLXAACf/ORvxlcv7P79XwEAtF/96lfu3/7t3+I//sf/ONO/f/tv/y2eeeaZeLpERERERERERERERERERBRz9+7dswkAswfw+rcGOE3bUn72AF4v21KOVWIdRrE+5sMewOtrWz5/l4X1sd14fmnVtuUa3JZy0HrblutsW8pB24s9gIkWx2c9EclswrPhrHoAy+cAJiIiIiIiIiIiIiIiIiKijcMAMBERERERERERERERERHRlmAAmIiIiIiIiIiIiIiIiIhoSzAATERERERERERERERERES0JRgAJiIiIiIiIiIiIiIiIiLaEgwAExERERERERERERERERFtCQaAiYiIiIiIiIiIiIhoozntf4LK2/GlHnv/K9Ae9v/t/1l89ezebiPf/uv40tl88Ndw4stUUm6rrIMP/mfkH/7K4nmOe7sN7eE27HDBX8N68itCHv4a1v7/nCrv0nP0dnu87OGvRI/llylYt3DZUtbxxjmtcsnSFe8LyXrZ9Wnv/xNYH0SX0XIwAExERERERERERERERBvL3v8KjBd/EV/sebuNAv47uB98D+4H30MP/4+JINTZ+zNUrv2b+EKFWbaVc978CbKvfg/H5b8TX7UEH+EkCOB98G/QGQirPvg3GBp/H7qwSCrhHOVeeDFc7r4KNNp/7dXJ//knKP2//OUfvIjSG/98gUDi4nW8nk6rXNPSnbZ+zDwoYvjPl9AogyYwAExERERERERERERERBvqz4BL38Pohc/EV3j+3m8h9+d/FfZGNA++h9YT0d6KYc/Et9vI77f9nqV+b1PZMp+9H+t5+nZb0sP4z1CJ9WB12l20B38KY//PYj1Z/d6Qb7eRf/KfQHu4DUvcVkzryaBn7XjZ3huxQ8PrKbv34i/Q/upk2rbfYzeSXry8YS/caNkDucvnMXzTr8c3/wrZy+Pz4Lz5V8j8X/6OtA4iVOdI5e1/g8EL/y2qDwcL/g6qb/xT4W+fqm5j5z1yPmR1EiGsD8si2WdaPcbXJ6QT9HIebye5DiTbRcs15RxI8/NnqIR18NewnpSlO0l1XOn1id9BEd0FgvekwgAwERERERERERERERFtqN+BmRQsfPi/xnHtr2DEA2YK/T//LRxGepvKlwGAefDfIfvi6+PgXfMjNP/b3wnXww+G4dWgp+pTMD4A9HIR5ewfYHTwOwD+vpf2B9/D6AVg+Bfefv1HinA/KKMqbBtJq/ZX2Gv/dWRZ/RFJL+iH/2scvvAZlF8dB0iDtI32P0fnSa+H7ejJn2AvVt7RCx+hcPvv+3n7CF1Zz2nj7yMz+jdw8Nc4Gv0Wikawwvt792F5HUQknKP+iy+MA5tfBerlvwPn5x8h+1m/N7MQ+JwcBlpet3Hi+XAUdRJ6+/VwvfsqUNj/M+U+0+oxfl2p0sFlr3d0sK/sOpBtFy3XlHMgyQ/wOyg+8hMcfeD37n7k78OM1ZeM6rjS6xP/f/b+L9aN684XfL8FyHm5ZxADd4DJdXZyrLhqwyE4A7djGNcsCw1HCUbFHdlsROZ5EHwIHzisdoCInPQhDAWEIQT7RmjsnjRLAZyQNlrYR9DDYRKEsbxZGihqoyGTvjBsJw9strGrHEmOovEAM4CMOffN3bwP9W9Vsar4Z3P/o74fYMPmqqpVa60q/hF//K0FKErytaH5MQBMRERERERERERERETL63jZDXwlBPUEuZPulMVfewiw7iaWOR5H4dS7TkDv5vtoP1oYy0KVywXgJS/z8jVshTcDR4EtN+tTnMY6pzwU2g0ALOtPaHl1vfQu+tZdWBaQ+ZqzXVESsqAjvLotCyh+2wmkyt9+cqy/8iMrse0IewireA9bN+8CyhPw47/C9M8TxwDJ1yg0BfTNshOAfGQFg4/da+gd98ZT4fqQPLZpksbEEwo+Hy9jtPF44jGTxjF6XyXWEzk27j6I2080zTWItgcAtBMraF/71JlG/ER8wDfNNPendz39daAn/EiDpsMAMBERERERERERERERLSW79WrMtMxhlhUEB71gGv54F3ADanFlHu3738Xg6ocwX3sPxUj2r+NxNL0A5htOME1k1l4DLjjbu6dCm8YoyldQ9rM4L2K08Xgoe1LsxzQUBX577GvvjfVtWtqJFQxfex9DLzAamv4ZE8dgmmsUcvwJZM+H1/w1r74r7uGUTRjbuPGaNCah4PPNt6CefAuYcEyS6H016dyeuPtgsvRrgJj2AO5YX3kTG1dWUEjLtE8wzf3pBdW1Dbd9V74zed1omogBYCIiIiIiIiIiIiIiWiLB2qVy+cfo4mf+NMHKlSexWf6SG0R0phde/yjITMx91AlNN5xU5jv6HdTRwTqexFp0DVovuBmZwhh4CBk4a6RqJ1ZQ/aazvYOnguCiL9g3nMXpTHkslon9mIZc/j6KV5wx8MdlHsefAH4FIUAYTP+MxDEIJF6jRI+jebOAoTtu0tEXsa6cRy9yTOzYxl53cYwnjMnxMuqWOy31N99D8cJ3oE06JkH0vpp4blfcfRAv6Neka4CY9jgeR+HRd9Fyp392BPXGi79ng/EW1xYOZwnT4kj37t0bRQunce3aNZw6FfOTiUNGkiSMRnMNwY7Zhgql2ncelLsYNYOnz17Zz/4vkiRJ+PzOMFp86BxZybAfBHAMx3A85nNkJbMUr/HLaFnefxeF47HceH1pvy3LPbgs/aCDbVnus2XpBy0vSZJw4Q+FaPGhc+axDp9rtG927bX+egvqx8+GA4lxZSGfwjh5FsPqRTTnyJCk+9TE+2qP7Vt7PoReA5pTZTFPtmuvDQt0+/ZtPPDAFwAADz74xejmHbt37zOAGcD7yDZQqmbRHY0wGnVRbq3D4KTmRERERERERERERESHw/UWpKNnUX30Bwz+Es3BrHWQiZ06nXaKAeB9Ym+1gUbNTZnXUGsA7S1GgImIiIiIiIiIFsLUoZviQ32GH9/bMHTDn5pw50zoqgrdnLfGcHtsY0JfTB1qqP0mdFWHNxy2aSCxKaYOVVXdP+c8E8/niu4XfTwmdC4VeurOHhv2NLvtgon9IaLD73h5PAMyrsxzvDzDGqxEgrT7aj/sU3u0jR+jEjN1Ou0cA8BERERERERERHQfGAj/b8OORBGDR/ZY4De8byQAaU94DABmByhuoqnJ48fHGDuf8AgA5EoTFTl4HO0LAGAwhJ9rYHZCvbe2AUVOaCuAbL2HXq+HXq8GlHRYqecbH0s4VU/XzuKme64emv7OkTrFdpob2LD8DWPtH2+b8BDCdU7oe+wx0QIiIiKiA44BYCIiIiIiIiIiWkqDbROm6fxtexFQU4eqW7CsLai6AdNQoeo6tkzbyRrWLVjGBtoDwDJUqLoBy9pwMmpNHaq+BcvSoesmbEOHblmwNpzs1ehjhw17e4ABrNDxzrm9jFInw9dpS/h8Yns8XiaqHd0/2AXZYgZDNwJsdjIoZr0tJraxBsS2NcrCEBkg6XyRsXTisjZMXcfWlO0ELNi2EPAduz6RMd4eYLBtx1yLuLZFtzvXOf46eecWr0+4Ti/uHGSTm9DFNHMiIiKiA4IBYCIiIiIiIiIiWkrZVQWK4vytegFQrYbNAoDtoZsUnEWx1kRFk2F2gEJTg1apuQHTLIq1CjSthiKArc4A2cwqgAIyg3VsDIFBZxvbhU3U3OzV6GNAhryaRXZVg9UB6s0KNK2JOtroDN1dfNHzRdsTFd4/ZHUNmeEWbJjoZNaw6pWb28BqUlsdg3Uduq5D17dR2KxA8bdEzjc2lkC7VEKnEM78HTtONNyGZVmwLMsJDMfUKbbTGUsZ1ti1iI5d3HbnOkfr9Jhj1ye+3VrNDa6bHaDgLPBGRPvpUxgnX4R09EVItQ9TykTJ2+3Wq9Cvh4pcH0I/6h5ztOVOqy/Uc/RVGDejx3jrBIvHTOnmp2MzQCxabF+vtyJtdfoY7PcpjNpbk9vm9zsyZtdbUFufRvdOFrd/XFmcm29BDbXhxemOE+3BdSDaDQwA7xN5rQhUN9wXURMbVaC4Fv6wTUREREREREREOyFDlp0/j6mXsAUFSmJQNU0WmTUnoLxWr6NWq2GzuYY1bKCkm5DXwo/3l4y1zBBbRgcZ4TsnextY1ZDa1my9iWaziWazAjdeGmsrZiyL9U1k1oP1hifKrEHTNGiaBjnm+iiJ7Qxfi0JG2DRhe1rfpyI7wXWD8V+ig+H6m2ifPI/RzYvo4mdOoDJU1hkPzMYdA8CsvQjl/J8iOzvsVgd44yJGNy/COnsH661PAdzF8NEfOOsA34xfy9S8egeNf3SO6USDrYk+hH7m/WjhHrqDbW/Mbr4fmoUCN9/HUHkCKW8PvtxZZ4xHNy9i9AacMVvEWrOz1HHKuz7O39THAQfgOhDNjwHg/SJXUC+3kJckSFIeg8Zm5JeRRERERERERES0aEomi+G2hS19A+3BENvCNq2WQUfVYUSmXPas1TIYljawtbWBUgfA1gZK+pabbarAjjyO8uvXVayjjmYBaJd06Hry+dLaM4m8lkG7nUEQ/7WxhVVowMS2TmM1biwVGZXNDNbnCazGXJ+tmHYO1g2gEL4W0R5Er5W4Panv0etTGwsqe2SsZdpoZ2pg/Jdo/9kfA8VvO0E97cRTGHwsBhk/xfZHK1iNBGZjj8GHwImLsM5+JbyzSy7/GM3j7v8/soLsI18Cbt7F4Fc/c7JLT8ZnxSoKMPzjp9i6soKCe3zYeGax3eqgNfg1lNqH4Sxj7xzXW1BrLTe7VcisjZaJdfvtC8pKV0IN8eVOrWB4zcmUta/dRfZUMCb2tbvIfPtLse2eipe9G8oQdo8PZexGM6qdcfCOTaxjGrHnGe9P+DrEjGXs+eP3U0++OlsbiXZIunfv3ihaOI1r167h1KlT0eJDR5IkjEZzDcFSWJb+S5KEz++MzZt06BxZybAfBHAMx3A85nNkJbMUr/HLaFnefxeF47HceH1pvy3LPbgs/aCDbVnus2XpBx1stqFjay061fV0JEnChT8UosWHzpnHOnyu0b4RX+vN2qvY/r6bfXu9BfXjZ93g74fQj/4MrVM/wGjj8dDxycc40yJvPBIEe8d9CP3kXdSufAeyeOzNt6BfewLNSIap3XoVynmg8Y/xGcLh830K++aXIB8NzoHWqyjh++iVvwTb+/9H3oTUeAiW2IaYsk28FtQdU2bWXkTnxMVwX6+3oH78BIrWXaxtPIGt2vtYVd5D55Efo3n8Uxi197G24bRrvN3heqSX3hUKnkL3Zhma2N6rT2C08XgwBl/7FPbRL0EWxwUtqB8/hOz595DxxjCtDrEvN9+C+s1fox9tw83x89Q+jutP+DpExzLu/KF6Yvaj3XUYPgfevn0bDzzwBQDAgw9+Mbp5x+7d+wxgBjARERERERERERHR9GzTwAZqcwV/iWjxFGUlWuR6HM2bFzE68f7Yuq/Jx0zyIfSj76Nw5TvOFMjiVMR/vOstXe7zArajf3wS7TNvwYxZc1cuF4CXvCzS17AV3gzLCrKV5W8/CVh3AQC5k+40zF97KLHMsv6Ellf3S++ib92FZQGZrzl1K0p8tjPwEFbxHrZu3gWUJ4JZFITpnye1G9EpoG+Wx2ZNyCkPhQuOAltutrM4FXf//K/RCu0YGKsjKjQFtNuGmPNM6k/cWCLm/NPuR7TbGAAmIiIiIiIiIiIimpKsVdBk9JfowJAfAdrudMXm1XeRfcTJlI0GWkVxx0x08y2oR99HQQhkRs+TWM/R76BXvYv8lSdRG8ssdgPVNy9i9MaK3y6PogRtta+9B7iBRC+wiD/eTSxTlK+g7K5bPLp5EaONx90pqZ3dLCt+vWMA0E6sYPja+xgKfQqmf8bEds/DrL0GXHDq7AoT0DqB5AKGZ+Kn2Z5V/HnS+xM3lnGm3Y9otzEATERERERERERERETzu96KrG3prNUpBsbCgbKYNU0jzJqXifcipNqH0c3xvHVBZ/YpjJPCeqM334Iqrj968y2oCe2MNXc7XDffghrps1mLroc6WTQ4uStuvgU1sq5pqK2htVbd9VsX7fizKF45C+noi8jjB2geB+Ty95FpuOdtPIRNb0po7zrGHBMvOMZ87dfo413khb6EznP1ibF65HIB2fPOeaSXgG71rruebMBuvRrc6y8B9fKXADyEDJy1Z+Xy9/22KleedPsC5D7qRI4ZLwtntXptDsrWP0rKAAZw/AngVxDWLf4UW9ZDWHOneY5v985oJ1ZQ/aZTZwfe2syex9GMGb95xJ0nvj/idRgfyziT9xPuQ6JdxDWAD8F84LtpWfrPNYAPlmXpx37iGIZxPObDNYAPrmV5/10Ujsdy4/Wl/bYs9+Cy9IMOtmW5z5alH7S8lnIN4OstSC/dCdY4ddfdzL7hrC1q1l5E/ldA2X0srtUZu27n9VZovczYdUoXbKxN1goGiru2a2SN2Ilm3T/q5ltQX3sIPSFzMLRm7ZRix3bRvDVWhXV2g7Z+CP1oJ1i3FZ/COPkacGG2fsS571/r4+6xuDKi+8xheG3gGsBERERERERERES7zoapq1BVFapuhLLYpmUbOoyZUnls2BP3n7SPDUM3hAwiE7qqQjdTD5rM1KGO1av742KbBpJPETOWpu48VlWoqjBOtgHdLdd1c8ZMqEljQ/shd2oFQ3+a2rvInvIyCz8ETlyEdTbINLSsFeCqkx2nxE2J+7WHkPvorn9faBtu8Pd6C2qt5WaUulmn11tQT77qPPYyb6+3gkw+Pzv1Q+hHX4R09FXotfHMWPnbT2Jw1ckstKwVFDaeQPbK+07m59U7zhqsoWxWL8vVq1c8FwDrzXA7xf287D+x7d5xk8S1IVRPcJ7SFfeY1PEQs7Dj+hJXFnHqB+jiZ2NjiuvvY3D2+0Kw90uoXNl58JeIiCZjAJiIiIiIiIiIiJaTHQ0URh8DMDfQKfTQ6/XQqwHremx4AwBgRw6OPk4ltsXcwIblbxirx47dJ7zH2JnNDlDcRFNz1qYNtkePFdptx9QDAIMhtvy2djAQNlnbgCLHjW3yWGbrblmvBpR0mLYBdWMVtZ5T3ix0UBqLoI+Piy91bGjfKE8gY70P250mtqB4Gx6HFg3w4l3ghLs+ZvUuStEpUt31UpWxACXQ/+ghbN68iNEbwLp7XP/RAkbCuqyAE5Qc3bwI6+wddK4DdqsDvHERo5vfR+ajmHVPjz6E7Ed3YeNDdD56CAoeQgZ3YeFTbH+0gtWjAPCEc+6bF2GdddZRDeq9iNHNZ6G4Ux977Rw/f7jPsW0HgF/9TAjaOhnUjvE2QKhHEc5Tf1ToZ+J4BO2J60tcWRxt4wfAS+EAsf3xnWBNXCEIPT4lLs3seHk80zeujIjuWwwA7wNTlyBJzp869uGWiGh25isZHHvjk1CZ/cZpHHnlRqhs3A28vHIu/tebCfVG2W+cnrjP/vgEF57L4MiK8DdxPBZvmjEkIqIkJnRJgqSKWUgAYMNQJUhSkI0EOBlGkqRGMrBsGGq0zITu12lCj9bjndf/ix4viD1nXLtjzjPXsV7fhb/YQEXMfn6904xJXP+jdYp1xLVbPGbavkevBe2vtGs+i/C1NfX5/y28k2N3H+/hg8Y2dOiWBWtDhW7YbmbrFiwrkuGqZDBY12GYJmy5gl5TEzJ6nSxb03AyWi1ry8lsjTz2YpGm7h1nQhden6NtsbcHGGzbsE0dqm5F6tWxZUb3cdqt6yZg6tB1C5axgbYfmXX3hxWqI9pnv91bG042rmVhQ8ju9WSLGQzdCLDZyaCY9baY2MYaEB1bT8xYhlkYIgNstZEtaHBC1QC0JnoV/5HbbnFcItcjZmzCWcu0Px7CKt7D1s27gPIE/PhvrKeEdUUTHC+7QceLsE6+5wdMcyefcO6drz0EWHedMuWh8LExZZYFZL4GAF/C2sm4dU8fR+HRu7Cuv4/ByScg40tYO3kHndb7aD/6hBOgPQpsuWsXK+ed4Gp4vc/XsOXW5rfTZVl/Qsvb76V30U9pOxAEbL2/rrcaY0wbINQT9BNQlKCf0fPEtSeuL3Fl8R5H8w0gL6zPKj+yEqzh6l3PN54KDiEiol3DAPBesw10MhZGoxFGVgOobox9yCYimpV2ooh3r/yT8I/dT9C98nt878Sx0H6z0v52iBsvfTVafIj8BX76zhCf3xni8ztX8dOP9D0PAh/+MSQi2m855NAOspAAwN5CGznkhCIAMDstlMtZVDcW8Qm7jO5o5HxuH/UgfictSj5nDjlUMVYsmP/YHBqW1zYLjUE+Jggso9Jz9rEaOeQa7r9BepXQF5HJkvovnLubRbUkftm+X9eKdlfaNZ+P1hyFAz2Jxn+sMP2xRI5BZxvbhU3UKjLMDlBvVqBpTdTF1yu5gl6viTVsY0tXoY69pgJAFsVaBZpWQR1tdIbRx85eWs0NnJodoBAOfoptkVezyK7KkLUaNgsAtodw0myzKNaaqGjBPlZngGxmFUABmcE61HWg0NSgVWpCYNbbX4Mi1BHts9/uSgHZbAEVTUOtCGxHn9ira8gMt2DDRCezhlWv3NwGVp3noNgfX8JYDtZ16LoOXd9GYbMCBVlk3OigM2V05AdNY+MSpvhjk3BNad9oJ1YwfO19DL2szwSK4mShevwsUZfdehWSEEgUeYFT/PEukBQ8jaEoQbasZcVkALvtWm8EWavyIysYXHnPP49Zew24EAnI4nE0vUDtGytou9NgRynKV1D2M2kv+uvlziq+DYFp+onE9sT1Ja4swfEyuvhZkK18/Alkz7/mTpXtMK++GzwgIqJdwwDwXpMraIofjHOZCb+GIyKawjPH8b0PrqJ7yyu4jX/5oIhnn3Ef3rqEY0ImbDQj1XrjtL/t5beD8mh2ry3slxhInXCu/fNVnPltE9+7/AtcuOW285VLTpbwc5ecLzIjbQ/G4gZefu4STKH/Qb/StkXH0Nn3witx5xjPWBavBRHR/SuLYhFoC9/o2lttZOt1+N95AwBMdFplFJoFlFudPfqRZdo5s6jXy2itJwXLdnKsSEal10W5tT5nZuYOaAWU+0M/6+1gXytaiNA1T8oUd5m6kKXeETYAtqEKWbxJ9dgwVAXVfh9VJQgMhY91fmStCsf78SPbgKobTgZzJDPd1IX9TF3YLgack9oV1BFsC2dPbhvqeHsw3la/HyltpZ2R12rYbK5hDRsoxQZ1HV62r6xVUGluojjopGS4AUAWmUzCY9kJnBqR+G9SW0y9hC0oUELB3KgsMmsKFEXBWr2est8iyVjLDLFldJBZC77HsreBVS25P3FjaQLI1ptoNptoNivQZEBeDd4vtGYPvV4XZb+WaceFDqTjTwC/wsTsXrn8fWQablZp46GxNYDl8o/RRTAFsnLlSWy6U9vmPuq4WatAfYbpbsVM1vWP4jKAnXWAMVgJ2n/8CWQHcNb/dQPc1W86dXTwFAYff+oEq72pmlPaFM6knX8a5Lg2iKbpJxLaE9eXuLI02sYPhOfz42jeLGDotlc6+iLWlfO7ME3xFOsUi0LrKL8YrF3srSE9j50cK5pUz81PZ/6sYLfG17yOK4sTu9+kNh4mO+nLTo5N4I+3WPe013wn7Znn2HmOESX1y58ufornMqViAHgf+P9QVIaoT/0LfCKiNMfw7Onf45e/cwONb1/H66ePu+vH3MDLT3+MH90JMmGfv3LWCYICANr4Jc472945i0HDDYZG3bqEF88puOLV87dx2cWTzrXfnHH6F++Xp5evAsYQn//2Bci4gZefvorn/YzhJvDC6aDtH5zHT7xxutNE9pzQr7RtUR+cxy+Vq+Pj/fY/4IePNp3yS0XgdBM/9wL4RET3udW1ItDe8gM0W+1sNKkKMDtolQvQoKFQbqET+peiG0DyAy95tMTNsVrIe/snBWRSz+lMZ9nNJmTy7uTYMRoK5T6GQSR2CpPGZMr+R37QuvNrRQda6JpraPpZ4iOMrCLafnawCT0/8DOHrcwg5TmXVI+MSs9CI+dmII9NIwvnPEobRT8jvgvkhUBtqw1sjme+a4UyWu6NZ29DyFy3MEQRTqwrqV1O0DiPbrBt1BTWbWyhjU33mAYG/g85TOjKEHX/GAvFdmliW2ln7K0NlPQtbHUGyGYUaLUMOqoOQ1exjro/u4FcKWBYUp0MVbWEYbGGyirQLunQdW+a5QHaJR2GrmM9U8Da2GOPjLVMG+1MLbSeZ7QtADBYN7CNLIbbFrb0DbQHQ2wLx3j7oJDBsLSBra0NlDpAxetHaAroeNE+10KB63TyWgbtdsZ9TsB5XccqtIT+IGEs45690JrYhDMNta7rUNV1CAvGQsmExwVj1yMYm7hrSvvAX3v0cTTd9Wzl8o/RFAK74cdfQuWKm1V65Tuxr33ahpCdKu5z8vtuubturrjuqff/Qpl3XnEt29DauKKj30EvtB7v42je/DEqR92HwrTUzQ3nHHL5x0E7Y9oU9FvIpL15caydIUe/g14kQ1jbcNsR04ZwPcF5elfcc0/Znri+xJWFjLU1MmYx51k08dpaZ+/4a0PH+xD6N++i7rfpB8BLr4aylPdV0j0BOG0/8360cO+ltpEWwh/jA3LNFy65X+bVO2j8Y7BeOc2PAeB9oDW9f0BmsO7+ithO+oUwEdGUxGmgzavtYPrnW7cwQBsn/czSE/jhB0IQFEX8yJui+OGHkf3gYyGTJ2D/7ipw7j+Nf9AXTTzXAfONE8g/7P7/29fx+um/xhnvcTRYLI7TTNuiphtvIiISyBXUvWCouYFqtjD2fmR2Wii7kUYxuOMQp0x2gkRillE8YQrkhIBM+jkdWk0MAAV2cuxiTBqTpP4LgeNOYXxsdnyt6OBJueZilq9SRd8v76BVFoNr9fTnXFI9k0TOM/ZjiJwXzI3QvOxzG1ttoF7POseYHbSyq5P7pxVQbuXHsoIdZdT9jq8i62VM29sYiD+skJzs5oltpR2RK030mhVUmj1nNja5gmaviUqzF1mbVkOz13MyVHvuvloTvZ6TtdrrOVMWFzebqDSb6FU0Z9YD4bFcaQr3YhbFyAUda4vm1FtpNtGsaE49vSYqYj3uPprmtrvSdNrt9aPibA+eAk04m4U6In0OtmloumMQbntQjzOds1O/1mxCg4xKJTgm1J/g4NixjPsNh1wRx7iHphbUI1fC46JFroccHZuxa0o0Tsx4zX/03bGsYzq8xB8XyI+sjE0pHnL9fQzOPpsc5LfedLODvexDIbv45FvuZ/NPYbjrMI9nKTrbxjIjr7eg1lqRuoV6vLq9rEo/CzLY32510Br8Gkp0evRQRrMXzA7aXbri7ZheFvQvbj9BShvH9ov2+XoL6slX3ccx/Y8d2/Q2xu4X157YunfxmsddFyFrNsiujhlvd7/Ea57Unt3qS9LYTnW+8bLkfnnT2H+KrSvCbAw0FwaA95NcQd39x6lc6flfvvDzKhHNxZ8G+gbevCxM/wwA3ziLj/ysXOdv17JL9/JcM7uBNy//Bb7u/wr1ADn6CJ66rDuB8xcs/PTluAxrIqL7lxcoFIOHAROdFtDKu4GVfAvY9amFpzynGxAtGWJO106OjWOi08r5aynuLi9w7Kw9HPfj1YN3rWhnEq65bUDNI/ihgNUYW+t5KouqZyYKMrkBtm0Lw2wBmpLBIHrPprbLyw7eBErS2BTQiXINWP6PLvjv/0NnNROsgxv32GWbBjZQYyYq0W7ZUeahkImakHVMh92H0GOmFBfZHwdrPMfpf/QQNt1M4s71cHbxqHoXpdanwPU30T553il7A8j7Qaz3oR911miOu0+9ukdvAOutT2G3XvPrsU6+59QtOvUDP6u5c935EUM5+11YY+tHP+HUe/MirLPOGtBxGe+Tyrz+xe2XKNLGqGifAaD/aAGjm2Uocf2PGdtJbRzdfBbKzUhf3LKQmLrFNi7+mo9flzhp4514zRPas1t9SRrbac4XV5bYL1frpdeACzEzDtBMGADea6YufEmyl1/UENHyczNPfy5O/+xlmYrrA89H/tYJ4Nw/pH+5taBz7RbzFT2S5St45niwPjCcKa9/Egqkt/ETby3fmbZNx/7dVWQveUHzy/FtJCK6n7kZd/lWOWFKYXE6VguN3C5PLTzDObVaA6hWgylwd3JsDFPPR7Ig94KMStI6xQftWtGCxFxzYQpwe6sdZMgqGeSEwL5trKfew4n1TKIVwutf2wbW4+67MTLWikC7tI5BRnEydQcddAaRYye2S0alN0J3mqnM5VVk+95U03QYyZqzdm3SY7E8nBFLRER740PoR99HYUJwX35kZWzdZFz/0P/ckjv5ROh4y/oTWt5ayS+9i751NxxEPl7GyA1i9c//OvUzj1/31x4CrLuwrGB9afnbTwLW3fD+ykOhx4mOAltuRqdy3gkgWhaQ+ZqzWVGctaDjy8b7F7dfkkltjPYZwjFx/Y8b27g2htewfg1bbrA0WiaKqxu7ec1jrkucWcbbk9Se3epL0thOc764siR261WU8H2M/vFJtM+8BTNuDWqaGgPAe00rAN6v3aU80O3t8Rc1RLTMtBNFvH5ZmP4ZAHAMP3/nBH75tDctcwZHVs6lB3LjPPwCfnRamN75lRvRPRZ3roX5PX4otOUkmglrF8Np+yUl2P/pq3j+nXPCL82KyFon3G3nkb007bbpyI8oeP0FYdyeS1iLmYjovqWhUAZyjfG1BMczTWWsFXMzTC0sTsvqZfKJZePLtMx0TrmCzUaQO7iTYx3h9Xvz6Casj7oT6f0HAGg1NPy1U0MbdnCt4q4FHRjiNZcr2Cy2objXSxlmg2me5Qo2GwP/WpZQx9ht7Emrxw3UVhUJUvxNiGY3GzwflDaKlrgebzJ5rQj0+8iuys49m22hJU5ZntIucQkn7zk4+SmooWkV0Q6tvc17nIiIaCFuvgX16PsoxK1RHHX8CWTPvyas+fspjMbPYrNX4Qbkyn7m40WMNh4PB5FvvgXVndY2d/Y8RjcLGJ7xpr4N8wNff7wLKA9BUYD2NXc64GvvAROCqUnMmpO1Obp5Ed1TTpkzja7z/5blBB/jy8b7F7ffvKJ9FsX1P25sEdPGUEb/GytuPXFlgbi6465T3JgkHZt2zeOuiyjtukyS1J6oRfVl0th64s4XVzbR0e+gV72L/JUnUzP6KZ107969UbRwGteuXcOpUzF37Q7ZhgqlGv5dba5hobdLUVJJkjAazTUES2E3+2/qEvLuT0Z28xrC7cfnd4bRYgA38PJzt/A3v30h9ZdfB8WRlUxCP9KZr2Rw8rLz/0+du4ob7vqi9hun8ei53zsbTgeBr/j9b+DlFR2vO8XONL5zjttc/Xj7nDPt7Tu7mfl4Ay+vXMezd8LBOfOVDH6iBOO2OJ/gwnMn8EPMPpZzjeES2//xiL93Jm+bnvlKBm+e8KbL/gQXnjsLGDt7PhxZyQiv8TYMVUHwFptDw5rnR0gmdKmDwsj5ctXUJaxndvc1fhnt5vvvJHv9WWsa+zketPt4fWm/Lcs9uCz9oINtWe6zZekHLS9JknDhD4Vo8cL8n5dv4Mcb/5f/+GjtW/hfTv+70D6LcOaxTvi5dvMtqN/8tTtjwlfQ+Ed3XdXrLagfPzs2pehesVuvYuORYI1Yx6cwTp5FdeBOYbvxeLjMb3/cfoKbb0F97SH0hHKz9iq2v/994MxrwAVhbdmbb0E9A2xGM1Rvfgr76Jem+N4ori1CWfa7sK58B3LsfoJFtPkAEF/rzdqLyP8q2JY7ex698l3oJ++iFtf20L0KlN+46Nwfwr0a3DcfQj/6Mz8z0qn7S8I53Xvlj8J9fr0F6eoT4bG/3oLauIP+4E8AnkL3Zhla3PXz2vDImzFtcfd/NHJdr7cgvfQuAKB86ikMlGed/rvtzmW/gmw13Je4MohjN7ZfcDp/nGLbGNkv2ufQ60FM/0PX03sejrdxE68JWbVO3Urr1bGy6Hd1Y3UL1203rvnc1wVe3Yi/5nvcFztubKd+vgR9DsqS+iUe/xS6bwD56LhOsLefA03oUh6tXANWr+K+1oS/O41z+/ZtPPDAFwAADz74xejmHbt37zPgIAaAw2wYagnYnOcL6uns7c1w8Oxa/20D+taaM+2RbUBVhqin3PA7dV8HgG9dwsu/+0v8/KWvArcu4djTH+NHd85BE/8fN/Dyyi/w9Xcu4wwS9l/gWM3TD/OVDN5EEa/jeEqG5k4tJlA3HXfML53ALxvAxRnHdZ4xXGb7Px5p907athncuoRjT5+H87Ew/KONeY0HgIX3VFOHtJ4RPpxMa/KHmHi7/55+mOza++/MDsZ1OTjjQbuB15f227Lcg8vSDzrYluU+O5j9sGHbMuS5P3OFj7cNHVtrTVTkaL02DH0La033c75pwFAqKZ/1bJjGBtbbQH2zCU0GTEPHehso1puo+B/6x/cDAFM3gGZF+LeBDUMvoY0sioUmKpoNQ9/AEAAyBdQqmv/vD9vQUWoPkK1vohk3n7Yv2sedio6RDrWTwab3GCZ0tYNCz/k3j20asJT4Kb/ntZsB4OF6B7/Y/h/x6n95BP89AOC/4Z/+4++B/88x/OV0M4tOLRQAvvkW1G/eRd0PuHwI/WgHmWhgYR8kBqbcNjnBTzfIVAOa0aCdv9+L6JxwA4WexGDqj7F2zZnK1Ot3bDvwYXKQMiquzXEBHz9wtFttPhgO5mt9in3+IcS+uB/7TPtub18bTOjSOga5PrL1kTsr0OTvTvcqAHywp4C2t9BGEWsT3/3owJEja94Iayftnxt42Z+SNoMjK6eDtT5xAy8/dwkXXgm2v/y2eJw4ha34OKXOW5dw7JVLuPCcM5XrhVfEOj/BhefE8+/Awy84wVy466/CgnXLWU8U5/6T+yJzDH9zDvjl7z5J3H9/3cCbl4t49m+P43uXr4emQTOFayJOJRxXbs45xvYbp3HMW7819V5wr6twzYPjoo7h53cu44z3i0k65I7h54kB3rRtM3j4Bdy4460BPNxx8HcirYByfwgLcD+YiNMRqsFaenCDxd42vSNscLJJVX/npHq87GN3ylJvCkfbgCrs78/saBtQdQOGKkFSY9aWpMXhZy0iIiJaejbs0AfK6GPA9gpse+yzp7/NeZR8rPMoebu5gQ3nw7dznuiJXOH6BOLxieXj7Ye2Bmwkf6a2jQ10Vpvo9WrY3jBgGrr/GNvBcdH9bNgwdBXrg/APdW2jBNR66DVrwLoO097CMFNDs9lEUwj+AiY22hls9jaR6WyNt08co2gfk8Y49nF0/5gxAoDBMFjSwOxgIGyytgFFTr9uB8afPsb/9quH8dd+8BcA/h3+8r8sPvgbZV97D9k3xGy7x9EUpwm98pq7dmTL/W7nQ+hHvfUkY8q86Uyvt6CefNXd50Po/jSnn8I4mXKcUFa64jQh5HjZDUp9iu2PVrB6FMDNuxj86meheuyPgzVKtRNPja8dm0IuF5C98r7f3q0rKyhEAql2q4PW4NdQah+6fYr2QxDX5hi73WYiIhJlUa+X0VpP+LyV9P3nHjjQAWBzo4psfdbMJDooTN29qZUh6jNnmO2GY/i5GFx55wR+WRHW2PzgPH6pXHW3ncWgMc36mxPqvHwVMIb4/Lcv4MyJIl6/6q6Zeuuf8EucQH4HU7vGunULg2/MUG90/w/O49GJgc1d8PZ1vH76ODQcw7On23jTC7i+fc5Zs9UfYzfIllCuLWqME++FG3j56Y/xI/+8V/H8lbNTBZmJDhyzg5b/4xwNzdEII+/PKqJd8j60mNDzAzQsZ5uVGfhTtoxLqkdGpWehkcs59TQ1p16ljaJb72jUBfJC4LnVBjZHGB2I94/lxc9aREREtNRMHaq+BcvSoetm6LGqGzANFapuwNragKrqMCwLG6qzNrPtbbO2oOoG7KRjrY2x7bpuCsc7283tAQbbNkxDh25ZsDZU6MKvLqPnM3RvjWjTqc89Pvo9hV9u6tB1C5axgbYYvYSMtYwQ3IywhgNkFACQsYohOkMgs61DVTeAteBzYnQ/C8Bas4d6NlQd5Io3s4yFITJQrCEG7Q3oqgrdFBuhoVZso6RuALXw51E7MkZiH+OvgTNm0cfRa4LEMQKyxQyG7iCZnQyKfr9MbGMNSLhuB87t/xs3T/2/kImWHwD9Rwvu2pHAeutT2K0O4K8J+SyUm04w1C+r3kWp5QQunWPL0PA4Co++h62bAG6+j/ajTzhZ2jHHiWX1R5PW1PwQ+tGzqLr14I93gbPnnXouAButT2FZd6IHjfOCxu5fMBVxfHtFcrmAcva7sDYeh916De2Tzvmtk+/5/Q+LtPl4GZtwguslfB/N49j1NtOc/AD+feR+7DNnvVMQAAD/9ElEQVTdn7QmutkqNsaCu/Hff+6VAxwANtFplVHgO8yhpTW9AEAG69Fssv3y9rkga1ScahUAUMSPxMzYDz52M+MmSKtTDK4+E2S32r+7Cpz8ywV/4f4JLlSu4nlj2qmGo/uLwewmsuf2LrBpXm3jeyecbMdQEPeZ4/jeZT2SrT2pfBFjnHAv3LqFAdo46WcAn8APP/g9/uWmk0UcmzFMdKC4GbiSBKlTCAdXxSxfpeqvgwOzg1a57k8ZJ1fqKHvb4iTVExWpF9BQKPcx9F54c8xK3X38rEVERETLzewA9WYFmtZEs6mFHtfRRmeYRbFWgVYpIJstoKJpqBWBbRsA3G1aBXW0UVpPOFaroQhgqzNANrMKoIDMYB0bke3KahbZVRkKgEFnG9uFTdRC8zKHz4cM0DFspxMFDbJ7fPQjsldudYBCU4NWqQnBS28fYGgBtmnCNE2E4rDIYjVUaQtDLwO45AWh4/Ybb0vAhqGuI7NZgawUsNlrotnrodDZCOozdZSGddSzAwwtE4YR/sZUHCOxj/HXwBmz6OPSeviaqOvJY4TVNWSGW7BhopNZw6pXbm7D63j8dTvI/g/818c6OPNYB2ceu4F/SoqB7pGc8pDzP197CLDuQi4XgJe8AORr2AJgWX9Cyyt76V30rbvhYwFoJ5ysYvvae8iecKYwjjvOsoDM15xjFCUp/flxNG9exOjE+1Bbn4aDVX+8iwEARVmJHjTu1A/cQLbz1xVWTYxrbxLLCjJ35W8/Cbj9Dwu32W45UzaPbl7EJl6D2vp0T9tMREQOrdbAIJoFnPD95145sAFg21jHoFHjL4yWgVxBXfxSf7/cuoRjLwBX/Gzds3gqus+sZqrTy279BN0rwPPfcgOMC2K+cgK/PHkeZ6bMeE3f/xiePe0ENnffDbx5GXj9BTeo+kIb8KeB9oLS54GKOAV0cvlujjEA4Btn8ZEfKHf+fv4MIL90OfSY6GByM3BHFhqDfHjK5TzQ9TN3G8hFjpzKouqhPcHPWkRERHT/sGGHo54zyiIbDRiOySKzpkBRFKzV6ygkpGDKazVsNtewhg2UEucAzGK1UkNmuAG9k0FtQR/YZMVpnyLEL5WMF/C2sQ0AyAWZvkKfx/dLYkJXN7C66WQC21vbsPyhH7h1AGZngGJNg9bcRGY9j+Fq0Mnpxigqi0xozLPIZsPXZCzoG+JmShsdZIRfotrbwKo2b5v2wb//73D0V/+7s+Yy/gf8hz8UcOEP38J3/6fojosnf/tJDF7ypmSGk6n60h0/oOkFc/HHu4DyUBDIvHkRI3eqaEX5Csp+VvBFjMS1eD3Hn0D2ypvYEKYmjjtOUYDhH53tljUe/bZbr0K/nl6WfeRLkB+BP421efVdZB+ZMZsxpr1JFCU4l33tPXecAtH2ebw2yY+soG/d3dM2ExGRS66gnq2iZKR/UtpLBzQAbGKjChSZ+nN4mbowl7mJTsv7B8Qeu3UrtG4LvvGIvxax/burkQzgJP8eX/9GsE6u/cYv8Lq4eYY6tRNFvN44O//UxLE+wYXnMviJchU3vKxVAPK3TgDn/sH94H0D/+s5LyAav3/IrUv4yeW/wNcT1hJZqLev4/XT4nTOV/HTbwjTQAMAvoozvx3iijg9dEL57oyx6+GHkf3gKrp7lBlNtHtkVKJrUwhrtdtb7SBzV8kg1+r4/4i3jfWUKaBT6onSCii31oPZIWwD68xG3UP8rEVERETLT6tl0FF1GHoJG9viYxXrqKOWEKR1DNAu6TB0HeuZApoTjl2rZTAsbWBrawOlDvzPxKLBugFjYwMlfcvNGBb3Cp9Pg4y1zACDzJqfaTtYNyLZu0E5Cm77vOmNTd2fqtjehvOdjCxDlsOZu/JaAcOSM0bDTA3NWtF9rGMdBWhuPdH9xj62u/uZ+joGWaCzoUPXDWANWC+545YJMmC0WhHtkg5dL6GdLQPCv03srfExCvXRvwbhMVuLuWbiNal41zBmCmgAkNcyaLczwkxENraw6kwxHNOmA+krj+B/PnULv/iPH+P/jG7bbUe/g94/PoR1f1rhDjL/+GNU3O+Wch913AxdoF7+EuzWq8EUxG5ZOCv4RScrd8zjKDz6LlrC1MRxx4ll6x+NZwDL5e8j03CPaTyEzfKXwmVXn0DzOIDjz6J45awzTTJ+4JTNZLy9YQ8hA2cNYLn8ff9cypUnsRmZOje+zULfXwK6G4/vQZsPoOut4H46+mKwrvTNt6CGyl+F4Se8iGtKT3C9lXA/TmGeY+c5RnTz0+n6NUHSjw58c51HWOu69mFKmSh5e3Ib49YZF+oJ3QtEi6HVGkC1Gnx3mvD9516R7t27N4oWTuPatWs4dUqYG2KRTB3SegbWHqz7J0kSRqO5hmBOJnR1G7U96Ns0dq//JnQp79/o5e4IzV38xCBJEj6/4/y+0XEDL6/oeB3AU+eCQKf9xmk8eu73zi6ni/jeR4/gb377AmTcwMsr1/Gst8Zs9PHb55zMVAA4fRY//ehjKL91tiXWeesSjlWAi78Vp2R22jUQ2iQ6spKJ9GMKYttcXp/NVzI4eTlclrT/RZwN+gHge5fmz2SdpR/mKxm8eSJ8LvuN03jU+mt8pPwi1CacbuLzvz0WHnOh3JE2xsF94Sjiyp1zUN44jRdx3t1/wr1w6xKOhab6duoYv72j55ptTGcZw3Gf4MJzJ/DDD7zHf4GfvnM5Idv7cNjZeMwjeh8cTkdWMsJrvA1DLQHuL/Gjj21DhVJ1w7XlMsqDjP9eJW7LNbootjtY7TWd10BDRQmb6Lnf5ExVT7nrrANs6pDy3jtFDg3LbZttwGnawXiv3A279/47pT38rDWNfR8P2lUH8fqaugTv5SfXsNCryDB1CesZ5//hvWYN6xg1tZj9AUNV4L3c+XINWL1VbAifg4PXN/fzca4Ree7Zbl1ldEfOa+v4+aLP1PBnbe91NdoH+P0oojGoJrRXbIsJXeqg4LYjaJtwDLzj1rAV3ea9vh8wB/EenMey9CNd9B5M4X+OCJ47e2eGdh4yy3KfLaIftqFja60pTNm3u3bvfDYM3ULlAL4+71R0zKKPDzJJknDhD4Vo8cIM1zv4hb+mK4D/6X/Eq//lEfz3QtEinHmss+PnGtG8Qq/111tQP342mMLbe/zt96G+9hB6fjb5h9CPvo/CzTI0fAj95F3Urnxn8r+Lo/XPYp5j5znGN0O/JrBbr2LjkR8n/IhgzvMIfTNrL6Jz4iKaEMtexfb3gx+PJB5zHDBrzvrV5TecxyKx7d5U6b3yXeg1oBk3uwAtjUV8Dpze+L8LnO8/s8G/UWK+/yw8cBsPPPAFAMCDD37Rq2xh7t37DDiwAeA9tLc3A+6jAPDeGg8AH1Q38PLKL/D1hGDc3ge5dsf+9iN9jA+LnY3hJ7jw3FnA2OkYLKqendvZeMxjGQPAdJAsy/vvonA8ltuBu76RH0CYug40m9BsA6oyRH3UhAYTurSOjNVDxUrY360u+kOYuH8ABuXrGOSAov9jHO9HL22gn3XOndS+sbq8czhB2mF9hCaiP+4QtrkVjLdXlNT2uOPiflikoJo9eEHgA3cPzmlZ+pEu+R6MMnUJncLu/tA42fTtPGyW5T5bRD9s04ClVKDFvVzugl07n23ChLb4eg+A6JhFHx9kux0A3isMANN+mi8ALAYGkwKYn8I4eRbVAQA8he7NMrTrLahXAfzqXfS9MnwI/ejPnB9lZr8L68p3ICcd+/Gz6JUB4+RZtE+ejwR2hXpmPt94GVqvQjn/J2edZzHQKYyRPwZIP08u+xVkqz9G82tvQf3mr91Z3r6Cxj/+GGvXxPNgrB1JL8V2q4Wtb5edAG/0uuFTGCffxOqVcugzVvwxd2FefxzKx2lBatf1FnSUw/2Y0E46vBbxOXC33b69NwHgAzoF9P3ChC5JkPw/NUgFp+X09nW8fvqv9z2YttQ4xilu4OUVd63llQyOrJzGBWE6a/uN08G2Vy65WcS/xw+fzuDIKzecnW5dwjGhjpe9KblvXcKxVy7hwnMZHHnuEi68ImzDJ7jwXPhch1ZS/+Fkswdj661LnVxOREQHg+YFV+UK6uUW1g0bMDtolYNpKmP3n0sWxSLQ3go+9NtbbWTrdSQtSzj5fDLWijkMtm1neql+G0H1Fob9vZpeX0al1w1Pb0U0DVMP/k2sd8LbbAOq8G9m1b25vCz5Vl6C5K09FNlXXJJIVw0YurdNhyns69UZV0doW1o7aSnJ2t4GEnftfPJyBn8RM2bRx0R0f+mfd6a99qbDridkz8qPrGDwccr0ytffRPvkeXd9aiDvTjnc/+ghbN68COvsHXSuA3arA3hrT1fvotT6NPFY4H3oR18DLlwcy+oN1XPzWSjutMTTnC+uTC4XUM5+F9aUWa7eeUZvAOuROuuPeutnP+Hsc/MirLPO+trieeLakcSy7kSLXB9CP3oW1Zipx+OPeRxaWtDX9yH0xkOoHXfXID/rXp8LwEZKO4mWAQPA+0pDczTCyPuzimiXhPUYafk8c06Yqph2BcfY5QZuQ0HHY/i5v9byEJ+/cwK/rFxyXnNuXcKL5xRc8bb97Qs489ur+Ok3/gI/fWfojukNvPz0VTz/jldHE3hBCOxevgoYQ3z+2xdw5kQRr1/1gsb/tDtrMu+5lP6/fQ4nIa5lHUwfH1tORET7R2uim61CiQZ3vPV62hvQ1wdo1NxX7JT9k7WQ9wJFavjz/epaEWhvuWU2ttrZcIB25vPZ2Gr3kV2VAWgolPtBgNnsoFUu7OF7j3P+oRUtJ0piQs8P0LCcfxNbmYEwfboJXRmi7v+b2UKxXYJhA1pzhG7ZWWrIyTg3oSttFN16RqMukBd+YN2vYlhwtnXLLeS9eq0GUN1wPysnny+9nURERHQQ5LzA3s2LGN0MZ5CK7I/vIPtIfHAY0e3Hy34Wbe7kE6FsUcv6E1r++svvom/dTTy2f/7XiZ8dwmtYv4Ytt3ya88WVzco/z9ceAqy7sCwg8zVnm6K462cfBbbctXOV815QODCpHWbN3XbyLUBZCW0LPI7mzYsYnXh/bP1jJfGYSdwpv71M3+PlIAD/x7uIWQ6eaKkwALzfxF8RK1V3GgUiop1yA7fRoOPb54JsVGEtY/t3V4Fz/ynxwzEQl119DM+e/j3+xf1lIr4hBHmfOY7vXb4O06v75F8e/ilV0vr/zHF877I+llWdWE5ERPtKazpBnPpQCc/CI1dQz7bQyoazfxP3T1RG1wsiRZd+kSuoZ6vYMAGYG6hmxwO0053PCzIraBctfxpcrVBG3w0wm50WynuT/ks0n0i2vVypo+xts7cxEH9MISmo9hN+YDCWtR/5MUKuAe83HUomh1yj5mb+rwbZ92nnS2snERERHSIfYuP8CgopmaOhDOGbb0E9+VZswpaifAVlP3P3IkYbjyce6wSnCxieiavLDXzevIjRGytoX4vPSo07X1zZNCwrCOL6wdo/3gWUh6AoToavuJ9Zc7KXRzcvohuzKuikdmgbbvmV70B7BH4fzavvIvuIMyW1fj10SIgcc8xEN9+C6q/37IieZ6p6iA4xBoD3k21AzSP4cshqIBfdh4hoUW5dwrEXEGT5vnMWT0X3WZhjePZ0G2++/Qm6V4Dnv/XV6A5LxsuuPg9U4rKuo+VERHQQaM0RrEZ4SmYlk0Muo4T288TtPw+tUEarY04M0KafLwgyh9bz9aeBNtFp7dX0zx4TnVYOCcNHNLtcA5Y4a9Zol9f83evz0e4zdaiq6v7pMGzANpz/ThLdL/p4TOhcKvTUnT027Gl2IyKi+f3qZ8HU0Ec7yPxjcnYw4GSJ1i13Oulvvofihfh1YsOZuy86Waupxz6OZvUuFH9aaIfdenW6qatjzhdXBjyEDH49dh4cfwJZd5rs9Y/czF4AuY86oXOLdXr7aSdWUP2mU9bBU26QOzhPfDs+hB4XPD/+LIpXnHbk8QM0jwNy+fvINNzjGw9hs/yl8PExx8QLjjFf+zX6eBf50HgJ57n6REo9RMuBAeC9Zm+HpxbIZeB9P2JvtZkBTES76xuPBK85v7vqZwDL3zoBnPuH9ODkM8fxvcu/CDJZb13CTy4X8ewzkf1c2okiXm+cXZLpn6ft/1dx5rdDXDndxpvC+sDJ5UREtNdsQxXWBgWsoTd9crxZ95+KVkC5lUc+JkC78/O5mY8bez39M2Dq+cS1k4liKRnkWh3/M6htrAfTI8qryIbWtE6hFcLrT9sG1mOeX6nSzpfWTjrwsvUeer0eer0aUNJhVZqh1yk7FIG1I4/dUhuQU49zFTfdc/XQ9HeO1GkLQV9zAxt+Vvt4MHi8bcJDYPxLdSKi+5U4ta/o6HfQ86eFvojRzR+jctTb+Dia3tTAEX7Gqre/UL9c/rEbOBQyd28Ga/umHStOC+2Ryz8W2ucGp6c+X1zZl1C5Mp6FK+7bu+LVCeDk98PnjtvveNk/R3PDa5t4nrh2JI2ve9xNsY1CmX+MeHzcMY5gfBA6JrgOMWMTUw/RMmIAeM+Y0N1pnlFcc1645Ao2i20o7hRTyjDLaaSIaPc8/AIunryKR90poB+1FHxP2Paj022c9KaHfuUGgK8ifxLOWsKv3HCyWS8pwdrCT1/F8++krGn7zHF874PfH+Lpn4XxWDkHM6X/9hung6m1VzI4iSZ+/kxyORER7R+5Ugfy3hSvEvLopmb4zbq/Q5xGVgoFdB0aCmUE09AK5jtfmFYoo9VKzy5OJrZdT/9xGPqoKuG2OuuxEk1JrmCzMfDvuRLqaPjTYmloWkW0hXss+Z7U0Oxmg/tRaaNoNceeX+lSzpfaTjo8LAyRAdxMXttQoeoGLGsDqm7ANnWougXL2nLKAQA2TF3HFoIM4LHjIuewbSHgG6nTNHTolgVrw8kQtrcHGGzb7rm3YFk6dN0cP0fsdh1bJkPARERERBRPunfv3ihaOI1r167h1KmYCd8PGUmSMBrNNQRLYVn6L0kSPr8zjBYfOkdWMuwHAUszhjfw8sov8PV3Lgvr5s5nOcZj7x1ZySzFa/wyWpb330XheCw3Xl/ab8tyDy5LP+hgW5b7zO+HqUNdB7JZAMigUKtA2dKxtdbEmvvfimzD0Lew1lwDTAvWdgfr7QzqxSHW2wNk6z00NScAHH+cu9a7qUPtZFAvrAIAFE2DDBt2tM5hBsXCGtY0GbKpQ0cThY6KTqaOwiqwvb6OYTaLTC04B9DGMHZ7pON0aEiShAt/KESLD50zj3WW4jWDDqdlec8iosU6DK8Nt2/fxgMPfAEA8OCDX4xu3rF79z4DmAFMRES75u3reP30X+84+EtERERERDSvbL2JZrOJZrMCLSVguqWXsAUFSqWGYtYpK9Y3kVlPyjyPkVmDpmnQNA0yADNSp7JWw2ZzDWvYQCk0PUQWmTUFiqJgrV5HISNsmmo7EREREVEYA8BERLQ7njmHz//2WLSUiIiIiIjowFnNZDHctrClb6A9GGIbABQZlc0M1sfn8p+KEqlza2sDJX0LW50BshkFADBYN4BCBsPShrO9AzhbAmu19O1ERERERFGcAvoQpIPvpmXpP6eAPliWpR/7iWMYxvGYD6eAPriW5f13UTgey43Xl/bbstyDy9IPOtiW5T5bln7Q8uIU0EQ7x9d6IopzGF4bOAU0ERERERERERERERERERHNhAFgIiIiIiIiIiIiIiIiIqIlwQAwEREREREREREREREREdGSYACYiIiIiIiIiIiIiIiIiGhJMABMRERERERERERERERERLQkGADeFyZ01YChS5Ak5083o/sQEREREREREREREREREc2GAeD90q+inbEwGo0wshoYrBuwo/sQEREREREREREREREREc2AAeB9U0a9Ijv/K68i2x/Ciu5CRERERERERERERERERDQDBoCJiIiIiIiIiIiIiIiIiJYEA8BEREREREREREREREREREuCAWAiIiIiIiIiIiIiIiIioiXBAPC+0NAcNaElPiYiIiIiIiIiIiIiIiIimh0DwERERERERERERERERERES4IBYCIiIiIiIiIiIiIiIiKiJcEAMBERERERERERERERERHRkmAAmIiIiIiIiIiIiIiIiIhoSTAATERERERERERERERERES0JBgAJiIiIiIiIiIiIiIiIiJaEgkB4D/jNxf+M/7zhd/gvT9HtxERERERERERERERERER0UEUGwD+82/+Hvju3+HvzjyJP//6N2AMmIiIiIiIiIiIiIiIiIjo4IsPAP/J+78v48v4EwPARERERERERERERERERESHQGwA+Mnvquj9/QVcuHAB7U+iW4mIiIiIiIiIiIiIiIiI6CCKDQADT+J/+bszOHPmu1C/Gt1GREREREREREREREREREQHUUIA+D38+sJv8JsLf48/feW7eDK6mYiIiIiIiIiIiIiIiIiIDpz4APCX/wpnzvwV/urM3+HMX305upWIiIiIiIiIiIiIiIiIiA6g+AAwEREREREREREREREREREdOtJnn302+td//Vf827/920x///zP/4znn38+Wh8REREREREREREREREREUXcunULDzzwBQDAgw9+Mbp5x+7d+wwAIN27d28U3TiNa9eu4dSpU9HiQ0eSJIxGcw3BUliW/kuShM/vDKPFh86RlQz7QQDHcAzHYz5HVjJL8Rq/jJbl/XdROB7LjdeX9tuy3IPL0g862JblPluWftDykiQJF/5QiBYfOmce68Q/12wD6sYqek0tumUKJnSpg8KoiWmPNnUV27UeKnJ0y7xM6Oo2ar0KJla5o746bEPFxmoPs1ax+H7vltmv6TT4Wk9EcQ7Da8Pt27f3JADMKaCJiIiIiIiIiIiIaNeZugRJcv900yuFLunwHonE/VXDjinX0Qkd4bINqLoOfexc8W2wDRWqqkKSdOh6Hq1+FYpwjMc21OBY1YDTok5wHr8sue3ROiyx3D1n0rET+53QP9gGVFWFGtNO4UD/ON30xlAcNxWGnTK2SeUh4Wsd10/xWsTVQERE02EAmIiIiIiIiIiIiIgWp5UPgpBeIM82sI4uRqMRRiMLjcG6E1BMYurI+/uPsImSE5gMlReAVvRAVwsouMd2kfeDmklt6GfrGI2aaDa7KOcasKIpubaBUrsIy63TKrZR2hgK57HQQBtbdrSNQttj6shX+0BHhzKsY9TUko+dpt+RY/1+AwCK2Iy2Uzy0M0DDco6rKWkXJmFs08rjJPVTuBaLzBgmIrrfMABMRERERERERERERItTDgJ7fiBPrmAzs+4GhRVU+9GDwuztQSiQrFT7GGzbsLcHKBe80KCGQjlyoKdc8AOIWqGMwbad2oZcRgkexLGGQHHNnxZarvTQq2WE88hYzTrbktoeV4fVyKE1GCDnliUdO02/w/sI/QaA7Kp73qCdIq1WRFtxzlnaim6NiBvbtPIYSf3ENNeCiIgmYgCYiIiIiIiIiIiIiHaVbagoYdMNCltoeBHPBPJqFrmGJQSSR+hVZMirWbQ6Xmqpje1B5EBPqxNMNdxpIbsqz9yGECUDtLeCqZNNHVKpHd7HldT2uDqUah/leg91ONnIScdO0+/wPkG/pyJX0BuNMLIaQRsH225bTXTEjOOYsU0tj5HUTyIiWgwGgImIiIiIiIiIiIhoV8lrRaCquBmfJQyzwNBbADeO1kR96O0vrE2rNdGFlzlaQnwIFkAZ6LjH5dFFU5uhDf0qlOg6uXIFm8U2FK89eaC7WRT3CCS1PaaOhhuF1mpFtEsG7KRjp+l3aJ+g39Pw1+NVqsjWK5DlNRRRddvaAcSM45ixTS2Pk9TPHUleT3qxdnYe04hZgzmReK6dnTfZDPVG1obeL/6a1GPlEiQpftvOzTBOAttQU+/t4H6Yov6U8U+6r0LrgseMjW2owlrjNgxV2D/6OuhKOlcs24CaUM+0Jo0hxZPu3bs3ihZO49q1azh16lS0+NCRJAmj0VxDsBSWpf+SJOHzO8No8aFzZCXDfhDAMRzD8ZjPkZXMUrzGL6Nlef9dFI7HcuP1pf22LPfgsvSDDrZluc+WpR+0vCRJwoU/FKLFh86ZxzoH97lmG1A3VtFLjUDSXJLGNql8l4y91ps6pHwLQBndXV8/2IQudVCY6zwmdHUbtV7Fnwp8ejs5b5oZ6t3j65zE1FVs13oIJ43P0I+5zFe/bajYWO0l/CBixvshcfyT6rFhqCVgMzpWLvd5k2tYTga+qUPqFJz1yN3gcacwirQ96VwJbANOE6bcP0b6GIaNvTYcQLdv38YDD3wBAPDgg1+Mbt6xe/c+A5gBTEREREREREREREREh5cNY7sw/bTepu5nOHpZhWKWZJANGcmeTEhBjD3WNqCqKtRIJqWp59HqV6HE1BV/rimyQhfcH5FtqMH+fhZnB/pYWULdCeMQzjTVoQsZvZPbrqPjlwZMPY8WWshLOgxDhaqqkNyxS2ybrvt9UQ072G+KjNXYOmPGzJtkwDbUsTEP3w/itU4en7jxT76vLAwBf33v0PltA+p6BlZXSO/Xmn7wFwCUzPgTKnqupHGYRtKxs4whJWMAmIiIiIiIiIiIiIiWh1yJyZCjhUga26TyPSGjUpn+3GZngIblrDtcU2zA1JFH11+LeBMlJ5BqG1j3yy00Bs46zeHKEo4FABSx6R2LNrZsQGt2Uc41YEXHKlJPF/mpp7xdaH9EtoFSuwjLrccqtlHaGAItoBDpV3rd4+NgGyW0i94a0AXAW2M6qe2hcmF/gdbsouxmgK8B6GfrGI2a0NLG1u9LF9mqgk7B3SdbxUba+CfVGTNm+Wof6OhQhvVQcBVem2Puh8Txgdjmae6rDlr9LOpeezLrbt9N6MoQ9bSsXNNpc7TK0LmSxmEaScfOOIaUjAFgIiIiIiIiIiIiIiK6L2i1op8RWdoC7O0B0ArWTlaqfQy2bWfN5sy6W66g2o/WlHIsAGRX3eCajNVs+Lgoe3uAciEIbGmFclDPBIvsT4g1BIprfoBQrvTQq2WAcsGdAlnoV1rdMeNgDfvIrno1ayi4SahJbQ+PT7B/mlxGASaNrd8XBZlcGcJuqRLrjBkzq5FDazDAeC5tsqTxAcQ2T76voDWdILj7UF7NOuNprLvZ0hKkfAv9qjKebS1MBZ0kcRymkHjsgsaQGAAmIiIiIiIiIiIiIqL7hVxBbzTCyGoA7S1gNYtcw8u2dP56FRm2oaKETbcsfnppOeHYWcmrWbQ6Qeqk2WkJAcAJFtifECUDtLeCqZBNHVKpHd7HNWvdSiYnBApNdNwM16TxDI+Pje2BV9NkOxrbBIl1xoyZUu2jXO+hjgkZ14Kk8ZmZqYcCu/b2ANlVGXKlF4xxtxysAexOPd0pjCYGf5E2DlNIPHZBY0gMABMRERERERERERER0dIxoces5eqvO6pUka1XIGtN1IdKsOaou5auvFYEql55CcMsMPQWI/UkHJuqX4USbZfWRBdB5mse3bGpd5MstD8iuYLNYhuKV08e6G4Wo3sBmL1uubKJYtvbvwN4Ga4JbQ+PTwnxYegEOxjbREl1xoxZw42Ga7Ui2qXx+zHufkgcnzQx9UTHs4TN1L6bupO93coH4y8GkH3euZLGIapfDcZEctf7TTp2njGkWNK9e/dG0cJpXLt2DadOnYoWHzqSJGE0mmsIlsKy9F+SJHx+ZxgtPnSOrGTYDwI4hmM4HvM5spJZitf4ZbQs77+LwvFYbry+tN+W5R5cln7QwbYs99my9IOWlyRJuPCHQrT40DnzWGcXn2smdKmDgjB1qb9FV7Fd62HaJMuk/U3DgFJJWf8yxuRjkts9u3Bd/rltA+rG6pzr7S6yffuLr/WHm5cx7GSdLs99uSgcn/kdhteG27dv44EHvgAAePDBL0Y379i9e58BzAAmIiIiIiIiIiIiooNFQ3NXgx0mOjOlEGLKYxbZbrGuac49jUW2j2h+4QzXPAaNGu9LAceHFoEBYCIiIiIiIiIiIiKan21A1XXo4vSebhabqqqQJB2mOFWtsI+pq8GajrYBVTVgw4TuHuPs4x2no+OWhcvD05Qm7R9sz6PVr0Lx2xBTj6n7Zbo5fown3Eex3c5aml47dLGf/nZvXxO65G33pi0O6ho/dycY6+iUr664sXbO49QZvTZEe0tGpbezdZOXG8eHdo4BYCIiIiIiIiIiIiLamRZQcIMVXeT9dVD72TpGoyY0U0ceXT+g4e2jFbKobrgh0622s4apWG/ouALQiisfYRMl55xJ+wu0ZhflXANWU0usx+wM0LCcsppih4+J8PsolNlGCe2ildIOGWvFATomALODQc5dM9XsYFBcC43B2Ln9sbbQQBtb0QiwbWDd75OFxmA9Enx2xLWbiIiWAwPARERERERERERERLQz5YIfSNQKZQy2nYhjLqMAAOztAcqFINTo76MVUG51YMLERjULYRdg7DgNhXJQjlbez3JVqn0Mtu3E/ZMk1aPVimgrTllpK3pUmNdHkTXsI7vqhXHj2yGvFTHomLC3gWLd+X+zM0BxbUK2nz/WMlaz0Y0A5Ao2M+tunxRU+9EdHHHtJiKi5cAAMBERERERERERERHtTKsTTNncaQnBT4e8mkWrE0w2HOyjodYYoKN3Yte5DB9nY3sQlOcaXoZtME1q0v5JkuqBXEFvNMLIagDtrdhpltMomZwfBAdMdMYygAHIaygO1lEaZrCmraGIDjooYlL8dxLbUFHCZpABnIvuQUREy44BYCIiIiIiIiIiIiLamTLQcbNo8+hibKZkrYkugkxbcR95rYhBKyHzNXRcCW2hvD5UgnVu3bV6E/eP6lehqAbshHr8NXSVajAttXdMtK4YcmUTxbZXbweIyQB2poEG+liFDBmraGGQCU//7Jvl3GtFoOqdu4Rh1p1eeomZhjc24fWjY9kG1Mhazp6gnjDbUIN7RDhWXGtZrDIoj679TES0N6R79+6NooXTuHbtGk6dOhUtPnQkScJoNNcQLIVl6b8kSfj8zjBafOgcWcmwHwRwDMdwPOZzZCWzFK/xy2hZ3n8XheOx3Hh9ab8tyz24LP2gg21Z7rNl6QctL0mScOEPhWjxoXPmsU7wXLMNqBur6I1Ffe9fXhZuryK7QckOClxvd2HCr/UmdHUbtV5k/egkifdrQj2mDqlTwMjd39QldAojNCGWC9fY1CGtZ2D1KpDF/xfrJKJdcRg+B96+fRsPPPAFAMCDD34xunnH7t37DGAGMBERERERERERERHRYoUzgPOx01vTYph6Hq1+FYpuRjKAbRiql4mrQ9fFbNwOdC+j182sDtcTsLcHKKPj1iNkr2tNPygcomQQmnU7u8rgLxHtOQaAiYiIiIiIiIiIiGh+ciUmm/J+J6PSi6wrTLtCa3ZRzjVgRe5B2yihXfTWdy4A4jrMLaDgrZGMNrbs5HqsYR8tFPxraWXWY6Z7FoL8cgW9+hCKJDnZv3xuENE+YACYiIiIiIiIiIiWlrg+o7oUCzEmr29pG+qS9JGIaOesYR/ZVS/wrqEgrsNcLrgZ2TJWs0J5DCWTQ7kQBHHl1SwG28FrrdZ0AsObKEE1bGe94I4bMN4ESgmv2UREu4kBYCIiIiIiIiIiWk6mjvygAcvN2qoPNw7Il/A2DFWcinSv7ff5iYh2n5LJCYFaEx0xA3gG8moWrU7w7mFvD5zAsqkn/ugml1Gc/5FXMSG+TES0KxgAJiIiIiIiIiKi+4LWbLoZX9Es2vBjMWtY8stN6KoB01DjM4ptA6p/THibLRwj6QYMVUG130dVkSB584imHA9TF47vBOWTROp0TmXHnj++zyIzWC9TkiBJQgDZNqDqhrPWpruWZvTcSUESIqKF6FeheK8/rvA6zB1AzABOElMPtCaszLr/elbCpr8GcH3o1S9BGdbRq8hj6z+j6733EBHtHQaAiYiIiIiIiIhoOWlNdLNVKLMEIE0deXT9tR5HI+GL+34V69h0y7vIVktuENSErgxR94+xUGy722wDpWoWXW9bs4JKz0Ijl0PDGmHU1NKPhwk9P3D2HY1gZQahZSyTmdCVNorucaNRF8irMGx5/PxpffZpaPrbRxhZRbRLQpCk1QY2Rxj1KpBT+0O0j2wDeuqNGP1xyGxMIxI4PETCP1SJGQHbgBpXPo2UTNnFcF+fehXI0NB0X8PG1wDOYlUeX7Naa/bgLNEs1hMmV3r+65+4nrM3/bPz+u7VGV7/mUsAE9F+YACYiIiIiIiIiIiWlvflvJOlNcW0x1oB5VY+Yd8y6v4X/xoK5T6GFgB7GwO0kPczXp0M26EF2FttoFGLCagKUo6H2UGrXHeDE4BcqU+VxBY9LtTeqNQ+C8RMZKWKvrgtV8Sad660/hDtGxtGaYiCELxbLBOddrTskDB1KMO6H7DsIu/OGLAgWg3F9t5PwR/NxB1Mei0mIloiDAATEREREREREdHS05ojWA2gvZUW4YSQ6boJlKSE6ZBj5IK1hufK+trp8TsyRZ9tA2oeQSaz1UAuuo9oX/tDe842oOp6ME24Gz20DRWqqvr3lDjVuJ8RKvywQHd2Cj+OZJ6auvNDhanqFtlbaGcLTgAwob1RoanRxenaVTWY4tydLtjU82j1q1CidSWca6r2R8ci+nhBY2NvD1BGx98nj27C87Uz1g8kjFO4DTLWigMIy+jukXAmrpi5S0S07BgAJiIiIiIiIiKipWQbaiiLzRr2kV2VASjI5AbYduMgtrEeM62yEzjolltC0KKFdS94YhtYb5VR0ADIq8j224iLLctrRaA6IfMt5XgoGeRaHf/4+LbG0Aoot9ZD6/T67U0U12dBLgPF/V97qx3OABal9YeWVwsoxGSQ9rN1Z1rxyFTjmyhBNwGzE0xxXlPsscdpJtUdYg2BjHcHJ7fXZxtY9+u00BgIzycUsemVw7nXtWYX5VwDVlzkNOFck9ofHYvo4zST6hZZwz5aKPj7WJn1sX2AhH6kjJPfBve1cBD7wkJERLuBAWAioqVyAy+vZHDE/zuNC7ei+0zPfCWDY298Ei0mIiLaJWaQUSBJwjSUbrmbXRHsG85OCq1bFslusA1VeDypvrh22DBUscz9Uw3YsfuL9UbLbRhqdIpNE3qoPcKWmIwNUx/vn5dtMb7/PG2PGyMIdQVjP36+qMg5hHZG93f6YaS0lw6u8efk/BZZ1wz8rKp9ODftGrlSB/LBa0mQ1SajUs+iqjjlyrCIhpvOGn0/CWfClZEdutOJKlVku95auRqaVhFtt77QvSRXUC8L0yHrJgAZa0U459fNicdvNgb+8SXU/bam09DsBn2UlDaKltfe8PnT++ySK9gstqG4+yjDbMpU1Cn9oeVVdrNrAWiFMgbuLyxybtDV3h4Arbx/TyjVPgbbNrRacK+UtjD2OM2kukX29sD9AYgrob0+uYLNzLpbp4Kq+IuH7Kq7RqyM1axQniThXJPaHx2L6OM0k+r2P8PpJpRMDmXh1yHyanZ8PABkhSmU/X6kjJPXBiIi2nsMABMRLZ0irtwZ4vM7Q3x+5zLOPBzdPj3tb4e48dJXo8VERES7qBxMLTnqCesW5pBDFRsJ3xybugSlXRSmmrRQbJdS1jFMr2+8HcH0cVYjh1zDcrb1Ku6Xf9H94QZL80DXLbeKaCefMJ6pIz8IptCsD50MMq3WELLJTGxUgUZNS9h/nrbDHaNI9pa9hTZywZSfseeL453DQmPgZItohTL67S0hqGtjq91HuVCZ0F6i3WF2Wih3R36mEi0Lb2pj90+MampNobyCSs/NUqv0gvLoMQAK7prCo+iUxnIFPfE44V7y1iEW6/PP41WScrzYpl5F89saJVd64SlOxT6GXuPD55/UZ09ov2YTTe+1Wa6gF32dTukPLSkhU93stMLBVjeo6L+v+/ezHNwrzhztsKOPAWCw7X5mMNGJSYFPrDuyTyioOaG9tqGihE23PmvKH14kmHCuxPZHxyL6GPOPjf+61NQgr2bRErJzx4LlroHw2c3rx9TjZA2TZw0gIqKFYwCYiOi+cAMvP3cJF14JsoNfftvb9gkuPCdmDQfb7DdOCxnAaXUAuHUJx4Q6mDlMRESLlUW9XkZrPSYL1J3Sshv64llGpRf+ojsspb5FMTdQRQO14Nt79BK+UJ+W1nS/PHezydYNGzA7aJXrsX31959LFsVieK1Me6uNbL2OpESXyeeTsVbMOV++agWUQ9ODWhj2J01NSoeObQRrJIayxJOyzyNMXcgaTDtmPNPdn7oysQ0BU5eQbwGtvJuNaRtQvWx0L/s8Uk8wNaaTwW/42fA6TGHfuPMRES2lMtBxX/tis8i1JupeBr3wWupnoipVZOsVWJHHsryGIqpu9nkHsannCXWHKBlgaAWPJ7TXmb7dq7OEYTZ8eKx+FUrcrCUTzpXU/j0bG60Jy8/ilVDC5ngbAQBtlCL9mHac7O1BKMt4sSKfA+KuARDzWWJ3ZiYwDe/84VlNgvL5OfdEwuemue1s9pVF9CtZdKam2drprYsdKZ25Hl9k3e39Et+v3bo/AuLsT9MMQ1I7aW8wAExEtHTaOOkFYp+7FHwA++A8fqlcdTKD3zmLQcPd9vY/4IePNp3yS0XgdBM/fyZUYSCpDtzAy09/jB/5mcdX8fyVszuafpqIiO5XwhSZ0S9utCa62ZisXWuIvjCt3tSS6gPS2xFrfH97e4BccS0ha7UfTMkpSZCkfPx6jm4blZggklZrAO0N6OsDJ/t3wv7JxtvuWV0rBtklsLHVzoYDtDOfz8nydTJKNBTK/SDAbHbQmuc60gFmQleGqPsZR2JmfiQr0yqiXYo812wDThK9MMVu0jHmBqpZd/3Bbhkoe1+up7UhoDVHcA4TMh9bbWDTyz43oSttFN11F0ejLpAXvtDqVzEsONu65Rby3jktMVufDj8NTWaxEqUoBK/TQqa7mIkbyoZ3s+jFsrjH3trUTlkTzabzI79p6g6R11AcBJm4ce0NPc9DWew9NJs9p87Ij/o0tz3++1Q0Gx6IPdc07Y+ORfTxwsbGbY+3PZo97e6AXq8XjIlXScI4hdsQ8zlykcTPAaNRwmd8E7q0joz/Xj6C1RggP28gMJGJTtv7f/F9Qyyfl4lOq4xuZEaH/bWIfk1rUe/Di6rnoNnl+yO0nngXyC/6uUOLxgAwEdHSEaaA/u0Lwj86iviRN53zww8j+8HHiPlB5gQJddy6hYEYeF45gR9+8Hv8y83I4URERBMJ0xHHfHmm1RoYpGbtxq25myy5vvR2jJt1/xwawpdPo1E3NmEDwhd2TuaG0Ce5gnq2hVY2nP2buH+ilLbLFdS9L9DMDVSz4wHa6c7nBZkVtIuW/6WjOA202WntYlYI7Qt7GwPxBwaSgmq/H2QF+WvuOplM4WkhvSBq5Mu51GNiTGpDmlwRa94TYizT3vkBg19PLsj2VzI55Lw1EuXVxIx5IiLaazIqmxl04j+s0G4yN9AuBusHL5zWDE1dr2Ri5qE2Oxg0Nsemwu+WW+iY45mdYuaimPXorNvu7q+qwewg7g8pTT2PVr8KRTfdf5s4QTKx3NQjM5XEpFLGndPU82ihNR60Fj4feVWJx4s/1IyrNyr22Kn6GxZ7LtuAquvBv9kmlYdEMqrj2hkq19HxS0VCPTFjJ7INNeiD/2PZTtBO4Qe0if2NGbdw1roOPeF+m6Vf4v1hGCpUVfWz3BPbJoy5aghrg8f9CDryPEsS1057jvbE3wM0CwaAiYjud0cfwVOXdSdw+4KFn758LLrHdL5xFh/5GcDOX2ImMRER0bzcgGTJ2A7KlAxy/rpqXoZgyvpjorj6FkRezaI/VZRpOlpzBGe5t+Cf4komh1xGCe3nidt/HlqhjFbHnBigTT9fEGQOr03pTQPt/Fo9pXo6rHLBGtHeX1MTs3vdcqsRrC0NACij0RggL37xk3aMkkGulXe+LMoLWfFIaQMRES3OApa62BNyBU0nRXbv2ruX5zqotGZ8VvFuMHUow/rYe33SusZKxl2eJIltYN3PerTQGKwLP3gsYtMrh7O0idbsopxrwIo0QCzXag0M3DWX7a02stEPwaFMyxG6yEM33TpQFmZHcXfvDPwfl9YUe+z4TZSc4GZqX7zKEo4FZupv6rlaQCHSt9TyOEntDJUXED/NUmBs7ES2gVK76H+OtIptlDaGQjuDcUjtb8y42UYJ7aK3NrfQzh30S7w/1gD0s3WMRk1oCfcTII55F9mqgo43o01sFr3DCd7mMfB+8BjemNjO2dozxT1AEzEATER0n7N/dxXZS17Q9jLOPBzdYwoPP4zsB1fR5ZTPRES0B7RaA6hWg39Luuvh5uN+pTyFsfoWRSug3BL/0WpCn/FfsLahhv7Raw296ZPjzbr/VNx+5GMCtDs/n5tFucHpn5eSvIpsaJ3niFwG3s8X7K32WDbvaqWHLvLh6cUTjrG32sh2nS+LRuK0d5PaMC2tgHJL+CLPXXs8+pwgIiKi/WPqEqROITZLUV7NJgZ6Uz+/yhVs+usjK6iKH1iyq+7sOTJWZ5nyw5+O3MRGdXxq7Oh6yVqhnNh2ANBqRbTd5WVKW87x8H4YJ0lQqn3n+LS+uBKPxYz9TTuX8Lk/1Lek8hhJ7QyPnYZC0jRLrujYhVhDQFjSR6700KtlhHYK45DW35hxC/+7KWjnovoFwP+hcOr95PdFQSY33WdbbwaoTZTGlgFKa+ds7Zl8D9BkDAATES0dcSrmDF5+O7o9TH5EwesvBPuH1g2e2jH8/J0T+OXTQj0r57gOBBERzUGcqjV+Gi7IFWxG0nu1pvMrZcU/VkEVwvStaWLqm6odIXH7a2haDQzyXvk6MmJW4hTkSh3wj5eQh7euabxZ93fEtV3k/MPdn9JWMN/5wrRCGa1WenYxHRbivaTDhIamFXypFpS7z7ti23/OKsNs7DToWrOLbNVdszflGHk1i5ZwLwbT1qW0YSYamt1ssHa30kbRWsa144iIiA4jZzrdTkFczzlCKyBbVdzPus6yMbppY2tY9JdxwGDb/fxgouP+OtQ2VJSwGWR2Rv/ZMBcZa8UBOnonNotSXs2i5WYIA85SKZOC1L2RMzsK2lvAaha5hpdd6vz1KvJUfZETjp1V6rn82ZsifUsqj5HUzvDY2dgeRA6Mioxd6DtRJRMuM3VIpfgFj1P7GyOceR7cbwvrl2Dm+ymJqY8FfKOmaWdqe2a4B2iyAxkADs3/Peev+Pda0ObwmldiX8a/SAkT1xVYBklz1e+tG3h5rmDW4WK+EgTdjr3xiV9uv3E6CMa9cmPC/jfwshA0nC8IuNsibVw5jQs7yDg1XwmP13I4hp/HTsN8DD+/c074QBk8Nq+28T0/A/gqfoogk1d+6TJueGv+ptQBAHj4BdwInVvcd//Yb5ze9+t8cO41cX2R8S8/bUMVXq/D66rES1pnM/086dvjziueRzxXtJ7leh/dTaE1bCZ9QFkKkXvI/XwZGgf3z3sOJI1R8ucb936MfHZN/lw7vv887Zm1HncHqNGyA8Obvjn4c76/0dCMTHMmV3rO9FFCmfdLZP9PWM9WrvSELy4m1ZfUjmDf8JcgKft7XyiMRkJWooxKT8hQ9OqIrr/rlYt1R77QmtiWWfdPGHOtKX7xI25LP59jfLxDtObYGHvG27toSe8x0W0x73Nj/1aN3z/pdSD5eX1YRe8l95qHngNCuf+88+6dpvAciN5jwfMl6Riz00LZzwAWpuOb0AaR1ow8d6PPSfdedf7E53D4+Tvp9YYojanvxnt03GdsWl7/Df/0Hzs481jw91/fie5DtFxM3cm4FH8MNv5aqqE56ro/XsyjBaCVV1BtuevXymsowvtBaQfer8zktSJQVdx6SxhmgYmrvPSrUMY+K4bL5UodaA1QjPvFqtZEF0EW6KQfWfqfN5UqsvUKZK2J+tBrs/PndHGKviQcmyqmv6nnKgOduL4llcdJamdo7EqID9cGxsZO3Bj58aGUB7qbRXEPX2p/Y8iVTRTb3v7B/baofoXMeD8lirRNGdbH/602TTvT2jPLPXAgHOzvJqV79+6NooXTuHbtGk6dOhUt3jnbgFoCNnsVyLBhqAqG9fgvAxZBkiSMRnMNQcDUIa1nYPUqkKP/7085YUKXOiik/MPP1FVs16JfBO2uhfQ/jm1A31pz1tSwDajKEPWUvu+UJEn4/M4wWuwGgG/hb377QsyXaQfPkZVMQj9S3LqEl3/3l/j5S18Fbl3Csac/xo/unIMm/j9u4OWVX+Dr71zGGSTsv8CxmqsfU7mBl1eu49kDEljcTbs3hjFuXcKxp8/jXe/x6SY+/9s51wHeJTsZD/uN03gR54VA9v3jyEpGeI133lPbRcv/cGYbKpRq1l87xvu1orN90vtW5D3aNqBurKLXVCacZ1I74s4bVwa3DSVg033vFN+DQ/sdPLv2/juN0PuyCV1aR8ba288fUbs/HiZ0dRu11HtDuJ+QMEaWeI+JY+f+f7eI9rr3OTbtc23C/rO2J+m8SfW4G01dxXYmizZq4/9Y2wW7f32J0qXfg2nvMXH/Fk163iXsn/Q6oCQ9r4VjI9L7Qc77WzWYRrrcTfhBAqVZlvvs8PRj/H16dyS91tF+kSQJF/5QiBYvwH/DP/3H3+HTcgH/4Wmv7P/Af31sG1+6cgx/+ZXw3jt15rHOwp5rsd+LxnynaOpOlud0L/Hz3/u2oWJjtTfleRYjdgwiTMOAUon73J9u1uOmact+Ozyv9QlCnxPvI/73R5EnV1L5kprtO7j7xILugb19bZjvu8nbt2/jgQe+AAB48MEvRjfv2L17nwEHNQM4LAd3avADy94eIOfNBa8VUO4PYcH9dfCcN2voV+LeT2xsA6qqQvXK435FdFDIFSf46xHWado/admjTqbwBSEzNpg29wZeDk1lKz5OqfPWJRx75RIuPOdk0154RazzE1x4bmfZq76HX3CCuXDXYYUF65azrivO/Sf3TeMY/uYc8MvffZK4/+GWdv0+ca6BcJ28beHM0LQ63Osp1HEwsjkXJJq5e8CCv4uVfp1js+Yj1z702hCq6xxMYd9oNv5091ry/bpj5gaqaGBTeG2WK5to5FoQZl2ZnlufP02SXHE+oE06z6TtOyG+B1Mie6sN+FNMaag1gPaOF0ZcAvYW2u50wUljFPrM561b6nzoc7LTJn7Y8T7XTrH/FO2ZtR7A+cdIHnVUViP7EVGYvYW2+D7nS3jeJe4f5bwOJD+vaW7RLN85/y1OS8rUhe9YDBiqlw1rRjJjxcdm8gwBtgFVN4TZAFL2hQldNWCMzRDn/Cik2u87U4u73/2MzcoTe6zLndXD2xbKdgv1uSMcREvtHRu/Xn1KCP4CwP+A//CHxQd/90xugPWJ6Yf3CxOd2HS6SeY9jnaLbajOchKb6UEiWl7hDOB87FTgdAhFv5tM+6y2Bw5eADiUVq9gWD/YvzTyBHORK8hE5nd3grkzPIltA+vouv9wtdAYrAv/cChiM25KqwMomD5hiPqEXzzsjcjUuO+cwC8rwjTHH5zHL5Wr7razGDSmmQJ5Qp2XrwLGEJ//9gWcOVHE61e9gNI/4Zc4gfzDQlWLcOsWBt+Yod7o/h+cx6MxwauDRVjfVpymOun6vf0P+OGjTaf8UhE43XSnRI6RVAdu4OWnP8aP/Gt9Fc9fObuYAD7tvaTrfOsSXjyn4EooEH4DLz99Fc+/4137JvCC8OOND87jX044266cbuOkd5+8cxY49w/JU6wltWGW+3VG9vYAyK5GXotlrGZDBVMLB8LC5WnnmbQ9mbCmYNIPoMwOWgfiB0d0IPWDtWHjPnCbGzHTPcXoR+ZwCtbsibGDz7XTtmeScD02jHWgy6AIUUTMe4w1RF943RhfziAiaf8dvA4Q0aKY0PMDNCznxwFWpo2qnyqeJjKtuVVEuyR8Dm21gU1vuYEJ+/araGfc9fysBgbrBmzIqPQsNHI5p21J78+xx8LplzJE3T+vhWLbXS97rM8DuEsL0n3g6NH/h/t/4amg92Ia6FkTWoL9dST+TCFbx2ZmPXYK2tjzpUhaziWtHttQ/bL4/cTpP3XowhJ/SecTJY1B3LGmnker705XnLAPvDYL421MeVxSW2jxnCUt7tPPhV4CQVRS+dKSUekFnx32YnauA28Z7oHQd5Npn9X2xsELAAOwhn2g3EW3DLT8D7YHW/Dln4Vh5B8S3lpkmyhBNezgzTTpg4lcwWZm3X3DddYv8Plfmk/zZfn+8tdgszJYPyhzn799LsisE6e8BQAU8SMxM/aDj6fLIkurUwyuPnMc37t8HSbc7NyTf7njL3XDPsGFylU8b0w7hXN0fzGY3UT23EENcBaDAF1ouuo5r19IQh23bmEgBp5XTuCHH/we/3IzcjgdEvHXOZw173r7Ol4//dc44/+o4hiePS1c+2+cxd+4AVpF+Qs85R3/8MNIf4mObwOlKaPrfWAK/ajIzZiQJGfZhQPxgyM6eMQvZbvIVqMfuE10WmUUJvw7Q65sojEQ1qlpiT8CjDff59rp2jNZuB7bKKFdnPIHiUT3lYT3mLL3o9wRuuUW1if9gyZh//leB4hoYcwOWuW6sI503V9mbyIxi1acYhwAcsIMG5iwL8qo+w1YRXamWWsSjrW3MRB/wCI52cRDa4d9pkPv5s3/n/t//w5/+V8KuPCHAl6t/T8je+2CWRNaTB15f/8C0n6lIFfqQD7yY6zQ8SN0kY8NEvsi+2+i5Oyf1u6ODmVYd36gkbCf8xnb/ZGG2I+k84mSxiDhWK3ZRTnXgNXUEveBbaDULsJyy61iG+1MY/JxSW0hIqIJEr6bTPustkcOXADYNlSsZyyMmhq0pvMmVZr0D+19Jq9m0W9vOf+QFyP8ph776y4/MNrUYOrB1D/bA2e7N/+7/4EiklF86MgV1P0pEvfRrUs49gKC4OE7Z/FUdJ9ZzVTnMTx7uo033/4E3SvA899a7Hqk5isn8MuT54VAVbr0/SNBrsPs6CN46rLuBG5fsPDTl+ec3vgbZ/GRHyB3/haVmUnkW9T9GkNezQKD7ciXzja2B/MttSCvZscyIb3ytPNM2j47N2NiZKExmPAPfiIgMnWzwzbWp5ypJfwL3W45/b6d93Pt9O1JF67Hxla7j37VnWIq33L+n08aoqko0WmeJvD2n/d1gIgOANuAmkfwAxGrgcRXgln2XaRcww/yeH+HPXGGduhpGd/dfhd/f/m/CYX/Df/8v/1fwuNdMmNCi709QNn/xaOGQuqvFDQ0u0Be+OwaPh7QCuXU2Xns7QHQCn7MqVT7zv4p7W4NBsFzOWE/a9gXfhQa9CPxfIKkMZj22Nh9rCEgzNYlV3roCeu/JB2X1BYiIpok5bvJff6sduACwIhMrWdF02kPIq2Jbtad7is/QMObu19roj705nGXoAzrY6n8Wq2BQd794JB1fp0prxUB78s5qYRhFvsfPJ2VqQs3uolOK/0L0l1z6xbcuLrjG4/4U4Pav7sayQBO8u/x9W8E6+Tab/wCr4ubZ6hTO1HE642zC57+2Vkz9CfKVdzwMgoByN86IUxBewP/6zkv6By/f8itS/jJ5b/A149GNxw+9u+uInvJC9peTgh4T/Dww8h+cBXdA5kRTYsSfs64njmO713+RWht759cLuLZXQr+L+R+TaIVUO5XsSF00DZKqIprg85CK6DcEj/UmNB1c/J5Jm2fm4xKvczMqik4nzM2/LXtNqpAcWeDf7jYBtZDn0vGx2CqMTJ15AeT79vZP9eOn2+q9oyJ7hcOXo+6ZeQaTlCKiGIoGeRaHfd55/yAIjXjP2X/uNeB+Z7XRDSX0PPT+YFUkNimIJMbwIurhLcBEJYXsbfakazeiFn2XQR5Fdl+wtJgqX2m5eZk/f7PN3/nT/185rHf4dNyIbIu8OLNmtAir2bR6vh3qZ8Yk0hroos88u7NHD4eMDut1PdqeTXrfP4VvoTvVeTUdpfrPdThZfrG76dkckJw1kRHaF/c+URJYzDtsbH7KBnAS1SC8+8WcR3wpOOS2kJERNOKfDeZ9lltjxy4APDY1HqDBjYPwfznflZvZO7+oDxhPRe5gl50u1g26qHZ7Dm/CojMga41D/A6AVoByHup7Xmgu9dtvYGX3SmZ/amWH34BF09e9de4fdRS8L3oYbG+ijNVBT982jvuBH76DXfTrHU+cxzf++D3i53++e1/wA8/AN49d8KfivrYG58AD7+AH532pi3WMTjnZvsm7G+/cTo0lXX20oKDTwsjTsWcwctvR7eHyY8oeP2FYP/QusFTO4afv3MCv3TvAefvXPo6cPvKCfIHbRXWrKVkoedMBkdeueFc+0vB8//I01fx/DvndpyVl2Qx92sSDc1RV3htlqC0i7BSp0wWpymJrn2ooWl5P2KSIEnryNS0Kc4zaTsSziuWebNnRGi1YDoxSiZXUC9745nHoLG5x+/Rey+0BpZSRVb8XGJ20IpO4Zg0RrYRrF2WB7r+fWtCd+v21gDVzbTPtfH7z9yeWeuhA8qEHnqNFdeRE/5UA3bcttgXRJpNzHuMXMFmY+CWK6hmu+4vtROedwn7J74OJD6vl4dtqGPrEcbNkDU/91rEPBcWey4T+pRLGpl68hqPtI9Cz08JJRSF6ZBlVOpZf9o+ZVgMgj+hNbwlKMNs8jTKs+wbIsPJAZjn9VxD0yqi7U05KEnh9cdDfa4H/bINqFPe03R4ZerO1M/e324Hf4E5ElrcgK63fzu6PYbW7AbPrdDxEvLw3qsTRBJ1JO8z+4R2azVnTW/3yTq2n1zZRLHtlXfgNzDhfCFJY5B2bL8KRTVgJ+0TeT2S8kC3WZh8XFJbYEIX1m0+yExjtnaG1nSe4nXRFNZ3JiKKFfpuMuWz2h6R7t27N4oWTuPatWs4depUtPjQkSQJo9FcQ7AUlqX/kiTh8zvDaPEBdAMvr/wCX38nPrh6ZCVzSPqR7iD1w3wlgzdPeNM1f4ILz50FjPjxP0h2NoaL6uei6tm5nY3H4bHo+/XISmYpXuOX0bK8/y4Kx2O58fpOYkKXOiiMmmM/MPIyTYKMDxuGWgI2vR8x2DBUJ9gY+2NTApboHjxs/Yjev9HHOyc+d5znwrDuTKm2+HMtWvS5fHActvssSXo/kl93ifaKJEm48IdCtPjQOfNYJ+W5dn8Iv+fw9WUvhV/rTejqNmqpP3IXzf5ebOoqtmvT709E+yP9c+DBcPv2bTzwwBcAAA8++MXo5h27d+8z4CBmABMttbev4/XTfz13MIdmp718FgM/o/IEfvjo/Tz+bmZ8QmZwKAv8lUu48NwJ/PCD3zvZr6/ccHa6dQnHhDr8DOxbl3DslUtO5vFzl3DhFTE7+xNceI5ZyNPg/UpERLORUel1UW45UxMS7a1IBu4UmTMh4qwKkpg562QaGUJWzljG1BgZa0VxCk5RNMtefDyeVT9+rsjxkXaL+4czj5P64f5wo9+fM+uTiIgOknAGcB6DRo3B331g6nm0+lUo7vtqKLs39r3WwhAIMvNi9xHr0eFNpG0bKlRV9TP5Ys9lG1B1Pfis5JWbeuxnCCKi3cAAMNFeeuYcPv/bY9FS2k0Pv4Abd7w1VYf30fi7gduVjDBd9TH8XByLd07glxV3iuFbl/DiOQVX/HF6AWd+exU//cZf4KfveON2Ay8/fRXPv+PV0QReEAK7l68CxhCf//YFnDlRxOtXvaDxPy143esldt/er0REND8NhXI/fYpFol2hoSmsHziynCky40Kw40zoyhB1/3gLxXYpCCD3q2hn3PUJrQYG3jpaiaZYpzmOueFk0I+ctdFRnjB9KEzoShtFy2t3F8inBL5j+yGj0rPQyOXQsBKWiqJdpqHJ7DwiWhgZlV54PV3ae1qzi3KuAaupAaaOPNz399EIXeTHg61mB61+1v8sYmXWY/YR6ylAXEy9n61jNGpCSztXCyhEys3OwHn/H41QU5I+QBARLQYDwERES8kN3N4Z4vM7wpq1b58LsnyfPo933WL7d1eBc/8p/UuQsQz2Y3j29O/xLzfdh98QgrzPHMf3Ll+H6dW9yHWviYiIiOhgELJYJKWKfnR7Ensbg9Day05GbPBDhjLq3hfo8iqy/SHif+Pg1aGgXbQmBG8XwOygVa4LUz9O+gHGtP0gIiKiRbG3BygXgg8FWqE8PkuI1nQCuO5DeTU7tk+4Hg0FYXH3XEaJ2SdyrnLBr98r12rBeqClLf8wIqJdwQAwEdH94tYlHHsBQZbvO2fxVHSfhTmGZ0+38ebbn6B7BXj+W1+N7kBEREQLYaLTysH9Dopo79gG1DzQ9TOAG8hF90mTa8DyM4Cdv9kDuGX//HNlXCkZ5Fp5JwidH6BRm7kBREREdMDIq1m0OkE6r9lpjc8SYurCsg1OIDe6T7geG9uD0GZgbJ/IuVodfwkJv1yuoOd+bkJ7a8IMJ0REO8MAMBHR/eQbj8D7ftj+3VU/A1j+1gng3D8Ia6PFeOY4vnf5F8GUz7cu4SeXi3j2mch+Lu1EEa83znL6ZyIiol1k6vlIRiLRHsplgs+WW+3pM4DlVWT7bWztybeeCjK5AbxkHNtY92dwtLfayHa9AHRv8vNIK4TX3LYNrLfKEBJ/iIiIaL/0q1BUA7bWRBfuD7wkCXnELPGgNVEfems3SyhhM3afoJ4S2pHNQHSfyLnKQCdS7q8XrFSRrVcgw4SuTlrqgohoPgwAExHdLx5+ARdPXsWj7hTQj1oKvids+9HpNk5600O/cgPAV5E/CWct4VduOGsIX1KCtYWfvorn3xGml4565ji+98HvOf0zERHRROJUuHr6D7LQR9WdNs77MolriNK+kCvYLLahuPeiMsxCmBlxAg1NK5gCcbp7f14yKvWs/7xRhkU03FRleTWLVl5ow8QvYDU0u0FdktJG0ZpnLVkZa0U49YwtOEhEdEiJywIIf7rpzhohSaGMy+AYdy1124A66XXYrSftHKFt4mtsZPtYWxbA1GPWhY9rl9fmmZnQd/B+aRoTxjeObUCdr7F7TENzNMKoV4EMQGsKs4wkfFYW90maSSTYp4dez/mxmFzphfZPPlfBaZNQLu7rFGloum0mIlo06d69e6No4TSuXbuGU6dORYsPHUmSMBrNNQRLYVn6L0kSPr8zjBYfOkdWMuwHAUszhjfw8sov8PV3LgvrBs9nOcZj7x1ZySzFa/wyWpb330XheCw3Xl/ab8tyDy5LPw4SU5fQKXhfwNow1BKwGc0ENqFLHRSEdQKX2bLcZ8vSD1pekiThwh8K0eJD58xjnZjnWszrpm1ALQ2RBVDoBeWmrmJ9ABQ3e6jAgPMynBIMs1P2sQ2oG6vo+QE48XXdhC6tI2N5r/E2DFXBsD7P8gPJTF3Fdi3yPpLW5j1lQle3UZu1HWPjenAc6Nf6AzxuRMvuQL82uG7fvo0HHvgCAODBB78Y3bxj9+59BjADmIiIds3b1/H66b/ecfCXiIiIiGg3aLUGBn4GsIJqNjKdum1AlfJolQv3RfCXiGh3ZVAoDhAsqWqgk6mjGNlrN9jGOgaNTeE1XkalFx/89afoFTOIbQOqqgaZvEKmcrC/jo5Y0TQS67VhqEG9up9ZLGQAJx4b7oOX6WzqebT6VShun+L2capVg/77dXagj5VRKrnC4C8R7TsGgImIaHc8cw6f/+2xaCkRERER0cEgV9DzpmYcm7ZR2B4tJyKiuShrRQzcCLC9NURmzVtJfgb9qr/8gBcg9ScobgVrsUZ/2JNdnSLv1Tawjq77vmChMRDWfUcRm1453HXsTd1ZjmM0wmhUgL/IfFRam2PqtY0S2kVrcr0xx4bbNMImStBNQGt2Uc41YDkL0cbuA9tAqV2E5ZZbxTZKG0OgBRSi5yEiogOPAWAiIiIiIiIiIiIi2l3yGoqDDkzY2BpmsDZFTHZMruEHKJ0/YarpshfU7KKMMrruD3jk1SwG25GopW3CjAYy5Qo2M+tBALkvbMuuulMny1jNOkX29gDlgnd2DYVysHtIWptj6rWGfSFgnVJvzLH29iAUCFeq/bG+J+5jDYHimj9FtFzpoVfLAP5MGMF5iIjo4GMAmIiIiIiIiIiIiIh2mYy14gAdYwvDTBBoXDwNzS6Q96Zw1grIVktCNq8No5THeiSV1TZUlLAZZADnQpvHyKtZtII5rbE9iOwwJyWTE4K2JjqJGcDj5NUscg0ve9j564UXt0/eR8kA7a1gimdTh1Rqh44lIqLDgwFgIiIiIiIiIiIiItp18loRg2obmbj03+hUyV4AN22fyBq2Pq2JLvLuNg1Nq4i2EkwP3S5a44HRtSJQVdx9ShhmgaEV2iXMPYe3f2KodNo2u+TKJoptrx0dICkDOI7WRH3oHev8+cPYr0JRDdhJ+8gVbBbbQVvzQHdzL1ZpXgxxXeO4WyfE1EP9Dx8nrLWcxDagJpzENOZdJ3mK805p/jYsjnM9vPWrF2FR4zNtPdPut/dMf13wxZn3nrENNXkd8bjniG1AjYyrqU/xnKW5SPfu3RtFC6dx7do1nDp1Klp86EiShNForiFYCsvSf0mS8PmdYbT40DmykmE/COAYjuF4zOfISmYpXuOX0bK8/y4Kx2O58frSfluWe3BZ+kEH27LcZ8vSD1pekiThwh8K0eJD58xjHT7XdoGXiewEqE3oUgcFcdpoAqKv9aYOqVPAqKnNOGaz7CuwDagbq+i504wHTOjqNmq9yi5muE9yQNowz7im2o06DydTV7Fd6/lrnO/cnPeMqUPKt5BruD+oCT0PncBupzBC6GliG1BLbSBb958/sfvtwGH4HHj79m088MAXAAAPPvjF6OYdu3fvM4AZwEREREREREREREREB0M4AziPQaN23we8JtKaftBp58TMTxuG6mUI69BDmZcd6F6mo+pkT5p6Hq1+FYqbzihmJftZkrYBVVWhRo4NnTdxn7T2ONLa4GVk2oYKVVUhuecL9hHqjGQ5i1mnsf0SmHoeLbSQH6s/uQ0+24Cq68HYxqWGJrZt8viExlnIBB8/zTTXI5LxqhowE8c2PFZxYxItj99fR8cvFSSNyRTjOc09M8Y2oK5nYHWDKQrs7QHK6PjH5tGND+pm69jMrI+PeaStqmEHbRHGnKbHADARERERERERERER0YEgo9JLXsOXkjnBosUFzW2jhHbRWy+5AIjrMbeAgrdeNNrYsgGt2UU514DV1ABTRx5d/zpuoiQEvIrYjBw7bnyf1Pa40trQRd5vQz9bx2jUhBbaJ77OkNR+ObRmF2WU0R2rP6EN4cOFsQ3vP8k04yMyOwM0LOc8NSX2IgjGrwdsA6V2EZbbVqvYRr7aTxhbYaxsA+t+uYXGYN0J1ibtP+s1ipowntPeMwETujJEPZIxbA37aKHgH2vFBXldcqUO5GOm2Pbb2kW2qqBTcNuRrWJjbGeahAFgIiIiIiIiIiIiIiI61LRmEDiLy0ydlTXsI7vqhbg0FMT1mMsFN3ApYzUrlLvs7QHQ8taIlqBU+xhsu23KrrqBs/hjgfh9UtsTw94eoFwIwqtaoey3IZdRYvaZrs7EfsWYpg1j/LEN7z/JrOOj1YK1wUtb0a0RMdcD1hAorvlBULnSg9XIhcY2dqzkCjYz6265gmrfOT5p/1mv0ZgZxjPtevn7GOtuhrcEKd9Cv6pANWwomVzoWHk1O3ZsQEOzC+SjEWK/rQoyuTKE6mgODAATEREREREREREREdHhZOoLCfhGKZmcEMAy0Zkh81JezSLX8LJRnb+dZnPP2h55NYtWJwiwmZ2WECCN28fG9kDYONj2p6f2zjVrv6Zpw5hWx88MTdw/pm2zjg/kCnqjEUZWA2hvzT7FsJIJH2fqULxobspYeet8O2UWGrn0/VOvkShmTIApx9M1zfWSK72gjd2yvwZw9Fh7ezB2bIjWRBd55CddJ5obA8BERERERERERERERHQ4aU3Uh966yRKUYd0NSprQd7B2aHg95g4wTeZlvwpFNWBH2iTFrjM7m6nbI7ShiyCjNHZN1tA+JbS9cnkNRVShRM81a7+maUNUGeik7Z/QtqnHx+WvL6tUka2HpzOeilzBZrHttkOClAcaXjQXyWMlrxWBqldewjALDK3k/ROvkShhTIApxhMz3jNJtCYsP7NZQgmbE491pgufxc6e0/cb6d69e6No4TSuXbuGU6dORYsPHUmSMBrNNQRLYVn6L0kSPr8zjBYfOkdWMuwHARzDMRyP+RxZySzFa/wyWpb330XheCw3Xl/ab8tyDy5LP+hgW5b7bFn6QctLkiRc+EMhWnzonHmsswvPNRO61EEhbl3QhVhc/aZhQKnMETSagm2o2FjtTQyeiExdxXath4q8uD6mW9R55qtnL17rvUxNP5g8RzsXaS/aE9xH0S17xDagbqyiN8vN79qL8Tl0djCeB5MJXd1GLbL+sGgvXht26vbt23jggS8AAB588IvRzTt2795nADOAiYiIiIiIiIiIiOhg0NDc1YDNouo30YlNwzsIFtXHSRZ1nkXVs3jhjNI8Bo3avrbzoLXnoOH43A80NFOCvxTGADARERERERERERER7Yg/naokBeux2gZUVYXqTWnqT91pw1C9/XXougrnEBO6pDvrVSYem3CuhHLbUKGqKiRJhzlV/UltC5h6Hq1+FYo7923ceaPlkjdPrm1A1XXowv7+fm4b5NUiMgoAU/ePj5tmN6hfRycoDfoYc7xtqEGbVAO2bUAVKje9/kaPjT4Wz5PW19gxFqW3d3/JqPSmW+t2b+x+e7TmPmb/wplWef5s1d0fn0NnR+NJhx0DwEREREREREREREQ0P1NHHl0/8LKJkhDAK2JzNMJoZKGBNrZswDZKaBctd/8C0ApXFxg/NvFcSeUA+tk6RrFZpuP1T9M2rdlFOdeA1dSSz2sbWPfLLTQG60EguQUURiOMRl1kqwo6BefYbraKDROAVkFFBszOAA3L2VZTxqLQwnnj2zl2vG2g1C7CcttqFdsobcQvuRU9Nvo4vHN4DLrIp17/JKnnICKimTAATERERERERERERERzs7cHQCvvZ28q1T4G224AL7vqTtcpYzXrFFnDPrKrXnaehkLZ/d+omGOTzpVUDgC5jCLWGoipf+q2uRLPK1ewmVl3yxVU+8JB5YIbjFaQyZVRGI9MAwC0WhFtxam3tBXeZm8PUPYPjG/n2PHWECiu+dOnypUeerVM5ChH9NjoY1G4LYBWKKde/yRp5yAiotkwAExEREREREREREREc5NXs8g1vKxZ5y9t+lUlkwsChDDRicleTZJ0rqTyWc3atqTz2oaKEjbdMguNXPTIKcgV9EYjjKwG0N4KTZ8sr2bR6nhptja2B8JGT/R4JROux9QhldrAYNstE/obPTb62KtjrC2A2WkJQfQZpJyDiIhmwwAwEREREREREREREc1Pa6I+VPwsWGnCGq5yZRPFtrd/B4jJXk2UdK6k8hlN3bZ+FYpqwE44r7xWBKpeeQnDLDC0opWk89fVVarI1it+5i7g9LcLL/O4hLa4zTV2vFzBZrENxWtrHuj2NlFE1S0L+hs91orWJZ4o1BYJeXQxz7Kj0XNOHUK2jWCd4ch1mI64nnF4bePZRNZFNuLWPN49tqGG1qCeVO6MW7ivpj7LuBHRQSbdu3dvFC2cxrVr13Dq1Klo8aEjSRJGo7mGYCksS/8lScLnd+LXqzhMjqxk2A8COIZjOB7zObKSWYrX+GW0LO+/i8LxWG68vrTfluUeXJZ+0MG2LPfZsvSDlpckSbjwh0K0+NA581hn7uealx3rZOia0KUOCrFr9O69g9w2CoRe620DagnY7M0QNA7ZjetsQle3UZu7TTMydUj5FnINK5z5nlQOb9zaQLaOnhuxN3UJncJorgA+0UFwGD4H3r59Gw888AUAwIMPfjG6ecfu3fsMYAYwEREREREREREREe2lcJZtHoNGbYGBt505yG2j+fiZxZIEyU1vtQ0VqqpCGsv2jWTxCsd6WbTTHGvqebT6VSihdFobhipmGqtwqjShq062cFxbYep+WWx2rm1AXc/A6kbS1ZPKRdk6NjPr4/XaBlRdhy703W+b21YiOtgYACYiIiIiIiIiIiKiPSSj0tvZWr275yC3jRL1vWmsvT830GobWEfXvZ4WGoN1N+gK9LN1jNKyfk0def/YETZR8gOlk47Vml2Ucw1YoVRaGWvFATomALODQc6dFtzsYFBcg5zQVrMzQMNy2lBToqFXE7oyRH0s0zipfJxcqQP5aDAbQAsojEYYjbrIVhV0Ck4butkqNsZ2JqKDJjYA/N6F3+A9AMCf8d5vLuA//+cLeO/P0b2IiIiIiIiIiIiIiIj2Wa4Byw3UOn9ucFauYDOz7gaFFVT7wiEZRahgnL09AFrB2sZKtY/BthOAnXRsEnmtiEHHhL0NFOvO/5udAYprcmJbtVoRbcVpQ2krXJ9trKOFFvKSBCnfQr+qQDXsxPJ4GppdIB9NAy4X3AC3gkyujEJStJuIDqRIAPjP+M2F/4z2J39yHv3m1/j/fvkM/u7vvos///o3YAyYiIiIiIiIiIiIiIgOA29NZz+rNhfdI5m8mkWuYQlB5QVkhMtrKA7WURpmsKatoYgOOihiTU5pq1xBbzTCyGoA7a3Q9MtypRe0r1v21/pNKk+kNdFFHvlWdAMRHVZjGcBPnvk7FL/q/P+f//QJvvJlAPgyvow/MQBMREREREREREREREQHy9gU0M66tfJaEah6azqXMMy60y5PQ2uiPvSOTVmDN0m/CmVsvVwZa0Wgj1XIkLGKFgaZNchudnBcW/21d5UqsvXJUzrPS2t2kbJacIxg7WIiOnike/fujaKF7124AJw5A7j/fVIoe9Ld59q1azh16lTkyMNHkiSMRmNDcN9Ylv5LkoTP7wyjxYfOkZUM+0EAx3AMx2M+R1YyS/Eav4yW5f13UTgey43Xl/bbstyDy9IPOtiW5T5bln7Q8pIkCRf+UIgWHzpnHuss7Llm6iq2az2kJSgeZqZhQKnsXuAumQld6qCQslbtNPz22wbUjVX0QuvaYmHnmQVf64kozmF4bbh9+zYeeOALAIAHH/xidPOO3bv3GRCXASz68leAP/8ZAP7M7F8iIiIiIiIiIiIiopmY6LSjZYfJNO3X0NzD4C8REU2WHgB+8v+NP/39Bfzmwt/jT1/5rp/9S0REREREREREREQEALANqMLcuKauwrDdclWF6k2hK0wX609rK+no+EeK5c4UvnDXcVVVFZKkIzQDr21A1XXoXv1uG6L7i3V6+wA2DDVog+62Oe1Yrz0wdb9Md3YKPxaYeh6tfhWKuyG+LYG5zj9Fvf41gXddnGsRW78g2n6gE4y3fz1N6N61iWkbERHtvdgA8JPeVM9ffhJn/u4M/urM3+HMX305uhsRERERERERERERUYoiNkcjjEYWGmhjy4k6Io8uRqMRRqMC0HJ3DZWPsImSH0TsZ+sYxWWZtoCCu38X+fH9I3V6+9hGCe2iNd6GlGO99pidARqWU1ZT7LHHIq3ZRTnXgNXUxvontlc06/mnqVcrZFHdcArtrbazlmxC/aHjxPZDHG/hegrG2kZERPsiNgBMRERERERERERERLRj2VV37VsZq1mnyN4eoFzwQrkaCuWgHK28n0GqVPsYbDtBxFxGcfePKBf8oLBWKI/tHz5XsI817CO76q3KG7QBkWPj2qPVimgrTllpC2OPkyS1JWrW809Vr1ZAudWBCRMb1SwKWnL9qfzxDq6nKNo2IiLaH9Jnn302+td//Vf827/920x///zP/4znn38+Wh8REREREREREREREREREUXcunULDzzwBQDAgw9+Mbp5x+7d+wwAIN27d28U3TiNa9eu4dSpU9HiQ0eSJIxGcw3BUliW/kuShM/vDKPFh86RlQz7QQDHcAzHYz5HVjJL8Rq/jJbl/XdROB7LjdeX9tuy3IPL0g862JblPluWftDykiQJF/5QiBYfOmce6/C5RvuGr/VEFOcwvDbcvn17TwLAnAKaiIiIiIiIiIiIiIiIiGhJMABMRERERERERERERERERLQkGAAmIiIiIiIiIiIiIiIiIloSDAATERERERERERERERERES0JBoCJiIiIiIiIiIiIiIiIiJYEA8BEREREREREREREREREREuCAWAiIiIiIiIimoptqFANOygwdUiSDjPYA4YqQQ8KDrxon6KP52Xq0kLqISIiIiIimhUDwEREREREREQ0FXk1i357C15Y094eABhg249zWhj2yyhowTHLy4ahqkiK8WrNEXoVOVpMRERERES06xgAJiIiIiIiIqLpaAWU+0NYAAAbW+0sGg2gveVGQc0OWuUCNACwDai6AUOVIKmGEzS2DaiSBMn9CzKFTeiqAUOP2+ZkFXvl4W0e53jTUP19guxbE7pwrCQlB21jRdrs1GvDUBVU+31UFQnSeIPGMolNoW/hrGkiIiIiIqLFYgCYiIiIiIiIiKakoVBuoWPCyfZFBmurWfSHbkh4e4BcRgl2b7WBzRFGvQpkmNCVNorWCKPRCKNRF8gLwdh+Fe2M5WyzGhisu0FjcwPVbNcp75aBchfNuAzjfhXr2PTrzlZLbt0amiPvnCOMrCLaJbfuiUzoyhB1/3gLxXYJhi2j0rPQyOXQsEYYxTZIYOrIw+3DaITRqOkEyYmIiIiIiHYBA8BERERERERENDUlk8Ng23ayfbOrkLUCyq0OTNjYagPFNWHa41wR/kOzg1a5jmBWZA2Fch9u7BhAGXVvo7yKrJ9pPC3h+Gjdph5k3ypV9IWjUtnbGKCFvJ+562T9Bm2eklZAuZWfPfuYiIiIiIhoDgwAExEREREREdHU5LUi0N6CuT1AuaAJWcEWhhACvouiZJBr5Z0AbH6ARm3G3FnbgJoHun4GcAO56D5pcg1YYgbxaBSfgZzKy0LeBEqcApqIiIiIiHYXA8BEREREREREND15Fdl+G+ttwJvtWcnkMFhfdzKCo/t7tALKrfUgA9Y2sN4qozAhmGpvtZHtesHXnpBBHNXCuld5tO5cBt7E1PZWe/oMYLev3hLHOyej0huh60+jTUREREREtHgMABMRERERERHRDJzplftCtq+8VgT6fTcjOImGZjeLquJNxdxG0Zq8Fq68mkUr703BLEFSk9bvLSM7VPxpnrNdt265gs1iG4p7vDLMohw9NJGGplVE22uzJGbvylgrwumPnh7NtQ1VOF5CHgnrGBMRHVom9LHXaBP6ks54YBsqVGFOf1OXQo/ntah69tNujc1kNgw1eg9GufuMvacjuIe9P/+9fdb7OLz/IvofHdPdM2tf99NBamtKW/xlSBK2L1xKW2a8NydtX4S9u7fvTwwAExEREREREdFMtOYIo14lyPaVK+hFp0aWK+iJ+wCA1hSmUhazeTU0R2IwOHhsdloo+xnAFhpIzsgtNOOnaZYrveC8zSaaQrvkSg89Ia04+tjrW9DuoJ1+vTHRXLGe0PkT9iciOvxyyKGKjfjIQwobhnq410jXmqPwe8ecFlXPQbI3fTKhSyWgnrbMgw1DVdAuWv77sdUYIB8KlpXdJSMsNAZ5TPh911T2pv/76fA/f3dT8Dl28o8e91r43hy/jst/7y4/BoCJiIiIiIiI6MDSag0M/AxgBdVsPWUaaCIi2j9Z1OtltNYTMjBtA6qQYekE15ygXLXfT5hRIZKVKSUHmkw9LrMzmg0nPjahqwZMYZaGIBMtbdu4sSy2SF/9bbYBVTcSM1Wj9cT3Kak8ra8pbQpJH+/486YL98kZV0OoJ3TJp2pjHA3NUQ8Vb72HOOYGqmhgM/Sjr000cnHLMshYK+Yw2J7y/H6WpwRJ74Q2TXdNZ7nfkq+RqYvjKQT00sY1pe2BpHOmP39nb8+E+yOtrbGvL5Ofc9HjFtIWl6lLyLfgzGTjHTxXO5PG39uc0paUbcG9GX8do/duYttTx2pC22lXMQBMRERERERERAdXNAM3Nns2mkFMRET7Qmuim43LAjahK20ULe/1vAvkVRi2jErPQiOXQ8OKe43X0BTfA6wi2qVocMQJcuTRjZ2tIVW/inVs+m3KVktBcCJtWyoTujJE3W+LhWJbOLbVBjYjM2nESepTUnmqCW3ypYz3XOeN0a+inXGzcK0GBv4PBqZt43zs7QGQXY2MuYzVbKjAZWOr3Ud2NfUKuUzo+YFz/45GsDIDtKK7eNLGcOr7LfkaaYUyWl40295CG0WsyWnjOm3bk86Z/vydvT0T7o/Etia9vribE59zu9GWgNYcoVuGkwHc1HbQzqTxx4S2pG0TpV9Hx4S2J45VWttptzEATEREREREREREREQLodXEL/9dZgetsjiDg7Oe/NASd0ogZrApVfSj2wFAK6Dcys+RXVZG3W9UtE1p21LY2xighbyf8eZk1vnH5opYmyaumNSnpPI0k9okShrvec4bSxhXeRXZ/hAWZmzjrvHO70wVHRsHi4rc2/9/9u49zq26zh//67RT7jeXO1YtkIwwRlug3pJWRVhtMoJB2rjabx0USejCl2Rhaxe/g1aclYWumFRZmBTU2f7KarAlW3bmjFvYrrQzooIUNw7aBJliVVBYCwWkMJ3z++Nccs7JOScnmdzn9Xw88oA518/5fM6t+eT9/nji/Yial1E51mEF55tjG2UhAigMZ4BILzxO9VpJ2e326aTS8gD254dTWcvdX+yuuXqUxUm15YRD/TuVxWlepcqV3a6u4FB2qjt2ABMRERERERERERFRbXji6Pcl0JfaY55TuUIKgRCUcVnlyDLrMV7VKLMhoE9wnZ64bvxJ5PVRb6ax6d2xOya76WW4KZNjfVe530q4KWOVPN0+ILfHFHlYwJ6cHz1a6mh1DOB6jX1agzos00bhaBpZsQC5v1U5hpnWq+M+ndSpPLXUSmWxU3X9t4B2LnsHYAcwEREREREREREREdVMcE0SSCSK6UaDYUTTA8Wox0IKA+kowm46Wvw9UPvnCsOZMtFjHsTHJIxE1XFdvejx56AO5VpIDZhSoKYxoBaqpExO8xx4uuEbz2C4JMKzWuZjspvucKyVlKlsfZv3WyOVlLEawTCi48b05IVUHxJwiLp0w9sDvxLlCnO927KqwwrON4c2CoajSA/0KemWy9RrJWV32KeTisrjxKms1d5f6lEWJ9WWEw7171QWp3mVqkfZqe7YAUxEREREREREREREteOJYyipj/MKYnDEh4RXTQOaQSSvjn/qQW8E8ryYqUfRE8dQJAOvkj7UO+GzTGFaSAWKKUYFASGMKFF8HsT7i/v1TkRgKBai8E14tdSkvhH9uLZO85wEMZiPIKMeq1BdpKfdMdlNdz5Wl2VyqG/7/daKyzJaEhFT2ml8PAGvICAmyp1UAS3dchCD0ggQKm7fm4kgXzLeqhV9mmBTmTxxDCVz2vw+9JvOsSLnOnR5vjm0EaB2dI/L6ZblCfb16rbsjvt0uH5RYXmcOJbV6f7ipB5lcVJlOZ3q36ksTvNKlGnHepSd6k7Yv3+/ZJ7oxvbt27F8+XLz5LYjCAIkqaoq6AidcvyCIGBq34R5ctvpmt/D4yCAdViC9VGdrvk9HXGP70Sd8vytFdZHZ2P7UrN1yjnYKcdRGyJiQhZhyfylk910dwqpAPowpKV8FGMCBnrydUoB2Zo65TwzH4e5bZ1U0+7m7VezjcpUcK6LMQihtJLW1MXydWCuD3N9mf82KiAV8CKBpKGTppAKwJtQYoiiI5CUHhTL6YUUAsqYg9GRYmpPMRbAnjVjuvEMG0cQBGzYHTZPbjvXLcq2+T3D6VpymketwHyvb2+1PN9ExIQB9OSbc38jarZ2uDfs3bsX8+YdBgA44YTjzbNnbP/+FwFGABMRERERERERlQoO1mv8P2quAlIBNRqsVC3avRbbqBUxm0Z0RIJUVaeCc11ZK12n+voQERP6gH7TeIGFFPoSPmU8wZFiSkqb6YXhDHwj8riDOSXXaiEVwEDPEDtHiKjziFmko/28vxERO4CJiIiIiIiIqJZExAzp84x/izGbNHuFFALadAEBfQ+SGCuuE8sWp1vYo0uvqG5DjCmpIAHLDiorhVRAVwYRsUAKKV3ZDdnxnMpOLUSJJh0ft01xaGx3h/PVQV3OHadrwGYbYkxAKA2kQ7pjtVlWnqVLTRpLla2r0rqxrl9znboXxKA0hrg6cKCiMJwBkmuUDu0g1iSBzHDBdnqJQgp9mQiG2DtCCGLQ9scRTvOIaq2G51twUMuKQESzGzuAiYiIiIiIiKgxxBhCGIEkScpH/bJTRMw7gX5teh6RTJ/SSSsiFsohmZfn5XtySJu3q0kjgyFlGyPwJeRtBMNRpJXIPxSGkUEEvZX2/YwnkOnJy9vOJ5EbSEHpZnMoO7UWD+JjeST9fvl8KvcFue35WqEZnztO14D9NoKDEkaictpj+VjtlzVGz0qQBuPOdWVZNxXWb4N4eiPIhZTxCtd4keqbQL+rMT+JiIiI2hc7gImIiIiIiIioMYJhRNMhCIIpArewBzmkEdKiCeUowok8SlIZeuL9iOpWNYqiX4vqCyIcVbYRDCOazkJUowcjvVV0/ui27emGb3wCeZQpO7U3u/O1YjM8d5yuAbfbKLOsMXrWhZrVTQN44hiTJEjSGHqH+zDRPwio0csWkc1EREREnYAdwERERERERETUIEEMShIkaQjoU9PGKvxJ5LVoQvlTuwDCIMLRNLJiAXL/b+Xdv47qWnZqHofztVZqce5Uso1KlnXUgLqptUIKfRP9GPSmMJBLIi/lkcwp4wcTERERdRh2ABMRERERERFRDXnR489hj9KpUkgNWKRs9iA+JmEkmkZWVKMiM7AarhPeHviV6F3Ybk+VxoDam1NIYSAdRVjp3AqGo0gP9FWX/tmJU9mpQ5jO11pxe+44XQNutwHnZT29ESCxvopO3DrVjQNjWUWsT8g/6rCbLivIqZ8Nvd0edPt0fxIRERF1EHYAExHNNjvWoWv+SmyYNM8oVbh7JZbe/Yx5MhERERGRAw/i/T4kvHKKVe9EBEm/PKeQCiipZ+VPCCNK9GEQg/kIMso68keJKPTEMZTMaWlr+9Cvba+EP4nIhFde35uAb0Q3ZmswjOj4eJXpn504lJ1akAe9EcjnZ5n0v/bna624PHccrwGX2wCcl/XE0R/VpYeOiY51ZV839utUTkRMuZbHxxPwCgLkYunLGkIuOSSnx7abDkCMeTHRr9wPPHH0++TthVBMrU1E7Uy5XwTUMdZVBaQC+vuispz2MaWxF2Ol0wCIatp4QUBAmykiVnK/1U9T9221L/tyWO+LiKhywv79+yXzRDe2b9+O5cuXmye3HUEQIElVVUFH6JTjFwQBU/smzJPbTtf8Hh4HAXWuQ3FtD7Yhgo24CFO3LjXPNijcvRKfxS3Y+fm3mmc1VD3ro5N1ze/piHt8J+qU52+tsD46G9uXmq1TzsFOOY7mEhETBtCTH2OHj41OOc865TiocwmCgA27w+bJbee6RVlea9Q0xnu9/IzP+YHIkO45X0gh0JcBxn3olwYRhIiYkEVY0v1ATEeMCcgiijTCkNRf/IgxCAM9yI/F4QEgxmLAoN229NMKSAX6ALU8hu1YrWteRr8vInKrHd4D9+7di3nzDgMAnHDC8ebZM7Z//4sAI4CJiGabndi2OYJLb70IV21+SPuVori2R4v0Ldy9El1rdxrW0kxuwtL5PehSPowOJiIiIqK2IWaRjjLaj4ioPkTEAimIuuhwQ/RiIYWALuJRm1dIIRBLyZGSSvSmPgLSENFu2kYxyFzed0q3nj4A3XZ7xSVMkZzGv23XtzsmHTGmK4sY00WoFpAKKFGfFnVg3ra7YzVHnBrrofP5EIkAGV2e+8JwBr7+frjL9i4im44iPBhGVJd23yxYbYdsMIzo+ATy5ukOqt4XERE7gImIZpkdD2HjyosQxFJcujKDbTvkycFbB+FbdyM2TO7E19d58YBlZPBOrF7yFL64bwJT+yYwtW8UKx640VUqaSIiIiKipgsOFqN5iIio9sYTGMAQJEmCJI3Al+hT0tqKiHkn0C9Jyrw8Ihl1HoB0BhiSII3F4RFjCGFEWU6CpEVIioh5M4jk1ekjQEiXUnc8gUxPXp6XTyI3oHSk2m7PJdv1yxyTIhiOIq0MkF3YA/ihjsOdx4R+THp9HVR9rOuR8CllHYkC0VqnrW993b0RIDOsdbIPZ3wIl9SBLt29PmW0mEU6GkYQQYT145oHBzGipI236uR3Tcwi7e+BV5tgUY5a7YuIiB3ARESziziawVXL5M7d4LIINo6qkb5LccM64PolMeTWfc76H0OTk8ghg0u0COBluP6xx/Hk0+YFiYiIiIiIiGj2iaJfS7MQRDg6jom83POZ03d2CV4kxpV5AODXdYQGw4imQ6XjsJZkcdBtHzDu29MNnxppabc9t+zWL3dMqqAaTVrAcAbo7/fJy4hZpH3dxTHp9XVQ7bGSNsb3elHtEA9bfMcVxYjaca+kWgYAMZtGVOkt1nfcA0BwUF6+f8Jbei44GpfHRBcECNmwYX925ah+X0RERuwAJiKaNXZi22Zg4yqlA3dVBtClgXblghvxKy0CWP7ceaF5ISIiIiIiIiIiHX8SeS1aVv5YR6cGMShJkKQhoE+wSdlciZluz2F9V8fkRY8/hz2FPCZ8YQS9PchlRUNnY814e+BPh+TOxlAOyTU13n6bUDtvK6tjEdk0kA4pnbWhNGCRBjo4KCGf1KeZzmGPYwetH8m8HCGezIUqSsldui8iosqwA5iIaLbY8RA2rhzUdd6O4vYLlDTQk5vw2XVePLBPTQVtXhnAggXwPTaKEat5RERERERERDTLpTGgG9t3IB2V0+96uuEbV1Mfu+VBfEzCiJqKNxhGND1QjIbUb98V0/YM1E5a+a9CagBp8yLm9V0fkwe9ESDTN4Bcj1deL5dFNudQ9iqPtTCcgW9E7Ywem71j3itR2yEXdaYRs0hH9am+80j65bYupAKGjtv8xDh83R4tMjuxvjizkBpQ0kibeRDvjyKtpuu2Yb8vIqLKsQOYiGiW0Kd/lr0VoUvOw8bRnRDvvAW+TesQVFNB36mmhtZbijt3LcN9S9QU0D3omr+u5NeQRERERERERDQbReGb8MoRlN4EfCPqeLlBDOYjyKipcAX7SNxCKqBbRkAI6ji2QQyO+IrpdL0ZRPLlx/O1356eB/H+4ra9ExEk/eXWd39Mnt4IMK7rNPSlkbZMTayq7lg93b5iBKtgGt92VgkiHAX8yTU2daZP3S0gJhrTP8s86I34kc6K8MT7AV296s+h4KAc2avO82YiyJeeYLLgGiS1MaBhWQ6nfRERVaolO4DFWPEm1y6DnRfLbMzLrz+WcikexFhn5fRvjXbcidUf39TxLzvi2mKH3NK7n9GmF+5eWeyoW1vs0LNefidWa516Pehq13rbsQ5d81daR7CaFO5eaaivThe8tTRds+fzmzF161LDPHWa+v87P//W4goLVmGnIQX0OpuX6dbRCu0srjVem51CjNXi/i4iZvOPZKofw5cY5V5QOoKImO4f1vovQvTvK3bT9ed5ZdPt9wsUkAqYp9lPt28z98ubv7wyH8PsobSLoc709yJTu2nv93b3K/3y5rHqYqXTLM8XpR1N7WNuV7syFFKB0vOuZF11H8X1i+s57d+uPizWabv7iVVdmevYrn2trz15VgoBl/cCq2uV6qyQQkBrA/N5bL5e7drZbrpV+1NrMl/rM2G/rdq8L7cy+2NvvFYqS/M9v3knrluU1T7f2PyyeZG6CSvjl5akQ/bEMWZIl6x0aHriGNONf+qJjxlSKkv6jQQHdfP0Ea5BDKrbM/3tuD09/bYH44iPuVjf7pjMlOWKnYYW2zGMDVvdsYrZNKJaBHDe1NnY6Yz1EhyUMKYbj7o4T03pXfwMBuXlzaeGJz6mtJNpHeOJjfiYbp6hHT2Ij+nbTv+3dTlKppsLRUQtxs2/KZun9TqAxRhCOXX8hBH4En0lX5i0HH2ZR3xI9CmNLcYQgpo6YgQItUajN0QhhWxPXj72fBJIrJ89x95ok5uwzTsqd8btuhFY9225rrWUvhOY2jeIqzbfJXeK2i0P0/iu/77K+OLZJsTRDK5a6bWJYCVqjuCtE8aO9A5h/AcVtY1CCn0JH0aU9xNDarFOph+fS/1HeSGFAe29M48kElgvOrzH2L2n2i1vt1+IiAl9QH8SSmCBwma6bZtVtrzxy6s8kn4/Ir2z9Rr2w6+2t6WoUn9SmfR5BaQCIUD9oi0fQUa3UTGbRjTqM6SFM55HEvon1kPUfXGUT/rhTyrnk/mLQNf88Ju/8CsMIwO/6ZxTldu/XX2oY5op51Qu1IadmE7ngql9tWO3ufYU4voMIsmocaLVvcDmWqX6Kgxn4OvXX1u681j/73nbdrabrsy1an+atRr3vlxAKmD+AQPNVhMDWdz8wzPwpd1hbNgdxobdF+P8Hz6OH/3WvCR1muCaJHJa9KgXCV+/w3ssERHVhtO/KZur5TqAC3ty8Ed6lX+MyXn0J/LmpVqLoczBMKLjE8hD+aVWlb/SMUSjqF+iFFIIBAIIWPxyvOV44hjUv2H4e+DVz28KU4SrIUpUjhTeoIuMXb1Dv54+za3+b4dtTm7C0rWbsOHjcjTthrX6bT6DDR93F6Va1oJVuFPtWFqwAD7kkZ8ECg+OAus+p/y6TU7re9+Dz9gu3xl2YtvmCC699SJctfkhrc300ZeFu1caoqENJjdhqa49OzFik5yudZuoedN5Ybg3GLa1DqJuWXM0viHa3rYMz8j3DMv9zVxplJEpIkkf9VJIIRBLFaNbzH8r2zNENCgRL+r2tHkW65rt0ZVN33dgeB5qv54zR+uUz7JBRYXhDKClwgpiTRLIzJ6fhZfhR4/X9B7j6YYP8nhgtu+pFb/3BDEojSFespD1dPs2q3R5w0LIIIJZ2/8LH/pdjMFVlrgeCSSxRn3l98Qxpr3/i8imowgPhhFNZ21/DBkctIkUmREfIhFju8udXv3wGZarJQ/iY+3YielwLhSGkdG3r8b62gOUDn70I95tnlHK1bXatkTEAimIuud7te8M1u8CpdsovgvI+05ZZuMqYDgD+V5vRf/vedt2tpteWftTY5W+B8vs3kHN55f+/LXbFiCfA9aZFlD23Cz/fmv37l5AKuBFYnxcThdrWlGMmfejrGd7jE7lVI9RPf6sbkbpNrX1LK5tg3qUZbb67VP44Q8W4Op/PRsnaROPwQf/dSk++BbDknVgjkylhjNHJFf5vTQREVXC4d+UKH3PKX3Hq5+W6wAGgHFTj29uj2W1tZTiYOxe9Jh+Biz/gzWEnO24AyaFFAa0yOE8kjn9lygRDKnTzb/qbzHaP9S9E+ivOnqhlpbiTn3q2l3LcF9cl+b4sVtwny4yNpd0kwK5zDY3jwIpOZr2umURbBxVO5R+hPuwDKEFuk3VwuQkchdUsF3z8o/dgnMsOq/axo6HsHHlRQhiKS5dmcE2peMseOsgfOtuxIbJnfj6Oi8eUNIbG+3E6iVP4Ytae45ixQM31qaTnlqL3bVuiJqfUNJg78TqJaNYsUs9LwaBVbofbzx2C55cJs97YGUGl6jnkDm63syuDDu+jevPGZSnb4oAKwdL0nZXzRBlpP5D0JRaKB9BRot6AZDOAEO6SCXz3wYiYt4J9GvbyyOS0WXxcFw3jQyGlDIkkVNfmAyZNKRiOi1xPRI+ZfpIFIhyTBxyYTwBr/lLRU8cQ5GMMt2LiX6LSM/CHuT8xY5Su/dU2/ceq/22AHF9whQBNwsFBzHis/uVrm48LqsvqhXGHwWYiFmko2EEEUQ4mkZW3Y+yX2+dz4nu3giQGVbKXsBwxgfDsGYVcVcf7fID3hJ250J+AuO6a9huXL+iAlIDwIjVQ6lF7wV1NZ7AgPp8N2T3quCdwe5dACJi3gwiWgT6CBDS/ZBtPIGMLjOD9m6BPCbGfdD++W4mZpEu+yMeOw7tT81l+R4M+3dQp3PUdlvKl3shYMSpA8zu3HT1fmv37u5BfEzO7JHMl3b4BMNRpNWHkPYDMIdjhEM5ISIWymlR8/meHNLanspcl7b/HqhHWWaxvQfw9PLT0WOeTkRERPVj929Km/ejRmm5DmBPfMgwcHoore9cbV3FTuo8JsaN84LK2BdD6EMgVSh+QWjX1e+JY6hnQKkDLxL67fm6lRdlD7rr9/P9mlCPW8r3YKBkLKUm2bGuGFm35Bb82DAzgi/qI2Mfe0r55XcZTtvUd65eWIxKLTw4ClzyQesvC6v2DDbER7Ei5TZ1s3l5fWe22mFqXqe1iaMZXLVM7twN6jvclQjo65fEkNOiok0mJ5FDBpdokZfLcP1jj+PJp80LUvuzvtaNUfOKHQ9h48qrcZ32o4qluHSl7ry44EbcoHTQer3n4f3q+gsWlImwsi5DPRmjjHT0v5r3JmB4hOk6vSz/1ivsQU7fQSDIUQhaJ4DTuoiiXx9tqWXSCCOaDlmMx0dUKf0XpsYhRvIT40B0BCNRWPxas4BUXwaRIfmLSqf3VOv3Hvv9NpcSmVpyQ5h9gmv0XyTr6VIel3xR7Y6YTSOqVLLhy3fd+dI/4a3fPc4TR7/6D1BxPRK+cOkzwLWZ10ersz0XosXOx5FoGgMOjVVI9SETsXjWtuy9oN50z3f9jwMqeWewexcQs0hH9WktzT8+sHm3KOxBrqSDV4maFAQI2XDV57h9+1Oz2b4HO50nNueo/bbSCHkn0O/U+QvY79Mtp3d3O8FiJorCcAaI9MLjcIwym3Karj1PvB9awvNy16XdvwfqURZSPIfva+MA72QKaCIiojqy/DelzftRo7RcB7B54PSRqJKKr4V5un0YV39dr//FsBiz/HW39gXhYFCXiqeAPTl5fiEVQJ/2S+k8klYDC7UTTxz9rRAJMLkJS1ehGN2360a837xMpSraphqV+gxGHgBWXFzb8UDFtctw3yW36DqqnDkvb+rkags7sW0zsHGV0oG7KgPo0kC7oh8DWfnULPqSyI0zz8b7N8eUcziP21dbRavXkBaloHZcWY9l55p+fEPlUxq5UAn1C/MhoE8oRl55e+BPK51woRySpbk5iRwUv4wspAIY6MlDGgwiOCghH8mgT/fuJsa8yESGdC/qLt5Tbd97zJ0TzVNIDbjPTNPplE7SvtQe8xxXPN2+kqhwmYhsGkirY7CF0oBFGujgoIR8HdP+qh3P+s7o+hKRTVtcF+3AxbngNad6MihgODOO8YRXa/PxhNfiR7+tcy9oKtfvDDbvAjWljgEsj2Nd0mSuuG1/ahuuz1FVFMlkDqFq29zN+23V7+5qJgo5BXpE7YWt+BjrqJXK0u7edizO/MEfMAEAOBWfVMYAvvxd5gWJiIioplz8m7LRWrADWEeMIZSz+YVgK9GlcRNCOSSVKBEEB5Vf9ctf/Hgn+jFmyisYXJNELqT8wtEn/xLA0xsB1H84Cn2Y8KH9viAQY4YxmJr2RdDkJJR+ddkFZ2u/9i48OGqKALbzNpx7QXGc3MLdd2GjfnYF2wwui2Bj8sYap3+Wxwz9mncUO9WIQgCei5fpUtDuxNfXqZ3O1ssbTG7C1zafh3PPNM9oYTsewsaVSurcfXIK59svUNJAa6l9HSKbFyyA77FRjFjNo1nBeM0oLrwIV22+yzC299c2R3BpnX4YUHhwFL5N6jm82eYHGtWRny3rS7801UXBFIYz7qIIrHi64Ruv19AEcqfbiJJCtTCcgW9E/XLIImUvOTKeCyLWJ3RfBM4GhRQGdO8l+s67vJbGRR6Hb6AnX/LuptG/p7p57zHttxKVtpnz8ua/KbgmCSQS1aWNVKIT9e0fi4nKr3z1aWvzSPqVe1gqYOhgyk+M1y/jkVK+UIMivsVYyPTr5vZSci54e+DXOu7lDj77tjL+QEQaicKflH9gYqC7Fzhfq51AFzFdSGFAPQ+remcwvgvI57ZuqCT99p04Rlx6EHcau8uRy/anprB9D7bjcI46bas7PoYRhCwDAcpx/X5b5bt7MBxFeqBPSf/sfIyODPdF+Udl2j1zRtdljcsym73lbHx0+STu+sxTeN48j4iIiOqq5N+UNu9HjdJ6HcD6AZFDwEiV6ZcaTYvqNb2oF6eXjsMCAPDEMWaer58mjWFwcEz+5aMnjjHdNoKDDv8oaLZgGFAjHuSGbHBZd2K1kpJZS7W8YBW+c8moNsbtOXkvrjKvZumtuC7hxfVL1PWW4fYLlFmVbvPCi3DVY4/XNv3zjm/j+seAH69bpqWiXnr3M8CCVfjiSjWlcQy5dUq0r83yhbtXGlJZ+zbVtvOp3vTpn2VvReiS87BxdCfEO2+Bb9M6BNVU0HeqqaH1luLOXctwn9LO8med5T/sW5/cyV88Dt2YtWTPcM30oGvtTvm82FS8/ruWjGLFrnV1i5rznO0tRrHP70HXx92MRe6SJ47+qC61Wkw0jX8qwDvhm0HatCAG8xFk1BSKwsyjdAqpgG5bAkKQx0LzdPuKUXVCufEoqYThXAghl9RHuHYmw7nkTcCnvJeUpHTOJTEU98jpcsdRjORSx+y0e0+1ee+x2y8gIqZMU8cXlTsEbabbtlmly0PJVtMGP7BsJE8cQyUpd/SpKNX2MU+PQUQQg3n1B50CBGEAPWuCFhG3HvRG/EhnRXji/brzpXhvc89cBidBhKOAf8YR33b1oUudqxyL5b952oX5XPDEMZTMKcfuRcKntpXNtWfD9l7gdK12hCh86g+ivQn4RtTUuO7fGezeBYAgBkd8xfPPm0EkXy71LgB40ePPQRvBySy4BkmoHVF27Ww3nVqW1XuwI4dztMy2goPVpXl39X7r+O7ugRxLUFomQPnycXxcTv8sT7A/RieG+6KAPvTrstZVe13WoyyzW09/GFd3/w9u1tI/P4gtOAPveIt5ydZRSAUMP54w/12RQgoB3TUkxpR3+YrIPwgtnpMWQ3aIMevp6rol17H1dMOzzur6nQFzPZr/rs5M6qa+tGEX1X+/uWFTVnNdmf+mSomI2dzbq7tGqf7s26zxWqksZZj/TWnzftQowv79+yXzRDe2b9+O5cuXmye3HUEQIElVVUFH6JTjFwQBU/vkBDetbSdWz78L5+6y7lztmt/TJsfhrFOOo5lmVofPYMPHbwRS1ueZe7XazszNrD7ah7i2B9uWqanHZ17/XfN7OuIebybGBGTDalq4AlKBPmCo0T80mplOef7WCuujs7F9qdk65Rxsr+MQEROyCJcdD7Xx1CGXbDM8zHLtdZ7Za7fj6IT3W6qMIAjYsDtsntx2rluUrcm1Zr43m/+2V3q9FFIBrO9WgmmqZtquGIMw0IO8LlBJjAnIIoo0wrofwImICQPoGYkgMwAMacvbTC+kENDGD1eWydfu2jfXo/lve6X1ajvPdd3UnuFeX0ghNtyLwbjHVK/O7Mpqrivz363Dqa1aSeu+Gxq1Yn02q0yt1GaVlaUd3gP37t2LefMOAwCccMLx5tkztn//i0BLRgATdbIdD2Hjyqur7swhmhklMt4mMtgQBb52EzZ8fBmuf+xxOfp1rRI1PbkJS3XbWL1DWXlyE5au3SRHHn98Ezas1c3DM9jwcUYhuxFcfSNyWgTwMlx/Du8XVorDJwiGIRSIiIiIyvH0RoDMcGl0JVET8f2WOoOIWCAFURfRWozqU7InOEWNOtFn4tG2W0Aq4EViXMlIEhMhD9kAw7ArxshNuYwpXaSoq6DbYBhRwxACIrLpKMKDYUR1qcjlsevHEC8Z9sV6emE4A2iZWoJYkwQyJfnQW6FeHbiumzrzxOXOX0BOLQ+HjB+aGpXVVI/FKnNqu9L1tHmFFAKxlC5i3K6dbdrKrjwl2zVGTVtnX7DbtzLP6XoSY8X1YlndDKNKrlHr8lZZz8q+i2VMNbk+rda3aWPd8sVJBaQCyvZsj9m5fh3brIJ6MKhHWcg1dgATNdKF6zB1qz5NMVG9KB23hlTWS3GnNkbyBKZ2LcN9cSXFsDZOsjLv1lW47t9HcfsF5+H2XRPKebsTq5eMYsUudRuDwCpdx+7mUSA1gal/X4XrlkWwcVTtNP5Rjce97mALVmGnvo14v7BmGCrBZogFIiIiaqIgBl3+Qr/hPHGMtclQUzSL8P2WOsV4AgMYUs5lfUr0IAb153g+gkyfRUeBJREx7wT6tfXziGT6kCp4EB/LI+n3I5lXr5s8JsZ96Ha6yY8nkOnJK+VIIudm7Hcxi7RuDG6IWaSjYQQRRFgdn76eml6vDppdN1YKe5BzM+xNTcoqIubNIJJX63EECOk69Wzbzq7+lfXSGWBIgjQWh8e2na3aqkx59NsVY/IQLtq2rd7d7PatsL2eRMRCOblckoR8T879OO1223QqbzX1XEihL+HDiDpvMN7c+rRc36qNdVsLR5FWT9zCMDKIoNfjcMxwqF/HNqugHrR11PVqXRaqBDuAiYg6ktJxu28CU/t0Y9buWFeM8l1yC36sTC48OAqs+5zFi4lOSQT7Uly68nE8+bTy5wW6Tt4LL8JVmx+CqG67luNeExEREREREVELiqJfC18PIhwdx4QaGqqP5vImMK5by1FhD3LQjb0tyNFw2nbNy+o7Iy3pyujphs8QvaqnRNwJAoRs2NCxIWbTiIaVuF19B0zdNLleS7RS3ZgVkOrLIDJk7ogqVZOyilmko/qsDab2sWu7cvVv7sB2287lyqPfbjCMaDpUEoVawnHfNteTqRyeeL9u3PpybLbpWN7K69kYgW+jkfXpdn29YDF6vTCcASK98Dgcs8ymfp3arJJ60KtHWagi7AAmIpotJjdh6SoUo3x33Yj3m5epmaW4dGUG23Y8g5EHgBUXv9W8ABERERERERHNBoUUAiEUI+3ySfjNyzjxJ5HXR81J6pjZ9aRE3El5JHMhQ1rfbBpIq2nbQ2lgJumDZ6Jp9dq6dSPGvMhEhlyk0W9+WV3X/0zb2ZYajToE9AnWKYvrtu9quCivFbf1PGMuyudYny7WL6FGr8vp7yNqL2zDjtmFVirLLMQOYCKi2eSCs7VfwhYeHNUigD0XLwPWfdv5xeLCi3DV5ruKKZ8nN+FrmyO49ELTcorgsgg2Jm9k+mciIiIiIiKiWSGNATV0rZDCQDoKJcAS0EXmFoYz9hGMZp5u+MYzKBka14pjRG+1PIj3R5HW0tBmkY7q07TmkfRXlz7Y0xsBEuu1cUzXJ3QdOAZNrldb9aubyhWQCggY6MljrHzvb+3KGgwjmh4oRmya28eu7Sqtf7ftXLY8VjyIj0kYsUuD7Xbfet4e+HUd6oXUQA1T+FqVt/J6Nl5/NppSn2XWNwmGo0gP9Cnpn52P2ZFTm1VVD3UqC1WEHcBERLPFglX4ziWjOEdJAX1O3ourdPO+uDKDS9T00Gt3AngrQpdAHkt47U55DOFN3uLYwktGsWKXLr202YUX4arHHmf6ZyIiIiIiIqJZIQrfhFdLbeobUcbA9MQxFMnAq6QB9U74KkjnGcRgPoKMmnJY0EfGedAbgZyOOCYC8KLHn8OeSjsbygmuQRJyJ4Y+bbDMg96IX0kfLCKmpnUdT8ArCEp0rM10Txz9UTU9agi5pF3karPr1YHruqkzcT0S48B4QqknQUAgVZAjLi1S6taurEEMjviKKbG9GUTy+rFfbdrOsf5NHNvZ3FblylNUSAV0+xYQwkhpZKbjvh144hhK5rTUv33oR3KGocPO5a2ing3Xn1p/zatP+/XNZTIJhhEdH5fTP8sT7I/ZiWObua8Ho3qUhSoh7N+/XzJPdGP79u1Yvny5eXLbEQQBklRVFXSETjl+QRAwtW/CPLntdM3v4XEQ0DF1uBOr59+Fc3dt1o0bXJ3OqI/G65rf0xH3+E7UKc/fWmF9dDa2LzVbp5yDnXIcboixCiJ4bImICVmEJTdfTs1cbcrcfJ1ynpmPoznt06hzsFH7oVoSBAEbdofNk9vOdYuyumutNc7FQiqAPgw1+Hqvp9ao11Zkvte3HrZdY7Ceyaj17w3A3r17MW/eYQCAE0443jx7xvbvfxFgBDAREdXNjoewceXVM+78JSIiIqLZJTgoteAX9wWkAqURRKrWLDOp3LePczsTUevz9EaAzLCckpiIiGgWYwcwERHVx4XrMHXrUvNUIiIiIuowhpR1MV0KTO2j61ArpBCIpZAKCBACKRTMfyvbC+h74AopBHTb0+ZZrGtJjBnTzdltDyJigRRE3fHI8wpIBbxIjI/bpt8zllneTipW3IfFKtRA7trHop2tzjHT+WNoWzGmuxay+hmIGVIeGv8uvYZK92O4Jmz3Q9RMQQy2QgSeJ46xsXgHDUXVIvVKVWDbNQbrmcgOO4CJiIiIiIiIqDqFFPoSPoxIEiRJgjQYVL6IU/6WJEj5CDJ9ug7adAYYkiCpX9Cb/zYQEfNOoF/bXh6RTF+xQ9lxXaUTLQSMaF8MltneeAIDGFLmjcCX6EOq4EF8LI+k349kXj3GMsYTyPTkleNPIjfg0EFNjWfZPjbtbDjHRMS8GUTy6vkzAoTUHziIiIVy8rqShHxPDmnTbi1ZXkNO52mV+yEiIiKiWYUdwERERERERERUlcJwBkiuKY260EcoehMY18/zR9Cr7601/61X2IMc0ghpkZByhOZEXpnvtC7SCHkn0K+PCim3PUTRr6UKDiIc1c+rhG47nm74xidQ1WaoTipoH/05JmaRjvajmE1ad46Y5nni/YiqizmwvIacztMq90NEREREsws7gImIiIiIiIiodrSoWzUCOAm/eZlK+JPIa5GQ8sdNEC4QRTKZQ8icf7nq7RE1EM9TIiIiIpoBdgATERERERERUVU8vREgsV43tqnC3wOv8r+F4YwxArgSnm74xjMYrjJ/cnd8DCMIFcdPLbu9NAZ0YwwPpKMIs9ONVMEwoukBw5jW2jni7YE/ndWN6zugS83sRY8/hz3aqVWcZ3kNOZ2njvshIiIiIpKxA5iIiIiIiIiIquOJoz+qS1UbEwFPHEORDLzKNO+EbwYpaoMYzEeQ8aqpcAUIQqy0w9lBcFAdyxcutheFb8Krpa72jajpoz3ojQAJr3KM1KHKtXMQgyM+eb4gQPBmEMkr54gnjqFkTrsW+tCPpBb67kG8v7iedyJSnGd1DTmdp477IWq2AlIBAULAPO653XQla4QgFH+oU2dirBb7EhGr8FlUkUIKAau6orqpzXlhVufzhIioDGH//v2SeaIb27dvx/Lly82T244gCJCkqqqgI3TK8QuCgKl9E+bJbadrfg+PgwDWYQnWR3W65vd0xD2+E3XK87dWWB+dje1LzdYp52CnHEdrExETsgjrxwyeZTrlPOuU46DOJQgCNuwOmye3nesWZXXXmoiYMICekQgyA8DQWBzyUNV205W1YgHs6fEhgzUYKw6w3eJq/bwoIBXoA4bGtPG9xVgAe9YU/6ZSxnt9aR02X63PEyJyox3eA/fu3Yt58w4DAJxwwvHm2TO2f/+LACOAiYiIiIiIiIiIiGhmghiUxhBX8/+XnQ5AjCGEfsS7zTOKCqlAMRI+Jiqdavro+IAhLXsglipGG5v/VrZniPRUIpDV7WnzLNa1JMaMmSTstgcRsUAKou545HkFpAJeJMbHDdkHvD1AxjIPPJWyqMOS9nM4b0rOC7mtUrHi8oakELZtrJ4P6vma1a1ERGQmKZ96kLfNDmAiIiIiIiIiIgQxyCgdIqIGKSA1AIwMOtx1Cyn0JXwYkSRIkgRpMKjcq5W/JQlSPoJMn66DNp0BhiRIaqSx+W8DETHvBPq17eURyahDBpRbV+kIDAEj2rOjzPbGExjAkDJPHZ7Ag/hYHkm/H8m8eozK+OCZYfuOZ9KxrkNj+5U5b8zGE8j05JVlk8gNqMs6tbGIWCgnl0GSkO/JcYx2ImoqdgATERERERERERERUcMUUn3IRNY4/uimMJwBkhbL6KMsvQmM6+f5I+jV99aa/9Yr7EEOujG4BTmKdCKvzHdaF2mEvBPo1/9wqNz2EEW/lp84iHBUP49qztx+TudNCV1bebrhG59AHmXaWMwiHe3XUlB74v2I6jdJRNRg7AAmIiIiIiIiIiIiogYpYDgzjvGEV+5EC6Xl/zfk2bWhRd2qkZxJ+M3LVMKfRF4fGSpJcApKLooimcwhZC5z1dujuqrlecM2JqI2wQ5gIiIiIiIiIiIiImoQD+Jjug60kSj8yXwxda+6VG8ESKwvjq+r8vdAHVK4MJwpE8npwNMN33gG1Q612x0fwwhCxTFgy24vjQHdGMMD6SjC7DhsnFqcN05t7O2BP53VztdCaoApoInIXv2HAGYHMBERERERERERERHNhIiYmlp3PAGvIEAOjrWb7oInjv6oLt1uTAQ8cQxFMvAq07wTvhmk2Q1iMB9Bxqum8xUgCLHSDmcHwUF1LF+42F4Uvgkl6tmbgG9ETR/tQW8ESHiVY1TTX0d6rcceJguldWicXavzxqGNPXEMJXPa+dqHfiTVMONCCgEhUBwPmoioAYT9+/dX1ce8fft2LF++3Dy57QiCAEmqqgo6QqccvyAImNo3YZ7cdrrm9/A4CGAdlmB9VKdrfk9H3OM7Uac8f2uF9dHZ2L7UbJ1yDrbPcRSQCniR0MJq/Ejmx7Tx8ABlDL5QrnS6ui6SyI/FdV96W08vpALwqjuKjpREjs1EIRVAH4YwphTQ/LdrhRQCfcCQ4XhaV/ucZ8465TiocwmCgA27w+bJbee6RVlea66JiAlZhPVjBjsQYwHsWWN+TpIe7/VEZKUd7g179+7FvK55AIAT3nSCefaM7f/zfoApoImIiIiIiIiotvxI5tW0nj4k+lLQB7yI2TSiUR8S6/UROiJiQh/Qbx6Tz2Z6IYW+hE8Zy28E0fRAi0TVFJAK6CJ8PHH0+2xSRRIREVkppDCQi6CXnb9ERDQD7AAmIiIiIiIiovoIhhEdn0BemyAim44iPBhGVDdOHhDEoDSGuDo4X5npheEMkFyjRFEFsSYJZEp6WUXEAimIqYCWplEbp1FNSap9KkzLWEghoFtf3q4a/TxuSEHp7bEqGxERzS5BDLqM/oUnjrE2yRxBREStix3ARERERERERFQfYhZpfw+0/lsxi3Q0jCCCCEfTyFoM01dT4wkMYEiORpZM4zRKSpSyJEHKR5AxRSrbExHzTqBfWz+PSKYPqYIH8bE8kn4lAlpJSe3pjQCZYZfbJiIiIiIimjl2ABMRERERERFRDSkRsIIAIRuGpItiErNpRMNK3G44inTde4Cj6NcGUAwiHB3HhBqOLMaKEcDeBLRhi8sp7EEOaYS0CGA56lfbLhERERERUZOxA5iIiIiIiIiIakgdAziPZC4EJROykv4ZSIeUjtNQGjCkgW6gQgqBEJQxhCVIefPYw2X4k8jrI4glCUrALxERERERUdOxA5iIiIiIiIiI6sCDeH8U6QEltbKYRTo6ous0zSPpry4NtKc3AiTWK53HItYngEiv1WiJaQyog/sWUhhIR6EEIAO61NSF4Yz7CGBPN3zjGXBYXyIiIiIialWWHcA/3XA/furwNxERERERERFRWcE1SELuLNWnf5Z50BvxK2mgRcTUVMzjCXgFQYkctpnuiaM/qqZhDiGXHIKW6dkgCt+EV0vz7BsZRBDy+kORDLxKGmfvhA9R86q2ghjMR5BR01wLAgQhpnRGe9AbgZwCWwl9LgxngEivlgabiIiIiIio3oT9+/dLxT9/h/s3fANjz7wVkX++Du8p+bto+/btWL58uW5KexIEAZKkq4JZplOOXxAETO2bME9uO13ze3gcBLAOS7A+qtM1v6cj7vGdqFOev7XC+uhsbF9qtk45BzvlOBpLREzIIiwpnb5NIsYC2LNmzKaDurV0ynnWKcdBnUsQBGzYHTZPbjvXLcryWqOm4b2eiKy0w71h7969mNc1DwBwwptOMM+esf1/3g9YRQC/57p/RuSt9n8TEREREREREZELhRQGchFYZqcmIiIiIiKqE1MH8JvxZse/iYiIiIiIiIjaQRCDTY7+hSeOsbE40z8TEREREVFDlUQAExERERERERERERERERFRe2IHMBERERERERERERERERFRh7DsAH7PddfhPQ5/ExERERERERERERERERFR67HsACYiIiIiIiIiIiIiIiIiovYjvPjii9KhQ4cwPT1d0eeXv/wlVqxYYd4eERERERERERERERERERGZTE5OYl7XPADACW86wTx7xvb/eT8AQNi/f79knunG9u3bsXz5cvPktiMIAiSpqiroCJ1y/IIgYGrfhHly2+ma38PjIIB1WIL1UZ2u+T0dcY/vRJ3y/K0V1kdnY/tSs3XKOdgpx0GtrVPOs045DupcgiBgw+6weXLbuW5RltcaNQ3v9URkpR3uDXv37m1IBzBTQBMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERNYKgfOpB2TY7gImIiIiIiIiIiIiIiIiIOgQ7gImIiIiIiIiIiIiIiIiIOgQ7gImIiIiIiIioQgWkAgIEQfkEUijYzRMCSBVn1pCImBCDaJ5cI2JMQMCx4PXdPxEREVVCef8wvJOUIcas31PEmPIOU+vnfOe/P82cc/nKv581gohYSftB14Zq+d0uZ1K3888NnqOdhB3ARERERERERFSBAlIBLzKRPCRJgiRJyEcy8Bq+IPIjmZfnSSM+JPrMX3y1mgJSAeOXWMFBCWNxj34hIiIiakkiYkIf0J+E3zzLgZhNIxr1IbHe2NUkZtOIjkiQpEEELd4RqtOJ70+weIcy/11bjXs/K3ccfviRwbB+fmEYGfhN56Db5YqM518jdeo5OnuxA5iIiIiIiIiI3BPXI4EkhnRfvnniQ0iav9xSBcOIjk8gb54OoJAKFKMIYsqXr4UUAlpkgQB1MqCPiBAgxLK6GaXr2UWHiDF95EIMovJlV2J8HAlvsRyFVMCwDcuyqsSYMUrDriyFFAKxVOURSkREROQgiEFpDHGveboTEdl0FOHBMKLprPYMF2MCQmkgHRIgxFKW7whVPefb+v1JiWTVPmrHqPkdyqq+7NaVWR4LgD266fpjMb6fiYgFUkjp3u2Ky5qjVU11AjiUzXxcJSsC8CESATK6xisMZ+Dr74evquVkxvOvTNuWnG8Ox+ymndv6HCUr7AAmIiIiIiIiItcKe3KArxvG2AsPun3jmLD6BkjMIu3vQcl3soUU+hI+jCgRBtJgUP4izptBRI0skEaAkPplnIhYKKdFHeR7ckhrGxMR806gX92WlEck01catSHGEMKIFtUgR1Z4EB/LI+lXIhoGLWItLMtanBcIASNalEaZsqQzwJAEaSxuqkMiIiJqGDGLdDSMIIIIR9PIKp1RwUEJI1HIEZiDcYt3hOqe8239/oQgBrVlJEj5CDJ9KRRK3qGs6stuXbtjAYA0MhhSlk8iN+Dwo7nxBDI9SsSqfllxPRI+5Z1PblCUvuLZlc18XCUrAgC6eyNAZlgpWwHDGR/CFou6XQ4l51+5tjWdb7bH7K6d2/scJSvsACYiIiIiIiKiGlMiJgQBQjZc8iUoIEc/ILnGmNpOzCId7Ucx8CCIcFT50sk0zxPvR1RdrLAHOaQR0qID5KiNki+rgmFE06GS6JNyLMsKAEgj5J1Avz5FX7my+CPoNVcGERERNZSYTSOq9MIFw1Gk1R7gcur6nG/R9yfAGKHpTWDcPN+JzbqWxwIAiKJfK3A3fDZRprJKlrVgUzZXPHH0+xJYL6odzmGLY6lgOStObQuX51sl7VxWC5+jVIIdwERERERERETkmqfbB+T2mCIxRGTTfvRoIQDq+GB5JHMhi5R7deBPIq+P4pAkh0iPIaBPMKZtrkoUyWQOIfMBuioLERERNYeIrJpmVxAghNKALg10WVU859v6/UnLdqIsk69grOWZrDsT3h740yGlfXNIrjEfVG3Kpv54QP+DAitul5sRp2N20c5tfY6SJXYAExEREREREZF7wTCi40oUg0KMhUy/6ld5EO+PIm2Rus/TGwES641ftgbDiKYHitG5hRQG0lE5TZ63B37dl7OF1EAxPZynG75xm/HJLHkQH5Mwokv56MSyrIru+BhGECqOR1ZxWYiIiKihxCzSUf2QEHkk/e7eCap+zrf7+5Mu1W9hOFNZpKzNupbHUiOF4Qx8I2r7jlnUscKmbK4p2WVCan3bcbucmVPbmtges9t2bvdzlEqwA5iIiIiIiIiIKhDEoDQCqFEzgoBQGvaRM8E1SMLiixtPHP1RXUq3mChve8RXTC3nzSCSV9Ire+IYSua05fvQj6QWphHEYD6CjLqeYB3dW0gFdPMFhKCOjeZBbwTyfq1CGSzLWhQcHIEvoY5H5q4sREREVCsiYoKSwnc8Aa8gyJGJhRQCFsM+lEZhetAb8dukgTa/I1T7nG/f9yd44hiKZOBVlvFO+Iopekvqx/S307qWx1Ibnm5fMcJbECAESjsqHctmPg5bQYSjgN+c8riE2+XMHNrWxP6YXbZzO5+jZEnYv3+/ZJ7oxvbt27F8+XLz5LYjCAIkqaoq6AidcvyCIGBq34R5ctvpmt/D4yCAdViC9VGdrvk9HXGP70Sd8vytFdZHZ2P7UrN1yjnYFsdRSCHgzSCSd4iyoJbWFueZC6XHUUAq4EVCDevxJ5HXxqwzzYMfybqcwyJiQhZh/XjRbUCMCRjoyWOs9hUyA+1Zl3qCIGDD7rB5ctu5blG2I+4Z1J5K7/Vtiu9PdSHGBGTDaqrgAlKBPmCos+u4bsfcZudoO9wb9u7di3ld8wAAJ7zpBPPsGdv/5/0AI4CJiIiIiIiIqCY8cYw5pdgjagq5gzcTySspESXkIxl4DZFA6nh2EqQRHxJ9FlFCs1RwUGqxzt9GKCAVKI0YJCKqC74/1UVwTRI5LZLVi4TPKo1xZ6nbMfMcbVvsACYiIiIiIiIios4krkcCSQzpvrX0xIesUxYCyvh3E8ibp5tTiKvpIAspBLSUhErKUZUY0y2f1c0oXU8bQ9pEjFmnPCwti5L+VPvoOzBFxAIppHTbKpbTaZ68n2LZnJYtIBXQ799UF8AMylimLjXyNkRd3RjKbrfvQgqBWEoufyCGWMCLxPi4i7SfRETUsjxxjGljPEuQ5LDYzjYbj7mNCcqnHtRtswOYiIiIiIiIiIg6UmFPDvB1K+meVR50+8YxYdXLK2aR9vfAa55eSKEv4cOI4UtVETFvBhE1elgaAUJqx6KIWCinRRbne3JIaxsTEfNOoF/7kjaPSEYdQ1pHjCGEkeIXuWrKY8uyBDGo/9I3H0FGH8k8nkCmR4mCzieRG3A5z8xuWXE9Ej6lrCNRIKqOr61XbRmd6tJkPIEBDGntYRib22nf6QwwJEEaG8TgWB5JvxIVXnoQRERERG2BHcBERERERERERDSLKdGeggAhG4akjQ9cVBjOAMk1xjFnxSzSUX16xSDCUaVj2TTPE+9HVF2ssAc5pBHSolHliNOSDulgGNF0yBQpa1MWmKJkvQlowxoDAKLo1wrTDZ8hytlpnlkly1qopoxOdVlCtw19e6DMvv0R9JobnYiIiKiNsQOYiIiIiIiIiIg6kqfbB+T2mCJaRWTTfvRoYb7qGMB5JHMhi9TFdeBPIq+PSJUkh4jZIaBPMKSALlFIIRBCMSo4n4TfvEw9eXvgT4fkztVQDsk1JQfT3DI2c99ERERETcAOYCIiIiIiIiIi6kzBMKLjCazX9ZyKsZApclflQbw/irRFCmRPbwRIrDd2wAbDiKYHDGPJDqSjCAfVDtGsbszegWLaYk83fOM2YxBb8iA+JmEkmkZWtCkLAOhSVxeGM6bo2voqDGfgG1E7s8cs6lZRTRmd6rJEGgNqg+jbA1Xum4iIiKhNsQOYiGi22bEOXfNXYsOkeUapwt0rsfTuZ8yTiYiIiIg6TiEVQKBkEFZqf0EMSiNASE23LCCUBqDrUDQIrkESFp2znjj6o7q0zTFR3vaIr5g+2ptBJK+M0+uJYyiZ05bvQz+SWshpEIP5CDLqeoJ1dG8hFdDNFxCCMq6uVVk8cQxFMvAq07wTPoc0ybXn6fYhratjIVDaiV51GR3r0iwK34RXaY8EfCO69nC9bw96I5DbtSHh4J1DjBXPAeP9tIBUwOa8sCQiprsmxJh5e9bcLjdzxvIRoQ7nX623506jzu1G7YdodhP2798vmSe6sX37dixfvtw8ue0IggBJqqoKOkKnHL8gCJjaN2Ge3Ha65vfwOAiocx2Ka3uwDRFsxEWYunWpebZB4e6V+Cxuwc7Pv9U8q6HqWR+drGt+T0fc4ztRpzx/a4X10dnYvtRsnXIOdspxtLJCKoA+DGHMNnSx83XKeebqOAopBLwZRPIO0arkmhgTkA2raawLSAX6gKFG162ImJBFWFI6fVuYIAjYsDtsntx2rluULV5rhRRiw70YjHuU62sC/dIgghAREwbQMxJBZgAYshhju1Qt2rKe52Etykcz5epePyvU8lxv1LndqP3QbNQO94a9e/fisK55AIDj33SCefaMvfjn/QAjgImIZpud2LY5gktvvQhXbX6o+GvatT1apG/h7pXoWrvTsJZmchOWzu9Bl/JhdDARERERzZQYE4pjrooxXYRYAalAQE6vW0ghEEsZI8gKKQR00ZHFQD0RsUAKKV0kWnGeEoVmuV6RoUz6clDn8MQx5pSqmCoSXJNETosA9iLhs0qxTR3NE5c7f1Vayu0gBqUxxLUxt22IseK9OZY1zDJmaLC/jxeXKyAV8CIxPm4byW2IsC9uwOa54lw+83qNj9okKM/u4nlRjC4tbWsRMV17CYL+Ge/0DuE0z3yeOi1rfw7ruduexble0TuT07ltjtI1/l1ar6X7MVwLtvshonphBzAR0Wyy4yFsXHkRgliKS1dmsG2HPDl46yB8627Ehsmd+Po6Lx6wjAzeidVLnsIX901gat8EpvaNYsUDN7pKJU1EREREZCcYjiKdlb84LOwB/Fr63TwmEEGv2p+QzgBDEqSxODwQEfNmEMmrY46OACHdF7jjCWR68vK8fBI5dUxXcT0SvhF5+kgUiCopdU30ZUJhGBl9OYiolCeOMUm9HiVIVhdW3QUxyGiyptI64LwT6HcV6asSEQvlkFTu6fmenP04z67u4x7Ex/JI+v3yNs0LFFLoS/gwYjhfnZ4rTuUTEfNOoF87//OIZPr4o6FGE2MIQTkvJAmSei+wbOsgBvX3q3wEmT5denK7d4hy88zslnV1Dluw3J7Nue76ncnp3HZgWa9O10KV+yGiGWEHMBHRLCKOZnDVMrlzN7gsgo2jaqTvUtywDrh+SQy5dZ+z/gfz5CRyyOASLQJ4Ga5/7HE8+bR5QSIiIiKiCgTDiKazEFHAcAbo7/dhIg9AzCLt6y52IPh1nbBiFumoPsIwiHB0XF4PABBFvzrT0w3f+AS0WW5oZQIKwxkg0ltBRwYR0ewUHFQ71HowYIiqLMN0T/fE+x3GaJ65wnAGSK4xfvfh9FxxKl9hD3LQjcktyNGYxecRNUQwjGg6ZIrmtWlryB3GWjSqN4Fxw0yndwineWaVLOtGBdtz+87kdG47sKxXp2uhyv0Q0cywA5iIaNbYiW2bgY2rlA7cVRlAlwbalQtuxK+0CGD5c+eF5oWIiIiIiCrhRY8/hz2FPCZ8YQS9PchlRYjZNKLhkq9sZ8bbA386JH8xGcohucZu+0GEo2lkRblTOsLwXyIi9zxx9Bt+lFNDru/jDeRPIq+PKJXU8bCpcdSo3iGgTzCkgC5RSCEQQjF6NZ+E37xMPbXiOVwrvBaIWgo7gImIZosdD2HjykFd5+0obr9ASQM9uQmfXefFA/vUVNDmlQEsWADfY6MYsZpHRERERFQ1D3ojQKZvALkerxzVkssim4vCtv83GEY0PVCM8imkMJB2WF5RGM7AN6J+Kek8/mswHEV6oI/pn4mI3BBjhrFSs2k/esqN+6vy9sCvZF0AgEJqwDY9bCX3cTue3giQWG/sIHR6rjiVz9MN37g6dAE1nwfxMQkj0TSyok1bQz9GtXxOGSOA66sW53BFqj23tR/olc6zrFena8FxP0RUL+wAJiKaJfTpn2VvReiS87BxdCfEO2+Bb9M6BNVU0HeqqaH1luLOXctw3xI1BXQPuuavK32JJiIiIiKqkKc3AoyPw9ftkaNvfWmkfeHSlI2aIAZHfEh41fSNGUTy5cf+9HT7kA6pqQkFCAGHsfuCYUTHx5n+mYjIjWAY0O6vIWBE7dgSEVPT7I4n4BUEXUexwhPHUDKnpY7tQz+SNiGZ7u/j8o+LEl4BgnmHnjj6o7pUtTHR+bniWL4gBvMRZNT1hDLRp1QXhVRAV/8CQlDG1bVqa08cQ5EMvMo074SvoemI3Z/Dbjmc68AMzm0P4v3F9bwTkeI8q3p1uhYc90NE9SLs379fMk90Y/v27Vi+fLl58gwUkAp4kUAS+bG49o+rQioAb0L5DU50pDiQeY0IggBJqqoKDMSYgFAaAPxI5ou/3ClOB6IjzikPxFgAe9Y04Fc/OrU6fiv6Y/cn8xir44EJgoCpfRPmyQB2YvXHJ3HDv69qi3+wd83vsTkOZ+LaHlyyWf7/968bxc7PvxUAULh7Jc5Z97g8Y+Ugpm6VO/+sl9+J1fNj2ChPllP9Vllv1R5HTexYh65Vedy+azOuW2CeaVS4eyU+i1u0+molTa3DFjST+miFdhbX9uBr3uK12Shd83sM9/hG3peh7G+gp8b7EWNyiiTds7Yd1fP560a9368qVf/6EBETQsVfGPvV90276fbXSz2m6/dr3Tb25azsHdppO/VT//athlIXJXWg1Od4FCPSIIKul9NT56l/G/99MFN1ubeWEBETsgiXHJuTatZpDOtzsJK2tb7OjNdUsZ2trnvDNamwnOdwT7Y+DqqUGBOQDav/Ni8gFegDhuyuURExYQA9NbyGW12nnGftexzO99LGPAOaxfnYO40gCNiwO2yeXDPPb96Jm9e/oP195pqL8XcrjzEsUwvXLco2/Fqr7D5Onaxd7/U8h4nqq7H3Bqt/V5Z/p9m7dy8O65oHADj+TSeYZ8/Yi3/eD7ROBLCImNAH9Jvy7RdS6Ev4lHz8I8ZUBa1EjCGUU/Lbj/iQ6FN+tSPGEMKIks5hBAjNol9/FVLI9uTlY88nS1NCUO1MbsI276ic0nfXjcC6b8t1raX0ncDUvkFctfkuOa2v3fIwje9aZedvs4mjGVy10msTwUrUHMFbJxre+VtC/6ySJPRPqPflAlKBQF2er8FBqeZfTonZNKJRHxLr+VSpWru8X9WafiwifQeO1XS79xjDdTQCX6JPrju75R2mD2jbySOJBNaLZdrGqpzVvENbbme28sMPU4qywjAy8JvGAHO7nJ4fyXx90rrV497qTv2eF83jpm1trjMUkJIHjzO2s81174mPKcsp173fL48p63S9Ul0E1ySR06JuvEj4+u2vUTGLdNRhPlFFZn4fbcwzYCblnMm61Wj0/trDxEAWN//wDHxpdxgbdoexYffFOP+Hj+NHvzUv2Z4quo8TtSCew0Sdxg+/+r1Oi2mRDuAgBqUxxE3jQhSGM0ByjdJLHsSaJJCxTCLfXIU9OfjVlFDBMKLjE8gDQHDQ9tfb5YgxXaoENXVDIYVAIIBAzdJD1JEnjkH9k0s3rkLz7MRqLW1tD7rmr9SNc7oTqz++CRvWFuev3qFfT5/mVv+3wzYnN2Hp2k3Y8PEedCnbLm7zGWz4uH7/M7BgFe5UO5YWLIAPeeQngcKDo8C6zynXj5zW974Hn7FdvjPsxLbNEVx660W4avNDWpuJa3uw9O5nAMjRoF1rbTqHJzdhqa491XWokzhd68r5oZ4D6nliOi8M9wbDttZB1C2rP38Kd6/U/W1ez3xv0N9TjOWrpeDgIIJalNO4MVVQIVV81ggCAvpvVOzmFVIIxFJIBYrPp0IqoFtXRCyQQkr3fCtmJirI6+m2a5m1CCKy6SjCg2FEdWPHlO7bvK8YRF25DcczC7XL+1VT6d9jPN3wQR73yPDOhyDC0XFM5B3ee+yml5DHR6u8bdr7Hbr5fIhEjHVTGM7A198PX1XLuWC6h2r3upL7mP19sRb3VsO/NVylKLR5Xoix4nZiWfNKbcBN21pfZ3JHcRJrzP/cc3PdF4a1MWV5vTaBJ44xrTNecv43+wz+TU+txOle6XBvNjBvw+79UpRT3WoftXPS+j5qSFmq2/Ee3XR9eWrxDNArfR5YldPumMzPrxhiJeuW1q/hXdzVc8Ru/1ZlJfz2KfzwBwtw9b+ejZO0icfgg/+6FB98i2HJ9lXJfZyoFfEcJuowPvT3R5EesOmvc/WuWR8t0gHc/uRxiqAMjm6cJ79Qh5DT/mFfRiGFAS1yOI9kTv8r8AiG1OnmX6u3GO0fEt4J9LdEhMlS3KlGt+6bwNSuZbgvvql4UT52C+7TRcbmkrp5tspsc/MokJKjaa9bFsHGUbVD6Ue4D8sQKpOiuGKTk8hdUMF2zcs/dgvOsei8ahs7HsLGlRchiKW4dGUG25SOs+Ctg/CtuxEbJnfi6+u8eEBJhW20E6uXPIUvau05ihUP3FibTnpqLXbXuiFqfkJJmb4Tq5eMYsUu9bwYBFbpfrzx2C14cpk874GVGVyinkPm6HozuzLs+DauP2dQnr4pAqwcxJ0XmleuUnAQIz55vKXily4exMfkKKRkXv1Hh4iYdwL9uiilSEaJcnScByCdAYYcogrHE8jooqJy6ouRuB4Jn/LcG4kCUWWsHjMxi3Q0jCCCCEfTyOor2Lzv8QQmwnI5R6JphNRyMyvF7KWMN1byxaPddFVhD3J+uaMGAMYn8obZuT3yOnbvPZbTDWNOeTHR7yJCtFw53arVdjpEd28EyAwr724FDGd8CFvcf9wuV6R8GS0Iug5WETFvBhEtMngECOm+RNffx9zeF1HFvdWQpUiC5JCWqsjmeRHKaZHO+Z5cMb14G6m8bRX5CW0cQ2M721z3OuL6BHz9pdOJqI7s7pXl7s16rt4vgxjU7q8SpHwEmb4UClb3UUMGAH0HQBoZDFmU1YLdcdk9A/QsnwcW5bQ9JoX2/BrEYMm6Tv9+cPscsdu/VVkJew/g6eWno8c8nYiIiOpH+d61NArY+l2zUdgBXCPql39AHhPGoZ0QHJQbdwh9CKQKxS8E7Lr6PXEM9QwoXyToxw8D4OtWvijwoLvikIPGUo9byvdgQP8L0Wbasa4YWbfkFvzYMDOCL+ojYx97So7kLsdpm/rO1QuLUamFB0eBSz5Y4y99nsGG+ChWpNymbjYvr+/MVjtMzeu0NnE0g6uWyZ27QX2HuxIBff2SGHJaVLTJ5CRyyOASLfJyGa5/7HE8+bR5QWp/1te6MWpeseMhbFx5tW486aW4dKXuvLjgRtygdNB6vefh/er6CxaUiQqzLkO9qffl/gmv8Zf7eoU9yCGNkPaFtvyr+ol8mXkAoOsksxZFvz6qUs2Y4ZKYTSOqfCsfDEeR1vcAm/ftL0ZleXv88Ks/wvJ0l2kb6kz6Lw51qZttp6sKSPVlEBmSO2o88SEkcyHtV5uhdPFHgHbvPXbT8xPjQHQEI1HY/0pUU66cbtVqOx3EE0e/+o80cT0SvrD1e4Lb5TT6FNBKB2tJKlldFDks7mOuVXhvDYYRTYfsnwNumY7HE+9H1LxMO6i4bXWixY6TkWgaA0qF2l33MiWbheudEFFt2Nwry92b9dy+X+qjWr0JmL4i0hgzAOjZlNVSJcuaVPI8cDomp+eX078fKnmOOO2fHDyH7y/K4rpFWVy3aGfHpIAmIiJqRcE1Fj/cs3nXbBR2ANeAp9uHcfVX42IWaTXNlxizjKzQvhAYDEKMqSHfBezJyfMLqQD61F97Snkk7QcXaw+eOPrt/gHVSJObsHQVitF9u27E+83LVKqibapRqc9g5AFgxcW1HQ9UXLsM911yi66jypnz8qZOrrawE9s2AxtXKR24qzKALg20K/oxkJVPzaIvidw482y8f3NMOYfzuH21VbT6zAUHJeSdUkzqxwhVPtoP6p3mVcvbA39a6VQL5ZAsyacJ5QtzIK2OkxNKA/o00ESu2X2xWzpdjHmRiQzpXtQ9iI8Vz/2RqJy62cDuvUc3vZAKYKAnD2kwKF+PkQz6LN4ZrZWWszq12k77U39Qov+RiRW3y9WEq/tiGbbbUH8IMAT0GSNXZ6tatK3XnAYK1veDQmrAfWYoImo/hRTk4cHVH4KYxw9vENtngJ7L58FMj2mm/36Y6f5nm7cdizN/8AdMAABOxSeVMYAvf5d5QSIiIqop5cfFfak95jlN09IdwJ7eiC6Njoj1CSBi+7PCJtKl1RRCOSSVKBEEB5UoK/nLau9EP8ZM+f2Kg74XB3yXj1tdrw8TPrTfl3NiTJfLXEQ2bfEFaSNMTkLpV5ddcLY2BlfhwVFTBLCdt+HcC4rj5Bbuvgsb9bMr2GZwWQQbkzfWOP2zPGbo17yj2KlGFALwXLxMl4J2J76+Tu10tl7eYHITvrb5PJx7pnlGC9vxEDauVFLn7pNTON9+gZIGWkvt6xDZvGABfI+NYsRqHs0KxmtGceFFuGrzXYaxvb+2OYJL6/TDgMKDo/BtUs/hzTY/0KhOIRUwjDGRnxjXDV+g4+mGb9xmiAGneTNQGM7AN6J+IWSTClfMIq2LtJJ/IGVKA02utM37Vb0UUhiwei8xTJfHzRvoyZe8u2nEGEI5JeLF7r3HbroplXReSR/jqm3syq9Tq+3MGkoEVKhcVKbb5ewEw4imdUO7FFIYsNmWq/tiGeW3If+gYcScUt8tbw/8uh/iFFIDNqk720A1bWs4/gKGM8pz1eG6t7oeXV2vRFQ/FdybXdON/V0YzthGqxqv/9oq/wzQc/E8cHlMJZz+/VDJc6Ta/c9GbzkbH10+ibs+8xSeN88jIiKiugquSQKJRPGdxuZds1FapANYRExN46KMoxQT1V9Mq6liQsgl9REYrUWL6jW9WBen24xHoh/0XZ1vGAh+DIODY/KvIz1xjOm2ERws9xLfRMEwoEZpCSFgpNFl3YnVSkpmLdXyglX4ziWj2hi35+S9uMq8mqW34rqEF9cvUddbhtsvUGZVus0LL8JVjz1e2/TPO76N6x8DfrxumZaKeundzwALVuGLK9WUxjHk1inRvjbLF+5eaUhl7dtU286netOnf5a9FaFLzsPG0Z0Q77wFvk3rEFRTQd+ppobWW4o7dy3DfUo7y591dfnHeP3JnfzF49CNWUv2DNdMD7rW7pTPi03F679ryShW7FpXt6gdz9neYhT7/B50fdzNWOTueOL9uvuygBDUccA8kH93pA5NEMRgPoKMNnalPhrAaV71PN2+YmSvIEAIlKbDLY3K8qA34jemgSZ32uj9qlYKqUDx/PIm4FPeS+ymQ1yPxDgwrv0gTxkvt5BCQF0+BIyoY3vavffYTC9JJZ1LYkieYdk2tuWs8B3afjuzXRDhKIqpPG25Xc5OEIMjvuLYwN4MInnr8Xfd3BfLsduG4TwwPA/M9Ck7YxDNzwtPHEPJnLZMH/rbOHORU9vaX2fF4/ci4VPq0ea6lzeVRdqcKtXmeu0kYqwRY46LiOnfSQopBHTXjTYMU8n45/IPftxfY8b9uD02t8tRM7i/N7viiWMoktHGB/dO+HRpjUvvo8Xr32GYsCrYPQP07J8HpeW0PyazCv5t4fY54rh/8/4IAHr6w7i6+39ws5b++UFswRl4x1vMS85ipudEKyikAnV7VjTmOaR7Rjapfu2f9w7EmLtU+Brl3bDk+JR3Cu09we1yJlrKe5v5daWWzerZYZpXUZ1VwvROVwczuR5msi7NEp44hgwvNNbvmo0i7N+/XzJPdGP79u1Yvny5eXLbEQQBklRVFXSETjl+QRAwtU9OcNPadmL1/Ltw7i7rztWu+T1tchzOOuU4mmlmdfgMNnz8RiBlfZ65V6vtzNzM6qN9iGt7sG2Zmnp85vXfNb+nLe7xYkxANqymgisgFegDhjq7Y6pTnr+1wvrobGzfytXivliLbXSKTjkHO+U47M3kPBURE7IIK2NuF1IBrO9WfkhdSCE23ItB+ZcwCHgn0C8NIggRMWEAPSMRZAaAIfVHPY6M+6nOTI6z/jrlPOuU46gWnwGtTxAEbNgdNk9uO9ctyrbBtVZ6DRieEy1CHRLQNgNRQ5TWlXvGZ6QYC2DPmmq2457hXm/7vHcmxgRkEUUaYV3wllM9yO8POT8Q0c8vpBDoywDjPsN7RvnljIz370YqIBXwIhMpZsEqpALwZiLIj8XhMdeJGIMw0KPMq6VavGvVitN5QK2sHd4D9+7di8O65gEAjn/TCebZM/bin/cDrRMBTDRL7HgIG1deXXVnDtHMKJHxNpHBhijwtZuw4ePLcP1jj8vRr2uVqOnJTViq28bqHcrKk5uwdO0mOfL445uwYa1uHp7Bho8zCtmN4OobkdMigJfh+nNmx/2iOByCYBgSgYhotqrFfbEW2yCyJiIWSEHURQ9qkRCFFAKxlCGq1hjRJK+b0kXoyEF78peOifFxYySfPvOCOZpHi5ARIMSyxekoYDiDYuptT1z+MlilpZINYlAaQ7xcKnzb/ZiPzRwZox6bfjmb4ySqMT4DqDkqez443eP1kZyGSEjbdSp5vhifE2KseL+GGNNFPRaQCihRji7KX7yl25VF3ab+2PTzigxl0pejuERFdd34ZzHg7QEylvnf60T/vPd0w4cc9pTdvYhsOorwYBhR3dAelvVg4EMkYjy+wnAGvv5++KpaTibGBITSkDM42NS/VpySdnY4t5zaUCWuRwJKZiqFJz6EJGzS+AfDiI5PwGrUSkOGiXLHAefzyLyeZdkbeD24W1dd36Y9NEqUuPbRXecW5bavC4ft0KzHDmCiRrpwHaZu1acpJqoXpePWkMp6Ke7UxkiewNSuZbgvrqQY1sZJVubdugrX/fsobr/gPNy+a0I5b3di9ZJRrNilbmMQWKXr2N08CqQmMPXvq3Ddsgg2jqqdxj+q8bjXHWzBKuzUt9FsuV8Yhj6wGTKBiGg2qcV9sRbbILIznsAAhpTzawS+RF/xi6Z0BhiSINlFhIwnkOnJy+vmk8gNpFCAB/GxPJJ+P5J59XwVEfNOoF87j/OIZNT9iIiFcvKykoR8T043dmgeE+M+dOt2rnUkeCfQb1cuS077MRHXI+Ebkcs6EgWiVunVrY6TqA74DKBmcf18cLjHizGEoNxPJQmSFgnosI6yb3fPF+NzIhiOakMLFfYAfq3DK48J6IZuKCl/BhHl+SBJI0BI1+liWRa3zwpjmVAYRkZfDpXrurZgWT6runKqc+dnpKc3AmSGG54GGpAbMmcedsOKmEU6GkYQQYS1cdCt6qFUt+H4ChjO+CzHj3e7HCAPJSmfFvr6dzjP9O1se245tWFRYU8O8HWbzhcPun3jmLDq5RWzSOvGZ9cUUuhL+DCi7q/scTidR+7KDjTqerBgua7baz2IQe3YJEj5CDJ9urTbJfccu7oosx2a1dgBTETUkZSO230TmNqnG7N2x7pilO+SW/BjZXLhwVFg3eec06uURLAvxaUrH8eTTyt/XqDr5L3wIly1+SGI6rZrOe41ERERETVZFP1ahEgQ4ajuy8GyX7jq1vV0w2cTPYLCHuQMY1HLURgTefUL22JEoyfeXxwTtLAHOdMXksFB9QuxHgxUEhXhtB8iIrLg8vngdI8PhhFNh0qj2JzWASp7vuifE0E1+lOODO7v9xWfNfoOMX35Tc+HkmN1WxY7WpnkiFFEei2+U3FZ15Zcls+pzlv2GVlAqi+DyJBNZ5+OmE0jqvTGGjrd3fDE0e9LYL2odvaFrb9Tc7uclXLnWdl2LtOGFVOiYQUBQjZs2aFaGM4AyTXGY3Q6DqfzqKKyN+B6sDSTdWGMfvYmMK6f5/aeiTLboVmNHcBERLPF5CYsXYVilO+uG/F+8zI1sxSXrsxg245nMPIAsOLit5oXICIiIiJy5k8ir49okGY4Jp4njn7DF/Q15O2BPx2Sv3gL5ZBcM5OCEhHNArb3eDWabQjoE4wpoG3XmQkvevw57CnkMeELI+jtQS4rGjoHa8b1s0KNSJU7pSPOvVf1VZc6rx8x5kUmMuQi7b2IrJpuWRAghNKAlgbaHbXTuNy54na5GXE6t1y0oafbB+T2mKJGRWTT/uKwGlCiYaU8krmQRUrjOnBR9pbk1B6qQgqBEIrR0vkk/OZl9OzqotLt0KzCDmAiotnkgrO1X7kWHhzVIoA9Fy8D1n3b+UX3wotw1ea7iimfJzfha5sjuPRC03KK4LIINiZvZPpnIiIioo6TxoAallVIYSAdtU1nWDVPN3zjNuPOeXvg131JW0gNFNMFmqMvxJhhXEbjF5llOO3HpDCcgW9E/UJuzMUXz0REncjl88HpHq/xID4mYURNzetqHRfMzwl40BsBMn0DyPV45fm5LLI5m7JDjdAdKEYoOx2rTiXPimA4ivRAn3X6Z8B9Xc+EU51X8IxsDHnM1YGePMacKlYlZpGO6lON55H0q2mgXVKi1UPl6t7tcmYVnGe255ZTG+oFw4iOK5HKCjEWMkXuqjyI90eRVtMd6+f0RoDEeuP3i07H4XQeuS070JjroQK27WGmy0ZQGM7YR+6Wqwu326FZhx3ARESzxYJV+M4lozhHSQF9Tt6Lq3Tzvrgyg0vU9NBrdwJ4K0KXQB5LeO1OeQzhTd7i2MJLRrFily69tNmFF+Gqxx5n+mciIiKijhOFb8KrpZnzjajjM86E/AV8witAiIlyBFg+goyaalDQRYF54hhK5rQ0eH3oR1ILdVAjuZQ/g2FAje4RQsCI+iWciJiaJm88Aa8glEayOO7HyNPtK0YRCQKEQOmXojLzcRIRdRK3zwf7e3whFdBNExCCOnam/TrOzPdd03NC7bQaH4ev2yNH3/rSSDum6g1icMRXTIfrzSCStzvWIvfPCrVDbtwm/TMqqOtKmOvKoc7LPCPtU1fXibgeiXFgPKHUiSAgkCrI0ZHmdOIwpn+WedAb8StpoM31YCeIcBTwm1Mel3C7nJn788z+3HJoQ4MgBqUR3TuTgFAa9lHRwTVIauNl63ji6I/qUhWr55HdcTieR27LjgZdD+7Zt4d+oTiGIhl4lWW8Ez6HNOoOdVHRdmi2Efbv3y+ZJ7qxfft2LF++3Dy57QiCAEmqqgo6QqccvyAImNo3YZ7cdrrm9/A4COiYOtyJ1fPvwrm7NuvGDa5OZ9RH43XN7+mIe3wn6pTnb62wPjob25earVPOwdY5DhExIYuwVIsv1uqjkAqgD0PuIoBqRIwJyIbVtIQFpAJ9wJBDxEeLap3zbGaaeRzm80+MVRCRVnetf/3OFoIgYMPusHly27luUVZ3rbXP+WW+ThulsmeFiJgwgJ681fzWr2sxFsCeNVZlr51m3utbTWXnVgUKKQS8GUQsz8NW0XrXQ93ag1xph3vD3r17cVjXPADA8W86wTx7xl78836AEcBERFQ3Ox7CxpVXz7jzl4iIiIioEp7eCJAZLo20qKPgmiRyWqSHFwmfVcpEmo2Cg1LDO5mIyFkznhOo9FkhZm3S77aBQgoDObvU1VQPFZ1blfDEMeaUwpgs1a09iCrEDmAiIqqPC9dh6tal5qlERERE1NaCGGyhCAtLnjjGxuKNSzsJ9QtSdaw3CZIc8kEtQoxZpEyEiJghlaT+bxGxQAqiLhVtQMsf6jSvVCEVMM4vpBDQyqJbt5BCIJZCKmCTKtJuPaU8Kd0xGjJVirHisceyuhlEtdYGzwdVM54TqPBZERx0mN/idd2s+p3NKjm3Ok4LXg+zuj2olbADmIiIiIiIiIiIOpMYQwgjxS9h3X5JPJ7AAIaUdUbgS/QVx5B0mudIRMw7gX6tLHlEMrp10xlgSIJU0nFSZr3xBDI9eXlePoncgNqBLCIWyiGZl9fL9+SQNmyXiIiIiDoVO4CJiIiIiIiIiKgzBcOIpkMQhIDLTlpVFP1avsYgwtFxTOTdzHNQ2IMc0ghpkbxeJMZ16/ptUqaWW09fHk83fOMTyKM0hawn3o+ougoRERERdTR2ABMRERERERERUYcKYlCSIElDQJ8+BXST+JPI69NCShJcZYasdj0iIiIimpXYAUxERERERERERB3Og/iYhJFoGlkRALzo8eewRxuCd8CUHjmNAd34vAPpKMJah6vTPAeebvjGMxiuKBJ5But5e+BPZ7UO79JjJCIiIqJOxQ5gIiIiIiIiInJFjAkIVJZHt0FExGwiO8WYmjbXWHa76faM+3BbF47LFVIIBNTxWqkeCqmA1s6CICCEESVy1oN4vw8JrzzdOxFB0q9fMwrfhFdez5uAb0Q/drDTPCdBDOYjyCj7lD/W561Rlet54hhK5rTU0X3oNx0jEVEns383qFwttyVzfD+oQK22U5na14e1Ru2HqDMJ+/fvl8wT3di+fTuWL19untx2BEGAJFVVBR2hU45fEARM7ZswT247XfN7eBwEsA5LsD6q0zW/pyPu8Z2oU56/tcL66GxsX2q2TjkHO+U4gAJSgT5gaEwbl7Q2RMSELMKSqSOukEJsuBeDcY/c2eqdQL80iKDddP26JWz2UZHS4xdjAexZU+v6qE6nnGczPw6ntnaaR+SOIAjYsDtsntx2rluUneG1RlS98vf6Wt6va7mtSpW+O1SnVttBA+ujUfuhTlL+3tB8e/fuxWFd8wAAx7/pBPNsvPDCC3jkkUfw+uuvm2dpDjvsMLzvfe/DiSeeaJ6FF/+8H2AEMBERERERERG5VUgFdFEmImKBFFK6SNqYLkRDH2ErRysWkAp4kRgfl6Mu1YULKQR0EZqG7eumC0IAhgAXMVacF8vqZuh44nInr8rfA695uqcbPhRTARs47MNYFwWkAvqyFuuiuJz18Xt7gEzFuX2JiIhIz5DxQfdCskc3Xf+eYv/+Yb8tQH03UKNS5XchUbe8IRrXtA/9pty9U1m/O+hVvZ1CCoFYSn5/UbOROJTX/p3IHKVr/NuyLh3q3n4/RLPH1q1bMT4+jkcffdT2Mz4+jq1bt5pXNWAHMBERERERERFVZzyBTE8ekiRByieRG1C+QBRjCGFEni5JkKRBBOFBfCyPpN+PZF6CNBiUvyT0TqBfWy6PSKZP6egNYlCbLkHKR5DpU9Mli4iFcvJ2JAn5npzt2KZaR7R3Av1jcZQEvRT2IOePoLdkhvt9QFyPhE853pEoEFXTDOtZHT/g6Y0AmWGmgW4pQQzaRhs5zSMioqYopNCX8GFEfWfQHsJpZDBU+p7i9P5huy2l4zIEjOifA+MJDKj7kEbgS6jvMSJi3gwiynuEJI0AIdOP2fQs36ms3x0cVbKddAYYkiCNxeFxLG8F70R6lnXpUPfV7oeowxx33HHmSZbKLccOYCIiIiIiIiKqUhT9+kja8QnkASAYRjQdKo3aNSvsQQ5pbYxSQZCjUybyynx9FIg3gXF1PTGLdLRfS2Hoifcjqs4zCQ4qXzDmezBQUp4CUn0ZRIYsOoYr2AcRERE1T2E4AyTXWPw4x+Y9xeH9w35baYQsh4zQ7QNBhKPKe4zpPcIwz5JNWStWwXb0P4BzKm+V70SWdelQ99Xuh6jTXHzxxTjmmGPMkw2OOeYYXHzxxebJBuwAJiIiIiIiIqIaU6N3h4A+QZcq0YI/ibwWBSJ/BoP6KBu1AzcJv3ndSnji6Dd98SrGvMhEhmY+Fp63B/50SP4iM5RDck3p18ZERETUQuzeP2xFkUzmELJIw0wVqrjuiWaXE088sWzn7sUXX2w5/q8eO4CJiIiIiIiIqE48iI9JGImmkbX6vtTTDd94BrZD4Kpj9ipRJFoEsLcH/nRWN77cgHWKQDGmG79ORDbtR48XcuRvQMBATx5jdr2/bvehlM03on6JOTbzDmUiIiJyzdMbARLr7X9sZubw/uG0re74GEYQMo5ZizQG1L8LKQykowgH1WwoA8XMI/p5rcipvI7vRF70+HPYo1VBcZ5lXTrUvfN+iDrT9PS0eRIA4N3vfjcWL15sngwAWLx4Md797nebJwOm7bEDmIiIiIiIiIhqqpAKFFM3CwJCUMfE9aA3AiS8AoSYKEcK5yPIeIvLatHCnjiGIhl4leneCV8xDaAnjqFkTksf2Id+JK3Cg4NhIKRuNwSMKJ2z4nokxoHxhFfbr/HL3Ar2AcDT7UNa248AIaCOMWhmPn4lPWKktzQFNREREbnjiaM/qksrXDZK1/n9w2lbwUH9OL8AEIVvQnmf8CbgG1FTRAcxOOKTn/mCAMGbQSRvTh/tRum7Q3XKbcehvI7vRB7E+4vreScixXmWdelc9/b7IepMhw4dMk/SXHbZZSVRvieeeCIuu+wywzQ9/faE/fv3S4a5Lm3fvh3Lly83T247giBAkqqqgo7QKccvCAKm9k2YJ7edrvk9PA4CWIclWB/V6Zrf0xH3+E7UKc/fWmF9dDa2LzVbp5yDnXIcnUqMCciG1fSFBaQCfcCQu0hgMRbAnjXulq23TjnPOuU4qHMJgoANu8PmyW3nukVZXmvUNK1xrxcRE7IIl4wLTETN0hr3Bmd79+7FYV3zAACHH3EEjjjyCPMimlwuh3/7t38DABx++OH4xCc+AZ/PZ15M89pfXsPB114DGAFMRERERERERDQzwTVJ5LQIYC8Svn53HbqFFAZyEfS6WZaIiIiIiDqKUwQwAPh8Pnz+85/H4sWLsWrVKsfOX5i2xw5gIiIiIiIiIqKZ8MQxJqljAEuQ5FDg8jxxjI3Fmf6ZiIioLQUxyOhfIpqBqTfewNTUlHmywZlnnonLLrsMZ555pnmWwdTUFKbeeEP7mx3AREREREREREREREREREQN9tqrfzFPqop5O+wAJiIiIiIiIiIiIiIiIiJqsEOHDuG1v8ysE/i1v/ylJJ00O4CJiIiIiIiIiIiIiIiIiJrg4GsHq+4Efu0vf8HB1w6aJ0OYnJyUzBOJVHPmzMHhhx+O4447DkcccYR5NlFLO3jwIF588UUcPHgQ09PT5tlEREREREREREREREQNdVjXPPMkAMDcuXNxxFFHoquryzyrxNTUFF57tTTyVyX8Yd8+dgA3gmCeUEaLtIokSZgGcGh6GscffzyOP/548yJELemll17C/v37MXfOHMwFIAiVXoRERLXQ6Ae623tdbcpl3JvbfVdKmnFp61WyjjTTyiYiItKZ2WOFT/B6mVm7lMFma4jq25AN1K6qb/M2wtNzhjqtAtv0rG/TYleq0862VtQ1bx7mzp2LuV1zMXfuXMyZMwfT09M4dOgQDk0dwqFDhzD1xhvm1QzYAdwolV4RLdgqB6emcOqpp5oigSWlrC1YYJolBOX6Kl5kBw8exHPPPYfD5s6t+NIjIqqtRj8f3d71Zlau0r2UTqmVmXb/1q9kHWxmVU5ERKSZ+SOFT/J6mXnb6LCZGmpmbcfGalcza/c2w9OU2tksuVh5mbYHdgA3SqVXRAu2yiFJwrzDDsMpp5wCAJCmDwES0+pSixDmQJgzFwDwxz/+EW+8/jq6GPVLRE3X6Ae62/te9eUq3YM8pfotllPdlkvLSa5VV+VEREQlavdI4ZO9HmrWPmyehqlNm7HB2k1t2r3N8DSlWqvFhVTuvKzFPtpAuWqg1sEO4Eap9KpowVaRJAlTkoS3vOUtkKRpSFOvmxchaiqh6zAIwhz89re/xTxBYNpnImoBjX6gu73vVV8u4x7q3fmLqrbuthbIQeXVTkREVKJ2jxM+3etpxu3E5mmYGbeVho3WDmrX3m2IpyjVyqy+kGqPl2Z7YQdwvdT6SmiRVjo4NYW3ve1tmH79NUjTU+bZRE0lzOnCnMOOwN69e3GEi0HS9f77xbn4zp8OwxOvzMGzb9T6AqZKnDZPwsKjp/HZk1/Hh463HsDeDbZpc9WqHdtfox/gbs/16stV3EPx/6rfmhuVb91tLZCDyqudiIioRG0fJ3zC18uM2onN0lAzaitLbMBWVfu2bjM8NakWZv2FVMRLanZiB3C91PqKapFWUjuAp159CZBapFBEKkFA11HHVdwBvO63h+Ou5+aZJ1MLuPrUN7DuLQfNk8tim7aWatuxMzT6Wen2BWTm5RKUfc18S+VUtge3NUBlVFbtRERElmr7OOFTvp4qais2RdNU1E6usDFbVe3buoPwtCW3eCFpeNnMTuwArpdaX1Et0kpaB/DL/2ueRdQSuo75q4o6gP/7xbn4m/yR5snUQr7n/UtFEaRs09ZUaTt2jkY/wN2+gMy0XG73UwvuytrIEs0K7qqdiIjIUe0fJ3zi15Pr9mIzNI3rNqoIG7QV1aetOwhPW3KDFxLAy2VWYwdwvdT6qmqRVlI7gN948U/mWUQtYd7xJ1t2AD/3wgs49cQTDdMAoK9wJH64f655MrWQj55wCEOev5gns03bTKXt2Dka/QB3+wIy03K53U8tlC9rI0sza5SvdiIiIkv1f4TwyV9vZduQTdA0ZdumamzUVlO/tu4QPGXJDV5IvFRmOXYA10qjr6QmtZraAfz6//7BPKtlfHPwHtz17SG85/zz8J07U+bZmp3jj+Dqv/sCAOCXP3nYPLulqMd09ef68H9jV5pnt4x3vPcDAIC7vnEblvrfZ57dEIf91ekVdQAveuJojg/b4k6bJ2H3wlfMk9mmbabSduwcjX5guz33Z1Iut/uolfJlbXSJZoXy1U5ERFTC6vHRNW8e5nR1Ye7cuZjb1QVhzhzzIkREREREbW96ehqHDh3CoalDOHToEKbeeMO8SEPxrZuqIk1Pufp8866NeMd7P1DyuWL1dbjl60nkC4WSdWb6gTQtlxFSyTzDRyqmIi2Z12If9ZggTZfMa6WPVp/SoZJ5jfpUih2Fra/SNqp0eWoMtkunaL12bL0SEREREQDMnTsXRx13HI489lgcfuSR6DrsMHb+EhEREVHHmjNnDubNm4cjjjwCRx9zNI4+9hjMndu8TJV886bqTB9y91E6Lo879hi8+7yFePd5C3HGaafiZz/fjf8vsxWfufo6/CD7QOl6M/lonaVS6TzDR1mukuNp1kfXAVwyz+Ijbn8I132hH98avKdkXl0/Wn26K2ddPkREVCet1dUqtFyJOohV+BYREVEFDjviCBx1/PGYa8rMREREREQ0W3R1deGY447F4Uccbp7VEOwApqpMHzrk6iNJ8jeIb/echXtSt+Ke1K0YzQzh/qFBXLjk/XjpwMtYd+s38PDYIyXrVvtR9wlIJfMMy+k6gM3zWu2jHpMkOR+T+snc/wD+a+e46+Vr9VFJ09Ml8xr1ISJqVb+ZnMQP7s+aJ7eJ1upqba3SdBCJnb9ERDRzhx1xBA4/6ijzZCIiIiKiWemII49sSidwS3YAJzckEfvbq82Tm2ZYFDE2Pm6cqIadNCv8pMn7N6fdtf2o6ZglYzrms972ZiQH/h8uXCKPE3vftuHSdav92Oyz5NNGKaCLx+QyBbTWYexy+Rp9tPpsoxTQ1AThE+TPVy43zyEo9XO//fjlLeHJR4rt2Opl7XiNeCGo13bdavb+Zwl2/BIRUQ3MnTuXnb9ERERERCZHHHlkw9NBC3/Yt6+lvu5Jbkhi565d+Odb1+PMM880z26K5194AT96+GGcduqpCPj98sRW+y6yQa14cGoKb3vb2/Dqb580z7J0x3c2I73p+1i86J245/Z/NM/G6I6dWPvV9QCAJ/5rGwBgy3/8ECP/9TAe3f0/AIAzTj0FH/vIhbjmsyu19Xb95DH84D9GsWPsJ9oy8Wgfll241LDPFZcswz333oc9T03i2GOOxt9Fr8DlH/uoto1rbvwKAOChHwxh4Bv/om3vwsB70f93f4uT/upN2j53//JJbPmP/8SOsUdw4OVXcOwxR+PCwPtwxScvw9kL3lqyzaFv3oobB76O3z/3RzzxX9vw1OQz+O7378eju/8Hv3/uj9p+rvibT2DRO87V9jO6Y6ehzJd+5MM4+uijkN70fURXfdJQD2b6/eup9X/l9f8Pj+7+H0RXfRKvvPIqNm99QNumm3qH0j7f+/dh7HlqUlvulv4bsOgd52Lhhy8FANxxy5ex5L0X4Pn//TNWr/0y9jw1aSj77l8+ie9+b6tW391nL8DffLxXaxt9G4Y+/AF8I/1dOYrc4hwyO+ot52Lv3r04wpRq7LkXXsCpJ55omAYApz16jHlSeTu3AF+/0jwV6PsKcFncPLV9PfkIcOMy81TgvIuAL28xT3Xn6vOARR8Grv66eY6jZxe/bJ5Umzb9yuXA4w8B2f3mOUVfuRz4w2+Aux43z6mP8Am1PZfuTwFDXzZPrX4fz00CsUXADfcASyvrxK+kHTtH8QH9m8lJ/Pzx3Vh+WdiwxMxU+0JSyYtDtfuopWJ5W6E0HamSU4KIiNraIz/9KW79uvzv8LU3rMH73vMe8yJVO/K441ylfX7hhRfw4IMP4qWXXsInPvEJnFjmfTCfz+MnP/kJfve73+Gll14yz6ZZ7LjjjsOb3/xmvPe974XX6zXPJiIiIqqLF154AVu3bsVxxx2Hiy++uOz7LABMTU3hlQOl34/WS0tFALdi5y8AnHTiifjgBz6AZ597rjQSeJaSDk25+mjj7EpSyTzp0BQ++oH3a9vc/YscpENTuPn2O/DSSwcQXbkCn76sFwdeeQXpTd/Hd7/3A0iHprDzxz/FNTd+BTvGfoJLP3IhoitX4Jijj8JTv5k07PPXhd9g4Bv/gnPOPhPdZy3AgZdfwc2334GdP/6pvH/deLGrv/Bl/O4Pz2HxQh+OPeZo7Bj7CVZ/4ctaOXf/Iodrb7wZ2374EE4/5WQsXujD6aecjG0/fAh9161F4amnS7b5j9+4U+volQ5NYfShH2HH2CNYvPAdiK5cgcULfdgx9hNce+PN2n5GH/pvrP3qeux5ahLdZy3A288+EzvGHsG/3f8f8kanp0vqUP857aS/QnTlCpxx6skAgMULfYiuXIHghUvkulEig/977CfYvPUBwzbL1bt0aAo3/dM3cPPtd2DPU5NYvNCHxQt9OOO0U3DgpQPy9hXS9CFIh6a0Y7n0Ixfibz/zSUi6unz0iRw+fVkvoitX4GWlbdR9qW34+z88i2+kv4sDL79iew6ZPw01uFvuOMzuB24ZlTvZ7rrBvFR11AjL5+SO9qa6ZbR4nNn9cmfo1eeZlyrvuUng2aeBD64wz2meyBr5vzttOrSfm5Q7iD96hXlO+9G34eDu6s/XPY/J/62w85daTft1o9YzxpmIiIhmrmvePFedvz/72c+QTqfxi1/8ApOTk3jkkUfMixiIoojvfve7ePLJJ9n5SyVeeuklPPnkk/jud78LURTNs4mIiIjq4pFHHsHk5CR+8YtfIJ1O42c/+5l5kRJdXV3omjfPPLluWqYDuFU7f1XsBDYyp921/Sipi+GQjln10ssHIE1P4ZsDN+L7d96G1Z9ZgTVX9+H/XXcVAGDnI49Bmp7CE7+Uo48v/esP4Ss3rMbqz6zA9++8Df7F7zLs88DLr+CbX/0HfOWG1fj+nbdh8bveAQB44pdPKssVO2tDH16C7995Gzbe9iVs3fgNHHvM0djzm0mM7ngY0vQUbrzlGzjw8itIfP7/aMt9/87b8KH3vxsHXn4FQ5n7S7Z53DFHY/u/pfH4DzOQpqfgX/wubN34Da3MG2/7ErrPehsOvPwKdv7kZ5Cmp5C6exMAGPYzlPxHHHu0nEKrXErns956OlZ/ZgXOOPUUAMB573g7Vn9mBT6x7EK5rpUO4D2/mcQ/fTGBx3+YwerPrHBV7zt/8jNs+88dOPaYo/Hdb3wVG2/7kvYJKHWvkqRDuO2Ou/HoEzl0n/U2fOWG1VoZb7zlGwCArRu/gTVX92H1Z1Zgw1f/AQDw/X8XlXpUOoCf+xMuufiDePyHGWy87Uslx2v1aZpz3ydHRI7eU5tO2+d/Z57SOr5yv9yR+6TzFzUl/vdZ85TmO1dOQ49f2tzXx/9d/q//4+Y57e3UBcXztVLP7zNPIWoAdv0SERG1KnUIecFF5+/999+PbDaLl18uRj68/vrrhmX08vk8du3aZZ5MZGnXrl3I5/PmyUREREQ1p3+Hffnll5HNZnH//fcblrHSyDTQLdEB3Oqdv6pW6QSOrb4al69YjmQqWZz2t1fj8shyJDckte9IDdNqbfqQu4/S4QhIpfOmD+H551/QNnn6SX8FTB/C6Sf9Ff7lu9/DVWvW4ZNX/z3+4Wtq+eVtvOscDwBgx49/hn/57vfw1NN7gelDWHiOx7DPxe/qKU6bPoTz3vF2AMBzf3pemaZ0TgPou7xXW+6kE47FJRctBQA89fQzeCL3JH7/3J9w7DFHG5bD9CFcsfxjWlnM2/yHv70CJ51wrLbswnM8ePjHP8OX//kOXLVmHT5w+Wex5zd75YWnp233c9IJx6L3w3J5IMl1sOsnj+G8j0YMn3/57veKZVPzOCrLm6df+tcfxEeXvtcwr1y9b/+RfM5fctFSQ70aty/b/qNx3JsdQfeZb8UdX/0Hbb56jAdefgV//amoVvblUTkK8ffP/UleVmnDM045CWtiq0r34/RpppPeLP+3FTs666GVO6krsexK+47QXzwsp7w+dYF5TueoxQ8WiOqM3b9ERES18773vAf3f/8+3P/9+2ac/lk/goDTl1m5XA633347Hn30UfMsRz/5iTxsEJFbPGeIiIioWR599FHcfvvtyOVy5lmauV3278y11vQO4NjfXt0Wnb8qrRP42ecw3ITUMv+6aROef/55AMDOXbvwk5/81Hra/2ea9tOfGrYzU9L0IVcfGCKAS+f/6BH5H3+nn3ISznrL6dj105/js3+/Dhv/bSuOOepIfPC95+NTl8rjwqrbCFzwTiQ+9ykAwMZ/24rlV6/BVV+4GX964QXHfarTf//sH43LWRzP0Uceoc7AAeWXyW8/860ly73rnLMBJdrYvM2z3nK6Ydm/+8o/46sbNuJnT/wS3gVvwd987K/RfaY8dnC5/RSPaRrS9CGcdtKbcNXfhA2fd51ztm55tQNYXt48/dQT32SY7qbef/+snM76/ee/s6R82vYV27b/CADwwfeejxNPOFabrx7j6aecVFJ+9SOXUz7eM049uWQf5T4t5blJOY2z/nN/yrjM1efJaXjvT8nzrz5P/qhjDMcWGddTl1dTRKsfqxTG5mXCJ1QetWtF7eDuvsA4fecW47706YW/cnlxPOEbl9mXuRnUlNTm8qjpnz/8aeN0KO1Qrl3t6kLvK5e7ax/1/LDbXzWe3wecdmZp5/ZdNxj3pa+X8AnF8YTV+exALvHY44/jB/ffr3yy2ufnj+8GAMM0/ec3k6zLUmpMEQeorStWLxER1YBd+uenn34aW7duxQsvFH8A7tbvftchPzqlhuE5Q0RERM2kjg389NNPm2cBZX40WWtN7wC+9JJLAQATv5LT+raDP/5R7gg7822NjwgzDyR9yiknu5t2sjwmbK2Yx121/SgdeRJKx2/90/Mv4PsP/CcAoPdCP6RDU9gy8hAOvPwK+q+5Al//4v/F1Z8O4/3nyamb9dtYFf4o/vveO3DLmtXwLngLHv2fJ3Hjrd9y3qd5uq6z0Fy2Z/8kd55L0jSOPuIwAMCvf7O3ZLndOfm8Pfbooxy3uTv3JP77kcdw+ikn4T/u/mf8/ec/has/HcaxxyipnXWdl1b7efmVV7TySIemcNb803D1p8OGj/+8dxTXUb7JVZcvN91NvR9z1JEAgMLkMyXlUz+q+Gc/iWOPPgobv5fF7tyT2ny1Lv/wx+dLyq9+pEMWbVXBp6l+pfzSWE0rfP83jePnquMEmzsad/8X8Nwz8jJ3PS5/blAiUtVxhi+LF5cfvQfIrC9ut+8rcoexvvPw/pTc0arf/w33yNNm2nl44zJ5n/qOw/tTchn04yKP3lPs+PzyFrks0I0p3CpjyJ77Prkj1JwGWk3/rC+n2qm/6MPG8XSd5qt1YR43Wf1bv5zaSa531w3yeaPf39CXZ9aOTz4ibyN+p3H6Vy6Xz0d1X7eMyu2qnrNZ5XxT/z+7v7QDmagm2OnbEKxmIqJZ6ZGf/hSXfXIFLvvkCjxSwx+LC3Osv2LavXs3Dh48aJ7sCsf8pUrxnCEiIqJmO3jwIHbv1n1nrDPH5p25Hhq3Jxu9wRA+99nP4dvf+TaGxRHz7JYz8eSTePJXv8K555yDnp5zzbPrrjcUwscvlcei/MLffwFnnnmm9bRg6bRaMkdd2n2KkajGaNynJp/BtV/+Z+Qnfwvvgrdg+bIPQZo+hANKR+dRRx6uLbtldIdhG7snfq3N++vAYly7Su6ceex/fuW4z9LpxWjdraM7tOV2T/wa//3IzwEA7z/vHXjX28/C6aeciAOvvIp/3Tps2ObQVvmc/eB7zyvZpn65Ay/Lx3XMUUca9vPY//xKWXYa/vPegWOPPgoHXnnVUJ4/vfC/+I//GlM2ah1Jbf6cfrLyA4CydaCUz0W9By54JwAgM/wgnpp8pmSfkq7z+6z5p+O6PjmqMn7zN7Q2e9fbz9LGMzbX5e6JX2vT7Mrp5tM0O7fIHWpqxy0AXP31YmcwlI7G8y4q7WiEsqxbp50pd6iqLovL0350n/z3c5PFsuj3v/RyufNOjeB0S43YVT9ZU4e0fn/6zsBajolcbx+9ojQN9A+/K6eH1vvyZXIb6tvr1AXF+rjrhtL5UDryn3262JF6f0r+W9+OUDrH9Z58RC6XfvqpC6prR30bqj8g0J8fO7fIEc9f0Y1Vce775DrYPFCcRmVdcN55WH7ZZconrH3OP28RABim6T9nLWBnOjUQO36JiKjG9P8e1lu0SH4HqsZxxx1nnkTkiOcMERERNdvhhx9u+w48bfPOXA9N7wBGG3UCN7vzV/WZVauw5b4f4L3vLY7VUzJNsJhWS9MWY69afZRIzj1P/xax/tsQ678Nl1z1BUSu+xLyk7/FBb6345s3XYeTjj8G0HVc3nLnJvzzxnsR678Ne37zjGG/P37sF7jkqi/gnzfei7s2b8U/3bUJAPA3vRcZ9qkuby6LNl3394ah+7TyJb6awoFXXsXHLvRjYfeZwPQh/N//8wkAQOq79+FTiS8j1n8bPpX4Mn70k8fhXTAf164Ml2xTv+/TTzoBAJCflOvhnzfei8RXU7qO2mlg+hA+GboQAPCP/zKklWfFtf047eS/MixX7nP2/NMBAN8ffgix/tuwLnWPPE9l2o6ber/s4gC8C+bjD398AVfe+E9a+WL9t2Hs0SdKtn/ZxQH8Te9FOPDKq/inuzbh+Rf+F5g+hOs+I3fYq3V51+atuOFr38SV/3ALXnnlVXk7NvXo6tNIanrm8AnF6FerqFZ9x9vjD5V2iC76sPHvcqyWP/2s4v/veUz+r1VZznmv/F+7VMNW1IhdNdLVnM7Ybn9qiuh2GBNZrRe1g/a5SbmD9h3+4jLqtMia4jQzu5TRpy4wRhn/4uHSzmXoosdVv/qJvJ55ulpe87nkRI3YveEeuZzmSPRfjluPd/wOv3zc1ESCw6cTsWeSiIioHR2ass7IdOaZZ+JTn/pUSaYyN9785jebJxE54jlDREREzXTiiSfiE5/4hG1Q5qFDjevDaIkOYLRBJ7Ch8/fc5nX+tgpz1KXtR4nkPPDKq3gs92s8lvs1Xn71L/jguxfii1evxF3rEjjx+GO05a/99KX42IfejwOvvIrvDT+E00/6K1z7f8LKTuVo0DPnn4ZjjjoC3xt+CHffNwxAwpXLQ7jhs8sN+yyJHjVN13cWJr/4t3jpwMt4LPdrAMCVy0P48jWrtHX/2n8+7vnHv8cH370Q+cl98nG88io+9qH345v/71rtGPTb1O/7zDefin/8uytx+sl/hcdyv8aPfvo4/iH6KZxxivIPYGW52Cc/hiuXh7Tlfv/cn/AP0U/hA4vfJW/TfEw2n+DSxfjguxdq9a4ds1IH5u24qXdp+hC++f+uxZXLQzjmqCO09oQk4bQTj5e3r1KWv+Gzy3HBO7qRn9yH/3tzEs+/8L8IX+THP/7dlfC+7c3IT+7D3fcNY8/Tz+DK5SEs/8hSeV92beji01D6dMdWqXDVcWBvuKe4zHkXGZepJbUz8Pl95jlFf3WaeYp7py4oRvXqO5DV/ek7usMnyB3kAPB8G4zBpKaB/q975b+t0j+X68gu1xmr76T/w2/0c+w994zc+WquWzVVdLkyWVl6udz5rI4zrVLHPDbvS12u3PFRnXRqJ6+d5nb+qhmR1Q8REVEnet973oP7v38f7v/+fXjfe2r3g3GnL7N8Ph+uv/56LF682DzL0Xvfq/zwkcglnjNERETULIsXL8b1118Pn89nnqU5NGX/zlxrwh/27Wup77eGxRF8+zvfxuc++zn0BkPm2U1h2fnbbt/H1qiVD05N4W1vexv+/HNTmlKiFvGm85dh7969OKKryzD9uRdewKkWvzg/7dFjzJPK27mlGPFr7vRV2S3zFaVDUU39e/V5ckSvOWWw3fp2y+u3q66b3W9cBkrkrzo2sDmq1MxuWfMxOO1Pz257Ljy7+GXzpNq2KZS0zOpYu1b17Kb8aoe/ORoapraz2r4qfIKc4vmyuFymH35XHhe6Wvrj0tPvB0pk93OTpWmpzey250Il7dg5ig/g30xO4ueP78byy5Qf2LhSrxeOSl4M6lUGPefy1LsEkrYH+3LUuwwNZ3+oRERErukfJ13z5uHIY4/VTbH2s5/9DA8++CBefll+N/T7/ejt7TUvphFFEbt27TJPJiqxZMkSBINB82QiIiKimhseHsb4uJzt8ZhjjsHFF1+Md7/73ebFSrzy8iuYeuMN8+S6aJkIYJUaCbztgW3mWU3z9OQkI39NpENT/PDTkp+WY+4gfvwh4992TppB2io19bI5xS8cUgpXIrLGmEJYLWslaaVbkV8eNx133SBH3X5QHsdao0YJq2MtWznvomIUsZ6aPlrd5qIPA7v/y7xUaZudNF9erx7Rt+o4wuq2T32r+/OT2hhjW511XDcvERFRiUd++lNc9skVuOyTK/DIT39qnl2WXbaMqTfesE0Drffud78b0WgU73rXu7BgwQK8733O/zYJBoO44oorcO6553J8Vypx3HHH4dxzz8UVV1zBzl8iIiJqmPe9731YsGAB3vWudyEajbrq/J2ammpY5y9aMQK4bbT794NVtroaAfzCT1qng55I78T3XtoaEcBqtKg+wvIrl8sdbOddVD4C+LlJOYWyOZrUbnlzVO5dN8ipmvXRqmq5zdu04xTxqh6LGgWq7k9fJ89NytPVMjltr4xKIkeralOVelynnWkddavWob5dn5uUU0ZfFi8e47IrjW0UPsHY7mr7Wk2D0jlrPm/0EbdPPiJ3RJvPAytOEbvmcl19nvxf/bHv3CKn+VbL47S9Mippx04kRwA/juWXXWae1SBVPvzr/tJTvlz1LEEx+rc4xYp5qbZnfZhERDQLPPLTn+LWr68HAKy9YU1FaaDLPT7mzp2Lo44/3jyZiIiIiGjWe/mlA47DptRay0UAU3uQpqf44aclPy3j3PfJHa1DXy6OpRpZ434M4FMXyJ2AX79SXvf+lHkJZ1d/Xd7/jcuMY7kO7nbX+VtOZI38X7Xj+eqvy52esUXF/cUWueugbCXv+oD8349eYZ4jW3q5XIf6do0tAs5Rxpk6931yx+joPcX5aqplfWrlUxfI29GPufvly6w7Vb+8RT5v9Nu7cVlt6rbvK3IZ1PNL7fjV72vzQLHzl2bkrAULmtj526rKfY3sTB+BVN2n47p1iYiImurQoUM4+Oqr5slERERERLPaa3/5S0M7f8EI4Blo9+8Lq2x1NQL4T7sy5llELeHkJZH6RwBTw1USOco2bV2VtCPVQ5UP/7q89FRWFnMJ6ttxa122eu6xKawPk4iIyJHbx8dhRxyBw486yjyZiIiIiGjWee0vf8HB1w6aJ9cdI4CpOtOH+OGnNT9ERERERETUVK+/9hpeffFFV2MCExERERF1oqmpKbz80oGmdP6CEcAz0GlhIC7PAjUC+Pkfb8H0wb+YZxM11ZzDj8JJ7/8EI4Dd0I83a8XtOMENUknk6KxqU3VMYjtO41Q3QSXtSPXg8mFfotYvPdWVQy1FM6J/UYdaaCr7wyQiInJUzSOka948zOnqwty5czG3qwvCHMYiEBEREVHnmZ6exqFDh3Bo6hAOHTqEqTfeMC/SUOwArlZHfQvo/l9xB6emMH/+fBzI/TcOPr/PPNvgnP8eMk8impFffajPPMng8JPfgmPf8UHs27fPdQfwoieOxrNvdNoF3VlOmydh98JXzJPZpm2m0nakenD5sDeo9bVUTRn0al0eVfly1WvPTVH+cImIiCy17iOko57UDVfTdmVT1ExN26VpeEI0SmecL0T1w7sRzUb82SVVRADw+uuv46j55wDTU84folozn2Omz1Fvfjtef/11+YHu8qm+8Ohp8yRqMZW2UaXLU2OwXdqN4P5G6orUwl9JtGq56qCVm4GIiIg6A981yIAnRKPU8l9vRETUGRgBXK1Oe6q6PAveOHQIhx9xBE455RQc+PUjeGXyF+ZFiJri6AXvwrFvfx/++Mc/4vWDBzFvrvL7ljLn9n+/OBd/kz/SPJlayPe8f8GHjnc/vjPbtDVV2o5UD2VuiAa1ftGpZN92al0mlbuy1WvvDePuMImIiEq0xyOk7Z/UTVWXNmaTzFhd2qVpeEI0QmedM0S1xbsQzUbsAK5Wp98xbM4KSZLw+qFDeNOb3oTjjjsOB5//LV7Zm8MbL/4Rh14rTe1JVE9zjzga844/BUe/zYfDT3oLXnrpJfz5z3/GvLlzMFcdV8rmXNZb99vDcddz88yTqQVcfeobWPeWg+bJZbFNW0u17Ui15uKGCNThJcftfsupdblU7spXr703jLvDJCIiMmifx0fbP6mbqm7tzGaZkbq1S1PxpGiGzjyXiCrDuw/NRuwArlan3zEczoqp6Wkcmp7GkUceiWOPPRaHHXYY5s6da16MqCEOHTqE119/HQcOHMBf/vIXdM2Zgy41+lfP4ZyGEjX6nT8dhidemcPxY5vstHkSFh49jc+e/PqMIkbZps1Vq3akWipzI9TU+npxu99yal0ulbvy1WvvDePuMImIiAza5/HR9k/qpqprO7NpqlbXdmkanhDN0pnnE5F7vPvQbMQO4Gp1+h2jzFkxPT2NaeW/ZRYlqjsBwJw5czB3joA5gsPFyZOViGY1tzdBh/toRdzuz61alcvMXTnrtfeGsjrUWh+Y1T6IiKhttc9tvdYPtNml4e3M5nKl4e3SEGz8ZurMc4rIHd59aDZiB3C1Ov2O0ayzotb12qzjaEW1rltFnTZbPzwniGjWcnsDrMWd3e2+KlGLcllxV9Z67b2xzEfh7tgrUodNEhFR87TPbd38jKNKNLyd2VyuNLxdGoKN30ydeU4RucO7D81GFnlSiZQ7ov7Trtq57G2CL49ERNS+2ucpJlX5KeJLEREREZVqyttQU3ZKzcf30WYzf93b7l/7EhGRM3YAU+fjm0zdlX7J3ML4dktEVGft8ERoqycXEREROeI/8KrBtyFqHH4R0+rYOkREnYkdwDQ78F2zIdrqH488H4hoVmnEHbpdvkZshzISERER1Q/fhojIjF+TERF1HkGSJL73ERERERERERERERERERF1AOGVV15hBzARERERERERERER0Sz3pz/9yTypLZ188snmSUREswpTQBMRERERERERERERERERdQh2ABMRERERERERERERERERdQh2ABMRERERERERERERERERdQiOAVwDQ0NDePjhh3HGGWfg8ssvx6JFi8yLEBERERERERERERG1tJmOAfwv//IveOqpp8yTXfvwhz+M3t5e8+SKzXQM4Ntuuw2//vWvzZMr8va3vx1f+MIXzJMbKp/P4+DBg+bJFTn88MPh9XrNk4moxbEDeIZuu+02bNu2DZdeeil+/etf49e//jWGhoZw9tlnmxclIiIiIiIiIiIiImpZM+0AvuGGGwAA73znO7Vp27dvx2mnneZq2l//9V/jiiuu0KZVa6YdwFdeeSUA4PzzzzfPcuXnP/85AOCee+4xz2qoXC4HADjqqKO0aS+++CLmzZtXdhoAvPrqqwAAn89nmE5ErY8dwBXavXs3AGhRvgsXLsStt96KZcuWAQBWrFiBD33oQ7jmmmvw/PPP41e/+hXOOeccnHTSSYbtEBERERERERERERG1klp0AL/zne80dOLOZFq1atEBfP755+Oaa64BAOzatcu8iKUlS5YAAO644w78/Oc/b4kO4KOOOgpnnXVWxdMA4De/+Q1effVVdgArrr32WvMkAMC3vvUt8ySipuMYwBW47bbb0NfXh76+PgSDQQwNDZkXAZS0CjfddBMuuugiXHPNNQiHwzNKe0FERERERERERERERM1xzTXXuPoQEbWKtukAXrhwYdM7UTdv3oxbb70VW7duxcc+9jF873vfAwCkUinccccduOmmm7Bnzx7s2LEDBw4cwK233oonnngCxx57rOtfCBERERERERERERERUWu544478MQTT1h+7rjjDvPiRNRkN910k3nSrDKjDuCFCxeWfJrdSVtPZ5xxBkZHR/GHP/wB11xzDURRxB133IHFixfj3/7t3/CrX/0K119/PR566CEkk0ksXrwYQ0NDOHDgAMcEJiIiIiIiIiIiIqKOt337dtxwww3a56mnnnI9rdVt2bIFV155peGzZcsW82JE1OHuvfdeQ9/oV7/6VW3eiy++iI985CNYuHAhAoEACoWCNm98fFxbZ3x8XJt+77334t5779X+roUZdQADwNatW7VfuXzpS1/CJz7xCfMiHeOWW24BlHQPK1aswJYtW7BkyRJ89atfxa5du3Dfffehr68PL774Im666SaEw2F873vfw6c+9Skt9z8RERERERERERERUac67bTT8M53vlP7HH300a6ntbpTTz0V559/vuFz6qmnmhcjqju78Yipce68806tf1SNNj548CDWrl2LdevW4YknnsD69evxt3/7t3jxxRdx8OBBiKKIhx9+GA8//DBEUcTBgwdRKBTw7LPP4tOf/rR5FzMy4w5gvcsvvxwADL/UufLKK7XebH0a5C1bthh6x82/ktGvp0+fYP5Fza5duxAMBrW/62nRokVIJpPYunUr3v3ud+Pmm2+2TO38ta99Db/61a/wd3/3dxBFkbn/iYiIiIiIiIiIiGhWeOc734krrrhC+6gdvW6mtbrTAtXMvwAA//RJREFUTz/d0K+xcOFCnH766ebFiKjD2WUs+O1vf4tjjz0WF1xwAQDgggsuwFlnnYVf/vKXeO211wAARxxxBI444ghAiRYeHBzEpZdeathOLdS0A1hNh6ymO77ppptwxhln4IknnsDWrVvxj//4j9qyu3fvNkQO33zzzdo8tadcna8XCoUwMjKi/f3DH/4Qn//85w3L1NvZZ5+NL3zhC+bJBh/60Ie0DnEiIiIiIiIiIiIiImpvo6OjuOaaawyf0dFR82JUAXOHutXHHEBIZMV83mzbtq1kWi3PpdWrV2PhwoX4yEc+ghdffBEA8Mc//hHHHXccDj/8cADA4Ycfjje/+c2A0vELAK+99hp++9vf4rXXXsMvf/lLnHfeefB4PLot14bwyiuvSOaJbi1cuNDwdzQaNUS7Lly4EFu3btU6hK+88kp88YtftBwPV7+seT2r+WrHcDAYxLe+9S3LbdbbQiU62Zze+corr8T555/PyF8iIiIiIiIiIiIiaht/+tOfzJMqcsMNN2iRvbWYVq2TTz7ZPKki5u/47foCVLt27cI111yj9Vvccccd+PnPf4577rnHvGhD5XI5vPzyy+bJlk455RScddZZhmm/+c1v8Oqrr8Ln8xmmtxKmQp59vvWtb5knWbrpppsMY/PWy7333ouHH34YqVRK62DWp3NWx/b99Kc/jfHxcaxevRrHHHMMvvnNb+L+++/Hhz/8YSQSCUBJK+33+7V1Z2LGHcBqp+yWLVtw9913QxRFQAl/thoPWL1J3nTTTdi2bZthnlUHr0q/r5tuugkf/ehHAQDf+c53mnYTtbvp33bbbTj77LMtI4B3796Np556ynIeEREREREREREREVGz1KID+NlnnzWkc37qqae0MX/LTQuHwy3dAfzcc88ZMpRCyVp66qmntmwH8Lx583DiiSeaZ5U48sgjS8ZhbocO4Eay62x22yFZS9dee21T9ttOGtUBfPDgQfT39yMWi+GPf/wjHnroIS3TMQB89atfxUUXXVTSsfvVr34Vixcvxr333qu1pdquxx9/vGHZatQsBfTll1+OxYsXawelRuRu3bpVS+X8xBNPYMmSJdi1axd+//vfG6ab6fNnm3NpL1q0CD/84Q/xxBNPIBQKGeY1yu7duwEA55xzjnkWvvCFL1h28O7evRvXXnutti4RERERERERERERUSdRx/dVP2pHr5tpre7UU0/F+eefb/iceuqp5sVayrx583DSSSeV/bRD/RO1otdeew3PPvus9sOT3/3udzh48CCgdA6/9NJLOOWUUwzrFAoFHH300fB6vTjvvPNw/PHH44gjjsCCBQsMy81EzTqAofRWb9u2Dbt27QIALF68GN/97nfNi+G5554z/H3HHXcY/l68eDG+9rWvaX+bt3H55Zfj0UcfxX/8x39YdrQ2wn/+53/iwgsvxEknnaRNe/755w3L6KmdvxdeeGFDfnFARERERERERERERNRoahpn9aN29LqZ1srUQDV1LFH1o59HRJ3vxRdfxJ133qn9PTw8jO7ubhx//PG44IILAACPPfaY9t8DBw7gLW95i7b8wYMHMTQ0hCuvvBInn3wyHn/8cbz44ot47bXXAN1YwTNV0w5gmMYBvueee/Doo49qN8Irr7wSUDpwobtRmt1zzz34/e9/r81ftGiReREsXrwYixcvNk9umG3btmHp0qXa388//zzC4bDlANLs/CUiIiIiIiIiIiIial+33347rrnmGsvP7bffbl6cqK6Y/rm8evbH3X///Vof5sMPP4wvfOELAIDDDz8cf//3f481a9Zg4cKFWLduHW699VYcfvjh2rpbtmzBueeei+OPPx7HH388gsEgPvCBDyAUCqGvr8+w7EzMaAzgZrrpppuwaNGipkQA7969G319fXjooYcMEcBbtmzBzTffjC996Utaudj5S0RERERERERERETtoBZjAKuRvbWYVq1ajwFcqVYaA/ioo47CWWedZZ7lCscANmqlMYCJymnLDuCnnnoK1157LURRNM9qCKebt74T+Oyzz2bnLxERERERERERERG1hVp0AD/77LOGdM5PPfWUNuZvuWnhcLhlOoB///vf44wzzjDPckVd16oPoZFyuRzeeOMNzJs3zzzLFXVddgDL2AFM7aTtOoBvuukmbNu2DXfccQeWLFlint0QW7ZswTe+8Q1ceuml2LFjB771rW/h7LPPNsy/+eabceyxx7Lzl4iIiIiIiIiIiIjawkw7gIeHh2e0jZ6eHrznPe8xT67YTDuAt2zZgmeffdY8uSKnnXZaUzKY6v3ud7/DwYMHzZMrcvjhh+PNb36zeTIRtbi26wBuFWoUcCgUsryJb9myBbt372bnLxERERERERERERG1hZl03raSmXYAExG1O3YAExERERERERERERERO4CJiDrEHPMEIiIiIiIiIiIiIiIiIiJqT+wAJiIiIiIiIiIiIiIiIiLqEOwAJiIiIiIiIiIiIiIiIiLqEMJ/ZrOSIAiQpqchzJkDSdINCSxJkAAIACAIgG6e+n+CbrowZw6k6Wl1BiRJwpw5cyBNS8U1HJbXSFLpPGV1CRIEYQ4EAZieNg5fLMwRMD09LZdJLRuAaUnS/l9PPVZBECAAmJ6expy5c411oC4LQJqWIMxRtqNVgLy+YR3lGCVlv5IybXp6GnMEQTtW4f9n770DJDnKs/Gnumd293YvSTrpkkARCUkoAEICk0QQ0WRMEmBsIyEUACNhfvCBJJLBBBNNNhhjJDD2hw02mKRIUARlIemU7053p8ubd6a7fn9UPVVP1/Tszu7tCcTn2pvr7qq33lTvU1Xd1UF0Ux429Xtg62hUb4gqKV2qV0rHPCNtkW5LAFlqH1wla4Eso07VssxksHD5Gl9CglIqZVkW2s66SsGHWhb8mfLwdVhuvB8pU32W+qZuP/VdyoPH3K+jnzElfJQf98uyRCY20AdFWTobffuof7rpUlob2pJyoL6qqZfSaj7EF9zX+pb4lzzqnNKrBMsyj3/jYwHSptRZo9oYxknIqNiWJrXBwPs6F31t+C/EWhbax5EY4/6zpa3IhbUVesD1Vw7/JPP1MgPAwFpnrxX8V/T2zmPMK29r2V9Evxrj+qygWE1MBDlZ1MVtHf6tx29d76FlytoEHRAkpG3gXCRtx36HusPAwgI26kbbtAOotpWXC1/fxv6aPFmnjg/Lg1MsAi/yoIxwbFDhGxhW/EW7yVhTp181lbZEZqr3aZksQ1m4OGcbODqHfcZjoPd0sQ2cHrF+LNM2Af0m7ab5EF9wX+vbGvxrSuk1dSujPnXlRvrB2SbWzXLOVzpTN1+kuvA4pWdbMp40Fo20GeM+xBYTY7LG967HiLHI+pZxLTSVRDmhz3Bbjrng+F1b19P7/ZAYh9KPpb5A4rMsMyjLKL9n/JfWmys+EduJHStYDXaKzyrl7D+8fDZB6vfgW+FLvSruYpNIV6zJi1ZRYb8y/vs842OVAOaxyTIZn6ICbIsw/lOOz2dbkI7JBr+5CFKTSBfan/MQ5sO1TZZnlXm6iiC9symQhD4t+hsILKzr0w0MyqpGYR7khESe0/kdnr9Jxv8qZ5cq839JFV3lOJ3z6hyNtGGOII6x0neQVlPp537KOzjIuH49YMBjCmlM+K2L9Tj+EvcB/2JPqomVeErjjbHk1eiYC6nPIPLTfFs3/9fYE58xL62bltO3aV63cqaqDNIBAPXy56sdaInenm1K/Qbvq7IoKrqSzvhYCufOQIit3vHv4yWcvzl8KCroGsePfslQeh+wP8yymOdoTMQd+3VXEGiIcVv6+Km0hYUxWYhtTeH8n/4mT2uBGtwGc3wblmWJXOf/SSpLiyzMJ10e2z/GgjsGbIUeAf/u2gXp6Pc0loPfk7aH1wN+zGSKsYkgP9WrzqxUPrccj7nfrS7L1GfkB4mf1BfUjaky/pcWJgNs6WIw4B/G97+x4aLPIh/aUW2vaj+Y+rU2L63n/R7OKWROYuRaRDVeYxt2kxGcxK3kVcYQn5cZg0Ln/5mn8343Mg7DxwTbiO0CdJv/h2qh/VCDf+6aCv6j3WGe5duDSfmk9EwWMQ7TOk5f6l5R1tkt491skqtbIsty6cerqa790KW9bd38P8EA6RyNqchN6yp98EuNLkj4pj5KE+linQzWn6eUDoCuTNs+VJYyLTbwfGyItdQeJ0/HBSeXW/Zh1uq1QeVb5UEznYwoM47/jifr1PPp7AfJy/Go+t1aj3+XGcsjPMIxKpyqiflazv1KH+bzjMlQlHH8d/NePy82bm5ciWEP9N7H/6hDiI/EJtpKfgh+jD4ovf+Zx/xaenGMU6laRhYWnA/Fcibjr4OwLwk8rXpWU9AEJoxRTt9aaonh0If5AHB1fC1vpNKD478/d4l09K/22XHcVL2dH6wfh9xYGE2kr2JbGd8GlXhNkyfMkrj/vY7/1lbGrHT+r+1GHtxSH21PltOfsV2qfKK/6T1tB867TLDD6evspQx4+1N/sFzjgUn9ntIWZYnc28C2zEyGoigCMMK8188NiGcmWsTzV/JWS+vOM2wyD1We3NXYUBr1f9UXsW5Kz+RkVstYx/qYS+PH0UU/sJ6rk/DnVtrLsK+dZv6v5//RBgTsUgbnK+n1Asa30un5f2Us80qr3soXiPPQUEf0sf4alupVZ5a5/+abQ3YahNp4RVGE4xBAoh3zQwdqCMQ46KocXlzQCw1MvAChiQM2dcyyzC2CiQ7uBC53g4DYohPzakfiEm3UjsblORoOZEpLHkUZ/YIwiXS0RVF4fdyCCn3I+n4n2K++D7aGoM8cWKWcfJivbVCWZYUH6+SNRsVGdirkl+c5yrIMdmRZhra/2EAejabjUZYlGp4fZbAeZdCHQRdrked5oFX74e3IvK+M+JP7kLgsNE6kvalrsNPzTsupJ8scm8iHeaRtt9tRXg1elH+0PybGK+uVZYm80ajYlparL1PdVP+0Ho9ZVvp4UF+SHpYXYav20M+YI/4hdOSj+lCGtj8AlIIT+AhS3dR2dXFJ/IttnNhA5Nbpjjr8+3xrbRiElZcxpuIX8qfuxD/LiqIIfCifdRzOY8wEHyr+k7zIxw38toL/okLPOql/SEN+eZ6jLKr4JxbJg5gvBf9MrEcZKptyFP+0n8kYg7xH/KuvVQbldtOBeRp76s/UJ6SdDv+u/SL/VDZEH9YrSxcfalu1vBv+nf2qf1qPxywru+K/6nvagHnAv9KRD+VoW2r7o+v4X22Xuhgra/CvstXuVHfU4V/KqY/yMnPAf5bloT8jH9pPurp9lZHqwa3tMv4z2V7xn4z/RdGuyN29+K/2OWXhFuWUjr4oC983+BGeMii3mw7M09hTf6Y+Ie10+CcP8k9lmzr8FyXyRu4m6l1wrL5MdVP903o8BuLCKOuofmqj8keC//Zc8B9OeDrlVNqyB/zr/C7YLuMl6vAvFxQci97xrxfQrXUnhkpLHnX45xhftNs1+K8f/4OcJJZCfoJ/zk2Ujw0XbHjzltAn+Nf5gpGL6Y1a/Beuz5on/DemxX/v83+WpTIot5sOzKOeLMOs8F/FI3mQfyobAEp/0Zb1Sh+valtarr5MdVP903rhWGKMdVQ/tTHydzbSz5jF+G9mGv/9RfzSz3nVBiZtV2rXzXbVoUjxn7SjSXzJZK27nKs81S+Ux33MgH/S1o//iv8YK+RNvdJ9lZHq4baxDWiH0rNO6h/SkF/9+P8gzf/99aIsz1C0E/xnbi4AINykV5ZubpBeY6DcbjowT2NP/WltXBRhyjrwX41J8iD/VDZqxn/Gq/pAy1Nfqjw7E/79YhDLylnhX/wzS/xrnCpdKod6qw1MtFuT8uP1uNTHZVkiz6vXt1S22p3qjt8L/qu+IF3dvspI9eDWzgv+I7bzOeJf+1mVTTld8e/tUJn0p9LRF+prlUG53XRgnsae+jP1CWnr8F+9wB75p7JRg/9yd+Jf7CR/1lH91EbljzmO/xqnSleRw77cdMF/USDzMcLUzXbVwV1PifgH1wG4YDIL/OtqCeUpLXnsKv55bkbezE/3nQzqFv3J8wX6RX2jPMinG/5prysvgh3ZHPBf1zaUQx1IS58xmT94/Me4VFryIP9UNnYB/1w3yEJ/Y2Dlxhj4G6a0Ho/Js+wB/3oTAGbEv+PDxHzSkLfqxUT5lKHtjx7Gf8pJfUx/qm0q2/DBuQr+nd6Ycfx37a68zDzgX31Burp9lZHqwa2dA/4zY0wIQiUAgHa7jdIDPRWshrFcA0Zpi8ItRpBe9+Edr/QM0lR5GgXf2DSW/MK+dPhcvKQMbmmjOoOdjnZ4AJCLDIie3E8DjnXZ0cHr0mw2K8dqS0pPH9Auraf+Ji15sFzrkZZ6UceUR+Y7Xh5bGxeIoYEo/iU95VIXxgf5kqcxBu12G0C8o4XxRzkEDgA0Go3ge9JSni6mmRk6HMpWW9rtdqBTH7OcW9pJnyABHBNPluiHwrcDafIsQy6dTN5oVGRBfGploFS9SW+SQcP6OIT4mXHArdKpvxp+EZoyyWdX8a8nj/SD+o086XvWzZJ4YBntQAX/Tg+3X8WpmSv+/cUHppSv2ki91J+sm+K/rwv+i3nAP3mwXOuRlnpRx5RHlrkLLzymzaynPiafXcE/ec8V/2qf+QPAP/fVD0pDX7D98nyu+Hf1GcPUhce0lfK5Vbroryz4nzLJZ1fxz/1Z439Xx/8kPqmbyqKN6otu43/Kl1vuV/3ZDf8Zms0+OY4xSl12Bf8aC+ob5pEfj/lTHlnN+E+b8PvCf3Ma/PtFOZ6MqP+1jWinyrB/CPhvVE8q0DP+I+5YbqfBP+chSqf+6ob/VruNoiwrN1pS18YfAv7lDmM7j/jXGx6BuOBAvqmNyiPriv+Z5/9cGMVc8O8XR1iu9UhLvUwH/t028zd7kid9yXrqY/KZC/5b8zT/V/vMQwL/echXW1Jd5wv/xD31UDr1VxX/DZSla9PdM/53xhV9T/q0rVhGO1Az/nNRiLwhvjTGhAvKlEVfqS927/g/M/6Vnj6gjVpP/U1ajQX1DfPIj8f8KY/s9z3++ycainYRxsYw/vubeZhvMh3/Hyr4r47/7O9TXXcZ/3LDHPNZh8fqr+nG/3Le8R/9Rp70PenTtmJZWZaVayw2wbzuI8W/xCDrc0ud/hf/7mZPHtNm1lMfk8+84t/L+eMd/9Pz/92Ef28r5XOrdOqvbvjfLeM/3+xRi3/2X12u/3k+CPh3NymQd7wWSL/EG4k0BlmfW9r+0MB/Fm4kVJs0FtjeLCct9aKOKY/s9z3+/y/+gywr+M+Mf7LXJ+oU29zpxWPaSvncUuc0Xh9U/IvfyJO+J33aViyjHdiF8T88Tf2Qxf/8jv/5Waeffl7gLsGFpJHVMFVencEyVZzKUglVlHRKz0Snp3lMqRyI7nyMO9WfssmLurOM/AiCIENszjyIjeG7P3xKOhfS8ClV6wOFOoVf0tiRXdTFJp0K9SKdLnKRR9j3dGmQBjoJutLf0UO+WRbvAFWZKoOJmpMuyov0LEt106Q84WVpB8U8kJ/nZaQjo6+YaIPW03LqY6XdmLS91AeqD/MauR+sUH3iJ9B7PxkTX9OgNlEntrPypl06ALKe6sf6pMl8vFKO7tMG6kt+5JPip852bplIR3vKMr6aNrWLdErvku/M5RUemBb/0ReUY+cD//4OfU8UdExjhDyYRzrypSze8W2lzVDBf9RPdcEM+OcTetV2jr5lffLkFsmgU5YlGs1GvBM/8ZHa52RUsQqhU3kpD/IlP00pT/pAdVZ+yqsb/rvVYyIPu4v4Jy1Tin8m7ju+rs0pGz3hv9oWqh/rs042I/5jzGE34Z95qV2kU3om6pnmMaVysDvwX2Mz/cl8JqUlHfk6WWV44htd8R99qbpgRvx3H/9J1zP+k/FffaT2oQarELq54z/qg17x72U9JPHP137PCv8Jjxnwz4skLFO9VV90wT9fUZQZeaIw8SkTfUR7esE/7zyuaxPm2Tr8+zEu0Cj+S4u8kVeeQu4V/5ni388tjHEXrrLZ4F9wa7vM/zFf+PeLuMqT/mB98lRZKf6b0+Bfn07GLuK/ZFwlKeVJH6jOFZ3EzocG/mObqG8oG/OI/2xO+C/DE8C0h3bX2Z7WJx3tqeDfP13iCQOd0jNRzzSPKZVjUvzXjf98bV6NHzRe890y/tfh39UlrfpSdcGM+K+b/88N/7/38T/P9A2MzgeN3PX1/iqD8uNFf/OQwX/ct9bduMB96sR2VlraNRv80866uGC56gvBEOCuDanddban9UlHeyr47zL+Kz0T9ezI8/upHPSC/x7H/wcP/7FNyF/5URfMiP/5nP+7i9QcO9RHah92F/4TnvSB6qz8lNdDEf+qG3ViOyst7Xow8Z/ip872tD7paM+84l9i1dWv0pAXx4Q8zyuvxn9o479AluXh0x+Ulc0T/k1l/K/2o9RH7aOMNJHuf/E///gvyjLcNKaftrI2LvCyPutkf0z4l/1UDir4d3VT/TvxH3X5w8f/bhr/zzrttPOUSAcYEpdyB4E2jBpHoUyOZwwc7axVCa2jDlAQ2+Sd4IHG1+cdBiE/bcxkgEQS6JpPmSEvaVTAf3PFd5KUpQtE5M27Y8rSvepXU7AnAYL+ytK9IjnYJvqmnY2dppNigOX+bpq0XGk0n4vXLFMAkY+1nV8HqcqIfCkrpau2dRUEKS3zjYmvXU3p1RfW52ucMbHtaFca0yyzMggx6X7p3xbsaP2THDIR4SvP9PsyqS2YZiBSGtqb6qKdHTrwE+Mi9T/rG+MukMwv/v3WxFcUq295zOT4OF4V/eWbQNHqiMmZ8G93Af/cWuteb2dqfGPEt2pfBf8yebWQ7yXOgH+WaTK1+I9P1Kju1EnrpOVKA8B9Q8APWFkP+E9TKoP7lJXSpbHKxHpKy3zlmdJTjtJrnDHRv7QrjWmW2Wnwb0VeSpvy4bHWN/INEZbbtD067LXhIi3L07ZNfUoe6q/IK9bZHfhX2eoTHjOpbnX6aznzswcR/1rG+pRVZ18V//Xjv9blPn9qR1q3E/89jP+94t/nsw1cmbND5dXppmWoid1UZ9oZ2zoUh3pKy3zlmdKrL5ivccZE/9KuNKZZZqfBP0ReSpvy0YWYoJvczEF6W9Meqb2pLmnbqk91XFB/pbxcnFbxn/kTT2vdWEUbUl9hF/FvkrasxkR9rFn/zZ4O/BceN+U84t/LYh7rp/inf0wH/uP4n/IIvphH/Bttw57w31mvin+/gCby6nTTMkj7Mz/VOevAfyeemd+NZ0qvvmC+xibTg41/d/zgzP8L399gTviPtNSd+9Qx9RV6wT9sZcGOfJhUt8B7mlhj/aIowkIa65K+gn//7TDWVR1Zm/poGem1TH0T7Ev6t5nxH/3DOvrrHf8Rx6wbZfSK/5nG/4gTTNMmWgZpf+YrPekoB5DvOtv0G2fKk7pW5adyVAeNMyb6l3ZpTBMzKaaZdJ/yUlqNhRQrof5uwn/FpxIX6q+Ul15g5nUn9YHapL4iH/Vxqjtlq094zKS61emvGGd+Vjv/j/znbfzfLfivtgv3+esd/9WYp86qk9ZJy5WGfX9pLewc8U/soCZ2U53JV9uaifWUlvnKM6VXXzBf44xpOvyrbnYa/FuRl9KmfHis9dUWltvfE/41TklL3blPHVNfoVf8+4ez0ps3kbSlW/Cs6q/lLr9EluUoCj7JaQGY8ISste68u9vnUFRHJsrkzYksU11T31Ts223497b7OcPuwz/zq5+BoD4qL+pWTakM7lNWSpfGKhPrKS3zlWdKr75gvsYZ03zgHyIvpU35KFbqbGG5rWkPY6rrHZnRm6Gqi7V4UPDvFknVJvVxqjv5qU94zKS61emv5czPasf/LvP/jnhy+5pPmaq/o6+WqW+62Te/+K/WnS/853/zlrecR0YsYFJjtKGYlF7pmG9l4db9orNYXx1JGdrw+u7tyDcapUEYGig5cWCQqG4qK22gNAjYEORHXawPsLq7OI0xyPNGWPhWX2nSJ1iZrAAqvP9d9KW98JMt5kEAF3j5berzLMugJx+sp2BnMv61DXwdg8pSXqq3K3d6KkhYxsVlzSM/3cL7g98aCHmIid8cIS3toF7Mh5ehvlT7uS39nVCFLIhmIsPROZ8X/qkJ2geRRX2DHN9RM+k+5ZKPtgP9Qd7MozyNB7WjkFcZsB5p1ffW+ifRkxhlGenSRN5I+KcyLQdI0Z31O9rLP/3L+mEfnDTW4d91bKRN9crmEf+lt4ML2toRpzpwIkAbNTF+1cd6cYplGkPMYx3SZlne8Tr0KkKqcaH+03xj3LdZUn1ND/jnPhL/2S74Z3trHukDX4mjFP+ajEziWF/5M5+06kuW67Y3/Ds+haelfRBZHfhPMO/2o16zw381ltU+bnvDf95xUZqJtKyXJqVXulSmDeN/L/iP8UM9lZfmaz2lTfXK5hH/aoedFf4D+8pNLOpjJvKjbmZG/Hcf/5lSn9MXmm92YfznPnYZ/45WdbAz4D8zGYrSfaeU9R4s/JOW9kFkaduxL+vEv0uUSz4z4z/K03hQOxT/6Ir/zrpMmVwIp890VFF66lXxuVyI5U/1Zpnxi8zaLuSZZdVFIM03frziRaUsc0+PpXpls8C/TfFv4oIyvE3Uxc4K/1XfMtH/xrjFV0j8UDfTK/5lQSlNzAt6d+Dfl3XDf6v1IOE/+pY62Bnwb34v47/zea/4Z5mO+bsT/1nyKnPWI636Pq3LEYplpEtTpBe9Ep9Td2vja3z1Rua0vSDxw3Nb5cV96s96zCNfJmvjTSJ8taTKyPwcbveP/1EnTepjJvLLZoX/6NM6WcyjPvSf5ps/hPFfxgxex7GlRaPR9Hzq43A+8c85/fT4d3zmhn+X8ty93Y385g3/vi/vbf7vxngrPmAiLenSpPRKl8q0PYz/dfinnspL84uyRGtqClZe51kU7vuVRVGgKIqQP+XpWEZaay1arRbgX1WpZaRttVphv91uh1dj8lWm7Xa7Iot14WOgkNekpkl9zGTnhP+IoTo5qc/ZTprPdrC2ei3IPJj4l5ihbvYPcvx3fIqyQKPRrNzITVnadixL8c9EuWY+8O+3veI/rcvEMtKlSemVLpVpFf+84ZXzzdBeccGXWy7wKq+Yn4XXIcfrf442+ADVm0RVN5VVPmTGf491U5XJb3XDy62TFXzSE/6rODP/i//QFkzkQ1raB5E13/i3ijMT1zayGgybOeB/dtf/q3GmdKlMu5vGf62ntKleWXL+b4MMV1Y+ZPDv8liHtMyDl1sni3nUh74wG265xbKAwtRgKpHSUAkqoobSoUXhGkcdXJbV95u7vMifhhAArm71yVXQSWKM6lH6R+JDvjRWu90Oxqd2sizK0o9u+0bJqx1BlrkLVEVRoNFooNVqhaAwxgDGfVeDr9NhHfJgMNKX1I0B2/Z8i6IIi8XkbXwwQzpUllmZ1Ftbfa0d/Ml1tLMaGMwv/WS22XQnX5QR5PlvzRTiD/JytHHwrkvUD+J/2sVjF0fy/v2ko2SeJo0HXkSgvzPpDGgvY41+RpdOhPtOZCxPY4T7xsTXFLJuWRThSWwkgwSTkxF1U96QDir1Q92WyeHIdUg6MDAZtlnS4anvSEN9qSfLKJOy6GceQ3Ct37tT/s62eDcV66b22LL66sj0dQ4xP/qD+OfFz9TOTvzLICbxE/SVtuiGfyNYpq+UB4+dL+OkhXXIl21Gn5O3S97nFXujP+gLtVf5pHR6EWZa/IsfNTGPtLS7LlE+/U+78ixDq91GI8E/eZOujrf6Wm1n2a7j3/tHylUX7qc62iSe4cdDM2v8RyypjLotE+WaWvxX/apxor7TMvqvzmbKmg7/sxv/a/Avdmp7U77mk272439n26o/eIye8e/q8DvwyoO+pG6zw3/9+I+54l94RPy7i1raPupHTcwjLXWpS5RP//PGBh6n4z95035rrVv4Cmh88PCv5XU+Vx1NN/z7xUXyVxnaZqSHxFzqh7pt4Dkt/qvYTnHB+Z2W0X91NtPGoj17/Os3emzy2YSKPWInF4DJgzcxacxQ5nT4b3XDv/9uGcz0+G82GpiamnIXSqRtNN5YJ+VhrXuNDHWbCf98Wpip9OdaQfcZ8I8O/Dtbq3MIwX9RhCeCMI/450WHrMf5P3mTro63+lptZ9n84L+KV9WF+6mO1trwGQDmKZ6Un+qW2qltoDJqt75OOSv8x7hQ3ykN/ZfazPMzbbeyLP23W11ZOQ3+1bZyluO/FR01n3R5ozE3/Iv/1R88Rs/jf8ojyqYvqdtM+CdvJl5AT/VVH6m9yielUx4B/w/G/L/l8Z8ZZFmOdquFvNFw10/kyXHaoXZqUl+r7SzrBf96TYF03Fe/Ma/O56mOtmb8T2/wJ53qltqpbaAywjb5/A9p6/BPrupXjRP1nZbRf3U2U1YF/z2O/2qb+kufKi2tRbvVwtDChejr70dff58a4nSiPzzKrB9rgm3UN1SLZawDX4/1SadtEfzo470o3SevAg9jMDkxidbUJEZHRtFoNJw9NeM/29zMCf/zNf93sclrK3PBP8cAxUy3RPnZQ278F9/LTausSxrNtzX4py3kTzrVLbVT20Bl1G2ZKNf0NP4/CPj333JnHnlw/s+3Dun1UtVZ7dT2pnxrS+RZfAW07WH+r+f/+vAB65OO+vIYcx7/4zVE+pK6dcW/9wvPk+mRchfxn15LZb254J95pKUudSn1P33G4z88/MeY0PI6n6c62jngn+NJ2YH/1A+xzXTLRLmmC/51bNQ4Ud9pGceJOpspa1r8z3L8T+1RO7W9KV/zSZfneZjjO7roh2zG639OrvqDx9gF/POYvqRuXfE/z+N/fvYZZ5xHp6kzSERBqhTplDnrMDl+vpMSevJVJ6shmtyF7iifRjFZ6VwqxiPeMaJy0n11FhuEeVlW/d6ItdVXwFEeF1LZSNr45JvL3SuqpzY87TAJEBu5u0tU69BeJtpUV97N5jABlvbVcnY4rMsUZOlT1okOSlsXM3mehxMfyiP4+KuLRz0JMMbdba4narRDwUUZ3E9jIq2n7ad8mPTiSC6L6mldtaEsyuAvXYgvwzcXom70FY8pS33I1JA7j/jTdrfSgTLZpGNEEnPw7UNa5V3XluSn8Yhkcqr05Ftaf2NGyLfyc4k8yYPt6DIj/m3Af4yp6fBv3UE87oL/IMq4iZfqQx+Sz7T4lzZX33Ofv7qFuLQtqENVv6perrxqM/d5TP24z2Nd/CVPTTzuJd90iRn1B3XoBf9qC3XWxDy2JfPUljQm0noz49/rPRv8J7bEfDe4Q3Sjr+rqRZ2dPbsF/zX+5q+uLclP4xE94D+VX5fIkzzYjpqYpzbZGfDPfaVnWzNP7VE7eUx5/M0G/+nTmPyRdxpTdXql+qleWt7NZurHfR6r7sqbSWXNlG+6xMz0+M+RzRb/Piy4KMa2JF3qW+XDfJb1in/MEv+60BXyi+o318ue8e9Sr/jXm63sLPDP+ZYxbl5Q15bkp/EIxIXtUF9iQ+NM8+GbkkfkSR5sR03WuhsAsqx649K8499//5fH9CF/xH+DF6t4flCDf5WhPGzSFqxbpxcvlFEfxhDLNQ7qbKbd3OdxuHBeg38jx5qvxxX6LjFTwY11F9seauM/Zol/tUXz5zb+uzQT/nUBlcn2hP/dP/9P5dcl0yv+6VeJ3Xr8RxtVB+tvNGG+qcP/PI7/KkN5kHcaU3V6pfrx3CEtr9o/M/5V98g7Jh73km+6xMy043/u5gBl6W54R008kk+dDmae8M9FrDQpTnYV/3zSGKIbfVVXT3VGN/z7a1RsS40h5jPueO2kThZplXddW5KfxiPmCf9Z5q/BJfhvt1rYY6+9MDC4ALk89cdPRVXqavx7XiEx1qUfgadRnYzQ8jjVOfP9D+UayrMWjWYTzWYTzWYfJiYmgg/ZDvwhaQttO40rymNSP6bl6mf1O/3JfR4zb8brfz3kmy4xMy3+H2LjP69jpnXVhtQWzZ93/Iuv7Az4J786WaRV3nVtSX6sw0R+/JGefMPbQJKY0RE+y+JbKikrTXzQQW2y1qLZaISHzVRuRQehZ1tr+zGpnTymPP7mOv7z+qGdDf6tjU87i/9U77QNuc9j6sd9LgC7PEdLnppU1kz5pkvMPLTxH+vu6vhf9oB/vW6QPqHbbDSg+KBczBH/Kou0yju2ZcQB+bEOE23kj/Tkm8qvS+RJHmxHTcxTm2zX+b8vnxP+66//8zdX/CsP8k5jqk6vVD/VS8tT+3lM/fK3yzeAU6WUEffVCRrYSIIrrRsNzIIzWZ/1XDn5xc6BjaOyKIcOh8iHfK9OdUASTFnSMTFfiKOjGu6OBtIBcbAyHhx1PEzmO3nRmYn2wZepLtwyWGkHOwnuV2jTjk546X7IEx+Qr/W6kgZ8VVECtMpr8ZIyp1/s4NTOwDdp97ST0pTawqT+h/gwAEiAmPu7X/hDjV+5ZR7rxfhz/GkPfaX2Zf6uDWPcnczd5NFXqpPmMXGfeil9qovxA6nyI8/c3/1GfpnHX9o2mT+RoW16oZH8SDs3/Md2V/zriZzWoZy0TO2ycE/npNggnSb6prTxNYiaTz3TvDzPUYhvNWXT4J/yU98wj7xc21b7QG5ZFzPgX5/6SX2WtrPyJb3qpzbW4l9kp2WqXzf800+knQ7/RVnWnnSnutKWcBf2vOM/xg75kk510FjoJo++UhrNY+J+Ff+xH1AbzZzwX40h0tM26st9Hpt5xr/y1TqUk5apXeStfGbCP2nVdubX0eb+jkbmaTLzhv+oi25Tu3RfadXHqc9UVsqX9Kqf2vj7xn9qC1PQNXN9X5blMH4cIH9u5xP/ypd05Jl1wb+pw7+/YMnXotF/aif3qVfKV3Uxc8J/tW1Ib7uM/3nmL3DOhH/r3pajZUjaXduJfiE/i7gAXdf+ape2Q9qePGZSv9GfaX6F1j/9mzfcE82k02QE/xx3OBZTfsU3PqnvMznBV520LqbDv3wP05j4xhLlUbG1C/51DsG0O/HP+Nol/IsPaQv5Bzm/Z/w7usibvlIazWPi/lzwnxOvs8K/a2vaRn25z2PTBf+88SGta61fcJoF/qlbXfvTVxqbXIBBN/wbVM7h6E8kbRvIJW/3jP+dsYsEI1oX0+E/uWib+oy+TPMol3yVB9PuxD9p6/HvaMuyAB8E0JTqqraQP7d/GPiP8ugrpdE8Ju73jP9WO1x3yGYY//mUHfNUB9pGfbnPY9MF/6yf1mUedc1mwD88nimHZUVRYMHgIAaHBl0eX33u7wg3xo9tnofyc3TJgq6nN3W49j8L/5kx34dVqTwNy1IectxoujcQtFqtYDfL2bZah1v1T3f8x3hMfUYe3fiSvtJ2ovds8c8bN3Yd/y6ltjCpvfi94j/6Ivt9438e5/+kYyI/0s4J/34+neVZeDBG/ZLyc3I6+3+1S9uBfMrSXTNSHZC0If2Z5tfR7p7xPz5pnOqiW/VPWRSVN8DpOUPw8Szxz6c/o37VGJwt/rUN/vjwHzFK+WpftpvwX1AvpTfVa5HmoYB/aXdtJ+WrdSgnLVO7yFv5sI7qAPIIMl1MMJ+6KC3z8jw+hat6kG6u+CevrFf8z/P4bzbccovVQgook5VrZaJGkKGROwQiPxdQDDzyZR3HM8qL+fXgSmVzj/mBpy9hHl8jZxLHWB/oqZ1h33/nycJ9Y4R3FRgPPKYO+b6DzDxgnU5dbJGAIu/C30lQlmWoT931dRjWB0bL+5f5xsQnK0sP8sx3sCnPSh3eCZGUa5uyjeFPOCkrtZ8dJeMolUO728krOVQu6/DE3hgH3rIoQBBXZbr9AJAkToO+Pp+dIhP1K/xrIHh3jqOP9chDddMOQNsvbzjb6Qe2Rzrgqf2UQV70P+sxtgr/vRraSxypnrmfuKh/1AdqC6bBv5H2YF2mOl3JL5sR/xwM4qs3TPB5F8wkqWKDBeDvClS/dsM/psE/dbbWot1qo9FsoPTtrHo4udVYpB81r84Wyoly3eskUp3UDm2H6F8/+Qr8ou2kizLqdbDJjR0qg3QB/7WYr+7TD3X4534v+KcO5E+6OplIBl1Nyg8AGv6VIEzUqR7/cas2ULeu+Pe2c5/tEfEv/dys8B9xTXuJL9WzN/xXY5980hhM/cdUpyvrxPicCf+d+dzW6a2J+d3q0hbuax31qfqANtGedPxXPerk04+a52iycMGJdVK5c8N/Jz/WIZ3KSPXmfl2580HUTfFF2rp98psd/iNNaif5sw2DTItKDHNRyc6A/3xW43/cqg3UrRf8N2rxH7+VS7sog7wYg6zH2JoN/itPsIgP1BYI/guvr77SMPUfU52u5JfJqz2pH+vA8+yWz22d3ppSG9K6bAfua53Sus9R8EkOpPj3r5cO4/8M+DderrtQU4f/euwB7jWSpkf8c6E5I/7lhlnqwTqkq9jWoYPXu+aiUpZl7g0o84z/zBi0kk9yqFzlMy3+k33VT5Pywy7jv+qfXvDv8jo/gUS9aBdlkBcxxXplD/i3nkcjz9GecfyPZY531F1jMPUfk+rKBWDWCfHpX+vLJ22VZx3+ee7WTW9NxsQLYUjayxA3jdx/M7AzxvJp8J9nbuFn/sZ/tSX6TuX2gn/KdP6tLiildUinMlK9uV9XzvijbvOFf1M3/lu/SCDzJepA/mzDOpmYB/y3e8J/tQ16x391/LdJnKa6zBX/8N/YzLvM/4kvtQW7OP8fGxvD7WvW46LLduB3dyzA5tECk/0bULQb6J9aieWLgUceNIITnrQEjzz0Yejv7w/60/agRxf8T01NYc9le6HRbEb58E//+qXZoJ0DmJNh4oVfV8fT2XjTiqvt29nIGCl+IZ16gMehvuitefDfIt6+dRv6+voizS7jf77n/z6e5oh/XZRIdU5lduBf9ErtDPx3M/57G/8dr3j9Ly68zAb/5Kv2UwZ5zQn/nkc3/NfZgl3Ev+rKOhqf5AvEGzeov7Y98902xmOdbM1P68LrTlu4r3XUpxUfeJtoz+4Z/6ufciHvrvgv/Ouw5U1H+Tzhn1h35ajqOEv8c5/8/rjwX7WBus11/CdftR+iS7sowhzUyrlqnnFe7+IM84B/Myv8+yBJ/NYz/oVnt3xu6/TWpDagpi5t4b4NdWJbqJ3cp8424N+9Cj3Vo04+/ah5dbZQjsrtiv/dMP6b+2++2SpzNUAJmc9ERTRRCQq11lacRhoel77R6zoU0rbb7fAO+tSBBAXrsrH4nd6gt6dXkKa6Q+w0Jn7XNsvcE4asY+XkGnUO9fuFX6QM9iQ+DPzEJ/QD6ayNd9P5Sh0+op6QDsAYfbWuv3uRPvd8FXRpx6R+hdeF7a2dTPj2WtKmHLC1PusRFDzhZpukHUfwo0y8y7JEo9kMurFumujbMJIlKZQnefSH6uB0ju+zh3Yw/mKzlThgmcncKx7ZT6YxTl9Y8bW2A49pt/LQtlOZ5E2enXZ04kz1mRH/lDkr/MdJE2lirLiBtk4v42mnwz9lsC79mWdZWKhlMtPgn1SpjvC6Ua617tU1XFxFgn+dzKksTZSrOlAe/cBFQdqkSX0AmQwB/mJV0Kez/YMNM+Dflj3iX3wT2zT6Q+uzXiaTPdMD/lnHEv/y/eyZ8F9XhsT3mkd/pH7L/ARP45SJeerflJ/Sqb+cXVW807c8pt3KgxdokdhC3nZW+I/tNiP+xe75wf+ujf+UwbqME8Zayqsb/pWGW9WNclUeaVPbuF+Pfx+XSbtRHv0Ab4/a1G630S6K0K8VZQlIbCAZ/8lX+asNpEUd/jvG/zjxZD3VTfmnfnf1Z4N/5wPyYB07Hf6DqtGf1sa7q9Okvtc8+iP1WzYP+NdFaeWrfW3v+J/9+K+fMNAy1Ufxrwu/ugDM1PDzRE2UXZZlsMvdNPWHh/9Ud9JwG3Tzc9xUHmlVjvEXUgB0vi3ELyZZT9f03wIM+pRl5WlryqJvNN+YeGE5xJh/DTb1MTX2qA2cKyDEnbtI0KjFv79g4WOIbRExu+v455OqqjN6xX+SaGddGaQ8zaM/Ur9ltfh3NMxT/6b8lE7HW9rFOvOJf10QVXlKp/tlBf+dcU1apm7jf9lt/Gcc94B/cjWzwD8vxNtu+M8yh0kff6nuxCWSttMYV3mkTf3E/frxP/rQ8XN5lEc/kI62aFIfIODfMUrtTu1RGzSGZh7/fx/z/4grlpUPIv4ZD5TfiX+XmKf+Tfkpnfory+KFXcwn/uWmUtJQHjxWWKb66Piv7ai0TIr/oihwx53r8JOLNuPHl+yDLdv2RnPhbViw1zUoGlswuGhPTI2sxuj9h6I1vBx77bUZz3nqRpx4wl446MB9K3L1mo2pwX+r1cI+K1c4nSzCwx7gDTmw8SmtwAmA8W/F8GNjtfU9SdiptiMXkmGDtLiwKzobXxfw10pknGYqrcWm+zeExW9XZVfx7xLjIm038jc94d/hS/3n8nvHf3rdTetlPePfbVnHPsj417xsBvxbIHxPkmXKj3Ssq3zpa8wn/tl+NXYone6Xu4B/JsqmDbbu/N9fF9Xro3V6kV+71UJfX1/t2woow9Utw9tLQqwZ45Du+wYdk1PdyZNbXuvUuFR5pE39xP3exv94LUDbh3S0RZO7STTmlaV70hm7gP/0xmS9JoU54L/O5tAmD3n8V+uyfdS/KT+lU3/RLtbphn+u8fD8MU9upHT0EfPkWWeH6pDqw09F2Z7wH9uBibJpg63DfxIrqPGN8kvHf+VDGaxLf6Y4IH2IF/GZplRHVPBfbSvSprZxv1f8c1/bh3S0RVPqozTGUn24Zb7yLcvSPQHMgmLeP/hdNZ4KZbJqbTz423P44LeVBoJ2NPJdgKKIdyXTaCvv7IbopTxsaITke7c23lXIutRVdbQeuGGgFFu0UdMF2dROfZ2KnrwGOjkOPMsSmX7wWwNLbITsM2B5Ap/J6wNSnay18dU7pvpO9XCRW/xB/iqTbcdjxhXt4FZ5Gw9ebUe1m74tiiJO1HtoK5a5uzziXT+RNvpBeWf+FWu8Y5gp4MXfyaw6MqV+IZ1uIfhiHCk/xWJarnUUQ8o79UXP+KduM+K/mqh3FvAf22w6/HNhtY43aSE+pY554l+NmxT/bCHScV/9zTxjqq9YVD/SN/S7TpTZDuRPOtXNsYh2ahtoW3Vu3ZOFpM1zf6NFzSQptTET/NuyR/ynOE0GY9WV/FUmesQ/y1WmtqPSGcG/5lGe+iy1yUyL/1hPedNHmocEL6mOTNEv7g5I0ukWXfEfY4Jp1/Dv9nvGvyTmpW1bl+iHbJ7Gf/JSexgbLOsV/0yk4z710HLVhfupjrYr/t2YofxUN+XRarVQFAUK/9q7hYsW+ScHgP6BgaBnZ6LO9T4DEK7RWF44UzqXyWteYSsE4NxO+aQTakej/qIfo+/QUbcTKy5VZcY6VXonS2PU6VDd77wIaHxbVNpanioJeeIIYwyQ9NdAVCt9MqWOKMhUR6vD0z6E5XW6SLnWsdZfzPPjXKjFdvZ51vonSxNfcJ8+qqQ6/bomR2OMvwjt88IxeUk7Of+xbg1vk9wAUOc71q3BLZwGZBBu9iS7yrH4IuWjNJ6wkl+WJSbGx2H8Ra2R4WGMj4wgy3M08hz9/f2uH02wqH2w0TFV5EYbXSr9ybyZZvzXGxJcP+n6Y3Sb/5fxQpPaxa2d4/hv/HHh+ad8lTfztB9XOvOgj//ue+WzG/+jj9QvpNMtvF46jig/HYvT8oJvHOhp/Hd5bvzvQ7kL43/djRWAx6m0X7fxv70L4z8Xgalj6t9MLrCl4z85s124r/5mnurC/VRH23X81/m/o6dMlqud2gYqo3MbqgS5Zhr8q430E3mxPbUdVCfmYR7wz+Oy9E//Gjem6kVu8qYs+krzMM/453UZpTUd+N/1+X8a77rFXPGfTT//J0ZT+xz+Zzf/37ZtB351xd34xZUGv73hYbjzroOBfmDP/b6LocU/wvDmJhYsWYzmwCLs2PA0bLvv6cgwiQP3vwPHHrUWT3lChuOO3Q9LFi/sCf9TU1NYvmplkG9MHP918ZdlfKuG1Vgg3kgXuPlZB9vL+gc00nK/hewbwPVv9C3b2MsG/Q1g04aN6OvrC3l2XvAftZwf/OeVm7JUJ5XHLe2Ax47qSv4qE3X4F36qM3kzj75K7TbziH+VqfXq8N8u4lOEmCX+d9f4Px3+yTu1by74Z17atnWJeme5fyuQf1V9nmVotVv+NavtsJDreBfu2lbSXkz0HcSn1DHP3E1fpNG4Scd/JtKZmrhjuerC/TrfahugdvwHeJ5A3VI7YxvI4nVp45sxamKMck2P+Od1UsouSxeTaVxqffLk1s7H+P+QwH+Mf/poV8b/XvDPuby1emOnYrF6456ZI/7LWeE/tpPSqk/TRD9k08z/U3+o7nW8SQvxKXVM/cuyMuDf9dvUS3lwn3rQXh5TJvdTHW2P+KcM6pbaqW2gMuq2TJRresB/ftbpp5+nmdqYrGikkVVYanwaaCq4rlEpt45XnS7UsU4f7cA4sAQZNYHJ49SJ3A/Hnleg9TLVDyxL/aNlkFcKaCCoL5TG+iBlXWP8ZFYCHolt1IF8mUcaK50nkjtorO9c1L9BhnTu9FFZuru3eKLk7HZ1jX/1AH3Bre4HnWrijnJ0Igm4xXD1mf7UJ6jphMmTMshD7aQc6uTqVWOdOqmuagfz9aYBlUP7ua80lMFyzYfozESQZzIIsX7uL3aQjv5gnu6zXtoOlEX96ROTuW/Fqb6k4b7qTXmkVTu0bZSX6mJni3+VL9jQxGPSaz2bDP6qK2WyXPllmTup1HyWYT7wL7pqcsfxu8battSVdbQsxT9tMJXJRSyDxGMdf/XXTPhPZWrcUY7WY576TH/Uj4n8tIz1WW56wn8sUztVV7WD+eTFffWXyuGlBLUjrcvjGCuuzvzgP+IgbQfKpf70ieZrG9W1C5PWjXZEbKS86nShjnX6dMW/T5STHpNe69maeCYtZaof0jLNZxkANBrutXV8+wVtVPpGo4FWq4Wx8XEsWLAAS/fcEytWrsKiJUvQP9CPRrMPzWYjecuGwz/4TVljZB1O7Tb+QrGnt3ExsXJJy7DfTMt8eeUSWJpcebRJablf9Y8x/iKeIU1dcvlBNckDkNhCMenSq4kLZaS3NsoN8qsLaikX+BuXKslfvDaeT1rfxQXFplp5w0JGdV/jT2tqfLLMme2fRPWO4lOppOO+MALH87BlvtRL80M9vx/0Mz6GUhkapz7baxMWab1Ex6/SDv4iLozbD350ufQvaX0jJHLqk5GFeu4zX/1EH9CHaaL/1D9BQ2PQ19+PZrOJvv5+LFqyBEv23BONZhNTU1MYHxtzNHJheLrxXzwbaKyMQbxBzfY8/se7+k3d/L+MC7RarvxZZuYw/vNNP0xpPeZpn6k/2sfE8UHLWJ/lZpfG/+or3FiH/MmL+xxrU/uVhjLSujxOx4rpxn++Ko509Aft1X3WY15qA/WnTzRf24jjmv6YMr8YTV4s07axHju0KdWFOtbp0+5p/Hd9hcolvdazNfFMWspUP6Rlms8y7Nb5f8QiY5BtS11ZR8u6zv/r8C96aLnyV3/NFv/a1q77//3iP73OQj7UKeia2MF88uK++kvlUILakdblcRorXfGfTT//t/OI/+tvuBv/8aMMP7/sKNy/eW+YbASLl9+PJct+BVvciAfuy1G0GhhcNIn+/kWwdgkmJ0ts2bYMa9fvgWJqM1YtH8O+++5dud5Tpwv9vHDRIqevcZ9nMzAowydAOI4DlflHihnJN4ZzC85OXOIx+Vjq4eul/JUP63OOBLmYu3PHDjQajUosM80N/+5YY7AOn+gZ/14v4a96MB5S/iwzu4r/xF7SmwcR/4x1LVM7VVe1Q+NV66q/VI7SUEZal8dprHTF/6zO/12qawfKov70ieZrG9W1C5PWDXaY6AN9yIY2uYVIN89ysmKblkWBTGKMb/dQHkawp77WY9JrPWvdTSKpHfSRlThQfql/tAzTjP/6pqru+HdzeuO/oRzmMY441GEMarzxhy74t0kMG+N0ZNL69Ecdf/XXHy/+q3xIzzrMJy/uq79UjtJQRlo3vFWqK/79Z56E/1zwz7dCpTZQf/qE155UX9Jwnz+mWFfwLz5IeaUxwXK2aVWf2V3/Y7wzP61na+KZtJTJcuWv+miirG74V/ru+I86qi2k5ZYxqPHGH2rwn//NmWeGBWA1VhtTK1KAJmVOegaJGpA6hk7gvjqvzpFMrEOH5/Loepa5SSGP6+ppUh3UwfrKKnU65QVZomfpV97L0r0GhXoZY8Ldx5qirxz/1A4g3tUMuAVQraN+SBMXZrMsiycz0pbUu+L3BLx1P7U3PJGcxAe6BDn14cl6xotVAmzW11c/c+EXSTxRDo8pQ/VRgHHLpINUHR1PSCzvJhOduEVN55b5GKQ+kLghfx6rv5hoiyZ29ukPUtfWdBraLqSjTN2n/spTj5VPqG/cBMtad0EyS+KTfHlsjL8iawF4/5CXmQH/ltV6wb927oFDPU5UB8okH6VJ29HCXdRSPUuP/6IO/8mAy3xuq3ZEHKkuwYeJ3mGSjJjSC7qqJ31EfrpvjL8MXhNrKR/mkWev+OdgnU2D/4AjL0/9QdmkU11YTrl1uGaaCf+pz1QnblmmfPSYNLYr/qt2sLxOV+brjTbYZfzn0AvTylOPlY/Wh7QJ2xCJD3mc2kT9uK/+1v00sQ79PB3+6+ppUh20zZSWeaRh3Gg7Ixn/TQf+Zx7/jTEYGx9HlmVYsXIl9thrL/T19cvNRMYP4axX5ZP0AJJXLQ/0Ff8qXbcy4/kqP9m3Ws/RdTZhXHQ1AbOsp/QqJ1FHk/XzmpTAyEpxKFL74OeoXo7XqUInKhjjFwmNszMcx8uNlXYMi5cJD7afU9tjgvW89Dp7SKe/6KoY504/8YkeB3+oX9UnUW5Q2x/rneaar7RBR0kxCk10REjSJ0Tj/bY6djNRtupAHj7iRGo1iccqydlUXXAOtH6jfQnlpVvusy1DOfcT/2fGoH9gAIuXLkXfwAAmJyYwOTGBLMs6+jTyJs+sMv539mu2ckGn2rfqkz2xLPKf7qd8KvrMcfzPM3fTXP6QG//jnd2qZ6o3aay1yPOGi2uf78b/aC8TbdFUHf/jD7s8/lfHPuWpx8pH67Mu0Hl+WilzASa1on7c15sn1fdpYh36mfNx1y7Tjf9x0Z5JddA2UxuZR5q5jf+zmf9H+bpvpD1U7zq77DT4V721rJef8mEeeTI+MAv8UxfqqfVVT/UHZZNOdWE55VK21mGaDv+Mpzr7qK/KUj56TBrbZf6vb3hjoi2a5gv/dh7xPzExgf/68Tr8+prV2Lx9DyxauhF773cLDj5sDZYsWYPx4c3YubnEwOCe2GefhVi1L7DX8m1AthOmaGBsbAnahcXCoQdwzFHLkEn/ob7XVBQFFi5eBEh7ZrwZMszL6lMdP9CXrrob7lPZCU8+1Usa42lg5cYBY1x/yPaUeBkdHgnt6aruKv5jezLZecA/37ymP+XDPPL8Y8I/ZoF/17aufqo3aWwX/Ku9TLRF03zhH/OIfyb1Oem5VV1Sm0xWHf/V37ofk0NolmWAt81a/9kSIFw3o0xU3gRVjxP6CCKT7as0aTuSRvUs5zD+myQeKEN1Cj7KMnfOai2Mce1guthldwn/sb3Sn/JhHnkyPvD/GP5Vz1Rv0th5wH/m+2T3y8LCMD+laHcR/+zvHc8HAf/SrvSJ1kvpmViHfk5xoz6vqxdzO2OLeqiNzCPNfOKf2zo70n31oeqdtgd8PdZNfat652eddtp5rERCKqPO4JZGqAAeUykHcAD+zvyUhkpQZlrGpABV4zO/iMgyKwGIhKeCjGXqOK1PGeFEVPThseqoPgi+qTjbX9xL/BPk1gQppB2yLL6KOixICw0T9Qi2eDnWxtdeMTBTHsZ3Wmpb6lfmha1xC9qc5JJeAz7lFfRJttrxUkZY9JZOXeVre2qbq+2F/5A2dSJNKkt9rTxcnptYwOuk9MorTRadnYPW0/x0UCGt+oX5Sht8JZ16KoO0TKoL62hMsJ7dBfzneVzgZ36WZ4Bxfgmy8xx6oqU+YeqGf76yRG3FtPivxgDpKm2ueLCd349MdQBQWWSlb8jPmHi5mb6ibMplWZqMvzMy9W2VplMPlZ222Uz4V9tSvzJPt7SBcsw84l9tpx51ZajBP2XtCv41jymlV15pUvtIk/JmPl+3k9r84OG/83U5dhfwT99TRh0NZVNmWsbUDf+UobYyHwnPuYz/dbqkOiDxAX1TV590PGmjXJYBQLvdxsTEBPZevhzL9lmORrPZocP0ycJdinJb1nVb6kOamBxZZ35ninGE4A/Wh5MZPgsR2yCUVfRxeZEn81SPbvpUddU3bYQ8Exc9nbzIM1AHc7wepLPegJBXTbrYW1lQTEiNcQuKao6v6dvD7WusBN8whnzVoIfGlbevErtK78trk8hjfWe2qxf2Uz56LHTOItlP4l9GQm+/2BTIOmOwGivR307vWMIU5bht0Mm4+qQJ/vZ/+sRvUC/uuE2Cf/Vdmi/VOhP5+ENa3ezrw+KlS5HlOYZ37IAxpnI3sPrTsYnH1lr/WrgYT1zkZb80/fjv+uvAM+lXAf/tMS8L8zj+h6dGhTfLycv+UY//u2f+z3MonreQr26z3TD/p+8pw1p3Dqo0lE2ZaRnTvIz/jTycq7KMdOoz7SvqdEl1QOID+qauPuko28mNfksTeaS+TWmYHP+q7LTNpsf/H9r8vxPXKp9l2A34Dzd9Pwj4t7sL//7TU6Rlokzluyv4v/Gmu/HVb67A2m0D2P/w3+CEZ12DF/9pA0c/cgmyoo0dG0fRGB/D0qVLse+K1TjykNV40nGLcdzxo1i093WYKIex7v7l2LJpEI979DYs22tp0AVd8F8UBRYtXuw+82YB+OsK1B8uyyXrHx6QdjKIn1UzHHekjHMb8mIy8oPWExnWVuds3Ff+xhiMj45VxvY0qd9J06FPB/6rsZW22ezwH3Vg4j63jDeN89wvxFV5deqj23r8V7FA+9Iy6qF0lDVX/JNHKielJ6/O1os6kg5JPc3fLfhPcMukurDOruBfdaZc+p4y6mgA9xpoykzLmDrx7+rk/pWxvJ7IOY76DwBQWuSNRph/sIx06jOWBZtr8MYfk/qAvmH9OjrKplxAP4UTU9Chxm9A/KYx4PoU5a9yyGP2+I+8mLjPLW2gHDOv4/9DB/91Se0jTcqb+bPBf1GW4YbZ0rqbuXj9rpv+1Jt8dZsl+OcYZh8M/CdY1TKmTvzHuj3P/2e8/ldtW/IzxuB73/9PfPGrX8FzTnxWRYfb16zB33/203jXOe/BV//p67jn3ntw3GOPRV9fX6U+k7UW23dsx2c//3ncdc/dePTRR1d0vO6G6/HiV/4ZvvL1r+ErX/8avvpPX8cNN92I5z/nuYEm9U3KX31BG+n7afG/7sYbLe8aUKalf8c6GdB4iEIUqEHMfSfUvWefDakyWFf3yYPJ+gYs/Hu89QlM/mhY0M0PyZlfJO4oT4KFTmF5eBWZn2zSN1bsZh0XQPGuD/f9ktyD0oRBrjZJY1E/+gB+YIi+cBepWBbqia+Yn/vvqDDVPf2bBgI4EIkOaiNQ1Vd94YpiGcGf8qJ/4Os25OPgoS7jLOk8KYNxYGsCPpdXnrGc9ZQPdeKW+qqPrHUXLVSHsixhS7eYybyiLR2dLPqmSfkE+kRH5qm/Ul5qr/LUpHVCLEmMs5xyyrIMMa78ytngX9qFupdlibyRo2gXyBtV/BvqUlq4i+G94b/il274F/tC31OU4XqzlqMG/5QBf7dxU+6oov6ujtPXGIOycHVUT8robCGXtA0VB0527N+YYlnUQ8vhFxMa3l887VQ5mAb/gWfZBf9JHOu+ypgO/04vV7cO/xpnyp8yZsI/dWY56ykf6sSt4p90SsO8UvDAPNZN66RJ+Sg9X92X8qjEuaSoZ2f/yKR12HYa4yynnLKMY5zyU3u1XSD2kJ/qy/2ST8PP4/ivcvjrBf/dytED/vWOSurPOowF1qnDf0zVtgo2G4Px8XEABitWrUL/QD8AhAWumGwHj84UMRGTqdQ18iBiNZFGt0hkqg6dPN1W61UxGsqsW7h1x6nMehsj71S+23bYzX0T/mOBX/RjG5Q1soUm5FRPvAGvj6hjTFxMrCRhpJcFg4pefNTJ4yRtqKqjfcUkaR2WqyC/TzmU2ZGkzFp/kUL5JX6gvjTVso39wqT3oLSEN1r3jYlZgGsHtmvFdlcWdO+IC6dr1Y+uPL1YzJhhu1h5CthadzGdKY1j5aHtVilP25CpYk+kMcZgcnwcG9atQ568Epr9Sbf4sGXsL+EtVr0g/X60yteVBSS+Coz0ISX9KPdVxlzH/2w3j/+lBdoACutuVHEy4/jf8fRp6WI3zwz6GoCBjv9xfNA61C1NVV/FPNWReeqvlJfaqzw1sY71F0rtjON/3fzftYXqQz9SBo+tjvndxv9GI5zPRj9UcWJt52t3bTL+b24B95ZNXDaR4zeTFg+UFjYrYEwJa9oALLKshT0bUzimAZzQbGDvZh9W2ByNZMGVcV36pyKpF/XHvI//1aRzOPqX/kYSHzzWMvWfp6j4iyn4NsF/mpRnNxuUj+6/+O8OQZkDZQMoc6DI3bb2l8V9m8VjW5efuX0eW+OPjfvdc/RtQY+Z8K82ZDL/T18dntJsn9yOj//m07jkvkuxc2o48Nkdaa+BPfGc/Z+FUx91MhYNuNcca1I9VV9N1sY5icY44Dof8mQbl7X4B8p2GxgZRr7lAZgN65HdeSvy++6BeeAB2PFR2CzD368/FBdsfy0WHbIWxzxmHQ5cvgK3r7kHW7beie3bdqKYGsDSRSuwcMkyDBRjsLAoGg00+xo4/IgDcfuGdfjtb1dhZMPheMVz78KZpx5bsdnWzP/b7Tb2WbEizsd8Xx7Hb5eMqX4yjZZVPRr7g1AufggPIkifarSO8Q94MF4Ex6G8Jm28fwP6+/uDrPnBf9VfTGms9Ib/iKVe8J/J+DnX8V/9kOoMb8eujP9M1Ilb6pvaRhrmlTXn//FBByePddKkfFSG6sg89VfKS/VUnpq0DtuOfmE9lk2L/zmM/7pfTnf+728QVvspS/W3NfjX9rfWrTFQP9YB7Wu33dwjmaexHD2c/3e//rer47+3uWf8l/FtbfINYCR911zxD2tx/Y034JQzz0hLcOUllwIA/vn88/G5L30RHzznXJz49KcHnsYY/Pb663DKGWfg8osursTG9TfeiO/8+7/jZxddCABYtHARjn/csXjly16Oox71qIp+GmeqM2X8YeA/vrmBddM6aVI+Sq86Mi+Nc03G97Pa36ZJ69TFOMsppxT8600P0d5u+I8Lzqov98vp8J/owv3UZjsj/ud2/c9WfOPPlaWdb7jpRnztn7+By6+8Eo8/7nh8+mMfB/z19fX3348/P/mv8PrXnIQXveAFMMbg7z7xCYyMjuCTf/exoCd1AICf/vxn+MJXv4J169fhjFPfjNe9+qRgszEGv73uWnzqc5/F2844M5xbDi5YgIMPOghM9A/31X9KM1v8m/tvvtmyIrwDjHRyZEKHsiyTzo+MrQSArxmEq4O5DzGmTkE2lhqhRmf+TqAgTweWSrD6iwCJbKg+Esx5o1GxLS2njoEvL/4RMHJhn/kqh2VlMqlQ/RzAvZzkjk6b2KV1uShsjHvqkjbqBTvyMb5T1Uks2xlwT2kWHETl9UEEFpLOjf5K89HF967I+4H+ygysjXd/VPwsA2XwNTsaiRny5ZZ1q/kZyrJAnjfCwnSWuVc3k4cm1V1toz6qJ7wv2PmQXnXTY+ULaR+lTS+gpHUrMSl+TVOd7nbe8F+6xVC58YHy1C/UEfBPlkyDf4ie3AIutLMU/wmt4x9fbcEnXTRpu7Edc3/3U1lWv3vHcqdj9UTHmM7F02BXTXyQv+3Av9OLPFmPdLRf/cp+gndwOf60sLPPJR+TfDshI/7bEQ86iKZ56BH/akeaWMZ96jJb/JNHtD/KTmWoXB0w6Rfy0KS6p7alemJW+I+yWK7trLRRbuTFRF+k9qWpU3en3/zgPx3/u+O/W7niR32Q+vDucgEuKfbAjjbbDChLi6WmjSxMEP2bG9z9IliRT+GFS0fwnjuXVOq4ch67JwssgLJ0/cfe/SVOO7iFPZpuwqy+TnVT/WN5tZ9hWVmWmJiYQLPZxMrV+1b8FpOFv+zkt2k+0jWkmlStS3q3rfJXH7O8mhftBSIft99NCfKvS1qmOrp8suy0MepNH4d86yvQJsfJl3uf+Tx3Iu3byy/61ukaRyxfr9IW3nYT6YLfgj5VM+UZEs9AitVYwUri7JgPcVBKnySqAsQ6zl3CV9obpGe7K48kLgKvUFPleb+gesd7Wl5tZ3FYhxO9/NJWTK7SIu4zlivSnT6uVmwrYyI9aBvpp8FDwEXadjV+qfhejpnKosDGtWvRbrcx4C8W67hg/Qm7ScfGMupFeWmfm2V8jZyO/65fo4zFe++N5sBA1esi2+9U8yUvpbFliYnhYRRjYy7fJ+oOuAvJ9ON8jv+TyHHj5AAuKxbh7lY/Jtre9wWoNcKuAVo7W9h+6QZM3juC/ZY38LLH53jSETkG+x1P186ur6Y+af+uesX4SMeF2N7ki57Gf/GvT3XjP8+JNCkP5Vsd/+MYRrqZxn8utLCMyVr/9irxC+WHctrYZfwfsTn+c3QI17YauLNl0DIlSrQA04ZFG9YUMKYAUCDL2sjyNpr5JPJsCnvkJY5t5nhWticeZgcqssE5q/iY7VaxLSmf/fifxkeMZ2stvpPvjQvMnth5b0W1adPihwOvKrfgNdjqecV5PCT+UeNzxpfpNv+X+XAv8/+X/e0hcdG34RaArV/sLfyisC7wFr7MyqIw6cMx940sAufVReB7Hn17aK80Zmgvfa5twm3Rw/z/Pb9+H/7rzh+G4wcjvewRL8Z7jnsXMBf8h7ewVOfwpFYeylfxn01OILvyl2hcfzWw7j5g505kReHHAYvSj5ZvuPmluG7BY7DnIy/HyhV3wIytxJ333gQztgUDjSXYe/mhePihR2HpXstgt6zFji2bsX7rdtyzcRMOPuQAFAvWY+36/bD1vqfjmIeP4vOfPLgW/9TTGIPJyUksX7Uy5MfY9jbFbtzx4L7nsXF8O/5xzUXY3nbjkPUErOfG/1h30T57VsZtq/dsSb3VfUvx2mWPw0DWjHrDyQVjyo/JXAAm/rUv1fbVPNKRN8v5UzonNmo9O/xX8dAL/sm7Em9JnKU6MLGM+9RlPsf/VIbKnQn/TKo7bbM+3+kZrweh6/gfddNj5Yt5HP+1PZiUh/Ktjv/VuqaH8Z86s4yJ8tQvdTdVsnwm/KvdWZah3Wp1POEbeKJ6fVH9w8Q81mO7BfqkDWhfWo9b1T+tx2OWlT42+PkT1Y88mccFYBt849ulBhvkn9rIVId/WIvrb7oRp5xxOr782c8FHmVZ4jHHHIOyLPHNCy7A5770RSxauAjf+/YFWLLYXUcxxuDa66/HyWecjisuvgTw+v/sogvxnve/Hy970YvxxMc/HgsXLsTo6Ch+8etf4dnPPBFHH3lkkEF5tOEPF/+xvZmf6okHAf/pw3+7iv/GrPFfnSPPCv8Si2n5rPE/0/V/4U/Z6rn0Ov627dvx9nf+DU561avwgx+6ed9nPv6JcMNFWZa4f8MGrFyxItS79vrr8KYzT8flF1+GLMvw5yf/FVavWo0Pnfc+XHfDDfjaP/8T3vDa1+HUt5xRWQBmbHzrOxfg6t/8Bp/66Mc79A4676bx36y/6SbLQCUDdYg2qApIUyrEpXisRsC/8pCKKJDhjWOA26QzYCKfsvRPGvrgNL6BU31Sh7Xbbcc3scvxcwueWXiqN9ofefmAkMCkLppomzHxrg3KTnlmWYapVguZv8vcZNJBK78kCLhfWotGw01Ay9INtCa5EJB5IAe9krsKwr74tytN8goIyg2+TjoF+p40lh0e7/LIM8DffY4kZtQHrEdenLGThvWpmzv2r6ghsMSHTJyY1NmZprp81ZVyjfc//d5ouKfiWZftgCQW4O1IY4/l9CXl6GCjMecrVOhT/eYP/2luTKxLXu12u/qawuSkgnLsNPg3MtAq/qH4p7rWwvgbREwNBtXn9AfbLK/Fv+l49XJZxD6MiW0RXhFVI5s8syxDqzVVwUod/tU3rszxttaGOxZ1YEv9pvhne0RebtGL+11p/D71CT4Q/LOMPFQf6gv/qg/qRJmYBf5ZpjqjA//VV4qQB7dav87ONNXlq66USx3p9078V/s78sGM+K/KmQ7/1JX0Vf2cX0if0qY6qL80qby6xLrkNdP4Tzm2C/7PmzwY2wqnd1kCZenujLXWoiwsSr/oaksbFnIP7Z/AOau24IXX7QVrXZ7ja2FLL7dk3cjPlsAzl7dwzqPaXqcyLBym/uzEf6dvif9Wq4XSWuz7sIfHuKmMZ4yF6FeXJwIqycUFplk4rfKs8q5PStO5nza5xoezGR20MU/pUt6o6KhyprOtttxnGBOf6o3VhMF0dgqVy61fTDSIVwV5rDESbA1vG1ZtqgaoFh0O6OgPZEGRslhOPnSI0Lrsan4t7xmSyqtP3k7Piwu39K71C/muMPwX7KE/IzfPR58y9yUhP1Crh/3iroxxVG3kvu+jnNyMqWIQAwuXoBxfj6lWE8sOf71wAkbu/neU7R0oslVYsv+Jle/Bpr4y3jfqW16U8hXc1vtZ+9GyLLH2zjvRyHM0m02gZvznXdvW912NZsP3eW7OQZ5MHIf4lC/7Yz4BDACDS5di6YoVoY7Kq9tXurpybkdGRoBt21y/LOUN/9YizrOoL9t1V8b/8dLgwp2D+OaOvbAefbBtNx64eEq2FkBmsfNn92Pk8k1o9GdoDgxgv+XAO19s8ZTDczScir4pq22tutra8b9dM/7Pbv5fbv4PtNZ+Drac8FKDMrLfj3zvlyJffTJg+mCnHf/r5v9VG3oZ//n2po7EPlfaEl3Gf31VNOVsaWf46PZluLNt0MoAizZK04JFG0CJ0rQA0/KwbyPL2sjzNvJsCn2NKTTyMTSzSSxuTOHpZk+8yB4AUzMH5/lgWTP/T9tAfZj6s3P8j3Mx+rbdbvnvQTueLzAHAwDuuXyyUne6tPqxDcBa/LBxFwCEuQif5qBM0wX/wefTzO3R4/z/Ze87uLq426g+6Vs0qgvAXOStPZbF4LongfVp4HuOXRPsRBf80xdIv/mX9E1aX+180j89HcONkUDTLfVlfVi5eCUWDyzGUN8QBvsGkZkMk+1J7JjYgY3DG7F5dDMKd9fJtGmxXYRLXvuzDuwxUb807krO//Pq/J/XnUiv9UyCf4yOoP/b/wRz07WwY2PhlrgCQKPiL4MTrn0Ptu6xDIv2+wlMdg22rc+QNx/Aook2lu9zMFYecBT2fNj+2GPv5WiM78TWdXdgzZ234eb16zHVzrF0ZRtl+ViMbngulvcD3//XvYN9lGOT+f/U1BRWrFpVbavMPX0LE2dkVvtElwEYgys23oYzfvs1lLamr6pJex6wOs2qTcZkuGD/12FZv/s+ccz3faaJ4//6+9ZiwYIFoRxe3yzL0ArX/2Zz/h99tuv4jzGCHvHPfcpNy8hD9aG+eIie/3c+gefsoa6USx3p910d/1lupsP/rM7/68b/3Xj+7x8OqRv/Zz7/j30nP+vGh3iKoh3mLczPjD/BSHxgasZ/ylNfss26X/+by/hfla3z92xG/Fu/CBx9U5n/7wL+YS2uu/EGnOIXcaMfI80/n38+rv7tb7B27To88+lPw2knnxLa8LobbsAbTz8NV1x8Cax/8veUM8/AB885F8982tMqNjFO6fOHFv675cc2JH/qprE0G/zzlc9axnJDX84j/vUatdKwXZgnVyVCUnl1iXXJa274r8YxBK/0KXVI9VG7UMFgNR7Ul2/7m3fAWovPfPwTgL9pU3lRz+tvvAGnnHEafnXhJcjzHF/4ypexcOEQXvfqkyptcdxTnogzTj0Nr3nFKyt9zz+f/y1c/Ztr8NlPfHIG/O+W8d9lkAkbnELglUwFaTk8uJgcfQStbkv/GpfM322adsJlWVaedlRdjLxnHgyOhg98+LuQBYikSfkUvKvNyynZIQHIGw202+2gT2q3axDnvFLkGGOiLsK31W7Dygky/csGok5Z5hZ26WvWV/lIFnNjfeMHRBcwjjaQBZ5MBBQDrcLLuO/7hjp+a7wPSUt/Ul5RFNE26yblGoTwfmcw0t8md09MZ3kGa+NrFfTHevQVU7soYKXDL8vSty2/r4LgmyxzrxC3gGsTibGyjHelUYa2iybm0yZtT26ttWgXBUr/jTP1MzxPrU/fUx/+mv47kPQ3E3Wm3ZDXUaR4AtwCO+srn9zn7x78xzq6LQX/poL/OFirL1QXtQ/Ev++sIbbZHvFPOSozz/MO/NsO/BuUpYt7yjFd8N9uu0WjXvBPecwnjdqhba71OVEI+JdEnkzT4l/iM/2prdS3Dv/kTf0pI8U/ZWm92eCfcUueZcB/nEjAy6Ac+MmHTfGv/ew84J9+YT7pMS/49+NPj/gnzlGL/3gHpOqrvqYOpOFP01zwn3UZ/9UXqovaN1E635U9Lv6W1tEAgJXFX1tixsXfsrTYNO70K4p2GNus9d8yh4ExWXgdlfWLCc7WFiDtTP9OTU2h3W5j5arV8lmB6rjtzGZG1L0uMbyc79LSamJ7OL2TQs+LP9K4H9uR+4yFGBfGuJNutqfyr9ctzmE8kd+POiLI0HoRi+qboIP6yhvABURXjz9eJKj6mdu40MjcJN+6NrOWr412K0rWxm30t0vGGE/rODofcD/qm0lDVDgQ2+IQp4dgTnQ2sTHjlnpIPwHr52SBoiZRbtIYFRtFb58Rtx5nxjg61dc1iU28HC/iuCqqHeNN/Mb8Srt5PiwN47r/s26LvodhePNdMP2rYPOVGN58FxqLDgx1uC0b+2DnpjuQL1gZ+tOKL62FLQu0p0YxObET7fY4yvak00/mFDxm/ZDnU5ZlWPnwh2Oq1QpzEu3zOWcC5//GfZYk6Broop/R4/jPZKW/T39Ko/227gddpIzH4Ampv9Bh/byZ+vI31/G/KC1uHG7g/PVDuGUzsH3dMLZvGMbOTfrbGX7DW4ex/bYtGL12Pfr6WhgYaGNB3xi2TeS45q4c20aiPfQb+3Pd2t04/k/c9RHYyfVAa2v8tbcl+xtQrP88Wre/DWjvmGH8343zf3kakVs3Js48/rctcFNrAc7esgpryn60+fpDU/rItijhXvvsIMe4MihL12e0iwzWGiADJrI2fp7fiR80bsFYOVGZ/xczzP8dX08b5v+ujuI/l4twtIXzf9fOjJPqBffWRAtT4y1cf/x9+O2xd+O64+7FtY+7p/LT/OuOuxej28Ywsm0stAP1YNxp0vZDj/gPbSg/tZUxUhQF8gLI/C8vgKztj0vJS3++rONYtqb0x/5nJM/4awWYBv9qT0Zsdjv/l3bW7UyLvwubC/GYVY/BG459A8478Tx88oWfxJde9iV88zXfxPknnY+vv/Lr+NQLPoV3nvBOvOjwF2H/pfujmbmbebqlnWYYpgv+ITii3dD5v38Age1pZ5z/O/zbskR2x23o+9xHYa/6BTA6AmP93THWIg+4B9owKGCxoTwQozsfjsmRfZGXe2HpYD/2XXwgbHsBbLYAUwDuvP1W3HPnrdg6Pol7Nm7B3XffhVV77oH+HGhPLsbE8CqM7liNDZvd02SKH40z2sRrO/C9gL42PrSh7MO6G8GMH2unWlM9L/7OJlnr3uZDnzu3JeOdbxPGItsI83D+//vEP7eub/vjPv8vffuSnrrrVv3CfNJjF8d/zIT/WZ//78bxX2ILcA/YlD2O//SF6sJzbCZrbTjnhthmrQ0LxHV8GCOUozLrxn9i2e7y+L8r1//8/MG3FWXyRibqsSv457kIn+6s+wHAue9+N/7pX/4Ft625vRLnrq6z47vf+x4e/7jj8OxnPjPU+2PAP/NJr+3JLe2gX9TPmAX++6bBf1GWlbWgBxf/nW3RE/5nMf+nL1QXtQ8B/7ty/d/JUpmK/3gGPT3+r7/xBqxetTrocuobT8ZrX/WaYCskRllH2x0ALr/yCjzuyX+CZ7/wT/HFr34F23ds74hLymXS+rR3tvjPyJiE/DaDVqbx6iTW45aCKZx5GnAsY/1UDl8VRT00qQN5bLJ40UR1yGQCo52BgkAvNABuIsmGaTQasBzsazqCVBful8kEyHg9lI66URZT4YPFmOrFStLD11Gd4S880x4kYDPGoCV3WhiZOBg/eKRtYP0JcVGWboHV02j7khdl0W7yVFBrIo21FlkjDxMC1Tn1D+WwHghL37aqh9OLfpUBXGI8lWMR70rTRHp2jqojfHsVpbvrtCjdU9Lctnw7ZvJKvVLuVEn1CfHiY5gXhIuiDNdaS78gwRTiQgY4LU95cuKatp/qYnYZ/xETzMtmwD81Nln1xoOe8J/Eei3+/Qmxu1nD7Wd+0CMNeTDmKJv2sg5Tqgv3y9LfyOBjSuOdKY1vptIvFlEflUs9dZ+J+d3wz8GW7VQK/qmz8uLTQ6VgXvf5Uz1Kwb/tEf/EbtqOqX8oh/WYTFf8x0GSx9xqXdVF21ZpMA3+1Y+0n1v249mc8e/y1OdlMgEmPfcppxtPlpEf/aZPfpldxn/EC/PUtyzrNv5TX+qhSdvUHdvOxV+/gGt9Xpku/nr3pIu7br9al+XBJgu/SuW++a26cAGwLN1TTNZ6/Oe5LNK4RBtbrRaWr1wZnuyj/nGxLPLmToiZKqxCO3Qk4+wL9YAwnuhxmkjjeNqw72i5RUVXJ8ONW50Lf0zGF6lOanOsSzp3EIuZjCxIV32W9hMuP2XhFgSNq5MWAoEneXnKSr61vi4XvOWJX3j9mG/lTlPO7eB5sqyie4g7v6Do85iMc0DYN0YWQukJT9MRG1aejrHim6BvTKlryDfQeN7OrtBiLs99G0VzAK1f0Yux4fyg3yOC95HfkWPSuNZkvLrg8PmeD9uG1Na6Y81rLD0M1+/8EzT3ehQaiw/G3cXzMdE8wJWLPuXQkbh682ORLdo/6MB4MMZgYmwLdm65DVs33IT1d1yJ26+/CDf95ke47YYL0Zoa9/Kq9lvrX1cXSwEAff39WL56NSanpvyFmQzGZIGG83/OG/m2HsbErMd/6ec55qT7jCc9rvulNCq32/jP1+FxPKUdrKe6zjT+b20Z/HjLAly3FRjfMYqJ8SlMTrT8bwpTE1OYnGxhir+ijdYd29FslxgYamDBYI6+wQayoQw3bc2wdTzGQVm6i1KU19v47+7+p55Mdhbjf1buDPVmSnb7JSjWfgrt1khHe6hPqYuZz/E/c58Smev4f1s5iI9tX4Zhk8OiBFCGxV+LwuWZEiXasP77zBYW1vLCj3F9AYxbrrIAMuDSvlvxnYW/wmg5HmSp/HJX5/9y/k97HJ2TwzzKAoCR7WMY3T4qF54ib/WJ7o9uH8Po9rGQXzdPNXPEP2l6nf93LO728uMisf7SReAiWQS21QXhmfDP47AVO7VttG2ZyHPaVAAN08Ci/kXYa+FesJnFUP8QVi9djcHmIJp5E4N9gyiNi6k9hvbAgsYCGH+DwnTJdsE/E/XnPttY65Nm+vm/22/cdQeaF3wNuGsN4GDmL5CWKODn0X5enJUlTGnR1xxBa6wfEzseBdhHYulewH4DJfr7+7Bxxw7cfvvtWHfPnWjkTWzbMYztw8PoR4mH97WwZHEJFIdhcseRmBpZCDTiOaTpYf5vbZy3GAAw7s0alm1n/AyPF4IlvndXarc8fhUfEncQXCr+Ec7/e8e/8ps//Mexajb4L/8fOf8PsfVHdf4fdTHzOf6n5//+HBk9jv8z4V8/5+bqZCgKt7CXZZl/+02GXMZy6pLN4fpfeLisRhfus/2DDhJjTMyjLKZyRvx7fv6tnoHfPOKf52q/ve5a/Pa66/Cba6/FbWvcWzaKonDnXBY4+sgj8fIXvwQf+ujHAK+76p3nOX564c9xwlOeEnkDuP6mG3HdDTfg2uuvx4aNG4M+aRuof2gH9WUyvwf861b9yHbn9sHAf+5jHL8X/MdvhnM7I/4lpucH/9W4UR2UD8ci5qOC/9iHUn5ZwT9CUjtUl5/8/Gf43Be/gHPe9e7Q/pRFPagzRFfKAoDXv+YkXHHJL/CrCy/Bxz/8EVxx1ZX40le/CjwI47/ZcMstVp1GRlQwk/dsq9IURBqIk13DO3BqHuswULKs+tSrOpB1Sa/yIE9rkl6PWZf55M+ALASMeZ4Dviz335JlEIRyaXT4i0dZ8poI3u1MfawEK3Unv9AQYjvzwoRVgMoLc9pweuFJn7Z1xxHc+pRyGqBcBA86MmgS4FIOksEz2GrjhT61uXafi/Y1A4e7sOVSsIW+S14RoFte6CM9+QbbEoAY4y/KJnGVeT/m+kokiT/ebcVEXowr5ZclAwHjR3lW82O7cxv0TzoRl6odMOtwa7wfNN5A+T4uGnIXHHEzP/j3T/j2gH/qmin+K3Fe9UXaLnxyROWzLvONcRd6C/86F/faGMG/YLOcAf+GcvPcvWYmsY02Af4CuPiqKAo0pD1oF386qaX+1fKqX0jHJwqqr/Co+hk1+Fe9dZteuKMcTIN/1Zt8uu0zpW2pZazDPMYyaXWb0pMv61Jn0pE25Z/NgH+Vp7x2Df/VgVttY16d7LTPYx1uzTT4p+15wL+znbZgl/Hv/EFZGjOkYz51pY6al9pDecYYnL3zQIyWBmXheHFBmDcwWAv/NHBcDD5sYALve/g2PP+aPfyCi7+oJYu/cUHYyWX5MXuU+NxxU06fMr55JMvche50/KfeoK/8Eyu5f/VzludYtXo1wmKPQc1FQTtDOQBYjE9Moq/Z8HdHSx1fHo9TfintNPmAq2+SJy6tz6/IQKJwus+UltfJZNI4T8vSVOXlYinO36I2QmejbcbwBrzUb6nguPDIOlxQhOECqKPiAibLSZvmB810XVp9ron53i+kUW3ps2qbeeu0zERblA7sYzSP+2K78qnmsVrVn+4oaOkVJrEYQCYVv2luJAzHIYsMXJ6zw7dTTd85OVXgJxdfjac+4XA0m3347Q0bcMB+g1i1fJ/oFwA7h6fwowt/ieefeBwWDS0MZWXZxvjwBozvvB8my9FuT2F8bBRjo6MYHxvB2NgIpiYn8PCDH4NHHP4ngHGfsajYX7GOyWDDffeibBfo63Ov9GWyfg7EftFa94XG0H92Gf/zjvHfSzIGC5YsweJ9os1W5lI8TvPTbV358PAwsh07Qnk6xuqif9o+HMtIq9uUvizdjZlXbWviXbctwn3jOWx7MniWvjWw7lFCn2cyC/vTLejf2Ub/wiYaAznKgQbKgX4MDOX4wDOn8MT9SjQzV9vMafz30jrm/9EP3Ma2iWPhxBVHwMZ7mWZMxjSAxiL3MVXNzzzmq9mAhf82sg/HvB/Z3i9F38NPr9U3xJTYVBRFuJmT55+9jP98W9KWdoazHliFnSZzi7so3EKvafv9Sf8q6Km4GAwgy5xXsqxAM5tEszGBZmMc/c0R9DeH0d8YQ19jDH3ZOI4pV+FlI08JMdXucf5P/Umb2tY5/jvb/v2WUbzzJ1tg3MQCBn5rSwz96WNgrcX4D64CbAljS/f0pdC4pzFLF6e2RPs5T4a1QN+PLoo8pfx9Lz0cLzhmVfAzbaB+qd66ZTxrok1aj7xOetch7rXP8hpoft+37pXQHa99Tn/6TWB++zf9BnAG3Hb8bUE/YsRMM/+3no60ijH6hv0MeRz9L8cFGUwN08DyoeXYObETI+0RWFj0N/qxctFKHLjXgThq5VF49qHPxmQxiR//7se4dv21uGPLHdg6thXtso3c5li5aCV2TO7ASMvVT9NvXnN5pU3of01qM9hGHOc8nnqZ/2N0BP2f+xiKO29Dbt3cmd2C9d/8LQE0YMPwXwJ48a1vxq1jT4NdUmKvfS/FsmU/wuCmErev24iRyRIm70PfggEc+/gnYcPGTdhw7x0wEztxyL77YNviFrbvfD52bDgBdnQJDj30Nnz3a6srfQJtjjYaTExMYMXqVV45zruorKczcY4DeFuMWyC+dO2N+Osbz2eNGVOvr4AGgK/u/XLsv2yl7zgrsw8A/iZ0Y7Bpw0Y0/KsaGY9sI23LbuUaC1bGEZaRnjx6x391PNNEmXX4j+0T6VTPdJ8ptVfL1BbSzmb8pw+wi+f/VnRTecrL+auqb9Z1/I/2dsvnlnl1sjW/W13awn2tYyvn/04X2oL5Pv/Pexv/NT7VZrXRXSOjvLLy+RUeh7q2BGzaTrGNdXznftnj+N/oefyPviI/2mp9f6D2pz5imSt3ctx1xUhXnf/PDf+ZMbj2hutxyhmnQ9PjjzsOn/nYx2GtxTcvuADX/PY3+OTffRQ7h4fx8pNeg9NOeRNe8oIX+NdHnxG+AXz8CU/Flz/7ufCdX2stjj/hqYHvGaeeite+8lUVe7mPmthmm5FWtyk9fRFs2wX8Uw7rxN68M66UX/Yg4Z9rSKipS1u4zzq0XfHPG297x381piiXvs528/U/lad0Kpf55E+94vpffBV7Hf7PPOvtMMbgMx//hH84wyX67vNf/iL+/T//A+e9+7144hOeAMyA/+Of+iScceqb8frXvBZl7fV/Z9uvLv81/vqd78CvL7q0tpx8KYPtwjLS0wdsH/WvtFNcVaZSTMxjEDEvpWEZkiDkPoOGygH+zryknhrJOhCnltbCmnhMw0nDBizkTgCIjsZU7+IyJj4hkfvFX/UFBwnaERYok2DNG9E/BZ+2lCDmrzKYqE7WXxATIBneBSGN6vQwYRJOXZisdd8Ac9nx5Jtl1JG+1ETZXPxV3bQt1K+Ml0KeDkhpALjrW5lBKac6BCNlpa/s0KdreWGgLa9ucHSZY57EmwLZyl08wRdywuVkx06DdTO/QF5av8CedCZqa5pnfHzonWT0facvc3DiDa8jdSIv0mo9d7cmAMTXgmu7wfvB+I6P+hkfF3nuvn+deRwa7+vSx6JjXT2JpD6qi8qD6KntUYd/6srEgaws3U0QdfgnPx5ns8G/3DmXbq20O+2px3/sP7j4y7rkRXpr3Y0Y3Ced9TczUI4xJtxprfoYj39XrvivxgLrwPuQMUf6EPMJ/pUH6QH3CkmNI9sD/rlV/UjDpPqjFv9VPdkWxHFWi/9q3JG/4p+yoPhP/EcdbM2FPdrCOuoX8krzqHdv+K/iPPUH81Vn8mOeYoC6YBr80860DtuRiXkPBv5Zpu3ORP+TX+b749ks/rqneimrZvHXunJr5cnf8ASx2wYf+DdXUK90/Keu9BV/uZ9wT0xMYO999oGeTNRcA6zeEOVWiPyRxQ03XI+PfvSjOPnkk/H85z8Xz3nuc3HyyW/E3//9J7F+/XrP2lZl6OJSKi8U+TpGq5KYC76+wFogXBR0+0zStMypHno5MQZEt46to9U2rE+u0Bi/UBli0Z+0cK4gNQzpvb+MkYVcb1/V994x/tAyKxzEfd4UAJWdGBAXfmNOxS/Ev1A4mT62lKeJT764Q5Fp4oVSK2XG16OFFe28H51/oj6p/2qT2Bl345XlsFArRc6vnkb9ZBLtvA5czGUe2875QxbGE1EdyV8kAgzyRtMTWywYGKqQ0WdZloexmfnGGIxsvw8PrLsNo6PDKNot5HkTjWYfmn1+2+yDyTKsuflyXHf1jyPWQDxSS2+d1wmw2HOf5ZiYnAx9SaoT4Nq50XBvFDA+PtJxlfsdcejLOFaSJh0TmN/tRxrWS39M6fjPT1jYmnGAfe1sxv+RqRLX7MywaaqFvNyJRjaORjaGZjaCvnwE/fkw+vOdGMh3YqCxHYMD29A/uhWNkQJ9g000FjRRDvahGOxHa0GOHQNDuGzLAuxsca5QHdPob3hf7q7xf2IKGJ4Ahse6/0YmMkyWQ8DAKqw46hU44PjX4oAnvBoHPP6VOOD4P8MBx78U+x/7Euz/2Bdgv0c/H/sd8xzsd/SJ2O+oZ2C/o5+G/R/9FOz/6CfhgEc/AfsfcRSWml8EPdTOoF/SDtzynGk24/+ONvDRrftgxPAJAAughC3baE9OoT05haJdovSLnXouV5YG1hrY0vUPcVwvUZYGpQXybBx5YxJr+tbgrr773ALXLOb/3FbG/27zf/9EnbUW7/zxZhhb+AXeAigLmLIAbIHRNRsxumYjTFnA2MIv6BYwpaMNx7b0NCUm77wfrTvXh2PSGc/3vH+7vhJf6nvqpEn11zmh7WH+n77iOT3O2i7PtIHxUYvhYf8bsZgYt8hKG2iLFjA2bjEyajE6ZjE2ZlG2ACNPBIffNPhnvwHp07SPYTIzzP/TZGDw9IOfjg8+94P45Es+iecd9jwsaC7AZHsSd2+7GxeuuRBf/PUX8a4fvgvv+dF78LWrvoZf3/NrbBrZhHbZxgF7HoC/ftpf45Mv/iT+5ml/gz0W7JGKAORcRduMiW3JPNrJT4mwTi/z/3xyEo1vfAntNb+DKUu0LYBKn+2O3Sug3T4skAE4sO8mDGAUFhZFMYVWawTbpyyyvn4M9Odo5CVQtnDPmt9h09o7MT4+giJrYNskMDU5DJNvQdYcRX/fFA7Yd1vAFbdMxBntNSbOSzTPkM5f9wnxwTmRrzf9L4idU6JsC04j4vUU3uCk/QxtYNu4Km5/tuf/dj7O/+eAf25VP9Iwqf6oGf9TPTUOiMfZjP91+FcZTJRN/RT/fAMi44/0aVukedR7d4z/3Fd5Af9/qOf/8sas1E6tR3ncMtH/5OeOS//gQ2xb9zroQp4Edjby2p/aoFv6g7LV7m7jP69Jsy7LZjr/x67gP3zCqup/JjsP+AeAKy+5FFddehmuuvQyfPqjH6vGrPf1ksWLcdrJp+AfvvwlbNu+vdJvkvemBzaFPGMMLr/oYlx5yaV4/HHHuU8O/IHjn23JdiY9ackrzaPe/4v/qn7qB8rVepTHLRP9T348zmZz/X8O+KetlKv13n3uObji6qvwjS//I578xCeGsunwz6RylIY8BgcHAQB33X13KOfDXaiJXyZrLZqzxH/+9tNOO4+ZkMezrR/Y1fnKlPt0FvOZxztz0kDmQk+YlPtOljTky2R8Z2tqXqnKferMpHRpkPCk1Nrq0wpcdKK+pEdoMP+KX3E4Ah+3n+fuaWL6RB1uTHIRTRtd7Ha+q3ZUtEHLgNjnUu/Ud0gCIdiaBD59wQVj6kYa1tF6EH+qTpqcbby25XRPg5++hbcjz923mbPkThLaHm2M/kIS4ORjJaYCTfJdKtar2JzgIW1LJiv+0gkt45k8FVN65yfg7KdflL/qRb7MK9mpAEDmXnPARXj1b4pL8iZflsPjEvOG/2onTZlqVx3+FQe88En+zge5P4ejHZyANdzJqU+qX/CtjfFqavxMOupLPpAOW+PAIznwgQy4FVq5IzvUdUaEfNqpuihv6qZlmrgYrYMEk/oh1cP5Tu+g7IwVraP1kAzEdYn03Fc7+FOflsRtT/iPuqX75EO5dTRpntrMfOx2/Me2K2eBf8fL6WDk2zOO32zxX5U7P/h3bcU8ylS76vBPvakL86iHyv2f8aWYCq+A5gKv84su/sZFXIu9GwWetmQc31o34K/3yOKv/6awLv46u1z9FQssnrsqvqKdSXWtxT9t9gs6U60WhoYWYvGSJZDLRNWUZhlPCoMHNj+A7373u/jKl7+MW265BVu3bcXixUtgyxJr167DjTfdiF/+6peYmmrhEY94RHjFdJWnHCT2dAqv0zEEn9+k5fB1NJ/zH8/PkEb4W1m0cx2nP/Z5xiTqqm7JvtGFiUSPyv/yCuQaU43hIiN1rNIE24NZPn5VFS4Ey74uCIeY92RGXOG2HhcqTxLrO2s8G8GRISNfJqp1JOUf5FnvAb8fbY5z6FDX6yHKk3Pgi/AK5uhfeoVtUqHlIrwxlcV4+tDJJTUwOb4TYzs3YGJ0I1qTO5HBIGsMSFtWE3kXRYm779uIh63eE3nWwI5hYGiwxEJ/QkbntlrAmrvX4uADVqLZcN9pmpoYxqb7bsTw8A7XV+V5KCvLEmXR9v1JgbJoY/OmtRhatCeWLN0naBGDSH3l7MvzHFMTkyja8a5lJl6MYhyoq5mnfbMx3otdxv9Gfz/6BgcrfZtN5gS6rzR15dyfmpoCxuOrd+kbxhNvNqQeuzL+by8zfGvDFB5ot9DETvTlY+jLx9HfGEN/Pha2fY1R9DfGMDAwAntPBmxYgv4hg3JBjvaCDO0hA9vfh2JBhvvsAPqaBg8bbGEw9wshsxr/SzQazQ5ds1mM/7m9GXvs91QsWnkMFq08CotWHIVFyx+FRSsehUUrjsCi5Ydj8YpHYc99j8HeDz8KfU0AxQ6gGAGKUaAcc79iHCgngGLCbe0UUE4BtuV+ZdstOqJE/+ACDOfPrejDfePPz5nPvEzO40CMil3p+G89zffG9sDlE4MojUFZtDG8eRt23LcJO+/fgZENwxh7YBQTW8YwsWUMxViBrD9H+knVzJTITQFjCuRZG3k2iUY2ib58Ao18ChmmkDVGMZxtwaGTh6CBhnsifhbzfya2Fyrjf1b59IK1Fp+7fBuM9U/zwj3Ryyd7swe2Itu0LRw7Gpb7Xzh22/4HNqF/86aEJj49bGyJNz3zkEqb0feqVx3+bYJf1tF6kPn/93+yzHvAJd+LueR3LIBW2+KsFwOvfwrwp4+2ePljDQ7aq8Qvbrdo5hmm2sChyyz++k+ANxwDvOxQ4HWPAn63sY3NE1ns8T3P0/fd3BFXmGb+z2tPzNd6ajPzAeBLN7hX8TE9dvVj8bYnvw3PPPSZOGz5YXjMvo/Bov5FuH799ZgsJgEA7bKNDcMbsGlkEwp5w89xDzsO7zjhHXjZUS/DYSsOw2HLD0O73ca1669Fq2xV5JzyqL+qtJ22n+pqdP5vY6yiZl6uday1aJdt3HbrZei78KcYnGg5WhtbL4yVWQazxx4YeNzjMfiCl2HoeS/CghNOwP3FZlx3z8MxnucYGLoF/fmN6MuWYeHiBVi8dCGGFi5AfyPDzh1bkecFFizox9DQQgwOLcTIyP2wjT1giwMwlA/i2U9fj2OOXBV0YzJh/u++V1iWJYYWLgxlgH94gXV8e3/2N/+Jb99yEX5811X4n7uuwo/vvBL/c+eVuOy+G7B2ywa0R8fRHh1De3QcrRHuj6KcmkKjvz+8ZXDBHouDLjOlFy08AkuHFjm9GGt+381dXBodGa20J6RNzJzO/+fh+h+cmmmsaB2thz/y83+9HqY6Kg31tD2P/3Xn/7Mb/1NdzS6f/0d5eAid/wNWrv/p9X+NE/dJJi5AUyfU+JltQH1JjxnG/9DvzHT+L3FojMGOHTvwg//+b/z05z/H5VdegVt+dwuWLVuGJYsXB7nUkboZA7eobS10kt8x/5fEPG0b1Yu+MwA2bNyAH/zoh3jjG97Q4R9jDK678Qasv/9+POfEEwEARxx2GK7+zW9w+x134OADD8QPfvRDnPyGvwAA/PLyy1EURXgyUn38Pz/7KVavXIWjjzyy4qfyQcL/FVddhUt+cRl+dfkVuOqaa3Dr7bdhfHwcq1b6N0skeEjbUmno198X/jFP+J/d9X8X58xL5ZgHBf/Rjir+u1z/nwP+f/zTnwIGePYzTwx6GGPwzQvOx/U3XI9Pf/wTWLZXnPsS/2940xtx9TXX4BknPK0i46v/9HUcd+zjcPSRR8GKTyG2GGNw591348c//Qne+fazYLqM/0Z+RVmGJ7itx3L4GTf/yP0cyRj3tlVD/J912mnnkSkdplsNKA0GKps6X40hT2Oqj6pDOlfSqdxCX73Axk7efY+aoOKW+dxSFnUw/gTV+EblgprWU96cfGoAKR0v6nU7wUgv6DBlsmCMJAhKGy+6RV9KGyX2aQCzPvVN+as+ZemeuDRGnhAR4FbqsZ3gv4kgQGQ9+gRwd6SWSQeoPiR95k++IQHOrUkGU/fe9mpnqPaxrt6hFXRKmkHlB3/7O0ms76zZOaX+gAe88kn9pHlGsEKbXFN0j9vgpxrfwjj/MtEOk/G1gjGvzkcqg7ZxX7fB97PCf9bxhITqgGnwz9d1NxoOGyx37V5tQHccT7ZSH3EbZPmLMsYvUBsZvFIfpf7hL+gjdEqbynY2+dirusnrVa2j/tI8eF7Uh2WOT165gMU6dW2vx0gmDE7IzPjnVnVETYySphf8pwOc2ljFfxVTqX2sy74w1UmTylf7Hjz8O7tSHbklr1QGU6qTytS8Oh+pDPLhvm7na/xXHTAN/rNk/Gd5avv/jC3BZOne8sTXNrsngauLvzwuS7cA/Iw9J/EvawfcuK9P+lobxlfdOt7AygUWL9w/2qU6qS/r/GtMxP/ExASW7b23X5jtjEmge3ZRtPHBD3wAF110IQYGBnD66WfgrLPPxhve8Bd43eteh2c/+9lYsngJLrzwIlx22WUYGRnGk5/05JSNJK9Uh0DNS8qM/8/ERbcOGqbEF5GvxovxZG7hKvUfAOhCoqmsj6X66za1K9Ux0jhZXidj/A1p8Q0OLtu4OsbXFV0DO7HNGLdYqTQmiz4LcSSqhgVN75MQap5FRZ4chxiUbSVf/RcrR9G+TPfFyTCsJ3QhP6FzO6o8S6rt0WELaYxx6maU6v3pHNRRpyrdYue2jfjd9T+DsZOAbWPD2rvQ17TIG/1uEZh/HWOCRbsocec9G7DfvsuQZznu3zSKRQuBxQsXVuinWgXW3HUvHnHgKvT39QEANq+/EZs2rEXbv1Yqy91Twn19C5GZBbBFG+2ihbJw344tizZarSk8bP9HiV+iD6pejjG1c/t29Pf3h2NwrEnm/+xLSxtfrcx849v+znvuxoZNm7Bl21Zs3roVm7duwcZNm2DzHAODg5iamsLk5GRl636TmJqaxOSkO2aZ6sT41v5ycnISecstNLDM+Kd/eXMtn9Lj+GDmMP6bLMMdIxP4zsYtyM0I+syIW/BtjKHPL/725e51wP1+UXigvw38bgFOeswgXvmUHM88Ajjx0AaesjjHk9oNPKHIcOxUH/YeWYxsbR/a9y7A+MZFaG3rQzY4iUZ/9C/1T3V1Y6WzhfNOLU/tUN+RZvnynVg41MDQwn4MDQ247cIBDA32Y2jI7Q8uaKC/OYXMjgLlpH+ns3U/ayEf+fT7CK8X7ix3ryseaf5p7+O/jzvVW9sJXcb/re0M/z68F7agicnRCdx3/e3YsWE7psZLFG2DwuYobQNlO0M5ZdAeLjC5YQwoMzSWNPzYYGGMRRYWgFvIsynkWRvNxjCaZhx5No4sa2PUbMFhU4dgsBjqiCNtg6xm/q90Ssubmat5Bp/7tXv9c1igrSwC1y/ypjSoLApb9zSx1OGxe8q4xKnPOqzDrrQdOub/YjMT66HL/P/7/+MugpFD5BTTzhGLt7/c4qQTMhzxMINHLHe/D//bDmwe74cxGfYcsjjlCRavf2yGI/YxeOQyg30aE/jvWyawdrzP6en5GQOcsd/WDvswzfy/GqWxbdSWLJn/f+G6Lwf6JX1L8LrHvg4vOeolGGgMIDMZ9liwBx614lHYd+m++NXdv8Jk2y0Ca8pMhj/Z70/w7me+G0856ClY1O8WCfsb/Th8xeG4bM1luH/k/srNSacedXIl1tQOprSN0ieA1bbUR8YYbGsN45+2XITxHZvxyA3jsd1s+A9mYAEGn3Yi9njbOzH4gpdj5wFH4/4lB2F0xcHY/8j9cMmvJrFpaz+yvvVYOHAnVi5djsWLB7F40SCGBvvR12ygr6+JoaF+LBwcxNLFC7FsjyXYuHkTJtsHA+2D8bC9J/Cmv1iMxYuGkHWd/zvbiqLA0CJZAKY9XmPjCnDyDz+O27atxZqt63DHtnW4fes6rNm2DuuHt6BsTaFstVG2WyhaLZTtKbedmkJ7YhIT92/CxI4dmNi2HabZh4kdIz39/mz5sdhjyC0YR192Xv8bGR52c4TkPN4k45rmwftCscl67Jvqxv+07fUY84R/1k1jlDQPxfP/8kE5/6/akNpBXqkMplQnlal5dT5SGeTDfd3Oy/l/8npsiO6kU7n1+E/b0PqxtjMWqjZ6+/w5vdpiduH6n9IpbVV2NY/p05/7LP7i5JOxc3gErXYLm7dsxR133YmPfuLj+O111+GEpzwFff68gnYB/ib3soxPNnu++Tzhf8PGjW4B+M/fENpH611/w424f8P9eO6znh14H3TgAfjQRz+K/R7+cFx5zdU4+Q1/AWMMhoYG8Q9f/hJOePKTsc/eewcfZ1mGH/3kJ1i1ciWOPOIImAcJ//fedx/+/rOfxTkf+iC+94Pv466778bwyAju37ABv7r8Cnzn3/8N3/rX7+Due+/BwQcdiCWLF3fBf2zv2eB/zR134JV//jrcv2EDnvQnfzJv+CeF8b5bc8cdWLt+HTZu2ohND2zCpgcewIaNG7DpgU3YsHETNm7aGMo2btqIDRs3YnBwgTun7Bn/Ufee8F8Td/Sn+otye8N/J8ZSH3GrsoyJaxnuRs1O/F9/4w3YuGkTLr7sUkxOTOLAAw7AyMgo9l62DNZanP3ud+LFL3gRBvr7sXHTJv/biHa7jcWLF2PDhg1YtXIljj7yKGzfsQO33X4bNm7aiP/60Q+x7+p9sXBoCEVRYMmSJVi3fj3ecvbbccD++2PF8hW49vrr8O5z34tXv+KVOPYxj+3wJX2k9s0V/wZw3wBGsopcJivm2gjcB9yEKzP+dUuyek6SVCD58pj7pdz5EeT7hiz9CTNT2lik12OlZTJez1AmeeospQf8BeAuIA/HfEZEApI28USY+b5i4EPZtCMAL/E5n6guigJ5chcJvG+tH+z0FbOUq7rr4mhZurukePc9wUfdyMOY+A3cqFPVZ9ZP9oqyqFyQIi+Wa3tZ657vUOCn5QggjrHJco07t3DY6Lj4EOI5LPq7u3X4umuN926JNpOf+gASl0xpGeljcsd5nqPNJ2ATOZDBTKoBCc86Gwzc64jUj9qWqU70Y8VfCf67PWGq9RHaLPJXGq3D/bIG//w2RlnMjH+1021j+zMZowsWcHcHim/SWE51pkzaBMTvd7Ae61jBv/K01j014mh5XI9/5an6McbVB8SF9Xf6uPis6qO6qxzuU9+i3R3/3XRissS/4ErtYbnTL+oGH2sz478zhjTu1DesS7+Sh/pZ9VQZdYk2s776ABKXTGmZ+i/SxD6XSeWgDv8+Wbl5pJsNykf3VYbTKcZB6i+1q86GunZI6ZVG63CfsUda+lf3majPWzfvh9Ei61z89a91Thd/bWlxxOAUPnTQTjz714tlodjxDPX8E79p+aP3KPDFJ8ZX6VD39Jg6qk1MRbvAxMQEDjj4YFm6sgDkBhFu02SA737nX/GNf/4nPOIRh+B97/8AliyRpxOkzq233opT3vQmjI+N4Zxzz8Xzn/c8VxB4U1A1NtP2UjoAWLNmDS6++GJcfc01ACz23nsfHH7YYXjyk5+MfffdF9rnh0VAw37XK8h84RuzWb9SFMoBX7WShJe1ePNpp+ElL3kJnvWsZwlJlO1c4J4orejpy7ulavPEPbaj4yDKeXy6XS8vbVjBcEgqCOis12F/lYdipXLxUfdrUqXdU3/ocdoAEvO19aWtaUdVC/+EL+PEsD4xIc4AApeY4+v7o9/++geYmtyOhYv2QKM5gPHRbdi+dQuOPvbJWLLsEGS5u7DCNgn7xmBioo0fX3wVnvbER6HRaOKa69bjoP2HsHI5n9J1/t2+YwL/c9Ev8KfPegIWDg6hNTWG9XdciTvX3IQFg0P+txCLFq5EWSyELUvkjRwjo3dh546NGBtz3wQ2eR+e+cLT4+J2iEenlZcICK7uvOV3WLzYX2SW9izT8V/LfduQR1mW+NI3vo6rr/1tiBvr+9V2u40XvOCFeMpT3fe6HD1pOBeiVJfHcsDiwAMPwsKF8bvIjsbxHhkZQd/oaKVPJ13u5+P8tlpaPpvxv1WW+I8HtuLrGx5A2ZpwC2nGL5aZ0vszHucNi8bkAM5cdAyO2rcPC/qc1yfWFpi4og/DW/owNtVGYfvRRh+sbQB9TdisgcUDA5hsbMYhL96OvoVxHLddx/+qX2Y7/q9ofsE9yWst+I1Yx9Mt/MV95gsN62h5j3zuX/AFsSEmY2rO//0vtSVtO+5zrPzt+AA+vHUfbHlgJ9bfejdKk8M0+mAaDb+4lcFkcIu8sO61x8UU0J5AY8hi4SGDaCwADEo08kk08xH0N4bR19iJvsYIFjRH0MyHMdA3gr58FI1sHA9rL8drh08Jcx3VS3WmHeqDumP4cSUd/w/9+K1hEdct0Dq/GzfBiNtQzuOkXBaCux77heCr/u4ltbqzrXSf+k53/q92Wpn/v/Eth7hv/db9GsCUBZYsLfHNcw322cPx62sAP7p6DH/++TYWL1uMCWvxrCMt/v7PDIb6HE27sLh93Q688+fAFTsWwzaz8P3fMgNuftrttfinntS/LN1reXV+m/U4/9dvAD/lgKfgb5/7tzhi5REVGgAYmRzBy//55bjqvqv868ljWti/EG96/JvwjhPegf6Gu3lH0w9u+AFO/d6pGGuNhbzfnnQFUIN/JtrGdgg2+JvCrdAoPaT9bhu9Fx+/45sYG96O9/zwfhx+/4Qrt3DXkgYWYNGrXo8Ff/Za3DW+EN//7RSuvbfA8LhFlgF7DRYYu/FK3HrtEO7ZvAaDCz+LHfeMI88XwGQLYG2OwrZhLJBnTcC0YctJFG2LBcu2wTZfh4P2PgLPfWKJ17zyKOTyUAbj1e3HdpmcnMTylSvcOAkOm503uB321b8ErJ9xhHMYd/5trXWziEo+z1GBcngcZqAB5Bn2OPQRQfZM6d8f9xYcsPeqwKvyZLJvEwDYuP5+9Pf3e3nzcf4fx3/GAv2HWeE/fveUOqQxU6cTk/0jOf+PFsVEm1lffQAgLIowVct0/I9J/cWkcjAX/M/p/D/6MfWXrYlFTXXtkNKHB6RmGP+pE/2r+0xOn9gnOJr4XWCldSfvbreSX+Mb2sqkdim9+oDHxLjyU5uYrLV40+mnYc0dd+CFL3oRli5dGsoAd3P4r375S9xx55340X/8JxYvXhzkUb+i3a68RYZWlbuIf1uWuOHmm3DKGafjy5/7XOgnjTHYf7/9sHTJEvzz+efj6t/8Bp/5uPsmMHl84Stfwb/9539geHgYV1/2i4Crd517Lq68+iq87EUvxhOOPx7WWtx97z343Je+hD8/6SS8/tWvCf7JdhP+t23fjq9+459wwXe/i8cecwxe8Lzn40lPeAKW7bVXBf9bt23DL3/9a/zgRz/Eb669Fq9+xSvwV6//c+y5h/tEA33HRUNtF8qiXB6z7LY1t+PNb3srAOCIRx6GT3/s44FmV/HPB/22bd+Ocz/4AVxx1ZUpaU/p/e89B8+RJ10xI/5jX4KZ8J9gicfcV6zw2EyL/2pfpjQpLVMlv4L/OAaT/vindj40cfzjjsOnP/YJGGNw/FOflBYDAM449TS8/jUnwQr+r73+OpxyxmkpKc449c147atc/H/rOxfgP37wfaxdtw77rl6NF7/ghXjdq14DiA+p33yP/5k+eVla6xajfGBZOsv/SusmNSaL3w3lYlvuV+wZzGwY7nPb8O+1z/xgg2RgLrx8uKZBJgO1GkJ+mqcGszGt9ReBveEuz9VlwMLrzfqs5y5Cdd5ZxXrGuAXqQgYJ/khDmWXpnrQlP/Kh39ho4buzYov71oFvVOm4WV6WJcDX7ibBTpqwrxMd65/klfbTtlC/6uIvZTse0Wb6oxT/MzDJm3xdMoC/s5M+Y3CyLuUX/t3qPCZPnazmfsFddQL8SVHVJcFPlKv78HYxr/BPbXAfFR8bWMvXcLjXTvurFO6ypMkA//pwGG8vn/z2mMuSO8wi7xg/XlQoy/0dpBU71b8SK/yxLu3h1sjdPcQBeWpS/Ne1Ayr4jwMX5Zoe8W+Mv6hkLbJ8ZvyzL2K++kTtL63DSeDj76RDV/w7GdRP9WXfUMq3JlSWxjC3xrgLve4k3bg3CyT41zgnT21X+iHKjDIoU+0gD01pjEPxn2fhG6e0Ofi5F/zLHVWYEf+OH/mzXH3H8l7xr/qo3LqkcnUfs8J/7IPV/yznvtpCefqZBP4ol0l9TX6Au/OO9GpnXbvxR75V/Lu4J6/p8K+6Kn/U4n/u4z/zKa8O/7Z0/YPzffyFxV8/5rvjWA6gY3GXNJaLv6GulMuCnrZzOQv8F2WBhYv8K+LguhDOdcJVhxq/wwDr1q7F+Rd8C6tWrcZf/uVfYolfBAqTM0mHHnoozjj9dIyMjuJTn/oU2u3q6wXjYGiDeG0j9pE6aN544434+Cc+AQA4+6yzcPZZZ+NFL3ohHtj8AAYG+r0SbiwEUnt4UL/4i2C2qx/DPxrm/BoOQwq+dAeJK/yR0mgycDTeZucP8Y3fwvoLhv5kIVQNlM4Ano6HBT2fuNjsnz2Nf+Jz/rwbQ0oXjdM68L5hXgW3xvvbVrlonGpd8LjDjz6xcfSn9UUXqC7eHgN+B8/XFX8Zb2sl7mzk49i7sugeV4tcAIMtD9wHYwy+8uVv48zT3wtrLcYnxrB58xaMbLuTUnycx3ayfn4w1YpPcI1NjHgVos8BoLQlWi33xKu1Fq3JUezYsQWt1hRarRbarSm0W1OwZT/arRb+7/e+h6nJKfT37xG+Bdxo9lVuXCMunP0aBHEcMsZg4ZLFaLValT6H+9ovaarEhKe7+dbfdcRB6EOZVzl2F9PIyi38FpVyay2Gh4eDvJQ/dVX9GMelLF5r38ny2Yz/bVvitrH7MbRgG4aaWzDUtxVDza1YGLZbsLC5JWyXLBnDE5dZHH9gE0uHMjRzwEy0kd0xhdaa7RjfuAlTW0YxvmUUY5tHsXPzGLavH8X2tTtx35qNKO5aiPW/iud11LFiX+3470/CZzH+oz3iL2y678m6xVt/rPvhxzypU0czEx/fntRT2w3J+E/MzGb8hzH4xfgQ7r93M+695T60zQBsYwFs3g+YBiwaKE0GiwzWNGBNE2gMwPYNAQOL0J5oYuS2URRTrq8zaHkb3NagjaJwY7Ut22i3XSyuz9cFvdXvjC/VtaKv2NjL+B++/6vf7C2r3/mNeXqc1CGP8L1grRO/IWz8q4eplybqprE20/m/+kNj0lr//d5Svvmr+wUwstPi7a8w2GORwVQLaLVd3bO/NIolQ4MwbWDFEPD8I4AFTYOJtrtN4bb1IyiyfuQmdzz9z/gt9U7xzx9jk/amiXbRZm039Q0ADDQGcMzKY/DI5Y8UDjF9/aqv4+aNN3cs/gLA6NQoLlxzIS6/9/K0CADw7MOejf2X7l+Rx5TiX9uL/QXbJstnN/+/a2QdNk/sxGifwb8+dg9sH8hgS4sCFtYY9D356VjwZ6/F929fgHf+6xj+/eop3LahwPrtJdZtK3HDOoNbs9WYWLADg83lsOZZWLjqMCzYZ1/s9bC9sd+h++LgRz4ahx5xLB72iJXYc99lGFz+cCxctR/6lzwVQ839cdgBEzjhKSvRbDZR1s7/44JisIH9iR8pYdycgN6zfnyy1sKWJYaaA3jmQcfiBY98IpYNLnFlZYlnPeI4POeQ49E07vqaLUvYsoBtl+HFCLNKNs611AZuqR9jLKu5/jf78/+5jf/Mj/Hkvh04F/xrfJX/e/4fdNR9tYXy2JbZLMZ/ltXif07n/9W4emic/0c/u7zq+Kw+2b5jB7bv2AGbYIY6MO3K+D/T9f+bb7kFZ73zb3D0447FmjvuxCte+cqOxV8AGBgYwNOf8Qzsv//+OOWM04Gu+I9zjnLe8B+vhZ5yxhk45cwz8Ka3nIlTzjwDd997T+RhqjFprcWrX/EKLF60CBC8W2vxoXPPxWknn4LLr7oy8PuPH/wAL3/Ri/Gi5/+pY7cb8b9l61ac+ta34Ac//CE+9oEP4qv/8Hm8+E//tGNRN8sy7LXnnnjh85+Pr33hi/joh/4W3//v/8apb30Ltmzdukv4X3PHHXjz296KE5/2dPz5Sa8F5O2TjOlsHvD/5X/8Knbu3Il/+9YFuPLSX+DKS3+BKy65DJdffCkuv/hS/PqiS0Lery+6pPL7/85+B875wPuxdt26HvEfX3Wu7YAHDf+Rn+ZpPerFfbYR86gDk8q94pLLcMUllwV/XXnpL8LiLwBceekvcfnFl4Xtry+6FFdc8gu8zt/QQL0B4MgjHoUrLvlFoGG91736JGR+/H/dq0/Cv33r27jikl/gu/9yAV73qtd0+KCK//kb/zMyZKJTKVQFM6lTSa+JtAxSrUOeGtjMz/M8PDnK/Ha7jSzL0Gq57+9pQxWlu7OTP1645QUsLlYxwIxxr35215/cYivzlbe1FhbxW6sEN33BLS8LKg/1RbgxHk6uBjKksyz4GmoBEnkZ4wBA22h74GP867Gz6uJvrO8WC0B/WQvrX23pFnuq7Uq9ssy/xku+8cQfE+m0PnXUNqQu9BvgLtvxBI10SII393cDWWvDYgl5sT3YOQd9fYpyqnxpEy+2kR/l80PzHEyMgI7HxmT+Wqi+ujr3343xFxWNv5Du//JGAzDxdeEWcUHStV+MK4jfnPL+V4OjPPnuBHy7lH5iwkVg+iva4OzSeMQs8K9YU7+jgv9G2E/1pq4soy2Uy/xWuw2T1+O/wkNkcIJI+zLFf+ZuBjBZhqJo+3bqxD/lUzfqRT+TjpjjT32p+1kykLmJVAHrbx6gDzvxHyc/PHb88nAxttI+vu+D8d87rsV/fAtA2q4AUBbxDiHay3pqE/2i9bUO82gL/ab06b6WV/Ef9eFxmeBf+ZFPypc8dF/t6g3/sW1oE2MsTayn7cp856MYO+of1VMT+ZU94F/jlP5SG1z7OzuZUnq1L9WBvLQ+dnH8p1zmdxv/S1td2A2LuFz8lYXfWObGPFfX6xQWOWTx1/NhubUA5Ptq6lfMAv+tqZb7fhmzPV/Zcf0R2N/7PGtx9TVXo9Vq4clPfjKOOuroWJ+JoeK3L3/5y/HoRz8a69atw3XX3+AyK81kPXFnjCEsdrt+CrC48KILcfjhh+GNb3wjDj74IBx88EE49rGPxVve8hYsW8bvoIgdtcpRZm8p6OCOfB7LAHDB0NqQ3zURV+7AsbN+H+7JEACwZQnAujE+pQ3qc4FUnj41spjoNiGFBcckL8WNtfS3Y6JLnUyczyj+yJv86BPHz8+FTVwMNt4Mrcvk3Or1FR4dDva8QL6aPK2p1HOaW+v3KnUcxoxxS8G0EXD4M8bNVxEWSL29NZ4eWrQUWZbh+c9/Bs44889de1qLK27ajvGJFlqTO2N9r4PzgcP15NS4b2qL8YkRd1E46eeKooXJlntaCgCK1jhg4BeA3SJwqzWF0rq+6tHHHOP7NqDRaIZF4IWLlsCFXrQktAcfBA42O5cNDi3sOI8w0j+zPvU1Mv6z/7d+7hb2Qx9YuotLPo/zBbaPaz9PJ4vDbCfXRqQh7+rcQeON+oc6av8ujP+TZQv3jt+DQbMRQ/1bMdS3BUP9WzHYtwVD/X5BuM/lL+zfikXNzTh+yR5oZHH8z8Ys7L070JgcRaM1hmZ7HM2W/kbRbI2h0RqDndyB0XvaHViC+KL7+B9xyHGF5XX8wuIs/M+WAAoPLC7c2limC76aB0/fwUf4e57WunhjSttT2xFzGP9dvJW4dBOw+f5tKE0TNmu6hV4YlNYEk7hv/c1ChywC/uqgPrz+EYPYs2hg/N4WjJ10Twmh5U1toSwAgymgbKHdKv3NCwUKuHmFmeP8H9J+7rywM6YBtwDcuWAbF3kxMQw7thV2bIvbjvotf6NbYce2uf3xrcDUaP3CsD927TYN/qeb/wueaC/rqX2BRwHksuCrv/YEcNwjLY49zC3+Tk4BfU3go+fvwPD4IPpMAygsDt/H4lmHG4xMAK0CuGNTG/dvL2AaTZgSMLq47BeBiX+ey/AcygJh3CmTfoU26b7alc7/mfYZ2gdHrTwKudw0zPTLu36Jz//q8xieHE6LAC/n+vXX4/zfnI97t92bFqOv0YdnHPgM5CbyVj01afuV4ZpZvH5g/Xkey2kf45d8jTG4d2IDrMf5rfv04Zbl/bDw3wFevBSLX/hS3DU+hG/+cgJrtxZoF1xU9zpYi2zxapT7LMDDDpjAvkuPhcFLUBQvhWk+GYv3fgQOPGwFHnbwMgzteSBs9kS0ixcB5gVYuejxeOrRwFOfsBCrV+0TbKGetLV2/i++qPjG/4wr9GO3+73hMc/DZ17w1zjluBfCliWecsAx+PJL34VnH/J4ZPBzndLPS+KFu9klP9cKSfQz/pxF+w22B7eY1fn/Lo7/84h/ra91mEddGI9Kn+5r+VzHf+WT8iUP3Q+2AWg96Of/sxv/ya+ct/P/Tr8pvdqX6kBeWh9zGP+Z3zP+2bcLD9Kr3+648y686qTX4FUnvQZr7rijYofy4m+u4z/fBJj6wlqLf//e9/D8F78Izb4+vOtd78L/967/D484+BFYvXq1/wxUZ3ryk5+Me+65Bz/+2U+DXryhhdePtd1Su7ilL3rF/9GPOhJXXHwprrj4Elxx8SW4/KKLcdWll+GoIx4Fay1e+6pX4dMf/VigJ48lixfj/55/Aa64+JIgk23z4he8AN/48ldw+UUX4/KLLsY3vvwVvPnkk7Fk8eIOX2Ee8b9t+3ac9ra3Ahb4z+/8K57xtPg91u//93/jY5/6FN54+uk4+YzT8bFPfQo/v+giwI//z3jqU/GD7/4bAODNb3truIGA8tW3jIXM4//2O9bg/7zvPLz1HWfjLe84C29665l41tOfgXed/Q4A8ZzeWotvfOtb+MnPfx54ktdPL/w5/vn88yu+YNL2K8sSDY////v9/8Qb3/AXGBsfw5lnvR1nnvV2vOXss/C2vzkbb33H2fjrd74DZ571dvyf887FzuHhoHOWZXjJC16Iww59JC685OIO/6p9qQ7aHppI+/vGP+1j26gdkVcsmyv+WT/1he5n6fX/LuN/48Ee/+GTVuA+HcfKNF4V4b4rz9Bs9gWaoiiC8hClObiqAYVfsAoN5r/5q487F3zFr5/oUk8OgipD+UcHmxBQhbeH9Rh8RVHAytMZ1K9Db+Of8PRP8lm/qGpMhlLmkFnmFpyt9ye0s/MnLbQZ0qm6rWs4vrrYyiSqLN3CY1w8MmGxmDryyWELPu3oaAAgb7inZekD2mv8RNV6nzBoTU2Q0W53R0gGG54ciqCAxEiWuYuq6fya5UxlmBi5BQrn42q70g/GuMX1trc76Oi/u1rha+MEiXpym+fuzhQnl1igTKcLf45XvMOYJ41FUQD+DimNFfKjXO7Tr4Eu8xeU/SDvLgJGHmqz6kkbIJ0efWhdZvAN67MuE22ljdqu6AH/XAhvNJshJttFEdqFutkUR4w5PyhQf+oYXumR4J/1yM8Yd/KVxgl15z7xX5b+29c+XjLBP3kzqRzl6081K0/lp23CeLQ1+M88vyzLQ5w7Hzjckj7YF2TE9lXbTDJYZL6fs15HTxSw3Q3/5Dcz/qtxBe3buuBfaZhYzqTtyzppuyoWqKf6WO1holz1mdqa+oBb7qc2sW4F/57/nPAvcpm0jG2f6kk9UIN/paM8/mK9eKxl2q70N21gflU3M+fxvwz4dzikHl3H/2Txl4u2XLzQxd9AB6Ddavtr5Iwl+Ovc/jhcQ4+Lv1wgTvVmol30gdKkMd/wd9oDYPfhd/yB9btWCIzBPXe7u3APOuhgqZckX4+yjj32WADAmjW3h/aKtOTNYy309pn4xO7NN9+C/R6+nxL5cvKqU4p5Mc6qx/Upujfydfq7dohbXx5iOT5lkZpbSb7dY+KNWeoM63n4la9QrDY4JpQd4oJY9n960hdSWGSX5MRWF369GAPna4O40JzGGvOc7JicGbKQy18Sx86lUmZEE9a3svCb5sM/4etp6nRzfqV+LPOLvtb5PNro2sXp5fzHOZLPck3jKgEA9jvo0ciyDIcdfhAe/ZgjUFqL7ROD+PEvb8bVt7UwMbpJzQvtSd0mJscdI2sxNj5S+QQNt0VRRDoAZdnGsuUHotWaQrvNReApjI9vRP+CATziEY/AgsE+mHwSfX39aDabaDT6sNc++zl/+D/KpYLMi3HibmBxMnsb/0mXjovaPrxIHo/Zbu7nmjPSFUW8YQ2IfatjW+WR/kijyfYy/ue9j//3T21BY8FmDGUPYFFzKxY3t2FJYyuWNrdhj8Y27NnYhr2a27GssR379O3EstEtOGLRvpV2LkYm0HpgGwzG0IdJ9GEC/dkEBrJxLMjG/G8Ug9ko+s0Imq3xHsb/2DZurJv9+B8XatMFX3mSNyzo2ngMWfCtLPLqz9OH4wLWPwFcN/5babuyLGEyg2bf7MZ/4rcsS2zcPoWJCesXft05CMdijsG2tCgLi3LnNjyveT++eNQUTj/E4K2PbOKCExbjqXkJO1EgsxP+O+BTMOUkMrsTtpgEykmUZRtlu42iXaDtH0fN5zT/dymO//HmNJ5DZ/6ct+NJXz6lywXb9jjWlZ/BWvs5rMU/4D7zBdxnvgiUBd565rvwlre8G295y//BmW99L85867mw7Qn3ume/mAzPE7IIPB3+aYvZxfl/af0TwLI4q08BT41a/MWLDLIMGJ8A2m1g07YS//DdFpYODiIrgEU58IrjDSZaBuMt1/39669HsHmsD8bksLrwq/ucI9ad/yd9NqTf0T5TbU19oHX3Xrg3Dl9xeDhm2jq2Fef99DxsGtlUyT961dE4csWR4biwBf77lv/Gf93yXxhvxbGD6WmHPA2ZvOqYifFmejj/Z7xpuysd25G/m4bvDPXHGwaXHjSEbQMZitJiwVHHoHHoEfjOlVNYvz0+aEE5+hvc/2jkB++Pxxy9GCsHDkL/yKEY33QEdm5dhRZKjBVTGN6+GpNbH4XmyKFY1jwETzpiCV79ktV44uMPC+e7rk9058K8DlE3/6e9HCczE280M9IvuTkFMDw5hvOv/THaZYHnHfoneNTyA/Hh55yGkckxfP3K72NsaiLO/xNszypZP//02IfEn9X9pD9km8HHJtuPeZ3n/34s2IXxf77wr3EFsU15Ug7rpz5mORN11jqUxZ9iIR3/WVe3ELmzwT/lUZbaxLoP7vl/Z1tRD8wS/1pPZaf08DZRB9Ux1Y1P8tsex3/KLme4/md6uP6nMm6//TacfuYZGB4exs7hYZzx1rdgzZo11et/4sv5Gf+r5/8333IL/ubd78J5556Lpz/jGdhrr70AAIWfB+69997YZ599QszC67FixQo8//nPx/s+9CE890UvxK233eavyZb+k3gZSv+GjzJc//9f/FMXAPjARz6M4ZFRfPEznwlP/P7Hf/0AT37Wifj4Zz6NtevW4dhHH4PHHvNorFu/Du/7yIfxlGc/C//53/8NYwz2WLoUX/rMZwELvP8jH+7wE/VAgv93vte9deq4Y4/FsY9+DE4/+U1459vPcvSlvyLg9V+5YgXe8/7z8OOf/Sz44Cc//xne8/73YYX/7BDlmC74L0WPoaEhXHn11bjiqivD7/Irq9ufXXQh7rn3HpgE/0uXLPGnnr3gP54Tp7r9oeBf+VMf+Bt84mcS6UsTHlabT/yzDN5PafwrfrIsg/k9jP+ZGsoK+mMldTAr85j7NnlEnoprfSrJYy4csQNut9uAX0RTg+GVLj09k4Jf5dNg7huT+e8IRdCQXh1n/BNRGiCktdZf0MvjAjLz2WBaxxh3AYv6g4GQuyed6TfqzDoOiP5JJQkKww7RuAVOt2DuFo6oQ6PRBGSh190p7croP9ZNbaMOudwxQHsYG3neiAvdMslw/JyfIYvi1CPL8nDXNgMeAi6NIye7Gksqyxh/0RfxpMQYg7zB7w9H/5d+gLRwuljrbADgF30zb4/rCPizlq8FiK/psYgLv9rGecMt8qt+1F1TWLzwPs58h0M96WvAqUFf1flI/cdj0jGf9FmWwRqDdum+92zDNdzYXo5HPBHjz/HSdp0t/t0rsNlekCfvITFWwb90bCyHAbJG9fsQqMF/u/CvoJM7tRU79BF/ReG+V134p+zTxdyUnv5kufNlfKJW63Bf9bXS9vQbfVZaC8hCvCs2KEsbTood3iMmGAfUudFwse1kOrksC/iXeNO+MOjn41l9QJtTHkxKC4kLPSb/rCf8+88BiK1MqU+Zx1ggT9YjX+YTzy4+oy80WRkbSM988uZWy+HlzA7/6YTEJfqlzkfqPx6TjvmkJ20hd6BR9ygvtrH+HK84EcyyHHkeL8K4fl7x7/Dr/OJuqtH69A2Pnd2Zn4Dl4XXF9JO2TSX2rK1d/LU+z13DdmW8eAzrxk3ab/13gnnxp+Qx+XBhWC4O0Z/Ug3llD/i3Mlk1xi+e+vxKSg5h3SJuWVocfPDBSaFP3j6dG+2/v1uwvevOu4I+UajU0y2Eh4XrQwxw7LGPxSWXXoJ169aFfsnv+GQBGIyOjuKCCy7A2886G6e++VR8+CMfwZo1d4heFldfcw0+8pGP4NQ3vxmnvvnN+PBHPox169yrOOG/NXzqm0/FDTfcgM989rM49c1vxg03+KeYAVx99TX4sNT/zGc/izVr3B3e1OjHP/4J3nvOuTj1zafiveecgxtvvDHU5w1W4UYr63R3mTHL+qdO2X6+JNga/aPldI36xmcz9vhEsNBZ6xf8hFWFDjZuPY7qtirXxVhcrHUyaJws4gp9iHPSxcKwDXyZL3RBPmOfBVI/6OFtdC50fgwLi9b7WWgpV7WmznD/sHjZfvjXn9+Fy665B7/8zd34z0vvxpe/fzO2bNuKdQ+MYnyqwNTEdic5LGxajO7cgo0b1mFsfAR33LkWa9asxcjoMO65dwNuvfUe97vtXtx66z245977MT4xhg0btnhcWeyz7xEYWrgErSm3+NtutTA2thU7h29DiU2w2RbkeYZGn3v6d2BgAVY+/DBvKv2XxJVv64hdv8AmY5uOq6WO/4xtzlnTsdv3n6G/8/Na9qF0aPRRvOnGJZfHYyc/zsPSH2nsDOO/l+xuCNbxv+h9/N/UXo8Vi3Zi72w79sm3Y3m+HcvzHeG3T74d+2TbsU++A/sOjeDIRYuwqDEYmbUK5JvHsGBsHJkdQ7+ZxEA2gX4zjn4zjoFsHANmHAvMGAbMOIbyCQz0uVeCU5f68T9eHKmO/zXzf++vdPyPr3Hmq5m7vMZZacKPC7/JcYWP+9myDVu2Aeu21Cvz83/ilO3m9IX7hJS0B21iffrG+L6adud5ju2bR2GRw1o39+UYrmM5Soty/d04fPNN+D9PWIqlQ31h/r+oCbz70YsxODIOgxHATsCUo7DlBMqihC0m3fzE20RbqZPGobZHGsvdx/9or03Hf//kLxdoUXlql+3Xmcw0+ekrnyv7/gKx9fgvPP55vYVbYr702Ct5oUuuzRg/l6zlAf9K5pqnf1sTwNOOs1i9HJiYcL++PuB9n9+OhQOL0ICBbQGH7mNx/CMMdoy510PfeM8UbrgXaJVNtAr3uQ9dWOYicMUfPoZ4bkn/E2+kIfbQ4/yfaUFzAfYachfwNX36sk/jdxt/V3n180sf9VL88K9+iO+94Xt42kHuySP4V0F/6zffwrXrrw15TA/b42EdC8CMNeqtWONnrdjPKx28raRnX5vO/9cOPxBwVViLax62AL/efwitzGDgMcdha6sPN6wt0PblDn66z5/B6OD+OOSEY/HZjzfwly/8Zxy7+jJkDwC/vWxf3HTlAWhubeJxq36Fv3jmx/C+s7fjjW84HI84eL+Ajzj/73L+3+X6Hx+i4JzGvcEF/nXO7tiWJX74u1/iW7/5H+y/x0p85kVvx4F7rsJ3r/8Zbrx/jXvts5v8AzLOzDr5OUyYE+kx0zTn/4xZ3cL7gu3LtmTc8pi+qp7/u8Syyvif9F+UZWe8/vfHd/7Pa6Ga7IN6/t/7+E9b1H88Jh3zSU/aFP+pPLax/shL5eSzuv7XffxHMv5n013/S87/mdjmtKkoCqxZswZvedvbMDw8jPeddx7ef+55GB4exhlveyvuuOOOQEt66qQ+1vZQetKwnHllzfn/177xDbzyFa/AylWrgr5pajQaWLlyJVavXo1HHvpIHHPMMTjooIPwohe/GF/60pdwwgkn4BWvPQnr77/fXf/zN4DymhHbljrMD/4dD/UBbU55MCkt/iDwD3zsQx/yC5sW537wg3j/hz+M1/zZK/D9f/0uPvXRj+K0U96EN598Mj7x4Y/gB9/9N5z0ilfi/R/5MM754AdgrcWSxYtx7rvf5T9b5BJ9Rb0pl2nd+nV4xUtfipNe+Sq87tWvwUte+MJQlud+Xuvx/5wTT8QH3nuOXwT+KX564YV47wfejw+ecx5OfPozgl/qfET/qW6my3WHNKkN6sd/+PIX8YznPw+f//KXUE6Lf73+94eHf4h/uG98DGdJzEf8+zc/dcW/04c0KX7KGvyntkPGV/VbUbi3mrCO2wLWlgDceXWWGRgDZJkB/MMJzI/n4m6BnOVu9h/LnP+KUNcYIKMSdDjB2fDv6lbFGRR0MuvCd0h0BvkVfsDhfjAwqMa6zuiiKNBoxg5MHUl5rKPOU8drA9ImN0n0uoud1DfwIr2XpzobTiYAP7erBjJ14MWZQC/BZHky5vlqsAbfeAOjZ+PADCBeNOQCrwQNbc79CTonNtSx3W67b6pKZ6r1s8w/oevr0aYivGbBAZB3ZVjfHlZORChL/coTh+Bnf2cIaemrqE+8C4Q+dDbHCTV1BvWVhXa1STtnrcN94+8y0bamTPg246KiJvqrLN1dWeQJ3yllMsBRVogDr0O73e4YUGkrF03cwqtL5EW52omwHNJ+LKNdWZa5CzSZCb8S7gIsZWcz4j/GbSqbumMG/GM6/MsEhvmhzizxX/jFf/qWP9pJfR2varuTN+WTB2WbCv79idkM+GfdgP92Hf6jjUz0IVPqE9ajfbmfoFMuafXuR+VFvRmzrMcbZiL+XV3FPxNlqF4s5z6PZ8Z/7HvoQ+brj/xSO9Unu4J/8mO8a7KKf5koYc74d7ycrQg3Xbgnt12MsU+gXMYNE+WnctSn9LvqxTrWP/WfZTkazabve7hQ5WjKMP77ugZBN+snt8RSUbSRefucf+VJdG8TEBfGiqKNRjPewMQ5BftAp6qrFy4K2+rib1gM9tjn4m9YDC68j/2TRfy5t7/546QO24TtTH9qDDNeWWZq8F9ai7zpsePvBIW0W9dkgNWrVqMsS9x7373VyYEkC3fhiytkGzdsBACsWLnCldvS+68LA6rB4nBs8ZxnPweAwQc++EF8+zvfxpo1a3xhTKOjo/jI330UN99yC17z6lfj7LPOxt7L9sbHP/FxrL1vLQCLzZs346c//Sme+MQn4uyzzsIZZ5yOoaGF+MTf/z1GR0eFm8HXvv51PPLQQ3D2WWfhgAMOAGBwwbcvwFf/8R9x+OGH+W8Rn4W9l+3lv6nkFL7sF7/Afffdiz9//etx5hlnYHBwEF/7+tcxNjYajDN6jc7HH+UGB0h/0pl8ZRf0Ps/Hs5EnOv3Wwq9QCnvrbzwLi7uWC5l+UTTwIKf4Zz32VDfGEfNcnIXCiHeTXJR0xEDSx1Zo2H9rvx5Lgy+Y5zATfcS6dcnALXpa65/m8bmQV227FOurHGePoxofn8JVN63H57/9S/zDt3+Ji66+B61WCzuHd2Lr9m0YnujH+M51CE9FwmJ8dCusLbFpyxTGxkexYeMw1m/cifGJEWzaPIx1G3a63/07sG7DTmzcvAMTE2NYt347pqYmYUyGRqMPhx3zdBRFgXbLvQK61ZpCa2ock1MjaLem0Gg00Gz2odlsYumyh2HRYneXtzM5CQ5J2k/neQOl9Dt2juO/6+NKd3Jo48KvLdk3xYVjLvSWIa5Yn+3sv59ofVmoJ3EocTPT+J8Zg3wXxv+x9l1YYeKi7z5c9M3dou/yfAdW5DuwPNuB1f07cNjgw1G045hfTrTQt2EnFuUWTTOJfjOJfjOBATOBBdkYBox7AnjAPwm8MJ/E4F7RnrmN/91tZXL7XMQtPWa5nyz+hjxPk9IpH5Cm8O2nC8F+K/HF+RDtAKo3VqHH+X+o630yMVW6GyBB1X2M6Xg8shPFnbfi+P2WYqCZo/AxTV8NNXMcvggwdhS2mAAwBWNbQFnAllNAOQm0x2FtgXargJlK50DVeZ+2hcao6TL+d53/69O/6Td7y+o3ezUZdMlPXyMtC788Ts//W13m//Q/Y5b1aFNbXrNc1Mz/syJ+l5eLv+6VzSWe/VSDRmYwNg4UBXDjbS38/FfAYF8/sjbQmrD4y2cCW3YC41NAuwAuvXESm3c2kJkcky0AbZHBRWAfH6ov7VSb5mP+DwD9zX4sWbAkHAPAr+/5NX5w8w8wMjUS8v7ycX+JL738SxjsG8ReQ3vhMy/+DE485MRQfvPGm/H9G7/f8cTwisUr4jAn/YbqYIx7oIDf+uX833L08LRpP0Nb0vn/VDkF6197bK3FWNPge8cswUjTINtzLzwwCgxPlOGNbRZungyODRW8W6zb0cTRj30Mznlzhu++79u46h8+iru+8Le4/TN/i6s+93f4t/efj/e89nocdeRB6O/vr9hlezz/D4m2eVs5pzEmzjesLcMrrttFGx/42T9i/fBmHLnyYGwe245PXnI+ptotPw2I41/NENxTMnB8DADQ/+zPPY2VfoX9KNtR20xTN8zqvp3l+F/l5eQT/6xH/Bf/D5z/8w0CKpP82E6a7Hyd/8tDDbW2yo18zAv4929FcYWzx7+e91B2xut/Tbn+588zaGvt+O/lKb8w/hed478m1p0N/rlPGaS/8847ccZb34Kdw8M475xz8MynPR3POvGZOO+cc7BzeBinv/WtuP3222Pfmeis8lRnUxOjGsPUQel/8rOf4uhjjgk616Vms4nVq1bjqU99Kh6+38PTYjz3ec/Ds5/1LPz9pz8d8mzdE5j+en85J/w7vSP+nV0PZfx/+mMfw+GPfCTyPMcXv/pVXHTZpfiXr/4j3vRXf4U999gj1Dce/0sWL8ab/uqv8M2vfBUXXXopvvCVr8AYgyMOOxyf+PBHkCb6i5iA2O6uodXg37pxgHq3220858Rn4YPnnIv3fuD9eM/7z8MH3nsOTnz60yt2MvGYcrPs/2/vveMtKcr08ae6z70zcycQZxhmyEGSgEo0AEpc14Did1WCGVEUMICuuiqIYVXMurpmVyW4uwbQdV0EBDESFAEBEVDSMMMMTLgzN53TVb8/qp6qp+v0uWkC+Nt97+fc7q566031vlXVXV3VzZ+9nAiUdrRhOA6uHcQ3Lvz2OM///XM9phFIS+skxn/D+F+BZTdE/DOuKSvLR9nDc8Hu+G9u93nN57PkbSYR/6RH/2RZ0vV2dCgKE2Lax3Y+AOkVs3qedPYTvcqXuJ1Ou4tWkQzQbWAWZnoh20uYMGuvZZjvpCNRXA4aVSga0jm/vRnfAFCalIUDzrw8K5eymuAIgN9mtar8Kj8XOmfqTLk8Lb99pdKF2MTBAYV3BMpFHi7o1RbZi8JvY83y6eFJch61Fx+gq43oVBU73LD+owojcg5uqLfHSTdE1JPA7x9SbtXVyMpMF5wn2do/jEcI7OhAobw6OMTGRWig1Jbk1aWbc3GVo/Innn6rOOKHt2B1gEKw1k/W11ebVmEFc9KB/BXoKxDb6Hm8Dt/e4eQzbd3hd8SkMULUMTzgkMAlPe8P3gZJZguEVUgm+HrTOXmrjRVyXrx2wd+cCZMo/llsLU5Jm/5qwwpwfRNI86mnx2X8p0FDTb7gdywzXvw7FyJg0vHvj50Qaxgv/g3Q15/in77dy67Uj3nO+XpHiMFCOoQmOlVVoSj9G301/RizPWIE0Sea45/5So+gdcNyPJpe8R98m7gaO5oW7ZbFP3XDpOI/2Yz8mUaZCaoHrykXxEbaSVt5g1Hzc1C6qjvPm64pNyYR/zxnmfgWf1mG3SHCjZ/x32OGtDXWppddaHflrTZWiLwou66EVR81iO0peTLfy1f4G4TCoKxtx+b7l7itedDFVl5e4noZfN/o5SpQddj/l35LxiCDp+npsV+gXF/cfgku3HkJLt7lIVyy+0P49ycsxX/u/TC+u/fD+N4TH8alT3oEl+63Aj8+aBV+9JRH8N+HrMJH916LslXiqiPW4uoj1+Gao4bwy+NG8atnj+FXfzeC657XwXXPa+O657dxwws6uP4Fbdx4Qgc3/YPDV55ZH0x1x7//XgmhV/zHjoV1YTRRzsUGcA477LgjnHO47957EyqruF7VkcStf/wjAGD33XcPGVmBvHxsK5z/OeYZbLfddnj/+efjiMMPw/XX34CPffxj+OcPfxgPPPBAKGfwy1/+EsuXL8eb3/QmHHjgAdhtt91w6qmvwfz583HttdcCALbeej7e+Y534LDDD8Nuu++GJ+6zD0468UQMDQ3hoaUPBf5ehoMOPBDHHnscdtttN8yeMxt33XUXrrnm5zj5pJNw/POPx2677YbddtsVJ554Irbeeqto4/nz5+M1r/HfKt5nn33wD//v/2FoaAj33POXUCdJ1VgvNUgGNYb/mM5fNI2chLq2fpzmJ3A5avNnnNTlJK8vGeixLQl/EU9wXIhRY3xH3SvW8zTEslm6GKPJEorv/TXt5NHFg22RyhB4Mh3UxRvWWyjc9Jgwxq+RDDakdevWCCaMOhiMjI2h3WljrNPGWLuNdif97n3gPgwOG/TNmIvRdY8AMBgaXI51a5ZjuNPC//zyOqwaBH57y634zc03Y+mKYdz0p7twzQ3X136/velmrB1u4WfX3YilS+9F/0z/lvmiHfbGvk85Gu2qit8CHuOK4M4YnAP6+voxf9Ge2GmPp0bfok6pttkOhz6gFpfpevz+P7WXBO3/OVHrnEz8Sn/gfzZO/iLUk/+lFzqZ74J/8YUZQk6TfjFe/2/DwyxNm0r/X1YPYhvzaG3V7zblGmxThF+5BvPLNdimbw3mrluF7WbuEWMRAMp2hdYDy9CCX+E7sxgOE8D+esAMYZZZF45DGDDrMHuHdC885f4/61Ni7Mg4JsWTRX0SOJ/QdfV8/UW8fOKYk7wV4MIKWdeJE8HOpYmKIkwCmq77f3+Ppj5WNDwrcNIeUC/e/48MdWIoO6cvaYU21Tq4e/8E06nQ39fvy4cxEfk457DzZh3AjqLACGBHYO0YnF0bVzbbqgPYMTjbwR5u3yhLX19fTS6EeuJR64X6Mc813f9LXPbaAlqvm8DImFbBryLOtpHmMfCK9g6gdQPRkXpxrOy67v/r/qg+CdQnfnneGXY48unAFpsZrBsCRkeA0jh89POrseWcuSitXyH81D0sdlxYYHAIaLeBG+8cxe33G/S3+tGpDEbb3j2Ljv/VVhvLfTplJuj4XmWf6vifYMI9OGHd2Dp8/pefxwOrHgAA9JV9eMPT34APP+fDtc98bLf5dvjA330Ax+x+TPx+8IW/vxC/e+B36FjxF1NIr5ZsW4t/jv9ZXzat0O7lp0qPefEaJny2K4xSnMPSgRYu3W8eRqsx9JWhm4bHSRPB6SctDmb2A8Y4OFvBVqGQs2iV7DccTFEfRxt9/jeZ+3+XJlgDgVq6kzQ49mue91YDm2HujAFU1mLejDnYctbcsDrB+mMo0/fwCGbcO4SZfx3Cyj/9edK/aqy+C0SUR44IunQ//6vfj5kefSTEJ8bv/xM9wsaKf/Ij/C3c/1fyfDAHpau657bQa8qN6fT/8f4/7FI50f1/uH+2fBbAe/Tsvj2CSff7pMtr/iiTH3fW6TC/KLx8rO96/5/6ROpZsP8v6v1/bsMpx39Wnj559913441nnYnBwUGcf955OPrIo/zz/06FY48+Bue/91ysXTuIN77ZTwJTB9Ja3/4/v/8fHBzErFmzYprCrFmzsPdee+HII4/Ek578JMyZMwc77bQTnvCEJ3SV+btnPxuXX3lFuE8aP/7deM///xfG//IVK/Dlb3wd577zXdgrTAj/5rrf4k1vOwdPefrT8KSnPRWvecPpuPLqqwEA++y1F8591z/hy9/4Oh5dubKme24LvabckIlD6h/larCFL5Nsx2f/xFNbm4bn//z+dIRU3eMCefOXg9YV82sxPZX4z8b/qp/ZgPFPHKPzf+GlF163ej3/h7835zwX07x+Jr50wXTqRxzXEP9GJnT1aAz84piiQFkU0S9IR3WgfZIs48c/85UeQeuG5QoSo0JUEKIYkZnHyqTh6cBkrOAQHljIUnmWJWiHZRre+kCgQRmYTnqNYPwNqXX+wbJPSvLb2vYJQU4JLtWDA22d8KKMNgwk8jLxwZ3xD3jU+FoJXpfwJoc4V6Tt/ESnRdiqyXZv0VJVftafq60IdG7n/ENIugLlrDX48rYcZbPWoqqSnUgTxsCErSgcvJysN9IlTQLrjPYjToL0fWYTnD/Wv9jV21senmZ+FfFDfaizI7wFgRigPp/yO/qr+EGkKb7JQRKBOMSj7LSv4YPNMMlWFGESOPg17WTCN5xzuh5SPdN2Kc9D1CPrwNXOzNMyYPyHFZ/Uj7I5+HhiPdTjP9Em/xwoB7cWyWXwPNODY8quOqqNff1PEP+MPdnSTOW32fYpoPzyAI6aUS/qzTTVw5cpomOkOq37RHP81/0s+o/tflvJhpsYlYt+Qb0ItfgXHyAfjX+1Uy3+O6nzVJoqP+Ugb/qn8lQ9FUehV/xTXojdCawXZD7CH+UkDXbSyif3W15TXuapjgq5nLH+JP6Jo4MRwLefzqVJHa4Kj3TDDRsAVJ3Kb3PP+NebvOnEf1j5jzh5O07/LzsscDLX2rD7QSiS29EXlPhvSf/PcuFmNPb/hd/uk7yN8fpTX96Qfvie2Xj7HXNwzm0DOPvWAbz1lll48+9n4M03zcBZv5uBM6/vx5k39OP037Twxuv68fpflfjErZ7/637RwqnXFHjtz0u85mcGr74KeM3VBV55pcOrrwJe/TODV10JvPoqg1ddZfCKn1p8+MbU7qFn/Ndtx3TQ3wBUcZAYcH3DFNIky8kPBvvssw+ss3516wP3S9lwNACknq+++mrcfPPNmD0wgCc96ckxHRB2xGexKH9E8Djhcvbs2TjxpJPw/vPPx6mnnorly5fjAx/8AO6//wHAAHf86Q4ceMAB8VtHJHzYM56B226/LaatWzeEa3/+c3zly1/BZz77Wbz7Pe/xOWFC04PBQQcdFH0EAO655x4MDAzgsMMOCzgeL8nt+e25xx4pDyZum71kyRK/wiOo6osZNVuAlKB5Jk8gRBMFOYyvQO8DQYFQj9GnY1EdmSW/YZ4+FGZZF8ZzObAsYwfw9qzRzNtlnmT+G4G4kmcMnxrXaTXaBimd9GOb51O1Mrwbq/MHti5ZMl41yTsyMop2Zwydqt31e2jZQ/ivn/0a3/zhDbj3vrtxz52/xp133oJ/v+JWfP5b38NVv/wtfnzlNfj+f1+O7//35fivK67GpT+5Il7z98MrrsZ/X3UtfnzVNfjdLX/E1773M3z+W9/FF779Pfz4uvtw7d2zsGzlMMbGRtFuj2JsbAyjo6O4b8lyXPyTW7HZ1jsn2aOK1DDY2gW7OcDEldB+/Mq3pNneTqf/d2FsZ0Oev7aepXV+O+ew8hJAfPjkq51lAr7QIDjpg/Ifxun/ufK3lJdHtZ4n0/9vaVZgQbEaC4o1WFCswfzst3UxiPnFILaftQ6LWnMxyyxI2686B/Poapi1qwG3FjPNCGbEb/7Wv/07q1iHOeUwXLUCM3ecGeWcUv+fxWrv8X+YrOKEL1fp6iRu09bOjddM85O7zsox/PyKWT8RjLAFtAljYvaDVl8G7tX/ix4cX7IsQWknfwpHeTHBrloO9+gyoNWPPzy4DmWIA4VB28avhu9H4dbCuDUwdhCwawA7DFuNwVZjgOug07YYqObgaPvcaH/Kzx+B6eP1/3n7qXUKIE3M5hO2ui10A/RKJ42mlb9cZTxe/KPH+B/5+D/z16bxf74FtGsDW2/m8KR9DcoCGFoH2Ar44f8MYcmSGZhR9AFtoKwsXvnsAg8/CoyMAqsHLX5xcxtLVpSY3SrR6QBjY/ArgGWFsV9d7OUpGuJff+s7/ieMdEaweni1z3cWP7j1B7hpyU1o2zZm98/GG576Brzn6Pegr+yLZQhPmP8E/NPR/4Rn7vpM9JV9GBwdxDdv/CYeXJ0+e7FscFmtjpDHv/H1VYb7f7aNCpSbfsnySld9dn7fXDhrpa33bfpP95iD348+hEXzLBZvEXaFi31E6jN4XjmHsgD2WdxCv1sJjC1FWfgt1p2rUHUcAH9uzYKaDJD45zllV/21bl3oKXX7yxz8jhT+Z63FVrPm4asvfjeqqsIlv78cZVHg/L87HXP7ZsVtosHjdEHlYfzHLD9mYn3U4kf6BzQ9/9uE9/+YRvxTDvJm3648VU/FUdgU9//tTgduCvFPmqSh9iV4nHTvTNl79v/ZwhXneP/vX4au0e26/2/F7Uo5WUHgy9bOpZ2u0gRuuo/2k8qeqI33//7lbqUZZQPv0X3elPv/sNOR1pOWo414zjqmzVgmtyXpIXw26Iww+fu+c8/D0UcdHXS38bnDMUcfjfedex7WhpXAd99zT6SN9ez/8zLOOcydOxe3hZewCdtssw2e+tSn4qijjsIuu+6Kvr56fzF37lzsvffe2H777aN+s2fPxuDgoB+XVzaOeyhXU/y7/4t/GGOw9VZb4fsXX4Kjn+U/xfDu89+H09/8Zmy3eDv866c/g3/91Kexx+5PwNvf/U849wMfAAAcefjh+P7Fl2CrLbeMNMlL/ZaQy8mYy+MfYR5A7em/+XsePvDec/HBc8/Du88/D5dfeWWNLkH7/zwPgH8W3x1+XZA/s4f0pfPmzsWrTnkZkMe/6Md5MDvZ+M/ilWUJNdtNM/6bgLjEI61WiJMyPJOjjpTft+WpjvyKeG59b4GwLbMfW1RA2HLZk3cA/DhKedKfeVTeqpPi0g68Zhr1obxN8Y9Jxn9RcHKExpeBXRzsBbU4IaFpdGoeuV2uDRMYClSIFQlvqqgYpDK0sp102MwjrpHGIhox/FzArcIWBgxIGtHLEyZ4RUbSLopCvu+a3lRgPoCwVWZyehuCIuKJU7PivCN5Wa1HiLpqXlEWcOD3Rf23F7UBID8T3sqO+gf5iOe3+U0yagPiQj3RTizr7e9tTtvSBziQ4KQAbUncovArwZAFN6RzSbhlbJBUBtqLerEOyZMyEdcFv6yC/e04e7IXYdAX6zr4K+VkHZB+lBf++6jKt5A3Xag7eRWhXiCNlTb+BOccYBKuAmVWPRDkpYz0X27NQd5Kg/WDzP8oF/FI07nwaNqFTsX4G1+/qVIe/wDCAzv1IdqXQBtRF+IpLtuWXN+u+A8T1NSVdGo4QJxUt9y6xvg3p1P81+WMPsH4F/s0xb++NYgs/uk9tH9T/DuJI5fHP28kgp+VoZHP41/9T+1KPE1HQ/zTN2LsOd9eGJMm3JQf6ZuA0xT/1JU4hO7497IzLY9/6hXjX/uFLP6pC3/0GeLznDzJF6IPxot/qR/yLSaIfxvaLPYjevPHwRrxiatAmY3UBcuozgDQCtsLk7fSoO0AxDbMmDQpSzylm9tA7RzL8M3iUNbH2ATxLxO+uQ4utDfUmbx0ctoYg9vXFLhpZYGbVpb4/coCv3+0wO9XFvjdoyV+96jBjY8ANz5S4MblwA0rgBuWA3es9HLeuNzgxhUG1z+M+m+Zw3UPA9cvA65b5nDdspAWrqca/wTav9XXQqdK31NsBBMmf8Q/AIf99tsfz3nOc/H73/8eF114Ub2MR4kwPDyMz37uc1i+fDlOP/10zB6Q71sC8A+nyASpsMhcc1JNdv6G9MADDsT7z38/BgZm4xe/+AXgHG677TbccOMNeP3pbwg//43e733/B1i+fDkAYMUjj+A9730vLv/pFZg/fz723GNPnH322ZFjslvodyiqc7jjjjuw0047pfxGuWOBOCivmTtcuzC33QTN9ZPGk+TrOEEbxgaIE7bBtoGRUZomTeZFiJN8XTkAfF44SRBVT/Go8aE6MI40X/O6gMaRPiym65F1xuwgD3E0BphGXeOKZvi0GFfEzSrO4/OaZcN5sKmDw9Llj2JkdBRj7bGu30PLluCPd/0FF/7gp3jTP38Hn/zmVXjnZ36ISy67EjfcfCfmzp6DuXPmTfo3b848fPPSG3HRD67AJZddiUsuuxL/8eNrcM+SR/Chb96AD3/zt/jkRb/BR77+M5z9sR/gtPO+hUt+/Assf3RVaOdoPeoW6igm+TT6mQkvCPmH21579kGxbQ02cy5tu6XpCP2/dWnlr3XWT/7aNOYLVRXOLZyD3wbaWn9zS5zYT6S+oemn/SPEJ/P+nytyKmvjjbqbYv+/ZauFRX2DabK3TL+tS58+vxjEdjPXYOGsfQGT+kNjLfqXrcCsmRambxT9Zdj6OWz7PMv4iV+eb9EaQ7lNG9iyP+pDWrH/n8T432R9NIH68te1upfnzslEr+TV0gIOwuSvtWHFL7d6TpM2cfVvmBxGqBO1O+Vz8L7MekLQifVK0HtU6qn1VrJNrk0C+wfIzgFm2X0wRQumKPHbv64JtNKqA+ccvrL6NjxSrfOzkK4C3Kj/3q8dgbEjMOh4/7UVnmNegC2wVU1OnrMu12f8TzDGpO2euQV0nMBN5zu1X4Gdx16OnUdfhl1GTsYuIyfBuAqf/9g78YUL/hFf+Ojb8YWPvg1f+Mg5YdK313eA/fV48c802t403v83x1qOo9szmw5QVA4HPNlg880M1g0C7VFg+cMd/PDHo5jdNxBXCL/gCKBlDIbCCuGb7hzDDXcA/eUMtABUbaQVwOFXhl9RBR9piH/+NuT4f3BkEA+u9BO2ywaX4Ue3/QhL1izBQP8ATn7KyXjrEW/FzNbMiJ/Dftvuhzc94004YLsD0CpauPLPV+KG+2/AaGcUAHDbkttq3xEmmDDur9WFxA11xjTu/7eZuTX8DuOpjm3hsKavxPdX34yibOOQXfpQFC6t9JVv/8b4dMD2WxbYb7sWivZSVGvvAeBXWSJuKW9hjMVoa/eoC7L45zVlpr7I7/+9WtJN+nEWrz2d8FmCIOhrD3kBnrxoD1x33x/xrh9+Bnctvw9P33k/PGnxE6JCfhI4dHzThFgvkmboX9kEWu6Xrsf9P315U93/q0zEUX45zv/d/xdhQmAS/X9YOKPg8dOzgjQeNHEywoTPQXneSX8XP01k0Orri7SKMj23jrTDAgW+wG1MESYTQ1zFXWPq7QtloY5NduFxvP6f9aQ+QXrEJW2tN+TxL2Vp5x9ceinWcOXvUUcJrp9Ut+H537FHH433hZXA3//BD7rkVDnUj9Gj/+8fp/8/9uijceutt6Kvrw8777wzjjzySBx00EHygnRvWLBgAfbdd19steVWuP2223DIwQejbLX8CwCdMIaJ3wdtjn/urKjp+F8Y/zuF3dOuvOYa/OgnP8G3v/JVnH3WWTjogANwyEEH4Zw3vQnf/PJX8KOf/DeuvPpqlGWJHbbfPtJXeXvHv5dhu8WL8e/f/S6+dcnF+PZ3LsF3L/1BtJGnE0nip1ddiXef/z68/z3vxbFHHY2jn3Vk/CYwJ4G1HigDNG7Ef8uynFTfpW2U+veZrz8dV/zox3j9qa+N9NUGyc4pXigTj49V/JNOjmN6zP/pvaXKqXJwzo3AF2+YjymM/8nTyCpktR3P6V+qF/2s3Aj9f0EBK+sndwlkoMZlWt3IqTIpJIOcRypBYHrZquPmClAuTdcA5FYbNjQWRVHEgSodkZVugrPz2tP0bzfmPKPu2fdyyzCjXpZ+0pyTcFrWhIfqReEnxJgPkcmysQxb1NK5i7Bc3Vr/QIaT6UWRBiTqoA6pRVFbx/ooC6DovhlgPYWErnIhI/KrbPj2MdIbZfpTh6dMWt+0KXGSDj4vNY6ef3RqsW3ZKuPEBctHeU16M53phQzyVNZU9x6HKz7JJ/IPW/M6Fx6KxQdj/sd6U7q8RvANKwGtP5VRbcM08EGYvFzh7Rq2vAp+xglvPde6huhEHVVmzdM61HI1Oygt4yd/4hHhLcJWCVMWcJzs6or/5I95W0EbINiPfqTpefxTb9Ji3kTxz8ljiG3Ih2YoOIEfQOOf+OTHsj6/FWNW29Q8/hF4eD/M4p8T1gGH/qTxj6xema5pfEBGMFn857orWOdQVelGyePU/cFl8Q/A77yg8S8+p22Dc/6mmJ0s+fv4L2M9OOf84FfePPP4/obGH/3KVNLh98q9bKmuWL+8SSrKMpanDj7+u+PW/zwey/Ka9FRmL3c3nSRjc/ybMGhhHu2iR7bDNtw0urATQ36D6VyYUA2x2iue8zrkea/2oulIv9KYJi31B6bnuKorzykX0xn/Phb8j6sXrA0Pi206t47XDmvGQnsAX4+gX3iG4ci68xfRJG4q8Z/aIuYDXh5udx0hTHbHe/4oGM8DEoDnPue52HOPPXHZZZfhPe99L2688cZIho+c/uvHP8bpp5+O22+/HQsXLsSz//7vWVygPrmWpKkjss/rdVcxe/Zs7LTTjli+wk/u7rjjjjjwgAPxtnP8t3nPOfsc/zvHnwPAT3/6U8weGMD7zz8fxx//fBx73LHYYvPNM8rwsihbY7Djjjvir3/9q8hDecOx1n75OOdPy9CshrbPwHFurkvv5COcxPQYDkxJJbzdTOi7E16SI58I5SQfEPwpqw9eG3h/qflWFpu90pV+BBNmxAWilMxjfPjE2jHWgtyoxrKk5byNtEAXbrBrKhRijGUMwpg9WFMmLEnruj/8EWPtMVRVp+u3bt1ajI4MY4t5m6G/bybue2gQ/a2Z2GLeZth+4WLMnjmAubPnTvo3Z2AOtttmMbaYt1n8bTYwB4888gg6VQd/Xboav7/zIdxw+wP4073LMDQyiuGREVx2+S9SPRnjzWj8udc32Jt1B+M9xPkVwOlBYLJxd/+f+pKiqH/SxLdNwbahfUwrwPyEsD/3d1PpO+guysGxSCwjOE0/hfp4ovf4n+VcGEfHtj8b//NIOgtmPgkLW2uw/axBLOpfg2371mCbcjXmF6uxoFiFBa3V2G7WamxuW5g781CE22A451ANrkX54L1w/WPAzDaKGWPo6xtBfzmMmcUQBoohDIRtnweKddi8bxQzd5+DIozfVGbK3WQL1oOZav/fa8I3fr/XhglcnssvrvTthIe5bb9dq+2E1b6VX/ErE8FcMWwz2ePRAJDPIuV9erTrJPr/7efQRmxy5LyywOrlQNECTIl25fDRH9+NThgvk1YfDAq0YTAC49aiwJhfbQsH6yq4jsWAnYsjzdHY1+zf3ebq/X82ju3V/zspy3z6QrSZzbZ8bviG76MnnoVHTnoTHjn5zVhxylux4pSzYZzFw2f/M5ad8xEse9tHsextF2DZ2z8Gg/pkMmqrgf21xj+B13nMqZ8RXIi1PF6j3uHHyVljAbSBxdsCO+/sV/2ODvuJ3B//eB3aQwMoXQk7Bmy3tcNT9zNYtdqv8n1kZYUbbu1gdquFPbY1mGkc2m2/LTRk8rfgNtO2d/xTxzT+T7JSfuLQRtQPDe0PACxfsxx/fNCv5vrlX36JOx6+A8YYPG+v5+HNh70Zc2fOjbhNYIzB03Z6Gk475DTsstUuaNs2vnvLd7F6xK8qvvK2K1HJd6B7xb8LR+ZZefBOuRWoA2moX+48sCic8x4JgHOwpcWN7mHc8PBtOO6JLeyxsIXC+LnRSFd+M/sMjtmnH7sssLDL/gOFWxlX1Trn0Cqt32XZOozMOLRn/KuuPG8c/wcZLJ9LOX8fSfsEAl53Z7HtnK1x0PZ746E1K/Dxq76F1cNr8c7LPotVQ4N48ZOPxazWjDT5K/E+LTB+pSRl4Q8ib2X9i/4u6K1xyu9tVzY9/+NOhnzW4cK9uQv8SIfpTDOFf5bEPOL7e27GSj5uSECfmij+WUcE1pteExeboP+nLfP45zMf8p1M/Pf6sSyvSU9ldj37f//MQj95l2j4PqYKLwozPdeX5bg6zZ/75yYJUl/GsrlezMvr0J96ebpkl906c9p5THtaqc40PcdVXXneGP9BTn3+f8rJJ+Ob3/g3HHXkUUCYrAH8jlveXun53zFHH41/++rXcPKJJwIiP/mQPn2IUDb0/3y+x7LML4oCr3r5K/Dr3/wGixcvxj777IOB/EXsCaAsS+y08074yU9+gkMPPtjzkwk2ZLb36fVni2YT9P+577De9Jq4eAzjH87h7DPPxN577QVjDC769+/gwu98B8YY7LPXXnjrmWd28e/1K3rE/0fO96uIb7jxRtxw4434wpe/hA9//GORPzsDYwyWPfwwPvDe83D0s46MNI47+hh88Nzz8NDSh6Ldcj1NQ/8PAGvXDuKphxyCQw8+GIcefDAOOcj/eH3owQfjmCOPwk477pBsEuitWr069Z3iX7kdPL73p1wu+pXGNGlt7PgnLeZN9PxfaXL1M9NUdy83efvvImv8E5dlma92Q6Aw7vP/4D+9nv+TlsYOMturHEwjXQKvqUPBQlqYBXOg8YmP8OFkyKwyhcwrlEobY/ybjmH7SS2jtIswaCllGTNxII0CwTm/FQ2VJS/qoj/n0uBJIZe53e7U3gKgDvxWppE3VmJ+UZ+MI57St9b6769kb7ZU/C5I/FZvGiBQ7iI4jJ+4SPITxxiuHGZbY+LgvijKMKHjUFn/yJHpJrxlxjooygKtvhaKVtgaRB5wqE4cJJRlKw6wtK5VbvqPp5Pqlvgc1LLuWdc64DAy0IoD4uzNO/ULyql+gWCbytrYiLAsJ0g8cpowYVnPqwTiinA2iDKx5UsDEhfMo08U0ri0Wv4tErWXdmbacHBQl+vKcqx3+rcLNwV640A5CNQv2iDGfz0+uuM/deZN8W+d/2428agfy2jM6zlEPvq54oDxL6sX+UBS6znpUm8Dovy94j/IzC1JuJpd45S0uuJfZOVgvnaTljXijfEf8FgPTuLfhHzGDoE41FmBdi2yDoZ55EMeTGu1Wv5lltK/KMFJUVP4a+8fBkVZprdKg18Thw+rFYc3FWXLd6j+m7KMM08vTXCkrYdM2IZIJ2fjm7eUjW+1GqSyYYsjvUb4vk6n3Y60lDYhXfuy5IVwc8FypEe+XmC/bZOXs1f8+zf3aX/WQe/4T/VpTFrBy3LkC5lYdI7bPqVYVx9hGmlSxhymGv+kRzzqxzJ2EvHfs/+v0mSvzwsTvtY/bKpP/gLWOsztC/I430C60F4iHmlbf0E1iadxSl3Gj/96/9/qa2HdunWeEYF16SsqVR54nmD33XfH2eecjd122w2X/8//4HWvfx3+4cX/gLf/4z/iTWe9CUcedRTe9ra34brrr8ecOXOwdOlSvP1tb8O6dUOeQOwj0o0IvGenC6+5j5m4rZnxciuaAdatW4fly1dg/tbzgfCm7b333YeFC7cN3+cNv139EcZ4/AULvH7GT4DeHreHHh8Wb7cYQ0NDuPVWbqsVKpK2ok7Z1mghMU8I4yLviyzsqyoZp34d6oVjCCe8abcMIk5wJk75ejf0JUywg4LGX/R5HkP9qW/R75pA44qg9MXRmdlgrVDGGy2m8cxJunPBRjwSz7tSLEQ9XJjE5R+IG+VM9ma+Cy8jRnDAzXfcg9vufBB7PWEv7L3HPl2/vXbfC7NnDmDLzbeo/bbafEtsv3Bb7LLdjnjibntO+rfHTrth1x12rNHaYvPNsXjBQhy431Mafgdgvz33xXU33Ykbb7kTjH3nwy22A4arzWsG88eR4RH0tfxOQLmP0B8m0/87Jyt/oxx+FVS73Q4Thq5r8je/TueJl7blmsd09g35+J+4lJ/3A+rj1I+0c5rGGMyZeQRm4ijMn7k1turvx9alw1amwjatMWxp29jSVti8nA/bPh4Y2gbF8FpgcDXcvX+BvfYa9I2tQtUahpnRgZnRhpnRRjljDK3+UfT1DWNGawgzWkMYaI2g41YBe2wJZA+9CBOP/yff/1fWT+ylnw1brFYYa1cYGelgeLSN4dEOhkd4DGkjbQyPtjE04n/DI2MYGm5jaGQMwyNtjIy20W53YCtuA+23fnbOTw6jqf83afes8fp/N8n+/8W7mtC8+LbEubT6140Ow6AMbbuPi8tufhh/XLIWEL97/Zb74k2bPQkH9W+D+cUstGyFPlehZS22tVvjBTOfjdfPeDWe3f/36Cv8d4QJ+ZiF43/WBXXQ/l+/Ial+TBvEeg0TtNzuufu623cAoOeElHV+YjvbAhpxgjmVo401/lkHTFffY1ortDPqs7QPbQTIN4A7wIyWw267O8ybZzCyDrAd4M47RnHHrQb96A+rhB2efTgwPGQwOgKMjjjccXcb7RGHd5zcj9f9PfCUnSsU1qI9hjgBzK2fi05aAdwU/5O5/0eor677/3gfUocV61bg+vuvx7LBZbjxwRuxZM0SHLT9QXj9016PBXMWdPXfTVAWJY7d41i8eP8XY6uBrfDLv/4SD615CPevvB9X33V1bQVwjP8ii3+pT9WVdadAXWknniPYY9/Nd8OMcC+Gjm/7SXvNyFp89oZvYWV1N979vFl40YEzsNVs/6JpFXBmtBx2XVDglc+YiRccYDG07D9QLfvP+DJJYSq/FS0siqID29oOo/1P7Bn/PKd8GG/8j2wLaLEJgDQBbS1WrluFf7z00/iHr70dN973R8A6XHPnDfh/XzkHn7ryWxgdHQUqC1c5/6JJHNVMDaJsmSz5UeuCE76Qz4PRBxl3pMU0tkk1Xx6n/7cN8c/nQcqHPJg26fiXZ3tm0s//Ju7/eU1eqh/l3Njxr9eqC6TPI03Wq0J3/+91Lmr9f9Pzv/Qy+7j3/4KncjON+E3xT2Ca2kDtROAL+M6FASs/ITVB/49J9v+R9mTiP3v+v+2222LXXXaRevbP/bhzWG7f3XbbDYsXL47lMc3+f7z7/yfusw8u+OcP47jjjsPHLrgA998fPt00Sfj1r36FE154AgYHB/GaV7wSzvmFCUXhn3GlOnJh4tfXuV8EkNpJ2rXYWP3/30j8H/XMZ+KUl/pJ/29fcgk+/pnP4GOf+TS+fcnFcM7hlJeeiGOO9JOxBNIlLfJCj/jffbfd8MFzz8OnL/gYPn3Bx/Avn/wULr/qSnz44x+LNKjDKS89EccedVTX+P+YI4/CK04+JeKPF/+toOuLjn8BvvS1r2FgYACfvuDj4edl+NRHP4ZPfuQCfPqCj+MD556HzeZtFnUAgO9deilu/9MdOPLwI6Js1EmB9acrgCnTZOJ/zeAafPSTn8CRz/k7HPLMw/CyU1+NO+/6c60ev3nRhXjRySfikGcehhee+GJcefXPot3Hi/9Vq1fhwx+/AIc88zAc8szD8K9f/XJNF2MM7rr7brz7/Pfh4COegUOeeRg++smPx/IGiN/jLYwfzXU6HQyuHcTHPv1JHP3cZ+Ogw56GV73uNNxx558izaqq8Oe77sKb3nYODjniMBzzvOfg8iuuiDYwxuDbF1+EE046EYc+6wi88MSX4n+u+GnUoaoq/O4PN+Ggw5+Bgw5/Bg591hE49FlH4Ky3nRPL0470PcaS1hFxqLMC66VoiH/zwB//6JoqG1lnSSAhTyAFOPOQNaQqWMXvH2R0lA8HMsTR8sqHSjLfb6XczTs/T5M+qRMuZTm48rFw4U2t9G1WTggwLepV+EkATlZosKodPGvPV2UlrpPGjnnk5VyaAKrCvt/8pg2D0wYcyqiykKafXK47SbRx6Dh4Y6ty6Lm3ZyrrhIa3pZ8A0zeSfDlfhk0s8fWofD1u3Q8CQswn8Jo4ZXjjg1CENywB30mwg3dhMtHrFCWr2ZDpxOevJlO4SSNfEzpklSvpmMqRhjZwBPWzBMHnZVvhXJ66LvWOLJen+1s6Sa4EqSzjhjg53SLbFpYyVVXlG1n4GzTSUT7E5zmvi4yP1ouRNx3LnvGf4ptA/rodRNQnTA4YiT/I9g1aLzH+ZfCS4j8NbkzoWAztnse/vGKtZciLfMvgx62G+Fcdkiz1WNY85Rd1Dx26luEkutKnvPkLGtb6h8d8eYL6KX0C8Y3x335VWsT1DwGtl6Ehn5DL0yrL2gO6okjf2ClbJTrttm/PbVP8e3raX5EG8ZxN23cT/DdaSlSdCqaoy1kYv6MF403tEu02qfhPdtP4Z99ZhP5QB2qMC+IqjZw2oSndTSr+x+n/JW5JR/kQn+daXvmcfP0cPDQU9J5w8tf74+7zgP841uGg75YYq0JP53gkP3/BaiDPPTYHvv8c329Q9snFfz1eRkdHsfOuu3mGk3hoiJqNfRlrLb76ta/i+9//PpYseQiVTOrsvvvueNUrX4nbb78d3/r2twEAz3/+83HmGWfEG16XfVvWM+G/zEdgcP8D9+ODH/wQjjj8cOy7776YOWsmRoZH8MMf/RDLly/Hu975Tmy99dZYseIRfOif/xnz52+NY44+GptvvgVWrVqJX/36NzjyWc/CE/d9Iq79+bW48KKLcMILX4hddtkF9/zlHtxxx59w22234Zyz/eT2XXfdhY99/OPxmvVhDPDPH/4w7r33XpzwwhOwyy67YGRkGLfccgtODG9zv/7003HCC1+IY489ruYzrz/9dJxwwgtx7DHHeL2M8e2F8Tp7XBqD0F1HJi6WDZPo0W4BtA/JbApwUpTI/kTR4gRoxFBa3em9YofXhKZ0tU9G3kND/MeKIG05j1oyTY+ZfA3ZtXSe08jKkvXlcfz56sF1+Ojn/wPDw35LzamAcw6r16yt9RVTga23bFrBPj7M6O/DW1/3Iszfcp5YX+s+OETU3cfAfXfdhTmzZ8e2P+//1f+Kwt/Qsi3iGMo5h1e/6QysW7vOXwcbOOdXGOy+++546YknRUmcs9HdJTE+WPaX/nzBggWYP3++YkboKwrMy9LMZMb/HLPIWFvzCbw2BjBuBfrN3bDt1TCug75qJWasuwNm5YPASAE3sg2q9m7AaAE3UgEjDuvuXwk7MoytdtsB7SEA7RKuUwBVCVcVQFUA1gDWtxUz+/qxdu5MjL3sSLi+9JJwGv/X+y2vY+rL9Uj9c53y/n9h++1I2zk7dDoVhkcrrBr0E75+qBfy+XN+xbBD5YNIz+FgnEWrdJg9C5g3YNDfsjCyytjB4pGFVwDBxrH/N+HlRqknyuyCH+rExET9/3XLHE78aRtjriRpgGPmsSH03/kbmKIfht9ZdRbbbTYD/3nGkzF3hh8HFeHF0zFUaLsOqmBv5ywKGMwsZqAMK77Jv9f9P69ZB5A403rhxA1kd6O8/3/KuVeGlboWRuwO5492eBVWvMzvkqGw4OsfwLK3pwdVhEUfeiNa/bMBhMnjQEfp/vyLbwIa7v8pvwLriLp3j/9TvtIBgHf9vz3hCqADYOEuDk9/NjAwz8AZwBqHS7+/BkuWzkLR34+RjsM++zscc3SB0Q6AAhjtVLj4x2ux394z8ZG3zgAA/PymYdz+QIlZs/pw8c/X4p5Vs4G+ArYEbAHYFnDNyXfW2iTKQ39quv/Xeqzd/+cvNwR6T77o0HAB7LXlXjjt0NNw5b1X4hd/+QU+/PcfxvH7HI+Zfb23fm6CB1Y9gLN/eDZ+dvfP8PkXfh63/fU2fP6Gz2MUqe/6/cm/BRB2oeOqFaFhGsb/eT2pLtSTuABw39AyvO+PX8SSNSuAMnXIDl7fsihw4KL98E9POx2LB3bE7+/r4Pf3tXHP8goz+wwO2LEPT9yuhe23svjDvT/Etks/iu3dfXAWKIp072EAVJXB2jn/gDXzXgdnZsA1xD9l43WTTmNjY9hm24UJJ9CnpibosNMnTvArekO/6dtAhOuwhzUAWBvy077W/cs66Ovvh2kVGNlp8qv2rnjJJ7Droh0BsTHlV72WPbQUrVar1k5qGWRxR7+lzXjd1P8rv7wtUr9ge0XLq40xxfin/MRhW5rrp/QJxNdjjqt6NeUTcnk0/t004582ZDrxu2Xy+eP2/wV19DRVF+qf60SZiUsg/vrEP2nktAlN6bRJfKYkz95yG1EOPiOZqP9nOq+bdNKyit/EG86/1KL2UF7kv779fyXPNSmX9v+333EHvvZv38BPr7wSg4ODkf9EsHjRIvzDCS/Cqa96FWbPnu2fmZZ+5XjV6aBstdBpt4HwPMs/J5P4LwvAGf95D5mrUfsROLam7lxBzbSbb70Vp515Bn579TUx7ZBnHoHFixbhexddHHFN8Kmz3nYODjrgALzspSdGmyt9AvH1mONq3TXlE3hNnPH6/4v/49/xsc98BgbAW844Ey8/6aTIh6B2Ynq+Il5lQo/4v/OuP+P0N/ux2N577oXPXJAmg3mk/rlOk4l/FyZA33P++fjt9dfV8CYDc+fOxdvf8lYcG1bPE3KeiDbx8UIcrSc0xX/Q7+WvfQ22W7wYb3jt67Bo223x7Usuxjcu/Ba+d9El2GzeZli9ZjUu/M4lOP45z8PiRYvi95G/9Nl/wZP227/GJ4//d513LgDgHWefjcHBtTjznLfgBc97Pl720pNgjMGq1avwopNOxCtOPgXPf85zAADX33gjjn7WkT3j3zqHV7/+NGy3eDFe95pTsXjRIlz4nUvwbxd+G9+/+DuYM2cO1gyuwated5rndeJJPk7OeAO++NnPYf9998MXvvwlXHfDDXjzG8/Ak/bbD3+45WacduYZ+OJnPocn7+91+sOtt+CTn/0s3nLGGSDMHpiN3XbdFWaj9v+AWXL77S6vOAIRjbyFUIRGsyhSB8o0MkFgqpVEoflGjqYZE7ZLEeGoiAmOnjsV6ZqwLa6ViUalEfFkNt2ne9rUjToweItWCYRVnnSQylq0Wq2YRj294t5hiKu6QQcOgB9wiq2qqkLZ8jP6lTTiqn9uo6Z869JDR9oglg1leMPOfOpA+YrSTy5RNj3STkF6gPJkDVXUNUzaIK7wQFxlTJp6TqDM8CVredSTaawzSAPEI/G97n47X9oM4WUB+jXTk33rtiGfmmy5PwpPtVe0fbBTJ2xLQrosQ5q90nlkmgkPBnNIOjeXpS6qL+DfUFZ6lMXr4hsaykY9ip7x3z3Yoz34ILIo/IScL5M6VbUZ5WVaPhEc+VX1esknvLweKX4oq9fND+BoF43vqtOJ9W5D/Num+Cffxvivt0dsACgv+RnjJ0FVd+qvujGfgzbmR/qZH/m85Pukwfqp2Tdrt/yx7s8K5KnlSItyKp7KmZ8Tcn01j2WYxjojrh5zfNJlWcpMPOLm9GnHieKfQFpVlW4wWaYsCrRD/JdF2mKck8I2+G5TOjJ7NPFO6bRp8ne1Q1mWYaJY47/e/1MWIytdKBv1KMILCbm8xFE6nRBnlLsIaaqjC7g2xLoJk+aUjWVf+utZeGgYk578tRY4cL7D1480OPA/DUYrH4cOACaY/HXWYc8tDb7790BfqxVfvqCeBOccWqX/bj31NcY/ZKEfrFu7DtsuXoxZs9KDpVinvrrCv+DzMS2BTuCuWr0Kf7jpD5gzdy723HPP+L3flatW4vP/8nlceJH/XvAJJ7wQZ55xJrbZZpsuGrUJ4dBG5hPEN9x4A37/+5vittMDAwPYe++98ILjX4Ctt946yOmwYsUK/PSKK3D99TdgaGgdBgZm46ADD8Qxxxzt8WBw6aWX4pqf/xxDQ0M48IADcOKJJ+Lsc87pMQG8a7IF/KrjX/7yF7j2F7/E8uXLMTAwCwcddBCe//znY/bA7DAB/AIce+xxIj0nhuvpefyY2iQjgXVB32vOq4O3nvNBWKtPY8KLKsZjccI3r4um9HAirjFe/He3vTkOgfmaFjLACZhIg0YiD03jecBX/rlMATmk+SvGH+2s6bloefqV1/4Bv77xjob6mxiqqsJNt92KNWsn/3BG4VlPfUaeNCnY+wk74EXPeap/kSjGfxgnA/5/SAMMhtauxcNLlmBg1izfrvTo/1lfRVHA8v4q2J7jp1ee8QasWxcmgOVnw2cfFi7cBgsWLKjlxXYyjtW8HuTrnMOxzzwCzzv2uFim5gPW1nypJrNUcFMfy9zcjybX/1sUbgz9q/+MgQcuR/nIMriVBmbdCMrhCljbwegaixUrHOY8eRcMLNgS1ZABOiVcpwSqAq4yfgLYz2rBOYOBmbOwat/dMHrg3jUHZb30Hv+3fV00jJvdOON/B2DbsXPALaCttVg71MH1D8zG5wZfhl+3D0LlCoBveNuwqs+Gidxw7rc7TefOWvRjDMfMuQbv2Oli7DF/LfpLC4APpCxWLLwqym+tX4nSabdhwgqRXF6Om5zoRHuwDpnGMiuGLU67usL1y/19quEkMAxM1Ub/bT9D0RqQCeAweQ2L80/YA894wpbYYqAFlz3LIC/yXTvcRlEYDMzwKy8oF32pNv6X+3/bcP+f+n9Pu3n8Dxzwnsu7Jmj12g6vxvKXvz3QSrDN187H0n/8ZJ6MxR88Ha3+AZlQDke5vvqLb6m1DfRLF2KzmPT43x97jf//6YV7wBqgf47DAUcBu+1vUFmgXTn87sYh/P4GB1cMwJYFZsyxeOkpBv0z/UuKHefw69+vw7W/A/bfdyb+8bUGu+9ocOF/r8Wa0RnYeusZuPDKQdy9cgCuVfoJ4PD72Sv+PMn497rTFtSJuhJPbUOc/b99cKTV7/rx5AVPxmq7Grsu2BXnH3c+dtlql5g/WXBw+OYN38SHrvwQnr7o6fjN3b/B0mpp7eUvTgDzZdapj/+7+3+1Q1mWGLFj+Pyf/h2XP3QdHF/4MPDtmwkTNzBYNHs+XrzP3+PYnQ/DFjO3RL+ZBYsKo9VaLF33MH72l1+h/eDX8NrN/4xZRYWqMihbzr+HEprFtpuHlVu8F6MzD4UJzxlyX1O/pKyUl2ntdhsLFnIMG8l7HdkGO4cnfu4krBse9ja1iBPAzvlJXrjw3V+5ds4BbYuZyyq0Zs+EaRUYWzj5yf3LX/5J7Lp4p5qdm+pq6ZKH0N/fH/PYnrCM6p7ToY2a8kmfeGzTmEf8ZGf/TcL1jX88zu//+bxwOvFP25BPk2yeX52nyft/fiYtPDc30+j/eWRa4l0HpvcqS11UX2R9JvELuf83sf/3etWe/4UdxnK7IdxP0takp2kqJ9MpK+XVtFwf8sttqDGvfFme9CkX7VLr3yfo/20Y05Jvr/5fbVvjP9X4z/OLsHBinPjnmF8XcUQbMYZq8e/9kzICwB9uuQWvPeONuO6an0ceBx9xOADgjNe9Hq84+eRa/J95ztk48MlPwctP8i+Sqs69zgl5XWoeyzCNdUZcPeb4pMuyF37nO3DO4uSXvDSm0zZKX33D8l5NZFN+5Gmy+L/r7rvx+jefhX94wQtx2qtfA7OB4p/jAsKf774Lw8PDNbxUFjAGsNahLAuEO0XsuMOO2GzevK7nf5SFukDH/9OY/7vv/vux/XbbRZsVRYEDD3savvS5z+NJ++4XbU+bGWPwitediqOOeBZecfIpXfbm9YNLluCFJ74Y37voO1i8yH/W4oqfXYWPfPLjuOKHP4ZzDhd86pMwBnj7W86O5fN6Yh1rfN97//3YYfvtYa1fZNFqtXDw4c/wMu+3H/7nip/iX7/yFXz3Ir+KvCxLfPjjH8Pg4CDOf8974wsfW2y+eeR71jln48CnPAUvP+lkAMC/Xfht3HjT7/HZj31i4vjfoP1/4VcAa0VBDKOMWTBVrE/XRp14xOE5aTtXXzHlMroIDkbI5aESXq70cDm2wFLOcOY8C+AqzqTXJ7tqZeU7ifFRjElbgKocBTs50Z1AfjFAjAljTe8oscEkvzDRojYDg0541jqf0AlQT6qU7JRsx4d2lJ80yMOFLT1YRmWJNAKo/UlLgTziMTxYN5xwk0abNui003cvCg4YSt/AUBZKQDzWAekw3csarrVT6bEqlzyZxnp3WV1FOhEv2DCc57gcEFA2ToLkchPHcpJRrtVWTfxrK/24EkSA+lJP51zk4fWud6CU1YbBg09L/DVGx4//5F/kS9oIFjbGr8TyeKkOWIY0qUOR1UHUVVQmn6IoaiuNy/A2tde53tlJ4ZjnfLACQQZNpxwqL3Un1OM/PYh1nCjKbpgijYbteqmT+gPrR21eo1OL/9QRkBZpkAevWSbpI21IAJZXWgpM13yeN8a/vBjhNP7DACPJ4oF4qjdlpo7EQzaoVF1Ilzy1DKYQ/zyv46abB8qm/UFerzxOPf5TvaT4pw6pHqin64r/6fT/HsaP/1Rn5EvaBKWLKfT/L/n1LCwdSm2HnWDy1zmHPTYD/uPvgIO/W2C0Ex63TWLy1wHYawuDS49PW2CpngTVF1n8803k0dFR9PfPwMJFi0LbohO/odpidWoiUyTe8jIZnU67g7e97W34n8svBwC85CUvwbnvfW9A8NA00aiTwdqu1iC5Vw9QgZL8CLZVH0D0A9/WsEzE42Sp+HmSLePTU+ZuORKksUkT0PcA+DozmV4ujUETrp8UNYaTudmkcE6HNIIcrIfcVr584BVO1C6mCIPRBqjhZW0g841PYIF0HqBJnloZwaF2Pg1R1yYz57L4NH/M8VUs54BHHh3Ev1/669oWmlOBdqeDy6/9GZY/4r9lPRUwRYFXnPDSPHnScNihe2G/vXdMnmmS4rQdLbnswSUYGx3BwMxZQNZXsy1ifTDNh4/4UWi/XvnG0zEYJoCZ5pz31Kqq0nagoW6af14+X3eB7kteilNPqd+s1/xrGv1/WfidPzgugvhvTe8J+v/CdTD3ju+j/6Fb0Fo9BKzrAGsruHUdrFlpsWqshW2O2g2l6YcdK8IEsF8BjMr4VcDOABZoFS10yj6se97foT13Ttz5KR8rdPf//qFJLjdx7AT9/zYjb/ae4RzanQpLHxnF6x74R1w/ul+a7LXW73jTY7I34aQ0ThafuOAn+PgTv47ZM+BXAcPTWrndL2r2DkEfV7/SzpSZaZwgZZ3QDgStRwC46M/Aub/tYAz++5UG3NHfoO/OX6BVOZiizzcALk2ils5hn+0G8KQdNsexT5yP/Xfw29xRFmst7n90GD/47X249b6V2H3buTjn+ftEOQj0PfUhBDk1nbql/l/Hyx60/3/Ku/4rTdBCJmrDtR1ejYdf8Y5YlrDwq+fioXd8Jk/Gdu8/DeWMga5J3zS57HDVl94a7U2ZVX5Mevxf7y94jWCv9xy/B2wBoGXRv/kozIwxVAawxmBwbYHKzQJKP3mLvgrzthrBmOvAhUX1q4daGMNMtGYZbLHFKGYOdLB80MD0FWj1d7BiqMBoMQDbKuDC5G9VAle+2k8ATzb+ea66UEfWu5ZBNgEMB/SP9cNai3c991049amnYu6M8b/92wvuXH4nTvnmKXjwwQcxPHMYrky2RZgANsZ/Li3e701p/J+A+lJPF8b/VVXhhkdvw6fuuAQrRldKjwPEwUgYm5RFiYVz5mOHuYswb+Zs2I7DiqGVuGvNvZhtV+ETi/+CfWeuQ1n6bz8Xpe8fjPGrf0cHjsQj886GK7eo2VdlwyTG/+12G/MXbhP7y7qmAZzDr+//I1YOr4HvpIwfWxqDW+74I/71P7/hy6mdHIDCoDAF+vv7UQ70A2H3p8nCf739i9h50fbxmjKrvwHAQw8uwaxZs3rf/0ubiQnu/2kbjQOlo7bjkecIuwmZ9Yx/nisovxx3qv1/sZ73/2494t9N6f6/G7dslXFnM2P85BpX0OX1yuN4/X8Tf62XqcR/rrfaxBgTds8oALiwcMePFTRGG+//q9D/hxXPpK11RFDZMIn4V1spjgLxysK/AFmUfoKadUOde5Vlnuabhv6fdUhtmEbQ/p8ys3zMm2r8V36xGJAWvXBsXJSFH9shrDYP+UX2GUmeQ/r/+LK+tf6eIYv/P9x6C047w68ARpDz4CMOx4uOPx6XX3UVvvmlL2PxokUgnHXOOTjwgKfUVgCT76aOf2zQ+E+2a6LdFf9d4/8N//xPJ4GnG/+mId5yXsneXh70in8Z/9sJ4v/gI/xk6n77PBFoiP8TTnopXnbiSXjR8S/oshVxfnrVlfjCV76M7110SUy76567ccprXoVvf/Xr2GP3J+DI5/wdPvnhC7DvPvtEnXM7sSzz1K5Gdhc+5IjD8KXP/Qv23eeJ+Nin/MuZb3/r2VG27192GT7/5S/iqh//xLc/Wfyf9bZzcPABB8QXD759ycW4/nc34jMXfLzLZsjjf4P2/0ChlaEI6iy8Jg7BBmfVSiOelQ9wg4Euk7+cTCV+mX3EOZbpciLAGD8h2l19Xj4GQdNbk/48OSzLGOMHCkXYChTB8HRkxwcjNafwD+q4ckkdU+W21tZwaC9j/ANLykp85hGPk6xF2Puby749YnoLuW6nVOHtTifyJ7BuSJe20npQnXLZOKHFH4K9SFdlQKhv8i1b/hufKi/5mCJ819LI26/Bl/LJZrWlBwMX5uyM33816kUdaBO1b1mW6Ovri+nG+Bsv6wmhU1W+fuhzht8S5arr1KHQR1R3rcei8G/F5w9MW/yGqrxtwzzWN2Um3VSffnBJ/fmdZ+eATqfy33yufMPtv0HicVO5QKUh/ql3ZcPke4gFF95+Hz/+k8+pbUFfCXRh/BYm/qUMBNma4z+3dwSvDozEvwv1lfwm1T3lQNCb19qBFuGbsMzT+I+2yNpI4qrcGhPqs1qPzCOwrpnP6zz+WQ8YJ/478p0bAmUiXeZNPv5T50I9xo3/cLRZB4Y8/rPvWhFP5SWoLQnKl/ojk1n1Ro/4Vzoa06TFOCQO8+rx7+lrPeZ1z/T1i/+6L1WyJXCn04G1tmswnZfjOWXP65F1pfh2wvjP+v/MV5Tu5Pt/2ogrf92kJn+ddZjTF8q7qU3+wgEO3q4qn9qLulA/lduGvsu3/yXWrVuL9lgbbOfSQCbR9pBsjUDTmLB1sQIvNdn5b0tecMEFOPbYYwEAv/vd7yQ7+HL4IxgTJlE9UrKFEg9jFr1G9I0eOkQWGsMJ19OLhPRQk6NuEimjSY3Qo8+AZ+R9uIkHedfzjElT5hC1nXPhvGGi1hdkokBYIaA0NDfzOZ2s94kSl9GnfZ4eNf6awIS+nYMoPWdwaGnSzMcyPLqa7M5bIqL6sUqs1tjuMh/eLuJrCTedD64dwtW/vhUzZ5YYmNU3rd+8OTPx1Kc8CUc9/ekT/J7WdTzu8MO76E3ld/Ntf8HyR1b7FyRrzqtx6TA6MoqRoSHMnDETbR3/Z20uaHvpl7T/JwffVoYJQRnnORtWNIR6pb+ZMMGVXxNiXWZtInF4tNPo/ytrazujEOwU+/8KJaqB7WE7fcCoBUYs0LZojzmsW2fRt80s9G/hgP42ivDtXzOzDTNzzB9njcHMasPMaqO1OdB+wmJUcwbivSy6+n8v6/r0/zbcv6Uy1q9sge9f2+0Kfx7bAa6q4Crrj7RXx6dZplehviNOJTgVXFXhz2u3RadT+W//Ou0B8WoAAGz/SURBVP89YDg/nsjltrba4P3/P+xmsP/8cB/ANsQCgIOdvwtQjYW2pNZQoAJw8/3rcNGvH8RpX/8DjvnwL3HcR36OV33hejz/o9fgmPdfhRM/eS2+cc3d+O2fH8HgcIohlatr/C/jpXz8T//ib7z+30/Mynd/g13jtSmw4OsfwDZfOx/bfO19WPjVc7Hwq+fCOItFH3ojFn/wdCz+4Oux3QdOw3bvf62Xy6ZvCfvv/ur3hdMLpxt9/G/9d4DRKTC0oh9rlszG4EOzMbhsAGZ0AC1borBAWQFoF3hk6QysXj4bq1bMxuoVs4HOLPSjhB0tsHTZDNz91wGsGRzAytUzsfSRAXQ6s1Daov4d4Grq8U+ZVW9MMP6vgQFGW6MYGxnD2sG16IRdsaYDQ6ND6KzsYG2xFq7I+BBC39fudKK/qT+qfJo22fG/MQYHbLkX/mGHo1C6Vq2rd86mI4COrfDAmofwqwdvxE/u/jkuv/da3PjwrVgzOojDZ6/E3rPWhhV3FcqyAhC2kYeFa83F4MCL4MrNI+9e8a86sT6IE+u2K/oTGPhnTU/dfh88Z4+n4e/3fDqes+fT8Jy9noHn7vUMHLjtXmiNAX1jQF/bpF/HoK9ToK9owfS1gPDsaUqQ+Qt1UV9yDX0A8/MYIx7tUDTc/2OK/b+W4Uvh6x3/Uqf0O5WBZch3qv2/XY/7f7ue8W/W6/4/2EUmcDh5onq4cfp/t4nv//1zT4vKUo8wPgxbPutY3z6G9/+Kp2Di87/AO7ShxqRn7SoHy/B6sv0/y1Em6kJclZt2IA7tRVzNU9rEo8xF+PZvp53Ff3gxUheOuDBR6ZxDu9OOPGKZcfv/9Pw0xkz2eTrKetwxx+CJe+2Fz3/5S/X4h78PVnuQ76aMf+pFmZmm9t3o8b8e43+3ieOfsqvP8jrHt+sZ/zfd/AcAwPyttu6K/9VrVuObF12IeXPn4lmHHxFpkI7qvnTZMmwfPm9mgv/stsuuAIChoSE88OCDcSXuCSe9FIc+63C84nWn4s933xXLUC6N/7Ih/inz1lttDWMMHliyBAsXLow2MsZgl513wuDgYM0WlH3lqlW47Y7bsXCbbVKdAfjNddfh4CMOw1HPeTa+8JUvY83gmub436D9v4N58LbbHCfn+DCAgpkirKALRiHBquO/kWErX8kUlOcmGzB4WiEARaleoE7SCW+FmPAt3nbYkpUO7cIDRRqfMubU1bmcS4MVADCl34qWK3GZ55xDq9VX+x4uwbnwjcvM4JqvsvBct2FA2DbahkaRJqEuXr9ET2UzxiCth2Uj020HEwZBek0gX1OELT4kD9Qxa7wqvt3iUn3TtlEvKW+Mf6jIyVzqofksR/r5itToXzIQ4eSKykza5Kn1SP4sQ16a5sarK8HrdDpotfw3v5Sn2lhp00b5N+ai/RrqhlC3S93OKpsJMcAGTOlpLOb5ipeXY37i63GqqkJfXx9saORj/Vi/lQhl8VCXT/2pCYwMGorC25q2LUJ7wPjXbWFzv88bgKhDWKlC32Ce2pcrtJ28Ke0HM4keaYSLmt2Yn9dPvg0z8ZzUG5De7Iv0pW4ot9JA0MFI28H8+jENUKHxH/xV8xB11JuXFP9OBrO5X2p50uSRemg+y2k9MB/ZAIp1ltNlvvKkrTSNZchL08iP5yqb4k0t/r1eOT9k/WUuIyG3C/H0iK74r9s+3rytd/z76/Hin/qk+PfAtLxum4D8i1r/X4//v7uqH2tG4V8yySZ/XXj5xMrkr7XOf8f3uSUO/k9guE19AUxi8nfPLQwuO97XOfFUF7Ub0/L6YVqn3UZZtrDtovBN3sayQDZLmFaFZtsEe8xQh7qCN0Cn08HlP/0p9tpzT+y8884xnWOncGdcKxOBpBx8A+jShGeUO1xP+GQOeT4LBTAIctTlr5fNGSgu80JalKebptbNeECVa9fh29+guIF+zQxZIU8n4xfF0pIeksr1lcC9fEBxEPjreaSb5ffE88ihvuu2cy58iqGBTxMtIOmf8iU7g8TOxFXhPs1fq9z33PsQ3vWRr0zr27+PB+hrtfDOM07CAfs/wetE24SVu4QH770XrqowY8YM345m/qttsDFpq2djjJ/UlWsD4JTXvRZruQV0qK+mHxxg+TAtxLyt9eG8ufV5rznpJLzmZL+1Ffkh87tUNsgj/UxT/8/VCS68MGiEHo9Km2lFQ//f9+j9mPvrb6N/6RJgyMIOVxgcdFix3GKrYxdg813noVpn4Lj6t1PA2QJ+SWMBZw36Wi2MFS0MHXYC2nO36NLD9Bj/+7RUZ1Pp/7nSduHwGZ6Gcxgdq3D/0mEcd98Xsaqa4x/S3XkL8OBfczLjwtjW22Fsi4WAdThwzq34/sHnY+6AQ2n8ZLODw8rt/YpEx/6/36+E1FWwTf0/tWVaXrcKinvcD8Zw2+rCx31oP42zmHHHz1GafqAsAefTaA8fOP4FLz8ZxWueA3AW+2+/OT7/ukMwR74brOMr9Zs4/lcflnpB9LtuX6S9AODgd14WV/vmq3/HvXYO9e2dvb660teX43U4wuKKr7yj5lu5j3G8SH/N/S/XkXYiLdbnuX+/B1wJuCJ8n7cI59yuWa8L+FW8kl/Jts61XyuVIR7LViXwk9ff2WVz1bEp/hHqMcVjSmNdqa1qK4ADuI7DVu2tcMbRZ+BVh78Kmw9M7RvwN/z1BnzgPz+AXz38K7T72/nQBABw0ynXAaHP1PjP61JlZn3mdtCxeJ7vnEPlKnzjrh/ie/f+DGNoh3jyfZAPyrALS+W/6WzCu2oGwG59o/jqLndim742qsrEb/86G3iXc7Fm87di3axnw7r6pEYv0PrLx/9DQ0PYdrvFqU+jmD4Ak8gZUNerfvdLvOEL/nuBdQTfzqAoYFoFTNlQKRPAf73tX7Hz4h3y5C54eOky9PX5bexd7fmflzz24VO8/9eyuY/okWCtRatM2+BrHqYQ/7lfannS5JF6aD7LkX7uI3pNX87pMl95FoXfATLX20wh/nOdzIT3/97+tf6f323dZPf/U4v/iOdc7RkR83O+VVWh/zG+/8/tkfu9h7A7kfN1wElM6kQZc/syz/Xo/5VGuKjZkfkqi9q6JuNU4t/6Vb5NWz5rHSgPY/w9nF/BXZeRfI3xK4tTXt1OAPD7m/8QVwCT9iHPPAJf+uznsGD+fLzgpS/Bpz76UTztkEMBAGe97ZzaFtCk7TZx/LMeFY+2nV78ex/sHf/+vBb/G/n5n9sA8W8a7Mf8nG9VVejr8+N/jWnVR3mSluL67yKfhVecdApedqL3EQDhG7lvBABst3g7vPWMs/D0pz4VZpz4/9YlF+H6G9MKWhfq65BnHoYvffZfAACnnflGHHrwIfjHt5xd+/7wdy+8GFtsvkVj/Fvn4iffAL+N9+lvPguvOPkUnPLSE1EURdzO+RRZ6f6HW27GaWe8Eb+95lrwvsMYg1WrV+NNbzsHm2+2GT4dvgPtsvj/wy034xOf/Sz23nNPvOPsc4JVUt1QNtUTE8R/fiRYa1HElbhV5b+TG358CsPJX0jAFlzmHlb0UjgTHL+p8p3z3+FVISgo86kExDAe1w/0+O3EiBt0cWGZfiwbz5LMlFH5W+eAMDFdlHXD0lk5MWplFh/wE5ouGFFpsyx51ydfUyXFB3fGhMYkNVqxMjO6dJKi9Ns1szxp0paUyYQBEGVxYmPLrQb4UEWCluV5XoW3WtqdTvANT4PysM4pA8vbEEQw/u0JbQCJq7LR5swnVNaiE2TgKlZ2XFqe+tN3SaNs+W0YCOQF8UEvZ5h0Fx9RO6gN+VZFkwwsQ10cV7oGv2FezM8CmOWJp7Ln8kEaV9Pw9hDTi/D2SG4Hyku8aMMA5Kf4hdwIsDzzOlUVdfVg4uAjl135xXzjd9nzMtX15GAw4oZ0l8U/EMJJHjpTRtYzyxnpmGgDxoTq6esl+QPlssHHSd/LXY858q/Fv9DhYAL0i7D1lNKkji5rJ1UO/6DMb01HvFwW9TO+dRb17op/n8b474RvPpDnZOKfeq5P/KsMRYib8eK/ZpMgp9IjL4gPsnzuo5SfulCGqca/8mOe1qPqzfJMV9lz+fA4i//x+v9cduXHfILKRND47z3569sNm03+WuswpxXkDHHs1eIx1XU++QsH8CaPOJRL/YI/6s9ryswyZauFdevWYWR42NPS1Qa6mlMgTdaiNjGkE7/+OV3yPxif3mq18PfPfjZ22nmn1PYhtEdBt0hDjuEi2cX53RoIXu704B3O8/QnqVy4iHxSnuoZyse0ugyprPFaG38UhJhXKwcAEpMxK7uOkJk+oVGnQC/ssJHQw42YSh7rMfkYSxhfWRFinQZbJo26J/pdNskf61wnmUPdq7/SDwnqm+qfxvixbbiI+Ao2o5N8JJ0TTJxHNuoCflInDtdcjZXHo0WZZpP9GH/OYnhkGEOjQ3+zPwtpL436hfeCobVrMTo8jJkzZ8JlYx9th1jHNoxJYt8R/ELLujAW4rmuBvbXbFtTmmWZ+OOLNimNsrgN2P9z/G/Dy3nsy/Ly1F9tgqz/72y2LVw1gGrMwQ5XGBpyWL3Swc5rYe4eLbgyrPbl6t9ZPHZgZrXRN7uDYp7F8J5PRmdgbqMM1HlD9f+18bQLK4BdFeLBr961nfCbvwj2Cfuj2m0/VLs+EZ1d9kFn573R3nEvtHfcE2Pb74HR7Z6A0cW7Y2Tb3TCycFe0B+bBdaq4CtjZjqdvq7AK2L9xTv2KokAlD2ZV9+n2//RXwmeO6MNuc0N74ZzvPlCgvWhPWNv2+8xKuzg5cDhszwX49GsOwrxZacUH/Y4+qb7IcU4VYortnvoY9eeP+qtd4krd2irdcG3z67CCl3iW5RKOnwxmWgUEGkzHBhn/18fevcb/hQOM7f4VNqzW5TXPw5EreXueZyt+a9c21UHNzhPEP/E1HlnnpmH83wSmZfBo/6O44PILcNJnT8LF11+MdaPrcrQaWGdxx7I78J7/fA9O/dKp+MXyX/Sc/FXI479JPtadmeb4vzQlXrTDUXjGNk+Cc4CtQpvegf8FOpWxQNjxDs5hM9PG2dvehwWtUcBVKIoOTG3l7yys3uwsDA0cB4f6RCHlVvtr/KvsBI7/kenvkHaYy4F+zKMpCxQDfd2/WX0oZrZQ9JfTmvxVIK/8nKDxZZru/6Xf0N9E9/+0JelPFP99Ld8GsixxVT47ifh/PN7/O9kZrcnveR3xe8S/2oF8ivHu/wvp/+U5jvLDFPt/lT2XDxsg/p1zYbvnevuJx/H9f47b9fwPAODv01gnKidEH/od+ZG36qn1j2n0/8pX69hMOv4tylYLzo4T/2E+hvQ5p6G01M+m0v9zqFVI/JPuwm22wRtPex0u+NSnsGZwjafjkFZhPwbxrzSa/J7XxGf53EfVDmrDnvG/Ecb/KnsuHzZQ/BNP7YeNFP8/verKOJH68pNOruXvv+9+uO6aX+C3V1+Ls896E8790Pvx06uuBAB8/VvfxKHPOhwHHf50HPqsw/HNiy/0DBzipypzcC4973/JCS/Com23hTHGf3/XAdfdcAOstTj0WYfj4COegUOeeRgOOvzpsGExG+f//ueKK3D6m8/Cy086GS878aRoI+quPysvmthglzvv+jNe/frXYbvFi/G+d78n2tRk8f/k/Z+E1736NfjeZZd20d3Q/X+r1UIRHSSb6C3yN3kbFK06YRI4PMBkA5QbJ58speA2DBogDQvLRiVN/WGH8icPpsP7gtcnOBvppHNPvwqTviyn9EH+sp0s6TnnH7TxQUjEFRpFkbaoZuXGrT8K/wDPOhedi40bQkNZlmXcNkRp05ZxMjHIy8aQ5yyvuhXZWyiUEbIVM3XUxtWYsNIj6OBqD4QTLunb0Iib4FOkQRyVhTR4bsR5y7AlAO2sdUrZcv28fRIPBHtX4e0OLc9jflOv8vgHXF4e6qC28jj1svyprpSS326ACX5AGcKb9L4+/BPRKqTR/mVZxok95WUCLm2lOrAsZSdQB56rbTGV+JdOAMKHfLXuECYTyYO0e8W/CS859NqimnRUZ8WjPkUZvtHNc41/0Vnpoyn+S7/bAPNVBq3j3JYp/unjqR2h/fhwExL/9BWWg7R1tBnlbYr/sixjG+R6xH+0YWP8p5gkMF9tMF78lxsg/slP7UqZKAdpKi2lOV78qz68VtnWP/7TjQntofik2cSHscmyikM+xM11Yx2QF8+xieJfy/Ca8hOXOqIh/rX+CNTNOYfZpT9al0/+2q7JX05mrB4NvOOEHI+pHpsmfxlD5E18nlNWTCr+vQ79/f24/4EH0Gm3UZsVo72od1I/3oRxQjBOBhrjJwQdANrQhGsCVxTS/jCRoNJDZnMFnXQEQnFjgpBh4sp5TCgdw3/pOvGozaImJQ0nwmh9mRiL+KJgbi+lGW2KepkcKH+TPDFR5KtR84Vp0SRPIlazK3nB10lsqU1Kg0u2od/4XF/vLlsdTNmZ3qs+SYfnhn22+DbLNPl7U1kIn5wfwZcPOsikpL82XrPMbHVS3mg0DQBYW/mJ1JG/0d/oEDqVf5iABpu2220sW7IkTv6aKfT/qb78WLyQ/n+sHbaFs37il+Pg2sRvGO8wjfWVtgXUNP8ba7djW76h+3/d8YVlCcRVHqSp/b8tSgzvdRism41itIWxtSU6oyV2PHJzlAtbMJs5FJs7lFs4tLYAWpsDfVs49G3u0Le1QbGFw9pFe2Bsu73gSv8AjXzUDrkcmEb/z/E/ALTiwxtOAFtAtmmO9ThzNuwW81FtMR/V5luj2mxrdOZtjWrelujMDb/Zm8dfe2AeqsLv5uU6Munr0iSwn2zuruuqSpPA1Emvte4wxf7/CVsU+MbRBRbMsD7WnYNzQDV3ATpzNofrjALWxvZkMrD/jlvg/Jfshy1m+9VL9BkC6wQiD8fR6ovI2kMd45ke/f8z916YJmhlkjdO2FpO3Mq20LUJXT8RzHxOHMdrThQ7b8+nP3mPmm70/8mP/7vb8iYblGUZJ3vjpC+vq/rEb21CWCZ7y2ySN/462bXSqqYX/07GyDySDq+Lwt/P8Z6sEUpgeGAYv3nkN3jz196Mp7/76fjgjz6Iy26+DLcsuQWrR1Zj5dBK3HDfDbjouotw+tdOx/M++Dz867X/invdvaj6q2ycUQfGBu2/scf/m8+Yi9fsfjyOWngI+o0fK9kw4RvHwc75Zsc5mA7w7M0exQEz14QJX7/q3FqHyjpYzMOquWdi3czjANMfeamtx4t/rT9C1Fuj3nGVn8Rx1r7GdJ4befOs6xfRpw3kjQY9og5y/9T0/I99BctDxga0GWlN3P83xz/9e73jfyPe/8fnc6E8n/eAz5eCLzCvCLGrNKcT/5RNY05trzha1jkfL3zW5J+BphgmqAyMg5wPY5NlFYe8iJvrxjogL56jR/yXRRleKEt1ovpG3cLPPsb3/6SjOiuet4ffvRRhIpgT8giy0GZajteUh3FEXOWruEpD6fa6/3fTjX/5rjJpla0Q/9ahbLV8+TBZTCga4p88tQ6ccyjDrgDkoaB6Q+z0guc9D8YY/OCHP/Iym/RSjlmP+Cc/tStlyuVQWkpzk8d/gxx4HMd//h1qLU9c1Y2/6cT/9y67FB/5xMfw8X/+CE55yYk1e2rZoijw9EOfilecfAou/I7/tu/LTzoZv/nZz/Hbq6/Fb6++Fi8/8WQvswFWrV4NgjEGd99zDwBgwfwFmD1rAACw7xP9d4YRZNln772xdNkyAIiTzr+9+lpcd80vojytssT3Lv0BPvbpT+KCD/4zTnnpiUAWB0NDQ5GuMQZ/vfev8XvYfa0WbrrlZrzhzW/CKSeeiA+d9z7Mmzu3Zr88/ufOnQsA+PPdd9X8h7akzQzjf5r9v/P17E/obKpY7pQqBGRCqyj8B99daIxg/NtPJjiWbqFMBei0BBoCADpV5Vd86sOtwCc2jNKYR+cJA5AmfaLhjPETS5y0FqdVPfnkiTJRl7KVbgiVB8vxnHKqPAgrYQmsJPINFeJXUYpTEKzz8rPOiO9Cow2+9ZY5CXVnmnN+4JQ7A/ERt5Iu/KNEU8TvArA89VUb5Pbg5FvNBlIGnNgMgeBlCW8VBj1Y52rfqqrQDg+alCYHh9RXJ/gpF2k4mQRkPnkoLxNkYHmes5zqonTIS9/epaxgRx++N12UadVnskNogBmL7FRCmgtp9FN6ikPYul14E7+yfgv2sq/l8Rkzwd6Um7Kz3pJt6r6ugxSWzdNMLf4LGOPrzI4T/5W8LWa5Ui2Pfy0rdaK+pvpw4OTjPtSR1Jf+KA9CW8TrInyDg36Q+7ubKP5jzCX7qX1Zx9Sf9UAgv6Ix/j0/1qO+JMLryvpN4+kP1I00iJ/iP9lCcdQH1Aa5PTRG1AZKuzv+6/0R65z5bpz4r9kyG+BTLtJgGcrIcjwnHmVgeZ6rbsRXOsqDoOdVGOiTpsqBLKYQZGlKU94e6rIRj9dFUcSbEuqh9nbjxn/W/08i/gsZdJCOnUL8K79C4n/NmEzuujT56+KDqpTPVWpz+5J9OZFEHsA4k7/hRor8WRdqs9w+48c/0OprYebMfjz44AOowrd7Quvt5XEuXCdwkFW+MgEYGrKAFCYN6fd8okWdBKh318QueQUwnqlmpmslqec6yUujEqGGx0lpEjQUNsgVHsxF8Laxln0faXr6UVYlKUW7EgQnTpjWlMsfCgaciFJnRAp1ubpOxWe8HolnOBrRgzn0sSY7CpBW9OuA6PiyQKDDc8Z8ig0PLE/cXmk8Vxp6TGUMABNjtBc/yuPPk62N+BTTrLMYGhnGupGhv8nf0PBwXH3h9Ur10akqLH3gQfT39aEMDwCMttkN/T9x2N6wjq1Nb2Y757BkyUN4ZMUjWPHIo3jk0Ufx6KMrsXLlSjy68lE8unIlVq1ahVUrw2/1aqxavRqrV6/GmjWrsXr1GqxZswaDg4Ndv4eWLYt1q/2Q20D9vw124USz0iRf6k9atAPPR3Z9ElYe9TI8vOP+WLlgB/Q/Z1e4/XbE2MgCjJoFGOufj9H+LTHatxlGZ27hf3O2wPDcxVi189EY2vnpMDP8QwXVhXyUF+XLzyfT/+s233Fs6Db3Y0Nw4jd8x7dTwXU6/ju/nQquCudc1ct04mg6z8NEMsIEpHMd/z3AcocoF20MIN5zFuvZ/7uQp/2/sxV2nGdww0v68JwdgTn9JrRgBdrb7YexuVuhch3Adry8PRpDA4ut58zAcw9YiM+9+kBsNXdGlAMik/6Yjqbx/zT7/1OP3ktW/spEcG0CV87HWw0sK3919bDa4BXHPyPKrTanjBj3/r/u19SdOKqvtdZ/tqfXCmBZ/ds1IZxf53lhcjjSChPCcRXwJOOf/sVzvR8uwr1yU90757DVzK3QEwzgZjiMbTWGe829+Pj/fByv+syr8Mx3PhO7nbobdj9tdxz33uNw5lfOxH/c8h9YMXsFOnM7QFrw0QhbzdgqPj/j/T99jnowjbIqMK7y+qZNmsb/zjksmLU13rL3SThz71Ow92a7YGbRgjUOrnJAx8F0wm4kDthm5giO22wFBooQf9b6z4KZLTA0cAwe3eZTWDfwQphy1oTxz7ypjP9Vb2P8GFHruMk2zjn0l31omQkqYBowq5yBQp4pxrZN6gpZH8C2hHZhHVN/liEwJrXOeD5x/98U/35nh/WO/yC7nqsNGJvkr7Sn0v+zXpv6fy6OoB/Qv1QvlZ9yUEbaiefEowwsz3PVjfi+rH/GlXh4PyYuYTL9fy5zU5ryJqhsaNC3Kf45BnV/I/f/WlZ5qa/5erB+W+sibJ0sMcpj/tN8lZ38WRese5WR53n/H/000MN04r+qwrP4LP7DxG/EKfyWzoj6pWeuqMX/5Pt/nrN8ru+8uXPx3ne8E5/74r/igQcfhEFalZnbQGlPJf7Jr/q/538xTXkTVDY06Kvxz5dqqYfbiPF/86234PNf/iI+/6nPYL99nhjlxDjxr8P6okf8P+2Qp+L2P92Bh5YujTLf89e/YPGixVi07bbYbdddMXfuXNxy661RdmMM/nj7bdh1l12ifqonjzfe9Ht8/stfxBc+9Vk8ef/9u+L/WYcfjsuvvLJmnz/ffTcOPfgQAMDKVStx9jvfgbe/5a044fnHTyr++b1ifseYoDHBeuK5tjdm0v1/BfPQn/7k1Il5roy457k6CYHXsbxzsJWffFOjKI6Wyfl2QmBY2f6VCpRlGR9iUflOpwM00GMZ4iEMEvStlNz41vpJR83nhKQJDmpkWw/yyvVXerGSNXgDz7SlSmrIqAtpUn5dRZ3zJE3Iw3+XdR5Kz4XJ+458TNoPXMLbCPLmEunwqHajbGzAWb4Mq1U5wUk7sD7orKRrosN6fWifSvZlZzkbGjF2kNRXJ//9te+Eiedt5W8U+KabZ1XXR9MAwIXvRZMXY4EyMT3aVtJ48xZ5yJbpOf8ko08DgKqTOnEEnbQcBzTMjz6kZTK9oB1C5etIB0b8voQxBmX4bka700FfLf6b7UfarCNNI46plUkykTb9h9eRR1WhLFvxGyW0cW1bmAniv4smG9RQvitfGthC/BFALEv99FzpNTXyPNctlVh3xAH1DFu+kH6v+Of5xPHvy5fZx+RpO3ZQrVb6RpEeVQfapyn+VXeesz56x78HpTXZ+C/y+A+D8Hr81+NBrzVdz8mDx6nEf6KX9OzFn/lMQ3bzoUee01+Z7m1Yx0386v5C/DzWlCZ1mEr/7yaI/7xMzrdX/Ks/GWNw5H+XWDPq4OKWddafxxVs/sGVblF68DYGFz6nD0+8yJejbMDEk7+HLDT41rP9W6ksp/rl57TDRPHf5veAt11Ujwuu7tRJTZ9Ry8/Pc7yeIG0B0D1pGPuanI4JabUjT9QWYUxCo+bnBKWlkNGt0Qh5Tkkp/UCA9k6FpgNS1nh/KAojk7k+38TF1cFxaAMWJF6marpOfKLGZBLZ13Wo1Xu4JuS4TaC+qv4L1NuaHC/KFfCayjPPp6GuX7BVzQ1YvTUeip94JDAYHhnGX+5fGh60+XogkG9dtroM0Hl29beQSLcyLE8GWlaTMxvl9lFwoZ/YYdE2mD0wq4ZvqwoP3f8AqqrCwMyZsTz7SdKkXMzP+39y9TipPfvmJRfjov/4d7/yM+DQd6Mf6SHQ6zrntTGYv9VW+PQHPoAdtt++1vZpP+PWo/9v8b4ivFTonN8SGtPp/8PPGANnUlsL70XppYmwvZiDQ2EKdCqLVtg6k7+J+/96u980fs5lRDb5yGNf9VeUbgUMHNqVxfCoxbVrD8CY9f0zEComOKZx/iVKOMCEY5xUqio/rnVhFR2ALcrVePrWt6Gv5fV1zmCsWAQzsHd3/294P1WPMe3/XUjL9avZY7z+3wCjVYEbHu7gR/caXHpXB+usf8m8HFqJvkcfRGtwBVC1YYrwYMs5uKLA7JbB/ztkMZ7z5EXYY9u5MNIWdMnQMP7XFywoW3P/n+qI6aSn/f+Pr/8L3n/RL0I92HG+88trftc3z0/f+WUsKvzja56HY5++by1N5ULD+J92SOP/yd//n3/k7nD8zi+/AWz8dfzeb36efRO413eAqwJw4VvAFb8zHM6/95Y7Yn2MF/98JqPyE3J9cpwLbvgELvrTdyL+pCCvEgbXJOGVT3wZ3vKUsxrjn2B6jv9TPo+qF6QutV3mZ72stbBwWD6yEreuugu/evgP+M2ymzFSjcJZB+MMUDocv8UjeP/iv2DAWFQwsH07YXjWkRie8QyMtnYDynnxxW03QfyTr2mKf9G1LEuMjo5im0Xbxrbbyy702PyFNOXrnMPDj67AT357NdaN6KodhpGLlZXopGRvt+bKnL/ZVjjukCMwb45fvYOsjYDI9PDSZZgxY8a49//qk3ovRbxcL57n/T9B6aEW/+mZjJlm/G+s+//O39L9f22bYVtbMKM8evHPZcS07/9TPo8qBxri3y8a8OWUJvUe7/6fz7qUNutI03L91B7Kd6L4Zzkn9dFEj2WcsyjDDh2cHIULOzCGOQae5zzJg7R79f9sizSddlCZczk7nQ7KqcZ/w8S4nsdtx2X1r5GFO64r/j3Un//5z0ZBfOWmm2/GaWeegeuu+XmkdfARh+PLn/sX7LvPPlGnd513LtauWwfnHA4+4EC87ES/ynM68Z+P/x8/8b++4/9u/sxnGqYR/7rYTMuoHMjinzsLMU9pjh//dfpKm3Wkac45vPv89wEAXvyiF4H3jAYGswcGsOsuu+APt96CP9x8M17wvOdh7py5uPnWW3D2u97hv7n7khPHjf+z3nY2tlu0CK8/9bVYu3YdzjznLXj9a16Lo591JIqiwDcvvhBX/uxn+OC578PiRYvw0U9+ArfdcTv+7UtfifTy+LfO4T3nnwcH4MUn/D9YW8WXvGbNmoUn7LY7Vq9ZjReddCLeeNrr8MLnH4+bbv4DXnfmGfjuRZdg24ULcdl//QjfuvhinPuud8X7ShOeTT1x773x0NKleNf7zsVb3ngG9t93P/zh1ltw9jvfgRc9/3ic/trTop5aP7Sp2pfn2j4pqN0g8W+W3HGH4001ghOxUVKHQmgkmO8amCgkgUp0Om0YcapOw4ecUXPoFDwKuqKThqGMbBQ0WNkgtPghZwkWpcFzvVFgWk0W2bZXjeno9MFBIYFUFOl7yuRB2RKNVHkuC0LnwupFqUCVsQqNqzFpIKaQ62g4YAt2YrBqPUR9M+fi0YWA1nzKVpT+4UzuiDU7S2dXoxs6KuWp9ai60bZVmLBmmtdBGyZpnAWPjRqiPpnNY2eY5CA/BW3sWC73XNpF/bOGH2zkXwTgRGfdDvomIRtC5ttssE09lLbyUpvynPWj+rCePIFg04ibfKAJKHchjbSR+G/F+E92yP0+hzK80Qfxa8rIuimKAmiI/7wzBfwkLvVGZm+fVK8fHezSFsTTOiBt6qv0VO5cT60Dw4lp68INat1nCORrgr9qHsROes6t+yh3URSyvWK97VV+PFIPzSe9Wj2EfEwy/pmvPLUeFY+21XhUe6qtNJ153fFfxzVyM4wpxn8O/oZwMvFfj2Wlp7GY52sZvjiV652/OEGb8lx9j/ooT4h8ed02AeUuesR/3v+Tdi63AnEB4Bt3GnzpjgIjbe9Prtfkr0urhA/Z1uCi5/Rj72+nuAUmnvx1zuFle5c472m+Xc5l9Havxz91oa2IpzY3Ib5HR0fhAGy33Xbo75/RNbE3Hrj4UDs+xeoGknKAPO3ySfQxw/xwbAIVKeKwUACDQD+TX2VIPXHKr4GUj/J002S7mBB7QK5TmAhrnOSu2aGe0eiXTmcyu2VkOm/Ca08Uuwzu68YYjiGEnvBlbMWXBKSd8DzQ5T8RN6rm6VEnLV+jJdCE2wuIA5jQZ5tgJn+ttGgWT8/jNZGOJMXsxGP5Oj1420uf1kTDY9XNHROz6mGaJrMweUui2EHloR/VqETc4aEhLHtwCVplib6+vtq4Q+0PuYk34/T/vLdz7J/loRnHQHm/BPhJQeUXaef9v4yNtJ9jPjZC/1885v2/l0X7y1xGQt0u3XWpMtf6cqGnffH4/f/6jP9T/24a7v/Jqyj4WRX13jpQbjNB/8/7UNKuyW0Q7QwAY9Zg5YjDJX+2+N49FR5c69BxQOEsTHsErbG1KKsxbF528MqD5uOFe83B3BkFBmb2N4//s7Ex5SDoPTfLEqdu2zQOZ1qv/v/OBx/B1//7Zlx7619lgpcTuX6S119bH4MZDid9udWzwtOe9AS88gWHY9cdFsS0XEf6IeVnfRZd8Z/Kx7oMR9qK5x86es804ctJYL3mxK3k5xPDTRPArgjpDRPAtgR+8M67J4x/9Iz/du0lV+qpdVxVFdaNrcMnb/osrvzrVVjdWRNpbAzYasZWeO6uz8aZT3kDSpPGmtjI8V/JdyU1/ttVByPVGB4efhS3rLwT1y67EX9cdQ+Gh0fx9d3/jIM23wp25h4YmXEwhmc8A66YB2f64fvw1H6PF//qdyo7X1JRKIsCI6Oj2GbbhUBDfbO85lFH4nU6HaxZswajo6M1fOZPFpR3URSYNWsW5s2bV4s14im4MAHcavltVpWv1gHtoPWmRwLr3ozT/08U/2WRtlvNZVJ+aiviMJ/lSD+3g17Tl3O6MV94Fj36f/OY9/8eYrxIv55Dbhfi6RHiw3l8Y6PHf6ovjX/lCZEvr9tujVOdFtOMf9JWIC7EppQxt2/S0X/rulN1YID4UoqnYePnG1yDj6nNMJ5Prc/9v0sv32kdKI/aUdos4votoNO4XsE5FyfAyTuP/6L2/M/UXlBk2k233IzTzjgD1//82qjHIc88Al/8zGfxpP32i/QeWroULzv1VMAArzj5FLzspScCqLdBrDPKqjKTNtNSPdbrhrbdtPHvfVZB4yWXkeA2cvxX4R7QyU6eud7KS21aTuv5X/KnXkC5C4n/N739HPzmut/mqDj0oIPxmY99An/68534wQ8vw+VXXYnBwUEsXrQYL3ze8/GyE0+KtFQf6gEAg2sH8U/vOw+/vf46zJ07F688+WU45aUnwsnz/y985Uv47qU/wODgII458iicfupp2H677SI9tTfC+P/NvWQ++BB8+oKPAQDuvOvPeMd73o0HlyzB4kWLcfZZb8KhBx8MYwwu/M4l+Ny/fiEvDgD47dX+ZYpvXXwxfvCjy/DgkiXYbtFiHP/c5+HlJ/nvDGu96ZFAfzHT7P/Ng3fc4WjUnLBeq+MqAR8YKRB5XvLNwrAqtao6YcuobsemG6X0MAhUGUQvYwwq6+AfpjD4bJw4s/JBewaEy5wmyZfeiCYvlmU+t9RlGjsviF2aBqzG+DekwWAR+l5OG+WHTOYyOInnv4Xa3ZBRJwBdb5zFsmprlpXgrNu4O+hRq5dkI6Z5W/sBUF6eMiifJG9qeKxz4WFcvTHM6ZCn5+tt1el04urqGAAG8aGfczLp3aC38vFveKT68Gmp00bN3v5aG3UrbykR1xh+I7ted2obJx1xLpfqxXwtTzzWg+YhdBbRz22FVqsvTiYTr8nmNb/I458DjUnFfz0NapfYsXn+qo/J4x8ejW/xqx2oRz4ILoQG9aQNo3yifyG8cx48Oo1/qT+tWwLpoUE3lZPpKhfxnXVRZ5ZTiLJL56i4ytfnp/LqbwjyWnlzkJDLrmmqA68JlEH5qLw2+LzKqTrkdIhDPoz/Io//rAz9j3lNcYZs8KNppIEJ4t/1in9jwH6PoLZxGyT+WY91P+mO/7RSSG3Ea4L6BfL4n1L/3zv+yYeg6aYp/gMwj+eUJY9/pUE9acO8nkhLaSoP5RvjX+xCGgoqe65bLmen3cHw8DAWbrsIc+fOlQm7IFvjbTZ653uXGx9ynPw6QG1Cmmwc8XnSu3xjOtOa8nLIcWJZ4ycTIUsxczsEJt7+TFPmCiFNk52kK0SWksc2jMLGLJbtVoKTsmEAFI6pTOQRJnXzVYqsF+JoHhB8kOI4PxbydkqQ+7+mEXrlMV1p0NeJ5tVK/q9QZ5NsyTJddq/lwWtLsxlvU5oSmVkhk68qX6qXaMBg967kyCfp6/MycwGSB5FDgfolGg5r16zB8qXL0N/Xh74+/6Y5Qt+sfOs0/MNxrQPiOud3JIm4Ur4oitoDJVPrv9ODKa07Y7zHMc1aCyPyaXtOGbRfi/qsR//Pcd1j2//7vmzy/T/LJv1I103Q/3em1P/X/bPe/9sJ+v/0sJL3zQTKabT/h4MJkwe9+n83Qf+vk8yazh2dVIYIm6j/p2yazrL1/j/RUFDZa7oFefK6VrmIr7LptdKF1I/Hrdct6edl1d98uXr8EnLZNU11yMtTBuWj8trwMJFy8iUSl9ku14V8Jop//1yB8Z8ejhdFKc+Iks/7+/+w3WRgz7oouuJ/nPF/+KSHyqtlkdnGMf7LAlW2q5fqRZtpeeLl9UheE8d/9/OvnB56xf9GGv+z/nMZAGBsbAwLF20b9dN8nmue2jzSF7vn+IS8rKZpXhPeRPDw0mXo6/PfITcbJf4TLukoLsHHgf8GJMtpfRCUhtIiPvnl5SnD+PFf7/+bfDHXhXwmin+Wof8xT+VRPpQnTyMN9Ir/sDDJTar/96C2cRP0/xs3/vnsOtHK6WGC+C83cPxDfFFlIDCP55Ql7/+5YI35nPC1tkKrbPltrwH/0rz4HGkqD+Wb9/+QMZSCyp7rFut8qvGfxSfzWT8RN6xqds7v5KK4hJq/1eza3cbcfOutcQUw0/IJYJb//mWX4cOf+DjOeP3peNlLTwx8ks8ob8rdpC+B6cQhn8cm/n06r6um/v8xiP8q+JKTPMT49+fWVnEnT6XRZHPKQaCcSR5/XWyE/h/iiyoDgXk8px55/CsN6kkb5vVEWkqze/yfYlT1VRsqmBBXaNAtlxOTjf+MD68pR46rfPOyRVF0TwCzoMkqIC/MNCOOqcat4hJ9Tkx2C14UnPzTwKjvcW/CtzuLEHDE0RtH8tMAcs7BhknhqvKThLmRbLhBZZo6OfWAdCJMz+loPst7+dNWirpSGRJgnABWZ6vZOpQnXQIxEr/kqEzToLPBln5Ftmyby8Yx2Ic6Eoinequu/i/xVp9RXUiXPGN+4ONcqkfiKp2cdgxCqStr/Rbf1L0ovJ/k9cqjbmsQ6xuAc/oB9uYGnI0NgTagrXz9O7RkoA+xA48Qn8jr2IQ3lXizoPnkRRloVx6VJ/FpW1+2299S3iTjP+TrW0S0Y4r/FCu1spLnnJ/kRJChli4x5wv6kKDtME78O24bKB2o6koaHFQVYTDHvBg7WfzXHrZm+ZSZ/Hlzlde1llFZWJZgQieSv/lHUH7M53lTp1sURdyRwUn8F+ENNz5cJRCPdUA6qiPxMI34J7jQgU81/okb4z/Ipv6gchPHjhv/qXNW/lovefwjsxVtk3gkHOWJDRr/XiaNA6XFh2Asq3R4zmuVk/RzIJ7amXacavwTSI/plIM2Ig5thwniX/1EZVEaTMv9pFf8N9HJbafykwZ55DSN8dv5V1WF4eER9Pf3Yev5CzB79mysDyj/CMbESdOuFaQGALLll8a3uY4PCFxII3RVbY6gEMZEuUwBaDcPTXRSmse1APWgbKDMxM3p+GvnwgrgKL/OGia8XmAM7VdLDTqmpXHEi3J7DH9GXaM96jy9Gl5Oj1qn41MCDU5MyosD+UsBzhs/WoV9nfpyjs+0VC/dQBr5MeXlJQDEyVh/nsA0TN52+3HNRSNfLQPh4e2Wu12iIfVAE9d092khOaIhoXbRRpae2ziXae3gIFY8vBy208GsWbNCOyF+3WADBDoep15XRvp/L6NPK4oCnXa9/7ex/9fxf3oo5rL+XyejnfOTyjrOoRzJ9v7cbsD+X8d1bKu1Td34/b9/2ViB+lJPV+v/Ey0+DPN2Hr//b0+p/5/K+D/VSzr39e+C4yqNXFcgtD3hfp12ph2rsPWu9pW1ss6/jKI6IMjDnbSoL2kDITzFdthI/T9fxsaE/X/iSb7Kn/bL61rLqCwsS2B5paWg/BKup834V7xCVmS4rvH/NO7/xZ6YcvynMZ0L92p82SGnk9PO24o8/rkLGV/qptzEsdai1deKnzyy1q+koiwer95Oab2MO/6vJor/xBP0Cb7UFG3i5Z3a+H/q8Y/a7hh1H1Yaua5MMxt4/I8Jxv/5BLAvUo87Qm4LzddzTcvL5vk5n6bzXI6cxrKHlsYVwPzRF/KylIl0c1B+Oe5k4r8Mq9qKxyT+6/YuN2D8b/z+P8S/VAn1pZ5uKvHfUMdmE8S/MZx0r9erykn6ORCvKPyLhOS7PvEf6fWIf+LQdhi3/7fp+b/MK+Q0nPPfsc/9ZHL9f1qVq7ZT+UkDDf1//uIkyxJYPtGqb7ui/HJcxr/e4xc9+v+yFv/dq2pVb9VV7YBajDb4mc0+2yj+6aY4/s9xN138J/7UjUB97eMg/usvcHo/64Tnf3zRTunwnNcqJ+nXoe5TtDPt+PiI/+mP/6mHq8W/P2+ik9uO/DfE8380+AZB+eW4k+r/zz7jjPPUuESGOETOWIkRTxWiMmXt491JQdDYcp3yssYlvM3KfDq3llFnUDw+XWHj3wlbT5C+4qrsKS/c3EqQIbz1QfzmijFwzm9ZTbsgc7CImd1sMj/aIDxQzPM1KPJtP5W2MeFbRuEtNZZTmYxJq3epv/qE0lYblC3//QjqRdlyHRXYcBrjp/ys9d/UQtCNvCkX+UFkJW3WS/TDsA0LfYjAOiBdZH5HSGkm3vwV2WCK/kC9rUurv2m/oggrouFd0N+QNzd22nip7XI8Xmu9oMFfiE9cplnxMW+LMj58bKJJPLW35hv53nSRPQRpjv9u2fQ6PuwUffMyxpi4lXasqXHi3wQfK6Tha45/bwtj/GCunpdsyGMt/msdbQInHTE7AdJSfMqfx7fawDH+w0oDlqEN1fY5bdIh717x72lWccU7t41UOqQFxn8YdJE2Zct1VND4R4z/+lYsxSTjn3nqS0xT/lOP/3ReNMS/2pEyI4//zJd5VH3MBo//hj42ypYGA7SF4imoDfnL80mDeOsf/+nc69Ij/kN9aJnx4l+ve8d/r/5/EvHfw9ddw404aSk+eZZlicIU6O/vQ7vdxtJlS7Fm9RoUhUH/jBnddQQX+6jaZF+DPTVdcY0fXMW21E8mdsePjsEI1KM+0eg8cjx2g6eT8mmnBGHWzGQrcYE6zdppF6IgSB2ZZIdcHw+aFs4N6vpElGwmMCaL/Aj8HPlmyLQry9Rsl3jKlG1N15poQp66cSIYAc9IXXediz1or9xPc4h85Gga2mB/oO55mZSW8rxJ6solXGkaBZf5/uh/KlfSC1oTxIv2qBNv9q0gl6mf1jC6Jq9pm6SHtRVWr1yFB+67DytXrMCM/v44+WtMGou4Ccf/4/f/0P5f+hrArxwmHvsvxmSsMaGtbaD2/9jE/b8J+ExHkDP3PTzu+v9639Wr/+c9hdJAj76aNsl1p3xoHP839f+hToQOfwrO+ZdSTFgFbXr0/8V0+//MrjE9vGw62ft/LVdMof9X/dWGPNb7f39vl4ObRv/Pcol2Nv6fZvxTFjfh+H+K9//rPf53cVcaTDH+ic90BDmZlvj7dtYYf++ouDkYpBeAxrv/VztSZkw6/pM+Zpz4z/FyXQnEb9Kd8qFn/Ps2vokm8fjL80mDeOqDjMeNMf53zmFgEi9G5nQpVy+/Ip6mMy0H6j8RkB75s8y6tWtrdfG/N/67+3++NNSrnlRH5jXVn/KnfUg3zydoGs+L/1/Hf8JTUDr85fmkQTz1QbsR45/1oWX0WvFSufD8v91u7P/LsOsDdx3RPLUhj/n9P5/vKbiN1f+HZ/3W+h0jkMc/P2sk9efH/2l1ZF73xKP/UvacDmXCtOM/rdJkvp3m+J/4TIf4Dc8JtA/p5vkETeN5dx3W7UiZ8TiIf+vCq+XGP/cuZe7KWotW2fJ30xsk/ut2Vx+0j7v4n9r4P8/jCzJMz+NfdSC44Mcb9Pm/5NPPkMd/Rpt0yDv3z/Ktb3zjeaoIlVRhKQQLKSNlTByWLYoirjrygZMCCUK3qVKdCzeZQp84XOWpstEYSgPimKoX6TCNQPmTvOkVfvLgkXqw00C0madFnkXR/b3kaAP4BoBgQ2NIXBMa+ISf6CLWQd3+SsuYtMLWV3x3QAL+noe6qzxRDrF/1Nv4p17qJ2oXppNOTYeiqH37iXl5IKjNlTdEZoh9iixI+Dah8iCYHn7NY87PhAaWfqZyIQtCdsy8LstWfKsqrYhPMqiM1LnGV2TRAM7xmYYmmwuulyXJrnJQNq3XJjulCW6VHbFjIC82lkpPebow2UhZcnn0F+PMFCj028494p9l9I0nr38e/3U/bZKXPCivTw/2DFt+MZ/8iVvnlfwMoZMk5PGv9epPwjPnLG54rjxy/1W/QSYPr40p0k1CFl+0pfJE5idKX22hdmSelmPeVOKfOMhkYbrJ3njNy5oefs1jzo/45KFyIY//LB45UNZySlNlVB7EUVm0HnN8ruBBg80VV2XWPB4xmfjPzpUGyxaTjH+VKZdHf2pD5ZnbjDRYhngsSzpMIyjPXF7y4JHpSo/5aPAX5cWyaIr/vj60yhYGBgbQ7rSxbOlS3HfvX7Fu3TpUnQ6qqsLIyIj/NigfwHdNP6FrBSivm3AJBsb7kL/QDA8unRvjGyPVxc+6hQI1NlIQppZPOhGP9GguXmb+jBqKT+/Kz9qXZshl46EhXeUznPxlG0ddTEThpKLvK4Nf1AwT0k09J5QKF5wgDpnZRK5HEbkFLwnC9DBxRs4N7VBTGhrsz3M91u1dbxNSWeJ7tSAvfhH8tZcymDTgu9r1+DT8MenF9HQeLaE2oxGNr9+gitR9vYxPSrImPuITAKqqg8E1azA6OoLVq1bhgfvuxT1/vgsjw8Po7+vDFltsgaIo6v1/WQK0XxCxyaY81zZG+wyj/UZTeyR2msz43yF93kLbyTQu2vj9v0H31qXa1pqN2v+n/kH7UvKhHLyu9/+Ph/F/7/5fX6plWpOd6Ee57EYemhTr1f/bOJ7hz9q0pbTyzG1GGixDPEyi/4fUocpLHjwynduo+vMN0P+PN/5v8BmmqY6Y9vh/cvHPNGR+UrfLZOM/lbFTiH/iIJMlpjfFvwO7YZgefg3wmY4vSyA+eahcmFL8d/tIkjH5l/JV3bUec5mYhgabKy5lqWyFvJ+mbFqvTXbKz5UGyxZTjH96pNLSn7V+l5y58+bWZMh1JQ2lo+nUMc9jvtLOeeRlNC2nxXxkvHQC+LGOf44sSHPTx3/SI18I49Yj/k1T/AuYHn7NY86P+OShcsEBNjzbNusV/3UexNlY8c+jMSbKT9m0fprslJ8Tz6xH/BOUlv7Uhsoztxlp+DJVbFcRnk2SDneQQvivK3lzecmDR6YXXG3Zo24pF9OZR5h6/Ke65Q5WagulxXJmnPiPUIv/FLeo2XIq8Z/GucmOSS8txzL2bzX+N1j/v2Hi39E2UX7FTXHEo8pB2bR+muzkz5PcSoNli8dF/He3a6TDNILyLMI9DG3ot49vjv/x6naDPv9vsA3TVEdMpf9/8I47nBZQBvlRiZVhJp0VrKAV4s/LOBHsZPWkOkUSPvCTCSbSIY7NGj06mvIE/ECe1zZbHRXpCm2m8abO0QGCeiY4RhX2/3ZSIT5fGrWwGjVq1fDh8VwP2hMAXOislB+B9lN+OdAunYrfqKg7T5I5rUDO7aBBWcsvDKrKb5nkpHFWXSgDr4vQUfI8yZg6iiZ+yJzehhsFBgvr3Tm/WtrjhjKRmgfy1uCw1sYtFnidByWkrgmUhecE2kevGXxe7+AXWT2oXbSs+rbK78JbITktpUO+POrqA4LaQeuv6Uiwoe6NMag6VdcbcGws/Xm9I8jt4Vz69pMOPMiPR+qGsArWb53SbSPiIhsQcJvnnC7gB37kaaRRz/U2Ev9BKq9T+MaC2orngG8+TEP857hG4h8yUKrFv4NfzRka81zGiNbgO4qvq0W9z/uOR+1A/0Ye/7HM1OKfNs19g/hN/NAQ/8Ttiv8e/kpQOZhvJxn/mEr8Z9fchq7mjyIr05ivZfM6VDvmdeIYGxs7/qfc/48f/2oHliFNHqmn5rOc2oj5yOI/ryuVmbSZpjZWPJP1/0wjP7VVrpOZVPwXqDqdWKYo/fcVx0bHMDQ0hKGhIVRVBWsrjI214Qz8YEj6mwjWb7Fpqw5MWSY8PQJAYeCqCkXZ8qtFrU2fnahsHPsURenzfecatvzyaS5sowhT316I+rGOrPXfXNdxGX0ASFvxI+jeZNdanLZaXr/CT5RRtnjMIfB21sZ8F3Yg4fjQWRtfJMM04p830r4r83XsLD+/sbHjf7z+X+yZGETZN3z8pxt56kBa1ln/Etcmin/7GMY/SxdhcrfVaqEsSwwMzMLArIFoR5ZLtL0Ni8K3CWph1muNn+Qjszs/WeHxw/bvKnPj+F9s1tD/axlr698BJu3Es+63Wk/0AWSxNpn+v+8x6/+9nrlPIfNdXrO+kt7Jt9RWzAfSfSnrkDqqHbvqZNz4T3ZWUDsY43fNyu2Y62RD26uTbArOdbfxTf2/vgQcZYsPOH150qZutIuZQvyTp9LrqiPRUW2seKZn/Ot5XTbFm7j/n8T4v0f81yH5gfqO4lM2k43llZ76fp6vZbzvTHf8n+K8iR/Gif/xxv/1/r8eY5SXdPr6+2GDjaNvB1CZ1M4qi6ar/XivyvpSvWuyUrayCBvv+8KUd2PEP88YZ1qHSo/HqqowNjYGa63/tFpYTOCcw8yZM2ttpsqgOhBf7aE8KBfTvHz1+B8bG8M22y5srAtNYzqkrKblkPNkmRxfZR0PcjyVkd8AJn3img0W/3W753ZW2bh7W+5L6BGPzNcy6jtKW3mp3+a+4UK73sQP04z/8WyivmKn1f9n8Z8971M82od1yTSVlWnM17J5Haod8zrhOemQL4/kpUBZq/hN9LqPNNmTNjI9+n801PFk459lSJNH6qb5LKc2Yj66+n8fQ/m4IuKLT6iNFc/06P85AFBb5TqZHv2/jpnNhPHvn3/SflouB+d8f1J1KpShj1V8ymaCH7dqvuRpqO/nvkYfcD3jv87L27S+BTTPKUsTPzzu4j/5JfOUV86b9mFdMk1lZRrztaz6tsrvesS/lUnHuEupTXbOZ0XUDlp/TUcCbWRq8V/XOa/jxz7+63Wl+pA202hjvSfgs37yIqjsaqt4LnhN8V/DnTD+PdB+Wi6H3C7E0yMAmAduv73uEZOoAE2jschEIWdoTO5+qbIQHvpBgk4FJZ8gQTSWKmekYbLWP+SLwSLfd1HautWWh/pbcJW1MOGtiUg3lE9voNeDk/ngc0DiS2NSFKVfsp/px3L523AE5zipnJzfZR2/piPIThmbypiwPJ7lWZ+kRVtFWxdhu4HM+VxolPJBgXMORVmiHb49pnnskIlHGrm94rX4HtOjL5QFag1RPEv1nfOg3rQ9ZcvpA2nFAXGpv5YpW+nlgdwG+bVPS75DPWhDtWXOT9OVPuWup3l5WadaXvHzcsRlmtqEN7e0nX4XN1CpyZzrH7FIMzbY9caa+RpbcP5hY1X5ulO7aJzy2oXvS9X40R+sq3mKaXgrJ6cLeP46iepCJ6uyE4z6bwCNQV6TF7KBiNrVOT/RYcJ5HsvEUbuov6a8dDNWFCU6nXZ8aG/ZwWR+pTRJS/V048R/2TP+u2NivPgnvmuK/2wApaAyK4+pxD/T1J55Pn2k2zZJduISx22w+K/HoNI3xqCQl6rWO/7Fz+gvOS3lnduDoGVYfxpDzNfYYt5E/T+vXagXZPWqOilMJv5VNp6rjLmupEHQuPXXSWYgvWSDzEa1c5s+7cBz4vSM/4YyRVGg0+7IllL1wbTqp9c894jJ/6uq/lIQ0zdE/Nf7f+/zhnHzOIj/FuM/bNXFvqVmK9GVdDZM/NfjWdNM2OoMefyLjfNyxGWa2oRpveO/LnOuP0HLbMj4rx5H8W8mFf95/1+hLMPNovUTrMjsRZ7Ohe/w9uj/ubLBOf8inPIuigJlz/F/wBH9SBN5/PuCNZ8luA0Y/8R3Ln2j2Dwm/X/d75hPH8ltk65Te8A0J/Hfqar4LdQNHf+0j5ZP+OneXGVX+sQ1RdrViraLfhg1TDbXowJpEHj/5h/WJp0h8aG0x4t/jVs3Tvx33/9PJ/69DJSR+QqkQdAY5LX6N/khs1F+nseyT0/1Qb6Ut6lM0TP+6z6kNFle9XTTHv/XfWyy8c900xD/9Vr1zyxc+LyNc/4+3Ri/Laja3pjw3CYQUHnJU+2Z53fFf6DTZCu1ZVH6F/o7VSd+t3Jjxr/fHS3vs+vliAsADy5Zgt/9/ndYu3ZdnCBwDthi882x//77Y9uFC7toKe9cf4KWKUK70hRjrKN2u42ttt4KLZlAVdpO+0ShP1oBv1vaxlk/WY17VqWXLKcDe23dwqeP2xz7LmhhRln35dwGBOaNjY1h5SOPYsaMGXAbLf7rsTpe/JfhJbPHMv6pUZRpA8R/Diqz8ph+/y/xyBdmm+I/QNM105z0/9VGHP9r/Gv/HyKlqxxxmUbamkbbacwROG5UGXLQMup/6BH/BOqgPmka+/8Kzrr4Uo/q4HUKvER0xh0m2f/r+FjzFUiDEO011fgXGuTJutGYLcoi3IMWcLIKuqlMUfiXTJP9p3H/L/7vfUv64hj/Y7GeCHl54ub24jXx3WMW//X2NM9/PMQ/vSWleT34fMSYtI0x9VRQWZW+2oRptF30Z48R8VQullNQ/sn/GmJs2vE//vi/SX+N//QcIW15jkw2nquM0X6BDmUhaAzyelLxn50rHY1ZtYv6a16mPPvMM8/LC6kBCEVoKGhopvG6yVFVoLL0E54sS9DtcaPRZKZdl0QT8pvvnK8LN3a8BtL3YU1Ykk+aLlS4f5CY9FFaOY+i8MvD/Xl6qKZ6W+tX0qjxaQ+/ckb1SXicXCU/DS7S4YMhLc88XkOcV2UkzYiXBRmDijQILOfElpqHzDkJTsqqv/hfvZNgvgaKBoW+nU6bEJJMznfqPd5sVZ9U0DczSLuy/oGzkzdIUh2mNzBi/Uh9E0/5q02pP9O1Tqgjj0xX/upXKkfOw4m/2NAYsi6Uruoxqfh3yQZ+MrYp/hNtxpzKhxB7NX/01Yxi3PgP+mZbxKkt+CNNHYxq/MP5NsiHgtclp5Xz8HZKE6hRpvDQv5DG3Nq0BbX6jgLxcj1i+a74LwHdMlTK8RriIyojafrJE5YDELY11PjXmkrlkv01Dw0xRVA9yJM/Au2jfJDFP/mapvgXmYij5ZlPW+SyNsW/xhhl0jpUmuSZ2zzxT3aC1AV/uW31yHTlr7IlOfygVnk4iWe+gcm6ULqqx6Tifxr9v+pDaI7/ifr/eozkfF1D/Gt+Lf5j/9+bVp4e/SOPf9Gb3/7gkeXQM/677efTe8U/4ujSmLTjCK/RK/5lCyATPrHhXNoey8d/qmMCZeG52s+Y8NCUq4pDv6/5Gy/+HYDmlcdanmXVJxU2ZPyjMf7r+mqa6qw6qh485nQVlzIpDyf9RRXeau2K/+zG4P/iv7sONJ124nlOv8j6f2P8mJ434CxDULycJ7/Zq/Lk9WPCuIU6mXHjv36TakL9I8jVNP53Yfyk5ayrv90M8oulElA/9ZfIOwBtSVwCdSCdWIePef/vfUbxKbsZN/5THekv6tzge8RX/iqbykE8lnG1/r/3+N+G8bziK/BFIRNWCWOc+Of9q9p6UvHvXzmECbsDVFUHrZaf6FFQvfWntuCP/DSfspDq+sd/vUzREP8Jd4rxP17/L+WZx2v0iv8sjrWct3l3/BNXy7EMr9EQUwTVgzz5CxjRPsoH48Q/bUJQmYjjy0u/xJfkwstqcZYXQKuvT/pBrmxKD0kpk9Yh87R+cptrvSZ9k+1N4X9VZWUHs/qR+Mpf/UrlyHm4LP7r/X+SSfXI/QsA/uenP8WjK1ei3R5Du93G2FgbnU4bg2vX4pFHHsUTdt896kSZKCtpqj4Exr8DwHaFZZv6f+f86u4ZM2Z02UbPWYbXjwxbvO2KNbj54XbEnS6sGLJ4aG2FZ+04A3P667GMzE/zOlw7uDbaWvH/t8Y/S9AmygcbJP43Vv8v8R9eqKXslA+Tif+GOiEt1YPHnK7i5vXG9In6fzeJ+C+mMf43RVpEMFH8Q3Q048Q/8yMP9SWxRdplpQAManMGXO3qwflvo5rQFjfQynnQTjw3Db7J+tF6Ut/J9cn9lOesqyiPTS+Ga3mW4zXCSmFj/FhV8dTekV8t/lMdK4/cRzUPDTFFUD3Ikz9CtOXfYvyvT//fUCekpXrwmNNV3GhfpHkX57x/I8wHOZe+U6x0VY/1j/+6DUhT9SFsvPifePxPmNz4v4CRHUdJX+1I3GKTPP+vl2cerzHJ/r9gIpn0Uo4EmYdQscRTGkaMbMPgbqzdTtdS3itYotXXVxOQdDuyJaIqSj5KizKY8ICgEKflCj0XtrNx4QbQy5AcRn9phW83TxcmjnL+np6FKesz+kqDFaBliMdJW9qBeHSqovCrG7Q85MPUhE5VxYfClDHnRRrkkzshyxDPlEV8243ptCnLqj1yR2e92vCxdOJXssRd0618ID5te53koS7qUwiNH8szuEk31r34LmWgHDHPB0hMo3wI9o7l+Se6az7ETkrfT1bX7Uxc8slB5TYSZ6SvPBBped2Kwn/jNa9fM9X4Dw/6c1lYNsmV7NUeN/799oiUhTjFpOLf5/FaZeHPmPT9Zid148vZODHW9CPfOs+w1YZ0JM6Ft8xFp+jLU4h/lqEdiEd6PML4Feksl8c/r5v0UDwvT9r+jLy1DPFoS02nTaOuYg/6D4H1aqcR/9Rd5aEupKvA8usT/7QF09Ar/jN/IT3mA34Qrvl6jo0e/zault8g8Z/pQVlYVuWiHhsv/iX+xol/0nNZ/Nvwoo8NMZ3/nGccr/W8DC+1uUCHeeyr2Je7ScV/9w2D4rEeedTyWO/4z/v/1FcRlzLwmkfalGVZzrm0DSiB9WqnEf+9+39vD/IlsPz04t/fKBl5aYP0aauJ4r/D/DBYJx7z9RybMP5bmyT+fTvjHqP45wQ8f8SjfBr/KlPTj3xznq6p/xe/pd1pOy1Hm2gZtXGyQ+qPSI9HLY8pxX+SiTR4P6G8tQzxaEtNp01ZVu1B/yHQznYa8W+tDavkkjwc/5CuAstPL/5TXSs/TCH+NR+TjH9qUG6U+B9v/O/jJKfDHSF4z0c753pQlqLwL0arXNQjj38ndVQw/gsvi422K6cV/zzyRzzqVlWV769FBtLMf+Sb83SbJP4fq/5/U8d/qmNNt3n8N/b/E8V/K/hUiP9OFv9h8qbqdBr6/w0Q/yGGiMd85/xLd7yXZox53PRQNIco9xTj3z8P6hX/k+v//QpqyD23/8cJA5ZVuahHHv+UkfXaN8n+v9VqYeWjj2JkZCSmK1BW0tI63NDAF9xzoA14JAwPDWH16tXJng149H/agXisRx61PNYj/u1jEP+VtbXFFZPu/6cV/387/T9B6zgHldtMIf7H6/+LScY/7ZzrQVlYVuWq7GSe/2/Y8b8/luFXxPtZysd7M8C3aZwY0x0i+CPfnKd7LPr/yu9yaasNF/8qj/LWMsSjbTWdNmVZtQf9h8B6tV39///Fv9YJfacJVG4zyfivQvyXRRHGQ/X6NRsx/qnHRP3/ho//8cf/uQykmf/IN71QMrX45/yRlqNNtIzaWO1AvEhvA/f/5dlnnnmeIigiDaZ5vUDza4yEFhXz1954fgsGA1slx2jia6XSmW74wEf4go4Z0mp6cJVfjX4qn9OPEGb+mW5M2gJLcUnXGBPf5mSalzPQbAhAY4y/WRDbsWzJbRXDW+d0AJZTWrHhqOmZGjLiF4Xf+ln5JDkTeDy/eiSf4GIZyssf+UdbSP3zXGUuQqDSadWOCHXPtKif2rswYZWri509Ow7yID/KQdpO3qjIZTRhBVeOH2nIqiumEdg4kF5ugyRTvQEmryI8TCnDUf2Nkw3EZX4R6q4K33RI8qTGKm8okhzJj5mW19N40ETTy5fZLKMddZKOoYkvcY3xb7cZE745WRTQVRXEJSgvI/4W6Yu/R/oN+qo8Pi/dCRNX65BHprFuiJ/TI25T2RT/Pj/GvydQ003bhiY7kr4fHJvaw79cTohfs2Nyk4x/1YN09VzlKiaIfy3TGP9hwKF8N1T8a4dMfKWR0yV0x38awGo6sroiXV6rrfRIvFwGhFjiwDfJ04JzfiCo6bkcmpbX03jQRFPly21G2qQ/pfgP6SbGf+JLXEKTHvm14ip9BcXP+fBa65DHmDZu/Hvb5P7Bsj3jP6v/PK9JT+IXMjjWukj2THVBuizbM/4LE/clUD1c6MdM6KvYp6mcRVGgU/mtowvmm+630+vxn3hwi3/ym37812N8w8V/vQ3UsrQB0/WaR/LmkXi5DBg3/nv0/+IzMa0hbsaDOs26Lqp7Tpv0//8e/7mcOT3iNpWdTPybcN0U/8yLvEP8kh5X0+ZyAuKzDfHPFXOUlys+Ih+xheqW25+yTKX/d2GilHibtv/3sdVEl7A+8a/3bmorPZJ/LgN6xn/v8b+2xTBpNyVOjsW8YPcm0HzVkedqd9WL9K31D2Dh/EszXXz/L/5jflP881p3U2vSk/jFhP2/B+XJsj37f7GN6kG6eq5yUZaq6tTuR0hLy9T7/4S3XvEfVlTVZSzjy2U5vtLI6RIa4z+8wOJc2pI6PZMifr1O1FZ6JP9cBjTEv5sg/lme6UxT3ltuuSXWrh0E4NDf3x9/W221FQ4+6CDMnTO3i6bKl9ss1meg7ydhkh65TE78sygKPLLiEVjrtzDWum4CYwxaBbDbli385oE2Vo4kH5oO7L5lCx86cjPssFmJlkwCq115bYzB8PAwBteswYrlKzAwaxZasqqJOGaDxX93/89rHpMdy9rkH9MVlCfLrk/867M84rFOp9L/UzbirVf8T7n/n2b8Z/Wb24Dpeq220iPxchnQEP8qT1P8+xhM9ibNvJ7Gg5ymykhaurseaZO+nWT8q4wm2En5EpfQpEftOpQ3YlelRdDyOR9eax3yqPVIYL7SI25TWR//HRRl6pO0rNJqin8jMhK/yPp/3QVKgTgbJv5710fxNxP/dRo5XcJjGf98/l+Y9FIpV737MVZ3rPJc0/J6Gg+aaHIso7rntEn/MYt/kTunD6T7HT9PmfgSX3G1DnnkPWoup5ZVXbQs6W28/r+AefCOOxwZmvCGhBYssrcRtOIoEMtUYcm2/75IcnzSJmgDwodFHAiTLgMPjZO/9eBguaqq4ge9uWJE+RnZ/hAAXJh8Yz5y5+FJEJ2TxfxmLvUqwjUryn8jycuVGhAJZNJVZw8r+tTetClxuPrXhQauCm+sqG2jXUJj6zhZJvmxbsQhqEuUMTS2ZcuvckKwI/VVeuTJfOIjG5QoD31IyCPBygCGvqRAfgDgEOwSGjYX3jorwgBXeWh50uSRemg+ddF6YD6QvlnlbVWvC5WZtI3xDXIZ3spJcqQyZXgQTlDZ1Va5Tmacj4wXwRcM7RnKqD6kOan4D2/KFRL/pcQ/O3IvQ70DRVf8B52yxinFf32QAeKFFf2INPzkFuNfY5rnuo0hwZi0zSIA6LZgOZB/URT+m7k94r8Q344xk9UXQW2tujOvHv8+z2n8q13y2MjsxjTa2Q/6k6wp3ePZMJBg2mTjX/XUOlAeTUeCxj99SSHXkXYirVjfmY9p+WizCeJf6StPZPHDOsvpMl9XXmk9Kp4JtmW7zjTyU1vlOpkY/31AVvepnH8zjKDyE29S8T9B/1+P/0SbwPphXq4febKM0snxlMZE8W+y+HeM/x79fw7kX0zQ/6tcud8jxCkhXxmu9qZNSY95bhL9P8/Vbkxrsnkuo98Zwcch06gL6ZOeymZCf0jQOlAeTUcC+ZpJxj/7HtJifWo9qEzKj0evh7d7bg8/vliP+LcO2GTx393/e1yPo7S5JbHidTqd2va66o8ulOF4nJP6ndD/d6oKfa2+xzz+q0nGP2kprto0B/Iv1iP+6548if6f3+aaIP5JlzR47pzfyYbgXD1Goy274t+PaTX+OQlM+gGxJrcJaQStg5odGo6EycS/+m6xweI/6a6ykr7aFeGTGbweN/5r/luvx8g/lNkY438tp/FfFHyROX0OoOr4VSakrf4I+El+0i6y/r8zyf6f92fMy/Ur5BteyHShnchfaTD+7TjxX22U+PcrlScT/zkQF+LLtfifVv/fbTfNb7J5LqPj/f9U+/9MT60D5dF05MiIfM048a/1RTuRVrr/V/+QcZ/YhCtveU8b88PLsUo/9xG9njD+w+eBAP/cwPuo50Pg5LeuiFZ7qq00nXlN8c8XxVmuHv/+wbfSVH/zOF7WTtXB2OhYog3/Caay9BOwfX2+359s/HMc0aSf+lLkp3UW4mp4ZATtdhtVpwMX6r2v1fK2dRYFd9UJ58YYWPEDADDwacRNS0e6gb1sUfhvNRvjX3jkdVmUqGy4//dPF2GdRX9fP/r6+jBr1qyaHUiL+qvuzJte/Nf7/zxfba7PKjTdbYT4z30xPxLWN/5tY/wnmZQfj9RD81lO64H5oG7h2dqE8S88tR4Vz2zU8b8/r8c/48PBhOfvveJfy5B2McX7f2rK+mFerh95mnHin3hKo6r1/1Vs33hueo7/K5RF6aNfPmOUA/kXWf9fTmH8n4Pea6nu6BX/YfViq68PVVgdSbkijbDrRHxO27DIrcvmNRl9ufWL/2SrVLbuw/mR8PiO/0RLZXg8xH+700GfxD/718L4vrYwpja2UPlJc/zx/3Ti38umem6a+G8e/6supKW4atN6tNbrbyr3//m9tQJxIb5MGWlT4jDPbcD+3zx4xx2OguYGVsMgLCumIYmnxuXNlTJW5koXgG+gQ3YUKO+wMkcIlMIxKUTj8FiWZdqGj0aOxfyJvo2WaKdAjBPPYeI4DphFd4JWfmXTalnnUp4x6QaafEgjfAWly3nK8HaK5Q2E2Dyno7ZDYeDCt25oP3UsJw06f8yPNAC4bBtEniswPR4lrQofM1c83jCzjDo6fclaWqTbH0knPYyg3NQrdRqqS6Qb3uJhGsHJ2xYm8z0eaTMYv6qGuKwr/eYQdYp+KfXKY6vlGyylQVkiL+FPXSBvGSlQX6+nt00r3BSRBidClXZ+rfYmVJ3m+OeDYNsz/pP9SRfSAYVCEYd4SS6iiK7h1IWOrYgxmuK/yuI/99yYF2wF+JbBhPhXPeq2CH7eI/653RjLxzyhC7EfZcG48Z9ilbIkmU30O040K39fB/X499dVfEtLZWFZT7vuezxXUH45bnP8pw7UjRP/BOKp3pSZOhIPGqO5LjH+Uyep+rgs/nM6Oe0c18d/qqd6/Oc+7Y8am6RBWZr4Uxfy12vIt+iopwuDBU8rYDXoll+rvQkT9f+2Z/x7ULrI4l/riHi5XHVdPRAv2bl3/NfKafz36P9Vj9wWqi/y+A8ys7z6SfTfSMPzJX/1b/UH0lRZ1Gaaz/IqP2mQR05T9fFl6/GHqcS/jDs2VfzTnph2/HfXVZ1O3WaYcvwXgMQ5jxs2/uu2om08j1R3RTa2qV3LjUaUO8Bk4p+Ti1pHBJUNGzH+q0nEP8syT/NJT/XIbcE0wmTjXx/4KA2mqX/bqkLZagHOxclXlSWWETup7cifE8DW2li/vGYZfTmOZXXcFoRM5wFMQ/wbsdvGin+9qVZ7Ytrx7+XLY1rp1Gn7VQdTiX+vf6KhExa83njxX6fFayc+pflqb0KnquKDVKXDOpvs/T/xlHasI5l4y+Vyrnt6hnhqZ9ZFU/xrec1TO5Ke6pHbgmnhatLxr7IoDaYlP0k+hSn3/3X+tB95UQ8to7KwLIHllZYC0zWf51OP/+4H9cRTvSkzdSQeqGfNl5NedqL4b7VQdTrxW+nMV9o8n2z8c8Iz2iTg2Mqi1dcX78P8Czd8gJu2yVT+Wi8TxT+fX/WO/2SDPF/tTZhM/48J4t9ugv6fddEU/3lZ5mk+6akeuS1UX0yh/1dZcpthg8V/ikeekwZ5JJppZSbzWZbA8kpLQfnluIx/N+n4n1z/r7qqHbDJ+n+J//DsqVf853ITx27S8X9T/KfrquGZKeUmbIj4xyaK/1Z8/m9rL1nXy0pe5m+sL5VD5VV9zXrEP58hMi33k8b4r8IknXw+gM8cubMEj86lCeDc7kqzPv6v21rtz3MFpmu+kxeOk097fsXfdPwnHXPcx1P8V7X493MMvA/0vOrxHnmFl0HV3oTpxX89ZkgXGzn+WTduPfv/NGfjdVcc6oEJ4r81TvyrzTDZ+N+A/X959hlnnKcFVKlohEC8CAFKYHp+49cKW5yQMUEVIx0jgcLtTJ1LN3q50f3ROxxl5mw4A7BoeIu6KAtUnfBARWjxnLLR4CBvA/gbPK8T5coNHnUyfnLQ65EcOuqRObMJjbZWNtPVmYA0eC4kCLW+HB068vfXeRnA3wiX2TYhEHlggKryE9lGHIx6uNBYkgfLumA3Gxqg3J6sp9w/lC6CfLxmGq9p83RM35zjzV6TLQHESXzWC2kU4uuqj+Iyz+MnX/N0uxszHosibXnZC5/1Q33Jk8Bz4lIOAu3NNOKXZZpsZxplUZrknfyJjRXS5GIZ4j+wpU9Y61d+kP904p+TyKoDop3q8lIXPmz28e/fwCHtKo9/vqEU/EJlI1/TFP8B8s7WWv+QgROutRiT+KOsXLFCvlpPtEmTz9LGLJPHMr8HwvyiCC9BhM6rkAcQqjMAlK0e8U/aNr29RDloE9cj/rGB4p+Q+wPL5ccU/x63yZYQPtSTNIopx39qV5UuesS/njfhFxsk/m1cfEX8evz7PJZTmuRtp9H/swxln0785/oTlB/p0TbEb+r/e8V/9IvMtpQt91dCU/yrDHlcUg/iqL7MN2HC3qxP/Df0/zzndV6GUPbq/40B5KUSyqd6uPHiP3yniDgErQPaRvMgvkmgHnptYn3xWvv/6cR/iuvcNxNu/UZO7ap0ITrwyDLsUxFWASo+64c6pHrwwHPiJpoe7IT9v/hMhqMrcWy+QnCK8W/DC2fUQYFpuY03ZPxXk4x/lY10zCaOf16bXvFflrDhxtGME//es3rHP7d8NsaPTTh+Gz/+07iP8qkejrHdEP9lkDviBNA6oG00D2IXAvXQa2P8vZD5m+3/Q7wHfOvCiuaNGv+JXixn/AvF5Ef9CWoTGIMifFOP0BT/bkP0/zJNq/yMSSuA+SO/yfT/nb+1+J92/+958zovQ5g4/pOOPKcebrz+fxrjf79rWrAbwmOXceI/P44f/2G3Lsddu8SHwoNyrnrhw3WEsZni0o65XdEj/vWen2kmrDRLix9MnIigPnxQXrOP+ECxQeK/fk3e6k/koXWvejKdZci/Kf6djDPUbqYp/kUv5Ud61IX4k43/v7n+f9rxn/iThpYhlGUrTgoQKA82cfwrXQXqoddmyvG/Eft/+cY3gTLwyDKKl+OzfqgDeRJ4TlyliWnFf8Kpjf83Uvwz34T5ArXxxoj/TtVBem7o5a46nez5f6LHlxtzfyWMF//W+Rc0qQPEFsRRfZnPazPp+LewlfBxIf6DWI6x6GT1bxz/d/f1Zc/+38s6/fj39UAcQlHICyF/s/GfdFZc9RXKwCNpK16OzzqlDuRJ4DlxlSZCXVnX/VnCVsP9P8vF6zCpTf194oaK/6QD03Ibb4z431D9PyXh/B9BY4M2og4QW/D5uerLfF6bScd/N59YX+IbPOd1XoZQlqWfAFZFiKgVogpYeYMipvcwJqTSNb8o0vdnmaZvbDI9N2iiXR9IMI/5zvlv7infqqrit4ViuvBU/YrCT9hZ6ydArWwPlE/k1eQLPP3bOPWGxjk/IUM6al+6Va6r6kN+Crlt6zqkG4omuioLwRhTe9NBG+oia3A8rveFpjSWIVAPtUt+NCZNIKtN1A+iTmFiWiGnxWttcMDVm9JI85p2Tjy6g8k5/5ZwTjeXT/GZHul2yebtzGAnXTaMlCGno/zYmZMu03Qbv7w+dFKSdLz+6U0sL28RJ875YI/5PLImVEfy0WqqlcnqKz9P9W5qb7Ub47eqKFtlHOgY2V5E5SNUlZ9kVtnisSt26h2f+jmPeb0rT2v9SijmUy70iH+C0tJypJ2D6gKJG23wFcexQ2Kblm13Q9nJqyz9A16zQeM/s32PeieQjuKpfRRyWryux3+igQnin2U0z8mgdsPFf7e/FdOK/2QnptkwsPDyJHupfkqT+qsdeI0e/T95khbLkE+ezzJM73WutEmHx4n6/1wu2lLl0aPq11Qfbqrxn+lDuWrlpR5zWnk58lNQXdDQhrH8eHQVKDvplOGhKO2Tyzpu/MsWqdho8R/RYh6PSu/xFP/WppdqlIbbIPGf6DLNx7+/ecnrQ2WPOgc6agdeY1Lxn7abIp96/v/u+OcNutqXkOua65NDTZdJx7+feIzyCFB20snH//HtIsHl/ZCmNW0VTX5ql/zIcy1HOoqn9lHIafF6w8f/+oz/04MDZNuhbrz4bx7/F/IwRHU2jfGf2rxGvEBXy5APzyOv8eI/rABGj/jnw+rHV/zXbTde/Gt5phNyXXN9clBdMOn4r9NVoOykk8d/LqvaJU9jGQL5URY9uswHimIS9/+TiH8OEKJODkB4KZ9yk1bts0ZBV8pP2WmDifp/G571qM04Nvf8qI+J25M652Ql8PrHv50w/us+TDq0NY+0D3F7xT9By3g+dR/VMkzvda60SYfHx1f8h/b0by7+0y57oO9uhPh3E8Q/jzxXXUlH8VQPhZwWr1Un5lNu0lI78zrKP178ywslSlvxmd4key9/K9Yz/pnWO/7TtdKk/moHXmMDxD/CYgiVtde50iYdHicX/wU4AVV1/Dd0VR49lqV/IYcTrG4K8W82WfyLHRtsWxS+j2uO/7rvqSwEyu55ef9hGdokx+2VxjIE8qO8TUeeaznSUTzVQyGnxesNG/9pclnp5vIl/O64bZLNbeD4t1x5ai1aPe//SyB8qkB1Nhsx/rUM03udK23S4XFy8Z/4Tqf/jzu1WBsXFrqG+Gc6eW68+K+D6oJp9f8O5TlnnnmeDbPIRmbj1bkpAIVlACiDXBEjjhyZSUdkq6pmqCLcBBPXhEqpGvCcDOK1IiiDnhPHGP9GPR2HeeRF+sgbjGygrBWh5YxJNxx8iKY2UXz+qJfJ3uhQur34ocEBIvQIKIidTY8GuijK+ACHeEb8griUl7YlPq+JB3FspvEGX+V3DArWn+Q7aRxJj515rS6FJ32aclJWn5Y6NqXLRpRleVQ5jfFbcOQvGJAHH/AQlz5PW3JQVshbKk2rkovMJ9T2ise8mnzZGzlMVz0QOokyxDpxxo9//7bZBon/sMWk6pBsmMd/2q6CePHNbdapCfKJXBDZTRh4dsV/ePsp2i+Pf7E9ZSIY41cA81xlpHwKfPCv9iFN6tVEi6DpyPxSoaZPHv9h6xhj/Ipu3gHS7tG+bF+nEP96TTzKQFCZc/nVzprvmuI/8Ne61OP48Z90nFb8s93O9OJPcdMgxZdpjv+kN3+5T6jtFY95/jz5lcpE2to2Mb+YUvx7Wps+/rvxyFNtV9e1O/5JryzTlmSkpXaZSvyznJ6Tn9pEcfiz1n97rNiU8S/2U9q0Rd2+yc+nHP9hG2jKoHx4ncuvdtZ81zP+/eRmQI5lMKX4T33Lxo1/n97aqPGf5FOZ/EtvSWcCbVKL//DNWdujvjFh/Af5H+fxzzzSUrtsyvgnTbVvTisvT6DsQP3RUC+5QPsJX4JzfnI6ty/L94p/fZgXba00gwzKh9d6jinGP1/me2z6fz9Rk+vFX03OLP61/+cuVfmLmKbBJ9T2ise8unx5/KeYUJmttfF7u8Rp6v/zyaym+M9fBKAcan/agtvrNsV1eqGzOf45OUfe6jO5rsjiv3H8L/YkTC3+63VHfJWhjp9+GzL+FYx8tikvQz7kS6AtNF9t0yv+qSvxeU08BBmUj+Ybk14eUDvX8hvin/x7xb9uM+6cjat84fzzmfiMQ+M/7IhkK7/ivXf8j9//6z1hin8LE3YqoX/xe3zd9/9ebvUJtX3Cq/sbaVjrJ/YoD9NVD9Iq8v6/If6JR1pN8c88plMOluOEtPJsjP//6/+7aOXlCZQ9h15yoSv+Qz2KLXL7svz6xL++qaky5/KrnTXfTSP+6dPEo2yaZvL4n3T/n8W/7PiW447X/2+68X+KiSiz1GNl07ckN1b8u8cs/r0MkV74VqfPS+2yp598h3TJk3Q1nXoaOSd+bpMavtqnoa5zWrXyck075KDl/XldF7VvhFr8e3sTz6xn/KuMKnMuv9pZ893jKv6971JnAnnUcR+b+M935HUSE0lm7/tF4Xdri2U3ePwn/R+b+E8+SXrT6/+7Y0bL6Tn5uWD7HJ8/6lVMJf4zn9NrQi+50BD/5VvPOOM8MlFjUEASIfCcFchVLFqORteK0iN58Q3kMrypQBw6CkRgpUc5iGPlLSfKzWDmtTFpdSn5k446tJEKoW78MXhVhkg7C37KrDQ74SPZOW6+Eoh5XceQr3wjjQxURtJWWyKzgeIxjTaouA2d0FTQspRNdae+Pk06HeFtQsPlZLJU5SE96qBv93pcX1aX6qsfqRxNb5iP56+qrwt+qzoSz8pASnkWRXqrmHlV8AV/Xe+IyEfxKYfiMJ24BNavP++OS8rOG1X1B+XTHf/+bSFI/Ee6Uo58kh3rAwryIl8+FCdOd/yngSTLG5MmWCcb/7pdIekbxn8oqwMyysNfin942caL/zA5TRmK0Pk0xT/LE5Ld6keC6uT1ilk1HB5JuwyTv0Xpt7an/UhHZaDMZoPHf3dZ/myIf9WbwLL0A0Juf/Wd3vGf/F7Pla8eVWbq0Rz/9Xhhnvenej3W4z/poXwUn3IoDtOJS6CP85zlmmRXfNW3SR89t1n8aznyye2o+hAHoZ6UVnf8b6D+f7z4Fxv7+hov/pMMuf/l+inN7viXF57WJ/4bQGUkbbUlJtX/+/Qpx79sU8U8tUdelr+px7+smnF+Amt68T++vyaZkw9NPf7Dizd8I32Tx3+q+3Hjn/iFnwRGVt8q73jxr7tt5EfyIt//vfHfrQvL+jTr6y3zDeUbacTchMMjaSdbJhmJU2QyUGZjvK/WeKmfZjwom+pOfdXnCMRhObWNysOy0a9Cem7/6cX/VPv/XuP/CeJfeFdVhb5W2oKT97/KR/Eph+IwnbgE+jjPWY6yjBv/WX0gq2+eTxT/49nTTRT/IUYoW06PchBnsvHPiWz8zcR//UhQvpqu0ERbbYnMBrkMlNlMp/+fRvxzwtXjhnbPpThnWepAyO1PP3DjxX9o/4qyTPTlxViPk/xNZaYeTfEfJ52DjzPP+1PyTwCoqg5arb74LEJfRCMfxaccisN04hKKIq2gzushye7jgzjYiPGvz3NYnjhoiv//6/9jmh4JylfTFZpoqy0RbeD7/lwGymw2UfyznNpG5WFZ6kDI7b9p+n+Jf7mvz+OFNOhPynvTj/+TLFo/AFCGFwFU3yZ99NxOIf7zI3lRzo0f/95/nUtzDixrwku5PDeFiS9lswx/GyP+TaYLyzJNjyHX7+DHb/5m/kBIMhZxYYzaEpkNeo//N2T8d8tLHJZT26g8pEcdCLn9N3n8C14eL8wrNnH8lw39P+vXy17V+/+wi4HqawxfhKvXt8r7txP/G6L/9zSnGv/sW4se8Z/rwrJM0yNB+Wq6QhNttSUCn/8PcQBmUPINanoAAAAASUVORK5CYII=</t>
-  </si>
-  <si>
     <t>2025-07-18</t>
   </si>
   <si>
     <t>problem2</t>
   </si>
   <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAB4AAAAQ4CAYAAADo08FDAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAP+6SURBVHhe7N17fBTV3T/wT+73DbkAS7iYhKvcBMP9IhBvULFVWlta+VGreGlVihaFWvWxtbWo2Fr1eVotj1Ue7MU+SluoIOgCTxASSCCEAIFAEiAkC9ncdjebe/L7I5lh5+w9u5u95PN+veb1Ss7Mzs6cOXNmdr5zzgnRXq7sBgWnEDGBPI0nj7cEQuHl0SciImsC4Rom4jWNAlEgnmvkDazBvClwcldZI/h7/RA4+UpERP3Pn69ivIIR9Tf3aoRQMYGIiIiIiIiIiIiIiIiIiAITA8BEREREREREREREREREREGCAWAiIiIiIiIiIiIiIiIioiDBADARERERERERERERERERUZBgAJiIiIiIiIiIiIiIiIiIKEgwAExEREREREREREREREREFCQYACYiIiIiIiIiIiIiIiIiChIh2suV3WIiBYkQMYE8jSePtwRC4eXRJyIiawLhGiby/jWtu9v730EDTSCea+QNrF28KXByV1kj+Hv90I2QEH/fRiIi8hV/vkIEzp0BUbBwr0ZgADiYuVc2yAk8ebwlEAovjz4REVkTCNcwkXeuad3d3eju7kZnVxe6u7rQ1dUlLkLkhkA818gbvFODUY/Ayd1ACgCHhoYgNDQUoaGhCAkJYTCYiIgU/PmqEDh3BkTBwr0agQHgYOZe2SAn8OTxlkAovDz6RERkTSBcw0Sev6Z1d3ejq6sLHZ2diImNRXNLCzo7O9Ha2iouSkRENGBEREQgIiICMTExaG5qQnhYmBwIJiIigp//ovT8L0ciss+9GoEB4GDmXtkgJ/Dk8ZZAKLw8+kREZE0gXMNEnr+mdXV1oaOjA9FxcTCZTIiLi4NKpUJoaKi4KBER0YDR1dWF5uZm6HQ6qFQqNDc1ISI8nNdHIiKS+fMvSs//ciQi+9yrEXiHSUREREREHtXZ2Yno2FgYjUYMGzYMgwYN4sNtIiIa8EJDQxEXF4eRI0fCaDQiJjYWnZ2d4mJERERERG7jUxgiIiIiIvKY7u5udHR0wNTcjMTERAZ+iYiIBKGhoUhMTISpuRkdHR3o7mabKiIiIiLyLD6NISI/4163BkRERL7Da5iks7MTHR0diImJEWcRERERgPj4eLS2tqKzs5MBYCIiIiLyOI4BHIz47LHf8OTxBn8vwDzqREQk8vdrlyOevbZ1dXXBaDSiE8CYMWPE2URERNTr/PnzCOsNBrPHDCIigp//uvTsL8ceXd3dyL9Yhl1nilBUeQlaQyOuGhoBAEMTEqFOSMTUEaOw7MapmHFDJkJD/DmHiLyh72WeAeBg0/eyQH3Ak8cb/LkQ84gTEZHIn69bzvLs9a2rqwsGgwFdISEMABMREdlx/vx5hHZ3IyEhgQFgIiIC/PwXpid/ObZ2dGDLV/vwh6800BkN4myrUuMT8Nj8bKyZvwRR4eHibKIg53rtwABwMHH9+JObePJ4mj8XYh5tIiKyxp+vXc7y7DWOAWAiIiLnMABMREQif/6F6alfjv8+VYgXd36CqsZ6cZZT0hKT8Ivl38Rdk6aJs4iCnGs1BO8uiYiIiIj6xLUbbyIiIiIiIqKBqru7G5v27MCaj7b0OfgLAFWN9Vjz0RZs2rMD3d2eCkuTe/h8xB8xABwMQnh+EXlPtwffbyMiouDAmy8iIiIiIiIiZ3V3d+OHf/sAv9v/uTirz363/3P88G8fMAhMA4hrZd2rXUBXNtfhseN/Qm1bkzhLljgkBWFx0WIyAGBi9FC8PnS5mOyWg7mHr1cIISEIDwtDSIhzcfDu7i50dHYCvZ8PCQnBgjlzxcVc8sU+DZIGJSFr+nRxFnS1tbhQVgZdrQ7NLS0AgPi4OAxTD8PozEzEx8X51bNHY1MTLpSVobq6GsamnmMeEx2N1NRUjM7MRGpKivgRFBw/jvr6etyWnS3OCgheO3kGLD8q0ACPMBERWeFv1ypP8Oz1jl1AExEROYddQBMRkciff3G688tx054dHg3+mvvx4jux8Y67xWTqVyFulhBynePawqsB4H9UHcOr53aKyQpxg5MQFR8rJsv+fcNDYpJbcg4fQmJiIiIjI9HW1gaD0YhxY8eKi1l1rrQUCfHx8mcbGxuxcO48cTGX2AoAnzpzBmfOlmBQYiIGpw5GQkICAKC+vh7aq1q0d3Rgxs03Y8Tw4YrP+UrllSvIP3YMEeHhUKvVSEpKAgAYDAbU1NSgobERN06YgEk33qj4HAPApOS40uo/PLpERGSNP12rPMWz17z+DAAfPnwYhw8fxtmzZwEAiYmJuOGGG3DnnXd6/buJiIjcxQAwERGJ/PkXZ19/Of77VCHWfLRFTPaoLfev4ZjAPiWW3L6WFnKNmO9KA/LuMjIyEklJSYiK7ml5rFarnZoAICo6GklJSYiMjBTW6jlS8PfG8RNw25Js3DRlCjLT05GZno6s6dNx19JlSE1JQf6xY6i8ckX8eL+Tgr+pKSm4a9kyZE2fLm/vTVOm4LbsbNw4YQLOlJTg1Jkz4seJiIiIAoT9G2vqX//5n/+J7du3Y/z48fjVr36Fd999F4888ggGDRqE9957D//+97/FjwwIGo0Gb731Ftra2sRZRERERERE/aq1owMv7vxETPa4F3d+gtaODjGZfIbPT/yBxwPAVQYddp4/jJ3nD6Pwylm06Q02pw6jSfz4gGce/BVby8pCgAXz5iE1JQUniorEuf3uRFERUlNSsGCe7dbQk268kUFgChDdfEOJiIgEHPPX33z00Ue4evUqnn32Wdx1111ITU0FAIwZMwb3338/Vq1ahT179uDw4cPiR91WWVmJp556Co8++qg8MeBKRERERERkactX+1DVWC8me1xVYz22fLVPTCY/Ul5Rgdy8PIupvKJCXDRgnSwuFpNscmVZ2+zHMTweAP7uP3+B9V/+F9Z/+V/467HP0FSttTkZrlyBvrJKXMWA5WzwVzLtppvQ3tGBs6Wl5kv0q7OlpWjv6MC0m24SZ1lgEJj8n/0Kk4iIBiIGfv3N+fPnceTIEaxdu1YO/IqmTp2KO+64A/v2efYBgEajwRtvvIGf/OQnePfdd/Huu+/i7bffRkZGhrgoERERERHRgNbV3Y0/fKURk73mD19p0NXN57v+6EuNBqsfeADPbNhgMa1+4AE89/zzqK2rEz8WUE4WF+NHTzyBHTvtD4sLADt27sSPnnjCg0Fg6+Xe4wHgq02uvc2hP1aGas0J1JVfsToNFK4GfwEgPi4OgxITUVNTo5zRj2pqajAoMRHxcXHiLKsYBLbtlU2bsHDxYnlau26duIjFMgsXLxYXsbDl/fctPrNw8WJsef99cdE+u2/lSrsV29p16zz6fe7a8v5/Y+26Hwup1itJc2vXrbPIR2m/pWPjKa9s2oRXNm0Sk4He7bA175VNm6yWHXd4et+cdd/KlcjNyxOTZY7mSxyVT3t27NyJ+1auFJM9LjcvT1GuxOMrzre2jDXWyoN5OZb2zdpy9thaXjwmtpbzFlv1nbffJLR3vpozzw9r9Ym3tnPL++/363Ewd9/KlR47h7xdF3l7/QCwdt2PsXDxIsW0Y+cOcTELr2z6NRYuXiQmD1gnTpzAuHHjbAZ/JXfddRcaGhpw/vx5cVafGI1G7NmzB3fffTdGjBghp0dGRuLuu+/26hAxREREREREgSb/Yhl0RoOY7DU6owH5F8vEZPIZqTe1ENyanY2c/futTq+/+iqqq6vxxm9+I64goEyZPBnPrl+P1zZvtvssesfOnXht82Y8u349pkyeLM52g2V8w+MBYHN/vv+XyF+3FSMHDQUAPDp3BfLXbcWjc1colmuvci1oHGxqdDWOg782JCQkoKWlRUzuNy0tLUhISBCT7TIPAvsyeO1P1q5bB61Wq6j4pHGnJfetXInjhYWKZZ5dvx4LFy92GASbPm2aRcX64datXn/QHYy+v3q1Ih/vXr4cAPDcxo3I2b9fXNwrbr/tNuzavVtMBgDs2r0bt992m5jslv7cN5gFYbRarTgLcDB/x86dPgt0uUOzb5+iXB0vLFS8NFFTU2NxHj+3caNiHSLpRuOtN9+U0+5buRJqtVpex9//+leg9xhPnTrVqRc1rK3X1jFxZb2eIuZTzv79yEhPFxfrd9byzbw++f7q1Vj9wANeCwJ7iivnmPm1ydF1SmTtezxZFzm/fs+3/u057gfk6e7ld4uLWHhu40+Rs/+AmDxgabVapDt5Xg8aNMgn95tiN9Hbtm1TzG9ra8Nbb72l6EZaXGbbtm146623cPz4cTz66KPYuHEjjEYj0BuM3rhxo/zZp556CpWVlYrPX7lyRbENGk3/vXlPRERERES064xzw1fO+9Y76N60CsoBJtPx5qaNeMQs5ZEfb0f3j+2/HO3sd1L/+FKjwdp1P8badeusTq9s2oSxY8fi0UceQc7Bg37/XMyRu5cvtxsENg/+SnEFb/JqAPh/i77E6JQRePWuJwEAaxd8BwDw7uFPhSV969y5UqcmbzE2NSE+Lg4tLS0oOH7cYvLUsHM1tbViElpaWtCg14vJHiXuT8Hx42hpaUF8XByMTU3i4jb1x/YvWLzY7vSkkw+9XVFeUYHjhYV4ysqDaInUskwK1kikCuWZDRsU6c7I6Q0yO9NqLbjZ7iLBX0kXBzGgIv3fHxcPb9mxc6f8ooP4EoQz8wOVGMxdvWoVPt+zR/7/6rVrLu/v1m3b8F2zlpdb3n8fw9Rqi++SrHnwQXy4dauYbEFcr6Nj4ux6g52Yb6I1Dz4ItVqNL4MoQKPZtw933nEHpk+bBo2Hu+H1Pg/dfFFQiY+Px+TJk/G3v/0NJ0+eFGfLKisr8cYbb+DBBx/Eu+++izfeeAPFxcWKAO/Zs2exZMkSuRvpF154AQUFBRZB2lOnTuHUqVN49913sWnTJsTHx6OyshIvvPAC7rjjDvnzjz32mMXnduzYgVdffRXvvvsunnjiCYfbTURERERE5ElFlZfEJCvS8e0ZwHnMwbdHifOum/etd/DMlacQ8jv7L0c7953UH8oryvHSL36OMaPHYOrUqVan0tJSvPvee5gzezYA4OrVq+JqAo6tIHD/BH+VcQ6vBoA/PbkPB8qOYfHoLLz7rZ8iTTUYT25/XVzMZ8LCwhAREYH6+jqnpoiICISFhYmrcUtCfAIGJSYiPDwc9Q31Vid76uvrnWqB29LSgms6Hc6VXe8CoaWlBRcuXsQ1nU6xrCsSEhJQX+94G61N4eHhGJSY6NPtFx3cv9/u9LZZyy1PkVqmFdvp733X7t34yVNPicmAWbDP2hsljqxetUrRkrS8okLRHanYbafYDa34Rs59K1fK88TgJMxaCVpbN3q7ZjbvFvOVTb9WzC+vKFfMv29lz0slkvtWfgc7du6Q50ukrjMtP+O5wK/YBazU7bB5npjnl6O8dsRaQEWzbx+WLV0q/y92h2v+/dL2SfNg5/iK+wYr6xbnO9p/W+5evtziRQdz9uavXbcOr23ejOOFhTa3SdoWa+XTGeJ+SHkm6et+e1puXh6GqdWKlq+f79mD7333u4rlRN9fvdpua11r67V3TCSO1tsfrHXve9/KlYpyYn5OLDTr4h1Wyrwrx9VavlkzzCyAbu0chZXtEMs5nKhrxe0XyzFs5IWjc0y0a/du3JqdjewlS2z2WuDK95jXRdJboua2vP++vL/26ljH678e+HV0XZKuO/et/I68THlFuWIZZzi6vr2y6dcW3z2QqdVqVDh5DjY0NGDw4MFicp+tWrUKCxcuxDvvvINHH33UIqDa1taGTz/9FFlZWZgyZQrQGzi+//77UVxcLLfgnTJlijwfAEaMGIGsrCxUVVXJaQCQlJSEe+65R5G2f/9+ZGVlITs7W04bP368olvq2NhYrFixQu6Wevz48Zg0aRJOnDghL0NERERERORNWkOjmGRp7kr8uPrvGPvPStw1y/pzk3nfegdfDf87xv6v49+BTn2nD+Xm5bk0BTIpmLv2ySex5sGHsObBBy2m+fPnW/QoGAzEIHD/BH8lUoO3bu8GgAHIAd9v33Q7dpUcwuGL/vPWeUJ8PG4YNQojR450arph1CgkxMeLq3HL7JkzcduSbOtTds9ki662Fg2NjRielibOshAdHY1J48cDAM6VlcnB04T4eIzLzBQXd9rwtDQ0NDZCZ6V1rkTaD1vT7JkzxY9Y8Nb2+4vvr16N1zZvtniYDbNWndJbMNZMnzatTwOGT+7tY176ji81Gmz94AO5S9JhZi2Eyysq8MyGDfL81199VbGu1zZvxmubNiFn/34sW7oUb/z2t4r5H27diimTJyvWbd795iubNuHDrVsV3WIeLyxUPPC+vn0983u2T/lA/LXNm+Vl0PvQvKd1Ys9nfvLUU/3WGlHMk2fNWl7ay2tn3H7bbTheWKhIO15YKI8b8MqmTSgqKpLX/+z69Vj9wAOK5a/n1X6Hx9fc9WOl7LJY3H57++8Nb735Jp5dv17uAti8pau4LWL59CTxu/qy33u/+ALTp02T/7927Rp27d4tB7PEvBZp9u1TdAVeXlEBrVaLmpoaRVBMvJGcPGkSiopsd5UjrtdZjtbbH57buBHTp02TA9FScFcqJ1vefx+vbd4sl+mtH3wgf9aZ88keZ/OtWqvF0CFD5P/Nz1E4ee69smmTYriAvtR5tvLC3jkm2rFzJ9S9Qe85s2dDrVZbvKjkzvdYqwM/37MHq1etAhzUsc6sH73XD0fXJSjO+QN9Puedub7RdTfddBPOnTsHnYOXAL/88ksMGjQIY8aMEWe5ZdWqVXj77bcxadIkvPPOO4quma9du4by8nLcdNNNis8kJSUhLCwMDQ0NcprYDXROTg7q6urQ1tYmL5OWlqYYW9hoNKK4uNhi/aKMjAwMMatPIiMjkZycrFiGiIiIiIjIm646EYx9ZNZs7DpyADh8GKUzFgjdQAOYuxFfDf+7w5a/Eme+01dOFhfjmQ0bXJr68szff10fE3ggMA8C91/wV8nrAWBzsZHRYhI6WlrQVH0V9WdLrU5knbGpCfkFBRiUmIgRw4eLs22SgqVS8HSUC5+1ZsTw4RiUmIj8ggKXunPuK09vvzX/stKStryiwiJQ4klrHnwQWz/4QA7w9FdLObE12poHH1Sk3X7bbfIbONIbO9L8ObNnK5b9/urV8v/ZS5ZYvLkzfdo0RQX31Lp1OF5YKLdC27V7t0XQ8SdPPYVdu3fLranWPPgQMtIz5Pnm2yfp2Y7ry4itp+fMnqNoJesqaexkabLXCtBentjLa2fcvXw5tFqtXC5z8/Kg1WrlPN61e7eiW/G7ly+3CMCYb5+j42vO/rG6nh/29r+/9ee2uPtdW95/H8cLCxVBKWlsUmnatXu33SCwVqu12uJt67Zt8jq+v3o1ntmwQXHMhg4dimo722trvY44Wq8nSa06rbX8/N53vysHQ1/bvFlRN3y4dauiXGekp7t0PtnjTL5Jx9O8njQvS3Dy3LOs82a7XOfZywtn7f3iC9x5xx3y/3fecQf2fvGFYhl3vkesA6WXHKTPu1vHwmF+X2/la37dceac77mOXG/tW15R7tT1ja4bM2YMZs2ahbfeestmELioqAj/+te/sGTJEnGWR0RGRmLt2rV44403AADvv/++InArtRCWppdffhk6nU7uOWfbtm148sknMXnyZLkb54ULF8qft6WhoQFhYWFISkoSZxEREREREQWYRbjn5jz84zAAHMA/qr+J5+eaz5+Ndx8DHnUy+AsAIX4cXDRvHOXsJDX2CT7+e5yCidcDwH+5/1dobm/FH/P+gUWZN2PFFO88hAlo5i8+OPEShLGpCQe/+gpw0CrUlnGZmUhKTPRY8FTahoNffdVvQWBPbr+58ooKvLZ5M75lFjAor6jA/3vgAWz2YotB9D74zultefnh1q2K1rHOMG/l4SwpYDB06FA5zbx70dc2b5aDNlILroVCt6gS81Zr0vrMA0tTp06V/4ZZoPHq1atmrZznKJaR/jfv+9+8O07z7ZOYb0duXi4gl9HrXR/0Ja8k31+9WnERthUkhRN5YiuvnTV92jQUnzoFACg+dUoO8kj5ufqBBxSBMDGYYL59jo6vxFaLdGvjNNjbf/PtchRI94T+3BZ3vmvtunVyC097nl2/3maXutZIx8U8MCiNOWuv+3lfcZRP9kitOqXJvHtqKRi6cPFiLFu6VC63tsq1+TxH51NfmL9Qcryw0KIrbWV9Zn0bzc89W8u4UufZWocrynvHtr/VrBeTyZMmKV768cT3LFu6VK4Dv9RoLALdztWx1m+8rl8/HF+XrJ/ztruB7rmOXG9VLAV+HV3fSOnOO+9EY2MjXnvtNfz73/+WA8Hnz5/HRx99hG3btuGOO+7A3LmKpwceJ3XvXF5ejmvXrsnpTzzxhBzYNZ+mTJmCyspKFBQU4IknnlB04+wsk8nkcAgWIiIiIiIiXxuakCgmKc2di2XHDuO93n/fO5KHZbOuD+sH5OHRFyrxzIcb8YhZqj1DElRiEpFPmHf7bG1M4P7g1QDwc7f+AJPUmXht/1Y8u/Mt1Jn0eO7WH4iL+VRISAiqqqudmkJC7ERl+8rFVZoHfxfMn4/4uDhxEaekmY0z6K74uDgsmD8f6McgsCe331xGejoO9gZevrVypRz8XbZ0Kf7XwRiXnjJn9mxs/eADHC8sRG5envww2V4L5OOFhYoH0M4qLi6Wu+hE75iTYjen5v7+179i6wcf4LXNm10OynjCfSu/07t9PQ/Nxe0LJI7y2hm333YbPt+zB+jt+jRbaOUkvjGWs3+/3dZ1/Xl8xe2yF0j3tv7cFnvfJbVUzXEQ/AXgsDWpSKpHzF/2QO+Ys1fNAhb+wl4+uUsKhroSFIWVbcpxcD45w/yFEjH4G8i+1GgAIWj+zIYNinmeMGXyZLkOLCoqUtSB9utYF2+++kEwXd/6g06nw1tvvYVx48bh3nvvxdmzZ/Gzn/0Mjz76KN577z00NDTgkUcewV133SV+1OuGDBmCjIwM1NTUiLMUYmNjFa1429raUFdXp1jGGmn9HMuXiIiIiIj8ndpuADgdb35jNnDzOnR/uL1nemw2cPNcZbD30jaM/QPw7qZVlt1DW2H/O8nfic8uA5U45q95d9D9GQT2agD4axPmI//yabx7+FMAwGv7e7pdfHTuCmFJ3zIYDOjq6gK6u61OXV1dMBgM4sfc5+LzR08Ff73BF0Fgb5KCvVLw92d9GM/PHebBjoz0dCxbuhR//stfFMtItrz/PtRqdZ8CEa9t3iyPlyh1IfzWm2/K860FhqSWytOnTXPpQb55qxgIrb+uB7l7WlxdX+Z6C6zcvNze7fudPN/a9l3XbdH6UuLrsUidzWtHpC5Qt7z/PrRardySzpmXBmxxdHxtrdsTrfn80dVr1zBMeOHEvOWfowf8zlq7bh2mT5umKBP21NTUQG3nRRi1Wq3Ytoz0dKutfcUxZ69evWqxv+bE9TrL0Xr7S3lFBT7cuhVbP/gAH27dKtcNtuoK83limXdFX/PNnK3tsFaXivthrc6zVY5trcMVn+/Zg2fXr7cImH9/9Wo5YOuJ7zHvBvp4YaGiRbe7dawz1yVPcf36NrBJwd+hQ4fi8ccfx9y5c/H000/LLWxfe+01PP744x4f9xe94+9++OGHiq6e29rasG/fPnnM3cjISCxZsgR/+9vfcPLkScVnd+zYAQAYNGgQOjs7sd/shZ+PP/4Yp3pbtNsjrT8nJwcas+v02bNnUVlZqViWiIiIiIjIl6aOGCUmXTdqAe7CJ5j//XsRYjY9emw2nvmW0BDg8CaE/HMEvnIiCHzTiBvEJPJbygDZSy++6NFGIL4iBn8lvggCezUAvOA/1+D2956Q/3/38KeY8eZqOSDsL0JDQzFq5EjMmDHD6jRq5EiEhno1qxzy5+CvJBiDwA+sXu314G95RYXFWJ7SGMDSw+znNm7E8cJCi26ht7z/Pj7culXRraszcvPy5C5QpUpIDC5IgRLzz5gHHsTAkSO7du9WfP6N3/4W31+9GjALckstxKwtIz6ML68oV2yfNRnp6Zg+bRqeNTuGO3buxPHCQsVy/c1RXrti+rRp+HzPHkXXp9J+i/kpljNzzh5fZ46Vr3ny+H6+Zw9uv+02+f/p06ZBs2+f/P/Wbdvkv/tK6i73u2Zdz4vMz/3y3q7qzcdXFU2ZPNlivNU777gDr23eLP8v1TPmNyLFp05ZdNduztp6neFovf3l2Y0b5XF1v796NX7bGyCUyrV5XVFeUYEdO3f26XwS9TXfzDlz7jlb59krx/byQiKuz5wUfJ1sZYyaW7Oz5YCtu98jWbZ0Kd747W8VdaD9Ovb6jwt7689Iz3CY357Sl+vbfSu/gy3v/zfQ+7mFixfJn39l069x38rvCJ8IDmLw1xfOnDmDJ598Uh7b98knn0RycjLWrl2LyMhIAMCUKVPwxBNPKMYBfuGFFzB9+nSgt9voJ554AgUFBfL8tLQ0p8YARu/6X3jhBezYsUP+/J/+9CcMGjRIXJSIiIiIiMhnlt1o+1nQI/d+E8g/iENC+nvbPwFmLLAM9B7ehPn5c/CVg+6gl944RUwiH6utqxWTZKYmU+9fIbg1+1abQ3UFClvBX0l/B4E9HtUcGne9KzNnhDS2IbK+HdEVJqtTUBDH9nWx/AZC8FcSbEHgNQ8+KCZ5XEZ6Onbt3q0YW/LzPXuQI3QDm7N/vzxGqzRJD4ilh8e2HC8sVHzumQ0bkLN/P54ze/AuBUSe2bABCxcvxrMbN1p0QSnNW7h4MaZPm2a1ErPl+6tX489/+Yvi8+b5+1xvYEYa/3Dh4kW48447sObBh4Deh/HXt2+R1e27rlv+S2oBJn3vyeJijz+8d5Uzee2s22+7DVqt1qL757fefBPTp01THPcpVgIy5pw9vteP1fV19xwr758vjty9fLl8nrgSoBPZyoen1q1TnK9SC3p3SC0xxTFmFy5erAjKy9/5wAN4dv16u/l99/LlqNZqFa0r1zz4oOK4fb5nj0W3wx9u3aoYt1Vkbb3OcLReTxLru4W941pLQXQp39Y8+CCOFxbK5eS5jRsV58zqBx6Qg5h9OZ/M9TXfRM6ce87UeY7Ksb28cHSO/fkvf8H0adOsvrEpBailHi3c+R5J9pIlFnWgM3Xs3cvv7l3/Iryy6deKeZLnNv7U7nXJU1y7vg1c/hD8jY+Px6ZNmyzG9V1l5VowZcoUxTK//e1vMWLECHn+iBEj8Nvf/laen52djVWrVikCyeL/5sTPb9q0CfHx8QCA7Oxsq59btWqV1W0lIiIiIiLyhhk3ZCI1PkFMBgC897t7MfZ/rTwnubQNYzduwyFUYN3GTfL4wABw6H+fQMj3lWnmUuMTMOOGTDGZfGTO7DkYM3o07lmxQvFsxXz6+yf/i298/RviRwPSyeJiu8FfiXkQ+KTQW6OnhWgvV16PlHhAlUGHY1dLAQC5p47h48/+IS5yXVsXuq41IWb0YITFWT7YAIDCX38iJrkl5/BhJCaq5IBZSEgIzpWWYvy4cTa709RqtTh77hzGjR2L7u6e7Kqvr0dNTQ0WzrV4F0XJhUCvNYEU/DUXqNvtKo+ePH0ktQIG4LBy8X9unjB+cUSI/MOOnTtxsrhY8aKHPVKLYHuBZXhxvcHO1XwjT3L32jIQePb6KQ2f0hUS4pGumP0h+EtEROQN58+fR2h3NxISEnze8xwREfkHf/4F25dfjv95YC9++fk/xWSveP7Ob+DxRbeLydQvbJdccXgtc0OHDkVGeoaY3KsvJc63ThYXO91oxJVl+8rjAWBz/zz8BX7636+JyQrhiTEIjQwXk2WeDgBfrqzExcrLSEpKQmpqqncDwLbLvFMCPYga6NvvDK+dPAOWOydN347GwsWLxSQAwOuvvhp049nSwPPKpk0WY6Fa4+xyEmeXd3a5gYL54SvuXFsGir5dQ23xZACYwV8iIgpmDAATEZHIn3/B9uWXY2tHB+a98XNUNdaLszwqLTEJh37yH4gKtx1rIm/ydsntS+kjrwaAvzh5GOv/fH28wb7wdAAYZkFglUqFqKgo1Oh0GDliBGJjY8VFAQAmkwmXKysxODVVDgC3tbWhsbHRawHgYAmeBst+2OK1k2fAcuOk4dEgIiIL7lxXBhLPXkM9GQD+8ssvUVJSwuAvEREFJQaAiYhI5M+/Yvv6y/Hfpwqx5qMtYrJHbbl/De6aNE1Mpn7ji5Lb1xI5cIStf/rpl8RET4mLisHeU7loaunbWL7zx03DXdMXicluS1SpEIIQXL1WgyaTCSEhITA1NaG+vt7qZDQa0dXdjaamJpiammAymdDa2oqQkBCMGjFSXH1PWXezvF+rqUFdfT3mzZ0b0EHTyMhIqNVqVFVXIz4+HiqVSlyEyExfThxW9EREJN18iRP5Qnd3N9ra2tAdEoLk5GRxtksyMzMxa9YsMZmIiCgo1NXVIQRAVFQUQkJ470JERMH5S3bcEDU6OjuRV3FBnOURP158Jx6c6/k4ErkiGEtu4PNqC+ABieV8QOHJ42munkA8AkRE5Oq1gyx59nrqyRbAREREwYwtgImISOTPv3Dd+eXY3d2NH/7tA/yzqECc5ZZvTM3C77/zAF+k8jlf5L87JXJg4N2lJ/mijBMNWKzgiYiIiIiIiIiIiPxdSEgIfv+dB/DjxXeKs/rsx4vvZPB3QGMPcI4wAExEREREREREREREREReExISgo133I0t969BWmKSONtpaYlJ2HL/Gmy8424Gf6kXy4E17ALaE1i2BiyePJ7mzMnEXCciInPOXDvIPs9eW9kFNBERkXPYBTQREYn8+ReuJ385tnZ0YMtX+/CHrzTQGQ3ibKtS4xPw2PxsrJm/BFHh4eJs8il/KLmeLKHBgQFgd/lDuSaf4cnjaY5OKOY4ERGJHF07yDHPXl8ZACYiInIOA8BERCTy51+4nv3l2KOruxv5F8uw60wRiiovQWtoxFVDIwBgaEIi1AmJmDpiFJbdOBUzbshEKFv8+il/OC7eKKGBjQFgd/hDmSaf4snjafZOKuY2ERFZY+/aQc7x7DVWCgCHRUZi5MiRfKBNRERkQ1lZGdDZyQAwERHJ/PkXrmd/OVJw8beSy9IKjgFMRERERIHL335gkCQ0NBSRkZEwGo3iLCIiIgLQ1NSEyMhIBn6JiIiIyCt4l0lEfq6bb+wQEZEghMFfPxYSEoKwsDBERESgvr5enE1ERDTgdXV1oaGhAVGRkQgLC0MIu7MkIiIiIg9jAJiI/BgDv0REJOIDUn8XEhKC8PBwNNTWIj4+HpcvX4ZerxcXIyIiGnC6urrQ3NyMK1euIDIyEvqGBoSHhzMATEREREQexzGA3cH78wGPJ4+nmZ9UzF0iIrKGN2Ce5/lrbmdnJ1paW9Hc3IyU1FS0tLaira0NXV1d4qJEREQDhjREQkR4OBrq6xETHY3o6GiEhYWJixIR0QDlz794Pf/LkYKHv5VcllYwAOwmfyvT1O948ngaA8BERGQPb768w/PX3G4AnR0daGtrQ3NzM1paWtDZ2Ymu7m6g2/PfRwMR6wPqYb1GsZ7af1g++8f143w9x/0470NCEBoSgrCwUERHRyMmJgaRkZEICw/3560mIqJ+5s/XBF/fYZE/88eSyxLLALAr/LEMk0/x5CEiIuoPvAnzLu/c0XR3d6O7uxudnZ1ob29HV1cXuhn8JY9hvUD2ai/bc/oHy2f/6TnWPTnu//keEhKC0NAQREREyGP/svtnIiIy589XBV/fYZE/88eSyxLLALAr/LEMk0/x5CEiIvI23oB5n3fvaKRAsPQ3kWewbiB7tZftOf2D5bO/BUqO9wR7uxn4JSIim/z56uDrOyzyZ/5YclliGQB2lj+WX/I5njxERETexpsw7+MdDQUi1g1kq/ayntr/WEb7U2Dltr+UUSIi8kf+fE3jFYxs8+eSiwFbekPFBCJyzsCsMoiIiIiIiPxNt9nkL/xxm4IXc5mIiIjIl3jf648YACbqA1ZlREREREREREREREREEkZO/AkDwEQuYhVGRERERERE5F8Cp92Jv3eRSEREROSOwLgjGwgYACZyAasuIiIiIiIicg1/SfanwMhtBoGJiIiIyLsYAHYkhPfl1CMwfkQSERERuYJ3OEQUmAKv9pLapwbelgeiwMhlPnAiIiJLgXENIwo0A/OeiwFgewZmmSAreOElIiKi4MM7HCIKTKy9iIiIKJjxtTEi8gQGgG1h8Jd68UJLREREwYd3OEQUmCxrL8sUIgTUg3M+gCIiItsC41pGRP6IAWAiO3iBJSIiouDDOxwiCkyWtZdlCpEoMEoJg8BERERE3iUNvzFw7rsYABYNrONPRERERANKYDwGJyISKWuvwGnbSf4hMEoLH0gREZF1gXEdIzLn7/frA+OeiwFgcwPjmBMRERHRgOTPP76IiGxj7UVEREQDnb+H04isY6n1pRDt5UoeATD4S9bx5CAiIvI13qR5Bu9qKNiwbhgoLGsvy5TAw/LrS4GR+8FQzomIyFt8dS3j1Yls2Vt+FG8e+V9c1l9De2eHOJucFBEahpGJQ/H0rPtwa8YMcbbLGACW+KrWJL/Gk4OIiMjXeJPmPt7RUDBi3TAQWNZelimBi2XYlwIj94OpvBMRkSf56jrGKxNZs1HzLv557qCYTG66e+w8vHbrD8Vkl7ALaA6xQjbwgkZERESBj3c0RBSYlLVXt0VK4JP2Kdj2KzAERq7zgRUREVkXGNcxGgh2Xchl8NdLdpQewmfnc8VklwzsADDvo8kGXkSJiIgo8PGOhogCE2svIiIiIvv4Ghn5g//K/4eYRB70+wL38nfgBoAZ/CUbeOEkIiKiwMc7GiIKTJa1l2UKkScEzoNzPsAiIiLbAuNaRsHqkv6amEQedFF/VUxyycANABNZwQsmERERBT7e0RBRYLKsvSxTgtNA2U//FBi5zyAwERER+Z+2znYxiTyovbNDTHLJwAsAcwgVsiEwfvQRERER2cM7GiIKTMraK3DaZnqOtM8Dbb/9Q2DkOh9oERGRdYFxHSOi/jawAsC8TyYbeJEkIiKiwMc7GiIKTKy9iIiIiNzD18go0Dw6d4WYRB42cALADP5SL/P3qnlhJCIiouDAOxoiCkyWtZdlClF/CJznA3zARUREtgXGtYwI+NaUbOx95B0x2S3567Yif91WMXnA8rsA8O/eeRsPrHlI/v/Jp9bhyafWKZYh6iteAIlsW7tuHdauY31LwFtvv40fPHT9WjwQDMR9dgbrhUDBOxwiCkyWtZdlysDEfPClwMh9BoGJiIgo8M0YOdGlIPBry9cif91W1L+sQf3LGlS9uAt/vv+X4mLUq98DwFvefx8Lliy2mKQgr7GpSfyI66RhUcynfrTl/fexYPFibHn/fXEWAGDB4sVYsHixmBz0pHzxFWs/4sorKrB23Trk5uWJs7xqy/vvY+HixYrpueef7/ftcETazkDiT8d04eLFfho4EStIsaIU061NtojLeW+yluf3rVyJVzZt6j3+lp/pmWzzVflxhrX9/cFDD+FLjUZc1G0euRb72CubNuG+lSvFZNnJ4mIsXLxYPtbBsM+O6uyFdu5NKJBZu8MhGghY9gOd9SMo3rcN5Il8yXr59DcsK0REZF1gXMdoIHpt+Vo5eDtj5ET8Me8fSIpVORUE/vP9v8Sqm5ehsvEaNn72DjZ+9g52nP4/DI4bJC5Kvfo9ACzZvOlVxfTIQ2sAAD/bsBEfbPlvcXHn8N6XbLB10bt69SqOFxaKyf3m9VdfxeuvvoqXXnwRRqMRz2zYgJPFxeJi5AJ/OabS9PCanrrNt7zxMElcpyfX7Rrz/F5xz73QarV4ZsMGbHnf1rXE9vb6uvw4w7zeGDZsGF76xS88HgR+buNG/Om/beVfYJg9axa0Wq3NYP6OnTuhVqsxZ/ZsIEj2OXjZuooPRN1WJqKBjOdBoOJRIyIiIvIu8Zcj75zJ1+pf1iB7zAwkvZAtT8/ufAsz3lztVBB48egs7L9QgHv+tB7vHv4U7x7+FI/+769x+3tPiItSL58FgOfMnq2YpkyeLC5C1CfiRc2fL2xS+b81Oxtvvfkm1Go1duzcKS5GAcS9uk0Mpnpq8g5/Oc/mzJ4jT99duRJvvfk7fH/1any4dSty83LFxQOeeb3xyi9/iTGjR3s8ABwMbs3OhlqthmbfPnEWAODgwYNYOH++mEzkp3xd0xL5O/GuxNmJvE3MceY8BZLAKa/e+81HRETBJzCubRRsLvz0H9j42TuY8eZqcRYAQHM+HzNGTsTcG6aIs2QxEVEwtDrXg99zt/4AF376D9S/rMGFn/4Dz936A8X8FVOW4ODjW1D14i55mdeWr1UsI40n/NrytfJykkfnrsCpZ/7m991Q+ywAbIszY/7m5uXhgTUPYcGSxVh29/Kg6c4wNy8PP33+ebmL6G+tXGmxb0+uW4cFixfjS41GXnbZ8uX4V2/Q8Hdvv41ly5djweLF+Onzz6O2rk7x+dy8PDzw0EPyd/z0+ed92uL0yXXr8OS6dfhSo8G3Vq6U91sMZpRXVCjy5oGHHkJ5RYU833y/vrbcskxIYxju2LkTX1u+XO6a95kNGwAAz2zYoOgK1FeGqdXQarVAb/ekzz3/vLy9961caTU4/KVGgx889BAW9u77jp07sXbdOos8yM3LUywnzu8LR9v43PPPWx1TUzoOUvnMzcvDc88/b7dbW1v7ZH7c/PGYmnNuP3+Mtet+jB07d+Bry+/CwsWLLNLvW/kdLFy8CGvX/Ri1dbX4UqOR0+5b+R2Lc3rtuh9btIbNzcvFwsWL7AZIe47vz+TtuG/ld7Bj5w7A7GaxvKIczz3/M9yyeBEWLl6EHzz0IMoryhXr8YU1Dz6E6dOm4V87erYXNvfnenm1V34clXVfmj5tGoxGoyLN3vlu67x86+235S6TrY376mid4vJ/+etfsXDxYsV1aMfOnVhop4tiT1s4fz4OHjwoJuNLjQYGoxF33323nBYs++wqe/tojZRPJ4uLXfqc+wbyT9SBvO9EFKgCJ3BG5FhglGUGgYmIiMh/mAdL/3z/L5F3qRjvHv5UsYzkteVr8c0pPS2CD188Kc6WHSg7hrsn3mIRqBUlxahw/81L8dr+rdj42Tuob9bjifnfxshBQ+Vl7hw/B5catPj53j9i42fv4IvSPDw8+x6LAHRSjArT08Zh9lsPIOmFbKA3+Lvpa0/gRFUpNn72Dt756mMsHp3ldBDY2vbPvWEKHp27Qkx2m98FgB3JzcvD+o0bsGDefGze9CrWP/00Ptn+aT88ePSuLzUarN+wAYWFhVi2dCnu++Y3AQAfbN2K3739trg4Nv/mN4iPj8eypUthMBrx2ubN+Onzz+N4YSG+uWIF1Go1cg4exB/ee0/+jPQdCQkJeGD1atz3zW+isLAQz27caBEo7k/VWi3+56OPsP6pp7D51VcxTK3G5t/8RrFNz2zcCADY/OqrPcsMG4arV68CUpnYsAHz58/H66++ip88/TQ+/dSyTFRrtThZXIz/2boVOfv34+E1a/Cjxx4DAPzoscfw+quvYuzYsYrP9DeDwQC1Wg0AKC4uRmZmJl584YXerm3vwWubNysC319qNHjpF7+Q9/3FF17Ap9u34/z582Zr7cmjZ5zII1c52sZbs7Nx/sIFxTYDwOHcXCxYsAApycnytqmHDpW7tp0/f36furX1x2Mqcbyf13+wK8vqATn9/PnzOFlcjJ889RReevE/cP78efz8F7/AH957F4898ihef/VVxMfF4Re/fFn+jDssj++9vcf3eoB3Q++5+dqrr+I14dz0talTpyLHLPhne38qAITg4TUP40eP/RCwUn4sP2t5PvpKzldfYerUqfL/js73uXPmWD0vc776CnfecYciTeLMOsWusw/n9rxcUGiWfrK4GAsXLDBbyruWLFkCg9FoUZfkHTmCMaNHIyM9XZFuLlD32RWO9tGWaq0Wf9yyBavuvx+vv/oq/t+qVfhw61aHn6O+CIxHzkSBTmydysn9iSjYBEa59m4PUEREFDwC47pGwWL2qMl4+2BPa1lxyl+3Fd+cko3Rv75H/JiFe/60Hkcun8LDs++x2mJXkhyrwtI/rpW7iX5y++uIiYjC/8v6mrzMo//7a3zvo+cVXUkDwAMzl5utqWddD378Mi43XH/e/ezi1ci/fFr+/Ctf/gk7Tv8fFo/OUnzWmrk3TJG33zztszW/w7OLrbeOdofPAsALlixWTM620tv8299i2dKlWPPQg5gzp6cLzP+3ahU+2W797QFf+mDrVrnFqvlkzebf/AYA8NqmTfjZxo348ZNP4t3/+i8kxMfj7598YvGgfumdd+JnGzfiZxs3YtnSpUDvA+c3Xn8dax58EOufegoAFA+nf//eexgzejTefvNNrHnwQfz4ySfxzRUrYDAa8fmePfJy/U2r1eKN11+XuzV9et06GIxGxQN0rVaLb9x9t7zMr3/5SzkwI5eJBx+Uu0X9f6tW4dNPlWVCq9Xi0UceQUpyMgBgyuTJyMjIAABkZGRgzuzZ8rz+Vl5RgVc2bcL5Cxdw9/KeSua7K1fK+zRn9mx8t7dlXm5vgAEAtn30kWLf58yejc2vvy7Pl7zhZB65ytE23pqdjYT4eMU2l1dUIOfgQWQvWQL0btvCBQuw9skn5fWsefBBLFu6VPECgzP84ZhKrXulSarbXNnP62U1RZEOAI8+8gjmzJ6DW7OzsfTOpTheWIjHHnkUt2ZnY87sOVh1/ypoewPI7vruypV46MGHMHv2HMyePQcre4/v4dzr9bVWq8XX775b7oL5V7/8FcaMHesXDwEnT5qk+L+nvD6k6C4aAHJ796en/PQEBHvKzxy5/Dgq6/0pNy8PuXl5+FKjwdp16xAfF4d777l+k+TofL97+XKL8/JkcTG0Wi1uze55k03kaJ2Te7s6lwKttXV1OF5YiIULFuDUqVPyeo4XFrrYLbp7pkyeDLVajbwjR+S02ro6HDx4ECvuvVexrChQ9xlW6iFpEjnaR1u0Wi2eWreut97pOR++v3q1w8+RPWKt6cvak2gguB4k4ZlGRO7htZuIiAITr1zUH+beMAXJsSps+97LirF/k17IRv7l00iKUTkV/JXc86f1+NqWH6OsthIPz74H+eu2Klr2AsCF2kpFwFZqVTxZPdpsqZ6WuP/4wWbkr9uKqhd3AQASouIUy4jrGjloKJJjVfjfk8rGJseunEVMRJRFC2LR4Ysn5ZbEF376Dzn4m3/5tEv54CyfBYA3b3pVMTnTSq+2rg7aq1rc2hs4kmRmZMBgNFoESX1NrVZj+rRpFpMoNy8PBqMR06dNUzwkTklOxtI77wR6H86bmz1rlvz30CFDAEBuUYneMSLR+5AWvd+h1Wpx/sIFRTD6g61bAQAmk0leX3+bPm2aIkgntcgyP55qtRp/eO89xYsCKcnJPWVCq5WDiZIMK2VC/B5/ID2UX/3AAzheWIiXXnxRUQZ27NyJt95+G2vXrcPXegPDTb3HqrauDucvXLDY95TkZIwZM0b+35U86gt724jecrln7175/9zcXKjVasyZPVvetq+bdcMqyV6yBFqt1qet0/tCat0rTWPHjhX2Uzk+7/X9rJXX0VNWLYO/Y8aMUaTHxsUCvYF2SVxvWlOTskvgvugGsGPnDrz19tv48bof42vL7wIAmEzXx1pQq9V49733FF1JW9t2X9xQNjVZ1mvS/qw1258ms/2xx1FZ7y/PbNiAZzZswEu/+AXUajX+9N//Lddtzp7v4nm5b98+TJ82zWqLWGfWmZGejjGjR8uBz8LCQkyfNg1z58xBzldfAb11ularxZw5cxTr8bYV99yj6Ab60KFDMBiNmDdvnmI5c4G+z2I9JE3mnNlHW6yVlcmTJjn8HNniixqSaCC73jqOZx8RucLyQbm/1iJsBUxERM7z16sZBYepaWOxq+SQ1eBmTVMDRv+6J4jrSvfHhy+exO3vPYGHPn4ZMRFR2P6AZYM4R/Y+8g5W3bwMAPDpyX34+d4/iotY9bUb5wMANn3tCUVL5k1fewLo3V9nSPkhBX9vf6/n857mswCw1IpKmpwJzJWeLwUArN+wQRHEXN87ZqO/dDsqWXrHHXj7zTctJlfExfW8cXDt2jVxlgUpEGzPmNGj5W6UzSdbrb78xeubNmHs2LFYv2GDYozgc6U9ZUIar1OapHE8/a1MiKSH8v/1zjv4+1//qjgOr2zahN//4Q8AgG98/et48YUXzD4JlPbuuyPSct7II0fbiN7Whubdze7Zu1fuZtaZfXBmGX9irW5zZh+cWaY/dQP49aZfmx3fb1g9vq9u2oRxY8fi2Q0b8O2V34HGTrfd/X1DWV5RLnepDgCvOLE/tjhT1vtLzv79yNm/Hz967DHs2r1b8WKMs+f77FmzFOdlzldf4fbbbpPXY87ZdU6fNk3udSLvyBHMnTMH8+bNg1arRXlFBYqLi6FWqy0Ch942Z84cGIxGeczmw7m5WGj2wpQ1Ab/PQj0kTeac3UdX9fVzRET943qr3/6+LyGi4CHVIf5dlzAITERERL737uFP8b2PnheTAcBmurM+PbkPHx3bjdEpI7BiirKBgz0rpizBjJET8c5XH+OeP63HK1/+yeb4xKKiqp7naR+f2IuNn71jMX12pqdRiDNG//oe7Co55LXgL3wZAO6LoUN7mnL/6LHHLAKYm/1orE9PamrqaZnmyYfH4gPhObNne3T93pCRno6fbdyI//ngA0yfNg3/8Ytf4HBenqJMiC2dpNaX/kzKf7F70JPFxdi1ezd+8vTTWPvkk3I3m+aklwMc8VYeObONMOuCNTc3F+UVFTh/4YIc6Ja2zZ6+bp8/CcT9LO49vuuf/gnWPvkksnu7mBZlpGfgpxt/ig97z82XfvFzRWtgX/p8zx4snN8z9ur18tqzP1KX2Y6FOF3W+9t3V67EwgUL8MZvfyu3lHf2fL81O1s+L7/UaNBkp0Wss+uc1RtUlrpYnjx5ck+PBKNHo7i4uGcs3Pk9b8n1p4z0dEyfNg2Hc3NRW1eHnIMHHb70FOj77Axn99FZ0v2Kq58j/31sTERERM7x31bBHBOYiIic409XL6K+qNbrxCSbBscnAQD2nc+X05wNIB++eBJ1Jj0SouLk8YPNJ/Puop3hbhDckcAJAIf0PMRVq9UwmUwWAcw5TrYi9kdzZs9GQnw8jhcWKrp6rq2rw+7PPwcATLPSdbQrxo4di4T4eJy/cMFivOVfbdqk+N/fmHcBLAWCAaD41Cm5TDQFWZmQHqRnZmbKaWI34FMmT0ZCfDyOmI1tid4uR83HfvZWHjmzjZIV99yDPXv3Ire35Z30woG0bZp9+8SPQLNvH8aMHq3Yvq96u1WV1NTUKP73VxnpGU7sp2W3yZ7kSt51AzD2diGdkdkzpjJ6g8LmzLutlgLBABTjn4r66y35Vzb9Gk1GI+6//3uAWZfYmWb7Y6u8ilwp6/3tJ08/jSajER999BHg4vm+cP587Nm7F3lHjiiGEBA5u845vdey7f/4B+Li4+UXW6ZPm4aTxcU4XliIScK4zP3l9ttuQ87Bg9j+j38gIT7eYQA4GPbZEWf30Zrz589bdM+fd+SIRZ1N9vRXbUhEPTjmLxF5g60u5f2/fTAREZGIVy7yd/nrtuLP9/8Sj85dgUfnrsBry9fiifnfxoXaSnmcX2d8duYrNLe34hd3PopH567Ac7f+AM/d+gNxMZs+OanBsgnzLLZl7yPviIv6XOAEgHutXrUKH2zdii3vv4/cvDzk5uXhXzt3+n0Q05EfPvYYAODZjRvxq02b8Lu338ajP/oRDEYjnl2/3u0HqinJyfjmip5+1H/+8sv43dtvY8v77+PJdeuwa/ducXG/Ulpaip8+/7x8vP/8178CveMNordMfCiUiR07d+IVJ8qE1FLpyJEjfhPQgVnA/i9//Sty8/LwpUaDP27ZIi6GFStW4O+ffKJY7hcvv6zo9hZu5hF6x5A2n04WFzu9jejtgvX8hQvYs3cv5gpjYT72yCPYtXs33nr7bXn9W95/H7t278ajjzwiL3f7bbfh/IUL8vft2LkTW7dtU6wLfndMrz9sfOyRR832Mxe5ebnY8v5/W+ynNyjzLhc7du6wmnfmxo4di/j4ePy19zMajQZ/3KIcC6G0tBTPPf8zeX/+0ntuOhPw8uQNpfT9Up7et/I7OHjwIF7d9KocWFeW155Wr+L+SMsBwJEjR+Xy40pZ728pycn4f6tW4e+ffCJvr7Pn+5IlS3D+wgWUlpZajAMrcnad06ZNw6effqpo9Tpr1iwcLyyEVqt1GHj1Fql186effooFC3pahTsS6PvsDGf30Zr1zzxjUWevuv9+cTGyypM1IBE5ZitAQ0TkCYHwgglbARMRkfP893pGBCwenYVNX3sCm772BO66cT72XyjAvR88Iy5m1+WGq3jnq4+RmTICm772BB6a9Q288uWfxMVsenbnW3h9//9g9qjJ8rbMu2Eq9l0oEBf1Of8OAFu5R/368uX4+YsvYveePVi/YQPWb9iAw7m5mDNrlrhoQJH2a+jQodi1ezf+/skniI+Lw89ffBFfX75cXLxP1jz4IH702GOIi4/H3z/5BB9s3QoA+PmLL4qL+hWpm0rpeO/Zuxcvvfgi5vR2wXr38uV46cUX8fmePXhmwwY801smZjtRJlKSk/Hs+vXY/fnn+NETT/hBwLBHSnIyfvL00zheWIhnNmzAH957Dw+vWSMuhjUPPojvr16N/9m2Dc9s2IBtH32ERx95BMOEALA7eYTeMSLNpz9u2eL0NqK3pdnCBQtw9epV3C2U51uzs/HSiy/K63lmwwaUlZXh9VdflY8xevfhvm9+U97XvV98gdWrVinWBT8+pj37+R84Xnjcyn460xVx3929/G7c981v4X+2/Y/NvBNv7lKSU7D+6Z/geGEhnt2wAX947108vOZhxTLSufnshg14dsMG7Nm7By+9+B9O74/4nX1lXja/+uor3HnHHfifrVsVXaunJKfgJ73701NeLfdHWq6n/OzGj554HCeLi6181nZZ94XvrlyJMaNH4ze//S3gwvkudc9ubGpSnGvWOLvOub3j7Zq/BDBn9mxotVosdDLw6g0pyclYuGABDEajRR1kS6DvszOc3UfRmDFjsOLee/HGb38rn3cvvfiiXwe7iWig4pi/RNRfGAQmIiIiMlf/ssapaXTKCPGjVs14czXSfrEMSS9kI+mFbEx6/Tv43kfPK7pdnvHmasx4c7XicwCQ9EK2orvlV778E0b/+h4kvZCN0b++B5+e3GexjK11Qfh80gvZWPCfa1wKIveXEO3lSt6fUkDw34Lqf+5buRJ33nEH1jz4oDjLZ9auWwe1Wo3nervwDn6BVYH56vwKrFyS+Cq3iHxv7bp1AIC33nxTnNUPArPGUGL9QdS//D0gQ0TB5Xptc/2uxR/vX1grEhGRY9auYLyCkOjGP/w/MYk87Mxj/yMmOc0/WwBf70GHCODFxSW5eXnQarUOW3D1J2lcYmdb3gW+wKnAfN0ixtff3zfSRSpwjjMR+Vpg1nZEgev6dZpnHhH1H/H3gfg/ERFR4OCvWKLA538BYN4fk4AXGtv+8te/Wozd+IuXX8b0adMU3d/6Sm1dHXLz8vCLl1/GwgUL/GKbvCuwgoL+dG7507YQEXkWazii/nX9XoxnHxH1v0B4WdSft42IiPwN76mJApd/BYB5D0oCXmDsy8jIwFdffSWP3bh12zasWLEC/+En4zpv/8c/8MyGDRg2bBh+8vTT4mzyIX88t/xxm4iIiCiQXG/1y/sKIiJ7+ACOiIiI3BcZFiEmkQdFhIWLSS7xrzGAef9JZvynYBI5K3AqMX89vwInB835a24SBZvArCFYRxD1p+sBYCIiXwucOxfWmkRERNQ3X//4pyitqxSTyUNuSFRj93dfF5Od5l8tgIl68ecH0cDEFjtERETkuuvdrfI+goiIiIiIqH/88OZviEnkQY/PuEdMcglbAHvY2n/9Bp+fyxOTA8Kd42bjra/7vpte/ymQRK4KnEosEM4z5iYRKQVOraDEOoLI+xj8JSL/FRh3MKxBiYiIqG9+svc/8dmFXDGZ3HR75ky8dcdaMdklDAB72PjN3xGTAsrZ9X8Tk/qV/xRGor4InEosUM61wMjRQMlNokAXGDWCJdYRRN7F4C8R+b/AuIthTUpERER982V5Pl7P/RsqDdfQ2dUlziYnhYWGYkTCEKyb9S0sHT1bnO0yBoA9jC2A3eM/hZHIVYFVgQXKuRYYuRoouUkU6AKjRlBi/UDkfQwAE1FgCJw7GdaoREREFKz8+Y7M8/dg/hEA9uc8p37l+8JI1BeBVYkF0nkWWDmLAMtdokATSDUC6wKi/sMAMBEFhsC5k2GNSkRERMHMX+/KPH8P5rEAcHd3N7q7+7Aqf81r8ok+lCAiHwq8CizQzjHmMBFdFyg1AusBov7FADARBZbAuKNhrUpERETBzB/vyHrvv0JCEBrime1zKwDc3d2Nzs5OdHV1yQHg7p4Z4qLWeWYfKIg4WXKI/ETgVWKBdo4xh4noukCpEVgPEPUvBoCJKPAExl0Na1YiIiIKVv55NxYSEtI7AaGhofLUV30KAHd1daGrqwsdnZ1ISk1BTGwswsPDEeKhqDQRERERERERERERERER0UDR3d2Njo4OmEwmNNTWIiwsrM+BYJcDwF1dXWhvb0f8oEQMSkrq05cSEREREREREREREREREZGlrq4uNNTXw9DYiIiICJfjsU4v3d3dja6uLrS1t2Nw2jAkp6S4/GVERERERERERERERERERGRbaGgoklNSMGTYMLS1t6Orq0tcxC6nI7jd3d1ob2/H0LRhiImJEWcTEREREREREREREREREZGHxMTEQD1sGNra2tDV1YXubuc6dnYqACz1OR2XmIhoBn+JiIiIiIiIiIiIiIiIiLwuOiYGCYMGobOzU5xlk8MAsNT1c3d3N5KSk8TZRERERERERERERERERETkJUlJSUBICDo7O+FMG2CnAsCdnZ1ITE7mmL9EXlBUVCQmERH5BOsjIqLgwTqdyDaeH0TBgecyBROWZyJyBusK1wVTnoWGhiJRagXc3e2wK2i7Ed3ubqAbQEdXF2LiYsXZRERERERERERERERERETkZTExMejo6HAY/IWjADDQ0/1zV0cHIiIixJlERERERERERERERH5j7969qKysFJNdVllZib1794rJREREPhMeEdETt+3qEmdZsBkAlqLH3V1d6OzqQkhIiLgIuaC8vFxMktmbR0RERERERERERETOu3jxIg4fPuzWdPHiRXG1REREPhUSEoKuri50O9EFdIj2cqXVJaQPtrW3w2RqwoTJk8VF/EJdXR20Wi06OzsRFRWFESNGIDbW/7qrLioqQnp6OlQqlSJdr9ejoqICU6dOVaTTwFFUVMTjT0R+gfUREVHwYJ1OZBvPD6LgwHOZbNm7dy9SU1MRGRkpznJJW1sbdDodbr/9dnGWx3mqPBcUFODSpUtislNGjRqFrKwsMZloQCooyEdZWRmuXbsmp2VkZGDMmLEYN26cYtn+5Km6wtyFCxdQW1srJvtESkoKRo8eLSa7xRt55munTxYjISEBYWGhCA212c7XfgC4u7sb7e3taGpqwo1Tp4iL+Ny5c+dQXl6OsLAwREREwGQyISwsDFOnToVarRYX9ymtVovS0lIsXLhQkZ6Tk4OxY8f63fZS/wnGCoiIAhPrIyKi4ME6ncg2nh9EwYHnMtly+PBhZGZmYujQoeIsl1y9ehVlZWWYO3euOMvjPFWey8vL8X//938AgMzMTHG2TZcvX8bIkSMtnl1T8KusrERcXBySkpLEWQPOuXPn8M9//gN79+5BU1MT4uPjkZFx/TwqLy+D0WjE0KFD8fWvfwNf+9pdGDJkiGId3uapusLckSNHcOXKFSQkJIiz+pXBYMDw4cMxa9YscZZbvJFnvnaq6KQcAA4LCxNnyxwGgNva2tBkMmGinwWAL126hOLiYqjVaowdOxYA0NLSgvPnz8NgMGDBggV+1xL4448/xtKlS+VWwHq9Hrt378a3v/1tcVEaQIKxAiKiwMT6iIgoeLBOJ7KN5wdRcOC5TMHEk+VZCgKr1Wrceeed4myrNBoNEhMT2QJ4gLl69SqKioowaNAgzJw5U5w9YFy7dg1///vH+POfP0JGRgaWL78bU6feJMedzB07VoAjR45Ao/kSJpMJ3/3u9/DAAz8QF/MaT9YVkiNHjkCv1+O2224TZ/WrL774AiqVigFgJ1wPAIchNCwUtgbwtd022JyDfqR9obq6GklJSYqTMDo6GpMnT0ZoaCgqKioUy/uDxMREnDhxQv7/xIkTSExMVCxDRERERO4pKioSk4iIiIiIiAaEjIwM3HLLLdBqtfj888/F2VZlZ2cz+DsAabVaREZGoqGhAfX19eLsAeHcuXN4+ul1+OKLvdi48af4058+xDe/+S2rwV8AuPnmLDz22A/x8cf/i+XL78Zf/vJnrF//E0VX0UTe5sz4v3C6BXBTEybe5NsI+fHjx9HU1CT/39jYiDFjxiAtLU2xHACcPXsWdXV1ihbAQ4YM8Wnf7ABQUlKCvLw83HvvvQCA7du3Y/bs2ZgwYYK4qNMqKipQVlamSMvOzlb8T/6tL2+gdHV1wWAwoKWlBS0tLeJsIkRGRiI2NhYqlQohIdbfAQrmcuTM/pOlvtRH5Bs8VvYxf4j6dh4E870BBae+3vP15fzoLwUFBVZfaDeZTGhqarI7xpc9XV1dGDx4sJgMg8GA6OhoREREiLOQnp4e0MEAW3lpTXt7O1paWpzu+tBevlnjq7x0JQ+8zRt54Mlz2ZVxU71dXjw5DqsrZcDb++XJMuDMfplMJoSGhiI6Olqc5ZSWlhZ0dXU57GHSU/vlyfIs6UtLYFccOnQIADBv3jxxllcVFRVBp9PJ/6tUKsyYMUOxDDlHo9Fg5MiRqKqqwtChQ92KUwSigoJ8PPfcT5GenoH/+I+XrN4rOXLsWAE2bfo14uPj8cYbv/V6l9DeqCvEFsCHDx9WxOIciYuLk7vKd+ezbAHsvOITRUhISEB4eHhvC2Dpt5Ay3OuXAeCSkhKLBw4VFRVISkpCXFycnKZWq622oK2qqoLBYJD/v3r1KsLCwizG2R00aBDS09MVad62fft2pKamAgB0Op0cDO4LaxdZ6ebHmf2qqKiATqfjBdLHXK2A2traUF9fj6ioKERERKCrqwtdXV3iYjSAhYb2DP7e3d2NxsZGpKamIioqSrFMMJcjZ/afrHO1PiLf4bGyj/lD5Pp5EMz3BhSc3Lnnc/X86E85OTkoLy/HsGHDFOmNjY3Q6XRWn4E40tHRAaPRiDFjxoizcOHCBQwePFgeqkpSXV2NjIyMgB4L0lZeWqPX61FTU4PRo0eLs6yylW/W+DIvbeVBS0sL9Hq9xx9SX7t2DSqVyiLg5q088OS5bCuvrAmk8jKQ96uyshKRkZF9LufXrl1DW1sbRowYIc6SeXK/PFmezXkrCKzVauVGSZmZmRbP3R3p63Pp/Px8AFB8zlt5F+ykhmXZ2dk4ceIEGhoasGjRInGxoHXt2jU8/fQ6DB2qxqZNr4qzXVJTU4PHH/8hRo8eg82b3xBne5Q3yrsYAP7iiy+A3pcrHNHr9QDgsc8yAOycgA4AHzhwADqdDpGRkXJaY2MjJkyYgPHjxyuWdcbBgweh1+sRHx8vp7W2tiIzMxPTpk1TLOttUitgAG61/i0qKoLRaHTrDau+XmjJs1ypgDo7O6HT6aBSqdDW1ibOJrIQGRmJxsZGDB48WB4QfiCVI2v7T7a5Uh+Rb/FY2cf8IXLtPBhI9wYUnFy953Pl/OhvOTk5qK6uxrJlyxTpFy9exNGjR3HzzTcr0p1x7do1VFVVYcWKFeIsHDhwAGPHjrXoXW3Xrl0YNmyYR4IavmIrL62pqqpCaWmp0w++beWbNb7MS1t54Or+OstWvngrDzx5LlvLq5CQEISGhqKzs1OxrKv5ZytfrPF0XlnbL1uCbb+OHTuGuLi4Pj1LRm8Pk01NTXbrXU/ulyfLs8gbQeCioiJERkbK946ubntfnksbDAYcPXoUM2fOdLqlOtl29OhRhIeHY/r06aivr0d+fj6mTp2KoUOHiosGpfXrfwKtthqvvba5Ty1/RceOFeDFF1/w+pjA3qgrrAWAnQ3E+uqzrvBGnvma7QAwFEHgvvUd1A9UKhXGjx8vT8nJyeIiTouNjcXgwYMxduxYeXL2zWBPmzBhAmJiYhATE9Pn4C96Ww9nZmaKyQoajUbRElqr1UKj0QC9b0uVlZVBr9dDo9GgiGPlBYSmpibExMTwwRw5ra2tDbGxsYquNwZSObK2/0RERKQ0kO4NKDjxno+IPC0kJATR0dGIjY1FeHi4OJsooPRlTGBHdDodhg8fjiFDhii6Y5b09bl0SUkJNBqNPJnPk4K+tbW1cprI3vei97tLSkqQn58vf4dWq4XBYFB8r7dZ68LcYDBAq9WKyV7R3NyMhoYGJCUlAQCSkpIQGxuLqqoqcdGgdODAARw+fAgPPrjGI8Ff9I4NLI0JzPGAybdC5MlvA8DBSq/Xo7m5Gc3NzXITd1dJFwJXu9YwN2PGDGRmZkKlUiE7Ozvo3oAIVs3NzS6NbUUEAGFhYTCZTPL/A60ciftPRERESgPt3oCCE+/5iMhTpOCvFPiNiYlhENgKsatv8m+eDAJXVFQgOjoaCQkJUKvViI6OthrQtMXWc+mioiJUVVUhOztbnoxGoyIInJaWhrKyMrcaM1VVVWHEiBHIzs5GWloaTp8+jZMnT8rfqVKp3Fq/IwaDAWVlZfLwjlLa0aNH5W61ve3ixYsICwtTDCOZkpKC+vp6xXLBaseOf+HWW2/1SOt9c4899kPExsbis8/+Lc4i8omACAAPGjQIkZGRqK+vx7Fjx1yeTCYToqOjFV1A+8qJEyegUqmgUqlw4sQJcbZTxPGRaeDgsae+6OrqQmtrq/z/QCtH4v676s9//jO2bNnS55d2Bprt27djy5Ytbk3bt28XV0t9ZO3t4ZKSEuzcuRM7d+5ESUmJOJucsH37duYdBZWBdm9Awcndez4iIgjB36tXr+Lw4cNobm5mEFgQHh6O2267zaWWc30Zw5z8k06nU/TWmZycbLUVsKt0Oh0mTpyoSMvMzIROp5Nb9U6YMAEzZ86ETqeDRqPp0++y1NRUuWHV8OHDgd7Asvl8o9Eo/+9pCQkJyM7OBgAcOnRIDv6mpqa6NdyjK2pra+XWv5KhQ4eis7PTajC/oKAAn3zyicemgoIC8Sv6zblz53D48CEsXtxzDDwtO/tW/Otf/xSTiXwiIALAMTExGDJkCJKSkhAXF+fyNHjwYKSkpPj8Rk2v16OsrAw33ngjbrzxRrmrCyJXdHV1iUlEdlkrM9bSgpU7+1pSUiK3JCktLRVny44fP253vrecOnUKzc3N8v9Xr171yXaYmzZtGhYsWODWNG3aNHG11EcajUbxdndRURHy8vIQGxuLiIgIHDx40O23v4koOLhzvSTyByzDRNa1trbi7NmziunSpUvQ6XQoLCz06KTT6XDp0iWL7wuklzPMg7+nTp1CdHQ0YmJixMUGtPDwcDlPkpOTnXreOm3aNPY+6GOeGgfYYDBAr9fLgVP0Nt7S6/WKrpddZavHS+l/82EepADqxIkTUVVVhfz8fLNPOBYZGSn/LXUr7YsW7VKwVwr+9tc5Ul9fD5PJhI6ODpw6dUqeqqqqEBYWhpqaGvEjMJlMaGpqkhu2uTM1NTX5tNeWEycKER8f7/HWv5JZs2bh6tWrOHfunDiLqN+FmnUHbX/ysYyMDMWYwK5O5m/x+IrU+nfChAmYMGECVH1sBZySkgLYaNVDRESec/HiRahUKqjValy4cEGcDfQGf+vr61FRUdGvwVdpvJZjx46hublZfkDhzbdUnZGRkSFf5/o6ZWRkiKulPpo7d66ii6+SkhLccsstyM7Oxp133olbb70VWq0WOTk54kep9yFJSUmJ3Rf2SkpKeE9GRERENsXExLjUStLTOjs70dTUZDG1trbiypUrHp1aW1stvqepqQkRERE+zQNnRERE4Oabb1YEf5OSkjB9+nSg9/dXR0eH+LEBRwr+mkwmnDx5EnCii+zIyEiMGzdO8RnqX54K/gLAlStXgN6gpTRe7unTpxXz+otarcbMmTOh1+sD9jfZvHnzkJaW1m/BXwC4dOkSwsLC0NHRAb1er5iioqLQ0NCgaGwgiY6Oxpw5c9yefBFsN1dRUYHJk6eIyR5z881ZiI+Px/nz/feMkAaibrNJ/P/6FBAtgIOBeetfSV9bASckJEClUqGyslKcZcH87Sh27UZE5DzpB8SoUaMwbNgwqz8opODvpEmTkJ6e7rUgsLUAU0xMDG6++WYAwLFjxyweUAxUUsDOnam8vFxcbcASx3mKjY1VBNgzMjIwefLkPt2PBLs///nPKCwsxJkzZ7B9+3aLctHQ0ICPP/4YZ86cweeffw6NRqOYT0RERANbSEgIIiIicPfdd2PChAni7H4TGxuLm2++WTGNGTMGUVFRmDhxokenqKgojBkzRv6erKwszJkzBytXrvRpHjhjzpw5GDNmDIO/DkRERABmv5elblxtBYEjIyMRFRUFk8mEgoICNDQ0+LTl30DkyeAvANTV1SEzM1MxTq80lm5dXZ1iWVeeS8fFxQFWGjzZahkskVrwmnPle/1Bf9ePDQ0NSElJwdy5cy0m6TnTxYsXxY8FjbKyMsXYx96QkZFp8QyByBdCtJWVUohYobu7G93d3Whra0NTUxMm9uNbKAcOHEBbWxtuuOEGAMCwYcPERfpEai2F3q48hw8f3m/dTObk5ECn0+Hee+9VpG/fvh2pqakudzkgjQ2gUqkwY8YMOV3qoz89PR35+fmIjIyU3yA6dOgQWlpa5DEGKioqUFZWJv9PvlFUVOT0W14XL17EoEGDxGQihxoaGuQ6dSCWI/P9d1ZBQQGOHz+O5cuXIzY2Fh9//LH8Iwe915TCwkJkZmZi6NChQO+1xWg0ejQIW1RUhCNHjkClUuHb3/62OBvNzc04duwYYmNj3f5eV+ojf7V9+3bU1taKyS5JSUmxuF77G1ePlfSjPyIiAt/73vfE2diyZQsWLFjQ7z88vcXV/LGmvLxcDpZrNBqYTCYsX74c6C1n7e3tWLp0KVQqFfR6PbZv347Zs2cHTR5S4HPlPBiI9wYUnJy953Pl/OhvOTk5OHr0KMaNG6dIv3r1KpqamhAa6vg9/u7ubotATFdXl1N5Izl37hxmzpzp8rMKf2IrL60xGAxobGxEbGysOMuqlpYWREREICwsTJwF9AYysrKykJ6eDr1ej8OHD6OqqgoxMTFYuXKluLjX5OTkoLq6GsuWLVOkX7x4Efn5+fKDfk85duwYZsyYgRtuuAEhISGIiYlBWFiY1/LA0+eyteDvv//9b4vfF52dnWhvb3e6FZvJZEJERIQcPLXHaDQiPDwccXFxCAsLczuvcnJycOrUKUVaa2sr2traFGnorTu6urpslmv0vtgwc+ZMLFq0CFqtFidPnkRycjKysrIAIVguBn8BICsry+nzzB5nzm+tVut24D48PNxm4BEeris9XZ7hheCvVqvF6dOnMXPmTIvAq/SseuLEiVCr1X16Ll1UVASdTqdIO3ToEJKTkzFhwgQYDAaUl5cr8qmkpARVVVXyZxx9b35+PuLj4xW/2zQajbzd6N22qqqqfhuPtz9JDRdmzJhhMQaw5Pjx4zCZTJg/f76cVlRUhNzcXEyaNMmtclpUVIRTp05hzpw5bq3HHT/84WOYOHEiHnvsh+Isj3nyyScwZcoUPP74E+Ist3mjrjhy5Aj0ej1uu+02AMAXX3wBlUqFWbNmiYta8NVnXeGNPPO14hMnkJCQgPDwcISGhdnsxDnoAsD2bsA7Ozvlt350Oh2SkpLk7pS9paKiAhcvXoTBYEBcXBzmzJkjj5PR3NyMgwcPwmAwICUlBTfccIPLb5/k5+crWuxER0fLFyfpwivJzMy0uLBKF8H+HGeAlFypgGw9nGuuPo3TVeZdcyQjMysD1i/jSvXlBaiOnoiJw3rKZX15Acrqrn9enO8scT3kW84FgJtRffo0WoZlIcPqQXM03385+zDQ3Pbt2wFADgR+/vnn0Gq1+P73vy8s6V07d+6EXq+Xg0/Wfnw2Nzd7ZFwqV+ojR0pKSnDw4EEx2a5gCkB6W1+Ola0f/3q9Hh9//LFcvvbu3av4HADcfvvtYpJf60v+WFNSUoKmpibodDqYTCa5Pti+fTuGDRuGOXPmyMtKLaztPfwRH0ZIioqKYDQaLR4wFBUVAYDF8t4i3lea471i4HHlPLB9b0AUWJy953Pl/OhvOTk5KC0tVTx0RW93jefPn0dycrIiXdTa2gqj0YhJkyaJs6zeR5aWliItLU1ueSX56quvMHbsWLvXNX9nKy+t0Wq1uHDhAkaNGiXOsurSpUsYPHiw1XvwqKgoTJ48GUlJSSgqKsKxY8cQERGBIUOGoKysDI8++qj4Ea/xVQB49OjRiI6ORkhIiFfzwJPnsrXgb0lJCaqrq8VFFbRaLSIjIzFo0CB0d1t9xAqDwYDo6Gg0NTWhra0NQ4YMEReR6fV6hIeHIzw8HPX19bj//vvFRVyi1WrlxjCSkpIS1NTUQKVSKdI7OjrQ3t6uKNdtbW3yc0tJdHQ0Fi9ejMTERJtB4NDQUK8Ff+Hk+X3o0CFERUXZDHI5Ul9fj9bWVot7dHOerCs9WZ5h5/efO6Sxds0bI5kzn9/X59JSQFeSlpZmEaw1Z/4sHE48Dx/oAWBrwV2RrSBxQUEB8vPzMXny5D6V1aKiIhQXF2PGjBlyfeELDABbcicQ66vPusIbeeZrAzYAHB0djQsXLlgdrNxV7l68m5ubcfjwYaSkpCAxMREXL15Eamqq/EPs1KlT0Ol0uOGGG9DY2Ija2lrMnTvX6g8ICl6uVECWD+d6AnJVzUKgtb4c5chwKkjnKMDraD4FBkcB4J6Afc/fyZmWAV5H8/2dsw8DJVqtFjt37sT06dPlm9Ki3pa4s2bNcvqcdZf5dhQXF2PkyJFe7bXBlfrIEb1er/jR5oy0tDSLhxBknTPHqqCgAMXFxWhvb5dbr5s/BJg7dy5MJhPy8/MREREhPxSQhpioqamBTqcDBmAAuLy8HIcPH4ZKpUJiYiLa29vR2NioCADfeOONiocG0jjK9u4frb3lDrMHH+Kb9IcOHUJaWprLLwh6gqeDzxUVFdDpdDYfFpHnuXIeWLs3IApEzt7zuXJ+9Dd3A3bXrl1DVVWV072ZHDhwAGPHjkVaWpoifdeuXRg2bJjd65q/s5WX1jibv5L8/HyMGjXKIpCXkJAg9yCSk5OD06dPIzMzE3PmzEFubi5aWlpw9913Kz7jTbbywNX9ddaxY8cwe/Zsefgzb+eBp85la8Ffo9EIg8EgLmrhwoULCA0NRWJiIjo7O8XZAIDa2lrExcWhuroazc3NmDhxoriIrKamBlFRUejo6MCVK1fcDgBb89VXX+Hy5csW29HS0oKmpiZFsPfatWu4dOmSxT1cWFgYRowYYTMIjN6Wz94I/sJO2Tb36aefIiYmps8vGZeUlKC5uRkrVqwQZ8k8WVd6qjyjj8FfjUaDxMREnwbmyLukxmgjR450eF5oNBqkpKTgpptuUqRLQWCpXndWbm4uysrKfB78BYCXXnoRBoMRmza9Ks7ymOXLv4Y1ax7GffdZ9uTnLk/WFRJrgVgATj2jk14i99RnGQB2jrMBYMd9BwWgmpoanDt3DtXV1X2aLl26hDNnzoirdVltbS06Oztx0003IT09HampqYpWFXq9HqmpqUhPT8dNN92Ezs5Oi25liOxpri5HFdIwUWxlm+Rc8JcI6HlhoKe1diastidwND8InT59GgAwduxYOW3q1KmIjY3FpUuXzJb0roqKCkRERGDs2LEYOXIkLl++LC7it1QqFSZMmODS5MzNITmnpKQExcXFmD59OmbNmiWPAWw+JvDHH3+Mw4cPIzExUfFQYMSIEWhuboZOp0NqaqpivQPFuXPnoFarsXz5cixcuBCJiYniIhYtKXQ6ncNu/aSHaebjWhkMBrS0tCA6OlpxHyile7u3GiIiIvIM8+Dv7t27UVpailmzZmHOnDkwGo2orKxU/L4IRqmpqXLwN1DyQAr+RkVFYfDgwaisrERlZSUaGhrQ2dnpcMrKypKP+0DS2dmJyspKNDY2Qq1WY8qUKairq5MDvt4M/pJ9UvAXvWOA5+TkODVptVqOzxzkamtrER8fLw9jZs/QoUPR1dUlJiMrKwszZszA5cuXsW/fPnG2Vfv27cPly5f9IvgLAOnpGSgruyAme4w0PFxmZqY4K2BIPcPo9XqHk/ny7n6WPC8oA8DovfFetmxZnybxDbi+SklJQVhYGE6cOCG3ejB/uK1SqaDT6VBRUYETJ04gLCyMD/nIBfXQVjUjedgw2G2b21yN0wUFKJCm09Uw7yxaVF9egNPVlks0V5+2sY5mVJ8uQHl9PcoLClBQUI56O+shz6q20h2VyWRy7WWSpAxkiS8RmHM034c8sv9WaLVajBw50iIgqVarodVq5ZsUbysrK4NarYZKpUJGRgba29vlVnlkn16vR0lJiUuTJ45reXm5xXpdncrLy8XVuuzMmTOYPn06pk6dKrdMaWxsVASBIyIicOONN1q8rV5aWoqKigqkp6dj8ODBinm2VFRUiEkwGAyKQGegkR5+6PV6qy9+XLp0Sd6/goIC6PV6h/eQCQkJiI6OVgSPa2troVKpEB8fryiDtbW1iI6OllsEHzp0CBUVFdBoNHK3ZwaDQf5fo9Hg0KFD8ufR2zqppKQERUVFNpdxVUlJieI7pZYx0neYO3ToEIqKipCfn4+ysjLo9XpoNBrWY0TkMm/d8xF5ihT81fcOrXHlyhXMnj0bY8aMAQC5ZxFHLa4CWUJCApYvXx5weVBWVobOzk6YTCacOXPG5Wkg10P2gsAM/vpOXV0dVCqV/NzZ2SkmJobHKsiNGDECc+fOdapb9EmTJsk9IoiysrKwZMkS6HQ6h0Hgffv2QafTYcmSJX4R/AWAKVOm4Nq1aygtLRVneURR0QnExcUhKytwe7+aO3cubrvtNqenuXPneuSz5HlBGwD2BzExMcjMzERDQwNKS0uhUqkUb35kZmZCpVKhtLQUDQ0NyMzMZPfP5Lz6BtQhGYMcXLObG1qQNDELWVlZyMqaiDRU4XR5vbiYXc1Vp1GODLvraK5uQPTELL8NFAYjk8mEqqoqnDx5UpF25swZl7veDUTe2v+ioiKYTCarww9Ib3ZLLYS9qby8HCaTSe7GMCMjo99bIAeyqqoqHDx40KXJnXIjKSwstFivq1NhYaG4WpfFxsbK3dv83//9H8aPHy+3/JWCwPfee6/FAzjz4K+zrTMMBgPKysoUgUVp3KWysjLFsoFi3LhxMJlM2LJlC7788kuMGjVK0Qo4MTERo0ePhkajwZYtW3DhwgXccsstFi+NWJOcnAyj0Sj/r9PpEB8fD5VKpUjX6/WIj4+X/0fvA8qZM2fKXUhfuXJF/j87OxuRkZEWwdWqqiqoVCrFMtLYXK4q6h2rWFpXZmamPL7W1KlToVKpUFJSApi9FDB16lTMmDFDvu/Nzs4Ouq6XiMi7vHXPR+Qp5sHf3bt3o729HYsXL5bHEz5z5gxqamo83t2yPwnkPJg2bRpiY2MRGxuLBQsW4Pbbb3dpGjFihLjKAUUKAre3t0OtVmP8+PGoqalBS0sLg78+kpWVhXvvvbdPk78E6Mj/ZWRkYMmSJairq8P+/fvF2QCA/fv3o66uDkuWLPGrnhKysmYgIyMDO3b8S5zlETt37sDtt98hJhP5RFCOAZybm4tqB+NA2HP+/HkcPXoUjzzyiDiLyONc6YNeMT5bfTkKyqAc+9cZ9eUoqI7GxIk9LYfFMX6t/V+GTGSZ9yndXI3Tp+uRNHEihsX0jENcn6QcJ1hcD3mP9DBs9OjROHPmDBITE+W3rCWOxgDuUY/ynkJlowtxR/N9w9X9d+Tzzz932NWySqXCt7/t+XE8zH3++eeora3F9773PTktNzcXxcXFWL58OdRqtWJ5T3ClPrJl+/btbr8Fn5KS4vS4dQOVs8cqNzcXOp0Oy5cvB3qPT3t7O6ZOneqR4K85KQA8ZcoUHD16FKmpqU5tozc4mz/ecPz4cbS0tNh8i1Wr1eL06dNyEFej0WDmzJkAgKNHj8rjAIvj/x46dAjJyckWx82cOM6uFOg1H7NNCs6L4w2LpECyeT5K22prnGLzfdNoNJg4caJcV4nbRt7nynlg+96AyH948p7PlfOjv9ka19LZMVs5BvB1tvLSGmfzVyKNATx69Gg58PnZZ5+hs7MT2dnZ8ktcRqMRu3btwtixY32Sl7bywNX9tcc8+NvfeeCpc7m5uRnHjh0DANx8882IiYmB0WhETU2NuKiF06dPIzIyEmlpaegcQGMAmxs8eDCGDRum6Pa5paXFYkxgT7JVts0N5DGAiWzRaDRobGwUky2kpqY6Va7Ly8tx4MABxMbGYuHChYiPj4fRaEROTg5MJhMWLVrkV8Ffyd///jH++Mf38Oabb/Xp+Yctu3fvwqZNv8af/vQhxo0bJ872CG/UFeIYwIcPH0ZTU5O4mE1xcXHyMxB3PssxgJ03oMcAJiIlRffNZXXibIdioqPFBItup2OixRTqL1OmTAF636q29iAs2Hly//V6PS5fvoyUlBSMHz/e6qRWq6HX6z3STa8ter0eWq0W7e3t2L59uzxJrX+tdbfrL6ZNm4YFCxa4NU2bNk1cLfVRdXW1Yhzf5uZmfPvb37Z4COJu8BcA5s2bB/QGMX0Z/PWkoqIieUwsa+d8c3MzTp06pUgbPHiwoiWvSAqIarVaaLVauZvnhIQEqFQq1NbWyuP/SsFfSbR4PRa6ZC4rK0NbW5tivtiKWAreuvKDDGbjFh89elTRBXRLS4u8jFqtRmpqKjQaDVJTU73yogoRDVyevOcj8oTY2Fi7gU/0Bqni4uKceogeiBwFfxEgeRATEyMHw48dO4bm5mbEx8cjISEBzc3NdqempibF/dBAYy34m5WVZTEmMBH5h8TERKSmptqc2tvbUVtb63TvBhkZGVi0aBEaGhrk34xarRYNDQ1+G/wFgPvu+zZGjx6D//7vLeKsPqupqcH77/83vve9+70W/O0v0vMCqTt5e5P58u5+ljwvbP3TT78kJprr7OxEe3s7BjsxOLinXLx4EZ2dnfJb6PZaJ4jCw8NRWVkJo9HY5weYdXV1qKqq8tpbakTmrl69iqFOnl+NjY1mD39b0FBjQETSYCRECAvK6lFecBqXOoZg4k3jMCotDWkxrag2hmPw4AREAGhpqIYxfDAG967E0f89WtBQbUT44MFIiOiAsaYGHQlpSDKLAVv/HHnL0KFD0d7eruhm3lxLS4tcpyrLkbkWNFTXA0nKY3mdo/m+48r+23P8+HFcu3YN8+bNw0033YQbbrjBYlKr1Th16hQ6Ojq89uCxuLgYV65cwdixY+XuyGJjY5GQkCDfjEsPQT3JlfrIlqSkJIsfEK5OzoxHM9A5e6x0Oh3Onz8Pg8GAY8eOITU11eIHmCeCv5KRI0eitbUVkyZNEmf1K2fzx57PP/8cV65cwdChQxEREYHm5mZF6yippUhLSwsGDx6MiIie611dXR3q6uowevRos7Up1dbWoqurCy0tLQgLC5O3Va/Xw2QyoaurC52dnYrvu3z5MhISEhR12aFDh9DZ2Yn58+cjIyMDISEhMBgMGDlyJNDb/XNkZCRSzV4CQO9b2oMHD7YIDpu7evUq0Fu/orf1Tk1NDbKzs5GRkaGYzLepvr4eBoMBgwYNUnxvQ0MDTCaTRQsz8h5XzgPb9wZE/sVT93yunB/9TRpjPikpCQaDQZ6uXLmCa9euoampyWLcRvOpoaEBRqMRnZ2dqK6utjo1NDSgvb0dBoMBdXV1iI6ORmtrq+L7Lly4gJSUFKdaVPsrW3lpbaqpqUFdXR3Cw8PR1NTkcIqIiMBtt90md3nc0dFhEfjMzc1FbW0tbrvtNrvXXG+6dOmS1edjjY2NqKqqcqnHPZHY7bMv8sCT53JERAQGDx4snyeDBw9GYmIiQkJCUFZWZlEGpMlgMAAAOjo6LOZJk16vR3t7O1paWtDR0QH0PvC2Nun1erS2tqKzsxMtLS1uv1Sp1WpRWVmpqCcuXbok37OJdUhdXR0aGhrk/xsbG2EymdBkpe6ZOHGi1eBvbGws4uPjERcXh4sXL6KhocHj94DOnN+XLl1CaGioXN+5OplMJnR0dGDQoEEW86TJk3WlJ8szkS1paWkWz7mkKSoqCiUlJZg4caJLz5ySkpJQUFCA4cOHIzk5WY6tSK1J/dW4cePwwQfvw2AwYMaMnl653LFhw7MAgKef/gni4uLE2R7jjbriypUraG1tle+xy8rKoOptiTt8+HC7k06n8+hno6KiMHz4cMX2ucsbeeZr165eRVRUFEJDQxESGsoWwERBJ2YQkmKaUaW1M55vcwuakYzM3u6ee5KahYUcaxbfZq1vQB1iwEa//sUTPzgCmSf2/9KlS1CpVBYBMnMqlQpqtVp+s9EbpO1YuHChxTR69GiYTCZ5nE1SKi8vR0lJiVuTtZaertLr9RbrdTTp9XpxNW5buHAhMjMzodPpkJqaKnc7LPFk8Fciti4OREVFRaitrcXSpUuRlZUlTxJr3QRKqqurHQYfUlNTYTQaYTQa5bdeAWDQoEHQ6XTQWxn/V6TVatHS0qLojs9a6xOxRbBUd7naOlf6AWuv7jMYDKiqqsLMmTNRVVUFQ+8DUSIiT/LEPZ+/a2hoQGlpqWK6dOkS2tvbUVNTY3fS6/Xo7OzE6dOn7U7SetH7wpD4fQ0NDeJmBSRreWltqqqqQmdnJy5duuRwMplM+PrXvy4HPtvb2y0Cn2fOnEF5eTmysrKgVquD7pooBn+dyQN/p9frrbYETk1NRWRkJC5fvixPFRUVKC0txeXLl9He3o6mpiZcuXIFVVVVVqerV6+iqqpKDiiK880nqZeY+vp6hIWFiZvpstLSUuzfv18xSUFZsWxfuXIFWq1WkabVatHU1GSxbGhoqM3gb2trKzo6OqBWq73aEtjR+d3Z2Qm9Xo+LFy/2aZLqU3G95lOw1JVE6O26V6VSYc6cOeKsoDRu3Djcfvsd+Otf/4I//OH34myn1dTUYOPGDaioKMeLL76EIUOGiIsQ+QzHALaCYwBTf3KlD/qLFuOz9YzJWheTJo/p25NcjnJkICPafKxeaezeKjSbLS+O1Wvt/7I6IFke97XnO5vTpGV6xgBuGaYcF1ZcD/lWMI8B7AxnxoMrLy/Hl19+icmTJzu82S0qKsKRI0cwffp0j/cWodVqsXPnTrvb8eGHH0KtVuPOO+8UZ7nFlfrIX/nLGMQlJSU4ePCgmGzXggULnA6eeuJYlXoh+Osv3M2fnJwc+UGmyFbwt76+Xm5tPWnSJLtvlxp6x+EFYDGmrkajAQDF+LkQxtqF2Tqk5aT/o6Oj5e648/PzodfrFetyZixh2BgDWFqfeb6Y57X5uktKSmA0GuUAdUVFBcrKyqzmKXmHK+eB7XsDosDizD0fXDw/+putcS0vXryIo0ePuj1m66lTpzBy5Eh5yA2OAdzjopNj4kqBTwDYsWMH6uvrcfvttysCn5cuXUJubi7GjRuHhQsX4ty5czAajQ7X7Q228sDZ/bWmL3ngLZ48l3NychAZGYnZs2dbvd9rbW2VX6yTXppYtGiRsBbrbJ1n1nj63LNVBqxxdr8iIyMRFRVlM/jb1taGkJAQREdHIzw8HFqtFidPnvTomMDO7NexY8cQFxeH8ePHi7OccvbsWTQ1Ndk9Tzx5vDxZnolclZOTg7KyMtx55519emnnvffew8yZMzFmzJiAia38/e8f4803f4t77rkXe/fuwZQpU/HQQ2tcej6Sk5OD99/v6Ub6qaeeRlaW7fHSPcUbdYU4BrArY/H66rOu8Eae+RrHACYaEJKQkTURaajCaWmM34ICFFRHQ50EIGYYMtKAqtO96eVARmayuBKHYtIyEV0trb8MdcmZDOxS0JFafYpjblozdepUREREoLq6WpzlttOnTwMOtkOtVuPy5cteaTEa6O69916sWbPGrcnd4C96W8GK63U0OQrIeVIwB389obGxUe7SWVRYWAiTyQSTyYSDBw9i79692Lt3L/Lz82EymRwGf9H74DQ6Oloe/9ec1CLY0Y/uhIQEpKWl4fTp09BoNDh58qTVLlHT0tJQWVkpj9kbHx/f57I2Y8YMqFQqxRjA0vbm5+cDZi3AJ0yYAL1eLweS09PTER0dDY1GI6cREREFEvPA5+7du3Ht2jVkZWUpAp9GoxGFhYUYPnw4Fi5ciI6ODhQXF8vd/vqCyWTCsWPHFNP58+fR2tpq0TLc0VRbW+tyHgSSixcvorW11aIlMABERUXZvD8cSJwJ/qK3YZHU5bW3WwITkXvKy8tx9uxZjB8/3uHv0GAhBX/XrXsKzzzzLN55579gMpmwbt1a/OY3b6C0t5cUW3JycvDyyz/HCy/8DGr1MPzmN2/2S/CXyFUMABMFvBgMm3i9e8qsrCxkmbUGjhk2UZmelKGYn5SRpQjmWv8/SfkdiuafPd8vtggV10OBIAkZWZbH8jpH8wNbRkYGbr31Vqdvdm+55RavjAHszHbMnTsXCxYsEJOJnMLgr2OpqanQ6XRiMgAgMzMTYWFhiI2NxY033ihPU6dOxaJFixwGfyXz5s2TW+qamzFjhtVWsvPmzbN4MWTChAnIzs5Gdna2PN/eOrOzs51+63Xq1KlWlzVfV3Z2trxNM2bMsPhu8fvmzZtnkUZERBQIoqOjFYHPK1euYM6cORg1apS8jNFohEajQXh4uHxNrKys9GnwFwDCwsIQFxdnMUlj7Dk7jRgxAkuWLAFczINA09bWpggCSz1kdHd3+/xY+hO9Xo+wsDCrwV+JtSBwa2srTCaTYjki8q2jR48iJSXFZi90wcY8+Hvffd8GeruD/v3v/4CHH34EJ08W4eGHH8K3v/0tvPzyz/GHP/xenjZu3IDly7+GF174GUymZrzyyiZs3vwGu30mv8UAMBERUW/g1d7Yv6KMjIw+t6Kzx5ntUKlUmDBhgmLsUCJnMPjrnIkTJ0Kv10Oj0aCkpARFRUVyq9WhQ4di0qRJaG1tRU1NDUaMGIERI0Y4HfglIiKiwJGQkIDhw4fL9+eff/45qqqqLAKf6O0NIywsDMuWLYNKpcKVK1f8ItAVFRWF8ePHK6ZRo0YhNTUV06ZNczjNmDEDc+bMwfz58wEX8yBQmQeBJ02ahO7ubjQ1NaG72+ooegOKlDdqtRrz5s2zGfyVSEHg+vp6xWeIyD/k5OSgubkZc+fOFWcFJWvBX3P33fdtbNv2Z7z11tv4xjfuQWhoqKInDLVajTVrHsaf/vQhNm9+w2GX+US+xgAwERERkYeUl5ejpKTErUnqjtwbVCoVg79OUKlUclfgZ86cwaVLlxRdNUtB4Pr6ehw/ftzsk0RERBQMwsLCcMMNNyAjIwMpKSmIiIiARqNBVVUVZs+ebRH43L9/P2prazF79myoVCrodDo0NjYqlgk0ISEhiImJQUxMDCIiIhASEuJSHgQ6KdDJ4K8lKW8A2A3+Srq7u7Fv3z6v/s4hItdJXT9Pnz7dbi90wcJR8NdcVtYMPPDAD/DSS7/A73//B3l65plncd9938a4cePEjxD5JQaAiQJMaChPW3KNtTJjLS1YDaR9Jd8rLCzEwYMH3ZoKCwvF1XrM0KFDGfx1kkqlQnZ2Nu69914sX77comW+FARuaWlBc3OzYp6/mDFjhld6KqDgxOslBTqWYfKUsLAwjBgxAomJibhw4QL+/e9/Y9u2bTh79ixiY2MtAoFS4HPRokXIyMiATqfDtWvXFMsEmpCQEERHRyM8PLxPeRAs2traGPy1oa2tDXl5eaioqBBnWdXR0YHKykoxmYh86OjRo1Cr1R4Zoqe7uxt5eXn46KOPkJeX53f1pivBX6Jgwl9IRAEkOjqaDzbIZWFhYYiKipL/H2jlSNx/Im+69957sWbNGrcmqeUp+b+hQ4di7ty5iInhmPcU2AbavQEFJ97zkackJiYiMTERZ86cQV5eHlpbWzFixAjceOONiIiIwIkTJ1BaWgpYCXwajcaAD/4CQHh4OMLDw/uUB8HG34IY/qSmpkZMIqIAodFo0NzcjFtuuUWc1SeLFi3C4sWL5cmfukZm8JcGshBtZaXVO5nu7m50d3fLb7tN9MCbIM46cOAA2tracMMNNwAAhg0bJi5iU3R0NHJzc1FdXY1ly5aJs51y/vx5HD16FI888og4i8jjioqKnH7TymAwyOcmkbPCwsLQ0dGBQYMGAQOwHIn7T7a5Uh+Rb/FY2cf8IXLtPBho9wYUnFy553Pl/OhvOTk5KC8vt3gO0tjYCJ1Oh8TEREW6q0wmE6KiouSx6y9cuIDBgwdbdNlbXV2NjIwMLFy4UJEeSGzlpTUmk0keo3Tp0qUwGAzYtWsXYmJiMHr0aMWyFy5cQFNTEzo7O9He3i4HPk+dOoXy8nKLurShoQHjx4/HrFmzFOn9wVYetLS0QK/XY8iQIYp0AIiNjcX8+fP7lAf9zZPnsq28skav16OmpsYiX2yxdZ5Z4+lzbyDvV2VlJSIjI62Wc2dcu3YNbW1tGDFihDhL5sn98mR5JrKnpKQEBw8exKxZs4K+zAVj8NcbdcWRI0eg1+tx2223AQC++OILoLdnNEf0ej0AeOyzKpXK4/dM3sgzXys+cQIJCQkIDw9HaFgYQsQFeoWtf/rpl8REc9LN3ODeHwf94eLFi+js7JR/uIWHh6Ojo8OpKTIyElVVVTAajX3u4rCurg5VVVXIysoSZzn0xz/+EQUFBVanCxcuYOTIkXwrmRSuXr0q//h2JDw8HA0NDYiPj0dnZ6c4m8hCZGQkmpqakJiYKLfsGUjlyNr+k22u1EfkWzxW9jF/iFw7DwbSvQEFJ1fv+Vw5P/qbTqeDyWRCa2urYmpubkZ7ezva29vR1tbW58k8ONna2oquri6Ehoaio6ND8X2RkZEYPHgw0tLSFNsXSGzlpbVJegY1evRopKSk4NixY6irq8PEiRPF1SImJgYVFRUICQnBihUroFarcfnyZZw7dw4hISEIDQ1VTLGxsUhJSfFJmbOVB52dnQgPD7dIb21txejRo5GcnOxyHviCJ89lW3llbWpvb5c/J86zNtk6z6xNnj73BvJ+dXZ2IiQkBJ2dnRbznJk6OjoQEhKCrq4ui3nS5Mn98mR5JrJFr9fjwIEDSElJ8ciLC/4sGIO/8FJdceXKFbS2tiIzMxPo/Y729naLOs/aBABxcXEYOXKk258tKytDVFQUhg8fLm+bJ3gjz3zt2tWriIqKQmhoKEJCQ20GgAOiBbArhgwZgpMnT/qsBfB7772HcePGWX0r9/Tp04iIiMDSpUudegOCBgZX30BpbW1FXV0d4uLiEB4ejs7OTnR1dYmL0QAmPWhA741dUlISoqOjFcsEczlyZv/JOlfrI/IdHiv7mD9Erp8HwXxvQMHJnXs+V88PGlguX76M//u//8OQIUNsPoA8cuQIsrKyMGXKFHFWUAiUPOC5TMHE3fL8ySefiElu+eY3vykmURDQaDTQarVYvnx5UMcngjX4Cw/UFdaILYB9hS2AnedsC2AGgK1wNwA8c+ZMjBkzRpEeHh4Oo9GIU6dOITk5OegKHPVdXyqg7u5uNDY2oqmpCR0dHeJsIoSHhyMuLg4qlcpmK4hgLkfO7D9Z6kt9RL7BY2Uf84eob+dBMN8bUHDq6z1fX84PGhhOnjyJU6dOISYmxmavcteuXcOVK1dw++2397lrWX8WSHnAc5mCibvl+b333oNarUZMTIw4yyXNzc3QarV9ei5O/k3q+tkZ48ePD9gWwsEc/IUH6gprGAAOPAEfANbpdIiMjBRnOTRhwgRotVq/CwBHR0ejtrYWDQ0NinRzaWlpQf3mDVkXjBUQEQUm1kcULFiWiXgeENnD84MkZ86cQV1dHZqbm9HQ0ACTyYSkpCSbY6A2Nzfj/PnzUKvVWLRokTg7IAVyHvBcpmDibnm21yulKxobG3Hu3Lk+PRcn/6bVau3GJswNGjTIZ937uyPYg7/wQF1hzZEjR3DlyhUkJCSIs/qVwWDA8OHDGQB2QkAHgEtKStDS0iImO2XkyJE4ffq0XwaAc3NzcerUKUW6JCQkBElJSeweegAKxgqIiAIT6yMKFizLRDwPiOzh+UHmDhw4gIsXLyIkJARjxoyxGTypq6vDlStXEBsbi8WLF/v8IaknBWoe8FymYOJueX733XfFJLc8+uijYhKRXxsIwV94oK6w5sKFC6itrRWTfSIlJcXmS2h95Y0887WADgC7KycnB5cuXcLEiRPFWU5x500nRwFga4Hp8+fPIy8vD1FRUYiLi3MpCFxRUYGysjJFWnZ2tuJ/8m/BWAERUWBifUTBgmWZiOcBkT08P0h07NgxnD9/Hu3t7YiLi0N0dLQ8prTJZEJTUxPa2tqgVqsxa9Ysnwc+vSEQ84DnMgUTd8uzrWfSrnLUMCo/Px96vV6RlpmZifT0dBQVFUGn08nPpouKigBA3i/xfyJP+s//fAdDhgwJ6uAvPFBXDETBmGfOBoCdHyQnwDQ1NeHo0aN9ms6dO4eQEFtZ5j2zZs1CU1MTdu/ebXEhtebQoUOoqqpCdna2PGVmZqKiokJclIiIiIiIiIiIrLj55puxbNkyTJ06FYmJiTCZTNBqtdBqtejs7IRarcYtt9yCW2+91S8Cn97APCAKbjqdDsePHxeT+yQtLU3xPDo9PR3oDeyyYRL5yuOPPxH0wV8iVwVlC2BfsvW2lTMtgO+//35cunQJR44ccdgSuKioCEajEfPmzRNnUYAJxjdQiCgwsT6iYMGyTMTzgMgenh9EwYHnMgUTd8uzrWfSkurqaly4cAELFiwQZyk40wI4Pj4eEyZMEGdZEFv8iv+LKioq5GCyxGAwoKmpKSDHoyXyBnfrioEoGPNswLcADkTnz59HW1sbMjIyUFdXh927d4uLyHQ6HTIzM8VkCyUlJdBoNPIkXWgl+fn5KCkpQVFRkbzMoUOHFPPFz5SUlCA/P1+R5knWWjAbDAZotVoxmYiIiIiIiIiIiIh8rKioyOI5srMMBgPKysoUz6UNBgOOHj1qMfwhERE5hwFgP5KXl4e8vDyUlJQAABoaGsRFAEAOhDp686moqMiii2ij0WhxIa6qqoJKpZKXiYyMlAO8qampMBqNiuWNRiNSU1MVaZ7Ciz0RERERERERERHRwJGQkCB3H33o0CH5eXBqaip7wCQi6iMGgP3AmDFjcP/99yum2bNni4vJWlpaxCSrdDodJk6cqEjLzMyETqeDwWCQ01QqlaJ7jfHjx0Ov18NgMCA9PR0tLS1y0NlgMECv11t0x+EpvNgTERERERERERER+aeqqipFj5Pmz5ndJT3/lZ4HB1u3rURE/YkB4CBlq5Ww9H9TU5OcFh8fb7ZETxAWZsukpqbKrZGvXLnitda/5nixJyIiIiIiIiIiIuqb06dPWx1qDw7mOZKWlqbocVJ6luwp8+bNQ1paGp8HExG5iQFgHyovL8fZs2cVU2Njo7iYhZSUFMAsyOttQ4YMQV1dHdDb/bNKpRIX8Qpe7ImIiIiIiIiIiIhcFxsbi8rKSotA7+nTp9HQ0GDRKMifTJgwQUwiIiIXMQDsQyaTCU1NTYqpra1NXMxCQkICVCoVKisrxVmyuLg4wEqQ2FrLYPE7xWXUarXcDbQ3u3+2hhd7ClbiWNzBIlj3i8jf8FwjIiJreH0gIiIiSXp6OkaMGIHKykrU19cDZsHfcePG9Usvj0RE5DsMAPvQpEmTcPPNNyumwYMHi4tZJY3Tm5+fr0ivqKhARUUFEhISkJqaitOnTyvml5WVIS0tTZGm0+kUgWJry6SmpqKyspI3BkRERERERESCiooKxXiIGo1GXMTjSkpKFM8EioqKHH6vM8t4WlFRkVsvJ+Tn51vkrdiajfrOnbIrHlvxfyJPYB3gHikILPXuyODvwCNd+6VJjCd4m7fP3VWrVmHs2LGK6W9/+xsAYMOGDRg7dqz4EZe8+eabWLVqlZhswdr3+6tDhw7h0KFDYrJN4j2nNc4sAx/diw5kDAD70LFjx3DgwAHFVFVVJS5mVUJCArKzswGhEq2qqpJb6E6dOhVpaWmK+cnJyRatatPS0lBZWSkvEx8fb7HMkCFDoNfrMWTIEEU6ERERERER0UB26NAhVFVVKcZDzMzM9MpDTnumTp0qPydAb2BPfBAnLhMoxPEm+7NnMmdZy29/5y9ll8gR1gHukYLAoaGhDP4OMPn5+Whra1OcP5GRkeJiLnO2vOfn58vn78yZM1FWVgaDwSAu5rbHH38cpaWl8vSd73wHAPDqq6+itLRUXNzjVq1aJW/DZ599hueff75fvrcvzBsCir3H9odAvRcNVH4VALb2Rpc3KgRvO336NHbt2qWYrN08jxw50uLtlOTkZHExu2bMmKGowOfNm6eYP2HCBMV8MbArMV+PtTF3W1paEB0dreg6moiIiIiIiGggk1o7ir/F09PT/TJAQSRh2bUULC2YS0pKLJ6vajQalJSUiIs6FCx5Qj3n9s033+x28HfGjBk2ny9PnTpV8VzZ0f/kXQaDAXq9HuPHj1ek9+cxaGtrw/DhwwGzYS2bmprExQJeZWUl7rrrLqC3JfDs2bOdbujX365du4bk5GTEx8fj2rVr4mwKMiHayspuMREAuru70d3djba2NjQ1NWFiP1QM+fn5itanJSUlqKqqwsyZM5GQkCAu7pSKigrodDrMmDFDnOUVOTk5YhLQe+KXlpaiuroay5YtE2dbOH/+PI4ePYpHHnlEnOVRYp7bcujQIauth8l9RUVF/XrhJf8QrMc9WPdroODxCxw8VvYxf4h4HgxUPO7O8WQ+aTQaTJw40eHL0tLzDUlqaqpiGw4dOoS0tDRUVVWhpaUFACyehRQVFUGn0wEAoqOjkZycDKPRKD/vkII0U6dORX5+PvR6vfxZ6fvMl5G4u20GgwFHjx6Vl4+OjlYEFa19pyscPbdwdvvLysoAANnZ2fI6jUajnE8TJ05EXFycYl/MW6jY209b+S2ytw70tsQxH8pLLAOe1Neya75N4rEV//c2T57L8MH2m/Pk88uSkhJF3SDR9Ha56UrLK1fzxJP7IQmmOsAed8vze++9B7VajZiYGHGWS5qbm6HVar3+TJr6h0ajQWZmpt0Xe1w9h1QqldPlvaioCJGRkZgwYYJ8jZPOK+mlFFvntrNWrVqFGTNmYN26deIsbNiwAehtCQwAixcvxg9/+EP8/ve/x5UrVwAAn332maKb6A0bNuDTTz8FAAwfPhz33HMP8vPzsW3bNnkZ0YYNGzBs2DCsW7cOBw4cwJo1a+QWwG+++SYAWN2+vnC3rtBoNJg5cyaampoUx8Oco3tOZ5exRryuOLrP9MS9kbt55o+KT5xAQkICwsPDERoWhhBxgV5h659++iUx0VxnZyfa29sxeOhQcZbHVVVVITIyUn4TKTU1FdXV1ejo6Ojz20kNDQ0wmUwWY9p6yw033GB1io+Px6VLl1BfX4+wsDDU1dXZnRobG1FbW4usrCzxKzxKzHNRUVERTp06hUGDBmHSpEnibPKAq1evYmg/nF/kXxwd9z/84Q8ICwtDcXExCgoKMGrUKPzpT3/qU1p/nruO9ssZGo0GX375JS5evIjhw4cjKipKXCRgfP7559i/fz/S0tIQHx8vzvY7njh+1D94rOzrS/788Y9/REFBgdtTRUUFJk6cKK6eqN/15TygwOet415eXo5du3YhLy8PDQ0NyMjIEBfxiIKCAuzduxcnTpxAZ2en/Dve09/vqXzSarWoqanBlClTxFkKRUVFuHr1KrKzs5GRkYGMjAxcuHAB9fX18nZcvnwZNTU1mD59OiZMmACDwYDKykqMHDlSXofRaMQtt9yCjIwMREREoKysDFFRUXI+Xb16FQAwdOhQpKWlISQkBJ2dnZg/f778PebLeGrbysvLMWHCBEyYMAEZGRm4evUqdDqdze90lb3nFq5s/8yZM+WHzFVVVdDpdBg9ejSmTJmC1tZWlJWVoa6uTs7j2tpaxX7Y209b+S2ytw6DwYATJ07I2xkTE4PIyEiv/B5ypew2Nzdj/vz5yMjIQEhICE6dOiWfg+KxFf/3Nk+dy5L+3n5znnx+qdPp0NbWZrGujIwMVFdXK84PR1zNE0/uhySY6gB73C3PFRUV6OrqQmtrq1tTV1cXYmNj+ZsmSLS2tuLSpUswGAxWy1dfziFXyvvQoUNx7tw5lJaWwmAw4JZbbpHnScFDa+e2Kz799FOkpaVhzpw54ix88cUXAIDbb78dAPDBBx/gn//8J/72t7/hpZdewpUrV/D73/8eDzzwANAbyM3Ly8OxY8ewdu1aZGRk4IUXXsCIESOwYsUKxbrN3X777di4cSN+9atfoaCgAMeOHZPn5ebmAoDV7esLd+qKiooKNDc3Y8yYMYiPj0d1dTU6OzsxaNAgeRln7jmdWcYW8bpi7z7TU/dG7uSZv7p29SqioqIQGhqKkNBQmwFgv24BbJ42fPhwm29ZwcabAGfPnrX5Nor4Zktf3hxwVU5ODs6cOSMm2xQSEoKHH35YTKYgE4xvoJBjjo778ePHoVarYTKZ0NLSglGjRuH8+fMup7W1teHGG28UV+81jvbLkfLycnz55ZeYNWsWiouLkZmZ6bEbJF/48MMPAQDjx48PiP1w9/ihN4Df2NgoJrskMTHR6huIzhgo3+/MseqvbbHFl9/vTP6I3nvvPYwbNw6JiYniLABAY2MjampqMGbMGHGW7PLly2hvb8c3v/lNcRZRv+vLeRDs9Ho9Tp8+jerqaqC3jrHX+q2goADV1dVYvny5OMtvuXLcm5ubUVZW5tTLgtu3b8ewYcMwceJE7Ny5E+PHj/f4y8p6vR7bt2+XHwx++eWXWL58OdRqtce/35V8sqeiogJlZWUOr1XWWlpKzzCkZxFir1tiKxlr6ygqKkJbW5vVFsCw0RJPXMbael3dNpH4veJ3ukpsWQezZzh92X70rjMyMlLeJqlln3krqYqKClRVVVl0kSwR91P83xnmn3GUr57kStkVn5dJLXXS09Mtjq34v7d56lyWiNvvTqske88d3WlN5wxbLYBh49jb21YxT+wtL56rnnoOK64XQVQHmPN0eSaSmLdeT0tLU5wLfT2HnC3vGo0GKpUKI0aMwOnTpxX1Qn5+PkaMGGHzXtxZq1atQl5eniJNatVrrQXwPffcI7fGFVvrjh07Flu2bMGiRYvkdW3YsAFXrlyx2wJY6vb54Ycfxpo1a7BixQr5O1etWoWHH35YsU53uFNXiPE3a9cLa2VCvOd0ZhlbxOuKWL7M74c8dW/kTp75K2dbAPvVGMDWtLW1ITo6GleuXMHMmTORbTZYuVRYDAaDXCllZ2fLbyjNmDEDmZmZUKlUyDYb27ao9w0FaV2ZmZmK4LK3LFy4EI888ojTE4O/5I6CggLk5OQopoKCAoub5v6Qm5trsS3e3I6cnBy5GxGR1ELL3+l0OphMJgwZMgSjRo0CAPntrCFDhiA6Ohq5ubmKNHE5vV6P+vp6Yc3+zWAwoLOzE+PHj0dMTAza29vFRQJGQUEBIiIiMH78ePmH/UCQmJiI1NRUtyZbAThnDPTvN+frbfH19/dFYmIixowZY3UaNmwYYmJiLNLNJ3e7WyMi79Hr9di9ezfKysrkOqaxsRGff/45tFqtuDi0Wi2Ki4uR6maLBGdotVr5fln6jettzc3NOHbsGBoaGtDc3CzOVtDr9dDr9ZgzZw5UKhUyMzPlFhueVFFRgZSUFLn1iVqtxpUrV/rt+71FKl/iw03pf/Nx8KKjo+W/4+LigN77Y1vriIyMVPzvKlvrdWXbJCVmY46WlZWhra1NnucJaWlp8jOc7OxsJCQk9Hn7Jeb5JwWirC1nzhP7aWsdarUa0dHR0Gg0qKioED/W76T8PXr0qLy9Go1GDoQOFGVlZZgyZQqys7ORmpqKkydPAnaeRcLJ545lZWXyZ209v/SGlJQUwOz4OrOt5uwtb2s/7H3GWcFUBxD1t4SEBLmeqqqqQn5+PuDGfYCzpJddZsyYAbVajezsbBiNRvl+V6/XW3x3Xz3++OMoLS2VJ/MunUXDhg2T/5Zaq5aWluLAgQMAYBGoNV/emsWLF+Pxxx/Htm3bsGjRIpSWliIvL08OPufl5Vms0xcMvWNCS2MyA8CgQYOg1+vlezpbZcK8vnRmGfQGic0n8/tGka37TH+7NwpEfh0AliqD9PR0TJgwQfFmWGpqqnyRlSojab5arbb7FplOp1MMfp6eno7o6GgWIgoqly5dwtmzZxXT8ePHsX379n57sASzlhOXL19GWVkZdDodYmNjoVKpxEU95uzZs6ipqRGTgd58uXTpkpjsd+rr6+3+sG5paXEY3DWZTF4NtHtaeXk58vPzMWzYMLS1taGzs1NcJKBUV1dDrVYjPT0dJpMJ5eXl4iJBKSsrCwsXLnRrcqdFz0D/fnO+3hZff7+rQkJCoNfrUV1dbXXS6/UICwuzSDefWlpaAr7uIpKUlJR4dPK1w4cPo6OjA8uXL5frmHvvvRcxMTHyQzBz+fn5UKlUXu/Bo6CgADt37kRxcTHOnj2LI0eO4OOPP/bqfYMU/AWAm2++2eHLK1VVVYp790GDBsFkMimW8YTGxkbFiz+JiYkwmUz99v19IQZSBqpDhw5ZBHeCkSf209E65s2bh5kzZ6KsrMzhw1J3uFJ2zYNu0mRvLMlgk5aWJj9jHDJkiPw73d6zSGeeO5qvtz+J3+nMtppzdXn08TP+yNH5S+Tv1Go1Zs6cCb1e71T97w6DwYCWlhZFsBG91zmdTicHhwNdaWkprly5grvuukuRvn//fnz66adycNgfSGMem7/YJfViIc3zJPHeQbz+OKu/7o2Cld8FgKuqquQCaDQaFd1slNh4y8qVNwH4BiMNNOPHj8eaNWvk7tPa29tx/PhxcTGvycrKkh+upaSk4N577+3XB/qBatmyZXKLXmtGjRqFZcuWickKU6dOxcKFC8Vkv1ReXo59+/YhNTUVS5YsAQB0dXWho6MDAHDy5EkcOXIE165dEz7pn7RaLbRardx6RaVS4dy5c+JiRORHQkJCUFNTgwsXLlidpNZmYrr5ZDQa2QqAgsaBAwewf/9+j0zS2/S+pNVq5VZJ5kaNGmXxAKyoqAharRbTpk1TpHtaSUmJ1ftyvV6Pw4cPe+VFPleDv2RfQkICVCoVKisrxVkyqRWDWM5stZ6wxlqLWwAwGo2K/13liW3TarVoaWlRdPfXX89XPLH9zvLEfjq7Dqmllkql8soDWbhZdgcaV1slOfvcsS+t6TxBqkfi4uKc3laJq8ujj59xlq0y6q91AJE/MA/C9ec5ZE56ecK8S2l/YN4a2Jy1l0Wd8ctf/hIA5O6mfa2urg6ZmZkWgdm0tDTU1dUBTt5zOrOMp/XHvVGw8rsAsHmXHubBX0dvWbn6JoBY0LMH2BuMNPCo1WqM6R230Bfd6ur1+n7pQi9YfPTRRzh//ryYLDt//jw++ugjMVkhNzcX//73v8Vkv2Mt+Cvp6OhAXl4eDh8+jEuXLuGrr77C5cuXFcv4o9LSUsTGxiIjIwMwe7jsjQe5ROQ5gwcPxoIFC/o8RUVFiau0kJ+f7/BeVaPR9PlHZn8wf3jn6OVLayoqKhTr0Gg04iLkB0JCQjB79mzcf//9bk2zZ89GSIitEYn6T3t7OwYNGiQmW6Tp9XoUFxdj/Pjx8nXcWy5evCgmyUwmE06cOCEmu62wsBAmkwkmkwkHDx7E3r17bU72AkN03fjx46HX6y3q7YqKClRUVCAhIQGpqamKcULR2/2rsy1fpGCd1PUsetfvzL2lvWU8sW3iw2ODwaAY59ObPLH9znJ2P+3lt6N1aHtfIpVIQ6J5izNlV6VSWeRvf/Yo5u/sPYsUnzn6y3PH2tpaREdHK4JA4nY62lZxWUfLo4+fcSTQ6gCi/mYwGCzqbKlnHqnXAnfOIXvlXbqGnD17VpFeVFSEsrIyxfCe/sJ8HF/J3/72N4vxhc1Jn/n5z3+uSN+wYQOef/55jBgxQu4K2pekl1ikHkDMDR8+HC0tLdBqtU7dczqzjKf0971RMPK7ALA1zr5l5cybAOIFm2ggkbpFjo2NFWd5VXl5uc2HbmTd7Nmz7b5pp1arMXv2bDFZITMzE1OmTBGT/Yq94K8kPj4eLS0tqKurQ2dnp93AuL+4fPkyRo4cKf8/ceJEtLe3W7xFGIw0Gg22b9/u9OStwE95ebnFdzmavNXdpq/zpLm5GadOnRKTZfa2z5PbcurUKavjTPbX9/dFaWmp1XtO9HZl15fgp8TWvao76+wP+fn58gub0gNPe8Fs0aFDh1BVVaV4+JeZmemx/a6oqLB4kE3uO3/+PHbt2oVdu3bJQ2lcu3YNe/bswZ49e+QeOi5duiQv54/Xa/NxzGylSeXnpptuUqR7g6NujKurq8Ukt2VmZiIsLAyxsbG48cYb7U7SA6K0tDTFA52qqiqvvNiZmJiIxsZG+f/q6moMHjy4376/r6TnEBBekKmqqpKDG1OnTkVaWppifnJyskstX6TnIdLn9Xq9w4ezUjerGo3G5kNWd7ctISEBaWlpOH36NDQaDU6ePGnxwr43ubv9znJmPx3ltzPrkOZpNBrEx8e7HSCzx5myO2PGDKhUKsV8sSeFgU58Funvzx3NAzuubqury6OPn3FFINUBRP0tISEBOp1OcX7U1dXJdT/cOIecKe/ivYum9/d9du/Y50ajERo/e/l527ZtQG9gd+zYsTh27JjDLpzFz0jjD5eWlmLbtm3Iy8vD2LFjsWrVKuGT/aeyshIqlUrx8o9ECuhKL3+Kx83aPaczy3hKf94bBaMQbWVlt5gIAN3d3eju7kZbWxuampowcepUcRGPy8/PR3x8vEUFYzAYcPToUUycOBFqtVr+Pzo6GvPmzZNvIqRgidSHfHp6OioqKlBWVqao2PLz86HX6xVpRUVFmNoP+0gk8lbZ2759O2pra5GSkoLU1FQ0NjZCq9UiIiICt9xyi9dbNJgrKCjA8ePHsWbNGnGWV2zZsgXjx4+32v3x9u3bAQD33nuvOKtfOTrue/fuRWZmJoYMGSLO+v/s/Xt8FdW9P/6/NiHcCVe5JMjNbLSItFUBDS1aTq0l1n6E4+XR6vnp5/HVcHr8VnL6KfLxSC+2Wg/SzznBfmxL5Pv76q/S81E84KNKUoulyimpIGjFFJEdkoAkBAwQcuMSwv79sfdMZtZeM7Nmz+yd2Xu/nj7mIZlZe2bNe9asuayZNUD8pmt9fb3td+nq6upw9uxZU28Kqea0XkZOjb/79u3DsGHDUFxcjOrqapw+fRqjR4/GuHHj8NWvflVMHhgHDhzAn//8Z73bdc0bb7yBnp6efi97dtxsPyt79+51vKFtNGzYsJR0C9/S0uK6wT0cDts+eJGsVMREdVupdPVplz+VvKiwy0cqlq8aH6MNGzYgHA7j2muvBeIXGW1tbZg1a5a0oaGxsRFHjx7FlClT9AuQbdu2obu72/bCTru4Fc9FNTU1NRg0aBBguKgKkpqaGlxzzTX6heOePXswZcoUpX1n3759CZ948VtjYyNaW1sDGbt0S2Y/MKqsrMS8efOA+KcYhgwZgjFjxujnJ7/73e9M6e+44w60trbi0KFDAIChQ4di0qRJOHPmDHbv3o2ysjJT+nSzOgfcsmUL8vPz8Y1vfAMNDQ344x//iC996UsJ16SpsD3+aSM7bs+fVbb78ePH8be//Q1jxozBF7/4RXEyEO9JZvbs2XpDzxtvvIH8/HxMnjwZH3zwAW699Val/d5Oe3s79u/fbzqfffHFF/XvRNbX1+Pb3/42kILlq8SJiILP731Za8TQ5mm8vwjD/cl58+bpDxDJ7kU63XcU54v4OYx4/zJZBw4cQGdnp+l8qKWlBfv378f48eNNMXPKqxgTp/Sy9XD6DcUwJkSkgnWFe9kYs9oPP8TIkSMxcOBADMjLg1WfW3nf/973fiyONOrt7UVPTw8umzhRnOS75uZmDBo0KOEm2+DBg3H+/HnU19ejoaEBp06dwtSpU9HR0YHLL78cnZ2d2L9/PxoaGtDQ0IDRo0frF42jR4/GsWPHEIlE0NHRgYkTJ6KwsBAnT57EgQMH9N9MmjSJbydSvzh+/DgmpmD/OnDgAM6ePYuzZ8/i5MmTej/8RUVFmDJlCkaMGCH+JGUOHDiA3t5eXH311eKklHj//fcxfvx4TJs2TZykd3Xyuc99TpzkSmNjY0Kd0dHRgdOnTyvF1mm77927F2PHjsX58+dx8uRJjBo1CnV1dRg0aBDa2trQ0tKCEydOIBQK6ePEdCdOnEBHR4fe9beKVK+Xpr29Hb///e8xfPhw3HLLLeJkAMDEiRMxduxY/OlPf0JbWxu++tWvIhqNore3N+FJWyde18uNvXv34uLFixgzZgxaW1v14dy5c2hubkZhYaGnZaZyXVS3n53CwkJMmzZNeUjVE4IjRoxIWJbT4DV+VlIRE5VtpTW6nj9/HtOmTcP58+fR3t6O9vZ2nD17Vl9fu/yp5MXK8ePH0dbWZlpea2srPvvsM1x22WXIz88HUrR8lfiI3n//fYwbNw6TJ0/G/v37cerUKUyaNAl5eXno7OxMGAYOHIhQKITjx4/j0qVLGD16NOrr69HT02N7YdHc3IwRI0agp6cHvb29pv25paUFp0+fxqhRo3DhwgXT+h84cAD79u3Tz13Hjx+vdzldU1OD3t5evP/++2hoaNAf8tq3bx/+9re/oaGhAceOHUNXVxcaGxuV5ytz+vRpdHd3Y/z48WhpacHRo0f13iYOHDiA1tbWhHN5zd/+9jfMmjXLcV+zy5O2rvv370ckEjFN37NnD1paWnD+/Hk0NDTo5/6q8xTj57dU1t8yyewHRnv37kVRURFaW1tx9uxZ3HzzzZg5cyaGDx+Ojz/+GIcPH8aSJUswa9Ys3HDDDRg0aBDOnj2LgoICjBkzBuPHj8fll1+OSZMm4dKlSygqKhIXIfXyyy9jzpw5pnGRSAS1tbWenvYOhUL45JNP0NbWhvPnz6O1tRV79+7FyZMnMW/ePIwZMwbbtm3DmDFjUvqQgtG4ceNw8OBBXLp0SZyk0x5KUaWy3UeMGIFhw4bhyJEjaGtrw+TJk8Uk+Otf/4rLLrtML5uTJk3C0aNHceLECcyePRtXXHGF+BPXTp8+jbq6OsyaNUsfN2rUKBw+fBjd3d249tprMWbMGCAFy1eJExEFn9/78vHjx4H4tSjiPTuNHDlSP35fuHABzc3NKCoqQk9Pj+W9SKf7juJ8YXH/MlnaNai27IaGBnz22WdYvHhxwnyd8irGxCm9bD2cfkMxfpdnIspOrCvcy8aYnTh+HIMHD8aAAQMQGjDAsgE4UG8AE+WiVD2BIr4BjPhFRnd3N/Lz8z0/Ne/Gli1bMGrUKF+eZFWR6jeAxV4IrMbZcdruHfHuNN99912cPn0aS5YswcaNG7FgwQK0trYqjSsuLsaAAQP0LpecyNZBNs6O03oZ7d27F3v27MGcOXMsf/OnP/0Jra2t+MpXvoIZM2Zg9+7daG9vd/UGsGwdZOP80N7eji1btth+Z9uqbKqQ5Vs2Llluth/1L5Vt9be//U36XSrEb/7feOON4mhf/eUvf9EfPhIVFham9KEglfiItDeAJ0+erL/BqGrAgAG49tpr8V//9V9KbwBrDSrimxn79u3T3/41Ttu3bx8uXLig/y2+WVFTU4Nz585h3rx5+pu5+4S3bbW3PgoKCpTna0VbnljvaA9Zyd6c1JbvNG+nPInrKq6n7A1gt/NMBVldLRvnp2T2AyPtDWDjOYZGOz9ZtmwZPvvsMxw6dAgnTpxANGq+tAyFQpgwYQKuuOIKaSOjKBKJoLS0FEVFRXj77bctxyXrwIED+Pjjj3Hy5Ekg3qh49dVXY8aMGXj33XfxySefYOnSpWnt3rSlpQUffvghWlpaUFBQgMmTJ+OTTz5BT08P8vPzcf/994s/seVmux8/fhz19fX4whe+IO0hIpu5iRMRBRf3ZcomLM9EpIJ1hXvZGDPVN4Az4hvARJS88ePH48tf/jK+/OUv4xvf+AaGDRumP6maLtqbqdnC+K2kmpoa/Qbu+PHjfbuBu3HjRtTV1eGGG27Qb7jee++9KC4uxg033IBwOIyNGzeaxonp3n33XWzdulWYs7V0rJfRddddh+uvvx61tbXYJ/leiNj4i3ge3UrnekUiEfT09ODuu+/Ggw8+mDBcfvnl+PTTT8WfKUvnulDmu/rqqzF+/Hjk5eVh7ty5uOWWW/Qh1Y2/AHDjjTealjl37lzk5eVh/PjxKW389Wry5MmYMmUKAGDKlCn40pe+ZDmMHTsWAwYMwKxZszBkyBBxVrauuuoqtLe36w/8dHR0oLW1VfqWZGtrq/5GCQzfW2o0fDe3sLDQVEe2traaekuYNGlSwpu5KvMVbd++HYMGDcLs2bNx7tw5U/3d2dlp+SaH1beURSp5Mq7rhAkTHOftdp6pkK3198CBA7F7926cOHECY8eOxZVXXolrrrkG11xzDa688kqMHTsWJ06cwO7du8WfSoXDYb37/ptvvllv/F22bJnnxl/E97ulS5fqx+VvfOMbmDFjBtrb2/HJJ5/gyiuvREFBARoaGvDGG29gw4YN2LBhA1555RXpuYofJk2ahFtvvRX3338/li5dihtuuEFvgE51Q/TEiRNx4403JnTL/+KLL+LFF1/E3r179fENDQ347W9/iw0bNujfb/PTBx98YPvphlQvn4iIiIiIKNsEqgtoolyUqi4ItC6gxxu6Qh48eLD+XdjBgwebultLlQMHDuDIkSO4+uqr9S7cUq2urg55eXnSro8/+OADTJ48WY+JF1pj3pEjRzBe+I6OE6ftnpeXh0mTJulvgokGDRqE0aNHY+zYseIkndal/mWXXSZOspXK9RIVFhYiFArhr3/9K6LRqP5bWeMv4m/YDhgwQOktIpGX9VL15z//GRMmTLBs3MrLy8PBgwcxbNiwhIYYN1K1Lm63n8z27dvx17/+FQcOHEh6OHbsWNJdsObK8lW31eTJk9HW1oYjR45g0qRJerfLRnZ5VsmLCq07atn3JlOxfNX4GBm7gB49ejQuXbqEo0ePIj8/X9owGIlEcOrUKdM3glW7gNbq546ODr075YaGBgwePBhTp05Fa2ur3gV0S0sLPvvsMzQ3N5u68dO6mh89ejQ+/fRT/d+Iv1H42Wef6V0za06fPu1qvqKamhpMmDABc+fOxYgRIzBjxgwcOnQIp0+fxsSJE3HgwIGEZWra2tpw+vRp2+2pkidxXaPRKJqbmzE+3qVzW1sburu79W6uk5lnKqWq/pZJZj8w0rqA7u7uRkdHB4qKivTzko6ODrS1teHqq6/WuzDu7OxER7xL61OnTuHUqVP6cTsvL8/UCO/kgQcewAsvvIBf//rXWLZsGdasWSMm8dW2bdsAALfeeisaGhqwY8cODBs2DF/4whcwdepUDBgwAPv27fN8/Fa1c+dOAMAVV1yhP5Ciyst2b29vx44dO7Bo0SJMmzZN/0bliBEj8Pbbb2Pq1Km4+eab8f777yd0U+9VZ2cnGhsbcenSJYwbN06c7PvyvcSJiIKD+zJlE5ZnIlLBusK9bIyZahfQfAOYKIdo335E/M3gdGhra0N+fr7tDV+/TZ06FZ9++qnprQUAePPNN9Hd3Y1wOGwa70VJSQkKCwt9v4Hb2tqK7u5ucbSuu7sbra2t4miT9vZ2nD59WhytJFXrJSO+CWzV+Iv4jVC3DdpGqVyvlpYWtLe32zZOz5gxAwUFBTh8+LA4ybVUrosXo0aNwvjx4z0NXnoMyPXly3zxi1/ErFmzLLv3tMuzX3kZOnQoZs2aldD4izQtPxnTp0+37bb28ssvNzX+JmPChAl6N92nTp3ChAkTxCS6xYsXJwxevoeqEedpNd+Ojg6cO3cu4Q3lkpIStLa26g1FVrQGnZaWFnFSAjE/VnlyQ5yfH/NMVlDrbyvjx49Hb28v/uu//gvvvvsuTpw4gc997nOmt1M/97nPYc6cOSgsLMS4ceMwbtw4FBYWYs6cOfjc5z5nmp+qt99+Gw8//HDKG38PHDiAlpYWzJs3D4h3n19QUIBvfOMbuOqqq3DVVVfhy1/+MiZNmpSyt4CNtGXk5+dj9uzZ4uSUamxsxLhx4zBjxgzMmDEDkyZNQlNTk34Nob2dPHPmTMfzULfC4TCmT5+OxsbGhDeB07F8IiIiIiKibMM3gIn6WaqeQDkQfwP47NmzqKurw4EDB/Dhhx+ip6cHBQUFuPHGGzF48GDxZ75pb29HQ0MDjh49CsTffGxtbfV0o1zVlClT8Nlnn+GTTz7BgQMHUFdXh927d6OzsxOf//znfX/zOZl1ctrue/fuxdixYy0bP06ePIkjR47YNmYfPXoUHR0d0jehVaRivawY3wQ+f/68tPFXYxUTVcmsl4pPPvkEABy/79vb24vTp0/7Ug79Xpdkt59RYWEhpk2b5mmwa0RykivLd7ut7LoRtcuzSl5UWeUhFct3Gx/E3wAeOXIk8vLy0NnZqX+/WPu3OJw7d05/61EbWlpacPHiRduGPeMbwCNGjMDJkyf1N361hjLjG8DaG65Dhw7Vvx0s+vTTTzFy5EjLt2I1WpfHqvM1unDhApqbm1FUVJRw/hAKhdDR0SFt4NcMHjwYJ0+eRHt7u+V2VcmTuK5ivsQ3gJOZZzr4XX/LJLMfGGlvABcXFyM/Px+nTp3CuXPn9POT6dOnY9CgQfjkk08wbtw4TJkyBePHj8eECRMwYcIEjB8/HgUFBWhvb8epU6dcvQGsueGGG8RRvmpvb8c777yDyy+/HNdeey0AYMeOHbjqqqsSymlHRwcOHz6sp0uVmpoanD17FrNnz8YVV1whTnbkZbsfPHgQQ4YMwbR4TznHjx9HT08PLl26hI6ODr2O6uzsxLFjx5Jq3D969KjeoCsOWi8Vzc3NpjeBGxoafFu+xkuciCg4uC9TNmF5JiIVrCvcy8aY8Q3gDNXQ0ICNGzfi9ddfR3v8TU0iL7q7u3Hy5EmcPHkS+fn5uPzyy/H1r3/d8ka8H9rb2/H73/8ef/7zn/W3Iv/85z+jq6tLTJoyt956K/7u7/4OM2fOxPjx4zFnzhwsXboU1113nZg0kJYsWYKpU6eKo3VTp07Vv/lrZe7cuY6NkUGivQls1/gbZNdddx2+8Y1viKMTzJ07VykdEaXfmTNncOjQoaSHnp4ecZaOxo8fj9bW1oTGJs3IkSNRUFCA/fv3m8bbvYmo/eajjz7SxzU2NprOLd3OV0uvPeyi2bdvH+rr6zFo0CDL32quvPJKtLe3Y8+ePabxjY2NaGxsdJ0nK17Wk+SKi4uxZMkSy/OTlpYWHD58GG1tbfq4c+fO4ejRozh58qQpbZB8+OGHAIDrr7/eNH748OGmv63G+e3NN9/EyZMncfnll6e88bu/fPzxx7aD9mbvp59+irNnz4o/JyIiIh90d3fzfJiIKAeEWo4ejYojEX9aPhqN4sKFC+jq6sJsmzcZyB8NDQ3405/+hPHxb8INGTIEf//3fy8moyyzb98+2zeFKDs5bfdf//rXWLBggeXbu3V1ddi1axfuvfdecZLu3XffxenTp3H33XeLk1LGab22b98ujvJk8eLF4qi0yaZ10ThtPwoObit7ycSnsrIS8+bNs6x3m5ubEYlEcNNNN4mTdO+++y7a29ttz9/27NmDESNG4KqrrtLHbd++3VQHHDhwAJ2dnaZGqT179pgaNmfOnKl3Yax1vyx2aVxTU4Nz584B8YbmQYMG4cKFC6bY2M1XRkw/3vAdW215BQUFCQ1qRuI8hgwZgpKSEsvpduva0dGB9957D/PmzdO/1azlw5g3N/PMFsnsB0br169HNCq9VATi3Xrfdddd+N3vfochQ4ZYfrpi2LBhOHfuHL75zW+Kk/pVQ0MD/vjHP2L+/PmmOG3YsAFz5sxJaIB999138cknn+D+++83jfdDe3s7/vKXv+DTTz/F5ZdfjltvvVVMoszLdv+v//ovwNCbifb3ZZddho8//hhLly4F4nWU8W8/ffDBBzh9+jSuvvpq/Sl9cXni38nwEiciCg7uy5RN0lWeu7u7sWfPHnR0dGDChAn6ZzCIKDOkq67IJtkYs9oPP8TIkSMxcOBADMjLs3wDmA3A/aC9vR0ffvghLrvsMv3mn7Hx9ytf+Qr27t2LxsZGPPDAA+LPKctkYwXUXxoaGvDXv/5VHG3Jy00jr5y2+wcffIBJkyZZdlepdTVq1VABACdOnDB1KZoOTuuVTY2m2bQuGqftp2L79u04c+aMONrSqFGjUrLubusDAPjCF76QkrfPUxETlW3ldrkyKnmx0p/LV4mPKF0NwP1p3759GDRokKnxmbJXMvuB0YEDB8RRJoMHD8aMGTPwu9/9DuFwGFOmTNHPPQBg0KBBmDBhAo4ePYpIJBK4BuAtW7YgPz8/oVcO7S3cb3/72/q49vZ2vPHGGxg3bpynxlmRdl1YX1+P/Px8XHvttZ73Ty/bfd++fThy5Igek1deeQVz585FYWEhtmzZojd+b9++Hfn5+b73NCNr/EU8Tn4vP9k4iQ+TQOHBmSDbt28fWltbkzrWBoVsm2iMDwLJyB7KEu2LvyFnN58g0LalxulhLDuZss7wsC8TBVE6yrPW+NvT04MpU6agoaEB48aNYyNwFpIdH7VzFvH4n0n1PgCsWrUKmzdv1v9esGABXnrpJVMaK6tWrQIArFmzRpyUMdJRV2SbbIwZG4ADqqGhAe+88w4GDBiAc+fO4brrrsPYsWNNjb/79u3D3/72N1x33XUZ010tJS8bK6D+0tLSgkgkIo625OWmkVdO2/13v/udOCopI0eOxFe+8hVxdMo4rVc2NZpm07ponLafir1791q+BSYzbNiwlBzr3NYHABAOhzFp0iRxtGepiInKtnK7XBmVvFjpz+WrxEdUWVmJSZMmYejQoeIkIN6dbXt7OyZMmCBO0p0+fRp5eXmBbABubGxEfX296U1Zym7J7AfJMDYAywSxAVh7m/fWW29NqPdbWlrw5ptvYujQoZg8eTIA4NixYwDg+2dUGhoacPDgQUybNs22AcoNN9u9vb0d+/fvN73t/OKLL+rfa66vr9cbwt944w3k5+dj8uTJ+OCDD6Sx80Js/H333Xcxe/ZsPd5+L99NnIxUGgyDoLGxEa2traYGQNm4bOP2BrbK9nQ7z/6gfVrBuG2NZdztts+EddYkuy8TBVGqy7Ox8Xfu3LkYMmQIPvvsMxw8eJCNwFlI5RinEet9t8eNdLrvvvsAwNTgu2rVKuUGXT8bgF9++WW8/vrryo3Pfkl1XZGNsjFmbAAOoOPHj2Pr1q0YOHAgbrnlFtTX1+Nvf/sbBg4cyMbfHJaNFRA5c9ruGzZsEEcl5bLLLsN/+2//TRydMk7rlU2Nptm0Lhqn7UfBwW1lL5n4/Od//qc4KiljxowJxP4se+I7CPmi9ElmP0jGH//4R5w/fx6jR49GQUEB8vLyAAC9vb3o7OzEqVOnMHjwYPzd3/2d+NN+88Ybb2Dy5MmW11vam7na23STJ082NUYGmZvt3tLSgj179pjegm5oaMDf/vY3AMDVV1+t94yhdVPd3d2NK664QnkZqiKRCAoKCvQ3f9944w1cf/31eiOv38t3EycjNzdT+5Psxq1sXDo0NjYmvCHd0dGBrq4uT434MuINbCcq29PtPEWpXn/ZpxBEbre913W2kopYJLsvU+5KRTn0SyrLs6zxV8NG4OykcozTiPW+2+OGKq/7XyQSQWlpKaqqqhAOh8XJStLdAPzyyy/jnnvuMY2LRCJobm627V3MTirrimyVjTFjA3DAdHd3Y9euXTh27Bja29txzTXXYO7cudi3bx9OnjzpuvFXdlMvU7uekq2L3cWL0b4s6LIqGysgcpat291pvbKp0TSb1kXjtP0oOLit7DE+ROnbD7q7u3Ho0CGcOnUKXV1d6O3tBQDk5eVh+PDhGDt2LK644goMGzZM/CmlQLq2e6ZLNk5ON1MPHDiA5uZm/W+xC2Ltm+P19fVA/PxPm2dnZ6d+XTx79mwMHz4c7733nv5b47mi1uinMX5LXby+Hj9+PC5cuJAwTrsfAcMNXy1/zc3N+jfkxWtz7Roc8eWOHTs24bv1Gi2fxvzJxvlFXB+7OMGwPS9cuGBaJ2MacZ6QbGcxRhrZusrGebV9+3bL+0FW5WHQoEEJ66RtR7fr3NLSgv3790unaWTrLRvnVrL7MuUmWZmTjesvqSrPdo2/mmQagbUehowytUvhbGR3ziJuH+PfsuOGls7uWCA7xzGS7WuycU7C4TCefPLJhEZVo4qKCjz33HP638YGY1kDsF16xBtxV69erf/95JNP4vXXX8euXbv0ccuWLUtoVNYarIuKivD2229bjnMrVXVFNsvGmOVEA7DXp0bSpbGxEQcPHgQAfPGLX8TBgwfx0Ucf6Y3AiBdC1cZfOFTiQaLyxJC4LtrBRHbR4JVKftItGysgcpat2z1b1ytXcPtlDm4re4wPEfeDXMXtribZOInXrkb7JA8n19TUYMSIEfqyampqcO7cOdO1rnajdfbs2Zg0aZJ+PSw26hob7A4cOICioiLTPIzTZde9snHiDWAxf/v27UNnZ6eeD/FvreHP6XuzNTU1AIBrrrkG7733XkLDuF/E9XGKkxZ7Y+PpHqE7ZXGe+/btw4ULF/TpWgOIeKPbKNXrr5UZq/mK276xsRHNzc0JjeHjx4/Xvw0JxXXWbt5rZaalpQXDhw+3vJfjdyyS3Zf9lCn3Jt3K1vVCCsqhX1JRnlUafzVuGoG1GBrrkcbGRgCQ1iOUfk7nLLBoAIbkuKGlsToWQHIOYcXr/qc11soaXBFv4G1qatLfytUab7VPhIkNwE7pteVpf0ciEbz//vu45557lN4ABoCbb74ZAPD888+jtLTUMu+qUlFXZLtsjJlqA/AAcUSm6OjoQH19vV5paOPee++9hKeP+suBAwfwzjvvYN++fSgoKMCNN96IIUOGYO7cubjmmmvw0Ucf6RUs9bnqqqswZMgQNDU1iZOIiIiIiIiI+k1zczO2b9+uDx0dHQCA1tZWzJ4925R25syZaG1t1dMAQGFhYcKN0fHjx+sNKkVFRXo64/TOzk7976uuuso0D+2tTj8Y8zdhwgT9TWDE13HmzJn635MmTcL48eP1v61oDQTJ3Oj1QiVOBQUFpkauK6+8Eu3t7aZtZtTa2qp/Jxvxho4hQ4boDR8yqV7/q666CvPmzUNrayu2b9+OAwcOiElMpk+fjnPnzqGlpQWI30trb29PaOzT2K1zV1cXAOhxnjRpUkL5Nkp1LNItE+5NJiNb10uTbeXQipvGX8Q/ITZ27Fh89tlnOHLkiDhZp93LFt/YnD59umU9kg6yerijo0Ov63KR1TlLMuyOBRrZOY7I6/5XXl6OqqoqbN68GeFwGBUVFabpmzdvxo9+9CP973vuuQdFRUV4+eWXTek0Tumfe+4502f6wuGw7dvHMtqbvn40/hK5lbENwCNHjjQ9YaKdiIwfPz7hAJROH330Ef785z9j69atOHToEPLy8vDFL34RV199tSmd2Ag8d+5cXH311dizZ48vjcIHDhwwVfDiPGtqatDY2KhPR/zJoAMHDmDPnj36+JaWFnR0dJjmZSROM54c7tmzB/X19Whvb5fmwc6gQYMAh/kjftJhnK+2XjU1NfpvtIObXX7EeBkPiLJYERERERERUe4pLCzE4sWL9UF76xHxxi8j7W+tkQzxLoZF2vUvDA1psnRGxmvY+vr6hIbNZBmXO3z4cEC4gS6uozHvdkpKSlBYWOj6Rq9XTnEaMWKE6W8t/sZtptFi8N5775nuHxgbya2kev21e2SzZ89Gc3Oz/iazlfHjx6OtrQ0A0NTUZNmQ77TOkyZNwpAhQ7B9+3Zp44tMqmORTkG9N+lVtq6XUTaVQ5nu7m6899576OzsVGr8BYCGhgacOHECxcXFmDp1qjhZJz4MpMru3qvT/V+ne7PZ/tBCsmTnLMlwOhZoVMoZfNj/wuEwIpEINmzYgOeeew733XcfAOCdd94B4g2t4XBYH6xeMnNKr01P9lu9Rm+//TYefvhhNv5S2mVsA7DG61Mjfhs5ciROnjyJYcOGYf78+fj85z+P0aNHi8kAi0bgyZMn2z5lpWLfvn1obm42VfCdnZ0JDbD19fWYN2+eqaui5uZmTJkyBYsXL0ZhYSH279+Pjz76SJ9PQUGBaT5NTU36PBYvXoxBgwbp06+//nrMnDkTBQUFWLx4sattc+HCBf0tYKv5W6mvr8c111yDxYsXY/z48fjoo48Am/zsi3djpS1j5syZeM/wnSBtnmKsiIiIiIiIiNKtpqYm4Ro2E8i6oUylVMVJm59xUHnrLR3rP2nSJMybNw/t7e22b71NmDABp06dAgB0dnaioKBATGIirq9xnUtKSjBv3jzU19cnNOpYSUcs0ilo9yb9kq3rpcm2cqjRGn/b29tx/vx5/bOEdhoaGnDkyBHMmjULs2bNEifrrB4GcuJ071Xl/q/dvdlceGghCMTjgOrxT8aP/e+mm25CVVUVdu3apTfWIt5NszjYvbUrpnVKn6zy8nJxFFHKZXwDMHx4asRP06dPx5VXXokzZ84gEong8OHDYhITYyPwu+++i88++wyjRo0Sk0lZdeOQ6V1PaQf46dOnJzV/uy6rZPzqwoKIiIiIiIhyj/amrNjgluyNcjstLS04d+6c6bt8Tte8fjC+DWxkvD8QJKpxEu8v2G0zq+0cNCr3LiZNmqR3A23X/bPqOmuNLwUFBZZvWmW7IN2b9FO2rle2Mjb+TpkyBZMnT8aJEycSGlONVBt/YVGPqnC696py/1fl3my2P7TQX1SPBf0hHA7r/9baMIyNwXac0mvTte//EmWirGgAhk9PjfjlqquuwuWXX46mpiZ8/PHHeOutt/Dhhx/i8OHD0gPl3LlzMW3aNEQiERQVFeHLX/6ymERK1o2D1cVK0LueMjZmd3Z2mp7Ocjt/qy6rZPzuwoJIVbaehGbrehEFDfc1IiKS4fGhf4wcORLjx4/H/v37TePr6+tND1T7QbwJ29HRgebmZiEV0N7eLo6SjlM1cuRIFBQU6D1sIf69RS/zTCXVOLW2tppuaNttMy0G4na2a1hJtY6OjoTla98ANt4Xkm2n8ePH4+jRo5bdP0NhnVtaWkzx03pzy1VBujfpp2xdr2wjNv4OGjQII0eOtG0EdtP4myzVe69O939V6xY+tOAP43HD6ViQLpFIBKtWrTKN074BfNNNNyEcDmPBggV48MEHTWnE32ic0ofDYSxbtgwPPfSQPi0SiZi+J7xr1y7930RBlDUNwEFz3XXX4fLLL0c0GsWIESNw5swZfPLJJ9ixYwfee+89HDp0SD/QnTt3DhcvXsS0adPw9a9/XZxVoPnVpZKxMdvY+OvX/J2I3Vd46cKCiIiIiIiIcsvcuXNRWFhourk9duxY3xtORo4cicL455q2b9+Ojz76KOE6WXuzavv27aYetsRxbmlv02rr197ejsLCQuXvAKeTSpwQvxdx9OhRfZ1GjBhhu82uv/56FBQUmLazU/fJqTRy5Ei0traa8nPq1CksNnSRarXtJ0yYgPb2dkyYMEEfJ+O0zlqMtfjxXgpR//jggw/Q2tqqN/5qrBqBk2n8HTduHJDkm6DifVfjvVe/7//a1ePkTHbccDoWpEM4HMbmzZtN3+t97bXXTG/ovvTSS1iwYIEpzbXXXmuaj5FT+jVr1piml5aW6tPvueceFBUVIRwOWzYyE/W3UMvRo1FxJABEo1FEo1FcuHABXV1dmM2nZpKyPd418xVXXIFBgwahpaUFXV1dOHv2LKLRKIYNG4a8vDwMHTpU+c1fANizZ4/0wkT7xsHs2bNNT3u2tLRg//79+kVATU0NCgsLTSfmsnlu377dNK/GxkY0NzejpKQkYZ6IP6116tQpvRG3sbERra2tpm6XRLLlQpJnSOavHYS0p7rE9dLiMW/ePIwcOTIhP1bxMhLn6bd98e8/ExH1N9ZHlC1Ylom4HxDZ4f7hn3379mHQoEEJ1/MUfMb7O5mK+zJlE6/luaWlBe+99x4GDBggvYfZ0dGBY8eOYcKECRg5cqTrxl/Nnj17AMNDQTLG+7VO915V7v+m+t4sUSbxWlfkomyMWe2HH2LkyJEYOHAgBuTlISQmiOMbwCl2ww03YOjQoTh06BAQ74LniiuuwJw5czBu3Di9O4XrrrtO+GVyMqXrKRWq83criF1YEBEREREREWUS7QHroqIicRJlgObmZowdO1YcTUQZatKkSZg3bx4uXbqkf1vXyPgmcLKNvwBw5ZVXor29XW8I1jQ2Nlou1+7ea6ru/xIRERuAU27YsGH40pe+hFAopDcCA0BbWxtaW1sxYcIEfOlLX8KwYcNMv/Mi6F1PqVKZv1uy/AShCwsiIiIiIiKiINuzZ4/purm+vh6LFy/GyJEjxaQUYPv27cN2he6uiSjzODUCnz17FqFQKOnGX8Tv12pv6xqPCc3NzZZv6Nrde03F/V8iIophF9BpcuzYMezevRtDhgzB4MGDcerUKRQWFuKGG24Qk1KOycYuCIgoM7E+omzBskzE/YDIDvcPouzAfZmyiZ/lWdYd9IkTJ3DmzBnMnj076cZfIup/ftYVuSIbY8YuoANm8uTJ+PznP4+uri6cPHkS4XCYjb9ERERERERERERE5BvxTWA2/hIR5SY2AKfR9OnTMXfuXJSUlOCaa64RJxMRERGRD7LtyU4iIiIiIiI3jI3AbPwlIspNbABOs+LiYkyePFkcTURERERERERERETkC60RmI2/RES5iQ3ARERERERERERERERZZtKkSWz8JSLKUWwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLKEmwAJiIiIiIiIiIiIiIiIiLyIBKJIBwOY9WqVeKkBDfffDNuvvlmcbRv2ABMRERERERERERERERERORBOBxGVVUVNm/ebNsIrDX8vv322+Ik37ABOE3C4TAikYje+v/OO++ISaS03/WnIOSBiIiIsk+y50dEREHG6yciIiIiIqLc5dQInI7GX7AB2H8333wzwuGwPoi0mwE33XSTOIky3Pbt222HPXv2iD+hHGWsI8LhMCoqKsQkrvFGIxmJ9Y84sD6idLvvvvtw3333iaN1mXZ+xDqX0kmsw8WBdbqzcDhsWQdxf85s4v4gDtw/iPs4kb+M+xT3LyJ/aPuS3YPRdtOI0sGpzrebnqvlN2zRCJyuxl+wAdg/WiG+44479Aq7qqoKL7/8spiUstjs2bOxePFi6XD99deLySmHVVVV6XVFeXm5OJnIM9ZHFBSRSARHjx7F0aNHLS8GiMge63Tvjh496stDdxQ83D+yl3afRRuMD3LY3WQkIjVOL7EQUXKM+5U2qDR8acc27cFo47FOnEbkB6eH9f2Sy+U3LDQCp7PxF2wA9s8TTzyBhx9+2NSQEw6Hcc8995jSaeONlfc777xje8LV3NxsO33VqlX6NPGD0S+//LLpt8YGaeOyjb+777779PS8SUKUXnb7s7YPG/dn7aYIAJSWlqbloE1E5MbWrVtxxx134I477sDWrVvFybqwcCNXPB8xTpfVh8b5iNPEv42MyzFelMvmwzqXKHM9//zzeO6552xvvhnrGfFvWZ0g/m3kdA1nV/fIrtGIck0kEkFpaSk2bNiASPzBWTboE/lDO6flSyxEqWN88SNXG74o2CJ8WD9twoZGYKSx8RdsAPbPrl27cNttt4mjlfzoRz/SDwYPP/xwwoW+3fRVq1ahqalJn75gwQLTzcj3339fn/bkk09i9erV+jQY5q0VOu1VdO03lLzGxkZxFJEtp/0ZAF5//XXT/my8MVlVVYWXXnrJlJ4IrI+on7322mu47bbb8MUvfhGvvfaaOFlKPB85duyYmCShPrSbpp0PbdiwwZR21apVKCoqQiR+0+tHP/qR7XxY51IQsE5P3pNPPokHH3xQHK1MrBOs6hYoXMPZ1T3iNRqp4/6RPZqbm1FUVGS6YV5eXo6I5GGs++67z9Rw9c477yTcV9FYPXzh9GA+UTZReYnFal+xwn2ISJ34sLNROBzGW2+9lXCs06Zp16NhycOJRuIyjL8lgsLD+mIZEjlNF6mW32w9nmjrn+5rPDYA+8BYcJPx/PPP6/8uLy/XG4BUpm/evBkPPfSQPv3BBx/Erl279L/XrFmj/1s7kTPO+4knntD/jfj8jDcg2DVtcvbt24f6+nrTDYiWlhZs377dlI5yV2lpqX4g0y6mnPZnxG8IwmJ/JpJhfUT96Z133sGUKVMQDof1G7gqN5DE8xHj+YzGrj4Up2kNPloejOdR2rRwOIwpU6bYzod1LvU31une3HPPPVi2bFnCA3aqxDrBqm6BwjWcXd0jXqORGu4f2UXbr8T91XjzUHsY6/bbb8frr7+up6mqqsJ3vvMdw69i7B6+ePDBBxExvKlFlM2cXmKx21escB8iUiM+7Cwzbdq0hGOdjPhwokZchuyBaiK7h/XFMiRymq7CqvzyeOIvNgAHUFFRkTjKRJxeWFio/1trhNZ2DmN3srIGauNvNbJ05M7cuXMxc+bMhBsQRBpjVzDGp9rt9meiZLA+ov5UVVVl6q7xjjvuwAcffGBKYyXV5yNa3Wp8IGfXrl1obm4WkxIFBut079asWdMv3wPWruFU6h7ZNRo54/6Rfd5++21cf/31CAvf/xXdc889pgdnd+3ahWuvvdaUBgoPX6g8pEaU6bQyb3eu7bSvWOE+RNTHeK5n3N/Eh529vHwlPpyo7afiMmQPVFNuc3pYXyxDYjm1mx6J99aiDeLb6Rqr8gseT3zFBmAfhMNhFBUVWRZmNyKRCJqamsTROtl02Y3KcPytQmN3sionaxB2NtXfUKLp06fzBgS5ZrU/E3nB+oj6y+bNm/Hcc8/pJ/7PPfdcwpOlVlJ9PqLVrfw2E2Ua1uneqXwP2E/GazjWPanF/SP7aN0+FxUV2V4XLVu2DO+8847phqaRdi5h9fBFJBLBgw8+aHujkigXOO0rVrgPEZmJ53pG4jEqFdKxDMpcKg/rO5Uhq+nheG8t2mD8vIAKHk/8pdQAHAqFxFEkeOKJJ7B69eqE/spVCqmxi68NGzZgwYIFph3IbvqyZctM3YutWrUKy5YtA+LdXRmpPOW+YMGChOVR8ow3IE6cOCFOJjKx259VOF2QUW5jfUTp9vLLL2PBggWmE/9IJIIpU6Y4Nrqk63xkwYIFSc+bdS71J9bp3oTDYf17wMbelYqKivTvX6lcO9kR6zDjNZyXuoeccf/ITmvWrMGCBQss77Fce+21qKqqwgcffIDbb79dnKzvf+INeePDF9q41atXO56rEGWqsMNLLCr7ihXuQ0RqIil+2BlpWgZlLpWH9Z3KkNN0L3g8cabaZqvUAAwA0UuXxFFkcNNNN6GqqgqrV6/Wd5wf/ehHSk843H777fpvdu3aldCvv910rQsHbXpTU5M+Tlu2Nk3FSy+9hKNHj+q/kXWbRO5oNyBaW1vFSUQmdvuzk2XLluHBBx+07RqNiPURpdPrr78uvQF7/fXXmx52kUnX+chLL72EXbt26ctRrUNZ51IQsE73RvsesLF3pSeeeEK/EeKV3TVcsnUPqeP+kflkD9Tv2rULkyZN0v82PoyldQP92muvWd6HUX34YsGCBeIooqzi9BKL6r5ihfsQkTW3Dzsn8+Cx22VQblF5WN+pDDlN9wuPJ3KXXLTVhlqOHo2KIwEgGo0iGo2ip6cHZ8+dw4wrrsCgwYPFZORROBxGVVWVLzcZKDhaWlqwf/9+cTQAYPHixaa/9+3bh7lz55rGERH5hfURZYNIJILS0lLfnyolyjSs04mscf/IPjfffLPpIY0nn3xSb9xdtWoVNm/ejAULFugPWKxatQoQvnUo3nMxzlP7rXaeoXn44YcTvnVHwcR9OXliuS8qKsLbb7+t/y3bVyDsU9q/Ee8yWsN9KDksz9lDdp/feAwz7l9PPvkkVq9enbBfhcPhhGOdbP/TliX+bbcMymxe64r77rsPt99+e8IDcxUVFdizZ49e3zuVIafpIpXyixQdT7zGLGguXLiA+kgEw4cPx4ABA5CXlycm0Tk2AF+8eBHnzp3DuAkTMHbcODEZeSQWdiIiIiIyu++++1BUVKTcKwIRERHlnlWrVuHaa69NuKFJRESUy/hANVF2OX3qFE60tGDYsGGODcD2XUDH+5HOy8vDZydO4FJvr5iCiIiIiMhXq1at0p8KDce/U8bGXyIiIrISiUSwa9cuNv4SEREJnnjiCSxbtkwcTUQZ6NKlS/jsxAnk5eUhFAo5fgvY9g1gALh48SJ6e3vR3d2N0WPHYnJRkZiUiIiIiIiIiIgo7bQuMjds2ICbbrpJnExERJRTtOOiZtmyZXygmihLHD92DCdbWzFkyBAMGjQIAwYMwIAB1u/5WjYAI94I3Nvbi0uXLuHc+fM4292NK668EsOHDxeTEhERERERERERERERERGRj7q6uhD55BMMHzYM+YMGIX/gQAwYMMD2LWDrpuG4UCiE0IABGJiXh8GDB6Ph0CF0dXaKyYiIiIiIiIiIiIiIiIiIyCddXV2oj0QwZPBgDBw4EAMUun+GUwOw1of0gFAIeXl5GJifj7xQCAc//hjNTU38JjARERERERERERERERERkY8uXbqE5qYmfLJ/f6yNNv7Wr9ObvxrbLqAR7wZa6wq6t7cXPRcvoufCBVy4cAE9PT2YXlyMgoIC5OfnKy2QiIiIiIiIiIiIiIiIiIj6RKNR9PT0oKO9HY0NDRgQCmHw4MF6t89aI7D2Aq+d0MWj+6OtKBDH6y5duqQ3Al+6dAk9PT242NuL7u5unDt3TkxOlHNsn6CQsN8l08dtvimIglKachX3IiIiUsVjdmBwU1hSO7ORBVDtl/1Llm+Sy4TtGXyBKHHclP3ALuiBKBWK7NaDiIiI0mnokCEYNmwY8vLykJ+fb2r8HTDAtpNn9TeAo9EoLkWj6L14Eb29vTh37hwu9PSIyYmIKK0y6SIy29gePomIiAyy43idFUe+7NgUKaG+fY1BVP9V6nHj+idI2zWz9Wup5GZMq37d1inBAkRERBQE+fn5GDJkCPLy8pBn+P6v0hvATg3AkDQCRw1vAhMRUdDYV/zkN8fDKBER5bzsODZn9BEvOzZBSqlvXy2Y6r9ID25kfwVt+2amQJRKbsq0cd7e2sZwThkMLDxERET9TXvzNzRggKvGX6g2ACPeCKz9/9KlS4gC+tvARLnGbqdx3u36j12+KdsEuSRmI+5dRERkJzuOyxl7tMuO8Kdcxm5fHTe0/zK/VARBIEomN2W/MW9/44YIRMlQwMJDRETUX7S3fkOA3vUzAKXGX7hpANbI3gYmykVWO47arpd+VvmlbBbU0piNuIcREZGd7DgmZ+zRLjvCn3IZu30BbuSUy+zSETT9Vlq5GftN3zbXNkK/lYIksfAQERH1h2Te+jVy3QAMQyMwAP1tYKJcIyv37na/9JHllXJFUEtltuFeRkREdrLjeJyxR7vsCD8RkTcZW4lnh8w+FLHwEBERpVso/tYvEHvj123jL5JtANYYu4XW/k2Ua4L8/Cb3SlITxNKbabi3ERGRnew41mbs0S47wp9ywd++3JDBEPySkgn6tTRzE/abft3unrHgEBERpYuxwTeZhl+NpwZgIzYCEwUP90hSl/yBhMC9jYiIHGTHcTZjj3bZEf6UC/725YYMhuCXlEzQ76WZm7Ff9fv2TwoLDRERUTok+7avjG8NwEQUPNy5yR1/Diy5i3scERFZyY5jbMYe6bIj/CkV/G3LjRgswS8xmaDfSzU3YyD0ezlwjQWHiIgoU8Q6kCYiIuKFHBEREVFOiQbqDDBkM1CwiNuH24qIiIiIKGhcvwEcjUbR0dWFi7296Ll4UZxMGS5/4EAMzMvDyOHDfXvN3I2Bgwah6+xZnD93DmfPnRMnU5oNHTIEg4cMwfChQ9Fz4YI4OYFWP/SyfiAiIiIiIiIiIiIiIkpa/sCByEuyzc5VA/CQESPQ3NyMMWPGYNSoURg6dKiYhDLc2bNncebMGZw+fRqFhYU419kpJkmdvDycPHUKkydPRkFBAfLy8sQUlGa9vb1ob2/HsWPHMG7sWER7e8UkuvMXLqCzuxuDBw1C0ZQprB+IiIiIiIiIiIiIiIiSpLXZnTx5EiOGDcPgQYPEJJaUG4Cj0ShOd3Rg6tSpGD58uDiZskxXVxeOHDmCMSNHun6qIBkDBw3C8c8+QzgcRn5+vjiZ+llPTw8ikQgmXnaZ9E3gaDSKU2fOYPr06awfiIiIiIiIiIiIiIiIfKK12Y120Wan/A3gjq4ujBkzho07OWL48OEYM2YMOrq6xEkp0XX2LCZPnszG34DKz8/H5MmT0XX2rDgJiNcPgwcNYv1ARERERERERERERETko2Ta7JQbgC/29mLUqFHiaMpio0aNwkWbLn/9dP7cORQUFIijKUAKCgpw/tw5hICEobe3F0VTpog/ISIiIiIiIiIiIiIiIo9GjRqFAS4+narcANxz8SK/6Zljhg4dip6LF8XRKXH23Dl+89el557731i27A4sXHgj1q59Rpzsu7y8PJw9d04cDbB+ICIiIiIiIiIiIiIiSpmhQ4eiu7tbHG1JuQGYiILhxIkT+Id/uBfvvvsX/Ou/PoOJEyfitde2YO/ePWJSIiIiIiIiIiIiIiIiyjFsAKaMceTIEXGUo2R+46fOzk4cPXpUHO3JM8+sQX19PcrL/xmzZs3Ct771bXz72/fiuuuuF5MSERERERERERERERFRjmEDMGWEI0eOYP/+/Th48KA4ydLBgwexf//+fmsE7uzsRE1Njas8O3nnnXfwl7/U4JZbbtEbfO+66248/PD/LSYlIiIiIiIiIiIiIiKiHMQGYPLV4z/8AZbdfSce/+EPxEmeTJ06FTNnzkR9fb1Sg+rBgwdRX1+PmTNnYurUqeLklNMafwFg/vz54uSkHDx4EBs2VAIA5s9fIE4mIiIiIiIiIiIiIiIiSkUDcAM2LA0jHA5j1XZxGgBsx6pwbLo2iOm2rzJPt0onTStLRFlh1qxZSo3AxsbfWbNmiZNTztj4W1JSghEjRohJXKmq2oqFC2/Ef//v96O+vh4A8NRTT2LZsjvEpBnOqe6I277KZl93rl90PsynYcNSH+oftWXBRX2n52vpBjSIE2Gz7g0bsFTIizxfKnlWSaMWQ5U0gM16xTnPRy3PRERERERERERERERB5n8D8PZfY03tMixbBmx+M/HO+fZVy4H1EUQisWH9MmDz8qXYILZSzFmFP8TTaMOaxcYEscai5QeFdOZElGWcGoGzrfEXAIqLw/jZz/4Vt9xyCwBg5syZ+NnP/hWPP75aTJrZHOoOvYF4+WZxgk6tfvFnPg0bluJra4BVf9DSrceyzcsljYp2GrBhqWxZYsOji/quYQO+twZYtmyOOMV53Wc8iC1CvRuJRPCHVXMALMOti6GYZ5U0ajFUSeO4XkrzUcszEREREREREREREZFbP/7xD7Fw4Y3Sti2jTZtewcKFN2LTplfESa743gC8/c3NwLJbsebWZcDmNyHeN1+8xtyQu/gfV2EOarH1j2ILsL2GDd/DmtplWL/lQcwQJ1K/eeonP8XmV17FUz/5qTjJN1aNwNnY+Iv4+t50003o7OwCANxww4246aab9G8AZwunuiO2z8/Bqj/8AatkbZuK9Ys/89mOX6+pxZxV/4YH9QpoMf5x1Rxp3q3NwINbZMsCDtaLeVap7xqw4XtrgFX/hn8Mi9PU1j1RbF2x7FbEsqmSZ5U0KjFUSaOyXirzUckzEREREREREREREZF7P/7xT3DLLbfgv//3+y0bgTdtegUVFf+O8vJ/xl133S1OdsXnBuDtiLXhLAYW34pl2IxfJLzaKzdrpn2zhlkD/ri1FnNW/WO8QYJyjdgI7Hfjb2dnpzjKVqoaf40++mgfAGDOnGuAeIP3c8/9b/z4xz/UnwQ5ePAgfvzjH2Lt2mdMvzVqaWnBhg0b8Oabb4qTEvz2t7/Fb3/7W3F0CjjXHTMe3IJIZIuhAU+dsX7xZT4N9TgoqbdmzJwFYDOkLzAnTb2+0xqKv2uxcsmse8OGX2Az5mDVPzot3SWVGKqkUVkvxfkQEREREREREREREaWKXSOwn42/8L0BePub2Kx3E7oYty4Darf+Uf4NSkB/W612zioktC3UrsHXDN9hXGpqDGpApBZA5NfC9yrFrl5z08GDB7Fw4Y348Y9/KE5KsGzZHb5+S/bxH/4Ay+6+E4//8AfiJN8ZG4H9bPwFgN27d2Pnzp3iaKl0NP7u3btHb5S+6aabAADHjh0DAPzlL39BRcW/Y+/ePfjudx/Gtm3b8NZb20y/N5o0aRK+8Y1v4NNPP7VtBNYafr/97W+Lk/znuu5QYVO/uCKZT0MEtZiDsNjgOCMM6QuobjREUGtqrFSs7xo24HtrarFs/RrHhmJ1scZnLPuudeMqZHmWENOoxFAljYpk5yPmmYiIiIiIiIiIiIjIA1kjsN+Nv/C3AbgBG34R68JVa3xYHGvFgbl35/i3GsNhhMNfk3ZrunhN4vcna9d8TWgEBmoPhvFvero/YNWcWqz52ioX3a9mp1mzZuH//X9fxLZt22wbgbWG382bXxMn5bxZs2bh5MmTjo3A6Wj8BYCPPvoIADB37uf1cTfddBMefvj/xre+FWug/Zd/eQwPPvgQdu78C95807oBGAqNwGlt/FWuO1Q41y9q/JqPW9uxavlmQNJo7VTfbf/1GtQuWy98K92j7b9GrPdnu5la57mPSpqgycQ8ExEREREREREREVHQGRuBn3vuf/ve+AtfG4Ab/oitYkPB4luxLOH7vrHvLPY17h7E8oQ3fM1mPLgF6yVvBM657e8MDTIz8OB3l7E7zzinRuBsaPw1dvss+yawF1OmTMG1115r2wicrsZfAKitrQUAzJmT+L7iNdfEuoSeMGGCq8rBqhE4vY2/buoOFe7rFzm/5uPO9lXLY90t/1tiY7Ntfbd9FZZvXob1vrb+xhvmHRpA7fKsUUkTNJmYZyIiIiIiIiIiIiLKDFoj8G9/u9H3xl/42QDc8MetqAWwebmxi9Ll2Aygds2vLd/KnfHgv2HVHPs0utqIfZewTt155hirRuBUNv4+9ZOfYvMrr+Kpn/xUnOQr8Zu/4jeB/WDXCJzOxl9Ivv9rdPnlUwEAXV1d4iRHYiNw2ht/PdQdKlzVLzYS5jMjjDmoRUSskKy6GlawfVUYyzfPwao/2HzL1shQ321/czOAzVhu6CL6a2tq9a70k2q41t7+/a51A6hKni3TqMRQJY0Kl/OxzDMRERERERERERERkU9+/OOfYOfOv/je+Av/GoC170SuN3XdHIlEEFmv+FbunLBlIwPQgPqDxjQzEJ6T+Eaw1c38XCY2Aqey8TddxMZfTboagdPd+Kt9/3fEiBH693+NXnzxBQDA8ePHceLECXGyI2MjMNLc+OtL3aHCtn5xQZvPjJmYBeBgvblFsaH+IIBZcPvJ2FiDI7BsvazB0bm+E7vNj721PAeYswp/iESwJXGmjmKNytp3mRPZ5znGNo1KDFXSqHAxH9s8ExERERERERERERFlAH8agO2+E7n4ViwDsDnWTylWhYVv9MZ/q3dv2rABS5duMDV0NGz4nvAmWrz709o1+LU+s/j3Gpd9lzftBcZGYKS48ffxH/4Ay+6+E4//8AfiJF9YNf5q0tEInM7GXxi+/3vjjTfq406cOIGDBw/inXfewb59H+Lb374XALBnz3v4/vf/B/bu3aOnVTFp0iQ8+OCDaW78dVN3qFCoX5SozGcxbl0G1K75HvSXaxs24HtrajFn1T/q3zJW0bBhabzBMWLx/d5+qO8aNiDW+7N8XZzzrJJGJYYqaVSozcc5z0REREREREREREREwRdqOXo0Ko6UOX7yJObOnSuOBvQ3ppZhfWSN9Ia8cfqMDUtjXZMamG+2N2DD0q/BnEQ+7wZxXsvWI8K79r7at28fJo4bJ4629PgPf4CPD3yMz131OVfdQNuVL41T46+Rm7Sqjh49ivfffx9DhgxJW+MvAHz/+/8Df/lLDZ599he47rrr9XEffbQPw4cPx+OPr0ZnZxf+5V/+J0aMGIEbb7wRP/7xT8TZ+MKqPKhsPxmvdUdM3+8T6oSE+kWeJsbdfGB4W1QzZ9UfXL5tux2r4t1dJzJ3QZyQJ4f6rmHDUnxt6234w5a+LpwT5qEzbwP77aKSZ5U0sb9UYuiUxt169U01z0c9z0RERERERERERERE6bZv3z5MkLTRyPjSAEzZy6rBz0qqGoCPHDmC/fv3u2rQ1RqBZ8+ejalTY9/J9ero0aMYPXp02hp/AWDhwhsxd+7n8atf/Voft2nTK9i1axe+9a1v6Y3Ca9c+g2HDhuHhh/9vw6/9ZVUenLYfERERERERERERERERJY8NwOQbqwY/v6mUryNHjrhuyE3mN/3tnXfeAQDcdNNN2LTpFVRU/Lvp7d/+ZFUeVLYfERERERERERERERERJcdNA7A/3wAmSoNkGnKT+U1/OnjwIP7lX/4n1q37d+zduwcbNjyP8vJ/DkTjL7mxHavCYYRtB+E7w0RERERERERERERERD7gG8Bky+qNT7+xfPX5znf+Efv2fYiJEyfiwQcfQmnpbWKSfmNVHrj9iIiIiIiIiIiIiIiIUsfNG8DKDcCnzpzB9BkzMHToUHESZamzZ8+isaEBY0eNEif5rr2rCzOvuAJ5eXniJAqI3t5e1B86hILhw8VJrB+IiIiIiIiIiIiIiIhS5OzZs2hqasIIxXYY5S6gB+bl4cyZM+JoymJnzpzBwDQ1yA4eMgTt7e3iaAqQ9vZ2DB4yRBwNsH4gIiIiIiIiIiIiIiJKmTNnzmCIRRuNjHID8Mjhw3H69Gl0dXWJkygLdXV14fTp0xgpedszFYYPHYpjx46hp6dHnEQB0NPTg2PHjmG4xZMlI4cPx8mTJ1k/EBERERERERERERER+Uhrs3PzyqZyF9AAMGTECDQ3N2PMmDEYNWoUu3vNQmfPnsWZM2dw+vRpFBYW4lxnp5gkdfLycPLUKUyePBkFBQXsDjoAent70d7ejmPHjmHc2LFAb6+YRHf+wgV0nTvH+oGIiIiIiIiIiIiIiMgjsc3urIs2O1cNwAAQjUbR0dWFi7296Ll4UZxMGS5/4EAMzMvDyOHDEQqFxMkpN3DQIHSdPYvz587h7Llz4mRKs6FDhmDwkCEYPnQoLl64IE5OoNUPobw8dHd3i5OJiIiIiIiIiIiIiIhIwbBhwzBkyBDkAa7b7Fw3ABMRBRkrNKI+7k4J/JNN+2F/xTAXycoN4+8fWXw1/Rlnu3xlFy3K6V5j/7ZuunOuzL9VTLv+j2kGB4+o3/T/nptKaa0VsjuUWSN9ZYIFgoiIyG/K3wAmIsoEIQ5JDZSd+usSmmWKksFyk1pBjW9Q80Vm/XU8yVZRxpQog4lXUtl1RcX6ifpP9uxHREREQcEGYCIi4qVWFuuvmzgsU0TBE9Rb1EHME/Xpj2NINmM8ibJVdh3N0lJXBfXEhPqR+GAFCwgREZEXbAAmIiKAl1aUAuKlOy/hicgK64dgSksDQA5hPImyXXYdydJWZ4kXC9kVRvKMBYKIiChZbAAmIiLKAWm7gUPkAe/9pQdj2x9YC1PQsCYgogBjFUUmLBBERETJYAMwERHpxMaXVA3UP4LS/JBJZUDrQjsosSPyS1Dr5KDlx1+ZU5Ow3stWQd3zibKJeOXDfY7IH9yPiIiI3GIDMBERpR0v3fpPUG7qswwQkRXWD/0rCMcIIqLsw6Oba2w7pwTigxUsJERERHbYAExERP2Cl2kkXrbz8p2INKwP+gcbf4mIUolHtqSIFwsMIyVgoSAiIpIJtbW1Zc11figUQltbmziaiHxy5swZTJ06VRyddaLRKEIhXkCkG+OeOowtEeUq1n+UTixvRESkgscLbxg/bxg/bxg/bxg/bxg/b4IUv7OdneKoBAPz85GXl4e8gQMxIC8PAwYMwKVLl3Cptxe9Fy+it7cXF3t6xJ+ZZNUbwA0NDeIoIvLRpUuXxFFZKRrNmudiMgrjnjqMLRHlKtZ/lE4sb0REpILHC28YP28YP28YP28YP28YP28yJX55eXkYPnIkho0YgcFDh2Jgfj4GDIg15Q4YMAAD8/MxeOhQDBsxAsNHjkReXp44C11WNQDnSuMUUX/JlX0sUw4G2YZxTx3GlohyFes/SieWNyIiUsHjhTeMnzeMnzeMnzeMnzeMnzeZEL9BQ4ZgeEEB8gYOFCdJ5Q0ciOEFBRg0ZIg4CWADMBG5kSv7WK6sZ9Aw7qnD2BJRrmL9R+nE8kZERCp4vPCG8fOG8fOG8fOG8fOG8fMm6PEbNGQIhgwdKo5WMmToUGkjcEY3AF+4cMH0d9A3IFGmy5V9LBOeBspGjHvqMLZElKtY/1E6sbwREZEKHi+8Yfy8Yfy8Yfy8Yfy8Yfy8CXL88vLykm781QwZOjShO+hQW1tbcNfaxoULF9DV1YUxY8bo4w4cOIDJkyeb0lFw1fz+IfzLQQCzHsbbX/+COJkC6NixY7jqqqvE0b7a/eydeGaHODZm0aOv4pH54lj/nT9/HoMHDxZHB9xuPHvnMzCFbvq9WPfzpSgyjguwIMfdrlxOv3cdfr402FEOcmwp+9jtL0Dm1U2U2Vj/qbPfdxfh0VcfQRpOwzIayxuRQdMWfH/FRjQax/EcgAgI3PGiCVu+vwIbIds/7ab1n2DFT7D7Wdz5zI603b9KRqDjp4kfQxDA+y1Bi1/sHF5+rq6f3y96FK8GpEAGLX7Q4nQkWPWcleDEr+8+tNV90aYt38eKjY0sfxbOdnaa/h4+cqRyt892ei9eRFdHh/53Rr4BrDX+inLl7cSscKoaLxwEvj7rBuDg7/B/TokJKIjSt48twqOvvopXDcO6e6djxzN34tndYlr/pW89/dG05fu4885ncOTedYaYrcO92IgVd34fW5rEXwRT8OOeWC5fXXcvsHEF7kxHwfQg+LGl7CPZX7QhAy6qKHuw/nPLat9NvKFEiVjeiGKatnwfd8Zv3Gfy9QlRqvB44Q3j5w3j502mxK9py/fxzI7YyzRBaXxDBsUvqIIYv8aduyE7tWv61PQYYCAEMX4AMDA/37Hxt6GhAVu2bEFDQ4M4ySRv4EAMzM/X/864BmCrxl8E/BVuMvv00Hs4iBuwaH4hZuFTbD90TExCAdSf+1jR0ruxCMCOd1Pf0Naf6+la0xb8+8ZGydNWRVj680exCI3Y+O9bpAfioMmouGuKluLnjy4CdjyTlocTkpWRsSUi8gHrP0onljei2NtvKyyvT9bh3umN2PifAT5xJkoDHi+8Yfy8Yfy8yYT4xd68BO5dF7w30TMhfkEWuPgtWoRFjZ9K7jvvxrs7FmHRInF8/wpc/OLEbptFtbW12LBhA/bs2YPf/OY3qK2tFZOYGOeXUQ3Ado2/CHALPon+io1/+RSYdR1Kxi7BA7OAgwf/ik/FZBQ4QdjHpl+e+vfGgnowkNn9nxvRiEW4W9LVBjAff//ooxnRhQkyLO4m8/8e904HdrwS3Ib2jI0tEZFHrP8onVjeiIDd7+4Apt+Lf5ZenxRh/sLpWHR5UWDPm4nSgccLbxg/bxg/b4Iev77G359DeijuZ0GPX9AFL3434IZFO5Dwvtbud7Fj0Q24QRjd34IXvxint3//8Ic/6P8+f/686W8Z4/wypgHYqfEXAWmcIgWH9uL3AL4ejn33tyR8A3ByMzYeEhNS0PTnPta05RXssLyR4K/+XE93duPdHQCmX27ZwFs0f77ltKDJnLiLilA0FYD0ibdgyNzYEhF5w/qP0onljSh+fTK1yPIapGjpz/HIUuvpRLmAxwtvGD9vGD9vAh2/3c8GuvEXQY9fBghi/ObfsCihx87d7+7AohsC9vp5QOMHAANs3gDesmULTp48aRp38uRJbNmyxTTOyDi/jGgAVmn8RYA3IJnVRN4FcAMWXREfccV1+DqA30f+KqSkoEnfPrYDz9x5J+40DCs2NqatgS2oTwNZsrnBkkkyLu4ZhLGl9Eusx7UhyN2lU/Zh/eeWbN99Ftxt1bC8Uc5rasKRNPXaRJTJAnm8aNyIFQnnACuwMXifcAxm/DII4+dNYOO3+1nc+cwOAI3YuTsdd0+TE9j4ZYhAxq/ockzf8a7hmnE33t0xHUE8HQxk/AAMGCBvpn3vvfewZ88ecTQAYM+ePXjvvffE0YAwP/mcA0S18RdpbZyipJ2qxgsHEev+WR/5BSyaBeDgXtSYElPQpG8fW4RHX30VrxqHdfdiOnbgmTS0HAT1YJDtGPfUYWwp/ST1eHwI2jeIKLux/nNLtu8+Au62aljeiOR2Pys2Kn0fW4J7b5oo5QJ5vJh+L9YlnAOsw73TxYT9L5DxyyCMnzfBjN8OPPPMEdy7LrbPNm7898AeZ4MZv8wRyPgVzcfC6YZuoHe/ix3TF2I+G4A9OXnyJN566y1xtMlbb72V8HawKNANwG4af5HWxilK1qeH3sNBADj4HG5+9iF9+JeDAPAuXnjvmPgTCpB+3ceKluLuRQBMTxSlRr+upytFuHw6gCNNaXkzOtUyJ+6Zh7ElolzF+o/SieWNcl5REWJfRjFfncx/pK9BaV0QW5OI0ozHC28YP28YP2+CGr9Fj/4cS4uKsPSf78V0NGLjimD24hPU+GWKYMavCPMXTte7gd797g5MXxjMTxIGM35yb731Fjo7O8XRJp2dnY6NxIFtAHbb+IsM24C56a/Y+JdPgXHL8JtHnsfbpuEn+MdxwMGDf8Wn4s8oMIKxjx1BU4pbOzPnaSDnb882bfl+xnS5mjlxF8W/dbbohsC+IZW5sSUi8ob1H6UTyxtRdj2gSpQqPF54w/h5E7j47X42o3qGCFz8AACLoH9utWgp/vne6bG3ggN4MzCY8cscQY1f0fyF8W6gY90/Lwzi678Bjp9Me3u7OErKKV0gG4CTafxFhm3AnHRoL34P4Os3LMHl4jRMxsJZlwMnN2PjIXEaBUUg9rE0dCERiPVUNP/vY11jvyI9U27C7p2NwPR78fdBbZk0yKS4m+x+F7H23+AGOWNjS0TkEes/SieWN6IiLL17EdC4Ef8ZvHvORIHB44U3jJ83wYxfI4TOIwAAU4tSfAMwCcGMn1nR0n+Odd++45nAvRCSCfELssDGr6gIU3EETVuC2/0zghw/iWXLlqGkpATXX3+95VBSUoJly5aJPzUJXANwso2/CMzbiWSlJvIugBuw6ApxSszl876JrwP4feSv4iQKiH7dx3Y/i2d2IC1dSPTreroVf7KvceMKfN/UCNyELd9fgY2N03HvPy9Necz8kFFx1+x+Fnc+swNY9Gigv2uakbElIvIB6z9KJ5Y3IgDzH8G6e6djxzN3CtcnsW8Br9jYmJaHeomCjMcLbxg/bwIXv/l/j3unQ+8+FgB2/+dGNBrfag2QwMVPqghLf/4oFgHY8UywuoLOjPgFV3DjNx83LGrExo3B7f4ZgY5fonHjxuG2227D0qVLLYfbbrsN48aNE39qEqgGYC+Nv8iwDZhzTlXjhYPArBtLUSJO030Bi2YBOPg7/J9T4jQKgvTtYzvwzJ134k7j8MwOLHr0Vfx8aeoPIZn0NBAAFC39OV5ddy+wcYUhZiuwEfdi3as/RxpC5ovgx926XL4a5NbfjIgtZR/J/qIPmdO9F2U+1n+UTixvRDFFS3+OV199FFNN1yd34pkdi/Doq6/i1Z9nxgOqRKnC44U3jJ83wYtfvLFyxzPC8eKRQH5mK3jxszIfjzy6KH5tHpxG4MDGr3EjViTcu0h8mK2/BTZ+AObfsAgI6Jv7miDHL1VCbW1tgVjrZBt/x4wZo/97x44d+PznP2+aTkT++fDDD7FoUawyz2bHjx/HxIkTxdGUYox76jC2RJSrWP9ROrG8ERGRCh4vvGH8vGH8vGH8vGH8vGH8vAlS/M52dur/LjC0cfql/fRpIEhvAA8aNAhjxoxxPRil7+1EotyUK/tYrqxn0DDuqcPYElGuYv1H6cTyRkREKni88Ibx84bx84bx84bx84bx8yYX4xeYBmA/5OIGJEqnXNnHcrE7iCBg3FOHsSWiXMX6j9KJ5Y2IiFTweOEN4+cN4+cN4+cN4+cN4+dNLsYvMF1A++GLP71bHEVEPvvgB6+Io7JOU1MTigL8vYJsxbinDmNLRLmK9R+lE8sbERGp4PHCG8bPG8bPG8bPG8bPG8bPmyDFL11dQIcARNva2vTWb9n/ZeOCOO3jjz/Go+8+DyJKnWdueEgcRURERERERERERERERA7mzZuHwQMHAg4NwJFIBLt27UJTUxPa29tRUFCAoqIiLFiwAOFwWEyu0xuAs+kN4G3btqFt4kJxNBEREREREREREVEgPPjlyeIoUnT48GFMmzZNHE2KGD9vGD9vGD9vGD9vghS/w4cPOzYAV1dX489//rM4WvelL30JS5YsEUcDhgbgrPoGMBERERERERERERERERFRJopEIraNvwDw5z//GZFIRBxtwgZgIiIiIiIiIiIiIiIiIqJ+tmvXLnGUlFM6NgATEREREREREREREREREfWzpqYmcZSUUzo2ABMRERERERERERERERER9bP29nZxlJRTOjYAExERERERERERERERERFlCTYAExERERERERERERERERFlCTYAExERERERERERERERERFlCTYAExERERERERERERERERFliVBbW1tUHJmptm3bhraJC8XRRDlp+Im94ijPuiZcJ47qd7mynkHDuKcOY0tEuYr1H6UTyxsREalI1fHiwS9PFkeTosOHD2PatGniaFLE+HnD+HnD+HnD+HkTpPgdPnwYgwcOBAAUjBkjTsbjjz8ujrL01FNPiaPQfvo0wAbgfrTrUTy08iVgzhN46pcPYYI4new1PY+nv/Uj1ON63PMfv8NXi8QENPzEXnzr778hjk7af/znG4G8qZUr6xk0ORn3NNXbORlbIiLWf/7j+bItljefsbwRUZZK1fGCDcDJC9IN/EzE+HnD+HnD+HnD+HkTpPilqwE4q7uA/mhtIR5aVIiH1m4XJwEATmz6Zmz6Pz2PE+JESp+m5/H0okI8tOibeKtJnEheRKNR3wZV+n5nGr6Jp9duT9l+JubVy2BFul7/9E38ZleDmDTAGnBi16N4+p/M6/H0Pz2Kt5JYDzF2XgaZXK7Dxfh4GawYy/TTm4Ttv+tR29gTEaWKWId5GayYj+lW55/b8Rvj8bK/68MUnS/n+rFALDNeBissb5oGvCWcgz60KH4+vSl11wmu+L3efs+PiPqNWOd7GYiIiIjSJasbgK9ZdF/sH6//Hh+JE9GAfX/aAwCY+ZWvpuxNrmzk1ChDwRH1cfBmD+pfvw+Pp6ihTsyrl0GuAcdl7aO1e7Bj5UL8Zpc4IYga8NY/LcTjK19Cfa15Sn3tS3h55a8k9aQ9MXZeBplcrsPF+HgZVNT/wv32JyJKBbEO8zKo2YP3aiQH+V2/xw7heOlGJp4v5+KxQCwzXgY1LG8Javdgxy/uw+MZ3kia0duAiByJdb6XgYiIiChdsroBGAu+jkUAgJfwV7GBpuktvFcLAPfhG3fNECZSWhU9hMd2NOP5HewqzHfilYaXwa3bX8LzO5rx/I5mPPXdeENe7Y/wprgv+kHMq5fBwczv7oyv107cMyc2bseO4N/o+WjtQrxcCwDXY9F3d+Kp+LZ5fsdOPLX2PsyMr4srYuy8DDK5XIeL8fEyOJg553oAL+EN8c0vIqL+INZhXgYHsfpP1vDZgLdefMmUpt+l+Hw5Z48FYpnxMjhgeevTdz7dHDsPBQDswctPpeZhUWV+r7ff8yOi/iPW+V4GIiIiojTJ7gZgLMYXbo/9S2yg+ei3P0I9ANz+dVxjmmJ2YtOj8W6bYl03id29JnanKuvCqgEfrY13VbqoEA/906P46Igpgc68vMIkus3VutZ6FB81mbsSi83LnJen15ovshPXx5gmNu9nX48nfv2+hKec7fO/Hb9ZFOuu9aNdWrpH8ZGkayz7fKiwi0PifBKXJ9uOmUfsasjL4MWEu7SGPDPnuFuUGQCIb1cEYD1nTtcaIPu6tjO9Fax1oRh/A9rqDQG9S2Ov+5Q+Pa7pebwR328Xrf0d/uGuGYY3ZmdgwoJn8Ngvn4nXhVbzNO9TSEvc3dfh9vFyUy+4qLe9lGMLYny8DE6m3F+ORdIb0maJ6ynGzS6+zscfOG4/IsoFYh3mZXD0ldvlDxoZHjKa9xXD+Dj7+jCTzpf7qB4LIF2ueNzLHGKZ8TI4YnmTmrDgGTy2VntY9HXsM7wFbJ934MSu5w15klyrW17Lq663+dzmLel5jM02SJhfTGIsxX3I7pzKe8yJyD2xzo9Go/jZmmdMw1NPr8FPf/Y0fvLTp/Djn/wUP/jxj/H4D36I//kvq90dL4iIiIh8kp4G4KYt+P6dz2K3OD4N5F2IbsdftcaQRYv1saITm76Jx3/xUqyRAQCwBztWrui7CN70TUl3qvEurAwX3R+tXYhnX491VQoAqH0Jz/4i9pS30UdrC4XlwUO3uS/h2W/dZ+pKrP71+/D4InNe6l//kSGv2/FmwvqIaawp57/2R3h2pTmdmbd8mMniYJ6P6nbMROKDpl6G5DXgo00V2AEAuB6Tp8TGuop7QpnZjt986z7sqI29JSHm1cvgpP4XC+M3YGJv1M68/SX8Xy7fQJXXS31dGmv1km/71NFIfNp9+MICcaIFy3nG9ilIYudlsCKPlbwOV46XQr2gWm97K8fWxPh4GZwtxq3fdXrzy029LIuv0/HHzfYjomwm1mFeBmdfjdd/5geNtIeMZn73O5hrSB3jpj5MpFzXOR4zvOUjkcqxwOVxLwOIZcbL4IzlzZLe68seHDsaG+WY96bn8f+s/JEhT3uww/BJE6dreUBlvTWxc5uXxfMYMY4K3O1DsnMqn2JORK6IdX4UwP98dCUQjSJ6KYreixdx8eJFXOy5iAsXe3DhwgX0XIj9/2dP/dTl8YKIiIjIH2loAN6NZ1dsRKM4Ol1kXYju+n28McquMWQ73vxF/PuSWhdV//GS3uWrdPqOZjwVv6jH6xXxi8u+hgr5fOL0N/Suxz3/Ee+a9T9eiuVdeBJa2Zz78Mh/mLuqBa7HorWxfOh5bTgUv3BdjFvXvoSntOUbu+5tOIQTmIGv/rIZj8TfyNO7+F252H3+b38p3gWt9tahkVM+XDLEQc+7Ph/V7ZiZxCdUvQyuaU+/L1qIZ+Mxxu3l8e7Pkoi7scw0HcJRxOaHfl7P+tfvw//j9iaMtF76VbyL5ni95OM+deLIgdg/5oQxMT5OfwtZHyRvpFrNc84TQLriLo2VpA53Gy+HekGp3vZajoVJRmJ8vAwqJtzl9OaXy3rZ7fHH7fYjoqwl1mFeBhUTSm6PdT+bcO5+PeaVyB7wcqoPM/R8WelYkMRxL+DEMuNlUMHyZmUGJhvPs1Tyrj3gOOc+PBKfbnutLj2Xc1pvgzlPxM9tDGW+9nXsa7LZBgkk+XLah2zPWYkoXcQ6XxtWPboSPT096Om5iJ6eC7jQcx49Fy7gwoULOH/+PP716Z8l/IaIiIgoXVLbALz7Wdx55zPxG/X9JbEL0Y92xL+x9N3vWF/kaQ1Mxu9LFi3GV38Z/36PoQHC+P1J7caJ/vSy1Xzuj18wa/Q39Pbg5W/FG2S+dV98GX1PQrux6P5ncE0RAMzA3K/ELypvL8c/LIjlY8LUq2LjaiM4Hv/NhCnAm0/1dW31uOSNNylX+b8e93x7saEL2kRJ50PCGAf9bUKN6nbMUNGof4Mnc+INP9qNENdxF8pM0RWYgthNEqR5PWU3a+plN2tsaW/Z2NRLPu5Tsn3dmfU8F93/EJC2uCvW4a7i5VAvqNbbXsuxDTE+XgY1zm9+uamXXR9/XG4/IspeYh3mZVBS9FXMmwMAe/BeTQNOaL2WzLkdcy2+2emmPjRxVdc5HzOSzoclh2OB6+Ne8IllxsughOXNQgOOGd+IVcm79pBg7Ut4dlEhnn7q95j4eLwR1+pcTruW1zmvt2bR/Q/Fz208lPkk9iHbc1YiShuxzjcOqx//F1zoiTX6Xjgfa/g9f/481j7zTEJa5eMFERERkQ9S1wDctAXff2YHpt+7DuvunS5OTStTF6JNTk9Zx+kXnTmk6Xk8/a37sKPW0O1pfwhKPrKA+KSpNqxZ+3N9+NnT/4onfvJT/Mvq1fj+ypUJaZN+SlV7+n1HM57/5e/0hh9/aG8JxMqImNd0rafdzRon5jdA+t5ysK2XkjUlHFuW4S3aa1bGt432zbUkiLFLVdyTqsMznBifVMXWaMJd63DPHIs3v1gvE1GaiHVY6uu/GfoDPvW/+BXe1D7HcP9D8kahoNSHKcqH7bEgC4llhuXNQqrzoTeM9n0uxtli/MOOnXjku/dhJoD62pfw7Lfi39rNxWt5Ikopsc4Xh58+8QTOnz+PC/Hh3/7X/0pI4+54QURERORd6hqAi5bi56++ip8vtXiUOZ0MXYi+8ZTzU9aAucFEfwK+aTve+qdHYxeVsulA31PcCd1LC/N5UXhiWp+foZsrw/APll1V+0jsRsvYtZcTP/PvJR9uud6OmUV80lQbVv6P/4GLFy/i3Nmz6OzqREdHOzrOtOOZNfInVH2/RvEa93h3yTO/uxPox/U8scn6ZtWOHfGwn24AAP/0SURBVNvjXdtK9neY3wB5+Vuxb7+Z6iU/9yl9WcCOld/Eb3ZJ3upxYceLzwPpjLtKHe5nvHSq9XaS5diGGJ+UxdZEuyn9Et54Md5tuCbV9XJKth8RZSKxDktL/Wc4zsS+tWlTf3upD/2s67zkw5bNscDFcU/71MTTsjeJA0QsMyxvFrzkw8GJXY/i6ZXxcyzt/E4l77sexdNrGzDxrmfwmP7Jidib1dKyaryWT8KOF5/HR00A0ICPJGVeiSxfFvsQEQWLWOfLhtjbv7FBnJbU8YKIiIjIo9Q1AAdKXxei9fGnlmd+5avyp6w1RQ/hG9pvfrFQ73bq5dr4jRDZ9EWFeFz/pk+8a1JZum/dF//Wp4GeztDNlT5Ivs2ZCtoFabwbrdj6JDZcTZyufaMo/o3Xtdv9zb9iPnwh2z6y7Zihojb//c9Vj6Kjox3tZ86gvb0dFesqEtIY//OVT3Gv/8VCIM3rac5vvFzq3zY2dHf7+n143Gp/B0xvgGhMb3/4uU9hBr76y5ewKH5jbMfKvnV4SLvh5kbtj4C0xl2hDvczXrLyKduOsnRJlGMZMT7G//yNrWDBd2Jvfolv+KS6XvZz+xFRRhPrMON/qav/+o4zAIDbv25dfyvWhxl9vmx1LFA+7jXgeLxtq74x4A3ANv+xvBko5kOVqfysfCn+tu59eOSX8XNhxbzXa+fbixbq52lTps6Ql1XjtXwyan+EZ78VW9az8TJv3HbSbSCS5Uu6DxFR0Ih1vuy/8xfO64M4zfgfERERUbrkSAMwcM23n4g/bYuEb+5YuWblTjxy+/WG312PRd9dp3836JqVfV1O6eLfOn3MMP9rVu7EPbfHLwgRf3L6P16KP/ndJ3F5aVb0EP6vtcb1uR6LvvtEQj4n3LXOtD4zp8fW1bf8K+bDL6rbMROJT5qKw7/+6xp0tLfjl7/8VcI0cfCbp7jrb07EiHkVB+/rOQMTZVmacz0WffclPKV92zi+fzyisL8D4nokPvHv2z4FxLrJ+2U85vG3gTUz59yHe9aq33Ba9N3YDT8xduLgPe59VOpwP+Plqt5OthzbEOMjDn7G1mwGvvq4MdZxaaiX/dx+RJS5xDpMHFJV/12zSKvjYt8EtaRYH2b2+bLFscDFcU87b9LWO6jEMiMOLG9xivlIinY+vSP+/d44x7wv+I5wzh0rh9qbzYm/N1/Lu7Xou9rDlDEzb0+8BpBtA5HqPkREwWKs73/+8/+Fn//8f+FnP3saP/jBD/G9730P0Sj0b/9e4BvAREREFBChtra2lJ9+NG35PlZsnIpHX30E88WJPtq2bRvaJsbeCCTKdcNP7MU3S78mjk7a76r+gK4J14mj+8VHawvx7OuxLqCfvOlUBq9nA976p/gbC7e/hOcNN5GCpy+vi9Y24x9nZG/56m/ZvO8SEdlh/UfpxPJGzsznv666zSairCE7Xvz0yZ+iu6sbXV1dePbZZwEA/59/+AdcutSLS9FL+O1v/48pvZF2vHjwy5PFSaTo8OHDmDZtmjiaFDF+3jB+3jB+3jB+3gQpfocPH8bggQMBAAVjxoiT8fjjj4ujLD311FPiKLSfPg3k0hvAmW87fmPq+ko2uOzKi7Ke+KSplyGI9C6gJflNdkirprfwXry7ukWLgtz4KyfGzstAZmJ8vAxERJlErMO8DEROxDLjZSAiouwl1vmrH/8BTp8+jXXrntXHvfj/+w1+89JvsXHj/0lIz+MFERER9Qc2ABNlsWg06tsQJFr3vFrXaWJevQzpdKLm9dg3z+Y8kdD9cyYQY+dlIDMxPl4GIqJMItZhXgYiJ2KZ8TIQEVH2Euv8aDQa/zxA4ningYiIiChd2ACcMRbjH3Y043nbwfzdJKKoj0OwzMBXV/4Oj+1oBiR59TKk04S7fhfbd3/5UAbsuzPw1V/G6hqt+zsxdl4GMhPj42UgIsokYh3mZSByIpYZLwNlo8TzXyLKTWKd72UgIiIiShc2ABNlMfFJUy9DkIl59TKQOjF2XgYyE+PjZSAiyiRiHeZlIHIilhkvAxERZS+xzvcyEBEREaVLWhqAi5b+HK+++gjmixOIKLXER029DEEm5tXLQOrE2HkZyEyMj5eBiCiTiHWYl4HIiVhmvAxERJS9xDrfy0BERESUJmlpACai/iFeZ3gZgkzMq5eB1Imx8zKQmRgfLwMRUSYR6zAvA5ETscx4GYiIKHuJdb6XgYiIiChdQmfOnIkauyGR/V82LojTPv74Y7RNXAgiAoaf2CuO8qxrwnXiqH6XK+sZNIx76jC2RJSrWP9ROrG8ERGRilQdLx788mRxNCk6fPgwpk2bJo4mRYyfN4yfN4yfN4yfN0GK3+HDhzF44EAAQMGYMeJkPP744+IoS0899ZQ4Cu2nTwMAQm1tbbEW1Cywbds2NgATERERERERERFRYLEBOHlBuoGfiRg/bxg/bxg/bxg/b4IUPzYAJ4ENwESp9dCiQjy/o1kcnXVyZT2DhnFPHcaWiHIV6z9KJ5Y3IiJS8dCiQjQ2NoqjiYiIKIewAdilbdu24c477xRHE5FPQqGQ3u16NsuV9Qwaxj11GFsiylWs/yidWN6IiEgFjxfeBOkNrkzE+HnD+HnD+HnD+HkTpPil6w3gAaFQCDB8X/fSpUu4dOkSent70dvbi4sXL6Knpwc9PT24cOECLly4gPPnz+P8+fM4d+4czp49i7Nnz6K7uxvd3d3o6upCV1cXOjs70dHRgY6ODrS3t6O9vR1nzpzBmTNn0NbWhtOnT+P06dM4deoUTp06hZMnT+LkyZNobW3FZ599hs8++wwnTpzAiRMncPz4cRw/fhwtLS04duwYjh07hubmZjQ3N6OpqQlNTU04evSosIpERERERERERERERERERLllgPbEWSgUQigUwoABAzBgwADk5eUhLy8PAwcORH5+PvLz8zFo0CAMGjQIgwcPxuDBgzFkyBAMHToUQ4cOxbBhwzBs2DAMHz4cw4cPx4gRIzBy5EiMHDkSBQUFKCgowKhRozBq1CiMHj0aY8aMwZgxYzB27FiMHTsW48aNw7hx4zB+/HhcdtlluOyyyzBhwgRMmDABEydOxMSJEzFp0iRMnjwZkydPRmFhIQoLC1FUVISioiJMmTJFXDciIiIiIiIiIiIiIiIiopwyQBxBRERERERERERERERERESZiQ3ARERERERERERERERERERZgg3ARERERERERERERERERERZwtcG4PpfjcDo0aPiwwj8ql5MAWDbMEOaURhdni+mICIiIiIiIiIiIiIiIiKiJPjWALytfBSufQx4+v0zaGs7g7ZNl/DYtaNQvs2YaBhG35WPBzbF07R144EXhqWpEbgO6xaGEAqFsLxanBZTt24hQqFYmlAohJAkYfVyw/RQCAvX1YlJAEk6cV7Oy6rGcuN0m3zbU5+PU541et4XroN07auXy39ftw4LhbzI86WSZ5U0KnGWrHfCeqktC7BZ9zhxWVblJ+PFt7U5DGpxVNlmgHOs/ZaQr1AIodBCWG5ChfyJ5cEuLeVqHZ4ODrGtXo5QaDlkk7T1jMWxbz6Wg1McJWnM6Wz2OUPMZdvV/bKMg2S51csTx8vGGcjnLTvuSEiOoelYT2k6yfzgIq00nWTZfazKqIsyZ7NtpPmR5Fuv16X7g3FfsKe6PGk6lWVIyoo8zxbLkOSlj9W2sGAZd/VtJ82jShwynvpxxOmYpdFjaVXnWJ27SMuULF8qeVZJI9nukkQJ652wXmrLAmzWPU5clpvyF1sX2T4oqTdk+0yydY90u5nnkRBny1j2kf8mcT+XpxPm7cP6Wi1HjIk0nWR7S9OJeTSSxFklf8Y49KWxWY7FeY7K/NVjql43J5BtSwNX+wEREREREfnCnwbg+sFY+wIw/+lufGdmfNwt3dj0APDC2sGIvQg8AL9amw/MP4dHbtF+2INHnu4FXhgsf1vYT9VrUV5ThrIyoPK1xMuOunULES4HKiJRRKNRRKNVKKssNV3gVC8PobSyDFXReJqqMtSUh4WLldhFU2ltBSJaumgU0fVL+lIoLasUqOr7fVUZUFlqfUElV4d1C2XzEW9+OOe5L+k63F8OlJWViFP6LhhLK8UJMcUrsNM4//gQqSgBUIY7lkAxzyppVOMsbNNoFcpqyhHWL5jVluW47rJlSctPtlKLo8o2U4l16hjLShRVZTUoD4v7pUr+XOxzFJOTdXiaOMRWXTFW7DTErKoMQIkhTsY4xuJsjqMhltIbhABQg1e2yoNYt+5JyPe6ZJalsq8nyzzvaDSK6M4VKBaTGVQvDyEULsccQ5mKRiO4+xVj+fW+npEKoDwsHt8AlBj3h/j8TI0DKVw27MqomzIn4y7fdQdr4/+qRKk0o07cLQ8QYx8bdq6wLi3yshJFpKIWpZ63md22cMvtthP2m1iBsW2kymxq500qx6y+pDyHly3Lcd1ly5KeP6ROMnWPel2AxP0r6nxcEn9jXYe7n3cy62tfVyZT36mtnzzO4vEZCfOzjkMy5zlwnL96TN3WzUREREREFGT+NAAfysNuALOLL5lGX3FlL7A7H2+munFXQfVrlUDZHVh/RxlQ+ZpwkVeNteU1KKl4EX331JZgZUVJX9q6dXiyEiipWAn9kmfJelSVATWvbDU8vXs/ymvKUCW9oIPasgAsWR+F8dpqycoKlNhcEMrFLuAS5wPUHjTcAnTMs6YO6+4vBypexMrZ4jRtPiWoiERQIbu3JBWLB8ruiMdVJc8qaVTiXIeDtTAs25CmZj8igOKyFNZdsfxkL5U4qmwzhVinkWy/VMmf+j5Hmtysw9PDPrap0bef7DTEEQCWYH2kAiXSG5RlqKgoQU35Wkke67D1lRqUVFSgTJyS1LLM+nX7VS9HaSVQVmUuU1q9qt3g9mM9i1esRhmcGva04+Qr0MKR6mWnqowml+9YOUTlk64fCEhueerq1i1EaWXsRr14f754xU5zY0CSeUnVtnCteAV2RipQUlOO+91uiIygct6kcszS8Bwe0mUprLvi+UPqqdc9buoCv9jV4clRX18nydZ3RtL1Uzw+q0vuPEedfzElIiIiIqLM4E8DMACgF1deIY4zuoTvrOwBdg/Bs3q30Pl49rE8YH4PbtXeHE6JasTuVy0BltyBMlTiSeNVT91B1AKYM8t8kVY8aw6ASrxWDSCyHzWSNOHZxhsN2oWZ4QaBSGVZNsTfeaeQ5zjtJtNqi4vZ4hU7EY2KF9b2Yk8yl6BipdPSXVKKczFmzQFQe9D0RszWV4w3s9Q4rrtS+clxSttMIdb9wJhn5/yp73OkYR2eOg6xTQmtnl0t30+KV2B17C5rwg3QWbfdjRJZnKvXorymBHffNkuYkPyyZNK//eqwLtbyAPvDpL/rWTI7LI4yiZV3TaqXnaoymny+Z614ERUlNSi/X3yLzk7yy1PjMH8Th7SWeUnVtkhSPJ/yxpJcoHDMiuM5vDXHdVc6f0gPtbrHYf9OscQ6PHlq6+vEIR6W9Z1c3/qpHp/dcX+e444/MSUiIiIiokzhTwPwFb2YjzxsedM8u0Of5AHIwyeH4iNu6Ubb++ew/65RGD16FEaPHob9T3eg7Q/nkdr239dQqXdPtgR3iE9sR/ajBiVIuF4Nz4b+ILjx3waxmxG1iD1IHsH+GgD71wrfATJ0G6myrASxp/Zr/LjATLiJoZBnALFu42pQVrXe1U0Vew4X5JqEPEuIaRTjvGR9vLu40EKsq6vG8lA49iaF+Li8kbgsFRbb11x+cowYR8VtFiTVa8tRo9ctqhT3OerDOjx1nGKbErE4290kDs8ukdeNxbfh7pLEN4xibyXKjiUelmWQ3L7uh3iZnDPL4W0tn9ZzeSkqUYK7b7NfWl9Xkkj9slNWRr3kuxgrYi2PWCvepLfkZXkK6rbiFYf590kyLynbFsmT5jNbiedNKscs8BzeRFyWCovje/+cwyvUPa7qAv9Y1uGeKKyvoyTrO0Hi+qken11yfZ7jlh8xJSIiIiKiTOFPA/DM81j5ALD7sWF93/LdNgx3vWBOtq18FEZfm4+l759BW9sZtLV1YOmWkRg9ehj0l4J9F3861/A0+JLYHSu960Il2sXYk8L3055M/BJPTe1svGj4BlBFSQ3Kw7JvC9mJf48qFEJIu6HhubuuaiwvlT+p7JTn6rXlqCmrSuhGzJPqtYj1HGc3U+s891FJY2UJ1kerUIYalIdLUQk43CBLclkuyk9uSDKO/a4SpYabrLFVcH7zRsZpnyMN6/DU8Sm2bsXf7kpO/MalsfvCePec0mNJ0svyb19PZJ53QmONhN2Na8DH9USV/Ztw6GtM0m9Ep3TZKSyjSec7Lt4FbGWpYt2Q7PJqyhF2UV6MDVt16xYafhfq+15uUnlJ4bbwwPw2ejazPm9yOmbxHF6T5LJcnD/YE+v+EEKhWL5dUax7lOoCnZg3+3omRqUOT0ynNm8DxfW1rCuTqu+QkG+r9XM8PutU4+DyPEenOn8XMU0JMZ+h5PYDIiIiIiJS4k8DMIBbKs5g0wN5eOza+Nu9a3vx/vvnMF/rGrp+MNa+AMx/uhvf0V/3vYTv/KEbDyAfa3/lW1bM4k9Bmy6YltyBMtff8ivGip3ak+baxUoY++eUAZgD44PkJXffZrjJH7+Ik3XlZCv27aDYzZwoIhW1KA2FsNDySs6Z9uRyxYuJjRC2ea5ejtJKhyfqXVPrNssuzxqVNFZiN0RKgSotziWoLA0hZPEdqOSXpV5+ckHycexvZajSb7JGEY1UAOVhyY00Z7b7HPVhHZ46vsXWpeJZUGuysagbhTzWbX3F+u3qpJfl376eSJi35IayqGa/QyejPqxnpKIEqCyF9PBn3G/C5UBFBFHtnCCVy05lGU06331i3xNV7AY52eWVVCDiorwYv20a69o29rsq40cjk8lLKreFB+a30bOX3XmT7TGL5/C65Jelfv5gT6z7o4hGq5L6nqtK3aNUF+jEvNnXMzEKdTiQ5LzNVNbXsq5Mpr4DlNfP8fiscxEHN+c5OhfzV41pSoj5jCa9HxARERERkTNfW11vqdDe7D0T69b5UB524xKKZwI4lIfdAGYXXxJ+1Ysr5wO7P8kTxvujbusrqAFiNwSEp0z1b4aFZ6MENUi4fkvogmwJ1gsXLCtn1wIls2H77G9CN6QqyzIrXvEiKkqS/85Z9fIQSitLUBGxvxjUGfJc/VplwtO64fIa/YZwUg0a2psDq61vwqjk2TKNSpzjbzGVVET0tyKKV+xENPZIdMJFvuWylCVZfrKMZRxVtlnQFK/AixUl/rwBZdHFYK5jHZ46SrHVWXSNaPGtRnthxD6dKAaxTyTWX6PFdol3PVu+FtWoxtryGqEBxMjrsuL83NddieXf/J1LGe/rWbxiZ+yNINNbbnHCjfWd5so7Zct2V0bd8p5vrVzUlN9v/aaVzofl2Yk3ctjNv4/7vKR2WyQvEuuD1UUjXOaxPG+ywnP47D+Ht6t7XNUF/rCqw31jt76O3Nd3Ivn6qR6fk+HmPCdJnmJKRERERESZwtcGYNG2rfnAAz24Bdp3goH9deIi8/DJbmD+lb3CeD9o36eqMl2wR6PR2A0C7en4+IWy8Ulp6G8V2N1Uis2/74IsfoEpfg/NeMMi6WXF2VycWond9ADKqmQ3PZzzvGS9EDvtSej4DWHzjWA1sRtS1t9TtM9zjG0alThbfQdM0hBnu6ykieUn+9nGUWWbZQXnfY40rMNTRzG2sLkZj2TLbTFmzYG5e0OjeFeHdnWj9ubKa8tj3yRdnVChaLwvq38V47a7SxS+1efPesa69HValihVy3ZRRpPiT76LV6yOdUG79jVxksCf5VlbgpUVJdbzN3Gbl1RviyRp+fSte/bgsT1vUjhm8RzeYVlJE88f0s+67nFTF/gnsQ73l/X6OnFb38klrp/q8Tk56uc5yUs+pkRERERElCnE1tgk5aN89CiMLs/Xx9T/agTueqEXTz/SExsh+04wBuBXXxuGF9CDld8R3wz2gd33qZbcgTIAla9VG56yNTwBqz9ZbnVTqQ7rFoZRjgq8qF+QxbtdM10Ixr83pX0rT2lZ1VgeEr7JE18Xp4tTUd26hfGbHlGLb3+p5NlnDjfsnPOskkYhzloZEJ5Wr15bjhrDjS3nZSVDVn6yiKRRyDmOCtsscGJP5bvbV/phn8tUrMNTRzm2AIpXYHUZUFkqfE+ubh0WJllul6zXvtsoxKluHRaGy1FT4lA3at9krKw0fZNUxvOygCT3dX9ob49Xloakb7Vpb/D5sp5LVsaW5fItrpQs200ZTZIv+cYSrK8qAyorHb9h6M/yrMXKSg3Kw2JZqYPYU7KrvKRhW7gmy2eWcT5vUjlm+Yzn8JCfP/QH67rHTV3gG7EO9531+jpxVd9Zkayf6vE5KS7Oc5KXfEwBANXL7b81TERERERE/a+trS3qy/D+2eh8RKPQhwvRTWKatrbo+09fNKSJRjH/bPR9Sbpkhk2bNkWNqsoQBcqiVaaxfcTpsb/7hpKKiCF1JFpRYp6OMvmcIxUljunslyWZBxCVzMZBVbRMmEffUBI1LjJheQ4Li1SURFFSETVFSJyHPpi3gRh3M5U8q6SJz80hzvJ5GfMmm564LOd1Vy8/QQZAHGVgjpU51mpxjCpsM+dYeydbT8vlCtvRMp2Qv4R0GVge/CbG3b6uSJxuX3bU90GVbWO/LMk8kqrD/QOPsY0ms05VZQn7t0iMoyyWUX3Z8vyY8xCra2TzcLesxLQJ5UC2flVlib8zLMdy3sLxVEb2W1n+3a1nYhmIjReObwr5i/q8bFkZNJJOl20ThWle8x01zEMsJjKulqcYexNZObSYj0pepLE2sJ0uy4tkGXbbR1b2oRjrqKT+ywzq500J8XEIjKxcJcxDH8zb1XZbK+VZJU18bg7HWfm8jHmTTU9clvO6q58/RC3Km3XdITlmSfYF69871D2y/U9121vUGVGb/EiPH+J8xXn7sL6yMi0jlimIsY+zWr64fubx1vOVTRfjIFum9jun85xk56+RxdQwUbrOUVk8ZOUt4RxIlofEdSLKBZAcL0hdY2OjOIpcYPy8Yfy8Yfy8Yfy8CVL8Ghsbo8eOHo0eO3o02tXVlTCUl5crD+Jvu7q69HmH2traomKjcKbatm0b7rzzTnE0EfkkFAohdq2S3XJlPYOGcU8dxpaIchXrP0onljfKFdXLQyitrUBkp/X3wInIGo8X3hw+fBjTpk0TR5Mixs8bxs8bxs8bxs+bIMXv8OHDGDxwIACgYMwYcTIef/xxcZSlp556ShyF9tOnAf+6gCYiIiIiIiIiouxWjdcqgbLVbPwlIiIiIgoyNgBnpGosD4UQsh2EbxwREREREREREXlQt+5JVJZV+fhtbSIiIiIiSgU2AGekJVgfjSJqO6wHr8eIiIiIiIiIyC/FK3YiytZfIiIiIqLAYwMwEREREREREREREREREVGWCJ05cyaqvTUKQPp/2bggTvv4449x1113gYiIiIiIiIiIiCiIGhsbxVFERESUQwYPHAgAKBgzRpyExx9/XBxl6amnnhJHof30aQBAqK2tLdaCmgW2bduGO++8UxxNRD4JhUL6QxfZLFfWM2gY99RhbIkoV7H+o3RieSMiIhU8Xnhz+PBhTJs2TRxNihg/bxg/bxg/bxg/b4IUv8OHD6elAZhdQBMRERERERERERERERERZQk2ABMRERERERERERERERERZQk2ABMRERERERERERERERERZQk2ABMRERERERERERERERERZQk2ABMRERERERERERERERERZQlfG4DrfzUCo0ePig8j8Kt6MYVaGiIiIiIiIiIiIiIiIiIics+3BuBt5aNw7WPA0++fQVvbGbRtuoTHrh2F8m3u0qROHdYtDCEUCmF5tTgtpm7dQoRCsTShUAghScLq5YbpoRAWrqsTkwCSdOK8nJdVjeXG6Tb5tqc+H6c8a/S8L1wH6dpXL5f/vm4dFgp5kedLJc8qaVTiLFnvhPVSWZZKGrX8ZIX4tjavns8xsipnKZKQr1AIodBCWFQBSvlLKHs2aSlX6/B0cIht9XKEQsshm6StZyyOffOxHJziKEljTmezzxliLtuu7pdlHCTLrV6eOF42zkA+b9lxR0JyDE3HekrTSeYHF2ml6STL7mNVRl2UOZttI82PJN96vS7dH4z7gj3V5UnTqSxDUlbkebZYhiQvfay2hQXLuKtvO2keVeKQ8dSPI07HLI0eS6s6x+rcRVqmZPlSybNKGsl2lyRKWO+E9VJZlkoatfxYif1Wtg9K6g3ZPpNs3SPdbuZ5JKyXNiTEso/8N4n7uTydMG8f1tdqOWJMpOkk21GaTsyjkSTOKvkzxqEvjc1yLM5zVOavHlP1ullklQ8tr/Lp1usrTS9bdgDWTUb6G4v5w0V6aTqbOOpk+5pBbL5OMSQiIiKiTONPA3D9YKx9AZj/dDe+MzM+7pZubHoAeGHtYNSrpkml6rUorylDWRlQ+VriaW3duoUIlwMVkSii0Sii0SqUVZaaTrqrl4dQWlmGqmg8TVUZasrDwslw7MKitLYCES1dNIro+iV9KZSWVQpU9f2+qgyoLLU+YZerw7qFsvmINzac89yXdB3uLwfKykrEKX0XVaWV4oSY4hXYaZx/fIhUlAAowx1LoJhnlTSqcRa2abQKZTXlCOsXzCrLUkmjlp/s5WeMHMpZShnLShRVZTUoD4v7pUr+XOxzFJOTdXiaOMRWXTFW7DTErKoMQIkhTsY4xuJsjqMhltIbUABQg1e2yoNYt+5JyPe6ZJalsq8nyzzvaDSK6M4VKBaTGVQvDyEULsccQ5mKRiO4+xVj+fW+npEKoDwsniMAKDHuD/H5mRoHUrhs2JVRN2VOxl2+6w7Wxv9ViVJpRp24Wx4gxj427FxhXVrkZSWKSEUtSj1vM7tt4ZbbbSfsN7ECY9tIldnUzptUjll9SXkOn7gslTRq+UmlZOoe9boAiftX1Pm4JP7Gug53P+9k1te+rkymvlNbP3mcxeMzEuZnHYdkznPgOH/1mLqtmwW22wEJ+ZTH1d32Stu6iTG2PA65y7/79EjIizyOREREREQA2traop6HTReiQDT6wCbz+PefvhgFLkaffl8xjThfl8OmTZuiVqrKEEVZVTRaVRYFyqJV5qnRMiBaUhExjY1UlPSljVRESyRpqsoQRUlFVBtr+o2UwrJkLJbvmmQ+jsvWRaIVJbHfRipKTOsd1edTEq2IxNKhzHmOWjxs00rynCAhjUqc5fl0jEfCsiQS0qjkJ/gAiKPk4utvt1mTjVFy5cwd2XqK+YiPTCgLKvmTzoukcdewDvcm+dhGrcdHo5bxiE0qi+8L4gTjfiJO6YuVcd/R4lthGWft+FSRkJ9kl+W0r0vXTzbOQDpvJ1VlUTjVp36tp+SYHKmwO97L/zbxsGx9ilMZ1djFXzIt2XzHyqH4O5t9IS6p5Qmxt2M7f4FtWkleNMrbQiOJu5RNOnl56cunXcyjDvVfRpGsr2VsEvAcPhqVLUsiIY1KfvrIyptVWum8JfuC27rHdv8WWOfNmvw3ieVBnk7g1/ra1JW28ZDUd/J8J66fu+OzOD8z8zrL0jqd58h+08dtTPsmJW4fK2rbQcxnYlyT3V4pX7eEvPflJ3F7WMzXMv9u04t5SYxjAof1lc83ah9D8kR2vCB1jY2N4ihygfHzhvHzhvHzhvHzJkjxa2xsjB47ejR67OjRaFdXV8JQXl6uPIi/7erq0uftzxvAAIBeXHmFOE6kkiYVqvFaJVB2xxJgyR0oQyWeND6RW3cQtQDmzDI/g1s8aw6ASrxWDSCyHzWSNOHZJUDNfkQAAHXY+koNSipWwvLZUZVl2RB/551CnuPq1t2P8poyrLZ486R4xU5EozthMVkq9iRzCSpWOi3dJaU4F2PWHAC1B01vxGx9pQYou8MxHq4o5SfHKcYomXKWasY8O+dPfZ8jDevw1HGIbUpo9exq+X5SvAKrywBUvpbwxsOs2+5GiSzO1WtRXlOCu2+bJUxIflky6d9+dVj3ZCVQUgH7w6S/61kyOyyOMomVd02ql52qMpp8vmeteBEVJTUov19868dO8stT4zB/E4e0lnlJ1bZIUjyfNeVrk4xZplM4ZsXxHN4Dpfykh1rd47B/p1hiHZ48tfV14hAPy/pOrm/9VI/P7rg/z3HHn5j6zxjXZLdXv6xbwnHIbf7dprfn5/5HRERERNnBnwbgK3oxH3nY8qZ5doc+yQOQh08OKaZJlerXUKl3T7YEd5QBNa9s7bswiOxHDUqQcL4cng29kzTjvw1iF/+1OFgHABHsrwGwf63wHSBDt5Eqy0pQh3X3l6PGjwvMhEYQhTwD8W7jalBWtd7HmyoOFzyahDxLiGkU47xkfby7uNBCrKurxvJQGOU1Zaiy6/5JXJaMmEYxPzklC2JUvbYcNXrdokpxn6M+rMNTxym2KRGLs91NqvDsEsN2MSi+DXeXJHY9W/1apcWxxMOyDJLb1/0QL5NzZkm6iTTyaT2Xl6ISJbj7Nvul9XW3iNQvO2Vl1Eu+i7EidscXa1XuyAIel6egbitecZh/nyTzkrJtkTxpPrOVeN6kcswCz+FNxGXJiGkU85MeCnWPq7rAP5Z1uCcK6+soyfpOkLh+qsdnl1yf57jlR0z9YxXX5LZX/6ybOT9u8+82vVxiHImIiIiIYvxpAJ55HisfAHY/Ngy/0j7mu20Y7nrBZZqUiD+da3gafEnsjhUsPq8jp12MPSl8P+3JxC/x1NTOxov6N1kisSdRw7Jvt9iJf4srFEJIu6Eh/U6QG9VYXip/Utkpz9Vry1FTVgW7eyquVa9FeU38TRJL1nnuo5LGyhKsj1ahDDUoD5eiEnC4QaayLJU0uS5TY1SJUsNN1tgqOL95I+O0z5GGdXjq+BRbt+JvUyUnfnOv8sm+Bo66dYithmRPTHpZ/u3riczzTmiskbC7MQj4uJ6ocn4LMN6YpN+ITumyU1hGk8533JL18W+FKtYNyS6vphxhF+XF2LBVt26h4Xehvu8UJpWXFG4LD8xvo2cz6/Mmp2MWz+E1KstSSZMsse4PIRSK5dsVxbpHqS7QiXmzr2diVOrwxHRq8zZQXF/LujKp+g4J+bZaP8fjs041Di7Pc3Sq83cR02RYbQedQ1yT3l5xqVw3C6bjkNv8u02vc4hj0sRyFEquniIiIiKiwPCnARjALRVnsOmBPDx27SiMHj0Ko9f24v33z2G+odtnlTS+iz8FbbpgWnIHylCDV1zdsSrGip3ak+bayXAY++eUAZgD44PkJXffZrjJH7+Ik3XlZKsYK3ZqN3OiiFTUojQUwkLLKzln2pOhFS8mNkLY5rl6OUorHZ6od02t2yy7PGtU0liJ3RApBaq0OJegsjSE0HL5xlJZlkqaXJe5MSpDlX6TNYpopAIoD0tupDmz3eeoD+vw1PEtti4Vz4Jak415u+iEPNZtfcX67eqkl+Xfvp5ImLfCDbua/bFOyi35sJ6RihKgshTSw59xvwmXAxURRLVzglQuO5VlNOl891mysgIlqt0gJ7u8kgpEXJSXWsMrQrFufWO/qyozJEomL6ncFh6Y30bPXnbnTbbHLJ7D61SWpZImeWLdH0U0WgXjrqlKpe5Rqgt0Yt7s65kYhTocSHLeZirra1lXJlPfAcrr53h81rmIg5vzHJ2L+avGNBlW20HnENekt1eflK2bBdNxyG3+3abXOcQxaWI5iiZdTxERERFRMPjWAIx4A29bW3z4w3nMPJSH3biE4pnu0vipbusrqAFiNwSEpxj1b7WEZ6MENUi4fkvo8msJ1gsnxCtn1wIls2H77G9CN6QqyzIrXvEiKkqS/85Z9fIQSitLUBERL8IsGPJc/VplwtOg4fIa/YZwUg0a2psDq61vsKjk2TKNSpzjbzGVVET0tyKKV+xENPbYcMJFlOWyDCzTqOQnR2RVjIpX4MWKEn/egOqXrgSDj3V46ijFVmfR9ZzFtxHthRH79LIYxD6RWH94Ftsl3vVs+VpUoxpry2uEBhAjr8uK83NfdyWWf/N3LmW8r2fxip2xt2ZMb8nHCTd0d5or75Qt210Zdct7vrVyUVN+v/WbVjoflmcnfhPZbv593OcltdsieZFYH6yWDQHZwPK8yQrP4bP/HN6u7nFVF/jDqg73jd36OnJf34nk66d6fE6Gm/OcJHmKqT/s4uple6V73czHIbf5d5s+kTyOREREREQxvjYAi7ZtzQce6MEt4gQDlTTJ075PVSU8xRiN3SDQno6PXygbn5SG/jSn3U2l2Pz7LsjiJ/Di99CMNwiSXlaczcm/ldgNDaCsSnbTwznPS9aLT4HGnzSN3xA23whWE7shZf09Rfs8x9imUYmz+I0vjaQhznZZcbZpVPKTAxgjKO1zpGEdnjqKsYXNzW8kW26LMWsOzN0bGsW7OrS72am93fHa8tg3SVcnVCga78vqX8W47e4She/Z+bOesS59nZYlStWyXZTRpPiT7+IVq2Nd0K59TZwk8Gd51pZgZUWJ9fxN3OYl1dsiSVo+feuePXhsz5sUjlk8h3dYVpxtGpX89APrusdNXeCfxDrcX9br68RtfSeXuH6qx+fkqJ/nJC/5mPpHFlc/tlfa1i3hOOQ2/27TyyXGkYiIiIgorq2tLep96Io+gGgUD3Tp495/+mIUuBh9+n03abwNmzZtippUlUUBRMuqzKNjqqJlQBTxiVVliAIl0YpIfHKkIloCREv0EaJItKIEUZRURE0pEpZpXk4sidOyqqJlKIuash2fr3V+5CIVJTYxiFPIsyhSUZK47rp4bKx+n7C+Zip5VkmjFufEbRj7XV/8VZalksY5P8EHQBwlV1VmXteUxMihnHkgW89Y/oX90nZfsclfEvtcLkiIe0KcjHKjDveLl9hGZesc7Vtvy3IrqQf6xJchxkmbp7BdEve/+PZLWH5svuY4e11WVBoT6frJxhnI5+2kb13FUFeVieXO63om7hf2x3tNCpbtsozGRtvEXzrNj3z35dV5H09ieY6xN7IqK4nb1VVektkWGmncJWzSSeMuy6eFhPovQ6icNyVuG4ft4ViubM5don1xtyrnKnlWSZNwzElYbnw9A3gOLytv0jIcjerrYZqPZF+w/L1l3aNeF1jO24b8N0nO24f1tS/TUXf1neXyE9fPOs7m47N8fmaJadTPcxJ/m8gyjUVMzdPldbM4zWk7yPMgi6sf28vjugmky7DIj9v8u00vzYssjuL6iX8L5PONSssc+UN2vCB1jY2N4ihygfHzhvHzhvHzhvHzJkjxa2xsjB47ejR67OjRaFdXV8JQXl6uPIi/7erq0uftUwNwW7Tt/bPR+YhGoQ8XopuSSeNhEBuAxZsAInF67O++wepCWh/EK7242MmzfTr7ZUnmIbmwdKZdTMgG2YW2fZ6NZBd4CfPQB/M2EONuppJnlTTxuTnEWT4vY95k08VlqaSJz80xP8EG24sUcxzM6+ZfjFTLmRey9bRcrrCvWKYT8peQzmGfywVi3O3risTp9mUnE+tw/8BjbKPJrJPDjaaoJI6yWEYtbkpp+THnwfomlbtlJaZNKAey9TPcbJQtx3LeCTcDE8l+K8u/u/VMLAOx8eo3dI38XLasDBpJp8u2icI0r/mOGuYhFhMZV8tTjL2JrBxazEclL9JYG9hOl+VFsgy77SMr+1CMdVRS/2UG9fOmhPg4BEZWrhLmoQ/m7Wq7rZXyrJImPjeH46x8Xsa8yaaLy1JJE5+bY35iIClv1nWH5Jgl2Resf+9Q98j2P9Vtb1FnRG3yIz1+iPMV5+3D+srKtIy4DSHGPs5q+eL6mcdbz1c2XYyDbJna75zOc5Kdv0YWU8NE6TpHJfFw2g5WeRDno/G6vaIe1k1kFWPpfONU869RTW+1vmIcxb+l9YFhGVbzlZU58gckxwtSF6Qb+JmI8fOG8fOG8fOG8fMmSPFLVwNwqK2tLSq+FZyptm3bhjvvvFMcTUQ+CYVCiF2rZLdcWc+gYdxTh7ElolzF+o/SieWNckX18hBKaysQ2Wn9PXDqP9w+wcfjhTeHDx/GtGnTxNGkiPHzhvHzhvHzhvHzJkjxO3z4MAYPHAgAKBgzRpyMxx9/XBxl6amnnhJHof30aSDV3wAmIiIiIiIiIqJsUY3XKoGy1WxcDCZuHyIiIiKKYQNwRqrG8lAIIdthOarFnxERERERERERJalu3ZOoLKvC+iXiFAoCbh8iIiIi0oTOnDkTjUajetcjsv/LxgVx2scff8wuoIlSKFe6KcqV9Qwaxj11GFsiylWs/yidWN6IiEgFjxfeBKkLz0zE+HnD+HnD+HnD+HkTpPilrQto7YRDe3N0wIABGDBgAPLy8pCXl4eBAwciPz8f+fn5GDRoEAYNGoTBgwdj8ODBGDJkCIYOHYqhQ4di2LBhGDZsGIYPH47hw4djxIgRGDlyJEaOHImCggIUFBRg1KhRGDVqFEaPHo0xY8ZgzJgxGDt2LMaOHYtx48Zh3LhxGD9+PC677DJcdtllmDBhAiZMmICJEydi4sSJmDRpEiZPnozJkyejsLAQhYWFKCoqQlFREaZMmSKsIhERERERERERERERERFRbgm1tbVlzSNn27Ztw1133SWOJiIiIiIiIiIiIgqExsZGcRQRERHlkHS8AZx1DcDsApoodXKlm6JcWc+gYdxTh7ElolzF+o/SieWNiIhU8HjhTZC68MxEjJ83jJ83jJ83jJ83QYpf2rqADoVCgOH7upcuXcKlS5fQ29uL3t5eXLx4ET09Pejp6cGFCxdw4cIFnD9/HufPn8e5c+dw9uxZnD17Ft3d3eju7kZXVxe6urrQ2dmJjo4OdHR0oL29He3t7Thz5gzOnDmDtrY2nD59GqdPn8apU6dw6tQpnDx5EidPnkRrays+++wzfPbZZzhx4gROnDiB48eP4/jx42hpacGxY8dw7NgxNDc3o7m5GU1NTWhqasLRo0eFVSQiIiIiIiIiIiIiIiIiyi38BjARERERERERERERERERUZYYII4gIiIiIiIiIiIiIiIiIqLMxAZgIiIiIiIiIiIiIiIiIqIswQZgIiIiIiIiIiIiIiIiIqIskXQD8LbyURg9WhtG4Ff1Yop8lOvTDUN5vss0RERERERERERERERERESkIqkG4G3lo3DXCz3Y1HYGbW1n0LbpEh67dhTKtxkT5eMF9OLp9+NptKGix10a39Rh3cIQQqEQlleL0wyqlyMUCiEkTVSN5aHYPLRBmgz+zKdu3UJTGvm8nKgtCwCql5vTWS1Pz9fCdagTJ8Jm3evWYaGQF3m+VPKskkYthippAJv1ivNrPlkhvq3Nq+jfNgPSH8eEfIVCCIUWYp1kJ0hIK8ljwv5mtT9RXK7W4engENvq5QiFlkM2SYvFwnV1pvlYDsICEmIkSSOj8jtpGot9FlbpJXmRptNjoMVLWI5snIHVPM31ghhf6/kBzsuUTe/Lh83vDOVfX2eI8xPzKhnisVVZd6s0puUTZR21Yw1k5xQWCfV9yeqcw+rYx3P4GIf5OHM43ibUnWJdbD09tg5i+r5tZ1dfxn4rO84bj/HaqMRjhx4X1XlopOXKPI+EbaMNVmUYsI0ToOVXlldI8yvNg8o5h3wjK6eVpjOti7iekiFhvu5/I81HwnzV05nIypOBq7JJREREREQJ3DcA1w/G2heABzZ14xZt3C3n8PR84IWtfW/u1tcNAHAJxTP1UQlU0vimei3Ka8pQVgZUvpZ4CaFfDJVWihN01ctLgaoootHYUFUGVJaKFyz+zKdu3UKEy4GKiJauCmWVpc4XUSZ1WLdQtizxpkMsz6W1FYjE00WjUUTXLzEmiiddh/vLgbKyEnGK87oXr8BO4/zjQ6SiBEAZ7lgCxTyrpFGLoUoax/XycT7Zy79t1r9xLEOVoexWldWgPOx+361eHkJppXFeVSirKUfY9mZWjsvJOjxNHGOrqhgrdvbFJVpVBqDEEAPjcSUWZ3OMDHGS3uwTlBiPWfHfJexD5n02UgGUh+XHQFd5MS07NuxcUSymcsmc12g0iujOFYjNtQ7rFoZRDsNyI3fjlfvF9fVLDV7ZKp9z3bonYb13aNyUBTisu0Wa2MaUbHOibKB23sRzePs0juvl43yU2B5vnep5++nFK1ajDDUoX2ueb/XactSgDKs9H6Os1R2sjf+rEqWK5znVy0MIhcsxx1AWYmWqFqUJ9brKMUJjH6ekqZxzOKZJ4nzD9jzG7bHW7W+SyK9jDIiIiIiIKJ3cNwDPPI8/tJ1Bhd76K3fokzzggZ6+RmIJlTR+qX6tEii7A+vvKAMqX0u4WKlbdz/Ka0pQEYmgQnZfBMCS9VEYr6GWrKxAiXCT1J/5VGNteQ1KKl5E37X6EqysKJHm3VrsAi9xWUDtQTHPZaiyvJDW1GHd/eVAxYtYOVucprbuiWLrirI7EMumSp5V0qjEUCWNynr5NZ9s5tc2C1Yck9t363CwFoYyb0hTsx8RfRwZ5WYdnh5OsU2FvjjvNMQIAJZgfaQCJS5uIsdo+9ArsGi3BPQb5OYb7/7nJRUi2F8DlNx9W99xungFdjoet5NRhoqKEtSUr5WUhTpsfaUGJRUVKBMnpVvxCuyMVKCkphz38w0gyjoq5008h7dPo7Jefs1Hjf3x1qmed5qu5fvJvgfS6tbhyUqgpGKl4ZwzVWLHDtPyLdStW4jSylijo9g+Wbxip03jrgqnOPlB5ZwjMY0f5xuy85hU8Z7fxBgQEREREVF6uW8Alqj/1TA8trsXTz+idd08AHX7gfn7B5u+7fu1XxkXp5LGL9WIXW8vAZbcgTJU4knhyrR4xU5Eo+LFjZo5s/p+5Mt86g6iVpgvABTPmgOgEv5e72k3c51vDGg3mayeIE9m3WNvEpWgYqXT0l1SiaFKGpX18ms+uS6D4+hu3y3GrDkAag+a3gjY+orxJiqZsQ5PHefY+k8r76vlcS5egdWxu5uSBkhrsfiqKZkdjv8rNXlJlZr96XlEZNZtd6NEVlar16K8pgR33zZLmNBP4ttH3lhNlO14Dm+bRmW9/JqPErXjrVM9bzddfAu4em05akoq8KK3jCubteJFVJTUoNz2bVuH465P7OLkB5VzDnMah/V2eb7Rdx6TKv7kVyVORERERESUOt5aW7cNw+jRo3DtY3mY/3Q3vqN35ZyHT3YDu2efN3zbtwNLt4zE6HKtm2iVND6pfg2VevdkS3BHGVDzylabC1MVsSfpa0oq4O2+h2Q+kf2oQQkSruvCs+HhofOYyH7UmG50xJ6Sxv61wjeYhG5R69bh/vIalFWtd7zJpM7hwlKTkGcJMY1KDFXSqPBrPrkmmW0WMFq3erG6RX0dlqyPd/kcWoh1ddVYHgrH3uARX4OgGNbhqZOS2DqJv52TEKA+4dklAGpheNHNUV8XlNaql5eiEiW4+zbzMdDvvPhPe7OrNPH4nArFt+HuksQ3jGJvrzkcs9MsGNuHKA3E8yaew9unUeHXfFQ4Hm+d6nmn6TC/BVwde/u3bLWfb746KcaK2FM5EHqi7lO3Fa84HHe9UYmTdyrnHOY0/pxvJJ7HpIo/+VWJExERERERpY63BuBbuuMNt92Y/dhIjP7aYNQDAHpQ0XYGbRXaG8EAcAnfWdkDvDAYv6pXTeOHOqx7MtbdlnbTY0nsijuJroji338KhRDSGmyS6k7Kr/m4VY3lpZWApMGjpnY2XtS/1xOJPb0d7vuuT/XactSUVSV00+VJ9VrEeo6zm6l1nvuopKFgydRtVolSw03W2Co4v3mTaAnWR6tib2mES1EJ+HxjNpuwDk8dP2PrQvyNK1/FGzgSGyOEfRZV5re4ks1LTTnCdg0uSTHnVZxn8YqdiEZi3Y2XhxOn+yt+E1/Slaj9MTtZ9utuh28XUW6wPm/iOXwmUDveOtXzTtNjaeJv4Za6fchNrIdDCIVi56iuLFkf/66z5PuwBsaHAurWLTQvN+GbsWLeEtfbSCVOnliecxiIaZI933A6j0mVpPNrIMYgaeL2T7JsEhERERHlIG8NwLoePPJ0L7A7H286Ntzm4ZND4jiRShpF8aeMTTcoltyBMuG7j2pi362K3WCJIlJRi9JQCAtdX1H6NR93tCeGK15MbKgwfSdJu/GrdX1WvRyllX6/nRi/EeJwY8IuzxqVNBQsmbvNylCl32SNIhqpAMrDkhtV9mI3ukqBKq0OKEFlaQgh2+9o5SjW4anja2xdKJ4FtSa7ObB7aczUCBsuByoiiCYcp/r22Uj8jSDTbpZsXkoqEDHWBb7cjBXqF9k8i1dgZ7zuid3Ytr/B7olQFuq2vuKyMcENhXW3wLeLKBfYnTfxHD4DuDneOtXzTtP1MuD27V+xHo4iGq1K6nvvse86y7u41hi/ZR3rYju2zCrpAsW8KRwjHOPkkso5h12aZM83nM5jUiXZ/NrFIGni9k++bBIRERER5RqfGoCBmcWX/G249Und1ldQA8QaV4QnRr1+My72hHUK5hOejRLUIOHTRVbdlCmoXh5CaWUJKiIKF8wwd31W/VplwpO34fIa/QIvqUYP7c0BmxsTKnm2TKMSQ5U0KvyaT47wtM2CpngFXqwo6XuDQ2Ud4k/Dl1RE9LdxilfsRDT2ukR6bupkENbhqeMuthZd/Fl8P9FeGLNL7L/PF4n1OwjbUAmNsDutDhRxxSt2xt5KetL4wIZPeUm34hXYWWVo5EmJeBel5WtRjWqsLa8RGpqCIbK/JvEGNFEWsTxvssJzePXjrF/zceDueBvnVM87Tfcx/67Fz49ryu9PfPM23rBod9z1lWWcXJ7XqJxz2Kbxfr4hP49JlSTzaxsDIiIiIiJKN/cNwPWD8bXRo1C+TRhdNwBAL668wilND267RTGNZ9r3qaqEJ0ajscaWhAvBJIkXPsnS5hO/MDY+GQ39LRf3NzljN1iAsirZTZj4xZ34zUfDjY8l68UnbuNPIMcv8JK5sIvdkDJ8O1Vgn+cY2zQqMVRJo8Kv+eQAz9ss6FTWQfzWnSYV35vLeKzDU8dFbK1ukCPZm+TFmDUH5u6FjeJdDaeisTHW5abx24T9lxfP0lBnaG9xvbY89u3K1QkVdz/Ttk9SXfETBZ/teRPP4e3TqPBrPrZcHG9FTvW80/R+VLxidexTJ2tfE6YYvlMsO+6mghgn389rVPhzvpF4HpMq/uSXiIiIiIj6l/sG4Jk9WDofeGFrvmFkPp59LA/zn+7Gd2ZapRmAN7fkYf7T53ALFNN4Zfd9qiV3oAxApeUVt6gay0NC11Hx+bu78FGZj/bWjeGpaf2tQXc3OevWLYzfYIlafPsr3k2Y6UIy/j0uz9/rseBww9Y5zyppVGKokkaFX/PJIpKbJ/5ss6CJvRXXt68orINW9whP71evLUeNzQ3VnMQ6PHXcxLZ4BVaXAZWlwjf06tZhYZLHiiXrtW9gC7GsW4eF4dh3C190O1MVS1Yidt+5b//rt7y4Ub1c6Gq+DuvuT0OdUXwb7i4BKivN364MhCBtH6IUcD5v4jm8fRoVfs3Hhurx1qmed5quqHp5yP9v4kotwfqqMqCyMuFbrfp3isMhoeebOnju1V8lTik4r1Hhy/mG5DwmVXzJLxERERER9a+2trZoMsOmB6JRoG+Y/3S7Y5oHNjnPR5ZGddi0aVPUqKoMUaAsWmUa28c4PVJREgUgGfp+L0tTJsxcliaZ+UT1/PUNJRURMYmDqmhZQj60oSRqnF1CnmQZMohUlERRUhE15ihhHvpg3gb220Ulzypp4nNTiKFTGnfr5X0+QQZAHGVg3i7m9fdvm6UjjrL1tFyuZF9xWgd5PPzLf6YS425fV+RCHe4feIitRnW9dVVlCfu3SIyRapxkxyBRLL+J6xgbn5gv1bw4Llu23lVlCfM2zl8WWwCm5SSksctD1HmZsnzKYqYt17ytY3WYKT6S+alMS1gvyfpZpbEtf0RxkBzTg092nqANsv3WMN1hx5DVYQnz0AfZuW5ivRqjkmeVNPG5KRxDndK4Wy/v84lKypt9zMzTE5bjtJ2sjgM2dW5sebIyJMujWl1v/fu+2EqLpew45bTOFumMEn5jkTYhnUU+ZfuMSCWNRixvEGMcZxXX2HjJ9pVsG0cKv3GVX8UY6GRlIOH8KDEG0rJJlGGQkecnwdHY2CiOIhcYP28YP28YP28YP2+CFL/GxsbosaNHo8eOHo12dXUlDOXl5cqD+Nuuri593qG2trao2CicqbZt24Y777xTHE1EPgmFQohdq2S3XFnPoGHcU4exJaJcxfqP0onljYiIVPB44c3hw4cxbdo0cTQpYvy8Yfy8Yfy8Yfy8CVL8Dh8+jMEDBwIACsaMESfj8ccfF0dZeuqpp8RRaD99GkiqC2giIiIiIiIiIiIiIiIiIgokNgBnpGosD4UQsh2Eb/UQERERERERERERERERUdZjA3BGWoL10SiitsN6LBF/RkRERERERERERERERERZLWu+AfzFn94tjiKiFKn/+ZviqKzC7/H0D8Y9dRhbIspVrP8onVjeiIhIBY8X3gTpG46ZiPHzhvHzhvHzhvHzJkjxS9c3gEO1tbXRxLdHYychmTRu5V8qQUTp0fC//iCOIiIiIiIiIiIiBY2NjeIoIiIiyiFpaQA+fPhwVjxydvOzDwE58GYiUX+a+f1bgRzYz/g0bv9g3FOHsSWiXMX6j9KJ5Y2IiFTweOFNkN7gykSMnzeMnzeMnzeMnzdBil+63gDmN4CJiIiIiIiIiIiIiIiIiLIEG4CJiIiIiIiIiIiIiIiIiLIEG4CJiIiIiIiIiIiIiIiIiLIEG4CJiIiIiIiIiIiIiIiIiLIEG4CJiIiIiIiIiIiIiIiIiLJE0g3Af3psKqZN04bJ+P82iimG4TF9umF4bJg52Z/G208nIiIiIiIiIiIiIiIiIiIlSTUA/+mxqXjgt9144fARHD58BIdf6METN03FY38yJhqG36Ln/8/e/8TIbeV5ou+XSqdlp/9k2i7bZbtw1S1HyGhBm+cGcgBmA+/NA+xGhGahGkhaDBpQYoDHGC9eBYF7hYYgAY3Bk6BFzr1g9CzUGYuBtOlFCnjWYhQBO4G5mEXGAwS0VoksWBHOzrzwn7JdtiPtkmw5S+JbkIwgDw/JwyAjFBnx/QCE5eDJw3N+/HPIc/gH//A/3TTedPWBL82vcOS/7uN/evP+5x7++p9/NaRB4A5qSxo0TUOlKc7zaVagaRo0aaImKpqThzdJkyGffDq1pUAaeV5J1JYFAM1KMF3U8nrlWqqhI85ETN07NSwJZZGXS6XMKmnUYqiSBoiplys5H7UyTwR3XQfrl6L+CbEGFNPkKLR+NQ2atoSaZCcIpZWUMbS/Re1P5JrWY/goJMS2WYGmVSCb5cViqdYJ5BM5CQsIxUiSRkbl76RpIvZZRKWXlEWarhcDL17CcmS/+UTlGTwuiPGNzg9IXqZsfr8cMX/n2/57dYaYn1hWyeTGVqXuUWkCyyeaOGptDWTnFBEJeQ4vn5+cj1qZkyW0t6Fjp3gsjp7v1EFM3193ccdL529l7by/jfd+Crcdvfiq5uGRblfBPELrxpuitmEgNk6AV15ZWSEtr7QMKucc8pWsnFaaLlAXsZ6SKZRv+r+RliOUr3o6P+nfiOsr7TZKREREREQ96QeAd+bxX/8Z+A/X/4h/6/32b/fwD38N/PPH/YHbnX+dBbCPv/yL3k+COVxYnsNf/7sH6CX5iz38H/+wD/zzHPxjyblorsBsGTAMoH4rfOnQuxgq18UZPc1KGWjYsG1nahhAvSxeoOSTT6e2hKIJWG0vXQNGvZx4ERXUQW1Jtiyx08Epc3nTQttNZ9s27NWSP5GbtIZzJmAYujgnue6FKjb8+btT29IBGDhVgmKZVdKoxVAlTWK9lPJRK/PkUq1/cqzV0gyLgYZv220YLZjF9Ptus6KhXPfn1YDRMlGM7cyaclN5DB+RxNiqKqC60Y+L3TAA6L4Y+NsVJ87BGPniJO3kE+j+Nsv9u9A+FNxn2xZgFuXHnVRlCSzbmTaqBTFVSsGy2rYNe6MKJ9cOaktFmPAtt30Wa+fE+ualhbXb8pw7tcuI3js8abYFJNQ9Io2zMiXrnGgSpDtv4jm8PE1ivZTyUSuzktj2Nuk4Hz+/UL0EAy2YK8F8mysmWjBwKXMbFa1zb9P9Vx1lxaA0Kxq0ookTvrg629QmyqHjukob4YmP08BUzjkS0wxwvhF7HpO2rU37NwOUNzEGMnF1JCIiIiKiLNIPAP/FHv6/u/8XrvZGf+X+tT0L/IcH/UFikfuE8L/7f+4Hfv6L//gldnd9g8s5ad6qA8YprJ4ygPqt0MVKp3YOZkuH1W7DkvWLACit2vBfQ5XOW9CFTtJ88mlixWxBt26gf61ewnlLl5Y9mnOBF14WsHlPLLOBRuSFtKeD2jkTsG7g/HFxnlrdw5y6wjgFp5gqZVZJoxJDlTQq9VLJR6XMk0yt/smxVkszKoPtux3c24Rvm/elaW2h3fuN/KbzGD4aSbEdhn6cN3wxAoASVtsW9BSdyA5vH1pDxLgl0OsgD3a851+WYWhjqwXoZ0/22+lCFRuJ7fYgDFiWjpa5ItkWOri91oJuWTDEWaNWqGKjbUFvmTjHJ39o4qQ5b+I5vDyNSr1U8lEps5r49jbpOJ803yv35f4NaZ0aLtcB3TrvO+ccFqftCCw/Qqe2hHLdGXQUxycL1Y2YwV0VSXHKg8o5RzhNHucbsvOYYcle3nAMVIyyjkREREREky79ALDEzn/7Ff7zv+zjHyre651n8a+fAH/9yXzg+77//r/N9v+m94Sw8K3gobz+uQnnersElE7BQB2XhSvTQnUDti1e3Kg5caz/R7nk07mHTSFfACgcOwGgjnyvhbzO3OSOAa+TKeoO8kHq7jxJpMM6n7T0lFRiqJJGpV6K+VCyxFgrphm1dPtuAcdOANi8F3gi4PaavxOVgngMH57k2ObP294vyeNcqOKS0/MnGYCM5sRXjX686P5rOGUZltbWaG4ROXbyLHTZttpcgdnScfbkMWHGE+KuH/lgNdGk4zl8bBqVeinmkw+19jbpOB83X3wKuLlioqVbuBEZgHwdq96Apbdgxj5tm9Du5iQuTnlQOecIpkmod8rzjf55zLDkU16VOEUZfh2JiIiIiCZftgHg//NXOHLkf8H//T/P4q//4Y/4j713Oc+i/S/Av7yz5/v+75f4d//9DWGAdw7LR+ZR7H0n+Ev8wydD+AZw8xbqvdeTlXDKAFprt2MuTFU4d9K3dAvZ+j0k+bS30IKO0DVP8TikN6+n0d5CK9DR4dwlja0V4RtMwmtROzWcM1swGquJnUzqEi4sPaEyS4hpVGKokkbFoPmIZZ42E1B/77V6zrFFfVsorbqvfNaWUOs0UdGKzhM84mMQ5OAxfHiGEtsk7tM5oQD1FY/rADaR5uGq/isoozUrZdSh4+zJYBuYd1ny5z3ZVQ63z8NQOImzevjpG+fptYQ2e8TGY/0QjUDovInn8LFpVAyaj1hmFYntbdJxPmk+gk8BN52nf41LeT75mqSAqnNXDoQ3Ufd1bmMtod3NRiVO2amccwTT5HO+ET6PGZZ8yqsSJ9Ho6khERERENPmyDQD/2z+6A7d/xDv/+Q0c+ffz2AEAPMDV3f8Lu1e9J4IBYB//8f/9APjnefw3JxEACAPH8jTZdFC77Lxuy+v0KDlX3KleReRwvyOladC8AZuBXieVVz5pNVEp1wHJgEdr8zhu9L6903bu3i72v+vTXDHRMhqh13Rl0lyB8+a4uEyjy9ynkmbcHMQy5+mg1r+Osq+T1alC8pM3YSWs2g3nKY1iGXUg547ZScJj+PDkGdsU3CeucuUOcIQHI4R9Fo3g02CDlqVlohg34DKQYFnFPAvVDdht53XjZjE8P19uJ77kVaLxbfag4useJ8vTRUQHR/R5E8/hR22QMqu1t0nH+aT5Thr3Kdxy2pvcxOOwBk1zzlFTKa2630iWfB/Wxz943qktBZcb+masWLZwvf1U4pRJ5DmHj5hm0PONpPOYYRm4vD5iDCKp1lHcDgbcRomIiIiIpki2AeCeB6j8wz7wL3P4H4kDt7No/6v37/A3gB3+NBm5dxkHOihKp2AI331U43wDyulgsdG2NlHWNCylvqLMK590vLtprRvhgYrAd5K8jl/v1WfNCsr1vJ9OdDtCEjom4srsUUkzbg5imfN0cOtvoNHrZLVhty3ALEo6quI5HV1loOEdA3TUyxq02O9oTSkew4cn19imUDgGtSG7E4h9uMo/CFs0AasNO9RO9ffZtvtEUGA3G7QsuoW2/1gg7ahMSzi+yPIsVLHhHnucju34DvZMhG2hc3st5WBCGgp1jzDI00VEB03ceRPP4UdroDKnaW+TjvNJ83vbQNqnf8XjsA3bbgz0vXfnG8nyV1x7/N9Pdl7V7SyzIV2gWDaFNiIxTimpnHPEpRn0fCPpPGZYBi1vXAwiqdZR3A4G30aJiIiIiKZFTgPAwF/85X6qgVsn/fB1bq+hBTiDK8Kdolm/GefcYT2EfIrHoaOF0KeLol5TpqBZ0VCu67DaChfMCL76rHmrHrrjtmi2ehd4Aw16eE8OxHRMqJQ5Mo1KDFXSqEiZT2SZp8RE1b9QxQ1L7z/BobItuHfD61a79zROoboB23lcIqLDY3rxGD486WIb8Yq/iO8nxiviuB7/fb62895BxIZKGITdSDigFKobzlNJl/03bORUllErVLHR8A3yDIX7ilJzBU00sWK2hIGm8dDeaoU7oIkmSOrzJp7Dq7ezKfOJLHOCdO2tK+k4nzRfUv6Rcc+PW+a58JO37sBiXLubq8g4pTyvUTnniE2T/XxDfh4zLAOWNzYGyUZbRyIiIiKiyZd+AHhnHv/+yP+CC/+n8PO/zgLYR/Evk9I8wPv/FsBf7uOvMYv//j9mg4mAfprMvO9TNYQ7RW1nsCV0ITgg8cJnUF4+7oWx/85o9J5ySd/J6XRWAEZD1lnhXtyJ33z0dXyUVsU7bd27c90LvLQXduh1SPm+nSqIL7MjNo1KDFXSqEiRT2yZp8DE119lW4j6blzS9+amEo/hw5MitlEd5IjuJI9XwLETCL5e2M991fAwBhudV276v0345MqS2QiOGd5TXLcqzrcrL43bgdtbPwO9ip9o/MWfN/EcPjaNihT5xJY5Vor2VpR0nE+a/wQVqpecT52s3BLm+L5TLGt3h0GMU+7nNSryOd8In8cMSz7lHcTo6khERERENPnSDwD/xQP8u78G/vnjOd+Pc1j9z7P97/lK08zif/z3Wfz1P+zh3wLAX+zh//iHffzLf55Hf5x4Fv/tv87102QV932q0ikYAOqRV9yiJiqa8OooN/90Fz4q+XhP3fjumu49NZiuk7NTW3I7K+yIb3+5rwkLXGS537ZK/F7PgBI6bJPLrJJGJYYqaVSo5ZNc5gki6TyZzPo7T8X19xWFbcE79gh3tjdXTLRiOlSnEo/hw5MmtoUqLhlAvSx8Q69Tw9KAbUVp1fsGthDLTg1LRee7hTfSZqqidB5Ov3N//3tiZUmjWRFeNd9B7dwIjhmFkzirA/V6PfDtyrEwTuuHaAiSz5t4Dh+fRoVaPslljqHa3iYd55PmK2pWtPy/iStVwmrDAOr10Ddae98pLmrCm286yPxWf5U4DeG8RkUu5xuS85hhyaW8gxhhHYmIiIiIJt7u7q49yHT9P9g20J/++h++SEzzH66H89m9fj8xH5XpL//X9+2//F/ft/0aBmzAsBuBX/v889uWbgOQTP2/l6UxhMxlaQbJx+6Vrz/pVltMkqBhG6FyeJNu+7MLlUlWIJ+2pdvQLdtfolAevSm4DuLXi0qZVdK4uSnEMClNunpF5aNe5nEm28/6gnUcpP4qsVZJkxUA8afo5Ur2lfhtwY6IR37lP6jEuMcfK6bhGJ4fZIitR7XePQ0j8fgmxkg1TrI2SOSUN1xH5/dwuVTLkrhsWb0bRihvf/6y2AIILCeUJq4MdvIyZeWUxcxbbnBdO8ewQHwk+anMC9VLUr+oNLHbH5ELkjZ9/MnOE7xJtt/65ifsGLJjWCiP3iQ71w0fVx0qZVZJ4+am0IYmpUlXr6h81MtsS7a3+JgF54fKm7SeotqBmGOuszzZNiQro9qxPvrv+7GVbpaydiqpzhHp/EJ/E5E2lC6inLJ9RqSSxiNubxBj7IqKq/O7ZP1K1k0ihb9JVV7FGHhU6xiVTrqNEh0QOJDnJ+NjZ2dH/IlSYPyyYfyyYfyyYfyyGaf47ezs2F9+9pn95Wef2ffv3w9NpmkqT+Lf3r9/v5e3tru7a4uDwgfR/+Mf/18AgO3/8pE4i4hycvR/+1tgCvYzTdPgXJPRKDHuw8PYEtG04vGPRonbGxERqWB7kc3u7i6OHDki/kyKGL9sGL9sGL9sGL9sxil+u7u7OPzUUwCAF196SZyNixcvij9FunLlivgTfvj+e2CgV0ATEREREREREREREREREdFY4gDwgdRERdOgxU7Ct3qIcrD9Xz6a+Kd/iYiIiIiIiIiIiIiIDjIOAB9IJazaNuzYaRUl8c+IBnT0f/vb0ERERERERERERERERETjhwPAREREREREREREREREREQTQtvc3LTDT4/aAHCgfjv//6uDiPK3/V8+kj7x+6//+8fiT0RERERERERElGBnZ0f8iYiIiKbI4aeeAgC8+NJL4ixcvHhR/CnSlStXxJ/ww/ffAwC0brfrjKYecP+3/89Z8SciykHUAPAkfwtY07TejSY0Ooz78DC2RDStePyjUeL2RkREKtheZLO7u4sjR46IP5Mixi8bxi8bxi8bxi+bcYrf7u4uB4DTWl9fx+nTp8WfiSgjDgDTKDDuw8PYEtG04vGPRonbGxERqWB7kc04deAfRIxfNoxfNoxfNoxfNuMUv1ENAPMbwESUaPu/fITt//IR/vV//7j3byIiIiIiIiIiIiIiIho/HAAmIiIiIiIiIiIiIiIiIpoQHAAmIiIiIiIiIiIiIiIiIhoJzZ2GwcmbA8BERERERERERERERERERBNi4AHgdXMeCwve9DyubYspZmH25vsmc9aZvX0Y74vzfJO5LuZHRERERERERERERERERERxBhoAXjfnceb6Pm5299Dt7qF78zEuvCsM2q7P4joe4epdN403WfvO/KMP8bH/9+4eut0HWAaAxZ/xu/d8eeWig9qSBk3TUGmK83yaFWiaBk2aqImK5uThTdJkyCefTm0pkEaeVxK1ZQFAsxJMF7W8XrmWauiIMxFT904NS0JZ5OVSKbNKGrUYqqQBYurlSs5HrcwTwV3XwfqlqH9CrAHFNDkKrV9Ng6YtoSbZCUJpJWUM7W9R+xO5pvUYPgoJsW1WoGkVyGZ5sViqdQL5RE7CAkIxkqSRUfk7aZqIfRZR6SVlkabrxcCLl7Ac2W8+UXkGjwtifKPzA5KXKZvfL0fM3/m2/16dIeYnllUyubFVqXtUmsDyiSaOWlsD2TlFREKew8vnJ+ejVuZkCe1t6NgpHouj5zt1ENP3113c8dL5W1k772/jvZ/CbUcvvqp5eKTbVTCP0LrxpqhtGIiNE+CVV1ZWSMsrLYPKOYd8JSunlaYL1EWsp2SS5AulvIOk6QN5q5SlppBmsLj200XXIfL8RSTbxn1S7S9ERERERE9Y+gHg7cNYuQ4s33yA3hjtez/j6iJw/bb7dC+A7c4hAI9RONr7KdG6OecMGv/TQ6T4MzXNFZgtA4YB1G+FT9d7Fy3lujijp1kpAw0btu1MDQOol8WLg3zy6dSWUDQBq+2la8Col6UXPNE6qC3JliV2OjhlLm9aaLvpbNuGvVryJ3KT1nDOBAxDF+ck171QxYY/f3dqWzoAA6dKUCyzShq1GKqkSayXYj4q631yqa0zlVirpRkWAw3fttswWjCL6ffdZkVDue7PqwGjZaIY25k15abyGD4iibFVVUB1ox8Xu2EA0H0x8LcrTpyDMfLFSdqxJtD9bZb7d6F9KLjPti3ALMqPO6nKEli2M21UC2KqlIJltW0b9kYVTq4d1JaKMOFbbvss1s6J9c1LC2u35Tl3apcRvXd40mwLSKh7RBpnZUrWOdEkSHfexHN4eZrEeinmo9LuK4ltb5OO8/HzC9VLMNCCuRLMt7liogUDlzK3UdE69zbdf9VRVjzPaVY0aEUTJ3xxdbapTZRDx3WVNsITH6eBqZxzJKYZ4Hwj9jwmbVsrSr6uUS+zSlmqCmmynidmPX8hIiIiIpos6QeA3Sd3rYQndD/9ZAZY3u8PEidxB5YXrz7AB7mP/gLNW3XAOIXVUwZQvxW6YOjUzsFs6bDabViyfhEApVUb/muo0nkLunCRkU8+TayYLejWDfSv1Us4b+nSskdzLsTCywI274llNtCIvJD2dFA7ZwLWDZw/Ls5Tq3uYU1cYp+AUU6XMKmlUYqiSRqVeavkkr/dJprLOVGKtlmZUwutQZVvo4N4mfNu8L01rC+3eb+Q3ncfw0UiK7TD047zhixEAlLDatqCn6ER2ePvQGuIOqU4HebDjPf+yDEMbWy1AP3uy304XqthIbLcHYcCydLTMFcm20MHttRZ0y4Ihzhq1QhUbbQt6y8S51KMwROMuzXkTz+HlaVTqpZZPcruvJr69TTrOJ833yn25P4DXqeFyHdCt875zzmFx2o7A8iN0akso152BP3F8slDdiBncVZEUpzyonHOE0+RxviE7j8mLbLvOo8yDGGy5B+T8hYiIiIhohNIPAEtsX5vDhTuPcPV37uudcQidLWBx63Dgu77vX4te3Po/PoM72Mf5Dx6Ls3LQhHO9XQJKp2CgjsvClWmhugHbFi8w1Jw41v+jXPLp3MOmkC8AFI6dAFBHvtd73sVQcseA18kUdQf5IHV37sTVYZ1PWnpKKjFUSaNSL8V8ooh/N80SY62YZtTS7bsFHDsBYPNe4ImA22v+TlQK4jF8eJJjmz9ve78kj3OhiktO76akAy+aE181+vGi+6/hlGVYWlujuUXk2Mmz0GXbanMFZkvH2ZPHhBlPiLt+5J29RJOO5/CxaVTqpZhPFPHv4qm1t0nH+bj54lPAzRUTLd3CjcgA5OtY9QYsvQUz9mnbhHY3J3FxyoPKOUcwTUK9U55v9M9j8tffrvMts7rBl3tgzl+IiIiIiEYkekRWxfocFhbm8e6FGeHJ3Rl8cge4c/yh7/u+P+K3H76ABbP/mui+Wdy+jnRPDKfRvIV67/VkJZwygNba7ZgLUxXOnfQt3UK2fg9JPu0ttKAjdF1XPA7pzetptLfQClzYOXdJY2tF+AaT8PqnTg3nzBaMxmpiJ5O6hIs7T6jMEmIalRiqpFExUD6S9T5txHV2AHmv1XOOLerbQmnVfeWztoRap4mKVnSe4BEfgyAHj+HDM5TYJnGfzgkFqK94XAewCd+Dbon6r6CM1qyUUYeOsyeDbWDeZcmf92RXOdw+D0PhJM7q4SeMnKfXEtrsERuP9UM0AqHzJp7Dx6ZRMVA+knZfRWJ7m3ScT5qP4FPATefpX+NSnk++Jimg6tyVA+FN1H2d21hLaHezUYlTdirnHME0+ZxvhM9j8hO6rsmpzOllWO4BOn8hIiIiIhqFbAPA7z1wB3cf4PiFF7Dw/mFsAwD2YXX30LW8J4IB4DE+OL8PXD+Ma06inu1rh51v//aeIM5TB7XLzuu2vGuZknPFHfPKpijud6Q0DZo3YDPQ66TyyietJirlOiDpsGhtHseN3rd12s7d28X+t3WaKyZaRiP0mq5Mmitw3hwXl2l0mftU0oyDJ7Xex9FBWWeiOsq+TlanCslP3oSVsGo3nKc0imXUgZw7ZicJj+HDk2dsU3CfuMqVO8AR7twT9lk0gk+DDVqWloli3IDLQIJlFfMsVDdgt53XM5rF8Px8uZ34kleJxrfZg4qvexyVp7CIDr7o8yaew49C1nZfrb1NOs4nzXfSuE/hltMOUovHYQ2a5pyjplJadb+RHPWNVof/poBObSm4XPHbuqGyhevtpxKnTCLPOXzENIOebySdx2SScF0zcJkzyrTcUZ2/iNvkgPsLEREREdGQZRsA7tnH764+Au7M4iNhcDdsBp98Gvzl009mgMV9/O0Qvv3r3WUcOOEvnYIxwHebvO9WOR0sNtrWJsqahqXUV5R55ZOOd8ewdSPcYRH4TpJ34eS9PqlZQbme99OJbkdIQsdEXJk9KmnGw5NZ7+Po4KwzkYFGr5PVht22ALMo6aiK53R0lYGGty3oqJc1aKFvWRGP4UOUa2xTKByD2pDdCcQ9NBYYhC2agNWGHWqn+vts230iKLCbDVoW3ULbfyzIpTNWOL7I8ixUseEee5yO7fgO9kyEbaFzey3lYEIaCnWPoPIUFtFBF3fexHP4UcjY7qdpb5OO80nze9tA2qd/xeOwDdtuDPS9VOdbsvJXXHv837J2XtXtLLMhXaBYNoU2IjFOKamcc8SlGfR8I+k8JpOE65qBy5xR1uWO5PxF3CYH31+IiIiIiIYppwFg4GjhsXRwN5n7+ufjjzGc8d81tABncEW4OzPrN+OcO6yHkE/xOHS0EPp0UdRryhQ0KxrKdR1WW+GCGcFXnzVv1UN3uRbNVu8iV7nzw897ciCmY0KlzJFpVGKokkbFgPmE1vuUiFxnB1GhihuW3n+CQ2VbcJ8I0K1272mcQnUDtvO4RI6dOpOBx/DhSRdbyWv20H9KI/b1niFFHNfjv8/Xdt79h9hQCYOwGwkHlEJ1w3kq6bL/ho2cyjJqhSo2Gr5BnqFwX1FqrqCJJlbMljDQNB7aW63oTmCiCZD6vInn8Ort7ID5hNr9BOnaW1fScT5pfkz5h849P26Z58JP3rqDe3Htbq4i45TyvEblnCM2TfbzDfl5TI7E65ocyjyYrMs9GOcvRERERESjkH4AePsw3l+Yh7ku/Nw5BOAR3nk7Kc0+Tvo/9Lt9CFsAlk8O5/XPzvepGsLdmbYz2BK6EBxQ5MVHSl4+7oWx/85o9J5ySd/J6XSwAEZD1gnjXmCJ33z0dXyUVsW7W907kN2LXOkFcAKnQ8r/jaGg+DI7YtOoxFAljYqs+eS1/RwAsetsEqhsC+K37jyx35ubVjyGD0+K2EZ1kCO5k1yugGMnEHw9n5/7qr5hdNY5r9z0f5vwyZUlsxEcM7ynuG5VnG9XXhq3A7e3fgZ6FT/R+Is/b+I5fGwaFVnzUTp/SNHeipKO80nzn6BC9ZLzqZOVW8Ic33eKZe3uMIhxyv28RkU+5xvh85hhyqfM6WVf7tifvxARERERjUj6AeCj+/jtInD99qzvx1n844UZLF59gA+ORqU5hI8+nMHi1Z/hH//FpzO44w0c5y3u+1SlUzAA1COvuEVNVDTh1VFu/nEXH2Eq+Xh3rfrumu49NZiuk7NTW3I7WOyIb3+5rwkLXEi63+OK+65RFgkdtsllVkmjEkOVNCpU8lFZ7xNE0nmSvM4OIueu8v6+orAteMce4e795oqJVkyH6lTiMXx40sS2UMUlA6iXhW/odWpYGrCtKK1638AWYtmpYanofLfwRtpMVZTOw+l37u9/T6wsaTQrwqvmO6idG8Exo3ASZ3WgXg9+u3IsjNP6IRqC5PMmnsPHp1Ghko9Kux9Dtb1NOs4nzVfUrGj5fxNXqoTVhgHU66Hvova+U1zUhDffdJD5rf4qcRrCeY2KXM43JOcx+RGva3Iq8wAyL3ecz1+IiIiIiEap2+3ag0w3l20b6E+LV39ITLN8M5zP3at/toE/21fvhuelnW7evGn7NQzYgGE3Ar/2+ee3Ld0GIJn6fy9LYwiZy9IMko/dK19/0q22mCRBwzZC5fAm3fZnFyqTrEA+bUu3oVu2v0ShPHpTcB3ErxeVMqukcXNTiGFSmnT1SpdPQpjHDgDxJ5/gegnWX22dyWLkTPH7j5gmK0jqGblcyUpM2hbk8civ/AeVGPf4Y8U0HMPzgwyx9ajWu6dhhI7JIjFGqnGStUEip7zhOjq/h8ulWpbEZcvq3TBCefvzl8UWQGA5oTRxZbCTlykrpyxm3nKD69o5hgXiI8lPZV6oXpL6RaWJ3f6IXJC06eNPdp7gTbL91jc/YceQHcNCefQm2blu+LjqUCmzSho3N4U2NClNunqlyycqzMjQ3oaWk7SeotqBmGOuszzZNiQro9qxPvrv+7GVxkvWTiXVOSKdX+hvItKG0kWUU7bPiFTSeMTtDWKMXVFxdX6XrF/JuokiqzsQffxQLXOPSlkU0qguVxYrr46J5y8i2XYZOmcLrxelvIl8cCDPT8bHzs6O+BOlwPhlw/hlw/hlw/hlM07x29nZsb/87HP7y88+t+/fvx+aTNNUnsS/vX//fi9vrdvt2uKg8EG1vr6O06dPiz8TUU40TYNzrTLZpqWe44ZxHx7GloimFY9/NErc3oiISAXbi2x2d3dx5MgR8WdSxPhlw/hlw/hlw/hlM07x293dxeGnnDcov/jSgjgbFy9eFH+KdOXKFfEn/PB9FxjoFdBERERERERERERERERERDSWOAB8IDVR0TRosZPwvRwiIiIiIiIiIiIiIiIimngcAD6QSli1bdix0ypK4p8RERERERERERERERER0UTjADARERERERERERERERER0YTQ9vb2bO+pUQDS/8p+G8d5v//973HmzBkQERERERERERERjaOdnR3xJyIiIpoih5+aBQC8+NKCOAsXL14Uf4p05coV8Sf88H0XAKB1u11nBHUCrK+v4/Tp0+LPRJQTTdN6N11Msmmp57hh3IeHsSWiacXjH40StzciIlLB9iKb3d1dHDlyRPyZFDF+2TB+2TB+2TB+2YxT/HZ3d0cyAMxXQBMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTYiBB4DXzXksLHjT87i2LaaYhdmb75vM2WCy9bn4+UREREREREREREREREREpGSgAeB1cx5nru/jZncP3e4eujcf48K78zDX/YlmcR2PcPWum8abrH1fmjksnJnF8k1v/gMsX58b0iBwB7UlDZqmodIU5/k0K9A0DZo0URMVzcnDm6TJkE8+ndpSII08ryRqywKAZiWYLmp5vXIt1dARZyKm7p0aloSyyMulUmaVNGoxVEkDxNTLpZyPSgwPOnddB0Ogts6A5FgDimlyFFq/mgZNW0JNsgJDaSVlDO1vk7ot5GZaj+GjkBDbZgWaVoFslheLpVonkE/kJCwgFCNJGhmVv5OmidhnEZVeUhZpul4MvHgJy5H95hOVZ/C4IMY3Oj8geZmy+f1yxPydb/vv1RlifmJZJZMbW5W6R6UJLJ9o4qi1NZCdU0QkTDz/jGr7eA7fkxjDWAntbejYKR6Lo+c75RLT99dd3PHS+VtZO+9v472fwm1HL76qeXik21Uwj9C68abY+EfHCfDKKysrpOWVlkHlnEO+kpXTStMF6iLWUzJJ8oVS3kHS9IG8VcpSU0gzWFz76aLrEHn+IpAuU5Jvqv2GiIiIiOgJST8AvH0YK9eB5ZsP8J7323s/4+oicP12f+B2u3MIwGMUjvZ+EhzCtZVZYPFn/K6X0T5+d/URcP2w5InijJorMFsGDAOo3wqfpvcuWsp1cUZPs1IGGjZs25kaBlAvixcD+eTTqS2haAJW20vXgFEvSy94onVQW5ItS+x0cMpc3rTQdtPZtg17teRP5Cat4ZwJGIYuzkmue6GKDX/+7tS2dAAGTpWgWGaVNGoxVEmTWC/lfHqJY2I4qdTWmUqs1dIMi4GGb9ttGC2YxfT7brOioVz359WA0TJRjO3MmnJTeQwfkcTYqiqgutGPi90wAOi+GPjbFSfOwRj54iTtUBPo/jbL/bvQPhTcZ9sWYBblx51UZQks25k2qgUxVUrBstq2DXujCifXDmpLRZjwLbd9FmvnxPrmpYW12/KcO7XLiN47PGm2BSTUPSKNszIl65xoEqQ7b+I5vDxNYr2U8+kljomhgtj2Nuk4Hz+/UL0EAy2YK8F8mysmWjBwKXMbFa1zb9P9Vx1lWdwkmhUNWtHECd+24GxTmyiHjusqbYQnPk4DUznnSEwzwPlG7HlM2rZWlHxdo15mlbJUFdJkPU/Mev7iiYs7EREREdHBkX4A+OhDfNzdg9UbtJX79JMZYHm/P0j8hDVv1QHjFFZPGUD9VuiCoVM7B7Olw2q3YUVc05dWbfivoUrnLejCRUY++TSxYragWzfQv1Yv4bylS8sezbkQCy8L2LwnltlAI/JC2tNB7ZwJWDdw/rg4T63uYU5dYZyCU0yVMqukUYmhShqVeqnl44iP4eRSWWcqsVZLMyqD7bsd3NuEb5v3pWltod37jfym8xg+GkmxHYZ+nDd8MQKAElbbFvQUncgObx9aQ0S/H9DrIA92vOdflmFoY6sF6GdP9tvpQhUbie32IAxYlo6WuSLZFjq4vdaCblkwxFmjVqhio21Bb5k4x6dsaOKkOW/iObw8jUq91PJxxMdQRXx7m3ScT5rvlftyfwCvU8PlOqBb533nnMPitB2B5Ufo1JZQrjsDf+L4ZKG6ETO4qyIpTnlQOecIp8njfEN2HpOX8PlsPmUexGDLHd75yzDjTkREREQ0TOkHgCW2r83hwp1HuPo77/XOh9DZAha3Dge+7/v+Nf/iHuOD8/vAnWfwj71XR8/iHy/MAIv7+NvIJ4cH0YRzvV0CSqdgoI7LwpVpoboB2xYvMNScONb/o1zy6dzDppAvABSOnQBQR77XHd7FUHLHgNfJFHUH+SB1d+7E1WGdT1p6SioxVEmjUi/FfKAQw2mXGGvFNKOWbt8t4NgJAJv3Ak8E3F7zd6JSEI/hw5Mc2/x52/sleZwLVVxyetkkHXjRnPiq0Y8X3X8NpyzD0toazS0ix06ehS7bVpsrMFs6zp48Jsx4Qtz1I+/sJZp0PIePTaNSL8V8oBDDZGrtbdJxPm6++BRwc8VES7dwY+Ayp3OsegOW3oIZ+7RtQrubk7g45UHlnCOYJqHeKc83+ucx+evvD/mWWd3gyx32+csw405ERERENAzZBoDX57CwMI93L8xg8eoDfNAbtJ3BJ3eAO8cf+r7/+yN+++ELwe/7vvcA3bs/Y+uMN0g8h62rP6L78UPkO/57C/Xe68lKOGUArbXbMRemKpy7wFu6hWz9HpJ82ltoQUfo+qJ4HNKb19Nob6EVuLBz7pLG1orwDSbh9U+dGs6ZLRiN1cROJnUJF3eeUJklxDQqMVRJo0I1n6HE8AAT19kB5L1Wzzm2qG8LpVX3lc/aEmqdJipa0XmCR3wMghw8hg/PUGKbxH06JxSgvuJxHcAmfA+6Jeq/gjJas1JGHTrOngy2gXmXJX/ek13lcPs8DIWTOKuHn3Rxnl5LaLNHbDzWD9EIhM6beA4fm0aFaj55xDCxvU06zifNR/Ap4Kbz9K9xKc8nX5MUUHXuyoHwJuq+zm2sJbS72ajEKTuVc45gmnzON8LnMfkJXdfkVOb0Mix3SOcvw4w7EREREdEwZRsAfu+BO7j7AMcvvICF9w/D+XTvPqzuHrqW90Qw+k/8+r7vu27OY+HdWfz2rjBIvDCH3kPBmXVQu+y8bsu7lik5V9wxr2yK4n5HStOgeQM2A71OKq980mqiUq4DkgGP1uZx3Oh956bt3L1d7H9bp7liomU0Qq/pyqS5AufNcXGZRpe5TyXNkzeUGB5YB2OdhdVR9nWyOlVIfvImrIRVu+E8pVEsow5k61ScaDyGD0+esU3BfeIqV27nfLhzT9hn0Qg+DTZoWVominEDLgMJllXMs1DdgN12Xs9oFsPz8+V24kteJRrfZg8qvu5xVJ7CIjr4os+beA4/fNljqNbeJh3nk+Y7adyncMtpb3ITj8MaNM05R02ltOp+1znqG60O/00BndpScLnit3VDZQvX208lTplEnnP4iGkGPd9IOo/JJOG6ZuAyZ5RpuXmdv6jGXdw2B9xviIiIiIiGJNsAcM8+fnf1EXBnFh+5g7vRZvDJpwC2D2PlOoQnhx/jg48fYBmzWAm8LjoD9y7jwAl/6RQM4fs2apzvVjkdLDba1ibKmoal1FeUeeWTjnfnqnUjPFAR+E6Sd+HkvT6pWUG5nvfTiW5HSELHRFyZPSppnrihxPDgOhDrTMpAo9fJasNuW4BZlHRUxXM6uspAwzsG6KiXNWihb1kRj+FDlGtsUygcg9qQ3QnEPTQWGIQtmoDVhh06xvb32bb7RFBgNxu0LLqFtv9YIO0UTEs4vsjyLFSx4R57nI7t+A72TIRtoXN7LeVgQhoKdY+g8hQW0UEXd97Ec/ghyyOGadrbpON80vzeNpD26V/xOGzDthsDfS/V+Zas/BXXHv+3rJ1XdTvLbEgXKJZNoY1IjFNKKucccWkGPd9IOo/JJOG6ZuAyZ5R1ubmcv6jGXdw2B99viIiIiIiGIadRVuBo4XF/cFfFpzO4A+B44bEw4xHeWQTufDIj/D6Yzu01tABncEW4KzPrN+OcO6yHkE/xOHS0EPp0UdRryhQ0KxrKdR1WW+GCGcFXnzVv1UN3txbNVu8id6BBD+/JgZiOCZUyR6ZRiaFKGhUK+QwlhgdU5Do7iApV3LD0/hMcCtuC90SAbrV7T5IUqhuwncclIjoXpheP4cOTLraS1+yh/5RG7Os9Q4o4rsd/n6/tvPsPsaESBmE3Eg4oheqG81TSZf8NGzmVZdQKVWw0fIM8Q+G+otRcQRNNrJgtYaBpPLS3WtGdwEQTIPV5E8/h1dtZhXzyiGG69taVdJxPmp8mDnlzz49b5rnwk7fu4F5cu5uryDilPK9ROeeITZP9fEN+HpMj8bomhzIPJuty8z1/GXrciYiIiIiGKP0A8PZhvL8wD1N4R/N255AzePt2Upp9nHwPwNuPsAhgqyMWwfl+8OI7j4TfB+F9n6oh3JVpO4MtoQvBAUVefKTk5eNeGPvvjEbvKZf0nZxOBwtgNGSdMO4FlvjNR1/HR2lVvKvVvRPWvciVXgAncDpT/N8YCoovsyM2jUoMVdKoUMhnGDE8iGLX2SRQ2BZC37rziN+bIx7DhypFbKM6yDFAZzsAoIBjJxB8PZ+f+6q+LJ11UZxXbvq/TfjkypLZCI4Z3lNctyrOtysvjduB21s/A72Kn2j8xZ838Rw+No0KhXyyxzBFeytKOs4nzX+CCtVLzqdOVm4Jc3zfKZa1u8Mgxin38xoV+ZxvhM9jhimfMqeXfbl5n7+MNu5ERERERPkRR1+THd3HbxeB67dnfT/O4h8vzPRf5yxNcwgffTiDxas/4z0AOPoQ55eBOxfmet8EBg7h2vtzuI59nP9AfDJ4AHHfpyqdggGgHnnFLWqiogmvjnLzj7v4CFPJx7tr1XfXdO+pwXSdnJ3aktvBYkd8t8p9TVjggsb9Hlfcd42ySOiwTS6zShqVGKqkUZFXPhNE0nmSvM4OIueu8v6+orAteMce4S7y5oqJVkyH6lTiMXx40sS2UMUlA6iXhW/odWpYGrCtKK1638AWYtmpYanofLfwRtpMVZTOw+l37u9/T6wsaTQrwqvmO6idG8Exo3ASZ3WgXg9+u3IsjNP6IRqC5PMmnsPHp1GRVz4xVNvbpON80nxFzYqW/zdxpUpYbRhAvR76HmrvO8VFTXjzTQeZ3+qvEqchnNeoyOV8Q3Iekx/xuianMg8g83LzPn8ZatyJiIiIiIao2+3ag0w3l20b6E+LV39ITLN8M5zP3at/DqTB4k/2XcnyVKabN2/afg0DNmDYjcCvff75bUu3AUim/t/L0hhC5rI0g+Rj98rXn3SrLSZJ0LCNUDm8Sbf92YXKJCuQT9vSbeiW7S9RKI/eFFwH8etFpcwqadzcFGKYlCZdvaLzEcliOO4AiD/5BNdLsP5q60wl1ippsoKknpHLlewryduCLB75lf+gEuMef6yYhmN4fpAhth7Vevc0jNAxWSTGSDVOKsdPp7zhOjq/h8ulWpbEZcvq3TBCefvzl8UWQGA5oTRxZbCTlykrpyxm3nKD69o5hgXiI8lPZV6oXpL6RaWJ3f6IXJC06eNPdp7gTbL91jc/YceQHcNCefQm2blu+LjqUCmzSho3N4U2NClNunpF5yOSxdCDDO1tqLxJ6ymiDHHHXGd5sm1IVka1Y3303/djK90sZe1UUp0j0vmF/iYibShdRDnj1rdHJY1H3N4gxtgVFVfnd8n6laybKLK6A9HHD9Uy96iURSGN6nJlsfLqmHj+IpDl1f+9X96odCrLILIl7QWls7OzI/5EKTB+2TB+2TB+2TB+2YxT/HZ2duwvP/vc/vKzz+379++HJtM0lSfxb+/fv9/LW+t2u7Y4KHxQra+v4/Tp0+LPRJQTTdPgXKtMtmmp57hh3IeHsSWiacXjH40StzciIlLB9iKb3d1dHDlyRPyZFDF+2TB+2TB+2TB+2YxT/HZ3d3H4KecNyi++tCDOxsWLF8WfIl25ckX8CT983wUGegU0ERERERERERERERERERGNJQ4AH0hNVDQNWuwkfC+HiIiIiIiIiIiIiIiIiCbeIU3TAOfjE7BtG48fP8bjx4/x6NEjPHr0CH/+85+xv7+P/f19/PLLL/jll1/w8OFDPHz4ED///DN++ukn/PTTT3jw4AEePHiA+/fv4/79+/jTn/6EH3/8ET/++CN++OEH/PDDD9jb28Pe3h663S6+//57fP/99/juu+/w3Xff4dtvv8W3336LP/7xj/jmm2/wzTff4Ouvv8bXX3+Nr776Cl999RX+8Ic/4Msvv8SXX36JL774Al988QU+//xzfP755/jss8/Euk2wElbd9RU9raIk/hkRERERERERERERERERTbRD3jcnvCdHDx06hEOHDmFmZgYzMzN46qmnMDs7i9nZWTz99NN4+umncfjwYRw+fBjPPPMMnn32WTz77LOYm5vD3NwcnnvuOTz33HN4/vnn8cILL+CFF17Aiy++iBdffBHz8/OYn5/HwsICXnrpJbz00kt4+eWX8fLLL+OVV17BK6+8gl/96ld49dVX8eqrr+K1117Da6+9htdffx2vv/46fv3rX+ONN97AG2+8gTfffBNvvvkm3nrrLbz11lv4zW9+I9aNiIiIiIiIiIiIiIiIiGiqaN1u1xkBngDr6+s4c+aM+DMRERERERERERHRWNjZ2RF/IiIioily+KlZAMCLLy2Is3Dx4kXxp0hXrlwRf8IP33eBSRwAPn36tPgzEeVE0zR4bw2YZNNSz3HDuA8PY0tE04rHPxolbm9ERKSC7UU2u7u7OHLkiPgzKWL8smH8smH8smH8shmn+O3u7uJpdwB4fggDwHvuADC/AUxERERERERERERERERENCH4DWAiIiIiIiIiIiIiIiIioglxSPyBiIiIiIiIiIiIiIiIiIgOJg4AExERERERERERERERERFNCA4AExERERERERERERERERFNiMEHgNfnsLAw35/MWTGFWhqfdXMeC+8fxrY4g4iIiIiIiIiIiIiIiIiIEg02ALw+h4WVR7jb3UO3u4fu3Z+xeH0uOMC7PoeFM7NYvumm6T7AspjGb30OZ66LP+apg9qSBk3TUGmK83yaFWiaBk2aqImK5uThTdJkyCMflTQq1PNpVoLpemXv1LAk5BGVn5jHUq3TnxmRRluqQUylkgZIijPQqS0F85GkU0kD5LEs9XVx4LnbTLB+avVPjqMrYX3kLVQuTYOmLUGyiYfTSsoobuOyfYX8pvUYPgoJsW1WoGkVyGZ59XS2334+kZOwgNC+Ikkjo/J30jQR+yyi0kvKIk3n34eblfByZL/5ROUZbPvE+EbnByQvUza/X46Yv/Nt24HjViA/saySyY2tSt2j0vC4SZNNvR0Rzyl4Di/IvCz1dREvob0NHTvFY3H0fKcOYvr+NiBbn+j9nayN97fv3k/hdqMXW9U8PNJtM5hHaL14k3SbEmMjmSpN5ThJl610nhFVPo9YzhG2m/KNjoiIiIiIJtgAA8CzMM/MYvG3+zjq/XT0If7p6iPg+izWAQCHcG1lFlh+AOs9L9E+rJv7wPXDuBZ6xNfJc6iaKzBbBgwDqN+SXfy4F13lujijp1kpAw0btu1MDQOol8ULyDzy6aC2JEsT1VkQRTUfp8zlTQttN51t27BXS87sQhUb/t/dqW3pAAyccpM1KxrKdQMNL03DQMssBi76Q2nsBoyWiaLvglUljUqcO7UlFE3AavvyqZcDF78qafJZluq6mFRq9U+Oo5dX/PoYHv92aaNhtGAWwwMoSXUIbeOSfYUEU3kMH5HE2KoqoLrRr7PdMADovn3B1664cQ7uK779RdqRLND9bZb7d6FO1+A+27YAsyiuhwHKEli2M21UC2KqlIJltW0b9kYVTq4d1JaKMOFbbvss1s6J9c1LC2u35Tl3apcRvXd40mwLSKh7RBpnZUrWOdEkUG1HeA4flyafZamuCwWx7W3ScT5+fqF6CQZaMFeC+TZXTLRg4FLmNkquc2/T/VcdZcWANCsatKKJE76YOtvlJsqhY7pK+wDldidVnAY4z4guHxLWoVr5+xSWq1R+IiIiIiKaZOkHgNdncR2P8Nu/fRz4+egHf0K3+wDvAcD2LD68Ayy+8yiQBm8/wiJm8OFHwcVuXzuM64s/4+py4OdcNW/VAeMUVk8ZQP1WqDO3UzsHs6XDardh6cJMV2nVhv+6q3Tegi50kuaTj3MBGE4DbN5Lc8mmlo9TZgMN8aIxVhMrZgswTqEEAJ0aLtcB3Trv/D8AlFbRMIDW2u1ex8W9TfT/xkmE85YOtLbQVk6jEmenfLp1A/3reDef3vpXSZPXstTWxeRSqb9KHFXWx+iE912FOijtKySazmP4aCTFdhj6cd7w7SsAUMJq24KeoiPZ4bUTa4gYtwR6HeTBjvf8yzIMbWy1AP3syX47XahiI1W7rcqAZelomSuSbaGD22st6JYFQ5w1aoUqNtoW9JaJc7x5hiaOWjvCc/i4NHktS21dqIhvb5OO80nzvXJf7t+QJlu3Q+G0G4FlR+jUllCuOwObgfFMAIXqRngQM3eDxkntPCNe0jocpjzKT0REREREB03qAeDtziEAj1E4Ogsz4fu+xwvBQWIcfYzjwV+A7cP4TxeAq//0cIgXPk0419sloHQKBuq4LFydFqobsG2x81fNiWP9P8orn9HxOnPjLnjDnCeAdFjn3b9qb6ElqUPxuL/Tp4BjJwBs3gs8BXB7zdcJpZRGIc6de9iUlKdw7ASAOm41FdPktSxKphjHxPXxBPTKrFIHpX2FgngMH57k2ObPO6Zfkse5UMUlZ5RWMgAZzdnP1OjHi+6/hlOWYWltjeYIcezkWeiy9qu5ArOl4+zJY8KMJ8RdP/LBaqJJx3P42DR5LSs3au1t0nE+br74dGtzxURLt3AjMgD5OVa9AUtvwYx9M0VCmzsig8YpzXlGnLh1OEx5lZ+IiIiIiA6O1APAjlmcWTiMd+563/f9EVe3fN/3/XQGd8Q/8bnzyYz7r0O49p+eAa4+wAe990kPQfMW6r3XnJVwKpcn7TqonXMuFr3+k8Eo5hPROZNaKB/nTmRsrQjfYRJfi+onuXgvHofsxnrnQnMT3g3ypVX3VXDaEmqdJipa0XlywXcLuEqaRO0ttKCj18fv8ZdTJY2KQfMJrYspI9Z/0Dg+Qd7r4rxXKCrVIaI+4r5CPjyGD89QYpvEfQImtKP0FY/rqfeH/msoozUrZdSh4+zJYBuYd1ny5z2xVE5on3NSOImzevgVpc7Ta0+24140HuuHaARC7QjP4WPTqBg0n9C6UJDY3iYd55PmI/h0a9N5qtW4NIqnSwGggKpzRw6Etyv3dW5jLaHNHY3B4qRynhFPZR0OT/byExERERHRQTPgADCwGBi0fYwPzkd93zfa9rU5XMDP+KcPhCeFc9VB7bLzui2v66HkXHEP8Poj9ztSmgbN69AY6JVNafNpolKuA0kDDImi82ltHseN3jeC2s4d3EXJdw/hPQHk3sHu8TqLLwvf+LosfnOrhFW74dx1XSyjDsBorApPLqikOeii18V0OKj1r6Ps62R1qpDuyRv1fYUcPIYPT56xTcF94ipXnRrOmbKnioR9Fo3g02CDlqVloqg84KIqWFYxz0J1A3bbed24WQzPz5fbkS95RWag7c9NfN3j8Ikmmg7R7QjP4Uctel1EU2tvk47zSfOdNO6TuGWFm9N6xGOwBk1z1l8q7qvD6+WI7c/lHzjv1JaCyw19o1YsW7jOg0gdJ8XzjKTyqaxDNemWG11+IiIiIiKaZAMOAIe/AeyYwSefet/6jbb4zqPAq5+H+fCvd6dxoKOjdAqG8N1HNc43oJwOFhttaxNlTcNS7NWWTLp8vCeWrBtxAwzJ4vIJfIvI6/iVvvrM7cAIXSgXUN3w7vr3LkSL2DphADgB7zrfucgvAw2v7jrqZQ2a7/uKKmkOurh1MQ0Obv0NNHqdrDbstgWYRUlnVRy1fYVcPIYPT66xTaFwDGpDdgn7g38fKpqA1YYdesqsv8+23aduAk3JoGXRLbT9x4K4V4wqE44vsjwLVWy4xx6n8zi+kz0TYVvo3F5T6yQfiELdI/CJJpoGce0Iz+FHK25dRErT3iYd55Pm97YBtadaHeIx2IZtNwb61rvzfWT56609/m8nO6/pdpbZkC5QLJt6+xBPIU4pzzOUy5e4DlUoLFep/ERERERENMlSDwAfFb/rG2OrI2S/fQhb7reBtz+axR3M4MK7/e8In7kO4M4zeHfh+VRPEsfp3F5DC3A6H3qdGs4dzVm/GefcOTzcfJoVDeW6DqstuahLIXU+Ua8+854ckF4ol7AqdB6cP74J6MdRRP/OY91qw7v2LFQ3YDu3ijud8ippVBSPQ0cLoU8s+V/1ppJGRcp8Uq+LCRNZ/5RxHAuFKm5Yev8JDuU6JOwr1MNj+PCki23EK3Yjvp8Yrwjn05LijtLXdt7LHL8/CIOwGwkBLlQ3nCeTAk+55VSWUStUsdGIGuTJi/uKUnMFTTSxYraEgabx0N5qhQfoiSZI6naE5/Dq54wp80m9Llzp2ltX0nE+ab6k/CPhnhu3zHPhJ1Ldm67i2tzRi4lTyvOM1BLXYUbDLj8REREREY291APAztO9M/jwI9mf7uPkewCO7uO3i/5v/bo+ncEdPMI7bwNHP/iT+/3g/nRzGcDiz7jb/VNO3wT2vnPVCHRo2LbtdEbkdbGVV8ewkI/TyQAYjXSdDKL4fNzOb/Gbj1EdH7fqgP+bp7Gc+Pc6jKO+lxX6pldCGhVuB4P/DnP0nhRyO4pV0qhIkU/8uph8sfVPEcexNXAdhH2FXDyGD0+K2EZ1kCO6rYhXwLETCL5e2M991fAw9gfnlZv+7xM+ubJklrZdHID3JNetivPtykvjtiF76yftq/iJDoj4doTn8LFpVKTIJ35dxEnR3oqSYpc0/wkpVC85rwFfuSXM8X17V9bmTqMxXYdERERERDQZZKO48Y4+xD9dfYQ7F57Beu/HQ7i2MovFqz/jPcD3TeA5mL1EszDPzALLD3Ma3FUg+86Vp3QKBoB65BW3qImKJryeyc0/XcewWj6d2pLbyWD37qIfRHI+7uuvAh3i7retxG8Epepo7aC2VIQJCze8TLyYB56+AporJlpeh5RKGiXek0u+u897TyZ45VdJo0Itn+R1MUEknY/J9VeL43hxnorr7yuD1EGyr5CDx/DhSRPbQhWXDKBeFr4v16lhSdZWKCitet+IFGLZqWGp6HyPbyj7Q+k8nL7nfhvzxMqSRrMivGq+g9q5tO3iALxvg9aD364cC+O0foiGILkd4Tl8fBoVavkkr4sYqu1t0nE+af5YKWG1YQD1eug7wr1v7xY14anwDib+jf4Hah0SEREREdFE6Ha79kDTzV9swO5Ni1d/SEyD5fvhNL7p5rJtY/En+65knsp08+ZN269hwAYMuxH4tc8/v23pNgDJ1P97WRpDyFyWJn0+DdsI/b036bbV9qeNo55PqExixRLj2bYtXViGJA95mcQ8k9OEyhuRzilzf9IlwUtKk8+yZHXypjTr9MkCIP7kE6zjoPWPj6P6+shCVs/I5Uq28/g6qO4r00eMe/wxZxqO4flBhth6kustaBiJ9RX3FYT2F7m2pdvQLTsupVPecB2d38PlUi1L4rJl9W4Yobz9+ctiCyCwnFCauDLYycuUlVMWM2+5sm08EB9JfirzQvWS1C8qTez2R+SCpE0ff+rtSGj/kOwYsmN6n+p5iaxMYp7JaULljUgnHpNlx+OkNPksS1Ynbwof15ChvQ2VVzjOJ83viTnmimTHfYfacT767/txlW9OkjYqqb4R6aQkZQ2JSZPY1g9YvtDfRKVNKpu4TCEvlfIT0ZOFA3l+Mj52dnbEnygFxi8bxi8bxi8bxi+bcYrfzs6O/cVnn9tffPa5ff/+/dBkmqbyJP7t/fv3e3lr3W7XFgeFD6r19XWcPn1a/JmIcqJpGpxrlck2LfUcN4z78DC2RDStePyjUeL2RkREKtheZLO7u4sjR46IP5Mixi8bxi8bxi8bxi+bcYrf7u4unn5qFgAw/9KCOBsXL14Uf4p05coV8Sfsfd8FBnoFNBERERERERERERERERERjSUOAB9ITVQ0DVrsJHzLkIiIiIiIiIiIiIiIiIgm3iFN0wDn4xOwbRuPHz/G48eP8ejRIzx69Ah//vOfsb+/j/39ffzyyy/45Zdf8PDhQzx8+BA///wzfvrpJ/z000948OABHjx4gPv37+P+/fv405/+hB9//BE//vgjfvjhB/zwww/Y29vD3t4eut0uvv/+e3z//ff47rvv8N133+Hbb7/Ft99+iz/+8Y/45ptv8M033+Drr7/G119/ja+++gpfffUV/vCHP+DLL7/El19+iS+++AJffPEFPv/8c3z++ef47LPPxLpNsBJW3fUVPa2iJP4ZEREREREREREREREREU20Q943J7wnRw8dOoRDhw5hZmYGMzMzeOqppzA7O4vZ2Vk8/fTTePrpp3H48GEcPnwYzzzzDJ599lk8++yzmJubw9zcHJ577jk899xzeP755/HCCy/ghRdewIsvvogXX3wR8/PzmJ+fx8LCAl566SW89NJLePnll/Hyyy/jlVdewSuvvIJf/epXePXVV/Hqq6/itddew2uvvYbXX38dr7/+On7961/jjTfewBtvvIE333wTb775Jt566y289dZb+M1vfiPWjYiIiIiIiIiIiIiIiIhoqmjdbtcZAZ4A6+vrOHPmjPgzERERERERERER0VjY2dkRfyIiIqIp8vRTswCA+ZcWxFm4ePGi+FOkK1euiD9h7/suMIkDwKdPnxZ/JqKcaJoG760Bk2xa6jluGPfhYWyJaFrx+EejxO2NiIhUsL3IZnd3F0eOHBF/JkWMXzaMXzaMXzaMXzbjFL/d3d2RDADzG8BERERERERERERERERERBOC3wAmIiIiIiIiIiIiIiIiIpoQh8QfiIiIiIiIiIiIiIiIiIjoYOIAMBERERERERERERERERHRhOAAMBERERERERERERERERHRhBh4AHj72vNYWJh3p+dxbVtMoZJmFmZvvm8yZ8WERERERERERERERERERESUYKAB4HVzHu9eAK7e3UO3u4fuzce48O48zPV0abA+i+t41E/jTda+L1FeOqgtadA0DZWmOM+nWYGmadBiEwGd2pKTbqmGjjCvWXGW05skaaTphGX2lhExX00TFX8eYv07NSwJ82VpQ2WV5eVRiGEov0HrnrAs1Xwiy6MYHyep2rKSyjwR3LgFq5iwLbrGMY7NSvR+3Du29MqhVk9gtHU4+Kb1GD4KMbH14imbliqouH8XObkZhmLRy0MSW8lxd6kWStWjlHevHhWIVfT2WekyJGUJ5dGsQNOWEPjzlMtTqcPgaYSyOSl76zw6TZ80X9/GonaMrAnLlEyhDdAli7GfZH6/zDF/5zteB9Z/ID8xVpIpxXYelUa6/dGUSzifkB6fwmlDbZUsL49CGxrKb9C2L2FZqvlElkcxPk5StWUllTmKk79aeyA7nqVtU3qkMQjmEaq7N0Ue0yP+RoxJnvUgIiIiIiKigaQfAN4+jJXrwOLVB/jgqPvbew9wcxm4vnIY26ppAGx3DgF4jIKXZpiaKzBbBgwDqN8KX3L2OvjKdXFGWKeGcyZgGLo4B82KhnLdQMO2Yds2bLsBo2WiGLiIdpZV3rTQ7qWzYa+W+ilqSyiagNX25VMvhy+uY3VQWyoDjf4yGgZQL/s6PQpVbPjL4E5tSwdg4FS/SIAulNe24SuyYgzzqnvystLkE1kexfikWVZcmSeXwrY4xnEsnTKAlokV2e7XuY21FmCcKinX80nU4cCbymP4iMTFtrQaOv7ZbQs6AP3seaxu+H5vGAB0X52DMQH8cXWnjSoKvhTNigataOKEbx+y7TbOrhUTOoXj8+7c23T/VUdZcR3Iy2KjbW2iHNMxjgGXl1SHQdO0LcAs+o9BHdSWijDh237bZ7F2Lr5OwXMAd3t246B2jKyimmp7yUsLa7flNevULiP5iFFIWe7068h2VlLsgAtNG4XzCcVzVEDcf52J5/DplxVX5mEapE1J14apHLcEMW1ClEHqQURERERERINLPwD86QzuADheeBz4+e13HgF3ZvHRtmIaAJ9+MgMs7+O9QKrhaN6qA8YprJ4ygPqt0F3Hndo5mC0dVrsNKzwm4NNB7ZwJWDdw/nh43r1NAMYp9LtCSjhv6UBrC20vVe0czJaBRuSFdRMrZgu6dQPVXgI3H0nZozmdlv4OntJ5p+N+817c5bmz/GA9kqnEMK+6Jy8rTT5x5ZER45NmWXFlnmQq2+IYx7F0CgYkg2MAOrfX0Op1JKrU8wnV4YCbzmP4aCTFNsiJX0u3cKNfuXw0KyjXAaMhDkw4+9VG5uUZsCwdqF+OeSLU0aktoVx3BvnEMclCdSO5YxxItbxhKlQvCcevNrZagH72ZL8OhSo2lOrk8faLNdx2RoAVj5Gj5qyDlrki2a47uL3Wgm5ZMMRZo1aoYqNtQW+ZOPckNxYaI2rnE2HiOaoalTY0r7YveVlp8okrj4wYnzTLiivzKKi3Kfm0YWkIbUIs9XoQERERERFRNukHgAEAj/DO2+JvoqQ0h9DZAha3Dge+//v+tQGLFKsJp3+75HZS1nFZuOIsVDdg2xu+i385r7PhkjRhAcdOANi8F3hS7Lbz6Ivb0eB1OJ6P7pjp3MMmgBPHgssoHDsBoA5J/2qunCdidFjnI0solRzD/OqeuCylfBTKIxGKj9KyFMo87cY6jiWcckY3hEEEcf9W82TqcJDxGD48ybENaK7AbAHGpbw7jzuoXa4DuoWUTU8qx6o3YOktmLFPu3rr/FLi9pREbXmjoR8vBv6/teXd0jAYZ3v25HuMzNOxk2ehy/a75grMlo6zJ48JM56QQhWXDEQMVhOpCZ2jKkpuQ/Nr+xKXpZSPQnkkQvFRWpZCmUdErU3Jrw1LI9gmxFOrBxEREREREWWVfrT17UdYxAw+/Cj4p59+MgNgBp98qpgGM/jkDnDn+EPf939/xG8/fAEL5mzg7zJr3kK99/SJ00nZWrud/oKzU8M5swWjsRrZ2VBadV8Xqi2h1mmiohWdu9N7t187T95ga0X4JpPvG0ntLbSgQ+irBYrHkfmm8/YWWpKOjr6YToOWiaKvzPGv45QZYd2V8lEoT4gkPkrLohBxWxzzOJac0Y3gIELg9c8RxHpSejyGD0+q2DZRcR7RDT1RlJ0b1xPHch5YFhVQdUbZ5K8rRn+/FgdMB6OwvCFrVsqoQ8fZk15kvafbygntXbz+qzwdAx8jh61wEmf18NPJzpPvknOdJ6h4XAewidgHPGl6JZ5PSM5RPTyHl8dHaVnjRKFNybUNUye2CfEU6kFERERERESZpR8APvoQ55eBOxfmcM37mO/6HM5cT5kG+7C6e+ha+77fHuOD8/vA9cP9v8vMfarI9/SJ8606lVdUBTVXTLQSO75LWLUbMNCCWSyjDkgHG1qbx3Gj992ktnMXdLEy5Kc+3M77uCesvKe7hM7a0qr4/SgdLTPpm4xyT6bu0VKVJyI+lJbCtjhuSufhvBGwv2V0bq+hFVuHA1jPscNj+PCki60zkOgfDE+rjnJCR/3gHdbJefeUVt1vacavL/8gS6e25MtbS/zOYYDi8tTqkD5NGY3Qk2uF6ob7LecWzGJUPjHcmykCAykDHSNHwR1o8L9utFODs+kPo2Aq60guzRN0NG0UzicizlF5Du+KiM/oiMcGDZrmnGekotimpGvDxLKpH7eAiDYhiWI9iIiIiIiIaHDpB4ABvGft4ebyDC686766eeUR7t79GYu+1z6rpInmPSWcA9nTJ6VTMNDCmqyHO0qzgnI9uePbucAuA41+J0u9rEGrBC9tA9/e8zonxSdncuY9BWTdiHp1p/orOAvVDTRinxSL9iTqHke9POrxoXjJ2+I4KuCk8xiZ21Hlvn4wsP0EHcx6jhkew4cnTWx73+cND4arM9DwDUKIg5LI9Fri5Lz9nG9pxr/u2v+dTef1n07ejQE+GKuyPLU6pEvTdp/0FTZfR6GKDdv2DQQndML7nyAsmoDVhh3Yn9IfI0dG2K6HOzCtso7k0j1BR9Mk+XxC/RyV5/DivFERjw02bLsx0DfIVdqUdG2YWDaF41Zim5BMpR5EREREREQ0uIEGgOEO8PZe3fzxQxz9dAZ38BiFo+nSDFvn9hpagNOBL9xtneY7a81b9dDd0UWz1bv4Xap1enc/61a794RZoboB27m9Wd4B6/G/aqx4HDpaCPWDR72mTEGzoqFc12G1Yy7oB/m2Y2sLYjFTG0bds+QT9dq3qPhkWdYUitwWD0AcC/5vSXZuY63lf61qUGQ9KRUew4dHPbYKT55lVoTz9lv/95eHqFDFDUtHyzwXfsqpcAwnMg1GS8Qtb4i8gZ76ZfFpL59CFRuNqEETH91C2zdAsCE5sKU5Ro6W+3pzcwVNNLFijsnAtKDtvAcdkW/4pamkdD4RdY4ah+fw2Zb1JMW1KcNow2QU2oREcfUgIiIiIiKizAYeABat354FlvfxnjjDJ5Bm+zDeX5iHuR5Ms905BGAfJ+MyUuZ966kh3G1tOx36SZ2dPuLr02zvyRr34nejWoj+NlegM8Lp5A7dde/vaHAv3P13bqP3ZEj6jkGn4wgwGjEdR70BEu9bkEk6uLcJQD8O9b6REdZdKR+F8vhExkdpWYSkbfEgxNH3LcnmiomWfhaysY3YelIKPIYPj3psO7XLCU+e5cF9enSE3wMsVC85r/peuSXM8b6R63tlcA6ilzdczmu9E+IaNWiSluIx8knwnjS7VXG+e31p3A7O7mupdet8hqfsadKonk9EnqNK8Ry+R2lZ4ym6TRlOGzYs0fUgIiIiIiKirAYYAJ6FuTCPBXO298v2tedx5vojXP2d9z1fhTRH9/HbReD67X4a4BA++nAGi1d/jh1IVhb3rafSKRgIfqsuMy9P4Umb5oqJVq/TwX09WaAz1n26qvfdJO9JFd/d0L0n09J1DHZqS27HkR3/3cu4jsdODUvCt6I6tXPyO+ljjbLuKvmolKf/t5HxUVrWlJF0wCVviwchjt4rTsso18VXDzqS60nKeAwfHtXY9sp9I3bwIQ+F6g3nG7JlLfS0dbPiPqWdqxJWGwZQr4e+weiUxfk+brAs7sDJQKKXN1Tet3m97bpZEb7/2EHtnH8bzyL5GPnEeIPT9eB3r8dCp4aloomWbuHGsHc0OjCUzyfizlF5Dh8fH6VljavoNmU4bdiwRNeDiIiIiIiIMup2u3bq6e5P9iJsG73pF/vmIGm6Xfvmsj+NbS/fDKdRnW7evGn7NQzYgGE3Ar/2+ee3Ld0GIJmi/75t6TZ0y24Hfm3YhkIeoeUZYgqvfP1Jt4JLSiYrizfptj+7+Fi1bUsX/z6cNlSniLShdAPUPZRHxLKS8rFleUWWJ1xnv6RlhZYTUeZxBkD8ySe4vQXrn3ZbjMpnNHFUq6dseWr1HEUdDiIx7kn73eQfw/MzaGwtsZ5xcWkYof3ZE4qXN4XiL08bFztZejFvJ428vt56kqxCt07R+fbTBOuddnnqdVBJE16u83vMMUisk0C+r0SJO0b6SOIWSbYe/NuFJC9ZLLx6B9e1U97ANibJT2VeKK6S+EalkW5/lAvEtunjStYWeZPsvClqf+M5fHx8HEnLCi0nosx2xPYmOx451I4/0X8vb1N8M8NlFo7lkXWLOeYrtQl51oOIaALJ2gtSt7OzI/5EKTB+2TB+2TB+2TB+2YxT/HZ2duwvPvvc/uKzz+379++HJtM0lSfxb+/fv9/LW+t2u7Y4KHxQra+v4/Tp0+LPRJQTTdPgXKtMtmmp57hh3IeHsSWiacXjH40StzciIlLB9iKb3d1dHDlyRPyZFDF+2TB+2TB+2TB+2YxT/HZ3d/H0U87bkedfWhBn4+LFi+JPka5cuSL+hL3vu8Bgr4AmIiIiIiIiIiIiIiIiIqJxxAHgA6mJiqZBi50qyPHLmERERERERERERERERER0ABzSNA1wPj4B27bx+PFjPH78GI8ePcKjR4/w5z//Gfv7+9jf38cvv/yCX375BQ8fPsTDhw/x888/46effsJPP/2EBw8e4MGDB7h//z7u37+PP/3pT/jxxx/x448/4ocffsAPP/yAvb097O3todvt4vvvv8f333+P7777Dt999x2+/fZbfPvtt/jjH/+Ib775Bt988w2+/vprfP311/jqq6/w1Vdf4Q9/+AO+/PJLfPnll/jiiy/wxRdf4PPPP8fnn3+Ozz77TKzbBCth1V1f0dMqSuKfEREREREREREREREREdFEO+R9c8J7cvTQoUM4dOgQZmZmMDMzg6eeegqzs7OYnZ3F008/jaeffhqHDx/G4cOH8cwzz+DZZ5/Fs88+i7m5OczNzeG5557Dc889h+effx4vvPACXnjhBbz44ot48cUXMT8/j/n5eSwsLOCll17CSy+9hJdffhkvv/wyXnnlFbzyyiv41a9+hVdffRWvvvoqXnvtNbz22mt4/fXX8frrr+PXv/413njjDbzxxht488038eabb+Ktt97CW2+9hd/85jdi3YiIiIiIiIiIiIiIiIiIporW7XadEeAJsL6+jjNnzog/ExEREREREREREY2FnZ0d8SciIiKaIk8/NQsAmH9pQZyFixcvij9FunLlivgT9r7vApM4AHz69GnxZyLKiaZp8N4aMMmmpZ7jhnEfHsaWiKYVj380StzeiIhIBduLbHZ3d3HkyBHxZ1LE+GXD+GXD+GXD+GUzTvHb3d0dyQAwvwFMRERERERERERERERERDQh+A1gIiIiIiIiIiIiIiIiIqIJcUj8gYiIiIiIiIiIiIiIiIiIDiYOABMRERERERERERERERERTQgOABMRERERERERERERERERTYj0A8Dbh/H+whzWxd8BYH0OCwvz/cmcFRLMwvTPj0qXmA8RERERERERPVlNVDQNlab4O9GodVBb0rBU64gziIiIiIimUsoB4FmY7z6DO+LPcAdtVx7hbncP3e4eund/xuL1ueDg7fosruMRrt5103iTtR/M58wslm968x9gWcxnIM7FgJZwcdqsOGl6U0TiTm3Jmb9Ug3h50ZsXmYdzkexPE0qilI+K5GWF6qyYLnxhlbwsSPKRxRAA0Kw482WZeBLSqMYwVKZAOrV65bOsCdGpYSkUp3zjmLTuc+UuK3Kb95VBpfyhbSBqHyCfaT2Gj0JCbJsVaFoFslleLPz7RqjemgZNW0Jo93FJ00sLEqT0d81K7LL7EmLgmx+sj/i7ZPIyjCuLe8z0/134eOMjy8s7JkrXVXg9AfJjtTSumnxfiS53PnGRlkW2ggapu09/OfJyOPr7vSyvdGWVlRPyssbEB1HLFfNISOtft/I0suWL61iWpk+ary8+zUrENgb0l1WpqW9XEyG5rQm1eYrpwttH8rIgySdynamcoyWkCW0zEelCZQqkU6tXPstSEHnMFJPF7y9Q3mecv5Hmpw2674d1apdR1y2cL3n/L8tLKO+gx21JDEN5yI6bKZenVAeB8zdq+Xuky4nZrlTTS9NFlEGUqh45xLpHYd1G1au/XgqoXjLQMlckyyYiIiIimj7qA8Drc1hYmMN18XfAGRg+M4vF3+7jqPfT0Yf4p6uPgOuzvaeFtzuHADxGoZdIdAjXVmaB5Qew3vN+24d1cx+4fhjXtoOpU2muwGwZMAygfkt2OeBcKJc3LbRtG7Y3rbpXsoGkNZwzAcPQxTno1JZQNAGr7eXRgFEvC51cZaDRX0bDAOrl4IWTSj7JOqgtyZYl6fzQhXrbNvxVb1Y0lOsGGt78hoGWWfRdvKktK5SP3YDRMlEMXEy7nRblev8PQ5LTqMUweb3nt76SlzW51LaPNHGMW/e5K62iYSDUmdCpXUYdBhruOlQpv9o+QCFTeQwfkcTYDsK/jdtoW4BZFNseZ50F4+SLlbTjUBBou9y/G2Rfio1BB7WlIkz4ltU+i7VzNXRQQHXDV/aGAUAP1ke2Dfo0Kxq0ookTvm3Ktts4u+ZvY5N17m26/6qjnHk7C64/27Zhb1RR8KWILzcyxiXdtpFf3VtYuy2PuXO8l0lX1uEQ1pezw0XsC8nrVkwT3n/j9okYMftr6ZQBtEysyILVuY21FmCcqmbcrg4StfMmQIyrM/Ec3pFfe528rCTxx0z/ulA7nqjtM/7y5bHvy3Rwe60F/ezJ2LzE5Q1y3JbH0Ebb2kRZerzrG2R5SXXIRn1dD5Ye4fLHtg35GSTW6dZtwnopnYKBOkKnc0REREREU0htAHj7MN4/M4vFqz/i7tVH4tzek72//dvHgZ+PfvAndLsP4I3lfvrJDLC83/v/kO1ZfHgHWHxHWMbbj7CIGXz4kVpxZZq36oBxCqunDKB+K3SB1Kmdg9ky0Ei8qOugds4ErBs4f1yc18SK2YJu3UC1fwWC85YeWGZpNdgxUzpvQQ90Oqrlk8zpmA4vC9i8l+Kyr1PD5TqgW+fRy8obEFu73b/bNnFZHdzbBGCc6ufj1au1hbaXqnYOZkuH1W7DCo/PAEpp1GKost7zWl8qy5pcKttHmjjGrfvhcMrr68jo1HDObPn2C5Xyq+0DFDadx/DRSIptHgrVSzAQHFzt78sbvjgBQAmrbWF/U+LtS2uIGMOLFB+DNrZaCHZuF6rYSNzWFDQrKNcBoxHcprxj5kYwMAoMWJYO1C8rPbU1sNzLHTTYtpG17s7fizf6ONwBDsuCIc4ZqKxDVqhio21Bb5k4N1gwAsL7bx77hLC/lk6FjhGezu01tGAgMJY18VTOmxTwHF5Sr/TttcqyYikeM1MdT0awz4T3fYnObay1dJw9OUhk1I/bndoSynXnhg9x3L1Q3VAcmFVf3rClWtcDpJfKuW2Ipx7rfNatXwnO6VxCPIiIiIiIpoDaiOrRh/i4u4ePPwgO8Hr6T/YK3/gNvLb5EDpbwOLW4cD3fd+/Fi7C8YKwnKOPEeqnT6UJp2+31Lsj9HLgSsTr2PN1jkTwOgAuyTo3O/ewCeDEseC8wrETgMJdqL2/y5hP7tpbaEnKUzyedtCqgGMnAGzeCzwpcNu5Rb0X+0J1A7YtXtwGJaZRiqH6epdJt76yLWsqKMVRYd0PS6GKG72ODGcQsaVbuOEVRKn8avsAiXgMH56k2OZLP150/+Vt95fk+3KhiktOr7NkMC6aE+O01GLQ2lJv7dR0UHNGZnqvzczDseoNWHoLZtLTmAMbTrn7Bt82stb92Mmz0GX7aHMFZkvH2ZPHhBmDl3Xo3GXLB7QH099/HVn3ieD+6nTYh2PFNjITnsNLpWuvsy1L/ZiZ9ngyun1G3Pf9nMHmExBCqEztuJ0QmxTUljdsCfUJreu06WMMoW2IohbrhLoNqHh8PG+6JCIiIiIatfDo68BmcWbhMN7pfd/3R1zd8n+7dwaf3AHuHH/o+/7vj/jthy/003w6I/++sOvOJzPiT2qat1Dv3QXtXCz373pH70kGbK0I350RvmfjPvFnNFblF9TtLbSgI3SNXDwO6Q3ugNMp4A4k9ToFBspHUURHEFomilHfB4pYrtM5sonIBxEkyyqtuq+L05ZQ6zRR0YrOHfXi7b5ZKcVQcb0HDLq+BlnWhBO3D6U4PlkFryOjWHTuwr/huyNdsfwj2wcmCY/hw5MY23w0K2XU4X9CyH2CMBSkvuJxPb6Nkei/djCFxBh4T4OVw9tUJu52e+JYyidbkjjfv4t8NWhmwyq3J8u2kbHuhZM4q4efGnKeEJd1Tmcp6/Dltezw/pvPPiHuryVnNCs4AC99le2UEs+bPDyHj273AwZtrwdZlp/qMTP98WTY+0x43w9rO4VGdKmTKBy33TrFxUadwvKGLu26Tps+Xpq02SjEOtd125d4jCMiIiIimhI5DgADi1cf4IPe930f44Pz/m/37sPq7qFr7fv+QkwzDO5d1767oJ1vJoVfEdnaPI4bvW/JtN2Bnv73dJorJlpGI/RqovTcb19pGjSv8yT1q40G0USlHL4DvbQqfmtHD34bzOsQvSx84+ty9Le7opYFlLBqN2CgBbNYRh2IHowZkaT1nuf6Sl7WtIjaPsad25EBRAwGqBi/fWC88Rg+POqxTa+Osq+jvIxG8Ikv96mrXLkD/On2TbUYFKobsNvOq0PNYpqO/2R5d3oC6L3itV4etH0Jrj9ZfYdSbuSwbWSqu3uM97+y0n2FrnQwJWtZh0z+RHzyuhXThPbfPPYJ2f5aOg/nzbu+M7Dba8EBu6klP2/iOXx8u59ne528rHiJx8xBjiep9pl89v0g99Xg0sFtleW5FI/b/hsSOrUlX95auu/aKi4vVR16xL/RoGnO/tKTdl2nTZ9A3jaIFOqhQjHW6datWDbJeikeh44WMr6ogoiIiIjowMtxADj8DWDHDD75VPxN5KZ5+xEWxVk+oW8Dq5DdBV06BSPw/SdH4FtmvYEe967qZgXlel53uTvfe+p31myiLN6xPwTeXdyBpxYlCtUNybfBvLv+vQutIrZOGEDEK7+iluVc0JWBRr+jql7WoCV9s2iIYte791tO6yt5WdMhavsYf26nKADUyxhksx3HfWCs8Rg+PClim56Bhm9AIrS/FI5Bpfsxqo3p8bdLRROw2rDTrOM0MShUsWHbvkGv+M5MVVlfoxvF+2657HXWyfrrz5nCAwDDKnce20amugvrP3owJZ+yDpP4hK0jed0m7r+etPtE4v5awEnnEWw3H/fVu4Fj+3RSPW/iObx4Xp1fe528rHiJx8yBjidp9pkc930lKsvrUzlu+79/7bxK3Mm74d6bmYbK8tLWwSH+jQ3bbgS/H592XadNn0DeNogU6qFIJdbp1q1YNpX1QkREREQ0nXIZAD4qfrM3o62OUKztQ9iSfRtYgfNdIjgdFMLdq4nfvvG9/qt5qx6627RotnqdWUu1TvSdplGvF3M5r5X1lWfAfOI0KxrKdR1WO8UFUuDbYCWsCheB549vSl/5Fbks92kP3Wr3nsArVDdgO7cFZ+hgkMgSw4jX5XlyXV8Jy5pEkdtHljiOiNMp6nQ6hO5mVyn/KPeBCcFj+PCki23Ea/Qivp/o5w1IBJ9AK8L5BKUYpD6l10rqFtq+dmlDuYFzpIuBq1DFRiNdx7+cE4PgNzVz5H63vGWeCz8Zk8mQy53HtpGp7u5rwM0VNNHEihk1mIIMZR18f0qj7bx3VmlAIIp8/xWo7hMK+2vB/x3mzm2steJfPzsNIs+b4vAcXirX9jphWX2qx8zBjifD2meU9n1PYt0UxB233QHQuNikFre8oUu7rtOmj5dH25BKXKyHsW6JiIiIiKgnlwFg58ndGXz4kSy7fZx8D8D2Yby/MA9zPTh3u3Oon+boPn67KPnW76czuINHeOft4M/JnLugYTQCnR62bTsdFr2OKveiSvzuoe/iX3zFmu3dGe12Zm1UC70LGP8drOjdZatwkeVdtGXNR+B05gBGQ7XjyH2dV+xFpPwO89hlSb4nBqTpQElBKYbJ6z1WqvWVcVkTInb7UIrjE+S9BtR93WHobnaV8o9yH5gIPIYPj2psYzrIoX4Mc16r7P8GXAHHTiD4ql0/d38T25h8pYiBKJd91n1yK+7beBkVqpec17Wu3BJnZTDscuezbWSpu3d8v1Vxvg99KdRgeQYoaw77kxJv2db5zK/oDe+/ErnsEwh8h7m5YqKln0UOY1kHVux5kxTP4ZX2oVTtdcZlKR8zBzieYLj7TPK+75Y5J9HHbe+74xGxGVD08oYt7bpOmz5Gjm1DGtGxHs66Vd8/iYiIiIgmXLfbtdNMd6/+2QZ+sW8m/v6DfXXRthev/hD4fyzf9/2dmKZrd2/+YgO2vXzTS3PfXob4d/Lp5s2bdkDDsAHYRiP4s6NhG4ANb2YorTBfom3pNnTLbvt+axiwAd22vB/blq0Dtt77oWEbMOxAru6y+2lU8lHTtvSYGLj5CnVI/Bu7bVs6QnVP/js3ptKYCTGx7f5yojOMTaMUw8T1nuP6SlzW+AMg/iTXMILxUNo+FOPYE73uswrXM26b75c3ufxp94HpEop7aJ/xm45jeF4yxVZWH7tfJzHGzn4hbs+yfchdjpjWy1dYNyLZ+guRHIuC8xRi0DCE5bh1EcttqyxPnOflFS5Hw4jZXiR5yePer6e4jfbnKeYTkLLckuXEz0u3bUSWOa7uPuG/79cvuH075Qrmla6sthujUJ0j9id5fPrCZY9etjStQJ5G2H/T7BMupf3V5Z0vJK23pNh4Qse/AyLxvInn8EKZxbYrx/Y6cVl98u1N9ZiZ/njizI7fZ+T7dZA8jXx78ZP9new3UWSayON2VAwlZZQcG9IuLzJ9jOi/yaPtSJdeWpaItCLp39q2vB45xDrNuo3MW6CajuhJkrcXpGpnZ0f8iVJg/LJh/LJh/LJh/LIZp/jt7OzYX3z2uf3FZ5/b9+/fD02maSpP4t/ev3+/l3duA8Ddbn/w1psCA7vudHO5Pz840Budj8rgb1cyABzdKeEQ5/svnhFxUe/XtuSdWU6+/Um8EA8tJ3Sx40jKJ5l3oSibvAs1XydnbxJjJkkTKrDKsqLSyToNxDTBdCppbMUYhvIS6haan2F9hfKSZTTGEHuREly38k4O2RTsNEiKYyiGvUncbgcn1tNZpqyTOdwhmlR+eSzyK/tBJsZdPEaLxPmhbSNh/xr/Y3h+ssbWTlHvqE63qP1IjJNqrKLWX4Cvs1HMX1ZHP//8UN2jlivpCFWZF8o/KQaSvKLibvti7KyvuGO1vCxRdZalFfOzbXl5VeapbhvqdZeT/b1Xt+DfSTq/vTmKZfXIYictY8w2bEfkE5VXVFqVznVx/w3lJdk+/JT2156IgQ5RzLbjh9hzl3ElO1fwJp7De0J5jcE5PGK2t1AeEcsSyxOVri9+n5EtFxhs3w+R7IdZlmcnHbdlx0Tx2BJZJvXlqdRBFL2M/NoO1fRR5ZfGVJCqHjnE2jczVF4x3lH1EtM1jPBvROMGMe0FJRunDvyDiPHLhvHLhvHLhvHLZpziN6oBYK3b7driU8EH1fr6Ok6fPi3+TEQ50TQNzrXKZJuWeo4bxn14GFsimlY8/tEoTd/21kRFK2PTaku/6000etwm6WCYvvYiX7u7uzhy5Ij4Myli/LJh/LJh/LJh/LIZp/jt7u7i6admAQDzLy2Is3Hx4kXxp0hXrlwRf8Le910gt28AExEREREREdEUcb7hGvpGMtGT0ryFOgxc4uAvEREREREHgA+mJiqaBi12qqAp/hkRERERERFRTgrVSzBaJlZ48UlPXAe1y3Xo1nmUxFlERERERFNI29vbs23b7r16RPZf2W/jOO/3v/89XwFNNETT8pqiaannuGHch4exJaJpxeMfjRK3NyIiUsH2IptxeoXnQcT4ZcP4ZcP4ZcP4ZTNO8RvZK6C9Ew7vydFDhw7h0KFDmJmZwczMDJ566inMzs5idnYWTz/9NJ5++mkcPnwYhw8fxjPPPINnn30Wzz77LObm5jA3N4fnnnsOzz33HJ5//nm88MILeOGFF/Diiy/ixRdfxPz8PObn57GwsICXXnoJL730El5++WW8/PLLeOWVV/DKK6/gV7/6FV599VW8+uqreO211/Daa6/h9ddfx+uvv45f//rXeOONN/DGG2/gzTffxJtvvom33noLb731Fn7zm98IVSQiIiIiIiIiIiIiIiIimi5at9udmFvO1tfXcebMGfFnIiIiIiIiIiIiorGws7Mj/kRERERTZBRPAE/cADBfAU00PNPymqJpqee4YdyHh7ElomnF4x+NErc3IiJSwfYim3F6hedBxPhlw/hlw/hlw/hlM07xG9kroDVNA3zf1338+DEeP36MR48e4dGjR/jzn/+M/f197O/v45dffsEvv/yChw8f4uHDh/j555/x008/4aeffsKDBw/w4MED3L9/H/fv38ef/vQn/Pjjj/jxxx/xww8/4IcffsDe3h729vbQ7Xbx/fff4/vvv8d3332H7777Dt9++y2+/fZb/PGPf8Q333yDb775Bl9//TW+/vprfPXVV/jqq6/whz/8AV9++SW+/PJLfPHFF/jiiy/w+eef4/PPP8dnn30mVJGIiIiIiIiIiIiIiIiIaLrwG8BERERERERERERERERERBPikPgDEREREREREREREREREREdTBwAJiIiIiIiIiIiIiIiIiKaEBwAJiIiIiIiIiIiIiIiIiKaEOkHgLcP4/2FOayLvwPYvvY8Fhbm3el5XNsWUwBYn/OlmceCOSumEPKRpyEiIiIiIiIiIiIiIiIioqCUA8CzMN99BnfEnwGsm/N49wJw9e4eut09dG8+xoV352H6R4rX57BwZhbLN9003QdYvj4XGODdvvY83r0wg8WrP7r57ANCmsF0UFvSoGkaKk1xXl+z4qTpTULi0PylGjrezE4NS/55wiQuN5RXIEETlYS/V6OeT3x5+jq1JWe+v+5+zYr875Xjo1JmlTS+snqTJJFKGiCmXn55pTno3HUdrGJ+6wx4AnFsVqBpS6hJN3pHctnVYkAy03oMH4WE2DYr0LQKZLO8ei7VOoF8IidhAaF9RpIGUNj/ZPO9Y4S07P5yO6Rl0WLaOgx3uf40PcrrwiOuE6+s4u+SyV0P8vJJ1oUkFvK/FWMqlkWSt59kOQGS+f1yxPydb58NxDCQn1hWyRQbt2Ddo9JI1z1NIfV2JL496uM5fMR85JgmVkJ7GzrGiMes6PlOLMT0/XUXd1wJxdGdUv+NvFJAivTSdLJ6CZy/k7WPkrZR0k6kbbt7pPtGMA95naL2Q3EdSyYhbtL8VWMrSRcgi5VPqrgTEREREdHIqQ8Ar89hYWEO18Xf4TwVvHIdWLz6AB8cdX977wFuLgPXVw7DeRD4EK6tzALLD2C95/3hPqyb+8D1w+7TwrP4xwszwPIDfPzB414+d68+Aq7PSp86VtZcgdkyYBhA/Vb4EsW72CpvWmjbNmxvWi31UjQrGsp1A43e/AaMlomid/FWqGLD/7fu1LZ0AAZO9bJKWlYHtaUy0OjPaxhAvRzVWRBFNZ+k8viT1nDOBAxDF+f0L1jLdXGGQyk+amVuVmRpwh2+RROw2l66Box6OXChq5ImsV5Ajmkmldp6zW99jF5y2dViQBGm8hg+IomxVVVAdcMXj4YBQPftE2KMNGGfcddJvRzRmZhO596m+686ysqB928f7rRRRUFMFiOX5bYtwCxGdA6r6qC2VIQJ33baPou1czV0Uq0rhMrnFE91e46LaVwZh6GFtdvynDu1y0huVbLFLVj3iDS5rHs6+FTbkaT2yJ+U5/ByeaVRENveJh0P4+cXqpdgoAVzJZhvc8VECwYuVZNaMtVjUdr2O216hMqSrs0ZzCBtd7OiQSuaOOHbnp3ybqIciptKe4CU7cwAsdX9xwo3XaisREREREQ0KdQGgLcP4/0zs1i8+qMzGCv6dAZ3ABwvuIO2rrffeQTcmcVH2wC2Z/HhHWDxHeHv336ERczgw48OAduHsAVg+eR+MA0A4BA6sldKK2reqgPGKayeMoD6rdDFUKd2DmbLQEN6IQYAHdzbBGCcQr9LpYTzlg60ttAOpPVrYsVsBf4ueVnOhZ+/76Z03oIOYPNemssztXySy+PpoHbOBKwbOH9cnOflo8Nqt2HJ+pakxPiolbm0Kkvj79h18tWtG+j3d7jrq7f+VdKo1SuvNJNLZb3mtz5GT6XsKjGgKNN5DB+NpNgOQ38/3vDtMwBQwmrbgp6iAzaeAcvSgfrlyKdXhiPjcgtVbLQt6C0T5wbKAADa2GoB+tmT/e20UMVG5HarzhlokA1gpDW8MoY566Rlrki28Q5ur7WgWxYMcdao5bLu6eBTa0eS2yMPz+Gj6pVXGhXx7W3S8TBpvld/X7vTqeFyHdCt875zH0URx6K07Xfa9DL5tTlJ1NvuTm0J5bozMCveb1GobkQM7uYre2y98+A1RNwbRUREREREB5zaAPDRh/i4u9d/KlfqEd55W/wtTBwkxtHH6PVDuMvpPyHs+PSTGQCPUfCeLk6tCed6uwSUTsFAHZcDV3Vex1/cxXEBx04A2LwXeG3h7bXgwIDIeaJEh3W+N3SgsKxRUi+P18kUdQd5oboB2xYvQOOF45PNiWPuwjv3sOn/f1fh2AkAddxqKqZRrFdeaaZajutj5BTLToPiMXx4kmI7DF7cL8n340IVl5yeXslAXXrHqjdg6S2YQ3uqVC7zct04yAcs1bW2om9vyEo/XhR/Gsgwy+h37ORZ6LJjcnMFZkvH2ZPHhBlPSE7rniadenvEc/hAsoC80iRTa2+Tjodx88WngJsrJlq6hRuDFjx0LErbfqdNHy+vNieOWtudUK+RSCiDYmydfYaIiIiIiCaV2gBwEv9TvD7OwO0MPvm0/5RwlDufzIg/Ae43gc9cBxav/gxhXFhd8xbqvdeTlXDKAFprt30Xdc4d1dhaEb7hE3wdWWnVfV2otoRap4mKVnTuuhdv++2RXZipLSukvYWWpKMjtVA+iuXp1HDObMForCZ2MqmTxUciVGaR81RDS7fQ64Nqb6EFHaF+guJx9G7cV0lDwyOu14O8PgYtuxgDkuMxfHgSYzsM7lNMoR2mr3hcB7CJfB6YLqDq9GBDeDPmkGVfbrY4eE+DlZO3z5SalTLq0HH2ZNbteXhllCqcxFk9/BSZ81RewrnIiGVb9zSRQu2IYnvEc/jxkNjeJh0Pk+Yj+BRw03n617iU7UnU4LEobfudNr1cfm2OCoW2u3Mbawn1Gr58Ytt/9TUREREREU2ifAaAjz7E+WXgzoU591u+zjeDz0g/GJzC+hzeFb8JnFoHtcvO67a8foWSc8UdetVRa/M4bvS+idN27v4t+r+dU8Kq3XDurC6WUQfiO1OaK3DejBZOkbwsvyYq5Trg7xwZSHQ+SeVprphoGY3QK64yiYlPX1SZ3W9xaRo0bxBnBK/aorxErddpwhio4TF8eNRjmyv3ya2RKq2635mMWkeeOspxAylpKS9XLuuTOYXqBuy283pVs5ilPsG4lNFI8TRcfEzzK6MKt2Nf8opU2X6eXXzd42Rd9zRpotuRpPaI5/DjQK29TToeJs130rhPsJaFgfUBBY5FadvvtOl7Bm1zxGOuBk1zzvdSUWy7/Tc2dGpLweWGvqsrli287lIZOLY+7s0hiTdyJBLrNmDciYiIiIgod/kMAAN4z9rDzeUZXHh3HgsL81hYeYS7d3/Govdq6LcfYVH8Ix/x28Db157Hgvvd4a4l+yawIvcO3UAHRekUjMC3phyBbyp5nYS+14g5F3ZloOF0srQtHfWyBk36bR33Qj/iwjtpWX7eXc/WjWydI3H5xJanWUG5HveU3CDi4+OJLrPznTGns8tG29pEWdOwlOlKmkYler1OD8ZAEY/hw5MitrkqHIPa0NYJRD40NgDnO5PyV272GWj0BlJsxQ7neGrLlcvlyZxCFRu27Rs0iO/QluvHpe0+gSbdbaQUYppLGRUJ23jn9lougyRyCnWPkMu6p4kR147Etkc8hx8PadrbpONh0vzeNpD96V+Ix6K07Xfa9D2DtjniMdeGbTcG+ra7Stvt/7a185pwZ5kN6QLFsqm3B1KDxrZlougN0hZNwGrDznx8EOs2eNyJiIiIiChfuQ0Awx0E7nbd6eOHOPrpDO4I3+7d6giL3D6ELeHbwOvmPN69MIPFqz9mePLX0bm9hhbgdPILd6QmflvN/xox9w5Z3Wr37qAvVDdgO7cHhy9KvTvjVS+8I15Z1qxoKNd1WO1sF4mp8/GVp3mrHrqzt2i2eheQA3XYKMQnTZmdu91967R4HDpaCH0my//KOJU0lLvI9XqQ10fKskfGgEJ4DB+edLGNeIVgxHcY4xVxXI//jmHbea8hct3tC1XcsHS0zHPZnrpJK8Ny21utcOftoOuiUMVGI/pGBVWF6obzZNRl8emmHORUxnjuq1fNFTTRxIrZEgbQxoN83dM0St2O8Bw+dN71pKVrb11Jx8Ok+TnFIXgsStt+p00fNtQ2J05c2+0OvsbVa/gGjK1uoe0bqN1I2kGJiIiIiOhAy3UAWLR+exZY3ne+3Xt0H79dlHzr99MZ3PGeEvZ983f55l7mwd/+96kawh2pttPp37tgdi+gxO8e+jsRor5hFdXpf6sO9L7z5KewLJfTeQIYjeTOkzjx+SSXp7Qq3tHr3o3tXkAOcuEYHR9HfJljeBe57oW5/85s9O5iD96VHpuGchW7Xg/y+khR9tgYkIDH8OFRjW1MRzvk9U5WwLETCL6G1899Je8wBuUK1UvOK8BXbomzhmqg5XpxsM73X1OedV1EbO9pOa8ujfk+YhY5lTGO92TXrYrzTc5L47aDytY9TaX4diS5PeI5/DhI0d6Kko6HSfOzCh2L0rbfadPLDbXNiRHddvu+tSyr10jkE1siIiIiIppsOQ0Az8JcmMeCOdv7xRnIfYSrv/Ne3/wYH5zfB67PwVz3/d2ZWWD5IT44CmD7MP6T++Sv9V4vq8HFfZ+qdAoGgPqtJnqvygpcWLrfrfK+ieOlF+4+bq6YaImdIKGLZT+FZcF5VanTeWJn+mZXcj5q5clVbHxUytxERRNed+au6/5FrveEj++u7d4TgN5yVdLQQCQDEcnr9SCvD7WyJ8eAAngMHx7l2AIoVHHJAOpl4Xt1nRqWBmwrSqvet5iFY3mnhqWi893CG2kzVVLCasMA6vURf5su5XKj4pBmXTQrwjcIO6idk2zvgyidh9P3nfGJrGGWMU7hJM7qQL1eD3yTcyxErXuaOsntiFp7lKvY9lGlzFN4Dq/a3iYdD5PmK2pWNLXvz0Yci9K232nTS+XV5qQW3Xb3vrVc1IS3yHQwqjf45xJbIiIiIiKabN1u104z3b36Zxv4xb4pzrv7k70I20ZvkqTpdu3uzV98aWwby/eFvP15+Kc/21fvSvLzTTdv3rT9GgZswLAbgV/7xPltS7cB9CdD/MuGbfjnQ56/mK9M/LJky/Em3bbavqSx1POJL09Y29Jt6JbtL0ooj94UjEV8fNTKLFuWrMjOsvqTLgleUhrZspwpZtsZMM24AyD+5BNcd8E4qq1XO6f1kZW0ng1Dssxg+eLLrh6DaSXGPf5YEZ4f2jZCBwXZOgjnL+YrE78s2XK86cms66yxtWV1jjju9jSMxPqK+wxC+00vYShdIK1kWU555XX0lusvv6x+AEJtXcAQlxsXW9nfyNKH0kXVRVIPT1R9nN99fyPJI7R8STlCaaLK6MlpW/CWG4ybs+8GtkFJfirzQvWS1C8qjWxd0uAga9PHnno7EtqOEjagtsVz+NhzhwHTeJChvQ0tJ2k9RR0vY45NzvIStiF3kq0Xjxh7SOLvp5pedrzu/y6vkx3zd6rH9ei/75ddGg9Zm5S03iLSSUnKKkoVW5Vl+snq58s/Om6SuBNRAA7k+cn42NnZEX+iFBi/bBi/bBi/bBi/bMYpfjs7O/YXn31uf/HZ5/b9+/dDk2maypP4t/fv3+/lrXW7XVscFD6o1tfXcfr0afFnIsqJpmlwrlUm27TUc9ww7sPD2BLRtOLxj0aJ2xsREalge5HN7u4ujhw5Iv5Mihi/bBi/bBi/bBi/bMYpfru7u3j6KeeNyvMvLYizcfHiRfGnSFeuXBF/wt73XSC/V0ATEREREREREREREREREdGTxgHgA6mJiqZBi52EbwERERERERERERERERER0cTjAPCBVMKqbcOOnVZREv+MiIiIiIiIiIiIiIiIiCYaB4CJiIiIiIiIiIiIiIiIiCaEtre3Z3tPjQKQ/lf22zjO+/3vf48zZ86AiIiIiIiIiIiIaBzt7OyIPxEREdEUefqpWQDA/EsL4ixcvHhR/CnSlStXxJ+w930XAKB1u11nBHUCrK+v4/Tp0+LPRJQTTdN6N11Msmmp57hh3IeHsSWiacXjH40StzciIlLB9iKb3d1dHDlyRPyZFDF+2TB+2TB+2TB+2YxT/HZ3d0cyAMxXQBMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTQgOABMRERERERERERERERERTYj0A8Dbh/H+whzWxd8BbF97HgsL8+70PK5tiykArM/50sxjwZwVU2Dd9M2PyoeIiIiIiIiIiIiIiIiIiAJSDgDPwnz3GdwRf3YHbd+9AFy9u4dudw/dm49x4d15mP6R4vU5LJyZxfJNN033AZavzwUGgdfNeZy5vo+b3Zh8BtJBbUmDpmmoNMV5fc2Kk6Y3CYlD85dq6HgzOzUs+ecJk7jcUF6BBE1UEv5ejXo+8eXp69SWnPn+uvs1K/K/V46PSplV0vjK6k2SRCppgJh6+cWmUSvzRHDXdbB+avXPdX3kqVmBpi2hJt3oHcllV4sByUzrMXwUEmLbrEDTKpDN8uq5VOsE8omchAWE9hlJGkBh/5PN944R0rL7y+2QlkWLaesw3OX60/QorwuPuE68soq/SyZ3PcjLJ1kXkljI/1aMqVgWSd5+kuUESOb3yxHzd759NhDDQH5iWSVTbNyCdY9KI133NIXU25H49qiP5/AR85GURq3MyRLa29AxRjxmRc93YiGm76+7uONKKI7ulPpv5JUCUqSXppPVS+D8nax9lLSNknYibdvdI903gnnI6xS1H4rrWDIJcZPmrxpbSTo/6d+IsUsbfyIiIiIiGhn1AeD1OSwszOG6+Ducp4JXrgOLVx/gg6Pub+89wM1l4PrKYTgP8B7CtZVZYPkBrPe8P9yHdXMfuH7YecrXzWf55gP0krz3M64uAtdvh58UTqW5ArNlwDCA+q3wpYl3sVXetNC2bdjetFrqpWhWNJTrBhq9+Q0YLRNF7+KtUMWG/2/dqW3pAAyc6mWVtKwOaktloNGf1zCAejmqsyCKaj5J5fEnreGcCRiGLs7pX7CW6+IMh1J81MrcrMjShDt8iyZgtb10DRj1cuBCVyVNYr0AhTRq9ZpcavXPb32MXnLZ1WJAEabyGD4iibFVVUB1wxePhgFA9+0TYow0YZ9x10m9HNGJmE7n3qb7rzrKyoH3bx/utFFFQUwWI5flti3ALEZ0DqvqoLZUhAnfdto+i7VzNXRSrSuEyucUT3V7jotpXBmHoYW12/KcO7XLSG5VssUtWPeINLmsezr4VNuRpPbIn5Tn8HJJadTqpSS2vU06HsbPL1QvwUAL5kow3+aKiRYMXKomtWSqx6K07Xfa9AiVJV2bM5hB2u5mRYNWNHHCt2045d1EORQ3lfYAKduZAWKr+48VbrpQWUWjXx9ERERERJQPtQHg7cN4/8wsFq/+iLtXH4lzgU9ncAfA8cLjwM9vv/MIuDOLj7YBbM/iwzvA4jvC37/9CIuYwYcfHQKOPsTH3T3fAHF+mrfqgHEKq6cMoH4rdDHUqZ2D2TLQkF6IAUAH9zYBGKfQ71Ip4bylA60ttANp/ZpYMVuBv0telnPh5++7KZ23oAPYvBd/eRaklk9yeTwd1M6ZgHUD54+L87x8dFjtNixZ35KUGB+1MpdWZWn8HbtOvrp1A/3+Dnd99da/Shq1eiWnUavX5FKpf37rY/RUyq4SA4oyncfw0UiK7TD09+MN3z4DACWsti3oKTpg4xmwLB2oXw49rTJcGZdbqGKjbUFvmTg3UAYA0MZWC9DPnuxvp4UqNiK3W3XOQINsACOt4ZUxzFknLXNFso13cHutBd2yYIizRi2XdU8Hn1o7ktweeXgOH1Wv5DRq9VIR394mHQ+T5nv197U7nRou1wHdOu8791EUcSxK236nTS+TX5uTRL3t7tSWUK47A7Pi/RaF6kbE4G6+ssfWOw9eQ8S9UVKjWx9ERERERJSV2gCwOzD78QfBAd6gR3jnbfG3MHGQGEcfQ9IP0bN9bQ4X7jzC1d/ti7NSaMK53i4BpVMwUMflwFWd1/EXd3FcwLETADbvBV5beHstODAgcp4o0WGd7w0dKCxrlNTL43UyRd1BXqhuwLbFC9B44fhkc+KYu/DOPWz6/99VOHYCQB23moppFOulkoYS5Lg+Rk6x7DQoHsOHJym2w+DF/ZJ8Py5UccnpWZQM1KV3rHoDlt6CObSnSuUyL9eNg3zAUl1rK/r2hqz040Xxp4EMs4x+x06ehS47JjdXYLZ0nD15TJjxhOS07mnSqbdHPIcPJAtQSZMPtfY26XgYN198Cri5YqKlW7gxaOVCx6K07Xfa9PHyanPiqLXdCfUaiYQyKMbW2WcGM4r1QURERERE2agNACfxP8Xr8+knMwBm8Mmn/aeEo9z5ZCb4w/ocFhbm8e6FmeCrpQfRvIV67/VkJZwygNbabd9FnXNHNbZWhG/4BF9HVlp1XxeqLaHWaaKiFZ277sXbfntkF2Zqywppb6El6ehILZSPYnk6NZwzWzAaq4mdTOpk8ZEIlVnkPNXQ0i30+qDaW2hBR+i6tHgcvZv7VdIMU2K9JpxY/ye9PrIYtOxiDEiOx/DhSYztMLhPMYV2mL7icR3AJlI+XBWhgKrTgw3hzZhDln252eLgPQ1WTt4+U2pWyqhDx9mTWbfn4ZVRqnASZ/XwU0vOU3kJ5yIjlm3d00QKtSOK7RHP4fOXWC+JxPY26XiYNB/Bp4CbztO/xqVsT6IGj0Vp2++06eXya3NUKLTdndtYS6jX8OUT2/6rr9WNdn0QEREREVEW+QwAH32I88vAnQtzzrd84QzgnpF+MFjRew/Q7e6h232A4xdewML73reE0+qgdtl53ZbXr1ByrrhDrzpqbR7Hjd73bdrO3b9F/7dzSli1G86d1cUy6kB8Z0pzBc6b0cIpkpfl10SlXAf8nSMDic4nqTzNFRMtoxF6xVUmMfHpiyqz+70uTYPmDeKM4FVb+Ymq17SY9vqDMVDGY/jwqMc2V+6TWyNVWnW/2Ri1jjx1lOMGUtJSXq5clidz4D3Z1nZer2oWs9QnGJcyGimemIuPaX5lVOF27EtekSrbz7OLr3ucrOueJk10O5LUHvEcPm9R9Yqj1t4mHQ+T5jtp3CdYy8LA+oACx6K07Xfa9D2DtjniMVeDpjnne6kott3+GwA6taXgckPf1RXLFl53qQwcWx/35pDEGzmU14dYxwHjT0REREREuclnABjAe9Yebi7P4MK781hYmMfCyiPcvfszFr1XQ7/9CIviH/mEvg3cs4/fXfV9Szgt9w7dQAdF6RSMwLemHIFvKnmdhL7XiDkXdmWg4XSytC0d9bIGTfptHfdCP+LCO2lZft5dttaNbJ0jcfnElqdZQbke95TcIOLj44kus/M9Lqezy0bb2kRZ07CU6Up6dKLrNR2mvf5gDNTxGD48KWKbq8IxqA1tnUCah6uSON9slL9ys89AozeQYkd0cKajtly5QZ7MCSlUsWHbvkGD+A5tuX5c2u4TaNLdRkohprmUUZGwjXdur+UySCKnUPcIuax7mhhx7Uhse8Rz+NxF1ytGmvY26XiYNL+3DWR/+hfisSht+502fc+gbY54zLVh242Bvu2u0nb7vwHtvErcWWZDukCxbOrtgdSgsW2ZKHqDs0UTsNqwE48PqutDrOPg8SciIiIionzkNgAMdxDYeWp3D92PH+LopzO4g8co+F7fvNURFrl9CFuybwP7HC087r9KOqXO7TW0AKeTX7gTNfHbav7XiLl3yOpWu3cHfaG6Adu5PTh8EeTdGa964R3xyrJmRUO5rsNqZ7tITJ2PrzzNW/XQHb1Fs9W7gByow0YhPmnK7Nzt7lunxePQ0ULoM1n+V8appBmCNPWaRJH1f0LrIxcpyx4ZAwrhMXx40sU24hWCEd9hjFfEcT3+O4Zt572GyHW3L1Rxw9LRMs9le+omrQzLbW+1wp23g66LQhUbjegbFVQVqhvOk1GXxaebcpBTGeO5r141V9BEEytmSxhAGw/ydU/TKHU7wnP40HlXXtLUyy9de+tKOh4mzc8pDsFjUdr2O236sKG2OXHi2m538DWuXsM3YGx1C23fAO1Gmg35Sa4PIiIiIiIaSK4DwKL127PA8j7eA4Cj+/jtouRbv5/O4I73lPD2Yby/MA9zPZhku3MI8NKk4n2fqiHciWo7nf69C2b3Akr87qG/EyHqW09Rnf636kDvO09+CstyOZ0MgNFI18kgis8nuTylVfFOXvfuX/cCMu2FI2Lj44gvcwzvIte9MPffmY3eXezBu9Jj0+Rs4HpNiNj6P4H1kZsUZY+NAQl4DB8e1djGdLRDXu9kBRw7geBreP3cV/IOY1CuUL3kvAJ85ZY4a6gGWq4XB+t8/zXlWddFxPaelvPq0pjvI2aRUxnjeE923ao43+S8NG47qGzd01SKb0eS2yOew+dn4HqlaW9FScfDpPlZhY5FadvvtOnlhtrmxIhuu33fWpbVayTyie0gntT6ICIiIiKi9HIaAJ6FuTCPBXO298v2tedx5vojXP3dvvvLY3xwfh+4Pucb4J2FeWYWWH6ID472B4mv3+7nA8ziHy/MYPHqAydNGnHfpyqdggGgfquJ3quyAhcy7vedvG/ieOmFu12bKyZaYidI6GLZT2FZcF5V6nQy2Jm+2ZWcj1p5chUbH5UyN1HRhNedueu6f5HrPeHju2u79wSgt1yVNPlJrtcEkQxEJNd/tOsjX2plT44BBfAYPjzKsQVQqOKSAdTLwvfqOjUsDdhWlFa9bzELx/JODUtF57uFN9JmqqSE1YYB1Osj/iZdyuVGxSHNumhWhG8QdlA7J9neB1E6D6fvO+MTQMMsY5zCSZzVgXq9Hvgm51iIWvc0dZLbEbX2KFex7aNKmafwHF61vU06HibNV9SsaGrfn404FqVtv9Oml8qrzUktuu3ufWu5qAlvkelgVG/wzyW2g3hi64OIiIiIiFLrdrt2munu1T/bwC/2TXHe3Z/sRdg2epMkTbdrd2/+4ktj21i+H0pzc9mfj20vXv0hlEY23bx50/ZrGLABw24Efu0T57ct3QbQnwzxLxu24Z8Pef5ivjLxy5Itx5t022r7ksZSzye+PGFtS7ehW7a/KKE8elMwFvHxUSuzbFmyIjvL6k+6JHhJaWTLcqaYbSeURq1e4w6A+JNPsI7BOKrXP4/1kZW0ng1Dssxg+eLLrh6DaSXGPf5YEZ4f2jZCBwXZOgjnL+YrE78s2XK86cms66yxtWV1jjju9jSMxPqK+wxC+00vYShdIK1kWU555XX0lusvv6x+AEJtXcAQlxsXW9nfyNKH0kXVRVIPT1R9nN99fyPJI7R8STlCaaLK6MlpW/CWG4ybs+8GtkFJfirzQvWS1C8qjWxd0uAga9PHnno7EtqOEjagtsVz+Nhzh1AatXp5kKG9DZUlaT1FHS9jjk3O8hK2IXeSrRePGHtI4u+nml52vO7/Lq+THfN3qsf16L/vl10aD1mblLTeItJJScoqShVblWX6RMVFXB9R6aTxJyLblrQXlM7Ozo74E6XA+GXD+GXD+GXD+GUzTvHb2dmxv/jsc/uLzz6379+/H5pM01SexL+9f/9+L2+t2+3a4qDwQbW+vo7Tp0+LPxNRTjRNg3OtMtmmpZ7jhnEfHsaWiKYVj380StzeiIhIBduLbHZ3d3HkyBHxZ1LE+GXD+GXD+GXD+GUzTvHb3d3F0085b0Kef2lBnI2LFy+KP0W6cuWK+BP2vu8C+b0CmoiIiIiIiIiIiIiIiIiInjQOAB9ITVQ0DVrsJHwLiIiIiIiIiIiIiIiIiIgmHgeAD6QSVm0bduy0ipL4Z0REREREREREREREREQ00TgATEREREREREREREREREQ0IbS9vT3be2oUgPS/st/Gcd7vf/97nDlzBkRERERERERERETjaGdnR/yJiIiIpsjTT80CAOZfWhBn4eLFi+JPka5cuSL+hL3vuwAArdvtOiOoE2B9fR2nT58WfyainGia1rvpYpJNSz3HDeM+PIwtEU0rHv9olLi9ERGRCrYX2ezu7uLIkSPiz6SI8cuG8cuG8cuG8ctmnOK3u7s7kgFgvgKaiIiIiIiIiIiIiIiIiGhCcACYiIiIiIiIiIiIiIiIiOgJe/HFF8WfpJLScQCYiIiIiIiIiIiIiIiIiOgJe+utt8SfpJLScQCYiIiIiIiIiIiIiIiIiOgJ+zf/5t+IP0klpeMAMBERERERERERERERERHRE1YsFvE3f/M34s8Bf/M3f4NisSj+HJB+AHj7MN5fmMO6+DuA7WvPY2Fh3p2ex7VtMQWA9TlfmnksmLNiioB1cx4L7x+GLCsiIiIiIiIiIiIiIiIioklRKpWwvLyMv/qrv+p96/fFF1/EX/3VX2F5eRmlUkn8k5CUA8CzMN99BnfEn92B2ncvAFfv7qHb3UP35mNceHcepn+keH0OC2dmsXzTTdN9gOXrc9GDwOtzOHNd/HFQHdSWNGiahkpTnNfXrDhpepOQODR/qYaON7NTw5J/njCJyw3lFUjQRCXh79Wo5xNfnr5ObcmZ76+7X7Mi/3vl+KiUWSWNr6zeJEmkkgaIqZdfQppQjKNieNC56zoYhvzWGZAc69w1K9C0JdRiVlhy2dViQDLTegwfhYTYNivQtApks7x6LtU6gXwiJ2EBoX1GkgZQ2P9k871jhLTs/nI7pGXREo7TQ1yuP02P8rrwiOvEK6v4u2Ry14O8fJJ1IYmF/G/FmIplkeTtJ1lOgGR+vxwxf+fbZwMxDOQnllUyxcYtWPeoNNJ1T1NIvR2Jb4/6eA4fMR/JaUIxjophrIT2NnSMEY9Z0fOdWIjp++su7rgSiqM7pf4beaWAFOml6WT1Ejh/J2sfJW2jpJ1I23b3SPeNYB7yOsVvQ/K/iY6DNH0gvuK2I5kqNYU0wegkL1dMF12HyHZYJFt/Pqm2BSIiIiKiMVcsFvF3f/d3+Pu//3tcuXIFf//3f4+/+7u/S3zy16M+ALw+h4WFOUjHY7cPY+U6sHj1AT446v723gPcXAaur3hP7x7CtZVZYPkBrPe8P9yHdXMfuH5Y8rTwLMwzEQPDg2iuwGwZMAygfit8OeBdFJU3LbRtG7Y3rfZH0ZsVDeW6gUZvfgNGy0TRu3grVLHh/1t3als6AAOnelklLauD2lIZaPTnNQygXo7qLIiimk9SefxJazhnAoahi3P6F5blujjDoRQftTI3K7I04Q7foglYbS9dA0a9HLgoVUmTWC9AKU3i9jPR1NZrfutj9JLLrhYDijCVx/ARSYytqgKqG754NAwAum+fEGOkCfuMu07q5YiOu3Q69zbdf9VRVg68f/twp40qCmKyGLkst20BZjG2czhZB7WlIkz4ttP2Waydq6GTal0hVD6neKrbc1xM48o4DC2s3Zbn3KldRnKrki1uwbpHpMll3dPBp9qOJLVH/qQ8h5dLTpN4/qAqtr1NOh7Gzy9UL8FAC+ZKMN/miokWDFyqJrVkqseitO132vQIlSVdmzOYQdruZkWDVjRxwrc9O+XdRDkUN5X2QBT8m4bRglkUBz5V46vSflUV0mQ9j8vaDhMRERERURpqA8Dbh/H+mVksXv0Rd68+EucCn87gDoDjhceBn99+5xFwZxYfbQPYnsWHd4DFd4S/f/sRFjGDDz8KFmX72mFcX/wZV5cDPw+seasOGKewesoA6rdCFySd2jmYLQONyAuxDu5tAjBOod+lUsJ5SwdaW2gH0vo1sWK2An+XvCznAs3fd1M6b0EHsHlPfsEkp5ZPcnk8HdTOmYB1A+ePi/O8fHRY7TYsWd+SlBgftTKXVmVp/BeUTr66dQP9/g53ffXWv0oatXolpxl0+5kUKus1v/UxeiplV4kBRZnOY/hoJMV2GPr78YZvnwGAElbbFvQUHbDxDFiWDtQvRz4pMhwZl1uoYqNtQW+ZODdQBgDQxlYL0M+e7G+nhSo2Irdbdc5Ag2wAI63hlTHMWSctc0WyjXdwe60F3bJgiLNGLZd1TwefWjuS3B55eA4fVa/kNIOeP4TFt7dJx8Ok+V79fe1Op4bLdUC3zvvKrijiWJS2/U6bXia/NieJetvdqS2hXHcGR8X7LQrVDYXB3fTC+0o+8R3EYMs9IO0wEREREdEEURsAPvoQH3f38PEHwQHeoEd4523xtzBxkBhHHyPUD7F9GP/pAnD1nx7mdOHUhHO9XQJKp2CgjsuBqzrvgiPu4riAYycAbN4LvLbw9lpwYEDk3MmqwzrfGzpQWNYoqZfH62SKuoO8UN2AbYsXgfHC8cnmxDF34Z172PT/v6tw7ASAOm41FdMo1is5zWDbz1TJcX2MnGLZaVA8hg9PUmyHwYv7Jfl+XKjiktPTK+kgTO9Y9QYsvQVzaE+VymVerhsHeUeputZWmuGJdPTjaq+bSTLMMvodO3kWuuyY3FyB2dJx9uQxYcYTktO6p0mn3h7xHD6QLCA5zWDnD2Fq7W3S8TBuvvgUcHPFREu3cCO6cvFCx6K07Xfa9PHyanPiqLXdCfUasv52n1COlPFVN/hyD0w7TEREREQ0IdQGgJNEPMX76SczAGbwyaf9p4Sj3Plkxv3XIVz7T88A/tdJZ9W8hXrv9WQlnDKA1tpt30Wdc0c1tlaEb/gEX7FUWnVf96UtodZpoqIVnbvuxdt+e2QXR2rLCmlvoSXp6EgtlI9ieTo1nDNbMBqrKTo6ksjiIxEqs8h5qqGlW+j1QbW30IKOUD9B8Th6N/erpMlR+u1nwonrdcTrI1eDll2MAcnxGD48ibEdBvcpptAO01c8rgPYRD4PTBdQdXqwIbwZc8iyLzdbHLynwcrJ22dKzUoZdeg4ezLr9jy8MkoVTuKsHn6KzHkqL+FcZMSyrXuaSKF2RLE94jl8ZunPHyQS29uk42HSfPjSXEat6Tz9a1zK9iRq8FiUtv1Om14uvzZHhULb3bmNtYR6DYP3Ou/+J0nyiW96GZZ7gNphIiIiIqKh09xpGNy88xkAPvoQ55eBOxfm+t/yXZ/DGekHg+NtX5vDBfyMf4p92jiNDmqXnddteddKJeeKG+LnZ1qbx3Gj9/2atnP3b9H//ZoSVu2Gc2d1sYw6EN+Z0lyB82a0cIrkZfk1USnXAX/nyECi80kqT3PFRMtohF5xlUlMfPqiyux+r0vToHmdMEN41Va+Um4/Ey1qvU4TxkANj+HDox7bXLlPbo1UadX9zmTUOvLUUY4bSElLeblyztNsgytUN2C3nVdGmsUs9QnGpYxGwhNzfvExza+MKtyOfckrUmX7eXbxdY+Tdd3TpIluR5LaI57D5yHl+UOIWnubdDxMmu+kcZ9gLQsD6wMKHIvStt9p0/cM2uaIx1wNmuasr1QU227/jQ2d2lJwuaFvAItlC6+7MCEO4uu8B45vRpmWO6p2WIz3gNsCEREREdEQ2e40DF7e+QwAA3jP2sPN5RlceHceCwvzWFh5hLt3f8ai92rotx9hUfwjn8V3HgVe/ZzXw7/eHbqBC4rSKRjC93MA4ZtK3sWJ7xVFzoVdGWg4nSxtS0e9rEELfd8G/Qv9iAvvpGX5eXc9WzeydY7E5RNbnmYF5XrKu9wTxcfHE11m5ztjTmeXjba1ibKmYSn5SvqJSbf9TLbo9To9GANFPIYPT4rY5qpwDGpDWycQ+dDYAJxv58lfudlnoNEbSLEVO5zjqS1XrnNv8C7WnkIVG7btGzSI79CW68el7T6BJt1tpBRimksZFQnbeOf2Wi6DJHIKdY+Qy7qniRHXjsS2RzyHz0W68weJNO1t0vEwaX5vG8j+9C/EY1Ha9jtt+p5B2xzxmGvDthsDfVNWpe32f9vaeZW4s8yGdIFi2VTaA+Fv2hZgFvuDywPHN6Osyx1JOyzGe/BtgYiIiIhoeIb/CHBuA8BwB4G7XXf6+CGOfjqDO3iMgm80d6sjLHL7ELbcbwNvfzSLO/ANIi/MO08R33kG7y4833+6OIXO7TW0AOciXbj7M/Hbav7XiLmvT9Otdu8O+kJ1A7Zze3D4otS7M171wjvilWXNioZyXYfVVrlIjJY6H195mrfqobtoi2YLaJkoDtphoxCfNGV27nb3rdPicehoIfSZLP8r41TS5CXt9jPBItfrKNdH3lKWPTIGFMJj+PCki63kNX5A5HcY4xVxXI//jmHbebcgct3tC1XcsHS0zHMKT93kKMNy21stSQfqgOuiUMVGI/pGBVWF6obzZNRl8emmHORUxnjuq1fNFTTRxIrZEgbQxoN83dM0St2O8Bw+dN6VSdrzB4l07a0r6XiYND+nOASPRWnb77Tpw4ba5sSJa7vdAdC4eg2FW6b+k+PZ4zuYrMs9GO0wEREREdEkyHUAWLR+exZY3sd7AHB0H79d9H/r1/XpDO64Twkf/eBP/QFkd7q5DGDxZ9zt/mmAbwJ736dqCHd/2s5Fe++C2b2IEb976O9EiPqGVVSn/606EPhGj0dhWS6n8wQwGsmdJ3Hi80kuT2lVvHvWvRtbt9C2bWyEM00UHR9HfJljeBea7oW5/85s9O5iD96VHpsmLym3n0kVu15HuT7ylqLssTEgAY/hw6Ma25iOdsjrnayAYycQfP2fn/sqwGF0Bhaql5xXeK7cEmcN1UDL9eLgf91j1nURsb2n5by6NOb7iFnkVMY43pNdtyrONzkvjdsOKlv3NJXi25Hk9ojn8DlIef4QlqK9FSUtI2l+VqFjUdr2O216uaG2OTGi227ft5Zl9RqZfOKbXvbljn07TEREREQ0IXIaAJ6FuTCPBXO298v2tedx5vojXP3dvvvLY3xwfh+4Pgdz3fd3Z2aB5YcDDO4qiPs+VekUDAD1W030XpUVuLB0v1tlXHI6L7z0wt3HzRUTLbETJHSx7KewLDivGnM6T+xM3+xKzketPLmKjY9KmZuoaMLrztx13b/Q9O4s9t213buD31uuSpqcpNl+JoFkICJ5vY5wfeROrezJMaAAHsOHRzm2AApVXDKAeln4Xl2nhqUB24rSqvctReFY3qlhqeh8t/BG2kyVlLDaMIB6fcTfgUu53Kg4pFkXzYrwDcIOauck2/sgSufh9H1nfCJrmGWMUziJszpQr9cD3+QcC1HrnqZOcjui1h7lKrZ9VCnzFJ7Dq7a3ScfDpPmKmhVN7fuzEceitO132vRSebU5qUW33b1vLRc14SnwDob3Bn/naVn//p1LfAeQebnj3A4TEREREU2Sbrdrp5nuXv2zDfxi3xTn3f3JXoRtozdJ0nS7dvfmL740to3l++E0vunmsm1j8Sf7rmSeON28edP2axiwAcNuBH7tE+e3Ld37NrIzGeJfNmzDPx/y/MV8ZeKXJVuON+m21fYljaWeT3x5wtqWbkO3bH9RQnn0pmAs4uOjVmbZsmRFdpbVn3RJ8JLSyJblTDHbjiSNvG5RcRhPAMSffIL1C8ZRVndvCm6LeayPrKT1bBiSZQbLF1929RhMKzHu8ceK8PzQthE6KMjWQTh/MV+Z+GXJluNNT2ZdZ42tLatzxHG3p2Ek1lfcZxDab3oJQ+kCaSXLcsorr6O3XH/5ZfUDEGrrAoa43LjYyv5Glj6ULqouknp4ourj/O77G0keoeVLyhFKE1VGT07bgrfcYNycfTewDUryU5kXqpekflFpZOuSBgdZmz721NuR0HaUsAG1LZ7Dx547SNLI6yaPAzK0t6GyJK2nqONlzLHJWV7CNuROsvXiEWMPSfz9VNPLjtf93+V1smP+TvW4Hv33/bJL4yFrk5LWW0Q6v8i/kRZCPb49khiEKKRRXa4svl4dE9thkSzmvr+RLcv9w+S8iUYIB/L8ZHzs7OyIP1EKjF82jF82jF82jF824xS/nZ0d+/PPv7A///wL+/79+7lPXt5at9u1xUHhg2p9fR2nT58WfyainGiaBudaZbJNSz3HDeM+PIwtEU0rHv9olLi9ERGRCrYX2ezu7uLIkSPiz6SI8cuG8cuG8cuG8ctmnOK3u7uL2dmnAQALC/Pi7My63T0gv1dAExERERERERERERERERHRk8YB4AOpiYqmQYudhO/xEBEREREREREREREREdHE4wDwgVTCqm3Djp1WURL/jIiIiIiIiIiIiIiIiIgmGgeAiYiIiIiIiIiIiIiIiIgmhLa3t2d7T40CkP5X9ts4zvv973+PM2fOgIiIiIiIiIiIiGgc7ezsiD8RERHRFJmdfRoAsLAwL87KrNvdAwBo3W7XGUGdAOvr6zh9+rT4MxHlRNO03k0Xk2xa6jluGPfhYWyJaFrx+EejxO2NiIhUsL3IZnd3F0eOHBF/JkWMXzaMXzaMXzaMXzbjFL/d3d2RDADzFdBERERERERERERERERERBOCA8BERERERERERERERERERBOCA8BERERERERERERERERERBOCA8BERERERERERERERERERBOCA8BERERERERERERERERERBMi/QDw9mG8vzCHdfF3ANvXnsfCwrw7PY9r22IKAOtzvjTzWDBnhQSzMP3zI9MREREREREREXk6qC1p0JZq6IiziIiIiIiIpkjKAeBZmO8+gzvizwDWzXm8ewG4encP3e4eujcf48K78zD9I8Xrc1g4M4vlm26a7gMsX58LDu6uz+I6HvXz8SZr35fRINwLQU1DpSnO62tWnDS9SUgcmu+/sOzUsOSfJ0zickN5BRI0UUn4ezXq+cSXp69TW3LmR11UNyvyv1eOj0qZVdL4yupNkkQqaYCYevklpBFjvFSTRvDgc9d1MAz5rTMgOda5a1agaUuIW2XJZVeLAclM6zF8FBJi26xA0yqQzfLq6RzL+vlETsICQvuMJA2gsP/J5nvHCGnZ/eV2SMuixbR1GO5ype2D8rrwiOvEK6v4u2Ry14O8fJJ1IYmF/G/FmIplkeTtJ1lOgGR+vxwxf+fbZwMxDOQnllUyxcYtWPeoNNJ1T1NIvR2Jb4/6eA4fMR/JacQYD7afJrS3T1AolpnqORxOGWVtoKz9Gw/yuMa1RQeban0P4rokIiIiIjqI1AeA1+ewsDCH6+LvcJ4KXrkOLF59gA+Our+99wA3l4HrK4fhPAh8CNdWZoHlB7De8/5wH9bNfeD64d7TwtudQwAeo+Dlk5fmCsyWAcMA6rfClxreBXl500LbtmF702qpl6JZ0VCuG2j05jdgtEwUvU6UQhUb/r91p7alAzBwqpdV0rI6qC2VgUZ/XsMA6uW0nQWq+SSVx5+0hnMmYBi6OKffqVGuizMcSvFRK3OzIksT7vAtmoDV9tI1YNTLgY4dlTSJ9QKU0oS2n4aBllmckgtctfWa3/oYveSyq8WAIkzlMXxEEmOrqoDqhi8eDQOA7tsnxBhpwj7jrpN6OaJTMJ3OvU33X3WUlQPv3z7caaOKgpgsRi7LbVuAWYwepFHSQW2pCBO+7bR9FmvnauikWlcIlc8pnur2HBfTuDIOQwtrt+U5d2qXkdyqZItbsO4RaXJZ93TwqbYjSe2RPynP4eWS04TOHwY9h8+tvR2WSTkeucfq0PH2SQnGtWG0YBbDg6JKJDc5xf7+RGQ5ZyAiIiIiojypDQBvH8b7Z2axePVH3L36SJwLfDqDOwCOFx4Hfn77nUfAnVl8tA1gexYf3gEW3xH+/u1HWMQMPvzIKcqnn8wAy/vojRHnpHmrDhinsHrKAOq3Qh3Lndo5mC0DjcgLxQ7ubQIwTqHfpVLCeUsHWltoB9L6NbFitgJ/l7ws56LV33dTOm9BB7B5L81VnVo+yeXxdFA7ZwLWDZw/Ls7z8tFhtduwZH1LUmJ81MpcWpWl8XfsOvnq1g1Ue5Vy11dv/aukUatXYppODZfrgG6d728/pVU0DKC1dvuAdaoMQmW95rc+Rk+l7CoxoCjTeQwfjaTYDkN/P97w7TMAUMJq24KeavA0jgHL0oH65RF3imZcbqGKjbYFvWXi3EAZAEAbWy1AP3uyv50WqtiI3G7VFaqXYCCPAYzhlTHMWSctc0WyjXdwe60F3bJgiLNGLZd1TwefWjuS3B55eA4fVa/ENDmewz+J9jYTHo+GIrzNT7b8zhmIiIiIiCgttQHgow/xcXcPH38QHOANeoR33hZ/CxMHiXH0Mfr9EIfQ2QIWtw4Hvv/7/jW1YkZrwrneLgGlUzD+/+zdvW/bWNo+/ksTeLMI9kH8HwyQkbKAkWoKF3Q988BKkwWStHFF/aZZqUkRIGWAFG6kbfJYVdLGxaaJhF3XVpEileHBRJrALjK1svtNdmYzyfkVJCXynEPy5pssW9cHEBKTR+fl5hEP34k+HkV2YoMDf6Ede0Md128AOHoTeWzhy+fREwM6744SB937s1MHgrIWSV6f4CDTw+jR+pl6+xBK6Qfzk5nxKebGdb/wyRschf/21a/fANDHi6EwjbBdqWnGxxhZympspJ18WiElLo+FE9ad8uI6vDppsa1CEPeH9t9xvY2H3pHCUg6OX28/Q9cZoVPZXaV2hcv142A/YSk3Oq5uhHE2GvqkXKqsY9j1m3fh2NbJw110Rg7u3ryuzTgjJS17uujk4xG34SPJIlLTlLYNLxhvtUdtR29mts/zHk1tPjVj2Ep41HcWcesjy2PBrddtCdINW96jt2eP2S6h3nr7gzIijyg2yvHvBtfqG4nv7DUPcXnI6X0qLVbDVnCn+gidhjd/qzeJnS7NF2nxCbe5QHvL2mYgIiIiIiK5omdWPdpdvIGff7oE4BJ++nl+l3CcV0HaV8Crjd9C7//9N/7y9/+Jvic4q+EL9GePJ9vGLeOKbe8OFBzvajtH0ccobe/5jwutbaE3GaJVa3hX3dseswbEHOSWlWWIOfiQmZGPsD6THu51RnAHe6kHmeRs8bEw6qzz7moYOV3MjkGNjzGCA2M/s7GB2cX9kjRlicnTO1B1hCW8KbB6+nJd5PIoW9666zEgO67Dq5Ma2yr4d30aP5i5xoZT4rqxjrZ39Bq7toPTlSlebrE4BHfDNdP7Z0bDVhN9OLh7s2h/rq6OVvWbuOuYdyF5d+WlbIssWLFlTxeSMY4IxyNuwxcTk2fmbfjU8XaIlvdMa//RuWNsPApOPMbP8+4m1S5s8e9adh+m3RkuY6yPhi3UGh3cCD3KWw1c9JuWd6hL0gFAv4kmBl6a1Dvac+o30Th+OH9keOTOZv+VBDf8OviPJ/ceZ+z9dia9LdSaCD3eeIwuQq8SERrudjCKvFpEFqvtPfPVA4fteux0ab4zlvg0ajXUXtyKiZlMedsMRERERESUVTkngK/9hvs7wKsHV2bv8sXBFdyxvjA4ySd0p+8x7X4KTfuCH+5H3xOczQS9R97jtoJ9rG1vjxv6U5dGRxt4Ft6hc0boNMJXVG9jTw3gYoROo4k+kHwwZbgL78loZor0ssKGaDX7QPjgSC7x+aTVZ7jbwcgdRB7ZVlhCfObi6hy+Qts/iVPVwYIyBAedH4UPEPh9cyXFLddVwhjIcB1eHXlsS+XfubVQ/uM6+824ZRToo5l0IiUrcbl23gmG/OrtQ6ix96hJ766gvO2JxsU7SJ9wx1xEckzLq6OEf1I+/Gju4ESJ5XdeXHLbkxRd9nTRxI8jaeMRt+ELKmUbPs94W0f7MG4bJTTPcmHL5OVz8wRjAdH1UdAWrU8Fj8We3SksTRdIuiAvTF+v1lCredt0qdxB6P3Y+kl474KKcJ/evuWGTnx7jx2PbjcGF3olLUcYdfZ+FuE797PGSipjvk4XYy0+tmnpFwpKtxkKLEsiIiIiIhIp5wQwgO+677G/cwkPvvUf3bz7Ga9f/4rN4NHQ33zGpv6lEOPdwAb/TuKsJi/hPeEztNezfQuu5b07kXfQBTt0oSuqvUciNQH/Ctpx10G/6T0uyeTvcBkHPTxpZYUFV812nxU7OJKUT2J9hi00+9Kdcqnk+ATi6+y9Zyy4knncPUJTf9zVUqmjfRi6kto/6HV8wwVwA7E3RlxQ8ct1dTAGQlyHVydDbEtVvw7Zqa1y143BXVLGIzcj3NCdPSrmgGU2snLtJm9KOFVeb+NQqdBJ1jwno+dxGft37Fp/NlaCmJZSRyGtj09ePo/efVgqQdtjlLLs6cJIGkcSxyNuw5eghG140XjrPRFh1GlYLhZJmlfHTe8M8OzEa9rrLbKKro/ME6WB6AlTaTqfuL76elV5d6bqyTJrYEM7kT580Z8vY//itX5TO2HZlJyu1Oo87gKdRuhxyhljJVZVvmmk2wxVLUsiIiIiIgqUdgIY/kng2aOb//kbrv18Ca/wBfVr8zTHE63It1/h2PZu4JJ4V0DrO2velaXGVa+68CO//MenOd3x7AraevvQe9ySbacmuDJe+uitmMeLDVs1NPsOumP5QUObzPmE6uPt/Eav0G10RoB/ICTXARtBfLLUud5+hq4TWqaNDTgYwXitYPiRcZI0pdrGnraTe3/jCHA2UHpRSyx2uS58eZQoY91jY0AGrsOrky22MQcJY97DmMw7yJr03tex94zocteN9TaedR2MOvfEd2GWokC54+OR5QRDzmVRb+NwEH+hglS9fejd1Ry5G64kJdUxmX8HU2cXQ/+OrugJtOVgX/a0ijKPI9yGN7a7iiu2DS8db733ESsM3OCJCPOLYZLnPZy/U9h2srmgyPoo9SkeGdMtm35ztoya/fnjnwNu+FHKs096P4/wtwtmdw5XFauq8s2g0m0GIiIiIiJKVeoJYN3ByzVg5xO+A4Brn/CXzeBdvyE/X8Kr4C7ht5fx/fpVdA6iSd5OvgLwCTe/i05PF1wBPX+Xz+wTOcDoH4zWH2cUPogQ9w6ruIP+L/qA9dFbgrJ83sETwB1k3KnUJOeTXp/tPX0n17+a1+liHH7HUAbx8fEk1zlBcCDGv8PsSDtK7l3B7u/sStJUyuufy3jguSqJy/XMl0cBGeqeGAPScB1eHWlsEw60w97udHVcv4HoY3jD/EfyVrFu9A6Sj9DZfaHPqlSucoM4hB8TWXRZxPT3rLxHl+Z/t3GikuqYZPbOzJb3Ts6Hy/YDtS17WknJ40j6eMRt+Kpk2YbPMN76tveCJyJI580fzTss+6kG+vrIj73+LnUEfUNbjqnplsXkJZ6P5u/Q9T6hk78xfa4UVcWqqnwzqnSbgYiIiIiIEpV0AngNnfWrWO+szaa8ffIn3Hn6GY//GrzPN3iX75XQCd41dO6sATu/4Ydr85PET1/O8wG+wj/+fgmbj3/1TiRnkfR+qu1bcGc7RMH7e8I7Jv57q9yH3sGLIL129epwt2O+Y0nfUY4QlAXvUaXewRNV6J1d6fnI6lOqxPhI6jxEK3TVuzfJW9bzAzHBHT6hO65mdwAG5UrSVGWC3lYDHXTxrJIgnzHLiYj05XqWy6MoWd3TY0ARXIdXRxxbAPU2HrpAv6k9dnLSw1bOsWJ7L3gXs7Yun/Sw1ehg5FS1btzG3sAF+v0Fv2MuY7lxcciyLIat0OMl4Y079yz9PY/t++ga78TMoco6JgnemdnvZ3js6ILELXtaOenjiGw8KlXi+Cip8wpuw0vH22Er+kqK8LZ00jxfcJKtaXmqwbBVszw6WsC6PvIeR208PWXY8pb97M5wabolUb+OG7N30Yc+szEqeAy39jQPYxyT8J4+Mf+dZohV3IVg1ukZ8q1SWdsMRERERESU3XQ6VVk+rx//roD/qn193uv/qE0ohdnHkmY6VdP9/4bSKIWdD0aa/Z1wPkrt7FvysXz29/dV2MCFAlw1iEyd0+ePu44CMP+4+jcHyg3Phz1/PV+b5LJs5QQfR3XHoaSJ5Pkk18c07joKTleFq2LkMftEY5EcH1mdbWXZquyVNf84luClpbGV5X0S+o6RZqy6jjbPVuElB0CfFBJddtE4yparKml5FGVt58C1lBmtX3Ld5TFYVXrck9cV5nyjbxi/MdsyMPPX87VJLstWTvA5m2VdNLbK1uaY9e7MwE1tr/6bgfG7mSU00kXSWsry6mtvY1BuuP629gEwxrqICstNiq3tO7b0Rrq4tljaEYhrjzc99B1LHkb5lnoYaeLqGCipLwTlRuPm/XYjfdCSn2Se0S5L++LS2JYl5QfbmL705OOI0Y9SOtC4y234xG0HI022bXgUGG/19oSLSZrnCepprpO875rTw+LiYJbjM9bFMfkL0g3c5JgGbOtyj7nuHrjR9a2tjGgaL37RJH5Mk9bbKWOWkT742NoriJWXbJ4mro9Eshfkq8cry7SwuGXkTdfXA2Y627IkuqhwLrdPlsfJyYk+iTJg/Iph/Iph/Iph/IpZpvidnJyod+9+Ue/e/aI+fPhQ+ifIuzadTpV+Uvi8Ojg4wO3bt/XJRFSSWq0Gb1/lYluVdi4bxr06jC0RrSqu/2iRzq6/ze9MHh8u6M7OC2TS20Kjc8N452/cdCKios5uvLgYTk9P8fXXX+uTSYjxK4bxK4bxK4bxK2aZ4nd6eoq1tT8AANbXr+qzC5tO3wPlPQKaiIiIiIiIiBZu8hLPRwt8rO+FpL9zOXhU85K9KoCIiIiIiEiIJ4DPpSFa4XcTWT/a+7WIiIiIiIjowhnuLuD96RdYvX2IcddBvxnen27iqDuGsr/QmoiIiIiIaOnxBPC5tI09paASP3xMFRERERER0UW3vcf9v6Lq7UNjn/qwzfupiYiIiIjo/OIJYCIiIiIiIiIiIiIiIiKiC6L2/v17FVzhCsD6r23aMs778ccfcefOHRAREREREREREREto5OTE30SERERrZC1tT8AANbXr+qzCptO3wMAatPp1DuDegEcHBzg9u3b+mQiKkmtVptddHGRrUo7lw3jXh3GlohWFdd/tEjsb0REJMHxopjT01N8/fXX+mQSYvyKYfyKYfyKYfyKWab4nZ6eLuQEMB8BTURERERERERERERERER0QfAEMBERERERERERERERERHRBcETwEREREREREREREREREREFwRPABMRERERERERERERERERXRA8AUxEREREREREREREREREdEFkPwH89jK+X7+CA306gLdP/oT19av+50948lZPAeDgSijNVax31vQUsjRERERERERERERERERERBSR8QTwGjrf/hGv9MkADjpX8e0D4PHr95hO32O6/wUPvr2KTvhM8cEVrN9Zw86+n2b6ETtPr0RP8B5cwfruZ7ye+mle/4pNPU0uE/S2aqjVamgN9Xlzw5aXZvbREhvzt3qYBDMnPWyF52kfvVwjr0iCIVop35eR55Ncn7lJb8ubH2572LBl/744PpI6S9KE6hp8LIkkaYAy2pWhrPPOj0m0eeUtMyBheVRl2EKttoWetdN70usuiwHZrOo6fBFSYjtsoVZrwTYraOdWbxLJJ/ajFWD8ZixpAMHvzzY/WEdY6x6ut8dal1rCWIdqyw2nmREvi4C+TIK66tMtH3852OtnWRaWWNi/q8dUr4sl7zBLORGW+fN6JHwv9JuNxDCSn15XyycxbtG2x6WxLntaQfJxJHk8muM2fN52ZSgrUcp4a6xj9HVW/Hyvfnr6eRuzrFeMtvqfpDys37E3EsiQ3prO1k6N9z3beGkZKy3jRtaxfMbap6J52NuU8LuM/U58HKzpI/HV+5Ll0+oJ0kSjk16uni6+DbHjchzbcgzJ1CeIiIiIiC4I+QnggytYX7+Cp/p0eHcF7z4FNh9/xA/X/GnffcT+DvB09zK8G4G/wpPdNWDnI7rfBV/8hO7+J+DpZf9u4TV07qxh8y+fEGSDa7/h/x5/Bp6uWe86FhvuojNy4bpA/4W52R/sBDWPuhgrBRV89rZnKYatGpp9F4PZ/AHcUQeNYGet3sZh+Lv+Z9x1ALi4NcsqrawJeltNYDCfN3CBfjPuYEEcaT5p9Qkn7eFeB3BdR58z35Fs9vUZHlF8ZHUetmxpzAO+jQ7QHQfpBnD7zchOqCRNOe2SlnVRyZarLEYpy+OMpNddFgOKsZLr8AVJja1UHe3DUDwGLgAn9JvQY1TTfjP+Muk3Yw7QZTN5c+T/r4+mOPDh/uF/Dtuo68kSlFLuuAt0GokHg9NN0NtqoINQPx3fxfN7PUwyLSsY9fOqJ+3PSTFNqmMVRnj+0p7zpPcI6aNKsbhF2x6TppRlT+efdBxJG4/CSbkNbxC1S1qWQOJ4m7Y+TJ5fbz+EixE6u9F8h7sdjODiYTvLSIYM66as43nW9DDqkm0MyifPWD5s1VBrdHAj1L+9+h6hacRNMj7oot8ZuCN0GvoJT2l8JeNZW5Cm6HZd0XGZiIiIiIiSyE4Av72M7++sYfPxv/H68Wd9LvDzJbwCsFH/Epn8zZ8/A6/W8I+3AN6u4e+vgM0/a9//5jM2cQl//8dXwMEanuIz/vK/0Xyu/fD/MJ1+xOy8cQ7DF33AvYW9Wy7Qf2HsgEx699AZuRjE7nhN8OYIgHsL80Mq27jfdYDRMcaRtGFD7HZGke+ll+XtkIWP3Wzf78IBcPTGvoNkJ8snvT6BCXr3OkD3Ge5v6POCfBx0x2N0bceWrPT4yOq8vWdLE96B9PJ1us8wP97hL6/Z8pekKatdsrIuLslylcUo3/KomqTukhhQnNVchy9GWmyrMP8dH4Z+MwCwjb1xF06GA67JXHS7DtB/FHtHSDUKlltv43DchTPq4F6uDABgjOMR4Ny9Oe+n9TYOY/utnHeiwXYCI6vq6mjylsmos2vp4xO8fD6C0+3C1WctWinLns4/2TiSPh4FuA2fv12ysiSSx9u09WHa/KBOoXFn0sOjPuB074e2fXKKWTdlHc+zprcpbwxKIx/LJ70tNPveyVH9+ot6+1Bwcjc787dTTnzzyFfuORmXiYiIiIjOMdkJ4Gu/4Z/T9/jnD9FhVAQWAAD/9ElEQVQTs1Gf8edv9Gkm/SQxrn1BcBzi7eQrAF9Qv7aGTqnvAB7C29/eBrZvwUUfjyJ7ccEORtLOcR3XbwA4ehN5bOHL59ETAzrvylUH3fuzUweCshZJXp/gIFPcFeT19iGU0nf6kpnxKebGdb/wyRschf/21a/fANDHi6EwTVntEpa10oQxyrM8KiesO+XFdXh10mJbhSDuD+2/43obD70ju5YDgtldbz9D1xmhU9ldpXaFy/XjYD8wKjc6jr+8oShno6FPyqXKOoZdv3kXjm2dPNxFZ+Tg7s3r2owzUtKyp4tOPh5xGz6SLJHRLmFZ6WTjbdr6MGm+fhfwcLeDkdPFsywBSGKsm7KO51nTJytrDEoiG8tT2lWxed9MqUfG+MrlL/fcjMtEREREROeU7ARwmvBdvCE//3QJwCX89PP8LuE4r3665P9vDXfWL+PPwbuEp//G4+OC7wAevkB/9hivbdxygdHzl6GdOO+Kahzvau/siT5SaXvPf1xobQu9yRCtWsO76l6/zHfGtjMkK8swPsbIcvAhMyMfYX0mPdzrjOAO9lIPMsnZ4mNh1Fnn3dUwcrqYHYMaH2MEB8ZxgcYGZjcASNLkYmlXZWWdY/pyPc8xylt3PQZkx3V4dVJjWwX/LibjBzPX2HAAHKGcG6braHtHrKE9GbNixcstFofgbrBmev/MaNhqog8Hd28W7c/V1dGqfhN3HfOuMe+uvJRtkQUrtuzpQjLGEeF4xG34DCztKqus1PE2bX2YNh/Ru4CH3t2/7sNy7zyNrpuyjudZ09uVNwZJCMbyyUs8T2lXFYLHe89fUVJOfLMrUO45GpeJiIiIiM6jck4AX/sN93eAVw+u+O/y9d4ZfMf6wuB0kXcJ4wt+uB9+T3BWE/QeeY/bCvaNtr09buivmxkdbeDZ7H01Y+9q30b4fTXb2FMD78rqRhN9IPlgynAX3hPEzBTpZYUN0Wr2gfDBkVzi80mrz3C3g5E7MB5pVUhCfObi6uy/06tWQy04iVPBo7VyEbVr1cUt11XCGMhwHV4deWxL5d9NtVDbe/57JuOWUaCPZtKJlKzE5dp5d5jlV28fQo29R0R2GkXaE41LE4MMd9Ulx7S8Okr4B/Itj0i1/c6LS257kqLLni6a+HEkbTziNnwGonblIRtv09aHafO9NP4dq03txHpJIuumrON51vQzeccgfR1cQ63mbf9lIhzLwxc6THpb0XKNdwDrdTOXpUmLg/5479zxLahQuWc9LufsE0RERERE50Q5J4ABfNd9j/2dS3jwrf/Y5t3PeP36V2wGj4b+5jM29S+FzN8NbL4D2OPfSZyVf0VuZAdi+xZc7X05gPZOpWBnJPRIIm9HrgkMvIMs466DfrOGmvE+G8x39GN2vNPKCguucu4+K3ZwJCmfxPoMW2j2k+6SyyM5PoH4OnvvGfMOdimMu0do1mrYSt9zrpisXasufrmuDsZAiOvw6mSIbanq1yE7tXUDsTeN5eC9K8/+yM05F4PZiRQlPMCcTFau3eRN/kOqM/U2DpUKnTRIPoBtN4/L2L8DzfqzsRLEtJQ6Cml9fPLyeSUnSTyCtscoZdnThZE0jiSOR9yGz0DWrlyyjLdp68O0+bM+UP7dv9DXTVnH86zpZ/KOQfo6WEGpQa53ykrG8vC7rr3Hj3tlDqwF6nWTjA/ad8ZdoNOYn1zOHd+CipabZVwetrSTt3r/T6PHPX+fICIiIiI6D0o7AQz/JLD32Ob3mP7zN1z7+RJe4Qvqs7t5geOJVuTbr3Dsvxv4mv5+4BJMXj7HCPAO8mtXeaa+Wy38aC//8WlOdzy7gr7ePoTyLgc2d0KDK8ilO94xjxEbtmpo9h10x5KdwniZ8wnVZ/iib1wt2+iMgFEHjbwHbATxyVJn72r30DJtbMDBCMZrssKPcZOkySquXVWUdU7FLtfzHKOMdY+NARm4Dq9OtthaHtsHxL4bMVkDG07yewzH3rMEUerPvt7Gs66DUeee4C6bEhUod3w8shwwzbks6m0cDuIvVJCqtw+9O6Ee6XczlaCkOibzH73a2cUQQ+x2RtoJtOVgX/a0ijKPI9yGN7a7ROLaVUJZ2cZbX9r6MG2+sG5ZRddNWcfzrOlNlY5BSZLGcv8EaFK7KuHXaX4nefH45lO03Azj8vaedvI24Uk+RERERERU7glg3cHLNWDnE74DgGuf8JfN8Lt+fT9fwqvIXcLmu4Q9n3DzO31amuA9TgNtR0F5B/1nO8z+Tov+3sPwjn3cO6ziDvq/6AORd/IEBGX5vIMngDtIP3iSJDmf9Pps7+lXyfpXXztdjJXCoZlpqvj4eJLrnCDYsfR3xMNXYmN21Xr0KvTENBnFtquCss6jxOV6nmOUoe6JMSAN1+HVkcY24eA37O1OV8f1G4g+7i/Mf/Rf7MG/Aurth94jwHdf6LMqlavcIA7hxzsWXRYx/T0r79GlCe9DLKKkOiYJ7uR60fLeyflw2X6gtmVPKyl5HEkfj7gNLxfbrsJlZRhvdWnrw7T5ZTPWTVnH86zp7SodgxLEj+Whdy/b2rUw5cQ3u+LlLv24TERERER0Xk2nU5Xl8/rx7wr4r9qPTP+gdqAUdj5o6X5Xj1+H0u3/VwFK7eynfS+c/7/U402lNh//y6iL/tnf31cRA1cBUO4gOtkzUC6gEMw00mrzg7+drhoHSZRSAxcKcFWkiHFXOYByuuGUIallKTXuOgl1lxPlI6iPbtx1jFjMjVXXSfh+SnzS6zxQrh5zvw3hPL1l46jZJEu5kjRzxdqVrazlBECfZDdwo20VLdesMUpZHgVY22lpU5ik7pIYrDIj7sa6KWw11uFlKRRbW/9W8zjF/gYTfzN+GTGx15dTcl72+d4y0PJX87brY0Zs+iRVlRsXhyzLYuBq3/fXmXpZyt6OgLV+QV7h/C152L8bkqWOAUs5EZb5Zj2CcvT+6/XLyG/fkp9knlmmyZomYdlTPsb675wQjSPGutxcf+u4DW+R+N1sZRn9zVhGYaHllbY+TJsflrBuMtpikW3dlHE8z5jeWhfbGKSxf0/Nyk9bz8d+P2YsD48r0WVt1jU27wT279h+79niO2OJgSExTbZyzfZkGJfjJNbPVmYgQxlEJTLGC8rk5OREn0QZMH7FMH7FMH7FMH7FLFP8Tk5O1Lt3v6h3735RHz58KP0T5F3SCeCpmr7+j9qEUph9LGmm85PAs0/o5G9cGsnJ36nlBLD1wH6IPj84aDH7GHvqwY5N+GPmr+drk1yWrZzgE79TY5Lnk1wfk+3gkZHH7BONRXJ8ZHW2lWWrslfW/GPbsUtLYyvL+2RplyetrGWHxJ2U6LKLtk22XJUgRtLlUYS1naEDPnH1S667PAarSo972m9Kn2/0DWOlYFsGZv56vjbJZdnKCT5ns6yLxlbZ2hyz3p1JORCnLL8ZGL+bWUIjXSStpaz4A33zcsP1t7UPMA9aRlRYblJsbd+xpTfSxbXF0o5AXHu86aHvWPIwyrfUw0gTV8dASX0hKDcaN8tBYEt+knlGuyzti0tjW5aUH2xj+tKTjyNGP0rpQOMut+H1NiS3y5NWVgAFxlujvmnLKW59mbBu8sqzzwsY5fgf23IK6PFJipHKkN62/p5Pj29H3Pek6/n478/rbo2HbYxKW44x6cJiv2OthDy+M5YYGARppOXa4hu0MXVcjmOLfei7tjL9L8rLICoRzuX2yfJYpgP45xHjVwzjVwzjVwzjV8wyxW9RJ4Br0+lU6XcFn1cHBwe4ffu2PpmISlKr1eDtq1xsq9LOZcO4V4exJaJVxfUfLRL7GxERSXC8KOb09BRff/21PpmEGL9iGL9iGL9iGL9ilil+p6enWFv7AwBgff2qPruw6fQ9UPU7gImIiIiIiIiIiIiIiIiIaHF4AvhcGqJVq6GW+GlhqH+NiIiIiIiIiIiIiIiIiC40ngA+l7axpxRU4mcP2/rXiIiIiIiIiIiIiIiIiOhC4wlgIiIiIiIiIiIiIiIiIqILovb+/XsV3DUKwPqvbdoyzvvxxx9x584dEBERERERERERES2jk5MTfRIRERGtkLW1PwAA1tev6rMKm07fAwBq0+nUO4N6ARwcHOD27dv6ZCIqSa1Wm110cZGtSjuXDeNeHcaWiFYV13+0SOxvREQkwfGimNPTU3z99df6ZBJi/Iph/Iph/Iph/IpZpvidnp4u5AQwHwFNRERERERERERERERERHRB8AQwEREREREREREREREREdEFwRPAREREREREREREREREREQXBE8AExERERERERERERERERFdEDwBTERERERERERERERERER0QWQ/Afz2Mr5fv4IDfTqAt0/+hPX1q/7nT3jyVk8B4OBKKM1VrHfW5vPeXsb34Xnap2MrlIiIiIiIiIiIiIiIiIiIgOwngNfQ+faPeKVPBnDQuYpvHwCPX7/HdPoe0/0vePCtdtL24ArW76xhZ99PM/2InadX5ieBr/2Gf06DeaE0ALD5K/76XSivzCbobdVQq9XQGurz5oYtL83soyU25m/1MAlmTnrYCs/TPnq5Rl6RBEO0Ur4vI88nuT5zk96WNz/c9rBhy/59cXwkdZakCdU1+FgSSdIAZbTLF5fPReLHJNrE8pYZcAZxHLZQq22hZ+30nvS6y2JANqu6Dl+ElNgOW6jVWrDNCtq51ZtE8on9aAUYvxlLGkDw+7PND9YR1rqH6+2x1qWWMNah2nLDaWbEyyKgL5Ogrvp0y8dfDvb6WZaFJRb27+ox1etiyTvMUk6EZf68HgnfC/1mIzGM5KfX1fJJjFu07XFprMueVpB8HEkej+a4DZ+3Xb64fMRSxltjHaOvs+Lne7HQ08/bmLReMeLofzJ/x94oIEN6azpbuzTe92zjo2VstIwTWcfuGWsfiuZhb1PC7zD2O/FxsKaPxFfvO5ZPqydIE41Oerl6uvg2xI7DMaxlW/LP1DeIiIiIiC4Y+QnggytYX7+Cp/p0eHfu7j4FNh9/xA/X/GnffcT+DvB09zK8G4G/wpPdNWDnI7qzE7mf0N3/BDy9bL9bGMBB5wqe4jMe/99vCLLOZbiLzsiF6wL9F+bmf7BT1DzqYqwUVPDZ256lGLZqaPZdDGbzB3BHHTSCnbd6G4fh7/qfcdcB4OLWLKu0sibobTWBwXzewAX6zbiDBXGk+aTVJ5y0h3sdwHUdfc58x7LZ12d4RPGR1XnYsqUxD/g2OkB3HKQbwO03IzulkjTltAvp+VxosuVayvI4I+l1l8WAYqzkOnxBUmMrVUf7MBSPgQvACf0m9BjVtN+Mv0z6zZgDddlM3hz5/+ujKQ58uH/4n8M26nqyBKWUO+4CnUbiweF0E/S2Gugg1E/Hd/H8Xg+TTMsKRv286kn7c1JMk+pYhRGev7TnPOk9QvqoUixu0bbHpCll2dP5Jx1H0sajcFJuwxtE7UJ6PlKJ423a+jB5fr39EC5G6OxG8x3udjCCi4fttJFMui7KOn5nTQ+jLtnGnHzyjN3DVg21Rgc3Qv3Zq+8RmkbcJOOBLvqdgTtCp6Gf4JTGVzJ+tQVpim7HFR2HdYvvK0RERERE54nsBPDby/j+zho2H/8brx9/1ucCP1/CKwAb9S+Ryd/8+TPwag3/eAvg7Rr+/grY/LP2/W8+YxOX8Pd/WKpiO7Gc0/BFH3BvYe+WC/RfGDskk949dEYuBrE7YhO8OQLg3sL8kMo27ncdYHSMcSRt2BC7nVHke+lleTto4WM32/e7cAAcvbHvMNnJ8kmvT2CC3r0O0H2G+xv6vCAfB93xGF3bsSUrPT6yOm/v2dKEdyi9fJ3uM8yPd/jLa7b8JWnKalfefC4KyXKtcnlUTVJ3SQwozmquwxcjLbZVmP+OD0O/GQDYxt64CyfDAdhkLrpdB+g/Mu4IqVbBcuttHI67cEYd3MuVAQCMcTwCnLs35/203sZhbL+V80402E5gZFVdHU3eMhl1di19fIKXz0dwul24+qxFK2XZ0/knG0fSx6MAt+HztytvPqbk8TZtfZg2P2h/aNyZ9PCoDzjd+6FtH6GYdVHW8Ttrepvyxpw08rF70ttCs++dHNWvt6i3DwUnd7MzfyvlxDePfOVWPw4vrq8QEREREZ0PlrOuFv6jmf/5Q/QEb9Rn/PkbfZpJP0mMa19gOQ4BADj42x/xCp9wP7FciSG8/e1tYPsWXPTxKLJXF+xwJO0c13H9BoCjN5HHFr58Hj1AoPOuZHXQvT87hCAoa5Hk9QkOMsVdQV5vH0IpfScwmRmfYm5c9wufvMFR+G9f/foNAH28GArTlNiuPPmslAqXR+WEdae8uA6vTlpsqxDE/aH9d1xv46F39M5ygDC76+1n6DojdCq7q9SucLl+HOwHSuVGx/GXNxTlbDT0SblUWcew6zfvwrGtk4e76Iwc3L15XZtxRkpa9nTRyccjbsNHkiWytStPPibZeJu2Pkyar98FPNztYOR08SxvxY11UdbxO2v6ZGWNOUlkY3dKuyo27/cp9cgYX7n85S5qHF5EXyEiIiIiOg9kJ4DTxNzF+/NPlwBcwk8/z+8SjvPqp0valDW8fApg5xMKvfoXAIYv0J89xmsbt1xg9PxlaKfOu6Iax7vaO3yij1ja3vMfF1rbQm8yRKvW8K661y/7nbHtHMnKMoyPMbIc6MjMyEdYn0kP9zojuIO91INMcrb4WBh11nl3NYycLmbHasbHGMGBse/X2MDswn1JmlyE7Vp1+nKtbHksQN666zEgO67Dq5Ma2yr4dzEZP5i5xoYD4Ajl3DBdR9s7gg3tyZgVK15usTgEd4M10/tnRsNWE304uHuzaH+uro5W9Zu465h3Bnl35S3XmF1s2dOFZIwjwvGI2/AZCNuVR+p4m7Y+TJuP6F3AQ+/uX/dhsTtRo+uirON31vR25Y05EoKxe/ISz1PaVYXgcd7zR5OXE9/sCpRb8Ti82L5CRERERLT8yjkBfO033N8BXj24Mn+X78EV3LG+MFjm7ZPL3rt///pJn5XRBL1H3uO2gn2lbW+PG/rrZ0ZHG3g2e4fM2Lv6txF+f8029tTAu7K60UQfSD6YMtyF9wQxM0V6WWFDtJp9IHxwJJf4fNLqM9ztYOQOjEdcFZIQn7m4Ovvv4qrVUAtO4lTwqK1cRO1adXHLdZUwBjJch1dHHttS+XduLdT2nv+eybhlFOijmXQiJStxuXbe3Wz51duHUGPvkZGdRpH2ROPSxCDD3XDJMS2vjhL+gX3LI1Jtv/PiktuepOiyp4smfhxJG4+4DZ+BqF15yMbbtPVh2nwvjX8Ha1M7sZ5TZF2UdfzOmn4m75ijr3NrqNW87b1MhGN3+MKGSW8rWq7xDmC9buayM2lx0B/nnTu+BRUqt+xxWNpX9Pjn7BtEREREROdMOSeAAXzXfY/9nUt48O1VrK9fxfruZ7x+/Ss2g0dDf/MZm/qXQvR3A//80yVg8xP+t+C7f4MrdCM7FNu34GrvzwG0dyoFOyehRxR5O3ZNYOAdZBl3HfSbNdSM99tgvqMfs+OdVlZYcCVr91mxgyNJ+STWZ9hCs590l1weyfEJxNfZe8+Yd7BLYdw9QrNWw1b6nnTFZO1adfHLdXUwBkJch1cnQ2xLVb8O2amtG4i9aSwH79159kduzrkYzE6kqJiDiNnIyrWbvMl/iHWm3sahUqGTBskHtO3mcRn7d6BZfzZWgpiWUkchrY9PXj4v5SSJnaDtMUpZ9nRhJI0jieMRt+EzkLUrlyzjbdr6MG3+rA8Uv/sX+roo6/idNf1M3jFHX+cqKDXI9U5Zydgdfre195hwr8yBtUC9bpLxQPvOuAt0GvOTy7njW1DRcrOMw8OWdtJW7+/SvqLHP3/fICIiIiI6T0o7AQz/JPB06n/++Ruu/XwJr/AF9dBJ3OOJVuTbr3BsvBvYf/zzxhcUP//7HCPAO8ivXe2Z+m618GPE/MenOd3x7Ar6evsQyrs82NzRCK4gl+54xzyybNiqodl30B1LdhLjZc4nVJ/hi75x1WyjMwJGHTTyHrARxCdLnb2r3UPLtLEBByMYr8kKPzJOkiYrQbtWXexyrWJ5LErGusfGgAxch1cnW2wtj/EDYt/DmKyBDSf5PYZj79mCKPVnX2/jWdfBqHNPcNdNiQqUOz4eWQ6g5lwW9TYOB/EXKkjV24fenVGP9LubSlBSHZP5j17t7GKIIXY7I+0E2nKwL3taRZnHEW7DG9tdIoJ25ZVtvPWlrQ/T5ueNgya6Lso6fmdNb6p0zEmSNHb7J0CT2lUJv07zO8eLxzefouVmGIe397STtvFP7jmzvkJEREREtMRKPQGsO3i5Nn+H77VP+Mum5V2/P1/Cq+Au4YB/UnjnZvHHP3vvcRpoOw7KO+g/22H2d2L09x6GDyLEvcMq7qD/iz4QeUdPQFCWzzt4AriD9IMnSZLzSa/P9p5+tax/ha3TxVgpHJqZpoqPjye5zgmCHU1/xzx8ZTZmV7FHr0pPTJNRWrtWXeJyrWB5LEyGuifGgDRch1dHGtuEA+2wtztdHddvIPr4vzD/UYCxBwMLqLcfeo8A332hz6pUrnKDOIQf91h0WcT096y8R5cmvB+xiJLqmCS4s+tFy3sn58Nl+4Halj2tpORxJH084ja8XFq78ssw3urS1odp84sy1kVZx++s6e0qHXMSxI/doXct29q1MOXEN7vi5VY1Dp9VXyEiIiIiWlYlnQBeQ2f9KtY7a7Mpb5/8CXeeht/h+wU/3P8EPL2CzkHoe3fWgJ3f8EP4Vl/bSeE8kt7jtH0LLoD+iyFmj8qK7Cz4761yH3oHL4L02hWlw90ORvrBAmNnOUxQFrxHlXoHT1Shd3al5yOrT6kS4yOp8xAt/fFP/rKe72gGVxaHrtqe3QEYlCtJk0FKu1aK5URE+nIteXkslKzu6TGgCK7DqyOOLYB6Gw9doN/U3lc36WEr51ixvRe8i1lbl0962Gp47y18ljVTkW3sDVyg31/we98ylhsXhyzLYtjS3kE4Qe+epb/nsX0f3rHvgnfZVFnHJPWbuOsA/X4/8k7OpRC37GnlpI8jsvGoVInjo6TOK7gNLx1v09aHafOFhq2a7P2zMeuirON31vRWZY05mcWP3bN3LTdq2lNkJqjuCf7e3bLh33cp8c2hcLlVjcNn1leIiIiIiJbUdDpVWT6vH/+ugP+qfX3e6/+oTSiF2ceSZjpV0/3/htIohZ0PRhqvjN/V49eW7yd89vf3VdjAhQJcNYhMndPnj7uOAjD/uPo3B8oNz4c9fz1fm+SybOUEH0d1x6GkieT5JNfHNO46Ck5Xhati5DH7RGORHB9ZnW1l2arslTX/OJbgpaWxleV9srRLns8yA6BPCokuu2gcZctVlbg8irC2c+BayozWL7nu8hisKj3uab8pfb7RN4yVgm0ZmPnr+dokl2UrJ/iczbIuGltla3PMendm4Ka2V//NwPjdzBIa6SJpLWV59bW3MSg3XH9b+wAYY11EheUmxdb2HVt6I11cWyztCMS1x5se+o4lD6N8Sz2MNHF1DJTUF4Jyo3HzfruRPmjJTzLPaJelfXFpbMuS8oNtTF968nHE6EcpHWjc5Ta83obkdsnzUZb+lpZ3eL5RTtpyiltfJqybvPJS+pD/sS2XgB57WOIfJk1vW1/Pp9vbpBK+J12vx39/XndrPGxjUtpyi0kXFvsdayXk8Z2xxMAgSCMt1xbfoI2p43AMW57z6fo6x0yXpSyiKuBcbp8sj5OTE30SZcD4FcP4FcP4FcP4FbNM8Ts5OVHv3v2i3r37RX348KH0T5B3bTqdKv2k8Hl1cHCA27dv65OJqCS1Wg3evsrFtirtXDaMe3UYWyJaVVz/0SKxvxERkQTHi2JOT0/x9ddf65NJiPErhvErhvErhvErZpnid3p6irW1PwAA1tev6rMLm07fA+U9ApqIiIiIiIiIiIiIiIiIiM4aTwCfS0O0ajXUEj/a+3iIiIiIiIiIiIiIiIiI6MKrvX//XimlZo8esf1rm7aM83788Uc+ApqoQqvymKJVaeeyYdyrw9gS0ari+o8Wif2NiIgkOF4Us0yP8DyPGL9iGL9iGL9iGL9ilil+i3oENN8BTERiq7KTsirtXDaMe3UYWyJaVVz/0SKxvxERkQTHi2KW6QD+ecT4FcP4FcP4FcP4FbNM8eMJ4BwODg5w584dfTIRERERERERERHRUjg5OdEnERER0QrhCeCMeAcwUbVW5SrVVWnnsmHcq8PYEtGq4vqPFon9jYiIJDheFLNMd3CdR4xfMYxfMYxfMYxfMcsUv4XdAcx3ABOR1KrspKxKO5cN414dxpaIVhXXf7RI7G9ERCTB8aKYZTqAfx4xfsUwfsUwfsUwfsUsU/wWdgKYdwATkdSq7KSsSjuXDeNeHcaWiFYV13+0SOxvREQkwfGimGU6gH8eMX7FMH7FMH7FMH7FLFP8FnUC+Ct9BhERERERERERERERERERnU88AUxEREREREREREREREREdEHwBDARERERERERERERERER0QUhPgF80LmK9fXg8yc8eaunkKXBwZVQmqtY76zpKWRpiIiIiIiIiIiIiIiIiIgoQnQC+KBzFXeefsL+9D2m0/eY7n/Bg2+vonOQLQ0OrmD9zhp29v0004/YeXoleoJXkiaPSQ9btRpqoc9Wb6KnwrAVTVNrDePn+Z9QEms6WzmBSW/LS7fVgy2Vnle4PhLG92PqPKtHbDlDtFLygCgfj1GvSDpJWZI06fWZz99C/GKal2VdlsOWNe9AWh1mFpTPQvi/t2gVyllmMwtup1GvWny/MdKG62hZF4U/C2rO+WOJm+33mLRuMebFxFxPZysnUPU6fCGEsQUm6G3ZYwZbv09sb468Yn5viEtvy1hj/V5NW57BuqbWgpmjt16zxssSVyOPYctsV8byJG3In8YS8xLqPCOJka6E8u1tjamjrbyZ5H5sSMzLPr/Qdkokv3ldYz9+I+Lik95fYmK4hIx1s//Rl6PRTj1Byds2Rr0i6SRlSdKk16dQv5vNTt5OS6vDzILyqZJRx5jY2tPZxqTFrAOt6Szxs6bT6xhmWfdL6mdfByWUE9NHJfnLYypft8ZLG0v0MvQ2x8/32qqnny8DfZkH4mIUlx5x37E3CMiQ3prO1iaN97205RdMKv67mrH0bz0Pe5vi9yeAmDqGZGovEREREa2M9BPAby9j9ymws/8R3wXTvvsVjzeBpy/9k7KSNPgKT3bXgJ2P6M4SfUJ3/xPw9LJ/t7CfZvNX/DWU5q+PP4fSZDds1VBrdHBjoKBU8Bnj7vNGaEPY23FqHnUxnqVRUHvb0cwcbb5SCCcZtmpo9l0MgvkDF6NOuJyQSQ/3OoDrOvoceX0kUuo86W2h0QG642D+AG6/GdoBm6C31QRC8Ru4QL8Z3UlNzyfIK7ldw5atrPDOTpn1CYzw/KVlGQGY9B6hr08EZm2pNe1zIa7D4vI5O2Uus7NsZ+i3rRQG7gidhnmwPrEN9TYOw33f/4y7DgAXt3L8xC+6lV+HV0gW2yDxLjojF64L9F/Y1qN6fP2+bzuYJclL+72Nu0CnoR8c9eIc/c2FyrYeCNNFy1FKQR22UffnTt4c+f/ro2kdP0z2uCqMu0do2uIRkqe8tDbkTWOPuSlPnYvESJenfL2tymusvb/GEfXjsuTZTgmro30Yau/ABeBEfzeR9VP2/pIrhmcpZTxIHc8r2LZJGjO4fWwqK5/FkK5fJb+9qFzrQEv/P2zPRr4cY6usffZ1v227QxqHPH0UqfnLY5p13WqROJZM0NtqoIPQ8hrfxfN7wXo2eX69/RAuRujsRvMd7nYwgouHs2VuI13HZ+0vWdPDqEtc/yqTvA/M2ft33LZNch8kIiIiIipD+gnga7/hn9P3oZO2FpI0b9fw91fA5p8/R6d/8xmbuIS//yO9KrkMW2j2AXcQPagT7KwFO7qT3j10Ri4GRTa6Jz086gNO9z5mRW3vYeACo+cvzR2lex2g+wz3NyIzvLll1EdkiN3OCE73Geb7f9u433WA/gt/58uLVTh+2/e7cAAcvQlaJclH1q7tPVtZ4Z378urjcdHtOhh1di07mxO8fD6C0+3C1ef07qEzctAdj9G1nf8R1mFx+Zyl8pbZMrXT7JuyNpi878G9NV93kIfr8OoIYxsYvugD7i3s3XJT+nPA7/uj59CPzWbPKziIGT04Ol8fHIZ+cwCwjb1xF06Gg3bJvHEC/Uexd14EJr0tNPvewV/9mG+9fSg8uCcvr0q2mMeT17mcGOnk5VvV2zgcd+GMOrgnzCBPP84n33bKwuWI4fKSjOdlb9skjxncPtaVlc/ZyLZ+lSi4DgwpY2y1ti/jdke6fH1UrryYJkkeS8Y4HgHO3ZvzdUO9jcPZuiJtfvCbCLXBtr0rEbOOz9pfsqa3sfavSsj7QDXbNkRERERExeQ66/r2yRU8ePUZj//6SZ81E5dmo/4l8jeufcH82PkX/HD/E/Dqj/jb7NHRa/jbg0vA5if877VZQqEJet7eDe4n7t0EO4gZd4J042OMANy4Ht20b2w4wOgY49C04ECP/arbkuojMXmDI0ud69dvAOhDvE8lyqdYu/S8E4nqM3f95l04luneFdkO7t68rs3wd+SUvuMaIqzDwvJZdue4nbM6C9ug8+5QcNBNXlGtIK7DqyONbWAI7/jkNrB9Cy76eJR2JGzW93X58go4Gw3/f16c4T60rw/qbTz0jg5aDgxnd739DF1nhM7srhublDplICtvMeYxTyarc3kx0snKT+D3GfvJBF2xfpxVnu2UM5Ephkss53huEOVTbMzQ804kqs9cnn6Xup0mrMPC8jlj0vWrROF1IJC+js44tobH7GzbHTJ5+mgW5cQ0iWwsGR2Ht0JNSfP1u4CHux2MnC6eWRdwCmMdn7W/ZE2frMzfTxxZH0hpFxERERHRGcl2AvjgCtbXr+LbB5ew+fgjfrCdkI1L8/MlvNKShr366ZL3n+8+Yvr6VxzfuYr19atYX7+C48f/xvSfv8FWXDLviljcuJ5ytaWf7nhXe1+L5R0row4aoTSRR1U1NmC7sNw7EHGE2cX3kx7udUZwB3sxB3oy1Eciqc7jY4zgwNh3imnLjH6iRJRPnnZ5d9mN0g4W5KpPSP0m7jrmVcTeFdk5d+Sy1iFOWfksm6LLbAkEj0+bPbY5Vxt4wCAe1+HVkcbWN3yB/qyvb+OW9a5o0/zxeSE58xq2mujDwd2bQY39u16MH9xcY8OJLrtC6mh7Rz2hPUlxbvISz1PqJCcor2JmzNMI6lxqjHSC8lOI+0zOfpxbFdspFRHH8KwljQe5xvO82zZ5xgxuH5eWzxnJvn6VKL4OLGtsNduXcbtDqoo+GlFGTBOkjiXBHbzNmHVC2nxE7wIeenf/ug/z340aXf5Z+0vW9HZm/6qSoA9Uum1DRERERJRfthPA333EdPoe0+lHbDz4H6x/fxnGa3klaRIcdK5i/ds1/OX1ez+ff+Mvf/8frK9fweym4IykG+Kjow08m72DZexd6dmYv4Nme09/l4sTfTdksAP6KHx1qH+1c8hwt4OROzAeDaRLq49Eap1zGaLVzH8Fd3q7/Hd11Wqo1Rqpj8QrWh+Pv2NneTyWy5eyVqCMZXYW+miGDs56Tch3x87McBfe058L5XKhrfI6vGqy2PoxCD2ifNs7Qmk82jnCP1EePQCbJS/t94ZB9C4u/+6v4qLlxB9AxeyR4P1m8nIM35E26W2F8q5Z3p2XQFierA3Z0xgxlxDWubQY6YTlx7Hfta7L0o/LsujtFEl/sZPF8Gyljge5FNu2SR8zuH18vknXr/l/e0CGdaB2AcSsnNxjq6x9su0OGPnFxyFvH5XmnyGmmcnGknr7EGrsPfK90zDrmjbfS+PfxdoUXDiSIrKOz9pfsqafkfUvk76ca6jVmgnvho4h7APZtm30upnLLTs9z5ztJSIiIqILI9sJ4JlP+Ovjz8CrNfwj9uyuluabz9jUk4Rs/vkz8PYydp9Cu7v4C37450fsYA27T/JVN+mRSGGRd+cEO5O2R0r56u1D7d2QdbQPB3AjO9QNHN9wAdzA9Tr8dx+5GKSdOchRHwmzztkFV9x2nyUddIqX3i7vPVDzg3JHaOp3ZoQUrc/M9i24oXepTV4+L7yDTHalLbOFczEIHTBW4y7QaVh26KWqeRzeRcN1eHVEsfXvaogcSNXWlzPh2DU6QHcMFY5VlrxCv7exf3dL5JVw9euQnWbyl10s7XedckDRe6em/RGNgfn7NoPHj3p5D3K8iFBSnqwN2dJYYy4kqXOZMdJJyo9jvWtdl6kfl2ih2ymS/mIniuGSMceD7Ipu26SPGdw+Pt+k69f8v72AaB3odDG2lZN7bJW1T7TdAWSLQ64+miF/aUyzyjKW1Ns4VN6+h3eiVzsRmTZ/tk4pdvcv9HV81v6SNf2MrH+Z9OWsoNQg13uhJX0g27aNXrfkPiij55m/vURERER0MeQ7owrgWv0LgEv46Wd9zpwtzfFEK/LtVzgO3g3sPybaeE8wPuPPm6HHRIs14D1B6E2+gznSR4hF3g25jT1to/v+xhHgbKAB/3FU2pWZjc5odtA87iAOkKE+EkGdGxtwMIKxLx7zWLVhq4Zm30F3rO2gZMwnIqVd3hXL9vfJlVsf/7FbnV0MMcRuZ6QdjMsoVx0syspnSZS7zM5YvY1nXWd+pX7WNgR3/xY8EHNxcR1eHXlsJy+fYwSg3zTvJjDWy9oB5UPtSFamvEKCkzPRu7O9NiQdTB57zxmE/tMrxP/djzr3zDs1/AObSXXKLKm8CtljLpRU5ypipEsqP8XYe0Zp4kUDeftxcSVvp1REEsOlxe1ji5L7Xa46WJSVzxkotH6VKLAOLGNstbdPvt2RXcl91KZQTO1yjSX1Ng4H+sUhGeaX8NuIruOz9pes6U32/rUASX1gEds2REREREQ5pJ8AfnsZ369fRUd7/vLbyVfeidlvhGmufcJfbCdxf76EV0Ea/y5h4yQxLuGnV/5dwpnUcfOuk/y+FmC+I6Jf9Z96AGGCN0dI3EEJ3u8Z7ITqj5xTwVWs/kFz72B53vpIaHX2d1bCV6tidmVv9OCddzAJcAeWq1NF+RRslxbn4vUxBVf2vmh572N6aGScQc46GMrKZwlUscyWSsY2eCcTQ+8QJg3X4dWRxjZ4R/XAaLdKPMBoUywv77GI4frWcf0Goo99DPMfAVn6QWAA9fZDuBihs/tCmxN6z56tTjnFl1ctM+Zy8XWuJka6+PITBH0m8dH+xfpxUaVup1RBFMNlxO1jvV1hpfa7nHUwlJXPGSmyfpXItQ4EShtbzfZJtzvyKbWPxsgfU5sCY0nKxSGp84sw1vFZ+0vW9HZm/1qM+D6wmG0bIiIiIqKs9DOtJv/E7dOXa6GJa/jbg0vzRzVL0uALfrj/CXh6JXSieA2dO2vAzm9+Pr/h/g7w6sEVPJk9WvorPPn+Cp7iE+7/oN8ZnC64Or7frBmPCRq2gru1/EciRXYi/PdmBe8unPSwpT3mddK7l3L33gS9rQY66OJZpp1QQX0kRHUOrpgOXcnqv7cxfPBu0tvyDyapmPdeSvKRtGuIVk17ZJV/l2R4R7Cc+lgE7wDtR9/HlE/OOhjKymeBLActK1tmZ8q7y2DefzO0wTiAQjYrvQ6vmCi2Se+o3r4FF0A/9gilpmhe2/e9+obu+NjeG3gH4vRHHU562Gp477nLtuyktrE3cIF+33iv2uw9ew09rv4Jplziy6uUJeZy8XWuJka6+PKtpH2maD8uqtTtlJJJY3jWROOBbDwvZ9tGMmZw+9hUVj5npND6VSLjOjCklLHV0j7RdkdepfbROPljapCOJcOW9qqZCXr3OhgFF5CmzZcattLfQRuz/LP2l6zprSz9azHi+0Dp2zaSZUJERERElGY6nSrJZ39HKWD+2Xz8r1xppvv/jaTBzgcjzevHv0fTbP5HvdbzsXz29/dVnHHXUQAiH6c7Tk7jDsJzVdeJfh9wVTiFNU0kD7tx11Fwuipam7T6SFjqY9TZM3Cj6aKxGSg3kkf446hw0uR8PGntMuYDKpqkvPp4ZUVjEpRvKzP8fVs9vU80P1kd9Dyqy6cIAPqkkOhyqaoPnVU7Y8u1/C7T2jBPU16dLwJb3AO2+OtxNdKc+3V4eZAztmn9NDw/Lg6BzHlZ0nrTo+sMZfnNhduQxNZ2AJF2xNVFhcq1LtqBm5jvPE20PVnLk7dBksYs14h5CXUOzUysk1UJ5cfFI76O8/Ky9GODrb3hvipsW1D/tO0UW36SeXHxMfuLmcYawzMGY/1nWdfHLDN93VLVto2yxZTbx5Y8qsunLDD6mz2e8+nzZRNb1/B60fLbjctfheJjrAPT1rWW2NriqxLK19sXnR6fr22+HgdbmYX7aEr+AVtMQzOtbdYljhXafKO+2rJLmz+TUDd9WRl5+h9rm33S/hKQpo9bFnqddXHfs/UJW2zivy/pA1rb0paZJZ3RPlu+oXbE19fSXloKsIwXJHdycqJPogwYv2IYv2IYv2IYv2KWKX4nJyfq3btf1Lt3v6gPHz6U/gnyrk2nU6WfFD6vDg4OcPv2bX0yEZWkVqvB21e52FalncuGca8OY0tEq4rrP1ok9jc6j4atGppHXYwP456KQ4vGZXLxcbwo5vT0FF9//bU+mYQYv2IYv2IYv2IYv2KWKX6np6dYW/sDAGB9/ao+u7Dp9D0gegQ0ERERERERERFdMEO86Ce9EoUWj8uEiIiIiMrBE8Dn0hCtWg21xI/2Th0iIiIiIiIiIt+k9wh9dxDz3nA6C1wmRERERFQWngA+l7axpxRU4mcP3F8gIiIiIiIiIpt6+xCKZxqXCpcJEREREZWFJ4CJiIiIiIiIiIiIiIiIiC6I2vv371Vw1ygA67+2acs478cff8SdO3dAREREREREREREtIxOTk70SURERLRC1tb+AABYX7+qzypsOn0PAKhNp1PvDOoFcHBwgNu3b+uTiagktVptdtHFRbYq7Vw2jHt1GFsiWlVc/9Eisb8REZEEx4tiTk9P8fXXX+uTSYjxK4bxK4bxK4bxK2aZ4nd6erqQE8B8BDQRERERERERERERERER0QXBE8BERERERERERERERERERBcETwATEREREREREREREREREV0QPAFMRERERERERERERERERHRB8AQwEREREREREREREREREdEFIT4BfNC5ivX14PMnPHmrp5ClwcGVUJqrWO+s6Snw9smf0vMhIiIiIiIiIiIiIiIiIqII0Qngg85V3Hn6CfvT95hO32O6/wUPvr2KzkG2NDi4gvU7a9jZ99NMP2Ln6ZXISeCDzlV8+wB4/DohnzwmPWzVaqiFPlu9iZ4Kw1Y0Ta01jJ/nf0JJrOls5QQmvS0v3VYPtlR6XuH6SBjfj6nzrB6x5QzRSskDonw8Rr0i6SRlSdKk12c+fwvxi2lelnVZDlvWvANpdZgpnI8sJgvh/96i5cvql95OX0q8ymbUq1aL7TdG2nAdLeui8GdBzTl/LHGz/R6T1i3GvJiY6+ls5QSqXocvhDC2wAS9LXvMYOv3ie3NkVfM7w1x6W0Za6zfq2nLM1jX1Fowc/TWa9Z4WeJq5DFsme3KWJ6kDfnTWGJeQp1nJDHSlVC+va0xdbSVN5Pcjw2JednnF9pOieQ3r2vsx29EXHzS+0tMDJeQsW72P/pyNNqpJyh528aoVySdpCxJmvT6FOp3s9nJ22lpdZgpnI8sJlUy6hgTW3s625i0mHWgNZ0leNZ0eh3DLOt+Sf3s66CEcmL6qCR/eUzl69Z4aWOJXobe5vj5Xlv19PNloC/zQFyM4tIj7jv2BgEZ0lvT2dqk8b6XtvyCScV/VzOW/q3nYW9T/P4EYr9jxiFTu4mIiIjowks/Afz2MnafAjv7H/FdMO27X/F4E3j60j9xK0mDr/Bkdw3Y+YjuLNEndPc/AU8ve3f5+vlsPv6IH64F+XzE/g7wdPcy8t4IPGzVUGt0cGOgoFTwGePu80ZoA9jbcWoedTGepVFQe9vRzBxtvlIIJxm2amj2XQyC+QMXo064nJBJD/c6gOs6+hx5fSRS6jzpbaHRAbrjYP4Abr8Z2gGboLfVBELxG7hAvxndSU3PJ8gruV3Dlq2s8M5NmfUJjPD8pWUZAZj0HqGvTwRmbak17XMhrkMZ+chicnZk9UtvZ5BXcryqE/ptK4WBO0KnYR6sT2xDvY3DcN/3P+OuA8DFrRw/8Ytu5dfhFZLFNki8i87IhesC/RcxK5ZIfP2+bzuYJclL+72Nu0Cnoa/TvDhHf3Ohsq0HwHTRcpRSUIdt1P25kzdH/v/6aApXqPa4Koy7R2ja4hGSp7y0NuRNY4+5KU+di8RIl6d8va3Ka6y9v8YR9eOy5NlOCaujfRhq78AF4ER/N5H1U/b+kiuGZyllPEgdzyvYtkkaM7h9bErPRxaTxZCuXyW/vahc60BL/z9sz0a+HGOrrH32db9tu0Mahzx9FKn5y2Oadd1qkTiWTNDbaqCD0PIa38Xze8F6Nnl+vf0QLkbo7EbzHe52MIKLh7NlbiNdx2ftL1nTw6hLXP8qk7wPzNn7d9y2TXIftFt8HIiIiIjonJtOpyr751/q8aZS2PlgmReT5vV/1CaU2nz8r2i68PT9/ypAqZ39aF6vH/+ugN/V49d6GdHP/v6+MgxcBUC5A31G1LjrKMBVSckGLhScrhrrMwLjrnIA5XSjKezfG6uu46Uddx1jvqQ+EvaywwbKtdQ5tXyjrbJ89L9FjLIsjDTZ6tONrVewnLpGft53HdUde2lgdLIsdSiej8GISXEA9El2ftlGU8KM+snamR6v4mzt1OvhT8zVBpP3vSracp7Y4r7q6/CyFIltYOD6fXTgWtsWHwdH6ashUV7GdPN3Epe/P1M5Kb8rezlRQRpvnNDLMn/ziXXSDVwjbb7yZG3InsaMeXl11tMJlVa+3tZ5n4msAyzlzWcl92NDQl5K2edH22YrI347xZafZF5sfEJi09hieMZs6z/7ej3M7Dcqqd0Bo/2yfPS/RYyyLIw02eqTp9/Nf99x22lZ6lA8H4MRk3LZ+pu9Tub61Z5OY/nt5loHJvT/eez1OfP4pdfbbJ90u8OeX1TxPmr7zlzWmM5nmcsnTfJYklCWUoL5luUp+A3ExsjyXSP/sNj+kjW9XhdL/9LYv6fsMbMst6x9ILFdmvi6xbN/x4yDPZ2y1pnOlm28ILmTkxN9EmXA+BXD+BXD+BXD+BWzTPE7OTlR7979ot69+0V9+PCh9E+Qd/odwBZvn1zBg1ef8fivn/RZM3FpNupfIn/j2hdsRCZ8xp+/iUwoYILeoz7gdHE/8cLbCV4+H8Hp3kdisjTjY4wA3LgevW6zseEAo2OMQ9MmvXvojOKuui2pPhKTNziy1Ll+/QaAPoyLkOOI8inWLj3vRKL6zF2/eReOZbp3RbaDuzevazOAevsQSh3Cugghr0NZ+Zx7wnamxusMzOosbIPOu0PBQTd5RbWCuA6vjjS2gSFe9AH31jawfQsu+nik3yFs4fV9Xb68As5Gw/+fF2e4D+3rg3obD10A/ReWO0myu95+hq4zQmd2141NSp0ykJW3GPOYJ5PVubwY6WTlJ/D7zKizK+gzxfpxVnm2U85EphgusZzjuUGUT7ExQ887kag+c3n6Xep2mrAOZeWz7KTrV4nC60AgfR2dcWwNj9nZtjtk8vTRLMqJaRLZWDI6Dm+FmpLm63cBD3c7GDldPLMu4BTGOj5rf8maPlmZv584sj6Q0q6KLSIORERERHQ+ZTsBfHAF6+tX8e2DS9HHNEvS/HwJr7SkYa9+ugR88xmbuIS//yNarZ9/ugTgEn76OTJZYIxj72h+yqN0/HTHu9r7Wsx3qmDUQSOUJvKoqsYGbA8C9Q5EHOFNkHTSw73OCO5gL+ZAT4b6SCTVeXyMERwY+wwxbZnRT5SI8snTrgl697yd1MSDBbnqE1K/ibuO+dit4Yt+/h25rHWIkzcfPSbLRq9f3naeoeDxabPHNudqw9keMFhuXIdXRxpb3/AF+rO+vo1bLjB6/jLhQJhn/vi8kJx5DVtN9OHg7s2gxl4bkg56NTac6LIrpI62d9QT2pMU5yYv8TylTnKC8ipmxjyNoM6lxkgnKD+FuM/k7Me5VbGdUhFxDM9a0niQazzPu22TZ8zg9nHufPSYnJHs61eJ4uvAssZWs30ZtzukquijEWXENEHqWLKN+10H6Ddj1glp8xFK8wi9YQ+P+oD7MO1Rw/Giyz9rf8ma3s7sX1US9IFKt23iLTYORERERHQeZTsB/N1HTKfvMZ1+xMaD/8H695b38krSxLn2G+7vAK8eXPHeCQzvhPKdp1q6jKQb4qOjDTybvVNl7F3p2Zi/g2Z7T3+XixN9N2SwA/oofHWof7VzyHC3g5E7iLxnzCatPhKpdc5liFYz/xXc6e3y3/lVq6FWa6AzcjFIfB9Osfp4/B27/qP5jvPE30E+ly9lLSMmVVr2+sXpoxk6OOs1Id8dOzPDXXRG57WfLcYqr8OrJoutHwP31qyvb3tHKBHz2j2Pf6I8egA2S17a7w2D6N1g/t1fxUXLiT+ACmB7z39/ZPJyDJ9YmPS2QnnXLO/OSyAsT9aG7GmMmEsI61xajHTC8uPY71rXZenHZVn0doqkv9jJYni2UseDXIpt26SPGdw+Lq6MmOQlXb/m/+0BGdaB2gUQs3Jyj62y9sm2O2DkFx+HvH1Umn+GmGYmG0vq7UOocRcORug0zLqmzffS+HexNgUXjqSIrOOz9pes6Wdk/cukL+caarVmwruhYwj7QLZtG71u5nIzSeOg552z3URERER07mU7ATzzCX99/Bl4tYZ/xJ7d1dJ88xmbepKQzT9/BgB8132P/Z1LePDtVayvX8X67me8fv0rNgs8GjrpkUhhzt2boYMo/s6k7ZFSvnr7EIPIVbp1tA8HcCM71A0c33AB3MD1OoBhC82+i0HamYMc9ZEw65xdcKVp91nSQad46e2qo30YPih3hKZ+Z0ZI0frMbN+CixGe+3vck5fPC+8gn5XSYlKRZa9fPBeD0AFjNe4CnYZlh16qmsfhXTRch1dHFFv/robIgVRtfTkTjl2jA3THUOFYZckr9Hsb+3e3tMKxq1+H7DSTv+xiab9r64G0ue37XTgxj2gMHIVuW/EeY+rlPXAjyUQk5cnakC2NNeZCkjqXGSOdpPw41rvWdZn6cYkWup0i6S92ohguGXM8yK7otk36mMHt46JKi0ku0vVr/t9eQLQOdLoY28rJPbbK2ifa7gCyxSFXH82QvzSmWWUZS+ptHCpv38M70audiEybP1unFLv7F/o6Pmt/yZp+Rta/TPpyVlBqgDybGpI+kG3bRq9bch/0SOOg552/3URERER0vuU8AQxcq39JfSyzLc3xRCvy7Vc41t4N/F33vX8X8XtM//kbrv18Ca/wBXXbI6cTNeA9QehNvoM5aY8QC0TeDbmNPW1j+/7GEeBsoAH/cVTaFZmNzmh20DzuIA6QoT4SQZ0bG3AwgrEvHvNYtWGrhmbfQXes7aBkzCcipV3eFcv298mVWx//sVudXQwxxG5npB2MyyhXHSwy5hMbkyURW7+M7VwK9TaedZ35lfpZ2xDc/VvwQMzFxXV4deSxnbx8jhGAftO8i8BYL2sHlA+1lVCmvEKCkzPRu7O9NiQdTB57zxmE/tMrxP/djzr3zDs1/AObSXXKLKm8CtljLpRU5ypipEsqP8XYe0Zp4kUDeftxcSVvp1REEsOlxe1ji5L7Xa46WGTMJzYmZ6DQ+lWiwDqwjLHV3j75dkd2JfdRm0Ixtcs1ltTbOBzoF4dkmG/5bWQVXcdn7S9Z05vs/WsBkvrAIrZtNGcWByIiIiI6V9JPAL+9jO/Xr6JzoE2efAUEd+VK0lz7hL9s+u/6Dfv5El6l3N178HIN2PmE7/QZqeq4eddJfl8LMN8R0a/6jzmAMDfBmyMk7qAE7/cMdkL1R87Nrt70D5p7B8vz1kdCq7O/sxK+WhWzK3ujB++8AyeAO7AcOBHlU7BdWpyL18cUXNn7ouW9j+mhkXEGOetgyJBPYkyWQGL9MrRzaWVsg3cyMfQOYdJwHV4daWyDd1QPjHarxAOMNsXy8h6LGK5vHddvIPrYxzD/EZClHwQGUG8/hIsROrsvtDmh9+zZ6pRTfHnVMmMuF1/namKkiy8/QdBnEh/tX6wfF1XqdkoVRDFcRtw+1tsVVmq/y1kHQ4Z8EmNyRoqsXyVyrQOB0sZWs33S7Y58Su2jMfLH1KbAWJJycUjq/CKMdXzW/pI1vZ3ZvxYjvg8sZttGd1ZxICIiIqJzZDqdquTPv9TjTaWw8yE07YPagVKbj/+VIc1UTff/qwCldvajaebf0/+eqtePf1fA7+rxa71e5md/f1+ZxqrrQAFQ7iA6Z+BCOd1x8IeWZqBcQCGYMO4qx+kqP7U/ybHmO+eXrX1PN+46Zpq0+kgI6zxwoQBHBaFQ465yEIpNzPd0knzS2zVQLlwVKcb/ThX18fIJlzfvL9FYe/WMtGXG/46lMpI6zBXLRxKTogDok+wGbrS+wvpJ2jkXH6+ibO00+4qy9N8MbYibvsJscV/pdXiJcsfWaEdYtE3WOIRlzcv4vdmWh/89Pa3/+0qsT2w5UbFp/PbA+B3HxdVS/9h1pby82PQh+dNUU+dMMdKVUL41fVyf0cvL0I8Nel46y3yzrhm2Uyz5SeaZZZqsaeJieMaM9Z9wPJCM57bv6ST5mP1K70vcPs6bjyQmZTL6mzWeat6uUF+0p9NYfrux30taByb+TrONrfbyzfbFr/u9ZRnU0Z5flJlG3kfN75pi08TENDrfvm6NMH7zYaHf/8CNiaFft7T5YUl10+ZZ2x+z/LP2l6zprXWx9q8o+/eUtU/o7VdJ34/tA3H926xrbN5hkmWSKW9Lu+lM2cYLkjs5OdEnUQaMXzGMXzGMXzGMXzHLFL+TkxP17t0v6t27X9SHDx9K/wR5C04A+ydXd5QC5p/Iid0MaYKTwLNP5KTxVE1f/0dthufjv2pfzyPmYz8B7PE2hP2dQusGuyVNZMs9tFM5++gb1pY09r26iLid8OT6SFjqY9TZ4x1AmX+isQl20myf6I5Scj6etHYZ842dqPLqY9tBCsq3lWkePNDLh5GfrA56HlnzkcekCCTupETrkLd+ye2Ux6sIWztjy7X8LtPaME9TXp0vAlvcA7b463E10pz7dXh5kDO2af00PD8uDoHMeVnSetPNdZr+mwu3IYmt7YD0QNq8XOuiDR0gtOU7TyM84BhTnrwNkjRmuUbMS6hzaGZinaxKKD8uHvF1nJeXpR8bbO0N91Vh24L6p22n2PKTzIuLj9lfzDTWGJ4xGOs/y7o+Zpnp65aqtm2ULabcPrbkkTUfeUzKAqO/2eM5nz6vR2ybw+tFy283Ln8Vio+xDkxb11pia8bXE1e+3r7o9Ph8bfP1ONjKLNxHU/IP2GIammltsy5xrNDmG/XVll3a/JmEuunLysjT/1jb7JP2l4A0fdyy0Ousi/uerU/YYhP/fUkf0NqWtsws6fT2xdVHms7abjpTsIwXJLdMB/DPI8avGMavGMavGMavmGWK36JOANem06nS7wo+rw4ODnD79m19MhGVpFarwdtXudhWpZ3LhnGvDmNLRKuK6z9aJPY3Oo+GrRqaR12MD9uJj16mxeEyufg4XhRzenqKr7/+Wp9MQoxfMYxfMYxfMYxfMcsUv9PTU6yt/QEAsL5+VZ9d2HT6HhC9A5iIiIiIiIiIiC6YIV70AfchTzQuDy4TIiIiIioHTwCfS0O0ajXUEj8tDPWvEREREREREREBmPQeoe8OsLetz6GzwmVCRERERGWpvX//XimlZo8esf1rm7aM83788Uc+ApqoQqvymKJVaeeyYdyrw9gS0ari+o8Wif2NiIgkOF4Us0yP8DyPGL9iGL9iGL9iGL9ilil+i3oENN8BTERiq7KTsirtXDaMe3UYWyJaVVz/0SKxvxERkQTHi2KW6QD+ecT4FcP4FcP4FcP4FbNM8eMJ4BwODg5w584dfTIRERERERERERHRUjg5OdEnERER0QrhCeCMeAcwUbVW5SrVVWnnsmHcq8PYEtGq4vqPFon9jYiIJDheFLNMd3CdR4xfMYxfMYxfMYxfMcsUv4XdAcx3ABOR1KrspKxKO5cN414dxpaIVhXXf7RI7G9ERCTB8aKYZTqAfx4xfsUwfsUwfsUwfsUsU/wWdgKYdwATkdSq7KSsSjuXDeNeHcaWiFYV13+0SOxvREQkwfGimGU6gH8eMX7FMH7FMH7FMH7FLFP8FnUC+Ct9BhERERERERERERERERERnU88AUxEREREREREREREREREdEHwBDARERERERERERERERER0QUhPgF80LmK9fXg8yc8eaunAHBwJZTmKtY7a3qK0vIhIiIiIiIiIiIiIiIiIqIo0Qngg85V3Hn6CfvT95hO32O6/wUPvr2KzkE40RWs31nDzr6fZvoRO0+vRE7elpVPFpPeFmq1mvHZ6k30pBi2zHS1Wg2tYTSdkaeeQJjGKG+rB71WknzSDdFKaROE9QEADFupdTHyCtJOetjS6mKrl/F9bb40DYQxlKQB0tueno9sWZx7/nKOtk3W9vQY+lKWRemGLdRqW7CsOmbS6y6LAc0ZMfU/q7UOr4ZRN/9ji23A+h1Lm6zpEn8/E/S2vHSW7LLlZ1v/CH6/c8l18fJqwTYr+I17MZznE/vRCrC201oJIrr4ZNsMkrEIkG03GXkFabn9LloW6VLGF2Pc0Met+PleG/T082UXN7Z737ONaeHxLJhkGUuD2ErzCFj7VDQPY7kEn7g+nvAdax0s7bF/P5xGXwaWT2uYe3mY+Qd56NMtn5zbFNZ0trrPpPVj30KXcXx9ren1ivv92Fwu/m9fT09EREREdF5Mp1OV+Hn9H7UJpXb2w9P/pR5vKoWdD9G/N/+jXoe++/rx7wr4XT1+XWI+ev1Cn/39faUbdx0FuGoQnagcQMHpqnFo8sA1p+m8/BzVnSUaKBdQcOclSNIMXGj18tOEypfkk26sug5U+Cte2bZpyfUJ8gL8j7UefpqUOOr05SRZFpI0khhK0kjaLsln4NriHv7OcgOgT7Lzf2Pztsr6oSSGkmVRlLWdAzdxWaXXXRaDVWaLu75u8Ceu0Dq8HEVjO//d6b8Bv01aPra8vWkx/X3gKsBVrmuPjy2/2PWnsf5J//1GpNQlmG+ZM4uHYysosQ7Z4ktEcrb13/KTbTNIxiLZdhO335PyybL9ntjfEscXyzIYd5Uz+zttvllvZe0jUfoynLOMZ5ZxLBjb7fG15BHTl1WQl7EdZatbPOt34rZtYtuTdfvF1hfyLI+0ZRwSW64K9Xt9vn2bIl+b4/qxZ9HL2P6bzBYH27KxlUVUlsTxglKdnJzokygDxq8Yxq8Yxq8Yxq+YZYrfycmJevfuF/Xu3S/qw4cPpX+CvNNPAFs/ZZ24LSsf7yM+AezNUI62Q5p+QMK+ExstQ5LG3xnR9oiy55OT0XZJfYK/HdUd29PP02Stn7mDnL4sJGkkMZSkkbRdlo/BWBbLTbyTYjsBozPaLoth+rIoztrOxAMtsrobjBisNlvcY2Noid3i1gn2vpc9n8UpGtv57y6SMpjpHVgNxcOet7mun80JDiLGnFy15mepZ3h6pJjE329UWl1ipysVu9y9WfF1yBpfIpKzrf/OJWOdJxmLwusXe/p5mrj1WhxznZ4+DkvS2NejecbY9LbL8jEYy2Iuqb8ljy/2usylzbeMJQn1DMS31VKeZRwLvt/Vy/a+YORh1DFBfN3ixX7HFouE9tiWjdl/7HkEjLba6hBhxitWlnKjM41tiqxtTu7HKeVr7GUns37HEtvEeljiYEyz5ElUpqTxgtIt0wH884jxK4bxK4bxK4bxK2aZ4reoE8CiR0Dr3j65ggevPuPxXz/5U77gh/ufgFd/xN9mj3New98eXAI2P+F/r82/G1ZWPrnU23joAqPOruVxVTEmb3AE4Mb1emRy/foNAH28GArToI7rNwAcvQk92miCl89HgHsL25DmUxZBfQDU24dQ6hDtaJVCvO843fuz70hMeo/Qh4Pu/SzfEpDEUJJG0nZhPnH0760kYQxTl8VZENadSsR1eHWM2AZte2j/3fnp0X8hWhbORkObMsSLPuDe2ga2b8FFH4+MR/DF02NcTLG65FNufIloVQjGItF2E7ff0/KJo38vmWx8GR2P9UkRSfPr7YdwMUJn16v4cLeDkdPFs9gAlOd6+xm6zgide/GP7k0d76pkbNtkZ26/JMu7PJKWcbqUGGfcpjDbnNaPU8qv2Pw3mVIPWxzqbTzrOkD/EXqTCXr3ZMuLiIiIiGiZZTsBfHAF6+tX8e2DS9h8/BE/hE/IfvcR09e/4vjOVayvX8X6+hUcP/43pv/8DcZ527LyKaix4QA4wpvwPsuog0bo/TCR98CMjzGCA2M/qLEBJ/i/JA2A7b0B3FEHjdoWepMhWrUGOiMXgz3/IIown1zGxxhpBy1S6yMyxvEIwPGu9r6f+HfyJO6cJS0LSRpJDCVpJHLlM9+xLPvY2bmg98NcMVwSeeuux4AyWdl1+AJEY+ut282DgHPWZaEZtprow8Hdm1p/H75AHy5ubQPANm65wOj5y4QDyJ7hbgej2fdKkrMuxZQTXyK64CzbDKljkQi337Plk3P7PXV82cb9rgP0mzGxT5uPUJpH6A17eNQH3Idt6IuoGnW0vTOs8M93miYv8TxlvKtS3rE0dvslVdblIVnGacrZpohtc1o/PqNlbG4T5otDPbiQodFAZ+Sg+yxpeRERERERLb9sJ4C/+4jp9D2m04/YePA/WP/+Mt76sw46V7H+7Rr+8vq9n+bf+Mvf/wfr61cwu5k3UFY+BXlXd89t7ykoNf+Muw5GnYb9wEVh29hTA++q4EYTfQDuYC/Tlff5DNFq9gHjoEV59RkdbeDZLI5jfyeqZb/KeLiLzsi/ijhEsiwkaZbPBL2t4ICXf5DucBV3LOP64SphDIpazXX4YkRi698hlV0fzdAB/iYGljuxJug96kfuVtv2jibipbHYtPz6yHzHWrIsdSlR7vgS0eqI22Yobyzi9nuSotvvsvGl3j6EGnfhYIROwzwJnzbfS+OfwGpmOUkdHV+9j9efMtnew8AF+s2YfuMLX8Qw6W1Fy93S7yDW62a2WUrfbown2X6Rybo8JMs4Ue5tCkmbZf0YC1nGKduEuePgX8gA2C9wISIiIiI6Z7KdAJ75hL8+/gy8WsM/3gJ4exm7T6HdzfsFP/zzI3awht0nccWUlU8+kzfJuwX19iEG+lWtJfF2hJrAYH7wo9+sodZK2l0uLriaV7+atcz6OHdvhvIOdqJsj1HzdyKFO8Npy0KS5uzV0T4MH/Q6QlO/82EFxPXDVcIYFLeK6/BFicS2fh2yQ6Y3EL2Z3cUgdIAf/SaM8Ph3ikROImzfgosRnutHE0P5KaWgxl2g07AcSMwpU11KlDu+RLQq4rYZyhyLuP2epOD2e5bxpd7GoT/GeScBtZOpafNDJ7CS7zYN08ZXpaDUAP5psEy273fhGI8FjjoK3XLpPabbK3NgLVCvm35SUi5tu3FOsP0ilmN5pC7jBLm3KQRtztCPq1/GKduEuePgX2wD2GNARERERHTO5D6jeq3+BcAl/PQzgJ8v4RWAjfoXLdVn/HkTePXTJW36XFn55DE+Hlk2+i1GxxgjeBzYCMZrecKPD5OkmfRwrzOC0x0jeEJbvX0I5V0y7e1oSPLJaNiqodl30B1rO1WS+hQR9xi14O4B6c4wQssiSdnLSyJnPt5V4cXeR3XexPbDnDFcChnrHhsDymTV1uGLFI1tAxtO8jvpxt5z9hDXrOAAf/9R9GTt5OVzjADvhMXsTg7vrqPU9WLwrjbLnSd5ZKtLzKMTY94nmax4fIno4ordZpCMRUVw+z02n6zb79nGF1+9jcNB3El4wfyE+lfKH5tHnXvmXZz+Sbmk8a5K4u3GkLjtl+xyLI/UZWxTfJsirs2ifnxWy9jYJswXB+9iG+/ksrcqzXDynYiIiIhoCaWfAH57Gd+vX0VHe/7y28lX3onZbwB88xmbAI4nenaX8NMrYPPPn8vLpywT7z08yY+PnODNEeY7Bv4OTfiKVsyuJvZ3JiVpxsfGO7wA7UCLJJ8MvINHgDuwnHCS1EfE39HSr+CPOYgyfNEHxO9v1JaFVUXLS6JoPontujgS+2HRGJ6lDHVPjAHJrdg6fKGM2NZx/Qa8d9jZjn4G6SN3j5m8xwSG3w0YvENyoN11pLwTGJkOeBaVoS5xJwwQP94lKye+RHTxJG4zSMYiEW6/584nsV2BDOOLLm1Zps0/I/X2Q++x5LsvtDmhd+LaxrsqGds2cub2ywJlXsblbFOYbZb24zNcxhE54uBPCx6jL7mbnYiIiIho6U2nU5X8+Zd6vKkUdj6Epn1QO1Bq8/G/ZtP2d5QCflePX2vfw3/Vfqn5xH/29/eVbtx1FOCqQXSicgAFp6vG4Wnhv2ffhXJDXx64UICjukFCPy9nNkGSZqBcvfzZ9+Z1Tc9HxtaOKFl95saq60DBluHA1cry89bTJrVFsiwkaYQxlKSZi297ej4D5erx9ONlL2v5ANAn2Q3caCxilo8uPYZh8cuiKGs7LW0Kk9RdEoNVZos71+HlKBRbpeZtFqa35h38ZoO0xngRFh077PnFjC+236ptWliGuijbslWhWNgzSalDtvgSkZxt/Xce2MawKNlYNJew3WSsA831nlIp45hkHJaksa1jLeVK0szFtz09n2zb70Z/M2IbForzwNWWpV/noOy0+WGJ402UfXxVs7pF2mjJN/b7frvNOAX11mOibSMk5Z3A+p24sVTcHrNuM5Y8DJI0qsxlnG2bQtRmaT9W6myWsVGH0DQ9rTUOZt28pE5CnImKMcYLyuTk5ESfRBkwfsUwfsUwfsUwfsUsU/xOTk7Uu3e/qHfvflEfPnwo/RPkLTgB7J9c3VEKmH/CJ22Dz+vHv0fSYPM/6nVF+dg+8SeAvR2Q8MfceZnvqMw/+o6FxztQMP/Ydv7T0wQ7JMnlpeeTxlZO8AnvzNjSResTF8vUdGawEw5OKeGykKTxSGKYlsZoU0yZefKxhGdpIXEnJdqHom239a/gE92pzhND72Nf/nlY2xk6kBVXv+S6y2Owqmxxj1ve5u9msesE+/I0y0vPZzFQKLZzenvi2mQ/OBc9kJY8DkTnx9V1Pr4krX+C32/87yxLXQK2OiXFLq0OKkN8iUgOlvXf8rONMcGH2+/SNEabYsrMk48lPEpZ+ltyzFLGOuvJqPj5M4LxJhA3Xhc+ARyKqzVWtu3qtPbGpAuL+058HWTtCW+/RFjyMEjS+Iz6x7VVkKfer6EvT5+kzVn6cWiiUb7eHqO9MenCYr9jXciyOMQu32Adm1AforxwLrdPlscyHcA/jxi/Yhi/Yhi/Yhi/YpYpfos6AVybTqdKvyv4vDo4OMDt27f1yURUklqtBm9f5WJblXYuG8a9OowtEa0qrv9okdjfiIhIguNFMaenp/j666/1ySTE+BXD+BXD+BXD+BWzTPE7PT3F2tofAADr61f12YVNp+8B0TuAiYiIiIiIiIiIiIiIiIjoXOAJ4HNriFathlrip4Wh/jUiIiIiIiIiIiIiIiIiurB4Avjc2saeUlCJnz1s618jIiIiIiIiIiIiIiIioguLJ4CJiIiIiIiIiIiIiIiIiC6I2vv371VwxygA67+2acs478cff8SdO3dAREREREREREREtIxOTk70SURERLRC1tb+AABYX7+qzypsOn0PAKhNp1PvDOoFcHBwgNu3b+uTiagktVptdtHFRbYq7Vw2jHt1GFsiWlVc/9Eisb8REZEEx4tiTk9P8fXXX+uTSYjxK4bxK4bxK4bxK2aZ4nd6erqQE8B8BDQRERERERERERERERER0QXBE8BERERERERERERERERERBcETwATEREREREREREREREREV0QPAFMRERERERERERERERERHRB8AQwEREREREREREREREREdEFIT4BfNC5ivX14PMnPHmrpwBwcCWU5irWO2t6ClE+b5/8KTUNERERERERERERERERERFFiU4AH3Su4s7TT9ifvsd0+h7T/S948O1VdA7Cia5g/c4advb9NNOP2Hl6JXISWJLPQecqvn0APH4dnyaLSW8LtVrN+Gz1JnpSDFtmulqthtYwms7IU08gTGOUt9WDXitJPumGaKW0CcL6AACGrdS6GHkFaSc9bGl1sdXL+L42X5oGwhhK0gDpbZfmY9Q9Jt255S/naLNk/VAaw7RlUbphC7XaFiyrjpn0ustiQHNGTP3Paq3Dq2HUzf/YYhuwfsfSJmu6xN/PBL0tL50lu2z52dY/gt/vXHJdvLxasM0KfuNeDOf5xH60AqzttFaCiC4+2TaDZCwCZNtNRl5BWm6/A7a6x6SLlzK+GOOGPm7Fz/faoKefL7u4sd37nm1MC49nwSTLWBrEVppHwNqnonkYyyX4xPXxhO9Y62Bpj/374TT6MrB8WsPcy8PMP8hDn2755NymsKaz1X0mrR/7FrqMzfpm6ttERERERBdU+gngt5ex+xTY2f+I74Jp3/2Kx5vA05fByd2v8GR3Ddj8FX+dJfqEvz7+DDy97N3BK8nHT7P5+CN+uBak+Yj9HeDp7mXkvxHYxUApqOAz7gKdhn3HwuliHE6rFPa257MnvS00OkB3HMwfwO03IztTkjTDVg3NfrheA7ijDhqhOknySTdBb6sJDObtGbhAv2kejEmrz2xnr9mff9HgpWkeaXEMglhv41CLr1IK464DwMWtUKzTloUkjSSGkjSStmfJJzY+F5asH2aJYdKyOAvpdZfFgGxWeR1eNWlsvd9dtD2hNlkPsEXz9rKO6e/DXXRGLlwX6L+wJYCR38AdodMwD/gVJqqLRB3tw1CsBi4AJxq/WefME18iurhk2wySsUi23ZSyfcrt9+T4SCWOLxP0throIFTG+C6e3wuWZfL8evshXIzQ2Y3mO9ztYAQXD9v1yPSyTN4c+f/ro2kd4E3DVg21Rgc3Qv3b609HaBrbH9p2ilJQh20kt0a6bRMnaftFNrbnWx5Jy1hW7jyfrNsUSW3WJPZjz6KXcWJ9iYiIiIhWWPoJ4Gu/4Z/T9+jOztrmJMnn50t4BWCj/iUy+Zs/fwZereEf+c8AR9XbOBx34Yw6uJfpyPEQu50RnO4zzPfZtnG/6wD9F/6OlCTNBG+OALi3MD9s4KcZHWMszkfC21kMH5/Yvt+FA+Dozew0haA+wKR3D52Rg+54jK4zSxjhpXExSN1pC/PaGi2/DJIYStJI2p4ln6zxuQgk/TBLDJOWxVmQ1F0SAxJZqXX4gsXEdv67Owy1BwC2sTfuwhEc+PUOhtoPFg5f9AH3FvZuueL4eL+fEZ6/zNIH0uWpS1FlxJeILhLJNoNkLJJtN+XbPuX2e1bJ48sYxyPAuXtzXka9jcNZmWnzg3o/ml8YNenhUR9wuvdLXkY6F1297BiT3haafe/EpX7+vN4+FJz4yyFm20YqafslXp7lkbaMZcrYpkhqc3I/PptlnFRfIiIiIqJVln4C2OLtkyt48OozHv/1kz/lC364/wl49Uf8bfao5jX87cElYPMT/je4m1dj5gMAn/Hnb0J/VqXexkMXGHV2jZ2WWJM3OAJw43p0l6V+/QaAPl4MhWlQx/UbAI7eRK7Of/k8dBBFlE9ZBPUJdtiUviMZ5n0nfqfWbtJ7hD4cdO9n+ZaAJIaSNJK2i/LJF5+VIYqhYFmcBWHdqURch1fHiG3Qtof2352f3nYQ0MbZaGhThvCOJW4D27fgoo9HGQ7Q6jEuplhd8ik3vkS0KgRjkWi7Kd/2Kbffs5KNL6Pj4NS9XdJ8/a7T4W4HI6eLZ7EBKM/19jN0nRE6szuWbVLGuyoZ2zbZmdsvyfIuj6RlnC4lxhm3Kcw2p/XjlPIrZtaXiIiIiGi1ZTsBfHAF6+tX8e2DS9HHNMN7VPP09a84vnMV6+tXsb5+BceP/43pP3+Dcf43Lp9vPmMTl/D3f0Sr9fNPlwBcwk8/RyYX1thwABwhcvPdqING6H0ykXfDjI8xggNjv6KxgdlF5ZI0ALb3/Ee01bbQmwzRqjW8K8uDy2SF+eQyPsZIO9iRWh8R76plHO9q7/tJekRnwk5i0rKQpJHEUJJGQpRPnvhcYHo/FMVwSeWtux4DymRl1+ELEI2tf0eK0Zg567LQDFtN9OHg7k2tvw9foD97hOg2brnA6PnLhAPInuAxipFHjxaVsy7FlBNfIrrgLNsMqWORSJ7tU26/J8fHInV8Ce4YbcbknTYf0btOh97dpu7D8u+2tKuj7Z1hhfbU47nJSzxPGe+qlHcsjd1+SZV1eUiWcZpytili25zWj89oGcfWl4iIiIhoxWU7AfzdR0yn7zGdfsTGg//B+vfz9/IedK5i/ds1/OX1ez/Nv/GXv/8P1tevYHZTcCAun2u/4f4O8OrBFe+9wfBOFt95Gv16Wbyru+e29/R31DgYdRr2AxeFbWNPDbyrghtN9AG4g72CV5ZLDNFq9gGni+gF++XVZ3S0gWezOI69q8EbtncNwX+HkH8VcYhkWUjSLKNM8bmw4vrhKmEMilrNdfhiRGLr3yGVXR/N0MHyJgaWO7Em6D3yHiUYxG7bO5oI88nOWn6Jj1HMI0tdSpQ7vkS0OuK2GcobizJtn3L7PTk+Btn4Um8fQo291xt0GuZJ5rT5Xhr/Ttymd7epbBszOr56H68/ZbK957+rOjku4YsYJr2taLnG+2H1upltltK3G+NJtl9ksi4PyTJOlHubQtJmWT/GQpaxpL5mOu+To28TEREREZ1T2U4Az3zCXx+H3sv79jJ2n0K7K/gLfvjnR+xgDbtP4orR8gHwXfc99ncu4cG3/p3Eu5/x+vWv2Kzg0dCTN8m7R/X2IQb6Va0l8XaEmsBgfvCj36yhlvI+nqKCq2O7z6JXH5dZn8h7i4Krwa2PPPV3IoU7w2nLQpJmGcjjc3HF9cNVwhgUt4rr8EWJxLZ+HbJDpjcQvZndxSB0gB/9Jozw+HeKRE4ibN+Ca3237zw/pRTUuAt0GpYDiTllqkuJcseXiFZF3DZDmWORfPuU2+/J8bHIMr7U2zj0xzjvJKB2MjVt/qxuaXebhmnjq1JQagAvl2y8d1XrjwWOmr/H2j/h6Zc5sBao1812kk8mbbtxTrD9IpZjeaQu4wS5tykEbc7Qj6tfxoL6Apa88/dtIiIiIqLzKO7MbKpr9S/zxzL/fAmvAGzUv2ipPuPPm8Crny5p0+ci+fi+6wZ3Eb/3HiH98yW8whfUjWdJFzM+Hll2fixGxxgjeBzYCMZrecKPD5OkmfRwrzOC0x0jeEJbvX0I5V0y7e28SPLJaNiqodl30B1rO1WS+hQR9zi24O4B6c4wQssiSdnLS6JIPnHxuaBi+2GRGJ61jHWPjQFlsmrr8EWKxraBDSf5nXRj73mDiGtWcIC//yh6snby8jlGgHfCQrszI/U9ffU2nnUd650neWSrS8yjE2PeJ5mseHyJ6OKK3WaQjEVFxG2fcvvdExcfi2zji6/exuEg4SRz2vy0+lfFH5tHnXvmXZz+ycmk8a5K4u3GkLjtl+xyLI/UZWxTfJsirs2ifnwGyziuvkREREREJDkB/PYyvl+/io72HOe3k6+8E7zfBO/uBY4nenaX8NMrYPPPn2X5xDh4uQbsfMJ3+owiJt57eJIfHznBmyPMd5D8HZrwFa2YXU3s70xK0oyPjXd4AdqBBEk+GXgHjwB3YDnhJKmPiL/DqV/BH3MQZfiiD4jf36gtC6uKlpeEKJ9s8bmIEvuhKIZLKkPdE2NAciu2Dl8oI7Z1XL8B7x12tiNrQfrI3VEm7zGB4XcDBu+QHGh3ZijvBEamA55FZahL3AkD5F2flxNfIrp4ErcZJGORSLbtU26/+2LiY8owvujSlmXa/DNSbz/0Hku++0KbE3onrm28q5KxbSNnbr8sUOZlXM42hdlmaT8+m2Vs1peIiIiIiAAA0+lUJX/+pR5vKoWdD6FpH9QOlNp8/K/ZtP0dpYDf1ePX2vfwX7Uvzsf7O5zm9ePftXzjP/v7+0o37joKcNUgOlE5gILTVePwtPDfs+9CuaEvD1wowFHdIKGflzObIEkzUK5e/ux787qm5yNja0eUrD5zY9V1oGDLcOBqZfl562mT2iJZFpI0whhK0szFt12UjzQ+SwqAPslu4EZjEbN8dKIYzsQvi6Ks7bS0KUxSd0kMVpkt7lyHl6NQbJWat1mY3pp38JsN0hrrw7DoutGeX8z60/ZbtU0Ly1AXZVu2KhQLeyYpdcgWXyKSs63/zgPbGBYlG4vmErabjHWgud5TKmUck4zDkjS2daylXEmaufi2i/KRxsfW34zvhoXyGbjasvTrHCzLtPlhieNNlH18VbO6mXGwbd9bvu+3G3oes3rrMdG2EZLyTmD9TtxYKm6PWbcZSx4GSRpV5jLOtk0harO0Hyt1Nss4U96Wvk10BozxgjI5OTnRJ1EGjF8xjF8xjF8xjF8xyxS/k5MT9e7dL+rdu1/Uhw8fSv8EeQtOAPsnV3eUAuaf8Mnf4OOdrA2l2/yPep01n9f/UZvhPGYnkNM/8SeAvR2Q8MfceZnvqMw/th2G4EDB/GPbeUhPE+yYJZeXnk8aWznBJ7zTaEsXrU9cLFPTmcFOODilhMtCksYjiWFaGqNNMWWm5aNseVnis6yQuJMS7UPRttv6V/CJHrxIi6ERv9nHvvzzsLYzdCArrn7JdZfHYFXZ4h63vM2fzWLXCfblaZaXns9ioFBs5/T2xLUp7qCbN93r78njQHR+XF3n68+k9U/w+43/nWWpS8BWp6TYpdVBZYgvEcnBsv5bfrYxJvhw+12axmhTTJlp+ShbXpb4KEt/S45ZylhnPVEXP39GMN4E4sZr60kyS77x35/H1Roq23Z1Wntj0oXFfSe+DrL2hLdfIix5GCRpfEb949oqyFPv19CXp0/S5iz9ODTRKF9vj9HemHRhkvompbP2baIzgHO5fbI8lukA/nnE+BXD+BXD+BXD+BWzTPFb1Ang2nQ6VfpdwefVwcEBbt++rU8mopLUajV4+yoX26q0c9kw7tVhbIloVXH9R4vE/kZERBIcL4o5PT3F119/rU8mIcavGMavGMavGMavmGWK3+npKdbW/gAAWF+/qs8ubDp9D4jeAUxEREREREREREREREREROcCTwCfW0O0ajXUEj8tDPWvEREREREREREREREREdGFVXv//r1SSs0ePWL71zZtGef9+OOPfAQ0UYVW5TFFq9LOZcO4V4exJaJVxfUfLRL7GxERSXC8KGaZHuF5HjF+xTB+xTB+xTB+xSxT/Bb1CGi+A5iIxFZlJ2VV2rlsGPfqMLZEtKq4/qNFYn8jIiIJjhfFLNMB/POI8SuG8SuG8SuG8StmmeLHE8A5HBwc4M6dO/pkIiIiIiIiIiIioqVwcnKiTyIiIqIVwhPAGfEOYKJqrcpVqqvSzmXDuFeHsSWiVcX1Hy0S+xsREUlwvChmme7gOo8Yv2IYv2IYv2IYv2KWKX4LuwOY7wAmIqlV2UlZlXYuG8a9OowtEa0qrv9okdjfiIhIguNFMct0AP88YvyKYfyKYfyKYfyKWab4LewEMO8AJiKpVdlJWZV2LhvGvTqMLRGtKq7/aJHY34iISILjRTHLdAD/PGL8imH8imH8imH8ilmm+C3qBPBX+gwiIiIiIiIiIiIiIiIiIjqfeAKYiIiIiIiIiIiIiIiIiOiC4AlgIiIiIiIiIiIiIiIiIqILQngCeA2d9atY1z+dNW/228v4Xp8X+nQOSkxDRERERERERERERERERERWshPAB2t4is94/Po9ptPQp/vJm3/tN/wzPH36HtPpR+wAwOav+Ot3JabJa9LDVq2GWuTTwtBIthVN09JTDNHS8jGShMzy2+phos/0JaVJr4+EvM7DlhYjW8JhK35eSFK7kFKWMU+vt3V5WtIJY2iUZ9RZFkNJWbCVF5Pu3PKXT7RZ5cZQ2g/LYtSrVkOttoWerXNDVr8L3w/KZP3Nr8o6vGKS2A5byf3dZ7Q3ps3WdLb8E8q15mEpy8vD7Cserz9sRQqYoLeVUq8Qaz1qWn8I1gfWetjq4JMsm0CWtDrLd231sbbVFnMiKoF8vBJtTwi2S5AypiGlLGOeXm/Lusaazra+sdTbKM+osyyGkrJgKy8mnc7L37Y+tqz/beNehWOI0fbgY8RyzvodPRa2dljNx9xoFvpYbPn4X7DWJ6UNREREREREq0B0Avjt5CsAX1C/ps+Jd9C54p00/r/fEPe1stKkGbZqqDU6uDFQUGr+GXeP0AztGE56W2h0gO44SDOA22+Gdmgn6G01gVA+AxfoN/Ud1iB5D/c6gOs6+py5hDTp9ZGQ1tnbyW4edTEOxUjtbRtpas1+aFqMhHbJygLgaPOVwixJvY1DbZ5SCuOuA8DFLT+dJIbDVg3NvovBLJ8B3FEHjVnfkMVQUpa47RdO+TEU9cPShfuJwsAdodPQD25J6req/SCf1V6HV0sa23Ren462N9Rm60Hr6O9p3AU6jZhlEZGnLKkJelsNdBD6bY7v4vm9tFhE26KUgjpso+7Pnbw58v/XRzO9gUDGZZMlrc7+3THuPm+ETihUGXMiMknHK8n2hGS7xJcwpsnK4vZ7FaoeQ9LGMKvIcvZjZuQrMNxFZ+TCdYH+i3Db6mgfhuozcAE40TEoEv8cbSAiIiIiIrroptOpSvvs7yiFnQ/G9NjP6/+oTSi1+fhf5ryy04Q++/v7SjfuOgpwVHesz9ENlAsoR0vofd9Vg8jUkHFXOZbvKTVWXcebPu46Ck5X6SmS0+Ssj4SlzpJ857H06g03LnVSu2RlDVwY30vnxWxeL0kM7W1JraMRQ0lZ5t/nDQB9kp0fn9guoorGUNIP87O1U6+HPzHmt5RcP2telBB3rsOLKhZbpdTATUybmJcf4/BvwR4HfR1uLzdrWV4eelkBfTnpf6eztyUqSNO11t0sM7GNmixpDQNXIW1dnVaGLeZES8S2/juXLOOVfP2TvF3iSRrTZGVx+93e3+K/byk/dtyrcgyx1S1efP8IlWlph83A9Zdj4lidnF+eNhARnTXbeEFyJycn+iTKgPErhvErhvErhvErZpnid3Jyot69+0W9e/eL+vDhQ+mfIG/BHcBfYXIMbB5fjryP9/sn8V89+Nsf8QqfcP+HL/qsmbLSJJvg5fMR4D5EO+3y38kbHAG4cT2asH79BoA+IhckC0x699AZuXiYUHBimpLrk8yLk9O9j6Tr2OvtQyh1mBrLxHYJy8pj0nuEPhx07we3D0hiWMf1GwCO3oSuWA/6zS15HUVlVdf2C0EUQ3k/XKRwndPrx34gx3V4dTLENlVKXvU2HroA+i9Ed4k6Gw19Uki5ZcUZHY/1SaW43n6GrjNCJ/GO4pQ2RmRJq5ug96gPOF0Ew6ZdShklxZyIspJtT6Rvl3gSxzRhWXlw+12u/DGkPF7MshriRR9wb20D27fgoo9H6c+MJiIiIiIiIqH4s7gzl/DTK+DVxm+h9/L+G3/5+/9gvbOmJwawhpdPAex8Qvwre8tKk2LyEs9HaQeTfeNjjODASNrYgO0haDPjY4z0AweTHu51RnAHe/EHCtLS5K2PhFHnMY5HAI53tfdE6Y+2FUhrV5ayRh00Qmms77aasRzsEMZwe89/ZFxtC73JEK1aA52Ri0HSY930GIrKytD2VZArhstluNvBKPTIQhn2AzGuw6uTJbapvD6dlFdjwwFwhDcJfXzYaqIPB3dvJh2xLqeseNu433WAfrOi32Qd7YcuMOpgN+5saZZlkyWtwV8X3bie8ojMqmNORCLGeFXi9kTamJalLG6/V6jkMaRE88dUZzB8gf5sO3obt1xg9PxlwsltIiIiIiIiykJwAvgTutP3mHY/haZ9wQ/3PwFPL+PJ29BkAG+fXPbe2fvXcPqostJIhQ/sT3pboR33Wr53Fc0M0Wqad88MdzsYuYP5+64sJGmqYa8zAIyONvBs9t6ksXeFeSPbe/2k7Uora3sv+g6ncdfBqBN+H6FmuIvOyL+CPLNt7KkBXIzQaTTRBxIOgCExhhJpbV8NxWJ4dvpohtYfXhPy3RHCfiDHdXh1SomtfwdVdtrvCYP0u9RylyVXbx9CjbtwMEKnIT3IH21L4ne29/z3UCb/3rMsmyxpdaknCRYQcyJKYx+vUNL2hHRMSyuL2+9J9HGihlrNq3cmFYwhZt0SxjAb/wKCbHcd+0+hCN2xve2dAcbLLGXPFGwDERERERHRBSQ4AZzkEn76OTrl558uAZuf8L/XotPDykojdRS6JcV7DJq38z5wI8kyC+5W6j5rz++eGbbQ7KdcfS5JUxFrnX3O3Zuhaf4V5lkeVZqhXVnLqrcPMYi9Klz6GEs776BIExjMD1b1mzXUWvbKJMVQImvbL6KiMTw7LgahA5tq3AU6DcuBtHTsB3Jch1enlNjWr0P24McbiD5lc/57Gvt33casdudyl5VRvY1D/zfunQhOPtBurBtSTmRv3+/CSXnUZZZlkyWtLvVx14uKORHFso5XvsLbExnGtKxlcfs9TB8nFJQaQLCaNpQ9hph1Sx7DAO1O70YH6I6hBH1oxr9TOXLyf/sWXIzwPNcZ4BxtICIiIiIiuuAKngDW+Y9t3viC+PO2ZaUR8A9aph7cRPCorxGMpDGPBhu2amj2HXTH0Z3L4Yu+cQVyozOa7SRv9SaiNFnrIxFX51gZH1UqalccaVmjY+ghmd098FA7oCOJoX/FutMdz+56qLcPobxL642TEbExlJQVR9r2C6KSGJ6VehvPuk6BuxVCVqwfiHAdXp0ssU3VwIaTnNfYe4Yw4podnCToP0q7mCJvWTGPJ455/+NMvY3DQdaD/AL+umPUuWfeoZRl2WRJa/BiGX2Hpk3emBNRGeLGq1gZtydEY1ocaVncfi9XWWNIEU4X49AJ10NR55ybvHyOEeCdtJ/1Pe+O6FFnN+WiKyIiIiIiIpJIPwH89jK+X7+KzoE2efIVgE+4GX5B79uvcAxg52bCY5vLSiMSvMvvkblzrPN3lsNXSwPB+4yid7V4BxEAd2AeiNEffRZckR7sJB+266I0WeojkVTn2cFd/ep8ycGPEFG7cpc1wZsjWA8weweuLO9hlcRQfxdYwHJQJzGGkrJyt/3iKB7Di4D9QI7r8OpkiG2qOq7fQHxekx4e9fW7p0zeox8T3msI5Csr7gA/hL87y3hQhnr7offo0t0X2pwsyyZLWl0dN+861cSciEqRNF6VtT0hGtNyl8Xt96qUM4acleDdzwOj76kqLroiIiIiIiJaVdPpVCV//qUebyqFnQ/GtM3H/4qm3f+vAn5Xj1/reVSQxvLZ399XprHqOlAAlDuwTHe6auxPGbhQgKO6wYRxVzmAcmYTlBp3HUteycZdJ1KOjS2NpD4SojoPXC3NQLmAgvVLfuys86Js7Uota9xVjvad2DakxCQ9hn7Z1ti7KigutvyQ9LIEbV9yAPRJdgM3GosyYzgj74dZ2drp1X/eJzxJyy+hfue8H1TFFneuw8tRNLa233SU34f134jfZj029t+TtNxsZSnbslCh9OHGD1zt+0GM9LrO2dsSFZvGXxfA6BcZlk2mtLq473oxM8ZKvQ0JMSdaFvb13/ITjVeZticStks0tjEttSxuvysV099ixwA/H7Ms2za05fsljCGxeSew9g+dpR3ReXrdAjGxTcgvTxuIiM6abbwguZOTE30SZcD4FcP4FcP4FcP4FbNM8Ts5OVHv3v2i3r37RX348KH0T5C34ASwf3J1Rylg/tnZN9O8fvx76onbstLYPvYTwL7QDvLsY9lx9Q4CzD/RnengAKjtY98hVcKd5Lg0yfWRkNc5OEgy+2g73sb82Sd+hzuuXUZekbLmBy3SytAP9Nikx9AWo3CetvnBJxrD9LLS2r7ckLiTEo1T3t9OWgyN+M0+yf0gC1s7Y8vN+Tsx0p2jflAVW9xnVnYdXo7CsbWlsbRHb68tjUo4WOtNDy2LhAO+0rICxm8u5uCzkU6PhcZIb/leXHtVqB22uljjHlefLGk1tjbYYpk15kTLAEnrv6UlH6+M32/O7ZKwuDHNyIvb7wZY+lv8GFDwBHAJY4jRrph0YXH9I8JWtt/WtOVvnW+JSyBPG4iIzhos4wXJLdMB/POI8SuG8SuG8SuG8StmmeK3qBPAtel0qvS7gs+rg4MD3L59W59MRCWp1Wrw9lUutlVp57Jh3KvD2BLRquL6jxaJ/Y2IiCQ4XhRzenqKr7/+Wp9MQoxfMYxfMYxfMYxfMcsUv9PTU6yt/QEAsL5+VZ9d2HT6HhC9A5iIiIiIiIiIiIiIiIiIiM4FngA+t4Zo1WqoJX5aGOpfIyIiIiIiIiIiIiIiIqILq/b+/XullJo9esT2r23aMs778ccf+QhoogqtymOKVqWdy4Zxrw5jS0Srius/WiT2NyIikuB4UcwyPcLzPGL8imH8imH8imH8ilmm+C3qEdB8BzARia3KTsqqtHPZMO7VYWyJaFVx/UeLxP5GREQSHC+KWaYD+OcR41cM41cM41cM41fMMsWPJ4BzODg4wJ07d/TJREREREREREREREvh5OREn0REREQrhCeAM+IdwETVWpWrVFelncuGca8OY0tEq4rrP1ok9jciIpLgeFHMMt3BdR4xfsUwfsUwfsUwfsUsU/wWdgcw3wFMRFKrspOyKu1cNox7dRhbIlpVXP/RIrG/ERGRBMeLYpbpAP55xPgVw/gVw/gVw/gVs0zxW9gJYN4BTERSq7KTsirtXDaMe3UYWyJaVVz/0SKxvxERkQTHi2KW6QD+ecT4FcP4FcP4FcP4FbNM8VvUCeCv9BlERERERERERERERERERHQ+8QQwEREREREREREREREREdEFwRPAREREREREREREREREREQXhPAE8Bo661exrn86a97st5fxvT4v9OkczHN6++RPoXl/wpO383melLKIiIiIiIiIiIiIiIiIiMhKdgL4YA1P8RmPX7/HdBr6dD9586/9hn+Gp0/fYzr9iB0A2PwVf/3Oz6ZzFd8+wDyf/S948G30BHFqWXlNetiq1VCLfFoYGsm2omlaeoohWlo+RpKQWX5bPUz0mb6kNOn1kUiv87Clx8aeLq0+0nysaUOJjHkx+STWx7rMbXmlx0eWJqU+PqNtluV+7vmxjza/vBgCAIat5PklM+pVq6FW20IvbuEJ6mf0hYS0K8/6e16VdXjFJLEdtpL7u89ob0ybrels+SeUa83DUpaXh9lXPF5/2IoUMEFvK6VeIdZ61LT+EKwPrPWw1cEnWTaBLGl1lu/a6mNtqy3mRFSC9PHK2I6ISWf8drUE0nysaUOJjHkx+STWx7I+sueVHh9ZmpT6+Iy2Wcb8OF7+tvWxZf1vG/cqHEOMtgvaZ/+OOVZK083Nx1/LIpiztCvc/mHLUn8/hkE6e92C7+nbAZZPYgWJiIiIiIiWg+gE8NvJVwC+oH5NnxPvoHPFO5H7f7/hGry7hHefApuPP+KHIJ/vPmJ/B3i6exnBjcB5ykozbNVQa3RwY6Cg1Pwz7h6hGdo5nPS20OgA3XGQZgC33wzt4E3Q22oCoXwGLtBvxuykTnq41wFc19HnzCWkSa+PzLBlq7Nl59vpYhyKj1IKe9vz2eL6pOQT7Nw3j7R00USp+aTWp97GofZ9pRTGXQeAi1t+XpL4SNKk1sfvi82+i8GsPgO4ow4a+kGKC0f225HEcHZwqNkPTVuU8LJTGLgjdBr6b0lSP+FvgACuwysljW06r09H2xtqs/WgdfT3NO4CnUbMsojIU5bUBL2tBjoI/TbHd/H8Xlosom1RSkEdtlH3507eHPn/66OZ3kAg47LJklZn/+4Yd583QgfUq4w5EdlItj2BEraXAyn5iLddUvJJrQ+33w1VjyFpY5idZJvYTJc41g930Rm5cF2g/8KWIK5d+pilmfSw1ewD7gCH7XCr4tpdR/swNG3gAnCi45/e74mIiIiIiJbRdDpVaZ/9HaWw88GYHvt5/R+1CaU2H/9rPm3/vwpQamc/mvb1498V8Lt6/DpnWaHP/v6+0o27jgIc1R3rc3QD5QLK0RJ633fVIDI1ZNxVjuV7So1V1/Gmj7uOgtNVeorkNDnrI2Gp88BFTB0Dsvqk52N+xyY9H1l9TN734MansMXHYKSR1Mdb3nrZ6XVeHgD0SXZ+fJLCnC+G4d+0PZ5lsLVTr4c/0egrkvpZ86KEuHMdXlSx2CqlBm5i2sS8/BiHfwv2OFjWz5Zys5bl5aGXFdCXk/53OntbooI0XWvdzTIT26jJktYwcBXS1tVpZdhiTrREbOu/c8kyXpW1vZyej/kdm/R8ZPUxWcYHnSU+BiONpD727bm4Otv6W1xaa/mx416VY4itbvGs3zFiG5MuYVkOXH963LgtHLOi/dAvT+uX9rrFsCwTIqKibOMFyZ2cnOiTKAPGrxjGrxjGrxjGr5hlit/JyYl69+4X9e7dL+rDhw+lf4K8BXcAf4XJMbB5fDnyTt7vn8R/9eBvf8QrfML9H75ocz7jz99okyKyl5VsgpfPR4D7EJGLfW0mb3AE4Mb1aML69RsA+oi5CDnWpHcPnZGLhwkFJ6YpuT42et6JSquPt0yc7n0Uum46Z30mvUfow0H3fnrpet42szSi+tRx/QaAozehq+6DPnqrWDwuAlEMgXr7EEodpv+mFyhc5/T6lfQbWAlch1cnQ2xTpeRVb+OhC6D/QnSXqLPR0CeFlFtWnNHxWJ9UiuvtZ+g6I3QS7yhOaWNElrS6CXqP+oDTRfKQmFJGSTEnIhl9XElU2lhU0rZLzvpw+91T/hhSPj2WccyxfogXfcC9tQ1s34KLPh5F7uiVjllh3pNf+nAxSL2jmYiIiIiI6OIRnFm9hJ9eAa82fgu9k/ff+Mvf/wfrnTU9MYA1vHwKYOcT/Ff/er75jE1cwt//ES3y558ueWX8jBxlpZi8xPORbQfTYnyMERwYSRsbMB/sGTI+xkjf2Z30cK8zgjvYiz8okJYmb31STdC718HItvM86qAR8y6lTPVJygdjHI8AHO9q726yPDIsKZ8s9ZmRHBBJiM+MJY2wPtt7/iPjalvoTYZo1RrojFwMVvExYvpvRxjDZTLc7WAUehyhTIbfwKrjOrw6WWKbyuvTSXk1NhwAR3iT0MeHrSb6cHD3ZuwKurSy4m3jftcB+s2KfpN1tB+6wKiD3ZgTHZmWTZa0Bn9ddON6ykHxqmNOROks256BsraXk/LJsu2SlE+W+sxw+32u5DGkRNJt4tixfvgC/dn3t3HLBUbPX4ZOdEvHrLmXLX85qZhtNSIiIiIiogtOcAL4E7rT95h2P4WmfcEP9z8BTy/jSfDyXt/bJ5e9d//+NZwewLXfcH8HePXgyvw7B1dw52k4UbaypMIH9ie9rdBBixpqxjuQshii1TSvRB7udjByB9p7s6Ikacrjv5O0VkMtOGChXQW9vRd9/9G462DUSXiXUgxpPqOjDTwLvbep64zQaczfISjNJ5PhLjoj/8ryiPT4yNJIbGNPDeBihE6jiT4QfwLpQrP/dpZfH83Q+sNrQr67YdJ+AzTHdXh1SomtfwdVdtrvCYOUu+eLlCVXbx9CjbtwMEKnUbOf4DBE25L4ne09/z2Uyb/3LMsmS1pd6kmCBcSciGzStz3L2l6W5pO27SLNJ5MLs/2ujxM11GpeXplUMIaYdUsYw2ak28SSsd6/uzd0R/W2dwYYL7V6pI5ZgVEHnT4AZwPx38jTbiIiIiIiovNDcAI4SXDn7tzPP10CNj/hf69FpwPAd9332N+5hAff+o933v2M169/xWbqo6FhLUvqKHRLivd4Vu+gxMCNJMssuIK5+yx0IGHYQrOfckW4JE2p6mgfhg/GHKGpX5GvqbcPMTCuvM4uLh/n7s3QwRf/avaER7/F5SOX9NgwSXwkadJ5B2CawGB+YKzfrKHWimn4BWX97ZwLLgahA5tq3AU6DcuBtHRZfwOrjOvw6pQS2/p13NCnWd1A9MmQ89/T2L/rNnVVmLusjOptHPq/ce9EcPKBdmPdYBzcjtq+34VjPN4yKsuyyZJWl/q460XFnIg02bc9i28ve+LyybrtEpeP3EXaftfHCQWlBhCspg1ljyFm3ZLHMI90m1gw1vt3LUdO8m/fgosRnmtngFPHrIDTxXjchTPqoGEUGMjTbiIiIiIiovOj4Algnf/4540vsJz/BfyTwLPHO//zN1z7+RJe4QvqcV8owj9oKdpRbGzAwQhG0phHgw1bNTT7Drrj6I7i8EXfuJq40RnNHoe21ZuI0mStTxb19jN0HWDU2U05oA1gdIwxssfHEOQTJ/HRbyF56xPcPfAw/YSjJD5GGkl9/EfGOt3x7K7BevsQyruM3zwYckHF/XZEMVw29TaedR3rHQqZSX8Dq4Tr8OpkiW2qBjac5LzG3jOEY+/CCU4S9B/pB451ecuKeTxxzPsfZ+ptHA6ST3Dk4q87Rp175t1GWZZNlrQGL5bR91ra5I05EZXJ2PZMknd7Wcft9+Xcfi9rDCmTYJs4bqyfvHyOEeCdVJ9tW3l3R8+Xp3TMCgnG8LNaTkRERERERGcs/QTw28v4fv0qOgfa5MlXAD7hZvhFv2+/wjGAnZva458THLxcm78vOEtZIsG7/B6ZO8c6f2c5fLU0AEzeHBl3tXgnDgB3YF4lrD/6bHa1s9PFWCkctuuiNFnqk1viwdoJ3hyF0uSuj5ZPcCBZvxMg7sDPTLH6eCds0t9LFZEYH1+W+oyPzXeNIsPBswsg6bcjiuGFkPc3sIq4Dq9OhtimquP6DcTnNenhUV+/c8zkPe4x4b2GQL6y4g7wQ/i7q2gdXW8/9B4nuvtCm5Nl2WRJq6vj5l2nmpgTUXUSt0+LbS/Pcft92bffyxlDFs8c64N3PA+MbSsVuQBLOmZpZo/M5uOdiYiIiIhoBU2nU5X8+Zd6vKkUdj4Y0zYf/yuadv+/CvhdPX6t5zFV0+kHtYNoPq8f/66lz1CW5bO/v69MY9V1oAAod2CZ7nTV2J8ycKEAR3WDCeOucgDlzCYoNe46lrySjbtOpBwbWxpJfdINlAtXRao7cBXC+Yy7ytHKtrUztT7CfILy59MGygUUggnCfFLrE4ibrpQsPqI0kvr47bQuZy3/JQVAn2Q3cKOxiFmGuvQYhvm/4aQMc7K106u/vpy0vhuRUL+038CKssWd6/ByFI2t7Tcd5fdh/Tfit1mPjf33JC03W1nKtixUKH10YNG+H8RIr+ucvS1RsWn8dYE+nmRaNpnS6uK+68XMGL/0NiTEnGhZ2Nd/y06w7VnW9rIwn9RtF2E+qfUJxE1XShYfURpJfbJtv9v6W+wY4OcdaaNl3Iv9fgljSGzeCezfMbdl7em0Ohj9KkzPM65d0TFr4OrLyxzL7XWLYVkmRERF2cYLkjs5OdEnUQaMXzGMXzGMXzGMXzHLFL+TkxP17t0v6t27X9SHDx9K/wR5C04A+ydXd5QC5p+dfTONeUJX+7z+j9oM5QH8V+3raYRl2T72E8C+0A7y7GM5YOntzM8/0Z3p4ACo7RO/U2g7MaCLS5NcH5ng4Ev4Yz0YEElj3yFOro88H6NOkQrJ80muTziN/fvKVhcjPrI0SlQfWx+Kr9uyQeJOSrRteX87aTG0LYuy42hrZ2y5WkeITafVz0hn61Arxhb3mRVeh5ehcGxtaSzt0dtrS6MSDrx600PLIuGgq7SsgPGbi1mPG+n0WGiM9JbvxbVXhdphq4s17nH1yZJWY2uDLZZZY060DJC0/ltitt8lt9/njLoY8ZGlUaL62LYf7HWDpb/FjwEFTwCXMIbYYmRLFxb7Hes2sVnv8Fiftpxt823lh2M4cC311y76suUR227LMiEiKgqW8YLklukA/nnE+BXD+BXD+BXD+BWzTPFb1Ang2nQ6VfpdwefVwcEBbt++rU8mopLUajV4+yoX26q0c9kw7tVhbIloVXH9R4vE/kZERBIcL4o5PT3F119/rU8mIcavGMavGMavGMavmGWK3+npKdbW/gAAWF+/qs8ubDp9D4jeAUxEREREREREREREREREROcCTwCfW0O0ajXUEj8tDPWvEREREREREREREREREdGFVXv//r1SSs0ePWL71zZtGef9+OOPfAQ0UYVW5TFFq9LOZcO4V4exJaJVxfUfLRL7GxERSXC8KGaZHuF5HjF+xTB+xTB+xTB+xSxT/Bb1CGi+A5iIxFZlJ2VV2rlsGPfqMLZEtKq4/qNFYn8jIiIJjhfFLNMB/POI8SuG8SuG8SuG8StmmeLHE8A5HBwc4M6dO/pkIiIiIiIiIiIioqVwcnKiTyIiIqIVwhPAGfEOYKJqrcpVqqvSzmXDuFeHsSWiVcX1Hy0S+xsREUlwvChmme7gOo8Yv2IYv2IYv2IYv2KWKX4LuwOY7wAmIqlV2UlZlXYuG8a9OowtEa0qrv9okdjfiIhIguNFMct0AP88YvyKYfyKYfyKYfyKWab4LewEMO8AJiKpVdlJWZV2LhvGvTqMLRGtKq7/aJHY34iISILjRTHLdAD/PGL8imH8imH8imH8ilmm+C3qBPBX+gwiIiIiIiIiIiIiIiIiIjqfeAKYiIiIiIiIiIiIiIiIiOiC4AlgIiIiIiIiIiIiIiIiIqILQn4C+OAK1tevzj+dNT1FxEHnKta/v4y3xgxBPpI0REREREREREREREREREQUITsBfHAF67uf8Xr6HtPpe0xf/4rNp1fiT8weXMGdp/pEP587a9jZ9/OZfsSOno8kTQaT3hZqtRaG+gwM0arVsNWb6DMwbNVQq4U+rfC3ve+F50dmhw1blu+bvDrWUNvqQa/NbJ61LlLyOse2fdLDlpZHXH56HrYYw5Iub5yT85HFUJIGEC5TQZq0Op97fn+JNku2TEtdFiXx6rQFoyv77Zz38fQ2Gss+Jh15uA6vTpbYGu0IPuE2B/ES5jlsWWLm5xGkk5dr+X2mmqC3ldAHMrZnrtx842JgL1tji02V5dvKm0mJi8ZabuiL1v4z45fV6s3KjP3EVSa2LfN2xH78PK1tiIsdkUE+XsWOe9x+90jGc0GatDrHMepp+65tnWObFpY2fyZ5/WutnyBf+/dCfcdWP9u0sJT5cWWGxwN7mvg8TcnxMscBPe/4+V7d9PTz36r5u9PzsnzSfjuWNFnShXnfkW0/WJdlxm2QGeu6LJqHtT21uG2F5YrrjC1mIZniT0REREQkOwG8hs6dNWz+5ROuBZOu/Yb/e/wZeLqGg2jiWXrTV3iyuwZs/oq/fhdM+4S/Pv4MPL2MJ2+laark7Qg0j7oYKwUVfPa2ZymGrSYwmM8buEC/qW+k+zsUzX54ot2kh3sdwHUdfQ4mvS00OkB3HJQ3gNtvyncgAL8utjrrO7Qpba+3cRie7n/GXQeAi1t+smGrhmbfxSBIM3Ax6jS0nZGUssqqszCGkjSyZSpPk1Tni0m2TMtbFuWqtx/CxQid3ehvb7jbwQguHrbr4jYCABxt+SuFC98FFiL993X+1uHLJLRuDz6HbdT9uZM3R/7/+mjmaeOkh61mH3AHOGwHuSK13NyGu+iMXLgu0H9h1jd3eyrJV4vBuAt0GjEHNZOdWfkpcbGKrCv9349f5vYtFxh1oK2WPZOXeD4C3FtttA9D9R64AJzQbzLP+FvPmGcJsaMVJN2mSBn3uP0uGM/laZLqnCphfVY50fo3uq7yVlX6srOwbNNGx/AqSLYLcrYHafGaoLfVQAehdo/v4vm9YFkmz5ftU4RlGXO8fhr9Xah5f7OdOFxwv8yzDTJs1VBrdHAjtG7xlukRmkZdJX0DFy6uRERERERx0k8AH6zhKT7jL//7JTL52g//D9PpR8zO0/rePrmMp5u/4vGONuMcmPTuoTNyMbDuJHi296Inarbvd+FghOcv55vzXj4OuuMxuuY5gZAJevc6QPcZ7m/o84bY7YzgdJ9hvh+4jftdB+i/MHcyYnk7N2adgaM3ep2T227y6gj3FrYBYNLDoz7gdO97fwPA9h4GLjB6/jJ0VXZaWWXVWRJDSRrZMpWnSarzRSVZpuUti/IF9Xg0P1Fo9HdJG6lKkt/X+VuHnzcuuvpvRWSIVqODkdPFOMsB9QKGL/qAewt7t9yEZZK9PVXlG1Fv43DchTPq4F6uDBZfviwuSfzfz+g5Xk4AbN+CC9vBeWDy8jlGoZNbSyVH7GgVybYpJOOeidvvYfI0SXXOSlufVSzP+tc7UWlfx55HWdqTHK8xjkeAc/fmvC/U2zic9Y20+ZJ9inzmffkw9LsAgG3sjbtwUk+6LqpfyrdBJr0tNPveiVl987DePow5uVuu8xNXIiIiIiJT6gngt5OvAHxB/doaOmnv5X17Gf/fA+Dx//1m2RD/gh/ufwJe/RF/m902vIa/PbgEbH7C/16TpqnKBC+fj3LveN24Pm9xvX0IpfQdBFNwMMG80hfA5A2OtHwBoH79BoA+BPuuGeRr+6T3CH046N73vzU+xshS58aGA4yOMfa+lasskyAfSQwlaYTLND2NoM6rrMRlUQX9iv3hrney6tmiK0Ixiv2+zvc6fLlcbz9D1xmhM7sbJo1311gfZR5cTzOEd3x32z+R2MejmKOQ2dpTVb4W9TYeusCosys6mK9bbPnyuCTxfj+BbdzyjuZr5XvrgtnJrWWUKXZEcfKNe9x+j0pPI6hzDtH1WZWKrX+djYY+6VxLb48sXqNj75cRJ2l+NfsUwdj30N6X/XHHHDOjFtUvZdsgKW1aiJQ6LFlciYiIiIh0qSeAPWu4s34Zf34dvJf333h8rL+X9ys8+f/+CDz+iB/iTtR+9xHT17/i+E5wIvkKjh//G9N//jZ/vLQkTSW8q3VxvKu9X0Z/NGiYd/fXyOkiOIYiNunhXmcEd7BnP5gwPsYIDox91MYGYi5OlzMO9ORru7EzFFM3b4fnCN7F/3nKyllnSQwlaUojqPMq0ZfpQpdFHqEr9ofelfruw5STVXobA6MOGqE+wPc1lSHP7+ucrsOXXh1t7+yW/fG8mpethndnlYqJZRWGL9Cf3SHqnUgM3+kWlaE9VeUbo7HhhMbXrBZYfqa4xJs/OtKz7Z0Bjl5QMXv888J6Uy7i2BEFjG2KfOMet9+zEtQ5B319Vpmc699hq4k+HNy9mbile26I25Mar2B/oBnTB9LmI98+RSr/zmPjRzEnGXcW1i8l2yD+eJ7Upuqdt7gSEREREUUJTwADm5ETu/6duqH38r59cgUP8Cv+74foo6LDDjpXsf7tGv4SOpH8l7//D9bXr8zeJSxJk10fzcgOew21WhO2Nz2NjjbwbPa+lrF3ZWoj/F4X/z1RtRpqNf+gdY47loa7HYzcgfEoo+oN0Wr2AcsJj/S2hwx34T09LpRJ/SbuOkD/UfhK3gl6j8xIZyqrrDovifNY5/LFL9NlVg+uVm9KThra27i9F353lPcePvM9exTFdXh15LE108Yd2MTs8aH9Zsq6bdRBpw/A2UD8obUM5Yr441LoDlHvfbIJj+YTtaeqfOMVvqNkIeXniIuNf9FF5MTV9n14T3wN/cJfPhesn8+eLHZEAfs2BUTjXgi333Mrtc629Vklsqx/o2NtE4OUO6N92kWNxcdoCcl2QZ72yOJVbx9Cjb1XiHQaZvlp8700WfYpBPy74gsR90s9/rWEbccEwm2Q8IW0k95WtFzjvbp63czYZ7LQuErpbcwZfyIiIiJaCcITwOY7gD2X8NPP0Uc/x96l+/Yydp9aTiT/8yN2sIbdJ1/J0uTiYhA64eJ9BnD1ZNDe1xNcmRq5u8R7v9X85M0Rmlnv4Bu20Oy7GJzBmYPg6ufuM/OER3rbA/7OsbGzWkf7cAA3ciCggeMbLoAbCN8EKS+rrDovj/NY57IlLdPlFiyv9Cv1pW2stw+N9+yRjuvw6shja6ZNPpDqvfvR/ujEGaeLsf8+1Ebs+9OylZvKdofo9i242rugdantqSrfBGXcUVJ5+TnjAmgnFhodoDuGivzu6rh5N/zOT/9RrZH1wHISxY7Il7RNkT7uBbj9XkThOqeuzyqQaf07H2vH/h2sscNymNPFuMwxWkSyXZCjPVniVW/jUKnQiV7tJGba/Az7FCL165BdVhT9Tefrl3r8VcK2YzLJNkj4HeLeI9u9MgfWAvW62fpGBlXEddjSTt7qfSON3sb88SciIiKiiy/1jOq1uu3Eb9Tbf6zhFS7hwbfzdwTfeQrg1R/x7fqfvLuEf76EVwA2jPw+48+bwKufLsnSLFrKo8S8q3ezvcdt+KJvXLnZ6IxmOwpbvYlf7gjG64PiHnkmMGzV0Ow76I6FO0JxbQ/uHrDurG5jT9shub9xlHJ3V3xZheosiaEkTdVi2n5RxS7TZVgWYsn1iW1jktl79qhUKb+v87QOP3fqbTzrOhh17iXffVFv49C7BST94GwJJi+fYwSg3wwffPPunEjsByntqSrfJOPjkXnQMauKy88dF5gnFg4tK9T6zbtwZu8FfYnnI8EjPpeAJHZEyLNNETfucfu9XDFtjyVYn5Ut7/o3uDgxelf4+SVtT654BdswcRcDpM0vrb824L22W/9RzI29ZxlHf9Nn0C8jkrZB/JOvSW2qXgVx3d6LrGvVIl+BQkREREQrJ/UEML75jE1cwt//YUv6CTe/A6798P/8xzXPP/s7ADZ/xevp//Pu5v3mMzYBHE/0fC7hp1fA5p8/y9JUxt+41+/Ckx5I0Df6E+iPgFXBlcn+jsJhuz7b4Qlf8YrZHSPZDxh6B2IAd2A7EJOt7d7Jj+DdSGn0u3HkZRWusySGkjSlEdT5gktcpgtdFtVJbKPVBG+Osq1DyKbg7ytD/M9iHX5e1dsP4WKEzu4LfVbU7DGABR/Vlyp4/+XAWIYq8QCtJ749VeWbYOK9N9Dp3i984LC68ovFRSR4fO2Lofdoduculv78ryh2RGnbFNnGPW6/5yWo81Iqtv71Hn2c8H7Wcya9PQXilXYxQNr8UtRx/Qa89wrbtqOCcWcJn5ARvw0SeleyrU0LcX7jSkREREQE0Qnga7/h/x5/xqsHfwy9g/crPNldw+bjX/FdJHGCa7/h/g7w6sGV2XuDga/w5PsreIpPuP/DF1mayviPYYrsGPrvrpq9r2WIlv6IHv9q+vI3+rfh7aeGrob13x+T9YDhpLflH4hRMe+rlLTdl+mg5QS9rQY66OLZLBNZWeXUWRJDSZqySOp8QVgOiqUv00Uui2qktnHSw5b2rqpJ717CHTkkJ/l9nc91+Pm2jb2BC/T7qe8m294r+E5FCdv7LwPbt+Ai+j5ZU0x7qso3zqSHrYb33sD5+FpEReUXjotE8BjoJprn4SCsNHa08lK3KUTjno/b7wVI6ryEiq5/g3esp9w1e26ktUcar2FLe+/sBL17HYyCiyvS5ksNW5nfX7u9N/BOpOrbUUs/7sRvg8zeldyoaU+J8S+gzWql4kpEREREBGA6nSrRZ/+/ClCzz+bjf5lpQp/9HaWw+R/1Wpv++vHvkXzyprF99vf3lW7cdRTgqoE+Qw2UCyinO45M9dJj/nGj3zTmA0pLYk3jfWz18Iy7joLTVdHaKDVwo3no9U3ntdOsCxTgqHB2Rr31hs3qE9eOseo6WhmWPFRqWVXUef6xxTAtjVHO7DOPhSSNNZ2lzssKgD4pJLrcojGUL9MylkVRie0cuEad/RmCNlp+IyXW+7yzxZ3r8HIUjW1sTEJtjs9vHodwrAdu9PtKKaXGXeWElpukXO83aaaxxTp5DIvOz9KeqvJVCTHQ+62VZX1VaflaeVnioov7TdkF6197XjOWeMSS9quEPDPFjioDy/pv+Um2KTxGP7N0sKTfmnXbxJKHSi2rijrPP8ZvT5DGKGf2mcdCksaazlJnFdPfROsz27okbT2UMD95mcvGJW+6ff2mJO0quU3KthyCj2B7JKk92eNlL1sJ5s/Y4uOLrWvCdwL67yIcv7DU5WcRF1vbtqOtrvHfn9fb+tOy9Yu0uFvSLWtcZ2ztNPq/LX6W+NPSg2W8ILmTkxN9EmXA+BXD+BXD+BXD+BWzTPE7OTlR7979ot69+0V9+PCh9E+Qd206nSr9pPB5dXBwgNu3b+uTiagktVoN3r7KxbYq7Vw2jHt1GFsiWlVc/9Eisb9RGYatGppHXYwP+YSgMjGutEw4XhRzenqKr7/+Wp9MQoxfMYxfMYxfMYxfMcsUv9PTU6yt/QEAsL5+VZ9d2HT6HhA9ApqIiIiIiIiIiCo2xIs+Xw9TPsaViIiIiFYPTwCfW0O0ajXUEj8VvkeRiIiIiIiIiEoz6T1C3x3EvEeb8mJciYiIiGgV8QTwubWNPaWgEj974P4NERERERER0fKrtw+heJaydIwrEREREa0ingAmIiIiIiIiIiIiIiIiIrogau/fv1fBHaMArP/api3jvB9//BF37twBERERERERERER0TI6OTnRJxEREdEKWVv7AwBgff2qPquw6fQ9AKA2nU69M6gXwMHBAW7fvq1PJqKS1Gq12UUXF9mqtHPZMO7VYWyJaFVx/UeLxP5GREQSHC+KOT09xddff61PJiHGrxjGrxjGrxjGr5hlit/p6elCTgDzEdBERERERERERERERERERBcETwATEREREREREREREREREV0QPAFMRERERERERERERERERHRB8AQwEREREREREREREREREdEFwRPAREREREREREREREREREQXhPwE8MEVrK9fnX86a3qKiIPOVax/fxlvjRnp+bx98qdQmj/hiZEJEREREREREREREREREdF5o/xPFby8ZSeAD65gffczXk/fYzp9j+nrX7H59Ir15C3gpb/zVJ/o53NnDTv7fj7Tj9jR8jnoXMW3D4DHr/00+1/w4Nur6BxEchKb9LZQq7X+f/bePs6uos7z/5zb3SSEkEQRQV0HhG7AGOVBjNpRx9ER7WaWDfIwM85vTHbR2yIu6ZWJs8wPHB8Y88OsTLcrg2l1TdyRccMCWXbSjWSdByWtRowwG8NDd2IY5UlAExIgIX3v+f1xzvec76lT5566j327+/N+vU5yu6pO1be+Vd+qOqdOVWHM9MAYBjwPK4YnTQ+MDXjwPHUN6LuD+7R/wlszNmC5P00gowdvxTBMaSI/qyyuuMucmffJYaww4siKz4zDpmNYwtWq58rxuOnQJQzgWKZZYarQ4YwnzGsyT25l2tCyaBCBTCuQqsphPuM6np/HVH3NCEcC2IY3j2p0m8qHXDrPoi/HOMcGLDoL45Bw7ula7DOXSQyvqFAHqsxPTGPjzdKBPW0Dm26amb4tvYgcvRhY01U3WutPRJjWwHCUZuaVJUxmXuJ8ZF5hnNY8ZOmOkBTu/VVmv1fF2NOMI6uemuFq7WMrx2OxH0tELmEA1e5l+aNCmCp0mEVKTls6tjbH5qbJ84+o3P5a5XOI136fqjs2+Wxumhz/rDR1f2APkx1nmsr6SvcDZtzZ/oFsZvi4nqXtzozLcuXZjiVMNeE0wT1u4wdrWVY5Bomw2mEyDmt+vKyxQnvpVbDea+qw2nIghBBCCCFzGocJ4C4MXtaF5RcfxWnidNoRfHVdCdjYhfS8bBA+TQG3rO8Clh/G1e8Tt6O4el0J2DgvWOW7dx7WbwSWr3sBV0pi73sBt60GNq63rCZuOMGDQP+uIUz4Pny5NvRFIcYG+oHR2G+0CIz0m4Py8IGif0Q72pkcxqpBoFjsNX0wObwCPYPA0ISkN4riSL/zA0TAJIZX2GQ2H2hz8t69Btu1e3hNDPUCKGJlGGxswEP/SBGjEma0iPHBHuMhJCetRsnsqEOXMG5lmhPGUYezE7cybVxZNJbuNdehiHEMrk/a3tj6QYyjiOvWdDvnEQDQa9RZ34eqtqRm8tuEmdeGtxOqbZdr+xp0h76Tj+wKf42gv5Y8Tg5jRf8IUBzF9jUSK3LTrZmx9RgcL6JYBEa2pOWtOT9NidfQwcQQMNiT8VKzMtOWfo5erCTaytB+wjT7VhaB8UEYzXLA5FZsHgeKK9dgzXYl92gRQK+yyWT74EZ3lXE2QHdkDuI6psjp9xzHnhy/VwjjqMNcKrRnTcep/U22VUFTZZadBcuYNtmHNwOXcUGN+UGeviYxvKIHg1D5nrgcm1dJWVb2d3um0FTT5wR1OWkXflzfbBOGLa6XtYxBxgY8eD2DWKbalqBMd6E/JatL3UCb67WOuksIIYQQQohB/gTwti5sRAkXv7+ccD7tykPYv/8FRHO5IXtvmYeNyw9j3WrDw4U9HdgBYGl3Mq3TzywBO7rw3SbPAE8Or8LgeBGj1oeEgL4NyYmavrVD6MU4Nm+Nh/NBPL0YmpjAUHpOQDGJ4VWDwNAmrF1q+o1h/eA4eoc2IX4O7MPaoV5gZEv6ISOT4OEmLTOw6xFT5sp5TxPIiOJK9AHA5DBuGAF6h9YGfwNA3waMFoHxzVvVV9l5aTVKZhcduoRxK1OXMGkMHc5aXMq0cWXReESOG+KJwlR9d8kjaSb5bcJMbMNnGkUMmbbixBgGegYx3juEiaon5GpjbMsIUFyJDSuLFcqk+vw0K94E3WuwfWIIveODWFVTBK1P300vlQjtZ3wztk4C6FuJImwv54HJrZsxXs3ETCupQXdkLuI2pnDp99Jw/K5xCZOm3vG70Z41mVra32Ci0t7GzkSqyU9lfU1g9zjQe/mFcf3tXoPtUX3O83d5pqiNuC5vV3YBAH3YMDGE3txJ11bVS/cxyOTwCvSPBBOz5vCwe832jMndxjLdeq2m7hJCCCGEEGKSOwG8d7IAoIzu07owmHN2L/bOw8euBdZ99YhlIF7GlWuPAjvm48vRsuEufPnaDmD5Ubw/Wl5cwpmnRze1kEls3Txe84PXsjPiHHev2Q7fNx8Q0sgLkPSXvgAmH8EuI14A6D5jGYARNHb8X1veJ4dvwAh6MbQ2vGtiN8YtMvcs7QXGd2MiuKumtNI4xOOiQ5cwjmXqEsYkpcO5TAPLohmYX+yPrQ8mqza1WhCSgUObUIGZ3Ya3F2es2YSh3nEMRqth8ghWjY2g0oRAoxlD8H63L5xIHMENGW8hq8tPs+K10L0G1xWB8cH1Ti/zTVqbvrteKhHYj9CHlcEbUSP9oC2ofWKmBVSlO0KyqK3fS409OX7PDWOS0mENJNuzZlJf+9u7tMd0mtHk58dNX+O7A8vIopJ/c54ppO+7zl6Xw34n3WcmaVW9dBuD5OSpJeTI0EK95tddQgghhBAy42j+EcD5E8ABXbhsyTycKefy7j+IdbvNM4ALuOVj8wG9fbPJ+17A/p2HsfsymUhegN3rDmL/PUeC7aVPL2E5OnDnd5Ni7Xm4A0AHHt6TcG4wwde62L3eOF/G3BpUE6z+Gu8dQtXP/5PDWDU4juLoBvsLkIndGEcvUuP8nqVw/jg9i9SLntrynnoYypAteODZheDj/1rSqlFmFx26hGkaFh3OJcwyndaycEF9sT8WfKlfvC5nssrMozA+iB5Vb3lOUyNwaBNSzNA2vO3pxppgdsu+Pa/B1oGeYDWYn6HLZjC2BSPRCtFgIlGvdEtSRX6aFW8GPUt7Vf9aLS1Mvyq9ZBNvHRnQF8wAJz+oiLZ/blltqgln3REipMYUtfV7qbFnRr/E8XsWFh3WgNmeNY0a29+xgX6MoBeXX1hHJtsI5/zk6kueB/oz6n+eP2p7psglXHmcMooYl36nZfXSZQwS9ueV8tR8pl+vznWXEEIIIYQQC44TwMa5vLKaV87uBbD3lgW4Fofx1SuT2zdrtg0uxpLzunCxmki++M7jsWTJguAs4dOOYO1qYMe1C6J4sW0BLtuYjKd6RtCfeMngwfP6YTvpaXzXUmyKzlyZCL5M7dHnuoTnRHkePC98aV3DiqWx9YMYL46mtjJqPmMY6B8BLBMe+XlXjK1HsPOZiqT7QlzeC4zcoL/kncTwDWlNV5VWo2RuN2w6nDNkl2k70y1fq/e7TBra89i3QZ8dFZwhlz5njyRhG9483HWbDpv1YhPR9qEj/Tnt8fggBkcA9C5F9qu1KtJ1IuyX1ArR4DzZClvzOeWnWfFmU/eKkpakX4NebIQfXSQmXfrWItjxVVn41s0O7fP046Y7QgT7mAJO/Z7CNvbk+L06bDqsFlt71hSqaX+TfW0/Rt1WRhsfNdbfR7vgMi6oJT9u+upesx3+RHCEyGBPOv08/yBMNc8UDoSr4uvCuV6a+vcqjB0r4DgG0R/STg6vSKabOlfXlC2t+6poqV4F17pr5rXGciCEEEIIIbMaxwng9BnAAeGqXLX1c9biX+ydh/UbLRPJ97yA1ejC+lsCUd43dAC3re7AteeFq4TXl7Bz52Esr2tr6CJG1YRLcI2iaAaDcV6PfJmaWF0SnG8VT97sQn+1K/jGBtA/UsToNMwcyBekQ5vSEx75eRfCh+PUw2o31mwfRTHxIqAHu5cVASyDXgTpnlajZG43snQ4N6hUpu2N1LH8L/Vd89i9ZnvqnD1iwja8ebjrNh3W9jIqJjj70b51YkTvECbC81B7Ms9Pqy7dXGwrRPtWomicBW2Sm59mxVuBelaUCE1Pv0a9AMbEQs8gMDQBP2F33bjwcn3mZ7i9bKIdaE+cdEdISKUxRX6/J2SNPTl+dydLhw7ktmdNoKr2N+5rJ8IVrJndsqZ3CBON7KOdcBkX1JCfavTVvQbbfV9N9BqTmHn+VTxTONF9Btw+K0radG310tS/X2HsWBmXMYg+QzzYsj1Ic9SaoCmbrW5UQTP0OjZgTNqadcO17pp5rb0cCCGEEELI7CV3Avi0btvEb5K93+3CDqhJ2yWLg1W7O+bjvCULg9W8ezqwA8DSVHwlnLkc2PFwR+TyviFZIXwg2B56Twd2oIzuzNnlJpKzlVjw9W5157iNbRlJfbHZMzgePSisGJ4M0x1H6vigrC3PHBgb8NA/0ouhCccHoay8y5fv1ofVPmwwHkTWLt2Vs7orO626ZHbRoUuYZlBRh7ObzDKdrrKoicryZOaxEtE5e6ShZLQtwkxqw2cc3WuwaagX44OrKq++6F6D7cESkIwXXI1lcutmjAMY6dcv34IVExXrQU5+mhVvJSZ2j6dfOlZLk9OvWS9ITyxstzSo3Rdejt7oXNCt2Dw+M7ZJdNEdIahlTJHV71Uce3L87kRFHebg0J41mlrbX/k4MbkqfObimp+a9CVjmKwPGPL8G1ZfexAc220aRcxEsJdx0qanoV4mqDQGCSdfK+Wp+TRBr30bEm2tX+EIFNe6SwghhBBCSBa5E8BZ5/IGHMWF7wNOu/JQPGEbXretBrD8MHbuPxSs+D29hOUAdk+a8XTg4R3A8jNLhnvMtq1dwOqjeJ/p0VDCwb25Cs/1RYI56K+AuQWsL193hg8K29d0Rw88+otXRCtGqn9hGLyIAYqjthcx1eU9mPyQs5HyMFfjuKdVt8wuOnQJ0wSq0+HsoWKZTlNZNJqKebQyiUd2VdeGEBsObUIlqtD/dLThM5XuNdehiHEMrt9ieiWJtgGsc6u+XOTsxtFUGfoVX9AGZOenWfFWYDI4N7B3aG3mi0NXmpd+fXpxQrav3TIWbM3eeznafv7XSXeE5I0pquv3qht7cvxuozodTjf1tb/B1scVzmedYeTnpw59ZXwIEZHn3xC6ccYyBOcK28ZR0u+04Q4Z2WMQdVayLU8tYfr1ml93CSGEEEIIycacjU1z2hF8dV0JO66dH5zTCwAo4Jb1XVi+7rD7pKztfF8UcMsFC7ARR7H2yjKALgwuWYwlg13RbXtvWYjLNpaw7uqjkVtzCLdhSgyuw7OrovNaxjBgbtETfgne+EF/H4KxvvoaNjw/ptoXhpPDK8IXMX7GeZUueQ+p6qXlJIZX9GAQQ9gUReKWVmNkdtGhS5gGU5UOZyiWF4L5ZToNZdFgcvM4OYwVxllVk8Oral9NQhQubcLMbMNnNn3YMFoERkZyzyTr29CCcyArnd3YtxJFJM+TTZORn2bFm8XkMFb0BOcGxv1rPTQp/br14oJsA92P/ia/hG0Irrojc57cMYVTvxdS1diT43crVemwDai3/ZUz1mfLysO8/Ljqa2zAOHd2EsOrBjEuHwbk+bsyNlD1+bV9G0aDiVRzHNX2/U72GCQ6K7nHM3aJCT+grZaZqNe8uksIIYQQQkgl9u/f7ztdt73kA350LV/3XDqMum5b7ftY/qK/03DfuW4qEU8qzM4X/eXaHy/5t1nit1233XabbzIx1OsDRX/U9PBH/SLg9w5NJFyD8IivYvLOlD/gG0GsYYLLJkfAxFCvj94hPymN748Wk3GY8uYT5DMtC3yg19fRpeQ2MxbJk5WPCX+o10jDEoefm1YzZI4vmw7zwqTSia5YFy5h/FwdtjcATCdFstySOnQv00aURb1UzOdoMSVz6OGQR4uNNFDumY5N72zDG0O9us3UicpzdnyxHrSuR4vJ+33f9/2JIb9XlZtLuoFNpsPYdJ3X/mr/avLTrHj9Cjow660VS3vV1PSN9KrRi0mWTdmR9tceV4RFH5m41qsKcValO9I0YGn/2h+XMUVAqp5ZKlglW7OOTSxx+LlpNUPm+ErZnkOYVDrRFevCJYyfq8MYWOqbU3tma0vy2qEK/nnyuvRLgbu9ffNd8tXgPPmVysthPFIpP9Xry5627+AfYdNPSKasFe4RTLvQ+tPklp+FLN3axo42WbPvj+W2NAf2epGnd0u4dtWrkKUfU+6scNZyIG0LLP0FcWffvn2mE6kC6q8+qL/6oP7qg/qrj3bS3759+/zHfvWY/9ivHvOff/75hl8St7d//37fnBSeqWzbtg2XXnqp6UwIaRCe5yF4VpndzJV8thvUe/OgbgkhcxW2f6SVsL6RRjA24KF/1xAmtnOHoEZCvZJ2gv1FfTz66KM45ZRTTGfiCPVXH9RffVB/9UH91Uc76e/RRx9FV2ewE/KSly0xvetm/2/3A05bQBNCCCGEEEIIIYSQJjOGLSM8HqbxUK+EEEIIIWTuwQngGcsYBjwPXsWriecoEkIIIYQQQgghpGFMDt+AkeJoxjnapFaoV0IIIYQQMhfxDhw44Pu+H209Yvvf5taOfg8++CC3gCakicyVbYrmSj7bDeq9eVC3hJC5Cts/0kpY3wghhLjA/qI+2mkLz5kI9Vcf1F99UH/1Qf3VRzvpr1VbQPMMYEKIM3PlIWWu5LPdoN6bB3VLCJmrsP0jrYT1jRBCiAvsL+qjnV7gz0Sov/qg/uqD+qsP6q8+2kl/nACugW3btuGyyy4znQkhhBBCCCGEEEIIIaQt2Ldvn+lECCGEkDkEJ4CrhCuACWkuc+Ur1bmSz3aDem8e1C0hZK7C9o+0EtY3QgghLrC/qI92WsE1E6H+6oP6qw/qrz6ov/poJ/21bAUwzwAmhLgyVx5S5ko+2w3qvXlQt4SQuQrbP9JKWN8IIYS4wP6iPtrpBf5MhPqrD+qvPqi/+qD+6qOd9NeyCWCuACaEuDJXHlLmSj7bDeq9eVC3hJC5Cts/0kpY3wghhLjA/qI+2ukF/kyE+qsP6q8+qL/6oP7qo53016oJ4ILpQQghhBBCCCGEEEIIIYQQQgghZGbCCWBCCCGEEEIIIYQQQgghhBBCCJklcAKYEEIIIYQQQgghhBBCCCGEEEJmCc4TwHtvWYglSxaH10LcstcModg7DxcsWYBtprvBtsHFWHLBPERR7Z2HC6I00tdgXoSEEEIIaSCTGF7hwfPia8XwpBmIEEIIIYQQQgghhBBCSBvhNAG8bXAxzrsWWLfzAPbvP4D9t5Vx7XlZE7JdGDxvPnaYzibbFuCyjYbbaUdwz/4wjeh6AasBYPlhXP0+I7wLYwPwvBXIe189NpB8we0NjGlfDGg/z0PC2zlMzOTwiiDcimGYokV+VllccZcnM++Tw1hhxJEVnxlH1gSBGa56PQdUjsdNhy5hAKlDWf4uMruEmWWEdSeZTzc9NKZcGksgk6UdCfMZ1/f8PKbqbkY4EjJn2/AW4KDbsYEeDGIIE74P3/fhjxYxPthj141DfJqUniy6soapkIY1vEVYa7isvmtsAJ43gHQsiOqN9T5LHxqES0+qp65IZjNsdt6BjDKQttKah7T81esmS6ZYdksRpLCmW2t9MOQaG7DbakAoZ0rILPnNMrFc4Q12eSvJkpY9hcU/TqfCfaqNS5RlIr7G5i0rjLUuEQvu/VJmH2hph7LiM+PIKiczXPX9bUDleCz1xxKRSxhAtYNWfxeZXcJkk5LTJovFtq1umjz/iKz2LPS1yecQr/0+VXds8tncNDn+WWnmtz3ZcaaprK90W2nGne0fyGaGj201bXdmXJYrz3YsYaoJpwnucRtPWMuyyjFJhLUtS8ZhzY+X1ee2l14jbDpTVKV/QgghhBBCnCaA987D+o3A8nUv4MrTQrf3vYDbVgMb16vVuwgmdZcsWQBzXjdNFwYv6zIdrWwbXICNKGHdV49Akm8sweC/f5d6we378Df0RSHGBvqB0dhvtAiM9OuB+SSGV9jCZDw0Tg5j1SBQLPaaPpgcXoGeQWBoQuIaRXGk3/2hAahCnpy8d6/Bdu0eXhNDvQCKWBkGGxvw0D9SxKgxQZB8AMlJq1EyO+rQJUz0YNg/otw0LjK7hJkLuOmhMeXSeLrXXIcixjG4PlloY+sHMY4irlvT7ZxHAECvUX99H6oKk6rIbxNmXhveLoxhywjQe/mF6BannqXoBbDrkQa9YErYQqir1Is61b/4PiaGgMEes2yCepDUvYrT+rIsGa8fRGxJv3rGBjx4PYNYpuqU70/g8s09WDEMrNmu3EeLAHqTcm/oC/NkTMBPXI7Nq6qTb/KRXeGvEfQ718MG6GZsPQbHiygWgZEtjuk2rD4k6VtZBMYHYTThAZNbsXkcKMqgRsiUv9ux/ARDl74Pf/ua2KYayjg2b7WX0OTwDcjvNZuRtwbUpTmJa7+U0wdyLJ8zZnSR2SWMA07tW5PIbM801betgJmv4Nq+pjktXEz1bY9zfpCnr7y+ubK/2zOFppp2uYaxUIvrZS1jEvuYysfE0C70p2R1qRuYdXolhBBCCCEki/wJ4D0d2AFgaXc54Xz6mSVgRxe+KzPAe+fhgsu6sHzdQexcV0qENdl7yzxsXH4Y61abPga2yecGMzm8CoPjRYxaHwwC+jYkJ2f61g6hN/GSLXiASIexvSSfxPCqQWBoE9YuNbwwhvWD4+gd2oT42a8Pa4d6gZEt6QeLTNzkccl7mkBGFFeiDwAmh3HDCNA7tDb4GwD6NmC0CIxv3qq+xM5Lq1Eyu+jQJYyk1YuhiQkMped5HGV2CTMXcNFDo8qlGYgcN8SThqm675JH0mjy24SZ2Ia3Cz1Y2mu05Vs3Yxy9uPzCLG3XQ6ir8c3ImMMCopenyZeycbuwXekeAPqwYWIIvS4vGrvXYPvEEHrHB7GqnhUUYwPoHwGKo+aHHUE9c38xPoHd48YEfPcabK9Q17MpYshsw6qhBt2MbRkBiiuxYWWxxvpfe31I0bcyM0xQp+OJMKF++VtNUMbjg+stsk5i6+Zx9A4NoWh6tZoa6tLcxK1fcukD03AsH+Mis0uYanFr3xpFLe2ZU9s6g6gmP5X1ldc35/m7PFPURv1joVbVS/cxyeTwCvSPBBOzyTEV0L1me8bkbmOZOXolhBBCCCEkTf4EMACghDNPN90Mwu2b77kyOVGcYu88fOxaYN1Xj+QO1rd9eT524CjW5sVZM/JCrLaHrWVn5OUgjbz0SH/dC2DyEeyyxNt9xjIAI3B4Xq2C2vIerCDpxdDa8K6J3Ri3yNyztBcY342J4K6a0krjEI+LDl3CyEOlbz7okabR5uVifrE/tn4Q471D2NRqQYjCoU2ogFnXXGifNrwVdGPNdbJyUlY/jKM42jz7C3TlRu/SnvBXUA9QvM4uV/caXBe89c1/6R2GtU+iuTCJ4eAtLqSbrJfx3UFPWi9nrNmEod5xDFa5gjiiKt0Eq8eLK/vCydcR3JD3ltdCbfXBRh9WWuuA1J1wIiyiMfK3mjMuvBy9trZmbD0Gx3tx+YVnGB7TRFV1iWRTWx/IsXx7UE37Vh/1tWeV29aZR35+3PSV1zdX8m/OM0VjxkKtqpduY5KcPLWEHBnaTK+EEEIIIYSY5E8An17CcnTgzu8mg+55uANABx7ek3DOoYBbPjYfcFrR24WtGwGsPopajv51I/hCF7vXG2fKZJ+7Iqu/xvNe7tpepkwOY9XgOIqjG+wvPSZ2Yxy9SD2Xhltu1kVKntrynnoAypAteMjZheDD+FrSqlFmFx26hKmVlMwWXMLMBUw9NLNcGoL6Yn8s+FK/eF3OV+dmHoXxQfSoOszzmmrFoU1IMUPb8OkiXAU20h9vZ2iuwGgk8daA2YwN9GMksQo5XG2TUnxMz9Je1SdVppqwacI6ueyMym2DE9Lm9OfUaVf0hL7p54azbsa2YCRaVRtMvuqVhK7UVh/s9AUzwMnJ0cztnxsjf8vpvhCX96ZXuAWr2TJeXk8TznWJxKT6pdr6QI7lc0jJbMElTA4u7VtDqLE9c21bZwrO+cnVV17fnOeP2p4pcmnMWKhl9dJlTBL20ZXy1Hxmml4JIYQQQghJkj8BfNoRrF0N7Lh2AW6R7Z63LcBl+Qf9pth7ywJci8P4qsOK3r23zAvO/r36qOnVcMZ3LcWm6IyWieBr1B59lkt4fpTnwfN6crYtA4AxDPSnVwCNrR/EeHG0qS/P7djlgVPeFWPrEewYpyKRl4036K93wxVQBlWl1SiZW0q2zDEuYeYCM1MP3fK1er/DBGJGHvs26LOjgnP40ufskWrIbxNmehs+XYxhwPPQP9KL3l6olWCIdNrQehtOsKcnqkbQryYK+jGaXNEVrgRrFI1YpVHpRWE1dK/ZDn8i2LJ8sMdhsiWPaEK/tj7TTTfhGECtqg3O4K1y68Na60MWfWsR7A6rWoatmy1teYPkj0jKW3cZViR8oW7ZWjQ1yd0Qas+bW10iMfZ+CU59oIJj+RyyZY5xCZNDZvvWaKppz2psW42PGqtpB2rHpe2pJT9u+srrm/P8gzDVPFM40IixkHO9NPXvwfP6Hc6ZN3Ack+gPLSaHVyTTTZ2ra8qW1n1VtFSvrph5rFH/hBBCCCFkTpA/AQzgfUMHcNvqDlx73mIsWbIYS9aXsHPnYSx32RpaUFs/5y7+lRXGy4/i/S6B6yRxRo+8PEusEgnOfoonbHahv8KqPfnCeGiTmmAYG0D/SBGj0zBzYJUnJD/vQta2lt1Ys30UxcTDfw92LysCWAb9Ybx7Wo2SubVUkllwCTMXmLl6kPqW/6W+ax6712xPnbNHqiO/TZjZbfh0EeihiFF/O7ZvH0URI+j35CVdsCKintVPgPHiuGcQGJqAn9JxEaPqgwmM9CNx1Fr3GXCbSkr2SVk0YpVGpa0fq6Z7Dbb7vnqZXPlFaR7B2ZX2LS3zcNKNbVVt30oUE+duZ9CI+pBJNy4MlseG+gu3ok20H3XKbyWWN7jyJiDqxJDVPsndKGrPm1NdIhHWfikkvw8UOJbPo5LMgksYK07tW4Opqj2rsW3tDXYHqaUdqB2XtqeG/FSjr7y+Oc+/imcKJ2odC9VUL039+/D90ZrOmHcZk+iztoNt3YM0R60JmrLZ6kYVNEOvYwPG5K1ZN/Iw81i7/gkhhBBCyOzHaQIY4STw/v3hdc8RnLanAztQRrfjBO3e73ZhB9Qk8pLFwSriHfNx3pKF8epiIN7+eWnZabK44eRsHxZ8sWs/u2xsIFgtNTSRfNgY2zKS+lqzZ3A8ejhYMTwZpjuO1HvjrG3OHMiSJ5OsvMuKAesDah82GA8ha5fuAnqXoqLIGWnVJbOLDl3CVImLzC5h5gKZemhCuTSPyvJk5rESidWVpC4y2hZhJrXh00dwBl58TmMfNvjxJPBweIZk3XkyXhxvzzEY+WAiuVKtB8FRlabiYyaC/fsq90khE8EezsZkccbWfqlzKANZsOuRxn/Q0b0G20cbMEnSvQabhnoxPriq6lUxdt0kmdy6GeMARvr1y81gZYrN5hI0pD5k063PyJ3cis3j6e1A65K/LQi3LB1cjzGMYf2gZZK7DXCpSyQgq1/KJKsP5Fi+Ii4yu4TJpMr2rRHU2p5V27a2O675qUlfeX1znn+N9TVNjWOhaaiXCSqNScLJ10p5aj5N0GvfhkRb6/sZR8sQQgghhBDSAJwngE22be2q6nze0648FE8gh9dtqwEsP4yd+w8lzwTeW8BuAKsvbPb2z+GA3lx55/rywBjoBy8FgOJo+qWAue2rL18jhw8H29d0Rw85+itXRKskqn9JVkmeavMeTH7IeUh5mKtq3NOqW2YXHbqEqYLKMge4hJkLVNRDg8tluqiYRyuTeGRXuj0hLji0CZVo8za8HUi+8IongQcHx9E7tCmlp1YQbMeoz4zrxhnLkNz2VhNuges0CSZho4nvChMNsNW1cJVppTPt6iFjsqVautdchyLGMbh+i+mVjU03KeR80dGUvfgVX4DXTro+VECdkTu2fhDjvZcjOf/bevmbgayo2jIQnGV53XQYaiWc6hJBTr9UbR/IsXw2lWUOcAnTXtTXnlXVts4A8vNTh77y+uY8/4bQwLFQi8kek6izkm15agkzV6+EEEIIIWQG4IVXMwjjdpgA7sLgksVYMtgVuey9ZSEu29jE83n3dGBHNdtL10y49VLiYTA81yk6o2UMA+a2POEX9HqgPzm8Inwp4NdxPqSs2lBfwIZnxlT7kixfHpe8h1T1om4Swyt6MIghbIoicUurMTK76NAljBv5MruFmXVYXgjm66Fx5TJd5OZxchgrjLOqJodXVViRQyrj0ibMzDZ8+gnyYm6ZODl8Q3TG2PhgT/52is1AznJVK3n6NowGLw/NLRYnh7GiJzhfL+6TMsgK270G1xWBkX7jHLnJYayw9Jmywnyk30vpZ2wge+vxFGMDxtl2kxheNYhx5wmcSvRhw2gRGBlxOzMuSzcmtvNFhb6VKCJ5Bm9DsNSHbGQb6H70217YTof8zUAmukdGEmdZtgWudYk49EsufWAIx/KZ5MvsFqbtqLc9q6ptnQHk5cdVX3l9c56/K2MDVZ9f25Cx0LSQPSaJzkruMcdU4Qe01TKn9EoIIYQQQgiA/fv3+7nXzhf95fB9RNdL/m1mGHXtXDeVG2b//v3+bat9H8tf9Hda75/y1+1M31Ppuu222/wUo0UfQOrqHZqIgkwM9Sb9i6OJKFL+gJ8MMuoXLWkEV6+vkkowMdTro3fIN71Hi9myuuEuTypvRt79SJ6in/bxfd+f8Id6jTQscfi5aTVD5viy6TAvTCqd6BJduMjsEmbmAMB0UiTzmtSnux7qL5f6qZjP0WJK5tDDIY8We2mg3DMdq97nZBveeNAo3er6Gt4fhXeIT5OlP02QftpGAvd02Zi6z0o/na/gsnQnEbZ7qg1vkyW7TbHEkaMvW1xZOvSVvnQ+UmlWyquRXuXxQmX/htYHix5ixN7T8VSSz8/yr5BWli4r5jPPjizp2fQiadvaukQ9tMTn4ueSt6ww1rrURGBr/9oe934ppWeLgq11N8IyNrHE4eem1QyZ48vWfuaFSaUTXc0by8NS31zaN6u9ObUHdv/KZZ6sE7Y2xLe1rQa5+WpwnvxKZZpqe6rLT/X6sqftO/hH2PQTkilrhXsE0y60/jS55WchS7eu/Uv2/bHclubAXi/y9G4J1656jbDlM1X/bfqz6J+0PbD0F8Sdffv2mU6kCqi/+qD+6oP6qw/qrz7aSX/79u3zH3vsMf+xxx7zn3/++YZfEre3f/9+35wUnqls27YNl156qelMCGkQnucheFaZ3cyVfLYb1HvzoG4JIXMVtn+klbC+kUYwNuChf9cQJrZzh6BGQr2SdoL9RX08+uijOOWUU0xn4gj1Vx/UX31Qf/VB/dVHO+nv0UcfRVdXsOvykiVLTO+62b9/P1DPGcCEEEIIIYQQQgghpFGMYcsIj4dpPNQrIYQQQgiZe3ACeEYxhgHPg1fxMs6mIYQQQgghhBBCSNszOXwDRoqjM+e86RkC9UoIIYQQQuYinACeUfRhg+/Dr3htAJ9pCCGEEEIIIYSQmUX3mu3wOUvZcKhXQgghhBAyF+EEMCGEEEIIIYQQQgghhBBCCCGEzBK8AwcO+LJ6FID1f5tbO/o9+OCDuOyyy0AIIYQQQgghhBBCCCHtyL59+0wnQgghhMwhurq6AABLliwxvepm//79AABv//79wQzqLGDbtm249NJLTWdCSIPwPC/66GI2M1fy2W5Q782DuiWEzFXY/pFWwvpGCCHEBfYX9fHoo4/ilFNOMZ2JI9RffVB/9UH91Qf1Vx/tpL9HH320JRPA3AKaEEIIIYQQQgghhBBCCCGEEEJmCZwAJoQQQgghhBBCCCGEEEIIIYSQVuCHVzMI4+YEMCGEEEIIIYQQQgghhBBCCCGEzBI4AUwIIYQQQgghhBBCCCGEEEIIIS3AC69mIHFzApgQQgghhBBCCCGEEEIIIYQQQmYJzhPAe29ZiCVLFofXQtyy1wyh2DsPFyxZgG2mu8G2wcVYcsE8pKLatkCltRhLBrvMEIQQQghpOpMYXuHB8+JrxfCkGYgQQgghhBBCCCGEEEJIG+E0AbxtcDHOuxZYt/MA9u8/gP23lXHteYsxaJ3h7cLgefOxw3Q22bYAl200HcPJ38u6sPq2MK39L2D1xgW1TwKPDcDzViDvffXYQPIFtzcwpn0xoP08Dwlv5zAxk8MrgnArhmGKFvlZZXHFXZ7MvE8OY4URR1Z8ZhxZEwRmuOr1HFA5HjcduoQBpA5l+bvI7BJmlhHWnWQ+3fTQmHJpLIFMlnYkzGdc3/PzmKq7GeFIyJxtw1uAg27HBnowiCFM+D5834c/WsT4YI9dNw7xaVJ6sujKGqZCGtbwFmGt4bL6rrEBeN4A0rEgqjfW+yx9aBAuPameuiKZzbDZeQcyykDaSmse0vJXr5ssmWLZLUWQwppurfXBkGtswG6rAaGcKSGz5DfLxHKFN9jlrSRLWvYUFv84nQr3qTYuUZaJ+Bqbt6ww1rpELLj3S5l9oKUdyorPjCOrnMxw1fe3AZXjsdQfS0QuYQDVDlr9XWR2CZNNSk6bLBbbtrpp8vwjstqz0Ncmn0O89vtU3bHJZ3PT5PhnpZnf9mTHmaayvtJtpRl3tn8gmxk+ttW03ZlxWa4827GEqSacJrjHbTxhLcsqxyQR1rYsGYc1P15Wn9teehWs95o6rLYcCCGEEELInCZ/AnjvPKzfCCxf9wKuPC10e98LuG01sHG9sXp32wIsWbIAtnndJF0YvMw2oVvALeu7gOWHcfX7xO0orl5XAjbOq7zquGaCwX//LvWC2/fhb+iLQowN9AOjsd9oERjp1wPxSQyvsIXJeGicHMaqQaBY7DV9MDm8Aj2DwNCExDWK4ki/80NDgKs8OXnvXoPt2j28JoZ6ARSxMgw2NuChf6SIUWOCIPngkZNWo2R21KFLmOjBsH9EuWncZM6vP3MBN101plwaT/ea61DEOAbXJ+1wbP0gxlHEdWu6nfMIAOg16q/vQ1VhUhX5bUK+DVZRdkAL2vB2YQxbRoDeyy9Etzj1LEUvgF2PNKgBS9hCqKvUizrVv/g+JoaAwR6zbIJ6kNS9itP6kiwZrx9EbEm/esYGPHg9g1im6pTvT+DyzT1YMQys2a7cR4sAepNyb+gL82RMwE9cjs2rqpNv8pFd4a8R9DvXwwboZmw9BseLKBaBkS2O6TasPiTpW1kExgdhNOEBk1uxeRwoyqBGyJS/27H8BEOXvg9/+5rYphrKODZvtZfQ5PANyO81m5G3BtSlOYlrv5TTB3IsnzNmdJM5fxzhgFP71iQy2zNN9W0rYOYruLavaU4LF1N92+OcH+TpK69vruzv9kyhqaZdrmEs1OJ6WcuYxD6m8jExtAv9KVld6gbaXK911F1CCCGEEEIM8ieA93RgB4Cl3eWE8+lnloAdXfiuTMrunYcLLuvC8nUHsXNdKRHWZO8t87Bx+WGsW236tJ7J4VUYHC9i1PpgENC3ITk507d2CL2Jl2zBA0Q6jO0l+SSGVw0CQ5uwdqnhhTGsHxxH79AmxM9+fVg71AuMbEk/WGTiJo9L3tMEMqK4En0AMDmMG0aA3qG1wd8A0LcBo0VgfPNW9SV2XlqNktlFhy5hJK1eDE1MYCg9z+Msc379mQu46KpR5dIMRI4b4pd9qbrvkkfSaPLbBBcbrKbsWtGGtws9WNprtOVbN2Mcvbj8wixt10Ooq/HNqNQ8Bi9Pky9l43Zhu9I9APRhw8QQel1eNHavwfaJIfSOD2JVVW/1DcYG0D8CFEfNDzuCeub+YnwCu8eNCfjuNdheoa5nU8SQ2YZVQw26GdsyAhRXYsPKYo31v/b6kKJvZWaYoE7HE2FC/fK3mqCMxwfXW2SdxNbN4+gdGkLR9Go1NdSluYlbv+TSB6bhWD7GTeb8cUS1uLVvjaKW9sypbZ1BVJOfyvrK65vz/F2eKWqj/rFQq+ql+5hkcngF+keCidnkmAroXrM9Y3K3sUy3Xqupu4QQQgghhJjkTwADAEo483TTzeC0I7hn/wHcc2VyojjF3nn42LXAuq8esQzWy7hy7VFgx3x8OdpeugtfvrYDWH4U75cVyA1DXojV9rC17Ix0DvKQlx7pr3sBTD6CXZZ4u89YBmAEjR3z15b3YAVJL4bWhndN7Ma4Reaepb3A+G5MBHfVlFYah3hcdOgSRh4qffNBr3GY6c952qRcsjC/2B9bP4jx3iFsarUgROHQJlTArGsutE8b3gq6seY6WTkpqx/GURxtnv0FunKjd2lP+CuoByheZ5erew2uC96c5b/0DsPaJ9FcmMRw8BYX0k3Wy/juoCetlzPWbMJQ7zgGq1xBHFGVboLV48WVfeHk6whuyHvLa6G2+mCjDyutdUDqTjgRFtEY+VvNGRdejl5bWzO2HoPjvbj8wjMMj2miqrpEsqmtD+RYvnGY6VdDNe1bfdTXnlVuW2ce+flx01de31zJvznPFI0ZC7WqXrqNSXLy1BJyZGihXvPrLiGEEEIIIWnyJ4BPL2E5OnDnd5NB9zzcAaADD+9JOOdQwC0fmw/o7aRN3vcC9u88jN2XLcaSJYuxZMkC7F53EPvvOYKsW2on+EIXu9cbZ8pU2tIrWP01nvdy1/YyZXIYqwbHURzdYH/pMbEb4+hFamwfbrlZFyl5ast76gEoQ7bgIWcXgo/na0mrRplddOgSplZSMps41p+5gKmrZpZLQ1Bf7I8FX+oXr8v56tzMozA+iB5Vh3lOU604tAkpHG3QVnbT2YZPF+EqsJH+eDtDcwVGI4m3BsxmbKAfI4lVyOFqm5TiY3qW9qo+qTLVhE0T1sllZ1RuG5yQNqc/p067oif0TT83nHUztgUj0araYPJVryR0pbb6YKcvmAFOTo5mbv/cGPlbTveFuLw3vUooWM2W8fJ6mnCuSyQm1S/V1gdyLJ9DSmYTx3FEDi7tW0OosT1zbVtnCs75ydVXXt+c54/anilyacxYqGX10mVMEvbRlfLUfKZfr851lxBCCCGEEAv5E8CnHcHa1cCOaxfEZ/BuW4DL8g/6TbH3lgW4Fofx1QqrhLcNLsaS87pw8c4D2L//APbvP4iL7zweS5YsQLQouMGM71qKTdE5KxPB16g9+iyX8Pwoz4Pn9eRsWwYAYxjoT68AGls/iPHiaFNfntuxywOnvCvG1iPYMU5FIi8bb9Bf74YroAyqSqtRMreULJmrrT9zgSxdtTfd8rV6v8uLP3se+zbos6OCc/jS5+yRashvE6q1QXvZTV8bPl2MYcDz0D/Si95eqJVgiHTa0HobTrCnJ6pG0K8mCvoxmlzRFa4EaxTttEqje812+BPBVqODPQ6TLXlEE/q19ZluugnHAGpVbXAGb5VbH9ZaH7LoW4tgd1jVMmzdbGnLGyR/RFLeusuwIuELdcvWoqlJ7oZQe97c6hKJsfdLcOoDFRzL55Alc7XjiBwy27dGU017VmPbanzUWE07UDsubU8t+XHTV17fnOcfhKnmmcKBRoyFnOulqX8PntfvcM68geOYRH+MMTm8Iplu6lxdU7a07quipXoVXOuumdcay4EQQgghhMxq8ieAAbxv6ABuW92Ba88LV+WuL2HnzsNY7rI1tKC2fs5cybt3HtZvBJYnVgiXceU9L2A1urD+FidxqyZxRo+8PEusEgnOh4onbHahv8KqPflKc2iTejEwNoD+kSJGp2HmwCpPSH7ehaxtLbuxZvsoiomH/x7sXlYEsAz643n3tBolc2vJlrm6+jMXyNZVuyP1Lf9Lfdc8dq/Znjpnj1RHfptQnQ1ay24a2/DpItBDEaP+dmzfPooiRtDvyUu6YEVE9gopR3Tf0TMIDE3AT+m4iFH1wQRG+pE4aq37DLhNJSX7pCzqWaUhVNr6sWq612C776uXyZVflOYRnF1p39IyDyfd2FbV9q1E0eW8zEbUh0y6cWGwPDbUX7gVbaL9qFN+K7G8wWV7idtADFntk9yNova8OdUlEmHtl0Ly+0CBY/k8smWubhxhxal9azBVtWc1tq29we4gtbQDtePS9tSQn2r0ldc35/lX8UzhRK1joZrqpal/H74/WtMZ8y5jEn0ed7Cte5DmqDVBUzZb3aiCZuh1bMCYtDXrhmvdNfNaezkQQgghhJDZi/OM6vuGZEXugWA75j0d2IEyujNnc5Ps/W4XdkBNIi9ZHKwi3jEf5y1ZGKwu3tOBHQCWdpsrhEs4czmw4+EOw71J5GwfFnyxaz+7bGwgWC01NJF82BjbMpL6SrNncDx6OFgxPBmmO47Ue+Osbc4cyJInk6y8y4oB6wNqHzYYDx9rl+4CepeiosgZadUls4sOXcJUSTUyV6o/c4FMXTWhXJpHZXky81iJxOpKUhcZbYtQyQazym662vDpIzgDLz6nsQ8b/HgSeDg8Q7LuPBkvjrfnGIx8MJFcqdaD4KhKU/ExE8H+fZX7pJCJYA9nY7I4Y2u/1DmUgSzY9UjjP+joXoPtow2YJOleg01DvRgfXFX1qhi7bpJMbt2McQAj/frlZrAixWZzCRpSH7Lp1mfkTm7F5vH0lop1yd8WhFuWDq7HGMawftAyyd0GuNQlEpDVL2WS1QdyLF+RamSuNI7IpMr2rRHU2p5V27a2O675qUlfeX1znn+N9TVNjWOhaaiXCSqNScLJ10p5aj5N0GvfhkRb6/sZR8tUUXcJIYQQQgjJwnkC2GTb1i5g9VG8z/TI4LQrD8UTyOF122oAyw9j5/5DwYrf00tYDmD3pClWBx7eASw/s2S410s4oDdX3rm+PDAG+sGLA6A4mn5xYG776ssXneHDwfY13dFDjv7KFdEqiepfklWSp9q8B5Mfch5SHuaqGve06pbZRYcuYaqgsswVMB8U5wAVddXgcpkuKubRyiQe2TU360P9OLQJlWjzNrwdSL7wiieBBwfH0Tu0KaWnVhBsx6jPjOvGGcuQ3PZWE26B6zQJJmGjie8KEw2w1bVwlWmlM+3qIWOypVq611yHIsYxuH6L6ZWNTTcp5HzR0ZS9+BVfgNdOuj5UQJ2RO7Z+EOO9lyM5/9t6+ZuBrKjaMhCcZXnddBhqJZzqEkFOv1RtH8ixfDaVZa5AW4/d6mvPqmpbZwD5+alDX3l9c55/Q2jgWKjFZI9J1FnJtjy1hOnXa37dJYQQQgghJBtzptVCFwaXLMaSwa7IZe8tC3HZxhLWXX00EbJubOcNo4BbLliAjTiKtRXODq6NcOulxIA6PPspOqNlDAPmtjzhF/R6oD85vCJ8ceDXcT6krNpQX8CGZ8ZU+5IsXx6XvIdU9aJuEsMrejCIIWyKInFLqzEyu+jQJYwb+TK71Z9Zh+WFYL6uGlcu00VuHieHscI4q2pyeFWFFTmkMi5tgpsN5padEzO/DscEeTG3nZscviE6W2x8sCdjS7omI2e5qtUQfRtGg5eH5haLk8NY0ROcrxf3SRlkhe1eg+uKwEi/cY7c5DBWWPpMWRk20u+l9DM2UMWWoWMDxtl2kxheNYhx5wmcSvRhw2gRGBlxOysuSzcmtvNFhb6VKCJ5Bm9DsNSHbGQb6H70217YTof8zUAmukdGEmdZtgWudYk49EsufWAIx/KZ5MvsNo5oO+ptz6pqW2cAeflx1Vde35zn78rYQNXn1zZkLDQtZI9JorOSe8wxVfgBbbXMRL3m1V1CCCGEEEIqsX//fj/32vmivxy+j+h6yb/NDKOuneumcsPs37/fv22172P5i/5O6/0qPUsY23Xbbbf5KUaLPoDU1Ts0EQWZGOpN+hdHE1Gk/AE/GWTUL1rSCK5eXyWVYGKo10fvkG96jxazZXXDXZ5U3oy8+5E8RT/t4/u+P+EP9RppWOLwc9NqhszxZdNhXphUOtElunCT2RaPReQZAQDTSZHUR1KfbrryG1Iu9VMxn6PFlMyhh0MeLfbSQLlnOla9z8k2vPGgUbrV9TW8PwrvEJ8mS3+aIP20jQTu6bIxdZ+VfjpfwVWpbbbdU214myzZbYoljhx92eLK0qGv9KXzkUqzUl6N9CqPFyr7N7Q+WPQQI/aejqeSfH6Wf4W0snRZMZ95dmRJz6YXSdvW1iXqoSU+Fz+XvGWFsdalJgJb+9f2uPdLKT1bFGytuxGWsYklDj83rWbIHF+29jMvTCqd6GreWB6W+ubSvlntzak9sPtXLvNknbC1Ib6tbTXIzVeD8+RnlAVga3uqy0/1+rKn7Tv4R9j0E5Ipa4V7BNMutP40ueVnIUu3rv1L9v2x3FbbstWLPL1bwrWrXoUs/ZhyZ4WzlgNpW2DpL4g7+/btM51IFVB/9UH91Qf1Vx/UX320k/727dvnP/6rx/zHf/WY//zzzzf8kri9/fv3++ak8Exl27ZtuPTSS01nQkiD8DwPwbPK7Gau5LPdoN6bB3VLCJmrsP0jrYT1jTSCsQEP/buGMLGdOwQ1EuqVtBPsL+rj0UcfxSmnnGI6E0eov/qg/uqD+qsP6q8+2kl/jz76KI7pDHZdXvyyJaZ33Rz47X7AbQtoQgghhBBCCCGEENJcxrBlhMfDNB7qlRBCCCGEzD04ATyjGMOA58GreBln0xBCCCGEEEIIIaTtmRy+ASPF0YwzqUmtUK+EEEIIIWQu4h04cMD3fT/aesT2v82tHf0efPBBbgFNSBOZK9sUzZV8thvUe/OgbgkhcxW2f6SVsL4RQghxgf1FfbTTFp4zEeqvPqi/+qD+6oP6q4920l+rtoDmGcCEEGfmykPKXMlnu0G9Nw/qlhAyV2H7R1oJ6xshhBAX2F/URzu9wJ+JUH/1Qf3VB/VXH9RffbST/jgBXAPbtm3DZZddZjoTQgghhBBCCCGEEEJIW7Bv3z7TiRBCCCFzCE4AVwlXABPSXObKV6pzJZ/tBvXePKhbQshche0faSWsb4QQQlxgf1Ef7bSCayZC/dUH9Vcf1F99UH/10U76a9kKYJ4BTAhxZa48pMyVfLYb1HvzoG4JIXMVtn+klbC+EUIIcYH9RX200wv8mQj1Vx/UX31Qf/VB/dVHO+mvZRPAXAFMCHFlrjykzJV8thvUe/OgbgkhcxW2f6SVsL4RQghxgf1FfbTTC/yZCPVXH9RffVB/9UH91Uc76a9VE8AF04MQQgghhBBCCCGEEEIIIYQQQsjMhBPAhBBCCCGEEEIIIYQQQgghhBAyS+AEMCGEEEIIIYQQQgghhBBCCCGEzBKcJ4D33rIQS5YsDq+FuGWv9pyHCyK/9DW4zTEek73zcMGSBVC3E0IIIYQQQgghhBBCCCGEEEIIycBpAnjb4GKcdy2wbucB7N9/APtvK+Pa89TE7mlHcM/+0C+6XsBqAFh+GFe/zzGeBF0YPG8+dpjOVTI5vAKe58HzVmB40vQVxjDgefA8DyssgcYGAr/oGhjTvtG9ciW8NWMDlvtjUumsGEZamvx48kilY5HbJQwS+g0vHWByGCsscZhxuaaVCmfRjxnGVp4VZa4iDJBfFq7xmHJnhZsxhGWfzIabrbjqLE/3DSVMK12fwjwpGSrK72gTJIZtePNohG6BSQyvsOstiN8Sd2gHUXxjA/C8Adi1EaSv007ZWG4eQsYG0uGkLKzpu6adoZsq86V1mcyT6W65QuXb5bPoxqIL+71mPTZlscStsMapKsrYgBm/JkxrYNg5/yks+Qww82G5KurULDtCGk+qTwkvXd1dwsBWj2sYm7imlQpnsXEzjM2eKspcRRhAtfUZ/q7xmHJnhUtjtjlNbN8jsvtnZMVnC2ilctxN7VsNgnvd0rH2CVXKGmG1m2QcWfmy2USaHB2n6o5ZF7L9ncdnhBBCCCGEkBlP/gTw3nlYvxFYvu4FXHla6Pa+F3DbamDj+nnIWsC7bXABNqKEdV89gtNQZTzbFmDJkgXYqN3qZhybt9ofZiaHb8CI6QhED079u4Yw4fvw5drQp/z7gdHYb7QIjPSbD2rhA1i/PRWELxT6R4oYjdIZRXF8ED22F68V4nGm18iT7yPKlmOYyeEV6BkEhiaUzCP98cuD7jXYbtzv+z4mhnoBFLFSp5eTlot+UmFGixgf7Em9YKgos2MYl7KoJp7sOjZbcLOVanRWSfcNp28DRovA+OB648XODRhBEaNheeXKX41NEAO24c2jFt2GjK3H4HgRxSIwsiX5hrJ7zXUoYhyD65PuY+sHMY4irlvTnXCvDq1rHxNDwGCPWW75TD6yK/w1gn7nm5Np+0Hiji90s5jE8IoeDELV1YnLsXnVMCbRjTXbVXqjRQC9qp0x+4x6dGPkzffhb1+DoKQqyViBRP8etomhrvpWFoHxQRhVJGByKzaPA8WVa6rMvwv16bQxZU6IAznjY5cwDR2b5KTl0hemwsz68XqltrO+tqhi+16hf46o0D5XJCfu9ulb86lF1rEBD17PIJap8WNQHrvQn5K3Ur9agYo6rlSn8v2bOz4jhBBCCCGEtBP5E8B7OrADwNLucsL59DNLwI4ufNc2A2yb7HWNZ+88XHBZF5avO4id60qJsLVTxNBQb2ryJmASWzePo3doCEXTZ3gVBseLGM18SAse2vVzed/aIfQC2PWIfomxCoPjvRiamMBQbxw2ZhKP7AJQXIk4qj6sHeoFxndjQkLlxtNKxrB+cBy9Q5sQPyOGMo9ssehZCO5L5jUPB/1MDuOGEaB3aG0cRibtNm8NH4ZdZHYJ41IW1cRTqY7NFlxspRqdVdJ9cwjkVS+HJoexanBc1Tk3+dPUYhNzDbbhzaM23QpjW0aA4kpsWFm01HOp/zfEq0xsbXUDCF5m2l6SuhDoICFnNXSvwfaJIfSOD2JVTREAwAR2jwO9l18Y19XuNdieWXfdqU83mkbIKHaxGVuDGeBM2Sa3bsa4OfnULjSkzAlpBa0cmzj0hbY+YNaP1xvRdtqp1L5X7p9tGO1zBdziboe+1RV3WSeHV6B/JJikN+f/u9dsd5vcdaCyjvPqVJ5/68ZnhBBCCCGEkOklfwIYAFDCmaebbtls+/J87MBRrL0yOdnrFE+4nfQ9qXvr44wLL0cvRpB6Ph5bj8HxXlx+4RmGh7z4rv8hqHvNdvj+dvViwaQbZywDsOuRxEqxrcHSlyj9/HhayOQj2AVg2RlJYbrPWAbY9BwSrCbrxdDaarTqoJ+J3Ri3yNOzVL90cpDZJYxLWTjF07g6Nitw0pmD7ptF9xpsil6WTGJ41SDGe4ewSQRxlN+kNpuYe7ANbx7V61YYQ/B+si+cyBvBDcabU3OVydh6w24aTO/SHtPJiTPWbMJQ7zgG81azZtG9BtdZdgmolvHd8rlA46lVNyb1yhi0iUIfVgazF4be0vbTdjSozAlpKi0dmzj0hXN4vF5v21mJdPue3z/bSLbPWbjH3S59qwtuskp9vi67TjUENx3n1alK/q0enxFCCCGEEEKmh/wJ4NNLWI4O3PndZNA9D3cA6MDDexLOALqwdSOA1UcRHv0bUHU8Dab7Qlzem/5COvi61vYQF3w5i93rjfN9LOflaDJebOTRtyHcIs1bgeHJMQx4PcGX5uanxY1ifBA9Kl/Ws34qhZnYjXH0IvW+oWcprB/YA5Ufmiul5aKfjHSDFxm78Miko8wuYVxwiqfGOjZbMG3FSWfTS7e8HOrpCVaUbFJf+dckfwWbIEnYhjePqnUbMrYFI9EKzWAiL17BJahVJmPB6pLidY1ZHaMZG+jHCHpx+YW1xtyNNcFbZvt2xA70LO2N+5uqET3159fRKqlfN0JjZIy32wzoC2aAkxNR0fbP7W0/9ZU5IQ7kjI9zwzR6bFIpLZe+MCPd2T1eb0zbaSOzfXfqn9OY7bOVquKe7r61GhxkDfum9IR7g8nVcV6dyvNHy8ZnhBBCCCGEkOklfwL4tCNYuxrYce0C3CLbNG9bgMsyDujde8u84Ozfq48mPaqMp/GED3WWrY4qvWAc37UUm6IzeybCyZ+BjK+QxzDQPwL0DqGqD+YBAH3Y4I8GX+L29GMEQHF0Q11fmmfRt8E8r6g3dfaWS5iqGVuPYDe5ZK7c0srRj0xg3GCct3lD9plf7UJ1dWy2UI+tTCdhOwLYX4xWS4ZNEBtsw5tHLboN21e1QjM4zzW9dWT04UR/sLqket3aGEG/ehHfj9HKq7xcCLchHenPqh+VcVs5lU33mu3wJ4bQi3EM9lQzuWBSj26S95oy1C1juHV+ov3sW4tgt9VY65NbNzewrjSPesuckEq4jI9dwlRNxtjELa2cvnCOjtfrbjsjXNp39/45ga19TlFD3C3pW82+y4PnBfWvKhxl1R8JTg6vSKabOgPYlC2v7N10nFen8vyDMM0YnxFCCCGEEELaifwJYADvGzqA21Z34NrzFmPJksVYsr6EnTsPY7llS+c9D3cAy4/i/XL2r6KaeJpC30oUMY7N4dOTywvGxNk50eSPfcs0+Qo7sSrQkeDhsR8YjV+qjPR78OS80SbSvWa7cfZWGpcwlQkfZnP0jYy08vXTjTXbZdWBPGD3YPeyIoBlqHIxX0uppo7NFuqxleklnCAEgJF+1Gee7jZBQtiGN49qdWtboWnEERN/ONG41SVFjKpJiPrtMUDO+rZttZiH08qpPLrXYLvvq5e2lV9C26lHN/G9wWVOLNQgo+6XewaBoQn4iZXx3bgwWIIexhNut5qw3fakIWVOiCO28bGJS5jKuI9NbGnl94VzeLxebdtpxaF9r6Z/zm2fDaqJW9H8vtXsu3z4/ijCTzarwkXWXWo5crDNeJDmqDVBUzZLv6qpRsd5dSrPvynjM0IIIYQQQkg74TQBjHDydv/+8LrnCE7b04EdKKM7MdEbbv+8tAzL/C/gHE+zCLdQGlyPMYxh/WANLxgzthYbG/DQP9KLoYmchzob4RfXvUMTkGfu7jXb4QefIKcf7JuFnL1VCQnTsxS9GEfqaKGsrdRkNUE1D5fRWWCu+unDBuPhf+3SXUDvUvTAUWaXMC7UE09GHZstZNpKPTprEcEEYfAiJ7VCoFr5a7GJOQ/b8OZRnW4nt27GOBC82DdW22Sf1Wexg4iM7R0zzmfUyCREckVZjYRnfY8PrkqtlMljYve4ZQKjxnx1r8H20SonFyw0VDcmrjL2DmFC9cvbLQbWrc+hntyKzeOWLU3bEHuZE9JkOF53C+NCPfFkjCdycW07c8hq36vqnx3aZ01VcWsa3rc2kUqydp+BZah8tm691KTjvDqV559X1wkhhBBCCCEzFucJYJNtW7vS5/zuLWA3gNUXGts/V8AaTxORr3q3DARn61yX+aDbg6W9li/oLS8EgokDoDhaw8QBJE7Li+BaXyxUzSQe2YX4xYsVI0z4AKy/gEb0lXb6IX1sywgQnWWUh5FWzfoxVhG5yOwSxgWneNzr2Gyhoq046WwakS1xw60MUysEqpS/OpsgAtvw5uGuWzkfcjTxAt/3/eBFf+YLxgyyXsDDXl42gu0RK5zbVwXda64Lti9dv8X0yiZsH3qH1sZbndabrwbVn0bqJkWDZNTnUI+tH8R47+Vo+/lfW5kT0lQ4Xp814/VcnbiRbt8b3D8nqC/uhvWtLSBbVnVurjk53BDq0HFencrzJ4QQQgghhMxO9u/f71e+nvdXw/ex+vnIbee6KR+Y8tftNMLe9pLdvdp4Ev4v+bdZ/GzXbbfd5ptMDPX6QNEfjV38oV74AHwUY1ffH/WLgN87NKGcij4APw4WhNH3BfHrMJUI004FDuPtHfJV6v5oEYbsQlY8DkwM+b1GOqk8uISJ5Ov1I5VNDPm9pg4ruYtfblrV6sePdWS9p7LMLmFissvCKR6HOtZOADCd7IwWk3m3lmsaJ51FZOu+XtL5tNenIE+xvM7yZ7nPcdJ6Fx2zDa+Xhuo2pVdNWseBc7pN0KRsx4/txIwrLbefaaMJLDLY44rzCKNOWcOLnJa0nfM1WjTul7LIks2uS6t8Nt1Y4rDfq6hGxpCJoV6rXmyILZo6T2GRPRPXsBXCWfVSocxJ+2Fr/9oel/GxSxhbO5Q1BslyF7/ctKrtC317++Qos0uYmOx+1ymeVL+X0dfZ6ls1bWe1bZGpv5ScmqTM1bTPvl9D3ClZ4zjMdt4a3rGdtd7r+5FM6XJ07PsyZNVjpaQu0nU5M+4sXHWcV6fy/DUWnRBCWkOqvyBVsW/fPtOJVAH1Vx/UX31Qf/VB/dVHO+lv3759/uO/esx//FeP+c8//3zDL4nbYQJ4v79/54v+cvg+oss+KZs3oesaTzK+ymH05TYBbHth4dsfElXY6ErcFD6IWa/4QSoVR3RpuWxx2eVOX5aHuUzUC/7M+13CBAQvTeLL1F8cxn6/e1p5+rHEY396rkLm7DCuZZEXj2+LK0PudgAVH1KSZZTMq6385Eq+dMjTWUpf0WWrN7Vh5jNI0/ZyJP2yM0/+OEzj5J0tmHr32YY3DDRQt3n11+rv8ILRph9bc2iTO3avkIZFhqy4fGXLWgabjGYYE9s9tvCpcFkvvS35ELLyk9KNJY5U+hY5UmGyZAyZGKpmgkFsKC1/AovsmagX+Poy24lKcabyHF62MiTtCSztX/tjGdembMMlTED9YxPXtPL6Qks8GcbkLnN2mCz7NWXPi8e3xZUhNyz1LXVvVruY2xalda7b98plmPSvrn2uIe6MsI3qW4XstCzjQot+s++3y6o8U/Ka+szKlxlOqF7H2XHm+UdYdEIIaQ2w9BfEnXZ6gT8Tof7qg/qrD+qvPqi/+mgn/eVNAP/rv/6rv3nzZv9v//ZvM6/Nmzf7//qv/5q6V08Ae/v37/fNVcEzlW3btuHSSy81nQkhDcLzPATPKrObuZLPdoN6bx7ULSFkrsL2j7QS1jdCCCEusL+oj0cffRSnnHKK6Uwcof7qg/qrD+qvPqi/+mgn/T366KM4prMLALD4ZUtMb3zta1/Dvn37TOcUp556Kj760Y+azjjw2/1APWcAE0IIIYQQQgghhBBCCCGEEEIIaQyLFi0ynazkheME8KxhDAOeB6/iNYAx8zZCCCGEEEIIIYQQQgghhBBCyLTz+7//+1i4cKHpnGDhwoX4/d//fdM5gXfgwAHf9/1o6xHb/za3dvR78MEHuQU0IU1krmxTNFfy2W5Q782DuiWEzFXY/pFWwvpGCCHEBfYX9dFOW3jORKi/+qD+6oP6qw/qrz7aSX95W0ADwE9+8hNs2bLFdI5YuXIl3vKWt5jOgNoCmmcAE0KcmSsPKXMln+0G9d48qFtCyFyF7R9pJaxvhBBCXGB/UR/t9AJ/JkL91Qf1Vx/UX31Qf/XRTvrTE8DHL16EQsG+WfOdd96J++67z3TG+eefj4svvth0BgCUy2UcPPAcMBsngC+77DLTmRBCCCGEEEIIIYQQQtqCffv2mU6EEEIImUPIBPCChcehqyv4beOmm27Cs88+G/19wgkn4JOf/GQijObo0aN44dDzwGycAOYKYEKax1z5SnWu5LPdoN6bB3VLCJmrsP0jrYT1jRBCiAvsL+qjnVZwzUSov/qg/uqD+qsP6q8+2kl/egXwvPnzMf/Y+WaQiF27duHv/u7vAADz5s3DBz/4QSxbtswMFnH4xcM4cvgwAJ4BTAipgrnykDJX8tluUO/Ng7olhMxV2P6RVsL6RgghxAX2F/XRTi/wZyLUX31Qf/VB/dUH9Vcf7aQ/PQHc2dWF4xYeZwZJ8Itf/AL3338/zjnnHLzuda8zvRM8f+h5TB09CnAFMCGkGubKQ8pcyWe7Qb03D+qWEDJXYftHWgnrGyGEEBfYX9RHO73An4lQf/VB/dUH9Vcf1F99tJP+9AQwABx3/EJ0dnYmwtTC1NQUnj94KPrbfrIwIYQQQgghhBBCCCGEEEIIIYSQpnH4hRdNp5ow4+EEMCGEEEIIIYQQQgghhBBCCCGEtJhSqYTDL9Y3CXz4xRdRKpUSbt6+ffu45wghZE5QKBQwb948LFq0CPPnZx+sTtqXI0eO4MCBAzhy5AjK5bLpTQghhBBCCCGEEEIIIYS0NXoLaGHe/HmYf+yxpnMuh198EUcOHzGd4T3xq19xArgVeKZDDjO0VKrNpo1WZb0RspKZhe/7KAEolctYvHgxFi9ebAYhbcxzzz2H/fv3o6NQQEd4bhIh7U+rejXB1S4aI1cyNde0q8WvW9pmSTYrqVfZhBBCiKK+boU9eLOor1xyYLG1hNrLkAU0U6m9zGcQrJ51MtsUOENr/QwVu1pmW21rJzo6OjB/wbFOZwJPTU3h8Avplb8CJ4BbRbUWMUNLpdps2mhV1hsh64ylEZlvVUE1AR/AkakpnHTSSYmVwJKlGZy1WYFUT11Njxw5gqeeegrHdHQ0pPoS0jpa3aK4Wkh9cqVTSbs0inqnf5sn2SymPpUTQgghEfV3KezJm0X9ZaNgMbWU+sqOhTVTqa/cZxispmQmM0eMlWbafDq7utDR0YGOzg50dHSgUCigXC6jVCqhNFVCqVTC1NGj5m0JOAHcKqq1iBleKtVmV9OqrNcj44ymkRlvVWE1gSnfR9cxx+CVr3wlAKDkA2V/BmdoFlLwPHSE9fXXv/41jr70Ejq56pfMOFrdrrjaSO1ypVMIXGqPMY/aYk7LSZypTeWEEEJIisZ1KezZm0HDyofF0zIaU2YssJlGY8p9hsFqShpNIwwpr142Io0ZQJ4aSPvACeBWUa1VzIJSqTbLwnRkvVZZZySNzux0FFgD8H0fR30fr33ta1H2gSMzNB+znXkeUPCAX/7yl+jyPG77TGYgrW5cXG2kdrmSKTR78hc1xe6qBVKB6tVOCCGEpGhcd8LevZnUXU4snpZRd1lFsNBmAo0r7xkIqyhpFHPakBoPTXNmwQngZtFoS2jDUnrx4XEc/OF3cOSXuzD13NOmNyEtoXPRiZj32mU4/u1/hAVn9preFTk8NYVTTjkFL5Z8TLWhjRGg0wOO7fDw6KOPYr7DuQeafzrQgW8+fQweeL6AJ482ulEmeZzc5ePs48r49ye+hHcvtp9DMTdodePiWtdrlytOIf5Ve2wuVB+7qxZIBapXOyGEEJKisd0Je/hmUVc5sVhaSl1lZYUF2K40vqxnGKyapBHMeUOKoUnNTTgB3CwabVFtVkrP/u/1eO773zKdCZlWFr/rwzjh3641nTORCeADR+s9YZI0Cw/A4q7qJ4A/88t5+OpTXaYzmSY+dtJRfOa1R0znOUKrWxfXAUj9cnlhWvXHlEd1KbhqgORQndoJIYQQK43tTtjLN5OqyopFMW1UVU5OsDDblcaX9SyC1Za4QkOKoNnMTQqmAyF5vPjwOCd/SVty4PvfwgsPj5vOuUz5wRnAvNrvqmVl9j8d6ODkb5vx1ae68E8HOkxnMqPx4LfZs5THBxpCCCFkltNOI4/ZB8dRcxXaFZmBsNoSUhXs4+cunAAmVXPwh98xnQhpG7Lq51PPPms6RUyFE4282vPKIqtMv/n0MaYTaQOyyiWrHAmpBj7MEEIIIe2DfCRWYShfB82JlQTwg7q5Cu2KEEJmK+zX5zbcArpRtNqSprHUfvn59/DMX9K2dC46Eb9z/T+Yznjq2Wdx0gknJNxkC+jHDpcT7qS5/P3/3Iy//dpX8eTjj+Ed73kvbhj+GzNIgtfML1i3gLaVKQCc88BxPPO3DTm5y8f9Zz9vOmeW4+yh1R22a92vRy7XNBpFvqytlmhOkK92QgghJIWt++js6kKhsxMdHR3o6OyEV+BaBEIIIYQQMrspl8solUooTZVQKpUwdfSoGaTpcNRNqoaTv6SdqaV+TpXdrq//12G8+41nJq4/6H0LvvD//mf8+tdPp8LP9MuW33e/8Uz8xdUfxwM7d6bCu1z/Z3QU/+Wz1+PQwYM4+/y3YsHCRakw5lUtnPxtT1gus4X2K8f2k4gQQgghANDR0YEFixbh2OOPx7xjj0XnMcdw8pcQQgghhMwJCoUCurq6MP/Y+Thu4XE47viF6Oho7RF5HHkTQuY8JcdL5iIXHr8Ibzr/rXjT+W8FANxz1534Dyv78fQzT6fuqeX6v/fvxI3X/2dcP/jxlF8rL1t+T3r1azD+j9/D//uJAfzf+3em7sm77rot2KL7iv+0Fl/8xrdwzef/v1QY8yKEtAvtNdXKLQqbiG35FiGEEFIFx8yfjwWLF6PD2MWHEEIIIYSQuUhnZycWLjoe8+bPM72aBieACSFzHnPFadZVDl+Iv+7M12Pd176FdV/7Fr56xyhed8ZZOHTwOfzdN0ZS99Ry/fjeH2DbXXfi0MFDKb9WXrb8/ret/4A3nv9WHDr4HP7HN7+euifvkjmFl594csov6yJktrB33z78zzu3mM4zhPaaam0vaWYRzTuwkRBCyBzimPnzMW/BAtOZEEIIIYSQOc/8Y49t2SRwW04AD315CAMf/5jpPG1sHRvD9vHxpKMsO5mu5SfTnf4M4O23/gZnXfNt0znBorPejrff+hu8bvWNpldb8aoPDODtt/4Gr/rAgOnVFrS7fHlM+b7TJXORPmK34094BS7590UAwN5HHkrdU8tlS2c6riw5Xn/umwEAhw4dTN2Td/nhzEKpirzNOVYuAe4cNl3biwd/FMg5E2Sd9bRiQNCseF2Z7vTnCHOwuSWEENJ4Ojo6OPlLCCGEEEJIBeYfe2xLtoP2nvjVr9rqdc/Ql4fwg3vvxX+5cT1e97rXmd7TwjPPPot//v73cfJJJ2FFb2/g2G7vIltYir9Y+0bTKZfXrb4RJ1/wUdMZALDvW9fiibs3mM518/Zbf4Pf/nQMD33pT0yviEVnvR1v+PRWPHnP1/CLjX9uercNr/rAAE798Lqm6ape2k2+09b/X9MJTz37LE464YSE2+GpKZxyyinY9ZzbMtNbbxnGbV//Gyx781vx+ZFvRe47t38fn7/6o5H7b595GmO33Yqf/PM/YN/EQwCAU3vOwiX/YQDvuKA/Fdc7+/4A3xpej9ed8Xrs+umPo3g1d/704cQ977/0j/CtL/8XPP3EYzjxVa/BpVd8DBdcfHkU/rfPPI07No7gx//0PTz9xGMAgOXvfi/e/8E/wnkr3qViziYrv1nuDz2wE3d+6+vY8U/fA8I89/3hn+CCiy+PdGRy2Uc+jg9ducZ0TrBsUQGPPvoo5hvbx9nKFABOvm+h6ZTNZy8BfvY9YMt+0yfms5cAT+wFvvoz06c5rFwCrPoscHFlvThz5zCw6S9N19rTeGofMHAOcM03gHdeYvpW5MnzD5lOmeU4e4g76L379mHnz+7HpRevTISoj1oHJNUMHGpNo5HE8raDNLOSaqoEIYSQGc2PduzAjV9aDwD482vW4m3Ll5tBaubYRYuctn1+9tln8X/+z//Bc889hw9+8IM4IWc8ODExgR//+Md47LHH8Nxzz5nehBBCCCGEAAAWLVqE17zmNXjrW9+Knp4e07spPPvss7jjjjuwaNEi/P7v/37u2BYApqam8PzB9LvSRtJWK4DbcfIXAF5xwgn43Xe9C08+9VR6JTCpip9/7kL88EMvj65937oWp354Hd5+62/MoKQOln3uHpx7009MZ5KBueI068paEbv7X4KJwWMXLsSU72Pyod247et/gxNf/Rpc8pGP491/cDH2TTyEL137n/Dz+3cm4nrq8V/hW8Pr8fzB5+DDxyUf+Tje8ObgBcyJrwruv+QjH0/c84tHHsRXv/CXeMObl+OUnjPx9BOP4ZYbro/ifubpX+Ozn7gCf/93weTsG968HG9483Ls+Kfv4fNXfxT//N2tqbzZLlt+n3n61/inrf8LALDiAxdG7j+/fyduWDOAn//0J+j/ow/jko98HM8fOohbbrged3zr63jZya/CJR/5OE581WsAAO/+g4txyUc+jp43npNK17yayuVrg/9/cLvpE/DUvmCC+P2rTZ+Zx5b98bXh/mBS+KvXmKHyeeSnwf9VTv6SdmPmTaM2c40zIYQQQuqns6vLafL3Jz/5CUZGRvAv//Iv2LdvH370ox+ZQRKMjY1h48aNePDBBzn5SwghhBBCKvLcc8/hwQcfxMaNGzE2NmZ6N4Uf/ehH2LdvH/7lX/4FIyMj+MlP8udmOjs70dnVZTo3lLaZAG7XyV+Bk8DN4Ym7N+CHH3o5pg79hhOWDaRr4ctMJ1IB88zZrEvmIn11zz13bMbd/+NvAQDvufgPMVUGXnbSq7H+O3+PT66/GZcWr8bAp9fhA3/0YQDAzvEfJOJ6+onH8M4LV+LvdjyE6275Fi4tXo0zzzkfAHDiq1+DS4tX49Li1Yl7AOBTf70BA59eh//v2/8LS8MJY4n7b79yEx6deBjn/+578eX/9T1cd8u3cN0t38KfXB1Mdv7tf/1SKm+2S9Lb98hD+MuBD+MvBz6MwcsuxNNPPIYP/NGH8e5/d3kUdui6PwMA/JfNW/Gnn/wLXFq8Gp/662A1+NjmW/GqU7txafFqnPjqYAL4rb/fh0uLV+ONb39XKl3zaiqvf1vw/88z2vXxYLIbvf/O9JnZnHRqsIL37m+YPvk88yvThZAWwKlfQgghpF3xw8tzmPy98847sWXLFhw6FK92eOmllxJhNBMTE7j33ntNZ0IIIYQQQnK59957MTExYTo3HD2ePXToELZs2YI777wzEcZGs7eBbosJ4Haf/BXaZRJ44MqP4ZLLLsXQ8FDs9vGP4ZLLL8XQl4eid6QJtzbnV3esx/yTT5+xZ8iSmc2U4yVzkbt/ugN/vPws/PHys/C1L3wazx98Diuv+DiW9b4LUwBOPq0bTz35ODbe9AV87soP4z/+u/fi7u8Eq3HLRlyveNVr8Cef/AtrOn5G+r9zxlk47U3nRu5nhBPGTz/1BKYA/OSfgy2Y+//0I4n7P/D/XIEFxy/CM088hgf/5WcJP9sl6T1/8Dns/ukO7P7pDjx/8Dn80dVrEzI/+C8/wzNPPIbnDz6HK/veGelm7R/9AQDgmScei8LKHHbJkl7W1XQ+cEX2ROi/fB84973BhOls5al9pgshbQenfwkhhJDG8bbly3Hn/7gNd/6P2+re/lnv11PpBdauXbtw00034b777jO9KvLjH9uPyCGEEEIIIcSF6RpP3nfffbjpppuwa9cu0yuiozN7/NwIpn0CeODjH5sRk79CNAn85FPY2qLl45pv/ff/jmeeeQYA8IN778WPf7zD7va3htuOHYl42g05N3bxG+KzSZd97h68/dbfJC4TM8yyz91jBsHrVt+YCPO61TeaQQAAZ13z7US4s675thkEi856e0omM75ln7sHbxmZxKs+MBCFWXTW2wEA5970k8S9bxmZTNwrmGm4ImnOP/l0zD/59ET6ogedB5HdzLuEMzHDZckPpXczjJmOppKMzaTku13l8O3GguMX4azzluOs85bjfX/4YXzyr0ewsnh1FO7v//s38F8Gi/jB1i044eTXoLfv3+G8d70XQBCHjusVr3pNZjp+le5PP/4YSj7wwsFgW7TT3nhuKu7f6TkLAHDo4MGUn3lJvGedtxwbf/wQPvnXI1hw/CJ858vrMX7PaBTu0MGDQJiXi/7Dx62XhJVVxaIHl6vp/O5lwf/mNtCy/fN7PpR0B4CPnRuc1SvXncOV/bO2Wv7sJclwD2Zsf3fncOX0auGZXwEnvy49uf3Va5Jpab2sXBKfJyz+nEBO8dOf/Qz/8847w2tLdO382f0AkHDT19591GUaWVPUisZgDkP1EkIIaQBZ2z//4he/wB133IFnn33W9MrlscceM50IIYQQQghxZjrHk3I28C9+8QvTC8j5gLIRTPsE8EX/9iIAwO6HHjS92pZf//rXAIDXndL6FWHm4dGvfOWJbm4nnpj4ux05/OQedC4O5Fx01tvRtfBlifOCDz+5JzGZeO5NP8GxJ5+WCGPysjf34bjTzo38D07eh5Mv+GhqcvMVvcFZlvps4pe9uS8xCfy61TfiDZ/eiifv+Voi3MkXfNQ68fxvPrg2CvfcQz/Eqz4wgKOHfpuSV299LROfv/3pWCKNUz+8TsWcjWypffjJPTj85J5E+sKZn/zv0VnMv9j45wCA4898a0Kug5P34Q2f3qpiDuR82Zv7EuFefHJvIozwqg8M4OQLPorf/nQMPyl2Axl5Ozh5X2oSGBkyNhPzzNmsqxy+IX9tz1n4s7/ZhD/7m034w/90LZa+/Z2JcP97Y/BBw3/e8G2svv4LuKj4H/Hq7jMAAOXwPF2Jy7ekn+Xn6r7g+EUAgIceCM4E1te/TjwEADjmuOC84kqXGe/St78TH/3segDAphs/g3/dM4Ep38cxxy0EwpW+FxX/o/WSOGWOoWRJL+tqOq9/WzARam4DLds/67Nun9oXTHqe857kebqV/LfsD1YYf+zcOBzCSWIYZ/Ne+4FkGIQTspv+Mn1+bz2TwA/+KIhjzS1J989eAtz/D3Fa6+4GvnRFPAm8ZT+w6rPx7y370xPIhDQETvq2BKqZEELmJD/asQMX/+FluPgPL8OPGvixuFewv2K6//77ceTIEdPZCZ75SwghhBBC6mG6x5NHjhzB/fer98eKQsb4uVE0N3YHLuzrx3/49/8B/+2b/w1bx0ZN77Zj94MP4sGHHsLrzzoLS5e+3vRuOhf29+PfXRScRfmpP/sUXve619nd+tJuM4nnHvohfvbJtyTcnrzn6+hc+PJo8rZz4ctw8OHk8v1dn74g8ffhJ/ck3OT3qy/8hAoFTB36LR760p9Efz9x9wb8i8CLBgAA//RJREFU9qdjeNmb+yI3mdDUE5JP3L0BT97zNRzffX5iUrlz4cvx8E1/Gv0tYU35nhm/HfNPPj36+/Til3H4yT1WWRrFM+O3JyaEAUSTtMK/3hqs8JMtuc+65tuYf/Lp+PnnLkyEM/OD8J5TP7wOByfvS+TDlje531xtbZOxmZhnzmZd0QrcnHtkBe684xdjqgw8+/TT+OHoXUC48jUvriUnvsrql3WP6X72O4PVxmP//RuJcKN/+9/wwsHncMLJr8Gpy85NpWteZrxTZeD1b3sXzn7ne/HCwedw+y1DmCoDpy47N5p0Hv3b/5aI4+EHfpZwk3mGUqgHl6slvH91ehvo724MtofW/OXFwZbQH/tS7HbSqcDFa4LfX70m7Q8Ek7ZP/iKeSL1zOPj7L41Vx+vuTv794I8CubT7SacGk7CyEtcVvap38/pg8lbOQEa4Avpn3wM+q86neP3bAh18+4bYjeTy5nPPxaUXXxxeK6PrvHPPAYCEm75OO5WT6aSFcOKXEEJIg/HL9sH7OecEY6BaWLQoeM4ghBBCCCGkFqZ7PDlv3rzM8XA5Y/zcKKZ9AhgzaBJ4uid/hQ//6Z/i9tv+J9761visnpSbZ3FrczoXvsx0Smw5LKtgjzv1TUA4afuyN/dVPDf4xcceMZ0wdSi94nT/v/yD6YQDP/8+EK5clTQe3/oVIxTw7I+2AABOeNvKyG3q0G8yJzD1ttUnX/BRIEwDAOaffHpFWQRzW+u3Z2xZbUPkNdFxyurf+SefBgA49jVn4ODkfZl5EuaffFo0+WtODmflTa/8FrJkbBYlx0velfsWP329/OTXAABu/Ogf43997cu48aN/nLrX/FtfJ50WTMg/snMHvvSJVfj8h1dWvMd0f++f/AcsOH4RHvjB9/AXH/x9fOkTq/ClT6zCHV9ZjwXHL8Lqz65PpWm7zHjl+rcfG4zi3/F/RlECsPLjfwYAuOMr6/H5D6/E//ral/E3f/4JrB/4EF58/lAqzrIlvayrJZz11uB/maB9al8wQfuG3jiMuF2+NnYzydoy+qRTk6uM/+X76cllhBOumod+HNxnuou81Wy/LCt2r/lGIKe55fXPx+3nHb+hN8g3mUa8CtdshDOThBBCyEykNDVlOgEAXve61+GP//iPUzuVufCa1wTPVoQQQgghhNTCdI4nTzjhBHzwgx/MXKBZKjX37XdbTABjBkwCJyZ/Xz99k7+zmc6FL8fze38GqMlIvTXxvm9dmwj/s0++BQcn78OpH16Ht2ec/5uFOeGYh0yE2sibFBVkMltvbf3kPV+L/M1tqSvxi41/ntiK+YcfenliZW01yLnBJ1/w0Sguc6WvbXLexskXfBRTh36TmvyVvJ18wUdTE9fzTz4dXY7xN4tS2e2SFbHw0376WvWX69Fz7nL85snH8E//89t4ywcuwls+EGx3Xw7vrRTXKW84F7972Z/i2OMXYWLnDrx46FDFe0z3V57Sjb/427/HW/suxovPH8TEzh341cRDeOM734uBL34Vp7zh3FSatsuMV65XntKN9/1p8FHE363/LH779NN427+9DKs/+yW8pvtMPDb5MMa+eQt+NfEQ3r/6SqxY+cfRvTKvI3pwuVqCbAP9D7cGf9u2f/7Nk/FvG3mTsa9S7cgT9u3TUzz1r8Hkq169u3JJvFV0nkw23nlJMPn8JWMCWs48NtOScHn5I01itk7yZjG9k7++cRFCCCGzkbctX447/8dtuPN/3Ia3LW/cB+OVXmAtW7YMn/zkJ3H++eebXhV561vDDx8JIYQQQgipgekaT55//vn45Cc/iWXLlpleEaWp7PFzI2ibCWC08SQwJ3+bz+tW3wiEE5sIz+Q9OHlfamtik12fviCaHD6++/zEebr1oid9D2ecdYsqJm5f9uY+/PanY6mtraebky/4SHRecL3s+9a16Fz48sRZzVCT5Pr8ZH1Nt07MM2ezrvdf8R9x0w9248ovb0z56eu1y87BlV/eiJt+sBt/NfojvP+K/xjd+/4rgvNw8+L6d1dfi78a/RFu+sFuXHfbtor32NwXvPwV+MO/+Ksojr8a/RH+/Rf+K1677JxUWlmXLV65fveP/30U74KXvwJTvo83vacP13zzTtz0g92R3O+/4j9G/lO+H+nljLcmz02udLWM968OJkCRsf1zHubKWRPXSV/NSb8TTEzrc4L1Za4MdkW2qNbnCJ90arAC2EyDZ/3OUlpoW05M75SrDw++ZbKdk8GEEEKIO+WMFcCaiy++GCtXrsTChQsjt2OOOSYRRtPT04N3vOMdpjMhhBBCCCG5vOMd70BPT4/p3HD0eHbhwoVYuXIlLr744kQYG5U+oGwEbTUBDDUJfNf/Ds7LbAd+sW8fJ3+byKKz3h6dr6uZOvB04u/Fb3hX4m+NnJOrz9OthuNOO9d0wpI3vQeHn9yD5x76IZ64ewNgOTsYautnfTZwFkee/VXib53ucw/9EFOHfmOV5YRetQrRgaOHfms6VcQMr7ezBoCDD/8Yx3e7fan9ww+93DoJnJW3dmDK59XOV8voDc5Nx1evCVbd/u5lSX9ZJfzPtyXdNee+N15FrJHtoyXOc94D3J/eEj21LfMr/k1wXzNW38o5whL3Sb8TT4CTWQynMyuTngQmhBBCZhs/2rEDF//hZbj4Dy/Dj3bsML1zyfpAauro0cxtoDVvectbUCwW8aY3vQmnnnoq3va2yh819vX1YfXq1Xj9618/7We4EUIIIYSQ9mbRokV4/etfj9WrV6Ovr8/0bgpve9vbcOqpp+JNb3oTisUi3vKW/AVvU1NTmDp61HRuKN4Tv/qVOWYnLsz094N1lPov1r7RdMrldatvxMkXfBQ//9yFiS2Tz7rm29HKWL2F8bk3/QTzTz49WpX6qg8MRGcA7/vWtXji7g0496afJFaOyupfcXv7rb9JxQsAbxmZxItP7sWuT1+ARWe9PTrv9sl7vhZN4opckpZ20+FELp3Oss/dg2NPPi21elkmRMVddAIg0ou46fh0OC1PJURWvao3qwyWfe4eHN99fuSepZO33/obTB36TSJfyz53D3Z9+oJIDyKfxKHD23SFsNz2jFydyL8pY7Wctv7/mk546tlncZJx5tThqSmccsop+J+PN7ehbUce/tH3sfHPP2Y6R6y+8as4823ZH120kktf3YVHH30U8zs7E+62MgWAk++LVxNUzWcvCSZBT34d8NVgS/oEP7g92BJ51WeBi9cEbk/tC7aMvngN8OCPgu2ZP3BFvMoWCLZSPve9wF+qM4YHzrG7IZyclfhFpi37w8gQpPPPtyXTyOLO4WCiV98vmHJ9LPxIQ+f9B7cDz/wqlqdSfDk8ef4h0ymzHGcje/ftw86f/QyXOnwB2Bxq7fybPejJl6uZEqRX/trlMUPNeOzZJIQQMgf40Y4duPFL6wEAf37N2qq2gc7rPjo6OrBg8WLTmRBCCCGEEKI49NzBubcCmMxu3vDprYnzX+WMX3OS9meffAumDsXhTr7gI6kzgDsXviwRl9xXC0/e8zUsedN7orhe9uY+/PxzFyYmWx/60p9g37euTZxjK5Oepvw2flLsRufCl0f3HnfauYkzgBGuIn7ynq/hZW/uS4Qz857HQ1/6k4T+Km1TvevTF+Dwk3uisjnzk/89dQYwwpW9U4d+m9K5jece+iF+/rkLo/y+6gMDeOLuDdj3rWsTeXv7rb/Bi489UtdkbyMwV5zOhev0t74Ln/+n3ZnX6W99V+qe6bpaypvCSe/3rzZ9At55CbDh/mACVM7IHTgHOCs8S+L1bwsmRu/+RvIc3VWfjSdZEW63vOH+5Jm7f3mxfVL1L28PJmnNM4BdJn/zWPXZQAbZClomfnVa374hnvwldXHaqadO4+Rvu1KfkesVSLVds25alxBCCJlWSqUSjrzwgulMCCGEEEIICTn84otNn/wFVwDXwUx/X1hHqdeyApiQVlLtCuC//eVLCXfSXvw/rz2mdSuASVOZ6yuAp59aO/9mDHqqk8WUoLkTt3bZmpnitGDPJiGEEFIR1+7jmPnzMW/BAtOZEEIIIYSQOc3hF1/EkcNHTOemwBXAhJA5Twkerza+CCGEEEIIITOLlw4fxgsHDjidCUwIIYQQQshsZ2pqCoeeO9iyyV9wAngO4xkXIXOYYzxgquzzasPrGLZPlfnB7cntms3rqX3mHYS0Aa5rh2L0HdOx+nfWMUeySQghZHoplUp44bnn8OLBgzjy4ouYeukl+OWyGYwQQgghhJBZR7lcxtGjR3H4xcN4/tDzeP7goZZs+6zhFtC10sx3j9NBFbXgl59/D6aee9p0JqQt6Fx0In7n0/+QqtO2bWYPT03h3/ybf4P/86yPR1+o/CLiz7/xAdOJNIAbr7jbdEpwyoICfv8ED7/61a+ct4A+54Hj8OTR2dZIz3xO7vJx/9nPm86Z5UiaQRWdfUSjbakWGTSNlkfIl6tZKU8L+dklhBBCrLRvFzKreuqW09ByZVE0jIaWy7TBCtEqZkd9IaR5sDUicxGuACZVM++1y0wnQtqGqH469OoegJdeeglLjy9gykfFizQHU8/mtfT4Al566SWX4ow4+7jKk/lkemC5zDQavUWI38avJNpVribQzsVACCGEkNkBxxokAStEq2jk0xshhJDZAVcA18ps61WrqAUvPjyOJ78+YDoT0hac/NENWHBmb+xQoW4fLZdxzLx5eOUrX4l7ny3hZwdauwUDqcy5izvwjhM68Otf/xovHTmCroLbN0v/dKADfzRxrOlMppnv9LyIdy+mjU0vFRrEFI0e6FSTdhaNlklwk61ZqbcMt2wSQgghKWZGFzLje+pppSllzCKpm6aUy7TBCtEKZledIaSxsBUicxFOANfKbG8xcmrFs/97PZ77/rdMZ0KmlcXv+jBOuGht0rFCXS77Pl4qlfCyl70MixYtwqMvlHH/cyU8dcTH81z2Oy0c1+nhpHkezlnUgVMWFPDcc8/ht7/9LboKBXQ4TgADwGd+OQ9ffarLdCbTxMdOOorPvPaI6Uxajmu71uhBjmu6eTRaLsFNvmal3jLcskkIIYQkmDndx4zvqaeVppUzi6UumlYu0worxXQwO+sSIdXB1ofMRTgBXCuzvcVwqBUvPjyOgz/8Do78chfPBCbTRueiEzHvtctwfO8fJVf+mmTU6alyGVPlMo499lgcf/zxOOaYY9DR0WEGIy2kVCrhpZdewsGDB/Hiiy+is1BAZxWTv8I/HejAN58+Bg88X+CZwNPAyV0+zj6ujH9/4ktc+ds2ZDSEKRptL67p5tFouQQ3+ZqVestwyyYhhBCSYOZ0HzO+p55WmlrOLJqaaWq5TBusENPF7KxPhLjD1ofMRTgBXCuzvcWYrlrRaL1OVz4caHRWc/Gao46W56MeMhRQKpdRBlAul7OCkBbjASgUCujwPBS8GVXLCGljXFu4Rtmca3quNEouEzc5m5V6S7FltdEZs6VBCCFkxjJzmvVGd2hzi5aXM4vLiZaXS0tg4U8ns7NOEeIGWx8yF+EEcK3M9hZjumpFo/U6XfloRxqt25AmRds8WCcIIXMW1wawES27a1rV0Ai5bLjJ2qzUW4uZC7e8V0UToiSEEDJ9zJxm3ezjSDW0vJxZXE60vFxaAgt/OpmddYoQN9j6kLlI9XtqkrmBZ1wzlZks+wyBg0dCCCEzl5nTi/k1XjEcFBFCCCEkzbSMhqYlUTL9cDw63Zive2f6a19CCCGV4QQwmf1wJNN00i+Z2xiObgkhpMnMhB5hRvVchBBCCKkIH/BqgaMh0jr4IqbdYekQQsjshBPAZG7AsWZLmFEPj6wPhJA5RSta6JnyGnEmyEgIIYQQ0jw4GiKEmPA1GSGEzD483/c57iOEEEIIIYQQQgghhBBCCCGEkFmA9/zzz3MCmBBCCCGEEEIIIYQQQgiZ4zz99NOm04zkxBNPNJ0IIWROwS2gCSGEEEIIIYQQQgghhBBCCCFklsAJYEIIIYQQQgghhBBCCCGEEEIImSVwApgQQgghhBBCCCGEEEIIIYQQQmYJPAOYtDWbNm3C97//fbz61a/GJZdcgnPOOccMQgghhBBCCCGEEEIIIaQB1HsG8N/8zd9gz549prMz73nPe3DhhReazlVT7xnAX/ziF/Hwww+bzlVx5pln4lOf+pTp3FImJiZw5MgR07kq5s2bh56eHtOZENLmcAKYtC1f/OIXcdddd+Giiy7Cww8/jIcffhibNm3C6aefbgYlhBBCCCGEEEIIIYQQUif1TgBfc801AIA3vvGNkdu2bdtw8sknO7m9733vw+rVqyO3Wql3AviKK64AAJx33nmmlxM7d+4EAHzjG98wvVrKrl27AAALFiyI3A4cOICurq5cNwB44YUXAADLli1LuBNC2h9OAJO24f777weAaJXv2WefjRtvvBEf+MAHAACXXXYZ3v3ud+Oqq67CM888g4ceeghnnXUWXvGKVyTiIYQQQgghhBBCCCGEEFI9jZgAfuMb35iYxK3HrVYaMQF83nnn4aqrrgIA3HvvvWYQK+94xzsAADfffDN27tzZFhPACxYswGmnnVa1GwDs3bsXL7zwAieA24hPfOITphMA4Ctf+YrpROY4PAOYtAVf/OIXsWrVKqxatQp9fX3YtGmTGQQIt6y4/vrr8d73vhdXXXUVVq5cWdeWIoQQQgghhBBCCCGEEEJIJa666iqnixBC2oUZMwF89tlnt8VE3549e3D22WdHX/y0i1y10i7yf/vb38aNN96IO+64A3/wB3+A73znOwCA4eFh3Hzzzbj++uvxyCOP4B//8R9x8OBB3HjjjXjggQdw/PHHO399RQghhBBCCCGEEEIIIYTUws0334wHHnjAet18881mcELINHP99debTnOKuiaAzz777NTVDpOJjcLM280334zTTz8dDzzwQLSVgxm+kfk/++yzK1bQ22+/veFpThevfvWrcffdd+OJJ57AVVddhbGxMdx88804//zz8Xd/93d46KGH8MlPfhLf+973MDQ0hPPPPx+bNm3CwYMHeSYwIYQQQgghhBBCCCGEtAnbtm3DNddcE1179uxxdmt3br/9dlxxxRWJ6/bbbzeDEULmAAcOHMAFF1yAW2+91ep+9tlnY8WKFZicnHTyGx8fj+Yjx8fHI/dbb701lYYLdU0AA8Add9wRfeXy6U9/Gh/84AfNIDManb/p2MLhrrvuyuz4vv71r+PVr3616TwjWbduHRBupXHZZZfh9ttvxzve8Q58/vOfx7333ovbbrsNq1atwoEDB3D99ddj5cqV+M53voM//uM/tk7GE0IIIYQQQgghhBBCCGk9J598Mt74xjdG13HHHefs1u6cdNJJOO+88xLXSSedZAYjhMxybr31Vlx22WW4+OKLE+5HjhzBn//5n+Mzn/kMHnjgAaxfvx4f//jHceDAgVy/sbExfP/738f3v/99jI2N4ciRI5icnMSTTz6JD33oQ4l0XKh7AlhzySWXAOE2ycIVV1wRzVjrrXpl9apc5lcy+j69fYL5Rc29996Lvr6+6O9WYK66/dd//VecffbZAIAPfvCDuOKKKyK/rPzL32effXZF+YvFIjZu3Gg64/bbb8f555+Pxx9/POF+/fXXR+nZ4s3Sq82/lVsrn3POORgaGsIdd9yBt7zlLfjc5z5nTf8LX/gCHnroIfyn//SfMDY2Ni2T8oQQQgghhBBCCCGEEELsvPGNb8Tq1aujSyZ6XdzanVe96lXR+3O5XvWqV5nBCCGznA996EO45557sHjx4oT7L3/5Sxx//PF485vfDAB485vfjNNOOw0///nPK/odPnwYADB//nzMnz8fCFcLb9iwARdddJFKwZ2GTgDLlr2yJe/111+PV7/61XjggQdwxx134K/+6q+isPfff39i5fDnPve5yE+2PRZ/TX9/P0ZHR6O/v/vd7+IjH/lIIkyr+Z3f+Z1IzjvuuAPf+MY3gJz8A8Bf/dVf4YEHHsDY2FjCXfOBD3wA9913X2oV8Oc+9zmsXr064Xb99dfj8ccfj/R2/vnnJyajK+lV/CvJ2wpOP/10fOpTnzKdE7z73e+OPjYghBBCCCGEEEIIIYQQQlrB3Xffjauuuipx3X333WYwUgXmhLrtMhcQEmLDrDd33XVXyq3ZdenXv/41Fi1ahHnz5gEA5s2bh9e85jW5fjLpe/jwYfzyl7/E4cOH8fOf/xznnnsuuru7o/irwXv++ed909GVs8NVr0KxWEysyDz77LNxxx13RBPCV1xxBf7iL/7CemarDmveZ/OXCcy+vj585StfscZZL2b+br75ZrzjHe9IyWL7Lfdn5f/scAVupe2L5f67774bTz75JD7/+c8DoRzyt5m+jnPPnj344Ac/GOnKlMd0M/0rlVezMfMiXHHFFTjvvPO48pcQQgghhBBCCCGEEEIazNNPP206VcU111wTrexthFutnHjiiaZTVZjvobPeVwv33nsvrrrqquhd/M0334ydO3dGi8Wmi127duHQoUOms5VXvvKVOO200xJue/fuxQsvvIBly5Yl3NuJT3ziE6YTmeV85StfMZ2sXH/99dG8WrOQs3lli2bzb+0m2Pw+9KEPYXx8HFdeeSUWLlyI//pf/yvuvPNOvOc978Hg4CAA4JZbbkFvb290bx51TwDLhOHtt9+Or3/969FqVpl8NJFG8vrrr8ddd92V8LNN8Ao6reuvvx7vf//7AQDf/OY3m9aImhOiNves33n5z4pbkxW3y++sOLL0inD7apNKnVozOTujQ/3iF7+I008/3boC+P7778eePXusfoQQQgghhBBCCCGEEEIq04gJ4CeffDKxnfOePXuiM3/z3FauXNnWE8BPPfVUYodShLuWnnTSSW07AdzV1YUTTjjB9Epx7LHHps5hngkTwHONrAlv10nRucR0TACPj4/je9/7XrQjLwB8/vOfx3vf+14AyPQzJ3Y///nP4/zzz8ett94ale0nPvEJfOUrX0ltO51Fw7aAvuSSS3D++edHgssk5B133BFtOfzAAw/gHe94B+69997EVsXmpCSMc4TN7Y/POeccfPe738UDDzyA/v7+hF+7UCn/tVAsFvGFL3wBN998My666KLMieMnnnjCdEqEzdJro+Wth/vvvx8AcNZZZ5le+NSnPmWd4L3//vvxiU98IrqXEEIIIYQQQgghhBBCSOuR833lkoleF7d256STTsJ5552XuE466SQzWFvR1dWFV7ziFbnXTNA/ITOBxx57DEeOHAEAHDlyBM899xxe+cpX5voJk5OTOO6449DT04Nzzz0Xixcvxvz583HqqacmwuXRsAlghDPSd911F+69914AwPnnn4+NGzeawfDUU08l/r755psTf59//vn4whe+EP1txnHJJZfgvvvuw9///d9bJwOnEz0Bm5X/Wrjqqqtw3333YWRkJPMLqIsuugjf/OY3o7+vv/76xOHQeXptpLz1cM899+D3fu/38IpXvCJye+aZZxJhNDL5+3u/93tN/5qDEEIIIYQQQgghhBBCSDayjbNcMtHr4tbOyIKqs40zRbUfIWRu8+Y3vxkA8NOf/jT6/+DBg3jta19b0U84cuQINm3ahCuuuAInnngifvazn+HAgQM4fPgwoM4KdqGhE8AwzgH+xje+gfvuuy9qCK+44gognMCFaihNvvGNb+Dxxx+P/M855xwzCM4//3ycf/75pvO0ctFFF+Gqq66K8pmV/1opFosVV//K5Kek9/jjjycmRPP02mh5a+Wuu+7CO9/5zujvZ555BitXrrQezs3JX0IIIYQQQgghhBBCCCHN5qabbsJVV11lvW666SYzOCFkmpmOOaN58+bhz/7sz7B27VqcffbZ+MxnPoMbb7wR8+bNq+gn3H777Xj961+PxYsXY/Hixejr68O73vUu9Pf3Y9WqVYmwedR1BvB0cv311+Occ85puxXApD7uv/9+rFq1Ct/73vcSK4Bvv/12fO5zn8OnP/3pqMw5+UsIIYQQQgghhBBCCCGNoxFnAMvK3ka41UqjzwCulnY6A3jBggU47bTTTC8neAZw+8EzgIkrM3ICeM+ePfjEJz6BsbEx04vMcCp1jHoS+PTTT+fkLyGEEEIIIYQQQgghhDSQRkwAP/nkk4ntnPfs2ROd+ZvntnLlyraZAH788cfx6le/2vRyQu61veduJbt27cLRo0fR1dVlejkh93ICuH3gBDBxZcZNAF9//fW46667cPPNN+Md73iH6U1mOLfffjv++q//GhdddBH+8R//EV/5ylcSW17LJPDxxx/PyV9CCCGEEEIIIYQQQghpIPVOAG/durWuOJYuXYrly5ebzlVT7wTw7bffjieffNJ0roqTTz552ncwfeyxx3DkyBHTuSrmzZuH17zmNaYzIaTNmXETwGT2I6uA+/v7rR3k7bffjvvvv5+Tv4QQQgghhBBCCCGEENJA6pm8bSfqnQAmhJCZDieACSGEEEIIIYQQQgghhBDCCWBCCJklFEwHQgghhBBCCCGEEEIIIYQQQgghMxNOABNCCCGEEEIIIYQQQgghhBBCyCyBE8CEEEIIIYQQQgghhBBCCCGEEDJL8O7ZssX3PA9+uQyvUIDvqyOBfR8+AA8APA9QfvLLU+5eoQC/XBYP+L6PQqEAv+zHd1QIH+H7ab/wdh8+PK8AzwPK5eTxxV7BQ7lcDmQS2QCUfT/6rZG8ep4HD0C5XEahoyOpAwkLwC/78AphPJECgvsT94R59MN0/dCtXC6j4HlRXj0lm47DN/UeRRuE0XJDiWKGM+Uyw4mbp8rC/L8MoGDmD8FNvg8UCiJT0q/gFeAjcNf1SwVBWd1UKBSisvODmyIdar9In2Yc4T3i74V6lDS1zkzd2H6bujPjkL/lty18LkY8Oj75XS6XUVB5EB2UyuUgj2H5aP1kyVL2/agsJR1oXVnuM8NqdyhdyG99vy/2r9xEZjO8TsEXv9D+vbAuQJWpyKxrtedJPYkcEnkz0XnwEOq6Q8nrR/9Eda0QlU8QxPOCf/yyn0gXvp8IDwTtVWD/Eiy8r+AB8OD7QX59Zf8JuUPlSZ3Xcfu+tBexXj0vaLMiwSx1IkqnEMsS/B/Yvx/ar6310H46ai+SAVEKZhkEKlJlJ+2OyA4PPnzAj2WTvOkGIFlWYboI7/fj9lrilHts8Yh/pBQfUVwSh6QR/e0hEW8UYUJfkm+JWJPWq6bsl1Hwkt9peYUCyqWgnksZBOEC25f6GIUPw8VlEMgR3x/76TKB6E2Vm3aH0oX81vf7FvvXmOE1WX4ij83fU+1gtci9hQ4Zr6TJ0oUpi/xthpeylPqk66KnykzqfVS3BKmTFt0HLUZcF+V+X+q1CpNA0onajOB/6XMh/bf13jB8+DtC6qFqx0xdwNBZoeChXI7Td7b/sh9mV+lE5V1sx1e2GuVT6SzhL+1HmL4Ugan3SLcqXpEroS4pEtUUa8KkdVLR70T/H7p5YV0VA5a/vUJB9U+xAFIWUf8v6YTuUhYSTvAjvQU1SGdJwkXlL+MQcUdQNoWOQmKcrpOQ8EGeoiBRmxbrG4ii8IM23YOHclKiaBwUJBLHWUnvCOP3jP4/GXNAYvyvSMiq/jbHvHqMJmGjMYJSjK/aDgmrKYdjPx13pCAvaNcjGwhtCmadCP8P6nrc/4rdR/av8mNK4qv6ZNY3qUuhGKmxkNYZVPqmu28b/+u6p3Qmbua9pr/o1nTL8heSaUg4ABC5wufVlLXE2q4WU28IdVUulRKySjgvrEvRszMQ1S13+w/rS/T8FtiHtgpRTRCf6KWAcqgDaQ8LhdgtCOPFdifteuARhREb98th/UmUhQ/PK0R1WxM9/4u+JU7fByx2G2UnLMNyuYwOPf43KJd9FKLxZOAm5R/XheBvwE+ER2T/wbsLCSd6N+typHej7BHKgbDPFOK6iSh9Uy5btsz05X/pj+V31r3ip3Um8UHVH1MXIpuQ6P/LPrwC4JeDOhjZP7yw/Y0LLtZZHI/kI1leyXbQ1KvVzbwv1Hv0TKHGJJ56F5Gsr3EZZqURKUn+V26JPiR0K3geSnr8XwjDhXr3VD+MsE5IGUm5AFnj/+i2qPxgsX/56SXsP853NM4Ky0PQ8ZjhBR9xPTTvCeQV2RPCBvlW/V01BPeWUSh0qHY8ia38kFHevm38b9iAhAvCeIl0zXt1+EgvFllgxGvqyETCxfcU4IfPKeXAAAM/XfbRzcpPe3sI4/GjumbmJ0hP9wtBuvK/tGG+r98N6niTcUg2gzTiNOP+P4hT7rHHk24HJa4gjqTefT+0/8Ax9o/NI/obiZiSiLv2l9+JNix087wCSuW4/w/GveG42AvGxok6HBq6e/8fyxDVDyNPkleJD5EeYx2UQ/2Lm7hbwyvFBCIl/SQKHzIeiv0FL3wPIm1JFKevNauJJIEX9VGBvNbQqg5HbVhYAYJ7wrvCTOrwkP4/fHaJw4l+dZsd95ta7kAPftgPBX1hnEXRVVxWXlgGifpqEgYsGPV+Wvt/30/0Web4X5ebxCH/izy6PMVf9BmXSzKeWN+iPV0OMu7yonwE8gb5lTQQ5t/Uh/jr+iBovZthS+UyOsI8SFkWvAJKpVJkGNG4NxwbiD0LkiN5fpW4dU5tzxm+MQ7VccpPXTd0GK3/pC7ie83wQpBm0k/u8cM6Z9afIFysB7kvuMeIX/5X5eVJW1th/K+f/+M8ILJdSUPGK+b7AqnfOpx+/k/0ZaHQWm4dLxCPQ6N7lDx++A5Ly2XLlvfE7t2Rs1kJdeGVSqXo76gCKenEPWpAPTHEuNPV6cjLBf2iQZAXEBrpsEXGQqEQTIIpGYIHuI6gE1B50QPzZEMSIHnUDU3gFoSRjkyHlThK5VgviAaRQdhSqRTKE0yoiA7l/vBHlH+t+yivUaUvBMaq/CUecddlUC6XE3HIPR2dnYk8SqMi8XV0dKBcLkf5KBQKmApfNkgcnV1BHOVyGZ1hfJKG3CdpiA4jWXwfHR0dUVidf4T5KIS68pQ+5TdUvSzpeqLKW2SN8hnGbfqLnOIXRBPHI24SdmpqKk7PYi86/jj/MVJf5b5yuYyOzs5E3kx/rUtTNi2/eZ/8LX7lsD5oXUp4+PISNpkf0TNqtH+ocBKPlkfS0OUPAGVlJwhrkJZN512ruCz2r/ImAxuodG2yw2b/obvv+1EnrOPyPC+hF4lfZBf7F79SqRTFI+nLPYGdx3Um0qG2f8Mtjifo+P2E/ZcS4eUeUz8SRuLr6OhAuZS0f7FFiUNsvqzsX5D7JA2dtqSj7V/yL3iehw5H+9e61mlIulkyiJuue1qfpk4kbCX7D8ovjt9MG0oeua9cDuqHzlvSP8v+g/xr+c375G/xK2faf1L3kgc0wP51OIlH0tFlqcsfmf1/slxsdaxssX+dts63KTts9q/8RR4dl1eD/RcKHVF7JvFI/iWc7bdOw5RD/vcz+n/Bd7V/o/8vlaYS6TbX/pNtTrkUTMrpcKKLcilsG8IeXtKQdLNkEDdd97Q+TZ1I2Er2L3FI/Gbans3+S2V0dHYEA/UMO9a6NGXT8pv3yd9APDEq92j5dB51/DDsf6oW+48eeNLpJMrSwf71+C7Ku+ovYbN/9UIhiMLd/vULdN8PHgx1WInDZv/Sx5empiz2b+//o3SMuhS5G/YvYxMdjx+9sJGPt1R4w/71eMFTL9M7rfZfCtqsBtl/Z0X7dx//i5+ZhqSbJYO4iZzih6rsP2mPEofEb6YNAOXwpa3cVw7rq86b6a91acqm5Tfvi/5WdUzu0fLpPMbxB3kUPaOK/t/L6//Dl/jlcMyr8yDochXpsvKuZSiZ9m+Uo2foUvD94HWujlPrRdKT38ixfwlr7/+1/cd1ReIWuczfOg1TjuD/uAwkHzq83GPqR8JIfPb+v0Xj//B9UaGjgNKUYf+FYCwAIPpIr1wOxgbmOwZJN0sGcdN1T+vT9+NJEaGQsv9knZQ4JH4zbVj6f6mvWgfa39SlTs/Ps/9wMkj8ylXZv9JPlfav66kOZ6Yjcus8CJJvjY5P3seZOi6Xy+joSL7f0mnrfJuyY1rsP6kLCWf7rdMw5ZD//YbYf2zbHTXav25nddqSTqb9h/nQaYo+dTjRhda1TkPSzZJB3HTd0/o0dSJhbfaffMEex2+mDYv9l5tp/yqfEr/co+XTedTxo8b+X9dTHS6RjrTlXob9l0oohHVEyMq7liF4nxLbP2QeQCZMqrB/PVsi6emwEke99i/PZhK3uJu/gzREtlif8rwgetG60XFIPFn2L/kN/EtRPgo12L+tbCQdkUHCis4Er+3tP66XOqzEIfGbaaMO+5d5g0LU3njw1YcxCD+Y0vfJ3xJn2cH+9UcAyLX/IB5B3CWMxK3lEiR9SUOXPxz6f0nH1LHoU+dNp+3JwrmE/QdyI7f/D8pdx+U1wP61LiSc7bdOw5RD/vdrsP+C53lRJdQBAGBqagrl0NDNhHXGxF9XGB22VAomIyS8/o1Q8Tq8VFJTeMkUwsKWzEp80W/V4MvkpaQh/0setTKk0dENHgB0qDSg5JTfZoWTe6WhQyhLV1dX4m+dFzO86EDype/T+pawEof46/skrMglMppxFMKGV/72/XiCGLoiKv1KeElXZJH6IfFKnJ7nYWpqCkD8RYvUP0lHDAcAOjs7I91LWElPT6Z5OQ2OpK3zMjU1FYXTOhZ/+V/yKTqBYXCCPCyJHkphOUiYjkIBHaqR6ejsTKQFpVNfdZRabgnvGZ2GH9ZDKD1LPZD/dTitr85wElrSlHjqtX/98Ch60HqTOEX3cm/BqA/iJ/lAwv4DOYLfSTv1arX/8OWDYMar8yhyaX3Kvab9H5Nh/6UG2L/EIf76PgkrcomMZhyFQvDiRf6WPMt9WscSTz32L3HXav86f14b2L/81nrQYUQXUn4dHbXaf3C/1GGRRf6WvEr68r8OF+urEOlf0pR46rV/+V21/dfb/xv1U2TTaUketS6y+n8zXvlffif1mWX/BXR1HaP+juuoyFKP/eu6oHUjbhKf/C2XjqNg6f8lT5gu+++qYP/hpJw8jGj96zKSfOo0/Haw/87kQwWc7T+2O/H3K9i/jEN0OK2vLPs/OjWFUrmc+NBSZO1sB/tXXxj7DbR//cEjEE84SLxmHnUchUz7zx//y8QoarH/cHJE/PV9Elbk8lL2H/xfCD/2lDhFl3Kf1rHEU4v9H23Q+F/nz5sR9t8Rueu8mLI2yv7F7kUOHU7rK2n/nSiXgzJtTv+frleiewlvlpX4ST5g6f9lUkjihtKl53nRC2VJS3SlddHc/j/f/nV40YHkUd+n9S1hdV3QuhE3iU/+lkvHUZju/j9c0VCaKkV9Y9T/hx/ziLtX0P3/TLH/ZP8v7b0pa932rz6YE3e5R/7W+qrU/5cbbv+x3iRO0b2EN8tK/MrlcuIdi2/YvP4N0/5VHZT75X+RifYffOwpf0ue5T6tY4mnofYfpjN7+3/z+b9J9h/mVdKX/3U4ra8s+29K/y87e1jtX9qvjPd/YTyI7D/4SEHijt8Fil7iD4l0HZT75X/J+8yw/0L0IaHOk64LUt7iL2FFLpHRjKMw3f0/7T9Ky1f2X/DClb0hIlNc5oFc8rfkVdKX/0Vms7621P6V3iRO0b2EN8tK/CQfqKP/j1ZTz1j7b2z/33HNVVd9JopdVS4YhawzpoXXyhA/LbgIK0JoQSWcDi+I0k03wUwHSnZZxm3KL2lLXCK7+El8YgRRGirPhdCIPU/2/ggxGhcJI6tU/bCiiEzRZRR2HF0si280KiKXhNOTXBJH9DsMZ1bSKJyqdOXwix6Jt1CIvwDVaeo0BJFcwsXpxeHFz5RNo+NEmJZuoMQNEl8Yl6caMtGVIHnQ92l/kcdX5Sbo8tI60PKIW2dH2FkhueInCh/qyfPibRp0nkQmKWcdt+RLd4Byn5ZP7pcwhbC+Sjr6t+RB5JX4JB7Tfmx5l/8FCSf5KZfjrWnNfEk4HT4gbMzVFh6oaP+xLiQdvxH2H36hHwaKZDTriMQhbhJO4pW05ItvX5UZEvYfy6dlQY79ywq9ZDnHupX7JU75H0anUy6X0dnVGX+Jb+hI5y9II2mrUOF0emYcEq/EpzHjFB1omXV8Oq4s+8+6T5A4/DrtX8IKpv0L8juINyhzSRtO9p8sCy2f3C/3FHLtP65zaJL9i5uZLwmnwwsip+kmmOmgGfZvybPoU9wFHVbCSbxBWuVoxTcy7T/WpZYFufaf3f9LOGf7N/p/rSOdP1hsFSpc7fYfywNX+w/TmpH2L9t+V2X/Rhw59i8vScRPy63lRYb9yxZFBU+tKDR0KoiOJD8u9i9fHtvKRNx8m/2HfVwURtt/2UdHZ0diFbKr/Re0/YdjC88LXlwVqrF/Zbd+xvgfjbL/cBJXxyn6kPslTp2Waf9dFexfr05GnfZflnplYMYpOtAyJ2RS+ZwZ9h+XidaNpI0G2n+hJvsvRyuAJT+Sb1vezfslnOQnYf/h6pIwYBROhxdETtNNMNPxTPu39f+ybZ5FD7q+djSl/7fZf3CvhNW61LIg1/5t4//a7H/a+/+Ogt6BMdBBZ0fQ1odvGXR88tLfmzH2H//2/eDDBfktMkk567CSr2rsX/Jpqxfir+WFsiEgeDek823Lu3m/hJP8JOw/o//X4QWRM+UW/jbTgYv9O/b/rbP/uEwkfh2fyIJc+2/k+D94SS19h9aRzh+aZf9GnKIDLbOOT8c1E+1fyyYySTnrsJKvVtq/aT+2vJv3SzjJT0PtX9XV4P5kGIlL+oSOjo7E1vgz2/5LKBQ6oqM/JK1Cg+zfS/T/yXZU5NH5kzRMJBztv/H2XyqXo4/G9NFWvh9P8Mr9ck9hNtm/+m2mg4T9B/ea8qftP5al/e2/Sf3/NR//+Gd0IN3BSOCy+oJAF4zOnCQqBHHGFUc31loIfY9WgDZi39gTPAoT3i9fGETuZmEaHSSMiq7dJc3IzShUIDxzJWwkJS09QSRxy9cx5XKw1a8myo9hCPoql4MtkqO8KXnNxsav0EhJBesIv6Yx/XUY7S6T1+KnDUji8f306SDJNOJ4JS0zXLKsk0ZghhV3z4u3XTXDa134obuuZ4KUneTLrNPi56tOSNC/y+FuwUHYcCWHGojIlmf6fBkzL6jQEekwkl9TFt3YIWU/cb0w9S/3e17wgqSx9h/+78VbFGvdyt9CEE8QV0J+dSZQnOvYJvPs36/D/uV/3w+2t/MsuvGUbnX+EvavBq8+1HmJOfYvfhrPav/xihotu8ik7zH9dRgAwRkCYYdVcLB/EzMN+S1pmeHMuirIfTqsuOs4zfCSjg6v65kg+pV8mXVa/PwK9u+r9MywZjzyt77fU2eIiL9vlkcqv370klb8zbI1dSpxaH3FccX3NMP+ddpaJ/K3oGWzya/9xb3QQvvXfnK/pGXLX9L+7f2/vld+y6XzYd6btn+H/t/V/kN3KYPAL8iHTs8mm/aDpe6aMks+47KOvKP7dFhx13Ga4bUuxF3XM0H0K/ky67T4+RXsHyo9M6wZj56IiWRTH3NIeN9SHmZ+TVnMstU61f2C1pcZV1BPk/ZfCB88fT/oqyQPpq5Qp/17Rlkm64S9rvnhmT0p+y+FdlNuoP2HaYmb3G/av+jHS9l/3P+bcUS6aKD9e7oMnew/fV/S/sMJNJWeTTbtB1X+4m7KXEjZf9qexT0rTjO81oW467optNr+g79bM/4vhe0NarL/OKzILr9FRlNXcLF/+IkJO4lH0LJFcVeoa3J/qVSKJtLkXgmfsP/w7DC5V8sod4s82k/Caz+tmyh/RvuWb/+xfuQefbnbf2zHcm+chqv95/X/sZ2gQploP6jyF3cdXsJJOoA619k3zzjTcYqsyfTNdLQMup4Jol/Jl67TYjOmTQv6t6RnhtV1wbSV6P4m2X9Cp6peaH2ZcekXzPLeSetA50nrSuLROjZll7S1TuRvQctmk1/buLgXrOP/OP6G9f9Nsf9kuchvudztP1nnRWYtk77H9NdhpO0v+z78Gu1fbAeWumvKLPHqshbkPh1W3HWcZnitC3HX9UyoZP9aNr+C/fsqPTOsGY/8re/XeRF/f5rsX9dTCSuyy2+R0dQVXO0/XJxlfrwJoyyDCc+k/No/cC+jUOhAqSQrOX0AXrRC1veD5+6s41C0jIKkKR8nip+W1dRNIn9Ns/8w7+GYoXn2L+7JYyBEHp1eLFsSMw35LWmZ4cy6Ksh9Oqy46zjN8FoX4q7rmdAI+4dKzwxrxqNtxZYX8fct5eF5yfmOgqc/hkpO1qIl9h9Mkuo8aR2bskt8Wifyt6Bls8mv/cW9YO3/M8b/qfoU/NbukqaWPwif9NO6ycpfY+0/eW+j7L/jU1df/RmJSDwEnRldUIIOr8OJu68mboMrVpbcrxUpaeiC13tvx/HGmdKVMCog48FBKomWTadlFpBZCaQgJD6RxQ8rmO0rTs/z0NHRGU18a11p9ApWwVcGFe3/ruSV/CIcbIkblMFFcYX/mzovFArQDx9ynzZ2wQu3bZDtGHRaOi4td+AfyKmNRPxkclm7SXz6f4T6kLMGIjfEyJkjElbyIXKJO8I0tC51/uX/cvglVElNiBZUGkG4QOelcNWE5A8qLZE3SidsqAX9W9KVeHQ5iD4kbnGT9HR90Pkoqa0M5D4Jq3Xv++FKdKOOip+EM5G4YcRvpulLB6lkl/tT5RWu/pX7o9+QQaPN/oOGTcKachUaaP/lMB8yoa0bYlMGGQhIHjVSf7WO9csp8dN1SNzkHglbKHSktkNPWkiyXmj9aXfPC85mMeX1HOxffsPQn59h/1Le2k3CR/GqemTav8ZTgzi5X8cv7hJW61L89f9u9h/EUwrDSv6g0krZv2Hzwe9YrursP1mXdf7kfzf770i9lBYkrNxnosPrcGaaftT/u9h/XH9ETh2Xdtf36bCmXIUG2r/Oh1+V/UfRJz5i0ToWJD6Rzcu1/+z+XzB1LrrQ7l4d/b/8Rt32H4TVMvg59l/wCiiVg3NK5b5W2b+ElfxBpaXLTtqytP0HSLoST779x+np+qDzoe0fmfafvlcoqBfhojPdq+jwIldC5+pFrFxabvHzwklmXS4SZ6GQnATS7l7YX8lLpUIhWD1mylWowv590/69eEIZYZ5EFr8q+0/qVhD9e14w+QpVf0Q2z9X+1YSSibhFcqfsP/TLsv+jR1tk/7FuRQY/x/69aen/A5272r/46T6/mfZfMLYyl/skrNa9ea/0UOIn4Uzi8EouQ+ciu+/H2/jqD5nN8oKqP/Jsq+OS3yK/3CduEq/g+/FHIrK1pE6jEI7hmt//xzJptI4Fia9Qlf3HOrWlJW4ij+hPu3vt0P+rPkPe4/hlH52dXWE89nrYSPuXMX1l+w/iqc3+Azo6gt3dJL6G2X/YlruN/4M+3lc6ECSshDPR4XU4M03fof+32b/IqePS7qVyGUdfegm+2s6zVArOryyVSiiVSpH7S2E48ZOwvu/j6NGjQLhVpfaTsEePHo1+T01NRVtjylamU1NTibTkXoR1oKS2STXROhb8muw/tiFbOqbOpZy0u5SD7yffBXmttH9VZ0Q2vy37/yCeUrmEzs6uxIfckpYuO/Ez7V+QdL1G2H/4v6v9m/cK4ifhTHR4Hc5M09f2Lx+8yngzKq94wlf+lwleHVfsXoi2Q47f/wVhIx0g+ZGolk2nVZ4x/X9o614yTTmrG2G6trQinTjZf9LOPNp/VBaCxCNhJX9QaTXa/n1tZ148t1Gw2LBXg/1X9/4/Wc90ODNNv0n9v75PhzXlKhjP/36URuBXnjH2H7jJPRJW3BCma0tL3EQe0YX35IMP+uIhiekMixBmGBFCBNEZFYWWSkHhaAWXy8n9zQO3OH7JiBhAcG9y5SpESSozWo5yuCQ+cleFNTU1FWXezKf4xWnpQ7fDQulINgSFQvCCqlQqobOzE0ePHo0qhed5gBecqyHb6cg9EodURtGlyCYVdiqMt1QqRZPFErcXVmaoBlX8fDWo9/3ktnYIH67jfCYrhriXw8FsV1fw8CVpROmFZ82UlD4kriBs3HnbEPmg9C/5kr+DeqT23zcaSnHT6PogLxFE3wXVGEh+pa6JnpHRiMjvIMnY36wj8tvz4m0K5d5yqRStxIbRSQhBGrFsOm6oBsrUg+1/IbCjoEHSHYPgSZkZDZ7WnYQReUVO8ZM0JS3Rs/wNZdf6vDsdf5C3+GsqudfMj19Obh1pbucQu8f6EPuXl59mPtP2rzoxVX8ieVVZZNm/p2xZdKXjkL8DXcaDFrlH4pUyE51L3AGhzhP5jfUhutD51fGY4fRLmIr2r/SoETcJK/m2IemL/iVfHYUCjk5NodOwf4lbwtni1rrWeRe/+u0/1I/y17LIb1NG36jPCPtDr2r7j21Jp2H7X5B0Pav9J/Wq64nWnfYT/dnyLGlVsv/q+n+L/at86vKW9LW7hKu+/0+XrdaH/A1n+w/ukXPgdRyiS5GtOvu39/+o1f5VHLH9By+1dPloPWrETcKKLDYkfdG/fNggf5v9v8Qt+fd9P5j4iqyxdfav/W061zJ6WfYfTi5K/DoNXWYSHqrOmXqw/R/FWdH+k7Zt2oWM77Sf6M+WZ8ljaap6+9dn9PjGsQmJ/Kh8ygSwxCEfMek6I2lWsv+jWfYfnlsGr7L9d3V24qWXXgpelKiy0fVN7jHj8P1gGxmRLc/+ZbWwUA6ftSLZc+wfKfsP8pocQyj7L5WiFUFooP3LS4eC4/hf4pZwtri1rnXexa8x9p+0Vy2L/DZl9H0/OgZA3LQ96fi0bGY+dRnoNKz/h/eUq7L/uF5o3ekwoj8zz/J8psutXC6HZ7cGfuUK9q/zVq6y//eVjNpdwnV0dtZm/0r/Wh/yN5z7fzOOOG3RpciWZ/8StyAv0E15tY50fnU8ZjgdR2T/rRj/Hw3tv+ChUOjA1NGj6OjsDN6fqJXjkg+dT43Wtc67+LnYv36nIOHkt9abuNl0bsroW/p/8wN/CadlM/Opy0CnEf1vHP8jYW32L7Fqvep6onWn/UR/tjxLWgn7d+z/dd60vvSq0rLvY+roURy3cCGOmTcPx8w7RmckkEn0EVqZH/Y1Ud5E3ui22E/uQXif3C/hdFlEegzre6kcHHkVxeF5OHL4CI6+dATPH3oenZ2dQX4s/b+UuVeT/Tdq/B/UTXm3Uov9Sx+gbSYLSb8w4/p/pXv10arcK2G0u2+xf8mLxC/htGxmPnUZ6DRs/wuSrufU/7fA/sOz3MVN4pDxv+w6pN+Xapl1PnV5S/q+X0ZHId4C2ncY/+vnf734QO6XcCKv/I2a+//4HaLoUmTLtP9QL/KcLBop12n/5rtUua8W+xc3CSuy2DD1LzqTv9vP/uM6of1tOjdl9Guwf+lPyin7N/UQl5n+X5B0vQz7132jridad9pP+glbniWtivZfZf9v5kfnU5e3pK/dJVxHR0c0xg/CxXoo5L7/C9LV+pC/UYf9y9+iS5Et0/4b3P93/NknPvEZUZpWhgSShLRQEk5HLvcIQXxhI6XCS7xayTojmuBFd5y+ZErwVeOSyDziL0Z0OuZvrSwpEHErFJLnjfh+cgs4SU8mUqWQdOFLvB3q6xUtpy54yYdnGGJnR/CVqL5H8itInmz+WXmOBsCqfLW/NDhyrxClpVdZGzLosLY609HRET34SHpifHLZ6qN+CPC84Gtz/aAm+dDGJWnIb7NOmPfp8tPxCPrlSIeaVDfv1Xkol8qRvvREfDk6cyGWTXQlf0taWodCp/rySC5d7r5qQAXfaBhh1DmE5SNhddy2spT4dH2EMTjV4SXesh9+mBG5++oKkDglDinHwDG2fz+y/7hOVbJ/P/gj/jvD/qOkvGDgpeURHUo8Fe1flbnWvfyWyzYRZ5aFyJCULylX4J/Ms/yWv0U++S1/68lfiVMjf7u4exl1RutDZHCxf50XkVkjblKW4qbzYtYJ8758+w/lrsb+jbzE7kHnDiWb6Mp2XyxzkJ+m2L9F33LZylLi0/URDvZvpm9D4pQ4pBw14qbz5OfYv/zW4aWsxU3nR+dT/pb05KrG/s3VmHJJ3Gadssllyqfl0v5ZeRb55Lf8rWXXcQs6rTx3L6POVLb/DhSqtf+wWsikmJSlhDN1q+MRd/FztX9Uaf96oityLyXPXC8723+Aq/3rj638KuxfxlueF4wLbGUp8en6CMQT29H9qm7oeqbdERal/CVxShxSjhrfDz4AKBSSHy413P7D83/lb9GhXGL/nfKySp4PLPav09Bx+EZZyL02ueRFmcgjdUj8dT2w5VnyLb/l7+jFucX+PfW3dtd/J8Jn1JmE3fjBy7aZ1v+jSvvXedHutfX/AXn2rydQBd/J/ps//jfTt+G52r/oVdVdu/3HedQy+OGHJuLu2ey/gf2/TkPHIXGbdcomlymfPDuY/sn859u/lj2OO0b+dnH3MupMxf6/IxgDlMvBB++w1EeJxyaD1yD7l0ksE20n9dq/rDSGkk10ZbtPy4ws+w/fUUlZ6jok7lLv5N2JLS0Jq+O2laXEp+sjGmT/hUL4Ds6w/6mjR/GyE07A/AXHokOt+pOjohL36vofxhUhdV21IwjDaJk8FVb+NmUuhO2PpOtJer6Pzq4udHV1oavrGBw+fDjSoZSDXDDKQpedrleSnqD1aPprPWu9iz7lt/wtbrnv/xzcvYw6U9H+Z1j/L+8xzXt1Hsy8aPeG27/SlZ9j/xKfLS0Jq+O2laXEJ/cIEp9cEl7ijXYDMeqM7uELhXiXSknLRBY66Dz5vo+uzs5osZlONyGDCi9lrctP0PmUvyU9uWrt/+X9oV+N/ft+vNpZ6U/LbZah/Ja/RT75LRPAgVsQVuLU6LTy3L2MOjOz7T++t97+v+xg//q9gblCt6uzE9o+JF3UaP86LQmr447LMrYDiU/uESSPckl4iddM34bEKXFIOWrETefJzxz/h/412b/9/b9ctdq/jkPiNuuUTS5TPi2X9jfzL3+LfB2fVGcAm0LpiOS3VoKu2DAql3lvnMFCpEy5X+4L/CW+uHGQwtFpSTqicKj0oc6r0zLAqEwFo2ESdxU4VlRn8EWDhAPizsoLjcMWh1cIG3klsyD5Q+inZZH/pbJKPqSRkN+JsGZDp+LSvyM3pQOJ1w9llTCQrYoMQ0tsi2f4BfLFDZzOZxSvUe5mI6Ux8yJo/UPpMDIgZYgd4dcvcsGiV/lf3OS+uP4F8Ut+RFc6f4Xwqw3PC75kzkpPdKVl0m6C/Ba5dHhTFi/sSHV8EmdH+PWbxFcI7c8sm0L4ICN50y8aJT4JW5v9x+Wu7V8/yOl7JB3TT+fLR7A6x7QNCacR3ZT9eBtE7S5ymm4dHR0oKd1qChXsX9I3dSNuEldQtsk2UP6Xe5Fj/3rVj6kzs5x1vBJey6fzaLV/lbbpp+XLsn/Rk4StZP+lctn60G3KKnmJvsJuuP3HdUfilXBaBl0XstITXekw2k2Q30n7j9sBnUevJvtP1iEJL3kTeeW3/O012P51vPoeScf00/mSuHU8efYvYXXexd0WtiP8olHcNF7D7D+WRf9v5kv/1mG1jk2d6bTMeCW8lk/ncbrt38yLEMlaCNq+QqEDXtgPSPzyfyPtX8cr4STOQob9ezb7D19YyrZooj+dT/ktcpnxalm8muw/WTYS3s/o/zsK4QvOPPv3g91ytB+MctflJHqR+HzEE9C28tf50uVglqf8LWi9iT5N90TYcPVvR2ewolnCaTxl/9LvSF8s6Sd0E6J1X1AP+FomfS8q2b86D9Pz4h1LdByJvGbYvx5DCM20f6lfddm/0qHkReKP0plm+w/CxXGLrnQY7SbI71rsv0PstSr7D8pa8ibyym/528uwf/nwwbzX98MJpyrsX2Szlb/oStdNmYBBlv17SDzDiT5hlG0UXLk1p/9P110YNqLvRSX7N17amjoTXZpukq7Eq+MQmmn/EtZu/0HYcrkEWQigMWXVeZH45f/2sP84PdGVDqPdBPntbP9Hp6L3DoWc/l9W2YmblkHyJvLKb/nby7B/ud+8V9xE1kKO/SO0Z0lH/EqlEo5dsAALjlsQuMnW5+EX4Z4X9m1hHDq+IJwxoRuG92x2HV4+wmPGwjYsGSoMI35mHOrvzq5gB4KjR49G+RZ/KVt9j/yv9ZNt/3F9NHUmcWTFK+ETZafkrtb+5cON+u0/wMyLoPOLabX/WBeF6bb/Bo7/JZwg8UnYmuw/HE8XOgrRwhitFzO+IJ10+6/zpctB4imXg3dGWgYYZSj6NN1tYZvT/8crjU1Z9P9aP+VSKbEDnH5miHRcpf3L6s9YvmQdrNb+dRnMPvuPbVTS1/krNMn+SyKXDu8l30V6M8H+VbnrctLx6nskHdNP50vi1vHIPVoGSBxRmkGdEHeRRYcVt46OeBWulkPC1Wr/ElfB1f4b3P97Tz74oK89JYGyMXOtI9GZkAg99YVAHF9QoaTiSbxyTxBnnF7sbjcuM235Je5RnKGPuMk2cp6hGD+s6GY+o9/hOU8+gjNG5KsCLzQ8IZV+2EAWQoMNZMrIi6pQEncp/JKgXC5H94vsejsMP6wYR0P9irvnxSsry6GRF8IG1owzcY98CWH46zKVMkb4wClpmfmXhlLqkZmO5HvK2JJDpyv3yIO95wXGWy6VIEacTDP4HRmIUU8jeUN3aRQFka8UbgMhX+cE4eP7JA4tm24AdPl1dAZ5Fz1IeZgdns6/pCFxif7lPqlbpfC8Gsmv2JGWsyMcuGj9aB3ovKCC/XuqPORewSarxFfItX/pDOKtN7xI5xk2Y5DIgw8g/CpQ6zXL/lHB/kVm3/cxdXQKnV2dKIflrOUI0k3WRdGjdrPlRdKJ0w22kzBl0vnQ5RDrNxx8RfHFeZdwcRp2GXzjww6dhoSL7N9q88nfogeb/ctvF/sXGSR+CWdLE0anq9HxAUBnuCWIIDLZ7T/+X+dBZMu0/zDv8lvKI7Z/1c5VZf+xXUt+xb60nG72n6z7Eo9ZB039CTZZ5Z64fubZf9pd/rfJrRH3rHslL/Jb36N1qnUgeZL8mP2/lsOWvuhRuwVhCtELJ7nHTLc2+0/HJ/dIOJ2GKbf8tvkHOohl0/YlYW2/Jb7q7D8OY+ZT4pcyjNL0kajDMqnk59h/R1X9f/y/zoPI5mL/nVb7j8/KlXxJGhKX1EG5T+pWNfafWMGidKDzAmX/pVBevaWhqT/BJqvEV1Bbe4p8cg/COLPc5X+b3BozD+a9Ug7yW99T9oPjKGQlB0z7D7eXjvr/HPv3wnSDFzU2+7fbHhBsI+k52r9MNBfE/tUHsyKH3CPhEnlLyRDKbXmpVCgUgh1QGmz/Bc/DUeNIDp2ujqei/Ru/tXwaHR/qtv+kflzsP3BLH4Ekckm+JA2JS2xK7is72L8fxtHZ0YGp3P4/9gvijmXXddDUn6BllQlguSeqn+G2vrLSVsdps395dsuSW+N58YswGOXlid10doRnBqbrWEcF++8oBBM/jev/dV5i3el0Xexf0gz0m5xQMu+RcDoNU275bfOX+ieyNcr+PVv/74eTBGq8JDJI/FKGtjTRAPufcrL/ZBm423+y//eNemrKUqv9IzxjsyNj/C/2pfOCOsf/L7zwAiYmH8c//uAAHtpzLJ55voQj855EaaoT8156FU5aBJx1+iG8+x2LcdaZr8W8efMi+SXvkRwZ9v/SSy/h5a84AZ1dXXH6CFf/hlOzkXSBgQVpePGL3+CeMJwff7QS3B2Ws6f6SKUXCac1IH9H9yu5tRvCs4j3/+a3OOaYY+Iwddt/o8f/YX2q0f71pIQps5lmyv6VXGY+o/ibbP9u/X8QV/z+L554qcb+JV6df0lD4qrJ/sM4suzflhfUaf9aVrlH10+JF4g/3BD5ddmLe/B/XB9taWt3816Eskte5Le+R+s0oYMwT5Kf5vT/yaNcJO5M+y+F22GrnY46GmT/YuuBP5IyVmn/8lvim132n8yDyFZr/y/x6vxDyTJVKkVjUF89q3YUZFwf1DM0wP69quw/rCSG3pztX8WZ5S7/2+TW6DzAcq/kRX770T1xWeh8ym+R2Y/sP9gK3ZTDlr7oUbvZ8iLp6HQz7b8J/b/3xO7dvo5cZ0AHFHdBBNGIEJKo7/sJpUkY+bscFrqtQZGwU1NT0R70pgLFKOReKSw5pzeSOwyvjdSUHSqfnhefa1soBCsM5R5fPVzDptDwdymcpIzyY+gwik/pRPQg4Xw//pouvCmlI5ETqgHwPL21bvj1oug8jFcbndkwab0ilEXKWzcy0dlrRplKh63vl/vEKOSBW8rEbDgiPaqBd7lcRmdXVySb3Gsiuo16MoPI33ATfWgZApnj/eyhG5jwZbOv6oH4eYVgi0dpJ806Lrrwla51Ocjfkm8dhy47nabELXGm85G2My1Prv1LmlXZfzxokjBxXQk6WptcXhi2kv1LGnKv6LOjUIgmagWvgv1LKFNGhLJJur4fbF0jk6sw7F8P5nRaGklXyyDpiR5kUlDypNE6gBoMAeHLqkiedPlHecixf7/saP9KN3GZxvrQ98t9BTXY8xzsX+7xxf7V+dl59m/zg6F77Sb6MPVWCAd4up4K4qb1a8anw2l9BflK2rvoVv6WfOs45AUtjLxI3H5V9h+XW679q3w3xv7r6/8lDblX6onUNTOuLPvXYeR/LZukq9OTsGbe5Lfd/sN6aZSbpCd6QJgfnaepqSlMlUpRu1YqlwFVN2D0/xKvjl/nQcLCZv+p/j8eeMp9WjYdv6n34P5q7D/QgcQh9/iV7D8SNdan78dfV5to3Ws30Yept0ID7F9PSut4dVvrbv/V9//6CAPtp+XR9q8nfvUEsNAZjhM1kna5XI7yFXw01X72b8ouYeT/SLZwjGumJ2F1Ol74IgVAereQcDLJD8N1hWcBRvKUy4nV1pKW6Ea7e178YjmqY+E22CKPZ8mPzoOMFRDVu+AlQafV/sMXFmEdkrKIbbZ++5eVqlpmuNq/geTT5gflb7qJPky9Faz2H4QRN61fMz4dTve3ki+5p5H2rydEdXo6nP5dTth/ul5LWCGr/y9n9f9Sjx3sX2L1qrB/eRHvZ9l/oRDYZFj/TNnFLmGUna7jOj0Ja+pJftv7/1iHQXyBm6QnepBwkheN1gEi+w8iMvNt5kfnQdeh/P5/Osb/sV2JX7mF9i/1QdJP23+AuGn9mvHpcFpfhUL8YheNtH/1UamEkfQQ2or4aXl0/6/LUYcVtP2XSiXs2fsY7vnHZ/Ddf34lnv3tieha+AiOPeGnKHU+iwXHvxwvHXoNnn/iTBw9eBJOOOEZfOB3n8L73n0CTj/t3yTS1e9sPIv9Hz16FK981cmBTD6ixR6QD3Lgx6u0opgAeOGuGGHfmCz9MEj0I1mOMpEMP0otnthVMnvhvUD4rkT100LZ9/HrJ56MJr+DW+q1/wCpF2a5Sfyek/0H9qX1F7i727/53k3fV3C2/+B/ucdvsf1rt0KO/ftAdJ6k+On4JJzcq+MVXaOR9i/lZ8mHDqd/l+uwf0HSljz4tuf/8L2ofj9qk0vimzp6FMccc4x1twJJI7i3HO1eEtU1zwssPWwbdJ9syi5xyv/yrlPXS52ehDX1JL/d+v/4XYAuHwknedEEH4nGbuVysNIZddi/+WGyfieFGuzflueoTGa8/SfvlfLR+jXj0+G0viRfck+W/cscjzw/dhgfUgbhY5uXOG350DKY8shRUb6T/cflIEjakgffZv9GXYFFNzo+s//X8Ugacq/o07QDCR/VF6UzjSkjEvafLCsJa+ZNfrvav/zW5SPhJC8aU0dmHTPlkf/FXcdbLpeDFcDiUWr4gd/JzItABTVr7YXGP1XDgd++KiDohkadC1AqxV8lS6Z9tWc3lFw6Dj8qBOO8Wz/+qlDuFVm1jH5ouFFHqfKiC9WckDXzqbdT0Q+vUTj1dxRnuYyCPvBbVyyVR6jfUmHlAb6gtg8wZfJ9P956x0vuqR695Fb6kPh1mlJ28rfUK8mH/K/j9kLj1eWo8y26LZVK8UDdoazEL/jKI/7qJw4b60HHXQi3WJMvhoXIXsIvmbWMgqkXCaf/h7IvqUc6Pm2Lpr++R9uQjtvUhbP9i2y59p9E5C5E9h+XWSX7l4lVW9wSFkqnImOHoV9db0z7lxKScPJb61vcPC+5xaLWo+hG9K4HylIOEr+E07IFUcT51GWgyyr9f7CyUMJ2dIQfWlgGSWYeC8r+/bKj/Zt2anTGWlaJX6cJR/sXf52mLkcdzlP2r90kPa0zM09eRfuP79Nxi460Gwx7MWUUYr0EX0BKOP0/Mu0/rhNCffYf/Ha2f4W4mWVrQ/RQaFD/L3Hp/EjdED9X+xcknPwWObS/lkV+mzL6mfYf9Bk6Pi2bjuPo0aMolUoohdveLTz++HDlADBv/vxIzjQis11nAKJ3NL68ONPhAkd55xX9rwJAxnY6HnNAHYTR+hI9xrpD6t60rQQk04zvSYYP0tJ1NJAh+Tv9EtALyyJR1mpVSeSmFOF5HmC010AslrkyxRYoSlMrWivcbEPE3yaL8tf3+H74Mi/s56K7pJxDN98PV5YaupDfoqMENvkyCcJ4XvgSOnSL/pa4VDkF+pN7LXF7xgcANt3JvRa7RSCBRBB97CnRJf5WujDj0WHCgAn3crmMwy++CC98qXXo4EG8eOgQCh0d6OzowLx584J21LBF3QZ7uk9V6cZ5DCiHD/Nehf5ff5AQtJNBe4ys8X85ftGk8yX/+zX2/174dymM34xXxy1uuh3X4byW9//BeeXV9f+xjrReJJz+H6Fcuh/R8em+2PQvyY4DTv1/4Bb0/8egXEf/b/uwAgjtVJVfVv8/VUf/L5PAIqOp34J6wWb2/xKzlIv81voWNy2L/DZl9DP7fz3+D8JLmuKv86nLQKeR/j+6JUrXq2D/Oo+iJ4lLylOXg5ZJ3NAA+5e/y+Vw9a8X9Kn6JbfELWmJrrQbGmz/8l5Gh/VS9l//+N+s7/p/1Gr/hcrjf7FRM3+B/Vc3/v/tbw9g/Mf7cO8ODz/7v6/F3l90A/OAl59yG45bNIaDz3Th2MWL0DX/eBx48vfw21++BwUcwWmn/v/sfXeAHMWV96+6Z2bzKmeBJBAIITICjG1yMsYYnLABZxtMhjNgHz4bMOAzBny2wefIOZ7B8bDBxsbkDEIiCJGEJJBQWsXNOzszXfX9UfWrfl0zu9qVBHe++95q1N0VXqr3qqrrdVcvxdy9VuLQgyMcOHcaRrQ2D8n/S6USJkye5OkrlY7/MvjLPO6qYaQt0N9YzmNzsw62l3EvaIT57ghxrgDbv1G3bGNHG9Q3gHVr21AoFHya2S7+n3K5ffw/zjyUJXmS9HikHHC+I3klfkkTtfxf4JM8EzfTqKtQbrUd/V/SlPVq+X8lSd8ixDD9/80a/wfzf+IO5dsa/2da2La1gHxHsdsVyG1VH0cRypWy22a14gO5Fndi17aC9iJQdxA6JY9xZB/6YhlpN+H4T2A5VcPumC954Xkt3co2QM3xH+B9AnkL5UzbQASvtUl3xqhhY6Srhuj/XCclba2tTYZ2KesTJ49me4z//xD+n9o/dbQt4/9Q/J9zeWPkg53SF7MP7qmt9H89LP9P20mWlToNgXqIBpn/h/qQvNfCzbIQOiWPoX6Zp73/236bfEkcPCcflJfXpMnzkEczRP8nDfIWyinbQNKodSSQrhqC/8cXn3vulTJRNiYrKtHIklgofGhoknCtRiXdWrhq8UIea/EjOzAOLJ5GDcPkdahEnvtrh8uXdTSlHpgX6kfmQWwpIA1B6kKWMc5IWVcpN5kVBo9ANvJAvExjGSM6TwRP0BjXuUj9ehqic6eOtLZPb/FGycpt6yq39QB1waM89zzVsDvSkRNJwAbDpc7kT+oENTph4iQN4pBykg55svWytk6eJK9SDqbLhwYkHcrPc1mGNJgv0yF4JtDJIzEIsX7sFjtYjvpgmjxnvbAdSIv8Uycqst+Kk/yyDM8l36THslIO2TYSl+TFDNf/JX3hGxJ4zfKyngkGf8kraTJf4osie1Mp05mH7eH/glcJ9jr9rrFsW/LKOjIv9H/KoDKTizQPwh5r4Zf62pL/hzSl3ZGOrMc0qTP5I38E4pN5rM98NST/T/OknJJXKQfTiYvnUl+SDpcSpBxhXV6ntmLrbB//T/0gbAfSJf/UiUyXbVSrXQiybipH6hshrlq8kMda/Azo/w5IJ7xmeVnP1LBnliVNqYcwT6YzDwByObttHXe/oIyyfC6XQ7lcRm9fHxoaGjBy9GhMnDQZLSNGoK6+Drl8Afl8Lthlw/o/+E1ZpUQcTsqt3EKxK2/SYGJmSUux3wzzXH5mCSwEm5/KJMvyPKsfpdwinmKZWmDTPWsiDUAgC8mEoVeVBspY3piUrqefDaiFWOAeXMqAW7xWDk9Y39oFyYZcOcF8QvZc2p+sKe2TeVZs9yaqUxTfSmU5ngtE4Hjuj0wX9cJ0X8+de/6Us6GQhrRTl+y48UFaR9Hiy7SDW8SFsudejzaV+mVZ1wgBndqgRKCe50yXeqIOqMMQqD+pH8+hUijU1SGfz6NQV4eWESMwYvRo5PJ5lEol9PX22jJiYXiw8V9o1pcxYgziA2pmyON/+lS/qjX/12mAVuZL/MxTWzH+c6cfQliPabLPlD/KR+D4IPNYn/lqm8b/7BZurEP8xMVzjrWh/LIMaYR1eR2OFYON/9wqjuWoD8orz1mPaaEM5J86kemyjTiuyR8hcsFo4mKebBvjfIcyhbyQx1r8VIY0/tu+QtJleVnP1LBnliVNqYcwT6YzD2/q/D/1Rdog25a8so7MG3D+X8v/BR8yX+KX+hqu/8u2tt3/f6//h+ssxEOePK+BHEwnLp5LfUk6pCDlCOvyOrSVAf0/Gnz+b7aj/y98/nX88a8R7n14L6zZMA4q6kbrhDUYMfYxmGQR1r8RIynn0NjSj7q6FhgzAv39Ghs3j8XK1aOQlDZg8oReTJ06LrPeU4sX6rm5pcXyq+zn2RQUtP8ECMdxIDP/CH1GpCvFuQVnJxZ4TTyGfLh6IX6Jh/U5R4JYzO3s6EAul8vYMmHr/N9eSxus5Z8Ysv87vgR+yQftIcTPPLWt/h/Iy/LqLfR/2rrMk3JKXqUc0l5lXakvSUeWIY2wLq9DWxnQ/4d1/2+hVjuQFvmnTmS6bKNa7UKQdb0cKtWBfMmGMtlApJ1nWVppm+okQSRsjLt7SBxK+J7UtbxmeVnPGPuQSCgHdWSEHUh8oX5kHgYZ/+VOVQP7v53TK/cNZT+PsYV9HdqgtDf+MID/m8CGlbI8EmR96qMWfqmv/73+n8XD8qzDdOLiudSXpCPLkEZY1+8qNaD/u888Cfxb4//cFSqUgfxTJ1x7kvyyDM/5I6R1hf8LHYS4QptgPts0y8/w1v9o70wP65ka9syypMl8iV/yI4G0BvJ/WX5g/095lLKwLI+0QWlv/KGG/8dfOP98HwCWwsrGlBVJQIJEzvI0EilAqBgqgedSebUUSWAdKjwWr65HkZ0U8rpWPQmSB6lguWWVVDrpeVqCT+0i71rbbVDIl1LKP30sIdWVxR/KAaRPNQM2ACrrSD2EwMBsFEXpzYxoS/Kd0XvgvLV+Ul7/RnJgHxjAyMkPb9YjLlYJx2Z9ufUzA78I7Il0eE0akh/pYDwS5CBVqxxvSAyfJhM88YganVvkbJD8QNgN8fNa6otAWSSwsw9/EHVNjU5DtgvLkaY8J/8Sp7yWeHx9ZSdYxtgFySiwT+LltVJuRdYAcPohLrUF/zesNhT/l527x1DbTyQPpEk8skzYjgZ2UUvyqZ3/J7X8Pxhwmc5jVo7UjyQvXocB336SjBTCBV3JJ3VEfPJcKbcMXsPWQjxMI86h+j8H62gQ//d+5OhJfZA2y0lemE+6tfyasCX/D3UmeeKReRKPvGYZM6D/Z+Vgfi1emS4ftME2+38MuTAtccpriUfWh2gTtiECHfI6lIn88VzqW56HwDrU82D+X6ueBMmDbDNZlmksQ7uR7Yxg/FdV/r/l8V8phd6+PkRRhImTJmHUmDEoFOrEw0TKDeGsl8UT9AAiLZvvy2f0K8sNlKccXolPnBtZz5arbsI06Kq8z7KeLC/pBOxIMG5eExZQIlLss6R8cHNUR8fxlCknWFDKBQmVldNfp8uNmXb0wcsAB9vPsu18gvUc9VrysJz8papK7dzyJ3Qir70+pF6lTlK6nm13LZ80l+myrOdRQGqFKlWEB9EnpMK7Y3bsJpC25IE4nMUJqlkQGsuAlSkbcPZl3UH2JaQXHnnOtvT5PA/0HymFuvp6tI4ciUJ9PfqLRfQXi4iiqKpPI27ijDLjf3W/ZjILOtm+Vb7Zk+al+Af7STwZfrZy/I8j+9Bc/A83/qdPdks+Q75ZxhiDOM5Zu3bpdvxP5SVQFgnZ8T/9YZvH/+zYJ3HKa4lH1mddoPr+NJNnDUzUSvnjuXx4Uuo+BNahnjkft+0y2PifBu0JkgfZZlJGprHM1o3/w5n/p/TluRLtIfmuJZcZxP8l3zJvKD+Jh2nESfvAMPyfvJBPWV/yKfVB2iwneWE+6ZK2rEMYzP9pT7XkI7+SlsQjr1nGDDD/lzu8ESiLhO3l/2Y7+n+xWMSf71qFxxdMwYb2UWgZ2YZx017CzNlLMGLEEvR1bUDnBo36xtEYP74Zk6cCYyZsBqJOqCSH3t4RqCQGzU3rsc9eYxGJ/kPqXkKSJGhubQFEe0Z8GNLPy2pDLXygLm11O9yHtAOcfKuXZZQrAyMeHFDK9odsT2EvPV3dvj1t1W31/7Q9CWY7+D93XpM/iYdpxPm/yf8xDP+3bWvrh3yzjBnA/6W8BMoiYXv5P7aj/xOkzlmeR8lLKJOKsuO/1Lc8T8F6aBRFgJPNGPfZEsCvm5EmMjtB1fYT6giCJttXlgnbkWUkn3orxn8V2ANpSJ68jqLI3rMaA6VsO6gB5DLb5P9pe4U/iYdpxEn7wP8x/5d8hnyzjNkO/h+5Ptn+Ih8Y5qcUzTb6P/t7i/Mt8H/RrtSJrBeWJ7AO9Rz6jdR5rXpparVtkQ8pI9NYZnv6P4+15AjPpQ4l32F7wNVj3VC3ku/44nPOuZKVWJDMSGXwSCEkAV6TKevgANyT+WEZMkGaYR5BOqgUPnJBROYZYYAIcEonY55UnKxPGv5GVPDDa8mj1IHXTUbZbnEv0I+nW8NIIdohitKtqH1AWpQhkA8vi6NjTLrtFQ0zxKFcpyVlC/XKNH9UNqDNSS7LS4MPcXl+gqPseEnDB71Fpy7py/aUbS5lT9yHtMkTy4S0pK4lDptmJxZwPMnyElcIBtWdg6wn08NBhWWlXpguy3pdiU49pMGyBMkL60ibYD2zDf4fx2mAn+lRHAHK6sXTjmPIGy2pE8JA/s8tS6SsGNT/szbAcpk2l/5gqr8fGfIAIBNkpW6IT6l0uZm6Im3SZV4Iyj0ZGeo2W6aaD0k7bLMt+b+ULdQr0+SRMpCO2o7+L2UnH7XyUMP/SWtb/F+mEcLyElcIUj6WCXEzndvthDK/df5fvV2O2Qb/p+5Jo1YZ0ibNMI8wkP+ThpSV6Qhwbs34X4uXkAcEOqBuatVnOd60kS7zAKBSqaBYLGLchAkYO34Ccvl8FQ+Dg4FdirJH1rVH8sMyKdhi1enVkNoRvD5YH5am/yxE2gY+L8OPTUtxMk3yMRA/WV7lThs+TaVBT0svxelLe3EcHyxnnAA+LQsy2JsJKAZFlbIBRSmOq+naw55LW/G6oQ25qp4PaVdOvoztyvIuvyYIeqxvxbb1/HmIR16LclYicR7YvxgJnfxCJl+s2gaztpLq2/Kd5hBSOvboeVK2Pst4fbs/+cavZy89sYfA/6XuwnRRrRqIx11S6nyhgNaRIxHFMbo6OqCUyjwNLPVp0aTXxhi3LVxqTwzysl8afPy3/bXHGfSrgPv2mKOF7Tj++7dGBW7mE5f5Xz3+vznzf95D8b6FeOUxehPm/9Q9aRhj70FlGdImzTCPsF3G/1zs71WZx3JSZ7KvqMVLyAMCHVA3teqzHGlbuqneQiCOULdhGYLFn6Udttng/v8/bf5f7deSPvPwJvi/f+j7LfB/82b5v/v0FMsSSFPi3Rb/X/TC67j5lxOxcnM9pu/+NA4/dgFOfk8Oe+82AlFSQUdbD3J9vRg5ciSmTpyCPXedgnce2IoDD+pBy7jnUNRdWLVmAjaua8QB+27G2DEjPS8YwP+TJEFLa6v9zJsB4NYVyD9skgXjXh4Q7aSQflZNcdwReZzbEBdBiR9kPUHDmOycjecSv1IKfT29mbE9BKl3lqnip8r/s7YVttnw/D/lgcBzHmlv0s5jF4jL4qrmRx5r+3/WFyhfmEc+ZDnS2lr/J46QTlieuKpbL+WR5RDUk+lviv8HfkuQvLDOtvi/5Jl0qXvSqFUGsNtAk2aYR6j2f1sndlvGcj2RcxypPwCANohzOT//YB7LSZ0xz8tcw9/4I0gdUDesX6scaZMuID+Fk4LnoYbegPSbxoDtUyR+SYc4hu//KS4Cz3mkDKSjtuv4/4/j/7VAyscyIW6mD8f/E639A7Pa2Ie5uH43EP/km3jlMQr8n2OYeSv8P/BVmUeo9v+07pDn/1tc/8u2LfEppXDb7X/CD27+Md51zLEZHl5dsgT/dtN3cNnlX8bNP/splq9YjgP3n4tCoZCpTzDGoL2jHTd973t4bfnr2HfvvTM8Pvf8Qpz84Q/hxz/9CX7805/g5p/9FM+/sAgnvOt4XybUTYhf6oIyUveD+v+qRYsMnxqQSLXbY50IKDwEQyQojZjnlqjdZ58NKWmwrjwnDoJxDZi4fbzlG5j8UTDPmxuSIxckrsoPjIVKYb7fisxNNqkbI+RmHWtA6VMf9vslsXNK5Qe5miAai/xRB3ADQ6oLu0jFPF9P6IrpsfuOCqHW27+hIYADkeBByghk+ZW6sFlpHp0/xEX9wNXNiY+D+7q0s6DzJA3agalh8LHY8oz5rCfxkCceya/UkTF20ULyoLWG0TaYybSkIjo6EfQNQeLx5QMemSb1FeKS8kqcEmQdb0vCxplPOlprb+MSnx6O/4t2Ie9aa8S5GEklQZzL+r8iL9rALoYPzf8zehnI/4V8vu9JtF9vlvmo4f+kAfe0cV48UUX+bR3Lr1IKOrF1JJ+kUd1CFmQbSj+wtNP+jZDmpXzIfLhgQs7pi7edkg4G8X+PUw/g/4Edy3NJYzD/t3zZurX8X9qZxE8aW/J/8sx81pN4yBOP0v9ZTpZhmhb+wDTWDeuEIPHI8ty6L8SRsXMBKZ/V/SNB1mHbSRtnPulonY5xEp+UV7YLhDzEJ/nluebb8Ntx/Jd0+BuK/w+UjyH4v3yikvyzDm2BdWr5fwrZtvIyK4W+vj4AChMnT0ZdfR0A+ABXCqYKRzWkPpGCytRV4kXELLCMPCKgKXmoxmmPsl7WR32esYFbex3SrC1jijukb49VcvNc+f+Y4YJ+bANdg7Yo41OyN96A40ewo1QaTMyAQCSXBT2LjnzKk/OTsKGyinYVA5B1mC8JuXPSIc0qEHnGuEUKiS/QA/mlqIZt7AKTToOiJZzQ8lypNAmw7cB2zchu8zzvVXZhec3q0eaHi8W0GbaLEW8BG2MX0wmhHUscst0y+WEbEjLypGWUUujv68PaVasQB1tCsz8ZyD6MTvtLOIklXxD9fiqVqysCSNwKjOU9BP0ozyWNrR3/ozd5/NcGqABIjH1QxdJMx/+qt0+1td04UijkAAU5/qfjg6xD3kLI6ipNkzwyTeorxCXllTglsI5xC6Vmi+N/rfm/bQvJD/VIGrw2cswfaPzP5fz9bKqHrJ8YU73trgnG/w1lYIXO4+FijKf7DdZrAxMlUErDqAoAgygqY3SuhH1ywOH5HMblC5hoYuSCgCvtWru3IskX+cd2H/+zIOdw1C/1jcA+eC3zpP5ciYy+CF63gf+HIHEOJIPEI89P/sau0DGgc4COgSS2x5q/KD03UXptaqVH9pzXRrlrZX/L917s+diS/0sZIjH/D7cOD8u097fjhqe/gwffeAidpS6P582AMfWj8a7px+KsPc5AS73d5liC5FPyK8GYdE4ibRywnQ9xso11Tf8HdKUCdHch3rgeau1qRMteQfzGcqj162H6emCiCP+2ehZubf8oWnZdiX32W4WdJkzEq0uWY+OmZWjf3ImkVI+RLRPRPGIs6pNeGBgkuRzyhRx2n7MTXl27Cs88Mxnda3fHKce/hvPPmpuR2dSY/1cqFYyfODGdj7m+PB2/LSiV/WQaJctqNO0PfL7Qg38RQfSpStZR7gUP2ovwY59fA9rWrEVdXZ2ntX38P6svQmgrQ/P/1JeG4v+RGD+3dvyXegh5hpNjW8Z/AnnikfyGsrEM03SN+//0RQdLj3VCkHgkDckj06S+QlyST4lTgqzDtqNeWI95g/r/Voz/8lwPdv/vHhCW8pOW5N/U8H/Z/sbYGAP5Yx1QvkrFzj2CeRrzMYT7/4HX/7Z1/HcyD9n/dbpbm/gGMIK+a2v9H8Zg4aLnceb554U5mPfgQwCAX9xyC777wx/gmsuvwDFHHulxKqXwzMLncOZ55+GJ+x/I2MbCRYvwmz/8Affcfx8AoKW5BQcdMBcf/sAHsdcee2T4k3YmeSaN/xn+n+7cwLphnRAkHlle8si00M4lKNfPyv42BFmnlo0zn3S08H/50EMq70D+nwacJb8814P5f8ALz0OZzRb9f+vW/0xGN+5eWbTz8y8swk9+8XM8MW8e3nbgQfjO9TcAbn199Zo1+MQZn8HHTzsdJ514IpRS+MY3v4nunm586xvXez7JAwDcfe89+P7NP8aq1atw3lln42Onnu5lVkrhmeeexbe/exMuOu98f2/Z2NCAmTvvDAL1w3OpP1lmuP6v1rz4omFFOAUo0ckRCRXKvEh0fkRshAG4mp64VDDPIYSpxSAbSwohhY7ck0CenhxYMsbqFgEC2pD8CGOOc7mMbGE+efR4ufhHhxEL+0yXdJing0mF5M86uKMTPNFpArlkXQaFlbJvXVJGuWBHPMp1qnISy3YG7FuaCQdRsX0QHQtB50Z9hekYQPc2y+mB+ooUjEmf/sjoWQyUXtfsaITNEC+PrJtNj6B1gjjO+cB0FNmtm4lDguRdykZ+JJ9wumDnw/KSN3kt8UK0jywbLqCEdTM2KfQaQi3ezXbzf22DoeLBB9KTeiGPgHuzZBD/h+CTR8CadhT6f1DW4k+3tuCbLhJku7EdY/f0k9bZ794x3/KYvdFRqjp46uWqYR/Eb6r83/JFnKzHcpRf6pX9BJ/gsvgpYXWfSzwq+HZCRP+vpP4gB9EwDUP0fylHCMzjOXkZrv8TRyp/SjukIenKAZN6IQ4JkvdQtpBPDMv/U1rMl+0sy6Z0U1wE6iKUL4Rq3i1/28f/w/F/YP8fKF/6j9RBqMPXdQMeTEaho8I2A7Q2GKkqiPwE0e3cYJ8XwcS4hPeO7MaXl43I1LH5vLZvFhgAWtv+Y1ydxjkzyxiVtxNmqeuQN8l/mp/tZ5intUaxWEQ+n8ekKVMzekvBwC07uWOYjjCGVAOydVneHrP4pY6Zn01L5QVSPPZ8ICaIvxbIPMmjTSfKahlTvqljn25cBcpkMbl8pzOXZm+kXXu5oG8tXtMRy9XLtIWTXaXlvN48P1kxxTskDoHIlsIKXwmUnaZDKCgsHwBZAdI6Vl0Cr2hvsDzbXeII7MLj8jUlPacXZJ94D/Oz7SwUVqVER1+bjMjZskjPacsZ6pYfWyttK6XS8qBsLD+IP3i/CNuuhl4yuhfXBJ0kaFu5EpVKBfVusViOC8bdsKtwbNQpX6QX9rlRxG3k5Phv+zXSaB03Dvn6+qzWBW13kk0XaWEZozWKXV1IenttugPyDtiFZOpxe47//YixqL8eDycteL1ch2LF6T4BuYY/VUC5s4z2h9aif0U3pk3I4QNvi/HOOTEa6yxO2862ryY/Yf8u+UrtIxwX0vYmXgxp/Bf6dVBr/Oc9kQSJQ+LNjv/pGMZyWxr/GWhhHsEYt3uV0Avp+3zKOMD4321i/KmnCc+Wc1hWVigrDY0yoCowqMCoBEolABJEUQVRXEE+7kcclTAq1pibj3FsNBo7mPoMbXDOKnTMdsvIFuQPf/wP7SO1Z2MMfhOPw61qNDpXZFgbFFp3BD6iN+I0bHK40nk8hP2jhs5pX2qg+b+YDw9l/v+Bf901DfrmbADYuGBv4oLCMsCbuDwjgsIs7695rkQQOM4GgZfv+6pvr9BmKC91LtuEx2QI8/8vP/5V/HnZnf76rYAP7HIyvnzgZcDW+L/fhSU7h2dpiUPilf4f9RcRzXsUuYXzgVVvAJ2diJLEjQMG2o2Wn3zx/XiuYT+M3u0JTJq4FKp3EpateAGqdyPqcyMwbsIs7DhrL4wcMxZm40p0bNyA1ZvasbxtHWbuOgNJw2qsXD0Nm944Evvs2IPvfWtmTf8nn0op9Pf3Y8LkST49tW0nU9qNWxw8dzja+trxH0vuR3vFjkPGFWA9O/6ndVvGj86M20Y+syXqTSmMxEfHHoD6KJ/yDUsXtCk3JjMATP+XfalsX5nGcsTNfP5kOUs25Xp4/p/1h6H4P3Fn7C2ws5AHAvN4Tl625/gf0pB0t+T/BMk7ZTMu3fKZrgdhwPE/5U1eS7zYjuO/bA+CxCHxZsf/bF01hPGfPDOPQHpSL7UeqmT+lvxfyh1FESrlctUbvh4nsuuLUj8EprEe282XD9qA8oX1eJT8h/V4zTztbIOfP5H8ESfTGAA2XjeuXWr4BvGHMhJq+T+MwcIXFuHM887Fj276rsehtcZ+++wDrTV+eeut+O4Pf4CW5hbc9utbMaLVrqMopfDswoU447xz8eQDDwKO/3vuvw9fvuoqfOCkk/GOt70Nzc3N6OnpwSOPP4bjjj4Ge++5p6dBepThf67/p+3N9JBPvAX+H778t63+nxu2/2fnyMPyf2GLYf6w/X9L6/8CP2lLzYXr+Jvb2/H5L34Bp3/kI7jjTjvvu/GGb/oHLrTWWLN2LSZNnOjrPbvwOXzu/HPxxAMPI4oifOKMz2DK5Cn42pVfxXPPP4+f/OJn+ORHP4azLjgvEwCmbfzqN7di/tNP49vX3VDFt+f5TRr/1eoXXjA0VCKQCpENKgmEEBKxkF5LIeC2PCQj0pHhhKOBm6AzIBCP1u5NQ2ecyjVwyE+osEqlYvEGcll8NuAZ+bd6U/lTXM4ghGGSFwmUTan0qQ3SDnFGUYRSuYzIPWWuItFBS3yBEfBcG4Nczk5AtbYDrQoWAiLnyJ6v4KkCfy70O2CZYAsI0vW6DjoF6p5lDDs8PuURR4B7+hyBzUgdsB5xccbOMqxP3uy126KGjiV0SODEpJacIdRKl7ySrnL6p95zOftWPOuyHRDYApwcoe0xn7okHTnYSJtzFTLlQ/62n/+HqSmwLnFVKpXsNoXBTQXpmEH8X4mBVvo/pP+TXWOg3AMiqoYPSp1TH2yzuKb/q6qtl3WS9mEEtoXfIqoGbeKMogjlcinjK7X8X+rG5lncxhj/xKIc2EK9Sf9ne6S4bNCL5wOWcefkx+tA+D/ziEPyQ37htvogT6SJYfg/8yTPqPL/7JYixMGjrF9LzhBqpUteSZc8Uu/V/p/t74gHW/T/LJ3B/J+8snyWP6sXlg/LhjxIfUmQ9GoB6xLXlsZ/0jED+P+V/TOxObF8aw1obZ+MNcZAJwbaBV2NNj6QO6uuiMsnb8R7nxsDY2yaxWtgtKOrWTfFZzRw9IQyLt+j4njSPnAY6rPa/6t1S/8vl8vQxmDqDjumdpMZz2gLqV5tmiCQAWsXGCRwmsWZxV0bZJnq87DJpX1YmVFVNk2T5ULcyPAo6QwmW818l6BU+lZvWk0gGExOUcqm1g4mKqSrgryWNuJl9bsNS26yAkguqhRQ1R+IgCJpMZ94qBBR1iZn02vi3gJIerXByelwMXBL7RoXyLeZ/j8vD/WZYnN45FvmLsen+9JSwy64K8Y4stb9xu3Q/RtQShpR3zwCum81SuU8xu7+cYEJ6H79D9CVDiTRZIyYfkzme7ChrpTTjdQtF6VcBXt0epb9qNYaK5ctQy6Okc/ngRrjP5/aNq7vyuVzrs+zcw7iJHAc4lu+7I/5BjAANI4ciZETJ/o6kl6tc1muVj6P3d3dwObNtl8W+Tm3axHnWeSX7bot43+fVrivsxG/7BiD1SjAVOx4YO0pOBoAkUHnPWvQ/cQ65Ooi5OvrMW0C8MWTDQ7dPUbOsuiaMtvWkldTc/yv1Bj/hzf/1xv+iPLK78LooqPqmRHndYjHvR/xlDMAVYAZdPyvNf/PyjCU8Z+7N1UB+1zRlhhg/JdbRZPOxkqE69rHYllFoRwBBhVoVYZBBYCGVmVAlZ3bVxBFFcRxBXFUQiFXQi7uRT7qR2uuhCPVaJxkZkDVmIPzflDXmP+HbSB1GOqzevxP52LUbaVSdt+DtjhPVDMBAMuf6M/UHQym7J8DjMGdudcAwM9F+DYHaaoB/N/rfJC5PYY4///AV2dmg7u57Ju+SS4bAGaQt+a1CAbXehNYvg28fO4SLycG8H/qAuE3/4K+SdaXcr7zZ0eiK9ftywwEhaiASa2T0FrfiqZCExoLjYhUhP5KPzqKHWjrasOGng1I7FMng0KracGDH72nyvcI5C+0O835f5yd/3PdieVlPRX4P3q6Uffrn0G98CxMb69/JC4BkMvoS+HwZ7+MTaPGomXa36GiBdi8OkKcX4+WYgUTxs/EpBl7YfQO0zFq3ATk+jqxadVSLFm2GC+uXo1SJcbISRVovT961h6PCXXA7b8d5+UjHRPM/0ulEiZOnpxtq8i+fQuVzsiM7BNtAqAUnmxbjPOe+Qm0qdFX1YDRM6aESTVBqQi3Tv8YxtbZ7xOn6a7PVOn4v/qNlWhoaPD5cPxGUYSyX/8bzv1/qrNt9//URjBE/+c56YZ5xCH5Ib/4B73/r34Dz8pDXkmXPFLv2zr+M18N5v/Duv+vNf6/iff/7uWQWuP/lu//076Tn3XjSzxJUvHzFqZHyt1gBDpQNcZ/0pO6ZJsNvP63NeN/lracv0db9H/jgsCpbjLz/23wfxiD5xY9jzNdEDfVY1rmF7fcgvnPPI2VK1fh6COPwDlnnOnb8Lnnn8dnzz0HTz7wIIx78/fM88/DNZdfgaOPOCIjE+2UOv/H8v+B0tM2JH7yJm1pOP7PLZ9lHvMVdbkd/V+uUcsybBemiVUJD5JeLWBd4to6/8/aMYS/UqfkIeRHyoWMD2btQeryoi9cCmMMbrzhm4B7aFPiIp8LFz2PM887B4/d9yDiOMb3f/wjNDc34WOnnp5piwMPfQfOO+scnHbKhzN9zy9u+RXmP70AN33zW1vw/zdl/LcJRMIGJxE4JkNCMh/OuQi2fOq08qjdNi6Re9o07IS11pm3HSUvSuwzDxpHzhk+3FPIwhFZJsST8Kk2R0ezQwIQ53KoVCqen1Bu2yBWeVrQUUqlvAi85UoFRtwgU79sIPIURTawS12zvqSPIJib1lduQLQGY8v6Yh4ngQ5FQ8vgUvb7vr6OOyqnQ5alPkkvSZJUNmMn5dII4fROY6S+VWzfmI7iCMak2yrIH+tRV4RKksCIDl9r7dqW31eB100U2S3EDWDbRNiY1ulTaaQh20UC0ymTbE8ejTGoJAm0+8aZ1DMcTlmfuic//OXddyCpbwJ5ptwQ21GE/gTYADvrSzyxS39z/D+tI49a+L/K+H86WEtdSF6kfKD/u84aQjYzRP8nHUkzjuMq/zdV/q+gtbV70lED+H+lYoNGQ/F/0mM6y0g5ZJvL+pwoeP8XQJyEQf1f2Gf4k7KS31r+T9zknzRC/yctWW84/k+7JU7t/T+dSMDRIB24yYcJ/V/2s9vB/6kXprM8tov/u/FniP5PP0dN/0+fgJT8Sl2TB5bhT8LW+H80wPgvdSF5kfIVtdWdHmLwVxtbBgCMCP4ajS0Gf7U2WNdn+UuSih/bjHHfMoeCUpHfjsq4YIKVtQyIdqZ+S6USKpUKJk2eIj4rkB23rdhMSHmvBTQvq7swNwtsD8t3kOlw8ccy9sd25DltIbULpexNN9tT4q/NWzqHcYXcecojPA1ZL/VFqRvPg9SVE4ABRFuPPy4SZPXMYxpoZGqQbmybGcNto21EyZj0mOrbglLKlbUYrQ54nvIbiYbIYKBvC4VYPoTPCZ5V2pjpkXyIfgLGzcl8iRpAukFjZGQUfLuE9Oj8TClbTvJrm8QEWk4XcWwVyR3tTeiN6Zl2c3iY68d192fsEYUd0LXhNai6yTDxJHRteA25lp18HR51bjw61y1F3DDJ96cZXRoDoxNUSj3oL3aiUumDrvRb/sScgtes79McRFGESTvuiFK57Ockss/nnAmc/yv7WRLPqy+X6hlDHP8JRvT34U+Wkf22PPe8iDxegzekbqHDuHkz+eVva8f/RBss6srhltVNeGkD0L6qC+1ru9C5Tv46/a9rUxfaF29Ez7OrUSiUUV9fQUOhF5uLMRa8FmNzdyoP9cb+XB7Nmzj+F1+7FqZ/NVDelP4qm4PztUhWfw/lVy8CKh1bGP/fxPm/eBuRRzsmbnn8rxjghXIDLtk4GUt0HSrc/lBpZ9kGGnbbZ+tytCsFrW2fUUkiGKOACChGFdwbL8MduZfQq4uZ+X+yhfm/xevK+vm/rSP9PxaLcJSF83/bzrST7IJ7uVhGqa+MhQe9gWfmvo7nDlyBZw9YnvnJ9OcOXIGezb3o3tzr24F80O4kyPbDEP3ft6H4SVlpI0mSIE6AyP3iBIgq7lqLtPDn8qquxVFpd+1+SqQpt1aAQfxfyhPRNwe6/xftLI9bCv4255ux3+T98Mm5n8SVx1yJb733W/jhB36IX572S9xy+i346Yd/im+f+G188fAv4qTdT8L0kdORj+zDPANBp+qCGsD/IfyIckPO/90LCGxPs8X5v/V/ozWipYtR+O51ME89AvR0Qxn3dIwxiL3fAxUoJDBYq3dCT+eO6O+eiliPwcjGOkxt3Qmm0gATNaAEYNmrr2D5slewqa8fy9s24vXXX8Pk0aNQFwOV/lYUuyajp2MK1m6wb5NJ/5F2Rpm4tgPXC8ht430binMY+yCYcmNtqVwacvB3OGCM3c2HOrdqC8Y71ya0RbYRtsP9/3+n//No+7b/3ff/2rUvy5N3eZR6YTrLYxvHf2zJ/4d9//8mjv/CtgD7go0e4vhPXUheeI9NMMb4e24I2YwxPkBcCw9thHQkzVrjP33ZbPP4vy3rf27+4NqKNPkgE/nYFv/nvQjf7qz1A4ArvvQl/Ow//xOLl7yasXNb18rxu9tuw9sOOBDHHX20r/e/wf+ZzvKyPXmkHNSL1DOG4f+FQfw/0ToTC3pr/b+6LYbk/8OY/1MXkhcpH7z/b8v6v6UlaUr/T++gB/f/hYuex5TJUzwvZ332DHz0I6d5WSFslHVkuwPAE/OexAGHvB3Hvfc9+MHNP0Z7R3uVXZIuQdanvMP1/4iIWZDfZpCVKbxUEuvxSMIkzjRpcMxj/ZAOt4oiHxKkAnmtonTRRPIQiQmM7AykE8iFBsBOJNkwuVwOhoN9jY4g5IXnOpgAKceHLEfeSIuQOGNRKrtYyfJwdSTPcAvPlAeBsymlUBZPWigxcVBu8AjbwLgb4kRrG2B1ZWT7EhdpUW7ilE4tgWWMMYhysZ8QSJ5D/ZAO64Fu6dpW8mH5ol7FAC5sPKRjkD6VJoHl2TlKHuHaK9H2qdNE27ekeSy7dozElnpaPKkS8uPtxdkwF4STRPu1Vu0CEgRvF2KAk/khTk5cw/aTvKht9v/UJ5gWbcH/ybGKsg8eDMn/A1uv6f/uhtg+rGHPIzfosQxx0OZIm/KyDiHkhedauwcZnE1JeyeE9k3QLlhEfiRd8inPCUwfyP852LKdtPB/8ixx8e0hLXxenvMn+dDC/80Q/Z++G7ZjqB/SYT2CGtD/00GS1zzKupIX2bayDAbxf6lHys8j+/Foq/3fpkmd62ACzPI8J52BcDKP+Kg3+eaX2mb/T/2FaVK3zBto/Ce/5EOCbFN7baqDvy6Aa1yaDoO/Tj1hcNeeZ+sy38tk4KJU9pvfkhcGALW2bzEZ4/w/jkWQxgJlLJfLmDBpkn+zj/ynwbIUN0+8zWTdyrdDFSgrn68H+PFEXofAMhan8ee2LI/I8Gpp2HGrOvBHUC5L8iRlTuuynL1IswlKBKSzOgv7CZseorABQWXrhJmAx0lcrmQm3RhXlwFv8cYvHH9MN+JJU87t4HAyL8O7tzsXUHRpBGUV4M+VEoFQasKVqbINI96OMUI3nt8UQtUQry/jcFu5fIvZNPttFJkCyPoZvmgbVg/ye0RwOnIn4pplbGvSXq1xuHSHh23D0sbYa5mWGzkbCzvfjvyYPZBrnYnXkxNQzM+w+YIf3bQn5m/YH1HLdM8D7UEphWLvRnRuXIxNa1/A6qXz8OrC+/HC03/F4ufvQ7nU5+hl5TfGbVeX5gIACnV1mDBlCvpLJbcwE0GpyJfh/J/zRu7WQ5sY9vgv+nmOOeE57Ule1/qFZSTdgcZ/bofH8ZRysJ7kdUvj/6aywl0bG/DcJqCvowfFvhL6i2X3K6FULKG/v4wSf0kF5aXtyFc06ptyaGiMUWjMIWqK8MKmCJv6UjvQ2i5Kkd7Qxn/79D/5JJhhjP+R7vT1tgSm/UEkK7+NSrm7qj2kTsmL2p7jf2Q/JbK14/9i3Yjr28eiS8Uw0AC0D/4aJDZNaWhUYNz3mQ0MjOHCj7J9AZQNVxkAEfBQ4RX8pvkx9Og+T0vS19s6/xf3/5THlrN0mEZaANDd3oue9h6x8JTiljqR5z3tvehp7/Xpteapaiv9n2WGOv+vCu4O5ccgsfyFQeAkCAKbbEB4S/7Pa38Ucsq2kW1LIM5BIQFyKoeWuhaMaR4DExk01TVhysgpaMw3Ih/n0VhohFbWpkY1jUJDrgHKPaAwGJgB/J9A/nnONpb1WWbw+b89z722FPlbfwK8tgSwbuYWSDUSuHm0mxdHWkNpg0K+G+XeOhQ79gDMbhg5BphWr1FXV0BbRwdeffVVrFq+DLk4j80dXWjv6kIdNHYslDGiVQPJbPR37IlSdzOQS+8h1RDm/8ak8xYFAMrurGHYdsrN8LgQLOz7zYJK2fmv9A9hdxB+Kf0f/v5/6P4v8W0//0/HquH4v/4/cv/vbet/1f1/yovanuN/eP/v7pExxPF/S/4vP+dm60RIEhvYi6LI7X4TIRZjOXmJtmL9z79cVoMXnrP9PQ/CxghMIy2C3qL/O3xuV0+Pbzv6P+/VnnnuWTzz3HN4+tlnsXiJ3WUjSRJ7z2WAvffcEx88+X342nXXA453yXccx7j7vntx+KGHprgBLHxhEZ57/nk8u3Ah1ra1eX7CNpD6oRzkl6D+G/xfHqUe2e48vhX+Hzsbx3+L/6ffDOdxi/4vbHr7+H/WbiQPEg/HIqYj4/9pH0r6OuP/8CDlkLz8/d578N0ffB+XX/Yl3/6kRT7IMwSvpAUAHz/tdDz54CN47L4HccPXr8WTT83DD2++GXgLxn+19qWXjFQaEZHBSOyzLZkmIZaBULJteOucMo11aChRlH3rVSqQdVle0oN4W5Pl5TXrMp34aZCJcMY4jgGXF7tvydIIfL5odLjFoyjYJoJPO5MfI4yVvBOfbwghO9P8hFU4KhfmZMPJhSf5tq29Tp1bvqUcGiiD4J5HGk3guKSDYPD0spp0oU/KXPOcQfsaA4dd2LLgZaHugi0C5JELfSxPvF62wEGUcouygV1FTo+x3BJJ2B+ftiIQF+1K4ouCgYD2I3Fm09N259HzH3QiFrIdMOvwqJwepL2B9J1d5MRTcPSb7eP/7g3fIfg/eY2k/2fsPKuLsF345oikz7pMV8ou9CZuOxe7bYzwf+Gbegv+r0g3ju02M4FslAlwC+BCV0mSICfag3LxJye15D+bn9ULy/GNguwWHlk9o4b/S77lMVy4Ix0M4v+Sb+IZ6JwQtqXMYx2m0ZZZVh7D8sTLuuSZ5Vg2xB9twf8lPYlr2/w/O3BL2ZhWi3bY57EOj2oQ/6fssfd/KztlwTb7v9UHaUmbYTmmk1fyKNNCeUhPKYVLOndCj1bQicXFgDAfYDAG7m3gNBg8u76Ir+64GScsGOUCLm5RSwR/04Cwpcv8fUZpfPfAkuVHpzuPRJFd6A7Hf/IN6sq9sRK7rZ+jOMbkKVPggz0KNRYFzRbyAcCgr9iPQj7nno4WdVx+eh3iC8sOkg7Y+ip449K49AwNBAyH54QwvxZNgrTzMC+ELC5rS+n8LeVGlDOpbErxAbxQbyHhNPDIOgwoQjEAaksxgMl8lg3TPWcyLi11LoHpTi8sI7mlzrJt5qSTeSqVRZYD+xiZxnMhu8STTWO1rD7tlefSMczCQgAiyehNpqYF/bVPIgKbZuVw7VSj7+wvJfj7A/Nx2MG7I58v4Jnn12LGtEZMnjA+1QuAzq4S/nrfozjhmAPR0tTs87SuoK9rLfo610BFMSqVEvp6e9Db04O+3m709naj1F/EjjP3wy67vx1Q9jMWGfkz0hEU1r6xArqSoFCwW/oSjJsDsV80xn6h0fefA4z/cdX47ygphYYRI9A6PpXZiLkUr8P08Fgrv6urC1FHh88Px1gZ9A/bh2MZy8pjWF5r+2DmU5vzuGxxC97oi2Eq/V6z1K2Csa8SujQVGZi7N6Kus4K65jxy9TF0fQ66vg71TTGuPrqEd0zTyEe2ttqq8d9Rq5r/p3rgMW2bdCwsPjkHJn2WaYugVA7ItdiPqcr0yPl8NhkwcN9GduYY1yEa934Udjy3Jr/epoRMSZL4hzl5/zmU8Z+7JW2sRLh4/WR0qsgGd5HYQK+quPN+txV0KQ0GA4giq5UoSpCP+pHPFZHP9aEu3426fBfqcr0o5HpRiPqwj56MD3Qf6m2qMsT5P/ln2VC26vHfyvaHl3rwxb9vhLITCyi4o9Foes9+MMag746nAKOhjLZvX4oy9m1Mbe3UaFTedQiMAQp/vT/FKfK/+v7dceI+k72eKQP5C/mWR9qzBMok6xHX6Zftard9FttA8/u+tbaErtr2OfzJbwLz27/hN4AjYPFBiz1/9BE1yPzfuHIsK32MumE/Qxx7/+eBngYhp3KY0DQBncVOdFe6YWBQl6vDpJZJ2GnMTthr0l44btZx6E/6cdfLd+HZ1c9i6cal2NS7CRVdQWxiTGqZhI7+DnSXbf0Qnj7tiUybUP8SpMxgG3Gcc/40lPk/erpR993rkSxbjNjYuTO7BeO++asB5GD88K8BnPzK2Xil9wiYERpjpj6EsWP/isZ1Gq+uakN3v4aKCyg01GPu296JtW3rsHbFUqhiJ3adOh6bW8to7zwBHWsPh+kZgVmzFuN3P5mS6RMocyqjQrFYxMQpkx1znHeRWVdOpXMcwMmibID4oZWL8E+LbmGNLcJQt4AGgJvHfRDTx05yHWdm9gHAPYSuFNatbUPObdVIe2QbybYcKF/aghHjCPNYnjiG7v/Z8UwCadby/7R90nKSz/CcEMor86QsLDuc8Z86wDbe/xvBm6QncVl9ZfmNBhz/U3kHSueRabVoy/SB6lIWnss6JnP/b3mhLNje9//x0MZ/aZ9SZimjXSMjPZ35/AqvfV2jARO2U9rGcnznuR7i+J8b8vif6or4KKtx/YGUP9QR82y+pWPXFdNy2fn/1vl/pBSefX4hzjzvXEh424EH4sbrb4AxBr+89VYseOZpfOsb16GzqwsfPP00nHPm5/C+E09020ef578BfNDhh+FHN33Xf+fXGIODDj/M4z3vrLPw0Q9/JCMvz1HDttlmLCuPYXnqwsu2Df5POqyT9ubVdiXxRW+R/zOGhBp1KQvPWYeyS//ng7dD9/+sTZEudR29yet/kp4sJ+kynfjJVxr/S7dir+X/51/8eSilcOMN33QvZ1ig7r73ox/gD3/6I6780lfwjoMPBrbg/wcd9k6cd9bZ+PhpH4Wuuf5vZXvsicfxT1+8FI/f/1DNfOIlDbYL81ieOmD7SP2KdkqjymSKwDQaEdPCMsxDYIQ8p9GQOcA9mRfUk0KyDoRStTEwKr2m4CzDBkzEkwAQPCqVfYpLqfQNidgFf6UuOEhQDh+gDIw1zqX6Sfi2pTBi/jKDieTJuAUx4UiKT0GIRrV8KD8JJy8EY+w3wGxyevPNPPJIXUogbQZ/JW+yLaReaS+JeDsgLAPArm9FClrc6tAZSSvcskO+XcuFgYrYusGWiyzywN6kIxvxFI/XhbjhsrTTToN1Ixcg18YF2IPORMoapilnH/JJMuq+WpcxOPGG45E8ERfLynr2aU0ASLcFl+0GpwflOj7yp5xdxLH9/nXk/FA5XWtnixZ19iaS/EheJD0IPmV71PJ/8krgQKa1fQiilv8TH6+j4fi/eHIuPBrR7pSntv+n/QeDv6xLXCxvjH0Qg+csZ9zDDKSjlPJPWkt+lPN/my/9P2sLrAOnQ9ocy3ubD/xf4mB5wG4hKe3IDMH/eZT8sQxB8o+a/p/lk21BP45q+n/W7ohf+j9pQfp/oD/yYGos7FEW1pF6Ia4wjXwPzf+zfh7qg+mSZ+JjmvQB8oJB/J9yhnXYjgSmvRX+zzzZ7gTqn/gi1x8PJ/hr3+olrRrBX2PzjRFv/vo3iO3R68DtXEG+wvGfvFJX/MVuwl0sFjFu/HjIm4kaa4DZB6JshMhdGTz//EJcd911OOOMM3DCCcfjXccfjzPO+Cz+7d++hdWrVzvUJktDBpdCej7L1VGyKgsz4OsyjAH8oqA9J4imZUr20tFJbUDwVnW0ZWUb1gabqZQLVHpbdDctnCuIGorlnb6UEoFcJ19W904x7tIwyV+k53woAJJ2IEAa+E1TMnqh/4sSlqazLYlTpW++2EtBU6ULpUbkKVePEma4c3q0+kn5CfVXE4Sc6Wm6suwDtSLL6tWVkXpSAXeOBwZzmca2s/oQgfGAVBW4RSJAIc7lXWGDhvqmTDHqLIpiPzYzXSmF7vY3sH7VYvT0dCGplBHHeeTyBeQL7pgvQEURlrz4BJ6bf1fqa6A/kksnneMJMBg9fgKK/f2+Lwl5Amw753J2RwHl7CMcV3leZYcuj2Mly4RjAtMH+rEM64U/Qjj+8xMWpsY4wL52OON/d0ljQWeEdaUyYt2JXNSHXNSLfNSNQtyNurgLdXEn6uNO1Ofa0Vi/GXU9m5DrTlBozCPXkIduLCBprEO5IUZHfRMe3tiAzjLnCtkxjfqG0+WbNf4XS0BXEejqHfjXXYzQr5uA+smYuNcpmHHQRzHj4FMx420fxoyDPoQZB70f0+e+D9P3PxHT9j0B0/Z5F6btfQym7XUUpu19BKbveyim7/tOzNj3YEyfsxdGqkc8H1JOz1/QDjzynmk4439HBbhu03h0K74BYABoGF1Bpb+ESn8JSUVDu2CnvJfTWsEYBaNt/5CO6xpaK2gDxFEf4lw/lhSW4LXCGzbANYz5P4+Z8X+g+b97o84Ygy/etQHKJC7AmwA6gdIJYBL0LGlDz5I2KJ1AmcQFdBMobcv6a6NdGY3+ZWtQXrbaX7Occniv/P3CjH1J3ZMnCZJ/OSc0Q5j/h1s8h9dRxaapCtDXY9DV5X7dBsU+g0gbXzYpA719Bt09Bj29Br29BroMKPFGsP8N4v/sNyD6NNnHENQW5v8hKCgcOfNIXHP8NfjW+76Fd89+NxryDeiv9OP1za/jviX34QeP/wCX3XkZvvzXL+MnT/0Ejy9/HOu616GiK5gxegb+6Yh/wrdO/ha+cMQXMKphVEgCEPcqss0IbEumUU5+SoR1hjL/j/v7kfv5D1FZ8jKU1qgYAJk+217bLaDtOQwQAdip8ALq0QMDgyQpoVzuRnvJICrUob4uRi7WgC5j+ZKXsW7lMvT1dSOJctjcD5T6u6DijYjyPagrlDBj6mbvVzwS6GeUV6l0XiLTFMu5dR9vH5wTuXqD/zzZrQLSNuA0Il1P4QNOsp+hDGwbW8WeD/f+32yP+/+t8H8eJX8sQ5D8o8b4H/Ip7YD+OJzxv5b/SxoE0iZ/0v+5AyLtj+XDtgjTyPebMf7zXNLz/v8/9f5f7JgVyinrkR6PBOqf+Oy1di8+pG1rt4NOxJvAVkau/UkZ5JH6IG0p90DjP9ekWZd5W7r/x7b4v/+EVVb/BLMd/B8A5j34EJ566GE89dDD+M5112dt1ul6RGsrzjnjTPz7j36Ize3tmX6TuNetX+fTlFJ44v4HMO/Bh/C2Aw+0nxz4H+7/bEu2M8uzLHGFaeT7//t/lj+pB9KV9UiPRwL1T3y8joaz/r8V/k9ZSVfW+9IVl+PJ+U/h5z/6Dxzyjnf4vMH8nyDpyDLE0djYCAB47fXXfT5f7kIN+yUYY5Afpv/Hnz/nnCuZCPF6tnEDu1S+RMpzKovpTOOTOaEhM9DjJ+Wuk2UZ4iUo19mqGluq8pw8E2S50Eh4U2pM9m0FBp3IL8vDN5jb4lcoHB6PPY9j+zYxdSIVrlSwiCYbXchtdZftqCiDzAPSPpd8h7pDYAhe1sDwqQsGjMkby7COrAehT8mTBCsb17Ys76HxU7dwcsSx/TZzFDxJQtlTGVN9ITBw4jHCpnyZ4LtUrJeROfCHsC0JRuhLTmhpz8QpfUo++QlY+akXiV/yRbxM0+xUACCy2xwwCC/1G/olcRMv8+H8EtvN/7OdNGlKuWr5v/QDLnwSv9VB7O7hKAcnYDl7c+pA8ud1a1J7VTX0zHLkl3ggOmxpB86TPR6IATdTVjyR7etaIXw65ZS8SNzkTeZJYDBaDhIEqYeQD6s7+QRlta3IOrIegoG4FrA8z6Uc/EmdavrtkPw/5S08Jx7SrVUmTJMyMx1vuv+nbaeH4f8Wl+VBiW/PWHzD9f8s3e3j/7atmEaaUq5a/k++yQvTyIek+7e+kSj5LaAZ4LV6kcHfNIhrMC6X4IgRffjVqnq33iOCv+6bwjL4a+Wy9Sc2GBw/Od2inSB5ren/lNkFdErlMpqamtE6YgTEMlEWwiTlikJh/Yb1+N3vfocf/+hHeOmll7Bp8ya0to6A0RorV67CohcW4dHHHkWpVMYuu+zit5jO4hQXgTzVxGvx6I3PHcJ8uDoynfMfh0+xjMBvRNDOdpzu2qUpFbAreQvOlQxMBHxk/hdbINcQVSkGGcljtoyX3Yvl7FeywkCwOJcBYW/zrpgSqrBH5xeSngDWt9I4NMKPFBG5PMFaFUj8np5xGnDnqczpHNrXdXwI5onZ44XfgjnVL7XCNsmUZRBeqUwwnjq0dFka6O/rRG/nWhR72lDu70QEhShXL9oyC8SdJBqvv9GGHaaMRhzl0NEFNDVqNLsbMiq3XAaWvL4SM2dMQj5nv9NUKnZh3RuL0NXVYfuqOPZ5WmvopOL6kwQ6qWDDupVoahmNESPHey5SI5K6svLFcYxSsR9JJX1qmcDFKNqBVDXTZN+slNPiAON/rq4OhcbGTN9mgjmBPJdlauXzvFQqAX3p1rvUDe2JDxuSj20Z/9t1hF+tLWF9pYw8OlGIe1GI+1CX60Vd3OuPhVwP6nK9qK/vhlkeAWtHoK5JQTfEqDREqDQpmLoCkoYIb5h6FPIKOzSW0Ri7QMiwxn+NXC5fxWs0jPE/Ni9i1LTD0DJpH7RM2gstE/dCy4Q90DJxD7RMnIOWCbujdeIeGD11H4zbcS8U8gCSDiDpBpIeQPfaX9IH6CKQFO3RlABdAkzZ/nTFBh2hUdfYgK74+Aw/PFfu/pzpTIvEfRzoo0KucPw3rsxtvaPwRLERWinopIKuDZvR8cY6dK7pQPfaLvSu70FxYy+KG3uR9CaI6mKEn1SNlEasEiiVII4qiKN+5KJ+FOIicnEJEUqIcj3oijZiVv+uyCFn34gfxvyfwPZCZvyPMp9eMMbgu09shjLubV7YN3r5Zm+0fhOidZv9tS3DfPfz1/ZYt34d6jasC8qkbw8ro/G5o3fNtBl1L/mq5f8m8F/WkfUg5v+3/32s04AF14tZcCcGQLlicPHJwMcPBd6zr8EH91fYeYzGI68a5OMIpQowa6zBP70d+OQ+wAdmAR/bA3i5rYINxSjt8R3Oc6duqLIrDDL/59oT02U9KTPTAeCHz9ut+Aj7T9kfFx1yEY6edTRmT5iN/abuh5a6FixcvRD9ST8AoKIrWNu1Fuu61yERO/wcuMOBuPTwS/GBvT6A2RNnY/aE2ahUKnh29bMo63KGzpl7fCbTdrL9JK9Kzv9NaquoMS+XdYwxqOgKFr/yMAr33Y3GYtmWNWnr+bEyiqBGjUL9AW9D44kfQNO7T0LD4YdjTbIBzy3fEX1xjPqml1AXL0IhGovm1ga0jmxGU3MD6nIROjs2IY4TNDTUoampGY1NzejuXgOTGwWTzEBT3IjjjlyNffac7HkjKD//t98r1FqjqbnZ5wHu5QXWce1909N/wq9fuh93vfYU/vbaU7hr2Tz8bdk8PPzG81i5cS0qPX2o9PSi0tOHcjfPe6BLJeTq6vwugw2jWj0vW4KTmudgZFOL5Yu25s7t3MVCT3dPpj0h2kRt1f3/dlj/g2UztBVZR9bD//L7f7keJnmUZcinGfL4X+v+f3jjf8ir2ub7/5Qe/oHu/wEj1v/k+r+0E/tJJgagyRNq6JltQH5ZHlsY/32/s6X7f2GHSil0dHTgjr/8BXffey+emPckXnr5JYwdOxYjWls9XfJI3pSCDWobAznJr5r/C2CabBvJF3WnAKxtW4s7/nonPvvJT1bpRymF5xY9j9Vr1uBdxxwDAJgzezbmP/00Xl26FDN32gl3/PVOnPHJTwEAHn3iCSRJ4t+MlDr+2z13Y8qkydh7zz0zetJvkf8/+dRTePCRh/HYE0/iqQUL8Mqri9HX14fJk9zOEoE/hG0py1Cv/13+j+3k/8Nb/7d2zrSQjnpL/D+VI+v/A6z/b4X/33X33YACjjv6GM+HUgq/vPUWLHx+Ib5zwzcxdkw696X/f/Jzn8X8BQtw1OFHZGjc/LOf4sC5B2DvPfeCETqFkEUphWWvv4677v47vvj5i6EGGP+V+CVa+ze4jfNl/1N2/hG7OZJSdrdVRf+/+JxzriRSKkwepUFJYyCzofKlMMSpVPZVdYjOleUk3URuvcDGDva+Rw2j4pHpPJIWeVDuBlW5RmVATdaTuDn5lAYky3FRb6AbjHBBhxCJgDECI9AmXXRLdSnaKJBPGjDrk98Qv+RHa/vGpVLiDRHhuJl6bCe4byIIR2Q96gSwT6TqoAOUOmT5yN18Qxg4jyoYTO2+7dnOUMrHuvIJLc9T0AySvte3e5LEuM6anVOoDziHl3hCPck0JXyFMtmmGNhuvZ5q6BbK6pdAOVTEbQXTtFo6kjQoG8/l0et+WP4fVb0hIXnAIP7P7bpzOesbzLftnm1Ae53ebIU64tHTcosyygWolRi8Qh2F+uHP8yPKybIhbSuTs72smhxf2TpSXzINDhf5YZ7FE2cWsFinVtvLawQTBktky/7Po+QRNWyUZYbi/+EAJ2XM+n/Wp0L5WJd9YciTBElfyvfW+b+VK+SRR+IKaRBCniRNmVZLR5IG8fBcHrfX+C95wCD+HwXjP/ND2f/WOwL92u7yxG2b7ZvA2eAvr7W2AeCjRvfjP1fW23FfvulrjB9f5dHiBiY1GLx3eiqX5EnqspZ+lUr9v1gsYuy4cS4wW22TwMDJSVLBNVdfjfvvvw/19fU499zzcPEll+CTn/wUPvaxj+G4447DiNYRuO+++/Hwww+ju7sLh7zzkBCNAMdUFUGZFuQp959Kg25VZQiBLlK80l6UK2YDV6H+AEAGElUmPhbyL4+hXCGPaRlLy/GklHsgLd3BwSYrW0e5uoJXj07IppQNVsoyKkp15u1IsOoDmk4n3tQcigw9ce1tUBwz6VJ/aeWUtMuT50LJUKwnyvn0oJw9kcwzJ9seVbKwjFKW3YhUnT6tgqrqZKkbdG5uw8sL74Ey/YCpYO3K11DIG8S5OhsE5l/VmGBQSTSWLV+LaVPHIo5irFnXg5ZmoLW5OVO+VE6w5LUV2GWnyagrFAAAG1Yvwrq1K1Fx20pFsX1LuFBoRqQaYJIKKkkZOrHfjtVJBeVyCTtM30PoJdVBVsupTXW2t6Ours5fg2NNMP9nX6pNurUy05Vr+2XLX8fadeuwcfMmbNi0CRs2bUTbunUwcYz6xkaUSiX09/dnjvbXj1KpH/399pp5kifat+wv+/v7EZdtoIF5yr39y4dr+ZYexwe1FeO/iiIs7S7iN20bEatuFFS3DfjmelFwwd9CbLcDrnNB4fq6CvByA07frxEfPjTG0XOAY2blcGhrjHdWcjg4iTC3VMC47lZEKwuorGhAX1sLypsLiBr7katL9Uv+Q17tWGll4bxT5odySN2xzIQJnWhuyqGpuQ5NTfX22FyPpsY6NDXZ88aGHOryJUSmB9D9bk9nY3/GQHzk053Dby9cnW+3K+7Ov2fo47+zO8m3bCcMMP5vqkT4Q9cYbEQe/T1FvLHwVXSsbUepTyOpKCQmhjY56EoEXVKodCXoX9sL6Ai5ETk3NhgoZRD5AHAZcVRCHFWQz3Uhr/oQR32Iogp61EbMLu2KxqSpyo5kG0Q15v+ynCzLh5mzaQrffdxu/+wDtJkgcO0gb1gGmaCwsW8Tizq8tm8Za5x17OwqucJ2qJr/C5kJrIcB5v+3/80ughFDiimFzm6Dz3/Q4PTDI8zZQWGXCfb39d93YENfHZSKMLrJ4MyDDT6+f4Q54xV2G6swPlfEX14qYmVfwfLp8CkFnDdtU5V8GGT+n7XStG2kLFEw///+cz/y5UcURuBj+38M79vrfajP1SNSEUY1jMIeE/fA1JFT8djrj6G/YoPAEiIV4e3T3o4vHf0lHLrzoWips0HCulwddp+4Ox5e8jDWdK/JPJx01l5nZGxNykEI2yh8A1jKFupIKYXN5S78bOP96OvYgN3W9qXtZvx/UPUNaDziGIy66ItoPPGD6JyxN9aM2Bk9E2di+p7T8OBj/Vi3qQ5RYTWa65dh0sgJaG1tRGtLI5oa61DI51Ao5NHUVIfmxkaMbG3G2FEj0LZhHforM4HKTOwwrojPfaoVrS1NiAac/1vZkiRBU4sIAFMex7GyGTjjzhuwePNKLNm0Cks3r8Krm1ZhyeZVWN21Ebpcgi5XoCtlJOUydKVkj6USKsV+FNesQ7GjA8XN7VD5Aood3UP6fWjCXIxqsgHjVJfV63/dXV12jhDcx6tgXJNpcLqQvsl67Jtqjf9h28trbCf/Z93QRlnmH/H+X78l9/9ZGUI5iCukQQh5kjRlWi0dSRrEw3N53C73/8H22BC8s5ykW9v/wzY0bqyttoWsjE4+d08vZVHbsP4ny8myWdrZNMJ3vnsTPnXGGejs6ka5UsaGjZuw9LVluO6bN+CZ557D4YceioK7r6BcgHvIXev0zWaHN95O/r+2rc0GgD/xSd8+st7C5xdhzdo1OP7Y4zzunXeaga9ddx2m7bgj5i2YjzM++SkopdDU1Ih//9EPcfghh2D8uHFex1EU4a9//zsmT5qEPefMgXqL/H/FG2/g3266CZd/7RrcdsfteO3119HV3Y01a9fisSeexG/+8Hv86re/wesrlmPmzjthRGvrAP6ftvdw/H/J0qX48Cc+hjVr1+Kdb3/7dvN/llBOd0uWLsXK1avQtq4N69avw7r167G2bS3WrV+HtW3r0Lauzee1rWvD2rY2NDY22HvKIft/yvuQ/L+G3VGfUl+kOzT/r/axUEc8SlpKpbEM+6Bmtf8vXPQ82tatwwMPP4T+Yj92mjED3d09GDd2LIwxuORLX8TJJ56E+ro6tK1b535tqFQqaG1txdq1azF50iTsvedeaO/owOJXF6NtXRv+/Nc7MXXKVDQ3NSFJEowYMQKrVq/GBZd8HjOmT8fECRPx7MLn8KUrvoJTT/kw5u63f5UuqSMp39b6vwLsN4ARRJF1EDGXjcBzwE64IuW2WxLRcxYJCRIvr3muxZMfnr5rSO1umAlhY7G8vJZlCcrx6fNEmlSWLA+4BeABnNxf8x0RYZCUiTfCTHcVPR7Sphze8QKd843qJEkQB0+RwOnWuMFObjFLupJ3GRzV2j4lxafv6XzkjTiUSr+Bm/KU1Zlxk71EJ5kFKeJivmwvY+z7HdLxw3x4J05tk/nS7mzgMFe1+ODt2Qf97dM63O5a2vtAQJmJT+oAwi4JYR7Lp2Cv4zhGhW/ABnQgBjNRDQhw1pJBwW5HJPUo2zLkiXrM6Cvw/4HeMJX14dssxS/LyDo81zX8n9/G0MmW/V/KaY9p+xOUkgEL2KcDhW5CWw55Jk3KBKTf72A91jHC/yVOY+xbI7Ysr2v7v8Qp+aONSx3QL4x70sfaZ5Yfybukw3Pym1QG9v+BeCIY+r/wKykP8y1/KW9wtrZl/6+2IWl3UjesS70Sh9Sz5FPSqAWUmfWlDiDskhDmSf2lZdI+lyDpoJb/OzDi4ZGBZJB45LmkYXlK7SDUl5Srlgy12iEsL8vIOjyn7bEs9SvPCeTnwg3T0JNE1cFft61zGPw12mBOYwlf27kTxz3eKgLFFqev5974DfP3HZXgB+9It9Ih7+E1eZQyEZJKgmKxiBkzZ4rQlQEgHhDhMQQF/O43v8XPf/Ez7LLLrvjqVVdjxAjxdoKo88orr+DMz30Ofb29uPyKK3DCu99tMzxuEsraZtheshwALFmyBA888ADmL1gAwGDcuPHYffZsHHLIIZg6dSpkn++DgIr9rmOQ6QJvmsz6mSyfD7iqGRC4jMHZ55yD973vfTj22GNFkZS2VYF9ozTDp8sfCLLNk56xHS0GwZzzT3vq6IUNK3zYgyQEVNerkj+LQ/pKZvFRnteATLuH+pDXYQMIm69ZX7Q15chy4d7wpZ0o1qdPCGUAHkua4uq7q2cevwOl/nY0t4xCLl+Pvp7NaN+0EXvPPQQjxu6KKLYLK2wTf64UisUK7nrgKRzxjj2Qy+Wx4LnV2Hl6EyZN4Fu6Vr/tHUX87f5H8J5jD0ZzYxPKpV6sXjoPy5a8gIbGJvdrRkvzJOikGUZrxLkY3T2vobOjDb299pvAKi7g6Peemwa3vT1arhxFQPjVspdeRmurW2QW7anD8V/mu7YhDq01fvjzn2L+s894uzGuX61UKjjxxPfi0MPs97pseZbhXIhUbRrzAYOddtoZzc3pd5FtGYu7u7sbhZ6eTJ/OcrGbj/PbamH+cMb/stb44/pN+Ona9dDlog2kKRcsU9rpM72Ocwa5/nqc37IP9ppaQEPBar24MkHxyQK6NhbQW6ogMXWooABjckAhDxPl0Fpfj/7cBux6cjsKzek4bgYc/7N6Ge74PzH/ffsmrzHgN2ItThv4S8+ZLsqwjswfIp41Dd8XMqSgVI37f/cLZQnbjuccK5/pq8fXN43HxvWdWP3K69AqhsoVoHI5F9yKoCLYIC+M3fY4KQGVInJNBs27NiLXACho5OJ+5ONu1OW6UMh1opDrRkO+G/m4C/WFbhTiHuSiPuxQmYCPdp3p5zqSL8kz5ZA6qHUNN66E4/+sG17xQVwboLV6V3aCkR59Pq+DfBEIHvDaBYKf+sb7avLOtpLn5Hew+38ppxHz/89esKv91m+tXw4oGWDESI1fXqEwfpTFV8gBf53fi098r4LWsa0oGoNj9zT4tw8pNBVsmUpi8OqqDnzxXuDJjlaYfOS//6sj4MUjXq3p/+ST/Gttt+WV89toiPN/+Q3gQ2ccin89/l8xZ9KcTBkA6O7vxgd/8UE89cZTbnvyFJrrmvG5t30Olx5+Kepy9uEdCXc8fwfOuu0s9JZ7fdozpz8J1PB/AmVjO3gZ3EPhRpSR5SHab3HPCtyw9Jfo7WrHl+9cg93XFG2+gV1Lqm9Ay0c+joYPfRSv9TXj9mdKeHZFgq4+gygCxjQm6F00D68824TlG5agsfkmdCzvQxw3QEUNMCZGYipQBoijPKAqMLofScWgYexmmPzHsPO4OTj+HRqnfXgvxOKlDNqrPU/bpb+/HxMmTbTjJDhsVj/gNvvmTwPGzTj8PYy9/zbG2FlEJp33qIDu6oOqzwFxhFGzdvG0twR/OOACzBg32ePKvJns2gQA2lavQV1dnaO3Pe7/0/GftkD9YVj+n373lDyENlOLJ4L5X3L/n0qUAmVmfakDAD4oQsjmyfE/BakvgqSDrfH/rbr/T/UY6svUsEUJtdohLO9fkNrC+E+eqF95TrD8pH2CLZN+F1iWtTfv9jSTXkM3lJUg5ZLlpQ54TR+X+KRMBGMMPnfuOViydCnee9JJGDlypM8D7MPhjz36KJYuW4a//vFPaG1t9fTIX1KpZHaRoVR6G/3faI3nX3wBZ553Ln703e/6flIphenTpmHkiBH4xS23YP7TT+PGG+w3gYnj+z/+MX7/pz+iq6sL8x9+xPvVZVdcgXnzn8IHTjoZBx90EIwxeH3Fcnz3hz/EJ04/HR8/9TSvn+hN8v/N7e24+ec/w62/+x3232cfnPjuE/DOgw/G2DFjMv6/afNmPPr447jjr3fi6WefxamnnILPfPwTGD3KfqKBumPQULYLaZEur5m3eMmrOPuiCwEAc3abje9cf4Mvs63+zxf9Nre344prrsaTT80Liw4JrvrK5XiXeNMVW/T/tC/Blvw/8CVe81z6Cq/VoP6f7ctkmbAsIZOe8f90DGb5gw6rfmnioAMOxHeu/yaUUjjosHeG2QCA8846Bx8/7XQY4f/PLnwOZ553TlgU5511Nj76EWv/v/rNrfjjHbdj5apVmDplCk4+8b342EdOA4QOyd/2Hv8j+ealNsYGo5xhGSrL/bSxkxoVpd8NZbAtdhF7GjMbhuc85ty+9pEbbBAMzImjD9s0iMRALQUhPpkmBWZjGuMWgZ3gNs3WpcHC8c36rGcXoaqfrGI9pWyAOhGDBH8sQ5pa2zdtiY94qDc2mv/urJDFfuvANarouJmvtQa47W5g7Czjz+VEx7g3eUX7ybaQepXBX9K2OFKZqQ8t9E/DJG7itaAA92QndUbjZF3ST9ze6rwmTjlZjV3AXfIEuJuirEq8nkhXnsPJxbTEvbXBc2R0rGAMt+Gw2067VQq7LKkiwG0fDuXk5Zvfzuei4AmzFHdqP46Uz4vdE6QZOaV+ha3wx7qUh0clnu6hHxCnBOn/tdoBGf9PBy7SVUP0f6XcopIxiOIt+z/7IqZLnUj5tbF+4vG4J+kwoP9bGuRP8su+QYtvTUha0oZ5VMou9NqbdGV3Fgj8X9o5ccp2pR5SmikN0pRyEIeE0MYh/T+O/DdOKbPX81D8XzxRhS36v8VH/MyXumP+UP1f8iPp1gJJV55jWP6f9sFS/8znuZSF9ORnEvgjXYLUNfEB9sk7lpdy1mo3/og36//W7olrMP+XvEr8qOn/Wz/+M530avm/0bZ/sLpPfz7468Z8e53mA6gK7rKMYfDX1xX5IqAn21kPw/8TnaC5xW0RB9uFcK7jVx1q6B0KWLVyJW659VeYPHkKPv3pT2OECwL5yZmAWbNm4bxzz0V3Tw++/e1vo1LJbi+YDobGk5dtxD5SDpqLFi3CDd/8JgDgkosvxiUXX4KTTnov1m9Yj/r6OseEHQuBUB5e1A7+wott66fmnwpm9eovPXhd2otAFe5KlpGgYMs4ma0+hG7cEcYtGLqbBV/Vl7QC8HbcB/QcMNjs3j1N/4TO+XNq9BAGjcM6cLphWsZvldO3yWKRdirrgtdVenTAxpE/WV/wAsmLk0eB38FzdYW+lJM1Y3cmxWPR27xUPbYWsQAKG9e/AaUUfvyjX+P8c78CYwz6ir3YsGEjujcvIxVn52k7GTc/KJXTN7h6i92OhVTnAKCNRrls33g1xqDc34OOjo0ol0sol8uolEuolEswug6Vchn/ddttKPWXUFc3yn8LOJcvZB5co19Y+aURpOOQUgrNI1pRLpczfQ7PZb8kIWMTrtyLr7xcZQe+D2Va5touphGVDfwmmXxjDLq6ujy9ED95lfzRjrUIXsu+k/nDGf8rRmNx7xo0NWxGU34jmgqb0JTfhGZ/3Ijm/EZ/HDGiF+8Ya3DQTnmMbIqQjwFVrCBaWkJ5STv62tahtLEHfRt70LuhB50betG+ugftKzvxxpI2JK81Y/Vj6X0deczIV3P8dzfhwxj/Uel2C5v2e7I2eOuu5bn/MU3UqVVmS3hce5JP2W4Ixn/6zHDGfyiFR/qasGbFBqx46Q1UVD1MrgEmrgNUDgY5aBXBIIJRORiVB3L1MIUmoL4FlWIe3Yt7kJRsX6dQdjLYo0IFSWLHaqMrqFSsLa6OV3m+pd5pX5LXDL9CxqGM//77v/KbvTr7nd80TV4HdYjDfy9Y1km/Iazc1sPkSwJ5k7a2pft/qQ9pk8a47/dq8c1feZ4A3Z0Gnz9FYVSLQqkMlCu27iU/7MGIpkaoCjCxCThhDtCQVyhW7GMKi1d3I4nqEKvY4nQ/5Y7kO/R//miblDcEykWZZbtJ3QBAfa4e+0zaB7tN2E1gSOGnT/0UL7a9WBX8BYCeUg/uW3IfnljxRJgFADhu9nGYPnJ6hh4h9H/ZXuwv2DZRPLz5/2vdq7Ch2ImegsJv9x+F9voIRhskMDBKoXDIkWj40Edx+6sN+OJve/GH+SUsXptgdbvGqs0az69SeCWagmJDBxrzE2DUsWiePBsN46dizA7jMG3WVMzcbV/MmjMXO+wyCaOnjkXjhB3RPHka6kYchqb8dMyeUcThh05CPp+Hrjn/TwOKXgb2J26khLJzAmrPuPHJGAOjNZry9Th657k4cbd3YGzjCJunNY7d5UC8a9eDkFd2fc1oDaMTmIr2GyMMC0w615Iy8Ej+aGNRjfW/4d//b934z/TUnuy3A7fG/6V96f9//+95lOdSFtJjW0bDGP+ZV9P/t+r+P2tX/xj3/6mebVp2fJY6ae/oQHtHB0zgM+SBsC3j/5bW/1986SVc/MUvYO8D5mLJ0mU45cMfrgr+AkB9fT2OPOooTJ8+HWeedy4woP+ncw693fw/XQs987zzcOb55+FzF5yPM88/D6+vWJ7iUFmbNMbg1FNOQWtLCyD83RiDr11xBc4540w88dQ8j++Pd9yBD550Mk464T0W3Zvo/xs3bcJZF16AO+68E9dffQ1u/vfv4eT3vKcqqBtFEcaMHo33nnACfvL9H+C6r/0rbv/LX3DWhRdg46ZN2+T/S5YuxdkXXYhjjjgSnzj9o4DYfZI2HW0H///Rf9yMzs5O/P5Xt2LeQ49g3kOP4MkHH8YTDzyEJx54CI/f/6BPe/z+BzO/f77kUlx+9VVYuWrVEP0/3epctgPeMv9P8ck0WY988ZxtxDTyQJB0n3zwYTz54MNeX/MeesQHfwFg3kOP4okHHvbHx+9/CE8++Ag+5h5oIN8AsOecPfDkg4/4Mqz3sVNPR+TG/4+dejp+/6tf48kHH8Hv/vNWfOwjp1XpIOv/22/8j4iQQKWSqCRMkEpleQksSyOVdYhTGjbT4zj2b44yvVKpIIoilMv2+3uyoRJtn+zkjwu3XMBisIoGppTd+tmuP9lgK9MlbmMMDNJvrdK5qQseuSwocUhd+AfjYelKQ4boLBNuQy0cibiUsg5A2Si7x6Pc9thRNvib1rfBAlBfxsC4rS1tsCfbruQritw2XuIbT/wRWE7WJ4+yDckL9QbYZTveoLEcAuON3dNAxhgfLCEutgc7Z8+vg5ROFi9l4mIb8ZE+PzTPwUQJp+O1UpFbC5VbV8fuuzFuUVG5hXT3F+dygEq3CzdIA5K2/VK7gtCbZd79avhRHHx3Aq5dtJuYMAhMfaUyWLmkPWIY/i99TeodGf/P+fOQb/LKPMpCukwvVypQcW3/z+AQNDhBpHyR9P/IPgygoghJUnHtVO3/pE/eyBf1zHL0Of6kLuV5FAxkdiKVwLiHB6jDav9PJz+8tvhivxibaR/X90G57x3X9P90F4CwXQFAJ+kTQpSX9aRM1IusL+swjbJQb7J8eC7zs/6f8sNrHfi/xEc8IV7ikOdSrqH5f9o2lIk2FgLryXZlutVRajtSP5JPCcSnh+D/0k6pLymDbX8rJyEsL+ULeSAuWR/bOP6TLtMHGv+1yQZ2fRCXwV8R+E3z7Jhn6zqefJBDBH8dHuYbA0B8X03qFcPw/3KpbL9fxmSHV5zY/gjs712aMZi/YD7K5TIOOeQQ7LXX3ml9Ak3FHT/4wQ9i3333xapVq/DcwudtYqaZjCtcbWPwwW7bTwEG991/H3bffTY++9nPYubMnTFz5s6Yu//+uOCCCzB2LL+DIuSoyRxpDg08D/bKpTEPAAOGxvj0AYF+ZS8sOuPOYd8MAQCjNQBjx/iwrGefAVLx9qkSwUR78OADjkFa6DfGUN8WiQx1Ejifkf5H3MRHnVh8bi6s0mCwcmLIugSrVsevwFGlYIcLxCvBlVWZepZzY9xZpo71MaVsKJgyAtb/lLLzVfgAqZO3hqabWkYiiiKccMJROO/8T9j2NAZPvtCOvmIZ5f7OtL7jwerA+nV/qc81tUFfsdsuCgf9XJKU0V+2b0sBQFLuAxRcANgGgcvlErSxfdW+++zj+jYgl8v7IHBzywhY00sl8e3BF4G9zFZljU3NVfcRSvTPrE9+lRj/2f8bN3fz574P1HZxyaVxvsD2se3nyongMNvJthHLEHd27iDtjfz7OlL+bRj/+3UZK/qWo1G1oaluE5oKG9FUtwmNhY1oqnMB4YJNb67bhJb8Bhw0YhRyUTr+R70GZkUHcv09yJV7ka/0IV+Wvx7ky73IlXth+jvQs7xS5UsQuhh4/E/9kOMK82vh88FZuJ/RABLnWAzcmjRPBnxlGlz5KjwCv8NpjLU3Qtiesh2xFeO/tTeNh9YBG9ZshlZ5mChvA71Q0EZ5kXhu3MNCu7YAn9m5gI/v0ojRSQ59K8pQpt++JYSyE7UMnQAKJUCXUSlr9/BCggR2XqG2cv4P0X72vrDapgEbAK4O2KZBXhS7YHo3wfRutMced+SvZxNM72Z73rcJKPXUDgy7a9tug/j/YPN/4U+Ul/WkfB5HAsQi4Ct/lSJw4G4Gc2fb4G9/CSjkgetu6UBXXyMKKgckBruPNzh2d4XuIlBOgKXrKljTnkDl8lAaUDK47ILA9H/ey/AeygB+3NFBv0KZ5LmUK5z/E8Y3jcdek/ZCLB4aJjz62qP43mPfQ1d/V5gFODoLVy/ELU/fghWbV4TZKOQKOGqnoxCrFLfkU4JsP+3XzNL1A+Pu85hP+Wi/xKuUworiWhjn56+ML+ClCXUwcN8Bbh2J1ve+H6/1NeGXjxaxclOCSsKguuPBGEStU6DHN2CHGUVMHTkXCu9DkrwfKn8IWsftgp1mT8QOM8eiafROMNE7UElOAtSJmNTyNhy2N3DYwc2YMnm8l4V8Utaa83+hi4xu3E/ZTDd2298n93s3bjzxn3Dmge+F0RqHztgHP3r/ZThu17chgpvraDcvSRfuhgduruVB8KfcPYvsN9gePGJY9//bOP5vR/+X9WUdppEX2qMsH57L/K0d/yWeEC9xyHMvG4DyW37/P7zxn/j0drv/r9abLC/lC3kgLlkfWzH+M33I/s++XeBgeam3pctew0dOPw0fOf00LFm6NCOHxMXf1o7/3Akw1IUxBn+47TaccPJJyBcKuOyyy/DPl/0zdpm5C6ZMmeI+A1UNhxxyCJYvX4677rnb88UHWrh+LNstlItH6mKo/r/3HnviyQcewpMPPIgnH3gQT9z/AJ566GHsNWcPGGPw0Y98BN+57npfnjhGtLbiv265FU8+8KCnybY5+cQT8fMf/RhP3P8Anrj/Afz8Rz/G2WecgRGtrVW6wnb0/83t7TjnogsBA/zpN7/FUUek32O9/S9/wfXf/jY+e+65OOO8c3H9t7+Ne++/H3Dj/1GHHYY7fvd7AMDZF13oHyAgfalb2kLk/P/VpUvwL1+9EhdeegkuuPRifO7C83HskUfhsksuBZDe0xtj8PNf/Qp/v/dej5O47r7vXvzillsyuiDI9tNaI+f8/79u/xM++8lPobevF+df/Hmcf/HnccElF+OiL1yCCy+9BP/0xUtx/sWfx79ceQU6u7o8z1EU4X0nvhezZ+2G+x58oEq/Ur6QB9keElj2v9v/KR/bRsqR4krzttb/WT/UhTyPwvX/Acb/3Fs9/sOBrMBzKo6VKbxkhOc2P0I+X/BlkiTxzEMwzcFVCpC4gJVvMPfNX/m6c8Itft1El3xyEJQ0JP5UwcobVOLkYT0aX5IkMOLtDPJXxbdyb3i6N/mMC6oqFUGLOWQU2YCzcfqE7OzcTQtlhuhU7dE2HLcuNmISpbUNPKbBI+WDxeSRbw4b8G1HWwYA4px9W5Y6oLzKTVSN0wmNVtUwMsptnwiJYPybQ6lTQNhIFNlF1XB+zXyC9hMjG6CwOs62K/WglA2uV5zcnkf33dUMXpNOkMgnj3Fsn0yxdOkLpGl54c/iSp8w5k1jkiSAe0JK2grxkS7PqVdfLnILym6Qt4uAKQ4ps+STMkB0etShsYleN6zPugTKShllu2II/s9AeC6f9zZZSRLfLuTNhH5Em3ODAvknj35Lj8D/WY/4lLI3X6GdkHee0/+1dt++dvYSCf8nboKkI/G6W83MW/lhm9AeTQ3/jxy+KIq9nVsdWL9leS+fp5G2r5RNBYNF5Po543h0hbxvD+T/xLdl/8/aFWTfNoD/yzIE5hNk+7JO2K7SF8in1LGUh0C6UmdS1lAHPPI8lIl1M/7v8G+V/wu6BJnHtg/5JB+o4f+yHOnxl9ZLr2WebFfqmzIwPcub2urxX3v/t35IPgYc/4PgL4O2DF7I4K8vB6BSrrg1ctoS3Dq3u/Zr6GnwlwHikG8C5aIOZJnQ5nPuSXsA7D7cibsw7tSIAkph+ev2Kdydd54p6gXg6pHW3LlzAQBLlrzq2ystS9y8lplOPpW+sfviiy9h2o7TZCGXT1y1mGJaamfZ69qQqjfFa/m37ZAeXb635fQti1DcDLh2T4EPZkllGIfDRb58tpTBIiFtbxf0Zfcnb/o8+CC7AEs2G/h1ZBSsrhXSQHNoa0yztFOwYohALn+BHVuVijwlOGF9IwK/YTrcG76uTC3erF7JH/Nc0NdYnacy2naxfFn9cY7kkmzT2EoAgGk774soijB7952x735zoI1Be7ERdz36IuYvLqPYs06K59uTvBX7+ywiY9Db1535BA2PSZKk5QBoXcHYCTuhXC6hUmEQuIS+vjbUNdRjl112QUNjASruR6FQh3w+j1yugDHjp1l9uD/SJYNMS+3EPsBiaQ5t/Ge5cFyU7cNF8vSa7WZ/tjnTckmSPrAGpH2rRZvFEf5YRoIZyvgfD338X1PaiFzDBjRF69GS34TW/GaMyG3CyPxmjMptxujcZozJt2Nsrh3jC50Y27MRc1qmZto56S6ivH4zFHpRQD8KKKIuKqI+6kND1Ot+PWiMelCnupEv9w1h/E/bxo51wx//00BtGPAVb/L6gK5JryECvpkgr/y58v46gXFvANca/41oO601VKSQLwxv/Kf/aq3R1l5CsWhc4Nfeg3As5hhstIFODHTnZrw7vwY/2KuEc3dVuHC3PG49vBWHxRqmmCAyRfcd8BKU7kdkOmGSfkD3Q+sKdKWCpJKg4l5Hjbdq/m8hHf/Th9N4Dx25e96qN335li4DtpU+rNI3YqX5Llbi3/GG+j7eUD8AdIILz78MF1zwJVxwwb/g/Au/gvMvvAKmUrTbPbtgMhxOiCDwYP5PWdQ2zv+1cW8Ai+CsfAu41GPwqZMUogjoKwKVCrBus8a//66MkY2NiBKgJQZOOUihWFboK9vu77ePd2NDbwFKxTAy8CvPOUesdf8f9NkQ/Y7sM6WsoQ5k3XHN47D7xN39NWFT7yZcefeVWNe9LpO+9+S9sefEPf11YhL85aW/4M8v/Rl95XTsIByx6xGIxFbHBNqbGsL9P+1Ntrssx3bk74WuZb5+X07hoZ2bsLk+QqINGvbaB7lZc/CbeSWsbk9ftCAd+WucvjfimdOx396tmFS/M+q6Z6Fv3Rx0bpqMMjR6kxK62qegf9MeyHfPwtj8rnjnnBE49X1T8I63zfb3u7ZPtPfCXIeoNf+nvBwnI5U+aKZEv2TnFEBXfy9uefYuVHSCd896O/aYsBO+/q5z0N3fi5/Oux29pWI6/w98e1hg3PzT+T6E/Rl5HvSHbDM422T7Ma36/t+NBdsw/m8v/5d2BSGbxEk6rB/qmPkE8izrkBZ/0hfC8Z915RGC7nD8n/RIS8rEum/t/X91W5EPDNP/ZT1JOywPJxN5kDyGvPFNfjPE8Z+09RbW/9QQ1v8kjVdfXYxzzz8PXV1d6OzqwnkXXoAlS5Zk1/+ELrfP+J+9/3/xpZfwhS9dhiuvuAJHHnUUxowZAwBI3Dxw3LhxGD9+vLdZOD4mTpyIE044AV/92tdw/EnvxSuLF7s1We0+iRdBux0+tF/////+T14A4Oprv46u7h784MYb/Ru/f/zzHTjk2GNww43fwcpVqzB3332w/z77YtXqVfjqtV/Hoccdiz/95S9QSmHUyJH44Y03AQa46tqvV+mJfCDw/y9+xe46deDcuZi7734494zP4Yufv9iW125FwPE/aeJEfPmqK3HXPfd4Hfz93nvw5au+ionus0Okowbwfy34aGpqwrz58/HkU/P874l52eM999+H5SuWQwX+P3LECHfrORT/T++JQ97+p/i/xE9+4B7wST+TSF0q/7La9vR/5sHpKbR/6T9RFEH9N4z/kRSUFeSPlaSCWZnXPDfBK/JkXNYnk7xm4IgdcKVSAVwQTQoMx7R25QnS+SV9CsxzpSL3HaHUaVheKk65N6KkgbCsMW5BL04DyExng8k6StkFLPIPGkJs33Sm3sgz61hHdG8qCaNQ7BCVDXDagLkNHJGHXC4PiECvfVLa5lF/rBvKRh5i8cQA5aFtxHEuDXSLSYbFZ/UMERQnH1EU+6e2afAQziXtyNLO2pKkpZRb9EV6U6KUQpzj94dT/Ws3QBpYXoyxMgBwQd/IyWM7Av6M4bYA6TY9BmngV7ZxnLNBfskfeZfggxdOx5HrcMgndQ1YNqirWjqS+uM1yzGd5aMoglEKFW2/92z8Gm7aXhZHeiPGn8Ul23W4/m+3wGZ7Qbx5D2FjGf8XHRvzoYAol/0+BGr4fyVxW9CJJ7Wl71BH/CWJ/V514t6yD4O5YXnqk/lWl+kbtbIOzyW/RrQ99UadaWMAEYi32QpaG39TbP099QnaAXnO5axtW5qWLvO8/wt7k32h58/Zs9QBZQ5xEGRZCLuQ18QfDcn/3ecAhKyEUKdMoy0QJ+sRL9Ppz9Y+U11IMGJsYHmmEzePMh+OzvD8P5yQWKBeaulI6o/XLMd0lmfZRDyBRt5Temkby5/FlU4EoyhGHKeLMLafl/5v/dfqxT5UI+tTN7y2ckduAhb77YqpJ9k2Gdszpmbw17g0u4Zt87h4DGPHTcpv3HeCufijeU08DAyLxSHqk3wwTQ/B/42YrCrlgqcuPQPBJYwN4mptMHPmzCDTgZNPzo2mT7cB29eWveb5SYmKevIIgcPA9iEKmDt3fzz40INYtWqV75fciQMDQKGnpwe33norPn/xJTjr7LPw9WuvxZIlSwVfBvMXLMC1116Ls84+G2edfTa+fu3XsWqV3YoT7lvDZ519Fp5//nnceNNNOOvss/H88+4tZgDz5y/A10X9G2+6CUuW2Ce8ydFdd/0dX7n8Cpx19ln4yuWXY9GiRb4+H7DyD1oZy7tNTJOMe+uU7edyvKypfmQ+VSN145Jpe3wjWJQzxgX8BKpMOZj06Pyo1lHStTaWBmstDQongriivLdzlksz/dHjZboo5+nT9pkh6ns+nIxWhVaPPrBonJ5FWdKVXJNn2H9oHTsNv733NTy8YDkeffp1/Omh1/Gj21/Exs2bsGp9D/pKCUrFdkvZBzYNejo3om3tKvT2dWPpspVYsmQlunu6sHzFWrzyynL7W7wCr7yyHMtXrEFfsRdr1250fmUwfuocNDWPQLlkg7+Vchm9vZvQ2bUYGutgoo2I4wi5gn37t76+AZN2nO1Epf4Cu3JtnfquC7CJsU2Oq1qO/7RtzlnDsdv1n76/c/Na9qFUaKqj9KEbCzaN15Z+Og8LfyxjtjD+O8r2gWA5/idDH//XVVZjYksnxkXtGB+3Y0Lcjglxh/+Nj9sxPmrH+LgDU5u6sWdLC1pyjSmycoJ4Qy8aevsQmV7UqX7UR0XUqT7UqT7UR32oV31oUL2oV31oiouoL9gtwclL7fE/XRzJjv815v9OX+H4n27jzK2ZB9jGWZbxPwZ+g+sMHvszugKjK4CxR/IVufk//ZTtZvmF/YSUaA/KxPrUjXJ9NeWO4xjtG3pgEMMYO/flGC7HcmgDvfp17L7hBfzLwSMxsqng5/8teeBL+7aisbsPCt2AKULpHhhdhE40TNJv5ydOJspKnqQdyvYIbXng8T+V14Tjv3vzlwFaZN7aZftVgxokPdzyOXPuFoiN8//E+T/XW3ikz2vne5oLXWJtRrm5ZE0ccFsy13j7t1wEjjjQYMoEoFi0v0IB+Or32tFc34IcFEwZmDXe4KBdFDp67fbQi5aX8PwKoKzzKCf2cx8ysMwgcEYfzoZ4b0n9099Yhr6HIc7/CQ35Boxpsgv4Er7z8HfwctvLma2f37/H+3HnZ+7EbZ+8DUfsbN88gtsK+ldP/wrPrn7WpxF2GLVDVQCYtka+pa/xs1bs52U5OFlZnn1tOP9f2bXe+1ViDBbs0IDHpzehHCnU73cgNpULeH5lgorLt+4nz/lT6Gmcjl0Pn4ubbsjh0+/9BeZOeRjReuCZh6fihXkzkN+UxwGTH8Onjr4eX72kHZ/95O7YZeY07x/p/H+A+/8B1v/4EgXnNHYHF7jtnO210Rp3vvwofvX03zB91CTceNLnsdPoyfjdwnuwaM0Su+2znfwDYpwZNrg5jJ8TyWvCIPf/tFl5hNMF25dtSbvlNXWVvf+3wLzM+B/0X6Rltrj+97/v/p9roRLMW3r/P/Txn7JI/fGa5ZjO8iwb+n9Ij20sf8Ql6cTDWv8bePxHMP5Hg63/Bff/BLY5ZUqSBEuWLMEFF12Erq4ufPXKK3HVFVeiq6sL5110IZYuXerLsjx5kjqW7SHLswzzmaZr3P//5Oc/x4dPOQWTJk/2/IaQy+UwadIkTJkyBbvN2g377LMPdt55Z5x08sn44Q9/iMMPPxynfPR0rF6zxq7/uQdAuWbEtiUP28f/LQ6pA8oc4iDIsvgf4f/A9V/7mgtsGlxxzTW46utfx2kfOgW3//Z3+PZ11+GcMz+Hs884A9/8+rW443e/x+mnfBhXXft1XH7N1TDGYERrK6740mXus0UWqCvyTbqEVatX4ZT3vx+nf/gj+Nipp+F9732vz4tjN691/v+uY47B1V+53AWB78bd992Hr1x9Fa65/Eocc+RRXi+1dET9Sd7UAOsOIUgZpB7//Uc/wFEnvBvf+9EPoQf1f7n+9z/P/yH0w3PlbDgKbD71f7fz04D+b/lhmdB/dA3/D2WHGF+l3pLE7mrCOvYIGKMB2PvqKFJQCogiBbiXE5ie3ovbADnz7ew/zbP6S3xdpYCITFDhdM6c26tbMk6joJJZF65DojKIL3EDDs+9gJ411rVCJ0mCXD7twKQiSY91pPKk4mUDUiY7SXS8CznJr8fF8o6e5FlxMgG4uV3WkMkDF2d8eWFMhjdjDq80Vq8bJ2Cq2XRgBpAuGjLAK4yGMsfuBp0TG/JYqVTsN1VFZyrrR5F7Q9fVo0yJ32bBOiCfyjCuPYy4ESEtqVfeOHg9uydDWJa6SvlJnwKhDq3M6YSaPIP8ikC7lEl2zrIOz5V7ykS2NWnCtRmDihKoL63tU1nECdcpRWKAIy1vB46HSqVSNaBSVgZNbODVAnGRruxEmA/RfsyjXFEU2QWaSPmfhl2AJe1oi/6f2m1Im7xjC/6PwfxfTGCY7usM0/8TF/ynbvmjnOTX4sq2O3GTPnGQtsr4v7sx24L/s673/0ot/09lJFCHhFAnrEf5YjdBJ12WlU8/SlzkmzbLenxgJvV/W1f6P4E0JF/M5zmvt+z/ad9DHTJd/ogvlFPqZFv8n/ho7xKM9H8xUcJW+7/FZWWFf+jCvrltbYx9AunSbgikH9KROqXeJV+sY9xb/1EUI5fPu76HgSpbRvvx39VV8LwZN7mlLyVJBZGTz+pXvInuZALSwFiSVJDLpw8wcU7BPtCyauv5RWGTDf76YLDzfQZ/fTA4cTp2bxbxZ3d/c9dBHbYJ25n6lDZMe2WequH/2hjEeec77klQiHYbEBQwZfIUaK2x4o0V2cmBAAO78MUIWdvaNgDAxEkTbb7RTn8DICAbzPbXBu867l0AFK6+5hr8+je/xpIlS1xmCj09Pbj2G9fhxZdewmmnnopLLr4E48aOww3fvAEr31gJwGDDhg24++678Y53vAOXXHwxzjvvXDQ1NeOb//Zv6OnpEdgUfvLTn2K3WbvikosvxowZMwAo3PrrW3Hzf/wHdt99tvsW8cUYN3aM+6aSZfjhRx7BG2+swCc+/nGcf955aGxsxE9++lP09vZ44ZRco3P2R7peAaI/qQZX2Rq9S3P2rMQbne5o4CKUAr1xD5754K5hINMFRT0OYkr/jPM9yRvtiGnWznxm6u8qWJS0hYGgj82UYf8t+/U01+uCadZnUh2xbi1QsEFPY9zbPC4VYqttC2l9ScfKY0v19ZXw1Aur8b1fP4p///WjuH/+cpTLZXR2dWJT+2Z0FevQ17kK/q1IGPT1bIIxGus2ltDb14O1bV1Y3daJvmI31m3owqq1nfa3pgOr1naibUMHisVerFrdjlKpH0pFyOUKmL3PkUiSBJWy3QK6XC6hXOpDf6kblXIJuVwO+XwB+XweI8fugJZW+5S3FTkwDgGyn47jHLTod8xWjv+2j9P25tCkgV+j2TelgWMGerW3K9ZnO7vvJxqX5+sJOxR2s6XxP1IK8TaM/72V1zBRpUHf8Qz6xjboOyHuwMS4AxOiDkyp68Dsxh2RVNIxXxfLKKztREtskFf9qFP9qFNF1KsiGqJe1Cv7BnC9exO4Oe5H45hUnq0b/weWlWDPGcTVzmd5HgR/fZorE5aTeMAyiWs/GQh2R2FfnA9RDiD7YBWGOP/3dZ1OiiVtH4AEWXc2Jsfj7k4ky17BQdNGoj4fI3E2TV015WPs3gIo0wOTFAGUoEwZ0AmMLgG6H6j0wZgElXICVQrnQNl5n2wLaaNqgPF/wPm/fPs3/Gavzn6zV4LCAOnhNtIi8Mvr8P6/PMD8n/qnzbIeZaqIbZaTGvP/KEm/y8vgr92yWeO4wxRykUJvH5AkwKLFZdz7GNBYqENUAcpFg08fDWzsBPpKQCUBHlrUjw2dOUQqRn8ZQEXQYBDY2Yfkl3JKmbbH/B8A6vJ1GNEwwl8DwOPLH8cdL96B7lK3T/v0AZ/GDz/4QzQWGjGmaQxuPPlGHLPrMT7/xbYXcfui26veGJ7YOjEd5kS/IXlQyr5QwG/9cv5vOHq4smE/Q1nC+X9Jl2DctsfGGPTmFW7bZwS68wrR6DFY3wN0FbXfsc3AzpPBsSHj7warOvLYe//9cPnZEX731V/jqX+/Dq99/1/x6o3/iqe++w38/qpb8OWPLsRee+6Murq6jFxmiPf/Hiibk5VzGqXS+YYx2m9xXUkquPqe/8Dqrg3Yc9JMbOhtx7cevAWlStlNA9Lxr8YQPCRQsHgUAFD/7M9dGSP6FfajbEfZZhIG8ll5boY5/mdxWfr0f9aj/yf/B+7/uYOApEl8bCcJZnvd/4uXGmrKKh7kY5r3f7cris0cvv/L+x7Sjrj+lxfrf+4+g7LWHP8dPYnPj/9J9fgvgXWH4/88Jw2WX7ZsGc678AJ0dnXhyssvx9FHHIljjzkaV15+OTq7unDuhRfi1VdfTfvOgGdJT/KsatiotGHyIMv//Z67sfc++3iea0E+n8eUyVNw2GGHYcdpO4bZOP7d78Zxxx6Lf/vOd3yaqfUGplvv11vl/5bv1P+tXP/I/v+d66/H7rvthjiO8YObb8b9Dz+E/7z5P/C5z3wGo0eN8vWV8/8Rra343Gc+g1/++Gbc/9BD+P6PfwylFObM3h3f/Pq1CIH6ok9AyG7X0Gr4v7HjAPmuVCp41zHH4prLr8BXrr4KX77qSlz9lctxzJFHZuQk8Jp0o6j2Zy+3BBK316E7dnV34We/+s9B1v/tuh7TCMQl28T7f435vwTW3R7+T78mr6zveXfrgtX+X7vf5zXXZ0lbDcH/iY/2ybrEa/VoEEXK+bT17XACMpDPyvNUZhvolXRZtlIpV+GKUgVUK5iVmR6J7SWUi9rLOsw3YiCRZTlplExRkcbY7c34BIDESV444Qzrs3HJq3KGANhtVpPEvuVn3OBMmcmXxWW3r5R4IXRiYIDIGgL5Ig3j5CoL3qPIbmPN+uniSWo8Ul9cQJc6olElHHDd+x+Jm5FzckO5bZn0hohyEvj9Q/ItZVXizUzjjCfVtV2Mh3Nsb0CuvjRwCB1HroOSuiStKtmM8W85SvosJ79V7Mu7p2DlBIWgtQ3WZ982TdwbzKkMpC+BtgKhG3nur923dxh8pq4r/I6Y6IzgZXQLHMJxic/ag9VByrMG3FtIytl6rXPSljqWENLitXH2ZpQLoti12IyfEjftVbs3wOWTQDKfctqy9P900pDhz9kd6wzm/8Y4Dxiy/9tjxfkaBvN/BeQLqf/TtgfSK+VjnjG23eF8MBIDQi08SZIgiu0TfRn56LMD+Ai8TdT2f+ZLfATZNqzHoxrI/51ts6z0HZnm9Rb4P2XDkPw/1RnpM408E6QcvCZfEDqSg7QWTzDK/BAkXik7z2tdk28Mwf95zjr+Kf44drtDuBs/Zb/HDNHXaJ0+7EK9S9pSxxI8LfIu34SVNqrg+1PSZL7lL7I3CJFCnNmOzY4vfltzJ4tOLL8sa3mwY6PlK0JS4fgf2y0ZHQ8Wp8XHcYF8/XCH1fjVjNW4dac1+PUua/DbXdfi97uvwx92X4f/2mMd/rTPRvxprw2484B2/Hm/jfjrQe24bvduxLkY9x3WjQeO7MGDR/Xi0eP68djxJTz2riLmnVjBvBPLmPfeMuafXMFTJ5ex4P0VPPshg5sPz06mqv3ffq+EMJD/+4GFbaFkojgXOoAx2HHaNBhjsGL58rQomzjb1B7FohdeAADssssuLiOoENb3fYWxP8M8halTp+Lqq67CYYcegqeemo8bvnkDvn7ttVi5cqWrp/Doo49i/fr1uOjCCzF37v6YOXMmPvvZz2DcuHF4+OGHAQBjx47DZf/8zzjk0EMwc5eZ2GPOHJx26qno7e3FmrVrHH3LwwFz5+LYY4/DzJkz0dTchCVLluDBBx/C6aedhpPeexJmzpyJmTN3xqmnnoqxY8d4HY8bNw6f+Yz9VvGcOXPwoQ9+EL29vVi27DXXJqmovl0ykCpUKf7HdP68asSJa2tt52k2gMtZmz1jUJdBXlvT4WNf4v58OVHGOB9Vyg7UA/l6mAZfN0gXyqilCVne2mu6k0cVDfZFkgdHk+mgLFaxVkPupke5OX4GpdMhtZvVhlOhl0GhWCqhXCmjVCmjVC6jXEl/y1euQFefQr6uBf09GwEo9HatR0/nevRVcrjr0Xlo7wKefH4Rnli4EGs39OHZV5bgwflPZX5PPrsQ3X053D9vAdauXY5CvX3KfPKOu2PP/Y5GOUn8t4BLfCO4UoIxQD5fwLjJu2H6rIO9bVGmtLXZD7sxIOOX6fXg43/aXxLk+M9ArTEi8CvGA/vTPvgL1072lz7QyXzj7IsPzBBCnLSLwcZ/7RazZNpwxv84WYUJalPmrd8JcScmRO4Xd2Jc3IkJ+U609LRjav0s74sAEJcT5Fa2IQf7hm991OcCwPa6UfWiQfW4Yy8aVQ+adkzvhYc9/gdjivcdMY9J/UkjGwQOA7ommy9/vlwYOGaQNwGMe0PWVHwg2Jg0UBG5IKCquv+392jSxqIaawVG9AeUi/f/xd6Kd2Vj5ENark/VBmb5K1CVBIV8wdZ3cyLSMcZgxogKoPsRoQjoIrQuwehu/2azTiqALsHoCmaZPT0v+Xw+wxdcO/Eo24XyMc/Uuv8XfjnQFtDyuhYoMaeVYN8iDraR5tHR8vp2INsGQkbKxbmyqbr/z9qjtEkgG/jleaXP4Mh3AKNGKPT0Av1FIFYG132vA6ObWxBr+4bwwbM0pk2M0NULlMvAgsX9eOkNhUKugEqi0F+25hlV7C/ztrG4TyfPBDm/l7wPd/5PUO4enNBT6sH3Hv0eVravBADk4zzOecc5uPaEazOf+Zg6ciquedc1OGaXY/z3g3/1zK/w9MqnUdHCXlQkRrVUtxn/5/yf7aXTN7QHslOJj3n+Gsp9tsvNUozB2sYc/rRXK/qTEvKxG6Zhy6SB4PQnehzUFwClDIxOoBNXyWjkYo4bBirKzqOVXP8byv2/SQOsDkEm3Yg0GI5rlvaYxhFoqWtEojVa65oxuqHFvZ2g7dHVya8rom55L+pf78XmV14d8i8pZXeB8PyII5ws1et/2fsxNcAYCWETg4//KT7Cm+X/pEf4R7j/T8T6YAgSr5Q91IW8Jt/YmvHf3/+7XSq3dP/v7p811wJ4jx7ct3tQ6f0+8fKaP/Jk551ZPMyPIssf2zs7/qdjIuWMOP5H2fE/1OGw/T+oT5tcunQpzr3gfHR1deGqK6/E0UceZdf/KwmOPfoYXHX5Feju7sK5F9kgMGUgrm0d/8P7/66uLjQ0NPg0CQ0NDdh99mwceeSR2GfffdDc3Izp06dj1113rarzruOPx9/vvcfdJw3u/2aw9f//g/6/fsMG/PhnP8UVl30Js11A+Il5T+LCSy/Bfu94O/Z5+8H4zDln494HHgAAzJk9G1d86V/w45/9FJs2b87IHupCXpNviMAh5fd81dCFrZPqjmv/LCd1rWqs//P70x7S5h4USJu/EGRbMT/j08Px/2D+L+VT29H/WUbJ+J976IXXuYHW/2HvzRnnYpqVT/mHLphO+VjG1PB/JQK68qgU7MsxUYQ4irxdEI+UgfpJeRnc/5kv8RFk27BeRGQUiAJCCMbCzGNjUvE0YBKWYOAWLMSr8qxLkAOWqvHUBxwO8sB04qsJyt6QamMXlm1Syr/ObJ/g+BTOJeXgRFsGvMijdhOJsI5fuFN2gUcqXzaClcU9ySGMy+M2NtCp4bZq0tVbtCSJjfrzbSsCjdsYuwhJUyCfmQ5fPC1H3rTWSJJUT8QJpaDcVhQGlk+2G/ESJ4FtRv2xTArp95mVM37f/kKvVt9i8TSwK1/etYc0drinIOAd1OaTf0N7FXbgcQrb5CSJwDIsR96pX8WFTRdkiyIXBHZ2TT0p9w3nEK+FtJ2puzTPgpcjGMClnpkn64D+7974pHzkzcD6E9sh6/8pbtIPgXxwa5GQB0szXTgm71JGqWPb/lvwf/qe2NJM8q+D7VNA/sUCHCWjXJSbaVIOWyfyhpG2adYmavt/1s68/ejqp5W0u4mRfNEuKBch4//CBkhH+r/UU8b/K+ngKXFK/skHadM+JU0ppywjYSD/J78QeiewXRDYCH/kkzg4SEs6od3ymvwyT8ooIeTTt5/wf5aRkxHA9p/GpEEdvhXu8bobNgBIKond5p7+L2/ytsb/3Zv/8MHbQcZ/scMCg7lau90PXJVQj7ai8P+cGP9Zz92M+vE/stt9krZSVn7KyxvSa5c14QsvN+OSFxtx8aJGfP75Blz0TB0uerYOFzxdh/OfKuD8+QWc/UQO584r4KzHYvzbIkv/c4/k8NkHI5zxUIzP3K/w6fuAzzwQ4ZP3Gnz6PuDT9yt86l7g0/cpfOo+hU/crXHtgrTfw4D+n9Ud00F7A5D4SaIrazsmlyayjPhBYc6cOdBG27dbV74h6rqjAiDa+YEHHsDChQvR1NiIffbZ16cDghzLs5rn3xewZdxlU1MTTj3tNFx91VX47Gc/i/Xr1+Oar12DN95YCSjg5Vdextz99/ffOiLiQ975Trz40os+raenFw8/9BBu/vHNuPGmm/Dlr3zF5riApgWFAw44wNsIACxbtgyNjY045JBDXBlbLuXb0ttt1qw0D8pvm7169Wr7hocT1VZTUm0O0gSZp8IEgleR40PZBrQ24ARw7eht2leVM7PUbpgnF4VZ17j5XAisS98BrD4zOMN+mSeB/XpgWZGnFFeNs7hq6gZpOvH7Ps+mysawZiyN35E1qSb9VS1+i8V+lCslVJJy1W9N2xr85f7H8Ys75mP5iqVYtvhxLF78PH57zyJ875f/hfsefRJ33vsgbvvr33HbX/+Ov9zzAP70t3v8NX933PMA/nrfw7jzvgfx9PMv4Cf/dT++98s/4Pv/+V+4c94KPLy0AW2b+1Aq9aNc7kepVEJ/fz9WrF6PW/+2CCPGzkh59yJSQqdr4/RmAOXfhLbzVz4lzf52a8Z/4+Z22uXZa21JamO3c3ZvXgLwi0+22VnHlRc4CEaMQeEPg4z/fPM3Fg+PynYeyvg/Wm3A+KgD46NOjI86MS74jY26MC7qwg4NPZica0GDGp9uv2oM1KYOqO4OwHSjXhVR57/5m/32b0PUg+a4DybZgPpp9Z7PYY3/ga8OPP93wSoGfPmWrgzi1traueY102xw12hxdD/7xqwNBMNtAa3cnJjjoJYPAw80/gs5OL9kXYLEndqTO4oHE3T7ephNbUCugOdW9SB2fiChS5fxWN8biEw3lOmE0l2A7gR0H3RSgk5KgKmgUtZoTJpxtH6P1z/554/A9MHG/7D/lG0KIA3MhgFbuS10DRgonThqvfnLt4wH838MMP9HOP8P7LXW/D/cAtqUgbEjDPbZUyGOgN4eQCfAHXf1YvXqOtRFeaAMxInGJ4+PsG4TUOwHOro0HllYxuoNMZpyMSoVoFSCfQNYvGFs3y62/EQ1/F/+tnX+TyhWiujo67D5RuOPi/6IZ1c/i7Iuo6nQhHMOPgdfOforyMd5X4ew67hd8S9H/wsO3/lw5OM8uvq78IsFv8CqjvSzF21dbZk2Quj/yrZX7O7/2TdKIN+0S9aXeKXNjsu3wGgt+nrbp989qxnP9K/B5FaNKaPcrnB+jEjHDJ4nxiCOgDlTciiYzUBpLeLIbrFuTIKkYgDYc63GZ3iA8H+ek3cpv2xb40ZKuf1lCHZHCvvTWmNMQyv+45QvI0kS/PqZvyOOIlz1rrPRkm/w20SDx60FyQ/932fZORPbI+M/YnxArfW/t/D+H1vh/+SDtDm2S5pSTllGwltx/1+uVGCG4f/ESRxSvwRbJr13Ju8Djv/BiyvG8P7fPgydwVt1/5/z25UyWEHgw9bGpDtdpQHc9D7aBpUtUu3v/+3D3RKn5w28R7d5wx7/3U5Hsp1kPeqI52xj6ox1Ql0SH9xng85zwd+vXnEljj7qaCe79usOxxx9NL56xZXodm8CL122zOPGNo7/YR1jDFpaWvCiewibMGHCBBx88ME46qijsNPOOyOfz44XLS0t2H333bHDDjt4+ZqamtDV1WXn5Yn28x7yVcv/zf/3fyilMHbMGNx2669x9BH2UwxfvuqrOPuiizB1ylT84Ds34gff/g5m7bIrvvDlf8EV11wDADjy0ENx262/xpjRoz1O0pJ2Swj5pM+F/g8XB5D6tN/8vRLXXH4FvnbFlfjyVVfi7/fem8FLkON/mAfArsVXu18VhGv2EGNpa0sLPvXRjwGh/wv5GAfTQ/X/wF9Zl5DR3Vb6fy1gWZYjrpzzk9ityVFG8m/78rSN7Bvx3PpeA25bZju3SAC35bJFbwDYeZSkSXvmUdKWMsmy1AOvmUZ5yG8t/8cQ/T+KGByh8sXEzk/2nFgMSMg0GjWP3C5XuwCGBArEhoRVlRcMojFkYxsxYDOPZZXoLLwS3c+4sonbwoAOSSVaflyAV/BI3FEUie+7pk8qMB+A2yozNXrtnMKXE0bNhrOGZHnVtoCXVeZFcQQDfl/UfntRdgCkp9xT2V5+xx/L2W1+Ux5lB2JcO1FPrGv1b3VO3dIGOJFgUIC6ZNkosm+CIXBuiMElLRv7DknyQH1RLrYhaZInljXOLhOnfz3InuyRm/T5tnb2Sj7ZBsTv+YX9PqqkG4knXSg7aUWuXSA6K9n5E4wxgErLSiDPUg44fskj7Zdbc5C2xMH2QWB/5IvliNMYtzRt3KCi7I2v3VQp9H8AbsFO2hD1S6COKAvLybLsW0J5q/zfBagpK/FkygA+qK65dY2yT06n/p/l09sE/V/op5b/y6cGEfg/rYf6r+X/RviRCf2fNxLOzmLXyYf+L+1P6pXlZDpq+D9tw/uesf2FUmnATdIjfuXK1PJ/ysoyhGr/t7wzLfR/yuX9X44Lgf9TFv5oMyzPc9IkXQh5MJj/i/Yh3WgL/q9dn8VxRN78cbLG8iwrgTwr0RasI2UGgJzbXpi0JQ7qDoDvw5RKg7IsJ/GGOpB69nX4ZLGra31sC/4vAr6hDMb1N5SZtGRwWimFlzojPLs5wrObYzyzOcIzmyI8sznC05tiPL1JYcFGYMHGCAvWA/M3APPXAy9vtnwuWK+wYIPCU+uQ/bUZzFsHPNUGzGszmNfm0tz1cP2fQP3n8jlUkvR7ijVBueCPsA/AYK+99sYJJ7wHzzzzDG751S3ZOraIh76+Ptz03e9i/fr1OPvss9HUKL5vCcAuTpEI0sqC54yRymRjb0jn7j8XV191NRobm/DII48AxuDFF1/E/AXzcdbZ57if/Ubvf932R6xfvx4AsGHjRnzl8svx97vvwbhx47DbrN1w8cUXe4qp3ty4Q1aNwcsvv4zp06en+TX59hX8pDyjbndtXGy7FtRun3Q+SbqGAVo3N4AP2DrdOkJK4lRpMM+DD/JV5QCwee4kBS966o/SP6QM9COZL/OqgMoRY5hPl0e2GbMdPywjfYBplNW/0Qyb5v2KZYOGs+V5zbru3OnUwGDt+k0o9vejVC5V/da0rcYLS17Dr/54Ny78+m/wrV/ch8tuvAO/vv1ezF+4GC1NzWhpbh3yr7W5Fb/40wLc8sd78Ovb78Wvb78Xv7vzQSxbvRH/+ov5uPYXT+JbtzyBb/z0flx8wx9x5pW/xK/vfATrN7W7fo7ao2yujXySTaOdKfeAkF3cttJzDPJ9q9OZMem2WzIdbvzXJn3zVxttg786nfO5pnLnGsbAbgOttb25ZRk/TqRjQ62fHB8hbDIc//lGTqK1v1E3wxz/R+dymJzvSoO9cfobG9v0cVEXptZ3YmLDnoBKx0OlNQptG9BQr6Hy/SjEbutnt+1zg7KBX56PypUQTygDowteHuLy4/8Q5v8qGKMJlJe/qrd7eW6MCPSKvEyaKwMX/NXavfHLrZ7ToI1/+9cFh+HaROqd/BlYW2Y7wcnEdiXIe1TKKdstZp+cCQLbBWRjANW2AirKQUUxnny90+FK3zowxuDmjhexMemxUUiTAKbffu9XF6F0EQoVa786wQnqZIzCmAyfPGdbbsv8n6CUSrd75hbQPoCbnk8vfwIzSh/HjP6PYafi6dipeBqUSfC9Gy7D96//Ir5/3Rfw/esuxfe/cYkL+g70HWB7PZj/M426VzXv/2v7WlhGbs+sKkCUGOy/r8LIEQo9XUC5H1i/roI77uxHU77RvyF88mFATin0ujeEn11cwvyXgUJchxyApIz0DWD3i90vSpyN1PB//rbn/L+r2IVVm23Atq2rDX9+8c9Y3bkajYVGnL7f6fj8YZ9Hfa7elw9hr0l74cJ3Xoj9p+6PXJTDva/ei/lvzEd/pR8A8OLqFzPfESYoN+/PtIXwG8qMrbj/n1A/FnaH8bSNdWTQmY9xW8dCRHEZB+2URxSZ9E1f8e1f758G2GF0hL2m5hCV1yLpXgbAvmUJv6W8hlIa/bldvCwI/J/X5JnyIrz/t2KJYdLOs3ht8bjPEjhGzzjoZOw7eRbmrXgBX7rjRixZvwLvmLEX9pmyqxfIBoHdwLeV4NtFpCnaVxBAC+3SDHD/T1t+q+7/JU8sI+mFZf7//X/kAgJDGP/dizMSbPl0rSCdDyofjFDuc1CWdiq/8Z8mUsjl8x5XFKfr1h63e0GBD3ArFblgovMrv2tMtn8hL5Sxll54HGz8ZztJmyA+liVu2W4I/V/UpZ7/+Kc/oZNv/h51lChrg+rarf8de/TR+Kp7E/i2P/6xik/Jh7RjDDD+FwYZ/489+mgsWrQI+XweM2bMwJFHHokDDjhAPCA9MIwfPx577rknxoweg5defBEHHXgg4lzOPgBQcXMY/33Q2v7PnRVlOv4P+v90t3vavQ8+iD//7W/4z5v/AxdfcAEO2H9/HHTAAbjkwgvxix/fjD//7a+494EHEMcxdtxhB49f8juw/1sepk6Zgt/+4Q/45a9vxX/+5tf4w5/+6HVk8XiUuPu+e/Hlq76Kq79yOY496mgcfcSR/pvADALLdiAPkH4j7DeO4yGNXbKPkvZ9/lln454/34mzPnuGxy91kOo59RfyxON/l/8TT1hGDRD/k/eWkk/JB2NuBD54w3wMY/5Pmkq8hSx1x3Pal5SLdha/CeN/RAYTbYO7BBKQymVaVslpY5JJOjmPFILA9DiXLRsKQL5kunRAbrWhXWcRRZGfqNIQ2ejKGTuvLU77dGNI08sefC83dhH1OLZBcwbhZF3lFtWjyAbEmA/Bk2Zn6baopXFH7nV1re2CDIPpUZROSKSBGqQ9itS1b484AqLqmwG2k0uoqucyPL1Eu28fI32iTP6kwZMn2d7UKcukMti8tHO09L1RC93GudgHLljf86vSJ9OZHolJnuQ1bXtbhm98ko6n77bmNcYtivmFMftju0m8vIazDS0cWv4kj1I3TAMXwsTDFVavbssrZ2cMeMtz2dYQMlFGybPMk20o62X0IHEpG/zxR7inCHMxVBzBMNhV5f+pPYZ9BXUApz/akUwP/Z9yExfztuT/DB5D6IZ0qIaIAXwH0v9ZnvRY1+bnvM/KPjX0fzga1g4D/2fA2pWhPUn/R9CuTJdpXCAjqMD/Q9klaGOQJOmNki2TtQcT+D8Au/OC9H9hc7JvMMbeFHOQJX3r/7FvB2OMnfyKJ89seXtDY4/2zVTi4ffKLW9pW7F9eZMUxbGvTxms/1f7rf3ZcqzLa+KTPFu+q/GkPNb2f+UmLcyjXuSR/bB2N43G7cQQ3mAa4wKqzlcH8uewDXk+UH9R60i7kj5NXNIemB6WlbLynHwxnf5vfcH++PaC1m6xWKfn2vDaoLPk+gPYdgTtwhJ0R7advfAqMcPx/7QvYj5g+eF21x5csNvf83vGeO4KAXjPCe/BbrN2w+23346vXH45FixY4NFwyekvd96Js88+Gy+99BImTpyI49/9blYXkA2updxkC3LMG+iuoqmpCdOnT8P6DTa4O23aNMzdfy4uvcR+m/eSiy+xv0vsOQDcfffdaGpsxNVXXYWTTnovjj3uWIwaOTLADMuLJKsUpk2bhtdff13wQ37dMdN/WT/nT9ahWhV1H4BhbK5K7tRGGMS0JQyYktawelNu7E7LpXyEgVAG+QBnT0F78FrB2kvGtgLfHChd4vegXERcgOeSefQPm5g5+lYQN6q+LnEZqyNZoaqs02tayfkY6yi4ObvTpghYEte8515AqVxCklSqfj093egv9mFU6wgU8vVYsaYLhVw9RrWOwA4Tp6CpvhEtTS1D/jU3NmPqhCkY1TrC/0Y0NmPjxo2oJBW8vrYDzyxeg/kvrcQry9vQW+xHX7GI2//+SNpOSlk1Kntu5XX6ZttBWQsx9g3gdCEw1XH1+J+OJVGU/aSJ7Zucbl3/mL4BZgPC9tzeTaXfQTeeD85FfB1RptZPQnY+MfD8n/WMm0f7vj+Y//NIPOPr98HEXCd2aOjC5EInJuU7MSHuwLioA+OjdozPdWBqQwdG6hxa6t8GdxsMYwySrm7Eq5bDFEpAfRlRXQn5fBGFuA/1US8ao140um2fG6MejMz3o36XZkRu/iZ5Jt+1dMF2UMMd/wcK+Prv92oXwOW5+Pk3fStuMbdst2vVFfe2b2Lf+BWBYL4xrAPe/VEBEJ9FCsd0r9chjP87NFNH7HLEeaKBjvVAlANUjHJicN2dS1Fx82XiykMhQhkKRSjTjQgl+7YtDLRJYCoajboFR6qjsafau7rPlff/wTx2oPHfiLrMpy14nelgy+ca3/DddOoF2Hjahdh4+kXY8NHPY8NHL4YyGusu/jraLvkG2i69Dm2XXo+2L9wAhWwwGZm3ge219H8Cr0Ofk3ZGMM7XQn/1crsfg7NKAygDUyYBM2bYt377+2wg9847e1DubURsYugSMHWswcF7KbR32Ld8N25OMH9RBU25HGZNUqhXBuWy3RYaIvgbcZtpPbD/U8Z0/p/ySv5ZhjqifKjR/wDA+s71eGGVfZvr0dcexcvrXoZSCifOPhEXHXIRWupbfNlaoJTC26e/HWcedCZ2GrMTyrqMPzz/B3QU7VvF9754LxLxHeiB/N+4I/O0WHgn3xIoA3FIu5zRONmd8x4JgDHQscYCsw7z172I4/bIYdbEHCJlY6Mer/jV5xWOmVPATuM1dNvvEJnN/q1aYwxysba7LGuDYt3bBvR/KSvPa87/HQ+a61LG3kdSPw6Bld1oTGoeiwN22B1rOjfgm/f9Eh193bjs9pvQ3tuFU/Y9Fg25ujT4K/x9q0DZNyXJC38Q/CbaPuhvnNzST/m97USn63/cyZBrHcbdmxtHj3iYzjQV2bUk5rG8veemr4TzhhRoU1vyf7YRge0mr1kWb8H4T12G/s81H9Idiv8P9GNdXhOf5NkMOP7bNQv5ybsUhx1jEvegMNNDeVmPb6fZc7tukkI6lrFuKBfzwja0p5afKt7Fbp0h7tCnLa60zWR6WFbKyvOa/u/4lOv/Hz39dPziZz/HUUceBbhgDWB33LL6Stf/jjn6aPz8P36C0089FRD8kw7x04YIcY3xn+t7rMv8KIrwqY9/Ao8/8QSmTJmCOXPmoDF8EHsLEMcxps+Yjr/97W9424EHWnoiwIZA9zY9u7ao3oLxP7Qdtpu8Zln8N/o/jMHF55+P3WfPhlIKt/z2N/jVb34DpRTmzJ6Nz59/fhX9gX7RAP7/javsW8TzFyzA/AUL8P0f/wjXfvMGT5+DgVIKbevW4ZrLr8TRRxzpcRx39DH42hVXYs3aNV5voZyqxvgPAN3dXTj4oIPwtgMPxNsOPBAHHWB/vH7bgQfimCOPwvRpO6Y6cfjaOzrSsVPYV6gHW97aU8gX7Ur6NHG92f5PXMzb0vq/xMm3n5kmZbd8k7b9LrL0f5ZlXeZLvcFhGHT939nPQOv/xCV9B4HuJR9MI14CrylDxEqyMiuGQOWzPNyHkyGiymQybFAKrZSyTzq67SdlHYk7cpOWWLzGzDIQnQLBGLsVDYUlLcoif8akkycJIc/lciXzFABl4LcylXhixedH2WAcy0n8Wmv7/ZXgyZaE3wXx3+pNJwjkO3IGYwMXKf8soxTfHGZfo/zkPopiF9AxSLRdcmS6ck+ZsQ2iOEIun0OUc1uDiAUOKRMnCXGc8xMs2daSb9qPxZO2LctzUsu2Z1vLCYcSEy0/IQ6evJN2QT6lXcDpJtHadyKsywCJLZwGTFjX0ooB/0Y4O0QR2LK1AeEXzKNNRKJzyeXsUyRSX3Iwkx0HJ3WhrKzHdqd9G3dTIG8cyAeB8nkdeP/P+ke1/6eDeS3/18Z+N5vlKB/rSJ+X5xD80c5lGdD/xduLXJCU7ZzKku0DPP8D+b/jmVuS8G126afEVeX/gldO5jM3aUEnXtP/XTm2gxH+r1w+fYfAMpRZAvUaBQMM80iHNJiWy+XswyyxfVCCQVEV2WtrHwpRHKdPlTq7ZhkuVssyvKmIc3ZAtd+UpZ9ZfGmAI916SLltiGRw1j95S974VKtCWtdtcSSv4b6vUymXPS6Jm5Be27qkBXdzwXrER7qWYbttk+VzIP+3T+5T/2yDgf0/bU+l0jd4WY90IQKLxnDbp9TXpY0wjTjJYwjD9X/iYznKxzp6CP4/4PifpMFem+cCvtouNmWDv4DWBi15x4+xHaRx/SX8kbq1FxST5aSfUpbB/T87/ufyOfT09FhCBLalbai08cDzFHbZZRdcfMnFmDlzJv5+11343Fmfw4dO+RC+8MUv4sILLsSRRx2FSy+9FPOeegrNzc1Yu3YtvnDppejp6bUI/BiR3ojAWnZ6YSW3PuO3NVOWb1lMAT09PVi/fgPGjR0HuCdtl69YgYkTJ7nv87rfzvYIpWz58eOtfMoGQF/y20MPDlOmTkFvby8WLeK2Wq4hqSvKFGyN5hLDBDcvsrbIyrapUuVkr127cA5hBG3qLQBfxhkTQ77WDG0N5fQgQfqft3keXftJ26Ld1QLpVwSJXxg6M2toy9WxSvNpPDMi3RinIx5ZzpqSr0Q5jAvi8g8s6/lM9c184x5G9GCAhS8vw4uLV2H2rrOx+6w5Vb/Zu8xGU30jRo8clfmNGTkaO0ychJ2mTsMeM3cb8m/W9JnYecdpGVyjRo7ElPETMXev/Wr89sdeu+2Jec8uxoLnF4O+b6y7+X5A8W3zjMLssdhXRD5ndwIKbYT2MJTx3xjx5q/nw74FVS6XXcDQVAV/w+v0PKUl+3KZx3SODeH8n2XJP+8HpI1TPuIOcSql0Fx/GOpxFMbVj8WYQgFjY4MxKsGEXAmjdRmjdYKR8Tjo8klA7wREfd1AVwfM8tegH34Q+VI7klwfVF0Fqq4MVVdGXFdCrtCPfL4Pdble1OV60ZgromLagVmjgWDRi7Dl+f/Qx/9E28Be+tNui9UEpXKCYrGCvv4y+vor6Cvy6NKKZfT1l9FbtL++Ygm9fWX0FkvoK5ZR7C+jXK5AJ9wG2m79bIwNDqPW+K/S3bMGG//NEMf/U3ZWrnuxfYkx6du/pr8PCrHr261f3L5wHV5Y3Q0Iuztr9J64cMQ+OKAwAeOiBuR0grxJkNMak/RYnFx/PM6q+zSOL7wb+ch+R5gQzlk4/2dbUAY5/stvSEo7pg58u7oALbd7rr6uth0AGDAgpY0NbAdbQMMHmNN61LH0f7YB06XtMS3n+hlps9QPdQSIbwBXgLqcwcxdDFpbFYo9gK4Ai1/ux8uLFAoouLeEDY4/FOjrVegvAv1Fg5eXllEuGvzz6QV87t3AfjMSRFqjXIIPAHPr56iSvgFcy/+Hcv8P115V9//+PiQLG3o24Kk3nkJbVxsWrFqA1Z2rccAOB+Cst5+F8c3jq8bvWhBHMY6ddSxO2fsUjGkcg0dffxRrOtfgjc1v4IElD2TeAPb+HwX+L9pTysq2k0BZqSeew+ljz5EzUefuxVCxfT9xdxa7cdP8X2JzshRfPrEBH5hbhzFN9kHTxJWpyxnsPD7CJ99Zj5P31+ht+x2Stt/7h0kilditaKERRRXo3FT0F/YY0P95Tv4w2PwfwRbQQicA0gC01tjc044v/uk7+NBPvoAFK14AtMGDi+fjgzdfgm/f+0v09/cDiYZJjH3QxM9qhgeet4CX8CjbggFfiM+D0Qbpd8TFNPZJGVseZPzXNfyf60GSDmkwbcj+L9b21JDX/7Y8/vOatKR85PPN9n95LWWBGPOIk+0qoXr8tzJHmfG/1vpf+jD7oPf/opzkm2ksX8v/CUyTOpB6IvABfGPchJWfkNrC+I8hjv8e91D8P1j/nzRpEnbeaSfRznbdjzuHhfqdOXMmpkyZ4utjK8f/we7/95gzB9d//Vocd9xxuOH66/HGG+7TTUOExx97DO9/3/vR1dWFz3zikzDGvpgQRXaNK20j4wK/ts3tSwBpP0m9Rm/W+P8P4v9HHX74/2vvzeMsK8rz8afOud0z08MMjGzDDIKyKKCAiiwugKBCDFEEv4kMiyuCxAEX0KjfGJeoMeKucV8SI6BZXJN8ExU3TNxwYYkii4qyDDIw+/R09z1Vvz+qnqqn6p57+3ZP9wC/5J1Pzz2n6q13q/c5VefUWXD2GX7R/zOf/Sze+b734R3vey8+89kr4JzD2WeswlNP9IuxJMqlLOpCH/wfeMABeMvr34D3XvoOvPfSd+Bv3v0efPUbV+Jt73xHlEEfzj5jFU568pN75v9PPfHJeO5ZZ0f+QfjvBF+fdeoz8dFPfhJjY2N476XvDH/ehve8/R14919fivde+k68+fVvwM5Ld44+AMDnv/Ql/OKXN+DE446PttEnJfafPgFMm4bB/8ZNG/H2d78LJ57yBzj6ScfinHNfgBtvvinrx09ffhmeddYqHP2kY3Haqj/Bld/6Zoz7IPyv37Aeb3vnpTj6Scfi6Ccdiw9/4mOZL8YY3HzLLfjzN70RRx3/RBz9pGPx9ne/M7Y3QPweb2X8bK7b7WLT5k14x3vfjaf80dNw5LGPx/PPPw833PjLKLNpGtx088146SsvwdHHH4unPv0UfPXrX48xMMbgM1dcjtPPXIVjTjgep606A//x9a9FH5qmwU+u+RmOPO6JOPK4J+KYE47HMSccj4teeUlszzgy94gl7SPy0Gcl9kvVgn9z23//t2vrbBSDJYmCvIAEcNahOJCqYQ2/f1DIUT2cyJBH26seOsl6/yrlXt3ldlr0SYNwLY+Dqx4LF+7USt9m5YIAy6JflV8E4GKFglXj4FV7vWoreZ0c7FhHXc6lBaAmvPeb37QhOG3goY1qC2X6xeU8SWKMw8DBE1u1Q7d9PFNbJzJ8LP0CmN6R5Nv5NjzEkl9/Va/nzfMgMMR6EvfJU4c7PkhVuMMS8IMEB3gXFhO9T9GyLIYsJz//MpvCSRr1mjAgq13Jx9SOMvQAR9I8SxRyXl4rXNqT+5IPZKU9vd/SSXYlSm2JG/KUcqvitbC0qWkaf5CFP0GjHNVDfm5zvyr0aL8YudOx7ov/hG8S9evrIKI/YXHACP4gr2/Qfon4l8lLwn+a3JgwsBjGvcS/3GKtbaiLeuuQx50W/KsPyZYcy1qn+qLvYUDXNlxEV/m0t7xBw1p/8Zg3T9A/lU8ivzH+268qi7z+IqD1NrTUk0p7OnWdXaCrqvSNnbpTozs15Y/ntg3/Xp6OV5RBPmfT67tJ/hstNZpuA1PldlbGv9GCeNO4xLgNhf8UN8U/x84qjIc6USMuyKsyStmktnI3FP4HjP+CW8pRPeTntrZXPWf9aCfcuTX4Pe3ir8/HA5cC/3iSw5H/XGOyCSOd4y/1+R12A3U+fBfgC6f4cYO2D4f/HC8TExN46P4HeIVDXDREFmPfxlqLT3zyE/jCF76AO+64E40s6hx44IF4/vOeh1/84hf4+898BgDwjGc8AxeuXt/iIq0AAIdHSURBVB1PeF3xbVmvhP8VOQKD3932O7zlLW/F8ccdh0MPPRQLFy3EtvFt+Mq/fAV33303Xvua12C33XbD2rX34K1/9VfYfffd8NSnPAW77LIM69evw3997/s48YQT8MhDH4mrvnMVLrv8cpx+2mnYb7/98Ktf/wo33PBL/PznP8clF/vF7ZtvvhnveOc74z77wxjgr972Ntx66604/bTTsd9++2HbtnFcd911WBXu5n7xBRfg9NNOw0knnZzlzIsvuACnn34aTnrqU71fxvjjhfE+e14Gg9TbRyY+LBsW0WPcAukYUsQU4KIomf2GssUF0MihsnrL+2GH+6S2co1PId5TC/5jR1C2bEcvWaa/hX0t1Vk5txlkVcn+8jx+e8OmLXj7B/8R4+P+lZozIeccNmzcnI0VM6HdHtT2BPtgWjA6glec/yzs/qClEn3t+5AQ0XePgd/efDN2Wrw4HvvL8V/zr6r8CS2PRZxDOefwgpeuxpbNW/x+iIFz/gmDAw88EGesOjNa4pyN6S6F8cKy3/Xbe+yxB3bffXfljDRSVVhalJlh5v+cs8hcW+tJ3DcGMG4tRs0tsFMbYFwXI806LNhyA8y624FtFdy2PdFMHQBMVHDbGmCbw5bfrYPdNo5dD9gHU1sBTNVw3QpoarimApoKsAaw/lixcGQUm5csxOQ5J8KNpJuE0/w/H7e8j2ks11/6X/pUjv/Lp16F9Dpnh263wfhEg/Wb/IKvn+qFev45/8SwQ+NBpNtwMM6iUzssXgQsHTMY7VgYecrYweKe5V8HQozj+G/CzY3ST7TZhTzUhYnpxv8f3uWw6mtTmHQ1RQOcM09uxeiN34epRmH4nVVnsffOC/BPqx+NJQv8PKgKN55OosGU66IJ8XbOooLBwmoB6vDEN/X3O//nPvsAgjPtFy7cQN5uVI7/j3n9leFJXQsjcYfzv3Z8Pdae49+SobTHp96Mu16VLlSRVrz1JeiMLgYQFo+DHJX7nY+8FGg5/6f9Suwj+t47/0/1KgcAXvt/DoKrgC6A5fs5POFpwNhSA2cAaxy+9IWNuGPNIlSjo9jWdXjE4Q5PfUqFiS6ACpjoNrji3zbjsEMW4q9fsQAA8J2fjeMXt9VYtGgEV3xnM361fjEwUsHWgK0A2wG+fdaN2TGJ9jCf2s7/tR+z8//y5oYg79GXHxN2gIMfdDDOO+Y8XHnrlfjur7+Lt/3h23DqI07FwpH+r35uo9vW34aLv3IxvnnLN/HB0z6In//m5/jg1R/EBNLY9dOzfgAgvIWOT62IDNMy/y/7SX2hn+QFgN9uvQtv/O+P4I6Na4E6DcgO3t+6qvDYFYfh/z7+Aqwc2xc//W0XP/3tFH51d4OFIwZH7DuCR+7dwYN3tbjm1q9grzVvx4Pdb+EsUFXp3MMAaBqDzTv9MTYuPR/OLIBrwT9t436bT5OTk9hzr+WJJ8inpyb48JB3ne6f6A3jpj8GIuyHd1gDgLWhPr3XevSuLkZGR2E6FbY9ZPin9r7+7Hdh/xX7AhJj2q9+3XXnGnQ6new4qW1Q4I55y5hxv238V33lsUjzgscrRl5jjBnin/aTh8fS0j+VTyK//pa86ldbPam0R/HvZol/xpDl5O+1ydcPHP8r+uhlqi/0v/SJNpOXRP7twT9llLJJbeWMSbymJNfeyhjRDl4jmW78Zzn323zStsrfphvO39Si8VBd1L+9438j1zVpl47/v7jhBnzy7/4WX7vySmzatCnqn45WrliBPz79WTj3+c/H4sWL/TXT2j853nS7qDsddKemgHA9y18nE/zXFeCM/7yHrNVo/EicW9N3PkHNsmuvvx7nXbgaP/jWt2PZ0U86HitXrMDnL78i8pqQUxe98hIcecQROOeMVTHmKp9Efv0tebXv2upJ3CfPoPH/in/8B7zjfe+DAfDy1RfiOWeeGfWQNE4sL5+IV5vQB/833nwTLniZn4sdctDBeN+laTGYv/S/9GkY/LuwAPq6N70JP/jRDzO+YWjJkiV41ctfgZPC0/OkUidiTDxeyKP9hDb8B/+e86IXYu+VK/GnLzofK/baC5/57BX428v+Hp+//LPYeenO2LBxAy773Gdx6ilPx8oVK+L3kT/6/r/Bow47PNNT4v+1b3g9AODVF1+MTZs248JLXo5nPv0ZOOeMM2GMwfoN6/GsM1fhuWedjWeccgoA4Ec//jGecsKJffFvncMLXnwe9l65Eue/8FysXLECl33us/i7yz6DL1zxOey0007YuGkjnn/+eV7XqjM9Tlb/KT7y/g/g8EMPw4c+9lH88Oqr8bKXrMajDjsM11x3Lc67cDU+8r4P4NGHe5+uuf46vPv978fLV68GafHYYhyw//4w8zr+A+aOX/zClR1HIqORuxCqcNCsqjSAsoxKEJRqJ9Fo3pGjZcaE16WIcXTEhEQvk4pyTXgtrpWFRpUR+WQ13Zd72fSNPhC8VacGwlOeTJDGWnQ6nVhGP73jPmHIq75BJw6An3BKrJqmQd3xK/qNHMTV/zJGbfXWpYuOjEFsG9rwhJ319IH2VbVfXKJt+ss4BesB2lMcqKKvYdEG8QkPxKeMKVO3SbQZvmVWRz9Zxj6DHID4S37vu3+dL2OGcLMA85rlKb55bKgns63MR9Gp8YqxD3HqhteSUC7bUGa/cv6yzIQLgyUln9vb0hf1F/B3KKs82uJ98Qca2kY/qr74753sMR68EFlVfkHOt0mDqsaM9rKsXAiO+pq8X8oFL+9Hwg9t9b75CRzjovhuut3Y7zbg37bhn3pb8Z8fj3gAoL3UZ4xfBFXf6b/6xnpO2lgf5Rd55OtS7lMG+yeLb3Hc8r95PitRp7ajLNqpfGpnuU0q/dU6tmEZ+4y8+lvyUy7b0mbykbeUzzhOh38SZTVNOsFkm7qqMBXwX1fpFeNcFLYhd9vKUcSjTXcqZ0xTvmsc6roOC8WK/3z8py1GnnShbfSjCjcklPaSR+V0A85odxXK1EcXeG3AugmL5rSNbc/43iLcOY6hF3+tBR67u8OnTjR47D8ZTDQehw4Apln8ddbhoAcZ/PMfAiOdTrz5gn6SnHPo1P679fTXGH+RhXmwZfMW7LVyJRYtSheWYp/67gr/hZyPZYl0AXf9hvW45mfXYKclS3DQQQfF7/2uW78OH/ybD+Kyy/33gk8//TRcuPpC7Lnnnj0ysgXhcIwsF4iv/vHV+OlPfxZfOz02NoZDDjkYzzz1mdhtt92CnQ5r167F177+dfzoR1dj69YtGBtbjCMf+1g89alP8Xww+NKXvoRvf+c72Lp1Kx57xBFYtWoVLr7kkj4LwPunWMA/dfyf//ldXPXd/8Tdd9+NsbFFOPLII/GMZzwDi8cWhwXgZ+Kkk04W67kwnJeX+DHZIiOJfcHca6/LyUfPeRBm/WlMuFHFeC4u+JZ90VYeNiQ1BuG/99hb8pBYr2WhAlyAiTIYJOrQMm4HftVf2hSYQ5nfI/4YZy0vTSvLr7zqGnzvxze09N/01DQNfvbz67Fx8/AXZ5ROeNwTy6Kh6JCH7YNnnfI4fyNRxH+YJwP+/1AGGGzdvBm/v+MOjC1a5I8rfcZ/9ldVVbA8vwqx5/zpeav/FFu2hAVg+bPhsw/Ll++JPfbYI6uLx8k4V/N+UK9zDic96Xg8/aSTY5ssB6zNcimzWTq4bYxlbZlHw43/FpWbxOiGmzB221dR33MX3DoDs2Ub6vEG2NzFxEaLtWsddnr0fhjb40FothqgW8N1a6Cp4BrjF4D9qhacMxhbuAjrDz0AE489JEtQ9kv/+f+U74uWebMbMP93APaavAR8BbS1Fpu3dvGj2xbjA5vOwfemjkTjKoB3eNvwVJ8NC7lh27/uNG07azGKSTx1p2/j1Q+5Ag/ffTNGawuAF6Qs1i7/RrTfWv8kSndqCiY8IVLay3mTE58YD/Yhy9hm7bjFed9q8KO7/Xmq4SIwDEwzhdGffxNVZ0wWgMPiNSzedPrD8cSHPQjLxjpwxbUM6qLezeNTqCqDsQX+yQvaxVzK5v9y/m9bzv/T+O9lt8//gSNe99WeBVrdt+MbcPdzXhVkJdrzk2/Cmj97d1mMlW+5AJ3RMVlQDr+y/62PvDw7NjAvXcBmNfT83//2m///39MeDmuA0Z0cjngycMDhBo0FphqHn/x4K356tYOrxmDrCgt2sjjjbIPRhf4mxa5z+N5Pt+CqnwCHH7oQf/YigwP3Nbjs/23GxokF2G23Bbjsyk24Zd0YXKf2C8Dh75vPvWlI/HvfGQv6RF/Jp7Ehz+GfOSrKGnWjePQej8YGuwH777E/3nTym7DfrvvF+mHJweHTV38ab73yrXjCiifg+7d8H2uaNdnNX1wA5s2sM5//947/Goe6rrHNTuKDv/wHfPXOH8Lxhg8Df3wzYeEGBisW744/ecQf4qSHHotlCx+EUbMIFg0mms1Ys+X3+Oav/wtTt38SL9rlJiyqGjSNQd1x/j6UcFicckuxbtlfYGLhMTDhOkOZa5qXtJX2smxqagp7LOccNor3PvIY7Bwe+YEzsWV83MfUIi4AO+cXeeHCd39l3zkHTFksvKtBZ/FCmE6FyeXDL+5/9Tnvxv4rH5LFua2v1txxJ0ZHR2Mdjydso76XchijtnrKJx+Paawjf4qz/ybh9uIf9/Pzf14vnA3+GRvqabPN68t1mnL852fSwnVzM4vxn78sS7pzYnm/tvRF/UUxZpK/kvN/E8d/71d2/S+8YayMG8L5JGNNeVqmdrKcttJeLSv9ob4yhop51cv2lE+7GJdsfJ9m/LdhTku9/cZ/jW2mf6b4L+ur8ODEAPxzzq8PccQYEUMZ/n1+0kYAuOa66/Ci1S/BD7/9najjqOOPAwCsPv/FeO5ZZ2X4v/CSi/HYRz8GzznT30iqPvfbJpV9qXVswzL2GXn1t+SnXLa97HOfg3MWZz37jFjO2Kh8zQ3LczWxTfVRpynwf/Mtt+DFL7sIf/zM03DeC14IM0f457yAdNMtN2N8fDzjS20BYwBrHeq6QjhTxL777Iudly7tuf5HW+gLdP4/i/W/3/7ud3jw3nvHmFVVhcce+3h89AMfxKMOPSzGnjEzxuC555+LJx9/Ap571tk98eb+7XfcgdNW/Qk+f/nnsHKF/6zF17/5Dfz1u9+Jr3/l3+Ccw6XveTeMAV718otj+7Kf2MeK71t/9zvs8+AHw1r/kEWn08FRxz3R23zYYfiPr38NH/74x/HPl/unyOu6xtve+Q5s2rQJb3rdX8QbPpbtskvUe9ElF+Oxj3kMnnPmWQCAv7vsM/jxz36K97/jXdPjf07H/8o/AawdBQmMKmbD1LG+XA/q5CMPtynbufyJKVfIRUgwUmkPnfB2pYvL8Qgs7QxXzgsAN3ElPV/sytrKdxLjpRiTXgGqdlQc5MR3EvVFgBgT5po+UeIBk/rCQovGDASd6MwGnzAI0E+6lOKUYseLdrSfMqjDhVd6sI3aEmUE0vhTlhJ1xN9wYd1wwU0O2oxBdyp996LihKH2BxjaQgvIxz6gHJZ7W8O+Dip9nsqlTpax313RV1FO5AsxDNslLycEtI2LIKXd5LFcZJR9jVWb/uxJPz4JIkR/6adzLurwfucDKG21YfLgy5J+xehg/Kf8ol7KRoiwMf5JLM+X+oBtKJM+VEUfRF/FZeqpqip70rgOd1N7n/PBThrHOufBCgQbtJx2qL30nZTjP12IdVwoKk6YooyW1/XSJ80H9o/GPJOT4T8NBJRFGdTBfbZJ/sgxJBDbqywllms9t1vxLzdGOMV/mGAkWzyRT/2mzfSRfCgmleoL5VKntsEM8M/tnDedPNA2HQ/KfuXvzPGf+iXhnz6kfqCfrgf/sxn/PQ3Gf+oz6qVsksrFDMb/Z39vEdZsTccOO83ir3MOD98Z+Mc/AI765woT3XC5bYjFXwfg4GUGXzo1vQJL/SSpvyjwzzuRJyYmMDq6AMtXrAjHFl34Dd0Wu1MLWSJ4K9sUcrpTXbzyla/Ef3z1qwCAZz/72Xj9X/xFYPDUttCoi8F6XM0opVcfUoOS/Qix1RxAzAN/rGGbyMfFUsnzZFuhp6/NvXYkSnOTNmLuAfB9Zgq/XJqDJl6/KGoMF3OLReFSDmUEO9gPZax8+6ArbGhcTBUmoy2U8RXHQNYbX8AGaTtQmz1ZG+Ghd74M0de2MJe2+DL/W/KrWc4B99y7Cf/wpe9lr9CcCU11u/jqVd/E3ff4b1nPhExV4bmnn1EWD03HHnMwDjtk35SZJjnO2DGSd91+ByYntmFs4SKgGKt5LGJ/sMzDR/IoHL+e95ILsCksALPMOZ+pTdOk14GGvmn/8/b5vgtyn30Gzj07P1nP8msW439d+Td/cF4Eyd/M72nG/8p1seSGL2D0zuvQ2bAV2NIFNjdwW7rYuM5i/WQHez75ANRmFHayCgvA/glgNMY/BewMYIFO1UG3HsGWp/8BppbsFN/8VM4Vesd/f9GktJs8dprxf89tL/OZ4Rymug3W3DOB82/7M/xo4rC02Gutf+NNn8XexJPKuFi8ao9/xzsf+SksXgD/FDC8rHV7fzeLdwB9fPqVcabNLOMCKfuEcSBpPwLA5TcBr/9BF5Pw36804Bv9DUZu/C46jYOpRvwBwKVF1No5PGLvMTxqn11w0iN3x+H7+Nfc0RZrLX537zi++IPf4vrfrsOBey3BJc94RLSDxNzTHEKwU8vpWxr/db7sScf/x7z2X9MCLWShNuzb8Q34/XNfHduSln/i9bjz1e8ri7H3X56HesFYz6JvWlx2+MZHXxHjTZvVfgw9/8/HC+4jxOt1pz4ctgLQsRjdZQJmwSQaA1hjsGlzhcYtAmq/eIuRBkt33YZJ14ULD9Vv2NrBJBais8hg2bIJLBzr4u5NBmakQme0i7VbK0xUY7CdCi4s/jY1cOUL/ALwsPjntvpCH9nv2gbFAjAcMDo5CmstXvtHr8W5jzsXSxYM/vZvP7rx7htx9qfPxu23347xheNwdYotwgKwMf5zafF8b0bz/0T0l366MP9vmgZX3/tzvOeGz2LtxDoZcYA4GQlzk7qqsXyn3bHPkhVYunAxbNdh7dZ1uHnjrVhs1+NdK3+NQxduQV37bz9XtR8fjPFP/06MnYh7ll4MVy/L4qu2YYj5/9TUFHZfvmccL3NPAzmH7/3uv7FufCP8IGX83NIYXHfDf+PD//S3vp3GyQGoDCpTYXR0FPXYKBDe/jQs/eurPoKHrnhw3KfNmm8AcOftd2DRokX9z//lmIlpzv8ZG8WBytHY8ZfbCG8TMtuJf24rqb6Sd6bjf7Wd5/9uO/DvZnT+38tbd+r4ZjNj/OIan6Ar+5W/g8b/Nv3aLzPBf+m3xsQYE96eUQFw4cEdP1dQjLae/zdh/A9PPFO29hFJbcMQ+NdYKY8S+erK3wBZ1X6Bmn1Dn/u1ZZ3Wm5bxn31Ib1hG0vGfNrN9rJsp/hv/sBiQHnrh3LiqKz+3Q3jaPNRXxWckuQ0Z/+PN+tb6c4YC/9dcfx3OW+2fAEaw86jjj8OzTj0VX/3GN/Dpj34MK1esAOmiSy7BY494TPYEMPXuaPxjTvGfYtcmuwf/PfP/ub/+p4vAs8W/acFbqSvF29uDfviX+b+dBv9HHe8XUw97xCOBFvyffuYZOGfVmXjWqc/siRV5vvaNK/Ghj38Mn7/8s7Hs5l/dgrNf+Hx85hOfwsMPfBhOPOUP8O63XYpDH/GI6HMZJ7ZlncbVyNuFjz7+WHz0A3+DQx/xSLzjPf7mzFe94uJo2xe+/GV88GMfwTf+7d/98afA/0WvvARHHXFEvPHgM5+9Aj/6yY/xvkvf2RMzlPif0/EfqLQzlEGThfvkIdmQrNpp5LPyAW4Q6LL4y8VU8tfFR5xjm54kAozxC6K93eftIwja7pr02ylh2cYYP1GowqtAEQLPRHa8MJIlhb9QxyeXNDHVbmttxsN4GeMvWNJW8rOOfFxkrcK7v/nYt2dMdyHncUodPtXtRv0k9g3lMlbaD+pTaRsXtPiHEC/KVRsQ+pt6647/xqfaSz2mCt+1NHL3a8ilcrFZY+nJwIU1O+Pfvxr9og+Mica3rmuMjIzEcmP8iZf1gtBtGt8/zDnDb4nyqes0oDBH1Hftx6ryd8WXF0w7/Iaq3G3DOvY3babc1J9+ckn/+Z1n54But/HffG78gdt/g8TzpnZBSgv+6Xdjw+J7wIILd78Pxn/KOY0tmCtBLox/hYm/KQPBtnb8l/GO5N2BEfy70F8pb1Lf0w4Ev7mvA2gVvgnLOsV/jEVxjCSv2q2Y0JzVfmQdiX3Neu6X+Gc/YAD+u/KdGxJtolzWDY//NLjQj4H4D7+2GMBQ4r/4rhX51F6SxpKkeuk/CpvVb/TBv8pRTFMWcUge1uX49/K1H8u+Z/n24T/PpUZeCdztdmGt7ZlMl+24TdvLfmRfKb+dFv/F+F/kisodfvxnjPjkrxtq8ddZh51GQns3s8VfOMDBx1Xt03jRF/qndtswdvnjf40tWzZjanIKPM6liUyS7SnFGkGmMeHVxUrc1WLnvy156aWX4qSTTgIA/OQnP5HqkMvhH8mYsIjqmVIsVHiYs+g+Ym708SGqUAwnXi8vCtKfzI48JNJGi1qpz5gBr8jncJsO6s7rjElL5hC3nXNhu2Wh1jdkoVB4QkBlaG2Rc7pY7wsFlzGnfZ3+Kv7ayISxnZMo3SY4tDVllnMZ/rrMducjEVn9XCV2azzush4+LpJriTdtb9q8Fd/63vVYuLDG2KKRWf0t3WkhHveYR+HJT3jCNH+P7/k9+bjjeuTN5O/an/8ad9+zwd8gmSWv4tJhYtsEtm3dioULFmJK5//FMReMvYxLOv5Tgz9WhgVBmec5G55oCP3KfDNhgavcJ8W+LI6J5OGvncX431ibvRmFZGc4/jeo0Yw9GLY7AkxYYJsFpiymJh22bLEY2XMRRpc5YHQKVfj2r1k4BbNw0v8umoRZNAWzaAqdXYCph61Es9NYPJdFz/jvbd2e8d+G87fUxvonW+DH16mpBjdN7gPXNHCN9b+MV9eXWZY3ob8jTyM8DVzT4KbNe6Hbbfy3f53/HjCcn0+UdlvbzPn4/8cHGBy+ezgP4DHEAoCD3X0/oJkMx5LsQIEGwLW/24LLv3c7zvvUNXjq2/4TJ//1d/D8D/0Iz3j7t/HUv/wGVr37Kvztt2/BD266B5vGE4bUrp75v8yXyvk/84t/g8Z/vzAr3/0NcY37psIen3oz9vzkm7DnJ9+I5Z94PZZ/4vUwzmLFW1+ClW+5ACvf8mLs/ebzsPdfvsjbZdO3hP13f/X7wumG03mf/1v/HWB0K2xdO4qNdyzGpjsXY9NdYzATY+jYGpUF6gbAVIV71izAhrsXY/3axdiwdjHQXYRR1LATFdbctQC3/GYMGzeNYd2GhVhzzxi63UWobZV/B7iZOf5ps/qNaeb/GRlgojOByW2T2LxpM7rhrVizoa0TW9Fd18XmajNcVeghhbFvqtuN+ab5qPZp2bDzf2MMjnjQwfjjfZ6M2nWyod45m34BdG2D2zbeif+6/cf491u+g6/eehV+/PvrsXFiE45bvA6HLNocnrhrUNcNgPAaeVi4zhJsGnsWXL1L1N0P/+oT+4M8sW970J/IwF9retyDH4FTHv54/OFBT8ApBz0epxz8RPzRwU/EY/c6GJ1JYGQSGJky6a9rMNKtMFJ1YEY6QLj2NCMq8oW+aC65ljGA9SXGyMc4VC3n/5jh+K9teFP4duNf+pR5pzawDfXOdPy323H+b7cT/2a7zv9DXGQBh4sn6ocbMP67HXz+7697WjSWfoT5YXjls8717X14/q98SiZe/wu6wzHUmHStXe1gG+4PO/6zHW2iL+RVuxkH8jBe5NU6lU0+2lyFb/92pwr8hxsj9cERFxYqnXOY6k5FHbHNwPE/XT+NmCk+T0dbT37qU/HIgw/GBz/20Rz/8OfBGg/q3ZH4p1+0mWUa33nH/3bM/90Oxj9t15zlfslvtxP/P7v2GgDA7rvu1oP/DRs34NOXX4alS5bghOOOjzIoR31fc9ddeHD4vJkJ+XPAfvsDALZu3Yrbbr89Pol7+pln4JgTjsNzzz8XN91yc2xDuxT/dQv+afNuu+4GYwxuu+MOLF++PMbIGIP9HvoQbNq0KYsFbV+3fj1+fsMvsHzPPVOfAfj+D3+Io44/Fk8+5Wn40Mc/ho2bNrbjf07Hfwdz+89/7rg4x4sBNMxU4Qm6EBQKbLr+Gxm28Z1MQ7ltigmDlxUAKE71I02SbrgrxIRv8U6FV7IyoV24oMjg08ZSuiaXc2myAgCm9q+i5ZO4rHPOodMZyb6HS3IufOOyCLjWqy3c1tcwILw22oaDIkNCX7x/SZ7aZoxBeh6WB5neOJgwCdJ9EvWaKrziQ+pAH4uDV8O7W1zqb8Y2+iXtjfEXFbmYSz+0nu0ov3wiNeaXTES4uKI2UzZ1aj9SP9tQl5a5QX0lfN1uF52O/+aX6tQYq2zGqPzGXIxfS9+Q8rjkcVbbTMAAD2AqT7FY1itf2Y71Sa/naZoGIyMjsOEgH/vH+leJ0BZPuX2aT21kZNJQVT7WjG0VjgfEv74Wtsz78gAQfQhPqjA3WKfx5RPaTu6U9pOZJI8ywk4WN9aX/VO+hpl8TvoNSHf2RfnSN7RbZSD4YOTYwfr8N01QofgP+ap1iD7qyUvCv5PJbJmX2p4y+Us/tJ7ttB9Yj2ICxT4r5bJedTJWWsY21KVl1MdttU35ZoZ/71epD8V4WdpIKuNCPv1FD/7z2MeTt+3Gv98fhH/6k/DviWVl37YR9VfZ+J/j/w++MYqNE/A3mRSLvy7cfGJl8dda57/j+0c1jvonYHyK/gIYYvH3oGUGXz7V9zn51BeNG8vK/mFZd2oKdd3BXivCN3lb2wLFKmF6KrR4TbDnDH2oT/AG6na7+OrXvoaDDzoID33oQ2M5507hzDhrE4miHPwB0KUFz2h32J/2yhzKejYKZBDsyO3P25YKlJd1oSza0ytT+2YQ0eVsP3z7GzQ3yM/CUDTycgp90Sxt6Sm5nD8J3C8HlAdBv25HuUV9Xz7PHPo7j51z4VMMLXraZAHJ/1Qv1QUldSY+Fe7L/L7a/atb78Rr//rjs/r27/2BRjodvGb1mTji8Id5nxib8OQu6fZbb4VrGixYsMAfR4v81WOwMelVz8YYv6gr+wbA2ee/CJv5CujQX21/cIDlxbSAeZuN4Ty59XUvPPNMvPAs/2or6kORd6ltsEfGmbbxn08nuHDDoBF5/FXZLKtaxv+Re3+HJd/7DEbX3AFstbDjDTZtclh7t8WuJ+2BXfZfimaLgePTv90KzlbwjzRWcNZgpNPBZNXB1mNPx9SSZT1+mD7zf1+W+mwm4z+ftF0+vtrLcA4Tkw1+t2YcJ//2I1jf7OQv0t14HXD7b0oxA2lyt70xuWw5YB0eu9P1+MJRb8KSMYfa+MVmB4d1D/ZPJDqO/6P+SUh9CrZt/Ke3LCv7Vkl5T/7iJH6+ofK4D8dP4ywW3PAd1GYUqGvA+TLGwwPH3+DlF6O4z20AzuLwB++CD55/NHaS7wbr/ErzJs7/NYelXxDzrjcXGS8AOOo1X45P+5ZP/w7cdw756529v/qkr2/H/fALi69//NVZbpU5xvki87XMv9JHxomy2J+v/8OHw9WAq8L3eauwzdc1634F/xSv1DfyWufsr5PakI9tmxr49xff2BNz9bEN/wj9mPCYythXGqvsCeBAruuw69SuWP2U1Xj+cc/HLmMz+wb81b+5Gm/+pzfjv37/X5ganSqnJgCAn539QyCMmYr/si/VZvZnGQedi5f1zjk0rsHf3vwVfP7Wb2ISUwFPfgzyoAxvYWn8N51NuFfNADhgZAKf2O9G7DkyhaYx8du/zgbd9RJs3OUV2LLoabAuX9ToR9p/5fx/69at2GvvlWlMo5kegMnkgujrN37yn/jTD/nvBeYM/jiDqoLpVDB1S6dMQ//6yg/joSv3KYt76Pdr7sLIiH+Nvcuu/3nL4xg+w/N/bVvmiP6SrLXo1Ok1+FqHGeC/zEttT5n8pR9az3aUX+aI7jOXS7msV51V5d8AWfptZoD/0icz7fm/j382/vO7rTvs/H9m+I98zmXXiFhf6m2aBqP38fl/GY8y7z2FtxM53wdcxKRPtLGML+tcn/FfZYSdLI6sV1s01pmNM8G/9U/5tr3yWftAdRjjz+H8E9y5jdRrjH+yONXlcQKAn157TXwCmLKPftLx+Oj7P4A9dt8dzzzj2XjP29+Oxx99DADgoldekr0CmrLdDsY/+1H5GNvZ4d/nYH/8++0M//N8/c/NAf5NS/xYX+ptmgYjI37+r5hWf1QnZSmv/y7yRXjumWfjnFU+RwCEb+S+BACw98q98YrVF+EJj3sczAD8//1nL8ePfpyeoHWhv45+0rH46Pv/BgBw3oUvwTFHHY0/e/nF2feH//myK7Bsl2Wt+LfOxU++Af413he87CI896yzcfYZq1BVVXyd89nypPs1112L81a/BD/49lXgeYcxBus3bMBLX3kJdtl5Z7w3fAfaFfi/5rpr8a73vx+HHHQQXn3xJSEqqW9om/qJafBf/pKstajik7hN47+TG/54FYaLvxDAVnzMPTzRS+NMSPy2znfOf4dXjaChrKcTkMB4Xj/R47cTI2/wxYXH9GPbuJVspo2q3zoHhIXpqs4Dy2TlwqiVVXzAL2i6EESVzbbUnS++pk6KF+6MCQeTdNCKnVnIZZJUtX9dM9tTJmNJm0yYANEWJzG2fNUAL6oIaNme2024q2Wq2w254WXQHvY5bWB7G0AE4++e0AMgedU2xpz1pMZadIMNfIqVA5e2p//MXcqoO/41DCTqguSgtzMsukuOaBw0hryros0GtqEvjk+6hrxhXawvAMz25FPbS/sgB1fTcvcQy6tw90gZB9pLvhjDQNSn/JWcCLA967pNE331ZOLko7Rd9cV649+y523K/eRkMPKGclfgHwhwkovOtJH9zHZGBibGgJhQP32/pHygXTbkOOV7u3PMUX+Gf5HDyQSYF+HVUyqTPrriOKl2+Atl/tV05Ctt0TzjXWfR7x78+zLivxu++UCdw+Cffm4P/tWGKuBmEP6zmAQ7VR51QXKQ7cscpf30hTbMFP+qj3Xaj+o327NcbS/tw/0M/4PG/9J21cd6ktpEUvz3X/z1xw1bLP5a67BTJ9gZcOzd4m/q63LxFw7gSR55aJfmBf/oP/dpM9vUnQ62bNmCbePjXpY+baBPcwqlxVpkC0O68Ouv06X8g/HlnU4Hf/i0p+EhD31IOvYhHI+Cb1GG/IadFBfn39ZA8nanC+9wXqffSO3CTtST6tTP0D6W5TaktsZ7bfyvMMS6rB0ACCZjVbEfqQh9YqNPQV54w0ZiDydiannsx5RjbGF8Z0WKfRpimTzqXeh3xSJ/7HNdZA59r/nKPCRpbmp+GuPntmEn8ivZQk7KkbRNMnEd2WgK+EWdOF1zmSrPx4iyzKb4EX/OYnzbOLZObH3A/lnI8dJoXvgs2Lp5MybGx7Fw4UK4Yu6jxyH2sQ1zkjh2hLzQti7MhbitTwP7fR5bU5llm/jHG21SGW1xczj+c/5vw815HMvK9vRfY4Ji/O/uvBdcM4Zm0sGON9i61WHDOge7tIMlD+/A1eFpXz79u4i/XZhFUxhZ3EW11GL8oEejO7ak1Qb6PFfjfzafduEJYNcEPPind203/O2+AvZhh6M54DA0+z8S3f0ege5DD8HUvgdjat+DMPngh2Ni74dhYuWB2LbXAdi2fH9MjS2F6zbxKWBnu16+bcJTwP6Oc/pXVRUauTCrvs92/Ge+kt53/AgOWBKOF8754QMVplYcBGun/Htm5bg4HDkce9AeeO8Lj8TSRemJD+Ydc1JzkfOcJmCKxz3NMfrPP/qvcYlP6mZP6YZ9W+6HJ3jJZ9ku8fjFYJY1QJDBcszJ/D+fe/eb/1cOMLb3r7LhaV3uczv88knevtvFE7/Zvk19kMV5GvyTX/HIPjct8/82Mh2De0fvxaVfvRRnvv9MXPGjK7BlYkvJlpF1FjfcdQNe90+vw7kfPRffvfu7fRd/lUr8t9nHvjOznP/Xpsaz9nkynrjno+AcYJtwTO/C/wU5jbFAeOMdnMPOZgoX7/Vb7NGZAFyDqurCZE/+LsKGnS/C1rGT4ZAvFNJujb/iX20ncf6Pwn+H9Ia5kpjH/DV1hWpspPdv0QiqhR1Uo/WsFn+VqKvcJim+TNv5v4wb+jfd+T9jSfnT4X+k44+BbEtetc8Ogf/74/m/kzejteU99yN/H/xrHKinGnT+X8n4L9dxVB9mOP6r7aV9mAP8O+fC657z4yfux+f/JW/P9T8AgD9PY5+onRB/mHfUR93qp/Y/ZjH+q17tYzM0/i3qTgfODsB/WI+hfK5pqCzNs5mM/5xqVYJ/yl2+5554yXnn49L3vAcbN230chzSU9j3Af5VRlvec5/8bF/mqMZBY9gX//Mw/1fbS/swR/gnn8YP84T/r33jyriQ+pwzz8rqDz/0MPzw29/FD751FS6+6KV4/Vv/El/7xpUAgE/9/adxzAnH4cjjnoBjTjgOn77iMq/AIX6qsiTn0vX+Z5/+LKzYay8YY/z3dx3ww6uvhrUWx5xwHI46/ok4+knH4sjjngAbHmbj+t9/fP3ruOBlF+E5Z56Fc1adGWNE3/XPyo0mNsTlxptvwgtefD72XrkSb/zz18WYmgL/jz78UTj/BS/E57/8pR65cz3+dzodVDFBioXeqryTt8XRphsWgcMFTB6AyuCUi6U03IZJA+TAwrbRSZNf7FD91MFy+Fzw/oRko5y07eU3YdGX7VQ+qF9eJ0t5zvkLbbwQEnlFRlWlV1Szc+OrPyp/Ac86F5OLBzeEA2Vd1/G1ISqbsYyLicFeHgy5zfbqW1XchUIbIa9ipo96cDUmPOkRfHDZBeHES/k2HMRNyCnKII/aQhncNpK8dXglAOOsfUrbSv98fJIOhHg34e4Obc/f8qRe7fEXuLw99EFj5XnytvxTX2klv90AE/KANoQ76X1/+CuiTShj/Ou6jgt7qssEXsZKfWBb2k6iD9zW2GIm+JdBAKKHerXvEBYTqYOy++HfhJsc+r2imnLUZ+WjP1UdvtHNbcW/+Kzy0Yb/2r9tgPVqg/ZxGcuEf+Z4Oo4wfry4CcE/c4XtIMc6xoz2tuG/rut4DHJ98B9j2Ir/hEkS6zUGg/BfzwH+qU/jSptoB2WqLJU5CP/qD/fVtu3HfzoxYTyUnzLb9BCbbKs81EPe0jf2AXVxGzsI/9qG+7SfvPQRLfjX/iPRN+ccFtf+17py8df2LP5yMWPDRNAdF+T4m/qxbfGXGKJu8nObtmIo/HsfRkdH8bvbbkN3agrZqhjjRb+T+/EkjAuCcTHQGL8g6AAwhibsk/hEIeMPEwWqPBQxV9JFRyA0NyYYGRaunOeEyjH8L+0nHdkqanLScCGM0ZeFscgvDpbxUpkxpsjblET72+yJhWJfJs03ZkSTPUlYFlfqgu+TeKQ2qQwuxYZ542t9v7vi6WDazvJ+/Uk53DYcsyW32aYt39vaQvSU+ki+ffBBFiX9vvGeFWHLRfmgMTQAYG3jF1K3PUD/Jrai2/iLCWiJ6dTUFO664464+GtmMP6n/vJz8UrG/8mp8Fo46xd+OQ/OFn7DfIdl7K/0WkAt83+TU1PxWD7X47++8YVtSeRVHZSp47+taowffCysW4xqooPJzTW6EzX2PXEX1Ms7MDs7VLs41MscOsuAzi7AyDKHkV0cRnYzqJY5bF7xcEzufTBc7S+gUY/GobQDsxj/Of8HgE68eMMFYAvIa5pjPy5cDLtsdzTLdkezy25odt4N3aW7oVn6IHSXhL/Fu8S/qbGlaCr/Ni/XlUVflxaB/WJzb183TVoEpk+6r32HGY7/D1tW4W+fUmGPBdZj3Tk4BzRL9kB3p13guhOAtfF4Mgwdvu8yvOnZh2HZYv/0EnOGxD6B2MN5tOYiiuOhzvFMn/H/SYcsTwu0ssgbF2wtF27ltdDZgq5fCGY9F47jPheKnY/nEx798Mw35v/w8//eY3lbDOq6jou9cdGX+02+8JstCMtib10s8sa/brGvsprZ4d/JHJm/lMP9qvLnczwna6UaGB8bx/fv+T5e9smX4Ql//gS85V/egi9f+2Vcd8d12LBtA9ZtXYerf3s1Lv/h5bjgkxfg6W95Oj581Ydxq7sVzWhTzDNyIjYY//me/++yYAleeOCpePLyozFq/FzJhgXfOA92zh92nIPpAk/b+V4csXBjWPD1T51b69BYB4ulWL/kQmxZeDJgRqMujfUg/Gv/kaLfinrHp/wEx8XxNZZz28idZz1/kX3WRN1o8SP6IOdPbdf/OFawPWRuwJhR1vTjfzv+md/bjf95PP+P1+dCe17vAa8vhVxgXRWwqzJng3/appjT2CuPtnXO44XXmvw10IRhktpAHJR6iE22VR7qIm/pG/uAuriNPvivqzrcUJb6RP2NvoU/ex+f/1OO+qx8Ph7+7aUIC8FckEewhTHTdtynPcQReVWv8qoMldvv/N/NFv/yXWXKqjsB/9ah7nR8+7BYTKpa8E+d2gfOOdThrQDUoaR+Q+L0zKc/HcYYfPEr/+JtNummHLMd+Kc+jSttKu1QWSpzh+O/xQ7cj/Fffoda25NXfePfbPD/+S9/CX/9rnfgnX/11zj72auyeGrbqqrwhGMeh+eedTYu+5z/tu9zzjwL3//md/CDb12FH3zrKjxn1VneZgOs37ABJGMMbvnVrwAAe+y+BxYvGgMAHPpI/51hBFseccghWHPXXQAQF51/8K2r8MNvfzfa06lrfP5LX8Q73vtuXPqWv8LZZ6wCChxs3bo1yjXG4De3/iZ+D3uk08HPrrsWf/qyl+LsVavw1je8EUuXLMniV+J/yZIlAICbbrk5yx/GkjEzxP8sx3/n+9lvMNnUsTIp1QjIglZV+Q++u3AwgvF3P5mQWPoKZTrApCUxEADQbRr/xKde3Ap64oFRDuYxecIEpM2fGDhj/MISF60ladVPXnmiTfSl7qQTQtXBdtymnWoPwpOwJHYS9YYO8U9RSlKQrPP2s8/I78JBG7zrrUgS+s4y5/zEqUwG8iO+SrrylxJNFb8LwPb0V2NQxoOLb1kMpA24sBmA4G0JdxUGP9jnGt+maTAVLjSpTE4O6a8u8NMuynCyCMh66lBdJtjA9txmO/VF5VCX3r1LW8GBPnxvuqrTU58pDuEATCxyUAllLpQxT5kpDuHV7aKb/I31r2CvRzqen5gJ8abdtJ39lmKT57pOUti2LDMZ/isY4/vMDsB/I3eLWT6pVuJf20qfaK6pP5w4edyHPpL+0j/ag3As4n4VvsHBPCjz3U2H/4i5FD+NL/uY/rMfSNRXteLf62M/6k0i3G+sf2k884G+UQb5E/5TLJRHc0BjUMZDMaIxUNm9+M/HI/Y5690A/GexLCb4tIsy2IY2sh23yUcb2J7b6hv5VY7qIOl2Eyb6lKl2oMAUgi1tZarbU24b+bhfVVU8KaEfGm83EP/F+D8E/iuZdFCOnQH+VV8l+N84KYu7Li3+unihKtXzKbUlIym+XEiiDmDA4m84kaJ+9oXGrIzPYPwDnZEOFi4cxe2334YmfLsnHL29Pc6F/UQO8pSvLACGA1lgCouGzHte0aJPQvS7Z2GXugIZr1Qr076K1G1d5GVQyZDxcVGaAg2NDXaFC3ORfGys5dhHmV5+tFVFStOeAuGJC6aZc+VFwcATWXJFlJDb1bMpOeP9SDrDrxE/WMMca4ujEGXFvA6MjjcLBDncJuYTNjyxPXn7lXFbZehvamMAmIjRfvpoj99OsTaSUyyzzmLrtnFs2bb1Afm3dXw8Pn3h/Ur90W0arLntdoyOjKAOFwCMHrNbxn/y8HjDPrY23ZntnMMdd9yJe9beg7X33It77r0X9967DuvWrcO96+7FvevWYf369Vi/Lvxt2ID1GzZgw4YN2LhxAzZs2IiNGzdi06ZNPX933nVX7Fsdh9wcjf82xIULzSqTeuk/ZTEO3N62/6Ow7snn4Pf7Ho51e+yD0VP2hztsX0xu2wMTZg9Mju6OidEHYWJkZ0wsXOb/dlqG8SUrsf6hT8HWhz4BZoG/qKC+UI/qon3l9jDjv77mO84N3S5+bggu/Ibv+HYbuG7Xf+e328A1YZtP9bKcPFrO7bCQjLAA6VzXfw+w3ifaxRgDiOec1XaO/y7U6fjvbIN9lxpc/ewRnLIvsNOoCUewClN7H4bJJbuicV3Adr29fQ6GBha77bQAf3TEcnzgBY/FrksWRDsgNukfy9E2/5/l+H/uUw6WJ39lIThbwJXtQU8Dy5O/+vSwxuC5pz4x2q0xp40YeP6f5zV9J4/6a631n+3p9wSwPP3bsyBc7pd1YXE4ygoLwvEp4CHxz/zitp4PV+Fcua3vnXPYdeGu6EsGcAscJnedxK3mVrzzP96J57/v+XjSa56EA849AAeedyBO/ouTceHHL8Q/XvePWLt4LbpLukB64KOVdl2wa7x+xvN/5hz9YBltVSKuyv5mTNrm/8457LFoN7z8kDNx4SFn45Cd98PCqgNrHFzjgK6D6Ya3kThgz4XbcPLOazFWBfxZ6z8LZpZh69hTce+e78GWsdNg6kXT4p91M5n/q9/G+Dmi9nFbbJxzGK1H0DHTdMAsaFG9AJVcU4zHNukrFGMAjyWMC/uY/rMNiZjUPuP29ON/G/79mx22G//Bdt3WGBCb1K+yZzL+s1/bxn8+HME8YH6pX2o/7aCNjBO3yUcb2J7b6hv5fVt/jSvp8HlMXtIw439pc1uZ6iapbWjxtw3/nIO6B8j5v7ZVXZprvh+sf611FV6dLBjlb/mn9Wo79bMv2PdqI7fL8T/maZCH2eC/acK1+AL/YeE38lT+lc6I/qVrrsjwP/z4z222L/1dumQJ/uLVr8EHPvJh3Hb77TBIT2WWMVDZM8E/9TX/e/0vlqluktqGFn8V/7ypln64ecT/tddfhw9+7CP44Hveh8Me8choJwbgX6f1VR/8P/7ox+EXv7wBd65ZE23+1W9+jZUrVmLFXnvhgP33x5IlS3Dd9ddH240x+O9f/Bz777df9E/95O+Pf/ZTfPBjH8GH3vN+PPrww3vwf8Jxx+GrV16ZxeemW27BMUcdDQBYt34dLn7Nq/Gql78Cpz/j1KHwz+8V8zvGJMUE+4nberwxQ4//Dcydv/yl0yTmtiriO881SUjcj+2dg2384psGRXm0Tam3G4Bh5fWvdKCu63gRi853u12gRR7bkA9hkqB3pZTBt9YvOmo9FyRNSFAjr/WgrtJ/lRc7WcEbdKZXqqQDGX2hTNqvT1GXOikTcvHfFYOHynNh8b4rH5P2E5dwN4LcuUQ5/NW40TYewNm+Dk+rcoGTcWB/MFkp18SE9f4wPo28l53tbDiIcYCkv7r47/f9IEw+Hyt/osA73byq3B8tAwAXvhdNXcQCbWJ5jK2U8eQt6pBXppf6k42+DACabhrEEXzSdpzQsD7mkLYp/IIOCI3vI50Y8fsSxhjU4bsZU90uRjL8t8ePstlHWkYek7VJNlE284f7UUfToK478RsljHH2Wphp8N8jkwfU0L6nXg6wleQjgNiW/um2yms7yHNbX6nEviMP6Gd45Qvl98M/t6fHv29fFx+TZ+w4QHU66RtF+qs+MD5t+Fffuc3+6I9/TyprWPxXJf7DJDzHf44H3ddy3aYO/s4E/0le8rOfftazDMXJh/5ym/nKch/DnDfpy/OF/CXWVCZ9mMn476bBf9mm1NsP/5pPxhic+P9qbJxwcPGVddZvxyfY/IUrfUXpUXsaXHbKCB55uW9H24DpF3+PXm7w90/zd6WynfpXbjMO0+F/it8D3mtFjgs+3amLmr4iqy+3S76+JMcCoHfRMI41pRwTyrJfbmgswpyEQS23SSpLqZCbyQh1TkWp/CCA8U6NZkPS1vh8qCoji7m+3sSHq0PiMAZsSL7C1bSf9ESPqSSqz33I+j3sk0reNtJc1fwF8mNNyRftCnxt7Vnny5D7F2KVpQG7N9Oh/ElHIoPxbeP49e/WhAttvh9I1JvbltsAXWfXfAuFTCvD9lSgbbW4iFEZHyUXxol9VuyJxWOLMn7bNLjzd7ehaRqMLVwY23OcpEzaxfpy/KdWz5OOZ5/+7BW4/B//wT/5GXiYuzGP9CfI69nmvjHYfddd8d43vxn7PPjB2bFPxxm3HeN/h+cV4aZC5/wroTGb8T/8GWPgTDrWwmdRumkivF7MwaEyFbqNRSe8OpN/04//+XG/bf5c2ohi8ZG/I81vULu1MHCYaizGJyyu2nwEJq0fn4HQMSExjfM3UcIBJvzGRaWm8fNaF56iA7Cs3oAn7PZzjHS8v84ZTFYrYMYO6R3/Dc+ncozp+O9CWelfFo9B478BJpoKV/++i3+51eBLN3exxfqbzOut6zBy7+3obFoLNFMwVbiw5RxcVWFxx+D/HL0Spzx6BR6+1xIYORb02NAy/9cbLGhb+/if+ojllKfj/7/96Nf4y8u/G/rBDvjOL/f5Xd+yPn3nl1hU+rMXPh0nPeHQrEztQsv8n3FI8//hz//fdOKBcPzOL78BbPx+/N5vuV18E7jfd4CbCnDhW8ANvzMctj//8htifwzCP6/JqP2k0p+S59Kr34XLf/m5yD8UlV1CcA1Jz3vkOXj5Yy5qxT/J9J3/p3r+ql+QvtTjMj/rZa2FhcPd29bh+vU3479+fw2+f9e12NZMwFkH4wxQO5y67B785cpfY8xYNDCwIw/B+KITMb7giZjoHADUS+ON224a/FOvacO/+FrXNSYmJrDnir3isdvbLvJ4+Atlqtc5h9/fuxb//oNvYcs2fWqHMHKxs5KcVOzj1t6Zu++8K04++ngs3ck/vYPiGAGx6fdr7sKCBQsGnv9rTuq5FPlKv7hdjv8klYcM/+majJkl/ufr/L/7QDr/z14zbLMHZlRHP/2ljZj1+X+q56/agRb8+4cGfDuVSb8Hnf/zWpfKZh9pWemfxkP1Tod/tnPSH23y2MY5izq8oYOLo3DhDYxhjYHbpU7qoOx+4z+PRVrOOKjNpZ3dbhf1TPHfsjCu2/G14/L0r5EHd1wP/j3l1//8Z6MgufKza6/FeReuxg+//Z0o66jjj8PHPvA3OPQRj4g+vfYNr8fmLVvgnMNRRzwW56zyT3nOBv/l/P/+g//tnf/36mc9yzAL/OvDZtpG7UCBf75ZiHUqczD+c/kqm32kZc45/Pmb3ggA+JNnPQs8ZzQwWDw2hv332w/XXH8drrn2Wjzz6U/Hkp2W4Nrrr8PFr321/+bus1cNxP9Fr7wYe69YgRef+yJs3rwFF17ycrz4hS/CU044EVVV4dNXXIYrv/lNvOX1b8TKFSvw9ne/Cz+/4Rf4u49+PMor8W+dw+ve9AY4AH9y+v+BtU28yWvRokV42AEHYsPGDXjWmavwkvPOx2nPOBU/u/YanH/havzz5Z/FXsuX48v/+i/4+yuuwOtf+9p4XmnCtalHHnII7lyzBq994+vx8pesxuGHHoZrrr8OF7/m1XjWM07FBS86L/qp/cOYany5rccnJY0bBP/mjhtucDypRkgiHpQ0oRAOEqx3LUqUkkE1ut0pGEmqbsuHnJEldAKPkj7RycDQRh4UFKw8IHT4IWcBi8rgtp4osCyzRV7bq8F0TPqQoBAgVVX6njJ10LYkI3WeK0DoXHh6UTpQbWzCwdWYNBFTKn00nLCFOBGs2g/R3yK5+OsCoLWetlW1vzhTJmIWZxnsMrlhoFKd2o/qG2PbhAVrlnkf9MAkB2fh40EN0Z8i5nEwTHZQn5Ie7NiuzFzGRfMz4w8x8jcCcKEzj4PeScgDIettMdmmHypbdWlMuc3+UX/YT15AiGnkTTnQRrS7koO0Efx3Iv5THMq8L6kOd/RB8po2sm+qqgJa8F8OpoBfxKXfKOLti/L+0ckuY0E+7QPKpr8qT+0u/dQ+MFyYti6coOY5Q6JeE/JV6yBx0m2+uo92V1Ulr1fMj72qj7/0Q+spL+uHUI8h8c961an9qHyMreJR46mx0nLW9eI/5zVyMowZ4r8kf0I4DP5zLKs8xWJZr21441Tpd3njBGPKbc09+qM6IfaVfdtGtLvqg/9y/Kfs0m4l8gLA395o8NEbKmyb8vnk+i3+uvSU8NF7GVx+yigO+UzCLTD94q9zDuccUuMNj/fH5dJGH/cc//SFsSKfxtwEfE9MTMAB2HvvvTE6uqBnYW8QuXhRO17F6iWKcoBc7fJFzDHD+vDbRmpS5GGjQAZBfmG/2pBG4lSfkbSP9vTK5HExMfah0qewENa6yJ3FIa9ozUunK5m9NrKcJ+HZFcWegPu+MYZzCJEneomteJOAHCe8DvTkT+SNrnl59EnbZ7KE2nj7EXkAE8ZsE8Lk91UWw+Lleb420VGkhJ18bJ/Lg4+9jGltMjxXHu5YWHQPy7SYjalbCiUOag/zKJMSece3bsVdt9+BTl1jZGQkm3do/CEn8WbA+M9zO8fxWS6acQ5UjkuAXxRUfVF2Of7L3EjHOdZjHsb/6j4f/70tOl6WNpLyuPT2pdqcjeUiT8fiweP/9sz/0/huWs7/qauq+FkVzd6caLeZZvzneShlZ3YbxDgDwKQ1WLfN4bM3WXz+Vw1u3+zQdUDlLMzUNnQmN6NuJrFL3cXzjtwdpx28E5YsqDC2cLR9/l/MjWkHSc+52ZY8eWzTPJxl/cb/G2+/B5/6f9fiqut/Iwu8XMj1i7x+33oMFjxc9OWrnpUe/6iH4XnPPA7777NHLCt9ZB7SfvZn1YP/1D72ZfhlrLj91qcclBZ8uQis+1y4lfpyYbhtAdhVobxlAdjWwBdfc8u0+Edf/E9lN7nST+3jpmmwZXIL3v2z9+PK33wDG7obo4z5oF0X7Io/2v9puPAxf4rapLkm5hn/jXxXUvE/1XSxrZnE78fvxXXrbsRVd/0Y/73+Vxgfn8CnDrwJR+6yK+zCh2PbgqMwvuCJcNVSODMKP4an4/cg/Gveqe28SUWpripsm5jAnnstB1r6m+21jj6Sr9vtYuPGjZiYmMj4WT8sqe6qqrBo0SIsXbo0wxr5lFxYAO50/GtWVa/2AeOg/aa/JPa9GTD+T4f/ukqvWy1tUn0aK/Kwnu0ov4yD7jOXS7mxXnRWfcZ/c5+P/54iXmRcL6mMC/n0F5LDJb4x7/hP/aX4V50Q+8q+7fU49Wk1S/xTthJ5ITGljWV8k4/+W9fdpgsDxJtSvAwbP9/gWnJMY4ZBObU95/8u3XynfaA6sl85ZpHXvwI6zeuVnHNxAZy6S/xX2fU/k92gyLKfXXctzlu9Gj/6zlXRj6OfdDw+8r7341GHHRbl3blmDc4591zAAM8962ycc8YqAPkxiH1GW9VmymZZ6se8bxjbHYt/n7NKipfSRpKbZ/w34RzQyZs8S79Vl8a0ntX1v5RP/Yh2V4L/l77qEnz/hz8oWXHMkUfhfe94F35504344le+jK9+40ps2rQJK1esxGlPfwbOWXVmlKX+0A8A2LR5E/7vG9+AH/zoh1iyZAmed9Y5OPuMVXBy/f9DH/8o/vlLX8SmTZvw1BOfjAvOPQ8P3nvvKE/jjTD/f1k/m486Gu+99B0AgBtvvgmvft2f4/Y77sDKFStx8UUvxTFHHQVjDC773GfxgQ9/qGwOAPjBt/zNFH9/xRX44r98GbffcQf2XrESp/7R0/GcM/13hrXf9JfEfDGzHP/N7Tfc4BjUUrDua+KqAA+MBERu17yzMDyV2jTd8Mqo3sRmGqXyMAlUG8QvYwwa6+AvphB8Ni6cWfmgPQHhiqRJ9qU7oqmLbVnPV+qyjIMXJC5tE1Zj/B3SIFhEvrfTRvshi7kEJ/n8t1B7D2T0CUDPHWexrcaabQWceYx7QY+sX1KMWOZj7SdAZXvaoHqSvenAY50LF+Pyg2Ephzq9Xh+rbrcbn66OADCIF/2ck0XvFr9Vj7/DI/WHL0uDNrJ4+309qFu5S4m8xvAb2XnfaWycDMSlXeoX67U9+dgPWocwWMQ8tw06nZG4mEy+tphneVHinxONofCfl0HjEgc2r1/9MSX+4dl4F7/GgX6Uk+BKZNBPxjDaJ/5XorvUwV+n+Jf+074lUR5afFM7Wa52kd9ZF31mO6VouwyOyqt6fX1qr/mGYK+VOwdJpe1apj5wn0QbVI/aa0POq53qQymHPNRD/Fcl/os2zD/WteEMxeRHyygD0+Df9cO/MeC4R9LYuDnBP/sxz5Ne/KcnhTRG3CdpXqDE/4zG//74px6Slps2/AdiHbdpS4l/lUE/GcOynyhLZaoO1RvxL3GhDCW1vfSttLM71cX4+DiW77UCS5YskQW7YFvraTb61/uUG0wlT7kfKFuQphpHfm70b99azrK2upJKntjW+MVEyKOYZRyCEh9/lqlypVCmxU7KlaJKqeMxjMbGKrbtdYKLsmECFH5Tm6gjLOqWTymyX8ijdUDIQZrj/FzIxylRmf9aRupXx3KVwVwnm3cr5b9SribFkm164p7VwXvLsBkfU4YSRVghi69qX+qXGMAQ957iqCf56+uKcAFSB7FDif4lGQ6bN27E3WvuwujICEZG/J3mCGOz6s1l+Ivj2gfkdc6/kSTySvuqqrILSiYbv9OFKe07Y3zGscxaCyP26fGcNui4Fv3ZjvGf87r7dvz3Y9nw4z/bJv8o100z/ndnNP7n+ZmP/3aa8T9drOR5M4l2Gh3/4WDC4kG/8d9NM/7rIrOW841OakOkHTT+0zYtZ9t8/E8ylNT2zLdgT9nXahf51TbdV7mQ/vG8ed9SftlW8823y/FLKm3XMvWhbE8bVI/aa8PFRNrJm0hcEbvSF+qZDv/+ugLxny6OV1Ut14hSzvvz//C6yaCefVH14H/A/D980kPt1bYoYuOI/7pCU7zVS/1izLQ9+cp+pK7p8d97/auUh374n6f5P/u/tAEAJicnsXzFXtE/ree21mnMo3yJe8lPKttqmda18U1Hv19zF0ZG/HfIzbzgP/FSjvKSPA78NyDZTvuDpDJUFvmpr2xPGwbjPx//23Kx9IV6psM/2zD/WKf2qB7aU5ZRBvrhPzyY5IYa/z1pbNw04//84p/XrpOsUh6mwX89x/iH5KLaQGIdt2lLOf7zgTXWc8HX2gaduuNfew34m+Yl5yhTdajecvyHzKGU1PbSt9jnM8V/gU/Ws38ib3iq2Tn/JhflJWX5lsW19xhz7fXXxyeAWVYuALP9F778ZbztXe/E6hdfgHPOWBX0pJxR3bS7zV8Sy8lDPfcN/n0595u28f8+wH8TcslJHSL+/ba1TXyTp8poizntINHOZI/fr+Zh/IfkotpAYh236UeJf5VBPxnDsp8oS2X2zv8TRtVfjaGSCbhCi2+lnRgW/4Ue7tOOklf1lm2rqupdAGZDU3RA2ZhlRhJTg9vER/S5MNlreFVx8U+Bkb/j3oRvd1YBcOTRE0fqUwA552DDonDT+EXCMkg2nKCyTJOcfkAGEZaXcrSe7b396VWK+qQyBGBcANZky2Id2lMuiRxJX0pUlinobIilfyJbXpvLg2OID30kkU/9Vl/9v6Rbc0Z9oVzqjPVBj3OpH8mrckrZEYTSV9b6V3zT96ryeVL2K3/1tQaxvwE4px9gbz+A82BDYgwYK9//Dh2Z6EPiwF9ITpR9bMKdSjxZ0Hrqog2MK39VJ/kZW9+2N99S3ZD4D/V6FxHjmPCfsJK1lTrn/CIngg1ZuWDON/SQYOwwAP+Orw2UAVR9pQxOqqowmWNdxE6B/+xia1FPm6mfJ1dlX2sbtYVtSSYMIuWdfyTVx3putw26VVXFNzI4wX8V7nDjxVUS+dgHlKM+kg+zwD/JhQF8pvgnb8R/sE3zQe0mjx2I/zQ4q37tlxL/KGLF2CQdiUd1Yk7x721SHKgsXgRjW5XDbe6rnZRfEvk0zozjTPFPojyW0w7GiDyMHabBv+aJ2qIyWFbmST/8t8kpY6f2UwZ1lDKN8a/zb5oG4+PbMDo6gt123wOLFy/G9pDqj2RMXDTteYLUAEDx+KXxx1zHCwQulJF6urZkUApzotKmQIybpzY5qczzWoB+0DbQZvKWcvy+c+EJ4Gi/rhomvn5kDOOXlQYf06Nx5It2ew6/RV9jPHKd3g1vp2fN5fiSIIMLk3LjQHlTgPPBj1HhWKe5XPKzLPVLL1FG+ZvqyhYA4mKs305kWhZve/M4S9GoV9tAdPi4lWmXZEg/MMSZ774sFEc2JNYe2SjKyxiXNm3etAlrf383bLeLRYsWheOE5HVLDBDkeJ68r4yM/95GX1ZVFbpT+fhv4/iv8/90UcwV478uRjvnF5V1nkM7Uuz9tp3D8V/ndTxW6zF1/sd/f7OxEv2lny4b/5MsXgzzcR48/k/NaPyfyfw/9Uva9v3vQuKqjNJXIBx7wvk648w4NuHVuzpWZm2dvxlFfUCwh2/Sor+UDQR4SuwwT+M/b8bGtON/0km9qp/xK/ta26gtbEtie5WlpPoSr5dN/CtfJU9kuJ75/yzO/yWemDH+05zOhXM13uxQyilll8eKEv98Cxlv6qbd5LHWojPSiZ88stY/SUVbPF9+nNJ+GTj/b6bDf9IJ5gRvaoox8fbObP4/c/wjeztGnsMqo/SVZWaO5/+YZv5fLgD7JjnuSGUstF63taxsW9aXetq2SztKGXfduSY+Acw/5kLZljZRbkmqr+QdBv91eKqtuk/wn8e7nkP8z//4H/AvXUJ/6aebCf5b+tjsAPwbw0X3vF/VTsoviXxV5W8kpN7twX+U1wf/5GHsMHD8t+n6v6wrlDKc89+xL/NkuPE/PZWrsVP7KQMt43954yTbktg+ycpfu6L6Sl7iX8/xqz7jf53hv/epWvVbfdU4IMNoS57Z4rONkp9uhvP/knfH4T/pp28k+mvvB/jPb+D0edYN1/94o53K4Tb31U7KzynPKcaZcbx/4H/283/64TL8++02OWXsqH8urv+jJTdIqq/kHWr8v3j16jdocMkMSYhSsQojnzpEZ+rs493JQTDYsp/qioNLuJuV9UxubaPJoHy8usKDfze8eoLylVdtT3Xh5FZAhnDXB/nbO8bAOf/KasYFRYJFzuJkk/UxBuGCYlmvoChf+6myjQnfMgp3qbGd2mRMenqX/mtOqGyNQd3x34+gX7St9FGJB05j/JKftf6bWgi+UTftoj6IrZTNfol5GF7DwhwisQ8oF0XekVKZiSd/VTGZYj7Qb+vS09+MX1WFJ6LhU9CfkLcf7PTgpbEr+biv/YKWfCE/eVlmJcd8LOp48bFNJvk03lpv5HvTVXERpB3/vbbpfrzYKf6WbYwx8VXasacG4N+EHKvkwNeOfx8LY/xkLq9LMeRvhv9soE3kZCDmIEBZyk/7S3xrDBzxH540YBvGUGNfyqYc6u6Hfy+ziU+887WRKoeyQPyHSRdl07bSRyXFPyL+81exVEPin3WaSyxT/TPHf9quWvCvcaTNKPFf5DJ/1R8z5/hvGWOjbWkywFgon5LGkH9lPWWQb/vxn7a9L33wH/pD2wzCv+73x3+/8X8I/PfJdddyIk5Zyk+ddV2jMhVGR0cwNTWFNXetwcYNG1FVBqMLFvT2EVwco7LFvpZ4arnyGj+5isdSv5jYix+dg5HoR77Q6Dxz/O0lLyfVM06JwqqZKZ7EBXKZ2WYPozBIH5kUh9IfT1oWtg1yfyJLsRIYi8V+BH2OegtmxpVtstglnbJkm/mamSbi6RsXghH4jPR1z7bEg/Eq87SkqEd+Tcsx2P/Q97JNKkt1PiS5c4lXDo3Cy3r/6//UruQXtCfIF+ORC2/PrWCXyTczjp7Fa8Ym+WFtgw3r1uO23/4W69auxYLR0bj4a0yai7hp5/+Dx3/o+C9jDeCfHCYfxy9iMvaYyNZjoI7/2MHjvwn8LEews8w93O/G/3zs6jf+85xCZaDPWM2YlL7TPrTO/9vG/9AnIod/Ss75m1JMeAra9Bn/q9mO/0VcY3m42XTY839tV81g/Ff/NYb8zcd/f25XkpvF+M92SXYx/58l/mmLm3b+P8Pz/+2e/7v4VhrMEP/kZzmCnSxL+v1x1hh/7qi8JRmkG4AGnf9rHGkzhsZ/8scMwH/JV/pKIn+b77QPffHvj/FtMsnHv7KeMsinOUg8zsf83zmHsSFujCzl0q5+eUU+LWdZSfR/OqI86mebLZs3Z33xPxf/veM/bxrq10/qI+va+k/1Mz6UW9aTtIzb1f+v8Z/4lFQO/8p6yiCf5qCdR/yzP7SN7itfaheu/09NtY7/dXjrA986onUaQ/6W5/+8vqfk5mv8D9f6rfVvjECJf37WSPrPz//T05Fl35OP+UvbSzm0CbPGf3pKk/V2lvN/8rMckjfcJjE+lFvWk7SM2719mMeRNuN+gH/rwq3lxl/3rmXtylqLTt3xZ9Nzgv887pqD9n6H/5nN/8s63iDD8hL/6gPJhTye0+v/Us88Q4n/QjblUHeZn/UrXvKSN6gjdFKNpRFspIpUMXnYtqqq+NSRB04CEkRuW6c6F04yRT55+JSn2sZgqAxIYqpflMMyEu1P9qZb+KmDv/SDgwZizLws6qyq3u8lxxjAHwBINhwMyWvCAT7xJ7mIfZDHX2UZk56w9R3fC0jAn/PQd7Un2iHxj34bf9VL80TjwnLKyXyoquzbT6wrgaAxV90QmyHxqQqQ8G5C1UEyffKav6U+Ew6wzDO1CwUIOTBzv6478a6q9ER8skFtpM+ZXrFFAVzyswxtMRdeb0uyXe2gbdqvbXFKC9xqO+LAQF08WKo81enCYiNtKe3Rv4gzU6HSbzv3wT/b6B1P3v8S/3mettlLHbTXl4d4hld+sZ76yZvrSnmGMEiSSvxrv/qNcM25wA23VUeZv5o3KOzhvjFVOkko8MVYqk4UeaLyNRYaR9ZpO9bNBP/kQWELy01xx2vZ1vTJa/6W+shPHWoXSvwXeOREWdupTLVRdZBHbdF+LPn5BA9aYq68arPW8RfD4L/YVhlsWw2Jf7WptEf/NIaqs4wZZbAN+diWclhGUp2lvdTBX5arPNajJV9UF9uiDf8jI+jUHYyNjWGqO4W71qzBb2/9DbZs2YKm20XTNNi2bZv/NigvwPcsP6HnCVDut/GSDIzPIb+jFZ5c2jbGH4zUF7/qFhpkaqQhTFZPOZGP8hgu7hb5jIzFl/fUF8eXdipt409LudpnuPjLYxx9MZGFi4p+rAx5kQUmlJu8JrQKO1wgDpXFQq5nEbuFLxnC8rBwRs0tx6G2MrTEn9v6m8c7PyaktuT3bkFu/CL5fW9lCGngd9n+YBn+N/nF8rQdI6ExYxCN79/givR93sYXJVuTHskJAE3TxaaNGzExsQ0b1q/Hbb+9Fb+66WZsGx/H6MgIli1bhqqq8vG/rgHGL5jYFlNu6zFGxwyj40bb8UjiNMz83yF93kKPk2leNP/jv0Hvq0v1WGvmdfxP44OOpdRDO7ifj//3h/l///Ffb6plWVucmEel7UYumlTbNf7bOJ/hn7XpldKqs4wZZbAN+TDE+A/pQ7WXOvjLcr5G1W/Pwfg/aP7fkjMsUx8x6/n/cPhnGYo8yeMyLP5TGzsD/JMHhS2xvA3/DhyGYfrkNcBrOr4tifzUoXZhRvjvzZFkY8ov1au+az+WNrEMLTFXXtrS2AblOE3btF/b4lRuqwy2rWaIf2akytI/a/1bcpYsXZLZUPpKGSpHy+ljWcd6lV3qKNtoWSmL9Sh06QLwfY1/ziwoc8fjP/lRPgjjtgP/pg3/QqZPXvO31Ed+6lC74AAbrm2b7cJ/roM884V//hpjov20TfunLU7lNvnMduCfpLL0T2OoOsuYUYZv08TjKsK1ScrhG6QQ/tcneUt7qYO/LK/4tGWfvqVdLGcdaeb4T33LN1hpLFQW25kB+I+U4T/hFlksZ4L/NM9NcUx+aTu2sQ9U/M/Z+D83+HeMTbRfeROO+Kt20Dbtn7Y4+e1kt8pg2+p+gf/e4xrlsIykOqtwDsMY+tfHt+N/UN/O6fX/ltiwTH3ETMb/22+4wWkDVVD+qrA6rKSzg5W0Q/x2HReCnTw9qUmRjA/6ZIGJcshji4MeE011An4iz31bPB0V5YpslvGkzjEBgnsmJEYT3v/tpEN8vRzUwtOo0auWD4+XfjCeAODCYKX6SIyf6iuJcek2/EZFnjzJ5vQEchkHBWVWXxk0jX9lkpODs/pCG7hfhYGS28nGNFC06UOR9DacKBAs7Hfn/NPSnje0idI8UbeCw1obX7HA/RKUkL4m0RZukxgf3Sf4vN8hL4p+0LhoW81ttd+Fu0JKWSqHevmrTx+QNA7af22/JBv63hiDptv03AHHg6XfzgeCMh7OpW8/6cSD+vhL3xCegvWvTumNEXlRTAj4mudSLuAnftRp5KBe+m0E/8Eq71P4xoLGituAP3yYFvyXvEbwD5koZfh38E9zhoN5aWNka8kd5denRX3O+4FH48D8Ron/2GZm+GdMy9wgf5s+tOCfvD3475OvJLWD9XZI/GMm+C/2+Rq6LB/FVpaxXtuWfahxLPvEERvzjf8Zj/+D8a9xYBvK5C/91Hq20xixHgX+y75SmymbZRpj5TPF+M8y6tNYlT6ZofBfoel2Y5uq9t9XnJyYxNatW7F161Y0TQNrG0xOTsEZ+MmQjDeRrH/Fpm26MHWd+PQXACoD1zSo6o5/WtTa9NmJxsa5T1XVvt4PruGVX77MhdcowuSvF6J/7CNr/TfXdV7GHADSq/gRfG+La4bTTsf7V/mFMtoWf0sKup21sd6FN5BwfuisjTeSYRb454m0H8p8HzvLz2/MN/4Hjf8Sz6Qg2j73+E8n8vSBsqyz/iauHYR/ex/in62rsLjb6XRQ1zXGxhZhbNFYjCPbJdk+hlXljwkaYfZrpk/qUcSdn6zw/OH172pz6/xfYtYy/msba/PvAFN20pnnrfYTcwAF1oYZ/0fus/Hf+1nmFIrc5T77K/mdcktjxXognZeyD+mjxrGnTwbiP8VZSeNgjH9rVhnH0icbjr26yKbkXO8xvm3815uAo23xAqdvT9n0jXExM8A/daq8nj4SHzXGymf64l+3c9uUb/rxf4j5fx/855TyQHNH+WmbKebyKk9zv6zXNj53Zjv/Tzhv04cB+B80/8/H/xxjtJdyRkZHYUOMY24HUps0zmqLlmv8eK7K/lK/M1tpW12FF+/7xrR3PvDPLeJM+1Dl8bdpGkxOTsJa6z+tFh4mcM5h4cKF2TFTbVAfyK/xUB20i2Xevhz/k5OT2HOv5a19oWUsh7TVspJKnWxT8qutg6jkUxv5DWDKJ6+ZM/zncS/jrLbx7W1lLqEPHlmvbTR3VLbq0rwtc8OF43qbPswS/4NiorliZzX+F/gvrvcpH+PDvmSZ2soy1mvbsg81jmWfcJtyqJe/1KVEW5v4TfQ8R9riyRiZPuM/Wvp4WPyzDWXyl75pPdtpjFiPnvHfY6icV0R+yQmNsfKZPuM/JwAaq9In02f81zmzmRb//von46ftSnLOjydNt0Edxljlp20m5HEnyyUvQ3O/zDXmgOuL/1yXj2n+Cmhu05Y2fbjf4T/lJetUV6mb8WFfskxtZRnrta3mttrv+uDfyqJjfEupTXEuV0U0Dtp/bb8kxshk+M99Lvv4vsd/3lfqD2WzjDHWcwJe66cuktqusYrbwteG/4x3Wvx7Yvy0XUllXMinvwBgbvvFL/KMGKIDtIzBohKlUqExZfqlzkK46AcBnRpKPcGCGCx1zsiByVp/kS+CRb7vorL1VVue8rvgGmthwl0TUW5on+5Az8HJevA6IPnlYFJVtX9kv/CP7cq74UjOcVE5Jb8rBn4tR7CdNra1MeHxeLZnf1IWYxVjXYXXDRTJ58JBqZwUOOdQ1TWmwrfHtI4DMvkoo4xX3JfcY3nMhbpCdiCKW6m/Sx30m7GnbaV8ID1xQF76r23qTrp5oIxBue/LUu7QD8ZQY1nq03KVT7vzMm8v+1TbK3/Zjrws05jw5Jax0+/iBimZzaX/kYsy4wE7P1izXrEF5y82No3vO42L4pT7LnxfKtPHfLAuyxTTcldOKRfw+nUR1YVBVm0nGc3fQIpB7lMXiomIxtU5v9BhwnaJZfJoXDRfU106GauqGt3uVLxobznAFHmlMilL/XQD8F/3xX8vJgbhn/yuDf/FBEpJbVYdM8E/yzSeZT1zpDc2yXbyksfNGf5zDKp8Ywwqualqu/EvecZ8KWWp7jIeJG3D/lMMsV6xxbrpxn/uu9AvKPpVfVIaBv9qG7fVxtJXyiApbv1+shlIN9mgiFG2bdOnHbhNnr74b2lTVRW6U115pVQ+mVb/dJ/bnjHlf9PkNwWxfC7wn4//PucNcXM/wH+H+A+v6uLYksVKfKWcucF/jmctM+FVZyjxLzEu25GXZRoTlvXHf25z6T9J28wl/pv7Ef7NUPgvx/8GdR1OFq1fYEURL+p0LnyHt8/4zycbnPM3wqnuqqpQ953/Bx7xjzJR4t83zHKW5OYQ/+R3Ln2j2Nwn43+ed6xnjpSxSfvpeMAyJ/jvNk38Fupc45/x0faJP52bq+0qn7ymSm+1YuxiHkYPU8z1V4kySDx/8xdrk88QfKjsQfhX3LoB+O89/58N/r0NtJH1SpRBUgxyX/Ob+lDEqNwusezLU39QL+1ta1P1xX+eQyqT7dVPN+v5f55jw+Kf5aYF/3mv+msWLnzexjl/nm6Mfy2oxt6YcN0mCFB7qVPjWdb34D/IaYuVxrKq/Q393aYbv1s5n/j3b0crx+y8HXkB4PY77sBPfvoTbN68JS4QOAcs22UXHH744dhr+fIeWaq79J+kbapwXGnDGPtoamoKu+62KzqygKqynY6JIn+iAX6yZgoX/fsG/Gp9uslyNnTwbh289+RdcOgeHSyo81wuY0Bi3eTkJNbdcy8WLFgAN2/4z7E6CP91uMnsvsQ/PYo2zQH+S1KbVcfsx3/BI2+YbcN/oLZ9ljkZ/5t5nP8r/nX8D0jpaUdellG2ljF2ijkS541qQ0naRvMPffBPog+ak6Z1/G/grIs39agP3qegS0wn7jDk+K/zY61XogxSjNdM8S8yqJN9o5it6iqcg1Zw8hR0W5uq8jeZpvjP4vxf8t/nlozFEf+TsZ9IZXvylvHiPvndfYb//Hha1t8f8M9sSWXeD14fMSa9xph+KqmtKl9jwjLGLuaz54h8ahfbKan+lH8tGJs1/gfP/9v8V/yn6wjplecobOO22hjjF+TQFpJikPtD4b/YVjmKWY2L5mvZpr74wgvfUDbSAJCqcKBgoFnG/bZEVYPq2i94si1JX48bgyYr7fpINKk8+S71unBix30gfR/WhEfyKdOFDvcXEpM/KqvUUVX+8XC/nS6qqd/W+idpNPiMh39yRv1JfFxcpT4FF+XwwpC2Zx33IcmrNlJm5CtARlBRBontnMRS61AkJ8lJW80X/5cPEqxXoCgo9O50xoSUbHJ+UO9zZ6vmpJLemUHZjfUXnJ3cQZL6MN2BEftH+pt8ql9jSv9Zrn1CH/nLctWveaV2lDqc5IsNB0P2hcpVP4bCv0sx8IuxbfhPsok5tQ8Be1k++m5GNRD/wd/iFXEaC/5Rpk5GFf9w/hjkoeB9KWWVOnyc0gJqtClc9K/kYG5tegW15o4S+Uo/Yvse/NeAvjJU2nEfkiNqI2X6xRO2AxBea6j4155K7VL8tQ4tmCKpH9TJPxLjo3pQ4J96TRv+xSbyaHvWMxalrW34V4zRJu1DlUmdZcyT/hQnSF/wr4yt/rJc9attyQ4/qVUdTvDMOzDZFypX/RgK/7MY/9UfUjv+pxv/c4yUel0L/rU+w38c//vLKstjfpT4F7/57Q/+sh364r83fr68H/4RZ5fGpDeOcB/98C+vADLhExvOpddjefynPibRFm5r/IwJF035VHEY97V+/vDvALQ/eazt2VZzUmku8Y9W/Of+apn6rD6qH/wt5SovbVIdTsaLJtzV2oP/4sTgf/Hf2wdazjhxu5RfFeO/MX5OzxNwtiEpX6mT3+xVe8r+MWHeQp/MQPznJ6km9D+CXW3zfxfmT9rOuvzuZlBfbJWI/mm+RN2BGEvykugD5cQ+vM/Hf58zyk/bzUD8pz7Sv+hzS+6RX/WrbWoH+djGZeN///m/DfN55VfijUImPCWMAfjn+avGeij8+1sOYcLbAZqmi07HL/Qoqd/6p7HgH/VpPW2h1O3Hf96masF/4p0h/geN/9KeddxHP/wXONZ2Pua9+CevtmMb7qMFUyT1gzr5FzhifFQPBuCfMSGpTeTx7WVc4k1y4Wa1uMoLoDMyIuMgn2xKF0lpk/Yh67R/yphrvyZ/U+xN5f+axsobzPJf8qt+zSu1o9ThCvzn43+ySf0o8wsA/uNrX8O969ZhamoSU1NTmJycQrc7hU2bN+Oee+7Fww48MPpEm2grZao/JOLfAeBxhW3bxn/n/NPdCxYs6ImNbrMN9+8Zt3jl1zfi2t9PRd7Z0tqtFndubnDCvguw02iOZRR5Wvbh5k2bY6yV/38q/tmCMVE9mBP8z9f4L/gPN9TSdtqHYfDf0ieUpX7wt5SrvGW/sXy68d8Ngf9qFvN/U6WHCKbDP8RHMwD/rI86NJckFuktKxVgkK0Z8GlXT85/G9WEY3GLrFIH48Rt05Kb7B/tJ82d0p8yT7nNvor22HRjuLZnO+4jPClsjJ+rKp/GO+rL8J/6WHWUOap1aMEUSf2gTv6RYiwfiPjfnvG/pU8oS/3gbylXeWN8kdZdnPP5jbAe5Fz6TrHKVT+2H/95DChT/SHNH/6nn/+Thpv/VzDyxlHK1ziSt9oh1//z9qzjPoYc/ysWUkk/5yiQdQgdSz6VYSTINkzuJqem0r609w7W6IyMZAZSbldeiaiOUo/Kog0mXCCoJGn5hJ4Lr7Nx4QTQ25ASRv/SE769Ol1YOCr1e3kWps5X9FUGO0DbkI+LtowD+ZhUVeWfbtD2kA9Tk7pNEy8K08ZSF2VQT5mEbEM+U1fxbjeWM6Zsq/EoE539asPH0snfyCPuWm7lA/HptdfJHvqiOYVw8GN7gptyY99L7tIG2hHrPEBiGe1DiHdsz3/iu9ZD4qTy/WJ1HmfyUk9JarcRnFG+6kCU5X2rKv+N17J/zUzxHy70l7awbbIrxWtqIP796xFpC3mqofDv67ivtvDPmPT9Zid949vZuDDW9ke9uc7wqg0ZSJwLd5mLTzGXZ4B/tmEcyEd5/IXxT6SzXYl/7rf5oXzenvT6M+rWNuRjLLWcMY2+SjyYPyT2q50F/um72kNfKFeJ7bcH/4wFy9AP/0W+UB7rAT8J13rdxrzj38an5ecE/4UftIVt1S76MX/4F/wNwD/luQL/NtzoYwOmyz/nFcd93a7DTW0uyGEdxyqO5W4o/PeeMCgf+5G/2h7bjf9y/E9jFXlpA/f5y5iyLds5l14DSmK/2lngv//47+NBvSS2nx3+/YmSkZs2KJ+xmg7/XdaHyTr5WK/b2IH47+wQ/PvjjLuP8M8FeP6Rj/Yp/tWmtj/qLXW6tvFf8pZxZ+y0HWOibTTGKQ5pPKI8/mp7zAj/ySbK4PmE6tY25GMstZwxZVuNB/OHxDjbWeDfWhuekkv2cP5DuUpsPzv8p75WfZgB/rUeQ+KfHtTzgv9B83+Pk1IO3wjBcz7GufSDtlSVvzFa7aIfJf6d9FFF/FfeFhtjV88K//zlH/noW9M0frwWGyiz/KPeUqfbIfi/r8b/HY3/1Mdabkv8t47/0+G/E3Iq4L9b4D8s3jTdbsv4Pwf4DxgiH+ud8zfd8VyaGPO86aJoSdHuGeLfXw/qh//hxn//BDXknNv/xwUDtlW76EeJf9rIfh0ZcvzvdDpYd++92LZtWyxXoq2UpX0418Qb3EtiDPhLGt+6FRs2bEjxbOFj/jMO5GM/8lfbYzvwb+8D/DfWZg9XDD3+zwr/D5zxn6R9XJLabWaA/0HjfzUk/hnn0g/awrZqV2OHuf4/t/N//1uHvyqez9I+npsB/pjGhTF9QwT/qLfU6e6L8b/xb7m0zdzhX+1R3dqGfIytljOmbKvxYP6Q2K+2Z/z/X/xrnzB32kjtNkPivwn4r6sqzIfy/jXziH/6Md34P/f4Hzz/L22gzPKPetMNJTPDP9ePtB1jom00xhoH8kV5czz+1xdfeOEblEEZGTCt60danykSWXTM7/vg+VcwGNgmJUabXiudznLDCz6iF0zMUJb5waf8MvmpfSk/Ulj5Z7kx6RVYyku5xph4NyfLvJ1BZgsAjTH+ZEFix7Y1X6sY7jpnArCdyooHjszPdCAjf1X5Vz+rnmRnIs/nnx4pF7jYhvbyj/pjLKT/ua02VwGoTFqNI0Lfsyz6p/GuTHjK1cXBngMHdVAf7aBsJ3dUlDaa8ARXyR9lyFNXLCPx4EB5ZQySTfkBmLqqcDGlDr+ab1xsIC/rq9B3TfimQ7InHazKA0WyI+Uxy8p+GkRtMr19RcwK2dEnGRja9JLXGH93mzHhm5NVBX2qgrwk1WUk36J8yfcov8VftcfXpTNh8mof8pdl7Bvyl/LI29Y24d/XR/x7AZlvemxoiyPl+8mxyS7+lXZC8poDkxsS/+oH5eq22lVNg39t04r/MOFQvXOFfx2Qya8ySrmkXvynCayWo+gryuW+xkp/yVfagIAlTnyTPR045yeCWl7aoWVlPw2iNplqXxkzyqb8GeE/lJuI/6SXvKQ2P8p95VX5Sspf6uG+9iF/Y9lA/PvYlPnBtn3xX/R/WdfmJ/krmRxrX6R4pr6gXLbti//KxPcSqB8ujGMmjFUc09TOqqrQbfyroyvWm96703P8Jx18xT/1zR7/OcbnDv/5MVDbMgYs133+Ujd/yVfagIH47zP+S87EshbcDKJcZu6L+l7Kpvz/v+O/tLOUR962tsPg34T9NvyzLuoO+KU8Pk1b2glIzrbgn0/M0V4+8RH1SCzUtzL+tGUm478LC6Xk27Hjv8dWm1zS9uBfz900VvpL/aUN6Iv//vN/PRbDpLcpcXEs1oW4t5HWq4/c1rirX5Rvrb8AC+dvmunR+7/4j/Vt+Oe+vk2tzU/yV9OO/55UJ9v2Hf8lNuoH5eq22kVbmqabnY9QlrbJx//Et134D09U5TbW8eaykl9llHJJrfgPN7A4l15Jna5JkT/vE42V/lJ/aQNa8O+mwT/bs5xlqvtBD3oQNm/eBMBhdHQ0/u2666446sgjsWSnJT0y1b4yZrE/g3y/CJP8KG1ykp9VVeGetffAWv8KY+3rNjLGoFMBBzyog+/fNoV121IOzYYOfFAHbz1xZ+yzc42OLAJrXLlvjMH4+Dg2bdyItXevxdiiRejIU03kMXOG/97xn/v8TXGss8U/liupTrbdHvzrtTzysU9nMv7TNvJtF/5nPP7PEv9F/5YxYLnua6z0l3ylDWjBv9rThn+PwRRvyiz7aRCVMtVGytK361E25dsh8a82mhAn1UteUpsf2X5obySuKouk7Us93Nc+5K/2I4n1Ko+8bW09/ruo6jQmaVuV1YZ/IzaSvyrGf30LlBJ55gb//fujesDgP5dRyiXdl/jn9f/KpJtK+dS7n2P1YpXbWlb20yBqk8m5jPpeyqb8+wz/YncpH0jnO36dMuklv/JqH/KX56ilndpWfdG2lDd/438Fc/sNNzgqNOEOCW1YFXcjaMfRILZpwiPb/vsiKfEpm6QHEF4s4kSYcgk8tC7+5uBgu6Zp4ge9+cSI6jPy+kMAcGHxjfUok4cbwXQuFvObufSrCvvsKP+NJG9XOoAIkClXkz080afxZkzJw6d/XTjANeGOFY1tjEs42Doulkl97BtJCPoSbQwH27rjn3JCiCP9VXnUyXryo5iUqA69SMhfkpUJDHNJifoAwCHEJRzYXLjrrAoTXNWh7SmTv/RD6+mL9gPrgfTNKh+rvC/UZso2xh+Q63BXTrIjtanDhXCS2q6xKn0yAz4yXoVcMIxnaKP+UOZQ+A93ylWC/1rwz4Hc25APoOjBf/CpODgl/OeTDJAvPNGPKMMvbhH/imlu62sMScak1ywCgL4WrCTqr6rKfzO3D/4rye2ImaK/SBpr9Z11Of59nVP8a1xKbBRxYxnj7Cf9ydZU7vlsmEiwbFj8q5/aB6qj7Zek+GcuKZU+Mk6UFfu7yDFtH2M2Df5VvupEgR/2WSmX9frklfaj8pkQWx7XWUZ9GqvSJxPxPwIUfZ/a+TvDSGo/+YbC/zTjf47/JJvE/mFd6R91so3KKflUxnT4NwX+HfHfZ/wvifqracZ/tavMewScksonwzXejCnlsc4NMf5zW+PGsraYlzb6NyN4HLKMvlA+5altJoyHJO0D1dH2S6JeMyT+OfZQFvtT+0FtUn389X74uJfx8POL7cC/dcAOw3/v+O95PY/K5iuJla/b7Wav19V8dKEN5+Nc1O+G8b/bNBjpjNzn+G+GxD9lKa/GtCTqr7YD/3kmDzH+89tc0+CfcimD2875N9mQnMsxGmPZg38/p1X8cxGY8gNjZrcJZSTtgywOLb+kYfCvuVvNGf6T72or5WtcET6Zwf2B+M/yN+/HqD+0mY/5v7ZT/FcVb2ROnwNouv4pE8rWfAT8Ij9lV8X43x1y/Of5GetK/yr5hhcKXxgn6lcZxL8dgP9mXvDvn1QeBv8lkReSyxn+ZzX+98ZN69tiXtroeP4/0/G/8FP7QHW0/XJmRL1mAP61vxgnykrn/5ofMu+TmPDJW57Txvpwc6zKL3NE96fFf/g8EOCvG/gc9XpIXPzWJ6I1nhorLWddG/55ozjb5fj3F75Vpuab5/G2dpsuJicmk2z4TzDVtV+AHRnx4/6w+Oc8os0/zaWoT/ss4Gp82zZMTU2h6XbhQr+PdDo+ts6i4lt1wrYxBlbyAAAMfBl506MjvcRRtqr8t5qN8Tc8cr+uajQ2nP/7q4uwzmJ0ZBQjIyNYtGhRFgfKov/qO+tmh/98/C/rNeZ6rULL3Tzgv8zF8pe0vfi3rfhPNqk+/tIPrWc77QfWg76Fa2vT4l90aj8qn5nX+b/fzvFPfDiYcP29H/61DWVXMzz/p6fsH9aV/lGnGYB/8qmMJhv/m3h847bpO/9vUFe1R798xqgk6q+K8b+ewfy/JD3XUt/RD//h6cXOyAia8HQk7Yoywlsn4nXalofcemKe2ejbbR/+U6xS2zyHy1/S/Rv/SZbacH/A/1S3ixHBP8fXyvixtjImm1uo/ZQ5eP4/G/x729TPHYP/9vm/+kJZyqsxzdGa999Mzv/Lc2sl8kJymTYypuRhnZvD8d/cfsMNjoaWAdbAIDxWzECST4PLkytVrMpVLgB/gA7V0aBywCoSIUgKv8khBoe/dV2n1/AxyLGZ39C70ZLsBMS48BwWjuOEWXwnaec3Nj0t61yqMyadQFMPZYSvoPQkTx3uTrE8gZCYl3I0dqgMXPjWDeOnieXkgM4/1kcZAFzxGkRuK7E8/kpZEz5mrnw8YWYbTXTmkrWMSG8+Uk66GEG76VcaNNSXKDfcxcMykpO7LUyRe/xlzGD8UzXkZV/pN4foU8xL6Vf+djr+gKUyaEvUJfrpC+QuIyX66/30semEkyLK4EKoyi73Nd6kptuOf14Itn3xn+JPuZABKDSKPORLdpFFfA2bLgxsVcRown9T4L/M3FgXYgX4I4MJ+Fc/8liEPO+Df75ujO1jnciFxI+2YCD+E1ZpS7LZxLzjQrPq932Q49/vN/EuLbWFbb3sPPe4raT6St52/KcB1A3AP4l86jdtpo/kg2K09CXiPw2S6o8r8F/KKWWXvB7/qZ9y/Jc57X8Vm5RBW9r00xfq133It+jopwuTBS8rcLX4Vu5rvEnTjf+2L/49qVwU+Nc+Il9pV+6rJ/KlOPfHf9ZO8d9n/Fc/yliovyjxH2xme82TmL9RhtdL/Zrfmg+UqbZozLSe7dV+yqCOUqb649vm+MNM8C/zjh2Ff8YTs8Z/b1/lcvKYYcb4rwDBOX/nFv95rBgbryP1XVXMbbJ9OdGIdgcaBv9cXNQ+IqltmEf8N0Pgn21Zp/WUp36UsWAZaVj86wUflcEyzW/bNKg7HcC5uPiqtsQ2EieNHfVzAdhaG/uX+2yjN8exrc7bgpFpO5Bpwb+RuM0X/vWkWuOJWePf21diWuXksv1TBzPBv/c/ydAFC+7PH/5zWdx3klNar/EmdZsmXkhVOeyzYc//yaeyYx/Jwltpl3O9yzPk0zizL9rwr+21TuNIeepHGQuWhb2h8a+2qAyWpTxJOYUZj/+5fsaPuuiHtlFb2JbE9ipLieVaz+2Z47/3Qj351G/aTB/JB/qZ5XLyy06H/04HTbcbv5XOepXN7WHxzwXPGJPAYxuLzshIPA/zN9zwAm56Tabq136ZDv+8ftUf/ykGZb3GmzTM+I9p8G93wPjPvmjDf9mWdVpPeepHGQv1FzMY/9WWMmaYM/wnPHKbMqgjyUxPZrKebUlsr7KUVF/JS/y7ofE/3PivvmocsMPGf8F/uPbUD/+l3eSxO3T+34b/tN+0XDOl3aS5wD92EP478fq/zW6yzttKXZFv7C+1Q+1Vf8124J/XEFlW5kkr/puwSCefD+A1R75Zgr/OpQXgMu4qM5//57HW+HNbieVa7+SG45TTXl/1gMZ/8rHkvT/hv8nw79cYeB7odeV4j7rCzaAab9Ls8J9jhnIxz/hn37jtHP/Tmo33XXnoB6bBf2cA/jVmGBb/czj+1xevXv0GbaBOxSAE4VUAKInl5YlfJ7zihIpJ6hjlGAEKX2fqXDrRK4Puf33C0WauhhOAVctd1FVdoemGCyoii9u0jQEHdRvAn+B5n2hXGfDok/GLg96PlNDRjyKZTThoa2ezXJMJSJPnSkCo/eWY0FG/3y/bAP5EuC5eEwKxBwZoGr+QbSTB6IcLB0vqYFsX4mbDAaiMJ/upzA+Vi2Af91nGfcY8/aZvzvFkry2WAOIiPvuFMirJdfVHeVnn+VOuebm9BzP+VlV65WU/fvYP/aVOErfJSztIjDfLyF/XabGdZbRFZVJ3yicerJAWF+uA/6CWOWGtf/KD+meDfy4iqw+IccrtpS+82Ozx7+/AoeymxD/vUAp5obZRr2nDf6BysLXWX2TggmuGMcEfbeUTK9Sr/cSYtOUsY8w2JZb5PRDWV1W4CSIMXpVcgFCfAaDu9ME/Zdt09xLtYExcH/xjjvBPKvOB7crfhH/P2xZLiB76SRnVjPGfjqsqF33wr9tt/NWc4N/Gh6/In+Pf17GdyqRuO4vxn21o+2zwX/pPUn2Ux9iQv23874f/mBdFbGlbma+kNvyrDSUu6Qd51F/Wm7Bgb7YH/y3jP7e5X7Yh1f3Gf2MAuamE9qkfbhD+w3eKyEPSPmBstA6SmyT6ofsm9hf3dfyfDf4TrsvcTLz5iZzGVeVCfOAv23BMRXgKUPnZP/Qh9YMnbpM3yfRkpx3/JWcKHn0Sx5ZPCM4Q/zbccEYflFhWxngu8d8MiX+1jXLMDsY/900//Nc1bDhxNAPw7zOrP/75ymdj/NyE87fB+E/zPtqnfjhiuwX/dbA78gTSPmBstA4SFxL90H1j/LmQecCO/wHvgd+68ETzvOI/yYvtjL+hmProP0ljAmNQhW/qkdrw7+Zi/JdlWtVnTHoCmH/UN8z4332g4X/W47/Xzf2yDWl6/CcfuU0/3KDxfxbzf//WtBA3hMsuA/Bf/g7Gf3hbl+NbuySHwoVyPvXCi+sIczPlZRzLuKIP/vWcn2UmPGmWHn4wcSGC/vBCeRYfyYFqTvCf71O35hN1aN+rnyxnG+pvw7+TeYbGzbThX/xSfZRHX8g/LP4fcOP/rPGf9FOGtiHVdScuCpBoD3Yw/lWuEv3QfTNj/M/j+C/f+CbRBv6yjfKV/Owf+kCdJG6TV2ViVvhPPNn8f57wz3oT1gs0xvOB/27TRbpu6O1uut3i+n+Sx5sby3wlDcK/df4GTfoAiQV51F/Wc98MjX8L24geF/AfzHLEopOnf+P8v3esr/uO/97W2ePf9wN5SFUlN4Q8YPGffFZezRXawF/KVr6Sn31KH6iTxG3yqkyEvrKu97OEnZbzf7aL+2FRm/77wrnCf/KBZWWM5wP/czX+0xKu/5EUG4wRfYDEgtfP1V/Wc98Mjf9ePbG/JDe4zf2yDamua78ArI6QUTtEHbByB0Us7xNMSKdrfVWl78+yTO/YZHkZ0CQ7n0iwjvXO+W/uqd6maeK3hWK56FT/qsov2FnrF0CtvB6oXMjL7As6/d04+YHGOb8gQzkaX6ZV6av6Q31KZWxzH9IJRZtctYVkjMnudNADdVUccDyvz4W2MrYh0Q+NS/lrTFpA1phoHkSfwsK0UimL+3rAAZ/elIM09xnnpKMXTM75u4RLuaV9ys/yKLfHNh9ngp1yeWCkDaUc1cfBnHJZpq/xK/tDFyUpx/uf7sTy9lZx4ZwX9ljPX/aE+kg92k1Zm6K/yu3U7ya7q90Y/6qKulPHiY6R14uofaSm8YvMalv87cFOPvBpnvO37HfVaa1/Eor1tAt98E9SWdqOsktSXyC40QO+8jgOSDymFa+7oe3UVdf+Aq+ZU/wXse/T7yTKUT6Nj1Ipi/s5/pMMTIN/ttE6J5PaucN/b75Vs8J/ihPLbJhYeHtSvNQ/lUn/NQ7cR5/xnzopi22op6xnG5b321bZlMPf6cb/0i7GUu3RX/WvrT/cTPFf+EO7svbSj6Wssh31KakvaDmGsf0guUq0nXLqcFGU8SltHYh/eUUq5g3/kS3W8Vfl3Z/wb226qUZluDnBf5LLMo9/f/JS9ofaHn0OcjQO3MdQ+E+vm6KevP5/Nv55gq7xJZW+lv6UlPkyNP79wmO0R4i2U045/493Fwkvz4e0rO1V0dSncSl/ua3tKEf5ND5KpSzuzz3+t2f+ny4coHgd6vzhv33+X8nFEPXZtOI/HfNa+YJcbUM93I66BuE/PAGMPvjnxer7F/7z2A3Cv7ZnOan0tfSnJPUFQ+M/l6tE2ymnxH9pq8alLGMbEvXRFv11RQ5U1RDn/0PgnxOE6JMDEG7Kp92UlX3WKPhK+2k7YzDd+G/DtR6NGefmXh/9MfH1pM45eRJ4+/Fvp8V/nsOUw1jzl/Ehbz/8k7SN15PnqLZheb9tlU05/L1/4T8cTx9w+E9v2QNzdx7w76bBP3+5rb5SjvKpH0qlLO6rT6yn3ZSlceZ+tH8Q/uWGEpWt/Cxvs71fvlXbiX+W9cd/2leZ9F/jwH3MAf4RHoZQW/ttq2zK4e9w+K/ABaim67+hq/bob137G3K4wOpmgH+zw/AvcWyJbVX5Ma4d/3nuqS0k2u51+fxhG8ak5O1XxjYk6qO9bb/c1naUo3zqh1Ipi/tzi/+0uKxyS/sSfy9u22xzc4x/yydPrUWn7/l/DYRPFajPZh7xr21Y3m9bZVMOf4fDf9I7m/E/vqnF2vhgoWvBP8upc/7wn5P6glmN/w71JRde+AYbVpGNrMZrctMAGksAqILSESOJHJXJQGSbJgtUFU6CyWtCpzQtfE4m8doRtEG3yWOMv6OeicM66qJ8lAeMYqKsHaHtjEknHLyIpjFRfv7RL1Pc0aFy++lDSwJE6gMoSJxNnwN0VdXxAg75jOQFeWkvY0t+7pMPktgs4wm+2u8ICvaf1Ds5OFIeB/OsL0Unc5p20lZflgY2lcuDKNvyV+00xr+Co7zBgDp4gYe8zHnGkpOySu5SaXsquSpyQmOvfKzL7CvuyGG5+oEwSNQB6+QZjH9/t9mc4D+8YlJ9SDEs8Z9eV0G+eOc2+9QE+8QuiO0mTDx78B/uforxK/EvsadNJGP8E8DcVhtpnxIv/Gt8KJN+tckiaTmKvFTK/CnxH14dY4x/optngIx7jC+PrzPAv+6TjzaQ1ObSfo2z1rs2/Af92pf6Oxj/ycdZ4Z/H7cIv/ilvmqT4Nu34T37zr8wJjb3ysc5vp7xSmyhbj02sr2aEfy9rx+O/l486NXa5r734p7y6Tq8koyyNy0zwz3a6TX0aE+Xhn7X+22PVjsS/xE9lMxZ5fFOezxj/4TXQtEH1cL+0X+Os9a4v/v3iZmCObTAj/KexZX7x78s784r/ZJ/a5G96Sz6TGJMM/+Gbs7ZPf2Na/Af77+f4Zx1laVx2JP4pU+Nbyirbk2g7kF8a6mcXGD/RS3LOL06X8WX7fvjXi3kx1ioz2KB6uK/bmCH+eTPffTP++4Wa0i/+ZXYW+Nfxn2+pKm/ENC05obFXPtbl9pX4T5hQm6218Xu75Gkb/8vFrDb8lzcC0A6NP2PB1+u24Trd0NmOfy7OUbfmTOkrCvy3zv8lnqSZ4T/vO/KrDTl/+ptL/CsZ+WxT2YZ6qJfEWGi9xqYf/ukr+blPPgQbVI/WG5NuHtA4Z/Ut+Kf+fvjX14w7Z+NTvnD++ky8xqH4D29Eso1/4r0//geP/3pOmPBvYcKbSphf/B5f7/m/t1tzQmOf+PJ8owxr/cIe7WG5+kFZVTn+t+CffJTVhn/WsZx2sB0XpFVnK/7/d/zvkVW2J9H2kvrZhR78h36UWJTxZfvtwb/eqak2l/ZrnLXezQL/zGny0TYtMyX+hx7/C/zLG99K3kHj/46b/ydMRJulHxubviU5X/h39xn+vQ1RXvhWp69Lx2UvP+UO5VIn5Wo5/TSyTf4yJhm/xqelr0tZWXvZZxxK0vZ+O/dF4xspw7+PN/nMduJfbVSbS/s1zlrv7lf497lLn0nUkfPeN/gv38jrBBPJZp/7VeXf1hbbzjn+k//3Df5TTlLe7Mb/XsxoO92mPhdiX/Lzj35VM8F/kXO6T+pnF1rwX79i9eo3UIkGgwZSCInb7EA+xaLtGHTtKP2lLt6BXIc7FcjDRIEYrPJoB3ms3OVEuwlm7huTni6lfsrRhDbSIfSNfwSv2hBlF+CnzSqzGz6SXfKWTwKxruc31KveKKMgtZGyNZYoYqB8LGMMGr6GTmQqaVvapr7TX18mg47oNuHA5WSxVO2hPPqgd/d6Xt9WH9XXPFI72u4wH5Sv6q8Leas+ks/KREp1VlW6q5h1TcgFv58PRNSj/LRDeVhOXhL712/34pK280RV80H19OLf3y0EwX+UK+2oJ8Uxn1BQF/Xyojh5evGfJpJsb0xaYB0W//q6Qso3xH9oqxMy2sO/hH942wbhPyxO04YqDD5t+Gd7Uopb/ktSn7xfsSrj4S9l12Hxt6r9q+0ZP8pRG2izmXP897blnw34V79JbMs8IJXx19zpj/+U97qtevVXbaYf7fjP8cI6n095P+b4T36oHuWnHcrDcvKSmOPcZrs225Vf/W3zR7dtgX9tRz1lHNUf8iD0k8rqxf8cjf+D8C8x9v01CP/JhjL/Sv9UZi/+5Yan7cF/C6mNlK2xxFDjvy+fMf7lNVWs03iUbfk3c/zLUzPOL2DNDv+D8zXZnHJo5vgPN97wjvQdjv/U9wPxT/7KLwKj6G+1dxD+9W0b5S91Ue//XPz3+sK2vsz6fityQ/VGGbE28fCXslMsk43kqQobaLMxPlczXZqnhQ7apr7TX805EnnYTmOj9rBtzKtQXsZ/dvif6fjfb/4/Df5Fd9M0GOmkV3Dy/Ff1KD/tUB6Wk5fEHOc229GWgfgv+gNFf3N7OvwPiqebDv8BI7StlEc7yDMs/rmQjQcM/vNfkurVcqU22RpLFDEobaDNZjbj/yzwzwVXzxuOey7hnG3pA6mMP/PADcJ/OP5VdZ3ky42xniflm9pMP9rwHxedQ46zzudTyk8AaJouOp2ReC1Cb0SjHuWnHcrDcvKSqio9QV32Q7Ld44M8mEf86/UcticP2vD/v+N/LNNfkurVcqU22RpLxBj4sb+0gTabHYR/ttPYqD1sSx9IZfx3zPgv+Jfz+hIvlMF8Ut07fv6fbNH+AYA63Aig/rb5o9t2Bvgvf6mLds4//n3+OpfWHNjWhJtyuW0qE2/KZhv+zQf+TeEL27JMf0Otf4Mfv/lb5AMp2VjFB2M0lihi0H/+P5f477WXPGynsVF7KI8+kMr473D8C1+JF9ZVOxj/dcv4z/71tjf5+B/eYqD+GsMb4fL+VnsfOPifi/Hfy5wp/jm2Vn3wX/rCtizTX5Lq1XKlNtkaSwQ9/x8lbjKKo036LwAAAABJRU5ErkJggg==</t>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAB4AAAAQ4CAYAAADo08FDAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAP+6SURBVHhe7N17fBTV3T/wT+73DbkAS7iYhKvcBMP9IhBvULFVWlta+VGreGlVihaFWvWxtbWo2Fr1eVotj1Ue7MU+SluoIOgCTxASSCCEAIFAEiAkC9ncdjebe/L7I5lh5+w9u5u95PN+veb1Ss7Mzs6cOXNmdr5zzgnRXq7sBgWnEDGBPI0nj7cEQuHl0SciImsC4Rom4jWNAlEgnmvkDazBvClwcldZI/h7/RA4+UpERP3Pn69ivIIR9Tf3aoRQMYGIiIiIiIiIiIiIiIiIiAITA8BEREREREREREREREREREGCAWAiIiIiIiIiIiIiIiIioiDBADARERERERERERERERERUZBgAJiIiIiIiIiIiIiIiIiIKEgwAExEREREREREREREREREFCQYACYiIiIiIiIiIiIiIiIiChIh2suV3WIiBYkQMYE8jSePtwRC4eXRJyIiawLhGiby/jWtu9v730EDTSCea+QNrF28KXByV1kj+Hv90I2QEH/fRiIi8hV/vkIEzp0BUbBwr0ZgADiYuVc2yAk8ebwlEAovjz4REVkTCNcwkXeuad3d3eju7kZnVxe6u7rQ1dUlLkLkhkA818gbvFODUY/Ayd1ACgCHhoYgNDQUoaGhCAkJYTCYiIgU/PmqEDh3BkTBwr0agQHgYOZe2SAn8OTxlkAovDz6RERkTSBcw0Sev6Z1d3ejq6sLHZ2diImNRXNLCzo7O9Ha2iouSkRENGBEREQgIiICMTExaG5qQnhYmBwIJiIigp//ovT8L0ciss+9GoEB4GDmXtkgJ/Dk8ZZAKLw8+kREZE0gXMNEnr+mdXV1oaOjA9FxcTCZTIiLi4NKpUJoaKi4KBER0YDR1dWF5uZm6HQ6qFQqNDc1ISI8nNdHIiKS+fMvSs//ciQi+9yrEXiHSUREREREHtXZ2Yno2FgYjUYMGzYMgwYN4sNtIiIa8EJDQxEXF4eRI0fCaDQiJjYWnZ2d4mJERERERG7jUxgiIiIiIvKY7u5udHR0wNTcjMTERAZ+iYiIBKGhoUhMTISpuRkdHR3o7mabKiIiIiLyLD6NISI/4163BkRERL7Da5iks7MTHR0diImJEWcRERERgPj4eLS2tqKzs5MBYCIiIiLyOI4BHIz47LHf8OTxBn8vwDzqREQk8vdrlyOevbZ1dXXBaDSiE8CYMWPE2URERNTr/PnzCOsNBrPHDCIigp//uvTsL8ceXd3dyL9Yhl1nilBUeQlaQyOuGhoBAEMTEqFOSMTUEaOw7MapmHFDJkJD/DmHiLyh72WeAeBg0/eyQH3Ak8cb/LkQ84gTEZHIn69bzvLs9a2rqwsGgwFdISEMABMREdlx/vx5hHZ3IyEhgQFgIiIC/PwXpid/ObZ2dGDLV/vwh6800BkN4myrUuMT8Nj8bKyZvwRR4eHibKIg53rtwABwMHH9+JObePJ4mj8XYh5tIiKyxp+vXc7y7DWOAWAiIiLnMABMREQif/6F6alfjv8+VYgXd36CqsZ6cZZT0hKT8Ivl38Rdk6aJs4iCnGs1BO8uiYiIiIj6xLUbbyIiIiIiIqKBqru7G5v27MCaj7b0OfgLAFWN9Vjz0RZs2rMD3d2eCkuTe/h8xB8xABwMQnh+EXlPtwffbyMiouDAmy8iIiIiIiIiZ3V3d+OHf/sAv9v/uTirz363/3P88G8fMAhMA4hrZd2rXUBXNtfhseN/Qm1bkzhLljgkBWFx0WIyAGBi9FC8PnS5mOyWg7mHr1cIISEIDwtDSIhzcfDu7i50dHYCvZ8PCQnBgjlzxcVc8sU+DZIGJSFr+nRxFnS1tbhQVgZdrQ7NLS0AgPi4OAxTD8PozEzEx8X51bNHY1MTLpSVobq6GsamnmMeEx2N1NRUjM7MRGpKivgRFBw/jvr6etyWnS3OCgheO3kGLD8q0ACPMBERWeFv1ypP8Oz1jl1AExEROYddQBMRkciff3G688tx054dHg3+mvvx4jux8Y67xWTqVyFulhBynePawqsB4H9UHcOr53aKyQpxg5MQFR8rJsv+fcNDYpJbcg4fQmJiIiIjI9HW1gaD0YhxY8eKi1l1rrQUCfHx8mcbGxuxcO48cTGX2AoAnzpzBmfOlmBQYiIGpw5GQkICAKC+vh7aq1q0d3Rgxs03Y8Tw4YrP+UrllSvIP3YMEeHhUKvVSEpKAgAYDAbU1NSgobERN06YgEk33qj4HAPApOS40uo/PLpERGSNP12rPMWz17z+DAAfPnwYhw8fxtmzZwEAiYmJuOGGG3DnnXd6/buJiIjcxQAwERGJ/PkXZ19/Of77VCHWfLRFTPaoLfev4ZjAPiWW3L6WFnKNmO9KA/LuMjIyEklJSYiK7ml5rFarnZoAICo6GklJSYiMjBTW6jlS8PfG8RNw25Js3DRlCjLT05GZno6s6dNx19JlSE1JQf6xY6i8ckX8eL+Tgr+pKSm4a9kyZE2fLm/vTVOm4LbsbNw4YQLOlJTg1Jkz4seJiIiIAoT9G2vqX//5n/+J7du3Y/z48fjVr36Fd999F4888ggGDRqE9957D//+97/FjwwIGo0Gb731Ftra2sRZRERERERE/aq1owMv7vxETPa4F3d+gtaODjGZfIbPT/yBxwPAVQYddp4/jJ3nD6Pwylm06Q02pw6jSfz4gGce/BVby8pCgAXz5iE1JQUniorEuf3uRFERUlNSsGCe7dbQk268kUFgChDdfEOJiIgEHPPX33z00Ue4evUqnn32Wdx1111ITU0FAIwZMwb3338/Vq1ahT179uDw4cPiR91WWVmJp556Co8++qg8MeBKRERERERkactX+1DVWC8me1xVYz22fLVPTCY/Ul5Rgdy8PIupvKJCXDRgnSwuFpNscmVZ2+zHMTweAP7uP3+B9V/+F9Z/+V/467HP0FSttTkZrlyBvrJKXMWA5WzwVzLtppvQ3tGBs6Wl5kv0q7OlpWjv6MC0m24SZ1lgEJj8n/0Kk4iIBiIGfv3N+fPnceTIEaxdu1YO/IqmTp2KO+64A/v2efYBgEajwRtvvIGf/OQnePfdd/Huu+/i7bffRkZGhrgoERERERHRgNbV3Y0/fKURk73mD19p0NXN57v+6EuNBqsfeADPbNhgMa1+4AE89/zzqK2rEz8WUE4WF+NHTzyBHTvtD4sLADt27sSPnnjCg0Fg6+Xe4wHgq02uvc2hP1aGas0J1JVfsToNFK4GfwEgPi4OgxITUVNTo5zRj2pqajAoMRHxcXHiLKsYBLbtlU2bsHDxYnlau26duIjFMgsXLxYXsbDl/fctPrNw8WJsef99cdE+u2/lSrsV29p16zz6fe7a8v5/Y+26Hwup1itJc2vXrbPIR2m/pWPjKa9s2oRXNm0Sk4He7bA175VNm6yWHXd4et+cdd/KlcjNyxOTZY7mSxyVT3t27NyJ+1auFJM9LjcvT1GuxOMrzre2jDXWyoN5OZb2zdpy9thaXjwmtpbzFlv1nbffJLR3vpozzw9r9Ym3tnPL++/363Ewd9/KlR47h7xdF3l7/QCwdt2PsXDxIsW0Y+cOcTELr2z6NRYuXiQmD1gnTpzAuHHjbAZ/JXfddRcaGhpw/vx5cVafGI1G7NmzB3fffTdGjBghp0dGRuLuu+/26hAxREREREREgSb/Yhl0RoOY7DU6owH5F8vEZPIZqTe1ENyanY2c/futTq+/+iqqq6vxxm9+I64goEyZPBnPrl+P1zZvtvssesfOnXht82Y8u349pkyeLM52g2V8w+MBYHN/vv+XyF+3FSMHDQUAPDp3BfLXbcWjc1colmuvci1oHGxqdDWOg782JCQkoKWlRUzuNy0tLUhISBCT7TIPAvsyeO1P1q5bB61Wq6j4pHGnJfetXInjhYWKZZ5dvx4LFy92GASbPm2aRcX64datXn/QHYy+v3q1Ih/vXr4cAPDcxo3I2b9fXNwrbr/tNuzavVtMBgDs2r0bt992m5jslv7cN5gFYbRarTgLcDB/x86dPgt0uUOzb5+iXB0vLFS8NFFTU2NxHj+3caNiHSLpRuOtN9+U0+5buRJqtVpex9//+leg9xhPnTrVqRc1rK3X1jFxZb2eIuZTzv79yEhPFxfrd9byzbw++f7q1Vj9wANeCwJ7iivnmPm1ydF1SmTtezxZFzm/fs+3/u057gfk6e7ld4uLWHhu40+Rs/+AmDxgabVapDt5Xg8aNMgn95tiN9Hbtm1TzG9ra8Nbb72l6EZaXGbbtm146623cPz4cTz66KPYuHEjjEYj0BuM3rhxo/zZp556CpWVlYrPX7lyRbENGk3/vXlPRERERES064xzw1fO+9Y76N60CsoBJtPx5qaNeMQs5ZEfb0f3j+2/HO3sd1L/+FKjwdp1P8badeusTq9s2oSxY8fi0UceQc7Bg37/XMyRu5cvtxsENg/+SnEFb/JqAPh/i77E6JQRePWuJwEAaxd8BwDw7uFPhSV969y5UqcmbzE2NSE+Lg4tLS0oOH7cYvLUsHM1tbViElpaWtCg14vJHiXuT8Hx42hpaUF8XByMTU3i4jb1x/YvWLzY7vSkkw+9XVFeUYHjhYV4ysqDaInUskwK1kikCuWZDRsU6c7I6Q0yO9NqLbjZ7iLBX0kXBzGgIv3fHxcPb9mxc6f8ooP4EoQz8wOVGMxdvWoVPt+zR/7/6rVrLu/v1m3b8F2zlpdb3n8fw9Rqi++SrHnwQXy4dauYbEFcr6Nj4ux6g52Yb6I1Dz4ItVqNL4MoQKPZtw933nEHpk+bBo2Hu+H1Pg/dfFFQiY+Px+TJk/G3v/0NJ0+eFGfLKisr8cYbb+DBBx/Eu+++izfeeAPFxcWKAO/Zs2exZMkSuRvpF154AQUFBRZB2lOnTuHUqVN49913sWnTJsTHx6OyshIvvPAC7rjjDvnzjz32mMXnduzYgVdffRXvvvsunnjiCYfbTURERERE5ElFlZfEJCvS8e0ZwHnMwbdHifOum/etd/DMlacQ8jv7L0c7953UH8oryvHSL36OMaPHYOrUqVan0tJSvPvee5gzezYA4OrVq+JqAo6tIHD/BH+VcQ6vBoA/PbkPB8qOYfHoLLz7rZ8iTTUYT25/XVzMZ8LCwhAREYH6+jqnpoiICISFhYmrcUtCfAIGJSYiPDwc9Q31Vid76uvrnWqB29LSgms6Hc6VXe8CoaWlBRcuXsQ1nU6xrCsSEhJQX+94G61N4eHhGJSY6NPtFx3cv9/u9LZZyy1PkVqmFdvp733X7t34yVNPicmAWbDP2hsljqxetUrRkrS8okLRHanYbafYDa34Rs59K1fK88TgJMxaCVpbN3q7ZjbvFvOVTb9WzC+vKFfMv29lz0slkvtWfgc7du6Q50ukrjMtP+O5wK/YBazU7bB5npjnl6O8dsRaQEWzbx+WLV0q/y92h2v+/dL2SfNg5/iK+wYr6xbnO9p/W+5evtziRQdz9uavXbcOr23ejOOFhTa3SdoWa+XTGeJ+SHkm6et+e1puXh6GqdWKlq+f79mD7333u4rlRN9fvdpua11r67V3TCSO1tsfrHXve9/KlYpyYn5OLDTr4h1Wyrwrx9VavlkzzCyAbu0chZXtEMs5nKhrxe0XyzFs5IWjc0y0a/du3JqdjewlS2z2WuDK95jXRdJboua2vP++vL/26ljH678e+HV0XZKuO/et/I68THlFuWIZZzi6vr2y6dcW3z2QqdVqVDh5DjY0NGDw4MFicp+tWrUKCxcuxDvvvINHH33UIqDa1taGTz/9FFlZWZgyZQrQGzi+//77UVxcLLfgnTJlijwfAEaMGIGsrCxUVVXJaQCQlJSEe+65R5G2f/9+ZGVlITs7W04bP368olvq2NhYrFixQu6Wevz48Zg0aRJOnDghL0NERERERORNWkOjmGRp7kr8uPrvGPvPStw1y/pzk3nfegdfDf87xv6v49+BTn2nD+Xm5bk0BTIpmLv2ySex5sGHsObBBy2m+fPnW/QoGAzEIHD/BH8lUoO3bu8GgAHIAd9v33Q7dpUcwuGL/vPWeUJ8PG4YNQojR450arph1CgkxMeLq3HL7JkzcduSbOtTds9ki662Fg2NjRielibOshAdHY1J48cDAM6VlcnB04T4eIzLzBQXd9rwtDQ0NDZCZ6V1rkTaD1vT7JkzxY9Y8Nb2+4vvr16N1zZvtniYDbNWndJbMNZMnzatTwOGT+7tY176ji81Gmz94AO5S9JhZi2Eyysq8MyGDfL81199VbGu1zZvxmubNiFn/34sW7oUb/z2t4r5H27diimTJyvWbd795iubNuHDrVsV3WIeLyxUPPC+vn0983u2T/lA/LXNm+Vl0PvQvKd1Ys9nfvLUU/3WGlHMk2fNWl7ay2tn3H7bbTheWKhIO15YKI8b8MqmTSgqKpLX/+z69Vj9wAOK5a/n1X6Hx9fc9WOl7LJY3H57++8Nb735Jp5dv17uAti8pau4LWL59CTxu/qy33u/+ALTp02T/7927Rp27d4tB7PEvBZp9u1TdAVeXlEBrVaLmpoaRVBMvJGcPGkSiopsd5UjrtdZjtbbH57buBHTp02TA9FScFcqJ1vefx+vbd4sl+mtH3wgf9aZ88keZ/OtWqvF0CFD5P/Nz1E4ee69smmTYriAvtR5tvLC3jkm2rFzJ9S9Qe85s2dDrVZbvKjkzvdYqwM/37MHq1etAhzUsc6sH73XD0fXJSjO+QN9Puedub7RdTfddBPOnTsHnYOXAL/88ksMGjQIY8aMEWe5ZdWqVXj77bcxadIkvPPOO4quma9du4by8nLcdNNNis8kJSUhLCwMDQ0NcprYDXROTg7q6urQ1tYmL5OWlqYYW9hoNKK4uNhi/aKMjAwMMatPIiMjkZycrFiGiIiIiIjIm646EYx9ZNZs7DpyADh8GKUzFgjdQAOYuxFfDf+7w5a/Eme+01dOFhfjmQ0bXJr68szff10fE3ggMA8C91/wV8nrAWBzsZHRYhI6WlrQVH0V9WdLrU5knbGpCfkFBRiUmIgRw4eLs22SgqVS8HSUC5+1ZsTw4RiUmIj8ggKXunPuK09vvzX/stKStryiwiJQ4klrHnwQWz/4QA7w9FdLObE12poHH1Sk3X7bbfIbONIbO9L8ObNnK5b9/urV8v/ZS5ZYvLkzfdo0RQX31Lp1OF5YKLdC27V7t0XQ8SdPPYVdu3fLranWPPgQMtIz5Pnm2yfp2Y7ry4itp+fMnqNoJesqaexkabLXCtBentjLa2fcvXw5tFqtXC5z8/Kg1WrlPN61e7eiW/G7ly+3CMCYb5+j42vO/rG6nh/29r+/9ee2uPtdW95/H8cLCxVBKWlsUmnatXu33SCwVqu12uJt67Zt8jq+v3o1ntmwQXHMhg4dimo722trvY44Wq8nSa06rbX8/N53vysHQ1/bvFlRN3y4dauiXGekp7t0PtnjTL5Jx9O8njQvS3Dy3LOs82a7XOfZywtn7f3iC9x5xx3y/3fecQf2fvGFYhl3vkesA6WXHKTPu1vHwmF+X2/la37dceac77mOXG/tW15R7tT1ja4bM2YMZs2ahbfeestmELioqAj/+te/sGTJEnGWR0RGRmLt2rV44403AADvv/++InArtRCWppdffhk6nU7uOWfbtm148sknMXnyZLkb54ULF8qft6WhoQFhYWFISkoSZxEREREREQWYRbjn5jz84zAAHMA/qr+J5+eaz5+Ndx8DHnUy+AsAIX4cXDRvHOXsJDX2CT7+e5yCidcDwH+5/1dobm/FH/P+gUWZN2PFFO88hAlo5i8+OPEShLGpCQe/+gpw0CrUlnGZmUhKTPRY8FTahoNffdVvQWBPbr+58ooKvLZ5M75lFjAor6jA/3vgAWz2YotB9D74zultefnh1q2K1rHOMG/l4SwpYDB06FA5zbx70dc2b5aDNlILroVCt6gS81Zr0vrMA0tTp06V/4ZZoPHq1atmrZznKJaR/jfv+9+8O07z7ZOYb0duXi4gl9HrXR/0Ja8k31+9WnERthUkhRN5YiuvnTV92jQUnzoFACg+dUoO8kj5ufqBBxSBMDGYYL59jo6vxFaLdGvjNNjbf/PtchRI94T+3BZ3vmvtunVyC097nl2/3maXutZIx8U8MCiNOWuv+3lfcZRP9kitOqXJvHtqKRi6cPFiLFu6VC63tsq1+TxH51NfmL9Qcryw0KIrbWV9Zn0bzc89W8u4UufZWocrynvHtr/VrBeTyZMmKV768cT3LFu6VK4Dv9RoLALdztWx1m+8rl8/HF+XrJ/ztruB7rmOXG9VLAV+HV3fSOnOO+9EY2MjXnvtNfz73/+WA8Hnz5/HRx99hG3btuGOO+7A3LmKpwceJ3XvXF5ejmvXrsnpTzzxhBzYNZ+mTJmCyspKFBQU4IknnlB04+wsk8nkcAgWIiIiIiIiXxuakCgmKc2di2XHDuO93n/fO5KHZbOuD+sH5OHRFyrxzIcb8YhZqj1DElRiEpFPmHf7bG1M4P7g1QDwc7f+AJPUmXht/1Y8u/Mt1Jn0eO7WH4iL+VRISAiqqqudmkJC7ERl+8rFVZoHfxfMn4/4uDhxEaekmY0z6K74uDgsmD8f6McgsCe331xGejoO9gZevrVypRz8XbZ0Kf7XwRiXnjJn9mxs/eADHC8sRG5envww2V4L5OOFhYoH0M4qLi6Wu+hE75iTYjen5v7+179i6wcf4LXNm10OynjCfSu/07t9PQ/Nxe0LJI7y2hm333YbPt+zB+jt+jRbaOUkvjGWs3+/3dZ1/Xl8xe2yF0j3tv7cFnvfJbVUzXEQ/AXgsDWpSKpHzF/2QO+Ys1fNAhb+wl4+uUsKhroSFIWVbcpxcD45w/yFEjH4G8i+1GgAIWj+zIYNinmeMGXyZLkOLCoqUtSB9utYF2+++kEwXd/6g06nw1tvvYVx48bh3nvvxdmzZ/Gzn/0Mjz76KN577z00NDTgkUcewV133SV+1OuGDBmCjIwM1NTUiLMUYmNjFa1429raUFdXp1jGGmn9HMuXiIiIiIj8ndpuADgdb35jNnDzOnR/uL1nemw2cPNcZbD30jaM/QPw7qZVlt1DW2H/O8nfic8uA5U45q95d9D9GQT2agD4axPmI//yabx7+FMAwGv7e7pdfHTuCmFJ3zIYDOjq6gK6u61OXV1dMBgM4sfc5+LzR08Ff73BF0Fgb5KCvVLw92d9GM/PHebBjoz0dCxbuhR//stfFMtItrz/PtRqdZ8CEa9t3iyPlyh1IfzWm2/K860FhqSWytOnTXPpQb55qxgIrb+uB7l7WlxdX+Z6C6zcvNze7fudPN/a9l3XbdH6UuLrsUidzWtHpC5Qt7z/PrRardySzpmXBmxxdHxtrdsTrfn80dVr1zBMeOHEvOWfowf8zlq7bh2mT5umKBP21NTUQG3nRRi1Wq3Ytoz0dKutfcUxZ69evWqxv+bE9TrL0Xr7S3lFBT7cuhVbP/gAH27dKtcNtuoK83limXdFX/PNnK3tsFaXivthrc6zVY5trcMVn+/Zg2fXr7cImH9/9Wo5YOuJ7zHvBvp4YaGiRbe7dawz1yVPcf36NrBJwd+hQ4fi8ccfx9y5c/H000/LLWxfe+01PP744x4f9xe94+9++OGHiq6e29rasG/fPnnM3cjISCxZsgR/+9vfcPLkScVnd+zYAQAYNGgQOjs7sd/shZ+PP/4Yp3pbtNsjrT8nJwcas+v02bNnUVlZqViWiIiIiIjIl6aOGCUmXTdqAe7CJ5j//XsRYjY9emw2nvmW0BDg8CaE/HMEvnIiCHzTiBvEJPJbygDZSy++6NFGIL4iBn8lvggCezUAvOA/1+D2956Q/3/38KeY8eZqOSDsL0JDQzFq5EjMmDHD6jRq5EiEhno1qxzy5+CvJBiDwA+sXu314G95RYXFWJ7SGMDSw+znNm7E8cJCi26ht7z/Pj7culXRraszcvPy5C5QpUpIDC5IgRLzz5gHHsTAkSO7du9WfP6N3/4W31+9GjALckstxKwtIz6ML68oV2yfNRnp6Zg+bRqeNTuGO3buxPHCQsVy/c1RXrti+rRp+HzPHkXXp9J+i/kpljNzzh5fZ46Vr3ny+H6+Zw9uv+02+f/p06ZBs2+f/P/Wbdvkv/tK6i73u2Zdz4vMz/3y3q7qzcdXFU2ZPNlivNU777gDr23eLP8v1TPmNyLFp05ZdNduztp6neFovf3l2Y0b5XF1v796NX7bGyCUyrV5XVFeUYEdO3f26XwS9TXfzDlz7jlb59krx/byQiKuz5wUfJ1sZYyaW7Oz5YCtu98jWbZ0Kd747W8VdaD9Ovb6jwt7689Iz3CY357Sl+vbfSu/gy3v/zfQ+7mFixfJn39l069x38rvCJ8IDmLw1xfOnDmDJ598Uh7b98knn0RycjLWrl2LyMhIAMCUKVPwxBNPKMYBfuGFFzB9+nSgt9voJ554AgUFBfL8tLQ0p8YARu/6X3jhBezYsUP+/J/+9CcMGjRIXJSIiIiIiMhnlt1o+1nQI/d+E8g/iENC+nvbPwFmLLAM9B7ehPn5c/CVg+6gl944RUwiH6utqxWTZKYmU+9fIbg1+1abQ3UFClvBX0l/B4E9HtUcGne9KzNnhDS2IbK+HdEVJqtTUBDH9nWx/AZC8FcSbEHgNQ8+KCZ5XEZ6Onbt3q0YW/LzPXuQI3QDm7N/vzxGqzRJD4ilh8e2HC8sVHzumQ0bkLN/P54ze/AuBUSe2bABCxcvxrMbN1p0QSnNW7h4MaZPm2a1ErPl+6tX489/+Yvi8+b5+1xvYEYa/3Dh4kW48447sObBh4Deh/HXt2+R1e27rlv+S2oBJn3vyeJijz+8d5Uzee2s22+7DVqt1qL757fefBPTp01THPcpVgIy5pw9vteP1fV19xwr758vjty9fLl8nrgSoBPZyoen1q1TnK9SC3p3SC0xxTFmFy5erAjKy9/5wAN4dv16u/l99/LlqNZqFa0r1zz4oOK4fb5nj0W3wx9u3aoYt1Vkbb3OcLReTxLru4W941pLQXQp39Y8+CCOFxbK5eS5jRsV58zqBx6Qg5h9OZ/M9TXfRM6ce87UeY7Ksb28cHSO/fkvf8H0adOsvrEpBailHi3c+R5J9pIlFnWgM3Xs3cvv7l3/Iryy6deKeZLnNv7U7nXJU1y7vg1c/hD8jY+Px6ZNmyzG9V1l5VowZcoUxTK//e1vMWLECHn+iBEj8Nvf/laen52djVWrVikCyeL/5sTPb9q0CfHx8QCA7Oxsq59btWqV1W0lIiIiIiLyhhk3ZCI1PkFMBgC897t7MfZ/rTwnubQNYzduwyFUYN3GTfL4wABw6H+fQMj3lWnmUuMTMOOGTDGZfGTO7DkYM3o07lmxQvFsxXz6+yf/i298/RviRwPSyeJiu8FfiXkQ+KTQW6OnhWgvV16PlHhAlUGHY1dLAQC5p47h48/+IS5yXVsXuq41IWb0YITFWT7YAIDCX38iJrkl5/BhJCaq5IBZSEgIzpWWYvy4cTa709RqtTh77hzGjR2L7u6e7Kqvr0dNTQ0WzrV4F0XJhUCvNYEU/DUXqNvtKo+ePH0ktQIG4LBy8X9unjB+cUSI/MOOnTtxsrhY8aKHPVKLYHuBZXhxvcHO1XwjT3L32jIQePb6KQ2f0hUS4pGumP0h+EtEROQN58+fR2h3NxISEnze8xwREfkHf/4F25dfjv95YC9++fk/xWSveP7Ob+DxRbeLydQvbJdccXgtc0OHDkVGeoaY3KsvJc63ThYXO91oxJVl+8rjAWBz/zz8BX7636+JyQrhiTEIjQwXk2WeDgBfrqzExcrLSEpKQmpqqncDwLbLvFMCPYga6NvvDK+dPAOWOydN347GwsWLxSQAwOuvvhp049nSwPPKpk0WY6Fa4+xyEmeXd3a5gYL54SvuXFsGir5dQ23xZACYwV8iIgpmDAATEZHIn3/B9uWXY2tHB+a98XNUNdaLszwqLTEJh37yH4gKtx1rIm/ydsntS+kjrwaAvzh5GOv/fH28wb7wdAAYZkFglUqFqKgo1Oh0GDliBGJjY8VFAQAmkwmXKysxODVVDgC3tbWhsbHRawHgYAmeBst+2OK1k2fAcuOk4dEgIiIL7lxXBhLPXkM9GQD+8ssvUVJSwuAvEREFJQaAiYhI5M+/Yvv6y/Hfpwqx5qMtYrJHbbl/De6aNE1Mpn7ji5Lb1xI5cIStf/rpl8RET4mLisHeU7loaunbWL7zx03DXdMXicluS1SpEIIQXL1WgyaTCSEhITA1NaG+vt7qZDQa0dXdjaamJpiammAymdDa2oqQkBCMGjFSXH1PWXezvF+rqUFdfT3mzZ0b0EHTyMhIqNVqVFVXIz4+HiqVSlyEyExfThxW9EREJN18iRP5Qnd3N9ra2tAdEoLk5GRxtksyMzMxa9YsMZmIiCgo1NXVIQRAVFQUQkJ470JERMH5S3bcEDU6OjuRV3FBnOURP158Jx6c6/k4ErkiGEtu4PNqC+ABieV8QOHJ42munkA8AkRE5Oq1gyx59nrqyRbAREREwYwtgImISOTPv3Dd+eXY3d2NH/7tA/yzqECc5ZZvTM3C77/zAF+k8jlf5L87JXJg4N2lJ/mijBMNWKzgiYiIiIiIiIiIiPxdSEgIfv+dB/DjxXeKs/rsx4vvZPB3QGMPcI4wAExEREREREREREREREReExISgo133I0t969BWmKSONtpaYlJ2HL/Gmy8424Gf6kXy4E17ALaE1i2BiyePJ7mzMnEXCciInPOXDvIPs9eW9kFNBERkXPYBTQREYn8+ReuJ385tnZ0YMtX+/CHrzTQGQ3ibKtS4xPw2PxsrJm/BFHh4eJs8il/KLmeLKHBgQFgd/lDuSaf4cnjaY5OKOY4ERGJHF07yDHPXl8ZACYiInIOA8BERCTy51+4nv3l2KOruxv5F8uw60wRiiovQWtoxFVDIwBgaEIi1AmJmDpiFJbdOBUzbshEKFv8+il/OC7eKKGBjQFgd/hDmSaf4snjafZOKuY2ERFZY+/aQc7x7DVWCgCHRUZi5MiRfKBNRERkQ1lZGdDZyQAwERHJ/PkXrmd/OVJw8beSy9IKjgFMRERERIHL335gkCQ0NBSRkZEwGo3iLCIiIgLQ1NSEyMhIBn6JiIiIyCt4l0lEfq6bb+wQEZEghMFfPxYSEoKwsDBERESgvr5enE1ERDTgdXV1oaGhAVGRkQgLC0MIu7MkIiIiIg9jAJiI/BgDv0REJOIDUn8XEhKC8PBwNNTWIj4+HpcvX4ZerxcXIyIiGnC6urrQ3NyMK1euIDIyEvqGBoSHhzMATEREREQexzGA3cH78wGPJ4+nmZ9UzF0iIrKGN2Ce5/lrbmdnJ1paW9Hc3IyU1FS0tLaira0NXV1d4qJEREQDhjREQkR4OBrq6xETHY3o6GiEhYWJixIR0QDlz794Pf/LkYKHv5VcllYwAOwmfyvT1O948ngaA8BERGQPb768w/PX3G4AnR0daGtrQ3NzM1paWtDZ2Ymu7m6g2/PfRwMR6wPqYb1GsZ7af1g++8f143w9x/0470NCEBoSgrCwUERHRyMmJgaRkZEICw/3560mIqJ+5s/XBF/fYZE/88eSyxLLALAr/LEMk0/x5CEiIuoPvAnzLu/c0XR3d6O7uxudnZ1ob29HV1cXuhn8JY9hvUD2ai/bc/oHy2f/6TnWPTnu//keEhKC0NAQREREyGP/svtnIiIy589XBV/fYZE/88eSyxLLALAr/LEMk0/x5CEiIvI23oB5n3fvaKRAsPQ3kWewbiB7tZftOf2D5bO/BUqO9wR7uxn4JSIim/z56uDrOyzyZ/5YclliGQB2lj+WX/I5njxERETexpsw7+MdDQUi1g1kq/ayntr/WEb7U2Dltr+UUSIi8kf+fE3jFYxs8+eSiwFbekPFBCJyzsCsMoiIiIiIiPxNt9nkL/xxm4IXc5mIiIjIl3jf648YACbqA1ZlREREREREREREREREEkZO/AkDwEQuYhVGRERERERE5F8Cp92Jv3eRSEREROSOwLgjGwgYACZyAasuIiIiIiIicg1/SfanwMhtBoGJiIiIyLsYAHYkhPfl1CMwfkQSERERuYJ3OEQUmAKv9pLapwbelgeiwMhlPnAiIiJLgXENIwo0A/OeiwFgewZmmSAreOElIiKi4MM7HCIKTKy9iIiIKJjxtTEi8gQGgG1h8Jd68UJLREREwYd3OEQUmCxrL8sUIgTUg3M+gCIiItsC41pGRP6IAWAiO3iBJSIiouDDOxwiCkyWtZdlCpEoMEoJg8BERERE3iUNvzFw7rsYABYNrONPRERERANKYDwGJyISKWuvwGnbSf4hMEoLH0gREZF1gXEdIzLn7/frA+OeiwFgcwPjmBMRERHRgOTPP76IiGxj7UVEREQDnb+H04isY6n1pRDt5UoeATD4S9bx5CAiIvI13qR5Bu9qKNiwbhgoLGsvy5TAw/LrS4GR+8FQzomIyFt8dS3j1Yls2Vt+FG8e+V9c1l9De2eHOJucFBEahpGJQ/H0rPtwa8YMcbbLGACW+KrWJL/Gk4OIiMjXeJPmPt7RUDBi3TAQWNZelimBi2XYlwIj94OpvBMRkSf56jrGKxNZs1HzLv557qCYTG66e+w8vHbrD8Vkl7ALaA6xQjbwgkZERESBj3c0RBSYlLVXt0VK4JP2Kdj2KzAERq7zgRUREVkXGNcxGgh2Xchl8NdLdpQewmfnc8VklwzsADDvo8kGXkSJiIgo8PGOhogCE2svIiIiIvv4Ghn5g//K/4eYRB70+wL38nfgBoAZ/CUbeOEkIiKiwMc7GiIKTJa1l2UKkScEzoNzPsAiIiLbAuNaRsHqkv6amEQedFF/VUxyycANABNZwQsmERERBT7e0RBRYLKsvSxTgtNA2U//FBi5zyAwERER+Z+2znYxiTyovbNDTHLJwAsAcwgVsiEwfvQRERER2cM7GiIKTMraK3DaZnqOtM8Dbb/9Q2DkOh9oERGRdYFxHSOi/jawAsC8TyYbeJEkIiKiwMc7GiIKTKy9iIiIiNzD18go0Dw6d4WYRB42cALADP5SL/P3qnlhJCIiouDAOxoiCkyWtZdlClF/CJznA3zARUREtgXGtYwI+NaUbOx95B0x2S3567Yif91WMXnA8rsA8O/eeRsPrHlI/v/Jp9bhyafWKZYh6iteAIlsW7tuHdauY31LwFtvv40fPHT9WjwQDMR9dgbrhUDBOxwiCkyWtZdlysDEfPClwMh9BoGJiIgo8M0YOdGlIPBry9cif91W1L+sQf3LGlS9uAt/vv+X4mLUq98DwFvefx8Lliy2mKQgr7GpSfyI66RhUcynfrTl/fexYPFibHn/fXEWAGDB4sVYsHixmBz0pHzxFWs/4sorKrB23Trk5uWJs7xqy/vvY+HixYrpueef7/ftcETazkDiT8d04eLFfho4EStIsaIU061NtojLeW+yluf3rVyJVzZt6j3+lp/pmWzzVflxhrX9/cFDD+FLjUZc1G0euRb72CubNuG+lSvFZNnJ4mIsXLxYPtbBsM+O6uyFdu5NKJBZu8MhGghY9gOd9SMo3rcN5Il8yXr59DcsK0REZF1gXMdoIHpt+Vo5eDtj5ET8Me8fSIpVORUE/vP9v8Sqm5ehsvEaNn72DjZ+9g52nP4/DI4bJC5Kvfo9ACzZvOlVxfTIQ2sAAD/bsBEfbPlvcXHn8N6XbLB10bt69SqOFxaKyf3m9VdfxeuvvoqXXnwRRqMRz2zYgJPFxeJi5AJ/OabS9PCanrrNt7zxMElcpyfX7Rrz/F5xz73QarV4ZsMGbHnf1rXE9vb6uvw4w7zeGDZsGF76xS88HgR+buNG/Om/beVfYJg9axa0Wq3NYP6OnTuhVqsxZ/ZsIEj2OXjZuooPRN1WJqKBjOdBoOJRIyIiIvIu8Zcj75zJ1+pf1iB7zAwkvZAtT8/ufAsz3lztVBB48egs7L9QgHv+tB7vHv4U7x7+FI/+769x+3tPiItSL58FgOfMnq2YpkyeLC5C1CfiRc2fL2xS+b81Oxtvvfkm1Go1duzcKS5GAcS9uk0Mpnpq8g5/Oc/mzJ4jT99duRJvvfk7fH/1any4dSty83LFxQOeeb3xyi9/iTGjR3s8ABwMbs3OhlqthmbfPnEWAODgwYNYOH++mEzkp3xd0xL5O/GuxNmJvE3MceY8BZLAKa/e+81HRETBJzCubRRsLvz0H9j42TuY8eZqcRYAQHM+HzNGTsTcG6aIs2QxEVEwtDrXg99zt/4AF376D9S/rMGFn/4Dz936A8X8FVOW4ODjW1D14i55mdeWr1UsI40n/NrytfJykkfnrsCpZ/7m991Q+ywAbIszY/7m5uXhgTUPYcGSxVh29/Kg6c4wNy8PP33+ebmL6G+tXGmxb0+uW4cFixfjS41GXnbZ8uX4V2/Q8Hdvv41ly5djweLF+Onzz6O2rk7x+dy8PDzw0EPyd/z0+ed92uL0yXXr8OS6dfhSo8G3Vq6U91sMZpRXVCjy5oGHHkJ5RYU833y/vrbcskxIYxju2LkTX1u+XO6a95kNGwAAz2zYoOgK1FeGqdXQarVAb/ekzz3/vLy9961caTU4/KVGgx889BAW9u77jp07sXbdOos8yM3LUywnzu8LR9v43PPPWx1TUzoOUvnMzcvDc88/b7dbW1v7ZH7c/PGYmnNuP3+Mtet+jB07d+Bry+/CwsWLLNLvW/kdLFy8CGvX/Ri1dbX4UqOR0+5b+R2Lc3rtuh9btIbNzcvFwsWL7AZIe47vz+TtuG/ld7Bj5w7A7GaxvKIczz3/M9yyeBEWLl6EHzz0IMoryhXr8YU1Dz6E6dOm4V87erYXNvfnenm1V34clXVfmj5tGoxGoyLN3vlu67x86+235S6TrY376mid4vJ/+etfsXDxYsV1aMfOnVhop4tiT1s4fz4OHjwoJuNLjQYGoxF33323nBYs++wqe/tojZRPJ4uLXfqc+wbyT9SBvO9EFKgCJ3BG5FhglGUGgYmIiMh/mAdL/3z/L5F3qRjvHv5UsYzkteVr8c0pPS2CD188Kc6WHSg7hrsn3mIRqBUlxahw/81L8dr+rdj42Tuob9bjifnfxshBQ+Vl7hw/B5catPj53j9i42fv4IvSPDw8+x6LAHRSjArT08Zh9lsPIOmFbKA3+Lvpa0/gRFUpNn72Dt756mMsHp3ldBDY2vbPvWEKHp27Qkx2m98FgB3JzcvD+o0bsGDefGze9CrWP/00Ptn+aT88ePSuLzUarN+wAYWFhVi2dCnu++Y3AQAfbN2K3739trg4Nv/mN4iPj8eypUthMBrx2ubN+Onzz+N4YSG+uWIF1Go1cg4exB/ee0/+jPQdCQkJeGD1atz3zW+isLAQz27caBEo7k/VWi3+56OPsP6pp7D51VcxTK3G5t/8RrFNz2zcCADY/OqrPcsMG4arV68CUpnYsAHz58/H66++ip88/TQ+/dSyTFRrtThZXIz/2boVOfv34+E1a/Cjxx4DAPzoscfw+quvYuzYsYrP9DeDwQC1Wg0AKC4uRmZmJl584YXerm3vwWubNysC319qNHjpF7+Q9/3FF17Ap9u34/z582Zr7cmjZ5zII1c52sZbs7Nx/sIFxTYDwOHcXCxYsAApycnytqmHDpW7tp0/f36furX1x2Mqcbyf13+wK8vqATn9/PnzOFlcjJ889RReevE/cP78efz8F7/AH957F4898ihef/VVxMfF4Re/fFn+jDssj++9vcf3eoB3Q++5+dqrr+I14dz0talTpyLHLPhne38qAITg4TUP40eP/RCwUn4sP2t5PvpKzldfYerUqfL/js73uXPmWD0vc776CnfecYciTeLMOsWusw/n9rxcUGiWfrK4GAsXLDBbyruWLFkCg9FoUZfkHTmCMaNHIyM9XZFuLlD32RWO9tGWaq0Wf9yyBavuvx+vv/oq/t+qVfhw61aHn6O+CIxHzkSBTmydysn9iSjYBEa59m4PUEREFDwC47pGwWL2qMl4+2BPa1lxyl+3Fd+cko3Rv75H/JiFe/60Hkcun8LDs++x2mJXkhyrwtI/rpW7iX5y++uIiYjC/8v6mrzMo//7a3zvo+cVXUkDwAMzl5utqWddD378Mi43XH/e/ezi1ci/fFr+/Ctf/gk7Tv8fFo/OUnzWmrk3TJG33zztszW/w7OLrbeOdofPAsALlixWTM620tv8299i2dKlWPPQg5gzp6cLzP+3ahU+2W797QFf+mDrVrnFqvlkzebf/AYA8NqmTfjZxo348ZNP4t3/+i8kxMfj7598YvGgfumdd+JnGzfiZxs3YtnSpUDvA+c3Xn8dax58EOufegoAFA+nf//eexgzejTefvNNrHnwQfz4ySfxzRUrYDAa8fmePfJy/U2r1eKN11+XuzV9et06GIxGxQN0rVaLb9x9t7zMr3/5SzkwI5eJBx+Uu0X9f6tW4dNPlWVCq9Xi0UceQUpyMgBgyuTJyMjIAABkZGRgzuzZ8rz+Vl5RgVc2bcL5Cxdw9/KeSua7K1fK+zRn9mx8t7dlXm5vgAEAtn30kWLf58yejc2vvy7Pl7zhZB65ytE23pqdjYT4eMU2l1dUIOfgQWQvWQL0btvCBQuw9skn5fWsefBBLFu6VPECgzP84ZhKrXulSarbXNnP62U1RZEOAI8+8gjmzJ6DW7OzsfTOpTheWIjHHnkUt2ZnY87sOVh1/ypoewPI7vruypV46MGHMHv2HMyePQcre4/v4dzr9bVWq8XX775b7oL5V7/8FcaMHesXDwEnT5qk+L+nvD6k6C4aAHJ796en/PQEBHvKzxy5/Dgq6/0pNy8PuXl5+FKjwdp16xAfF4d777l+k+TofL97+XKL8/JkcTG0Wi1uze55k03kaJ2Te7s6lwKttXV1OF5YiIULFuDUqVPyeo4XFrrYLbp7pkyeDLVajbwjR+S02ro6HDx4ECvuvVexrChQ9xlW6iFpEjnaR1u0Wi2eWreut97pOR++v3q1w8+RPWKt6cvak2gguB4k4ZlGRO7htZuIiAITr1zUH+beMAXJsSps+97LirF/k17IRv7l00iKUTkV/JXc86f1+NqWH6OsthIPz74H+eu2Klr2AsCF2kpFwFZqVTxZPdpsqZ6WuP/4wWbkr9uKqhd3AQASouIUy4jrGjloKJJjVfjfk8rGJseunEVMRJRFC2LR4Ysn5ZbEF376Dzn4m3/5tEv54CyfBYA3b3pVMTnTSq+2rg7aq1rc2hs4kmRmZMBgNFoESX1NrVZj+rRpFpMoNy8PBqMR06dNUzwkTklOxtI77wR6H86bmz1rlvz30CFDAEBuUYneMSLR+5AWvd+h1Wpx/sIFRTD6g61bAQAmk0leX3+bPm2aIkgntcgyP55qtRp/eO89xYsCKcnJPWVCq5WDiZIMK2VC/B5/ID2UX/3AAzheWIiXXnxRUQZ27NyJt95+G2vXrcPXegPDTb3HqrauDucvXLDY95TkZIwZM0b+35U86gt724jecrln7175/9zcXKjVasyZPVvetq+bdcMqyV6yBFqt1qet0/tCat0rTWPHjhX2Uzk+7/X9rJXX0VNWLYO/Y8aMUaTHxsUCvYF2SVxvWlOTskvgvugGsGPnDrz19tv48bof42vL7wIAmEzXx1pQq9V49733FF1JW9t2X9xQNjVZ1mvS/qw1258ms/2xx1FZ7y/PbNiAZzZswEu/+AXUajX+9N//Lddtzp7v4nm5b98+TJ82zWqLWGfWmZGejjGjR8uBz8LCQkyfNg1z58xBzldfAb11ularxZw5cxTr8bYV99yj6Ab60KFDMBiNmDdvnmI5c4G+z2I9JE3mnNlHW6yVlcmTJjn8HNniixqSaCC73jqOZx8RucLyQbm/1iJsBUxERM7z16sZBYepaWOxq+SQ1eBmTVMDRv+6J4jrSvfHhy+exO3vPYGHPn4ZMRFR2P6AZYM4R/Y+8g5W3bwMAPDpyX34+d4/iotY9bUb5wMANn3tCUVL5k1fewLo3V9nSPkhBX9vf6/n857mswCw1IpKmpwJzJWeLwUArN+wQRHEXN87ZqO/dDsqWXrHHXj7zTctJlfExfW8cXDt2jVxlgUpEGzPmNGj5W6UzSdbrb78xeubNmHs2LFYv2GDYozgc6U9ZUIar1OapHE8/a1MiKSH8v/1zjv4+1//qjgOr2zahN//4Q8AgG98/et48YUXzD4JlPbuuyPSct7II0fbiN7Whubdze7Zu1fuZtaZfXBmGX9irW5zZh+cWaY/dQP49aZfmx3fb1g9vq9u2oRxY8fi2Q0b8O2V34HGTrfd/X1DWV5RLnepDgCvOLE/tjhT1vtLzv79yNm/Hz967DHs2r1b8WKMs+f77FmzFOdlzldf4fbbbpPXY87ZdU6fNk3udSLvyBHMnTMH8+bNg1arRXlFBYqLi6FWqy0Ch942Z84cGIxGeczmw7m5WGj2wpQ1Ab/PQj0kTeac3UdX9fVzRET943qr3/6+LyGi4CHVIf5dlzAITERERL737uFP8b2PnheTAcBmurM+PbkPHx3bjdEpI7BiirKBgz0rpizBjJET8c5XH+OeP63HK1/+yeb4xKKiqp7naR+f2IuNn71jMX12pqdRiDNG//oe7Co55LXgL3wZAO6LoUN7mnL/6LHHLAKYm/1orE9PamrqaZnmyYfH4gPhObNne3T93pCRno6fbdyI//ngA0yfNg3/8Ytf4HBenqJMiC2dpNaX/kzKf7F70JPFxdi1ezd+8vTTWPvkk3I3m+aklwMc8VYeObONMOuCNTc3F+UVFTh/4YIc6Ja2zZ6+bp8/CcT9LO49vuuf/gnWPvkksnu7mBZlpGfgpxt/ig97z82XfvFzRWtgX/p8zx4snN8z9ur18tqzP1KX2Y6FOF3W+9t3V67EwgUL8MZvfyu3lHf2fL81O1s+L7/UaNBkp0Wss+uc1RtUlrpYnjx5ck+PBKNHo7i4uGcs3Pk9b8n1p4z0dEyfNg2Hc3NRW1eHnIMHHb70FOj77Axn99FZ0v2Kq58j/31sTERERM7x31bBHBOYiIic409XL6K+qNbrxCSbBscnAQD2nc+X05wNIB++eBJ1Jj0SouLk8YPNJ/Puop3hbhDckcAJAIf0PMRVq9UwmUwWAcw5TrYi9kdzZs9GQnw8jhcWKrp6rq2rw+7PPwcATLPSdbQrxo4di4T4eJy/cMFivOVfbdqk+N/fmHcBLAWCAaD41Cm5TDQFWZmQHqRnZmbKaWI34FMmT0ZCfDyOmI1tid4uR83HfvZWHjmzjZIV99yDPXv3Ire35Z30woG0bZp9+8SPQLNvH8aMHq3Yvq96u1WV1NTUKP73VxnpGU7sp2W3yZ7kSt51AzD2diGdkdkzpjJ6g8LmzLutlgLBABTjn4r66y35Vzb9Gk1GI+6//3uAWZfYmWb7Y6u8ilwp6/3tJ08/jSajER999BHg4vm+cP587Nm7F3lHjiiGEBA5u845vdey7f/4B+Li4+UXW6ZPm4aTxcU4XliIScK4zP3l9ttuQ87Bg9j+j38gIT7eYQA4GPbZEWf30Zrz589bdM+fd+SIRZ1N9vRXbUhEPTjmLxF5g60u5f2/fTAREZGIVy7yd/nrtuLP9/8Sj85dgUfnrsBry9fiifnfxoXaSnmcX2d8duYrNLe34hd3PopH567Ac7f+AM/d+gNxMZs+OanBsgnzLLZl7yPviIv6XOAEgHutXrUKH2zdii3vv4/cvDzk5uXhXzt3+n0Q05EfPvYYAODZjRvxq02b8Lu338ajP/oRDEYjnl2/3u0HqinJyfjmip5+1H/+8sv43dtvY8v77+PJdeuwa/ducXG/Ulpaip8+/7x8vP/8178CveMNordMfCiUiR07d+IVJ8qE1FLpyJEjfhPQgVnA/i9//Sty8/LwpUaDP27ZIi6GFStW4O+ffKJY7hcvv6zo9hZu5hF6x5A2n04WFzu9jejtgvX8hQvYs3cv5gpjYT72yCPYtXs33nr7bXn9W95/H7t278ajjzwiL3f7bbfh/IUL8vft2LkTW7dtU6wLfndMrz9sfOyRR832Mxe5ebnY8v5/W+ynNyjzLhc7du6wmnfmxo4di/j4ePy19zMajQZ/3KIcC6G0tBTPPf8zeX/+0ntuOhPw8uQNpfT9Up7et/I7OHjwIF7d9KocWFeW155Wr+L+SMsBwJEjR+Xy40pZ728pycn4f6tW4e+ffCJvr7Pn+5IlS3D+wgWUlpZajAMrcnad06ZNw6effqpo9Tpr1iwcLyyEVqt1GHj1Fql186effooFC3pahTsS6PvsDGf30Zr1zzxjUWevuv9+cTGyypM1IBE5ZitAQ0TkCYHwgglbARMRkfP893pGBCwenYVNX3sCm772BO66cT72XyjAvR88Iy5m1+WGq3jnq4+RmTICm772BB6a9Q288uWfxMVsenbnW3h9//9g9qjJ8rbMu2Eq9l0oEBf1Of8OAFu5R/368uX4+YsvYveePVi/YQPWb9iAw7m5mDNrlrhoQJH2a+jQodi1ezf+/skniI+Lw89ffBFfX75cXLxP1jz4IH702GOIi4/H3z/5BB9s3QoA+PmLL4qL+hWpm0rpeO/Zuxcvvfgi5vR2wXr38uV46cUX8fmePXhmwwY801smZjtRJlKSk/Hs+vXY/fnn+NETT/hBwLBHSnIyfvL00zheWIhnNmzAH957Dw+vWSMuhjUPPojvr16N/9m2Dc9s2IBtH32ERx95BMOEALA7eYTeMSLNpz9u2eL0NqK3pdnCBQtw9epV3C2U51uzs/HSiy/K63lmwwaUlZXh9VdflY8xevfhvm9+U97XvV98gdWrVinWBT8+pj37+R84Xnjcyn460xVx3929/G7c981v4X+2/Y/NvBNv7lKSU7D+6Z/geGEhnt2wAX947108vOZhxTLSufnshg14dsMG7Nm7By+9+B9O74/4nX1lXja/+uor3HnHHfifrVsVXaunJKfgJ73701NeLfdHWq6n/OzGj554HCeLi6181nZZ94XvrlyJMaNH4ze//S3gwvkudc9ubGpSnGvWOLvOub3j7Zq/BDBn9mxotVosdDLw6g0pyclYuGABDEajRR1kS6DvszOc3UfRmDFjsOLee/HGb38rn3cvvfiiXwe7iWig4pi/RNRfGAQmIiIiMlf/ssapaXTKCPGjVs14czXSfrEMSS9kI+mFbEx6/Tv43kfPK7pdnvHmasx4c7XicwCQ9EK2orvlV778E0b/+h4kvZCN0b++B5+e3GexjK11Qfh80gvZWPCfa1wKIveXEO3lSt6fUkDw34Lqf+5buRJ33nEH1jz4oDjLZ9auWwe1Wo3nervwDn6BVYH56vwKrFyS+Cq3iHxv7bp1AIC33nxTnNUPArPGUGL9QdS//D0gQ0TB5Xptc/2uxR/vX1grEhGRY9auYLyCkOjGP/w/MYk87Mxj/yMmOc0/WwBf70GHCODFxSW5eXnQarUOW3D1J2lcYmdb3gW+wKnAfN0ixtff3zfSRSpwjjMR+Vpg1nZEgev6dZpnHhH1H/H3gfg/ERFR4OCvWKLA538BYN4fk4AXGtv+8te/Wozd+IuXX8b0adMU3d/6Sm1dHXLz8vCLl1/GwgUL/GKbvCuwgoL+dG7507YQEXkWazii/nX9XoxnHxH1v0B4WdSft42IiPwN76mJApd/BYB5D0oCXmDsy8jIwFdffSWP3bh12zasWLEC/+En4zpv/8c/8MyGDRg2bBh+8vTT4mzyIX88t/xxm4iIiCiQXG/1y/sKIiJ7+ACOiIiI3BcZFiEmkQdFhIWLSS7xrzGAef9JZvynYBI5K3AqMX89vwInB835a24SBZvArCFYRxD1p+sBYCIiXwucOxfWmkRERNQ3X//4pyitqxSTyUNuSFRj93dfF5Od5l8tgIl68ecH0cDEFjtERETkuuvdrfI+goiIiIiIqH/88OZviEnkQY/PuEdMcglbAHvY2n/9Bp+fyxOTA8Kd42bjra/7vpte/ymQRK4KnEosEM4z5iYRKQVOraDEOoLI+xj8JSL/FRh3MKxBiYiIqG9+svc/8dmFXDGZ3HR75ky8dcdaMdklDAB72PjN3xGTAsrZ9X8Tk/qV/xRGor4InEosUM61wMjRQMlNokAXGDWCJdYRRN7F4C8R+b/AuIthTUpERER982V5Pl7P/RsqDdfQ2dUlziYnhYWGYkTCEKyb9S0sHT1bnO0yBoA9jC2A3eM/hZHIVYFVgQXKuRYYuRoouUkU6AKjRlBi/UDkfQwAE1FgCJw7GdaoREREFKz8+Y7M8/dg/hEA9uc8p37l+8JI1BeBVYkF0nkWWDmLAMtdokATSDUC6wKi/sMAMBEFhsC5k2GNSkRERMHMX+/KPH8P5rEAcHd3N7q7+7Aqf81r8ok+lCAiHwq8CizQzjHmMBFdFyg1AusBov7FADARBZbAuKNhrUpERETBzB/vyHrvv0JCEBrime1zKwDc3d2Nzs5OdHV1yQHg7p4Z4qLWeWYfKIg4WXKI/ETgVWKBdo4xh4noukCpEVgPEPUvBoCJKPAExl0Na1YiIiIKVv55NxYSEtI7AaGhofLUV30KAHd1daGrqwsdnZ1ISk1BTGwswsPDEeKhqDQRERERERERERERERER0UDR3d2Njo4OmEwmNNTWIiwsrM+BYJcDwF1dXWhvb0f8oEQMSkrq05cSEREREREREREREREREZGlrq4uNNTXw9DYiIiICJfjsU4v3d3dja6uLrS1t2Nw2jAkp6S4/GVERERERERERERERERERGRbaGgoklNSMGTYMLS1t6Orq0tcxC6nI7jd3d1ob2/H0LRhiImJEWcTEREREREREREREREREZGHxMTEQD1sGNra2tDV1YXubuc6dnYqACz1OR2XmIhoBn+JiIiIiIiIiIiIiIiIiLwuOiYGCYMGobOzU5xlk8MAsNT1c3d3N5KSk8TZRERERERERERERERERETkJUlJSUBICDo7O+FMG2CnAsCdnZ1ITE7mmL9EXlBUVCQmERH5BOsjIqLgwTqdyDaeH0TBgecyBROWZyJyBusK1wVTnoWGhiJRagXc3e2wK2i7Ed3ubqAbQEdXF2LiYsXZRERERERERERERERERETkZTExMejo6HAY/IWjADDQ0/1zV0cHIiIixJlERERERERERERERH5j7969qKysFJNdVllZib1794rJREREPhMeEdETt+3qEmdZsBkAlqLH3V1d6OzqQkhIiLgIuaC8vFxMktmbR0RERERERERERETOu3jxIg4fPuzWdPHiRXG1REREPhUSEoKuri50O9EFdIj2cqXVJaQPtrW3w2RqwoTJk8VF/EJdXR20Wi06OzsRFRWFESNGIDbW/7qrLioqQnp6OlQqlSJdr9ejoqICU6dOVaTTwFFUVMTjT0R+gfUREVHwYJ1OZBvPD6LgwHOZbNm7dy9SU1MRGRkpznJJW1sbdDodbr/9dnGWx3mqPBcUFODSpUtislNGjRqFrKwsMZloQCooyEdZWRmuXbsmp2VkZGDMmLEYN26cYtn+5Km6wtyFCxdQW1srJvtESkoKRo8eLSa7xRt55munTxYjISEBYWGhCA212c7XfgC4u7sb7e3taGpqwo1Tp4iL+Ny5c+dQXl6OsLAwREREwGQyISwsDFOnToVarRYX9ymtVovS0lIsXLhQkZ6Tk4OxY8f63fZS/wnGCoiIAhPrIyKi4ME6ncg2nh9EwYHnMtly+PBhZGZmYujQoeIsl1y9ehVlZWWYO3euOMvjPFWey8vL8X//938AgMzMTHG2TZcvX8bIkSMtnl1T8KusrERcXBySkpLEWQPOuXPn8M9//gN79+5BU1MT4uPjkZFx/TwqLy+D0WjE0KFD8fWvfwNf+9pdGDJkiGId3uapusLckSNHcOXKFSQkJIiz+pXBYMDw4cMxa9YscZZbvJFnvnaq6KQcAA4LCxNnyxwGgNva2tBkMmGinwWAL126hOLiYqjVaowdOxYA0NLSgvPnz8NgMGDBggV+1xL4448/xtKlS+VWwHq9Hrt378a3v/1tcVEaQIKxAiKiwMT6iIgoeLBOJ7KN5wdRcOC5TMHEk+VZCgKr1Wrceeed4myrNBoNEhMT2QJ4gLl69SqKioowaNAgzJw5U5w9YFy7dg1///vH+POfP0JGRgaWL78bU6feJMedzB07VoAjR45Ao/kSJpMJ3/3u9/DAAz8QF/MaT9YVkiNHjkCv1+O2224TZ/WrL774AiqVigFgJ1wPAIchNCwUtgbwtd022JyDfqR9obq6GklJSYqTMDo6GpMnT0ZoaCgqKioUy/uDxMREnDhxQv7/xIkTSExMVCxDRERERO4pKioSk4iIiIiIiAaEjIwM3HLLLdBqtfj888/F2VZlZ2cz+DsAabVaREZGoqGhAfX19eLsAeHcuXN4+ul1+OKLvdi48af4058+xDe/+S2rwV8AuPnmLDz22A/x8cf/i+XL78Zf/vJnrF//E0VX0UTe5sz4v3C6BXBTEybe5NsI+fHjx9HU1CT/39jYiDFjxiAtLU2xHACcPXsWdXV1ihbAQ4YM8Wnf7ABQUlKCvLw83HvvvQCA7du3Y/bs2ZgwYYK4qNMqKipQVlamSMvOzlb8T/6tL2+gdHV1wWAwoKWlBS0tLeJsIkRGRiI2NhYqlQohIdbfAQrmcuTM/pOlvtRH5Bs8VvYxf4j6dh4E870BBae+3vP15fzoLwUFBVZfaDeZTGhqarI7xpc9XV1dGDx4sJgMg8GA6OhoREREiLOQnp4e0MEAW3lpTXt7O1paWpzu+tBevlnjq7x0JQ+8zRt54Mlz2ZVxU71dXjw5DqsrZcDb++XJMuDMfplMJoSGhiI6Olqc5ZSWlhZ0dXU57GHSU/vlyfIs6UtLYFccOnQIADBv3jxxllcVFRVBp9PJ/6tUKsyYMUOxDDlHo9Fg5MiRqKqqwtChQ92KUwSigoJ8PPfcT5GenoH/+I+XrN4rOXLsWAE2bfo14uPj8cYbv/V6l9DeqCvEFsCHDx9WxOIciYuLk7vKd+ezbAHsvOITRUhISEB4eHhvC2Dpt5Ay3OuXAeCSkhKLBw4VFRVISkpCXFycnKZWq622oK2qqoLBYJD/v3r1KsLCwizG2R00aBDS09MVad62fft2pKamAgB0Op0cDO4LaxdZ6ebHmf2qqKiATqfjBdLHXK2A2traUF9fj6ioKERERKCrqwtdXV3iYjSAhYb2DP7e3d2NxsZGpKamIioqSrFMMJcjZ/afrHO1PiLf4bGyj/lD5Pp5EMz3BhSc3Lnnc/X86E85OTkoLy/HsGHDFOmNjY3Q6XRWn4E40tHRAaPRiDFjxoizcOHCBQwePFgeqkpSXV2NjIyMgB4L0lZeWqPX61FTU4PRo0eLs6yylW/W+DIvbeVBS0sL9Hq9xx9SX7t2DSqVyiLg5q088OS5bCuvrAmk8jKQ96uyshKRkZF9LufXrl1DW1sbRowYIc6SeXK/PFmezXkrCKzVauVGSZmZmRbP3R3p63Pp/Px8AFB8zlt5F+ykhmXZ2dk4ceIEGhoasGjRInGxoHXt2jU8/fQ6DB2qxqZNr4qzXVJTU4PHH/8hRo8eg82b3xBne5Q3yrsYAP7iiy+A3pcrHNHr9QDgsc8yAOycgA4AHzhwADqdDpGRkXJaY2MjJkyYgPHjxyuWdcbBgweh1+sRHx8vp7W2tiIzMxPTpk1TLOttUitgAG61/i0qKoLRaHTrDau+XmjJs1ypgDo7O6HT6aBSqdDW1ibOJrIQGRmJxsZGDB48WB4QfiCVI2v7T7a5Uh+Rb/FY2cf8IXLtPBhI9wYUnFy953Pl/OhvOTk5qK6uxrJlyxTpFy9exNGjR3HzzTcr0p1x7do1VFVVYcWKFeIsHDhwAGPHjrXoXW3Xrl0YNmyYR4IavmIrL62pqqpCaWmp0w++beWbNb7MS1t54Or+OstWvngrDzx5LlvLq5CQEISGhqKzs1OxrKv5ZytfrPF0XlnbL1uCbb+OHTuGuLi4Pj1LRm8Pk01NTXbrXU/ulyfLs8gbQeCioiJERkbK946ubntfnksbDAYcPXoUM2fOdLqlOtl29OhRhIeHY/r06aivr0d+fj6mTp2KoUOHiosGpfXrfwKtthqvvba5Ty1/RceOFeDFF1/w+pjA3qgrrAWAnQ3E+uqzrvBGnvma7QAwFEHgvvUd1A9UKhXGjx8vT8nJyeIiTouNjcXgwYMxduxYeXL2zWBPmzBhAmJiYhATE9Pn4C96Ww9nZmaKyQoajUbRElqr1UKj0QC9b0uVlZVBr9dDo9GgiGPlBYSmpibExMTwwRw5ra2tDbGxsYquNwZSObK2/0RERKQ0kO4NKDjxno+IPC0kJATR0dGIjY1FeHi4OJsooPRlTGBHdDodhg8fjiFDhii6Y5b09bl0SUkJNBqNPJnPk4K+tbW1cprI3vei97tLSkqQn58vf4dWq4XBYFB8r7dZ68LcYDBAq9WKyV7R3NyMhoYGJCUlAQCSkpIQGxuLqqoqcdGgdODAARw+fAgPPrjGI8Ff9I4NLI0JzPGAybdC5MlvA8DBSq/Xo7m5Gc3NzXITd1dJFwJXu9YwN2PGDGRmZkKlUiE7Ozvo3oAIVs3NzS6NbUUEAGFhYTCZTPL/A60ciftPRERESgPt3oCCE+/5iMhTpOCvFPiNiYlhENgKsatv8m+eDAJXVFQgOjoaCQkJUKvViI6OthrQtMXWc+mioiJUVVUhOztbnoxGoyIInJaWhrKyMrcaM1VVVWHEiBHIzs5GWloaTp8+jZMnT8rfqVKp3Fq/IwaDAWVlZfLwjlLa0aNH5W61ve3ixYsICwtTDCOZkpKC+vp6xXLBaseOf+HWW2/1SOt9c4899kPExsbis8/+Lc4i8omACAAPGjQIkZGRqK+vx7Fjx1yeTCYToqOjFV1A+8qJEyegUqmgUqlw4sQJcbZTxPGRaeDgsae+6OrqQmtrq/z/QCtH4v676s9//jO2bNnS55d2Bprt27djy5Ytbk3bt28XV0t9ZO3t4ZKSEuzcuRM7d+5ESUmJOJucsH37duYdBZWBdm9Awcndez4iIgjB36tXr+Lw4cNobm5mEFgQHh6O2267zaWWc30Zw5z8k06nU/TWmZycbLUVsKt0Oh0mTpyoSMvMzIROp5Nb9U6YMAEzZ86ETqeDRqPp0++y1NRUuWHV8OHDgd7Asvl8o9Eo/+9pCQkJyM7OBgAcOnRIDv6mpqa6NdyjK2pra+XWv5KhQ4eis7PTajC/oKAAn3zyicemgoIC8Sv6zblz53D48CEsXtxzDDwtO/tW/Otf/xSTiXwiIALAMTExGDJkCJKSkhAXF+fyNHjwYKSkpPj8Rk2v16OsrAw33ngjbrzxRrmrCyJXdHV1iUlEdlkrM9bSgpU7+1pSUiK3JCktLRVny44fP253vrecOnUKzc3N8v9Xr171yXaYmzZtGhYsWODWNG3aNHG11EcajUbxdndRURHy8vIQGxuLiIgIHDx40O23v4koOLhzvSTyByzDRNa1trbi7NmziunSpUvQ6XQoLCz06KTT6XDp0iWL7wuklzPMg7+nTp1CdHQ0YmJixMUGtPDwcDlPkpOTnXreOm3aNPY+6GOeGgfYYDBAr9fLgVP0Nt7S6/WKrpddZavHS+l/82EepADqxIkTUVVVhfz8fLNPOBYZGSn/LXUr7YsW7VKwVwr+9tc5Ul9fD5PJhI6ODpw6dUqeqqqqEBYWhpqaGvEjMJlMaGpqkhu2uTM1NTX5tNeWEycKER8f7/HWv5JZs2bh6tWrOHfunDiLqN+FmnUHbX/ysYyMDMWYwK5O5m/x+IrU+nfChAmYMGECVH1sBZySkgLYaNVDRESec/HiRahUKqjValy4cEGcDfQGf+vr61FRUdGvwVdpvJZjx46hublZfkDhzbdUnZGRkSFf5/o6ZWRkiKulPpo7d66ii6+SkhLccsstyM7Oxp133olbb70VWq0WOTk54kep9yFJSUmJ3Rf2SkpKeE9GRERENsXExLjUStLTOjs70dTUZDG1trbiypUrHp1aW1stvqepqQkRERE+zQNnRERE4Oabb1YEf5OSkjB9+nSg9/dXR0eH+LEBRwr+mkwmnDx5EnCii+zIyEiMGzdO8RnqX54K/gLAlStXgN6gpTRe7unTpxXz+otarcbMmTOh1+sD9jfZvHnzkJaW1m/BXwC4dOkSwsLC0NHRAb1er5iioqLQ0NCgaGwgiY6Oxpw5c9yefBFsN1dRUYHJk6eIyR5z881ZiI+Px/nz/feMkAaibrNJ/P/6FBAtgIOBeetfSV9bASckJEClUqGyslKcZcH87Sh27UZE5DzpB8SoUaMwbNgwqz8opODvpEmTkJ6e7rUgsLUAU0xMDG6++WYAwLFjxyweUAxUUsDOnam8vFxcbcASx3mKjY1VBNgzMjIwefLkPt2PBLs///nPKCwsxJkzZ7B9+3aLctHQ0ICPP/4YZ86cweeffw6NRqOYT0RERANbSEgIIiIicPfdd2PChAni7H4TGxuLm2++WTGNGTMGUVFRmDhxokenqKgojBkzRv6erKwszJkzBytXrvRpHjhjzpw5GDNmDIO/DkRERABmv5elblxtBYEjIyMRFRUFk8mEgoICNDQ0+LTl30DkyeAvANTV1SEzM1MxTq80lm5dXZ1iWVeeS8fFxQFWGjzZahkskVrwmnPle/1Bf9ePDQ0NSElJwdy5cy0m6TnTxYsXxY8FjbKyMsXYx96QkZFp8QyByBdCtJWVUohYobu7G93d3Whra0NTUxMm9uNbKAcOHEBbWxtuuOEGAMCwYcPERfpEai2F3q48hw8f3m/dTObk5ECn0+Hee+9VpG/fvh2pqakudzkgjQ2gUqkwY8YMOV3qoz89PR35+fmIjIyU3yA6dOgQWlpa5DEGKioqUFZWJv9PvlFUVOT0W14XL17EoEGDxGQihxoaGuQ6dSCWI/P9d1ZBQQGOHz+O5cuXIzY2Fh9//LH8Iwe915TCwkJkZmZi6NChQO+1xWg0ejQIW1RUhCNHjkClUuHb3/62OBvNzc04duwYYmNj3f5eV+ojf7V9+3bU1taKyS5JSUmxuF77G1ePlfSjPyIiAt/73vfE2diyZQsWLFjQ7z88vcXV/LGmvLxcDpZrNBqYTCYsX74c6C1n7e3tWLp0KVQqFfR6PbZv347Zs2cHTR5S4HPlPBiI9wYUnJy953Pl/OhvOTk5OHr0KMaNG6dIv3r1KpqamhAa6vg9/u7ubotATFdXl1N5Izl37hxmzpzp8rMKf2IrL60xGAxobGxEbGysOMuqlpYWREREICwsTJwF9AYysrKykJ6eDr1ej8OHD6OqqgoxMTFYuXKluLjX5OTkoLq6GsuWLVOkX7x4Efn5+fKDfk85duwYZsyYgRtuuAEhISGIiYlBWFiY1/LA0+eyteDvv//9b4vfF52dnWhvb3e6FZvJZEJERIQcPLXHaDQiPDwccXFxCAsLczuvcnJycOrUKUVaa2sr2traFGnorTu6urpslmv0vtgwc+ZMLFq0CFqtFidPnkRycjKysrIAIVguBn8BICsry+nzzB5nzm+tVut24D48PNxm4BEeris9XZ7hheCvVqvF6dOnMXPmTIvAq/SseuLEiVCr1X16Ll1UVASdTqdIO3ToEJKTkzFhwgQYDAaUl5cr8qmkpARVVVXyZxx9b35+PuLj4xW/2zQajbzd6N22qqqqfhuPtz9JDRdmzJhhMQaw5Pjx4zCZTJg/f76cVlRUhNzcXEyaNMmtclpUVIRTp05hzpw5bq3HHT/84WOYOHEiHnvsh+Isj3nyyScwZcoUPP74E+Ist3mjrjhy5Aj0ej1uu+02AMAXX3wBlUqFWbNmiYta8NVnXeGNPPO14hMnkJCQgPDwcISGhdnsxDnoAsD2bsA7Ozvlt350Oh2SkpLk7pS9paKiAhcvXoTBYEBcXBzmzJkjj5PR3NyMgwcPwmAwICUlBTfccIPLb5/k5+crWuxER0fLFyfpwivJzMy0uLBKF8H+HGeAlFypgGw9nGuuPo3TVeZdcyQjMysD1i/jSvXlBaiOnoiJw3rKZX15Acrqrn9enO8scT3kW84FgJtRffo0WoZlIcPqQXM03385+zDQ3Pbt2wFADgR+/vnn0Gq1+P73vy8s6V07d+6EXq+Xg0/Wfnw2Nzd7ZFwqV+ojR0pKSnDw4EEx2a5gCkB6W1+Ola0f/3q9Hh9//LFcvvbu3av4HADcfvvtYpJf60v+WFNSUoKmpibodDqYTCa5Pti+fTuGDRuGOXPmyMtKLaztPfwRH0ZIioqKYDQaLR4wFBUVAYDF8t4i3lea471i4HHlPLB9b0AUWJy953Pl/OhvOTk5KC0tVTx0RW93jefPn0dycrIiXdTa2gqj0YhJkyaJs6zeR5aWliItLU1ueSX56quvMHbsWLvXNX9nKy+t0Wq1uHDhAkaNGiXOsurSpUsYPHiw1XvwqKgoTJ48GUlJSSgqKsKxY8cQERGBIUOGoKysDI8++qj4Ea/xVQB49OjRiI6ORkhIiFfzwJPnsrXgb0lJCaqrq8VFFbRaLSIjIzFo0CB0d1t9xAqDwYDo6Gg0NTWhra0NQ4YMEReR6fV6hIeHIzw8HPX19</t>
   </si>
   <si>
     <t>In Progress</t>
@@ -217,7 +214,37 @@
     <t>Should be done</t>
   </si>
   <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAB4AAAAQ4CAYAAADo08FDAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAP+6SURBVHhe7N19XM73/sDxl1RKkkrlrqQQQm5CwmSTYbk9G9aZdrYYu3HzczLOHGacHNs6DnNszNrObMewDVOTsU0mCZm5iaJaakIhlZQkvz+uq7qu73VVV6ko7+fj8X3Q9/P53l7fz/fu/f18Po1atWp1HyGEEEIIIYQQQgghhBBCCCGEEPWekXKEEEIIIYQQQgghhBBCCCGEEEKI+kkCwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRoICQALIYQQQgghhBBCCCGEEEIIIUQDIQFgIYQQQgghhBBCCCGEEEIIIYRoICQALIQQQgghhBBCCCGEEEIIIYQQDYQEgIUQQgghhBBCCCGEEEIIIYQQooFo1KpVq/vKkUIIIYQQonY1b94cKysrmjZtiqmpqTJZCCGEEEIIoVZYWMjt27fJzs4mJydHmSyEEEIIIRQkACyEEEIIUYfMzc1p3bo1xsbG3Lp1i8LCQgoLCykuLlZmFUIIIYQQ4rFnZGSEqakppqamNGvWjKKiIi5fvkx+fr4yqxBCCCGEUJMAsBBCCCFEHWnevDlOTk7cvHmTmzdvKpOFEEIIIYQQlWjRogUtWrQgNTVVagMLIYQQQpRD+gAWQgghhKgD5ubmtG/fnsuXL0vwVwghhBBCiGq6efMmly9fpn379pibmyuThRBCCCGEBICFEEIIIepG69atuXnzJnfu3FEmCSGEEEIIIargzp073Lx5k9atWyuThBBCCCGEBICFEEIIIWpf8+bNMTExISsrS5kkhBBCCCGEqIasrCxMTExo3ry5MkkIIYQQ4rH30ALAjT3HUjjjY4yfnkkjy5bKZCGEEEKIBsPKyors7GzlaCGEEEIIIcQDyMnJwcrKSjlaCCGEEOKx16hVq1b3lSNrnesArgyeAQV36DzcF4C8fZsojvyS+xnJytxCCCGEEPWam5sb165dk+afhRANQp8+ffDy8sLe3h5TU1Pu379PQUEBFy9eZN++fVy+fFk5iRBCCFErzMzMsLW1JSEhQZlUs1q64jPYhy4OJuoRWST/vJe9F1Qt/Fh3GsGIJ12wVqfevRpPZFQkSddK5yCEEKW6d+/OwIEDady4sTKpSu7du8fx48f59ddflUnV9ris2+HDhzlz5owySYgGpc4DwMXdniTD+2W4dw/u3KGzzzCt9PzjP1K0bTn3s9K1xgshhBBC1Fc9evTg4sWLFBcXK5OEEKLeaNasGc8++yydOnWioKCApKQkbt26BYC9vT3t2rXDyMiIw4cPExERoZxcCCGEqHFGRka0b9+e06dPK5NqhoU3M//xKn6dSkK72rKOhrKdiQT2Lyf9Qjgf/X090XnKFCHE42ro0KG88sorNdZ6QW5uLuvXr+fAgQPKpCp7lNetf//+vPHGG9jY2CiTqiU3N5e1a9cSHR2tTBKiwajTAPDdXmO53vc51R/3iuFOAZ19nlRm4/7RcHJD/085WgghhBCiXurRowe///67crQQQtQbzZo148UXX8TBwYEjR44QERGh81GLtbU1zz33HE5OThw9epRdu3ZppQshhBC1oUOHDrUUAPYkKHQpPg5lYwoLClX/MTLF1LRsvCqxkEL1pdHUTCPxaiRLA0OILRsjhKgj3t7ezJo1C0tLS2WS3uCkvvz379/n2LFjvP/+++Tn55eOr67FixczYMAA5WgtR44cYfny5crROvr06cOCBQs4c+aMQfkrs3jxYrp378677777wDV3H/a6VZS/ptdNiEdV3fQBbGTEHa8/c733s1B8XzXcVw3qf7QG+vkp5/BI+Otf/8qOHTuYNm1a6bjFixezdetW+vTpo5W3IejTpw9bt25l7dq1peP07YOGZNq0aezYsYNx48Ypk2pVz549+eKLL9iwYQNOTk7K5AatcePGrFy5km+++YZnnnlGmSyEqA+6eOLZUjnyEWRqhuZ7GCGEEIYbNmwY9vb27N+/n++//14n+AuQlZXFJ598wvnz5+nTpw8eHh7KLFUTsJItW0JZMESZYJgXVm5hy5YtbNmykheUiXXshZVb2LJxAYOUCUIIIR5ZFi9MwdsBoJC0Hz/g1cl+THx2omqYGMRezR4PLu8laKI67dmJ+E1+lQ9+TKMQwMGbKS9YaGQWQtSFrl278tprr3Ht2jXCw8N1hmvXrjF9+nS6du1aYf7IyEg8PDx49dVXlYsQQohH2oMHgBtX8ia1sQl5g6eT1fVp7fGlEV/0D3Vs7dq1OheBkmHx4sUANGnSRDnZI23atGk621IyfPrpp9UKND5q+6Bx48ZMmTKFjRs3snPnztLt27VrF2+++aYy+yPLzMyMRo0aKUfXOw4ODmzcuJFt27YxePBgZXIpV1dXPv/8cz7//HPc3d0fuN+GR91TTz3FmjVr+Pbbb0uP0R07dvDxxx8zceLER3b79Z1Ddu3axf/+9z9mzpz5yK63qGMt/Vi6aClLQ5YyorUy8RFi6siAEeMYN2IAjpXcugghhNDWpk0b3N3dSU1NrbT5tuLiYiIjI7lz5w59+/ZVJteZF1Zuwc/2BGunTGHKlIV8qcwghBBCVMKvlwumAJcjWbF6L2lazTjHc0pjRF7aKeI1k/PS2Lt6BZGXAUxx6fVoVnYRoiEzNzfHxMSEjIwM1q9frzNkZGRgYmKCubl5hfn3799PUVERFhbyIYcQNcHIyIiAgIByY3IffPABf/3rX+nXr59y0nohPDxcOapCVc1fFdUOAN9vZETBE9O4Mj+Coi66zTgDYGpO9lNzye3gXVbzV6MGsHl6nG7g9yEFgAEKCwvZv3+/zgEXExMDwIoVK5gwYQKffPKJctJH2qlTp3S26ccffyQrK0uZtVL69kGnTp1YvXo1Cxcu1Mpb2xo3bsxbb73Fn//8ZywtLUlISGDfvn2cO3eOzMxMjI2NlZM8dPb29ixfvpz33ntPa/zRo0d54YUXmDFjBqmpqVpp9cnVq1dJSEjA3NycXr16KZNL9erVCysrK1JTUzl16hTz58/n2Wef5fvvv1dmrddatGjBihUrmDNnDo6Ojly5coVffvmFEydOkJWVRatWrfDz86Nt27bKSR8pJeeQH374gcTERJo0acIzzzxT52VePIJa+rH03zPxtM4j/sct2l/AP2oKr3ItKx+au+ItQWAhhKiSDh06YGpqSnx8vN6av0qpqalcunSJli1bYm9vr0yuAy/Q3RnyzkdxSJlUAwbND5XavEII0eA54mClemjISztFmjLZIGmlQWJTKwcclclCCCHEY6i4uJhNmzYxa9Ys/Pz8dIbZs2dz4MABnnnmmXr54YWfn5/BQd3w8HD8/GrvI7FqB4Bvj1nEzYHPw324Nm4Rt4dM164NbNacG0+/RX4rd902nu/fx+b4VqwO/kc5uqwZ6Ifg7t277N+/X+droH379imz1ivJyck627R582Zyc3OVWavF0tKS1q1bY2JiokyqVU8++SS9evUiMTGRmTNnsmDBAtasWcP8+fMJDAxkxYoVykkeOjMzM9q2bVv6ZVlDdOTIEQoKCujSpYve/jUAevfuTXFxMVFRUcqkBqNFixa8/fbbdO/enRMnTvDqq6/y+uuv895777F48WJefvllgoOD60WfoCXnkLVr1zJv3jwWLFjAtWvX6NGjR4WBftHAWYwoC/5ueZugL7W+d38EFZJ0aA+xF2+pgsCjvHGVILAQQhjEysoKgMzMTGVSua5du4aZmRktWrRQJgkhhBD1gCPNzJTjNFng2rLspbRFS1cqfEVt1kwCwEIIIR5r5ubmTJo0CX9//3KHSZMmYW5uTmxsLI0bN37wboUeEkOCwLUd/OVBAsD3i+5qRWxzBk4m67l3ud+sJcXm1mSMWEShZSsoLtaJ7trtWYHp2R/UM9IT/X1YEWBRr7Rv354mTZoQFxfHzZs3lcniIfntt9+4evUqDg4OeoOD3bt3p0OHDly/fp3ffvtNmdxgPPfcc3To0IFjx46xbNkyrl69qszCkSNHWL58eb2r9Z2UlERycjJNmjShffv2ymTxOLAYwdL1s+tR8LeERhDYwhlPCQILIYQQQggh9IrmqrrhPJPmDspE6BKIt4vG3y7eBHbR+FvNobm6skTWVaKViUIIIcRjZNasWaUfF5fHysqKWbNmAXD58uUaq8T4MFQUBK6L4C8PEgC2iHgPy+PhUEzpcKddDzL/8gmZk1ZRfN8ICm5D0d3SILBZZhIOX8+mccb5shkpm35+iE1AV2batGns2LGDcePGKZN0TJ48mc8//5xdu3axa9cuPv/8cyZPnqzM9kgo6UdXc30//vhjXFw072RVlPtg7dq1LFu2DAsLCwYMGEC4um9TQ/bRg8rKyqKoqAhnZ2eD+iLt3bs3//73v0v7Ct62bRsLFiwwqFaCodM6ODiwcOFCtm7dSlhYGGFhYXz11VeMGzeOxYsX8+GHH2Jvb0+HDh1Km+OeNm0aTk5OfPrpp6xdu1ZrfiW/zX//+1++++670v3773//m969e2vlXbx4MVu3bmXIkCH8/e9/Z/v27aXrGhgYaNA+qgm5ubnEx8djZmbGgAEDlMn07dsXS0tLTp06VRoULVn3Pn36aOWtqBzZ29uzYcMGNm3aROfOnUunady4cWl/u76+vlrj165dq5O/Njg4ONC/f3+ys7P55ptvuHfvnjJLuarymz9MRkZGFBUVcePGDQDGjRvHjh07mDZtmjKrzu/bp08ftm7dyuLFixkxYgSfffYZu3bt4rvvvmPt2rV06aLnqVk8Oupt8LeEBIGFEKKq7t69C0CTJk2USeUyMzPj3r17pdNW7gVWbtnCltJhJS8os6gNmh+qkW8LofPLGmNWpfnhDFj0naWTzpAFhGouR29TzoNYsFFzXbawZeULpdPO6msBlr2ZtWULW7aEsmCIcnpDlbMcPXS3+QXVtHryv7BSe54rA1T7Vms/YMC+GLKA0C2hLBhStp5CCPE4iU1TvbMw7TKRNQsnM6K3Bx69RzB5bjCh/xiBA0BhHnmFAA6M+EcowXM18i1cw8QuqoeNq2mxWvPWq8sEJg+vsB4xANajpzJBHpuFqHEnT57k1KlT9OvXr/S9bXh4OMuWLaO4uJiffvpJOYkQogqsra2JiYlh8+bN5Q4xMTFYW1uDxnNofaYvCFxXwV8eJADc6H4xFj+tpsXBT7Vq7hY3seB+y3bQpoNq3J18KLpLi5M7aLHnHzQq0I7YKyv+NoQKwDNnzsTf35+ioiL27dtX2oS0v78/AQEByuwP3fTp03n++ecxMjIiMjKSH374gTt37uDv74+ZWYXt3bB//372799PYWEhv//+O+Hh4ezevZuEhARl1hr3008/8fvvv+Ph4cHq1at1goeavL29efPNN2nXrh0xMTGEh4dz6dIlBg0axFtvvVVhcNTQaV1dXVmxYgXe3t5kZGSwZ88e9uzZw7Vr17CysiImJoYffviB3NxcMjMzS28iyqsF27hxYxYuXIi/vz+NGzfmwIEDhIeHk5iYSIcOHXjzzTfx9vbWmWbq1Kk4Ojry008/ERkZyf379xkzZgzjx4/XyluboqKiyM3NpVOnTlr9vjVu3Jju3btTUFDAiRMntKZRqqwcZWRkkJycjKWlJV27di2drmvXrrRs2ZImTZpoBRK7du2KjY0NqampnD+v8RFKLejcuTMtWrQgLS2Nc+fOKZPLVZ3f/GHw9vamS5cuXL16tdzj1xCOjo68/PLLXLhwgd27d5OSkoKzszNvvPFGuc2H16WSsq9vn7do0YLp06czffp0nQ9BUE+7aNEinnjiCWVS/Vbvg78ltIPAA0YPkSCwEEJU4MqVK6C+3zVE06ZNcXR05NatW3pbQdExZAGhW/ywO76WKVOmqIbd4DfaWZmTF1ZuYVbfTMJL8q07AX1nlQY3D70fyJQp4aQAeer5Bb6v7gk4YCVbXu9N5m71tFPWcoLezNIKfL7Ayi2z6M0J1pYsQz0/Dr5L4JQprD2eB7kl6YG8e7B0YsMNWUDolln0vh5ets1Twklx9tMJxOps85S1nO/sR2+d2yVVoNbPVnvdGa0KiGsxaF+odA54GTap8gkhxOPEwaKZ+n8WuA6eyuzlwQQvn83U4R44mAHkEb/9bd7eHk8egJkDHsM18g0uaxa6mYWeWsQKXTwHMXHWepZWEAS2Hr2UD2aMwLOLNCgtRE27d+8eK1euZNOmTVoB4O+++47g4GCio6Uev6hdmsedoYN49GkGgcPrMPjLgwSAS5gd2Yz19+/p1uC1sAKnztDEnJY/vY/Z6TDlpCrK6R5iDWALCwuWLVumVYD01UqsiJeXFz4+PqSkpPDXv/6VtWvXltaSvXHjBoMGDdIKiNWF8ePH65wYSmrplazvtWvXWLp0KatWrWLdunXMnTuXI0eOYGRU8SGyfft29u/fz927d8nIyGD9+vVs3LiR+PjaDwrcvHmTlStXEhcXR/v27Xn77bcJCQnR+b0sLS157rnnaNSoEf/+979ZuXIl69evJygoiNjYWFxdXXnyySe1pilh6LSNGzdmxowZtGzZkt27dzNr1izWrVvHunXrmDVrFps2bWLfvn1899135Ofnc+vWrdL+mGNj9X8F6ufnh6enJ0lJScyaNYtVq1axfv165s+fz+eff06TJk2YMGGCVvDazMyMvLw8FixYwLp16wgJCWH79u2g/q3ryunTp7l06RJ2dnZatVZ79+6Nk5MTly9f5vDhw1rTaDK0HJUcZ506dSqdtnfv3piYmJCTk0PHjh1L90+3bt1o2rRpnXycYGNjg7GxsWEvPDVU5zevCy4uLsycOZNZs2bxwQcfMH/+fG7fvk1oaOgDNcPRsmVLtm7dyooVK1i/fj1vv/02aWlptG7duk6PV31cXV2ZMWMGTzzxBK+99prWRwYAL7/8MmPHjmXs2LG8/PLLWmldu3bltddeY+DAgcyYMYPu3btrpddbFiN4a11DCP6WKAsC32vqKEFgIYSoQFxcHFevXsXd3V1vK0FKgwcPxtbWlnPnznH79m1lso4XnumNRUp4WaAWYNNCVaBV05AFDHOGlN0L+bJk3MF3+fR4HhZ9x5RbY1hlEAuGOENKOAs3lYw7xLubTpBn2Zsx6u90X1jph3PuCdZOf5eytfmShQtLl1gjSrZ5itZ8v2ThOu31UW1zHifWaWwzh3h3ujoorSlgDL0tUwhXrvu6E6rARCnD9oWKBZz/tHpBbiGEqLe6MPW9rcz2VAViC/Oy1LV81e4VknUxmi/eepmgL+OJ/zKIl9/6guiLWRRqNgBWmEeWekILz9lsfW8qFVXcjf8yiLe/vkrXcoLAquCvK0kbZrNoZ5oyWQhRA+7du8c333xT+t625F33mTNnlFmFqHF+fn5VHkT94KcOAtf1b1ZxdM9AjW7dgBtXdKvxGhlD6w7cN22qnKSMMvD7EAPAhYWF7N+/XytQumfPHi5duqTMWq5+/fphZmbGoUOHtPqlTUpKIiUlhRYtWtCuXTutaWrbqVOndALAJbX2PDw8aNq0Kb/88gtJSUml09y7d4/9+/eTn5+vMadHz9WrV1m4cCHBwcGkpKTQuXNnlixZwpw5c0qDZL169aJdu3YkJiZqfal17949Tp06hZGRUbn9mBo6be/evWnfvj3nz59n48aNWvOorn79+nH//n327Nmj08fxrl27SEtLw9HRkR49epSOv3v3LgcOHNDKHxcXR15eHmZmZnUWOCzZP8bGxlr9AHt5eWFmZsavv/5aYbPIhpajM2fOkJOTg4uLS2mNUTc3N65du8b58+dp2bJlaeDOzc2N/Px8Tp8+XTq/2lZYqPmEqLJ27VqtsqjZZHp1fvO60LNnT/z8/Hj66adp3749hw8f5o033qi0FndlLl26xK5du0r/vnnzJsnJyRgZGWFhofuwKx4u77lT8W4JYEGXKSE61xVDh61LfJSzfmDOQ5/F39+/GsOzDGjfjMYATR3pOUC+ohdCCH2Ki4s5dOgQRkZGjBs3DicnJ2WWUgMHDsTLy4urV68aWEviBbo7Q8pZ3QDroauZWn8P8uqMRe4JwkqDliqqfHa0ragp5iGD6WyZx4nvFcs5eIlMwM5hUOm65J2P0gigGihgpXZTzvqaXC5V/jZzMIrzueDcTRXOHuTVGQsyuaQTgP2dLMV3eC90c4bcLH7XHl26jaUM2hdlMq9WeW8IIUS95jl/PpO7lT2T3o0LZfJEjRfu4yYy9fUVbD1V9nlN3qmtrHh9KhPHaeSbOJnQuLLmKy26TWb+fM/Sv/UpLwhsMbws+Lt0t7pzYiGEEELUC+Hq4G94HdfafuAAcEHXkdzwehluZEDGH1p9ApcM15/7F/l99fd/q4wZP8wmoO/evcv+/fu1vvD57LPPqlSLr0WLFhgbGxMQEKDz0rtfv36Ympri6Fi3L5iTk5O1tkmz1qm9vT137twhOTlZORlFRUXcf1g/RhUdOXKEOXPm8N5773H9+nWGDx/OvHnzQKM2Zq9evXR+k2nTpmFiYkLr1q2Vs4QqTNu2bVtMTU1JTU2tMLBZFVZWVty6dYvff9d5hcO9e/e4du0aTZo0oW3btqXjCwsLSU1N1cqbk5PDnTt3sLCw0Mpb244cOcLNmzfp2LEjDg4OWFpa0qVLF27dusXx48eV2bUYWo6SkpJIS0vD1tYWNzc3OnfujJOTE+fOnePs2bOYm5vTrVs37O3tadeuHZmZmXUSAC4qKgKgVatWyiStj0yUv211fvO6sHPnTvz8/HjrrbdIT0/H29ubZ599VpmtyjIyMnTKy82bNzExMaFly5Za4+taUlISGzZs4JdffuHDDz/Uacr7008/Le2b+tNPP9VKO3fuHB9++CGHDx9mw4YNDeYr0ZNHklC9Zsgj6UA44WHVHKLLPjaqKfk518i6kVW9ISsf1VF4j4Jb2cpZCyGEUGjZsiUvvvgiY8aM0eoGwd7enqlTp/LMM8+Qk5PDjh07uHXrlta0eg1pi51yXDk62Gr2vasx6GkqWkcHayywoPfrimnV/QVD2bpUK+C5aaFGU86qQatGs6aqbrO+oK6OQbS1Ba5fqjx4bci+KJVHVuULF0KIBsQHv94VN9dsMXAyM2dMxlvzu2ULbybPmMnkgRV/zOzQ24/KPomN/zKItzel4qoOAlsMX8r6Wa4krZ0pwV8halnjxo159tlnmTlzZukwffp0nRYnhRDCUOEaNX/rOghc/QCwUWPy+j7PzZ4TVTV9jZtAzg0apZ6jUVGhTkQ3e9DLZP3p39xvouioSBn5fZgR4BpSWFhY2nencqir/nGr4v79+9y5c0c5ul6KiopixYoVXLt2jV69emk1vRoXF6fze5QMMTExWvNRMnRafTU+H1fnz5/n4sWLtGzZEi8vL3r16oWDgwPJyckGBcQMLUcJCQk0adKErl270rVrV0xNTYmPj+fs2bPk5+fj5uaGs7Mz1tbWJCYm6gQca8PFixe5ffs27dq1w8FB+8Fx+/btpR9iZGRkaKU96k6dOsVHH31EXl4eI0eOpGfPnsosDUp0dDTvvfee3tpLN2/eZOPGjWzcuFGntjbqaYODg/nll1+USfVW3o9Lmbk6liwscPXsSN6B9azfUPXhix9rvqmyqyciidgTUfXh5/Pkm5nTmHtkJ0bz04kc5ayFEEIA3bt3Z9y4cRQUFPDll1+SmZnJgAEDePPNN/nHP/7BsmXLmDt3Lq6ursTGxvLRRx+Rnp6unI1+ytqpFfj9umbfu8qhkr54f88ijzxOrFNOpxGsrcK6PJC6Wk55DNkXQgjx2HLFurlynCYPXp02Fb8xU3l1rnfpWO+5rzJ1jB9Tp72Kh1Z+hebWuCrH6RH/7SKCN6XiOmsrW0uCvz8qukYQQtSoxo0b89Zbb/Hiiy9qNbE7btw45s+fz9ChQ5WTCCFqUXFxMVeuXFGOrlfC9TT7XJdB4GoHgHP7v0iuq09ZsLaxMaY5l7CLWELLz1/G6Ha2TrPOd9p04+or31Bkr9HjhbLp54fYBHRNyM/Px8jIiIsXL+rUui3pM6Au+sc1VH5+Pqampjg7637rbWFhUWkfwI+iklqhxsbGmJqacvv2bYqLi7l7967O71Ey7Nu3TzkbAIOnLcnXsWNH5SyqLTs7m2bNmtGhQwdlEo0bN6Zly5bcvn2bixcvKpMfGSU1zXv27MmAAQMwMTEpbX68IlUpRydOnCAvLw83Nzd69uxJdnY2J0+e5MyZM6Snp9OuXTt69OjB/fv3DVp2TThz5gzJycnY29szYcIEZXK56sNvfurUKSIjI2nWrBnjx4/XaVZc2cd5yXqLhqE0CGzRhcnvhDC1og6sHnWmrvg8M4A25vfIOh/JvqNpyCc8Qgihq02bNowaNQojIyMiIiI4d+4c69evJyQkhIiICI4ePcrRo0fZsmUL//znP9m5c2cVPy5VNWVc0uSxphe6aT+jHLqaCZadGVxRU8/lOXiJTCzo7FVes8xUuC41q4LlDBlMZ8uy5qG/PJuif5vV+cocIup8Hjh31+0LOaC7ds1eg/aFEEII/axpZq76n2lj09Kxpf83b4Z16dgHE//tIoI37OCLlRL8FaIueHh40L17d44ePaoVAF6yZAlGRkY88cQTykkaJAsLC5YtW6ZTIaeqw7Jly6SLN/FA9uzZQ2bmQ/109oGE6wn+lqirIHD1o3vF97Rq7Fqe34f1wf9gVJBN41sZtPxyOiaZv0PxfZ3h2nOrye8xFhpgBeDTp09TXFzMoEGDtJpEe1RduHCB+/fv66yvubk5I0eOxNxcfVdrABsbG+WoWuXv788rr7yis46urq44OjpSUFBAdnY2p06d4saNG3Ts2BFv77KvMw1h6LTHjh3j6tWruLq6GhTwa9q0aaXN+J44cQIjIyNGjhypcyyNHTsWR0dHLl26pNM07aMkJiaGa9eu0bFjR7p3705mZiZRUVHKbDqqUo7OnTvHtWvXcHR0xMXFheTk5NKatefPn6dFixb06tWLmzdv1mnt+6+//ppbt27x9NNPM336dJ1AqT715Tf/+uuvuXTpEr169WL06NEA3Lhxg6KiItq1a6e17oMHD6ZNmzYaU4v6Lu/Hpcz+UB0E/scaAutjEFgR/P0p9qoEf4UQQo9mzZoxYcIEzM3N+fHHH7Vacbl58yYHDx5k165dhIeHc+rUqSoGfksc4t2DKeDsp91nbsBK/JTfqG4K40SuBb1fX6kd5ByygJXl9rdb4kvCjudh0XcWKwM0xw9iwcoFqKY+xLubTpDn7MeWlZpLeIGVGn8/UCAaKl7O672xSAlnYUk/x3q3eRALAnqjfJ126P39pOCM38aS7UE1T50msg3ZF0IIIR4F8btD2XpYgr9CCCEeP5cuXVKOqjcqCv6WqIsgcLUDwJbHvqD52e/h/n1sYj7B4uS3NCq+W5puVJCN9bf/R5OLv+pGd+/fJ3vQDLKGL9St+VvPawD/+OOPnDhxAhcXF9auXcu8efOYOXMm8+bN46OPPuKtt95STlLrXFxctPotKOm7oEuXLvz8888kJyfj6urKv/71L2bNmsWsWbNYu3YtdnZ2FBQUKGen49q1a+Tl5dG+fXvefPNNFi5cyMiRI5XZalzTpk0ZO3Ysn3/+OatWrWLOnDm8++67rFixAhsbGw4fPkxSUhJXr15l9+7dmJqaEhQUxDvvvMPMmTN5/fXXef/991m3bh1OTk7K2QMYPO3Nmzf58ssvuXPnDi+++CLvv/8+M2fOZNasWaxbt46AANWblUuXLpGbm0vLli2ZPn06b775JpMmTVIuFtT9rh4/fpyOHTtqHUvvv/8+L774IllZWWzYsKFOmjSurqtXr5KYmIiNjQ02NjYkJiYa1Kd2VcrRvXv3OHPmDDY2NrRo0UKrhn3J/x0dHfnjjz/qtMnlU6dOsWbNGnJzcxk3bhz/+9//CAkJYdasWSxfvpxPP/2Ufv36gUafwfXlN7958yYREREAjBkzBgcHB3777TdSU1NxdHTk3Xff5fXXX2fhwoXMnDmTnBxpVrehydqtDgKbuTKhvgWBJfgrhBAGMTIyYuLEidjb27N//34OHz6szFJzNi1kyu4ULPrOKuuPttsZpuxOUWQ8xLvTpxCe4oyfZt+1r1tzxoBmiw+9H8iU3Sk4j9bs93YW1mffLes39+C7BE4JJ8XZT6tvXNQ1ckEzKLuFLVtCWVCdQHA5y7E7vpYpCzWWxSHenb6WE7ma2/wybFrLiVyNbAB8ycIp4aRo9ZPcnTNTwtHZk4bsCyGEeCzt5dSFip4QIjmXUggUknb+WOnYY+dVLQoVppwjUiu/tsILp9irHCmEEEI8Bg4cOMA777yjU1tcc3jnnXc4cOCActJ6xZDgb4naDgJXOwDM/WKaxoXhsGM2pmmqZl6VjO7m0yLibZqe+0k3wHv/Pnfa9tYzvn4HgO/du0dISAi7d+/G2NiYYcOG4efnx6BBgygsLDSo9mNN69mzp1azFX5+fowePRo3Nzdyc3NZvnw5Bw8exNLSkqeffpphw4aRkZHB5s2bDQo0paamsn37dgoKCnjiiSfo3bt3Nb/+r5qwsDB++OEH8vPzcXV1xdfXl86dO5OZmcm6detYv359ad4dO3awfv16MjMz6dWrF35+fvj6+mJnZ8exY8cq/JrE0Gmjo6NZvXo1v//+Ox07dsTPz4+nnnoKExMTfv/9d1AfH//73/+4ceMGffv2ZeDAgTRq1EixRJV79+6xYsUKduzYAYCPjw9+fn60b9+e2NhYli5dSlJSknKyR050dDQFBQXcuXNHb1+q+lS1HMXHx1NQUEBWVhYnTpwoHZ+QkMDNmze5f/8+p06d0pqmLhw9epT58+ezb98+ioqK6NSpE08//TQ9e/akadOmnDp1iuXLl/P9999DPfvNd+/ezdmzZ2ndujWTJk0iNzeX1atXc+7cORwcHBg1ahQ9e/Zk165dpKQoXzmKhqBeBoE1g7/xPxEhwV8hhNDLyMiIMWPG0LFjR44fP87BgxV1rltDNi3U7ot24Zfqcbp9+365UNlv7UI0Q6aqQGg5fdkqlzNlSllt21Kq6cvPowpEq9J010+fLxdOYcp0ZXBVdzl611lredrLzLuues4oo5xn2b7JvKqYd2X74uC7BBq4fUII0XCkEfr39URfKxtj0XMqS1/wLG3aeetbE/Hzm0jQlrKauXlbgpjo58fEt7aqx1jj+cJSpvbUaK/hWjTr/x5KWtkYIYQQ4rGxZ88eJk6cqBOr0hwmTpzInj17lJPWK34GBn9LVDV/VTRq1apVrYdb7zcy4taAl8jr9aeykcX3oCAPZ/femllLFSxwU44SQgghxCOmy5+CWfSSB9YF8XwxK4itl5U5HhHK4O+vGm906kCPHj1KPwYSQohH3dixY+nfvz/nz5/nyy+/pLi4WJlFPGxDFhD6em8ydyuD03oErGTLaDtOrJNgrhCiYerQoQOnT59Wjn5AXZiwfBGBvTV69L2XRdrxQ+w9sI/IA0lkaWYHwBrXoT74Dh3BoL6OWGv0BJV1IpTgxTsoa7NMCFHbunbtyt/+9jeys7OJi4tTJuPu7o61tTXBwcGcO3eu3PwWFhZ4e3tz6NAhVq1apTWP6li8eDEDBgxQjtZy5MgRli9frhyto0+fPixYsIAzZ84YlL8yhqxbVRm6LZVZvHgx3bt359133+XXX39VJuuoKH9N7zchHlXVrwFcBY3uF2MZE4rl4U+hmLLh/n31vyV/q/4titmmnIUQQgghHkHx3y4ieEs0ez8NfnSDvwCFSZy5eI1rDyH4W8KQvsCFEOJhGzJkCH379iU5OZnt27dL8Pehe4GVWn36qscp+wpGHRTW6lNYPW60M3nHP5XgrxCiQaq9e+x4diyeytT3d3DyD3VN38bWOPb3I3D+Gr4IDyf8m+1sLx3CCQ//gjXzA/HrXxb8zfvjJDven8pUCf4KUefOnTvH+vXrsbGx0all6Ofnh42NDR9++CHnzp2rML+Pjw+//fYba9asUS5CCCEeaXVSA1hTfucRZA+dDfeK4E4ezt37aqUXxkVyL/wfNLr5h9Z4IYQQQoj6ys3NjRs3bpCfn69MEkKIR8qAAQPo0qUL3377Lbdu3VImizo3iAUbZ9HbUnts3vG1epqLfoGVW/xwVoxNMaSWsBBC1FPm5ubY2NiQkJCgTKpR1p4TmDpuBP3cHbE2VaYqFGaRFneMvd99wY5Y3XrCQojHW//+/XnjjTewsbFRJlVLbm4ua9euNbjrvYo8yus2dOhQXnnlFaysrJRJ1ZKbm8v69evrfX+zQlSkzgPAAAWO/bk5bD7cuUX7ngNV445t5/6hTzHKTFRmF0IIIYSo1xwdHbl//z43b95UJgkhhBBCCCGqydpa1URzWlrd9axr0c6Dfp6edHEw0Rp/92o8sbHHymoMCyFEObp3787AgQMfuBWDe/fucfjwYc6cOaNMqrbHZd2OHz+u0zS0EA3NQwkAA9zvMYaCdr1pcvsGjY79j0a35Ys4IYQQQjRMzZs3p127dqSlpXH//kO59RJCCCGEEKJBadSoEY6Ojvzxxx/k5OQok4UQQgghHmsPLQAshBBCCPE4cXFx4e7du2RlyUdvQgghhBBCPCgbGxuMjY1JTk5WJgkhhBBCPPaMlCOEEEIIIUTNu3z5Mi1atKBJkybKJCGEEEIIIUQVNGnSBCsrKy5fvqxMEkIIIYQQEgAWQgghhKgb+fn5XLx4kdatW9OiRQtlshBCCCGEEMIALVq0oHXr1ly8eJH8/HxlshBCCCGEkCaghRBCCCHqlrm5Oa1bt8bY2Jhbt25RWFhIYWEhxcXFyqxCCCGEEEI89oyMjDA1NcXU1JRmzZpRVFTE5cuXJfgrhBBCCFEBCQALIYQQQjwEzZs3x8rKiqZNm2JqaqpMFkIIIYQQQqgVFhZy+/ZtsrOzycnJUSYLIYQQQggFCQALIYQQQgghhBBCCCGEEEIIIUQDIX0ACyGEEEIIIYQQQgghhBBCCCFEAyEBYCGEEEIIIYQQQgghhBBCCCGEaCAkACyEEEIIIYQQQgghhBBCCCGEEA2EBICFEEIIIYQQQgghhBBCCCGEEKKBkACwEEIIIYQQQgghhBBCCCGEEEI0EBIAFkIIIYQQQgghhBBCCCGEEEKIBkICwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRqIRu7u7veVI4UQQgghhBBCCCGEEEIIIYQQQtQ/jVh4pjQA3Oq/w7VTH3O2trZcv35dOVoI0cBJ2RcNiRzPQtQdKW9CNFy2trbEjdmqHC3EY8s9bLJc84SoZXJvKUTFpIwIIUTFJABcAbmICPF4krIvGhI5noWoO1LehGi4bG1tuXXrlnK0EI+tZs2ayTVPiFom95ZCVEzKiBBCVEz6ABZCCCGEEEIIIYQQQgghhBBCiAZCAsBCCCGEEEIIIYQQQgghhBBCCNFASABYCCGEEEIIIYQQQgghhBBCCCEaCAkACyGEEEIIIYQQQgghhBBCCCFEAyEBYCGEEEIIIYQQQgghhBBCCCGEaCAkACyEEEIIIYQQQgghhBBCCCGEEA2EBICFEEIIIYQQQgghhBBCCCGEEKKBkACwEEIIIYQQQgghhBBCCCGEEEI0EBIAFkIIIYQQQgghhBBCCCGEEEKIBkICwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRoICQALIYQQQgghhBBCCCGEEEIIIUQDIQFgIYQQQgghhBBCCCGEEEIIIYRoIBqx8Mz9kj9a/Xe4dupjztbWluvXrytHCyEaOCn7oiGR41mIuiPlTYiGy9bWllu3bilHC/HYatasmVzzhKhlcm8pRMWkjAjxgLr4ETi0HSbK8VWRHc/WLZFkKcc/qEd53eoRCQBXQC4iQjyepOyLhkSOZyHqjpQ3IRquOg0AG1lh6jqAZtZNS0fdyzpNblISxcVaOYV4aCQALETtk3tLISr2SJQRi0b07GuGp+t9oj8rIF6ZLsSjqksga1ZMwNVUmVB1WbHrmb00vOYCrY/yutUzEgCuwCNxERFC1Dkp+6IhkeNZiLoj5U2IhqtOAsBWA7Ad9RyOHawwMoLiwtvcKwKMTDAxM4HiuxSkHSEtbDO52XeVUwtRp+okAGzaDZsRo2hWeJLMXw6QX6Bx3Jt2w8pnODamKaTv3cWdQs0JhWgYav/e0gQT12dp7dmC27/t5kbCRcq+MzLBxHUc9p5tuBv7DRlJ6VpTCvEoqP0yolAS7O1tQddOzXB0MMPCrJEq7fJlXnvlJmnKaYTAh6CNs/GxSCN8w1LWH3g0QpE+S7YS1P8KO/zmEKpMVKupPFVlyDxrKk9D93D6AG42mr9/9QP79++v8vDDV39ndDPlDIUQQgghhBBCiPrIBBOPv9L9tWm07wA5Rzdz5l+v8dv7czj97zmc/tdr/Pr+34jfc5q7DoPp9FoIjh6tlTMRooExwWZyIM0ufMP1693oMHct3UZ4YoQJJu6v0m3m8zS7Hk36xU64vRLwYM0DCvG4cpxGpyfucvXAbxj1D6Jv0F+xbmECpt1oOXUlbp4m5ByIxmj4Ejr0kFImHnfGBH3QheD5zkwYbkeX9uZlwV/g6oVbEvwV5XDFsbUpNHfFb34ooUsm42GhzCNE7XgIAWB3Xv33HJ5qVb3626atnmLORgkCCyEaPseexri0VI4VJTyeX0zw8iBGOSpTxKOoNo9np7FBBAcHMabax4Il7mNnsHh5MMHBwQT0VaaLGmfkgf/iYILnjcJJmSYeXMvG9OzZiNp5pvQiMDiY4EAvZYLhHLwICHqH4OBggoPG0EaZLmqAE2OClL+T6rcLGlu7pc5u+OsEL19MQF8zZZIoR+O+f6WbXxcaZ0YR/68gkn/aT6FmTUeAwmvcPvERF/69hKQLYOe3GOe+tXRhFXVu3CfHSEk5xea/KFOqwpHpixcxTDlar2EsWjydat861YlumOccJjXhInnHP+DseyFcc5xGz3mr6NEnkwv/Wcyl47HcOf0JV+56YGujnP7RYjcwgKB3VPeaQX5y5asKee6rRa3h1s/fcOfKYTK+mMWJ7+/iOHMVveYG0iRqMWe2fkXulViu/HwBq+5DlVM/WizdGTNzser+cnkAnsr0h6m2n31qe/5CrTEW5d7e3iEttkg5ssY9TudD5XWzxp8xHkK5yTsbSexlcOg/leCNa5g51FqZRYgaV+cB4CHLljGpoymk7mbe/HkGDru5qDEPCQILIRqCl9d0JSysK2H/a0nJo5RFTwve/qgjYWFd+TC4E2s+60rYzs58OMdYMfXjzgyT6n1HJGpJfT6e7UYE4j/AibuJUUT8GMvlfGWO2uMVqHqg0RqWv8PC2f54OShzNyBmJjxaR0E9M6wlW8JUZW7NtJKRjRj6ams27exK2GedCQ7uosqzxYFJ2lM/XEYe+M8cg5tFBrE/RhAV/3CavzK282DUi3NZ+Lai/L29GP/eytyiKsyNzZWjREVs/ek4whUu7+Xcp59zu6QZW6MeOLy2kT6LNtLlqR5l+Ysvk/3N34g/cRubEX/FzrYsqSpUAccU7SExgVM/fcYinZ6hFvF9oiJv6XCMzyYq8wN48+4PCaSkpHDqiwBloloQ2+OU8ytZj828+xd35QQqEz/jWMmyn1MmanCezuZf1fP84d2y8aXT6xkSv2eR5jzqSPc2dlCURtx/lSmGG/nBZhYFTmfN7mWVBIGHsWz3GqYHLmLzByOViY+Qphgba7TrXHyRO7dNMDKCoqwL3C1tpzabokJTGlf3qyfHMQQp78XU14OFswMY06/Ng9+z9PTnDT83LDNj2bc7ioS6vPSVt33BwQQHB/IAn3PVEXnuq01GZk25p9G3fFHmTYqNgOJs8jNvlyUU3Aazsn7pq6q8Z57Fi4J4/VkfXB44BmKH70v+eLW9S8LBCPaduEzdPdKpP7oLGlN+EKm2n31qe/6icgV5nNqvHFnTHqPzoZ7rZo0/YzyMcnMrlqXTp7IiLIk8C6kNLOpGnQeATRurz1SFtzgRe8LA4RYlt/2XEy9Q+JgEgX2WbCU8PFx3+CAQCGRNeDjhm5fio5wQH5ZuDic8fA2B5c5nK0uf1JjkyaVsDQ/XeImon755bV2iZw305AvXM//AD3TzaM1TvV7KdNU+EKKBsbBg6dtOeLZTN61UqP56sDHkXa39LwnrlwJiP1/OosUhREgbO4+menM8t8Grpx1kxbD58wii9u9g31llngdljefkuSz8c3nfoWdycncEEbsjiDh4koTLuZjbuTPmjQep1Vw11v0mMXehf919KX87lk3LF7FoVQSpyjRRLZ7z2xM0ugXWjQHuU1h4X5WQV0i8Iu9D1dsDd1NI3rOOHfujiAiPosZ7lOvoy+vz5pbzZbwxLiNfZ/HcSQzuaE1RZgJxR/apyt75BNJzjTGuixcrFa5j/Za6J4RFi5ez6XiBMknosKLFqMFYFKdycdvXFGq8hKf1AGzVL8Sbdh2Adl2H29ze8zlXclvSZtQz1Xqo93a0AxLZ6uyMs7Mzzs7PsODL49xpP4zp721murNG5r+442gMOQeXqPNqDv14abtGXjXHeUGMd2sCQHP78gK57jhaKOf7DC/9YyPRRd2ZvPR7jn2hp5ZqP0fsALCj78TpylS1YbwbGoS3ulZoZlp0WZJ6+sSvlNvijHPHZwguy1lHAnBvBVxJ40HeHe+ZvYRNZ3No3i2ggiCwKvgb0K05OWc3sWT2HmWGR0g2d5u3RfW61wQTr7/han2Ac59+QobTq3TqrzoKoBtm1oXcy9OauMoKkqNU92K79xFzJoGEzHxMbN3wGv867yz0x/MBAlSevd0xLk4m4sMdRB6KIOxQjV/5Kr2XK9s+zSGKJGXGR44899Wm4lwLmrZVP6+ZeuIU0I+879cQty8Pp1dexbzkAtPSDpMCjYBwtSieeRJTyb1rSZvevgQGvcPrI12qH4xp7YWHA2Qd28ymPVFEbt9HnDLPA3PB97Ug5o4sN8xbvuo++xh6v1jd+YsqMsGmuXKcSuHFPJKetmDmAmte7qVMrSnlnA8NPU7qEX3XzRp/xnho5SaP6A1zmLwgVLs28ECJAovaUZ1nxYfq1olXmPf14xMEhiR2+PnhpznMDgVCmbMqlrzmnryqCMD6LHkVz+Z5xK7S7Nxaez4hR8FzniIIXCFVwDmoyzlCtNZnB1f6B5UTiFas+84kXMfrBoHJiVXM04/JyyK1siTt1F5mkssECQKLhmdSC7qYAtwjLew8Y/50gTFjzvHamovsCFNmFuIRV2+OZzssLYGszFq86bektaMdlmblvdLIJfVQFFGHoojas41NH4bw9iexZBlZ4/Vkea/xapZlayfsLM2r/9JFPGQm+PZQfxGdc40PpsTzpz/FM+alC3zweQ6nlNkfImtbGyCLjJp/913G1ok2tsZ6j2ensXMJHNKGoov7WLf8bUI+3MTmXZGqsvf5JtateptNR5RT1YIK1lE8RqyfwaG9CYVx33PzliLt8hGuq2sJ3j5/BJ1XXcWnST8QD+0HlwaKDTcdx9bAjQyNF+RxbF3qT0hUJth4M35qWW7Hno40B9LObyobWaHpvPuXPjTJ+5VfUwA7R/TWAVYHYrXnG8f+/4Yw8+lnCD6cg92QID77p7dGOkx3tgfSSEuB5u7D0BcCHvb+Isa7NiEtJVPVLOPZ70rTVNNnknZMa5KHx7kvjjaQk3YcjTB1Nexnyeg5ZUHgHcrmoIexaEdZ8HfO6CUPFHCuXU0xcfPAwmEg7vPW0uvvoXiOtON2rjNtnhmHRe5NLEb/iwEL19Nn4V9xNMumyKj6tRMB8jPjVPdihyIJ+2oTmz4MYfk7y9nwYypFlu5MmDEJt2q9QbPG2grIziBd8yOPGlbZvVzZ9mkOCWQqM4rHh5kHNi5WtBixll7z1jPgrdnYF93EqKc/Tj0tyC/ypNeSUPq8uR7PMR25k3sTo2qVgRKKZ57PQ1n93tu8vXobJ7OMaTMkkBlDLZUTGcbOEksg62rtPdGBPU5trevmQ8EScr/4iCnr71fJ1M2R4DeceKZnY5J+U6bWsgZ3nNTNdfOhi9+hXRt40ReELplAF2U+IR7QA126H5a4Dx+3IHA5fl7KR0fzsOg/gbJQaCAT+luQd/Qjlv6slVtL5LKPiM2xwHO8IUFUH5ZunoBr8g78/JeiHZoNZY5fCLF4ElRZQPaTOexIBteeleSrVChzdiaBS0+N7RaiAWis+f+yvhvTfrxD9AN+0S5Enas3x7M55o/ik9LF46rmAe1al9+UmBCljDDVKHOmJa1jXSti3y/3yhIeAeV/CFEHHMcwaYA1RclhrP44knSNlkWFeCg6umJBNtdO/KpMgeLTXP1wOr8GTyd+72llqkrcr9wsaknzrlbKlIoN6Ytjc+BKHMqQ7tbMbADsXSeXjpvcQR1w1X4QLNfkT17BuzmkRa7l+G3Axh59dYCDujhWMN80Nv5tK3F5Tej4zBsaQV5v+jo2h5w09idmQvPuDFM8FDrO2Mya5zpC0lZ+vW0HpHFhlWL6vDTi9NRcfiietsMKyEjZqEypBlUQeOOJHJr3nq4RBFYFf6f3bk7OiY2PdPDXqEMg3d5chVsvuJ6Qya3YZfyelEn6/+YR/8Uykr5YRtIXCzmz5yJ3L37D6dib3E06C08tp+cbf8XGXl2bsSYUF5C6fwP/OZAJlh6MGlFS67gqLDGry4CREJUxaoP15LV4vjYO85ST3Lx1gQubosm9FMFvHyxWl7FlJPznAy7l3CT902+4XpzOtcsedJr9L9xGDK3RQFNR5km2rdpGXCG0eXICHtV5U21e/scPQtSdeyTvv84B5WhRRY/TdVNZGziQkM1SG1jUrEYsPKNuHw5a/Vens58a91RwGH/3bgaJ2xg2/SNlcjle5eP9k+gEXIyYxxp1YLP1yPnMf6o1AIVXfuK95//BT9oTPhBbW1uuX7+uHF1nfJZsJaj/FXb4adbkVQpkTbg6ODs7lMAPwpnQMpYQjUBtefMJ/CCcCaim48mlbJ3nyZWdfsz5RCMTwLQ1hI9vReyqyeUHlaetIXw8pcswaJklfyvWV0t566VYnqgfLAZOZs5QV5IOrGHrYWUEqAt+r02kJ6fY/mG4TnOVFgMnM8e3K2n73ucLnWlrVl2V/ZfXdGWCC5CTScifr3HArQWfhLSmtNvPrJvs/TaTL78ronrdRFniPnISo/o5Ya1+4V50PYGwzzcRq7F5dgP9+fNQN+wsjaG4iNzMBCK3bibmakkOJ8YEzcArK4yVh+3wn+CFU1NIOZuKczcnUvcsZ8NBRb2UpoOZ8bdRtDm/jbe/OAmAZbdRTBrphYttybokE7NnGxFnc0sncxobxIwBWYStjMHuzxPxcjSD5DAWhcaU5tHJuyiU0lQHL/wn++BmZ4mxEVCUS+aRbazenaw98WOk4RzPgGkbBv9pEoO72GFpDBRlkRy5nf2WEwkcADHrQwjTaAqpsmPOKzCYMS5l+VWSy44pS3dGTRqFl7O16ngqzCL5SATb9sRRdtQCGNNm0CQmDXLDzkr96qEwi4TdoUS2DmTGAN2qWcm7FhF6pGQdNJZZyokJb87A89Y+ln8YWVbzq2QfdLbDUv1QVJSdScLB/7H5cFkdDr3lQ5VSWp4Xhcao+oWb6YXOGmqWO4P2g2HnmzKK9VBT/WaeOFmblS4rYXcom45V+6ipU3VV3hjWki3z7LAAkr87x5xPYEJwR17uqX7pfe8uaaevsmNDLvv+UE5sOOvuo5g4oqwMFVw9ScQXqXgEjcFFeW42ssNr8p/xKS2fuWTGR/K/rTFkFqv7INRzrGUd2UDILlVtjcqvR2rW7oyaOApPJ2vMjFHnjWHbB1kMCx6DTrHOimFDSBjWU99hUucM9r23jkjtQlwh1X7QOC6LCshKjSViWwRxpfPROKa35zJm8hg826quRUXX4wj7bDOxWQBeBFawjqnqdOsjG/g804cXR7phbZxVdn4zssZ9xETtslaQReoxZZnUV8bK5l2yz8HAMj4gkOCx1sR8/DmZPi8yqqM1xtkl66xQklfznFxyfJScu0p/swjqyxXa1taWW7eU1XQfjNnIELr1vUZy8EpuaiZ0mEaX8T0oC2MlkfrvD1CFZjV1weGNv2Kb+AFn95QTJNZn8fekBLqT+eMc+k0rqxkL4L3uIJufcSTxK2eG/w1gHJ8dW8OwJtEE9/Sn0hDl8DUcXD8Ox9uq/He+OMWyIRC9vCf+Wg9uhs333R9SmOyWyf55JU1NL+L7xOm4J23FeYM9x1YNo/mxENye+49qguHv8uO6yXTMiyZ44n6G7VqE9539zOn3EqotVU//x3cM8ZmDwS3KzttOwuw+pH3tzJy4NayZPY6ONkDRHdIiQ/CfthFeWMP614fh3lrVPmTOqU3MGasdaHUcG8SiaZPxdrOjuaqFbO7cgSZNNLexJmgGfLcSwSgmlwR/JwTXSPC3WbNmNX/NaxlAl0kmpH0SSl4hYBNAt7/0wyhrH2c/24V2RaCOtHrjbzi2uMml9X8l/RrQYihOL4zlXthCLl28q5W7XOrrE8pzoyYjDwLenoTb9UhCPthXdi9byflTdT+mc+XTOKdXcu3UYNx2MJP+NLjsOae4iKzzYYRGtiZQz/W19F7OkO1T07cMfdfi8p/Z0suuPeEQ8OdRuNkaqwLph/5H6J5kihy8NMYXkZUYwedf6G6vJn33tRXdM9qNmMvcoXak713JugNlV0azvgH8baIbWQdWs3pv/aj7XPP3liZYPb+SlvH/IumEqjkWq+fX0r51Ide//iuXlCfFHgvxHNeJ4t+/4tf//Qg0pYnP3+jqeIwzX+zC0I59yn/mKWM3ci5zh1gTt/VtNms0X1Px/WE591Ua96mVPROW0nePlZtJzDeryRqq77mxpCyr77ko574Iyrkvq+g4dtO/XaX3i0r65l/B81mWB/6LJ+F+5ySb3ttGQmn5U8/HIo5F72wuGflIq/kyUgGNZzC9St6FKMdXwmzIDBaPNOzdmvb5sJzjX/M4qcJ1Rke5z1xl9+9Vvm4s3k6u3yTG9HVSrU9hFnHhoWw+rrqyVnjdbKPnGYOy9Sy9Ft/O5OSez0ntFVTJeUdfuamoXD7IOwlV/KbV0RCdVk/LWOA9YwVzRrti0biQq0e/4P1lO3Tej9ek8uI3mgzJ4/HSUmY+2YzYqUHl5qkqQ5ZbU3mqzoAYRoXxjyl4msayZbXutLWhOt9VPVTtR61i1fuqoST4C2DayonOWjkfFyW1YUewdNpSRrhA0s/lBFO1+ODYEvKuVd7ji0+bVpBzjsjygr8An5wiCVd6Kpt31mL4MiujWqesetBfjSjjx1tzp+I92Jup89+hrE6Bise8+cwc7Y336JnMn+ehSJ3MO/On4t3fk8l6pm0wEm4S8lkmV0vu96xbMGJaJzZ9ZscEN0VeA3j8OQj/QW3Ij9uv7mcnjixze1prtI7mNDaIuX7umN2IZd/uCCJ+/o1cK3fGvDEXX+UH7pZeBIw0J+rDRSxatIiNX8WQUAROPbwU/dKBWT8PnIxy+e2wOvg7IJCgPw/GiQSiSvqbMnZh8J+D8O+pmBhLvF4chXnUf1i0aJHe4K9edr7MfWMM7mbpxOxR99+VWoS1nb0yp6gLNXw8Y+TEmNmvM6qbJQXx6j7MDqdjOTiQF3vrNhVmyDGXdCiCiN0nVU3fZZ7U7gvN0ovAef4MbgcJh1R9VUWlGOMyxJ+gP2ueoyzxClzM66PdsSwsWVYEUeeLMLe1JONkJBG7o0i+rbmMCKIqiXhYDvCllxWkno4pC/5aehGwQL0Pzqv3wY8xpGKHu99cgsZWo67w9ZNE7o4gKrlAu1+uQ+orrIH7wZDzTaV6+hP058G0KTjD/j2q3yIuyxz71rq/r9C1Y8VFvr9wR/VHYxMce7Vj9ked+PANk/JfUlTAckAgc58fjItxKjE/qs6pv+W5MGH2KN1a6UZOjJk3lzHdzMg6vo+I3RHsO5mLZbcxzH3DV9VXp9axVkCy+niKPJkBVbketR9D0Dx/Bjsbk65eVsTPsWSaWmNDkqoMnsrUWkbE/pNk4IabkzFcjiOmCsFfJ78ggp4fjItxOrE/q8tAfC7mzoPxnxeIl/LwNHcn8I2JOGXEsG9PBPuOp4OtOxNmTFC/nKloHcsYO08k0COVzcGLWLSoJFDgxJi5QfgPccE4Xb2fdkeRkGuuKpOBXihXp1IGlnEVY1zHBeKRupnlixexSO8LSH3s8H1DdXykH1EtY9+xVIps7ZArNJB9Tbd5598/IX7N19ykKSZNVYP+RgfjuXMTzFrqlMoKBXRWdRKXcVE7+IvzdN4Y4gh34ti/oWSkN452wOW0coO0ZRxZNG8kjsZ3iPt6ARuBTVcygObY67Rnp57vjUwq6oU28UYO0IQmJe8C1f0RZ6ZFw/adnMmEJt2e5A0AJvPZPyfTsUkO0RsWsNFRVdP5zh9x6uCvRn/GaccND/4C3q52NCGHO+1+5KtpdkT/8xmcfeaw50oTHIcHsOhvm/l+sTfZuxczxPkZQo7l0LxnAEGLy+bhPnsz21e9wTCbC+xc6s8QZ2ecfV5ifya1UCN5P8ETSmoCT67x4G+tcXHmXqw6+Atw4yTZQM7PyuAvQCJXjl7EOOcsmdfUo24eIDUsEbsnarhyQ/FJzqcCDk6U3sYacP7Uug+8nay+T4zk5HUDr50lixoQyOLXRuFuVVC6rIhDCRRZ2GFZ2b2cgSwHBPC3mdrL2HcsFezcGfNGEGPa60xR/jObuTuB03zg7D71dcoMpyEv8uIwHwJnjsIyRXW/GJWYj3XnMbzxvPJ6U4lK7hkz924nJgva+Iwpq01q5MZYXzeMr0byv3oS/K0d3Whmlki6OvgLkJ2UiUX2Yd3gL8DpCC7fNiH7zI/qEbe5E7mMVFNf7Fsp8j6gzLgksjCmjXPZNa3y+0PN+yrIPKV9/BvyTAgl5VF5j7WP2ExjrK20nxvL+tNWl+XqqvA4Nux+sSIVPp8Vn2R7eAJFlh6MGl52trEcOgYv6yLidtSP4G+du1vMrYIC0s5mEn+5tD6dWvVr/xYcMvzdmrZKjpMqXGd0VPjMpVL164YZ7i+9wcR2GcTsjSDix1jSscZ94gwmdFTlqPC6qY+lF4GzVeuZeky9jadzcRk/l1HtlJkNUGG5rG3q2sCB64muZ7WBT362lFdrMPj7qHN8bU7lMYwK4x+eeA6fyfz5ymlrR70LAD9+XJkQHk64xqDTh+4nc9iRbIHneE8sknfo1uDVI/CDIDybJ7G33K9Oyri2tIBraQYElSum6ptYzzKbexKktY2V9E385FJe7W9hYKBbiPolfvs1pv0lng+2Z5KWo76hbNmSF6ZbVPEFviceXYwhbR/rtkeq+9nZzOp/ribikjqLuinMrGMbWPlxGJGHoojav4N1q8NILbZj8AjFhcgOkr/YRlzJR2/FJzl5vgja9mKIrWZGa4Z4tIGsOI4nAk29mDTaBS6GEbJqMxGHoog6FMGmkA3EZhnj7uOr+GLdDhI/Z9uZqn1d12aAB3ZGucRu3aReRiRhoSEs/ypWmVXUkZo7nsHJbxJe1kUkh69m9VcRZcf0u9tIUjb4ZeAxlxkfRdShVFUNt9xUjb7QzPCaNAoXo1TCVoWweY+qr6qIz1ey4VgWxt2G4as+5u1GBDLGxZisIxtYvrpkWVFEfLWaDXtSKbgYS9ShODLuaC4jigSt906WOA0azOBBgxk8chKBsxezcKwLucc3s7n0C2DVOrmZZhHzyfKyfbA/jND3VhKWXIT1gImMqvApTo/bqcQeiiIuM1+7X674zNJlVr4fDDjfGMCztzvGpLJv/Q7V+ehQBJs/WM7qPYaFmB57eXdZPy+ZgKUp7D2bj+rduTGOT7dldn9l5kqoy5BxVgwbQkIJ219yTl3JuiNZyhKnLp9ZxH6ykg27VMdA5PZ1rN6dSpHDYHx7Ko+1fDJOq46n2IsFhl+PjDzw/4sX1kXJhL23klD1sqL2hxEasplYMkk4FEVUSq7WMqKOp1KANZZNoSDjsm6wrTyOY5g0UNVk9Mr3SvaDqnwv/ySGLGMXRo1XXCtbO8He1aVlIXL7OjafyAXLXnj1BCpcxzKWtjeIUDRT7eQ3CS/bIpJ3rWRlqHo/HYpg8+rlbDiShbHLKCb01phJpQwt4yUssc6KYMP+dINr/ADQ2gsPB8g9vplN6mVE7golJHgzcoUGrFrqvOwDoDibu5VWYOyBWQu4V3BbmVABR1UTyFpNL7sz7LV32f5VEN5NM4leNZPgFHXSDEdVoN5tMikpKVrDwXXaffM6zltDQLcm8Md+QparIwnxGeQA9u0UPfWq51vVQKyqP+KSPn2/Y+PRNLBw58nZjkz/ahHD7O6Q+PUc/DekgY8jjkDG71sV00PzIcsU25PA9nlai9Li3cYeaI57xwzWvuDPkq/jIOU7jqflAI6M/Isj+1/vh//y70gjjv/sOUMO4NhNvd3D17B+tjfNL25l5mB/lnwVrdrulL7YWwOZaZSt5WPs7G/gtRCrki6+bDywBpp6DlRkBLDDvrcd+cbdsGupHmXaDfsRnhRdvqDI++DSr2t+PWTY+VPrPvBOBnGHoog6FEvqbQOvnag+cg30U1+Tg1eXLitqz2ZWr48gtcJ7uTLWA2YQHBysNZR+PNjUi0mj3TDL1l5G5K5QVr4XRnKRNV4TRimCBRU8s7W2I/frlepzfgSb/hNGcpExLsN9sT4RWnqNjPg8lKhMMO7sTlVegVZ+z5hK2NcxZBm74+un2kYnvzF4WGQS+dW+x7zf47PcyGxPh+Fle9zK1Y58q27Y6+tar9NwbMnGsnvJRxUmmLjPpp3DJfIMjUQa6lKmditLBt0fat5XQW6KxvFv4DMhgMfzgapnTa17LNX7hM3HtZ8by/rTVpXl6qr4ODbsfrF8lT+fFRzfQURyEXaDxuLVVH0eeLINRWe3a9XAFhqibjDtud95bcF1UpWf5uXcYPsnyqCwgQx9t6aj4uPE4OuMUqXPXNW9brTBiX2s/lB9zO/fwbqvTpKLJb0GqM5JFV03damvxcZZxHxStp6Ru0JZ+UksucqHVgNUXC7ryLVwVkyfytIf06C5K37PT1HmeARY4PHcW3z0hTqW891WQpdPxaOqL/pEnaj5AHCz0fz9qx/Yv3+/3uHv3vruKCrzEa8MG8YwfcPXNX9j/2hJYoefH34ag26AV1WztmLageQJLWMJqdGq7/poL/NVPsJP3zJzYgnR2kbdpqZdx2sEiKfBR3r3g3i0hbNi9RdER0Xzxftv67zgOLnqfdbvjiZ693reX6X8sm0rb7//BdFHY9mqZ9r6qrS/xoJ72k3i5t1n32fXeO3PF9h7WZ23fTNGaOap1A1y84DW7nhpRleLiyhSfz7vNqAX1qQTu1dxI5Mbw8lLYNzaSbuWV/ZF4hRPyyeP/EYudrj307its/PC3QEyz8SQCpj164uLcQFxkTHaD3TFqRxPzNX+kh6AXC6eq/pj+Y3sXMAS194uWsGJosIqvaYW1VS7x7MTfbtYQ2YMu44oqu4VniTypPa4qh9zCk296OtiTMHpSJ2agqknksjFDqeOAE549bSDzCg+r6RJvYrZ4TF6FKNGj2LUEA9crG4QGfo2Ids1ml9Vr1PR+X2EXdSeGnKJ2RtLFna4D2ijTKw+g/dD5ecbQ9zIzQXa4K5o8qlI+mnV1bjkhcM9ChUt0mYdz2ftghQCPstSB4HNce2vv+5guTw8cDEuIuGnMFIVv2H6XtW5vYwbXj2s4VIsEYpjM/fISdIVNTn0Mfh61M8Td9MiEnaF6hyThsovzFeOKpdqvTKJ2aU4lwBcDCMqBYw7e+CpOT77N/YpzlMJ51MpwhjLqjwQXzrPSa19r97P+s6DQGp4FMnFxrj11FqbihlcxsukJyrv0QyQnUVuMVh27IuLZn9ehUVVCyQ3QAXXs4GWmLVVphjIyAkzSyi4XpWafpNVNW9xZOQXJcHP71n/Ul84tZEFE/upgqdq3j0daU4O0UudcXbWHoa8Hq0x3+m8+0IfmpBD9Gczy2qZhqaRATRv3R1VvWMV1Xwh7byyF2JNjnRv3RzIJlPd15OqP+IM0tS1ZaO3xJFGEzqO+4xZA5uTcziEl+arlq6q6ZxD2qmy7VFNn8hWxbY4O7sxsbSfYKVxuLdrAmSy/z1/NpYExwErM1U7zmk/LmFOSQU5gI72NAeyL+/RqBmdxv5/LtCugTvRHUcLyLl8pkqB8MppNwG9VadP4EfUrV1c+PQwzSb/i26Tn8dmqAdFR5dx2XgcbTQPIIAegbTJ+Y4zsXex6T8QqxFL6LXwr7S8vIn4H/W+KX8g1hbmZX9U4/ypzfBrp9NAD+yMMon6XPeaXBVltRbLhpJWOFT3zvqv++TGsO9EFti541XWCF/Fz2zZCcSc1/j79m8kXQVIJ/ZHzWt9JnEpuWBsj71W0KNiBt0zXgxj2/EsrPuNwcfFl4n9rMk8+D/2lbPKj4+75IcvJunWKLrPXkLbvgHYt77AhU0pWE8YpXhJ3JFWvnZkbNpMloM3Nh2epcPs9fQZZcIfn/yLbOWx8qCsLdEoZYbfH5bD4GdCIy88uxhTFL+dUD33WLXFoOO42gx5PsslZlsEqbjgM9odjwmjcCmOY/tX1bjXe+w0xUnrnFX92r8lDHm3VjWGX2d0GPDMVd3rxm8/Ksrj+QRSi8BY8xprKKNeuDuX847kYhhR1bixqt1yaShrfF5bwfzhjkAeSacevTLZZdoK3n7RG0fzLNIuJJF0GRx6T+btfwai0+hPA5T24ZrKYxgVxj9iif1xPe+/r5y2dtRwANidV/89h6daPTY9dT8SSmrW7lgVS57LBN0awqAbSC6vz109kq7lQUtHfJQJlSpbZsjRPCz6v1pxzd4KJO1Ur/eqWPKae/LqkqqvjXj48g5vZcXKFXravweIJ/zDFazQ03Y+JdMuW1rr/f/WNgv1y1+Lns3pqb4RKswq5BRAezNmvtQEx5IXxBaNUHcNBvl3UXaBWLFkfvwhjlxjF8YEBbN4tj8+Xey0AqPWVmZAG3wXaX8JHhwcrGqqxdoerVDSzcu6N52Jx4nLArsunqVf9jkNdMeuOJXYX1RP1/ZW5oAZHi/qLmdGP0vAGjutFzpZXK7GjVrBoQgiLxVg3S+Qd94JInCsJ056q9SImlJ3x3MbbKyg4I9k/V/sF2uHEKp+zCnYql4+mPUO0Jk++BVPLAFrByegDfbWFayXwZIJW6RqWn3551GkG7XB58+Typqso2ydMlITNEZqSMskC7C2rcEAsMH7ofLzjSGS90UQl22Mi18QwYvm4j/MDTu5pSxjgbrmfCOeGWqp/n8hV9UXzaF/bs6EvmWB3tKPMoC8vKp9je5kZwlkoPdwK0YRtFPVrKWtL4uVx8nyMTgB1nYVH5eGXo+cHKzLX69KFXG3GKxbVbwumqytzOB2OsnlFPD0zCwwsqe15ouN63qulVm55AKWduW8ZNEjN6OsaUYVdQ3m8s43xelkZAN2rbWv3RUxuIyXyEVntQxxO4qIg+kUWHkSuPgdggLH4OkoF2gAEpPIwwqrLq7KFIMY9e+DjVE22ed1jrryqQOOd078RxX4HLuEPSl3aGJnRfaPIWxV1PoZ1sFRFXD9r/Z4pWHrAvC2Ac7uZIHWF7+JZOQANnaM1Birmm8mGXEaI5Wcp9OxHZCZyM8plAVib6RxvCQIe3ATcX9Ac9eONM/cT/DzG9WBVHVN56I04krXvWT6DCparA7nJ+loB5yNYMnXmgnq+eX9ynevazesHNDOXhV8TkgDAvDu3ASSognWDBIDuNtjB2SkVN7AtuE0g78bmTNhAQtKm4OuD0HgA1wKXUh8NNi52WH5xEo6dWpD++dX4jp1iXpYTs9x3Wji+iy9Btth4eVPy+u7OfPeTM6GH6iFj0vMsLYyhtu5qg8dq3z+VDL82tnGzrrCa5Ghymotlg2xF1V1CVX3zuVfX1OvZgHWWGtdYCp4ZtO5FhZQcEf9r7IWV3ERYIxZFboNMfSeMXVXGCfz2uD7kg92mY9708+a7nInZiVn1n9OjpMHLZt50PWVobRwfZbuL5WUsSW4vhZEB3s72r0yDftmHXEdYcW1bQs5FrKSGxmVNlFRdbbWWAL52aoPEwy9PyyPwc+Ebe2wNqrgOauWGHocV4+Bz2e5MWz+OR1LD38mdYO4HZsVHyAKvfqbYn03n7SScvAgtX9LGPBurWoMv84oGfLMVb3rRiaXlYFassjNBZrbVfhBh16Vld17yhGVq91yWTmLnpNZGhpK0GhXTK7G8sVbLzPnk0etzSQ/pvq6YpoTywcvTuXV/5vDnJmTCfrhKqYuzzDtUaywXOMMiGFUGP9YytI66v+Xmg4AD1m2jEkdTSF1N/Pmz9M7hJ5QVFMQD0bdHHLe0R2E/ryUvcngOn4Ngcp8DyAy/Qo074pPRcHbaT1xJYlT5dTKjVw2WdVM9bSl1Qgka/h5KZN3Jj1QMFmIh6cRL/+7K2Ffd2ZLcFscTVF9KRiruiBY+NryzEQXPtzSlbCvOxG2pRNDW6vz/JKNZh0LQ+Se2MzK5avZdjCBXEt3fKfO5Z15Y3DSPPMXpBKj+BK8bFD3hVpC781TKjFnMsHODU87ABf6drOm6HwMUVoP91nE7VHOv2RQ9udRhJ5OvipXnMq+D5ezfH0EJ6+CU78JzFi0mIABddFXx+Oobo9ngLtFhtfcq9oxp1/WGeV0ZUNJjQmqvF4VKzgfwbodcRSZuTOxqv2h1RJD9oNB55vK5J5k83tvs3prFAm5lrgPD2DuYn19Bz2mhjuwaWdnvt3ZhZm91J9TZGQT+RtAE3xGt+XlpV0I29mZb7/twqYAa0wBsjIJ36Y9K8MUUWBYG3MAFFyM0Tk+SgdD+iE0+HpUtfUqk8TlTKBtZ+2PKx5RVak9/6AMKeMqVavVryl17zqWB28g4mQGOHkxYeZiFr9YjT6LG5qs78m8BBaez9GiCsEPAIwG0HqAE2T+yvUqNLdPP0dVwLGkWeRTm5j5xXFysMPbP0iROQD3VlQeMB3yLoueVn9Z1S2Ag1pNKy/CuznQ3JHuziUTqOdbSb+33vOG4W4MaYc3qvvwVfcbfCWOsnrD0Wz6NQ3uJLL1by9pfGWvrul8JU2jxq16+sw0jekNMFHVXHXa73sUtXTV8/vjAiFa40ua2c4gbQMQqO53OCNRp5bvooHuQCZpxxQJ1TaMZbs1g78lff5q9gk8nTW7lz3aQWDuUpx2lltXD3NmRSCx/wjgWORtrKwzyfjhO/KaNiX7u8Uc+8dMYld8RUZRJlnHYykqqIWgFEBTT9xaQ1FqApqvmQ0/f+pn8LXz7l1q7m6zplTzma0mGHrPWJxPfpHqzWdRQa6BTec+Rgovknspm2t7AoldEciRZR9w3doOowvfkXoqD/O7B/ht5UxiVwTyW3Qmdy/Fknsls9Z+dpfuLpiRSfJZjV/K4PvD8hj+TFhUWMdHiKHHcTUZ+nx291YuRUYAueRna6eJchzNYtqUFP554k6N1P5VMfTdWtUYfJ3RUd1nrrpXo2W3lstl+azxeW0Nn66YimfLuyTtDiEwcClbT+kLID5k7V1oZQF58ZHs1Vi9+F0nuYopjp0fKPIjakGNvv4wbaz+JKLwFidiT+gdLj96d631mA9Lp3likRPLR+p+dUNn7yAJV0bUZA3ZT3YQm2OB5/jywsqBrBnvqgpCK5M0hM7eQVJN1N4t6fP4QYPJQtQ5U2wsADN1tax7d0gO+52lW1R/eppAVoH6q0Ez9beZefmc+jqZtz7RG32tXGEmJ/dsYnXw26zbn06RrReT1P0g5RcUgZkxuSe0vwQvGxL01zJSyPzlN9Kxw32gE3T2pLtlLr8dLmvGIregCDCn6Kpy/iVDef15VE9BWhTbPgzh7VWbics2w81vEl41erUTKnV5PKte3li2cdHbT6K5qXZzQQ98zN0uoAgwv5upZ1rVoKoxoV4vJzdFP9YP6NR2ws4XYdzNlwklDxrXc8kH7J3Kabza0U7Vr/FlzYc4a+y0mlwCjNpgb6UYVx6D94NaBecbwxWReSqCTR8s5+0PI0kvtsbruTHKTI8lCwcTTBs3VtfsvU/eH5l8+l6Wqg+m1kZQcIfCe0DjxpiaNgLuk3XxMuvnXWNfFZ8bVWXIXn/zlU3NFOVQVQ7MjHOJ1XOMRB3S7YdQydDrkWq92uDSXTkHQ2Rx8EQqGLuV9gdYmazsAmjaBhftzqtKtbGzhqJ0UtXN29euLHJvg1k7F0VfWmrqsl10ORWDK+lWtYw/qIJUor5ZR8g7IWw+k4VZ5zFMGqDM9LjJ5sa+KG4budJ+4jOUVty3HkGbKc/RsjRC7kSrF17FqvRi05IW/i/i0CybKxFfU5WQ13Rndc1UjWaRCf2VxDxo4toHrZ56nfviaFNZwNSRRX8bT0fjO/z6wRCdZqKdnZ1ZcjAHsMLuafUkGvNVNotWavi7LHvaEXKi2bRK/dmYut/gtN+1a9tGzx6Cs9twFmjWri1pWjnteNlHZyX9DldY7VjXuG6ONCGHtF8Vn6+p55eZpvysTR18zkzT+uAt+7Ii35B3Gda58kC44VTB34Buzck5u0kj+FtCFQTedDaH5t0C6kEQGMi8VBr4LDr6T84ld8Nt2qvYp23i4umL6kBUJoW3rDC10ZqyBlni9bwvTkZZxEaqn3Ee+Pxp+LUzv6AIrNrjVoUmkqsqIztfdd0v5zZTVRssk8sazZ8/fPrvGTWv8E5jJ+FllUnU3jhoPwr/gY/9Z0d6ZHK75D6m+CSXPt4HT87Gw9eCS//7inz1RxV3c7IxsdR7B1Iz2o9hYm9LipJj2K++bTT0/rA8Bj8TqstzG5eH8fFt5cfxA6ns+czSiz/7ucHZfURdtcbzuQk6AWJRvoHO5jVT+1etsndrVWP4dUbJkGeuR+K6oW7uw76tvpUwQ91LRzXoL5e1RavW7+VYvlj8MnM+jNTuWu1RcjGPW4BJM2t1q2RqrjY0A25lVfRhgXgY5LRej6mafs4j9hPN5pxD2fGAzS3rimSp/w6SXCYQvlkZdA1kTfgEXJN3MFkdhC5fza1b6E5pClrUR3d458/nCJh3gUWvnmPM+GTmfHyXkvfyBz66RMBz8YwZE8+cxed5bco5xkxJYdGmotI8hjPGWKuZkiLSfz5OOmBpqXp7ePJsEkW0wXPEAz5e3I7hZBpYd/bAt587ZllxHNfodivrRAKZmOHuU8s1fUwVDRplxRGVmAtGlqg3WdSoujyeT5KcCrT1ZJTyy0trH4Z7aIejHviYu/4bCZlg1sMHrwpncJLjp3PBYTATDalpbm1XYTNlZQqI3b6f9GJrPEteAKjLmXFnXz1fn1riNcIT6+JM4k6oHhNUD2TWOHXWXi/LIX1xKffuTxEwNng/VH6+MYSxogwXXdrH8UuAZYULf2zkffwHY6bEs2jxeQLGxDPl1WvsKKmGdDmfdwKT+dP4c0x59TyL5qnKXsAbN/n+mmJGBsg6l0SW3jJkjPs4L8VxfJK4xCL95dNAhl6Psg7/RnqxMe4jdGsv6LLG2l57TMHBCGKywHpAIK+P1O4vXp+E386Qix1eY5X7QfWicrAzFJ2Po7qvZfStY/kSiD2XC3ZejNVzvnHyG4yLUREJp6uwNgaX8QdkZIyx5u9VnEVcdJKqWeyyiObj69LnXNibBO3H0/0vz2FqCmQf4eoPn5CwfjmnP1zO6Q9XkvT9TnKzASNXbAOW4dLehNvHPic9rSrh33F4d1Q2iwywlQtXgOad8J6oMXpqRxwrCZg6zniXyd2aQNJOQlYp67eqbPojA2iOY09v1Qh1jdpy+70dvojt702mY+NMotctKO1zd1y/TjQnh7RTyoCrHiU1nTWaVlZNDxl/lB/O1sfb0U61zxRfO6v6Mb5D2llV/eRSJcHnxGhVzWX1d29WrdXbD4AjQfPG09G4kkB4FYz8YFlZ8Hf0EkXwt8R+lowuCwIv+0CzYe5HkGULTEr/aIGppQmNTU3AxETrZVZjI1MaV6WfdUOZtmHwi68zxsWYrCPbCCs5YB/4/Gn4tfPksThysWPweD3XIh16Pv4zQMGxk6QWG+P2lJ7rq6UXvr2t4WocvxnQgk5dqOiesfSq0n4Mk/pZk3VkOxEHwoi4CE4j/av5ezVkVpi20PjTtgUmmNDYFBqZlpU+jEwwrko73VVg3X0Mr//FC+uiZCK2xZTW1Db0/rA8Bj8TXo/ht0tg3EXfc5Yua8Nv3ipk0HEMVbxfLGHI85klXpNG4UICYTsiifgulixrTyaNrd7+fvyY4GpPDdX+Vavk3VrFlMeJ4dcZJUOeuR6J68blOJJy9V+LjbtNxKut9jhDVFQua56eWr/TH9Fav1r2ciq5ENNuUwmZ64M1YO05leCXPLEoTCJ6l967e/EQNWbwa0tL/mj2W9UehJRcnvLnCUdTuBHH52H62yc3JE+V9BvDX9xtgRvEfR6mqgVRQ5o2bUp+/sOrsuw89Dm82zrQ1d8ff83BrzPp1hMIesoBkr/nlQ9PaE2XcuAanf188PQZgPnmPWQNfQ7vtreI37wH7ZwaOvjw3MA2OHRRLMt/HJ2vfEPk7yfYs3kz5kODCHxdM70rWTv9CAjWnrNq3XWXqVw3RvnTtVUbvJXb6GXO5ogTpet1K34ze37VmNHvkVzrOA6f/j5s3rxZI0GIB1fbZb/gRjFXc5RjtWVduU9OVd7n6ejPS0tfYmgrC4ytWuHk5EJfv2F0bZ7P6d3fEncduJJMQQcvPLr3Z1DPVlg0tqKVkxNO7l74jp5ID37h5CUAK9y8PWlXcJ6fT/yhXBBQROq9dgzt2x0nK2Oun/iGHxI1qlfeTiS9WR/6u3sw2LMDFqYW2Ld1wqmjB4NHj+Uphz+IOa9qa8jKzRvPdgWc//kEWktyHEPQ/Bd5yimHoyfTKdKT1+mZecwb0xXLJur5u/vwzIA2NEmPZssvKRRqzu8x0jCOZ/jjmgV9+nTCtU9/OlkaY96yHS69fZky0ZWcP4qwblHMH7HRnM+p2jEH7ejzlBvWWZrH920SL1vQp687HoP608HSGIuW7XBycsFj8DOMfbIVfxw5TzZwPT4Vi9796dFrMP07WGDc1J52Ti54PDmeYa3TOZ6YDWRj0/Up3Nq0olXTIszbDsbD9jTnL0O7Pk/hZp2le8wXpnDVog+enTrR3vg0MUk5pCbcpsMAD3p4DqJnSdnu6IHvpCl4tS4mOWwd35xXHelFmfdp59WVDh096WptRBObdrgPnsSk7kVcKbDEMl+7PGe36MpTbm1o1dqCoiZtGOzRktPnEw3cD5Wfb8z6BrD4jUl4miYSnZit97zS/y/LeWlIKyyMVecil35jGOZmSf6pPUSdrc0nx5pT2+WNu3D1yv0KmzC8m3OfqzeUY6soJ5VCx0G4u3bFq1crzI2saOXkzuA/TWbQ/atkWFtjqVFmrv5eQIf+HrhrHptOTrgP8MVvQg84eLL0+Faduykrr1ThelSYQvztDnj16kF/7560amqMlYMq35jxHtyPPq2q/WrUjj6e7WjXqhXFjazo0c+NgnPJZJPN+dNXserqgVuXPgwb2oeu7dvRspk1rdy98BnkxbCnx9O5KFK1vBvxpDbrQ/8e2ucS98ETef5pNyyzY9i48Rey76P3mC5l5Ya3Zzu4dJzoBPW5p9x1VJ2TzDXzqmUl6DvfuDP4T88zqrMlWUc2suGXkmn0rY9y3oaf62jXh6fczLV/NwCcGBP0Ji8+1Y6c2JOk39WTt90zzJs3lq7NTdXzd8dnlBdtTNOJ3voLKfXkAt20aVMKC2tnZe9fPkLWvR7Ydu9Da6+hmJLBrZSz3M3LprhAPRSbYd5nGi6T/4SdbTG50es4/9Np5awq8TKzFnXHJv1X/vVpuEbwNYfbA/7Enzq35l7Ot2zap/qRA6YvZFj7JqRFv8SmnzRmU2oya9a/TBeLTPb/cxL/OatMV3MeyctDHbHKu8x/tkYT8NoifNs3IS0qQGO+jng/E8Aby1awaoYvzvcS+S7Yn+mfla3ly68vonvLNKKnbkLZla7S9GlBPOGYw8nPNvLdOdU41fQ5xH/7Ed/+ppwCVW3mXcf44p+v0L/4I749AjCdl998Asfryn0GAW+8TV+7yxxd8Bl7bmomzGJRD5uy7fvNmP5/9qWLcxs6pO5nz51hLPpoHX9unc2d5lbw+48EbzUgqF2JxIgfybO8x+YZy8oJ/pZIYf//4rGwjGPJ37ZRyW1cuUxNTWv3mkcBJv0m06rxDQpbjsIp4CXsMv/HqfWfcMP2eTqP6MO9m1cocnia9h65XAk/XL37ffU52rywgOKmqvsYj8FPMOTJUYwfNRg3m/ukR33Ouu9TNJq+rcL5s+R8zB8cjy4ZV4Vr5/U4vdcil94+jB/WhvTYRLLLvZdL138NUrqbynk911eX3r5MmeRFq+Jkwj76BvVtps5zWBl91x6V8u55de4LDHjuq+ie8duz18HIiQnTxuN6J5ZNm46Qfb+QP85D18F96OV0m+PH/6jesfIQ1Pq9pVEP2j3pQf4NM5oPe4MuPi24EvpXzscUY/OnV7C3yuN2TnOsn3ga45RtZP5ezjFUCdXvX0TBHWOs1fd4PoN88B0/nqd6tcPyVhw7PtrEUc3ZG3p/qFoAT7lZk5XwMydKxhn8TFhISrye5ywnd7zGjMejOJrTlwGMaNfHk3ZtWtEKI6y698UtP57kHPVx36SQgmIL1TpqDPZGGaRnW+iUjUqPY8q/X7xT6bNV5c9nlgNf4sUBlvwR8SlhvxdCdjzXbfrj1bcrVknRxFfvp65ztV5GymNhgf+4u3zz99vodGtbbZW8W9NzPoTyj5PzBl5ndJ7VDXnmqunrhtY1Ut84Pc8YZJGS345B7q507d+HVuZGWDmontUmDy7maqY11pZl1x2d7dQpNxWXywd7J9GHUf5daXYpmm8OpKhq/b67lIkeNnA5ls0rFxASfqHC5/zaUF78RpMyj8XwV3jlKVeaNW6MlYs3E/39mejTnVamWZz8chUhh6vxBboeyuXqU1N5GjrlNxriERK5bDJ+fn66g/9SIj+Zo/r/bH2NLkey1N8PP785hJbOR/X/cv28lMnK5fj54ec3maU/l2ULna1M92OOnn5/y1+m9rrpm5/WdqnXq/xl+ClHCyEASCchJR/LLoMZNXoUo0YOo7vZRfaFrmPb+ZI8ucR8tprNB5PJt3Jn8OhRjBo9Ct9+LlhmHiSqvJd4+pw8SVKRMcbGqcT+otuMTOqu1azbHUemkRNew1XLGfVEL9rcSSDqWKoye7VkpCSRpTn/AW3IOrGD1esjyVVmFvVPWhgh/wkjLhPa9PNl1OhRDOsIJ7duYN8Vdds/Gh74mLsYxur1EcRlgpN6eaNGDqNX6wISDsVQOofiVMI+WEfEmUxo54VvST7bXJKTy/p+i9m2jbgscBo4ilFPumJuwDNq6u4wTuaC3ZBJ+FgCuTGErgplX6JG2X7SE7uCOPaFhhB6RONIvx3LpvVhJGQZ06avav09rRLYti6MVH0ddx3ZxrYzWdDWi1GjfXE1U6+gQfvBkPNN5dLPJ5Nv5VZ6Lhrmbs7Fn0NZ941mb3uibhQQ+3kImw8mk2upvj6M8MD+6j7Wfxan+2CaG0PoB5uJSsnHulvJceCLp4slGdFRFfcdClW6HuUeCWX1V1Ek51niNqjkfO+CyaXkspcvaWFsO5BKgZU7vqNH4Wl/t+w6kBvHjlVvs273SdKzzbHv6KFa3hAP3Do6YUkWmRrP9qm7Qli9PZZUys4lgzsbk35sB6tXlVOeDFHROpanOJWwVavZcTy17HwzejBuRunEbF9NyC4Dzm1KBpXxB3Q9laTrxhrz96JNTiw7/rOOyEo3+nFxl8Lo5cT993uu5zXFdug0eszfSK+/rqHH/62hx18/pM/8f9LFtwfmhUlc/DKIC/urGvzVaAJZs1lktehf08gBOroHqMeU9GMLHZ/X7NNXPRz7jL+te4NhdnDnxFaWfK01O22haWQATew64l3ufA+yedUsRjnmEP3xAp7pOZw5X2qGW6fj2Fq3WWX9vFXL0GpaWT09zfFeqmd7di/SmkNpcyVD+uLYXN8+K+kfOY3jiuYNVc1sa/bru5UlyzcRl9eRcR8cJOXH9xjJTuaog9t3CmrqLXsaG5crm30uz36Cl2/UXwP7kZHNjc8/4kbrodi3zybjv7M4teMARdzmTvRKzn7xI7g/i1Ovu1z8+IPKz6GVMHNRX79G++LV3Q0nyyIyTu4jdNVy1u1JLmlpssyDnj+rcO0sva/VuBYN87AnNzmZ0rvN8u7lDJR7JJSQ0H0kaFxfffvaUXB2H6GrQol50B1cgyq7Z3Sb6I+ndS4nd+0ou07nRhJ2JAtjaQpaW9pHxO+9jfXgfpgmfsVv7y0mI+Mu3DzApdDFpKY54/DMszRN+ojzPz9omMsOD/VvNmqIB24uNhhnJRCzcx1vv7eZWJ32Tg2/PyyPwc+EGuWx7JnGCxfjdFVLVKq5EfZ1JKkF1rgPH8Wofvbc1YzNNXUpXUfNwcdDf/Xdyo5jqOb9IlT+fGbpQ8BoJ4wv7Wfz4bI5Juz+kYRCVVPQohKdGpH8Yw3W/i1Rybs1vco7TqpwnVEy5JnrUbhuFBzfRMj/okjOtcR9iGr7POwy2PdxKHFVuwyCoeXygTTDZ+5HfLFiKh7WeQ+91m9Wzi3ABpcZM5lZzuDtYALXrpIEWAwP4oPXfHAoTmJH0FSWfrKDvUdjif42lKWBU1n0bbxyEdVm8LoZkqfwLreUC3iMNGLhmdKG6lv9d7h2ahU9FRzG372bQeI2hk3/SJkMBuapktc+Zv9znYALbBv2CjUwx1K2trZcv/4gX3cIIeojKfv1g9PYIGYMyCJsUSgxykRRSo5n8WhyYkzQDLyywlgU2nBKsJQ3IYABgQSPtSZmfUhZc6kNgK2tLbdu1dGrAzNXLLoOxsqtdWnzt8U3k7h5ei+5l2oqWCjEg2nWrJlc80SdeJyf++TeUhimYT5bGULKiCiP1yvBjHFMYMfiTeW0GFuX5Ubdhab6r8LLsXzxr6XsqLl4aTVZMGLRemYPrKBbnmvRfPD6Cg4NfIv1s7yxvpvEjr/PIbTW192AdTNEYRI73qqL9X10SQ1gIYQQ9VIbO2soyqcaH/UJIR66NthbQ1GBlGAhGhonB2ugiALtFutEVRQkkXfic9K3rOSiekjb87UEf4UQjyV57hOiMvJsJYQWIw86twUyL5OkTCtVl+XmFrcKgHt5JIWtYOr0RyH4C5DH3uCpui2zag5/WcHePE9efaEug78Ytm6GDBPran0fXRIAFkIIUf8YedDZCUhN5qQyTQjx6OvdGScgNVFKsBANix3uLtaQlUSCVMYQQgjxoOS5T4jKybOVEFqc/HxxM4bM+N/QaV2+RJ2Wm60senYqUwMnM2dDdGlPI/VHLCGvL2JRnQV/RU2SALAQQoj6wXEUgS+OYvCgUQQETcLNKIuYvbXdTIsQoqY4jQwkYORgBo8MYOFEN4yzYth3RJlLCFH/eDLptQn4DPJhwmszGWxXRML+fZX3fymEEELoI899QlRKnq2EAKeRcwl6LYBJIwczeNBgBg8bQ8DcxcwYYE3R5Ui279XuR/nhlpsssq4px9UjeSc5KcHfekkCwEIIIeqH2/kYuwxm1OjBuBqlEvPVhgbVt6AQDV3uHWNcB41i1CBXuBTD5g1hEiASokHIB2tPfEf74mmXT0L4f9h0vECZSQghhDCMPPcJUSl5thICMtKTyDdrj/ugUYwaPYpRw71wNc0l7sdQVn+o+0GqlBvxOGrEwjP3S/5o9d/h2qlV9FRwGH/3bgaJ2xg2/SNlMhiYp0pe+5j9z3UCLrBt2CvUwBxLSUfyQjyepOyLhkSOZyHqjpQ3IRouW1tbbt26pRwtxGOrWbNmcs0TopbJvaUQFZMyIoQQFZMawEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRqIOg8AF94rVP3HtBm9PXs/+NDMVLkIIYQQQgghhBBCCCGEEEIIIYR4LNV5H8A0G83fN87hqVY1Gbgt5GL4P3jjXwepyV6ZpB8BIR5PUvZFQyLHsxB1R8qbEA2X9AEshDbpA1iI2if3lkJUTMqIEEJUrM5rAHNrN/+YvoafrqhrAteAG9Frajz4K4QQQgghhBBCCCGEEEIIIYQQ9U3d1wCuitc+Zv9znYALbBv2CjUwxyqRr4iEeDxJ2RcNiRzPQtQdKW9CNFxSA1gIbVIDWIjaJ/eWQlRMyogQQlSs7msACyGEEEIIIYQQQgghhBBCCCGEqBUSABZCCCGEEEIIIYQQQgghhBBCiAZCAsBCCCGEEEIIIYQQQgghhBBCCNFASABYCCGEEEIIIYQQQgghhBBCCCEaCAkACyGEEEIIIYQQQgghhBBCCCFEA9GIhWful/zR6r/DtVOraMiyb1k2xAZSdzNv7Y/K5Kp7cg6rRrUHLrBt2Ct8pEyvZba2tly/fl05WgjRwNna2ipHCSGEEEKIx9ytW7eUo4R4bDVr1kw5SgghhBBCCPEIqdEAMM1G8/eNc3iqlaky5QEUcuHrebzyYZwyodZJAFiIx5Otra284BNCCCGEEEIIIYQQQgghRL1Us01A39rNP6av4acrhcqUanp4wV8hhBBCCCGEEEIIIYQQQgghhKhvarYGcAMjNYCFeDxJDWAhhBBCCCGEEEIIIYQQQtRXNVsDWAghhBBCCCGEEEIIIYQQQgghxEMjAWAhhBBCCCGEEEIIIYQQQgghhGggJAAshBBCCCGEEEIIIYQQQgghhBANhASAhRBCCCGEEEIIIYQQQgghhBCigWjEwjP3S/5o9d/h2qmPOVtbW65fv64cLYRo4Gxtbbl165ZytBBg2pKmnQZjZlE26u7VKPIuXqNYM58QD8jiyUV88HofWigTquPmr3zyZjARcksjhBBCCCGEEEIIIcRjQQLAFZAAsBCPJwkACyWj1s/Q6ukR2LdtihFQXHCbe8WAcVNMTIHi2+Ql7Of38J0UFiqnFqKKPOby0ZIhmJ6J4HCqMrHq2g0YRY97B1n66mpOKxOFEEIIIYQQQgghhBANjgSAKyABYCEeT3UbADan+7gZTBjYBksjyD2zieWbzigzPV76vMyyKV3g7Fcs+e8JZaoe7endC078dlGZUAOa0vSphXTyak3jgmtkHvya9N9+5Z5mkNfMFQvP8bQf0gWzostc2raSqxdva2QQ9Z3f3Pd4ok06v7y5mnBloh7m3XvjmnSCM/nKFAMNXcSm2X3ICPsTQf9VJlbdiyHfMtb2V1a/FMxBZaJ4BJnz1GuLedopnzPblrPpV2W6EEIIIYQQQgghhBAVkwBwBSQALMTjqS4DwObDX2fxiPaQlciJswWY8yubvpMAcFUCwN2nLCSgT1Mu/hjKur01GQQ2wWzkP+nW14rChK9J2L6XuxW182zaB4eAabS1u036l3/jStpdZY6KjZnLe0PaKMdSlHeDS7+F8+l3ZyiLJ/bm5befp4tGU9Sa0g++yeow5VhgyCusGNMR47x4vnrnU/Tu3XLWg8IicrNTiI/+mfBDiRrroqIKkgLZZ/g0eBPxinRt5ox8YzFPOhlD+i+8uVodVlX/9mbK7AAYHoCtaVUKALd8itdnP03b/BPsXP0VR5U7yhAPOQD8xIwV+Fkc5e1VO8nnCV75hx9ND7/J6u+VORXKOXb0H8OPiW4BLP5Ldywzowl5fycZyvQSA19h2YSOcGEnSzYm4jd7Lk+0kQCwEEIIIYQQQgghhKgeCQBX4GEHgAM/CGeCi3KsWk4sIf5LidQcN20N4eNdNceUSd6B3+zQCueZtNOPOclL2TrPE70xhSosM+l4LK36ljOfUnnErprM0p+V48uUrW8SO/zmEKrMUCqQNeET0F6TSub/ZHnbWs6yytlWzf1S6f79xIelm4PwbK5MVVHlUY4Vda0uA8B+s9/jiXbp/PL2asIfcmSk4zOv8OwAE84sWVd5kKs2VTEADO0Z+UYgTzpRs0Fg97/iMb4Ld899TsL2KO6VjG/2DM4zxmNjepfru//GxZPZZdMYtaaF/2JcWidx4V//IreigLGSOniWmxTN6SsAzbFvb49DG3t17fCvWL6pZH+oA8AmGZw5lkiO9py4cWEnv5xVjCwJulrlk2tlwtUdS/j4sDJPeethQ3MLG2yszDA2gqKsM4R/uIlojU0vDQBTQGJ58y7R7XkW/qU3NqA3AGx85QxHk3S2ivjvfqkksFw7qhQABsz7Pc+cCb1pnlvNILAhAWCnp/DvncXm7yqPDlYtANyR5//2Ch0vqVsj6PQ8C6e35+LGlXx1QZlXQe+xU94x/DB0xG/Gs/Q3OcOS/xjyS9YE1f7sbZ1B9KoQdl5Rpqt4T1/G+E5UXHYGPU/Qk+3J+H6lBIWFEEIIIYQQQgghRIWMlCNEPdHck6DwcNZMUybUlUDWhIfrD4jWMZ8lWwnXCf4CWOA5L5ytS3wU431YujmccL3BX33qbltdx+tbX9FwdcTSAsjL4VJVA0S1wNKuHTZmJsrR9cBF9vwnlJ9Tof3wQF4f0V6ZoRp60GpYFxpnHyF5p0bwF8CtBzZmgJEJtj0Ga6ZA8WVu7tzLTaMuOI7ooZ1moNz0nez8bic7v9vExx+EsPydb4jPA8vuQ/FTZr57g9PfleQvG3SDv0Crp+nuZEz6qR+4lGeGc9+RmCvzaNBej9WE/HMJb/3zU35OysXYujvjZz6H7p4uoqiw8nl7D+qKTVEBBeX0l1x047TONu18SMHf6sg/9hVrdpwgx7I34+c+T/+KdkZ1dfBi5JDqHWMV64KDdRE30tUtEXR2wKbwBpcqC/5qqNIxXKcssW9lg5mxcnxtSuSn8zcAezoOtFcmqj1B9/ZmkJ3IL+UFfwFsHLC3bEqdrr4QQgghhBBCCCGEqJckAPxALPDw9DAwiFjCAu+h3lWcJokdfn74qYeQo3mlKa7jt7L0Sa3MoK5JWpLfz88Pv9nK+qza8/Tz0615mnc0RHsepbV/tWvbKvOFHM2DtKVMLh0XQmxJRa6cWEJKx1dQO9dQ09YQ1F+9N7XmXbZMi/5BGoFyRQ3c5B3a26i5rlDptvr57SBJM3upyvev1vruLJuLRRcfJAT8uLDE3FQ5TlRPDQeB3UfgYAXZsV9ToKzFm3CaGwVA8V1unDuiSARu7SQt9hpmHiOwVKZVR/5RTlwsAGyw76NMNJz9wI7Yk07ij6r5GbdxZWhVA5PZ8ezZEMIPqUVg2xu/EcoZZJBysQBjp348102RVMJ8JL07mFFw8Q9yGvDxX+NB4D+v4Ntvv+XbLSG82Fk9rrkbS/+9hkXPtVP93dmfFZ99y7fffktIgObEVdDPHhtyyFDHf/u3soEbGRxT5quKGjqG66uMQ/FkAPadh6I3BDy8B86mkHvxaL35yEEIIYQQQgghhBBCPNoaM/i1pSV/NPttk3bqY65p06bk55dfLc9h2gesmfkMfSzjOXj8KpX39mjBiPkfMNv/CXrdPcjes2WBXH36jPKnqzVAFvGb95T21Zhy4BvSO47Du60pYEobB3M2R5yAPqPw72IDQFb8ZvboaR6wvHmW6uDDcwPbYArcvRTNNwdSlDnwWbIQv7aqt/Z5R0OYvEyrUWhSDnyjWLYzPn/ypk0T4E460d9GojtX/SpeXx+WBvmp5ksSO/60kB2laSlEfmvOAP+u2AA2bTqT/m0kKdP+jyAP1T4qaRZbWwqR35Ytp7JthRPs0dieiteX8vfFr21L17Wq+0jUvKZNm1JYWE7VxBrS+y/LmOffm5amgGlLevj64us7BMfr+znhOZf3po3G8WYm7Z+dwct/8sPX25FrB05wBcC8I09NeZkXJo3Hb6Qvvr6++A71wqMNXDp1kbJWef2Y+940Rre9RixevDY9gIl+T+Pr68uQXq25E3eStDvqZnf/73l62xkDlrT3Vc/TvQn7Ys6rZmXenfGvvIz/n8YyaoQvvk8NoW9nK26eiSejqIrLK2VJ7wnT+Yv/c4wdpVqmV4+WFF02oWPXlpB5hv2/ldNeql7ZJB5N5o5LD/p7etCh8CLHL2q0UVwFZv3+hIPDJdK3/URBaUcJaoUXuHk4jMtR33Pz8m1FokpxTjua9+9Co/Q95GYpU8vh5oVve0tyU/dRsttLOPUdRreWt/l9bxRnbwG0prdPD1pyjTMlx0WFuvCnPw3GJuMY/41OJK3QEa8+nbExO0l0vOJaVMF6qBTx+622ePVqhY1xIT8d/R2Azl6+tLfM5UzYJWx6OWJnkcf+X9OUE9NlyvMMa11I/K4LNOnVHsvci2XHWeveDOtejd9+jLrMXE/G8unpBE4ZrzpOvTrT+NIZErPa8sRfNMYP8cCx+BInFMeHuetT+L/0ApPH+fH0CF98h/Slg9kV8lv2xdEyl4v7YtC7S8pRlH6G41db0MOzL717tuDqibMa5aUCzk8wYUBr8s5vY+9vqlH2d7KITfwD245P4Mg29t58ggmDm3H6UAEDh7Qn4fsY3F6Zz9ONf2Lxy5/xa/51Snqx6DViMm5NLxPz3UFStRak1uo5Fi75C2N9ffF1b4kx5rQdqCqT3VoaQzNHhvn64uvrgUVUNPHlbUMFx47uMQw4PUFAYEDZ/h7mhUdr5XnMnI5P+vPyC5MZrz6f+A7zwr3ZDU4mZKC9KupzyuQJjH2mLG9ns3SKBs0tO+datlel+fribqa7ruVTneO8qjQNcOsG9r28cWxpjnlKFGduaCaaM3K0H65WNzn1v52l+0Z1jfCgyb4YzquXO7G9JWBMy+7qc7TWdcGQc7QQQgghhBBCCCGEeFxIDeAHcPWTt1gfm4frmLdZMaOymsCq4O/ModZkHQjl7a+vKjNUSeSyvWU1T1s61mGNUR98upRsaRJ7dQKidehJH7qW1uQ9pdtnL6GcSlb/t3lXfJ6EwJ6ldXmJ3ak7hba621afJSPKahnHR2r3sywapEtx0UQfOkNGIVCYwZlD0UQfiuZMelke++GT6HglnOVvvsmb73yq+qDAvD8B817h6Z72mNyI59gh1Xwu5ptj39OPGXP9dJvltRnK3Cl94PejqmX8UYCZXXfGvzJeVRst/Yxq/JUiIJdE9bpEn0hUTW/en5eDAvB2bkpO/DGiD0VzLOk2zZ29CZj7PF0Ui6t0eQCY0/8vc3l+YHua37mo3v4z3DDvwfgxHR+gidOL/LJhE+FJ0PGZAF4ZqrM3DGJmYwW513Rq/5r0X0i3/1tDj5Jhmj96K7Fev8yd4qaYtFAmVIOTH96uZpAZz4EqxES19PGmo1URl84fIB/g7FEuZoN9l6foqMxriLOnuZQHxrbt6a2TtocT6UWYdejNSJ1ar9480dkSMk+zR18z1Q/I5okAhjvkcPpwNMcu3KDIsj1PvvA84/8SgJ9LEYmHo4mOTeSGsT1dnnme5zVrKTv5MSPwabrbm3Cj5DhPLqLd0Jfpr7fapmHyz3zNus3HuGHdD/83nqO7zj4xTN8pc5n/pIP2yD9O88nveRSaWdACcLG2oPDa7ySQQEJVApRXvmblm2/y5ptvEp5UBOm/8Pabb/Lmm+EkFkL6AVXam2+GsLP87+LKp+8YdvJj7kw/ureES2fU578rJqrz2BtPlTUh3ud5AkZ2x6b4Uul5Ir3IkjaD/JnxjOYP0x6/uX9TnVOKSvJGc+aPu5hbW2qfc7MTVee4Q9H8qr8ZjxqWwQ8nL1KEDe37KUqc+VBc2xhXUr4T+fVQNNFJuUARGafU5+ijZ7hENc7RQgghhBBCCCGEEKLBkwDwA8kifOlsA4LAmsHf9cx+fy8V1/01RBJZJU0VN7fW6f/WdXw44eFlg25fwa5M0EgPD19DoCKHRf8grXmo+qZ1xbok6JqTVU7zx3XExbp0f+dd078mSdc097QPji1L/n+FtJLmp6et0drO8PBwwj8ILHdbVX0Oa+fX7be38v1b0o9zeHh4WTPWyTv01DIWDVHGsT3s/O40N+5q9uO6h6OlAQAzmudGs27bCXI1pus92Y/uVkWkH1zHklWf8rW6n811wcv55mwuxm28dZrlNWtlyaVv/8nqL1X9cm76IJRj1wG7LjzVCbhylD3f7eT0DVUAOL2kz9UDqsZIe0/2o4tlAfFf/5OQ/37Nzu928vXGlWw4lEGRdQ+eGq61uMqXhyqo49fNkqL0X9gQvI5NpdvxT35O5wECwOgEgQOq2+TszcsUKEbdPbqSsxujKGjaFJOmTTExa1rOhfQyBbnQ1K7qfbRathnP+HHjGT8ugFfmLWTZa0/QJi+R8K07yVBmtujC8++9x3uaw9sv6wRlvfs6Y1Z0iaSDJdG7eI5ezAXrjniX11RzheK5oXlgaskg/EgKBcbt6TVaOwBvP6Y/zmYFJMb8oLstGsy6Pa+9Te+9x7K/KLdKyQz7JvGEvvsxX6uP0a/PFoBFF7w75/LLJ6tVx9m2j1kTqQ7G9SoJxtnjN9GbNsa5xH+rcZz/N4R/bo4n58EOSO0g8HQ//c0AV8K+mQVgX3ZdAmjnxVJfFyyu/8GvwE+Jf2Dh8SJr3lvD/Ika+QzWkbY2xtzIiFd9KNCpLTamN7halWCyQcewen+TQfT65awrPVf8k28SVE2Ijy85V5DPH0c2sVzjPLH6/9m797io6vzx4y+BQWAAuYsKKqKCJVqIaeQtbU0Lr+RW7qZuWGv1/Zp91/pu2oXadPeb9E39fVO31TZtM9uii1Kam+alUBNxFVNQEbkoF7kJDJcZwN8fc2HmMCDDRUHfz8djHsrnfM6ZM+fyOWfOe96fz8ajFONA75BIU6A4dO7jjOvtQPnpz83qfsWWdX8h7h/HLdtczeXmx8vuAFUH07lUC15BkRYBWecHQunnAJdTmzsnUjnw9Vd8dVkfAC4+bWijd/5MQSvaaCGEEEIIIYQQQghx67P+3FrYoISE2EWs/bmpILCayP+Ma+fgr8LNDsSKdqH5Oc5Kl9TidlacbcjWNBnHyIFO+nFYd2RaTIEqfv70OJdxoF/oJMtJeSl8ctR8SZkczy4GXHC+boaq4T2LUkiwWAZk7j5PMQ70DFAE5lrwfvfc3R8nykndnYDlJyln15HzjQKvtiumthbAGafrfsYmePTCSVkGUFHZgi7/++LUA+pqbO+C2i04ksj7Iom8bygD/d2pPPk5f1rxPges9d1rlj1uehmzAk0mcXeQE7WX09lvtltSj5ynGDcG3hdpXrmF+uDcXVlm5tABzl8Fr+EP0rD0UKYM643D1fMcMAWiravN02elW7x+sfxU1hSkWh5Px9NzqAVqM5NJMNt+VQcvUQy4exkC1M6RhPZ2oDbrqOLYhaqTn5HaZGamDap01AIOzs6Yx3Bb6vMtWzlceJYD/9zJgVNAxmF2/fN7ckqOsfH9zWiAnPdfZ/VnKRSUpJFm7Xi5rlB6etZSnG3I/h/cEy9tMZfOKes177rHsP94hvZ2oDbzZ76yWM8qfj55kWq86GmMkiZ/wvvxpyzbwqzzFGgANy9DMPVuIgd5wdVTfPbhz4p2s5Oo2kXq5Vro0Y97TD+68OPB0N5Qm0nq961d61a00UIIIYQQQgghhBDilicB4HahYfeb1oLA+uDv0gd7tn/w17z7YyvSv4oiKqrh9fzGRjX40mx6VNTzjbpQ1vwcZ7GMRpmpVjKPW6NxRu2nxE5U1mqe2sf6mgT7WM/JBn8Cje+x8XnDZ/yy6UC62Wfd9+aj+vr/m9TM/rz+9qUsibioKOJ+1i9Ffc9SK5nE4vZVTfFlZUDAHRdHqC28iD43V6HqEmUaoIcXQ82Kq4szGwVEzpdX67OM/RUTGtG/J94jWarMNH0jEj/AyaOPxRwteT8/NyfQ5nPRWvZdnbLAVm5ExixhZogzlw/+lfeN2f42qC6+Cm4+OLX2KtmnFy7oqCywPQp3+aC+u93X477iVAl43TWTeQ800W+wKXvc7GXICjRynhxKHwez7p+Nzh0lswSc+g1lnHl5i/TGTQ1UlyuCzUap7Dp5mVqn/txtzEi/dxwDe0DB6V3Wj18ztcUplp/p66/YdbTp/Ei9aoqzFUeeplYfAK5RpCtX6csdHAzrNsQLd6AsN7nRsQtV1Cq6AreVc/BMfh8TSW/NKT5f+xmG8KpNNKfiWffOVuK/2Mj2JCBrD1u/iGfjO+vYacrQLeXgZ6tY8ed1+jot9PjLxvN6HL1xYOA0w9/je4PjQKIM5/wfo1uWu3zdY7i3Gy6AQ3BUo0zvt+eE4gR4eTcELd1CxzFzwXMs+a8/8uZbK1n5l8cxjdAAQB/c1c20ja0WxRKL9RtHb6D3WMt1XjJNOZ91e05cpBY3+oUbotv+kQz0hdrLqexqfOC1kO1ttBBCCCGEEEIIIYS49bX20bZoxBAEPmQMAkcQ8fuVLH2wJ/nfxbVv8BeYMGZIQ/fHN3TMWLNxdQlm8s0MWG482RCwHTCscRfLxDBsgOG/ZWfYt3cf+1KNe0HNkDHXW3fLzzqsUTfa7WPfm+tJMnTnrb7nGZuD3+IW1uZAaPupvWIlI9P4Mo4VbCtdbTtk+ipZBn9XN8qUbpnqzFzq7PrS406VclKLuNwdhlN9FuVnlFNarqogkS2r95BZ60C/iU8yqYkYcPP8eHB4PxxwoN8DbyiCbU9ztyfg2J8wRbfh13VvKAGOUH4ppcluawt2/MzFagf6DX8QP/yYOWYgTrWZHN/V1Bw3X21tk/1at5op+FuVyuf/u4WfWx3o6zif/FkfsI07UgyaVD43jPd7tAiq0z43jP/7En+Jt23fXe8YLr+oH6/W6uuXS/qxwue9yqtPRhE52AuH2mpyUn/m50PHuWzlpqq2tr1bFMPYu6bXecqB8nTLdW3xOMIHT3GxWp8hfTfgd18oflRz8dgeZU2bdUgbLYQQQgghhBBCCCG6LDv/Dx/A+BJtpWH3CmMQOJbYaYHkfxfH0v+X2K7B35i1ZmPGliWxXpmZ28E2fdWQ+Wota3XCa59aGXO4aaaMWtPrUWJblLG3iS8N2bMQzKytsTSsSQxrEmaZsnbT98ayD9j35m5T0NjauiuZf9bgmdbGUm4P+4jda1orImY2DmULoVdGpRYcfPpbjCFp4mzIgiu5xCnltFarQlcLDnZVJCozTY0vw1jBtqiqrQW1H/2sZSCrHVo5BnD7BH8B+OUHrlSo8B4/33o30M1xnUOvMBfqzh2htI2Zo1Tt4bOfLlPr0I/xc+8xjXfaYv7jCfWF2qLUxkEhQ0CrGGOQtoWc7+HJBwbiVHuZ4983t+8TOXC2HHzDmDJ+CmG+UH56D3s6YQCU8ioqAS//kcopgF/z3V03wyL4G/dBpwz+mgvr5Q4lBfys/wu/HrXkZ+r/ajVrx7BhezvX5TduT8wzvp0nETnUjdq8RN5b9ifi1q7m/X98xVdfp2P43ZTxTdDVgpNfMMZRnduHYexd0+uyPgB82XJdWz6OcCJHL1SDuj93hw9k0mAvqM7h1CFlPVt0TBsthBBCCCGEEEIIIbo2yQBud/og8MrNCSRsbq/gbzCzzLpInmXMaiWdL+fqA5tKwTPNu1ROIMEiONoy6nuWKrpmXqPPst0by6NfNaS7KOuZgtPtynIbJCQk8OlrE9j35qN8aczSdY9gqWl6Q/BX83OcWRfYm3jerOtmy3VvmMdE8Vkttut/RSjGezZnfX2btPH5hs8xYFYHBZpF13eAU5nV0COUKdMMY5eaOHPPo3fTm1oupSYqptnCDa9h5n8nkn65FrzDiBppc/ixSYmZBYAXYQ8rgprOA5kTObAVAeB2DP4CkEzevnTqeoyi/5SwhuKgufT77Rh6GP92CyPwsbm4GP+2C8N/wWR61GeRuesH02xtUfDNlxwvAqeQB5kTrpzavNAHQvGilkvHPmgcFDK8Uq8AvgOJtBaMV3AOnsSTS2YS6lbL5UNfknCdsXFT44+SWetG6IOhuFFASrMB45voXCoFGnDodw8z+1pOchs/hzBvy7KW6GrBXxhKH08HigsN+2hYH7wcyihoh1+TNDqGzx3n8lXr29vCIC/cgNqrly3GdnYeexf9LS7AiaRkVoNnGFGN2kYr3Cy7yb+Rjv98nnKc6B/5IP08ofzsAWxrsZ1w72X+d8e00UIIIYQQQgghhBCia5MAcIfQkPjZBjZ81h7BX+v0Y/xaGVf2Rtn4PFFRcaauiy2lc7LRmMMdZ9Pipsbj1Y/D22js4r2xPGo29q6S5uc4ohabbVnDGMGmAK1C+ldW3qMVLLON1yimCqGX+I8EUssd6D32Od78ryeZM2MmM2fM47nlr/LIHW6Un/6KD75vXaQptagYcCP0wSeZOWMOz82LAqrYtT2Ry7VOhM55lVefncfMGTOZOWMm855ayh/fXEKUckEtULVjP6fKwSnkEV42fo5fP8nSl54mtKbAxq6h2zv4q1d/4h3Sjl3FZcRiQqePQWUHXNrN5W/Wc3rdn0hZ9ydSNrzDxe9269fXdQy9Fy2mt5uO4u/XU1qhXGJrZfLZv05RjhtDH3zcMvtb5UWYYX9YvMaHApGMG+wG2oukfG8+k7kCvku9DPgR9oBlXrlbb+Py5vH04iUsfXUlb/z+QUJ71JL5wwf8tSXbuWoXxzOqcXBwoDbrON9dJ2Bs5OAV1vgzzZjJuDsA7mbeq2/z9ltLiGpB0LpljpOQdJlaBz8iF73Kc781HOPPvsrLv1JRXKSs37w2B3/3f86edB1B0+KJj2/7a3qQjoz9n3NQ+T7mnAfi51ZLcba+u2DnID/cNAVktnCfNU95DKfy2e5Uyh38iHz2TZYumGPYx3N48tmlvLp8HncDnDxPfjU4hUSZ6sx56o+8+qAXlRaX8CoObLHWNs7hycV/ZOlvjeMJp1JwFXALZcqCmcz89XPMe9h8OTfA6Z/JvApOffvhRTmZyTb8KOJSGdVA7/DnmDNjJk8+9Th3d1AbLYQQQgghhBBCCCG6tm7+/v7XlIVCz9vbm6IiG5/6CiG6PG9vbyoq2i1614y7efJ1fTDkkzc+4LixeNoS3h7rReq21/gg2XIOAJyHMuW3U4gM8sPJkCpbW17A+aRdfLLzFA2xpiiWvD0Or9Of8NqHpqXrTVvC22N7c/ngS6zeYSzsx5Rn5zGxvxsA1ee+47W/6cemdA6exJwZkYT6ueFg+OlQraaYS2cOkPDPREN2no3v5zyUmb+LIryvF052QG05Baf389npgcQ8FgrWlmNF6NxXefIuZy7/9AF//fq82edvDz6oo/7AoOE+UJlLwb7PyDuRQr15185OwbjdN4fAe4JxopIrCX8iO6XQrEILWdtGJs6M+/3LRAU7UXzkPf4S76U/dprqhuDyAV460ps3Zw3EIT2BZX89oKzRwHkKz706kX41huPQsB5KtZpiCjJPsf/LBI5fVU6FqCVvM673ZQ68tJoE8wl3zOPVBf3I/PBPbLHoKld/vPS+fICXVhvmCH+SNx8LbbLbbf22uZt5rz7O0O6XOfB/q/VZyE2dM4blNT6WrLw30G/8POaMC8XPTX9iVZdkkrzjA2ofeMP6Z7PGZxLPLXmQfjWpfLX2AxKtbKuWCWHuy08R7qkst11F2ues2nTYyg+l2plNx3AmbnfNZN7UcPp5GvZ4fS21mmKLtsx56Ex+P+seepv2yXkS//lvev/2kcZtZ4+7mfmbBwkP8LJoG1P2beGTg4bxi/tO4bn5E+nnBtRXc373a7zfomEnAEIZNyMUztnS7XNjftF/ZOkoLyg6Stz/fGZ1HO27F7zJ43cUK445Z+6Z+xxRw/z0beaVo7y/6jPOt7iNFkIIIYQQQgghhBC3CwkAN0MCwELcnm5cAFi0j1Ai76vl+E/tHfw1UqEaMp++U0bRw9DXc11lJfUADi6oHPVluqJksj7ZyNWrOvOZxW3IeWQkd59NbEPwVwghhBBCCCGEEEIIIVpPAsDNkACwELcnCQCLpti5hqO+KxyPAB/TGAq6K8lc/fePaIoqFbWFEEIIIYQQQgghhBBCiBtPAsDNkACwELcnCQALIYQQQgghhBBCCCGEEKKrMiYwCSGEEEIIIYQQQgghhBBCCCGE6OIkACyEEEIIIYQQQgghhBBCCCGEELcICQALIYQQQgghhBBCCCGEEEIIIcQtQgLAQgghhBBCCCGEEEIIIYQQQghxi5AAsBBCCCGEEEIIIYQQQgghhBBC3CIkACyEEEIIIYQQQgghhBBCCCGEELeIbv7+/teUhULP29uboqIiZbEQ4hbn7e1NRUWFslh0As7OzsoiIYQQQgghhBBCCCGEuKVVVVUpiywMnPUS5798m0GPLKc8+zT1uhq05YV07+FHflIC3kMnUHRqH/0e/D1XL/yb7j186WavIu/Il8pFiZvgapmG8BHhyuI2kQBwMyQALMTtSQLAnZcEgIUQQgghhBBCCCGEELeb6wWAPQaNovTcETwGjcLOQYWdoxPaq1eoq6lEk3sORzdvtOVFuAXeib2jM7rKq3T36EnxmR+VixI3wdUyDX/4w2JlcZtIALgZEgAW4vYkAeDOSwLAQgghhBBCCCGEEEKI2831AsCia5MA8A0mAWAhbk8SAO68zAPActMjhBBCCCGEEEIIIYQQoqu7Wqahh7taWdwmEgBuhgSAhbg9SQC485IAsBBCCCGEEEIIIYQQQliKjo5GpVJx/vx5HB0dSUxMZMqUKahUKrp3705FRQVlZWW4urpiZ2eHSqVix44dTJkyhZKSEtRqNVqtlurqakJDQ7l69SpFRUUkJiYyefJkdu/ezSOPPMLFixfx8PCgtLSU/v37U1ZWRkVFBYmJiURGRuLt7Y1Op6OiogJXV1d27drFlClT0Gq17N27l6lTp+Lg4IBOp2PXrl28+OKLpKamUlNTQ1FREb6+vuzatYtf/epX1NXVodFoCAwMNL2vSqVi586dRERE4OHhwffff8+TTz7JyZMn8fHxMX2uX/3qV5SUlODj44OHhwfbtm1jyZIl9O7dmytXrrBq1SomT55MfX09/v7+/OMf/yAyMhInJye8vLyoqalhx44d/P73v6e8vJwzZ85gb2+Ph4cHDg4O7Nq1i1GjRqFSqaivrzfFExMTE5W7pkU6IgBs7+rqGqssvJm6+4dwb+R4xo0fx9j77uPe0aMYNWoUoyLu4q4hg/Fx01GZX0RFnXLO9ufi4iIBBiFuQy4uLmi1WmWx6ARUKpXp/7W1tRbThBBCCCGEEEIIIYQQ4nZUUlJCTU0N165do7a2lry8PK5du0a3bt2orq6mR48eZGRkoFarycjIoFu3buTk5DBs2DB++eUX1Go1JSUl2NvbU11dTUVFBdXV1eTl5ZkCsD4+PlRXV1NVVWV6n/r6evLy8iguLsbHxwetVkt2djZqtRpPT0/OnDnDtWvXcHR0JCcnhwkTJpCZmUl2djYlJSVotVpqamro1q0bFRUV5OfnU1JSQkBAANXV1WRlZYHhWXBVVRUhISEkJyfTs2dPqqqqyMvLo7q6Gnt7e3Jzc02fyzh/bm4uFRUV5OXlodVqOXbsGDk5OVy+fJnAwEBKSkqorq4mMzMTHx8frl27Zvr8OTk5dOvWjcLCQgDq6+upqqoiNzeXkpIS6uvr8fDw4MqVKwBUV1dTV1dHZWWlxb5piZoaHU7dHZXFbdJpMoDt/cJ5OGoM/V2VU6yrzEnmh+9/JL1MOaX9SAawELcnyQDuvCQDWAghhBBCCCGEEEIIIcStpCMygG9+ANjOnTsf/DWTBrk0lOnKuJJ+nrQrlWiunKdYFUighwvufUMYGOCFi72hXn0l6Xv/yTenOyYKLAFgIW5PEgDuvCQALIzsR/wfYVOC6V5fQtY/niI3W6OsIoQQQgghhBBCCCGEEJ3erRcAtuvFvY/OZqSvIaJbcZEfv/2O5LwaZU0z9vgOncAD992Jb3d9SdmJz/hwf66yYptJAFiI29OtHQBWEzDxERbOnERYHzVkbCd66WZlpU6rIQA8Fq+FLxDgoSX/yxlcPAXOD33OsBFqdCc3kvx1vGLOlvF6YieD+isK67XoSvPJ/eE9ck+fUEzsZFyi6Tn1QXz796Ry3wwuHFNW6Dzs7n2fkQ8EAlBx6DV++f6oosZIej3zJn19gIoTnHr3jzSEeP3xfvLvDOyj/6v+/DaOftLUcTwSrxlP0at/T0hbzS+7flBWEEIIIYQQQgghhBCiS3vooYcoKytDp9MB4OfnR1VVFQ4ODpSVlaFSqdi/fz8AU6ZMoa6ujrq6Ovbu3cvEiRPx8PAAICsry9R1tJeXl2l83ylTplBWVoadnR1ubm5cuXIFDw8PKisrTeMEX716FT8/P3bs2MHkyZOprKzExcWF4uJiHB0dcXV1xdfXl4yMDLy9vTly5AgFBQUWn+N21REBYDtlwY3jwrCZxuBvHVeSv+C9D7ZfJ/iLvu6pPXzywSccytMPBOw+fA4L7u+lrCisiZnLb75+huH3Kyd0tD4M/+hlfrN6hHLCzXX/ZGZ8/TIzXjFEEYS4ZakJe+hZ4jZtYc1z0/XB3y7NE3tHAB26En2JSq0fH7hWV2xRs83sHFF5BdI3+i8MmTBSObVz8RxOzzsCUbs43swLfIvUnzhNqeH/rsH30zC6s4HX/Xj56P+ru3DULPgLkEfpiXRq6oHaEnJ+/NxiqqXheA0LxNXdEfvOvlGEEEIIIYQQQgghhGiFS5cuUV9fT1ZWFllZWRQWFlJUVMS5c+e4cuUKdnZ2BAUFAXDu3DlqampMY9VWVlZy6NAhDh06RF1dHVqt1vSvcXxbFxcXrly5Qn19PX369KGuro6ioiJTL41ardb0vsa/i4qKTMu6cuUKWq2WzMxMrly5QmFhIdeu3bz81NvBTcsA9or8Lb+N8ALqyE38hM+SWvPA3oVhs3/HhAB7qC/j5Bcfsu+ysk7r3ZIZwDFz+c30HpxavZ4TNzQJqg/DP5rH0KLdfLykE6Wk3T+ZGUtGwNEtfP3WJeVUcYPZOdjj1EPfHXz11Urqa/U/8rjRbskMYPVcVm6KJkQFlGWw84yKqaMCunAG8AL6LJ2ON+mc+9N/UIwarwWfMygQir6dyvlWNjMNGcDG5XqiGvrfhMwYjtoOqDzBqXfMM1E7mT5vMuzJkTjTtu3QtIUMfDUa73ZZfiC+C99nQC+APC688zuu6O85AbC77++MnOgPaMn9ZAZZ581mtUnDOlcde5uT397Qi58QQgghhBBCCCGEEEI0qyMygG9OANh5GLOfnECAPdSlf8d736Qpa7ScXS8mzZvDne5A0VH+8fEhWhNKtkYCwO1JAsCiac6erngN9MfZQw123QCor62nulRDyYU8qkpubLjtlgwAo2buW2sJz/qQt94/SOmCOOKnBXXBAPAz9F06HX2HJM3RkPPBI1yy8bRuHADWc5/zNUNCHRuVA2A3HPeJz9F3RCBqR31RXXE2l6x1Ge0xDd/x0+g5OBC1k6GsVktVcTqXtv+JolxDOrMZu14L6fXARHoGeKJyAOqhJvcoF774H8pKNRYBzua0PWBLOweAQTXx74Tf5w9A0bePcP6Y8VxX4/XE5/p9UXuGM3/+L8qwDHCbaxzYvZ8+//kSAdc5UBrP50n3Ua8yMHIIrq76kvqKPK4kbiHryA/Um9UUQgghhBBCCCGEEEKI9tARAWB7V1fXWGVhR+s1dir3+neHuov865NEitoSgr5WQUaJB2GhPqhcPLHPTSbjqrJS67i4uJjS128Z4WEMC3Gi4HAS+ReVEzuSO/6zh+NXlU7KrvYfr7nVgoIJHd0bLp8g7UC5cqq4AVx83OkZ1pfubs7QTR/8Behm1w2VS3dcvNzQVlSjq9JazNeRXFxc0Gpv3PvdGDpS9m5n97EsqgHumsyjIZ5QmsY/d3fycW3NqFQj6REZgjF22jQdZcf/SbmNp7Xz8N/i7QFQQvGBb9FfAdSoRzxupRywe5Bez7zCwME9cDQMZw9g59yDHnc8gKdrIQXn0k3lXnPWMDCkB44ODXWxs0el9sXrrvuoPfM1GrMsWPsR/0f4o/fh4eHc0H1xN3Bw74NvT3sunUwGwvEafwf63PmmVZ37mOI2N78N79Uey6u/GoLHPUE4At2v1XP5F8OxaDefPlF34NIN6s5+S8bpU/py9/vpeXefRt1F1+b+RP4584taEO6j7sP9OgeK5XxD8Hr8/7hzpD+OhkA+QDdHV1yD78O/nzP5J5Npyy2LEEIIIYQQQgghhBAdwaP3nVSXXyEiIoJpQ3rj0l2Fn7srw/v6c0eALz1cnOjn64mbkyMRA/rg18OV/r4eDA3oSQ8XJ+4M8MPB3o5B/t6EB/Wiv68nHmon7urrj1e/gXh7e3P//fcTEBDAwIEDGThwIH5+ftTU1NC3b198fX0ZOXIkHh4eDBs2jIiICDw8PBg7diwpKSmMGDGCIUOGMGLECK5du0ZoaCh+fn4MGzaMIUOG0KNHD/r374+rq2ujadeuXeOee+7Bz8+Pfv36ceedd+Lh4cEdd9yBvb09gwYNIjw8nP79++Ph4cHw4cNRqVQ8+OCDuLm5MWjQICIjI6mtrWXChAkEBATg6enJHXfcQffu3YmIiGDAgAF4eHhw3333ERAQwODBgxkyZAg+Pj64uroSERFh0/ur1Wry8/MZM2YMAQEB3HXXXfj4+JCdnU1ERATzIoJRd3fk3kGB9Pf14OTFXJy6mz2UbAc3YTS8AO4Idgeg+MSPpLVHOk3mUVJLAFwIDQtRTu06QiOIMIx32GKhE5gQqiwUomtQuTjiPdAfBydlOKeBg7MjXgN74eDcvo2f6Ko+JCtuNie/z9D/mfsdR/80lSN/ikffX0M251ZM5cifbM/+tcouEOdR/0Pfvoa/LzWMWwvgPOUp+noBaCna/Zp+XVat5mKu/gcE6ruj8TaLzNZXlJC/byP/fncuR/40lSMrnubkwTzqAOz88Y24r6Fyn1cYMiUYe4DqbC589B/65f/Pf3DqmxOUmZLUN3L+T1P1y/vgqCk4XfStoczwamu2boco/oFi/bAg2A8Yjv7uALjjDjzsALQUp+1oqH/pNU5a+ayN/cCl/2f87MZjQ5/xa75NzLN/7UY8x4CB+nZGk7yOoyumcuR/XuPMaX1Wsn3/KfQaYKouhBBCCCGEEEIIIUSnUVmifxhaXV1NWVUNheWV1NXXcy6viMLyShwd7KnS6iiv1uLSXcWVMg319dcI8HKnrr6ewvJK8koryCy6SmF5JdraOrS1dZzL04/zq9FoSEtL49y5c5w7d86UQHnt2jXKy8spLy83jQ187tw50tLSqK+vJzMzE19fX7RaLZWVlRQUFFBeXk5RUZGpbmFhIY6OjlRVVVmdlp+f3+QYxPn5+aaxh7VaLVqtlnPnzlFeXm4ab7iyspLMzEzKy8spKCgwjUtcVFREeXm5KSHMOI6xVqulT58+FBYWmtbJ1vc39jBaX19PVVWVaVnGffRjWhba2joyC0spLDfLCGpHN74LaP8JLPj1MNwp5uiWf3DI/El6G3SPeJzfR/pCVRrb//Yd7ZHcemO7gJ5M7NbFRNQlseGFWBIMD8SbFfoEcW88SmjFPlbGxJGonG6NWRfQ6QNnM+7+YDzVDlBXy9WcYyS9t5c88x65vXsSvHQGQwd64+oIUEtVzgkS1+62rAcQFsLQpyYyJMDDkAlXS1XBMQ48tZfCJrqA9nzlGR4a6UFV2nYSXvoFLYDam+BXohke4o2zPVCnoSTtJw68dYwKU0/AI7j/68m4H91CwoEA7ntyHL09HbCnlqqcYxx4bS+FFrvOgR6LpnPfOMPnpZarmT9xeKcr9y2SLqBvim7g2d8Pr4G96Gbo9rkp1+quUXTuMqVZV7gR6Xe3ZhfQCl22C2h9578OY9dzx6iecDGeIx9tBP9XGPrUfajr00lb8R8WQVpbNHQB3Vh9wQnOfPxHGg6NaPr+YSG9XGhYD6PANxm2QN9VcfGuRzh3tLluzBu6Va5L3UzSZ9sAUM/4mqHDHG3rzrrdxwBuWVfKNq2jguqBrYTf62kx1q/ps9ee4cz//Bdl1n4sZvZZG3flbK4lYwCbjUdcepST/+81syzvZxm0fBpeQFXyak5+853lrEIIIYQQQgghhBBC3GTDhg3jjjvuoLS04cloWVkZ58+fx9tbP3hceHg4V65cwdfXl7KyMoqKitDpdKhUKhITE4mIiMDd3Z3c3FwcHR05ceIEs2fPprS0FI1Gw5EjR/j9739PRkYGFRUVuLu7s2vXLl588UVSU1NRqVRcunQJPz8/ioqK6Nu3L9u26Z91iuZ1RBfQNz4DuKevPsOn6gq5rX1Cb0VNTq5+fEBnX3pd90F1Z7SbVX9JIF0dwaJ3Y4m6XiawMfhLKp+uamHw14zzfXOZ+oAPxf8+wOGEvZxIq8C53ygmvTwZT7NjrP+rTzI6xImyE/s5nLCXo/8uwj5gBJNenkwP8wVOmkzUW7MZHqCiMFlf9/CeE5SoPBqN1Wjk+tw8Hhjpgfb8brPgbx+Gv/c0o+9wosSwnKMpFajvmMyM1eMxDMnYwG88U5eMgtMHOJqwlxPna3AOGMWDb47CPF/U85WniJoagro6nRMJezmccIxC11E88OTwJtdPdCw7e3ucPFyvG/wF6GbfDWdPV+zsbnyTJTon++761qCqyNC9sspRf0ErK6bGomY7qTxDmkXwF3AJxNmY3ds/mlGv7mx4GYK/AM6+9zTM43g/Xg+9z9A/fM1IU/2G8XvtnYyt3HBc/Q2tWNlpilsRWO0qdGfOG4KtjngMvh+4H4++hs+ec9p68Lfd3YOz8aLmMZJh5vvSEPwFcPYKNJtHCCGEEEIIIYQQQojOoSUZupmZmWi1WjIzMyksLOTKlSumzFtfX1/q6uqorKykvLzclCB16NAhKisrycrKAmD79u1otVqqqqo4d+4cAD/88AOFhYUcOnTIlA1bVVVFWpoyi1DcSDd8DOBed9zDnT27Q1kGh1Jy2u9BfYU7A0b1xx0dRWn/5mI7JO/d6DGAdflJHDzjTvjkCUyeOJiyg/s4ay3z2zz4+/pSPkpVVmhGeBjDQvzxcsvku6e2cX7fJUqSL1GwJ4nz3oO5c+ggPL1OkX64GgC3u704/39bOPVlNiXJlyjad5zi4SMZ0NebuitHyM0A1Hdy31v341+XyU/LN/JvQ92SI+lc/OqMPjCvGAPYMWYuUQ8FQsZuvv6vY/rgL9Djv3/LmOBqzqx9j0ObG97zvNsAQu8OwflaItm/APQm6PFgvD3g/P+9x8//MHyO3aeomTCKPn3cqUk9RmEecP9kHoweoH+vZ/aSm3yJkuQMcr5OonjkvQzwsUMrYwDfcHYO9rj19kTVwq6d62pq0Vy5yrW6jo8G3ZpjACt00TGAXadu487ZT+BjCI6qet9HwPjfEnCXYVxYpz70HP9bvF0vK8aEbZmGMYDTOfenp8ksDME91B9HR198+/uSl3y4IQnd+wF6jehr8WMTa7SXfqDgfDa4LmTg4qcICOyBo8oeqz99KD1jGNd3IO6R4+jhBNRcJv/ID9Qq61pjNkZue4zRCxcp//ljLh0wvpxxNowBXPTtVFK2GcttH2/ZpBwchuvH61U5aCnI6EOfcfpxgYsSX6M4V6ecQ8/sszYeA9hcw7jFTde7D9+J+jGHm1V4hkunkpWlQgghhBBCCCGEEELcVNece3Px3EmCg4MZ4+9M5oXz1FWWM8jHjQD37nSr1dKtqpyivMv4OdRRU1aCu3097tdqqCorJchLzZWCfJxrqxjoraaH/TU81E4Ee7ly+fIl+rg5MaSPLw7XaqlTOaPT6bjrrrsICAjAxcUFJycnXFxcKCoqws7OjtraWgICAmRMYMP7d+vWjdDQUEJDQ/H09MTPz89ijODz5y/cCmMAG1RpDIFBYU5zcgPPL/uy6Uzg0FmsWN7K4K+ZvMN7KVH0SKp97wgXteAzINhUlv3n7Y26es47nw+o6WHsJvWx4fR3rOXil1u52IIfdDjOms7k6f0gYzcJyxuCvxDM4DAPyD3BqT0Ws6Dd+gv5OOAzqI/lhMyfOWFRV0P2uSLACWdDSp3n2FBcKeLMx+bvBVDL5e9+oR1+KyBa4VpdPfW6OmVxk+pr625I8FeIBhp0p/9ExilDY9lrDH0GmnWRkJdHteGQrDu7zWJsWfPXqV0/AdB9zES8HQG0lB5cTdL/NB6jtsFPVBmHAnC/Ay9F09cS3ezat8uQjvMDpRcN29hvCH6jh+h7e6jPpuRMc11nt0K3pm6izqAx3pQU/kSylf145E9TOfKJWTffQgghhBBCCCGEEEJ0Eh05BnBeaQVVWh01ulq0tXUyJnArxgTOz8+nqqqKmpoatFptozGCO8INzwB2C7pLnwFMGRf+fRFrCa6t4tyXu0YEoqaG/F+6ZgawSeFxdp1wZtTUSZaZwKGzWLE8huGObQj+hocxLERF9jc/6bN3LTjiNX04fs6lZH2Zrs/OVjvhOXscYU+OZMjcydz9+FiG3+mFHVCe9iMXj0OPh8cwuE85594/TtFV5TKNDBnALt4EjOqLa8ER/vVSIuUWz/YHEPJEMG5u/bnz8bEMM39FB+MGOGrzSdmVa8oA7nbup0aZu7V3hDAsxBddvn79/GdNpK9zBifWpDU+3voHETq6N0gG8A13jWs4dFfh7Ol23W6gr9Vdo+xSEVWl7RwMaoJkAHde3bJ3kJ94mWt33ourk5bcT6I4/dXHFLvOomdvR6qSV5O88Y0msjyvryEDuITiA99ShQ5dUX88RgTh2M0RN58eZlnAadT2nomvtz12noNxoYSreelcqwOchqMe9hz9H7iPqpMHqAUcBz9Oz96OQB1XkzdTkluGnc98es+dib+bvX4FTBnAUG03gl6hvtjhiPuQ8Wgvn6a6tIRrjsGoh/83A0f3pzBVkY2qvg9fQ1ays3sfClMOUNfy31m0QEM2bftkGOvp6sPpGeaPPa64+7tCNyDvMOlHzDKulWzJAB6rz+5VufVAk/oj1dXKrOJsatwfplegM7j0xb2HA1ezzlNXqwPHYLoHzyfw1zMh6Xv0/WMIIYQQQgghhBBCCNF53H3XUO4P8mF0oCeZhVep9eiFzr47w+8ZzTVndxw9fXH18cfJrQf/vpCDq5cvVXaOlKtc8fAPoLqbAxezsrlz+N3YuXpQWFWLg2sPzqRf5OHpM+jm7EaVnSPJp9OYNWsW3bp149q1a/Tu3ZujR48SFRWFVqslKCgIgIEDB5KVlUVwcDAHDx4kLy+P7OxssrKyTIHfnJwcMjMzKSsro7CwkLy8PEpKSsjJySE7O5u8vDyr02pqajhz5gzFxcVkZ2eTnJxMXl4eeXl51NTUUFFRQU5ODhcvXqSgoICSkhLKysrIysqiuLiYnJwcsrKyKCsrIzMzk4sXL5rmLysr48yZM6Z5L126xMWLF0lOTiYnJ8eiji3vX1NTQ15eHpmZmaYywPQ5a2p0XT8DOLfQkGKjVpvG1GsXfl76sYWpQdNkELILSd2kzwR2NmQCD4oidnkMwznBptYGf010NJtIWV2jz5QNGcG4D17gobkjCHR3QJf7C6e+P8BPx/KVcwC11Bmz1ZqjKaJEA/Ye/fEfrZyop805ph9D2Nprf1MP+K9DW0u7xkBE212DioKraMuv/yOLmvIqKgqu0nQkSLTE/Lh44uMNr2n6CzFB0xvK/r6cscqZOqVgnNzQZ+gafuzj7K3Pdq2ryrOo2S4K3yP7vOEHAb3uJ3CoMbNWQ9k3OyiqBuwc8ZqwhIj/Nowb++JfGPrwSLw8Gi7aVannDcMeONJz1vuMenUnI595jIBejmCtTT75Ny4Y39cpkAFP/J9+3OD//j+GPjwc90aDogN5P1FUavi/333cZVyfV3cycISibmdy/iiFxl/oGO5MSs/EN9oszg993jA275Nm4yyPeKmZz/kdhRcM29F1CCH/2bCMYQ/db6ql27uZrGL9/9V3PcZdLxrq/ff/cdejD9LTx/XG3zQJIYQQQgghhBBCCNEC1dXVpOYWsv/MRXKKy1qcpWuelerr60tWVpYpy1XGAe7abvyzzLxifdfP9gH076ec2Hq9BvSiO0BZLjnXjyd1DambeP4VYxB4ERGcYNOK5XzZpuAvgAdeA5RlQL9++LhDXUkhVUCPOfcQ6FTKmbWr+OKprRx4eTdn/3aE7FzLkSi1VXVAT/yjLIqtq07npzd2c5mehC+aS3CYxUS0WnC0ryD7b0dIt/b6snFHqdej1daCuz++1o43NycMeXfiJqit0lKUnkttlTIbr0FtlY7i9Fxqq27xjFzRcs4u2NsBFFOTBzAclYt+Us3Vjshm1lD24wn0lxZHet73nH68YYCKjZxf8zbnT2ajMUsNra/WUHH6J858/q5hPuDCnziz6wwVxkBnPeiKs8mK/yPn9PdOCmco/mQB//7mKMXFWuqN0dB6LZqLP3FmxyeK+gA/kPv3jWRdLGn+hz6ttpHzhu6Qzx9TTmuLeIqMwW4A8ig+nm32d1tkU/rp25w7nUdNcwMp139H7vo/cuZQOhVlWlPwuV6rRXPxKOc//huG+LAQQgghhBBCCCGEEJ3KqVOnOHbhMj+mZXEiM4+UlBTS09M5fvw46enppKen88UXX3D8+HGuXLlCTk4OOTk5HD9+nAMHDpCSksKVK1fIzc3l+PHj5OTkkJ6eDkBubi6HDx8mN1ffHWBubi779u0zLRsgKSmJQ4cOkZubS25uLocOHeL48eMcP37cYj3FjdPN39//BufU9WLCgjkMc4e6jO94b0d7RP8DmLRwNne6QOXpL9j4fY6yQqt4e3tTVGR7wLHdhUYRM74n+fs3kdDW4G/MXH4zvR/k7ueLPyRSZdajrs9bi3kwrDsXt67ip08h8J2XGTfwEofnbiHdVE/N4A2LGdkLLm//Mz9sAkIimfT2ePxLjvHtc7sbjS2s14fhH81jaNFuPl5yDCZNJuq5EfSoy+SnVxrGDu799ovcH1LBmbXrSVaMA2xpBPd/PRn3o1v4+i193/Ymhs9oWj/D3xXHtvD1m2Z11R4MfucZRvaCCmvLETeMs6car4G9cPZQg7E76PprVJVoKE7Ppcr6QdVhvL29Tb9uEp2Ls7Mx55Ob00W/EEIIIYQQQgghhBBCCNGOrpZp6OFu7HmyfdzwMYChgjKXQQzr7YxdDy/szp0kp40D6rlEPMyUAWqgmJRdP5LVxuUZ3bQxgJUKz3L82HHOtqSL5esJD2NYiBNXa/szbHoA+LjiNqIfA59+hFHBLmgzvmfvO7nUAdUDBnDnoD74TfDDzs8dtxEhhL0wA//6EpzVLqYxgCnK5pK6L4PuGkLow3egHuBA9zsC8HpgBOFP3UntV2coM44BXJWuH8M3I52zhS70ixzCoPF9KT+ZQmkRlGfV4DP+TgZEjiRwuAv1A/zwGhFAnxnjiXh6CLr4X9D3bqofA7i7tbF7w8MYFuLRsH7Hi7GbMpyAAcMZFOlCXYAPHmPu5K7fP0Sv8lxqPd1lDOCbrLZaR/nlYspyS6gpq0JTcJXCs5e5mnWF2kZjdXa822IM4C5KpTLl3lJb21w6pxBCCCGEEEIIIYQQQtweBs56Ca8h91Gc+hNBD/8ndg6OuPcfhtp/IGr/YLzuHKcv6xeGa+AdaC6n0TMiCs/Bo3DpGUzFpVSCHv5PXAOGYGevwsknUF83IBTN5bN4DLoHt7534tprED2CR2Dv5EqP4BE4efXCyas37n3DcO0TgkrtaaqnyTuvXE3RhFtiDGCA4sNHSdcBdl6MnDGBXm1ZC5eRzBjtC0Bd+lF+1I+bLJpVTfZHf+OnCx4MnjqR0VHjCfau5vJPX/D1kmP68X8B7YZ49hy9RJ1HCMOjJjJ6agj2x/7Jd4cbZ0ZqN20l4aMjXK5S0/++iYyOmsjIkf3pnptJk7tkz252b09H69iP+978Nf1DgLRj/PDmF5zIrEYdMorRURMZHTWOIQNcKT58hMvKZbTIJU489z6HTxdBwAhGRk1k5NhgSNnO7q87YLxQ0Wq1VVrKLxdTfrlYunwWQgghhBBCCCGEEEIIIVqg8NR+Ck/tB6Dk7M/U1+qw766mvk6LtqyQqoKLUF+HtqwQZ58AACoupVGRfQZt2RXTfBU5Z6BbN1Pdikv67lvrdTXUVWvQlhVSfOZHqK/TL6e+nqqCTOrrtPq69XWmeuLmugldQBsMfpjnpgRjD9Tl7OOjr05SZut4hS4hPDz3QYJdAF0O+zZ/wUnj2IrtoNN0AS2EuKGkC+jOS7qAFkIIIYQQQgghhBBCCHEr6YguoNuSe9s2Z3exL6sOAPuACSz47SSC3ZWVmmbvN5I5TxiCv/VlnPy6fYO/QgghhBBCCCGEEEIIIYQQQgjR1dy0DGCXsNn87v4A7M0L62u4kvoj+w7+Qm6N+QQz3XsRPnESI4O96G6nD/6m7fwn36W3f/RXMoCFuD1JBnDnZZ4BLIQQQgghhBBCCCGEELeD6/WGGBUVhaOjI1988QXjx4/H3t4erVbLjz/+yOTJk7l69Sp+fn7s2LGD3/72t1y9epWSkhI8PT0pKirCyckJR0dHCgsL8fDwQKVSsXPnTiZPnszu3buZMmUKJSUlqNVqevfuzcWLF6mqqsLX15fCwkLc3d2xs7Pj+++/Z/LkydjZ6fNPy8rK0Gq1XLt2DW9vb+zs7BrVB/jVr36Fk5MTO3bsYNSoUfj5+XH58mV69OiBl5cXADU1NVRVVeHv788//vEPxowZQ319PVqt1mKdo6OjKSwsxNnZGZVKhZubG2lpaTg4OFBXV4ePjw8Au3bt4le/+hUlJSX4+Pjg4eHBtm3bmDJlClVVVab5U1NTCQoK4tq1a3Tr1s1iW0ZGRpre38HBgV27djFq1ChUKhX19fWmOGNiYiLTpk2jqqoKOzs7fH19ycjIwNvbmx49evDeur+2ewawvaura6yysMP1nsBvpg7CuRtQdpJv9ubj2bcnapUDat8B3Bkxioi7wgjpF0D/wf3xdenFkFER3HvfRCZEDqWvtzMO3YCKdPZ88hmH8nTKd2gXLi4u1z2phBC3HhcXF7RaGYO4M1KpVMoiIYQQQgghhBBCCCGEuKXV1tYqiyyo1WpSU1OpqKhgwIABpthWdnY2gYGBXLhwAUdHR3JycvDw8KCiooKSkhLq6+spLCxEpVLh5eVFcXExVVVVhISEkJycTGBgIBcvXmTYsGH88ssvqNVqKioqqKuro6qqivz8fBwdHbl27Rrl5eXk5eURGBiIu7s7KpWKjIwMVCoVOp2O7t27k5GRYVHf2dmZ0tJSAgICqKioICcnh/r6ehwdHamqqqJbt25UV1ej0WioqKigvLyc6upqMjMzCQgIoKqqimvXrlmsc0lJCX5+fri7u1NQUEBBQQFarZbc3FzUajV+fn6cPn2akpISAgICqK6uJjc3l4qKCvLy8rh27RoeHh6m+TMyMvDz86O2tpb6+nqLbenk5IRKpaKqqorc3FzTNvXw8ODKFf3YytXV1eTl5eHt7U15eTkqlYqSkhIKCgoAqKio4OzZ8zh1d7TYp2114wPALsOY/egofB0M4/Zu3Ulq/kVOHT9DoYMP/n7udLcDOwcVzu4eeHj40KtfL3w83HF2NPRYXVVM+uGv+GTnv8lvKlO4HUgAWIjbkwSAOy8JAAshhBBCCCGEEEIIIW431wsAh4eHExISQlBQEIWFhfTr14/vvvuOiRMnotPp6Nu3L/v27WPKlCn4+vqiUqn46aef8Pf3J1R9DV+HOv65ex9393TD076W2sLL9PPxoLKkkDv6+FJXUkBgDyfKu3WnoqKCgQMH4ujoiLe3N66urmi1WjIzM+nbty8ajQZXV1dyc3MJCAggICAArVZLYGAg+/fvp0+fPri5udGnTx9KSkoIDQ2lqqoKLy8vhgwZgp2dHfb29lRWVuLq6kpVVRU9evTAzc2NgoICfH198fb2xtfX1xSkDQkJoaCgAE9PT/r27WsK9hoDyQMHDjQFdQHs7OxwdXUFwzPn/v370717dwYNGoS/vz8XLlygW7duaLVaQkJCcHZ2JicnBx8fHwIDA03v4+DggKenJ25ubvj7+3Pt2jX8/f3x9fXFzc2NiooK/Pz86NatG7169aK+vp6ysjKOHj3KhAkTTIH09AsZ7R4AvrFdQKsCmPSb2dzpbhi394sP2XdZWckel4CB3DloIL3cu+Pu7Yu6tozcqxpqitJJO3Oei0UdGPU1I11AC3F7ki6ghRBCCCGEEEIIIYQQQnQVw4cPx87ODicnJyoqKnB2dubnn39m9OjR2NnZkZ+fT3p6OsHBwbi7u+Pk5MShQ4cYOnQoRTmZ9PZy49iFywzs6YVfDzUqe3t83Fw4mZVPgJc72UVX8euhpry7B5WVlbi7u1NWVmZ674yMDHJycujevTsAU6ZM4dixY5SVleHu7o6zszN2dnakpaXh7+9vCs5euHABNzc3nJycKCsrw8/PDzs7OyorK7ly5UqjadnZ2XTv3p3Kykr69+8PhiznAQMGYGdnx9WrVwG4cuUK99xzD8XFxRQVFeHs7IyLiwsDBw7kl19+obq6mitXruDp6UlhYaEpAJydnY2fnx+//PILffr0sfrefn5+qFQqfHx8SElJoU+fPhbzqdVq0/KKiopMn8UYsC4rKyM9PZ1evXrRr18/MjMzSU073+5dQN+4ALBdLybMm8MwQ/D3l68+Yk9OnbJWpyIBYCFuTxIAFkIIIYQQQgghhBBCCNFVREREmDJcS0tL0Wg0BAYGUlZWZnXc3YkTJ5r+/9hjj1FQUIC9vT3/+te/mDJlClqtlr1795qW6+DggEqlora2luLiYnr06IGdnR0qlYodO3bYNO7u5MmTqa+vN43lGxERQeqpk4wN6UeVToezSoXKwY7C8ipqamtR2dlRW38NXzcXANILignt7UNhub4HX21tHZ5qJxzs7DiYlskdw+6iurqaO+64g9LSUtM2Kisr4/z583h7ewPQr18/i7F+i4qKqKmpabTO6enphIaGmuKFyjF/IyIicHd3p6ioiBMnTpi22ffff28xHrNOp+PIkSMW4ymXl5frt8PH29o9AGzoU7mjuTBs5mx98Jc6cvb/s9MHf4UQQgghhBBCCCGEEEIIIYTo7Orq6igqKuLQoUNUVlaSlZVlGvv23Llz1NXVUVlZaQpimv8/LS2NyspKamr0ve+eO3eOyspKi+WeO3eOwsJC+vTpQ1ZWlmm5hYWFAPz000/Y2dnh4uJCYWEhaWlpaLVasrKyqKurw8XFhXPnzoEhgFpUVERWVhYYxsitqNZyLq8Iu252uHRXUVheSZVWh7a2jsyiq9TV1+PSXcW5vCLySitM06+Uaairr6ewvJJzeUVUVGupqqpCo9GQlpbGuXPnOHfunGnIV+PYw+Xl5Zw7d85inauqqqyuc35+vmn6lStXLLaJr6+vadsak8qM0zF0NV1ZWUl9fb3p87q4uJCVlUVlZSWOjo6mbdjebkgGcK/7FzAnTN+vdlnKZ3z4Q66ySqckGcBC3J4kA1gIIYQQQgghhBBCCCGEEDfC1TJN18sAdgmbzWxD8LcuZx//7CLBXyGEEEIIIYQQQgghhBBCCCGE6Go6NADsEvowc8cHYG8I/v79i5Pok8aFEEIIIYQQQgghhBBCCCGEEEK0t44LAPeewK8fCMbFDig7yRdfSfBXCCGEEEIIIYQQQgghhBBCCCE6UscEgF2GMXvGMNztAF0O+/65j9x6ZSUhhBBCCCGEEEIIIYQQQgghhBDtqZu/v/81ZWGb2PViwrw5DHMH6ss4+cWH7LusrNQ1eHt7U1RUpCwWQtzivL29qaioUBbfErr3uoe7hw/Bt4c9dkB9ZSnZv+zn5IUi5Hc6QgghhBBCCCGEEEIIIcSNdbVMQw93tbK4Tdo5A9iFYTNn3xLBXyGEuLU40vOex5kybig9DcFfADsXD/qNnMGEoX6K+kIIIYQQQgghhBBCCCGE6IraNQBs3/dewnvbA3Xk7P+nBH+FEKLT0FKcV0R54VmOffcPvv70A77+/AsOny8HwC1kKD2VswghhBBCCCGEEEIIIYQQosuxd3V1jVUWtta1qxn8O70eV+0Rvj1Wopzc5bi4uFBVVaUsFkLc4lxcXNBqtcriLq/+ajoZGVmUVdfpC65Vo8kto/vAYDwd7anMOU1hjXIuIYQQQgghhBBCCCGEEEJ0lJoaHU7dHZXFbdKuGcAAFB1lT2KuslQIIUSnVkVlmbJMCCGEEEIIIYQQQgghhBBdTfsHgIXoUmJYk5DAp69NaChauIaEhE+JnWheT4hblE8wvZ2AvItcvqacKIQQQgghhBBCCCGEEEKIrkYCwEIIcbvqPoTR44Lprsvl2OFT6JTThRBCCCGEEEIIIYQQQgjR5UgAWHRu05ay/qNNLJNsXCHaV/f+DJt4Lz0dyjm7dyc5MvavEEIIIYQQQgghhBBCCHFLkACw6Nx6BhLo6Ur7Dn0txG3OaQj3TJ1IkLqcs3u+4EypsoIQQgghhBBCCCGEEEIIIboqCQB3ZaERRPgoC68jdAITQpWFQojbhZ33vUyMupdedkX88v1nnCmqU1YRQgghhBBCCCGEEEIIIUQX1s3f3/+aslDoeXt7U1RUpCzuJCYTu3UxEXVJbHghloRC5XQrQp8g7o1HCa3Yx8qYOBKV05vkyYRnl/PEmAH0dDfk4mpLSN0Rx9K/n9D/rR7Oo/+5iKiIQDydDLNVl5Cd9AVr/vIlqaZlTSB261IiCr/k0Y0VvPjsbCIC1IZFpvLlqtf56KQGiGFNwiyCTfMZlCURNzeWfQvXkDDTn6TVa8h7+BmiBnk2TAPwmcCil57g/oE9URtXuSyfC/s38fpfE9GYFqh/H/+f43j0zX36IuOy//dRYveaKkLoLJb952wiAjxxtNdvg+yfFZ+vufVSR7Lo9RiLddLkJ/JRzEoSzN5G3Hze3t5UVFQoi7u87oETuf/e/nTX5vDvXbvJrFbWEEIIIYQQQgghhBBCCCHEjXS1TEMPd32srL3Yu7q6xioLhZ6LiwtVVVXK4k4inaPn3AmfPIHJEwdTdnAfZyuVdcwYg7+k8umKWL5pScAYgFBi1q4l5p6eOJaf48iew5w4e5ZC/PGxP8s3P14E9WSWvbeMqNAe1F9KYt/BZM6cLaS+Z3+CQ0cyYbQzJ3YeR/+W/ZkQHUnva46ET4nEN/Mg+5LOcLGyB/2D+jN89GDKPt/LWexxdqvgco0vg3vak/3jTg6eOMvZtJMcOZFOWfhU5oa6Yh80Gt+z7/Mfi1fyQfw+LgKExrDmf2MY3csRTdoR9hw+wdnsMlz7DCZ42FgeGFjI7v3p6AAIZ+rcIbheSuTz/Rf1H9mw7MuHPmdfhnEzxLBm5VyGu1Vz7sgeDp84S6FqIEPvHsWE8DoSdv+iX16T6xXB0g2vMrlvN7KP7CbxxFkuXnXGf6Azhdt2cdzwNqJzcHFxQavVKou7uCGMnBpGj26Agzv+oXcTOlTx6u/E5XM53GqfXAghhBBCCCGEEEIIIYTorGpqdDh1b9/BUCUA3IzOHQAGXX4SB8+0IAhsHvx9fSkfNaTjXlfEi//DM3f3oOTntcS8sJ69x5JIOpbEwX9t1wd/gQkvr+TRQZD+1X8T89bnHDmWRNKxg+z+KoHCgQ8QOfRO+tolsPukriEA7ONKScIynnnnG5KOJXHkhz1ohz5EeGBPXOs/Zfepy6QeSyIpaAJzQ1049/kfifs8iaQT6ZRhDLT2xDHnS555c7u+DIBAYl5bTKRvGUmrY3j+r3tJOpZE0uF9fBOfjPPoCdw9dAh9zn/JwUu0MABsWKb7ZRKWxbDyK8M2+G4nhYMfInJYIL5ntpOY18x6jVnAM1MCqU/eQMxbn+o/8/5v+PL7I1ysrEYSMTuXWzMA7EvA0EBclcXmtIVkSABYCCGEEEIIIYQQQgghhLhhOiIALGMAd3Gakxt4ftmXpKsjWPRuLFHKMYFDZ7FieeuCvzCBqLt7QmEia97cbdZtsrlZ/GqYGgqT+GijcuEadr+zj3QcCR3xmOWkspN8Y1Ffw5cns9HiiLpHy9Pc8899Yble/WYROcARbepuVn2vXONUNn11Eg2eDPlVpGJaM8yWucHiI2rY/eMZNPQkcIR5uZX1yi6mAlAHR1ruo8ISSsz+FKLjnOHwpx/wdXOvbw5RrpxNCCGEEEIIIYQQQgghhBBdigSAbwWpm6wHgUNnsWJ5DMMdWxP8BQjG0x20l8+QpJxk4oWrUzN1NOmUlAE+PbEIuRZms9v8b4CCCnSAV8+RyilN0JCfrgjyBnvhCpRk7rMesN6bTR7g6TNEOaVphmU6DoshISHB8rUkAjXg33uC2QxW1ivzI77cn4/WM4JFHybw0XuxxDwQSMtD3UIIIYQQQgghhBBCCCGEEEJcnwSAbxXGILCzIQg8KIrY5TEM5wSbWhX8baDTWg2ldg71yoKOU3J6Nwk7Eqy/EtMtKzdaLw27V8XwxKK1JBzPhoAIZi1Zz0fvxhCqrCqEEEIIIYQQQgghhBBCCCFEK0kA+FaSuonnXzEGgRcRwQk2rVjOl60O/lag04I6cBjDlZNMiqmoBsfeQ4hQTgJQG7KI89NJVE7rCOn6rpY9+02wnl07MRB/IP+y1Xxl60oq9N0312az4a8brL4++j5bOZdVmpzdbHj1GZ6Yu5yPTmtwHDSLZxZaXVMhhBBCCCGEEEIIIYQQQgghbCYB4FtN6iaef2UDX+74kg1tCv4CJPBTqgZ6RvLkwqbyVL/k0BkN+ETwRKM6aib/YQLBaLmQlKCYZgs1nv2UZU3I/JKjOeAYOpkXH1AGVkOJmTkMNfmc2X9CMa0Zx/eRXqhf5iLlR2wptSee5qujOcGnu8+gAVw9B5pNEEIIIYQQQgghhBBCCCGEEKL17F1dXWOVhULPxcWFqqoqZXHnV3iW48eOc7ZQOcFWOlIPlzH4gUiG3j2ZGfcNpndgKHdHRBL126d59O4yvvnxImd/tlZnMo/953/w8CBXSn5+j6XvpaIDoD8ToiPpXZnK1p3HLd8uaAJz7u0NlxL5fP9FfZnHaGbc25uevcLx8RvA1JkT4IdELoZPZW6oK5cPfc6+DPOFlJF03plRE+5m6H0zmHpXMD0H3EnE2ChiFi9glH8d6V/9idd2GDdOOFPnDsHV/D0bLfsyyRWDeeC+IQyfNIOxg3sTGHo3ERGRRD26gJjfDKfkq4NctDqvwdg/8rdVMUweHGiYdzJPzBpFz+75JP7f+xxp874S7cnFxQWtVqssFkIIIYQQQgghhBBCCCGEaFc1NTqcujsqi9tEMoBF8zS7iX0hjoTT+dArgsnTooiaNplhPlrSUw3j3mp2E7toJZ8ezzarE8kA+3ySPlvJojd30+pRhPeuYtP+bDTuoUyeFkWEr5YSZR2l1E08v2wDu89pUIdEEjUtiqgHIvCqSmX3umU8v9H2tGjN97EsXpVAaiEE3jNZv8yHJjCsF6T/sI+jyhmU0s+QXuhIzxHGeSPwLzvBpysWs9b21RFCCCGEEEIIIYQQQgghhBDCqm7+/v7XlIVCz9vbm6KiImWxEOIW5+3tTUVFhbJYCCGEEEIIIYQQQgghhBCiXV0t09DDXTmsadtIBrAQQgghhBBCCCGEEEIIIYQQQtwiJAAshBBCCCGEEEIIIYQQQgghhBC3CAkACyGEEEIIIYQQQgghhBBCCCHELUICwEIIIYQQQgghhBBCCCGEEEIIcYuQALAQQgghhBBCCCGEEEIIIYQQQtwiJAAshBBCWBEwL45t8fHEv/8ik9TKqUJ0fWP/sIn4+Hi2vT2fEOVE0f76zifu43ji/7mJFye2c6PSkcsWQoguYywvvh9PfPw24hZ0rStbV70m3y73y111/whxa+u6bb4QQghxo0gAWAghxC1sLMv/Hk/835czVjnpOiYNC0IF4B3G6AjlVNE0wzaPN3u1YvuLjjaWcUM9AFAFhzFaOfk65sfFEx+/heXjlVNEkyaGEeQE2HsQNipcObVtOnLZLSLnvRCiHY1fzpb4eOLj5iunNG/8OMK8AVQEDbX1ynYzte2afDPdHvfL7b9/xr68Re6jOgm5p+3Cumyb3xHmE2d+H96aa6gQQohbkgSAhRDidmHvTcCwqUyc/SQzHtW/HoqazV0DvLvOxcD4QPB6r3b4srPnZAY6gKIUDicpp944U/+wni3bNslDCTNh81ay6eN44hYop4iWO8iBU6UA6NJTOKycLNrf3hQyqoG6UlKOJCuntk1HLvs20GXblOHzWblpG/Fvt/2a15l1yP5ZENf43uGf29iyfiULx+gDPZ3abbLvbbb/AClFADoyTnWlK9tNvCZPi9Vn8Db3o52+z7I+Pp74LbFMVUxq+f3yVF5cv4Vt7zfzPp2WDfvnpp+bhiBQE9+F9IFns/bU1BauYWFfy7rhhqzn+Pg4TEvr6m2naAMrAUbzl5VjzmPMQlau38K2fzYcK5veXc58K8dKqwLxHdjmy3dwIYQQt4ou88xfCCFE27jdOZERQ3rhpmooU6k96DdyBhOG+plXFUDOlqU8Fh1N9NOr2KNRTr1x/Hr5oVaZ7bRO7yArfhdNdHQ00dGrSS5TTm87jz4BeDgpS4WtDr4TQ3R0NI+9tJk05UTR/rI2s/Q30UT/OoZVe9u5UenIZbdIx5/3HanLtikeAQR4qG75b3Q3bP/Yq1D7hTD1hXdY3tm7Ur9N9r3tDrLq6Wiiox9j6Ydd68p2067JO5JJrQbcBzSZwRvwUBh+gObMHnYqprX8ftmPnn5qutQtrZkW758ue24GEGrR7o1lqiHr+bq6Utspbpixi9ez4YWphPipUdkbCu1VePQNZ/oLrzT8qKBNOq7N73rfwTezNNp4L76dDOVkIYQQt60ud1sqhBCileqqKDz3I/u+2szXn37A159/wr7kAnSAW79g3JT1O6P9K5hn+mITTfTaZDQAGdsbyqKjiV66WTmnEEIIIYQFTdJq071DzIp4kgt0gAfhDz2ChDHE7WE7yef1x33oeGtDCAQwPcwP0JCWeFA5UXRxY3v5AQXkXIKgoWbt3vhxhLiXknbWelRf2s7bWFkyq82/d1v7/q2ez4zxfqjQkPHdOpY+bagz73lWfbiHjFKt+RKFEEII0YG6+fv7X1MWCj1vb2+KioqUxUKIW5y3tzcVFRXK4ltUf+6aPZF+VWfYu/MQ5crJnd345WxZHI46Y3sTQd+xLP/7EsJJZvXSA4T89wKmBht+zV6aw56Pl7HOIlvOUN/drKgsmdW/W0GTj7zUo5m7+HEmDQ/Aw/AjYV1pBgf++TfWfde6XyKPfXkLSyKu8/jEynp5jFnIS78ZR4ifYV5dKRl7P+St9w+i77jO0HXbND+S39uMJvopxvqroOgw617YTsDry5kerIayFLa+Hkt8FobuvqYTcHYrMV95snxBw/J1pRl8//7rbDxi/eGQxfZvcht6MHbeczwyPkyfMQFQp6P00jG+3bSO+FOGZS+II35akMWcjWWwPXop5keCemg0z8Y8xIg+Hvpfn9dpyDn+NRvXxpPS1Gq3gH4faTj45mouPPAsM0Ya9n+dhpzjn7Puz9stMkTmx8UzPSiD7dGvkzx7CQtnhhOgbro+3mNZ+MJcxg32Q2341byuNIPv//4WG3807s1wXnx/OaO9NaS8P4/Y78wXAKjnsnJTNCGkER+zjK0aTPvTYks2ef7oGY+rAd5mv+CvA+w1JK+dx4r9FrUZ+/RLzB0TQsNhqFzvBupRc1ny2CTCTPtHR+nFA3y+cR07zypr26KFx5WtbD5/rJ3P1rabnr5uAdvnbaZi8UJm3B2g3/91GnKOfMLr7+xsOJdtWXYr1rv127Al572tQpj63HymjzI7rspySP3+E1Z9fFj/QyAzLTrvW9Gm6Lc3Vrax4byyOJfa0nY2x8o5bEXGjmiWfmhW0KI2pZXUYUQvXsiM4QGorSXLKK5XHbV/bGJYviZpNfP+bHaUTlzOlufCUVu5xqIOI3rRQh4ytveA5lIyX7+/uvH5oA5j6oLHmR4xAD93482BhoLzB9j67kYOWvmK2Xi76Ci9+D0f/o+xfiv3fUv0fZb1707Cr7nrgeGey/HsVh57OV5fZmWb6MpySNmxkdVfpFicm+bnz3t1C3nldw8QZJipNH0nf3tjI4eNMzRxfxeyII43pgWh0hVw8P2lrDbew1k5XprcDsb2cO1iDoS8woKJQYbrt47Ss9tZ/eetje8PvMey8L8X8EB/w75Ram67NcvKPm1yWfq6fkmrWXwwxGL76UrT2P7uCrYqj8OWejCWLU+HoS46zIqnV2ExkIDx2LCY1tL7ZSv1rGh0Htp4L9ES09/YxvyhWivtdwP9vVoBB998htUnsGH/WKlnhfkx2XA+GI7DB4LwsNcP5ZCzfyvL3tvT6NrWMtauRw2M9w3GdTHed+z5TsWkB3Vsn7eUzRqY+toWFvocYHPuOOZH6Dj8TgyrElvZdtpAPXQq8x+bzuiBfqbria6sgAuHtvK2+fcZ47FVtJ15H1aw5OkZhPcxHCyaHA5//Dqrvmt8rNh2T2ubkAefZf7M0WbfwzTknN7FJ+9sbWjbjFp0TW74jMuSQlg+OwS1vY6MHa/zetZ01i4ajYe9joL97/HMWrMtbqVdbvJaZRPDsdWSfWxsw1tS10B//rVwP9jS5tvQdja+r7bChs/UiGG7kLSaee9jeV0pzWCnxb1h0+dy0/ejRk3Pa67xfYeV+zET2+7FhRBCtM7VMg093K9zLbKRZAALIcTtysGDniNG0k9VR/4v/+56wV9bOA5gwdolDcFf9F20TXp6OdFtuq6GsyTuRaIjGr5gA6g8gpj02CM3dIyzgDkrWWvoZstE5UHQg0vY8PZ8Aswr40jAnPn6IBCA9wge+fMSfRAIwD2MB6LDLOZQ+T/E2pcsl6/yCGLqC23chgteYcmM8IYAE8buwUYz96UXmd6WZY9fQtwrcxnd1+yBrb2agIi5xK59sR32jydhi99gfqTZ/rdXExAxnyUvWMuiURHw0lpif2MI/tJE/cHziXtvCVOHNDwUwrS9NxC3IMRQkswnSTmAmgGjlKPygXraUAaoQHP6oCH4a7uQBXGNu28DsPYAnACi31rLkgcbHgxgvt7zLI9CIpYQ91I04Rb7R4VH8CQej27j3unI46oV549tApi0fjlzIwzBXwzHSeR8Xlmg2IY2sXG9O3Qb2kJN9J/fYOFExXHlHkDY7Ed4xLwqN+K8t02HtZ22aHGb0hohzH/DcLyaHSpN6mT7pxG1CkeAeq1+XFOTsSyJW85c8/YeUPcJZ+4ba3lRMUbg2MUv6o9ZY/AXQKXGb8hUlrz5LMotrp64nLVvKLeLCo/gqTz19A3YKln5lOgATz9GK6cZ+alxBEoKDL/OUU9i+drYRttE5R5A+G9iWfvyJKuZgOpI/XXF+AAewCN4KkteibZa36gh+JvDnnfNgr+toiYkZi1LHjQEfzFs7yHRvLhYsb3Vk1j+tv4e0mrw9wZTD3mKtYrtp/IIIfoPS1p//nx3hAsawDuUSYpuoI3dP5em7bEMDHcYG+8lWiijtARQ49lPOcUoDE81oCsh+4RyWkdxZMBvNuiPQ9N570HAxKdYPqe5s6H9aT5OJoMgwuaogamMGqgm59QuSgBQ4Xi99r3JttMWY1nyh4VMGtIQ/AVQufsR8uAS/rxI2XICAZNY/8rchuAvgDqA0b97hfmKMY1tu6e1jXrOSt54epLie5iagOHRPDLHvGYrrsneo1kyM8RQV0VQ5LOsfHq04ZhR4Rc5lWhTZduuVR0mKYcC9PeWjzw3lhZ2Jt6hOqTtbC31OOIMzyZMx+KNvje06X7MxntxIYQQnYoEgIUQ4nbS415+9eiTzHj0SWZEz2Z0EGT+9AWHs6qUNW8tTh54OOnI2buO5+dFM2/xRlLKAFUI9zZ8Y7Z9HMvISYT5AXkHWbV4Xrt1bXXwz4ZlRUezPQNDVp+imy3zXx6ro3k2OgQ1paR9rf+M0dHzeP697aSVgip4EgsfNH8HFX5+agr2xhLzbY7+7z5+lCatI2ZLGjrAr5cigOnugYeugOTPVpm2YXKpfhs+8ETrHsYZabKS2b4h1rDe+q7kUkoBdSijHzJU+nCp6bOvTtI/9M3Yoex+zDwTLJwlj43FT6UjJ3EzKwxdj8Ws2MzhSzrwGM0jT7dtvUGFh4cKTfpO1r0UQ3R0DCu+y9Bvv4jpTFdWJ4DwUR7o8pKJXxFDdPQ8Yr811B88Dn3oLYD5T08lSAW6S3sMy41m3uJVxJ8q1T/4mTLf9KAn5+MjpOlAHTJK8X5qHokIQUUpKd+aj9hnw/hQ6rnMnxKECv25Y+y+bd7iWPZcUlYG9ZxnmTNEDaVpbH/veX137fOeZ93XaZSiIuiBhZiHqUdP1D9ULvhRf0wZP+fmvRmUtP70MWnRcdUqtp0/5uez8dhtngq1WoUuaw/rFs8jet7zbDyh0e/7OyZZ1LRt2batNx26DW3xCPcOVkF1GvGG8yE6OoalG7aTkqfsrcOG897mNqWV2r3tNDuHmxoGIdo8C8a2NsVmDz7OpCAVaDLYaTjvG5YNpUdWm12vOuH+MfEg6FcLiZsThgooOLWHw2ZTw1+Yy1g/FbpLh9m8wnAcPr2CzYk56PBgdPRCyx9a1WkoPbOHze8uJSY62nBN3kOODvAPY+pws7rqaJY/HY4HoEnfY1p+4/bQ1n1vi0uUaAAnNX6GkulvbCM+fg0LDUEUtbsaFaApSgFg7OL5hHsApSnEv21o859eyrq9OegAj4hHeMr8c+qXQkhEEKqyhuMl5v1kSgFV0AimKKsbmIK/1Rlsf+151imz582Ol+gdzV7ZTNRqNRSlGK7HMaz4l3691QNHWwTBA34znXAP0BUYr93RxLy0jj2XdICOjK+fbzbDqnk2XJON1GrUdaWkfLaCmOhoYlYYjiv3AYyOVFZuqZ0cOa+x0g20sfvnAlK+Nw//tvR+2bye4fNZ6T7WPJPU1nuJlkop0h8zahfDmdr3WdbHx7PlNePS/FA7AZoSGm5xWrp/WntuqvDwVunbZsX1PmRkG0MqQdOJj49v9FJmNw7wNPyt+ZyUDAgImYF62ihC1Rkkf5xjUde65ttOW2krS0nbu5nVxuv9vOdNbYrf8KmGe2UzKjVqlbXveEGETTCrZ+M9ra0eGRmCCh1pXxjbfH07sf1EARX15jVbcU1298NPm8bmp9fpzzXvAALIYPvLy9iTB6h6MsBw7tt8rWoN93CWWDm2trxsFjLUbOZvOzLQoSJg4hI2bVnPyuemE+5tvqA2aEWb35K20+bv4K2kHhJOkErfPfbz86KJftp4bziAETfk/tqG+zGw8V5cCCFEZyMBYCGEuJ3Zu9EvcgajB3aG3+V2JH13Wc+/t4ccDWgu7ST+ZIF+UluuhDklVAB4hzBp1AB95oomh8M71rH0hVVt/nLYYg+NYIAKShPfY9kW/WcEDTl7N7PsqxR0qAkcrsjpKUtm63splJ4v0D+o0qTw9do9lJZq0GJlu2jSiH/tGVZsO2zahiu+StE/kBlgGZSyyYdLmffCCjb/K8Ww3lCavJU95/UPwBxb+yvo4eMI8QPd2e0se2c7yYbuNkuTt7Mq7gAFQMDANqw3ADoKEtfxzEsb2ZNeCpSS/P5qDuQBToGENHoQq6PgyEYWPbeCrcmlgIaUTSnkoH/o7gHQdzqjg1SgSWHry+sMywXNpcNsff1tw4OeAYRNMyxS8zWnMnTgFMpo8wwD9SOEBQF5x/gkyazcBuo54YSoQHNiM8+/t4cMwzbUXEpBYyVAOyV8ACpKObx+GZv35hiOqxz2bFnG16d0oA5kqNk2ySnVPzDwHDyJUUH6Ha25dJjt7y3l+XfaePZ01HFlZOv5YyPN2Xhef2Edey5pQJPDzq+T9ZkUbVyuTevd0duwxQqo0ABOAYRPCjNkkZSS8a/NxD4XaxkAvCHnvY06qu1sKVvbFFv1ckUNlJ7YykbDea+5dJitaw+RA3j4DWio2wn3jzpiieHh9SbiFk0lSA269O2sftc82BXGuMF+oEtj+8ur2J5s6J6zKJnt76zSt/l9QjFf84NvP0PMK+vY/mOGoctSDTl715GcA6BGbXbbpZ5zLyEq0GXtZMVL60zLb7f2sEUOU1AEOLniCcBYwvqqgABCJ+pP9nA/T0BDSSbAdCYNVQMF7PmfWLYeMbT5RRnseW+ZoTtNP0LubRxq0JyNJ/Y/lpqOl9Lv9pBaCqgccVVWBkIeW8nyaUGoNGnEv7GUzW0aHqCBruAg616INVyPS0necIALOsDOEfNkxyBv/Ra5sN947YbS9D2s+yYVDSr8+lyv4992pivg4IbFxG7TB85Lk9dxIEOnb5evl6XZjJ1HLqABPEImYQoB951OmD9QkMaeG5QVa+u9RIudz6cUUHvq95d64gD8AHVQuCHTLQBPd6CkoE0BTFvp0rfz+uIOuN63lB1QXUEJGj4/lYEqaCjP3j0AVUYKn2sgo0QDOKJSdOPdsrbTVgdZ9VwMy97bzkHDtQpNDnveS7a8V7agIe2z63/Hs/We1lYFFfp7o4DhkwgzBDlL0/ew+c1niN1iVrFV12QdGXvXsb1oDzmG9S7Y9zc2n01DU4XZuW/7taojpX24lJjXt3I4qxTUfoRMnM/y9+PZ9PazTB2srH0DdFDb2SqaNOLffIal7xu+txftZE9a6Y27v7b5fsyGe3EhhBCdzo26rRRCCNEZXD3Evz79gK8//YCv4z9j39EcKusd6TliKsPa6xe5nVFZCl9/aDkeb0qJIaLRFlkbWbcjA53Kj/DfxLLln1tY//Zy5k8MaLYbw/Y2OqgnKsAjcnmjX2PHL9D/It/Dx7I7Mc3ZAxYBas2ZPWxvbpMUpLFV+dB1bw75tPVuIoSpz61k/d+3NZuhYLPhAfgBqsHRbFFuk3cn6TOcvJvp6rJFtOQkKcdoyyHtsiFA1uhhgpacI5ZjuJqyRoy/Jg/yRA3oLqVY2R9ppOTol+1qOl81bN2nfwg9ILwhXyDgN+EEATkntusfmrVCeC99HljBRfMM4qaMZoCfCvBg9MuNswLmD9VP6zmwYY6c99exPV2Hyi+cuW9sIX7LeuJens8k8278Wq2DjisDm88fm2hI27XVckzoEyXtMraWbevdsduw5Xay6sPDlNapCXpwCZv+uY1Na2N5dpo+Y9LCDTnvbdRhbWcL2dym2Eij7+7TY/gjzB+lv/ap+4xm/tJxBAA6jb4DUeik+0eh4MfVLHpps+X5RzgBfoAqhOgtyvZtDZP8ATzxMw9KqUcz9+U1bPrYsv50K7FCY1ubc3yj4n1vrAslGsCPgPHA8BEEuBeQcwmChj6CGvBzdwQKyNkP4Imrk/74Pqg8vtGwPUMfgDEG28wVpCnH2D3Mqpho6xndfpNYPicEtS6D7W8ta3wutUHOkdXssViPAkMwxVJptb7SgPEvMt0wlIhH8HRenBmKGtCUtDD7rL3kHG7U/XVBWTtEsEzdQA9gnCFz29j9c8GJz9HnfXc02+8lWiyxgBJA7a3/UcqUkAB0l3IodQ9h3HhguL6t1BRdUM7ZgTSkfKNob9rpem8tAzm6qd5CtDpKAM1nKWSoQhg93JG0pM/RADnVLbtGWG87baceNZfl725i2z/N930z4yuXpbFz2/W/49l2T2u7ne9s5nARqIOnsuT9eLZtWkOstYzXVl2Tc0j50PxuPoPDG6xt6VZcq1rDShZ/tCKT30hzKp5VL8Tos5D3plFaDR7Bk1j4Zhzzb3QQuKPaztYoSGs0Zvvht/WZtY17CugANt+P2XAvLoQQotO5EY8dhBBCdEa15Vy9sJt9/y4CnOnZR//FWNgm7cOlPPb0arYmppBT7ohfcDjTn1vDlvdfZNINipOo7BtFGm8Mb0f9eF+tFsD8tw3jCZmPk9gebuIdjtqxbVsF9A/jWuy77aQU6bvPnKsGCGDK0ADQpXGkRd33NUeH1soD8cZUONq8zdPY/NJjxLy7lcMncih19CMoYjrPrt3Cppesjx3ZMh14XN02Otc21OxdRczvYtn4XTIZRVo8+oQxacFyNn2seIBo8zF4k7S57WwFW9oUW3y2me8vAeoQpr+0hi3x8WxZ+yLTB6tBl8HOj7c31O2E+0eTtNrQ7aG+e3O/Mc/xinL8RZuN5cW1LxIdEYCHk3JaU1ra1nacg7kFgCNqPwi4NwS/gjQ+P5UDASHMUIOrSgVlJViEx+q1hjFCO0jBYfak60AVxLjfTG80dvKNkPL+dlLKQOU3mvlvbyI+Pp5Nb89ntJ8KSpP5/KO2Xmc7i53sOaP/EUDIxDDL7p+/vVGfsTX3Ei11gZIyQO1JGNMJ6wsXDu4iW6NmQEQ4eKhRAwW5jYNYt67R+OkT3PUM3UCju8CpHY2ikxY6pO0c/yJrX4om3HxM0nbVge2sZg+rnp5H7KadJKcXoHULIGzifJa/v63xmL504DW5sypKZvt7y4h5OpadGfo2ffrT89twry/apBXtbIvvxYUQQnQ6rWj2hRBC3Ep0dXUA1NXr/xWtUHSQ+HdieT7mMaKfXq0fF857NI883Wikqg6hf2gLBf96vtGvsU2vlxrl1bRZwJQQ/JQZXrboO53RwSqglBTD+JjNZijYIkOfQaE7tbnxtjC+YlZ1QDd/UwkPUgEaWpUUVKpBA6iCwq2McRdCWIDayrKT+SQpB1QDGDpNDX2nM6IPaE4fZGsbNqM+60mFp7eiC8/B8wlr1KvnQUO3dAXsecHKtja8lpp3g2dQ+mM8q958npjHool5Vz8el8coa2NHtlBHHle3i864DTUp7Hx/BUufmUf0vFi2nioFpyCm/s5spLwbct6r8exn+ffoReE2janX5rbTFq1qU2wwfjr39gFdWSka4/PsOh2aS8lsfet1y+56b8j+aZ3S5K3EbklGg4qgKU8x3zDurZ4hcFSdwmbl+ppeMaxKNFSfNokRHoAuhz0bGsaDjDaNKWhJ38WqioCh02/uw/CMEjSo8PQOYdJAPzRZxzi4K40C1QCGPjSWAG+gNB99B68V+viFfwhTLLYVgJrpQYZsu9y2dAcLoGHzS6+zPUOHx9D5vPRyW34c1DoB0ZMIdQdNaSk6461ynY7S9J2sfmmFIou4azuYmIYG8Bs8iTBj98+XjrE9S1mzo7T+XuL6DMt29yBofBgDnHJI+3YnyRk6PAaOIyzIEzUaSm7YZ+0MlAF3DZuXRhP92LIW3z8233baZvrEEXhgOTau/tXc+MstY9s9bWtpSPl2IyteeoZ5v55H7Mcp+nGrzcf07dBrso3XqptBk8LGb1P0We7eAQ3dzYumeSp6Rhk8nUkD23glbO39WEvuxYUQQnQ6EgAWN8yE1z4lIeFTYicqp7RUKLNeW8+nXyeQkJDAmt8pp4t2sXBNo/2k33driDGv197UjxL3eQIJHy5jgnKa6BgObrj1vpexw/3gWilZxsGQRMvNW8mmd5cz/1dhBBi/h1VnkHw6Hx2gdmp7p0gVOh2gJiz62aa7xt2bSg7gN/ENVs6bRFhT9drC2ZOxQw1dW6sDmDRvJW88EKB/2LHXLMPLFgFqfRacroKCs6nkaPRdh05/biULhjb9GYzdMQaNjWVueBPbeH8yFzSgGjqXNX+YzlhDt43tyxF1QBhBhm7aPMKn8+K78wlTgy7jcOsemJ44wIUiQB3G/HefZZJhvdV9JrHw7eX67tuKUti533K2nI+PkKZTERLxCCEPheFHKSnftq2bu5TT+foHwRNe5NkxHoAH4Y8tZ/2b0wmykhS652wO4MekV1ZanhNNmP/nTax5eT6TjMcVoMtIJi1Xf8ybj5Fpk1YeV8JMZ9qG419kzfqVPDttrOlcQ5NNcnK2/iGqymzU0Fae9y1qU8zqBYxawlhvwDucuS/HseRXARZjhlroiLbTyPAgmaBxxD7WRDd8rWxTWmpsZBgeaEjdsZpVf47V/1jg148xb/EK4hXdG3b0/mmz/av5+qw+M2nSAvNH8wdJztCAUxhz332R6WOCrG9rI09X/fFQVULG6QJK0Xd5Of/lNUyyEhzJSUqjAFAPnUvca/NN+wjvICY9HceaP+hHKLXQkn1vq6R8fRe5AY8QFqDhQvJByNpOSp6KAaOm4ukMujLD+OHs0o8/TwBTX4llrqH7b+M5MXeoGnRpJH/WwihSs9LY/PrfSC4Fj4hnWXuDg8CThgWhqsvh8N9Xs2KFIaD/68eIeWkjB2+1W+f9B0grA/xCmDJH3/1zzqldrR5KwpLhRwPuYTzy3KQm7xFsvZewRU6JBpw8CRsTgvpSKns0sD0pFZ1fOI+HGAJv55Vz2agjzs1OwK+XlXbIqMm20zaezvorqbYwg7S8UsCDoF/NZ/m7k5ruArqFbL2ntc1YXly7npXPmV/XNGSfSCa7DMvxzTv0mmzjtaojzYtl01vPMn2M+TnsQdCY6bw4M0zfDXZeqsWwJJ1Ni76DdyhDm+kRxvTZYahREzBxIXGvzCesrTvW1vsxW+7FzQ2eT9zH8cTHb2P9Czf22i2EEKJBN39//2vKQqHn7e1NUdGt9q2ueYHDHFBdruVCoXJK20147VOW3gNJ//sosXuVU68v4sVNxI7vieZcIj9kqnG9tJy4z5S1Opg6kMnzFzHr3iEEelp23qfN3UfcU3HczB9UtouFa0iY6W+xn/T7Lo8vo55nk7J+e+kXw5p3ZhFckUjcgpXsU06/gby9vamoqFAWd3F+DHk4isHW7s2vack9HM/PWR3VJ1YHGr+cLYvDUWdsJ3qptQzXsSz/+xLCSWa1cYxVowVxxE8LImOH2Vg7hrKmZbDdfIy6ZuuXcnhtDKta9QW+gXrOSjY9FtI4uFBm+ZnG/mETSyKb+vKmIXntPFbsb1hnTdJq/VhNhm2I4u+GbTqfuGbG3ipNWsfiP5uNg9vsNkGxDQ37x11Zp4HF/jGKWML6l8fqxyeyYLl/AubFETcjqPG2M7C67BYa+/KWpsdC1WWw/bWlFplv8+PimR5kth+aoZ64nLXPNfHQsK6UwxsWs0oxhhXA1Ne2sPCOEnKKAgio28nzizc2emjb7HqjPK7CWbJ+OWOVG7qulIxLKoL6ovg8Y3nx/SWMVo53ZqQ4ZvXbRFHHqPQwq2NWtfLBUCuPq5Zo5/MHxbro949yu9KwHIu2zoZl27zeNm5Dm857GxnXTVkOgI6Mr5eydEvDkd6q876FbUqT9apLKcUDj9yW759GbWerNHGOKj5na9uUlghbvJ7Y8VZWAEBXSs7Rr1n3znbTuJAdun9soTwnjAY/y/o/T8KPAva8/AzrjO143/nE/Xk6QU116Wx+bvadT9zbzQUVlNcCNZNeWsuzo6zuocbrCC3e97aZxPK/P6s/76tT2PybWLYDYS+sJ3aMIaP3x1ieedcwGuzg+cQ1GTzRkbHjdZZ+2DBOpfH606L1a9Qm6bOeYv9b/+C79Mg6Fr9tPH+u315ZbENr93/Q5D1j9FvbmDvE6ocETQFp+zezYtPhVp3Ltl2TrV0H9Jq+dtjOcp0y2D5vKZuVH65Vbb6a6D9vYu7gxtvS8hi37V7CFuqYNWx5SJ/uWfCv53lmQw4QzcptcwlRAbo0tj62jHhDfdv2j1HLzs2m91nT+7llmp/f8jw0fPYqa5/DQNlWKv82aqrttEHAgjjipjV9fbDc3tbPV2jqHG9ivzR5T2uL5tsgXfp2lr602XRP3vJrsnG5DeeT/t5Z+bfZNcWWa5XNmr+vsVj29dqIJr8rmVcyZ37dbH5706hNafqcaPo8bPl3cJtYu7Y1qek2s7RIg4e35Xrb2l7ZdD9m4724kcU6tWW7CSHEbeRqmYYe7tZb3Na6IRnA7oPGMHve73nuPxazePFiFj+zgNn334lvU1ca0WGeXDOEHTuGsONjH8YbytTD1Ly+fiA7dgxh3YpBrPn7EHZ8NZh1zzso5r6ZIpk8rCeUJbH+hZVsWN0Rwd/hxKzcxKdx1vNc1cOeIO6D9Sx+aDiBjiVknztB4o7dJJ1OJz0zH53qxoznNvx3K9j0aVzHZuPeDJmbeP6RKKJucvD3dlKvq+Jq9ikOf/NJ1wz+dgafbWbj3jQKyszGcarTUZp1mK2vL25z8BdA89kKVn+reA8rDr6zmNiPD5NT2ny99qIrzeHwx7FtDGAcZPU78aQUmC1BV0pO0nZWf5FGk58kaTWrt1z/s+ZsWcqid3eSVqBp6LaxI+k0FJzZyernLB9o2EqzdwWL31ast/G4erPpQM3Ob1MoVQUQ4K8jLfGTRsFf2yWz+pWNHL7U8H6aS8lsfXMxX+t7HVc4yKoXYtmamENptXJaY59/uJE9Zwoauo1FH0jLSdxK7OLWBn9p/XElzHSibbj/Pf72dbLl+V6nQ1OQxs53FzV64NSq876FbQpJq1n9WQqmzWLsBnbxh1zQKuo2oX3aTqNkVr+7mcNZZl3TWtHaNqUlUjZtJ8Uwu65asf1UHgREzmf5aw0ZYR26f9rD2XVsTdIAfoz7XXTDw86szSxdvJqdyjbLmqzNvPX3g5brqykgbe9GNiZaazw17HnbyjW8Tn9N+dv71lrDlu1726RRUqn/ny4rBWN+espefYYy6CjJMQR/Ac5uZulrjdfBdG6aBX/bxdntxP7PdjJ04DHqKeJuUDZR/LYD5Bg+X6NjXO1HyEMvsvLpdutD9qYzdgMNQEYKn7e+eVDQEP9WS84h2+4lbKEpKDFcvwpIO2S8dsRzLMOwQiUFtOH2zaAjzs2O4oqjCijKafqey9BV7HU11XbaIOfDt9i8PwfLpjONPZs2ctha02kTW+9pbXGQ9zZtJ1mxz3VlBaR9t5pFZsFfOviabNO1qiN9tpmNe1PIKdVZbpNqw71kG78r3Qgt/Q7ecTTEv/U39mSVmhXlkPxxLIut3kvYxqb7MRvvxY0Oxu8hQwOgo+DkYcMQEkIIIW60Ds4AdmHYjCeY0K+7coJeTS6HPv+Mo500yfZWzAB+cs0QZg0Ayq4Q95tC9qvVrNrSl1Bj5FJbC44OQB2pH5/lxW2KBbRB2zKAHyXuiycIzfmSqMUdlYM6gditS4kotPIeoTGsWTmLYPsSTvwjjpWfnWjZF6EO0OHZuDcrA7gTuTUzgIVoraZ/NX07a+4X40IIcXu0nQHMfzuO6cFaUt5fTOx3Zg8p8SB80Ru89KsAVJL1Ibqssby4aQmj1TnsfGsZG827NVcHMPUPK1k4XN3GrDohhBBCCCGE6IIZwL3u/7Up+FtTkk7y3u188sV3HDp9hZp6oHsv7p31IP07dC1Es37tYQj+1pG94yzTos8xbdoZnl2TyZc7lJVvJldUNyK91qpAYp59mGDHEpL+3yKW38TgrxBCCCGEEJ3DJMKC9V06OXo2jIcOagKGjiB8oKe+a8GiHMn6EF3T+HGGsRYdce01wHIsy7vHEd5L/wVVU3TBbCYhhBBCCCGE6Bw6LgPYOZw5MWPoZQeV577h7zvTsehVovcEFswehrsdFCd9yD8Sy8yndgq3RQbwwj7smOGuDwB/e4EX19e2PbjpM4FFLz3B/SE9UdsDdSVk7/+Ub1yfYJGVDODQ6GU8PzPCNKautiSbpK/WsDI+FYCYtQn6dbaQ3pCNGjqLZf85m4gATxztAW0J2T9/wZq/fIl+CUaeTHh2OU+MGUBPd0M0WVtC6o44EgKXsfSexr+uSP8qiudPLuOj1yJxPLmJJ5d92fLtY9wOA3uiNr5dWT4X9m/i9b8mNizHlHG7iH2hscQ8EIyno77bt+xDH7HsLwmUAEyM5dP/imjcndIFfcayKUt36T4ClzxGRIDaNA3Ac/wils+7nwE+av12qtOiKbzADxtfZ8Mhs09lQwbw9fadeVb10v2BPP/rCALVhu260WxBirrmGdjK9zDus6V/P9EwazuTDGAhzN0OWWy2kwxgIUTzboe2s4kxFc3pCji4/hlWSzspuiJ1NCs3GcaHbYomja2vLCM+SzlBCCGEEEIIIVqua2UABwXQyw6ozyV5nyL4C3B5H4cy9aVevfsrp4ob5aCGfADsCXxoENu29OI/ZzjgqazXUurJxL67lKg7PNGmJZKwI4GEQ/m4Ri7iybsaf3MOXbiGlb+LpGfdBRJ3JJCwI5Fs+0Aif7eSuMf0B/uJ/Qkk7DihD4IWntAvc8c+TmDsmjmGyF5w4VACCTsSSMx0JHBMDCvjHjULloYSs3YTSx8KxVNrfK8EEs9rUff0JD3R8N7V5u+RwL6TEDgqGE+0nP/ZhuBvaAxrNhi2w3nDdvg+iXx6EjptGRtem9wokNtz5lqWjoEz3+nXJb1aTeCYRax8NlBfIV2/nMRMLVDCCcM6Juw3D4R6EfnibFR7VvJoVJQpkBq6cA2bXowitIfWtJ12H8sHn1Cilm8g9gHl2lxfS/adiXskL05TsW/Fo0RFWQv+Wqd+LE7/HtVn2G14j9QSR3oGtvoIFUIIIYQQ7SKZ1a+sZntSDqXKsVGrS8k5sZPVz0nwV3RhmnhWvGUYr14xHq2urICMxK3EPiPBXyGEEEIIIUTn1HEZwGGzWXx/AJSd5LMP95GrnA70un8Bc8Lcm61zM90WGcBA6Gwflj7uS08ns4qFhXzwlyt8mWZW1gL6TFEV6V8t4/mNZvm3Pk8Q9/6jhDpqGjJL+8Ww5t1ZBOYmsOy5DQ3ZuurJxP5tMRFV+1geE6cP9BLDmoRZBJtltEIgMWvXMCsgn4Rlz7ChYQFMjv2AxREV7Hs1hrjjEPHiJmLH96Tk57UsenN3E4Fc6xmo+s9Uwe7nYlibaTFDEwzrNUBD0upFxH5v/m6hxKxdyawBGhLffIKVPxszboOhJIm1i2LZbaweuphNcZPpmW++HZrOxtWXqyn5MZYn/pLUMMGwnYM1iuVjNrZxWSKxC1aSRAszgFu87wzb1L2k4fM2qfH2j3k3gVmDskl49Bk2mNZbjacPlBRa34vtQTKAhRBCCCGEEEIIIYQQQghxI3StDGAjtTvuTbxLd5V+fGCqNRQrJyrYu7jj7qF/uTROJBVtkPpFIQsXpLL2iytklxl+D+Djw2+fUjfKUm3eZCaEqqEwiY/Mg78AhR+x+6RlwC5weiTBjlrO/MssgAig2U3iWQ30DCTCvFyp3ywiBziiTd1tFvwF0LD7xzNo6EngCIAJRN3dEwoTWdNk8Pd6KtC0KPhruV6rLIK/AKls+uokGjwZ8qtIiynZP66yDM6m7udMPuDsSk+z4uZpSE8yC/6abefU7xTLB0jdxJf/1oDPECaPUUxrhs37riydpC3mWGEAAP/0SURBVGaDv9blV2iAngz57XCzY1HTocFfIYQQQgghhBBCCCGEEEKIrqyJ0Gw7OH+R3HrAvj8jR3spp4LLMEYO0geAi3PSqVFON/IexvQFz/HcwgUsmKd/LXxmMQtnjyHYRVlZXI+jveE/1XX6LpWNNNf4198LefY359htSMV27OfKZPM61xWIpztoL5/RZ5IqaOst/w72dAUcGb4wgYQEy9fiCDXgT+BEy3ksBHvhCjgOi2k0f8IS/Vi5/r0nAMHNrtf1aOu0+nV5QDmlCYb1KsncZz3YvDebPMDTZ4hZoYb8c8raJyjRAO6eGDqBboFi8g5Zlui3cwlZB5XL19t3OQ/wpOcg5ZSm2bzvSvL4yezPlkr4OIHUMkeCp63g0083EbdkFhE+ylpCCCGEEEIIIYQQQgghhBDCqOMCwFXJnMwwjPEb8TiP3x+ClwrAHpeAcKbPnUAve0B3kePHmsj/7T2BBY9PoL+7MWrZwCUgnIfnz2aYBIGvS21InVQPc2dYL/3/tSVaTgL0c2LR77oTaEyvVHfDkJcNVTrD+MC20WmtBxqtKyH1O8NYtlZeienK+o2VnN7daD7Ty2wBtq1Xg8T0fLSoCY5oNh+5k9Cia93HbAUb9l2dznow/HpSP2Lp3CeI3ZZIeoUroQ/EELvpI5a1YsxiIYQQQgghhBBCCCGEEEKI20HHBYCBtJ1fcLIMwB7fsAf57TOLWbz4ORbOHkN/F6C+jF++/Y5fqpRzAnYhPDxjmL77aN0VTu76B++tXcva9Rv54uBFKusBVQATZt2LlfxiYdKNJ98dwo7PBrNtRR8CHQHquJCkD8epf+XNw7MHsG7bEHZ8Nogd2wYxvpehzoGrJCqW1rwKdFpQ9wm1mrHq6WTZd3dJVQWgpiZ7Axv+au31Ebub63a5pIIKQF2bbWVe/euj77Mb1itwGMOVy2iJbfs4owHPe54gJlQ50Yr0YioAz34TrHehPTEQfyD/cmvykW2XXlIBeNJ3rNW1YUJvfyCf7H8rpzStzfvOJiUk/WMlz8c8yhOr9pFf50nkky8yQVlNCCGEEEIIIYQQQgghhBBC0M3f398w6GsHsXMnePyD3H9HL1zMEnlritI5tOsbThaZV27QPXwOvx/TC+qvcOiDTzhaaTndJWw2v7s/AHsq+eWrjezJspzeHry9vSkqamIFu4zuvP7xACLcDX/W1XDh22yWva/PyBz/TB9iJrrh6dStYRZNFSe/zWHlllobszbVxKz9lFkDNCStfpJYs/Fv1cMWs3blZHqiIel/HyV2L3DPMj56LRJ1ZgLLnlOMJdtIDGsSZhF84UuiFm8ylEWw7MNYIt2zSVj2jGIcYHNqZq38gJhhKtK/WsbzyvGJTSYQu3UpEXWJrHxipUXwO/B3a1gTHYyjJpVPV7zOR4rxjC0FsmjDeqICSkhavchiO0AoMWtXMmtACfvejCHuZ2DhGhJm+jdsFzMxaxOYNSCdL6Oex/ipJ7z2KUvv0ZL4lydY+WNDXX15nkVdAPotYv17UQSWJLF2UazlOMChMaxZOYvgkn3ExsTpu8i2sj6Nlt3ifWfYpoXm+60pjet6+nhSUmjeWbmaRe99SlSvVD6avZRPzaa0J29vb2WREEIIIYQQQgghhBBCCCFEl9DxAWCTXkxYMIdh7pDzw1q+SFFOtxTy8HM8GGwPl/ex9vOTyskWyytL+YwPfzAMXNuObo0AsJ7nIAcCq2o5maOcYtSNAXfZoTtXR3Zzsc3rmbiMj/4rEk80ZP/8EyfytTj2HM59I1zJy3EkuB9mgUU1k1/bwOJ7PKEsm6SfT5BXBTj7MzA0mJ7Zm3hixT7Dgq0FgEH9QCwblkTgWach+5j+/cAR/+AhBPtls2nBSvYBqCcTu2ExEZ6gyUzip5N5aHHEP3Q4PfM/4pm/7DMLYGvJ/nk3J8oG4nV1KSv/rl/XyP+MY+mDgTgCmvxssjPPcD4f/IOD8XT3ItDpDGuN72cMrDpqKTmdxE/pxeDsz/B7Igh011oGoq0EXI2sBYDVC9fw6cxgtDlJ7D5ezEAfDUtXbGocpDUTunANK2cG41hdQmrST5wvwbBfAlHXpfPlsufZZIziWlmfxstu6b5rHNQ1MgbVNT/G8cRfrNeNWZvAZHUqJ34+TzHgGDCSCXf3RHdyE08u+9LGHyi03K107gshhBBCCCGEEEIIIYQQ4vbSoV1At0X37vp04criK8pJBrkUVyjLRFNKzjUX/AW4xoV/tzH4C7B3JYtWJJCaD4H3TCZqWhQTBsGJLSv4stGAwhp2v7mYuG9TybcPJOKBKKKmRRE1bhg969LZvfeocoZGNN/HsnhVAqmFDe8X9dAEhvWC9B/2YVqCZjexL8SRcDofekUweVoUUdMmM8xHS3qqcbBaDZvWfUpqiSOB90QRdX8gatMxpiHx/z3DE8s+IvFcPngGEnrPZKKmTSbijmCCfdRoCvMx5aqmbuL5ZRvYfU6DOiRSv14PROBVlcrudc1lIV+fZuN6Pj1dgmNABFHTJhPodP0TIXXj8yxbt5v0KjWhY/TbefIILyrSdrPBPPjbYm3fdy2Rfi4bbY9QIqcZ1nmII9nfb+D1Dgz+CiGEEEIIIYQQQgghhBBCdGWdNgO4/+TfMz20O5Qk84+PfqRYWcEuhOnPPEh/eyhO+pB/JJYpa7SZZAEKcSM1zgC+WeTcF0IIIYQQQgghhBBCCCFEV9VpM4AvZuVSB+A5nAlhLoqp9gRMuJf+9gDFXDzT/sFfIcSNFoynO2i1189oFkIIIYQQQgghhBBCCCGEENZ12gAwqd9zMKdOH+y9fyELZ4zhziBfAgaP4eEnFjJ7qDsAZSl7+NHU764QoqtS/3YIgUB2aoJykhBCCCGEEEIIIYQQQgghhGihzhsAppKTX33B0YIaAFz6hTNp2uPMnhJOsGd3AGoy9/HPH3IV8wkhuooJf1zPmj8uYtEf1/DBnFAcSxL5cqOM7iuEEEIIIYQQQgghhBBCCNFanTgADNTncmjbX/nwq6Pk6uPAUF9HZdFFknd+yF+/PkmlYhYhRNdRUg3BY6KIGhMMuUlsWrGSfcpKQgghhBBCCCGEEEIIIYQQosW6+fv7X1MWdoxeTFgwh2HukPPDWr5IUU5vRu8JLJg9DHc7yP3xr3yWbIwGdyxvb2+KioqUxUKIW5yc+0IIIYQQQgghhBBCCCGE6Ko6dwawXXd63T2dhYbgL2Un+fEGBX+FEEIIIYQQQgghhBBCCCGEEKKruXkZwKle9L97JPeG9sddP6SvggPdne0b/qy5yL6PtnPyBvb5LFmAQtye5NwXQgghhBBCCCGEEEIIIURXdVMygLsHTODxhb9l+ugQfD26093Z2qsh+FuZ+SOffHBjg79CCCGEEEIIIYQQQgghhBBCCNHV3JQMYJP6OsoKz3M+7QpWY7uaAlIzcqjUKSfcGJIFKMTtSc59IYQQQgghhBBCCCGEEEJ0VTcvAFyWxjdffEd6maJaJyJBICFuT3LuCyGEEEIIIYQQQgghhBCiq7pxXUB3705347vV5bLvn507+CuEEEIIIYQQQgghhBBCCCGEEF1Nx2cAuwQzIeoBhvl3tyiuK8vhxMFd/JhutfPnTkGyAIW4Pcm5L4QQQgghhBBCCCGEEEKIrqpjA8Auw5g9fwIBKsPf9XXU1NnT3fg3deT88He+SOmcQWAJAglxe5JzXwghhBBCCCGEEEIICH0ohgmBpgf6NtCRn5rEBUUvoBXZJ0gvtCwTnVUEs34fgWv6N3z0fbZyYhehJnLOEwzzUpbbQkfOoW0knNQoJ7QDTyY89iihPZTlUHLyIz491BHvKW4XHRgA9uLe3/yWkd5AfRlpu7fz/dli6gDcg5k082Hu9ADqr3Dog0842gljwBIEEuL2JOe+EEIIIYQQQgghhLjtjVnGR3+MxFNZ3hZlSaydG8tuZbnohGJYkzAL/5/jePTNfcqJXYCaya9tYPE97XAEa9NJiF3GhnYOAgc+u571DwUqi/W0qXw0eymfKsuFaKGOCwD3e5DfzwihO3Xk7v87n51QRHjtQnj49w8SrILK01+w8fscy+mdgASBhLg9ybkvhBBCCCGEEEIIIW57v1tDQnQgJzbOZvlXyomgDhjOQF9laVM8efg/lhLpmMjKJ1aSqJwsOqGuHgBuyfq3V53WmfDapyy9J48vo55nUwvKhbCFnbKgvfj270V3gLqLnFQGfwHq00hO05e79AzEXTldCCGEEEIIIYQQQgghhBA3xXAfV6CEkkzlFD1NzglOHG/pyxFHZ6AwX4K/4jYVxdJ317DG7PXoIBXgT2QLy2N/N1y5UCGa1GEBYAfjkjUaFN38/3/27j++qep+/PhrViKaDAkgQW1Q07mGz1bYWtSCFqsgn4GBCh8YyEdWtBQKfC3oKqzU0ZZROrCfAXVAsdbB6hwIAwsRNkYdAyaoFAeds502/ij+CCJBbESD6PePm7TJTdrmlpb+4P18PO5De8/Jzbn3nnMvue97zmnw7dfKf7tdgV6dJoQQQgghhBBCCCGEEEKIdmE1GYE6XK+rU1rCjLEHuF016gQhLhEmzDdHEeW3mI06QI8pzPUDzK0wnLVoHdZxTBoRXmRTP2IS46zqtW2vzQLApz7/SvmfHtcSeaU6VXGN0dvvt+4UH6kTRQvoGXrn0IsWTE9ctAm7fRM5d6tThBBCCCGEEEIIIYQQQnReZkxX6+CMi1YJ2d5tph/w8YetO4Ruh3d3Dpta4xm6ejvqv0UnUMJcm42CV91ADdtsNmxhLP75W3sIatFSNvJyU5g6u5CMZoLA+hEZFM6eSkpuHjZ1YhtruzmAr4xlYsodXHsZnD++l9IXjnHmm4bkq2LG8+BdkUQAHx1Yx+Yj3oBxB9LZ5gE1TSygMNlC3d+LSH9iN607HXkwZRx6OPybSeS8pE4VovNq77bff2wGM29Tv83l4lBRATtqvX+ax5CRFo86F44dZJUcUq8F4knJG4MlYJ2DHVklBOYOlQ9cr6yjYPv79X/Hp+QxxniIdQU7aFhbnxpyG/77UL+PjZbX67YU8sZagvKFOkbqMnZE4Za7/9gMZn6/OvTxNY8hIy2a6qICdlznPT6NUs7xhyG+N3Sd8m7Xt65ef8ZkzCT6P+soeH1Q6LpXT7XdjqKxNgM4tmdR8krguviUPMaEOLS+8xXqXAa3KaUtEGL7+L6D0G0g9Pert98Y5XzFq4qnrmuh9kGdB/98jbXXkHUn1HUgVPm15TOGKB80dX5Dbau9JZLzXAaDm5j/xP1qAZMOJLLp0cEhXuyrqZ8DKKXQzrigeuJW/dtMmasoKmi9mq9cfvnuzmHTo4P5+AUbc59Wcvm+093Y3EfTV2G/j5DzFCn/dtRT47c9fymFdsb1OUzBlBxCbLmDCVV3m7gPh6qjrhD30VD58Nuu777YKF+dD3Ud6KDXZyGEEEII0UGNJOe5dAaf3IYt3fevez1DR9zCm3v24lLlbtaDq7D/Tz8Or5xEzh51Yhd2dw6bHh3Am03+HguDejvqv9tE2819e3GEU/7WyhM+//l9d4+Yyr1RdRxetw1nI/9vkPmAA1ltpNxpwvn3EuxV6sSLRwnsJmLCyd416RTsCY7IhZOnLbVZD2DOHuHAG8rgzxGRiUxLeYB774gl9sd38N+TpzPdG/zli2pe+2fHC/52Rs7N2ZT83YXxzjQKHxsZ4oFhBzImg7WlJSyUN5SEaISDHVlZZHmXda9AfFoGY8yqXNsb8mRl7cBhGUNeSnxAnv5jM8jzBqEa8max7hUjY/LySLktIDt4g0D1eYsOwW0zyRjbX52tSQHbyMoiKyvEQ2fLDwgsbaD4HwY/5I5PyWPmba6A45NVdEj7D4+LKp6UvDwlqBtwTHbgum0meRlj0HZ0vV4p8dvWOg651MfdP/AVXp1qVu0OCvy2s8PhDUw0dZ47kMA2o9Qd49i80OfAdUh1vrJUwcfAY7rDYWFMXkqTdbpZ5jFk5HkDw6rv3uGw8IMQ7TXAbSnk5SnB+oDPb3f4ZWphfbSMCXm9CGIeQ4Y3WBtY/sBsLbk2NSfo/Ha44C/AXnKm+L3N+0JN0Ju//j8oa15Qv/2r+sF35jAFAW8Gw+BHQ70FrmfAHYnqlQ3uTmRAE0FpNf2ts0J8R1MSSbTqcZ9xE3V3Dk2UpFMJvOaGvg/Hp+SRlxZNdVFg/dzhimdmXujrcKP397Cu+/Gk5M0k3hV4HVn3Sse+UwohhBBCiI7GO2TzqYYf+abkpWTMy6CkeCG2PgGZm6XMJ1zHqbfUKUJcuqKG2rCNSWRQE/8v/FjHkZeVxrgx40hbsoqUdhhW2ce9p4D0NXtxYiJxdgHpQwIjcvoh6RS0Y/CXNg0AAx/97Xn2vucN7l7Zi6jYO7gjIZbovlcp6756l73P/4V3/XoGiwvhZvcT6RR1hiCwyYzZaECnXi+ECOn97c9zyGUkfmRToaVDlGx3BAZVb0th5m1wqCi4B+L72wvI2u7AMjb0w+d6tTs44ADjNdepUy6My4HDZeGOxgLL5jHcYXHh8n9e7V13qEgV1KndQUmoXoEdQn/GZIzB4thBlrqnF4coyVrHIeKZqQoYtLXw6tQloHYHBVk7cBgv/Bwc2n0IF0auaao9NcXb88+1PStkD8JDJcHtOMBtKeSNNXKoSB2oVl4WUNa1sD66DnHIAZaxzQe440fGY3TsCCrDoRK/dtsa1yYR0t7Fazl8JjjYW+OoQX/rOFIC1jZIuW8w+jPu8EaQcRzm8Bk9g6drCOTenciAHjXsfvpN3D0GkKgpeNxZ+O7Dd9TX3f5jMxhjcbAjxMsxh0p8L+M0165C3N+b0H/sHVhch1inuo68v70kqAxCCCGEEEI0yjtk86mP/lG/yrlhLaWvu9BdO5S0orVBAY+mWE1G8LhwvqdOEZeEMOdLNY6e2i5zpYpOwDqOvKwUBnGYokeKOHw2inEdIQj8xG5qMTPysYYgsH5IOgWPjcRMLbufaJ/gL20dAIYvOFb2NH986RjHT59vWH3uDMcry/njM9s5pnQSFq2mEwWBhRAavM8nmjvu9GdMggUcBxp/4PvKXznkMhL940aCsG3JCCf+48J42z0hH2grQaQDHAjabyN9WzkW3aZuu4d4o4tDu4MDeor32bE//Af7racldaqr0hZcaSu+wKk6IBoepb27Xnm+8fbOBdRHY18+KdmBAwtj1MHhUIzXhO5FDB3/2tRF9TvpooYoRi4KEbK9O4eRFjeHX3pTnRJaH9j79GHcPQYzK9T2Qki8YwB6xzFKXsphtyM4QN1lfHjCb0SKeO65zYjrlb822hP9/e0HcBBG736tjH3pTLdKIYQQQgjRAd1gRI+HU07/wEUV2345lYzfHcXVzczIrGcoSB4UxvNn73zC7lM09jPQJ6XQjr0wxTvHrR27d9kU4rdH4qJN9el2ux37c34vqU5fhV09R653m6um+60jhVUB6xLJea6RbXrTNi1KVMpp95Y1VFm86xs0tV2v6asCthFYztZmI2PFKlY1uQylH9Dt5kkh0gKXnAeb7qtqHXw74x8uIqeJILBxdA6FM0cy2Cpvg18s+iGTWPiLhUwK+TKHFdvshSycbSNUjFU/ZBILF+UwNeRnW5l1KgW5KQziKCV5OdjfspPjCwIvbecg8MFCMvyDwJP9g78ZFB5sn+AvbR8ABjjPJ//ay9bfr6awsFBZ1q5n69/e4JNz6ryidShB4IK/ODHemUbBw0PDuAk3oU8iactL2FTmvfmUlbL2URsGdT788m71uzkX5fi9taPcUO33RQF6Bj+qvuHpGTRxIWtLtzbc7LaWsmrmBe6DEJ1ef64xguuTD9UJAfqbjOA6gZLrOvoawfGvxh47A7zP0f+4MH5/UOPBmttSlN5LIXokXqhPGn3wHc8PLCHKXnuUahedqmegck6qOdrUL5xX3mjkOLSl8OrUJePDE7gu6Bz0Z8ykeGguANuoRup8uMyDiDa6qH696Z7wF1Yfg3s3hnLoXw5oskd1K12bRCOiMPaAjz9Uz0u0l22vutFbE4MeMiTeMQD9mTfZqxqmu0kv5bD2VXeTvYobpDDuVj01x5TBq0uONd0buVO7ri9GXHxSC5ivwUhz7fIQbzjA8sPG2osi8P7etPdfr8aFhTGNDecuhBBCCCFEGJQhm124QvTYrfpTFmm/3ESVW491Yh5FvxoXMkDUYAC99IDLycvqpFD6jGTTdFjrm+7mN4fh1gy/ILASTM2wvuk3JU4BhxlMhu8589PHqEGP0W92scQ7BqAHogb6/RqZPpAoajj2NN5n1xnKvMfe7W476bdNH+ssRp4sUPKkl8D0Vd45Wn1l2UaNf370DH50FjzdsD/qF2oTF23Cfl8/Dv+mIU+/+9oyCGzCfHMUUU0uJvSAzmgOkRa4DDAb1V8QoOrZDLI3OxnQSBBYCf5GUbMunawXmnpoIVqPjYXzpjL0jqFMfSyXSarUQY8+RtrooQwdncZjj6oD/JPIfWwqQ28dzKQQn21V1qkU5E7C6jlKSV4W23zz/p70BoHdHSwI/EDHCP5ycQLAon24efnJDAr+4sT03xktDwLrR5KzIgPbfxnxVL+MfYcd+0EnhqFpPPSjburcpCzKwBZt4NQ/d2PfYWf36066RQ4mJWuh9yZ5lL077NiPuQAPtQfsyjb/8rJyU7z7MRYmD8V03sHLO+zYd7xMzTkjUWMyWPpgE0+bheji4lNmEm90cEA9rKs/8xh+epsRx37vsK7eB88nwnlarGK8bSZ5eXnKMtaCY7v2eTQDtpHXyByrHOKvr7iwJASm+Yav/GtQT8j32VGwThm6OC2PvAudb/UiuE6JsqqG2m1/YdWpS0ntJ8HzSBvjmelfh4Pm6rQwpj5tJvEc4vmWHs8LaK+gCjo14YLr4ysl7HAYiZ8Uqj17vVKizDlsGUNeXl7w/OEXuq9NsIz1P195QXOxdkZR9/m9IR7yLfJAKYXjiDpzmG1Pq1Ng7+Ld1PQYzDjV2+7jbtVT81IO6pBxc5ThpqMY10yZAh+o+B7ERDGwzR5ktBPzGDLGWhp6/IbZLpulvr83p3YHBUWHcPmuYV2gHQghhBBCiIvPYjQCdbheV6cA+kHY7kvEoge+dFJzzNFMz17vfMInA8OijerxMbun+P1GUb+AOn0cg3u4Ofy0/++YveRM2eb3m6cG15nAYG9UHz01jhqwDKx/ITXxun7gOEYJkLhoJFHUsC1deXkVoCTdf5sKPW+ydnHDN6cMjKrfhqKEuX7bAHC/upacl7x/+Pan/gVd5XdZqDxRd4foKdwqSphbH7BubFEC2e5XvcHuJpZJfsejMY0FgfUjGoK/OTuDns6IS5kv+EsVm/yDvz6qIHDawBZFwbosCQB3aYFB4JYEUBN/nsJgo4eaFxYydf5SitYVUfTrDKambcIRagZf51FKFkxi1uJCitYVUfjLdEr/7QHjIBJHABxm27oiihyngHM4Xy1Strlht/cfCXW8/ZelTJ2WwdJ1RRStW8rc7N040RE1+N6WBbGF6JT8A0t5jDEeYl1WcBA2INgxCZ7PCp5PsyVcr6wjKyvLu+yAsdofIAduIyvEfKOK91+vxmWMZlD9JUoZMrPxB93vs6NAKZfDd5w0lu3SFF6dEn5ch1jnX4eD5vB0sMMvfd1/opkZFCS+MP3HZgQENIOCqe3gUIkyZ/JPmyrLKyXKMXnF5X0ZpHWPS2Mc2/3PV+i5lDubmhdUP6xVDxHoMZgMvwDxwGM2bP4PSgKUcMwR+AAkcdHIRgPGzdtLztOHcVvGNflWeqiHIepydFYBLzt55/BWz3/dEhd8f6/dQUFWVsDLGClBvfqFEEIIIYRojF4ZsvmMS9WTFaz/k0PJhjym3mrE9WopWckp5Gw+SpP93HzzCTtfU6eEFuJ79x54Ezf9MN/t/Y1x5k32+oKl9fyDvnvZW+WGPub6IOtAixvXC8eo8W4HEkm06r2BaeX/A3+7NGyz33V+YdiTtQG/uUqO1YBlXMhhqn2CR2kCehiJwvfSrJs3DwTm2fvhxw15uoiqZzPI/v37RHmDwPoRORQ9HEXNk2kS/L3o7CxdWcrLB16m9IlsNqlSj/7mCYp2vszLO4t44jdHVambyH6ilJdfPcymEJ9tFf7B3+wMStXBXx+/ILAtZ2m7BIED5vx9NnhO4PYiAeBLgNvjAXQYru6lTmrGSOWmd/IwpU+rWtfJUnYfC76tB3TBB8DNtv/UAnqMN/qvb8RLBWQ9+XLgPxiqjlF7BjD24xb/9UJ0aYGBpcaCp/XBDm9Pn4CATO0nuFplvtxDlBQdwtXMsK8tVruDAw4j8SO9QdzbfoAFB280+6D7ECW+fbeM6bBB4A8/cTUzH+rFEl6dumS1Qq/U97cXKL1jfXVZi0ba6/vbC7znbB2Hmv0dZOSaZtpo69RHpee+8bafNntN8JV/h8NIfJo3CNzIvooWOnO4fsizbQ6Ium9Vk0Mrl7xwGLdlpHceLO/Djqq9jQSMw/BSDrub+t67cxhpASzjAnoyj7MA9eXovNQvOwUEaT88gSuMdhlKk/d3LfxexrCMlSCwEEIIIYQI1y30M6oCnX0SSVuxiYIHB2Py1GDPm0rK4k0cDX5EHCzkfMJNUAVYQwqZZy+1J/3+OvAm7h4DSLzbG2Q98yZ7XyrhmEPPgDsSvVPoqAKvqt8udnsGg3s0JEOInsxPz8X2Qg36WzMaGbnJjavZKXf8pkv0Lfd1pdBvg6o/ZZH3+/eJengTm3zB3z1h1g3RqtwHN7H010vZFHKo4irsa5aydI2dULFX98FNLF2cQ2nIz16ooWQ8Fkbw18c/CPyLxxipTm9DAcHfJzIo3KiaE7gdg8ASAO7S9AyauZTsMVG4DxaSvlL9lkZzlKE5PB++yWF1EuD5Rr0G0JsZOXkheStWsbZ0K1u3bNV8ozIOHkfaogJWrS5h05atbC0LvskKIVRqd1Cw3aEKyHzICVdz8wr2Z9D3jbj+c7TpYGAbB2wO/cs3r2h/xiT4DZ8ZDu++Y/lBhxwO+n2nCwJ6OIcQdtBbtJX+P47G2NzcuGFoeYA1nPbahFfewIGR6B83/c2tVR/f3/68MhR7U0NB+zlUogzdrpQvnH0N89okApSkFzQ/JPNLe3nzjJ7B96V4h02rYXcYQ3U1pSR9GzWE/l5ljq0av7mw/IcS8z106aK8986m22Uz83+HvL9rp7yg0ly7E0IIIYQQwicqeMjmPgO5xQI1OwuYOmUuRQfdmEdMJW1mWuhlug3frKFNzSccNosRPR9T6+v1W9+z118i5j5+f3p//xgtSq9h38uvNSfd6PtE+QWFGz7S2HDHzQ5x/PRcJe9vlFGS7Op5g5sV6neTDZttrqpHctdQ9acs8tZto/TXEvwVobxMwRMFFIQT/PU5aSfnkRxyFuewW53WRvQjMij0D/56g+EBcwI/VkhGiHmvLwYJAHdZfsHfVwtJy9vd9DAcTTjnCfOT1hRWbVhL+gND+V4PHZ6PjrH3r7vZdtipztkIPSOzSinNScH2IxM6Tx1vH97N7p17qTmjziuECBI0N+f77NjvC6yqMyv6j/1pePPAtkLvyCa98lclODTyHqLDKU9n4t23xnuFxpPiP2dkyGGxG7RWoDJI7VGq6wN0KuZBRBtdVL/ehc6LP63zazYhcI7dQ7zRaMBFHfRpvr02zdcr956mX4RoQX0M7X12bPL2TBzZV53YjOb3Nexrk1AJZ0jmveS8pMx5tWpgFO5Xt7XCw4QS5r6gDHm2aqD/+saGUKN+GOiGOa+6oubbZXzKmEbmvPcTdH8XQgghhBCijd1hopd6yOaqEtKnTGLumr34BqgaOXYStjG20MvdgzF681lNTcwnHIrfHL0+yrDPytDQJcdqGhkaWQlc1xzz/QJRegRHDczB3Kehp+/eA2/itgwk57p+fj2JlSGjL/g3yks5THqhsfI14ulj1BDFwEZ/x3VNVTtLGul5KgRQtZe94QZ/fU4e5rDWz7SQfkQGhbMTMeFk75qG4K+P+2AhGWv24sRE4uz2CQJLALhLUgV/F7c0+FvHOQ/or7cS6vmssXu3gL8TfzqSqO5uDq+cxKSUWcydn0PhuiI2fuQJyNco/WTuHWLE856djPFTmfXIXLJ+XUTRumP1/6gQQjTt0G7VUJGvlLDuFYhPCx72sf/YDGbeBoeKmpsHNp6UtHiMjgOq+U9bkxIQMlosGB1vNF4e8xgygoZ6Djdg1V7eZ0fBDhyWMeRlqB/ex5OSNwaLY0fgnJG+YbHTUgKDBrelMLOVApXBvOfgtpmqunIxzn/76T82g7y0eHhlnbb5NUPoPzaDMRYXh3Y31MRDu5UhygPn7u3PmIwQQR+/9ho81+919PX9cm6E0sNPmetZ3d65LcW7zRbUx8bU7uD5V1xKu/VbHZ8SPN9vUEC3Va5NIqTmhmQGeHobh89EEWUJnmOqxZ6eqwxBbfF7xHF3IgMCHr4EUh7aeIdj66Ia2mVwu4hPyWOMxcGOMIbkD7q/N6H/2IygdsVtKUHXJyGEEEIIIRoV2SvEkM1u3AEPmfVszPT2Up00i6xfZgUuvy5BCR+bG51PuHGqEYamr2KcBWpeylGCtd7fNOMCetkmkvPcOKIc25j7dMNHlfl5BzMYv56+L9XyMVEMvlUf8Htl7+Ld1PQYTEbA6EaJ5DzXxO8rIKUwMN0/WB2eEra96ibqvk2B0+RMX9XkvMJCiPZiY2GqL/ibTkEjvdjdewpI9wWBUxdiU2doY9/p16/ft+qVQtG7d28+/fRT9eoOrrWCvwB6Ugo3Mc7i5vDKhwKGYtAPTKdw6UhMuDn8m0nkvAQpK+yMu7kW+6RZFNVntZJeXMDIa6HmBVvDzXf6Kuz3RVHzJxtzf+ddd8dCSn8xFN3hQiblNHTS19+XxzPTB6E/c5iCKd6bvBBtqL3bvhL8cLEjq4ngh3kMGWnxuLar5hus/7wRh3+aN39A/Mh1iHVBD529AaCAdcoch/4BIeWhdUAWhWMHWSWE3AbeOQ1LXmlsH+NJybuDE0UFAYHG+JQ8xrCDrJJDoffDb7sdXajj1lTZg/O7OKQ6Pg36MyZjJtH/CTxXhFunfG5LIW9sYCHV599fwPnpyBqpO6HbQahj7+VQ9tXXzlSJoY9xqO/2bie00O2wsbIGCXEOQ9WdUPsYqj42XX+UehdvbNh+qO02WvZQxyZk3kaOia/MH4bYDoTc7w5n+irs98E29bBed+ew6dHBBL8f6vdvr0I74/qE+vdRCqvs44g6c5iCKbWMs4+j36sFAUOWJS7aREaf3djS/b717hw2PTqAN73b95XhY79/wzX+nTR8LzVss82FQjvjLMr/hw4BJ5LzXAaDT27Dll6ibDvkSVbSOxalThqbuD4GCNUuQ10HNN3fQ1/3NV2fhBBCCCGECGHQYyXk3Ql7f5lCQbi9dhs1kpzn0uv/3d+clEI749hGwcmRZNzq+0XU8DsoKK/fP7Pdqt89Cu/vFNXvCuWzoX6v+H7XNGjYrvIbZkBV4Peoy4H/c2z17yyvxEWbyLj144DvV9b5/wr0K596O+q/24RyLNS/JzuPcMrfWnnCF+rcN0VrfnGRWMcxKXI3mxoJ/vrTj5jEyOOb2HaReif7SAC4Ce0dBNKuNYO/XncvpPTRoRhxU/vqPzjq9KAzDeL2OAMfH9cRdQP1N1/z7LWsHW3Gc7KKwwff5hS9GHDnUAxnXZhMxsAAsO+hpquK3Qfeplekgb2/rOKeTWkM0vt9V+QtJA4Al8eEicYeNgrRujpf2xdCCCGEEEIIIYQQonWMW7qVlIG1rRRw8gbPVJ1+GuMLAIcTLBZtrXUDnxffJPK2TGWA82V2HzulTvQyc/uYQejfaz6P56UsUn5zVJ2o2aBHS8i7W8fRHf8gnPfVew0cydBrHZSOz2CTOlGIJkgAuAmdLQhkmlzA2gesuA8XkZ5jb7Vhk/VD0sidfhdWk/L2kcdVy+EXVvHyD3LJuLUhAAxWxi2ay+Q4M/oI4LyL2r9vYuGZeyi9LyowAIyekY8VkHKHN+/x3WSlFfL2kDSWzh5JlFEHgNt5FPuqvxP1i3QGSwBYXCSdre0LIYQQQgghhBBCCNE69KSt3oTNeJTSJ56nsQ5rp/5zlNpweh95OwLV/WUWKU82H+6SAHBH0tkDwIA1hVVLxhHVXZ2gjau1OtyBEhvJKiJ9iHrkpkZ8WcO2x+dS0lhjFKIREgBuQucLAukZOeYuXtvResFfIS5Fna/tCyGEEEIIIYQQQgjRGgaRUZJHokm9/kJ4qHp2PBkb1euDSQBYCCFahwSAmyBBICEuTdL2hRBCCCGEEEIIIcQly2oj5c5IuqnXh0Fn+h5RxsBP1lVtYum6l8PqPSkBYCGEaB0SAG6CBIGEuDRJ2xdCCCGEEEIIIYQQQgghRGd1mXqFEEIIIYQQQgghhBBCCCGEEEKIzkkCwEIIIYQQQgghhBBCCCGEEEII0UVIAFgIIYQQQgghhBBCCCGEEEIIIboICQALIYQQQgghhBBCCCGEEEIIIUQX8Z1+/fp9q14pFL179+bTTz9VrxZCdHHS9oUQQrS2j6ftUa8SLdBv/Qj1KiGEEEIIIYQQQgihIgHgJkgQSIhLk7R9IYQQQgghhBBCCCGEEEJ0VjIEtBBCCCGEEEIIIYQQQgghhBBCdBESABZCCCGEEEIIIYQQQgghhBBCiC5CAsBCCCGEEEIIIYQQQgghhBBCCNFFSABYCCGEEEIIIYQQQgghhBBCCCG6CAkACyGEEEIIIYQQQgghhBBCCCFEFyEBYCGEEEIIIYQQQgghhBBCCCGE6CIkACyEEEIIIYQQQgghhBBCCCGEEF2EBICFEEIIIYQQQgghhBBCCCGEEKKLkACwEEIIIYQQQgghhBBCCCGEEKJT6t27t3rVJU8CwF2KnqF3DkWvXt3pxHFXWSb/uzJOndDFXOB+pkzhf8tmMegudYIQQgghhBBCCCGEEEIIIYS4VEkAuAsxTcxl7mMZFD42sgsEgcWl6LLLI7iq93e5qvd3uezyCHWyEEIIIYQQQgghhBBCCCGEaIYEgLsQ5+ZsSv7uwnhnmgSBRadypdHA9bd8D8tdP+S6wVFcNziKG+/8AdfFRXGlUWqyEEIIIYQQQgghhBBCCCFEuCQA3KW42f1EOkUSBBadyFV9emAaeANX9jLAZd+pX3/Z5ZdxVZ/vYoq5gat6fzfgM0IIIYQQQgghhBBCCCGEECI0CQB3ORIEFp1Ht6t09P5ePy7v3k2dVO/yK3X0+t61XH6lTp0khBBCCCGEEEIIIYQQQgghVL7Tr1+/b9UrhaJ37958+umn6tWdhJ6hDxeQ8d8mnH8pIOPJl3Grs4QjZQr/O/Zq/rWymHejx5MwPIqrdcB5Nx8fKmPv8vc4759f35Pr5owmNu56ru5+OQDnvzyNs+Il/rG8Go9/XuDKCXcTb4vDZLycCODsiTd4rfADvrdkJNe9s5s/zKtoyKzvTdTj/8Og6N5cGaGUwVX9D/YtqaAu7J2L466ykfR47ffseuMHJEwcRD/95XD+NDXb/sih0tPoxo30W/8lHx/Zyf4lqrK30X5e/fgsbLd8xj+SnuPdgC1cz6DSn/HDT/2OSf25WcvRv/lljY7mh3PuZkBkT3QRcN5zGudr6nLp6Tc/icF+5fe4aji08nlq/+m3rbb0HTDe2Jde37uW7/j1/A3l2/Pf8ulbH3L6/U/gIlyxOnfbF0IIIYQQQgghhBBCCCEuHRfrmf5PfvITbrzxRvXqZp0/f563336bzz77LGD98ePHOXHiRMC61iIB4CZcrArTdlohCJwyhf8d24cP3zmHqfen/Gvfe5xFz/V33YZZDx/vWkF50ZdKXv31DHryZ/ywN9S9V8GblZ9xHj3XDBlEVO/ueN7ZTdm8ivogpC5lCkljbyDizHu8+VoNdWcjMMQMZsC1V3Bedzk6/wCw/noGrf4ZPzS6+fC1w7zvPE9E5A8Y9CMTuhMvU5b6d+rqC90UbwD4vfc436c7zkNvcIrefO/2QfTpfpo37TVcN8rKmUOv8IErgl633s73+16Oa99T7Pw/b11ow/284ABwdBx3LRnJdZym5rUjfOKCK6238cPv6TlfvZ3N898A4Lrlj3FX9Nec/OcrvH38PBivJ/pHJj4oVgWT29Bll0dgirkBfd8e6qSQ3M7PcFa+xzfnv1EntbrO3/aFEEIIIYQQQgghhBBCiI7HeTIwCNoa/iva0ubP9O+9916mT59Ot26Nj2iq1YkTJ/jVr37FO++8o066YBIAbkLXCAI1BIFr/zSXub+rVWdoWsoU/nfsDeCqYOec3bh8EeTooQxffif9TrzM1tS/c7Y+eGngw+1r+FtJYKjZ+PgsRt9i4N1NT/CP54Ab4rirYCTXuVXbBa6ePwPb7b0hKDAKbxau5Uh5Q15d6s8YbzNR+9wT/GNTw/rGKQHg63Dy2vxn+E+1d/VdI0maF4eBrwPLr/8Bt68fy42nL+Z+tjQA3J0bVz7M7dc7OfT476nx7RtgXDSL0XHnOZL9FG/+cxDDykZjfm83f0j372F9ORF8zXnNbwm0TITucvoNulGZ+zcMZz+t4+Nj73Le87U6qdV1jbYvhBBCCCGEEEIIIYQQQnQszpOfYepztXr1BbkYz/QffPBBkpKSeO6553j++efVyfTv358+ffqoV4ek0+l48MEHufzyy1m0aBEffPCBOssFa5c5gCP6xnLv1JnMnHAL17ReoFw0wu3xADoMV/dSJ4Xtw38EBi+p/jcfngC66+kOQBTfj+kJn1bwmiooCuBa8Sofcjk3xg1SVoz8Adfpvubd3artAp+truDDgDXebX90lH/5BX8BPM+9gZPL6XPz9YEJzXnvaEPwF+BvNXz4JfBlNZX+5Xe/wccfAT17Y4Q23s8LdEMsUTddztnqfwQEfwFc/3iPOnrTLw7gNGfdwLXRRMX4ZXJfvOAvwLfnv+GbcwEDiDfpm6/P8+1F6P0rhBBCCCGEEEIIIYQQQgjhr3fv3pw/fx6Xy6VOAuD999/nyJEjYS1Op5MrrriCM2fOtEnwl/YKAP/gjjuIMl7BFdcN4f6Z0xn742uIUGcSrUDPoJlLyR4ThftgIekrj6ozhOk0p94OXnfWDfToifKeRk8M3eHsh++FHorZ/TGnzgC9TVwNXG3SA5/yyT/UGSF4nGpl21x7JxPLMvlf/+W5kVwHGPr0U3+oSXUnPlat+RKPB/B8yTlVyvlvAF13dNDG+3mBLAYMwJUxPw08RmWZ/G/6IAxAj2uvB97jqL2auogbiF+Syfji8Xx/bO+L3ga/+eYbzrrq+PZ884MQfHv+W8666vjmGwkACyGEEEIIIYQQQgghhBDi4jKZTJw7d45PPvlEnaSZ0Wjkyiuv5NSpU+qkVtMuAeAAl13FjQn3k3Z/IlHhTQUqwuIX/H21kLS83a0eb7xwX3P+pHpd4zzHKzhkfyn08vfAAZM7Fm37eaE++3eI4+NdjhxUhkDwPLeVstSn+Ns/avhSH80tKTOY+MxIjHr11trQt1B34jM8n59VpwT56vOz1J34DJqPFQshhBBCCCGEEEIIIYQQQrSa7373u+j1er744otWCdqazWZ0Oh0fffSROqnVtGsA+My/yznw3hcARFwzkHt/NpP774qiR7uWqitQBX8XX4zg72nqvoQrr7uBkDO66vvRqwecP/EBnwGes+eB3vQars4I3HCFqmIqvXN1EXXUFr9CTahlW9uO7d6gLffT52quvl21yrvdJrm+4hygO38y+Ph4l9ryLxvyf/opHy5/np1TnsD+Nyf0jmPYIxqH0r5AX5/18GnNR3x9Vt3vusHXZ89xquYjvj7rUScJIYQQQgghhBBCCCGEEEK0qT59+nDVVVfhdrt5//33AYiIiODOO+/kyiuvVGdvVq9eypStJ0+2Xe/B0PGni+X8KY6UPc3qjQf56Cvgsiu4JuZepk0bS2zfiz0gbVfRHsFfgBreqXJD7zhuSQnuRmp85Fau42tqK94A4OyRd6mjO1Ej4rxDK/tcTr+0wQQO6PwG77zzNVw7iB+GCqReVG25n3DW9RXQkz4/Cty2btogrgtYE8I//8X7n8KV0bcTFa1O9Hc5Eb39//6az4qP4gSu7NHTP+Gi+OLk5zgr3+XsqTr4xq+L7zffcvbTOpyV7/LFyc/9PyKEEEIIEVJkaiFb7XbspVkMD/6nmhBCCCGEEEIIIYRmviGb/QO2P/vZz3jkkUf4v//7P6xWa0D+5vTu3Zuvv/6aTz9tu86N7RsA9jp/4jU2F6/nxcpP+OobwHAjd0yew/SkgfTqECXsLNor+Ks4ufxP/Mt1OdeNTSepcCTfT72NqNS7iX/mEUbf0pPPXnuOf2zyZv7bPo68/TURN4wk6Znx/LA+78MkXHkS9TsPH5a8xIeengxIf4TR+XcTlXobUam38cPcKYx+7qfcqMrfltpyPz32Cmo90G/kDP47d6iyj/mzSLodPj6jyhzkU/71hwo+011PfH46dz2ufD4qdSiD8h/C9sxI73zNgxhW7H8ch3LL/w3jOtzUHFAC1xfbWZebD157m3cPvImz8n2cle/z7oE3+eDw25x1XcxaLERbSKXQbse+MZcEdZJof6mF2O12ClPVCRdRQi4b7Xbs7VqIxmiov/pkCrbasa+drU65iDSUt9O50H1LIHejHbvdb2nxtlpZK9adUTEW5aU7YwzDYtWpot204jkWQgghhBBCCCEuNt+QzR9//HH9um3btnH06FEiIyNZtGgR99xzT8BnmmIymfB4PLhcLnVSq+k44dVvzlDztz+y7vfl1NQpq666IZEHUu8n8ebmxr4VAKbJuUrw93AR6Rc5+AuA+wOOznmKff/8AK6N4xbb3cTbbsN8mZN/bXkK+5IP/DJ/Se3P11D+j/c4+91oBtnuJn7UD+nl3MeurGqCBvutruBvi7dy9L0v0UffRrztbuJtwxhgMXDq0Ct8qM7fltpyP987yr7/202t63KMP7qTeNvdfL9HDftz/xIULA6pfDe7/u8laj4F0y3K5+NH3U7UtV9S+7cKPgPgY94/7n8cb+fG7h/wWlEJr21Xb/Di+vqsh88/PMXnH56SIZ+7uJjUAkq3tnPQrSvrGcvYeYWU2u3Y7RvJbSLCkzC7gBK/oNDW0rVkjQ09jICWvAAxo+ZRULJR6Y3nXZo65/rh3kBoGMFQLXnFxRGdOgyrzkPVoQ3qJCGa1Jp1Z1elQ/n3lauSfUfUqR3LpXQvbOwcpxY2f5+Chpd1Gl1CvczQM4HZBSVs3Op339pYQsFs/5zeFysaW+pPjt8LFBvzGeW3BWjkZSJ9DBOy1lK6datfOUsomDeKmIDe6eGWQQghhBBCCCFEe+nVqxff+c53AgK2p0+fJjs7m02bNqHT6Zg9ezapqalERDQ9wrFvPuEvv/yyTQPA3+nXr5/fmKsXx8Dx6SRGwpnKzaz/W6gJjiO45sf3knT7jVzlDVF/deIIL/7pAMcbnyq01fXu3btNu1+3Pj0jx9zFazvstF2VEaLr63xtv/NJyN3IgjgDjjIb6cXq1K4mlUJ7Epa6CpZNzma/Ork19UwgdcEUhseY/eYpr6Ni2WSyQ3zx2PyNzIgJNaO5B0dZJunF1fVrtORFH8+8gvmMMAcOfg80fs71EygonYbV9xFHGbaQGTXmbU5qIfYkS+PluhgSctm4IA7DhexHmwm3/o4if+McYqhk9eRMdqmTL5pwy9sZtea+JZC7cQFxtMa2LlRHqTsX36VzL2z8HKcW2kmyNH6fque9VjdK1S70w7MoemQIRlU2hf/3eduVOotP/XXZ22a8t8HanWnMWnO8IZ/6XhI5gYKCaVhD3TaBuoplTK7f4XDLIIQQQgghhBBdg/PkZ5j6KOOVtpa2fqafkZHBkCFDKCoq4q9//as6maFDhzJ79mx69OjB66+/zooVKzh9+rQ6GwA33XQT2dnZfP755zz88MPq5FbTcXoABzjPJ69v5+nfv8ixE18BcEXfWMbPnM7YH19D07HzS5mb3Zdw8Dfiez258kdNLN+7XP0RIYToUmLnzCApxowBD86KfVR5R9QIRT82nykxBsBF5eZF2Gw2bA8sYnOlC9BhGZXKBG8PJS15ASbkeoO/dbVUlK0gM22S8hlb40GO1PwpSu+wfRU0UWzQmFdcHPrk4UQbwHlo/SUVwBMXTupO19cq57g4vf4+YlvmvfY7yhrW+b/IEJlK/hwl+OtxVlK24uH6fGlLnmKPwxU8Ck9dBct82/Jfgm5aLlwuMA9JpqkRxhNSJ2A1gMdZweYlafXbe+DhFZRV1uIKKoCWMgghhBBCCCGEuNh69uzJuXPn+OSTT9RJmEwmhg8fzne/+12++OIL/vOf//D555+rs9XzzSd84sQJdVKr6qA9gAP1uDmRe0cM5Jpu3hWn3+DFF8qpaXZO1AvT1m8MiNZ148pMbr9JvdbPO7v5w7wK9VohgnTKtt8zgdmPT2OYxYTB2yuyrraCLWuWs6XSNyC8t4eJowxb5iEmzJ/NhDhvT9G6WiqeW0n2dr9enN4hf6cNs2Ly9mDxuBzseWoRa/YHvr2kjxlFavIE4v2+31PnxLFvPRlrvI9km+u9A4CDMls6/o86wy1DWLw9LU+U/ZyK6FwmWg3gcVCWmYljQhGPDDGCx8m+FSksr+9GFMOEebNJijNjrN+3Wiq3rCF7S6X/1qG+vBZMvgPhE6LXXqvuG0DsfNbO0VO+cjlbKmO9vZVC96xSel15qN2Zyaw1/uc9lqzSxQwxeqhaP56MLdryEptF6eIhGF0VrEjLpjyM+QiiUwvJT7LgrlhB2p5hlDTRG1ZL3rDU99qaRLFrPrMnxGE2AHhwOfawOnMNh/z2Iay67i+cttlID2Dfvuo8TvatTme538EMq+6kFmJP6kvFsjT2xCxmxgiLtw57cFWVsTx7A/WXBy8t9dff7LV2Rpuq2Dw1gw3+29Rahs7S3jrKtUTd67Becz18m0tXaDlmo+YVMCHeL29dLdW7NpC54ZA6a4BG646vXfitChDQXgJ7Z0LoOgC+YxZJ1fqpbOmbS2r9/oVu81o1exw03wvb+d7dkrqu0ug5rr8Xhb5PNaqRa6ZPbFYpi4cYwXmQJel5zZzPcHvW++qYgz07uzFitImq9VPJ2OLduKotKvvVxKgXAcItgxBCCCGEEEJ0DZ2tB3BERAQrV65Er9eTk5PD+++/X592//33k5SURPfu3amoqOCpp57C6XQGfF4tKSmJadOm8ec//5l169apk1tNB+0BHOjMW3v549N/5MB7Xygrev6Ae382k/vviqJHp9gDcTG8Oy+fPyQ1sUjwV3RV0akUPrOA0daGB7gABnMc01Kn+OdUdIskqyifab4HyAAGM3Ez5jPfrzvLhIKNLBjd8AAZQGe0MHrBMxSmRjasJIH5WXMYofp+ncGEdfQCSuY1Pkdsc8IvgzZ94+eT5BuXUWdh2LwC5gzxDhSpMxGfNEH5f/1wcovymTakIWADoDOYiZuWT2nu8IaVQGrhVm95VQGbENpk344sZ1ZKtl/QvzFjsUQCHgfl/gHdnrEk56YSYwTQERmToDEvxIywYMRDVVl4wV+i5zE/yYLOdZCnssubnr9eS16N+g4rIn+aL/gLoMNoGc38XG9dAO11XWvb9NMQ/K1lz/LA4K+2umMgek4RC0b7Aq8o+2adSNb8wBkztdTfAKPyGWaGuuryoOCOIswydLb21kGuJW1FyzGbULCVOSNUeQ1mYiZOocnZS5utO41zOavUqzTQEZlUxOMB+xeqzWvT4uMQjna+d4dd19Uu4By3TDyjrEbAQ2VZc8HflnFvOESVR4d1eLI6qV6VSxmfwjIsnwmBE/4KIYQQQgghhOhkrr/+evR6PW63uz74e9NNN/HEE09w//3389VXX7Fq1Sp+9atfNRv8pZH5hNtC5wmfnvuEI2VPs3rjQT76CrjsCq6JuZdpD40ltq8MCi2EuFTFMn9+Ehadb5hD7zCDDzzMirJKnKEefJrjGGL04KzYzKIHbNgmZbLT4QFMRI+IAUA/oYApVgO4qhq2abOxoqwKFzosw+cwym+THreLqj1PsezhBxry7qnFA5hikoghcPjGZRXKg1FHmXqow4bev1rLoIXBZMJT9RQPrFCGkTSazeAo4+c/34MT0JmiiQcS5qcSZwRclQ1DOD7wcP2+GeOmMF85ZOiTCxhl0YGnlj3+w01m7qFW9f1tuW/hMaHXAa4TVKP0TBw1r5CNzy5mol9wwWC0aswL8ZEmwMkJzzwKSjZit9u9y0ZKCmYTH/AcPIGsx0dg8tSyc0leM72etOTVzmA0BgzVmba6Ahegs45inl/MJKy6Di1rm14NwV8HZZmzWOkXwWhJ3TEYDEodXqSUeZG3vAbLMOJ929VQf9WSh0djwMmRzY0P7hpOGTpje2vva0lb0XbMUhlm1YGnis1+7eLhFWVUNlXRm6s7+7OZ7N1W/fLzMhwe8DjKmJrnfxXYT/ZkX75leG8xTQq3zYcvzOOg8V5Yr73u3V7h1nW1Js9xm4jBZAQ4jmO7Oq0JhjgW1N+vGpaNuYEvygDg3kBZZR2YhxEqGWD/8mIOugBjDNPyN1G6NpfU4c1ULC1lEEIIIYQQQghx0fTp0we9Xh8wZHP//v259tpr2b17N2lpafztb3/jnnvuIS0tLeTys5/9jN69e4O3t/L58+clAKx2/sRrbC5ez4uVn/DVN8BVN3LH5DlMT4ptGCJaCCEuFQlJxJqUoS5Xp2dSXH5cWX/6HcqLM0nJDHqEDB4nB1c/REr2Bo6cBtyVrKlUPqfX9wRgVLwFHS4Orsho2CZQXpzB5koPGCKJrX/Su5+8lKlkrNzO/ncahpcsX3mE4wB6PcpWtdFWBo08DspXbud0+XGU27aTfauLqa52K71Ku+k4xFhGxxgAJ3uWZLLhkN+xXTmL9ZV1yoN37wPdKXFWdNRRWTyLleXv1H/V8Uo35+r/UrTpvmnhrqPn7AJKS/OZM8KCAe98hZsrg+fW1ZIXM8NmjMDq3wUNAybraB4vnF8/b+Lw3BkMMXpw7FpJwMjSIWjJ2xJ1VZsZn5Jdf56P78pWzgUmLPUREw11vSVtE4hOLiA3yYKurorNmekUq/a1JXXH49zHirRMNhxRynxkZTkOj1LPff900lJ/A0TOJt6qw1O1j+VH1IkNmi9DJ21v7XwtaSvajtlx3HWALpK4UQ0hw3fKi8lMyQwOZPqEWXfq6YeT+3gSFncFqxtpP1qE1+a9Q/uGCMrZN+YSGJZr4XEIV3vfu8Oo60E/xbSe405kf/E+ajEQk9RIL2B3OXlTbSzbWYWzDozmOJIeKcK+cS35yS294AghhBBCCCGEaA/XXnstOp0uIAB84MABUlNT+e1vf8vZs2cBGDt2rOoF74YlMTERvV7pGWMymRqdT7g1dboAMADfnKHmb39k3e/LqfE+db7qhju4f/r9JN7cQ51bCCG6LqsRA+Cq3BXecLsAnuPs26Wav9HbI2ly9n4gnmiTDjAyZHHwQ+8ZMUqaya9rkD4+mdy1pWwNyJtEc7McNk57GTQ5Xklxw7NxcBxiZVBQ0dvz1VlNeVAabHcoN3y98SYggci+ACdwNNvJqY33TQvLaBaMtmLUgcdVxc5lDygBEYdHnVNbXrx5VmTW/yPn4RV7qPUAplgmjgL98FxS44x4qp4jXR3lVNGSt6VOVG9Qr6K8NnjIlrDrekvaZt/h5E60YvA4KMvOYEPQrras7hw/tFxVBifugNOmpf4GSkgdhpk6qsuDj5+/5svQSdtbu15L2orWY7aLJcUHcWHAMnoBdvtWStfmM2+s37jEIYRbd3xS8+cQp3dQtiTM4eWbEW6bD1/LjkPY2vveHVZdD6T1HLerugqWhfiBrhzbEI6vYVdlHTrrsIAhuNX2r8kgZbKNtBVlVNTWgcFMzMTHg4Z9hxaUQQghhBBCCCHERdGrVy+AgB6758+frw/84p0neP78+dhsNh544AEef/xxFi1aVL8UFBTwwQcf8N3vfhe9Xs8XX3zBqVOn6j/fFjpnANjnzBu8+Mxq/rj/Xb74Buh2DQNHTWPmT6LUOYUQokvznGuFp+H1uqEL6sbThIQsih6fSJzZiE6d1mIay9CmPFSqVzXG46H5gTs6wr658PiCb3UO9qzOZPzUDNbsV4IL+pi+SvDSWakxr08te9IyWFPesO6d8pXk7XMCBvSREDssGgOgs04LDFQsiFOGlbYkedcVasp7wfNs+jHqVDW6BXVdU9s8cYhyh0eZX3PaWHVq29edsOqvH30ySTEGcB6h9UZ37Yrtzae1962taD9m7vI8pk7KZPXOChxOD0ZzDCNmLMa+tZDUUNPAa6w7w3NLSYp0smd5ZlCv+NYU1OYJHLI5YJmcHTQUvebj0Ko0nrcWXM800XiOW4/v5ZJILKEuo61o++ZKXJiIndj8IPLHy4vJnjWZB7xDjRvjUhsdPloIIYQQQgghRMdiMpn45ptvmhyy2T8gfPr0af75z39y5MiR+uXf//4358+fp0+fPlx11VUB8wm3lc4dAAbgPJ+8vp3n/36cr7xrrrgqYIJBIYToupxuZa6+6BA9SVpsP8dPoAxXmhbiobd3SfeOZzl2dBxGwFO7hxV+8wjabGU4VFsOn7YytA1v4NMUzewQ0/aNtfQF4MTxI8Bp3G5AZyRSlTc6NYbAVR1h37bgcAJ4cJQvZ+WuwLBUapwZ8OCsPqQxLzhcynC2luHB9+K++jYJM7SZsdEmwIPb2ylQU11vUdt0U5w+njKHB2PMjBA9xNqq7mipvw0ik+Ox6jxU7VvNhY/u2pXbW1vtWwNj38AhZaPHjsbiPwK7Ji08Zu5Kdq3JJj1lMrZJmayvdIHOwqjUCaqM2upOdGohc+KgYnVGwHzYbUHd5ltEw3FoXdrOm6brWQtoOcetaztVDg+gI3rUbHVi6zqSxz6HB0P0cJLDDL6f3pXNwVoAA0arOlUIIYQQQgghREfUs2fPVhuy2Wg0cuWVV3Ly5El1UqtrlwDwG3/eyoG3Tilz+F6oHlEkTp7JtLsiuQLgmy949y3/8cmEEKILK69Q5tE0jWBj4TzGxjeEB+KTcynJb1l/yF1VtYCJEfkFpA5vemxUkzeo5zldTbl3HsGbhqeSu3Z46GEkgdNu5SG+ZVg+ybGhZwjWUoa2kMAWKh0ewMzo/HySfce2ZyzJuSVMizGAp4qK59xAJZUnlMDnsKx5JPRsyJefZAnqXdXe+waw/YgDDzoso3LJTfaOX9kzluT8UkaYgLpKyrZoz1t+6B3q0GGdks9s75ymAPHJ+TwyxAjUUrUL9mdPDgpM2Gw2bMsqlDmFHWXedema8qpjUuHSGxOIiVSC1vrIeJLzSxltVvZt53Ylj6a6fgFtszhzNRUuMMY9EhQEbpu6o63+KmJJHmKGumrKN7RGUK7rtre2vJbg8uABjDETmBCj1N/hswvJnRGDUZ1XA03HLCGLtSUFzBubwE2+y7m7koqDx6kDdDp1ScKvO9GpheQnRXK8bAnZrTHus5/ANj+c1ILgNq+J5uMQ3r1QCy3nTdP1TLPwz3Fb2FCmzE2vM49ma0kuyQk31afdlDCWeYVryWql3rfFu6qp01mJ97Y/RQJZa9eSmzqcmPrKAPrIGIanFjDEDODkuPLelBBCCCGEEEKIDiwiIoKrr76ar776iquvvprY2Nig5Uc/+hE9e4b3u95sNqPT6dp8+GeA7/Tr1+9b9crOIYJrfnwvSbffyFXeMPZXJ47w4p8OcPycOm/L9O7dm08//VS9WgjRxXW2tq88IA8RGMAbGKvvppVKoT0JS10Fy0IMXRkogazSBQwJfl6t8NtGZGohhY19P4F568XOp2TxMEz+6wBwUFYfxAu/DGFLyGXjgjgM9cfFe0zUf/u2HZ1KYX4SlpA758FRltkwJ21j++RyUNvNghn/8rbBvuG3f+r1fhxlDT3AUgu3khRy51xUrEgLCLi0Tl7VMQsl6Bw1QUvexqQWYk9qLNwRuG9a63rYbTPUfkSPJf/xGcQYwXVwBVPzyr0f1FB3vPvmf84VCeRuXECcf53UVH9Bn1xA6UQr7oOLmJrXRP8+LWXoTO0t6Jy107VEP4GC0mlYg7brwlVnxOift8m6Tsuvv01edzw4ytJJ95s8Nuy6k5BF6YIhTQSy/cqrZd+azBt8PQubxuMATZzrgHPRzvdurXVdyzkGUgvtNHo6qKNi2WSy9zd33oLb8fD5JcwZZmpk//y26yu/OotP/X56r1kG/3OjmFdiV16Gqr/H+vL6ZVJxVaxgarbvuh5uGYQQQgghhBCia3Ce/AxTn6vVqy9IWz3T79u3L4sXLyZSPVTbBfjmm2/YvHkzpaWl6qRW1cY9gJUg7QMPzSE9PZ309HTmPPQA9/74GiLUWTWI6BvL2IfmcH+CN/j71Scc27WedRtbL/grhBCdRXVxOg8t20mVsw7fVK3gwVV7kPXFzwXkDd9+8tIyWX+wFlfDRkM6XpxO8b7AfHXOKvasXs3BxobRPLKc5U8dpLbJjYdfhjZTXUx65lMcrHX5HVtl/3YueygwkHlkOT9ffZDauvpc1FasJzNtMycacnl1gH0DijOzg8pQ56xi55LgAMiF5vW4lPmDmwz+toeKPRysrMVVP9ExDe0nM3DftNb1C2qb1dvJXFKGwwPGIXMome/rCdxGdUdT/YXkeCs6TxV7VjYd3NGkK7e3tto39xayV++h1m8KmrraCtZnprEvKLMWGo7Z/mxWl1Worucev30LDHqGXXespiaCv60tdJvXRONxgHDvhVqEf960Xs+0CPsct6Hy5Sk8tGwnlao253HVUlG22hv8bR3F+6oCvgP2s2J1GRUOJ3UBCUp92LM60y/4K4QQQgghhBCiIztx4gS//e1vKSsrw263a15eeeUV3nrrrYBlx44dPPdcM88GW0Hb9QC+7FqGTBrPLdeEDvWe/+Q1tm46yEdahoG+rAdRd97LiB9cwxXe0PUX7+1l645jnNKynTC11RsDQoiOTdq+EEI0ITaL0sVD6Fa5msmZu9SpQjSuI9SdRnuli1bREc6xEEIIIYQQQogOrTP1AO7MWrEH8FVE33EL114GcAU/GNMQ/P3ivSMc+PNWtv75AEfe+wKAiGtuYfyYHyjz9l52LbfcEc1VAdsL1OPmRO5Pnca9Md7gb927HNi4mqfL2ib4K4QQQgghgk2YEocRF5WbJbgjtJG60/XJORZCCCGEEEIIITqGVuoBfBUDxz9IYmQEnHmDrTu/InFyLL04z0f7S9n8+pmA3D1+PJGpCdcSwSmObNzLFaPH84MecP74Xn639RhKiNir2zXEjk7ijhu84eFvvuKTN/bw4t9rONPGgV95Y0CIS5O0fSGEuNQ0MwenSl3FMia35hiy4uKRHsBCCCGEEEIIIUS7kh7AF0cr9QD+grffquWrb4AeP2D8T2PpBXDmDQ6ogr8AZ14/wBtnAHoR+1Ml+Avn+eitt/2CvxFc8+OxTJ95f33w96sTx3jx9+v449/aPvgrhBBCCCGEEEIIIYQQQgghhBCdTSv1AFZcZb2XKSOiuMoXVnZVc+Bfn6hyKa754R1EG31/nef4337H1sqG8G/UT2Zy7/evUP745gve/UcZL77+Cefrc7Q9eWNAiEuTtH0hhBBCCCGEEEIIIYQQovVJD+CLo1UDwABRo2Zy783ewG2YvnrrRdbtqglYN3B8OomR8MV7ByjbeYRPzgUkXxRSYYS4NEnbF0IIIYQQQgghhBBCCCFanwSAL45WGgK6gf5KbcFfgCuu1KtXcf6LTzi2az1Pl7VP8Ldz0jP0zqEEH00hhBBCCCGEEEIIIYQQQgghxKWg1XsA+3runqnczPq/faRODnDtXdOYGNMDju+lcOsxdXK762xvDJgmFlCYbKHu70WkP7EbtzqDECIsna3tCyGEEEIIIYQQQgghhBCdgfQAvjhaqQfwQManp5OergR/NYtMJD09nfT08QxUp4mwOTdnU/J3F8Y70yh8bGSn7gk86ME8SjYVkKJOEEIIIYQQQgghhBBCCCGEEEI0qpUCwKJjcLP7iXSKukAQ2Gj+HiZ9N/VqIYQQQgghhBBCCCGEEEIIIUQTWikA/AZ//v161v9+PQc/VtZc0U3DXMAfH2T979ez/vd/5g11mtCo6wSBhRBCCCGEEEIIIYQQQgghhBDatPocwPXz+rqO8GzpAU6pM9S7ilvun86Qa8KbL7g9dO4xw/UMfbiAjP824fxLARlPvtyyOYGnr8J+Xz8Or1zFx/fOwnazEc4cpmBKDnsB+iSSNn8qd33PhF6nfMRzxonj7yVkr/P7zrtz2PToYD5+wcbcpxs2D5C4aBMZt37MNttcSrz5goLWjm3Y0kuU/7eOY+HD4xkcaUQXAXhc1L66lVW/3kZV/QesjPvFXMYPNmPsrqzxuKp48TcZlLxen0mIkDp32xdCCCEuXZGphRQmWdC5DrIiLY/yFv0DWAghhBBCCCGEEG2lq88BbDabueeee9DpvEEzDc6cOUNVVUOkC+DLL7+kurqa8+fPB6xvTqsHgLn5XmaOiuIKzlPz59W8+B91Bq/v38ucn0QRwVfU7FrHi2+pM7S/jlRhWqYVgsDeALDTCZ7KtSxcuReXL82awqol44jq7sH178P8o+YUXNmPQbcOxtwDXK8WkrZ4t/Kd4QaAbxjJ1J9YMA8cydAb3Bzd8Q9qAU4epuhPh5XvXDqOKFxUvfoP3nZBL+tdDL1Zj6eqlKkZm3CjZ1JBKVOt4Hx9L68d94Dxe9zyYxO166aS81Lg9wuh1vnbvuhYUim0J2Gpq2DZ5Gz2q5NF+0otxJ5kwVFmI71YnXiRJOSycUEcBkcZtnYrRGM01F99MgWlE7E6d2KbtUadepFoKG+nc6H7lkDuxgXEGfxWtXhbrawV605qoZ0kC0AdFcsmk93uOyegdc+xuFAXei0RQgghhBBCiAvT1QPAK1as4Oabb1avbrFvvvmGF198kXXr1qmTmtS6AeDetzDxp0O41jd167lPOLLjeQ4cD4xKR0TewU/HxHKNL983Zzi2dT17PwzI1u46UoVpuYYgcO2f5jL3d7XqDE2bvgr7fVF4qjYxNaPUL4BsJqVwFeMsbg6vTCNnj39o2UpK4VLGWdy8vHgqS1/VEABuYl39d0Y6sS+cRVH9SxB6RuY8Q/rgOvb+MoWC11NYZR9H1Ht2Js0paiiz3ogRFy7NUXBxqekabb9ji0ktYP4oK65d7Rh0u2ja4UFrz1jGTpvGxBEWjM0EQRJmFzBtmBWTNyjkcdVSsXkledur1Vk15QWIGTWP5AnxWEwGfO+7NRVo1Q/PpeSROAwAzQRDteRtkgSAmxF+/Y2eV8L/jTBStXkqGRva62Ybfnk7nwvdt44bAG7NutOZegBfSvfCkOfYe/0N5KHO6WDf+iWs2X/ab723/vutCdDI9TO5YCsTrTqgjsrVk8nc5Z8aok3gHV2ouoLtzxWzq9JXgRry1lWuZrL/hnzBbR3UVSxjcvb+Fpf34rjQa4kQQgghhBBCXJiuHAC+/vrrWbx4MV999RULFizg888/D0i/8sorufnmm7n88ssD1jcmLi6Oe++9l7KyMn73u9+pk5vUSnMAq4K/585w5gug2zXEjp/D9PGJ3PLDaKJ/eAuJ46czZ7w3+PvFGc6cAy7rwcCk+xlynXqjojW4PR5Ah+HqXuqksDnf2hrYe/iGcQy16PBU7eaJgOAvQBUlLxzDjZEB9wxVpV0Av+9sCP6izHt84E3cmDDHATipcwPXDmDqQL/BpN0S/BWio+gZGYlR+wgYojk9E0jNX8vGZxczY4QFozpdZWz+RhaMbgjoAuiMZobMyKcwNdo/q6a86OOZt3Yr+XNGYPUL/jZJP4HcOd6AbnO05BUXySimxZugrpryCwzgibayn+zJNmw2GzbbMirq1OntpXXrzvHidMbbbNimduzgL5fUvVDLOdZhMFkZveBJcocHTQqjjT6ZGIsOj8OBEwPRw8aqc4SmM2KOGcGc/CLyx6rub4DhpngS/P7WT4nDekmcRyGEEEIIIYQQzTEajXTv3h232x0U/AU4e/Ysx44d48iRI2Etl112Gd9++y0nTpxQb6pZrRQA7sUdo33B3484+Px61j+/l3e/UlKvihzIkLv/m/++ewgDI69SVn71LnufX8/65w/y0TklWHzL8DtoeYhSBNMzaOZSssdE4T5YSPrKo+oMYXLjrFE9rInqhQFwvbc39LDSL9XyMWDsM0Cd0nLe79QNTMFutwcu85R5g/tdlwjYKd1RhTsiCtvSTWwqKSD9vsHNBkKEEKKzi50zg6QYMwY8OCv2UdVEgEc/Np8pMQbAReXmRUpQ6IFFbK50AToso1KZ4H32riUvwITc+Yww66CuloqyFWSmTfIGnRrv5ZaaPwWrzkPVvgqaKDZozCsuDn3ycKIN4Dy0noAOdkI0Q+pO19fcOa6rWFZ/j3hg0WYqnB7ASFzSFHVWpde6N2/AEuLmogRmPVTvWY/DBbroIYQMAau2mbmijEpvGWKmzSE1EsCK0QB1tbXUGaIZ4RcBnhJjwVNVpUxbo6ahvEIIIYQQQgghOr9rr72W7t2743LVT6Z6Qfr27YvH4+Gjjz5SJzWrlQLApzjwp79Q4/qIg89v5rVPgTPH2F68nhePvMupLxqGgD7/xSnePfIi64u3c+wM8OlrbH7+IB+5avjLnw5wKmC7ouX8gr+vFpKW552Lt6W+Ua9oP65/78a+wx56ebkGgKpnM5iUksOmAzXUGayMnJ5D6fqFjLzAjgRCdFg9E5hdUMLGrQ0vRmxcm8uEGP9Kn0qh3Y69MBX0MUzIXctG30sUG9eSG6KXS8LsAko2Nmxza2khsxN6qrOhjxnFPNX3b91YQsFsvyekqYX1aQu84y1aklQvc9gLSW34BGgoQ1gSctlot1OYGk1ywUZlm1sLSY3WMzyr1Pt3CfMDuvbEMCFrLaUB+7aW3AkxfpkaKOXd6rdPjQ8B2ar7BhzZVUmts4L1mVNJyT7Y5HV/yogYDHio3bmEzA1HlJWnj7AhcwUHXYDOQvwo7XmJzSLJqgNXBStSZpFdXE7l8aZKAtGphYyy6HBVrCb7oDo1kJa82uiJmZDL2vrzsZXSwtnEq+4bYdV1f2G1zdCiUwvZ6quTqp5wYdWd1ELs9o3kJvQkYXahXx3eSmlBMqGKoKX++kuOt6LzVLGvWDUcuNYydJb21lGuJd7raqH6wkkCuRvt2DfmBvRU1ErLMRs1T5V341ryk+PV2YI0Wne8x7hh/1VLwE5799c/vbF9Ty3Ebt9KwQQ98QH7F7rNa9XscdB8L2zne3dL6rpKo+c4hNNHNpD9XKXyck/fyNDnMExTYizgcVCx/Qj7HHWgi2ZIyAhwoMryYjLTV1Phu79N8WujJyp5p85AtC8CHDmbWEsd1eXVnAMMRmtD3tbWwnMR1rVECCGEEEIIIUSrMBqNREREtKjHbih9+/bF7XZz8uRJdVKzWikADHxRzYul3uCvzzdnqDmwnWefXk1hYSGFhYWsfvpZth+o4Yx/QPHT19hc+iLVX/itExdAFfxdfIHB31BqTlEHGG9IJORzsrvN9AOcHx4OWN3LpB4SWk9Un5BbCOaqow7Qf11L0bqikEvpHr93708epvTXc0mZNJWCl5x4+gwl5eeJ/lsUomuITqXwmQWMtpow+A1BaDDHMS01RO+ZbpFkFeUzLc7cMISuwUzcjPnMj23INqEg1JC/FkYveIZCpTuMVwLzs+YwQvX9OoMJ6+gFlMwLfjgdrvDLoE3f+PkkWb0b1VkYNq+AOUO84wToTMQnTVD+Xz+c3KJ8pg0xBwzTqTOYiZuWT2nu8IaVQGrhVm95mx8Lsk327chyZqVks6V+zsLGjMUSCXgclK/xeyDfM5bk3FRijAA6ImMSNOaFmBEWjHioKssOb/jV6HnM987X+VR2edP3Ky15Neo7rIj8aXGY68+HDqNlNPNzvXUBtNd1rW3TT3RqIflJFnSeWvYsT2e538HUVncMRM8pYsFoi18d1mG0TiRLFSXQUn8DjMpnmBnqqssJPbprmGXobO2tg1xL2oqWYzahYCtzRqjyGszETJwS9FJPgGbrTuNczoD5QDTSEZlUxOMB+xeqzWvT4uMQjna+d4dd19Vaco71OmXqgHMezqnTwqVPRYn/VrIF2L+nmjp0RIcTAQZwl1Nc4QTAdJP/tbKSndV1GKJHkABEjo3BXPcO+0J1bW4jWs5FR7iWCCGEEEIIIcSlxGg08u233/LJJ5/Ur7NarQwcODAgXziuv/56rrrqKtxuNx988IE6uVmtFwAWHcRFCP4CvLeN146DzjqSx0aoA7hWUu4biB4nb/7dO+y0L2B842AC3ou3pjC00VfQe2G6w+/P1/dSc1L5zrQmX643Yuzj/7eLvetewwl062HyTxCiC4hl/vwkLDrwOCspW5HmHZ73YVaUVeIMdQEwxzHE6MFZsZlFD9iwTcpkp8MDmIgeofRy0U8oYIrVAK6qhm3abKwoq8KFDsvwOfg6fAJ43C6q9jzFsocfaMi7pxYPYIpJIgagOL0+bZl38klHmXpYxHR8gyJqLYMWBpMJT9VTPLBCGULYaDaDo4yf/3wPTkBniiYeSJifSpwRcFWyeYnfsfXumzFuCvO9HYP0yQWMsujAU8ueFQ/Xlzctc0/QsJBtuW/hMaHXAa4TVKP0TBw1r5CNzy5mol9wQenJpCUvxEeaACcnPPMoKPH2ULLbsds3UlKg7l2XQNbjIzB5atm5JI/9/klBtOTVzmA04nFW1J/ntNUVuACddRTz/GImYdV1aFnb9GoI/jooy5zFykMNmVtSdwwGg1KHFyllXuQtr8EyDF+/RC31Vy15eDQGnBzZ3HgEJJwydMb21t7Xkrai7ZilMsyqA08Vm/3axcMryqhsqqI3V3f2ZzPZu6365edlODzgcZQxNc//KqB9fuNw23z4wjwOGu+F9drr3u0Vbl1Xa/Ich3DT8NkUTolBBzgrd3FIncEQx4KA3tLKsjE38IUW/ZQYLMDx6i3Kiv17qK4DXfQwGglVBzlecVzpiWw0QXzf+ulk9u+pps5gYVhsJBPizNRV7ww5tDWEX14twj0XHeFaIoQQQgghhBCXmr59+3Lu3Ln6IZuvv/56Hn30UXJyckhJSSEiIkL9kUb55hP+7LPPOH++YaTlcEkAuEu5SMFfAGopWrmNGo+RwfNKKV2+kLSZaaTNy2HtcwWMs0DNC09Q8Ko3+3vbePktD1w7kqXFeaTPTCPtFwWULr0dPgou5WsffgwYGfxADmkz0ynISgEOs+rZw7h0ZmzLNrF2UbrynTPTyVm+ltL1C1H6944np2QTJb4yzUwnb+VIzLh584Bd/VVCdG4JScSalDnmVqdnUlx+XFl/+h3KizNJyQx6hAweJwdXP0RK9gaOnAbclaypVD6n1ytDRI6Kt6DDxcEVGQ3bBMqLM9hc6QFDJLH1T3r3k5cylYyV29n/zumGvCuPcBxAryd44MnmaSuDRh4H5Su3c7r8OMpgHE72rS6mutqtXDe76TjEWEbHGAAne5ZksuGQ37FdOYv1lXXKg/fhSqRgSpwVHXVUFs9iZfk79V91vNId1IOpTfdNC3cdPWcXUFqaz5wRFgygBEQ2e4ffbGlezAybMQKrfxc0DJiso3m8cD6+zmrDc2cwxOjBsWsl/p2LQ9GStyXqqjYzPiW7/jwf35WtnAtMWOojJhrqekvaJhCdXEBukgVdXRWbM9NRj5jakrrjce5jRVomG44oZT6yshyHR6nn3bx5tNTfAJGzibfq8FTtY7l3dPBQmi9DJ21v7XwtaSvajtlx3HWALpK4UQ0hw3fKi8lMyQwOZPqEWXfq6YeT+3gSFncFqxtpP1qE1+YDh2wOWIKGmG7hcQhXe9+7w6jrvutJvTDPsSFuQf1xffKR0VgMSpA/pakPNSM51gI4qHzO9ztjP4feqVOGdA43AuzPu39u1zveYLIRS1Iy0aY6qvfsB5y4Pcpxa3NhnouOcC0RQgghhBBCiEtN3759+eKLL+p7AH/wwQds3ryZL7/8kqSkJBYtWkTPnuE9LffNJ3z6dMPvdi0kANyFmCbnKsHfw0Wkt2nw16uqhLkLi9j9lht99FBsY2zYRgym19kqdq9ZyNyn/Yfmq6Xk8QLsb7mg7yBGjrFh+7Gemj9kUxriFXT302vZ9G8XusjB2MaMxNxdCS+49+SQ/oSdqpNgvnWk8p2jExl4LdT8bS+vAVBDzXEPRl+ZxoxkQPdadq/JJuuFNj8qQlxcViMGwFW5K7zhdgE8x9m3S3XT8PZImpy9H4gn2qQDjAxZHPzQe0aMkmby6xqkj08md22pMl9p/XIhc8xpL4Mmxyspbng2Do5DrAwKKnp7vjqrKQ9Kg+0O5bGr3ngTkEBkX4ATOBrtBuTTxvumhWU0C0ZbMerA46pi57IHlICIw6POqS0v3jwrMv16we2h1gOYYpk4CvTDc0mNM+Kpeo50dZRTRUveljpRvUG9ivJaZfhPf2HX9Za0zb7DyZ1oxeBxUJadwYagXW1Z3Tl+aLmqDN5ART0t9TdQQuowzNRRXR58/Pw1X4ZO2t7a9VrSVrQes10sKT6ICwOW0QuUuXTX5jNvrN+4xCGEW3d8UvPnEKd3ULYkzOHlmxFumw9fy45D2Nr73h1WXQ+k9Rz7OPctY3x6IyHzugqWqXuG1x8Dr8jZxJiB2iqK/erKroPv4EGHJdwIsE69Atzu48B+9lTXYYobgtlVSdl+ABceD6A3Br4YEE55tQrjXOzvENcSIYQQQgghhLi0+IZs/uKLLwLm7P3rX//KggULeOedd4iNjSU/Px+rtclhbsHbAzgiIoJPP/Wfezd8EgDuQpwbsylaV0R6jh2XOrGlnp6LzTaJnJfUCV5Vdgofmcr4pIYHGpNSMijcGWJeNvfLFPnnnTSLnD9VsXfxJGy2uZQEZK6idP7Uhm3+clN9iuvvRWSkTGp4iJI0nvFTZ5Gz4WVv0HsvhXMCyzR+6tzQZRKii/Cca4Wn4fW6oQvqxtOEhCyKHp9InNkY6llpC2ksQ5vyUKle1RiPJ4zrb0fYN++DaoA6B3tWZzJ+agZr9ivBBX1MXyV46azUmNenlj1pGawpb1j3TvlK8vY5AQP6SIgdFo0B0FmnBQYqFsQpw0pbkrzrCjXlveB5Nv0Ydaoa3YK6rqltnjhEucOjzOk4LdQ8lW1cd8Kqv370ySTFGMB5hDBHdw1DV2xvPq29b21F+zFzl+cxdVImq3dW4HB6MJpjGDFjMfathaSGmgZeY90ZnltKUqSTPcszg3rFt6agNk/gkM0By+TsoKHoNR+HVqXxvLXgeqaJhnNcV7EMm83GA4s2U+kC07BHKLyAAxY5NgYzgHl04D1jhjK0tM4SH9Yw0LHxymgXnDhe/1KPjzKnMLiqdtHyfsoXQbteS4QQQgghhBDi0uIbstntdvP5558HpNXW1vKLX/yCgwcPcv3117No0SLuueeegDxqvvmET506pU4KiwSAuxQ3u3e0YvBXCNHxOd3KXH3Rw9UpF2A/x0+gDFeaFuKht3fxdc4ZOzoOI+Cp3cMKv3kEbbYyHKoth09bGdqGN/BpimZ2iPkgx1r6AnDi+BHgNG43oDMSqcobnRpD4KqOsG9bcDgBPDjKl7NyV2BYKjXODHhwVh/SmBccLmU4W8vw4GEw++rbJMzQZsZGmwAPbm+nQE11vUVt001x+njKHB6MMTMozVV/tq3qjpb62yAyOR6rzkPVvtWtEADpyu2trfatgbFv4BjW0WOVYXRbpoXHzF3JrjXZpKdMxjYpk/WVLtBZGJUaHGrTUneiUwuZEwcVqzMC5sNuC+o23yIajkPr0nbeNF3PWkDLOfY5fWQDmU9VUIcOy6g5pDZW4ZsxNsasXhUonGGgo1OZFmcEPFRVPKdOrZ+jempeuHt3sbXsWiKEEEIIIYQQAqZPnx74QrFqeeaZZ+jfv7/6YxiNRnQ6HS5X6ChdQkICAwYMAO/Q0G+//bY6S4C+ffvi8XiorQ0xjG4YJAAshBCdWXmFMo+maQQbC+cxNr7hkV58ci4l+S3rD7mrqhYwMSK/gNThTY+NavIG9Tynqyn3ziN40/BUctcODz2MJHDarTzEtwzLJzk29JwHWsrQFhLYQqXDA5gZnZ9Psu/Y9owlObeEaTEG8FRR8ZwbqKTyhBL4HJY1j4SeDfnykyxBvavae98Ath9xKENhjsolN9k7RGnPWJLzSxlhAuoqKduiPW/5oXeoQ4d1Sj6zvXOaAsQn5/PIECNQS9Uu2J89OSgwYbPZsC2rUOYUdpR516VryquOSYVLb0wgJlIJWusj40nOL2W0Wdm3nduVPJrq+gW0zeLM1VS4wBj3SFAQuG3qjrb6q4gleYgZ6qop39AaQbmu297a8lqCy4MHMMZMYEKMUn+Hzy4kd0YMRnVeDTQds4Qs1pYUMG9sAjf5LufuSioOHqcO0OnUJQm/7kSnFpKfFMnxsiVkt8a4z34C2/xwUguC27wmmo9DePdCLbScN03XM83CP8dB9mezpUoZCWH4HP/JmMPkG/7ZuY9M9T3DZmPS5irvMNDJ6k8CoI+MYXhqPiX5SVh0gKuCMi37YDDS/CBejRueVao8UNhYQHLLO0GToPVaIoQQQgghhBAiyLlz53C73UHLF198wfnz59XZ6d27N5dffjknTijTffmYzWaeeOIJ/t//+3988803/Pa3v+Wxxx7jnXfeCcin1rdvX86ePdtoQLk5EgAWQojOzL2F4l0OPIDBMoIZjxfVv4n0+MQ4TMGdMMNyfM1zHHQBRitJj+QHveVk35hbP8fdrkrv98fMqU9/8pEk4syNdz+r3FONE8AYw8TFz/ptu2EIXy1laCsbincpQTxjDBN9x/bZxUyMM6HDg2NXMb7nwrs2H8EJ6MwjWPCsXz6Xg1plGvN6bbZvCblsrN/OAuIMAAbiFjRsu9B7gI8Xp7PL4QGdibiJixv2LcYIuKgoXl4/vKmWvOzKVIYxNlgY/Yh/fYzBiAdH2UrW+M9d2EGYhi0gv2gTdrudTUWPh9w3TXX9Qtqmu5zsJU9R6QsCZzUEgduq7mipvwD65CnEGcFVuZlmRncNW6drbxq01b6x65CyXYOVaflK/X1ktAUDLlzqvKmFfvvtvT4Y4lhQv66l118dRpOVETMW8OSzDXmenBGDAQ+OysAaEnbdScji8SQLOnRYkv4vuAz+Q75r2DefwDb/CEnW4DavjbbjQJj3Qi20nDdN1zONwj7HjdhSvA8nYIiZwDx1EDTgvPot3ptb5IQ4zIDLsSfkkOvuLdUcB3QWvwC53zY3FeXzSFIMJh1QV8XmJXnsB2KMTV20m9BMeQOlkjTE+6KAwUrcMHW6NpquJUIIIYQQQgghghw5coRJkyYFLf/v//0/PvjgA3V2+vTpA8Ann3wCQEREBP/7v//LE088wc0338yrr77K3Llz2b17t+qTwRqbT1gLCQALIUQnV12czkPLdlLlrMNTv9aDq/Yg64tDDFsYlv3kpWWy/mAtroaNhnS8OJ3ifYH56pxV7Fm9moONDaN5ZDnLnzpIbZMbD78Mbaa6mPTMpzhY6/I7tsr+7Vz2EOn+k1EeWc7PVx/0e6haR23FejLTNhP4zhcdY9+A4szsoDLUOavYuSQtqLfdheb1uJT5gwOOWUdQsYeDlbW46ic6pqH9ZAbum9a6fkFts3o7mUvKcHjAOGQOJfN9QeA2qjua6i8kx1vRearYs7IVhz/tyu2trfbNvYXs1Xuo9XsRtK62gvWZaewLyqyFhmO2P5vVZRWq67nHb98C3/gIu+5YTRfUi1mb0G1eE43HAcK9F2oR/nnTej3TIuxz3Jjqlayv8PZe1Th09oQYE+Cialcj3+0uptKhDAMdmoc6p4OKshXYJmewwds0e+r1QB2uKnV+H98Q3BeimLKD3sZcV0XFPnW6RlquJUIIIYQQQgghLti1114bNGSz1WrF5XKRn5/PkiVLuOKKK3jwwQdJS0sLuSQmJoJ3OOnG5hMO13f69ev3rXqlUPTu3ZtPP/1UvVoI0cVJ2xdCiCbEZlG6eAjdKlczObMl/fvEJasj1J3UQuxJFhxlIeYxFheuI5xjIYQQQgghhBAdmvPkZ5j6XK1efUFa85n+9OnTue+++3jllVf41a9+pU5u1IoVKzAajeTm5tYP73zllVfi8Xjqh4xOSkpi2rRpdOvWTfVpxQsvvMDTTz/NPffcQ1paGhUVFSxdulSdLSzSA1gIIYQQQoRtwpQ4jLio3CzBHaGN1J2uT86xEEIIIYQQQohLUd++fUMO2Xz27NmA+YJ3797NhAkTsNlsPPLIIyxatChg2b59O3h7AEdERATNJ6yF9ABuQmu+MSCE6Dyk7QshxKUmlUJ7Eo0NCqtWV7GMydktmylWtDPpASyEEEIIIYQQQrSrrtgD+Ic//CGZmZl8+OGHPPbYY+pkzWbOnMlPfvIT1q9fT1lZmTo5LNIDWAghhBBCCCGEEEIIIYQQQgghWsBoNKLT6XC5XOqkFunbty/nzp3jo48+UieFTXoAN6E13xgQQnQe0vaFEEIIIYQQQgghhBBCiNbXFXsA33fffSQnJ7N371727w89atznn3/OW2+9pV4d0pNPPsnVV1/NkiVL+M9//qNODosEgJvQmhVGCNF5SNsXQgghhBBCCCGEEEIIIVpfVwwAT5kyhUmTJhEREaFOarEPPviAX/7yly2eB1gCwE1ozQojhOg8pO0LIYQQQgghhBBCCCGEEK2vKwaAIyIiGDduHH369FEnNatbt27079+fyy+/vH6d2+3mT3/6E6+//npAXi0kANyE1qwwQojOQ9q+EEIIIYQQQgghhBBCCNH6umIAuCO6TL1CCCGEEEIIIYQQQgghhBBCCCFE5yQ9gJvQmm8MCCE6D2n7QgghhBBCCCGEEEIIIUTr6+g9gLsK6QEshBBCCCGEEEIIIYQQQgghhBBdhASAhRBCCCGEEF1CZGohW+127KVZDNerU0VHJect0IT8jdjtdkqzhquThBBCCCGEEEKIsEgAuBMz3tydn87oQdqMKxmsTuRyxs3oQdoMPffc/B11ohBCiIsmlUK7HfvGXBLUSaL9pRZit9spTFUnXEQJuWy027G3ayEao6H+6pMp2GrHvna2OuUi0lDeTudC9y2B3I127Ha/pcXbamWtWHdGxVjQARhjGBarThXtpplzfHHO24W2oYsllWExBgCMQ5JIVicLIYQQQgghhBBhkABwJ2V+8Hqe/s1NTB1zPfeO6cVAdQauJHHM9dw7pj/pv7mZVQ92tiBwIjnP2bEXpqgTOpGLsw+JizZht69C07foJ1GwxY59/UIS1WlCXAQxqQWUbm3noFtX1jOWsfMKKbXbsds3ktvEk+6E2QWU+AWFtpauJWtstDobaMwLEDNqHgUlG5VeXd6lqXOuH+4NhIYRDNWSV1wc0anDsOo8VB3aoE4SokmtWXd2VTrwALgq2XdEndqxXEr3wubOcWc6b22vmH2VdQC4DpYR+ogJIYQQQgghhBBNkwBwp3Q5k+7oobwl7zrF8098zDZ1FupY9dvjVLkAIrDc0TNEkFhcsvoY6KZeJ8RF1DMyEqNOvVZcsJ4JpOavZeOzi5kxwoJRna4yNn8jC0ZbMSkdjQDQGc0MmZFPYWpgYFdLXvTxzFu7lfw5I7CaDMr9qjn6CeTOicNv843TkldcJKOYFm+CumrKN7jViaJD2E/2ZBs2mw2bbRkVSnypA2jdunO8OJ3xNhu2qXmUX/jm2tSlcy9s/hx3pvN2MWzJnIzNZmNqXrk6SQghhBBCCCGECIsEgDulCPTdlf9zVpykdN95XOosfIvjL59T+Kr36V73iGYDAeIS8l4JcyfYsE1byl51mhCi04qdM4OkGDMGPDgr9lHVRIBHPzafKTEGwEXl5kVKUOiBRWyudAE6LKNSmeCdh1FLXoAJufMZYdZBXS0VZSvITJvkDTrZSC9uyOcvNX+K0jtsXwVNFBs05hUXhz55ONEGcB5azy51ohBNkLrT9ck5FkIIIYQQQgghLr7v9OvX71v1SqHo3bs3n376qXp1B3AF2X+wMLgHuF91MPlXX6kz1Bu68CYyh3QHl5P8n53iZXWGDiuRnOcyGHxyG7b0EnViJ3Fx9iFx0SYybv2Ybba5tN23XFo6bttvQs8EZj8+jWEWEwZvb6K62gq2rFnOlkpfV5pUCu1JWBxl2DIPMWH+bCbEmZVelHW1VDy3kuzt1X4bVYb8nTasodenx+Vgz1OLWLP/dEA+fcwoUpMnEO/3/Z46J45968lYs19ZkVqIPckS8LlgDsps6fjHCMMtQ1gSctm4II4TZT+nIjqXiVYDeByUZWbimFDEI0OM4HGyb0UKy73FRh/DhHmzSYoz1/fU8tTVUrllDdlbKv23DvXltWDyHQifugqWTc7Gt1lae98AYuezdo6e8pXL2VIZS+7GBcQZ6qhYNpls/y8GUgvtJFk81O7MZNYa//MeS1bpYoYYPVStH0/GFm15ic2idPEQjK4KVqRlh9WTKzq1kPwkC+6KFaTtGUbJgjgMjjJsIaLFWvKGxVsvHWWTKHbNZ/aEOMwGAA8uxx5WZ67hkN8+hFXX/YXTNr31Ur0fvn3VeZzsW53Ocr+DGVbdSS3EntSXimVp7Inx9grXoexbVRnLszdQf3nw0lJ//c1ea2e0qYrNUzMI6OCntQydpb11lGtJff1Vv1yRoLR/go9DeOkKLcds1LwCJsT75a2rpXrXBjI3HFJnDdBo3fG1C79VAQLai3d//DOHqAPgO2aRVK2fypa+uaTW71/oNq9Vs8dB872wne/dLanrKo2eY83nTcO1JNw25BXOMUst3EqSRUdd5VNMztze8GH9cHKLHiHO6MFRlkl6ceD5aFZTdaKR+1uz9UwIIYQQQgghOjDnyc8w9blavfqCdMpn+m1MegB3Sl/h9Hb57da96bl9TfrLlf9xnetEwV8hhCbRqRQ+s4DR1oYHuAAGcxzTUqf451R0iySrKJ9pvgfIAAYzcTPmMz+2IduEglBD/loYveAZClMjG1aSwPysOYxQfb/OYMI6egEl8xqfI7Y54ZdBm77x80myejeqszBsXgFzhnjHSdCZiE+aoPy/fji5RflMG9IQsAHQGczETcunNHd4w0rvw2GlvKqHzSG0yb4dWc6slGy/oH9jxmKJBDwOyv0Duj1jSc5NJcYIoCMyJkFjXogZYcGIh6qy8IK/RM9jfpIFnesgT2WX0+RHtOTVqO+wIvKn+YK/ADqMltHMz/XWBdBe17W2TT8Nwd9a9iwPDP5qqzsGoucUsWC0L1iCsm/WiWTND5wcWkv9DTAqn2FmqKsuVwV3fMIsQ2drbx3kWtJWtByzCQVbmTNClddgJmbiFJqc3rbZutM4l7NKvUoDHZFJRTwesH+h2rw2LT4O4Wjne3fYdV3tAs5xsDCvJRrbULjHrDjzOao8YIiZRoHfsBfD508jzgieque0B39boE3rmRBCCCGEEEII+vbtS2xsLP3791cndSoSAO6kPOeV/+qu9AZ4G2FsJr1Z01dht28i5249Q2cWULLJjt1ux162ldLVCxlnVeXvk0ja8hI2bfXms9vZVJQTnA/QD5zEwtWlbC3zy1uyEJs6Yz09IxeVKvkKpqJsUs+giQtZW7q1fhv2raWsmjkUv9FIFb6y+b6vrJS1j9qwLdrk3cfA7Nb/Cdzu1tK1LPyfEDuiWYgyN3Y8AfSDmPSLtZRuaThO9k0lLByjzthAPyKHUrsd+6YCpobaJonkPGfHXpgSsFa9z/atpRQ8OCggj/HONApKNjWct7KtbCopIG2I6ojX1x0jibNXUeqrE2WbWPsLmwxJ3mpimT8/CYsOPM5KylakeYfnfZgVZZU4Qz1sNccxxOjBWbGZRQ/YsE3KZKfDA5iIHhEDgH5CAVOsBnBVNWzTZmNFWRUudFiGz2GU3yY9bhdVe55i2cMPNOTdU4sHMMUkEQNQnF6ftsw7+aSjzDcfpW9p6P2rtQxaGEwmPFVP8cAKZQhho9kMjjJ+/vM9OAGdKZp4IGF+KnFGwFXJ5iV+x9a7b8a4KcxXDhn65AJGWXTgqWXPiofry5uWuYda1fe35b6Fx4ReB7hOUI3SM3HUvEI2PruYiX7BBYPRqjEvxEeaACcnPPMoKNnYcD2xb6SkYDbxAZeKBLIeH4HJU8vOJXnBPb4CaMmrncFoxOOsqD/PaasrcAE66yjm+cVMwqrr0LK26dUQ/HVQljmLlX7dEVtSdwwGg1KHFyllXuQtr8EyjHjfdjXUX7Xk4dEYcHJkc+ODu4ZThs7Y3tr7WtJWtB2zVIZZdeCpYrNfu3h4RRmVTVX05urO/mwme7dVv/y8DIcHPI4ypub5XwW0z28cbpsPX5jHQeO9sF573bu9wq3rak2e45actzCuJVrakKZj5t5C9uoKXOiwTsknNRL0w3NJjTOCq4LV2VsCNx4uvzpRvyxrbIqDMOuZEEIIIYQQQogWGzt2LIsXLyY5OVmdFBaz2cxDDz1EWlqa5mXKlCnExsYGLP/1X/9FRESE+muaJQHgzuaGK5g6tx+J3lHCat9q+of+X9/yPjqw9OGJuQbuuUGdIzyGO5aScY8J1+t27DvsvFztRn/DUFKychjp9zA/ZVEGtmgDp/65G/sOO7tfd9ItcjApWQtJ9NuefkQORUunMjRSh7NCyWvfc5hTul6Y/PI10DP04QLSbjXieWsb2RmlVAHc/RgLk4diOu/g5R127DtepuackagxGSx90Oz38ZHkrMjA9l9GPNUvK9930IlhaBoP/aib3/corNNXsfTBwO3WRpgZ+uBSCiYHhZY10DMyq4i85KGYI5wc3qM6nktXkeIfsNWPJKcoj6l3mNE5D7N7hx37jt0cPqmjVx+/fH70Q9IpmD0Y45c1bMvOoDTMDjL6yQXKPn/5pvd7XqbKpcNkbgjVWqevouQxG9arPTgOKmXfXeGEPlZsWUXkjAg+Nqb7Csm4A978i/f8fKnHfEcaS2f7nR/RcglJxJqU4QxXp2dSXH5cWX/6HcqLM0nJDHqEDB4nB1c/REr2Bo6cBtyVrKlUPqfX9wRgVLwFHS4Orsho2CZQXpzB5koPGCKJrX/Su5+8lKlkrNzO/ncahkosX3mE4wB6PcpWtdFWBo08DspXbud0+XFOAOBk3+piqqvdSq/SbjoOMZbRMQbAyZ4lmWw45HdsV85ifWWd8uB9uBIpmBJnRUcdlcWzWFn+Tv1XHa90c67+L0Wb7psW7jp6zi6gtDSfOSMsGEAJiGyuDH7wrCUvZobNGIHVv3sSBkzW0TxeOB9fZ7XhuTMYYvTg2LWSgJGlQ9CStyXqqjYzPiW7/jwf35WtnAtMWOqf/muo6y1pm0B0cgG5SRZ0dVVszkxH3ZmsJXXH49zHirRMNhxRynxkZTkOj1LPfXdALfU3QORs4q06PFX7WH5Endig+TJ00vbWzteStqLtmB3HXQfoIokb1RAyfKe8mMyUzOBApk+Ydaeefji5jydhcVewupH2o0V4bd47PG/9iyx+y8ZcAvuctvA4hKu9791h1PWgf1FrPcdhaP5aoq0NaTtm4C7PZsnOWjw6C6Pm55ObGofB46BsSZijXlywNq5nQgghhBBCCCEu2KOPPsr48eODX/YNY5kyZQqLFy8OWH79618zffp09dc0SwLAnY3lu9w7woiR8zj3vUPW2qancK5de5zCfW48dMc6oi9DG5leqml6rFYXRclTyfh1EUXrilg6fyoL/+IE42AmzfbrIeo8SsmCScxaXEjRuiIKf5lO6b89YBxE4gjf5iaRO3swRk8N2/zyFq3MYdbUjJDz2FqnLyXjv83g2MbCR0qU4C8Adbz9l6VMnZbB0nVFFK1bytzs3TjRETX43vpewIk/T2Gw0UPNCwuZOn+p8n2/zmDq49uoRTU03A0pzBodBe/ZWei/3dRCDp/RYb1nFoF9YjW4+zFShhjxOLaRMWUWOSsbjufUlYdx6aK4d/pUb7n1TMpN85Y7g0lzcihcV0TRukJy5kwl43fqjQPWFJY+NhIzNWx7fC4lYQZ/ASbfZkVHLbvnZXm/ZykZKQ+RvuY1JYP3uOhchyn0qwuFi2cxacE2ajxGBj8wl8EBW9VjNtZQmDpXdX7AHDep5cdRNLAaMQCuyl3hP3j0HGffLtX8jd7eJ5Oz9wPxRJt0gJEhi4Mfes+IUdJMfl2D9PHJ5K4tZWtA3iRadMmBFpVBk+OVFDc85wXHIVYGBRW9PV+d1ZQHpcF2h/IIXG+8CUggsi/ACRyhOjkFaON908IymgWjrRh14HFVsXPZA0pAxOFR59SWF2+eFZl+vZP2UOsBTLFMHNXQayqcITO15G2pE9Ub1Ksor3WqV4Vf11vSNvsOJ3eiVQkmZGewIWhXW1Z3jh9ariqDE3fAadNSfwMlpA7DTB3V5cHHz1/zZeik7a1dryVtResx28WS4oO4MGAZvQC7fSula/OZN9ZvXOIQwq07Pqn5c4jTt16gLdw2H76WHYewtfe9O6y6HkjrOQ5H89cSLW1I+zEDqF4zi10ODzpLDFaDB8eu1UEv67SdNq5nQgghhBBCCCEuyPXXX0+PHj14//33uf/++4MCvBMnTmThwoUsWrQorKWsrIxvvvkGjyf0M9imSAC4s3F8zosHzuAmAtOw/iycrM4QSD/ZRNowPTq+5NjGWp55VZ0jPM6DJexWPWyrenI3VR4w3TikPtBakpfFtoCgo5tt/6kF9BhvVNbo7x+KVeehauvCsAKU1v/JI+u+KHDYyc30D/4CLxWQ9eTLgfNAVh2j9gxg7MctACSSaNXDycOUPq36wqoSXjwWuGPmsUOJ0nl4869Fgd/l3s3L/3GDyawKcoZv3IiB6HFx+FnVfgDuPU+w1wE662AmA+gnM9Sqw1O1jYXqcodiHUde1jiiqMGeE96x9eescwMmBjwwyG/4bDeuk8rx8R2Xqr88EVQXqCph2z/d0GcAI+8ITKo9oMpf9XfedAJXGhrp7S1awnNOfVIuRDd0Qd14mpCQRdHjE4kzG9WvU1wAjWVoUx4q1asa4/HgnaK9CR1h31zU/5uhzsGe1ZmMn5rBmv1KcEEf01cJXjorNeb1qWVPWgZryhvWvVO+krx9TsCAPhJih0VjAHTWaYEP3RfEKcNKW5K86wo15W3N+Q+NOlWNbkFd19Q2Txyi3OFR5tecNlad2vZ1J6z660efTFKMAZxHCDm6a4t0xfbm09r71la0HzN3eR5TJ2WyemcFDqcHozmGETMWY99aSGqoaeA11p3huaUkRTrZszyzTQNtQW2eRobntdmwTc4OGope83FoVRrPWwuuZ5poPMetLqw2pPGY+elW/zkdxsgWjRneYu1bz4QQQgghhBBCNMVoNNK9e3fcbjeff/65OpmzZ89y7Ngxjhw5EtZy2WWX8e2333LihNKBQAsJAHc2731F6bIP2HTsayACy+DgIXf93Tu4h/JQx3GSrD+co1bDc+gGbmrfVM+YBeCk7kv/QCugNzNy8kLyVqxibelWtm7Ziv2+qIBP3XJdP8DF+/vDKEyfRLIeHITe+TJFmUUcDfER4+BxpC0qYNXqEjZt2crWsgwG9/DPEYWxB3g+fJPD/qu9PN8E/h1lNAA6Bk0P7gmQPlgP9MPsnS84pTA4j3peXX+9DDr48n3eDBmId1Nz0g30wnQHcJuZfoDrvb2BAe6Q+pGYlcIgvZOX1yykSBXUDof9D3aqzuiIGpPHpk0lFMwbx2C/YaaV49L4edv74cdKL4mb/de6cQYNU34UlxvoYUQGgW4FTrcyV1/0cHXKBdjP8RMow5WmhXjo7V3SveMMjh0dhxHw1O5hhd98dDZbGQ7VlsOnrQxtwxv4NEUzO8Sz3bGWvgCcOH4EOI3bDeiMqJ8DR6fGELiqI+zbFhxOAA+O8uWs3BUYlkqNMwMenNWHNOYFh0sZztYyPPj+1FffJmGGNjM22gR4cHs7BWqq6y1qm26K08dT5vBgjJlBaa76s21Vd7TU3waRyfHKC137VnPho7t25fbWVvvWwNg3cAzr6LGjsfiPwK5JC4+Zu5Jda7JJT5mMbVIm6ytdoLMwKnWCKqO2uhOdWsicOKhYnREwH3ZbULf5FtFwHFqXtvOm6XrWAlrOcevS0oa0HTOf4bmljDbrcO57in1OMMalkhvintem2q2eCSGEEEIIIYRoyrXXXkv37t1xuZp/LTkcffv2xePx8NFHH6mTmiUB4C7u3FfeIaIj8OvV2QKqIGmAs3XKG/bWFFZtWEv6A0P5Xg8dno+Osfevu9l2ONRTNA+ek+p1IbidON2gM0YxcIh6D/SMzCqlNCcF249M6Dx1vH14N7t37qXmjCorcM6j5aGhi6q/KHPchlperlFybX0yi6xfqpYnt6o3dkE8nlPqVSHU4VQOFFE/vr1l57qqlIwpU8nZ+DI1dQasI1LIKSllYYh5fUUHUl6hzH1nGsHGwnmMjW94tBmfnEtJfsv6Q+6qqgVMjMgvIHV402OjmrxBPc/pasq98wjeNDyV3LXDQw8jCZx2K+3RMiyf5NjQMwRrKUNbSGALlQ4PYGZ0fj7JvmPbM5bk3BKmxRjAU0XFc26gksoTSuBzWNY8Eno25MtPsgT1rmrvfQPYfsSBBx2WUbnkJnuHjuwZS3J+KSNMQF0lZVu05y0/9A516LBOyWe2d05TgPjkfB4ZYgRqqdoF+7MnBz1kt9ls2JZVKHMKO8q869I15VXHpMKlNyYQE+kdgD8ynuT8UkablX3buV3Jo6muX0DbLM5cTYULjHGPBAWB26buaKu/iliSh5ihrpryDVrur43puu2tLa8luDx4AGPMBCbEKPV3+OxCcmfEYFTn1UDTMUvIYm1JAfPGJnCT73LurqTi4HHqAJ1OXZLw6050aiH5SZEcL1tCdmuM++wnsM0PJ7UguM1rovk4hHcv1ELLedN0PdMs/HPc+rS1IS3HjPoXEozg3Mfq5dtZvnofTgzEzclvtPft8KxS5SXRjQUkN5InbC2oZ0IIIYQQQgghLh6j0UhERESLeuyG0rdvX9xuNydPhhNQCyQB4E7KaLgcgHOffa1OCnDqy/PK/xivaPGwxaDHaAkRBLxhIOYe4HHVchRI/OlIorq7ObxyEpNSZjF3vjJn7caPAscmd51VHsp8b0zA6tDOvklG9jZqMJE4eylpA/3KoZ/MvUOMeN6zkzF+KrMemUvWr4soWncs5JBv+uutIXucGrsHjv2mlE/PV7XKHLfBSym73/PmfesoR19XLW+F+nbFqToPdO/PgFvVKQB6ovroweOk5gDgqqMOMN1sU2cMoY43M7LZ5gDTnWksnek/jLMWLg4/u5S5KZOY+sRenOeNDH3oMRKBGlcdYKR/QugtJ17XD3BS+091imhT7i0U73LgAQyWEcx4vKi+N/rjE+MwhT5dzTq+5jkOugCjlaRH8oN7um/MJcGbd1el9/tj5tSnP/lIEnHmxrufVe6pxglgjGHi4mf9tt0whK+WMrSVDcW7lCCeMYaJvmP77GImxpnQ4cGxqxjfs+1dm4/gBHTmESx41i+fy0FtXeB222zfEnLZWL+dBcQZAAzELWjYdqH3AB8vTmeXwwM6E3ETFzfsW4wRcFFRvLx+eFMtedmVqQxjbLAw+hH/+hiDEQ+OspWs8Z9HsoMwDVtAftEm7HY7m4oeD7lvmur6hbRNdznZS56i0hcEzmoIArdV3dFSfwH0yVOIM4KrcjOtNbprp2tvGrTVvrHrkLJdg5Vp+Ur9fWS0BQMuXOq8qYV+++29PhjiWFC/rqXXXx1Gk5URMxbw5LMNeZ6cEYMBD47KwBoSdt1JyOLxJAs6dFiS/i+4DP5DvmvYN5/ANv8ISdbgNq+NtuNAmPdCLbScN03XM43CPsctOG/h0NKGtBwzoucxP8mCDid7li9XejYfWc7qfU7QWUh6PJfgjsCpJA3xBmUNVuKGqdO10l7PhBBCCCGEEEJcPEajkW+//ZZPPvmkfp3VamXgwIEB+cJx/fXXc9VVV+F2u/nggw/Uyc2SAHCn1A2T9zlC3ZmmA8AO1zn1qhaJui2FQQEPNPSMm3k7Jjw4DtuVPEY9cIqPD/q/6W8lZXBg2PXojqM40WG9N4eRQQ9JQqgqYeGal3FFRGHLWUqK1bv+xyZ6Aec+cQTMp6u/704GBAwBvZs3jwPX3k6KqjerfmA6toGBfQGO/r0GFzoG3JOG76tay7YDb+LGyOAHUoK2rR/xGIkW8Dheww7wup2jH4HOaiMnrF64VZRkFvHySR1RY7JZOl39DU0z9gnsMeD6+1pe+wjorszVW7v9NWrRYf3vx4LPmzWFcT/Sg/NN9r6uShNtrro4nYeW7aTKWUfD6xYeXLUHWV/8XEDe8O0nLy2T9QdrcQW+wxHkeHE6xfsC89U5q9izejUHQw0AgPLAdPlTB6ltcuPhl6HNVBeTnvkUB2tdfsdW2b+dyx4i3X8yyiPL+fnqg34Pl+uorVhPZtpmgt/36gD7BhRnZgeVoc5Zxc4laUG97S40r8elzB8ccMw6goo9HKysxVU/0TEN7SczcN+01vULapvV28lcUobDA8YhcyiZ7wsCt1Hd0VR/ITneis5TxZ6VrTi4a1dub221b+4tZK/eQ63fu2d1tRWsz0xjX1BmLTQcs/3ZrC6rUF3PPX77FvjGR9h1x2q6oF7M2oRu85poPA4Q7r1Qi/DPm9brmRZhn+O2oqUNhXvM9MPJfXwEJsC5ZzkrA5rsavY5AWMc0+qv1T7FlB30NtC6Kir2qZK1akk9E0IIIYQQQghx0fTt25dz587VD9l8/fXX8+ijj5KTk0NKSgoRERHqjzTKN5/wZ599xvnz3s6eGnynX79+3jGChVrv3r359NNP1as7hLTfDuDeG8Dz0ccUrTnD4X+eV/V6/Q6WH13B+Nn9ufPaCDjxMVkpLo4F5AnD9FXY7zPjcoExopaX//4mp9BhHpzIoGt1eBzbWJheQhVgnr2WtaPNeE5Wcfjg25yiFwPuHIrhrAuTyUjNCzbmPq1s1jp9FUvvi0L3pYuqw//gbRdgNDPoB1dweGoGJSSS81wGg09uw5ZeAoB+RA5F8wZj9NSwbeFcSqps5G1KY5DeTe2r/+Co04Mu8hYSB4DLY8LEYQqm5LAX4O6FlD46FCN+eU2DuD3OwMfHdUTdAId/M4mclwD0jFxURPqtRjhTy+FXj/LxWeDKfnzPGoWptoSpeXv9j1IjgvehsW33irqdwf9lROc6TGFaDrt9zx6tKaxaOo4onQfXvw/zj5pTQC/MPx7AFa9MJeN3kLhoExm3fsw221xKAPQjySlKZ7DRQ80LC5n7dBXmB1ex6n+icB8oYOqv94YsW0qhnZH6Ko6++janQDmWPzZx7lgJDy3chruR86YcRzP6877z4i379FXY7+vnd1wbpBTaGWepaShzB9OR274QQrS72CxKFw+hW+VqJmdKbzOhQUeoO6mF2JMsOMqC53YVraAjnOOuYHguGx+JQ1f5FOMzWzImuRBCCCGEEEJ0XM6Tn2Hqc7V69QVpzWf606dP57777uOVV17hV7/6lTq5SU8++STf/e53yc3N5Z133gHgnnvu4cEHH8RgMPD666+zYsUKTp9WpmNqyj333ENaWhoHDx6koKBAndws6QHcSb1YcQYPoLu2H+m/6sc4dQYMzP3VTUrwl69xHDitPfhb7xw1G3LZVGNg0GgbtjEjGdTbTe2BkvrgL0DtmlWUvFrLOaOVoWNs2EYPQHe4iIyDwXPYVj29kNwNL1N7Vo/1Dhu2MTZst34P3UdvclSd2cu9J4e8F2rw6KIYt2QVKVY7S1faqXF1w3zrSGxjbNx+3cdsW7yJWvWHX1pKWp6dKif1eRNvhqO/z2NbUC8HN7sXp1OwswpnhJnBI7zlGzYQ0/kadr/0mvoDGrjZvTiNpZuPUoupfttDvwfOVzex1D/4i7f3c04pL7/nRh89VCnH6MF8r5uTN9/wy+fPvZucvG3UfKkj6r6lrAqzJ3DNW7V4rvaeuzE2Rg7QUbuniGxv8Beg6um5LFyzmxq/8zYyrhd11bsp8g/+CiGE6LImTInDiIvKzRLcEdpI3en65Bxrl5pfQn7q8Po5fXveNJx5E7xDOleVq7MLIYQQQgghhOigfEM2f/HFFwFz9v71r39lwYIFvPPOO8TGxpKfn4/V2nzcxjefcEsD29IDuAmt+cZAWzAO05N2Tw/66b9k96MuXgxIvZxxM67CdO4cx/56lpdbOhpYE704u4qROZtIH+zh5V9PZekBdWpXFdwDWDTo6G1fCCFEa0ul0J6ERb26EXUVy5ic3bKZYkU7kx7AooNJLbSTFOri49zHohTvXMNCCCGEEEII0YV01R7AP/zhD8nMzOTDDz/kscceUydz5ZVX8sgjjxAfH09dXR2/+93v+Otf/6rOVm/mzJn85Cc/Yf369ZSVlamTm9WJegBHcM33Y4n98Q+IvEqddmly7XOT/8uPmBsU/AX4mm1PnaHodxcQ/L0kDGbwjXrwOKm5ZIK/AFEYe4DHUz85mhBCCCGEEOIie+65zVQ2TFgMHhe1B9eTmS7BXyGEEEIIIYRoT7fddht2uz1oeeaZZ+jfv786O0ajEZ1Oh8sVOGGrT0JCAgMGDADggw8+4O2331ZnCdC3b188Hg+1tUFj3oalk/QAjiDy7qmM/2EP5c9zx9m7YSvHvlDna12t+cZAp9XFewD75rSlqpSpGZvqhzru6vQPFFA62UrtC5OY+/Slstfhk7YvhBBCCCGEEEIIIYQQQrS+jt4DeOrUqdhsNvXqep988gn5+fl88MEHAevvu+8+kpOTefHFF3n66afr15vNZtLT04mOjsblcvGHP/yB3bt3B3w2lFDzCWvRZgHgq6yJjIj2Bmw1+OrdA/zlqP+csargr89FCAK3ZoXptLpKAPjBAjbdoaf2vTd52+kBemH+8SAGRerBXUXp/Aw2vaf+UNeS+Iu1jOMobzKAu4ZEoT/zMgVTl7JXnVFI2xdCCCGEEEIIIYQQQggh2kBHDwC31PTp07n33nvrh2yOiIhg8uTJjBkzhu7du3P48GF++9vfcvr0afVHg1x//fUsXryYr776igULFvD555+rszQrwmAw5KhXXrB+ifyvbSAmY0969tS29LnxB5g+P0b1J+eDgr9f1PyFLYe/Q9RNveh2eQ9ujLmes/9+E+c5dQFax1VXXcXZs2fVqy8tsaOYYjXw4cEt7NX+gkHH0ctKwsBobvzeAAZYv8/3o83007mpPfJninOX8eJH6g90PVcPtjEh8Ra+378X5z48TOkTv+LPDfOQCz/S9oUQQgghhBBCCCGEEEKI1uf+4isMV3VXr74gHeGZ/r333kvv3r3ZuXMnH330EZdddhkTJkzgsssu47e//S1//OMfufrqq/npT39KfHw8gwcPDloMBgPvvvsuN9xwA3fddRenTp3CbrervyosbdMDOGY86XdFAnD+7Fd8rU5vxOVXXEHEZXCmcjPr/3YiKPj73IvVfAFcZb2XKSOiuOqytu0J3BHeGBBCXHzS9oUQQgghhBBCCCGEEEKI1tdVewCvWLECo9EYMGTzlVdeicfj4fz58wAkJSUxbdo0unXrpvq04oUXXuDpp5/mnnvuIS0tjYqKCpYuXarOFpY2DgAfZ2/hVo6p00O6lsRpExnYA85UbmXPd0bUB3+/em8vpWXH8I/xXowgcEeoMEKIi0/avhDi/7P3//FNXvfB//9qCWoSqQkKzEoWq22UZla2Kllt2tmsdllNchei4ISZQlk80zgiBhqHNI6ZcYoxBVyoNxOvBieuW5i73OYDI3Wiwj1idym0Mc0wWaL7e0duh1gr0lSEVDSV8uOiNN8/9MPSJdm+LmGBbd7Px0OPR3Jdx5euc673ORLn6JwjhBBCCCGEEEIIIYQYf1NxADgnJ4dvfOMbnD9/ftQlmxMHhG+55RY++tGPJp0/deoUp0+f5ktf+hLLli3D7XYn7Sesx4fVByYCo70sPvh7/lTq4C/AO94f8nTfCd75IzA9l7mVi7jtalUiIYQQQgghhBBCCCGEEEIIIYTIkpycHEwmE+FweMTBX4B33303Phv4F7/4BcePH096nT59GgCz2cwHH3zAm2++qbqCdhNyAHja9GkQHfz93v7Uwd8YGQQWQgghhBBCCCGEEEIIIYQQQlwqZrMZg8FAMBhUn8pITk4O586d44033lCf0mxCDgCjYfA3JnUQ+C5uVicSQgghhBBCTHm5rjb2u924uxsoNarPCiHEpSVtlH5SZkIIIYQQYjKYOXMmV1xxBeFwmPz8/LSvW265Rf1nI8rJyeG9997j7Nmz6lOaTdAB4HfwvjT24G/MOz8/wiunI1Ommf4R5N8EQgghJg4XbW437p4mitWnxKXnasPtdtPmUp+4iIqb6HG7cV/SmxiJjvg1VtKy34175yr1mYtIx/1OOheat2Kaety43QmvjK81zsYxduY7bBgAzA5K8tVnxSUzjs84cxdahyayC83b5dE+jKsMvz9IG6Xf2GV2keN3osakEEIIIYS4pK6++mo+/OEPc8cdd7Bx48a0r9bW1uTvraO8brrpJt59992pOAB8NX9xz3Lm/qn6eBofvo7PlFdQdP004DxvHhvgVXUaIYQQE4rD1UL3fv2dZkKjGfksXNNGt9uN291D0yg9YMWrWuhK6DTb372ThoV56mSgMy2AY/4aWrp6IrM2oq/RnrmxNDoQ6h57MFRPWnFx5LlKsBsUvEd3q08JMarxjJ2DHh8KQNDD4ePqsxPL5fRZOJ7PWFxeplrsTKY2Klv0tn0TrcxGiklX29jfu2H4xwMjvtINXs8oZlVLFz37E76H93TRsioxZfSHICO94gWeMGDe08z8hCvACD9uMDoob9hJ9/79CffZRcua+TiSZmBovQchhBBCiKlnz549dHd3p34H0vD693//d1577TV+8YtfxF//9V//RUdHR3xP4ExM0AFg4MPXcNuiMQaBP3wdnyn/csLg737+94uZr4cthBDi4piRm4vZoD4qLtiMYlzNO+n5/kZWzLNhVp9XWdjcw9oFdiym4WMGs5WiFc20uZIHdvWkxVjImp37aV49D7vFFJm1MRZjOU2rC0i4/Mj0pBUXyXyWF1ogNET/7rD6pJgQjtC41InT6cTp3MpgSH3+Uhnf2DnVWcMipxNnxWb6L/xyWXX5fBaO7zMW2XB5tA8TwWRqo7JFb9s3dpldzPi9+DFpLG2g+/trWWC3YEooN4PJgn3B6rEHnEdjcrBwVa76aLLcclq6mlleZMVsSLgBkwX7vNU01F3IDQghhBBCTB3nz59n3759dHR06H798z//M4899hiPPPJI/PX444/z8ssvq99Glwk5APz2L17l1LkxBoE/fANFS2TwVwghhIjJX72CMocVEwqBwcN4R+kAMy5sZpnDBATx7F0f6TS7bz17PUHAgG2+i/LoL/r1pAUob6pjntUAIT+Dva3UVy+Jdso5qekcTpfI1bwsMpvi8CCj3DboTCsuDmNlKXkmCBzdxUH1SSFGIbEz9ckzFpmS2BETzbjEZGdN/Huxc2v0u6yvd/jY0kaOxNLmumheXYQZUAIeelsfiqer3vQUfb5gZHZ0otAgW2PXSnylfAkPEgyCtaiStCtrRxW7yrGbQAkMsndTdfx69z3USq/HTzDlBvTcgxBCCCGEyKYPXX/99R+oD14wxyJq/iYXOMULbfs1Lsl8A3OXL+a2a+Btz152/exPWFQ5l9zpwB/f5tX9u3jh19GkH76Bufct5rYZZHXwd+bMmbz11lvqw0KIKW5S1v0Zxax6fDkltuFfhof8g+zbsY19ntiv0120ucuw+Xpx1h+lvG4V5QXWyCzKkJ/Bp7fT+OxQwkUjS/4uLxme9akEffQ9tZ4dR5L3HjA65uOqLKcw4f2VUADf4V3U7oh2YbjacJfZkv4ulY9eZw2JXQNa70GT4iZ61hZwuvdRBvOaWGw3geKjt74eX3kHjxSZQQlwuLWKbbGeF6OD8jWrKCuwxmcrKCE/nn07aNznSbw6xO/XhiXxJ/pEO0ISO3TGO28A+XXsXG2kf/s29nnyaepZS4EpxODWpTQmvnF0mboym4L/QD0rdyQ+93waujdSZFbw7lpE7T59aclvoHtjEebgIK3VjSPM1EiW52qjucxGeLCV6r4SutYWYPL1pu0k0pNWk2hc+nqX0BmsY1V5AVYTgELQ10d7/Q6OJuRBU6wn0lI3o3GpzkcsrwYlwOH2GrYlFKam2HG14S7LYXBrNX2O6KxwA5G8eXvZ1ribePMQpSd+E63a6WaBxcveilqSJsTovYfJUt8mSlsSj1/1jyuKI/Wf1HLQdj5CT5nNX9NCeWFC2pCfoYO7qd99VJ00yYixE6sXCYeSJNWXaH4SE6eJAYiVWS7eXRXsy2nCFc9f+jqv15jloPuz8BJ/dmcS6yojPmNpH6R9yLR90Bq/kFEd0vTZPeL3hxABz0Gq6hOXB9bYRsW+Q4U8tC+tTxlgNFa20L3YDt69LKodvr62Z5FBOWihNc50t30ayyyFtvjNRkxGvi+n/949ohG+A8bkN3SzscgMgQE21Wwe4/Mp+ozHLKdY2froOzCdeQsseHdVULtPHduRZxrJF2mecTpa70EIIYQQl7vAmd9hmXWt+vAFmZR9+lk2IWcAA/DOq+zf/ULqTOCLNPgrhBCTRp6Ltu+mLgtmshaw3LUsMWXE9FwaOppZHuv0ATBZKVhRR13Cz7/LW9It+Wtjwdrv0uZKXCqsmLqG1cxLuyzZWrrWjLxH7Fi034M+OYV1lNmjFzXYKFnTwuqi6ILJBguFZeWR/zaW0tQRW/Js+O8NJisFy5vpbiodPgi42vZH71fVIZtGVvJ2fBsrqxoTBv1HshBbLqD46E8c0J2RT2WTC4cZwECuo1hnWnDMs2FGwdurbfCXvDXUldkwBAd4qrGfUf9ET1qdcko6aF4e67wFMGC2LaCuKRoLoD/W9dbNBMODv376tiUP/uqLHRN5qztYuyA2sEIkb/bFKUv26YnfJPObKbFCaKg/pTM0QuM9TLb6NkHakmzRU2blLftZPU+V1mTFsXgZo+72N2bsjCwY8KoP6WAgt6yDx5Pyl67O65NxOWhxiT+7Nce62pjPWNqHbOYtW/SUWcb1YtTY0Re/oL0O6f3sTv3+YMLiWExX0kU1Or6ZAT9guomSlI1Zodxhw0CIof7hwV89zwJ0lMMUlp2YzIZC5tvNgIKnd6zB38yEdx/Fqxiwl1aqT8V5g5H1dmwlzZQnb/grhBBCCCEmuIk7AEy6QeAHWH6/DP4KIcSwfOrqyrAZYsuCRZfluu8hWns9BNJ1FFgLKDIrBAb3sv4+J84l9RzwKYCFvHkOAIzlLSyzmyDoHb6m00lrr5cgBmylq0nsl1LCQbx9T7H1ofuG0/b5UQCLowwHycudbY1uzuXrVS8NNjz7V+896GGyWFC8T3Ffa2TZNbPVCr5eHn20jwBgsORRCBTXuSgwA0HP8JJn9z0Uz5u5YBl1kSLDWNnCfJsBFD99icuz1ffhV71/NvOmjQWjAQieZojIzKP5a9ro+f5GFid0CJrMdp1poTDXAgQ4rayhpasHt9sdffXQ1bKKwqR+o2IaHp+HRfFzYNPmMWYJ6Emrn8lsTlrarrp9kCBgsM9nTUL/qaZYh8zqZtTw4K+P3vqVbE/o8cskdkwmUySG10fueX30fk22Egpj19URv2qVpXmYCHB8r3qu0jAt9zAZ69ulbkuyRV+ZuSixG0DxsjehXjzU2otntEAfK3aONLI0eq3469FefAoovl4qNie2Avr3f9Ra57XTWA46PwvjLtVnd5TWWFcb9RlHSfuQnbxli74y01gv0hgrdvTEL2irQ5l8dpvM5rTxa3HMT6gT2tuo3Ue9KJjIK1mYfMLoosBuiLxXtEj0PYsoTeWQBbrbPu1lpk/2YnL8ObCYAU7he1Z9bhSmAtbGv38Pv3rSbRYc3k2vJwTWkhH3Ej6yrZOBIGB2sLx5D907m3CVjvFBqecehBBCCCFE1mR5ADiXuTU11Gh6RZZ/BrjGsXj4+APRZaABPnw111wdu/Y0/mR2NN1XH2Th7dE/voyYb7mSL624huoVVzFbfZIruHfFNVSvMHLHLR9SnxRCTBXFZeRbIkuitdfU09l/KnL87En6O+upqk/pQgYlwED7/VQ17ub4WSDsYYcn8ndG4wwA5hfaMBBkoLV2+JpAf2ctez0KmHLJj/dqHWFzVQW125/lyMnhpeb6tx/nFIDRSOSq+ui7B50UH/3bn+Vs/ylOAxDgcHsnQ0PhyKzS6QaOspAFDhMQoG9TPbuPJpTt9pXs8oQinWXRDpBlBXYMhPB0rmR7/8n4W53yhDkX/7+IrOZNj3CIGata6O5uZvU8Gyai+3vt9aTurasnLVZKVszDnji1AhMW+wIeb6uL7zNW2rSCIrOC7+B2klaWTkNP2kyEvHtZVNUYf86nDjZGngUWbPHeUx2xnkndBPIqW2gqs2EIedlbX0OnKq+ZxI4SOExrdT27j0fu+fj2fnxKJM5jX7H0xG+S3FUU2g0o3sNsO64+OWzse5ik9e0StyXZoq/MThEOAYZcCuYPDx6c7O+kvqo+dSAzRmPsxBlLaXq8DFt4kPYR6o8e2up8dCnMNJ3Y7p4mkruxMywHrS71Z7eGWI+1J3Ean7G0D9nJW7boK7MM68WYsaMzftFWhzL67A4OjBG/+oT3efApYMgrIXFevXGZAxsQGNxNrEj0PYsoLeWAnrZvsslWTE5eRzoP48eEo2yEWcDhfjZXONl6wEsgBGZrAWWPdODu2UlzpTrAhBBCCCHERJLlAeCL5MMf4ROfn8dt6uNTmPUrN/Kdf7qJirtv5K67r0uT96uYe/eN3HX3x6j5p1t44iuTbRB4LhueduNuq1KfmNBmf60Lt3s/T3zFqj4lRHbYzZiAoOegtuV2AZRTHD6o2p8t+qv8pY1HgELyLAbATNHG1I6fFY7IOUvCJAFjYSVNO7vZn5S2jLF2+hqZ/nvQ5ZSHzuF+MvAdZXvKoGJ05mtgiP6Uc/CsL9KdazTfBBSTmwNwGt+YkwKynDc9bAtYu8CO2QBK0MuBrfdFBkR8ijqlvrRE07TWJ8ys6MOvAJZ8Fs8HY2kTrgIzivdpatSjnCp60mbq9FDiXn0R/f6A+pD2WM+kbuaU0rTYjknx0dtYy+6UrGYWO6eOblPdQ4Bw0mPTE7/Jil0lWFXLUaYz9j1M0vp2SduSbNFbZgfZ1DlAEBO2BWtxu/fTvbOZNQtHX0tUa+zEuJpXU2D00btJ4/LyY9Ba57XLrBw0u9Sf3ZpiPZnWZyztQzbyli16yyyzeqEldnTFL1rqUGaf3b7Dm8eIX53Cu+kfCoHBRmHCCHBlvg3wM7gvFlR6n0WUlnKY0rIXkxNGaJCtSTOrI68Rn++pHRz0hDDYS0ZdBvzIjlqqljqpbu1l0B8CkxXH4sdTlqmHDO5BCCGEEEJkRZYHgN9g4F92sUvT64cMRacQveP9YZrzI7yOXo5LQF/Bks9dgwEg+Fv+v2/9hmfUSQjxxLdP4Q0CTMP2uRlpBonFeDMZDOpDQlwUyjmNvVSaTMegZ8pCcQMdjy+mwGqOtEvjQuc9ZJWCR31oJIpCUH0sxUTIWxAl1jkZ8tHXXs+iilp2HIl0CBodOZEO0IBHZ9oYP33VtezoHz52sn87mw8HABPGXMgvycMEGOzLkzst1xZElpW2lUWPtelKO+rebTqZ1W16BrGuq26ePkq/T4nsFblctfQjZD92NMVvAmMlZQ4TBI7Hl6O8cFOxvsWMd96yRX+Zhfs3U7GknvYDg/gCCmarg3krNuLe34YrzVacemOntKmbstwAfdvqU2bFj6eUOk/ysqVJr6WNKUvR6y6HcaXzuWXQnumi8xlrM951SGeZZdV45y1b9JeZ7nqhJXayHL+6Pruz4OBeT2QJ58LojMzcVTisoHiPsiP+owL9z0IXHW3fZJOVmMyK2I8JcrGl+1o4jp7d6yGIhfzFKYuGpzjV30njyqXcF906wVzgGnH5aCGEEEIIcWlleQD4PO+ffZu3Nb3e4f0/Rv7qD+feSXN+hNe759VvehmYhvHKyH8FBs/Qffh8mk6AD/D9++9peyk6qn7lNMzqJGLcvfDNCpzORTz8vYu1C5e47AXCkX3G8tL88jpjRzh1mshyhNVpOn6ir5roGmkLFxRgBhR/H60Je2k5nb34VFfWTt89ZEd04NOSx6o021wttOUAcPrUceAs4TBgMJOrSpvncpB8aCLkbR++AICCr38b2w8mdzu7CqyAQmDoqM604AtGlqu0lSZt9gtAjjEb3bTZszDPAiiEo5MCdcV6RnUzTGfNInp9CmbHijQzKrIVO3rid1huZSF2g4L3cHt8OcrMTeX6lq28DTPnJC/BmLdwAbbEFdh1ybDMwh4O7mikpmopziX17PIEwWBjvitxEdMIPbGT52pjdQEMttcm7YedDeo6nxEd5TC+9D03Xe1ZBvQ847Flqw7pK7PsyFbehk3F9iFr8ZvRZ3cWHN/MgB8MNgeVRsgtL0gz+zTDZ5El4xtnF8E4x2R2PIvXpwAG8uavUp8cX8c3c9inYMorpVLjDwvOHmxkwA9gwmxXnxVCCCGEEBNBlgeARbaZrrlCfSiJNXb+/B8v2r5QQoiLqH8wss+YZR49bWtYWDjc/VdY2URXc2bzIQ96/YCFec0tuErVa8cls0QH9ZSzQ/RH92G7qdRF087SEZfhOxuOdOLbSpqpzE/ZpQ103kM2FLMPj08BrCxobqYyVrYz8qls6mK5wwSKl8Gnw4AHz+nIwGdJwxqKZwynay6zpcxOudR5A3j2uA8FA7b5TTRVRtd7m5FPZXM38yxAyEPvPv1p+4+eJIQB+7JmVkX3LAQorGzmkSIz4Md7EI40Lk3ppHQ6nTi3Dkb2FPb1Ro/V6EqbaT+n0VyMIzcyaG3MLaSyuZsF1kjeDjwbSaMr1i+gbnbWtzMYBHPBIymDwNmJHX3xG5FPZZEVQkP07x6PQbmpW9+y2ZYQVFAAs6OcckckfktXtdG0wnFBP/zTVWbFDezsamHNwmJuijXnYQ+DA6cIAQaD+k60x06eq43mslxO9W6iUet6rBol1/lSXC2pdV4X3eWg7bNQDz3PTVd7ppv2Z6xN9uqQnjLLBmkf1HeiLXayFr8X8Nk93nYf9aIY7BQsy6PcYYGgJ2X2qa5nkS0ZxNl4t326ZCkms2V3rydyX9YF7O9qorL4pvi5m4oXsqZtJw3jNPu28+AQIYOdwuhzjCimYedOmlylOOIFBsZcB6WuFoqsAAFORX4HKoQQQgghJpgPXX/99R+oD14wxyJq/iYXOMULbft5VX0+rRuYu3wxt10Db3v2sus/NC7tnNF7aTNz5kzeeust9eEJofrbt3LXx0F59SR/2/Ce+nTcvZtv4f7brgDfKe5++Pfq0xPYXDY8XcvsM8/grOlSnxQiqyZy3U8n0kGepuOP6MBY/Kf/LtrcZdhCg2wdc/m2Yhq611Kk7gOJSbhGrquNtpHen+S0cfl1dG0swZJ4DAAfvfFBPO33oFlxEz1rCzDFyyVaJur/j107z0Vbcxm2tJlT8PXWD+9JO1Kegj78021YSbzfLOSNhPypjyfw9Q7PBnG17acsbeaCDLZWJw24jE9aVZmlk/KMRqEn7UhcbbjLRuouTs6b3ljXXDfT5SNvIc2Pr8BhhuBAKxWb+6N/qCN2onlLfOYRxTT1rKUgMSZ1xS8YK1voXmwnPLCeis2jzIfRcw+Tqb6lPLNL1JYYy2npXo495bpBgiEz5sS0o8Y6mbe/o7Y7Cr7eGmoSNkLVHDvFDXSvLRpxACHpfvXkbdS0qe2ZZjrLAUZ51knP4hJ/duuNdT3PWNoHaR8ybB80xy+klrc6rYrmz2498aurfGPm09yzmrygn6DVinKgmpXD6z9H6XgWOstBMz1xFjNSHGtuq8k8bZZiEsDV5mbk2wgxuHUpjUc03K/qGZXWdbG6xJI+JhOvG3vG6iQx8fiNxqgpNe7WdLkjP+6M/5shljYhkUpwsJWKxtj3VK33IIQQQojLXeDM77DMulZ9+IJMtj79i0FmAE9SSnTla8NVo88ANo9xfkwPPIHbvYcNXzAy58EWuvZE913s3U93+zruVS/1M2su1du62LN/eI/GPR0bUtMBxtuWsK69m/29CWm71uFUJ4wzcuf67ki6lgoilzRy++J17OzeP7wn5P5unnhwDimLj8buLfZ+vd3s/JoT5/o90TwmJ7f/bfJ193fvZN3fpslIonh5JRwzzkktE3U+jbez5B920r0vYW/Lfd3s/Id7o/mMqeIJt5s96+di/nw1TyTc356OdThnJSUWl4mhzhru33oAbyCEEj+qEPQPsKvz6aS02h1hc3U9uwb8BIcvmtapzho6DyenCwW89LW3MzDSMprHt7HtqQH8o15c+z1kzVAnNfVPMeAPJpRtJH8Htt6fPJB5fBuPtg/gj668DyH8g7uor97L6eFUURMgb0BnfWPKPYQCXg5sSh0AudC0SjCyf/Cog7+XwmAfAx4/wfhGxwzXn/rkvOmN9Quqm0PPUr+pF58C5qLVdNXFZgJnKXZ0xS9UFtoxKF76to/eGarLVK5v2cpbeB+N7X34E/YCCfkH2VVfzeGUxHroKLMjjbT3DqracyUhb8kDFppjx24ZZfB3vKWv87roLAfQ+lmoh/bnprc900PzM9YjW3VIR5llTbbyNoXbh2zG7wV9do+rg+z1BDFYrVgUL0d3p2lD9DyLbMkkzsa97dMhSzGZTf3bqrh/6wE8qjZCCfoZ7G2PDv6Oj87D3qT3gCO0tvcy6AsQSjoRKbO+9vqEwV8hhBBCiMvDF7/4Raqrq3W/XC4Xf/M3f0N+fn7SKycnsvVPNsgM4FFMyF8MfPwjVNxj5o55ZsyA/4CXVTtHfoTWlVZ2LDAB7+Hte5NDPwjx/C/VqUbxwBO477ke70u/wXbbdfiO/ZT/DsJ1N/81s//cjCF4jLbqDRyK9pVVtbm59+Nh/IM/5ZWAgiH3M8z9tAVD8EVaKrbwQvSyxnkb6FgzG/P54bRcdT23F5g4VlFLV8oMYCNzHmqh9n9Z4RfPsO6RLrwAX9jAnq/NZvoZL8cG/pvfch23fmEONxsVTvzbw8N78RrvZENHDbPNCsH/d4yfnvgtmD/JX8+2Y/ywgsFwjmP/tIQNP4oktz/wBFvuuRkSr/v5Odx8jYL3+xXU9ozQORgtr+Frzaa2awNzZ4U5MfAfvBYEg+V2PlOg8ELZw3QRubd17TXMmQXhXx7jp6/+BoXr+GTRbOyzDCi+Z1hXE80vVTzhvpfrf3kCJfd6fhu95nX2v2HOLUY45WZldQeyA/GFmZB1XwghJor8Bro3FjHd087SetV6lEKMZiLEzoiz9sS4mAjPWExOEjtiopGYFEIIIYTImsk6A/iuu+7igQceYPr06epTGTt9+jTf+MY3OHnypPrUBZMZwJON7aPcNc+MmfMEDp+kYZTBXwD/zlO0HQ6jcCX2eTnMGXEtntEYsduDdFRWUPvNDjqe7GBLXQXr/j0A5tksWXX7cNLAK3StXcLKjW10PNlB29dr6P5/CphvZ+682OWW0LRqNmblBM8kpO3YvoGVFbWRQVEV+wNbIoO/voTBXwBC/Pe/b6FieS1bnuyg48ktPNx4iAAGbp59V3wW8NxHq5htVjjxg3VU1G2JvN83a6l4/Bn86sWUPl7FygU3wy/drEu8rquNY28bsN+xkoQcj+5zd3K7BcIvd/FwtOzaNq6komoD+6NJ5j5axZxZCid+UMuS1Rtoi75f7fIK2l4KYrDdxQP3Jc9nNn78Ok788/3xa255pJFDbwC5n2HJp5OSCiGEEOOqfFkBZoJ41JsRCjEGiZ2pT56xyJTEjphoJCaFEEIIIYRaTk4OH/rQh/iXf/kXnE5nymvVqlWsX79e02vTpk28/vrrfPDBByhJKxOOHxkAnmx8v+eHP3mbMNOwlHyMdUvVCZIZl1qoLjFi4D1e7fHz3ZfUKbQJDHTFZ/nGeP/5EF4FLJ8oig+0dm1u4Jnh0VkgzDM/9wNGzJ+IHDF+eQ52g4J3/zq6ktKmZ//bzTTcczP43DTVJw7+Aj9qoeGfXyTp1ryv4n8bMF/PZwCYy1y7Ec4co/s7qjf0dvHDV5MzZl04h5sNCq8935H8XuFDvPjzMFiszE48Phr/bwkBxpvnJC/PfCZIZJWse7njthHujTCH/vEFTmDAXqB60L/8Kd/qS7xvLz/+eQAwYZqZcFgIIYQYZ/tqF+F0VjDGVniTjIu22BYMGl49TcXqCwgNpmbsiERT8xlL+3AxTM3YEZOZxKQQQgghhFCbOXMm58+fJxhM2AMlwa9+9SuOHz+u6RUIBPjIRz7C22+/zeuvv66+1LiQAeDJ5pfv0731dfa8+gdgGrbZKTvdJrlr9jWR+a2+MzT86zn8I6xcPLow/tfSLSocIPRe4kArYLRy59J1bG59gp3d+9m/bz/ue25O+qvP/On1QJBfHdFwM7Pm0vCV2zEGXqSjvoNX0vyJefa9VK9v4Yn2Lvbs28/+3lpmX5OY4mbM14Dy69c4lng4Svlj8v/fbDYBBm5/ILVDp2a2Ebgeq2q/4BH9sptnfhxAMc+mepeb7vYNVM2zJuxPfB2mK0e+N8InCL4NzLIwJ/FwwJs86A28EgwlDbQLIYQQQgghhBBCCCGEEEKIC2exWDh37hxvvvmm+pRuZrOZq666it/+9rfqU+NGBoCnuHPvR5eInkbCoGMGVIOkSd4NRWaz2qt4YvdOau6bwyevMaC88SovPH+IZ44F1H8BKChn1MfSCAcIhMFgvpnbitQ5MHJnQzfdG6pw/qUFgxLiv48d4tCBFzjxtiopcE5RD5mOJoj33924n0v/evGEOv1Iwhz6VhUV1W24X/ZD7mzuXbOT7tYq7OqkQgghhLhEOqlJs3TPSK+ljUfUFxCTRWcNTqfs/yv0kPZBCCGEEEIIIS53H/3oRzEajbzzzjvjMmhrtVoxGAy88cYb6lPjRgaAJymz6QoAzv3uD+pTSX773vnIf5g/on3Z4hRGzDb14Cvw8duwXgNK0M8rwNwv3cnNV4Y5tn0JS6pW8nBdZD/bnjeS1y8PvhsCLHzy7qTD6b37GrWNz3ACC3NXbaH6toT7MC7lriIzyi/d1C6qYOUjD9PwzQ46nnw1urxyMuONdqzqg4D5yuQNuyP3Z+R9f2R/3dRXN4d+mfQnYwqfOkTH11dSsayB7v8XxnDLvax8wAj8ltB7YPjTW9M/H2N09nLgBC+qzwkhhBBCCCGEEEIIIYQQQoismjVrFldffTXhcJhf/epXAEybNo3Pf/7zXHXVVerkY7ruuusAOHNGy0zJzGR5APhPuK1sIQs1vT7HJ6Jje8aPfy7N+RFet/2J+k0vA9OxmCP/FXp79AFgX/Cc+lBGbv6rKm5PGgM2cu+Df40FBd8xdySNOTKg+ZuBxJm2dqpmJw+7vvLcKwQwYL9rA3emGVdO4e1i3Y4XCU67GeeGLVTFps5+2sJ1wLk3fUl79Rrv+Ty3Ji0BfYjXTgE3/DVV85Lf0HhbDc7bDEnHXvnxCYIYuPWO6gufpWs0Y058y/Ar7Dn0GmHAZP4k8AwDr4Vh1mwqHlC/m5E7H53LzQllLIQQQgghhBBCCCGEEEIIIS6e2JLNiQO2f//3f88jjzzCP/7jP2K3q8d3Rjdz5kz+8Ic/8NZbb6lPjZtpJpNpg/rgBfuojdl/dh0f5gqumjGDGZpeH+Uj0eHoD3/ko2nOj/C6OjITlj/+lqGXhhjPorr66qt599131YcngD/yqdI/4c9mgOGqcwT95wj+5gPeS0rzIWx/eSWLnbP4xEc/DL/7PT989j3SLcY8qvz5LLObCP7hE9xVNodPzPoEfzF7DvdWf435n7wKxfcs3/rWzzgDnLm5GOctVj7xN/ncbLHxF7PvpOLRKj52PojJdBVB79P8n+PAmZ/x86v/irmf/hRz7p5Pvs2C7S9mM/uOe6l6cAHXP3OIl/kEc/92Dn/6jpenD77MOd8RDp35M+b99af49Ny/4qpX/g8vH7+W2WWzsX7iUxR/8k+x2j/NnHtW8rVSE2+/Y8LEr3nx317gf3ibY+98gvlFN3Nz4YLhtHdV8dDf3cRv/X/kuhnw64F9vHASeP044U/OY85f3M6dzmL+zGrFfvtsZhc7Wbq8iorbgzxz5H+Auazr/jZr/+6vuOpn/4eXfzdcXvFrFf8Dnd+q4s4/s2K1f5rZs++k4t6/wvKRAC9++yl+dgZ+/tLb/Nm8OXzq03dS9td/xp9a7Xx69p0sfeir3HWLieBL7dS2e4kM5eczf9mtmF5/kX0//p80z+q64XIWGZu4dV8IIYQQQgghhBBCCCGEmLzC77yP6eor1YcvSLb79D/72c9SUFDAf/3XfzE4OAjA//zP/3DTTTeRl5dHUVERb7/9Nj6fT/2nad17771cffXVPP/885w+fVp9elxkZwbwiR+y/9gbvPPu+7x/MV6hUwz872cZUt/HFPbDwbdRAMMN11Pzjeu5V50AEw9/4yY+f8M04A/4fnKWV9VJNDvHid1N7Dlh4vYFTpx338ntM8P4f9LFupqu+Oxb/44n6HrJzzmznTl3O3EuuBXDsQ5qB1LXQ/d+Zx1Nu1/E/64R++ecOO924vzsJzG88RqvqBNHhfs2sPkHJ1AMN3PvpieosrvZst3NieB0rJ+9E+fdTv76T3/DMxv34Ff/8Y+2UL3ZjTdAPO3cW+CVf9nMMymj4mEObayh5YCXwDQrs+dF76/kNiznT3DoR/+p/oORnXiNE2cMWAoi7+lcMJvr336FPZtraIsVXPgQG6q3sOdlP9wwmzvvduK8ew62aQGO7d1C9cZD6Nm9WAghhBBCCCGEEEIIIYQQQoyP6667jg996EMEg8MbkJ49e5bGxkb27NmDwWBg1apVuFwupk2blvS3arH9hN97772k6423D11//fUfqA+KiJkzZ2Z1+vWFMpcYqb7jGq43vsehrwX5YdLZK7h3xdVYzp3j1eff5cVTSSe1e+AJ3Pdcz7F/WsKGH6lPTg13bthDzWyFF79ZwZafqM/qdBmU1+Vgotd9IYQQQgghhBBCCCGEEGIyCpz5HZZZ16oPX5Bs9+nX1tZSVFRER0cHzz//vPo0c+bMYdWqVVxzzTW8/PLLtLa2cvbsWXUyAG666SYaGxv5/e9/z0MPPaQ+PW6yMwNYXBTBw2Gav/4GD6cM/gL8gWeeepuO713A4O9lYTazP2EEJcCJCx38Beb+6fVAiFD2frQhhBBCCCGEEEIIIYQQQgghLpIZM2Zw7tw53nzzTfUpLBYLpaWlfPSjH+Wdd97h5z//Ob///e/VyeJi+wlna+nnGBkAFpc1+wMVzJ4Fiu8/catP6jabOTYjvO3n2Mvqc0IIIYQQIttyXW3sd7txdzdQalSfFUKIS0vaKP2kzIQQQgghxKU2bdo0rr32Wt555x1++9vkLU+//OUv88QTT1BQUMCxY8d4+OGH+dd//VfOnz+flC6R1WrFYDDIALAQ4+IrLezp2knL+hqqH6ym+sF1bO7YQ8s9N2MIe9nzz3sy3Ge3is2dm6l5sIbNneuYM0vhxPNdvKBOJoS4jLloc7tx9zRRrD4lLj1XG263mzaX+sRFVNxEj9uN+5LexEh0xK+xkpb9btw7V6nPXEQ67nfSudC8FdPU48btTnhlfK1xNo6xM99hwwBgdlCSrz4rLplxfMaZu9A6NJFdaN4uj/ZhXGX4/UHaKP3GLrOLHL8TNSYvSxfa9gkhhBBCaHPjjTdiNBoJh8P86le/gugyzt/61rf48pe/zPvvv88TTzzBN77xDQKBgPrPU6TbTzgbZABYXB5++St+w3XYCu7EebcT591zuH2Wgv+lZ2hZXcueX6r/QKsQXHM7d959J7fPDHPiuRbWfc+vTiSEUHG4Wujer7/TTGg0I5+Fa9rodrtxu3toGqVHpHhVC10JnWb7u3fSsDBPnQx0pgVwzF9DS1dPZNZG9DXaMzeWRgdC3WMPhupJKy6OPFcJdoOC9+hu9SkhRjWesXPQ40MBCHo4fFx9dmK5nD4Lx/MZi8vLVIudydRGZYvetm+ilVnamIz+ICD5tZ+erhZWFc9I/PPhQcuRXiMUTGXL/miaHprnq8+mGQR3u3Hv72Zn8xrmOxKnTg+n7VFfKDa47XbTE/8HRGb3K4QQQggxlcyaNQuj0Zg0Y/djH/sYN9xwA4cOHaK6upr/+I//4I477qC6ujrt6+///u+ZOXMmRPcrPn/+vAwAi0vsOw/jdC5hw4/UJyaZH7XxcNUSFpU5cTqjr/IKVm7s4oUz6sR67KFhSfR6iyp4+MkXM5xJLMTlZUZuLmaD+qi4YDOKcTXvpOf7G1kxz4ZZfV5lYXMPaxfYsZiGjxnMVopWNNPmSh7Y1ZMWYyFrdu6nefU87BZTZNbGWIzlNK0uIOHyI9OTVlwk81leaIHQEP275ZNwYjpC49LY96CtDIbU5y+V8Y2dU501LHI6cVZspv/CL5dVl89n4fg+Y5ENl0f7MBFMpjYqW/S2fWOX2cWMXz0xacBksbNg7T/TdKFrVxsrcdgMKD4fAUzklSxUp0jPYMbqmMfq5g6a0/xo03RTYdLMWeOyAuw6no0QQgghxOXihhtuSFmy+Sc/+Qkul4tvf/vbvPvuuwAsXLhwePxJ9Zo7dy5GY+R7ocViGXE/4fEkA8BCCCHEFJG/egVlDismFAKDh/GO0gFmXNjMMocJCOLZuz7yZeS+9ez1BAEDtvkuyqN9VXrSApQ31THPaoCQn8HeVuqrl8S/7NR0DqdL5GpeFplNcXiQUW4bdKYVF4exspQ8EwSO7uKg+qQQo5DYmfrkGYtMSeyIiWasmAwNbo1/571v/V4GAwpgpqBsmTophAbZmqZj0Jnmy3JkYFZhqG8XviAY8opIOwSsumZ9ay+e6D04lq/GlQtgx2yCkN9PyJTHvIQR4GUOG4rXS9o1zXTcrxBCCCHEVHPdddcBJM3YPX/+fHzgl+g+wXV1dZHvgvfdx+OPP8769evjr5aWFl5//XU++tGPYjQa0+4nPN4+dP3113+gPigiZs6cyVtvvaU+LISY4iZl3Z9RzKrHl1Nis2CK/mo75B9k345t7PPEfp3uos1dhs3Xi7P+KOV1qygvsEZmUYb8DD69ncZnhxIuGlnyd3nJ8KxPJeij76n17DhyNimd0TEfV2U5hQnvr4QC+A7vonbHkcgBVxvuMlvS36Xy0eusIbEbQes9aFLcRM/aAk73PspgXhOL7SZQfPTW1+Mr7+CRIjMoAQ63VrEtetsYHZSvWUVZgTU+W0EJ+fHs20HjPk/i1SF+vzYssYKICQ2ydWkjscsy3nkDyK9j52oj/du3sc+TT1PPWgpMIQa3LqUx8Y0BV5ubMpuC/0A9K3ckPvd8Gro3UmRW8O5aRO0+fWnJb6B7YxHm4CCt1Y0jzNRIludqo7nMRniwleq+ErrWFmDy9abtUNKTVpNoXPp6l9AZrGNVeQFWE4BC0NdHe/0OjibkQVOsJ9JSN6Nxqc5HLK8GJcDh9hq2JRSmpthxteEuy2FwazV9juiscAORvHl72da4m3jzEKUnfhOt2ulmgcXL3opakibE6L2HyVLfJkpbEo9f9Y8riiP1n9Ry0HY+Qk+ZzV/TQnlhQtqQn6GDu6nffVSdNMmIsROrFwmHkiTVl2h+EhOniQGIlVku3l0V7MtpwhXPX/o6r9eY5aD7s/ASf3ZnEusqIz5jaR+kfci0fdAav5BRHdL02T3i94cQAc9BquoTl6zW2EbFvkOFPLQvrU8ZYDRWttC92A7evSyqHb6+tmeRQTlooTXOdLd9Gssshbb4HfeYjOYvNLiVpYlfukub6HmkAFPSvUefhab8RLja3JTletm1qJZAUw9rCwx4nlpE/bOxFKPk21hKU8cjFJghcLieqm2FtLnLyBk8wMm8Bdw0FL3n3FXs7CjhbHs/xtXRWKnpzOh+x5RJO6m17RNCCCHEpBA48zsss65VH74g2ezTr62tpaioiI6ODp5//nn1aV1uuukmGhsb+f3vf89DDz2kPj2uZAawEEJMdnku2r67lgX24U4qAJO1gOWuNL82n55LQ0czy2OdPgAmKwUr6qjLH05W3pJuyV8bC9Z+l7bIz8ejiqlrWM081fsbTBbsC9bStSZ1uTGttN+DPjmFdZTZoxc12ChZ08LqouiCyQYLhWXlkf82ltLU0czyouEOWQCDyUrB8ma6m0qHDwKutv3R+1V1SqSRlbwd38bKqsaEQf+RLMSWCyg++hMHdGfkU9nkwmEGMJDrKNaZFhzzbJhR8PZqG/wlbw11ZTYMwQGeauwffRl9PWl1yinpoHl5rPMWwIDZtoC6pmgsgP5Y11s3EwwP/vrp25Y8+Ksvdkzkre5g7YLYwAqRvNkX01CXvDm0nvhNMr+ZEiuEhvpTOugjNN7DZKtvE6QtyRY9ZVbesp/V81RpTVYci5cx6s6AY8bOyIIBr/qQDgZyyzp4PCl/6eq8PhmXgxaX+LNbc6yrjfmMpX3IZt6yRU+ZZVwvRo0dffEL2uuQ3s/u1O8PJiyOxXQlXVSj45sZ8AOmmyhJ2eMVyh02DIQY6h8e/NXzLEBHOUxh2YnJERgNka1QzimcU5/TyujCYQPF52EfcKRviBAG8orSzgFOFe6nczAAgOWmxO9+Hg4MhTDlzaMYyF3owBo6yWH1Lw+ySHM7OUHaPiGEEEJcvmbMmDFuSzabzWauuuoqzpy5oL1JNZEBYCGEmNTyqasrw2YAJeCht7U6ujzvQ7T2egik65ywFlBkVggM7mX9fU6cS+o54FMAC3nzHAAYy1tYZjdB0Dt8TaeT1l4vQQzYSleT2C+lhIN4+55i60P3Daft86MAFkcZDoDOmvi5rdHNuXy96mXEhmf/6r0HPUwWC4r3Ke5rjSwhbLZawdfLo4/2EQAMljwKgeI6FwVmIOhh76aEso3mzVywjLpIkWGsbGG+zQCKn77Wh+L3W13fl7KMWjbzpo0FowEInmaIyMyj+Wva6Pn+RhYndAiazHadaaEw1wIEOK2soaWrB7fbHX310NWyisKkLdCKaXh8HhbFz4FNm8f41b6etPqZzGaUwGD8OVe3DxIEDPb5rEnoP9UU65BZ3YwaHvz10Vu/ku0J0xEziR2TyRSJ4fWRe14fvV+TrYTC2HV1xK9aZWkeJgIc3ztyj6GWe5iM9e1StyXZoq/MXJTYDaB42ZtQLx5q7cUzWqCPFTtHGlkavVb89WgvPgUUXy8VmxNbAf37P2qt89ppLAedn4Vxl+qzO0prrKuN+oyjpH3ITt6yRV+ZaawXaYwVO3riF7TVoUw+u01mc9r4tTjmJ9QJ7W3U7qNelHR7vBpdFNgNkfeKFom+ZxGlqRyyQHfbp73M9MleTKrdVLqKtmUODEDAc5CUucWmAtbGvycPv3qakn+gZ1zmwAacGtoXOXCkj6EQGPJKGOGnNylODZ6KbJtitkBhDtEh1shgsslGSX4u5QVWQkMHUmaex2m8Xz20tpMToe0TQgghxOVr2rRpXHvttbz//vtce+215Ofnp7z+8i//khkzZqj/NC2r1YrBYMj68s/IALAQQkxyxWXkWyLLXrXX1NPZfypy/OxJ+jvrqapP6UIGJcBA+/1UNe7m+Fkg7GGHJ/J3RmPkg2p+oQ0DQQZaa4evCfR31rLXo4Apl/x4r9YRNldVULv9WY6cHF5qrn/7cU4BGI1o+/hLpu8edFJ89G9/lrP9pzgNQIDD7Z0MDYUjs0qnGzjKQhY4TECAvk317D6aULbbV7LLE4p0lpVGRgqWFdgxEMLTuZLt/Sfjb3XKE075xX9W86ZHOMSMVS10dzezep4NE0QGRPZ6UvfW1ZMWKyUr5mFPnFqBCYt9AY+31RGbYFLatIIis4Lv4HaSVpZOQ0/aTIS8e1lU1Rh/zqcONkaeBRZs8d5THbGeSd0E8ipbaCqzYQh52VtfQ6cqr5nEjhI4TGt1PbuPR+75+PZ+fEokzqdH0+iJ3yS5qyi0G1C8h9l2XH1y2Nj3MEnr2yVuS7JFX5mdIhwCDLkUzB8ePDjZ30l9VX3qQGaMxtiJM5bS9HgZtvAg7SPUHz201fnosp5pOrzdPU0kd3lnWA5aXerPbg2xHmtP4jQ+Y2kfspO3bNFXZhnWizFjR2f8oq0OZfTZHRwYI371Ce/z4FNSB/dig4CBwd3EikTfs4jSUg7oafsmm2zFZISpYG28rP75kQXYTJEfLVWN9kdjqMy3AT48T8cGqI9w9GQIDDYKtY4AJ4rGZjh4MjqYbMZWVkmeJcRQ3xEgQFiJ1KOs09BOTp8gbZ8QQgghLl8zZ85k+vTpzJw5k8cee4yNGzemvDZt2sT3v//91O/PaV4ul4tp06Zx9mzq9jnjTQaAhRBiMrObMQFBz0Fty+0CKKc4fFD1ARP9VX5kz6pC8iwGwEzRxtQPqRWOyDlLwiQBY2ElTTu72Z+Utoyxdvoamf570OWUh87hfjLwHWV7yqBidOZrYIj+lHPwrC/STWE03wQUk5sDcBrfiD+bj8ly3vSwLWDtAjtmAyhBLwe23hcZEPEp6pT60hJN01qfMLOiD78CWPJZPB+MpU24Cswo3qepUY9yquhJm6nTQ4l79UX0+yPL5SXSHOuZ1M2cUpoW2zEpPnoba9mdktXMYufU0W2qe4h27MXpid9kxa4SrKrlKNMZ+x4maX27pG1Jtugts4Ns6hwgiAnbgrW43fvp3tnMmoWjryWqNXZiXM2rKTD66N2kcXn5MWit89plVg6aXerPbk2xnkzrM5b2IRt5yxa9ZZZZvdASO7riFy11KLPPbt/hzWPEr07h3fQPpQ7uRQYB/QzuiwWV3mcRpaUcprTsxWQ6gcNbWZS8OfKw0CBbk2ZAR15JzyF3FQ4r4PfSmRBnBwdOomDApnUE2KA+AOHwKeAIfUMhLAVFWIMeeo8ABFEUwGhOHuzXcr96aWgnj0yItk8IIYQQl7PTp0/z7W9/m97e3pTv3VpeP/vZz/jFL36R9Hruued4+umn1W817mQAWAghpgDlnMZeKk2mY9AzZaG4gY7HF1NgNafrW8iQznvIKgWP+tBIFIWg+liKiZC3aMcOQMhHX3s9iypq2XEk0iFodOREOkADHp1pY/z0Vdeyo3/42Mn+7Ww+HABMGHMhvyQPE2CwL0/+YrS2ILKstK0seqxNV9pR927TyWxQRXQGsa6rbp4+Sr9PieyBtjzdvm5Zjh1N8ZvAWEmZwwSB4/HlKC/cVKxvMeOdt2zRX2bh/s1ULKmn/cAgvoCC2epg3oqNuPe34UqzFafe2Clt6qYsN0DftvqUWfHjKaXOk7xsadJraWPKUvS6y2Fc6XxuGbRnuuh8xtqMdx3SWWZZNd55yxb9Zaa7XmiJnSzHr67P7iw4uNcTWcK5sDJyIDoIqHiPsiM+WKb/Weiio+2bbLISk1Ghwa04nU7uW78XTxAsJY/Qlvai2uQudGAFsC5I/g68IrK0tMFWqGkZ6PzCyOo9nD4V/6FDTGRPYQh6D8Znl09Il7TtE0IIIcTl7v/+3/9LZ2cnHR0dul/f+MY3eOSRR5JenZ2dnD9/Xv02404GgIUQYjILhCP7jOWVqs9cgCOcOk1kOcLqNB0/0Vfsx+wLFxRgBhR/H60Je2k5nb34VFfWTt89ZEd04NOSx6o0+0EutOUAcPrUceAs4TBgMJOrSpvncpB8aCLkbR++AICCr38b2w8mdzu7CqyAQmDoqM604AtGlqu0laYuG5djzEY3bfYszLMACuHopEBdsZ5R3QzTWbOIXp+C2bGC7ib132YrdvTE77DcykLsBgXv4fZx6DCcyvUtW3kbZs5JXuMzb2Fk2cnMZFhmYQ8HdzRSU7UU55J6dnmCYLAx35XaNa0ndvJcbawugMH22qT9sLNBXeczoqMcxpe+56arPcuAnmc8tmzVIX1llh3Zytuwqdg+ZC1+M/rszoLjmxnwg8HmoNIIueUFaWafZvgssmR84+wiGOeYVDt7fDf1Tw0SwoBt/mpcI1XQMSx0WNWHkmlZBjrPxfICM6DgHUwzy+RII0udTio2a83dxZZZ2yeEEEIIIWQAWAghJrf+wcg+Y5Z59LStYWHh8D+BCyub6GrObD7kQa8fsDCvuQVXqXrtuGSW6KCecnaI/ug+bDeVumjaWTriMnxnw5FOfFtJM5X5Kbu0gc57yIZi9uHxKYCVBc3NVMbKdkY+lU1dLHeYQPEy+HQY8OA5HRn4LGlYQ/GM4XTNZbaU2SmXOm8Azx73RZaOm99EU2V02bsZ+VQ2dzPPAoQ89O7Tn7b/6ElCGLAva2ZVdM9CgMLKZh4pMgN+vAfhSOPSlE5Kp9OJc+tgZE9hX2/0WI2utJn2cxrNxThyI4PWxtxCKpu7WWCN5O3As5E0umL9AupmZ307g0EwFzySMgicndjRF78R+VQWWSE0RP/u8RiUm7r1LZttCUEFBTA7yil3ROK3dFUbTSscmNVpddBVZsUN7OxqYc3CYm6KNedhD4MDpwgBBoP6TrTHTp6rjeayXE71bqJR63qsGiXX+VJcLal1Xhfd5aDts1APPc9NV3umm/ZnrE326pCeMssGaR/Ud6ItdrIWvxfw2T3edh/1ohjsFCzLo9xhgaAnZfaprmeRLRnE2Xi3fbpkKSbTOtLIPm9kZZfS1Ymby2sUW/45cJh69Xdgp5Mle73RZaCjM8VVjLkOSl3NdDWXYTMAwUF69eTBZMauPqZDaUN3ZLZyTwuVmU+Cplhv2yeEEEIIIeI+dP3113+gPigiZs6cyVtvvaU+LISY4iZb3Y90kI/wj19fL874T/9dtLnLsIUG2Trm8m3FNHSvpUjdBxKTcI1cVxttI70/yWnj8uvo2liCJfEYAD5644N42u9Bs+ImetYWYIqXS7RM1P8fu3aei7ZYp0kKBV9v/fCetCPlKejDP92GlcT7zULeSMif+ngCX+/wbBBX237K0mYuyGBrddKAy/ikVZVZOinPaBR60o7E1Ya7bKTu4uS86Y11zXUzXT7yFtL8+AocZggOtFKxuT/6hzpiJ5q3xGceUUxTz1oKEmNSV/yCsbKF7sV2wgPrR58xouceJlN9S3lml6gtMZbT0r0ce8p1gwRDZsyJaUeNdTJvf0dtdxR8vTXUJGzwpzl2ihvoXls04gBC0v3qyduoaVPbM810lgOM8qyTnsUl/uzWG+t6nrG0D9I+ZNg+aI5fSC1vdVoVzZ/deuJXV/nGzKe5ZzV5QT9BqxXlQDUrh9d/jtLxLHSWg2Z64ixmpDjW3FaTedosxWTsHkKDW5P3xM1bQ9c/zsNCgL5Hq6L720afRcKfJ4nGWe6aLjrmWQiO9N5GF217yrApXpyLeiNxlz5jEPKyt7GW3UPgqOuiucSSJnZjojFsipWbtvtNlvw3Ke+lt50cKWbStX1CCCGEmBQCZ36HZda16sMXZLL16V8MMgNYCCEmuaHOGu7fegBvIIQSP6oQ9A+wqzPNMl+aHGFzdT27BvwEhy+a1qnOGjoPJ6cLBbz0tbczMNIymse3se2pAfyjXlz7PWTNUCc19U8x4A8mlG0kfwe23p88kHl8G4+2D+APxVPhH9xFffVeTg+nipoAeQM66xtT7iEU8HJgU+oAyIWmVYKR/YNHHfy9FAb7GPD4CcY3Oma4/tQn501vrF9Q3Rx6lvpNvfgUMBetpqsuNhM4S7GjK36hstCOQfHStz1Nh2SmpnJ9y1bewvtobO/Dn7ApXsg/yK76ag6nJNZDR5kdaaS9d1DVnisJeUsesNAcO3bLKIO/4y19nddFZzmA1s9CPbQ/N73tmR6an7Ee2apDOsosa7KVtyncPmQzfi/os3tcHWSvJ4jBasWieDm6O00boudZZEsmcTbubZ8OWYrJEQ1tZ9dgdPZqmuWlR1PusABBvAdHeO9wJx5fZBno9BRCAR+Dva04l0YGfwFmGI1AiKBXnT4mtrz4heikdyAaFCEvg4fV53XS0/YJIYQQQog4mQE8CvnFgBCXJ6n7QggxivwGujcWMd3TztJ61XqUQoxmIsTOiLP2xLiYCM9YTE4SO2KikZgUQgghhMgamQF8ccgMYHEZM7Jk237cvd2s+4L6nBBCCCHSKV9WgJkgHvVmhEKMQWJn6pNnLDIlsSMmGolJIYQQQggx2ckM4FFMhV8MWG+7gum//gO+M+ozAqxUtT7BvbYwLz5RwZYfqc+Ly9VUqPtCCCH0GGN/O5WUPf7E5CEzgIVu0j4IIYQQQgghxHiSGcAXh8wAnuTuf+JWnnvuVp7711l8PnrMeJuRxp2f5LnnbmXH5lt44nu38twP/owdD1+h+uvLnZ+uRxbhLJPBXyGEEEIIIYQQQgghhBBCCDE1yAzgUUyGXwzc/8St3GsD3n6Tlr87w4+NRr71Lx/DbogmUP4AhiuA83j/9ec81qO6gBAixWSo+0IIIYQQQgghhBBCCCHEZCMzgC8OmQE81XxpRnTw9zz+537O3X/7C+6++zVWPfFLnnlOnVgIIYQQQgghhBBCCCGEEEIIMZXIDOBRTIZfDKTMAH7gRp4ruyYyAHzAx2M7/0BY/Ue62Ln3Hx5m0Wwr5isjR5Sglx/+Uy1dL8fSGJnzYBNVX7BjMUaOhANe/uM7jXQMxN59LhuermX2mWeo/bGVh780G6sR/Cf9WG+y4j+wkpU7/LELRny8mp3tTizePVTUdhMG7H+7jofvmY3VHJnirAT9HPvBE2z5N2/8z+au30PtZ3/DM7UvYF2zlNm5RvA9g7OmK+HiqrTOh4mdNRZV0/TA32CbZcQwDTgfJjDQTdU33aq/FlPVZKj7QgghhBBCCCGEEEIIIcRkM9VnAFutVu644w4MhthSvdq9/fbbeL3D410A7733HkNDQ5w/fz7p+FhkAHgUEylgRpIyAJw3g++03IAlliB4lkP/9ibf7/0DweQ/1cDIkpZuKuwQePkF/vOUAuZP8plPW/A/WcGGH0XS3Lm+g5rPmgn/8hg/ffU3KFdZ+cznbsdyZYAXNlbR8hLDA8BKgAC/4dA/bWHPq2EwVtDSvQT7W4dY6WojcQjY+lAXO/+XiVd2LKHhANgfeIIt99wMZ7wcG/hvfst13Pr5Odx8jYL3+xXU9kQGmyODugqBAPzm/7SwZe8rIw6CpwwAf7aWrvVzsbx9ghd//Bq/xcD1t32G2coLOB9JHUAWU9NkqPtCCCGEEEIIIYQQQgghxGQz1QeAW1tbueWWW9SHM/bHP/6RH/7whzz55JPqU6OSAeBRTKSAGUnKADBgXzSL2i//CZbojF0Azpzhu998k2eGEo6NqYon3Pdy8y/dLFndMTyIajRjJkgwDHxhA3u+NhuOtXH/hkPDaezV7NzixOLrZlHtnuEB4GuCvLixgi0vxd+EJS37qbAHeeHrVbTEZxXfTm3XZuZedYyWZRt44eNVPNF6L9Y33Kxb3UH89w/GO9nQWcPsd1+goaqFV+KDukaCP9lAxTePxd8nHfUA8JyGbtYVGTi2fQkb+obTmWeZCZ7RP4QuJqfJUPeFEEIIIYQQQgghhBBCiMlmKg8A33jjjWzcuJH333+ftWvX8vvf/z7p/FVXXcUtt9zCFVdckXR8JAUFBdx111309vbyve99T316VLIH8BTk3X+GB5Z7adv/Jv63o+P7s2Zxn8tIdIVmjQKEwsANt1JxW8JfhqODv8C9827DSICffi9h8BfA280rb4DhT29lbuLxt09wLGHwF2DPj14jjIXb/9fs4YOfvYvbLRB81c0LgHXhHG42KLz2fMLgL0D4EC/+PAwWKwl/DYQ5cWz0wd90/MEQYOTmzzkxJxyXwV8hhBBCCCGEEEIIIYQQQggxErPZzJVXXkk4HE4Z/AV49913efXVVzl+/Lim14c//GE++OADTp8+rb7UmGQAeJIzTIv+x3vnk5d4Dn/A8987w6q/+wWH3oim/biJOxPTjMlN93NewtNuxrllD3u6Wqi5Z3bSwOh1JgNg4c52N2534msPzo8D15i5OSE9wd/w08T/BzjwPK+9DWb7nfFB3LlfvB0zfn76vyODuDebTYCB2x9Qv4+bmtlG4HqsX0i86G/5zUDi/2vj3/0ML7yhYJ5dTXdvNzvXV3Fnrr5hcyGEEEIIIYQQQgghhBBCCHF5ueGGG7jyyisJBsdnUmFOTg6KovDGG9GBPh1kAHgSMkbHI423XcNtN0T+WwkqvArw8Sup/spHsMbGLI0f4iOxP3z3HIHYf2vk/X4tS6o2sOcnJwiZ7Nz5wAa6d63jzsQxUcXPi8+5cad9vcArCUk5fy7Nfrwv4H41CLNu5c7PAji54y+MKN4X6f5lYrog3n9XX3/49eKJxLQK51LfaGzhQ7S4Kli53c0rb4D1s/dS09HNEw/Y1SmFEEIIIcQEk+tqY7/bjbu7gVL5DZ8QYoKRNkq/qVxmkzVv5c09uN1uuhtK1aeEEEIIIS57ZrOZadOmZTRjN52cnBzC4TBnzpxRnxqTDABPOh/i/tZbeW7vn9Gz+UasBoDz+I5FRjuNd8zkrkU2dvTcynN7b+G5nlv4/A3RNId/x4uqq2ly5hjd33yYqiUVtPwogDJrDlWPRhZ2DikKGAyE/k8HHU+mez2DloWYj/3v/ySAmdu/OBfuKeJWY5jXftQdHywOvhtZmvl9v/r6sVc3h5IGiy9EGH9fBw3VFSxZ1433bQM337OSqkn0DzIhxETios3txt3TRLH6lLj0XG243W7aXOoTF1FxEz1uN+5LehMj0RG/xkpa9rtx71ylPnMR6bjfSedC81ZMU49qJZWMrzXOxjF25jtsGADMDkry1WfFJTOOzzhzF1qHJrILzdvl0T6Mqwy/P0gbpd/YZXaR41dDTOYtbGBn9/4x72nC5U0TFyUOEwDmojIq1aeFEEIIIS5zZrOZDz74gDfffDN+zG63c9tttyWl0+LGG2/k6quvJhwO8/rrr6tPj0kGgCcdA9cZgSujaz+ffx/fcyfZ0BP539nTIfhedN/fK6ObSIff5dW9PtZ953z0GlqZMc9K/P8gLzz5nwSA6ddYAHD/lw8FC3/9lTt17i+s8stn+M9TYLTPpfZzt2J4+zWePzB8+pUfnyCIgVvvqCabc3GNs8xJ+Qi/uodDPw8DJsx/lnBCCHFBHK4Wuvfr7zQTGs3IZ+GaNrrdbtzuHppG6SUqXtVCV0LH0v7unTQszFMnA51pARzz19DS1ROZ2RB9jfbMjaXRgVD32IOhetKKiyPPVYLdoOA9ult9SohRjWfsHPT4UACCHg4fV5+dWC6nz8LxfMbi8jLVYmcytVHZorftm2hlNlZMGhc207SiCKvZoD6VYqLlTZtODntCAAQHeklfCkIIIYQQl6+cnBzOnTsXX7L5xhtv5Gtf+xobNmygqqqKadNi+7qOLbaf8O9+9zvOn9c7vicDwJPQ+zT93Wv8/dd+QcPK17j7Hh8PPzW8rPKPd77O3y/2cvfdXh7++s9ZtfQ17l76PzT8yx/SLL08lkVs6NpD17Z1VD9YTfWDNWzefidWwrz2EzcA4e9/hx/6FIyza+je1cK6B6sjaf9hMzu79vDEA+prjsRP90+8KNfcxhybgeCrbl5IPP3SE3S/FMTwcSctT+9kw5ro+6zZQEtHN90NkRnJo/rCOrrdbva3VmFVn4v6zKo29nQnXP8fnqDq00Z44xXcL6tTCyEyNSM3Fw19IkKvGcW4mnfS8/2NrJhnS9qzPZ2FzT2sXWDHEvkRPwAGs5WiFc20uZIHdvWkxVjImp37aV49D7vFFJnZMBZjOU2rC0i4/Mj0pBUXyXyWF1ogNET/bv3fOMTFcITGpU6cTidO51YGI323E8D4xs6pzhoWOZ04KzbTf+GXy6rL57NwfJ+xyIbLo32YCCZTG5Utetu+scvsYsbv2DG5bJ4DEwqBgad46L7YfTlxLm3kiCrtxMqbdvvql+J0OqnY3K8+JYQQQghx2cvJyeGdd96JzwB+/fXX2bt3L++99x5lZWWsX7+eGTNmqP8srdh+wmfPnlWf0kQGgCep4C/+wKun1EcTfYDvv87jT/uPCK1OcOKUgjlvDs67nTjvvpNbr/RzaEcjDT+IXdhLV30T3T/xE77Gzpy7nZG0sz+J4a2f8vxPVJccRfiZV/ApBgwGPz/93+qFo8Mc2lhDywEvgWlWZs+Lvk/JbVjOn+DQj/5TlT4zJ35+gsA0y/D1P3s9v311D1vWtOFVJxZCiAkmf/UKyhzWSKfT4GG8o3QSGRc2s8xhAoJ49q6PdCzdt569niBgwDbfRXlsz3kdaQHKm+qYZzVAyM9gbyv11UvinV81ncPpErmal0VmUxweZJTbBp1pxcVhrCwlzwSBo7s4qD4pxCgkdqY+ecYiUxI7YqIZOyaLyc0BFB8HNz/Lycz66YQQQgghxCQVW7L5nXfeSdqz9/nnn2ft2rWcPHmS/Px8mpubsdvHXus2tp/wW2+9pT6lyYeuv/766HrBQm3mzJkZF6yYHOau30PtZ3/DM86H6VKfFJetSVn3ZxSz6vHllNgsmKK/qA/5B9m3Yxv7PLEfbLhoc5dh8/XirD9Ked0qyguskVmUIT+DT2+n8dmhhItGlvxdXjI861MJ+uh7aj07jiT3Zhgd83FVllOY8P5KKIDv8C5qd0R/6+5qw11mS/q7VD56nTUkjhFqvQdNipvoWVvA6d5HGcxrYrHdBIqP3vp6fOUdPFJkBiXA4dYqtsV+om90UL5mFWUF1vhsBSXkx7NvB437PIlXh/j92rDECiImNMhW1S//xzVvAPl17FxtpH/7NvZ58mnqWUuBKcTg1qU0qqYcuNrclNkU/AfqWbkj8bnn09C9kSKzgnfXImr36UtLfgPdG4swBwdprW4cYTZDsjxXG81lNsKDrVT3ldC1tgCTrxdnmtFiPWk1icalr3cJncE6VpUXYDUBKAR9fbTX7+BoQh40xXoiLXUzGpfqfMTyalACHG6vYVtCYWqKHVcb7rIcBrdW0+eIzgo3EMmbt5dtjbuJNw9ReuI30aqdbhZYvOytqCVpQozee5gs9W2itCXx+FX/uKI4Uv9JLQdt5yP0lNn8NS2UFyakDfkZOrib+t1H1UmTjBg7sXqRcChJUn2J5icxcZoYgFiZ5eLdVcG+nCZc8fylr/N6jVkOuj8LL/FndyaxrjLiM5b2QdqHTNsHrfELGdUhTZ/dI35/CBHwHKSqPnFhXI1tVOw7VMhD+9L6lAFGY2UL3Yvt4N3Lotrh62t7FhmUgxZa40x326exzFJoi99sxGSElvfPbt60xYMOoz27Eb6DZ1q+QgghhLh8BM78Dsusa9WHL8hE6NP/1Kc+RX19Pb/+9a957LHH1Ke56qqreOSRRygsLCQUCvG9732P559/Xp0s7sEHH+SLX/wiu3btore3V316TDIDWFzWbp5lBOWczCATk1uei7bvrmWBfbiTCsBkLWC5a1liyojpuTR0NLM81ukDYLJSsKKOuvzhZOUt6Zb8tbFg7Xdpc+UOH6SYuobVzFO9v8Fkwb5gLV1rRt4jdiza70GfnMI6yuzRixpslKxpYXVRdMFkg4XCsvLIfxtLaepoZnnRcIcsgMFkpWB5M91NpcMHAVfb/uj9qjpk08hK3o5vY2VVY8Kg/0gWYssFFB/9iQO6M/KpbHLhMAMYyHUU60wLjnk2zCh4e7UN/pK3hroyG4bgAE819o++XYGetDrllHTQvDzWeQtgwGxbQF1TNBZAf6zrrZsJhgd//fRtSx781Rc7JvJWd7B2QWxghUje7ItpqEveHFpP/CaZ30yJFUJD/SN0hmq8h8lW3yZIW5ItesqsvGU/q+ep0pqsOBYvY9QtHseMnZEFAxeyNouB3LIOHk/KX7o6r0/G5aDFJf7s1hzramM+Y2kfspm3bNFTZhnXi1FjR1/8gvY6pPezO/X7gwmLYzFdSRfV6PhmBvyA6SZK5qtPQrnDhoEQQ/3Dg796ngXoKIcpbNxjsriJHrcbt9uN2x0d2DUVsDZ+LPLSuufxhdAdD1mQcfkKIYQQQkwgDzzwQNJ3OfXru9/9Lh/72MfUf4bZbMZgMBAMBtWnACguLubWW2+F6NLQ//3f/61OkiQnJwdFUfD7/epTmsgAsLh8GSu4NRc49RqRHY2FmIzyqasrw2YAJeCht7U6ujzvQ7T2egikdJgB1gKKzAqBwb2sv8+Jc0k9B3wKYCFvngMAY3kLy+wmCHqHr+l00trrJYgBW+lqEvullHAQb99TbH3ovuG0fX4UwOIowwHQWRM/tzW6gZWvN2FfLKcTZ8LsX733oIfJYkHxPsV9rZElhM1WK/h6efTRPgKAwZJHIVBc56LADAQ97N2UULbRvJkLllEXKTKMlS3MtxlA8dPX+lD8fqvr+1B/RGczb9pYMBqA4GmGiMw8mr+mjZ7vb2RxQoegyWzXmRYKcy1AgNPKGlq6ehK+HPXQ1bKKwoSloqGYhsfnYVH8HNi0ecSZDBF60upnMptRAoPx51zdPkgQMNjnsyahv0xTrENmdTNqePDXR2/9SrYnTEfMJHZMJlMkhtdH7nl99H5NthIKY9fVEb9qlaV5mAhwfK96rtIwLfcwGevbpW5LskVfmbkosRtA8bI3oV481NqLZ7RAHyt2jjSyNHqt+OvRXnwKKL5eKjYntgL690jUWue101gOOj8L4y7VZ3eU1lhXG/UZR0n7kJ28ZYu+MtNYL9IYK3b0xC9oq0OZfHabzOa08WtxzE+oE9rbqN1HvSiYyCtZmHzC6KLAboi8V7RI9D2LKE3lkAW62z7tZaZP9mJSu+zkLaN40CLh2cVfW0fahiXz8hVCCCGEmIjOnTtHOBxOeb3zzjucP39enZyZM2dyxRVXcPr06aTjVquVb33rW3z1q1/lj3/8I9/+9rd57LHHOHnyZFI6tZycHN59990RB5THIgPA4vLyhXXsbF1H9YPreKJzCXZDkBd/0DWus8iEuKiKy8i3RJYNa6+pp7M/ujn42ZP0d9ZTVZ/ShQxKgIH2+6lq3M3xs0DYww5P5O+MxsgG9PMLbRgIMtBaO3xNoL+zlr0eBUy55Md7tY6wuaqC2u3PciRho6v+7cc5BWA0om1b+2T67kEnxUf/9mc523+KyMdxgMPtnQwNhSPtwXQDR1nIAocJCNC3qZ7dRxPKdvtKdnlCkc6y0shIwbICOwZCeDpXsr1/+MP7lCfMufj/RWQ1b3qEQ8xY1UJ3dzOr59kwQWRAZK8ntVNHT1qslKyYhz3xp/+YsNgX8HhbHbEJJqVNKygyK/gObidpZek09KTNRMi7l0VVjfHnfOpgY+RZYMEW7y3TEeuZ1E0gr7KFpjIbhpCXvfU1dKrymknsKIHDtFbXs/t45J6Pb+/Hp0TifHo0jZ74TZK7ikK7AcV7mG3H1SeHjX0Pk7S+XeK2JFv0ldkpwiHAkEvB/OHBg5P9ndRX1acOZMZojJ04YylNj5dhCw/SPkL90UNbnY8ufZnm177uniaS59BnWA5aXerPbg2xHmtP4jQ+Y2kfspO3bNFXZhnWizFjR2f8oq0OZfTZHRwYI371Ce/z4FPAkFdC4rx64zIHNiAwuJtYkeh7FlFaygE9bd9kk4WYTPrBUnRANzTIVtWgaZqVksdVRvEw7jIsXyGEEEKICer48eMsWbIk5fXVr36V119/XZ2cWbNmAfDmm28CMG3aNP7u7/6Ob33rW9xyyy289NJLPPzwwxw6dEj1l6lG2k9YDxkAFpeXYAhsc3DePYebp/k59r3NbPmROpEQk4jdjAkIeg5qW24XQDnF4YOqPaCiv+xe2ngEKCTPYgDMFG1M7fhZ4YicsyRMEjAWVtK0s5v9SWnLGGG3KA3034Mupzx0DveLgO8o21MGFaMzXwND9Kecg2d9ke5co/kmoJjcHIDT+MacFJDlvOlhW8DaBXbMBlCCXg5svS8yIOJT1Cn1pSWaprU+4Zf/ffgVwJLP4vlgLG3CVWBG8T5NjXqUU0VP2kydHkrcqy+i3x9QH9Ie65nUzZxSmhbbMSk+ehtr2Z2S1cxi59TRbap7CBBOemx64jdZsasEq2o5ynTGvodJWt8uaVuSLXrL7CCbOgcIYsK2YC1u9366dzazZuHoa4lqjZ0YV/NqCow+ejdpXF5+DFrrvHaZlYNml/qzW1OsJ9P6jKV9yEbeskVvmWVWL7TEjq74RUsdyuyz23d48xjxq1N4N/1DITDYKEwYAa7MtwF+BvfFgkrvs4jSUg5TWvZi8tLKMB7GXWblK4QQQggxVdxwww0pSzbb7XaCwSDNzc1s2rSJj3zkI3zlK1+huro67Wvu3LlAZDnpK6+8knA4zO9///uEd9FOBoDF5eXlNlaWRX+Fu2QlG/7tQvaPE2LiUM5p7KXSZDoGPVMWihvoeHwxBVYzBvW5jOm8h6xS8KgPjURRGHtBjomQtyBKrHMy5KOvvZ5FFbXsOBLpEDQ6ciIdoAGPzrQxfvqqa9nRP3zsZP92Nh8OACaMuZBfkocJMNiXJ3dSrS2ILCttK4sea9OVdjz3FjMbVBGdQazrqpunj9LvUyJ7RS5XLf0I2Y8dTfGbwFhJmcMEgePx5Sgv3FSsbzHjnbds0V9m4f7NVCypp/3AIL6AgtnqYN6Kjbj3t+FKsxWn3tgpbeqmLDdA37b6lFnx4ymlzjPC0pdOJ86ljSlL0esuh3Gl87ll0J7povMZazPedUhnmWXVeOctW/SXme56oSV2shy/uj67s+DgXk9kyd7CysiB3FU4rKB4j7Ij/qMC/c9CFx1t32STlZi85LIcDzroLl8hhBBCiCnkuuuuS1qy+fz582zZsoWvfvWr/OxnPwOgsLCQhQsXpn7Xjr4++clPQnQw+corr8x4+WdkAFgIISa5QDiyz1heqfrMBTjCqdNEliOsTv0Qir1iy5gtXFCAGVD8fbQm7PXkdPbiU11ZO333kB3RgU9LHqvS7Ae50JYDwOlTx4GzhMOAwUyuKm2ey0HyoYmQt334AgAKvv5tbD+Y3O3sKrACCoGhozrTgi8YWa7SVpq02S8AOcZsdNNmz8I8C6AQjk4K1BXrGdXNMJ01i+j1KZgdK+huUv9ttmJHT/wOy60sxG5Q8B5ujy9HmbmpXN+ylbdh5pzkNR3zFi7AlrgCuy4ZllnYw8EdjdRULcW5pJ5dniAYbMx3JS5iGqEndvJcbawugMH22qT9sLNBXeczoqMcxpe+56arPcuAnmc8tmzVIX1llh3Zytuwqdg+ZC1+M/rszoLjmxnwg8HmoNIIueUFaWafZvgssmR84+wiGOeYvPQmVjzoKV8hhBBCiKkiJycn7ZLN7777btJ+wYcOHaK8vByn08kjjzzC+vXrk17PPvssRGcAT5s2LWU/YT1kAFgIISaz/sHIPmOWefS0rWFh4XD3X2FlE13Nmc2HPOj1AxbmNbfgKh19rTBLdFBPOTtEf3QftptKXTTtLB1xGb6z4Ugnvq2kmcr8lF3aQOc9ZEMx+/D4FMDKguZmKmNlOyOfyqYuljtMoHgZfDoMePCcjgx8ljSsoXjGcLrmMlvK7JRLnTeAZ4/7UDBgm99EU2V0WbYZ+VQ2dzPPAoQ89O7Tn7b/6ElCGLAva2ZVdM9CgMLKZh4pMgN+vAfhSOPSlE4pp9OJc+tgZE9hX2/0WI2utJn2axnNxThyI4PWxtxCKpu7WWCN5O1A5HuXvli/gLrZWd/OYBDMBY+kDAJnJ3b0xW9EPpVFVggN0b97PAblpm59y2ZbQlBBAcyOcsodkfgtXdVG0woHZnVaHXSVWXEDO7taWLOwmJtizXnYw+DAKUKAwaC+E+2xk+dqo7ksl1O9m2jUuh6rRsl1vhRXS2qd10V3OWj7LNRDz3PT1Z7ppv0Za5O9OqSnzLJB2gf1nWiLnazF7wV8do+33Ue9KAY7BcvyKHdYIOhJmX2q61lkSwZxNt5tny5ZismJINN4KG3ojqyk09NC5YXO0NVdvkIIIYQQU0dOTg4mk2nMJZsTB4R/8YtfcPz48aRXbMDXbDbzwQcfxPcTzsSHrr/++g/UB0XEzJkzeeutt9SHhRBT3GSr+5EO8jQdf0QHxuI/9XbR5i7DFhpk65jLtxXT0L2WopH+jZ5wjVxXG20jvT/JaePy6+jaWIIl8RgAPnrjg3ja70Gz4iZ61hZgipdLtEzU/x+7dp6LtuYybGkzp+DrrR/ek3akPAV9+KfbsJJ4v1nIGwn5Ux9P4Osd/vW/q20/ZWkzF2SwtTppwGV80qrKLJ2UZzQKPWlH4mrDXTZSd3Fy3vTGuua6mS4feQtpfnwFDjMEB1qp2Nwf/UMdsRPNW+IzjyimqWctBYkxqSt+wVjZQvdiO+GB9VRsHmU+jJ57mEz1LeWZXaK2xFhOS/dy7CnXDRIMmTEnph011sm8/R213VHw9dZQk7ARqubYKW6ge23RiAMISferJ2+jpk1tzzTTWQ4wyrNOehaX+LNbb6zrecbSPkj7kGH7oDl+IbW81WlVNH9264lfXeUbM5/mntXkBf0ErVaUA9WsHF7/OUrHs9BZDprpibOYkeJYc1tN5mmzFJPD0jx/NT33qyetrniIicZF9P9S43kEKe2c6nhi2rjU8hVCCCHE5Stw5ndYZl2rPnxBxrNP/4EHHuCee+7hZz/7Gd/4xjfUp9MqLi6mpqaGl19+mS1btqhP6/b1r38dh8NBS0sLL730kvq0JjIDWAghJrmhzhru33oAbyCEEj+qEPQPsKvz6aS02h1hc3U9uwb8BIcvmtapzho6DyenCwW89LW3MzDSMprHt7HtqQH8o15c+z1kzVAnNfVPMeAPJpRtJH8Htt6fPJB5fBuPtg/gD8VT4R/cRX31XlIX6pgAeQM66xtT7iEU8HJgU+oAyIWmVYKR/YNHHfy9FAb7GPD4CcY3Oma4/tQn501vrF9Q3Rx6lvpNvfgUMBetpqsuNhM4S7GjK36hstCOQfHSt11LZ6hGU7m+ZStv4X00tvfhT9gOJuQfZFd9NYdTEuuho8yONNLeO6hqz5WEvCV39GqOHbtllMHf8Za+zuuisxxA62ehHtqfm972TA/Nz1iPbNUhHWWWNdnK2xRuH7IZvxf02T2uDrLXE8RgtWJRvBzdnaYN0fMssiWTOBv3tk+HLMXkxJBJPHTSOxB9eCEvg4fV53XSWb5CCCGEEFPJzJkzueKKKwiHw+Tn56d93XLLLeo/G1FOTg7vvfceZ89GVj3KhMwAHsV4/mJACDF5SN0XQohR5DfQvbGI6Z52ltar1qMUYjQTIXZGnLUnxsVEeMZicpLYERONxOTISpvoeaQAg+cpFtVnsm+CEEIIIS53U3EG8LJly1iyZAnTpk1Tn8rY66+/zte//vWM9wGWGcBCCCGEEEKz8mUFmAniUW9GKMQYJHamPnnGIlMSO2KikZiMcDV30ewqje/pO+OmUtaUOzCh4PPGtigRQgghhBB79uyhu7sbt9ut+/Xv//7vvPbaa/ziF7+Iv/7rv/6Ljo6OjAd/kRnAoxvPXwwIISYPqftCCHG5Sd4Dbyyhwa0sbUy7s5+Y6GQGsNBN2gchxOXL1eYm7TbEgcOsr9rGZFgcWwghhBATz1ScATwRyQxgIYQQQgghhBBCCCFEkqef3otneONxUIL4B3ZRXyODv0IIIYQQE53MAB7FeP5iQAgxeUjdF0IIIYQQQgghhBBCCCHG30SfATxVyAxgIYQQQgghhBBCCCGEEEIIIYSYImQAWAghhBBCCCGEEEIIIYQQQgghpggZABZCCCGEEEIIIYQQQgghhBBCiClCBoAvS0bmPPgE3b1u3G433Q1z1AkuP1/YwB63mz3r56rPCCGEEEIIIYQQQgghhBBCCDFpyADwZci4tInau2/GeOYVDj33Iq+dUacQQgghhBBCCCGEEEIIIYQQQkxGMgB8GVr6V3YMnOCHNQ20PbmFLU++qE5y0dz+lc107WmhSn1CCCGEEEIIIYQQQgghhBBCCKGbDABfdm7HfA3wdpATYfW5i89s/SQW43T1YSGEEEIIIXTLdbWx3+3G3d1AqVF9VgghLi1po/SbbGU22e4328qbe6Jbj5WqTwkhhBBCiCyTAeCJxD6b2bPUB8dgn8tcu/rgaMyYrlIfE0IIkT0u2txu3D1NFKtPiUvP1Ybb7abNpT5xERU30eN2476kNzESHfFrrKRlvxv3zlXqMxeRjvuddC40b8U09bhxuxNeGV9rnI1j7Mx32DAAmB2U5KvPiktmHJ9x5i60Dk1kF5q3y6N9GFcZfn+QNkq/scvsIsfvGDE59v2Ohwut8xeLixKHCQBzURmV6tNCCCGEEBNUTk4O+fn5fOxjH1OfmlRkAHjCuJMN6zewoXUDTq2DwPYKWppqqX2sljnqc2nMXb8Ht7uW2dcA18ym1u3G7d7Dhi8ADzwR+e95c6hu7Y78o+npDcyN/bHxdpb8w0669yX8o2pfNzv/4V6Sx5+reMLtZs/6uZg/X80T3fvj6fd0rBvO2xc2sMftpvazRuBm7o1dsy1hMWjjHKq3dbGnN3qudw9d26qZk/QrWo3vF2dm7qoWuvYM56O7vRbnlep0Qohscrha6N6vv9NMaDQjn4Vr2uh2u3G7e2gapWeoeFULXQmdZvu7d9KwME+dDHSmBXDMX0NLV09kFkT0NdozN5ZGB0LdYw+G6kkrLo48Vwl2g4L36G71KSFGNZ6xc9DjQwEIejh8XH12YrmcPgvH8xmLy8tUi53J1EZli962b6KV2VgxOdHu99Lq5LAnBEBwoJf0JSaEEEIIMfEsXLiQjRs3UlmZ2U/YrFYr999/P9XV1bpfy5YtIz8/P+n153/+50ybNk39NmOSAeAJ4xDf+qabE8bZVGsZBLZX0NK0BDte9nyrBS27+J540Y37uRfxvwe85+fF59y4n3Pz4onhNNYvP8ztv+yiwunEuWwDLwAY72Rd+2YqPmfFEDjGoeci1/GGjFg/V8WWtirVIDBguZe2r/0N/P8ORd7jF2GMuXOo3lSNFeDEi5Hjv1SAIK9E78X941cif2+8kw0d63D+uYnfDkaucejVEOY/d7KurZbZqrcb8/0AMHLn+jZqF9gxv+uN5v9FAsY5VD9wG7IQtRAXz4zcXMwG9VFxwWYU42reSc/3N7Jing2z+rzKwuYe1i6wY4n8MB8Ag9lK0Ypm2lzJA7t60mIsZM2EHDirAAD/9ElEQVTO/TSvnofdYorMghiLsZym1QUkXH5ketKKi2Q+ywstEBqif/cE2GNCpHGExqVOnE4nTudWBiP9sRPA+MbOqc4aFjmdOCs203/hl8uqy+ezcHyfsciGy6N9mAgmUxuVLXrbvrHL7GLG79gxOfb9Xl721S/F6XRSsblffUoIIYQQYsr62te+xqJFi6LfUfW9li1bxsaNG5Ne3/zmN3nggQfUbzMmGQCeQMKvdrBug4ZB4MTB38Zaur3qBOn5+7rpePJFAgqgBHjxyQ46nuzm0C9jKYyYg25qt79AMOHv5j5axZxZCid+UMuS1Rtoe7KDjie3ULu8graXghhsd/HAfcmb2xg/fh0n/vl+Hv5mBx1PdrDlkUYOvQHkfoYlnwZ+eYjuJzt4MXAO+C2+JyPpOv7tWPw9Z5vDHNt+Pys3ttHxZAdtX69i3XN+FMscli5Nerux3w/gC49R9Vkziu8Z1i2vZUs8H1Xs8aFtgEIIISaw/NUrKHNYMaEQGDyMd5QOMOPCZpY5TEAQz971kS8Z961nrycIGLDNd1Eebdr1pAUob6pjntUAIT+Dva3UVy+Jf4mp6RxOl8jVvCwym+LwIKPcNuhMKy4OY2UpeSYIHN3FQfVJIUYhsTP1yTMWmZLYERONxKQQQgghhBjLjTfeyDXXXMOvfvUrvvzlL6cM8C5evJh169axfv16Ta/e3l7++Mc/oiiK+q3G9KHrr7/+A/VBETFz5kzeeust9eHss1fxxJZ7uTl8jI5HNuA+k3juXjY3VHG7Qd/g77C5bHi6ltkcoyU2w5foEtD33Iz/uSWsfDLxZ6r3snlfFbeHXmTD8i1EhmcTGKt4Ys+93PyLZ3A+0hVdkvlebv6lmyWrO0i80u2PdbH58yaObV/Chr7Isbnr91D72d/wjPNhuuIpo+8ZPMRKVxv+4UuAsZqde5xc91ILSza+oOv97tywh5rZCi9urGDLSwkJAeZtYM+a2RC/rricXbK6fyFmFLPq8eWU2CyYor9mCPkH2bdjG/s8sZrhos1dhs3Xi7P+KOV1qygvsEZmUYb8DD69ncZnhxIuGlnyd3nJ8KxPJeij76n17DhyNimd0TEfV2U5hQnvr4QC+A7vonbHkcgBVxvuMlvS36Xy0eusIXGMUOs9aFLcRM/aAk73PspgXhOL7SZQfPTW1+Mr7+CRIjMoAQ63VrEtetsYHZSvWUVZgTU+W0EJ+fHs20HjPk/i1SF+vzYssYKICQ2ydWkjscsy3nkDyK9j52oj/du3sc+TT1PPWgpMIQa3LqUx8Y0BV5ubMpuC/0A9K3ckPvd8Gro3UmRW8O5aRO0+fWnJb6B7YxHm4CCt1Y2aZj7kudpoLrMRHmyluq+ErrUFmHy9ONOMFutJq0k0Ln29S+gM1rGqvACrCUAh6OujvX4HRxPyoCnWE2mpm9G4VOcjlleDEuBwew3bEgpTU+y42nCX5TC4tZo+R3RWuIFI3ry9bGvcTbx5iNITv4lW7XSzwOJlb0UtSRNi9N7DZKlvE6Uticev+scVxZH6T2o5aDsfoafM5q9pobwwIW3Iz9DB3dTvPqpOmmTE2InVi4RDSZLqSzQ/iYnTxADEyiwX764K9uU04YrnL32d12vMctD9WXiJP7sziXWVEZ+xtA/SPmTaPmiNX8ioDmn67B7x+0OIgOcgVfWJi91qbKNi36FCHtqX1qcMMBorW+hebAfvXhbVDl9f27PIoBy00Bpnuts+jWWWQlv8jn9M6rhfvW2f1jofpSUeXG37KbMZCHmeYmn9s8N/bCylqeMRCswKvt56ajp1xsRoz3mE7+uZPgshhBBCTG6BM7/DMuta9eELMp59+g888AD33HMPP/vZz/jGN76hPj2qT33qU9TX1/PrX/+axx57TH1atwcffJAvfvGLfOc73+GHP/yh+vSoZAbwROTt4uF1z6TOBL7gwd+xhAmcUPd4XYfpSlB+/Vrq4C9A+ATBt4FZlqR9iMMBb9JgLMArwRBgxPwJ1YkUkffkhjvZmbBvpNvtxr3HiRUwzro56S+0vJ/1OiO89yteUw/+AvxRfUCISSTPRdt317LAPtxJBWCyFrDctSwxZcT0XBo6mlke6/QBMFkpWFFHXf5wsvKWdEv+2liw9ru0uXKHD1JMXcNq5qne32CyYF+wlq41I+8ROxbt96BPTmEdZfboRQ02Sta0sLooumCywUJhWXnkv42lNHU0s7xouEMWwGCyUrC8me6m0uGD0c6UyP2qOmfSyErejm9jZVVjwqD/SBZiywUUH/2JA7oz8qlscuEwAxjIdRTrTAuOeTbMKHh7tQ3+kreGujIbhuAATzX2p7TlSfSk1SmnpIPm5bHOWwADZtsC6pqisQD6Y11v3UwwPPjrp29b8uCvvtgxkbe6g7ULYp2LRPJmX0xDXfLm0HriN8n8ZkqsEBrqT+mgj9B4D5Otvk2QtiRb9JRZect+Vs9TpTVZcSxexqhbPI4ZOyMLBi7ki7CB3LIOHk/KX7o6r0/G5aDFJf7s1hzramM+Y2kfspm3bNFTZhnXi1FjR1/8gvY6pPezO/X7gwmLYzFdSRfV6PhmBvyA6SZK5qtPQrnDhoEQQ/3Dg796ngXoKIcpLDsxqZfGtk9nndcaD531T+NVwORYTkvCMj6ldcspMIPifVr/4G8GMn4WQgghhBAT2A033MCVV15JMJi4zm7mcnJyUBSFN954Q31qTDIAPFHFBoGvig4C3+JkQ0MVt/MKXVkZ/I2aQAOhyqnIPsFpX7G9gvVSzo3rgIEQl14+dXVl2AygBDz0tlZHl+d9iNZeD4F0AW8toMisEBjcy/r7nDiX1HPApwAW8uY5ADCWt7DMboKgd/iaTietvV6CGLCVriaxX0oJB/H2PcXWh+4bTtvnRwEsjjIcAJ018XNbo5tz+XrV+xwMz/7Vew96mCwWFO9T3NcaWULYbLWCr5dHH+0jABgseRQCxXUuCsxA0MPeTQllG82buWAZdZEiw1jZwnybARQ/fa0Pxe+3ur4veSWDLOdNGwtGAxA8zRCRmUfz17TR8/2NLE7oEDSZ7TrTQmGuBQhwWllDS1dPwo94euhqWUVh0o4BxTQ8Pg+L4ufAps2pMySS6Emrn8lsRgkMxp9zdfsgQcBgn8+ahP5TTbEOmdXNqOHBXx+99SvZnjAdMZPYMZlMkRheH7nn9dH7NdlKKIxdV0f8qlWW5mEiwPG96rlKw7Tcw2Ssb5e6LckWfWXmosRuAMXL3oR68VBrL57RAn2s2DnSyNLoteKvR3vxKaD4eqnYnNgK6N//UWud105jOej8LIy7VJ/dUVpjXW3UZxwl7UN28pYt+spMY71IY6zY0RO/oK0OZfLZbTKb08avxTE/oU5ob6N2H/WiYCKvZGHyCaOLArsh8l7RItH3LKI0lUMW6G77tJeZPtmKSf33q6Xt01PndcVDeB+N7YMEMWBf1owrF4ylTbgKzBAcpL1xX/LFtUp4zvHX1pG2bMn8WQghhBBCTGRms5lp06Zx+vRp9amM5OTkEA6HOXMmcalgbWQAeCLzdvHw47FB4Gpm8wpdmxt4JluDv2n9ltB7YPjTW5mtPgVgvBnzNaAETvCi+lzGQpxTwDAtxA9jewOrX9G9gvUIKQpcY8X+cfUZ4JrpTFcfE2IyKC4j3xJZ/qu9pp7O/lOR42dP0t9ZT1V9ShcyKAEG2u+nqnE3x88CYQ87PJG/MxpnADC/0IaBIAOttcPXBPo7a9nrUcCUS368V+sIm6sqqN3+LEdODi8t1r/9OKcAjEYiV9VH3z3opPjo3/4sZ/tPEfkoDnC4vZOhoXDkRyLTDRxlIQscJiBA36Z6dh9NKNvtK9nlCUU6y0ojIwXLCuwYCOHpXMn2/pPxtzrlCXMu/n8RWc2bHuEQM1a10N3dzOp5NkwQGRDZ60ntqNGTFislK+ZhT/w5PyYs9gU83lZHbIJJadMKiswKvoPbSVpZOg09aTMR8u5lUVVj/DmfOtgYeRZYsMV7y3TEeiZ1E8irbKGpzIYh5GVvfQ3qyReZxI4SOExrdT27j0fu+fj2fnxKJM5jn3164jdJ7ioK7QYU72G2HVefHDb2PUzS+naJ25Js0VdmpwiHAEMuBfOHBw9O9ndSX1WfOpAZozF24oylND1ehi08SPsI9UcPbXU+upylekUatxt3TxPJc7QyLAetLvVnt4ZYT/kurfEZS/uQnbxli74yy7BejBk7OuMXbXUoo8/u4MAY8atPeJ8HnwKGvBIS59UblzmwAYHB3cSKRN+ziNJSDuhp+yabbMWkfmO3ffrqvN54CPc3sumAH8VgY35dM02uAkyKj95NGlfxuWAZPgshhBBCiAnObDbzwQcf8Oabb8aP2e12brvttqR0Wtx4441cffXVhMNhXn/9dfXpMckA8ETn7eLhxzt45rln6Ljog78AzzDwWhhmzabigcjsrmFG7nx0Ljej4DvmVp3T4zosn0v8fzev+BS44a+pmpc0VeyCuL1+wMJff+VOkq5qvJ2au25n7AWVhJiA7GZMQNBzUPs/1JVTHD6o2p8t+mvtpY1HgELyLAbATNHG1I6fFY7IOUvCJAFjYSVNO7vZn5S2jBF2gNJA/z3ocspD53C/CPiOsj1lUDE68zUwRH/KOXjWF+nONZpvAorJzQE4jS/dpIAkWc6bHrYFrF1gx2wAJejlwNb7IgMiPkWdUl9aomla6xN+zd+HXwEs+SyePzzLQMsSc3rSZur0UOJefRH9/oD6kPZYz6Ru5pTStNge6XxrrGV3SlYzi51TR7ep7iFAOOmx6YnfZMWuEqyq5SjTGfseJml9u6RtSbboLbODbOocIIgJ24K1uN376d7ZzJqFo68lqjV2YlzNqykwjl/HtNY6r11m5aDZpf7s1hTrybQ+Y2kfspG3bNFbZpnVCy2xoyt+0VKHMvvs9h3ePEb86hTeTf9QCAw2ChNGgCvzbYCfwX2xoNL7LKK0lMOUlr2Y1Gvstk9Pnc8sHoZ2rOSgT8Fgc2A3KfgOtqf8+DB7MnsWQgghhBATXU5ODufOnYsv2XzjjTfyta99jQ0bNlBVVcW0adPUfzIis9nMlVdeye9+9zvOnz+vPj0mGQCeDLxuup7swn3RB38j3N/s4ljQwM33tLCnfQM1D1ZT/eA6WnZ1U/NZM8GXOmjs0fgvZJX//PVvADOz79tA9YM1tDRUAWG6v/NDTihGZq/ppnvbOqofrKb6wWrWfWMnXXueoEp9IQ3C33mGF4NgnF3Dd2P5WLOBnZ2b+cy7flkaWkxqyrnxjODpGPRMWShuoOPxxRRYzeP4Qwqd95BVCh71oZEoCmPv7jAR8hZEiXUwhXz0tdezqKKWHUciHYJGR06kAzTg0Zk2xk9fdS07+oePnezfzubDAcCEMRfyS/IwAQb78uROqrUFkWWlbWXRY2260o7nfmFmgyqiM4h1XXXz9FH6fUpkr8jlqqUfIfuxoyl+ExgrKXOYIHA8vhzlhZuK9S1mvPOWLfrLLNy/mYol9bQfGMQXUDBbHcxbsRH3/jZcabbi1Bs7pU3dlOUG6NtWn9WO6ZQ6zwjLWTqdOJc2pixFr7scxpXO55ZBe6aLzmeszXjXIZ1lllXjnbds0V9muuuFltjJcvzq+uzOgoN7PZElewsrIwdyV+GwguI9yo74jwr0PwtddLR9k01WYjKbNNX5zONhevzvDJhzM9oDIWO6n4UQQgghxCSQk5PDO++8E58B/Prrr7N3717ee+89ysrKWL9+PTNmpKxZlFZsP+GzZ1U/4tRIBoDF2MKH2FC9hT0v++GG2dx5txPn3XOwTQtwbO8WqjceynjwNPydnez5f0EMubNx3n0n1iujC4l6u1i3oZsXfxnGmDcH591OnHc7mX2zgeDA8/xUfSFNXmBL9Rbc/y8AudF8lNwMr3ax+QcXMuNDiEsoEI7sM5ZXqj5zAY5w6jSR5Qir03T8RF810XW5Fi4owAwo/j5aE/Zvcjp78amurJ2+e8iO6MCnJY9VafpCFtpyADh96jhwlnAYMJhR95vkuRwkH5oIeduHLwCg4OvfxvaDyd3OrgIroBAYOqozLfiCkeUqbaWpKzjkGLPRTZs9C/MsgEI4+hGhK9YzqpthOmsW0etTMDtW0N2k/ttsxY6e+B2WW1mI3aDgPdweX44yc1O5vmUrb8PMOclrfOYtXIAtcQV2XTIss7CHgzsaqalainNJPbs8QTDYmO9KXMQ0Qk/s5LnaWF0Ag+21SfthZ4O6zmdERzmML33PTVd7lgE9z3hs2apD+sosO7KVt2FTsX3IWvxm9NmdBcc3M+AHg81BpRFyywvSzD7N8FlkyfjG2UUwzjGZHXrqfGbxUNrUzQKrgcDhpzgcAHOBi6Y03+GzSsezEEIIIYSY6GJLNr/zzjtJe/Y+//zzrF27lpMnT5Kfn09zczN2u3rF3VSx/YTfeust9SlNZAD4svMCG5Y5cS7bwAuJh7/zME7nEjb8KPFggvCLdH99JUsWDf/jYVHFSjbsflE1+NvFw04nSzYmXT3iOw/jdDp5+DuJB71011XEr7nk63viZ8Kv7mHL6goWlSW857Iqare7GZ4MrfP9wi/SUVfFktg1F1Ww8pvP4P3RBpaMdB0hJrL+wcheUZZ59LStYWHhcFdAYWUTXc2ZzYc8GF0yfV5zC65S9dpxySzRQT3l7BD90X3Ybip10bSzdMRl+M6GIy2HraSZyvz0v3jScw/ZUMw+PD4FsLKguZnKWNnOyKeyqYvlDhMoXgafDgMePKcjA58lDWsonjGcrrnMljI75VLnDeDZ4z4UDNjmN9FUGV1qbUY+lc3dzLMAIQ+9+/Sn7T96khAG7MuaWRXdsxCgsLKZR4rMgB/vQTjSuDSlU8rpdOLcOhjZU9jXGz1Woyttpv2cRnMxjtxIh5cxt5DK5m4WWCN5O/BsJI2uWL+AutlZ385gEMwFj6QMAmcndvTFb0Q+lUVWCA3Rv3s8BuWmbn3LZltCUEEBzI5yyh2R+C1d1UbTCgdmdVoddJVZcQM7u1pYs7CYm2LNedjD4MApQoDBoL4T7bGT52qjuSyXU72baNS6HqtGyXW+FFdLap3XRXc5aPss1EPPc9PVnumm/Rlrk706pKfMskHaB/WdaIudrMXvBXx2j7fdR70oBjsFy/Iod1gg6EmZfarrWWRLBnE23m2fLlmKyezQV+f1xkPkB1ZmCBymfduzbGs/TAATBaubR5x9W9rQHVl1p6eFyhHSaKb7WQghhBBCTHyxJZvD4TC///3vk875/X7+4R/+gYGBAW688UbWr1/PHXfckZRGLbaf8G9/+1v1KU0+dP3113+gPigiZs6cmfHIuhBi8ppsdT/SQZ7aCQDRgbH4T71dtLnLsIUG2Trm8m3FNHSvpWikf3cnXCPX1UbbSO9Pctq4/Dq6NpZgSTwGgI/e+CCe9nvQrLiJnrUFmOLlEi0T9f/Hrp3noq25DFvazCn4euuH96QdKU9BH/7pNqwk3m8W8kZC/tTHE/h6h3/972rbT1nazAUZbK1OGnAZn7SqMksn5RmNQk/akbjacJeN1F2cnDe9sa65bqbLR95Cmh9fgcMMwYFWKjb3R/9QR+xE85b4zCOKaepZS0FiTOqKXzBWttC92E54YD0Vm0eZD6PnHiZTfUt5ZpeoLTGW09K9HHvKdYMEQ2bMiWlHjXUyb39HbXcUfL011CRshKo5doob6F5bNOIAQtL96snbqGlT2zPNdJYDjPKsk57FJf7s1hvrep6xtA/SPmTYPmiOX0gtb3VaFc2f3XriV1f5xsynuWc1eUE/QasV5UA1K4fXf47S8Sx0loNmeuIsZqQ41txWk3naLMWkrnvQEzsjlVW6Oq8nHvLW0PWP87AQoO/Rqvj+5Pl1XWwssUBwkNbqRtUexdEYiv5f6v2PIKVNVB1PTBuX+iyEEEIIMbUEzvwOy6xr1YcvyHj26T/wwAPcc8896sNxp0+fZsOGDfzqV79KOl5cXExNTQ0vv/wyW7ZsSToHcOedd1JRUcG1117L0NAQO3bs4OTJk+pkcV//+tf51Kc+xdatWzl+fJTvoyOQGcBCCDHJDXXWcP/WA3gDIZT4UYWgf4BdnU8npdXuCJur69k14Cc4fNG0TnXW0Hk4OV0o4KWvvZ2BkZbRPL6NbU8N4B/14trvIWuGOqmpf4oBfzChbCP5O7D1/uSBzOPbeLR9AH90JXsI4R/cRX31Xk4Pp4qaAHkDOusbU+4hFPByYFPqAMiFplWCkf2DRx38vRQG+xjw+AnGNzpmuP7UJ+dNb6xfUN0cepb6Tb34FDAXraarLjYTOEuxoyt+obLQjkHx0rdd/5fPEU3l+patvIX30djehz9hc8CQf5Bd9dUcTkmsh44yO9JIe++gqj1XEvKW3HmrOXbsllEGf8db+jqvi85yAK2fhXpof2562zM9ND9jPbJVh3SUWdZkK29TuH3IZvxe0Gf3uDrIXk8Qg9WKRfFydHeaNkTPs8iWTOJs3Ns+HbIUk1mjp85rjQdjKU2Pz8MCBPq2xQd/AY5va+dwADAXsDz+3TOmk96B6IMOeRk8rDqtl85nIYQQQghxMb3//vuEw+ERX++88w7nz59X/xkzZ87kiiuu4PTp5G9rVquVb33rW3z1q1/lj3/8I9/+9rd57LHHRh38Jbqf8LvvvkswmPCFWweZATyK8fzFgBBi8pC6L4QQo8hvoHtjEdM97SytV61HKcRoJkLsjDjzSoyLifCMxeQksSMmGonJ8VHaRM8jBRg8T7GoPpM9FoQQQggxFU30GcCZeuCBB7jrrrvYtWsXvb29TJs2jaVLl3L33Xdz5ZVXcuzYMb797W9z9mxkK5vR3HjjjWzcuJH333+ftWvXpiwprYXMABZCCCGEEJqVLyvATBCPejNCIcYgsTP1yTMWmZLYERONxKR+ruYuml2l8T19Z9xUyppyByYUfN7YdiZCCCGEEFPXDTfcgKIo+P3++DG73U4wGKS5uZlNmzbxkY98hK985StUV1enfc2dOxfG2E9YK5kBPIqJ8IsBIcTFJ3VfCCEuN8n72o0lNLiVpY3jtoOiuJhkBrDQTdoHIYTQwtXmJu1WyIHDrK/axiVaSFsIIYQQE9BUnQHc2tqK2WymqakpvrzzVVddhaIo8SWjy8rKWL58OdOnT1f9dcQPfvADvvOd73DHHXdQXV3N4OBg2v2EtZAZwEIIIYQQQgghhBBCiIw9/fRePMMbFoMSxD+wi/oaGfwVQgghxNSXk5PD1VdfzTvvvMOZM2fix999992k/YIPHTpEeXk5TqeTRx55hPXr1ye9nn02sm2G2Wxm2rRpKfsJ6yEzgEcxEX4xIIS4+KTuCyGEEEIIIYQQQgghhBDjbyrOAP7Upz5FfX09v/71r3nsscfUp3V78MEH+eIXvxjfTzgTMgNYCCGEEEIIIYQQQgghhBBCCCEyYDabMRgMBINB9amM5OTkcO7cOd544w31Kc1kAHiCim30LIQQQgghhBBCCCGEEEIIIYSYmGbOnMkVV1xBOBwmPz8/7euWW25R/9mIcnJyeO+99zh79qz6lGayBPQoLuWU8blz5/LCCy+oDwshLoJLWfeFEEIIIYQQQgghhBBCiKlqKi4BvWzZMpYsWcK0adPUpzL2+uuv8/Wvfz3jfYBlAHgUlzJgZABYiEvnUtZ9IYQQQgghhBBCCCGEEGKqmooDwNOmTePee+9l1qxZ6lNjmj59Oh/72Me44oor4sfC4TD/9m//xssvv5yUVg8ZAB7FpQwYGQAW4tK5lHVfCCGEEEIIIYQQQgghhJiqpuIA8EQkewALIYQQQgghhBBCCCGEEEIIIcQUIQPAQgghhBBCiCkh19XGfrcbd3cDpUb1WSGEuLSkjdJPykykU97cg9vtpruhVH1KCCGEEEJEyQCwEEIIkVUu2txu3D1NFKtPiUvP1Ybb7abNpT5xERU30eN2476kNzESHfFrrKRlvxv3zlXqMxeRjvuddC40b8U09bhxuxNeGV9rnI1j7Mx32DAAmB2U5KvPiktmHJ9x5i60Dk1kF5q3y6N9GFcZfn+QNkq/scvsIsfvRI3JCf19cry5KHGYADAXlVGpPi2EEEIIIUAGgIUQQlwKDlcL3fv1d5oJjWbks3BNG91uN253D02j9IAVr2qhK6HTbH/3ThoW5qmTgc60AI75a2jp6onM2oi+RnvmxtJox5WGzis9acXFkecqwW5Q8B7drT4lxKjGM3YOenwoAEEPh4+rz04sl9Nn4Xg+Y3F5mWqxM5naqGzR2/ZNtDKbajE5OXVy2BMCIDjQizwJIYQQQoj0ZABYCCHERTcjNxezQX1UXLAZxbiad9Lz/Y2smGfDrD6vsrC5h7UL7FgiP6AHwGC2UrSimTZX8sCunrQYC1mzcz/Nq+dht5giszbGYiynaXUBCZcfmZ604iKZz/JCC4SG6N8dVp8UE8IRGpc6cTqdOJ1bGYz0m04A4xs7pzprWOR04qzYTP+FXy6rLp/PwvF9xiIbLo/2YSKYTG1Utuht+8Yus4sZv1MvJierffVLcTqdVGzuV58SQgghhBBRMgA8pRiZ8/k5TP5tcT7Nl2prqf3Sp9UnppgLzOdffonaWhelN6hPCCEuV/mrV1DmsGJCITB4GO8oHWDGhc0sc5iAIJ696yOdZvetZ68nCBiwzXdRHv1A0ZMWoLypjnlWA4T8DPa2Ul+9JNop56SmczhdIlfzsshsisODjHLboDOtuDiMlaXkmSBwdBcH1SeFGIXEztQnz1hkSmJHTDQSk0IIIYQQYjL50PXXX/+B+qCImDlzJm+99Zb68EUxd+5cXnjhBfXhUVkWt9BWaSP04w5qvnWIyft71E/zpdpSPvarflr+v5fVJ6eQC8znX36J2nnX8vK/dtL/hvqkuBCXsu5nbEYxqx5fTonNgin6i/qQf5B9O7axzxNrDVy0ucuw+Xpx1h+lvG4V5QXWyCzKkJ/Bp7fT+OxQwkUjS/4uLxme9akEffQ9tZ4dR84mpTM65uOqLKcw4f2VUADf4V3U7jgSOeBqw11mS/q7VD56nTUkjhFqvQdNipvoWVvA6d5HGcxrYrHdBIqP3vp6fOUdPFJkBiXA4dYqtkVvG6OD8jWrKCuwxmcrKCE/nn07aNznSbw6xO/XhiVWEDGhQbYubSR2WcY7bwD5dexcbaR/+zb2efJp6llLgSnE4NalNCa+MeBqc1NmU/AfqGfljsTnnk9D90aKzAreXYuo3acvLfkNdG8swhwcpLW6cYSZGsnyXG00l9kID7ZS3VdC19oCTL5enGlGi/Wk1SQal77eJXQG61hVXoDVBKAQ9PXRXr+Dowl50BTribTUzWhcqvMRy6tBCXC4vYZtCYWpKXZcbbjLchjcWk2fIzor3EAkb95etjXuJt48ROmJ30SrdrpZYPGyt6KWpAkxeu9hstS3idKWxONX/eOK4kj9J7UctJ2P0FNm89e0UF6YkDbkZ+jgbup3H1UnTTJi7MTqRcKhJEn1JZqfxMRpYgBiZZaLd1cF+3KacMXzl77O6zVmOej+LLzEn92ZxLrKiM9Y2gdpHzJtH7TGL2RUhzR9do/4/SFEwHOQqvrERWk1tlGx71AhD+1L61MGGI2VLXQvtoN3L4tqh6+v7VlkUA5aaI0z3W2fxjJLoS1+xz0mdX62aI/fKC0xqfP7pK57MDoiMeOwxtMmUT0bbTGpw2jxM8K/AzQ/Y63tr97PLCGEEEKMKnDmd1hmXas+fEEmZZ9+lskM4CkksLeRrh8HMX++mrbH7pwCM4GFEJrkuWj77loW2If/8Q5gshaw3LUsMWXE9FwaOppZHuv0ATBZKVhRR13+cLLylnRL/tpYsPa7tLlyhw9STF3Dauap3t9gsmBfsJauNSPvETsW7fegT05hHWX26EUNNkrWtLC6KLpgssFCYVl55L+NpTR1NLO8aLhDAMBgslKwvJnuptLhg4CrbX/0ftP1jCTLSt6Ob2NlVWPCoP9IFmLLBRQf/YkDujPyqWxy4TADGMh1FOtMC455NswoeHu1Df6St4a6MhuG4ABPNfaP/uMlPWl1yinpoHl5rPMWwIDZtoC6pmgsgP5Y11s3Ewx31vnp25Y8+Ksvdkzkre5g7YJYJxWRvNkX01CXvDm0nvhNMr+ZEiuEhvpTOugjNN7DZKtvE6QtyRY9ZVbesp/V81RpTVYci5cx6haPY8bOyIIBr/qQDgZyyzp4PCl/6eq8PhmXgxaX+LNbc6yrjfmMpX3IZt6yRU+ZZVwvRo0dffEL2uuQ3s/u1O8PJiyOxXQlXVSj45sZ8AOmmyiZrz4J5Q4bBkIM9Q8P/up5FqCjHKaw7MQkaP9s0Rm/OmMy0cjfJ/Xdg6u5KRIzGpod3TGZBZqfsc72V/NnlhBCCCHEBCEDwFNKmEPfqqFDBoGFuIzkU1dXhs0ASsBDb2t1dHneh2jt9RBI1zlhLaDIrBAY3Mv6+5w4l9RzwKcAFvLmOQAwlrewzG6CoHf4mk4nrb1eghiwla4msV9KCQfx9j3F1ofuG07b50cBLI4yHACdNfFzW6Obc/l6Y/t1xV7Ds3/13oMeJosFxfsU97VGlhA2W63g6+XRR/sIAAZLHoVAcZ2LAjMQ9LB3U0LZRvNmLlhGXaTIMFa2MN9mAMVPX+tD8futru/Dr3r/bOZNGwtGAxA8zRCRX77PX9NGz/c3sjihQ9BktutMC4W5FiDAaWUNLV09uN3u6KuHrpZVFCZ9MBXT8Pg8LIqfA5s2jzhLI0JPWv1MZjNKYDD+nKvb///s3X98W9V9+P8XJBFQCWJhZgWw2BBlFvtMUGza2gy76RzoEtQYModkGZkDRqmTFOMU41Qki3Ga4CZ4czB1YnDdJjXL1yxZWlE1aam9ZgmtUxqHMm3FHkXZkIEq/FCgEj8uJHz/uJItXf/SVazYMe/n46HHA59zdHXOuedehfvWOaeHEGCwz6Uq7llVUmMdUrs2owYf1vnxuFewNW7KSCpjx2QyqWN4vVrn9dH6mmxF5MeOq2P8apUV52AiyNHd2rlKg5Kpw9l4vU30vSRd9PWZiyK7AZRedsddF/c2evCNNtDHGjuHalkcPdbA634PfgUUv4elm+LvAvr3f0z2mk9ekv2g87twwER9d0clO9a1Rj3HUXJ/SE/b0kVfnyV5XQxjrLGjZ/xCctdQKt/dJrN52PFrccyNuyaSv0ftPNyLgomcovmJGUYXeXaD+lnRLtF3LqKS6oc00H3vS77P9EnfmETHd0vy41f/mIwZ7d+T6KnD3HqKbQYI+9kX/fxFFRujW8FAqHszzujs35TGZDLixs/Aa/NIW8Ekf4713H9jkvnOEkIIIYSYLCQAPOVIEFiIT5XCEnIt6rJbzZVuWrv61fQTx+hqdVPuHvIIGZQg3c13U167k6MngIiPbT71fUZjBgBz820YCNHdWD14TKCrtZrdPgVM2eQO/B/uITaVL6V669McOja4rFfX1qP0AxiNqEfVR18ddFL8dG19mhNd/RwHIMjB5lb6+iLqrNIZBg4zn3kOExCkc6ObnYfj+nbrCnb4wurDsmL1ac6SPDsGwvhaV7C169jAR/X7Inw08JcqrW3TIxImY2UD7e31rJpjwwTqQ6vdvqEPVPSUxUrR8jnY4392jwmLfR7rmmqITTAprltOgVnBv38rCStLD0NP2VSEe3ezoLx24Dz3769VzwUWbANPqnSM9VSuTSCnrIG6EhuGcC+73ZW0atqaythRggdprHCz86ha56Nbu/Ar6jifES2jZ/wmyF5Jvt2A0nuQLUe1mYPGrsNZer1N8L0kXfT1WT+RMGDIJm/u4FPSY12tuMvdQwOZMUmOnQHGYurWlWCL9NA8wvWjR3LXfHTJx4EfssS9OupInOuTYj8ka6K/u5MY67H7yYAkz7HcH9LTtnTR12cpXhdjjh2d45fkrqGUvrtD3WOMX30ie3z4FTDkFBE/Z9S4xIENCPbsJNYl+s5FVDL9gJ5739kmXWNSldx3i47xm8qYTOLfk7rqkG3EBIR8O9gW/fxI/2F2bu4mAJgt6o9ASXVMjrtkz7G++2/M2N9ZQgghhBCThwSApyQ1CNzwsyDmL1XQcO+NqQeBP3cH1dUuii+dTlbeAlz3VVNdXU111QqWfOkKpmvLnzuTq790B657q9Ry1dVU3eviji9dPWwdZubM5o57Bsveu+xWHCMt/X5uJtd/9S5WVA3W4a6vXk+mrlF8PXdUV+OacxnGq4tZsiL62VUuSv5S/eCE9G/cy5I5w9Q9Te28bI6L6uo7uF6bwWUUu6qpvmNozhDGq5l9h4uqb0T76b7h6mUcWv97FuAY8qRETHp2c/R/yPcnt9wugNLPwf2a/Zeiv6peXHsIyCfHYgDMFGwY+uBnuUPNs8T9GtqYX0bd9nb2JpQtYYSdmpKgvw669PtoHXwmAf7DbB3yYCQ68zXYR9eQPHjarz7ONZqvBArJzgI4jn/kSQFRaW6bHrZ5rJlnx2wAJdTLvs13qg+t/Iq2pL6yRMs0uuN+dd9JQAEsuSycC8biOlx5ZpTeXVQOfSqVQE/ZVB3vi9+rT9UVCGqTkh/rqVybWcXULbRjUvx4aqvZOaSpqY2d/sNbNHUIEkk4bXrGb6JCVxFWzXKUwxm7Dmfp9Tah95J00dtn+9nY2k0IE7Z5a/B699K+vZ6q+aOvJZrs2Ilx1a8iz+jHszHJ5eXHkOw1n7zU+iFpE/3dndRYT5TsOZb7Qzrali56+yy16yKZsaNr/JLMNZTad7f/4KYxxq9OkZ109YXBYCM/LgJclmsDAvTsiQ0qveciKpl+mNLSNybR8d2S9PhNYUyO/e9JVdJ1CCnqbFjHElz5ajDUmJ2Pa10RVkCJxNqX4pgcd8meYz3330Fjf2cJIYQQYqr7m7/5GyoqKnS/XC4XX/7yl8nNzU14ZWVlaT9i3OgKnYmzSYRfPVZNw8+CWL5SfXpBYKZjKbyLJTfAS88e4MAvjuD/0Mhln7+DOz5/3mCxcy+j+G4XJZ+/gulBH8/+Qi17LHI+V3y+BNcd1yfUwfi5O7jrqzdwxbTXeP6XBzjwi2f53XtX8JVlX+KyuHIQPXb5XRRffT7v/NezHPjFAZ7tjWC6upi7/uEmMrXlxzD9T25iyS2X89Zvn+XAL30cPzmTq//mDr6SW8ySr/45H/zuWQ784ll8b07jss+VcEdh3Ceks52ny3g9d9xTwg2XwrGeAxz4xQGO9E9X61VyzUCxa0pclORZ+PClwxz4xQEO/OYl3jkvk6wLEo4mziLKR8k+EUjGDAx6fr5cuJaWdQvJs5oxaPNSprMOaaXg0yaNRFFQF0MbzWRoWwgl9qAi7Kez2c2CpdVsO6Q+EDQ6stSHTUGfzrIxATorqtnWNZh2rGsrmw4GARPGbMgtysEEGOzLEh8QrclTl5W2lUTTmnSVHXXvNp3MBs2ITmGs67o2jx+my6+oe0Uu0yz9COkfO0mN3zjGMkocJggeHViO8vRNxestZrzbli76+yzStYmli9w07+vBH1QwWx3MWb4B794mXMNsxal37BTXtVOSHaRzi3uYWUzjZ8g1zwjLTjqdA8tdxtPdD+NK53lL4X6mi85znJzxvoZ09llajXfb0kV/n+m+LpIZO2kev7q+u9Ng/26fulxufpmakL0ShxWU3sNsG/hRgf5zoYuOe9/ZJi1jchRDvltSGL+6xuSY/57UWYc91XQGAJOdknUteL1enmpZp+5xrvjZv+PpaME0j0kd9J1jHfdfIYQQQnzq3XrrrXzta18b+u/kJF4lJSXcf//9bNiwIeH17W9/myuvTPzR2XiRAPCUlhgEfvguq7ZAkoxcNtPPv7bu5UDPEY70HGDvD57l+Cm47P99nthE1sv++lauz/iYVzq3s/1fuzgcLev53mPs+u07TL/iS3zlL6KFL7ieW2dfwfR3nmdX67/S1X2EIz2H6frX7fzgt+8MmVl82V/fyvUz38H31HZ2dR7mSM8RDv/0B3zvwGt8fMkN3DS46lBSjJeej2/HD/hZ9xGOdP+MH+x5nneYieOvHbzz7z9g73+o9fnZkz/D/zFkXnXNGWnn6TmP62/9Elec8xpd323F8x9HONJzhAP/tp1d//kO06/O56YMAAfXXDUdXn+WH/xU7csj/+Hh+9u/z38M/XGymOyCEXWfppxibc5pOET/cdTlsCqGflnFXpXR9bPmz8vDDCiBThrj9llyOj34NUdOnr46pEc08GnJYeUw+0HOt6m/zjrefxQ4QSQCGMxka8rmuBwkJk2Gtu3BHwRQ8HdtYev+xMcerjwroBDsO6yzLPhD6nJptuKhPzvKMo75iGlSmZ9jARRiExt0jfWUrs0IrZUL8PgVzI7ltNdp35uusaNn/A7KLsvHblDoPdg8sBxl6qby9Zautg0yZyWup5gzfx42U0KSDin2WcTH/m21VJYvxrnIzQ5fCAw25rriFzFV6Rk7Oa4mVuVBT3P1kP0Lx5v2mk+Jjn4YX/rOm677WQr0nOOxpesa0tdn6ZGutg2aiveHtI3flL670+DoJroDYLA5KDNCdmneMLNPUzwXaTK+4+wMGOcxORrtd4uu8ZvSmBzr35M661C4lgIrKOEQ4YGZrgrhQA87auN/mDW5xuTY51jP/VcIIYQQQpWVlcU555zDD37wgyH/znE6naxcuZL169cn9dq4cSOvvvoqn3zyCcrA7JvxJQHgT4GIogAGTDMv1mYl7bWeLl47FZcQeRH/28B5xuhsVxvX58yEt39L12+HPpx77d+P8Mqp6diuia73c801XDH9Y/y/1BwXOH7ot7yWkBI99h98HHg1IYPIb1/kONPJytY5l/Z1HwnPEF8/xmvvA++/xJH4+p96kWNBICMzOls3ne08TRdcj+OK6Xz4P4d5XlO11/77FSJkctmfAbxD5H0g62quj1+G+tTHfKypozgLdPWoew5Z5tDRVMX86LJcAPlldbTVpzYfcn9vALAwp74BV/Ho63RZokE95UQfXdE9pK4sdlG3vXjoEmJRJyLqILUV1VOWO/za43rqkA6F7MHnVwAr8+rrKYv1bUYuZXVtLHOYQOmlZ1cE8OE7rgY+i9ZWUZgxWK6+xDbkl/UT3TaAp4/6UTBgm1tHXVl0SbSMXMrq25ljAcI+PHv0l+06fIwwBuxL6lkZt2dWflk9qwvMQIDe/XCodvGQfyQ5nU6cm3vUPYX9nmhapa6yqT5TMpoLcWSr32jG7HzK6tuZZ1Xbti86sUHXWD+Na7PV3UxPCMx5q4c8tEvP2NE3flW5lBVYIdxH186h34f6Td3rLZ33ksFlGUspdajjt3hlE3XLHZi1ZXXQ1WeFa9ne1kDV/EKujN3OIz56uvsJAwaDtibJj50cVxP1Jdn0ezZSm/Tal8lJvOaLcTUMveZ10d0PyX0X6qHnvOm6n+mW/DlOTvquIT19lg5yf9DWJLmxk7bxexrf3eNt5+FeFIOdvCU5lDosEPINmX2q61ykSwrjbLzvfbqkaUzGJPPdomv8nsaYHO3fk3rqUDjHgZkwfXu2sKk2tr3LAhavqGWPL7FPUh2TxWvb1dV8OhooGzJDV6ekz7Ge+68QQgghhCozM5OTJ08SCg2/LtMrr7zC0aNHk3oFg0HOO+883n33XV59VRP4GicSAJ7SjFz3tYep/epVRLqbqNz6grZAkt4h+PrQtMh7wIUzsQAwE+MF8OEfXuEtbVGAU0He+iNwcRZZwGUXG4G3ee2YtiBwCj5OSFCPzaybuDe6X+3A6xvFXAbMvFitRbLeeUM7teMDPlAA5QM+0ORwEph+HudDmtt5mjKMnAec9xcLEvuouprqv3NgBGZechnwCs/+x0tEpl1Bsauae5eVkH9V5jjPRhZnTGQPrfv9KIDJNofl0WW5vF4v6xbmYRk6CTMp/dt20R0CzHZKVtcP2cPJ21FHYbTsfl/08x2rBvIfW11CnnXkn/37OvsIApgdLNzwZNyxB5fw1VOHdNnZul996GJ2sDDWt09uYGGeBQMK/v2txJ4F7d99lCBgsM5hzZNx5UJ+AuHE46atbYV1dAwcZw15JgATeWsGj90U7eD+1kr2+xUwWMhbuGGwbQ4zEKKndcvAEn96yrLfrS47Z7Ixb3X8eHRgRsHv2Rq3fOHkYSlaQ33LU3ijy9oN1zZdY/10rs1IF7Ubn8AXe2i3dvChXbrGjp7xC2AsW0KeGUK+3aSwGuKwzrrrTYd0tY39h9Xjmuwsq1fH7+p5NkyECGnLupri2h29P5jyWDOQlur914DZYmfO8jU89uRgmceWOzCh4PcljpCkx07hWtaV2DBgwFbyT0PrEL/ku462xSRe86spsQ+95vXR1w8k+V2oh57zput+plPS51iHdF1DevosXdLVtql8f0jb+D2d7+7R6OjfmMjOLvrCkJ1bhcMCge6dQ2af6jsXaaJnnEUlde/T02d6yqZpTMYk892ia/yezpgc5d+TeuqgBuxNOJbVU1+vGWd729m+dnCZ6dTGpIuSgmhQ1mQnr0ibr1fy51jP/VcIIYQQAsBisfDRRx/xxhtvaLN0M5vNXHDBBbz99tvarHEjAeApKy74+1wTFZueYfL9u/VjPvxQmzayD199Xt2vdrhXzyva4pOIvnaernf6humf6Ovwi2rYOvI7D9sf+z4/+Y2fsPFqbrr9LqruKeYyuSOclfpaK7l78z56g2GUgVSFUKCbHa27Esom7xCbKtzs6A4QGjzosPpbK2k9mFguHOyls7mZbu1vLWKObmHLE90ERj148nVIm75WKt1P0B0IxfWt2r59m++mMn4zyqNbuL+5O+4BbJhAzw7cFbs5PlgqahK0DWh11w6pQzjYy76NFUNm251uWSWk7h+c0GeTQU8n3b4AoYSlVqLXjzuxbXrH+mldm31P497owa+AuWAVbTWxh3ZpGju6xi+U5dsxKL10btU+jj4NU/l6S1fbInuobe4kEPfD03Cghx3uCg4OKayHjj47VEuzp0dzP1fi2pb4i4+kx47dMuLssfE3/DWvi85+gGS/C/VI/rzpvZ/pkfQ51iNd15COPkubdLVtCt8f0jl+T+u7e1ztZ7cvhMFqxaL0cnjnMPcQPeciXVIZZ+N+79MhTWNyeMN/t+gdv6c1Jkf496SeOvia9+CL3nOGLE1oMGMtWE5H/dxoQipjshVPd3QAhXvpOajN10nPOdZz/xVCCCHEp96FF16I0WjkvffeG5egrdVqxWAw8PrrQ2ZfjptzZs2a9Yk2UagyMzN5661h53mm3ezZszlw4IA2OUma4O+G0wj+fu4OqufM5Pl/aaVLMw6vv6Oa4iteoavhX3keG7euWsA17x/h+987MHR27LnXc0dVMZe9/BO2el5kZuFduL5o4sV/e4yfaGfHXpDPP6y6iaxXumj41+eBayipupWr33yWx548zOnFUq/njupiZv52F62d8QswX0axawnX8zy7WrsSlmY+c+2Ey+a4WPI5eP4HrXTF/w9z9LhX9A+WHXJuMm7irnvyMf1uL4/tG7Jzzyimk/VXS1hSkEVkSL98Ok3ktS+EEJNe7lraNxQww9fMYncy82GEiJoMY8fVhLfEht9zBvch/DSZDOdYnJ1k7IjJRs+YnMLfLa6mvZTYFHzNFbj3q8tFx+RWbWfdHCuGcA+bF9emuIJGiorr6Fidh8H3BAvcqezdIIQQQoiJFHzzHSyXxO9PefrS/Uz/yiuvpLa2lj/+8Y/ce++9AEybNo2bbrqJ5557jvfff1/7llHdddddzJ8/n507d/KjH/1Imz0uZL7flDOOwV9d/PhejsDFn6P4c0PXIbrsr2/ginM/5ljfiwC88/tXeIfzuDr/+ugewjHTuXrO9WQlpL3I//zfxzDLwezLEzImQDrbCW/98UNgJpdfmVja+HkHV4x1tZ54kWNvw3l/ns/1Q6sWZzrTZ8T//THHu30cB4zG8b3pCiGEmHpKl+RhJoRPuxmhEGOQsTP1yTkWqZKxIyYbGZMALhw2db/gGVmOwT11gWxHMfk2s7r/+PH+tAZ/XfVt1LuKBz4/48piqkqjSzr3dmmLCyGEEEKkRWzJ5jfffHMg7R/+4R9YvXo1//RP/4Tdbk8oP5bMzEw+/vjjtAatZQbwKNL9i4HRpDYDOA3BX+0s0ziJM2OBcy+juHwJ18+EyCvP8/zL7/AxJi6/zsHVF5/HOwmzS8/D8bcr+MqV0/n4xEv89vlXCUfLXhEO8s4VVyTMjMV4PXfcU8wV0z7krZd8+F5T1yAyWWxceeXH/LZ5r1qHMZ3uDOA0t/MCBwuWfwXbtA85/rvf8Ls3PsZ02fV8LvtD3j6VRVZolBnAAJcX41p0PTOJ8Mp/Po8/9DEwnZmX/Tm2zFf5yY4uXuN67vjGTRgH+nE6mdd8Hsesj3nx37YPnan8KTSR174QQoiJ4KLJW4JNmzyCcM9mFtem81GnSJspPEtLpIvcH4QQY5iy3y251LRtoMiiTY+jBDnYWM6WNN72XE1eSoa7CQcPsr58y5D9sYUQQggx+Z2NM4BLSkpYtmwZP/3pT3n88ccByMjIYPXq1Vx//fWEw2G+//3v8/Of/1z71mE98sgjXHbZZdTX1/Nf//Vf2uxxMdacQnEWsSyuU4O/R1qoHI/gr16nXqOr7fv87L9eg0uv56Yvz2b2l2/gynODPP/T72sCrh/i+7dWPL95hYjxam748mxmF17DxW88y649L/FBXEkAIs/zrzs8HOn/gJlX38DsL89m9pduwmE18vbRI/yPtnw6pbOd7/vY+y9d+N+dRtZf3sTsL8/GcZGfn/ygk1dPaQsP49Uuvr/rAC+9DZddq75/9pfy+QvLB/iP/DYa2A7i7/8A01Wxfsznz89/lWf/9QcS/BVCCCGEEEIIIQRwlC33b8bTEyCk3f9XCRHw7WPz3ekN/gLs2rUb3+Dm5+pnd+/AXSnBXyGEEEKcORdffDHnnHMOoVBoIO3EiRPU1tby1FNPYTAYWLlyJS6Xi2nTpiW8Vyu2n/AHH3yQcLzxJjOAR5HuXwyMJtUZwLd89cv85sde0jdkhJj6JvLaF0IIIYQQQgghhBBCCCGmqrNxBnB1dTUFBQW0tLQMO8v3xhtvZOXKlVx00UU8//zzNDY2cuLECW0xGGE/4XSQGcBTSoRnPsXB3+nGmczMGOVlnK59ixBCCCGEEEIIIYQQQgghhBAjysjI4KOPPuKNN97QZmGxWCguLubCCy/kvffe43/+53/44x//qC02ILaf8PHjx7VZ40oCwGLKcNzqwnXPKK9bHdq3CCGEEEIIIYQQQgghhBBCCDGsadOmMXPmTN577z3efvvthLy/+7u/49FHHyUvL48jR45w33338S//8i+cPHkyoVw8q9WKwWBIewBYloAeRbqnjI8mtSWghRDjYSKvfSGEEEIIIYQQQgghhBBiqjrbloC+4ooreOihh4hEIgNLNl955ZWsXLmSnJwcQqEQO3bs4Be/+IX2rcO66667KCkpYdeuXfzrv/6rNnvcyAxgIYQQQgghhBBCCCGEEEIIIYTQuOSSSzAajQkzdq+44gouvfRSnnnmGSoqKvjFL37BzTffTEVFxbCvf/iHfyAzMxOiweqTJ08SCqV3Q1cJAAshhBBCCCGEEEIIIYQQQgghhMall146ZMnmZ599FpfLxXe+8x3ef/99AObPn4/T6Rz2NXv2bIxGI0T3DB5pP+HxJAFgIYQQQgghhBBCCCGEEEIIIYTQuPjiiwESZuyePHlyIPBLdJ/gmpoanE4nd955J+vWrWP9+vUDr4aGBl599VUuvPBCjEbjsPsJjzcJAAshhBBCCCGmhGxXE3u9XrztaylWf1grhIgqre/A6/XSvrZYmyWEEEIIIYQQYgQWi4VTp06NumRzfED4xIkT/Pa3v+Xo0aMDr9/97necPHmSSy65hM985jNEIhFeeeUV7WHGlQSAhRBCiLRy0eT14u2oo1CbJSaeqwmv10uTS5txBhXW0eH14p3QSoxEx/g1ltGw14t3+0ptzhmko75nndNtWyF1HV683rhXyscaZ+M4duY6bBgAzA6KcrW5YsKM4zkeV5P6/jveXBQ5TACYC0oo02YLIYQQQgghhBhWRkbGuC3ZbDabueCCC3jzzTe1WeNOAsBCCCHOOIergfa9Exx0m8oycplf1US714vX20HdKBGewpUNtMUFhfa2b2ft/BxtMdBZFsAxt4qGtg51Nl70Ndo5NxZHH8Qn8TBeT1lxZuS4irAbFHoP79RmCTGq8Rw7+31+FICQj4NHtbmTy6fpu3A8z7FIVSsHfWEAQt0e5EwIIYQQQgghxNimTZvGzJkz+fDDD5k5cya5ublDXp/73OfIyMjQvnVYVqsVg8GQ9uWfkQCwEEKIiZCRnY3ZoE0Vpy2jEFf9djqe3MDyOTbM2nyN+fUdrJlnx6JOCALAYLZSsLyeJldiYFdPWYz5VG3fS/2qOdgtJnU23liMpdStyiPu8CPTU1acIXNZlm+BcB9dOyPaTDEpHKJ2sROn04nTuZkeNQ40CYzv2OlvrWSB04lz6Sa6Tv9wafXp+S4c33MsUrfHvRin08nSTV3aLCGEEEIIIYQQw8jMzGTGjBlkZmbywAMPsGHDhiGvjRs38uSTTyauujbCy+VyMW3aNE6cOKH9qHEnAWAhhBBiishdtZwShxUTCsGeg/SOEuAxzq9nicMEhPDtXq8Ghe5cz25fCDBgm+uiNLp/pp6yAKV1NcyxGiAcoMfTiLtiUTTo5KSydbBcPFf9EnV22MEeRqk26CwrzgxjWTE5Jgge3sF+baYQo5CxM/XJORZCCCGEEEIIcbY6fvw43/nOd/B4PEOCucm8fv3rX/PSSy8lvH784x+za9cu7UeNu3NmzZr1iTZRqDIzM3nrrbe0yWfE7NmzOXDggDZZCHEGTOS1n7KMQlauW0aRzYIpOpsoHOhhz7Yt7PHFZtu4aPKWYPN7cLoPU1qzktI8qzqLMhygZ9dWap/uizuouuTvsqLBWZ9KyE/nE+vZdijxF0pGx1xcZaXkx32+Eg7iP7iD6m2H1ARXE94SW8L7hvLjcVYSHyNMtg5JKayjY00exz3305NTx0K7CRQ/Hrcbf2kLqwvMoAQ52FjOlmi1MToorVpJSZ51YKaWEg7g27ON2j2++KPDQH1tWGIdERPuYfPiWmKHZbzbBpBbw/ZVRrq2bmGPL5e6jjXkmcL0bF5MbfwHA64mLyU2hcA+Nyu2xZ/3XNa2b6DArNC7YwHVe/SVJXct7RsKMId6aKyoTWoGXo6rifoSG5GeRio6i2hbk4fJ78E5TLRYT9mkRMel37OI1lANK0vzsJoAFEL+Tprd2zgc14akxnq8ZK7N6LjUtiPWVoMS5GBzJVviOjOpseNqwluSRc/mCjod0VnhBtS29XrYUruTgdtDlJ7xG2/ldi/zLL3sXlpNwgQ/vXU4W663yXIvGRi/2h9XFKrXP0P7Ibl8lZ4+m1vVQGl+XNlwgL79O3HvPKwtmmDEsRO7LuKSEiRcL9H2xBceZgxArM+y6d2xlD1ZdbgG2jf8Na/XmP2g+7twgr+7UxnrGiOeY53nIqn6xkvD/VdXHYwO9Xw5rANlE2jGaLLnLWmjjbURvjfHHL8xyd7P9H4HCCGEEEIIIT4Vgm++g+WSmdrk03JWPtNPM5kBLIQQZ7scF03fW8M8++DDSACTNY9lriXxJVUzslnbUs+y2ANkAJOVvOU11OQOFittGG7JXxvz1nyPJlf2YCKF1KxdxRzN5xtMFuzz1tBWNfIesWNJvg76ZOXXUGKPHtRgo6iqgVUF0QWTDRbyS0rV/zYWU9dSz7KCwQecAAaTlbxl9bTXFQ8mAq6mvdH6DvekN1Fa2nZ0CyvKa+OC/iOZjy0bUPx0xQd0M3Ipq3PhMAMYyHYU6iwLjjk2zCj0epIL/pJTRU2JDUOomydquxj1LXrK6pRV1EL9sljwF8CA2TaPmrroWAD9Y13vtRlnMPgQoHNLYvBX39gxkbOqhTXzYg/dUdtmX8jamsTNofWM3wRz6ymyQrivKzG4MyDJOpxt19skuZeki54+K23Yy6o5mrImK46FSxh1e9sxx87IQsFebZIOBrJLWliX0L7hrnl9Uu6HZEzwd3fSY11rzHOc7LnQV9/03H/11cFVX6eeryQu4+TPW/okPX513s+S/g4QQgghhBBCCDGuJAAshBBntVxqakqwGUAJ+vA0VkSX572XRo+P4HAPW615FJgVgj27WX+nE+ciN/v8CmAhZ44DAGNpA0vsJgj1Dh7T6aTR00sIA7biVcyNO6QSCdHb+QSb771zsGxnAAWwOEpwALRWDuRtjm4+6ffE9qOMvQZn/+qtgx4miwWl9wnubFSXEDZbreD3cP/9nQQBgyWHfKCwxkWeGQj52L0xrm+jbTPnLaFG7TKMZQ3MtRlACdDZeO9AfSvcnQQ0n5/OtiXHgtEAhI7ThzqTZ25VEx1PbmBhXHDBZLbrLAv52RYgyHGlioa2jrglTzpoa1hJftxS0VDI2nVzsCgB9m3cNHSmXgI9ZfUzmc0owZ6B81zR3EMIMNjnUhX37D2psQ6pXZtRg8EHPx73CrbGTYFLZeyYTCZ1DK9X67w+Wl+TrYj82HF1jF+tsuIcTAQ5unvkxV2TqcPZeL1N9L0kXfT1mYsiuwGUXnbHXRf3NnrwjTbQxxo7h2pZHD3WwOt+D34FFL+HpZvi7wL69zdO9ppPXpL9oPO7cMBEfXdHJTvWtUY9x1HJnovk65ue+y966jC3nmKbAcJ+9kU/f1HFxujWCRDq3owzOvtX73lLWtxYG3htHmnrhCTHr877WUwy3wFCCCGEEEIIIcaXBICFEOJsVlhCrkVdRrC50k1rV7+afuIYXa1uyt1DHiGDEqS7+W7Ka3dy9AQQ8bHNp77PaMwAYG6+DQMhuhurB48JdLVWs9ungCmb3IEndofYVL6U6q1Pc+jY4DKFXVuP0g9gNKIeVR99ddBJ8dO19WlOdPVzHIAgB5tb6euLqLNKZxg4zHzmOUxAkM6NbnYejuvbrSvY4QurD96L1afTS/LsGAjja13B1q5jAx/V74vw0cBfqrS2TY9ImIyVDbS317Nqjg0TqA/hd/uGPiDWUxYrRcvnYI+fRoQJi30e65pqiE1WK65bToFZwb9/KwkrSw9DT9lUhHt3s6C8duA89++vVc8FFmwDT951jPVUrk0gp6yBuhIbhnAvu92VtGramsrYUYIHaaxws/OoWuejW7vwK+o4nxEto2f8JsheSb7dgNJ7kC1HtZmDxq7DWXq9TfC9JF309Vk/kTBgyCZv7mDU51hXK+5y99BAZkySY2eAsZi6dSXYIj00j3D96JHcNR9dwnaYPXy8HXUkzl1MsR+SNdHf3UmM9dj9ZECS5zi5c6Gjvmm6/+qqQ7YRExDy7WBb9PMj/YfZubmbAGC2qD+aQvd5S5dkx6+++1nM2N8BQgghhBBCCCHGmwSAhRDibGY3Rx8w7k9uuV0ApZ+D+zX7yUVniSyuPQTkk2MxAGYKNgx96L3coeZZ4mZ3GPPLqNvezt6EsiWMsPNcEvTXQZd+H62Dz1jBf5itQx70Rme+BvvoGpIHT/vVR+BG85VAIdlZAMfxjzzJKSrNbdPDNo818+yYDaCEetm3+U71Ibxf0ZbUV5ZomUZ33CyiTgIKYMll4VwwFtfhyjOj9O6icuhT9gR6yqbqeN9ObRJdgaA2Kfmxnsq1mVVM3UI7JsWPp7aanUOamtrY6T+8RVOHIJGE06Zn/CYqdBVhJUxf19D+izd2Hc7S621C7yXporfP9rOxtZsQJmzz1uD17qV9ez1V8+PWJR5GsmMnxlW/ijyjH8/GJJeXH0Oy13zyUuuHpE30d3dSYz1Rsuc42XORdH3Tcv9VJV2HkKLOhnUswZWvBkON2fm41hVhBZRIrH36z1t6JDt+9dzPBo39HSCEEEIIIYQQYrxJAFgIIaYA5aNkn3AmYwYGPdMxCtfSsm4heVYzBm1eynTWIa0UfNqkkSgK6uKOo5kMbQuhxB68hv10NrtZsLSabYfU4ILRkaU+PA/6dJaNCdBZUc22rsG0Y11b2XQwCJgwZkNuUQ4mwGBflvjAe02euqy0rSSa1qSr7GnvsxnHbNCM6BTGuq5r8/hhuvyKur/msvna3PSPnaTGbxxjGSUOEwSPMsrqrjpNxestZrzbli76+yzStYmli9w07+vBH1QwWx3MWb4B794mXMNtA69z7BTXtVOSHaRzi3uYWZnjZ8g1zwjL6DqdA8v3xtPdD+NK53lL4X6mi85zrDXkXKRQ3/G9/+qsw55qOgOAyU7Juha8Xi9PtaxT91FW/Ozf8XS0oM7zlkb6xq+O+5kQQgghhBBCiAkhAeApxciNX7qRhO0VJ63ZPLTLi7epXJsxvHsexet9iof+OpZgZNGWvXg97Tw4kCbEp1Awou47l1OszTkNh+g/jrq8X8UwD72jr8roeoDz5+VhBpRAJ41x+8Y5nR78miMnT18d0iMa+LTksHKY/SDn27IAON5/FDhBJAIYzGRryua4HCQmTYa27cEfBFDwd21h6/7Ex7iuPCugEOw7rLMs+EPq8o+24qHfRlnGMR+ZTyrzcyyAQmyilq6xntK1GaG1cgEev4LZsZz2Ou170zV29IzfQdll+dgNCr0HmxllddckTeXrLV1tG2TOSlwfNmf+PGzxK7DrkmKfRXzs31ZLZflinIvc7PCFwGBjrqtUU1Df2MlxNbEqD3qaq4fsxzretNd8SnT0w/jSd9503c9SoOccD0d7LnTVNy33X511KFxLgRWUcIjwwExXhXCghx218T9k0Hfe0m7M8avnfiaEEEIIIYQQYiJJAHgKsSys474Hqml64JazJAh8Oi7GNEl+LS/EhOrqUfdQs8yho6mK+dFlBgHyy+poq09tPuT+3gBgYU59A67i0dcdtESDesqJPrqie+JdWeyibnvx0CURo05E1If4tqJ6ynKH3yFYTx3SoZA9+PwKYGVefT1lsb7NyKWsro1lDhMovfTsigA+fMfVwGfR2ioKMwbL1ZfYhswUmui2ATx91I+CAdvcOurKoks8ZuRSVt/OHAsQ9uHZo79s1+FjhDFgX1LPyrg9APPL6lldYAYC9O6HQ7WLhzzgdjqdODf3qHsK+z3RtEpdZVN9Rm40F+LIVr89jdn5lNW3M8+qtm1fdKKWrrF+Gtdmq7uZnhCY81YPCUKkZ+zoG7+qXMoKrBDuo2vneATlpu71ls57yeAys6WUOtTxW7yyibrlDszasjro6rPCtWxva6BqfiFXxm7nER893f2EAYNBW5Pkx06Oq4n6kmz6PRupTXot3+QkXvPFuBqGXvO66O6H5L4L9dBz3nTdz3RL/hyT5LnQVd803X/11KFwjgMzYfr2bGFTbWw7hAUsXlHLHl9in+g5b/GK17arq190NFA2ZIauTkmPXz33MyGEEEIIIYQQE+mcWbNmfaJNFKrMzEzeeustbfIZMXv2bA4cOKBNHoORWx5oouJLZkL/0ULlI88wef/XezYP7armhjd/iLOyTZs51D2P4r1tFkf+eREP/bs2U4jxNZHXfirUB+TDBAaIBsYGpo24aPKWYAv3sHmYpSsTFbK2fQ0FQ59Xq+KOke1qommkzyex7IDcGto2FGGJTwPAj2cgiJd8HZJWWEfHmjxMA/0S7RPt37Fj57hoqi/BNmzjFPwe9+CetCO1KeQnMMOGlfj6pqFtxLVPmx7H7xmcSeRq2kvJsI0L0dNYkRBwGZ+ymj4bzpBzNAo9ZUfiasJbon10H5PYNr1jPelrc7h25Mynft1yHGYIdTeydFNX9I06xk60bfHnXFVIXcca8uLHpK7xC8ayBtoX2ol0r2fpplFmeumpw9l0vQ05ZxN0LzGW0tC+DPuQ44YIhc2Y48uOOtZJ/f476n1Hwe+ppDJu89ikx07hWtrXFIwSyI6rr562jVp26P0saTr7AUY51wnnYoK/u/WOdT3nWMe5SLq+0T/Tcf/VUwdHTRv1RUPPLABKiEDPblZsiv3SIPnzNija79G/ht5jRzBce+PT48sO0IxfPfczPd8BQgghhBBCiE+N4JvvYLlkpjb5tJxtz/TPBJkBPKVEeOaRSlr+I4T5SxWfkpnAQoi+1kru3ryP3mCYgVUGUQgFutnRuiuhbPIOsanCzY7uAKHBgw6rv7WS1oOJ5cLBXjqbm+keaRnNo1vY8kQ3gVEPnnwd0qavlUr3E3QHQnF9q7Zv3+a7EwOZR7dwf3M3gfBAKQI9O3BX7Ob4YKmoSdA2oNVdO6QO4WAv+zYODYCcblklpO4fPGrwdyL0dNLtCxAa2OiYwevHndg2vWP9tK7Nvqdxb/TgV8BcsIq2mthMtDSNHV3jF8ry7RiUXjq3jhLc0WsqX2/paltkD7XNnQTiNgwOB3rY4a7g4JDCeujos0O1NHt6NPdzJa5tiUHPpMeO3TJK8He8DX/N66KzHyDZ70I9kj9veu9neiR9joc1/LnQW9903H/11MHXvAdf9BpWEr5f1CXerQXL6aifG01I/rwNasXTHb3ww730HNTm66Rn/Oq5nwkhhBBCCCGEmDAyA3gUE/mLgdRmAMecDTOBZQawmLwm8toXQohJL3ct7RsKmOFrZrF7vzZXiJFNhrEz4oxEMS70nOMpfC7UlTAUfM0VuPery0XH5FZtZ90cK4ZhZ/amWXEdHavzMPieYIE7lbXOhRBCCCGEEOL0yQzgM0NmAE9J6kzghp8FMX+pgoZ7b0x9JvA9j+L1PsVDf23kxq810PaUV91ryrOX9uYHud0eX7icR71enlo/Oz5RNXAcbQZgv50Hm9vZ64ke+6k2Gr42dp1nr38Kr/dRyjXpxmsXJR7P6+WptgdxasoJIYQQQr/SJXmYCeHbPUZwRwgNGTtTn5xjABeO6PrIM7Icg3vqAtmOYvJtZnUZ6eP9aQ3+uurbqHcVD3x+xpXFVJU6MKHg741tKyCEEEIIIYQQYrxZrVbuvvtuKioqdL+WLFlCbm5uwusv/uIvmDZtmvZjxiQzgEcxkb8YOL0ZwDFGbry3geqvWAj+rIHqx36lfyZwdOZt73N/wHbtxfiP/JLfh+Diq/6KG/7CjCF0hKaKh3gmQjQAfDuznmtg0QZN3YfM4I3OAA4d4chFN3DNu0f45X/+AeWCWVxXcANWo8LLP3qQ+77bO8L71QBw9Rf+wA+d9xGbQ2yc8xAtVTdgPhkh0PNLXggqcMEsrsszcWRp9UA5IUYzkde+EEKIiZC4n+ZYwj2bWVybztCNSJspPOv0rDNlz0UuNW0bGGkLYACUIAcby9mSxtuIq8nLsFssBw+yvnwLqSzQLYQQQgghhBDjYarPAG5sbOTqq6/WJqfs1KlT/OQnP+Hxxx/XZo1KZgBPaRF+9Vg1DT8LYvlKNQ/fZdUWSJIRuz1ES9lSqr/dQsvjLTxcs5QHfxYE8w0sWnmd9g3J+9NrsTxbzaJVD9H0eAstWx9ixd1tvBAxcNW8e1ikLT8a4yLqVt6AWXmZH65ZxIoNTbTEjinBXyGEEEIIIUTaHWXL/Zvx9Gj3lweUEAHfPjbfnd7gL8CuXbvxDW4mrn529w7clRL8FUIIIYQQQoh0ufzyy7nooot45ZVX+Lu/+zucTmfCa+HChTz44IOsX78+qZfH4+HUqVMo2v+/TILMAB7FRP5iYHxmAAMYue5rD1P71asIda6lfOsL2gKju+dRvLddRfBnKyh/LKDJXETD3qXYX/eyaFULkVRmABteoK10LT9MLM11D7Sx6UsmjmxdxEOdw71/6Axg4z2P8tRtVno7llL9pO65zkIMmMhrXwghhBBCCCGEEEIIIYSYqqbyDOC//Mu/xO1289prr/HAAw9os3X72te+xt/8zd/w3e9+l5/85Cfa7FHJDOApbTD4G+luolJv8HdAhMCL2uAvQJDwB4B5Fp/XZiUrGOAZbRrwQigMGDH/mTZnZJ+/bBYQ4pVDEvwVQgghhBBCCCGEEEIIIYQQZ86ll17K+eefTygU0malJCsrC0VReP3117VZY5IA8JQVF/x9romKTc/o3/833iltQpz3w6Q8lE9+NEq9FD6KW7UsOQrKm9o0IYQQQgghhBBCCCGEEEIIIdLHbDYzbdo0jh8/rs1KSVZWFpFIhDff1B/4kgDwlKQJ/m44zeAvRsw2ozYR/vRarBeBEgoQP7fYaL4q7i/V7MtmaZNUl1iZrU0DbrdZgRB/6NPmjCz0fhiw8NmvanOEEEIIIYQQQgghhBBCCCGESB+z2cwnn3zCG2+8MZBmt9u59tprE8ol4/LLL+czn/kMkUiEV199VZs9JgkATznjHfxVXfXFcq5LiAEbuf1rf4UFBf8RbzTtbXVJ6Mts3B5f1ng7N/+/YQLIABddg/NvzYlp9kqc1xog+CIHnk/MGs0LP36BIAbstz7ELSN8nBBCCCGEEEIIIYQQQgghhBDjLSsri48++mhgyebLL7+cb3zjGzz00EOUl5czbdo07VtGZDabOf/883nnnXc4efKkNntMEgCeUtIT/AWF0Pmz2dT6KA9+rYKKr1WyqbWd8muNKP6f8N2O2Kf8kJ8/HwLjdZTHylY9xPbvlTPr3aDmmFHvKlj+oY22b1VS8bUKKr75KE9tvgULIY78f9s5oi0/mt4mHvnRyyjmG6jc2U7DNyuix9zE9vYGyrXlhRBCCCGEEEIIIYQQQgghhBgHWVlZvPfeewMzgF999VV2797NBx98QElJCevXrycjI0P7tmHF9hM+ceKENispEgCeQiyL69Tg75EWKsct+AvwES/vrOOpl01cN8+J86u3cF1mhMCzbTxY2UZvXMkDmzbR9lyAiPEqbvyqE+eXr0L594ep/PUIm/m+eYDKx3+F8me34PyqE+dNV8GbvXg3VfBQp/4W9H73Qep2/orA+0bsNznVY37hsxhefzFhmWohhBBCCCGEEEIIIYQQQgghxkNsyeb33nsvYc/en//856xZs4Zjx46Rm5tLfX09drs94b3Die0n/NZbb2mzknLOrFmzPtEmClVmZmbKHXu6Zs+ezYEDB7TJYzByy1e/zG9+7CWkzUrVPY/ivW0WR/55EQ/9uzZTiKlpIq99IYQQQgyvtL6DZQ4Toe5Glm7q0mYLIYQQQgghhBDiLBB88x0sl8zUJp+WyfBM/y//8i9xu9289tprPPDAA9psLrjgAlavXk1+fj7hcJjvf//7/PznP9cWG/C1r32Nv/mbv2HHjh14PB5t9phkBvCUEuGZ8Qz+CiGEGAcumrxevB11FGqzxMRzNeH1emlyaTPOoMI6OrxevBNaiZHoGL/GMhr2evFuX6nNmViTun9PVyF1HV683rhXMudqPJ2x/nVR5DABYC4ooUybLYQQQgghhBBCCDEO7rnnnsRnLZrX9773Pa644grt2zCbzRgMBkKh4aN0hYWFXHPNNRBdGvr3v/+9tkiCrKwsFEUhEAhos5IiAWAhhBBnnMPVQPveCQ66TWUZucyvaqLd68Xr7aBulGhQ4coG2uICSHvbt7N2fo62GOgsC+CYW0VDWwd74/6BNNo5NxZHA0lJBJP0lBVnRo6rCLtBoffwTm2WEOOglYM+dUuRULcHGWVCCCGEEEIIIYRIp48++ohIJDLk9d5773Hy5EltcTIzM5k+fTrHjx9PSLdarTzyyCN8/etf59SpU3znO9/hgQce4NixYwnltLKysnj//fdHDCiPRQLAQgghzriM7GzMBm2qOG0Zhbjqt9Px5AaWz7Fh1uZrzK/vYM08OxZ1Uh0ABrOVguX1NLkSA7t6ymLMp2r7XupXzcFuMZHUqTaWUrcqj7jDj0xPWXGGzGVZvgXCfXTtjGgzRdoconaxE6fTidO5mR41Pjpl7XEvxul0yvLPQgghhBBCCCGESLujR4+yaNGiIa+vf/3rvPrqq9riXHLJJQC88cYbAEybNo2///u/55FHHuHqq6/mueee47777uOZZ57RvHOokfYT1kMCwEIIIcQUkbtqOSUOKyYUgj0H6R0lGGScX88ShwkI4du9Xg0g3bme3b4QYMA210WpUX9ZgNK6GuZYDRAO0ONpxF2xKBqgclLZOlgunqt+iTp79GAPo1QbdJYVZ4axrJgcEwQP72C/NlMIIYQQQgghhBBCiCnu0ksvHbJks91uJxQKUV9fz8aNGznvvPO46667qKioGPY1e/ZsiC4nff755xOJRPjjH/8Y9ynJO2fWrFmfaBOFaiI3jZ49ezYHDhzQJgshzoCJvPZTllHIynXLKLJZMEWnW4YDPezZtoU9vthsPBdN3hJsfg9O92FKa1ZSmmdVZ1GGA/Ts2krt031xB1WX/F1WNDjrUwn56XxiPdsOnUgoZ3TMxVVWSn7c5yvhIP6DO6jedkhNcDXhLbElvG8oPx5nJfExwmTrkJTCOjrW5HHccz89OXUstJtA8eNxu/GXtrC6wAxKkION5WyJVhujg9KqlZTkWQdmLSvhAL4926jd44s/OgzU14Yl1hEx4R42L64ldljGu20AuTVsX2Wka+sW9vhyqetYQ54pTM/mxdTGfzDgavJSYlMI7HOzYlv8ec9lbfsGCswKvTsWUL1HX1ly19K+oQBzqIfGilq6kpgMmuNqor7ERqSnkYrOItrW5GHye3AOEy3WUzYp0XHp9yyiNVTDytI8rCYAhZC/k2b3Ng7HtSGpsR4vmWszOi617Yi11aAEOdhcyZa4zkxq7Lia8JZk0bO5gk5HdFa4AbVtvR621O5k4PYQpWf8xlu53cs8Sy+7l1aTMAHY1YS3JJveHUvZk1WHa6DOk7d/ddXB6FDvpQ7rQNkEmn5L6rylrFC95hnlXOm8n6Wjf5M22nfGCNf83KoGSvPj+jccoG//Ttw7DycWTLYfUriGhBBCCCGEEEIIMbrgm+9guWSmNvm0jOcz/XvuuYfbbruNX//613zrW9/SZo+osbERs9lMXV3dwPLOF1xwAYqiDCwZXVJSwrJly5gxY4bm3aof/ehHfPe73+Xmm2+moqKCnp4eHn74YW2xpMgMYCGEONvluGj63hrm2Qcf0AOYrHkscy2JL6makc3alnqWxYK/ACYrectrqMkdLFbaMNySvzbmrfkeTa7swUQKqVm7ijmazzeYLNjnraGtauQ9YseSfB30ycqvocQePajBRlFVA6sKogsmGyzkl5Sq/20spq6lnmUFg0ECAIPJSt6yetrrigcTAVfT3mh9h4sEJUpL245uYUV5bVzQfyTzsWUDip+u+IBuRi5ldS4cZgAD2Y5CnWXBMceGGYVeT3LBX3KqqCmxYQh180RtF6O+RU9ZnbKKWqhfFgv+Ahgw2+ZRUxcdC6B/rOu9NuMMBs8CdG5JDJ7pGzsmcla1sGZeLHCF2jb7QtbWJG4OrWf8JphbT5EVwn1dicHfAQayS1pYl1Dnydq/+urgqq9T76VJdJm+85YGOu9n6enf9Clt2MuqOZr+NVlxLFxCwi7hevtBxzUkhBBCCCGEEEKIT6esrKxhl2x+//33E/YLfuaZZygtLcXpdLJ69WrWr1+f8Hr66achOgN42rRpQ/YT1kMCwEIIcVbLpaamBJsBlKAPT2NFdHnee2n0+AgO98zdmkeBWSHYs5v1dzpxLnKzz68AFnLmOAAwljawxG6CUO/gMZ1OGj29hDBgK17F3LhDKpEQvZ1PsPneOwfLdgZQAIujBAdAa+VA3uboRpV+T2zvythrcPav3jroYbJYUHqf4M5GdQlhs9UKfg/3399JEDBYcsgHCmtc5JmBkI/dG+P6Nto2c94SatQuw1jWwFybAZQAnY33DtS3wt3J4KIf0bJpbFtyLBgNQOg4faiz4eZWNdHx5AYWxv0wwGS26ywL+dkWIMhxpYqGtg68Xm/01UFbw0ry45aKhkLWrpuDRQmwb+Om4WcsDtBTVj+T2YwS7Bk4zxXNPYQAg30uVXGxuaTGOqR2bUYNBs/8eNwr2Bo3RTaVsWMymdQxvF6t8/pofU22IvJjx9UxfrXKinMwEeTo7pEXfz5b+hc9dZhbT7HNAGE/+6Kfv6hiY3RpdAh1b8YZnYmbynkbb3ruZ+ns36TFfWcMvDaPtOy7iyK7AZRedsedt3sbPfg0ldXXD6pkriEhhBBCCCGEEEJ8emVlZWEymcZcsjk+IPzSSy9x9OjRhFcs4Gs2m/nkk08G9hNOhQSAhRDibFZYQq5FXWa0udJNa1e/mn7iGF2tbsrdQ5fIRAnS3Xw35bU7OXoCiPjY5lPfZzRmADA334aBEN2N1YPHBLpaq9ntU8CUTe7AU+9DbCpfSvXWpzl0bHAZ066tR+kHMBpRj6qPvjropPjp2vo0J7r6Ub9SgxxsbqWvL6LOKp1h4DDzmecwAUE6N7rZeTiub7euYIcvrAbNi9Xo1ZI8OwbC+FpXsLVLXeIDoN8X4aOBv1RpbZsekTAZKxtob69n1RwbJlCDdLt9Q4MsespipWj5HOzxU/EwYbHPY11TDbGJ5sV1yykwK/j3byVhZelh6CmbinDvbhaU1w6c5/79teq5wIJtIDKnY6yncm0COWUN1JXYMIR72e2upFXT1lTGjhI8SGOFm51H1Tof3dqFX1HHeWyxGT3jN0H2SvLtBpTeg2w5qs0cdLb0r646ZBsxASHfDrZFPz/Sf5idm7sJAGaL+qMIUjlvrqa4H0/EvTrqSG3Oqb77Wfr6N136iYQBQzZ5cwejt8e6WnGXu+O2FdDZD1HJXENCCCGEEEIIIYT49DKbzRgMBkIhdWLA6crKyuKjjz7i9ddf12YlTQLAQghxNrObowGI/ckttwug9HNwv2a/yehMq8W1h4B8ciwGwEzBhqEBiOUONc8SN0PKmF9G3fZ29iaULWGE3RuToL8OuvT7aB2MwYD/MFuHBCqiM1+DfXQNyYOn/Wro2Gi+EigkOwvgOP6RJ0FGpbltetjmsWaeHbMBlFAv+zbfqQbp/Iq2pL6yRMs0uuNm4nUSUABLLgvngrG4DleeGaV3F5VjRIn0lE3V8b6d2iS6AkFtUvJjPZVrM6uYuoV2TIofT201O4c0NbWx0394i6YOQSIJp03P+E1U6CrCSpi+rqH9F+/s6F9V0nUIKeqMUccSXPlqwNCYnY9rXRFWQInE2pfaeRtfeu5n6e3f9NjPxtZuQpiwzVuD17uX9u31VM2P29cA9PdD1NjXkBBCCCGEEEIIIT7NMjMzmT59OpFIhNzc3GFfV199tfZtI8rKyuKDDz7gxAnNc3wdJAAshBBTgPJRsk/okzEDg54pTYVraVm3kDyrmYHtEU+bzjqklYJPmzQSRWHs33hNhraFUGLBi7CfzmY3C5ZWs+2Q+g8KoyNLDf4EfTrLxgTorKhmW9dg2rGurWw6GARMGLMhtygHE2CwL0sMiK3JU5eVtpVE05p0lU3Y6/M0mQ2aEZ3CWNd1bR4/TJdfUfelXjZfm5v+sZPU+I1jLKPEYYLgUUZZ/XlEk69/ddZhTzWdAcBkp2RdC16vl6da1qn7iyt+9u9Q92xJ6bwNt/yx0zmwpHTqdNzP0tG/aRTp2sTSRW6a9/XgDyqYrQ7mLN+Ad28TriFb0evrByGEEEIIIYQQQojRfOYzn+Hcc8/l5ptvZsOGDcO+Ghsbh0wMGOl15ZVX8v7770sAWAghPrWCEXVfypxibc5pOET/cdQlMiuGCUBEX5XRNTXnz8vDDCiBThrj9l50Oj34NUdOnr46pEc08GnJYWXiaqAAzLdlAXC8/yhwgkgEMJjJ1pTNcTlITJoMbduDPwig4O/awtb9iaEQV54VUAj2HdZZFvwhdQlVW3HCZr8AZBnHDKlNKvNzLIBCbCKnrrGe0rUZobVyAR6/gtmxnPY67XvTNXb0jN9B2WX52A0KvQebGWX15xFNvv7VWYfCtRRYQQmHCA/MBlUIB3rYUeuOW/44XedNDz33s/T1b9pFfOzfVktl+WKci9zs8IXAYGOuqzRaQGc/CCGEEEIIIYQQQiThqaeeor29fUggN5nXz372M1588UVeeumlgddvf/tbWlpaBvYEToUEgIUQ4mzW1aPuQ2iZQ0dTFfOjy5AC5JfV0Vaf2nzI/b0BwMKc+gZcxaOvS2qJBvWUE310RffMvLLYRd324qFLpkadiKizymxF9ZTlDr9DsJ46pEMhe/D5FcDKvPp6ymJ9m5FLWV0byxwmUHrp2RUBfPiOq4HPorVVFGYMlqsvsQ2ZSTjRbQN4+qgfBQO2uXXUlUWXSc3Ipay+nTkWIOzDs0d/2a7DxwhjwL6knpVx+2jml9WzusAMBOjdD4dqFw8JgDmdTpybe9Q9hf2eaFqlrrKpxtCM5kIc2WrQ2pidT1l9O/Osatv2RSdy6hrrp3Fttrqb6QmBOW/1kCBaesaOvvGryqWswArhPrp2jj1LNLF/i3E1TM7+1VOHwjkOzITp27OFTbWx5c4XsHhFLXt8iX2SnvOmh577Wfr6N17x2uj/FHU0UDZkhq5OhWvZ3tZA1fxCrox9pUR89HT3EwYMBnM0UWc/CCGEEEIIIYQQQiTh5MmT7Nmzh5aWFt2vxx57jAceeIDVq1cPvNatW8fzzz+v/Rhdzpk1a9Yn2kShyszM5K233tImnxGzZ8/mwIED2mQhxBkwkdd+KnJcTSMHafwenAPTylw0eUuwhXvYPOYyooWsbV9DQeyZuVbcMbJdTTSN9Pkklh2QW0PbhiIs8WkA+PEMBPGSr0PSCuvoWJOHaaBfon2i/Tt27BwXTfUl2IZtnILf4x7ck3akNoX8BGbYsBJf3zS0jbj2adPj+D2DMw1dTXspGbZxIXoaK6iN2/RyfMpq+mw4Q87RKPSUHYmrCW+JNrQXk9g2vWM96WtzuHbkzKd+3XIcZgh1N7J0U1f0jTrGTrRt8edcVUhdxxry4sekrvELxrIG2hfaiXSvZ+mmUWZLnmX9q6cOjpo26ouG9JhKCRHo2c2KTbFloHWcNz1G7V8S76l67mdp6t9B0Xtt9K+hY3QEw31WfHp82QEKfk8llbGN3/X0g55rSAghhBBCCCGEEEkJvvkOlktmapNPy3g+07/nnnu47bbb+PWvf823vvUtbfZZQ2YACyHEWa6vtZK7N++jNxhmYBVSFEKBbna07koom7xDbKpws6M7QGjwoMPqb62k9WBiuXCwl87mZrqjS7sOcXQLW57oJjDqwZOvQ9r0tVLpfoLuQCiub9X27dt8d2Ig8+gW7m/uJhAeKEWgZwfuit0MXahjErQNaHXXDqlDONjLvo2JAV3GoawSUvcPHjX4OxF6Oun2BQgNbHTM4PXjTmyb3rF+Wtdm39O4N3rwK2AuWEVbTWwmZZrGjq7xC2X5dgxKL51bRwn+jmjy9q+eOvia9+CL9peSMH7U5bStBcvpqJ8bTUjTedNDz/0sTf07qBVPd3TH6XAvPQc12XodqqXZ06P5TlHi2hYN/qK/H4QQQgghhBBCCPHp8t3vfhen03lWB3+RGcCjG89fDOglM4CFmDgTee0LIcSkl7uW9g0FzPA1s9i9X5ubaMQZlGc/daa7gq+5Avd+dbnomNyq7aybY8WQ6sxeMbziOjpW52HwPcECd2x2tRBCCCGEEEIIIc4mk30G8FQhM4CFEEIIIUTSSpfkYSaEb/cYwd8pzYUjuobwjCzH4L6zQLajmHybWV06+Xi/BH9T5Kpvo95VPNC3GVcWU1XqwISCv1e7pLQQQgghhBBCCCGEiCczgEcxkb8YkBnAQkycibz2hRBiSpmyM4BzqWnbwEhbAAOgBDnYWM4WiQCnxNXkZdjtjYMHWV++hVQWHxdCCCGEEEIIIcTEkxnAZ4bMAJ5SjNz4pRsxapOFEEIIIcQ4OsqW+zfj6dHuHw0oIQK+fWy+W4K/p2PXrt34BjelVvu1ewfuSgn+CiGEEEIIIYQQQoxFZgCPYiJ/MZDKDGDLwgaaymyE/6OFykeeIaItIIRIykRe+0IIIYQQQgghhBBCCCHEVCUzgM8MmQE8hQR319L2HyHMX6qg6YFbZCawEEIIIYQQQgghhBBCCCGEEJ8yEgCeUiI880glLRIEFkIIIYQQQgghhBBCCCGEEOJTSQLAU44EgYUQQgghhBBCCCGEEEIIIYTQKysri9zcXK644gpt1llF9gAexUSuGZ7KHsCJjNx4bwPVX7EQ/FkD1Y/9KsU9ge3c/s37WHCDFfP5aooS6uUn/1xN2/MA5TzqvZ1ZzzXxaPBWVsy7CvO0CEf+eREP/TuAmdkr17L0JhuWiwyxA9D74waqv/9C3OcIMXlM5LUvhBBCCCGEEEIIIYQQQkxVk30P4HvuuYfbbruNX//613zrW9/SZo/JarVy8803YzBEY2I6vPvuu/T29iakffDBB/T19XHy5MmE9LFIAHgU4zlg9Dr9ADDjEAQ2sqihnaV2CD5/gN/0K2D+LJ+/3kLg8aXRAG80ABwMwkcvsH1dEwfejL3fTnnTw9xuM6C82cuR7t/zNnDxVZ/H+nY7K759uu0TIj0m8toXQgghhBBCCCGEEEIIIaaqqR4Abmxs5Oqrr9Ymp+zUqVP85Cc/4fHHH9dmjUoCwKMYzwGj1/gEgEkIAgf+7T7u+35AW2AUanD3qv/zsmhVy2Dw2GjGTIhQJK6M0stTS6tpj4sw3/BAGw99yULouSYqNjyjM/gsxMSZyGtfCCGEEEIIIYQQQgghhJiqpnIA+PLLL2fDhg18+OGHrFmzhj/+8Y8J+RdccAFXX30106dPT0gfSV5eHrfeeisej4fvf//72uxRyR7AnwIRRQEMmGZerM0aQ5BwBLj0GpZeG7eTcCQW/I3z+u/Zm5A2G+f1FnjzVzwqwV8hhBBCiDOitL4Dr9dL+9pibZYQQgghhBBCCCGESCOz2cz5559PJBIZEvwFeP/99/nP//xPjh49mtTr3HPP5ZNPPuH48ePaQ41JAsBTmpHrvvYwtV+9ikh3E5Vb9e6566X9x71Epl2F8+GneKqtgcrbbsCsLQZE3vBrgrxXYb4IlNde5EhCuhBCfNq4aPJ68XbUUajNEhPP1YTX66XJpc04gwrr6PB68U5oJUaiY/way2jY68W7faU2Z2JN6v4dby6KHCYAzAUllGmzhRBCCCGEEEIIIUTaXHrppZx//vmEQiFtVkqysrJQFIXXX39dmzUmCQBPWXHB3+eaqNiU2izc3ierWVT+EE89+zJhk51b7nmI9h0PckvchGAATimaBNVHSiqfKoSY6hyuBtr3TnDQbSrLyGV+VRPtXi9ebwd1o0TuClc20NbhxetVX3vbt7N2fo62GOgsC+CYW0VDWwd7o+XHCrQai6OBuiSCdXrKijMjx1WE3aDQe3inNkucMa0c9IUBCHV7kDMhhBBCCCGEEEIIceaYzWamTZuW0ozd4WRlZRGJRHjzzTe1WWOSAPCUpAn+nu4SzG8eof3b91G+aCkN/x5EueRGyu+frS2lEeYjBYzWa7lOmyWE+NTLyM7GbNCmitOWUYirfjsdT25g+RzbsCs2xJtf38GaeXYs6oRBAAxmKwXL62lyJQZ29ZTFmE/V9r3Ur5qD3WIiqVNtLKVuVR5xhx+ZnrLiDJnLsnwLhPvo2nla/+oQp2mPezFOp5Olm7q0WUIIIYQQQgghhBAijcxmM5988glvvPHGQJrdbufaa69NKJeMyy+/nM985jNEIhFeffVVbfaYJAA85Yxn8NeM+ZL4v0McePw3BIEZF1niM4bh5Ze9EbDcyN332LWZQggh0iB31XJKHFZMKAR7DtKrTgQclnF+PUscJiCEb/d6nE4nzjvXs9sXAgzY5rooja72oKcsQGldDXOsBggH6PE04q5YpL7H6aSydbBcPFf9EnX26MEeRqk26CwrzgxjWTE5Jgge3sF+baYQQgghhBBCCCGEEJ8CWVlZfPTRRwNLNl9++eV84xvf4KGHHqK8vJxp06Zp3zKi2H7C77zzDidPntRmj+mcWbNmfaJNFKrMzEzeeustbfIZMXv2bA4cOKBNHsN4Bn8BynnUcwumvhf4zctvAwasN8zmuks/4oXv3s3aH0XUMt7bmfVcA4s2aOprvIWHWiq5wQyR/zvCL//zDygYmGW/DkuwnRXf1ts+Ic6Mibz2U5ZRyMp1yyiyWTBFp1uGAz3s2baFPb7YncBFk7cEm9+D032Y0pqVlOZZ1VmU4QA9u7ZS+3Rf3EHVJX+XFQ3O+lRCfjqfWM+2QycSyhkdc3GVlZIf9/lKOIj/4A6qtx1SE1xNeEtsCe8byo/HWUl8jDDZOiSlsI6ONXkc99xPT04dC+0mUPx43G78pS2sLjCDEuRgYzlbotXG6KC0aiUledaBWctKOIBvzzZq9/jijw4D9bVhiXVETLiHzYtriR2W8W4bQG4N21cZ6dq6hT2+XOo61pBnCtOzeTG18R8MuJq8lNgUAvvcrNgWf95zWdu+gQKzQu+OBVTv0VeW3LW0byjAHOqhsaKWriS+iHJcTdSX2Ij0NFLRWUTbmjxMfg/OYaLFesomJTou/Z5FtIZqWFmah9UEoBDyd9Ls3sbhuDYkNdbjJXNtRselth2xthqUIAebK9kS15lJjR1XE96SLHo2V9DpiM4KN6C2rdfDltqdDNweovSM33grt3uZZ+ll99JqEiYAu5rwlmTTu2Mpe7LqcA3UefL2r646GB3qvdRhHSibQNNvSZ03PUa7r45wXcytaqA0P64O4QB9+3fi3nk4sWCy974UxpkQQgghhBBCCCE+vYJvvoPlkpna5NMyns/077nnHm677TZ+/etf861vfUubParHHnuMCy+8kLq6Oo4dOwbAzTffzF133YXJZOL555+nsbGREyfGfhZ08803U1FRQXd3Nw0NDdrsMckM4CnEsrhODf4eaaHytIO/AC/zcr+COedGnF914vzqLVxzfoBnttVGg79jiDzDQ6sb8P4uCJfewC3RY1x7icLLvS9rSwshUpXjoul7a5hnHwxWAJiseSxzLYkvqZqRzdqWepbFgr8AJit5y2uoyR0sVtow3JK/Nuat+R5NruzBRAqpWbuKOZrPN5gs2Oetoa1q5D1ix5J8HfTJyq+hxB49qMFGUVUDqwqiCyYbLOSXlKr/bSymrqWeZQWDARAAg8lK3rJ62uuKBxMBV9PeaH2HiwQlSkvbjm5hRXltXNB/JPOxZQOKn674gG5GLmV1LhxmAAPZjkKdZcExx4YZhV5PcsFfcqqoKbFhCHXzRG3X6N9desrqlFXUQv2yWPAXwIDZNo+auuhYAP1jXe+1GWcwOBmgc0ti8Fff2DGRs6qFNfNiQTnUttkXsrYmcXNoPeM3wdx6iqwQ7utKDP4OMJBd0sK6hDpP1v7VVwdXfZ16L02iy/Sdt/QobdjLqjmaOpisOBYuIWEnbZ33Pj3jTAghhBBCCCGEEGIqii3Z/N577yXs2fvzn/+cNWvWcOzYMXJzc6mvr8duH3vl3Nh+wqkGtiUAPIUEO2ppebyFyoe8hLSZKTlA06qlLChRl+10Op0sWHofTft648q0cZ/TOXT2b8ybB2ipKWfRgvhjrKDhRwFtSSFESnKpqSnBZgAl6MPTWBFdnvdeGj0+gsMFY6x5FJgVgj27WX+nE+ciN/v8CmAhZ44DAGNpA0vsJgj1Dh7T6aTR00sIA7biVcyNO6QSCdHb+QSb771zsGxnAAWwOEpwALRWDuRt7lEX7vV7Bu8N6mtw9q/eOuhhslhQep/gzkZ1CWGz1Qp+D/ff30kQMFhyyAcKa1zkmYGQj90b4/o22jZz3hJq1C7DWNbAXJsBlACdjfcO1LfC3Yn2jpfOtiXHgtEAhI7ThzrTb25VEx1PbmBh3A8DTGa7zrKQn20BghxXqmho68Dr9UZfHbQ1rCQ/bqloKGTtujlYlAD7Nm4acXapSk9Z/UxmM0qwZ+A8VzT3EAIM9rlUxcXmkhrrkNq1GTUYnPTjca9ga9wU2VTGjslkUsfwerXO66P1NdmKyI8dV8f41SorzsFEkKO7R178+WzpX/TUYW49xTYDhP3si37+ooqN0aXRIdS9GWd09m8q5y0pcffVgdfmkZZGd1FkN4DSy+64tt3b6MGn6TA9976YZMaZEEIIIYQQQgghxFQVW7I5Eonwxz/+MSEvEAjwzW9+k+7ubi6//HLWr1/PzTffnFBGK7af8Ntvv63NSooEgKeUCM/8eLyCv0KIs0JhCbkWdZnR5ko3rV39avqJY3S1uil3D13+EyVId/PdlNfu5OgJIOJjm099n9GYAcDcfBsGQnQ3Vg8eE+hqrWa3TwFTNrkDT/QPsal8KdVbn+bQscGlK7q2HqUfwGhEPao++uqgk+Kna+vTnOjq5zgAQQ42t9LXF1Fnlc4wcJj5zHOYgCCdG93sPBzXt1tXsMMXVoPmxWr0akmeHQNhfK0r2NqlLu8B0O+L8NHAX6q0tk2PSJiMlQ20t9ezao4NE6hBut2+oQEkPWWxUrR8Dvb4aYaYsNjnsa6phthE8+K65RSYFfz7t5KwsvQw9JRNRbh3NwvKawfOc//+WvVcYME2EJnTMdZTuTaBnLIG6kpsGMK97HZX0qppaypjRwkepLHCzc6jap2Pbu3Cr6jjfEa0jJ7xmyB7Jfl2A0rvQbYc1WYOOlv6V1cdso2YgJBvB9uinx/pP8zOzd0EALNl8JecqZy38ddPJAwYssmbOxi9PdbVirvcHbf0vr57X0wy40wIIYQQQgghhBDibPHFL34xbnLL4Ot73/seV1xxhbY4ZrMZg8FAKDR8lK6wsJBrrrkGgFdffZXf//732iIJsrKyUBSFQGCs6RnDkwCwEEKczezmaABif3LL7QIo/Rzcr9ljIDqLbHHtISCfHIsBMFOwYegX3HKHmmeJm/1lzC+jbns7exPKljDCzpRJ0F8HXfp9tA7GYMB/mK1DAkHRma/BPrqG5MHTfjV0bDRfCRSSnQVwHP/IkyCj0tw2PWzzWDPPjtkASqiXfZvvVIN0fkVbUl9ZomUa3XGzDDsJKIAll4VzwVhchyvPjNK7i8qhUbgEesqm6njfTm0SXYGgNin5sZ7KtZlVTN1COybFj6e2mp1Dmpra2Ok/vEVThyCRhNOmZ/wmKnQVYSVMX9fQ/ot3dvSvKuk6hBR1NqxjCa58NRhqzM7Hta4IK6BEYu1L7byNv/1sbO0mhAnbvDV4vXtp315P1fy4tf9B571v0NjjTAghhBBCCCGEEGLy+/DDD4lEIiO+3nvvPU6ePKl9G5mZmUyfPp3jx9VnJzFWq5VHHnmEr3/965w6dYrvfOc7PPDAAwN7BI8kKyuL999/f8SA8lgkACyEEFOA8lGyEZBkzMCgZ7pW4Vpa1i0kz2ombqvI06SzDmml4NMmjURRkliFYTK0LYQSC8yE/XQ2u1mwtJpth9QfBhgdWWpwLejTWTYmQGdFNdu6BtOOdW1l08EgYMKYDblFOZgAg31ZYkBsTZ66rLStJJrWpKtswj6mp8ls0IzoFMa6rmvz+GG6/Iq6L/Wy+drc9I+dpMZvHGMZJQ4TBI8yyurPI5p8/auzDnuq6QwAJjsl61rwer081bJO3V9c8bN/x9PRgmk+bzpEujaxdJGb5n09+IMKZquDOcs34N3bhGvIdu067n1CCCGEEEIIIYQQU0R7ezuLFi0a8fX1r3+dV199Vfs2LrnkEgDeeOMNAKZNm8bf//3f88gjj3D11Vfz3HPPcd999/HMM89o3jnUSPsJ6yEBYCGEOJsFI+q+lDnF2pzTcIj+46jLf1Zo9paMe1VG1wudPy8PM6AEOmmM21fS6fTg1xw5efrqkB7RwKclh5WJK50CMN+WBcDx/qPACSIRwGAmW1M2x+UgMWkytG0P/iCAgr9rC1v3J4Z5XHlWQCHYd1hnWfCH1OVhbcUJm/0CkGUcM6Q2qczPsQAKsYmcusZ6StdmhNbKBXj8CmbHctrrtO9N19jRM34HZZflYzco9B5sZpTVn0c0+fpXZx0K11JgBSUcIjww01UhHOhhR607bnnpdJ23FEV87N9WS2X5YpyL3OzwhcBgY66rNFpAz71PCCGEEEIIIYQQQgBceumlQ5ZsttvthEIh6uvr2bhxI+eddx533XUXFRUVw75mz54N0eWkR9pPOFkSABZCiLNZV4+6x6JlDh1NVcyPLkMKkF9WR1t9avMh9/cGAAtz6htwFY++LqklGtRTTvTRFd0z88piF3Xbi4cumRp1IqLO2rMV1VOWO/wOwXrqkA6F7MHnVwAr8+rrKYv1bUYuZXVtLHOYQOmlZ1cE8OE7rgY+i9ZWUZgxWK6+xDZkJuFEtw3g6aN+FAzY5tZRVxZdAjYjl7L6duZYgLAPzx79ZbsOHyOMAfuSelbG7RGaX1bP6gIzEKB3PxyqXTwkAOZ0OnFu7lH3FPZ7ommVusqmGkMzmgtxZKtBa2N2PmX17cyzqm3bF53IqWusn8a12epupicE5rzVQ4KU6Rk7+savKpeyAiuE++jaOfYs3MT+LcbVMDn7V08dCuc4MBOmb88WNtXGljtfwOIVtezxJfZJqueteG27Oru9o4GyITN0dSpcy/a2BqrmF3Jl7LYb8dHT3U8YMBjM0UQ99z4hhBBCCCGEEEIIAXDxxRcnLNl88uRJHn74Yb7+9a/z61//GoD8/Hzmz58/9Dln9PXZz34WosHk888/P+XlnwHOmTVr1ifaRKHKzMzkrbfe0iafEbNnz+bAgQPaZCHEGTCR134qclxNIwdp/B6cA9PKXDR5S7CFe9i8uJZDmqKJClnbvoaCWDxAK+4Y2a4mmkb6fBLLDsitoW1DEZb4NAD8eAaCeMnXIWmFdXSsycM00C/RPtH+HTt2joum+hJswzZOwe9xD+5JO1KbQn4CM2xYia9vGtpGXPu06XH8nsGZhq6mvZQM27gQPY0V1MZt6Dk+ZTV9Npwh52gUesqOxNWEt0Qb2otJbJvesZ70tTlcO3LmU79uOQ4zhLobWbqpK/pGHWMn2rb4c64qpK5jDXnxY1LX+AVjWQPtC+1EutezdNMoM0HPsv7VUwdHTRv1RUN6TKWECPTsZsWm2DLQOs7bgOj9KPrX0PM4guHaG58eX3aAgt9TSWVsc3Q99z4940wIIYQQQgghhBCfesE338FyyUxt8mmZ6Gf6WVlZfOtb3+LkyZOsWbNmxFm7F1xwAYqicPLkSa6++mouvPDChPz+/n6OHz/OHXfcwZIlS/B6vXz3u99NKJMsmQEshBBnub7WSu7evI/eYJiBVUhRCAW62dG6K6Fs8g6xqcLNju4AocGDDqu/tZLWg4nlwsFeOpub6Y4u7TrE0S1seaKbwKgHT74OadPXSqX7CboDobi+Vdu3b/PdiYHMo1u4v7mbQHigFIGeHbgrdnN8sFTUJGgb0OquHVKHcLCXfRsTA7qMQ1klpO4fPGrwdyL0dNLtCxAa2OiYwevHndg2vWP9tK7Nvqdxb/TgV8BcsIq2mthM1TSNHV3jF8ry7RiUXjq3jhL8HdHk7V89dfA178EX7S8lYfyoy2lbC5bTUT83mpDKeWvF0x39lWe4l56D2nydDtXS7OnR3HeVuPtZNPiLznufEEIIIYQQQgghxKdcVlYWJpNpzCWb33//fU6ePAnASy+9xNGjRxNex4+rT+LMZjOffPLJwH7CqZAZwKOYyF8MyAxgISbORF77Qggx6eWupX1DATN8zSx279fmJhpxdujZT53pruBrrsC9X10uOia3ajvr5lgxDDuzN82K6+hYnYfB9wQL3LEZyEIIIYQQQgghhBCTw1ScAVxYWEhlZSXPP/88Dz/8sDZbt3/8x3/E4XDQ0NDAc889p81OiswAFkIIIYQQSStdkoeZEL7dYwR/pzQXjuj6yDOyHIN76gLZjmLybWZ1Genj/WkN/rrq26h3FQ98fsaVxVSVOjCh4O+NLRsuhBBCCCGEEEIIIdIpMzOT6dOnE4lEyM3NHfZ19dVXa982oqysLD744ANOnEicdKCHzAAexUT+YkBmAAsxcSby2hdCiCllys4AzqWmbQMjbQEMgBLkYGM5W9IYAXY1eRl2i+XgQdaXbyGVBbqFEEIIIYQQQggh0mkqzgBesmQJixYtYtq0adqslL366qv84z/+48Cy0HpJAHgUEzlgJAAsxMSZyGtfCCGmlCkbAAYyCnGtXkKRw4LZoM4GBkAJEejrZtfmbRxK/UeaSTHml7GubC4Oq0lNUEIEejxs27oHX+LW3EIIIYQQQgghhBCTwlQMAE+bNo3bb7+dSy65RJs1phkzZnDFFVcwffr0gbRIJMK//du/8fzzzyeU1UMCwKOYyAEjAWAhJs5EXvtCCCGEEEIIIYQQQgghxFQ1FQPAk5HsASyEEEIIIYQQQgghhBBCCCGEEFOEBICFEEIIIYQQQgghhBBCCCGEEGKKkACwEEIIIYQQQgghhBBCCCGEEEJMERIAFkIIIYQQQgghhBBCCCGEEEKIKeKcWbNmfaJNFKqJ3DR69uzZHDhwQJs8qnOMl2GxwIn/fY0PTmlzhRDJmshrXwghhBBCCCGEEEIIIYSYqoJvvoPlkpna5NOSmZnJf3/1KQC++IsV2uxPJZkBPFV85s/4s+uuwXzpNVx57VWcPynOrJFFW/bi9bTz4F9r84a64RtteL17efQuqzZLCCGEEEIIIYQQQgghhBBCCJGESREmFKfpHJhuymDGOdG/jX/Gldf+GefF/p4wF2OaoU0bmclg0CYJIYQQQgghUlRa34HX66V9bbE2SwghhBBCCCGEEFOYBIDPdp/J5oq8L3BR+Le83PsaHyrRtZ+NV2G7bqKDwAHaVi/AWbKUh/89Lvmr1WxvbxsyK/jAt5fidC7gvu8HEjOEEOKs5qLJ68XbUUehNktMPFcTXq+XJpc24wwqrKPD68U7oZUYiY7xayyjYa8X7/aV2hwxEl19puNcJCFn/lq2t+/F6/UOvsbp2GKycFHkMAFgLiihTJsthBBCCCGEEEKIKUsCwGezz2RzxV/mYDzvQix/mcuFkRfx/+YX+AMRNX9SBIGHYbFiNZuQ+b5CfHo5XA20753goNtUlpHL/Kom2r1evN4O6kaJ6BSubKCtYzAAtLd9O2vn52iLgc6yAI65VTS0dbA3LsA02jk3FkcDoUkEQ/WUFWdGjqsIu0Gh9/BObdakMBnvOxPVZ8b59dQtL8Bqnph/jSV1LqI/zkh87aWjrYGVhRna0mmVVH0npVYO+sIAhLo9nNlRJoQQQgghhBBCiIkkAeCzVSz4G1tiecaFXHC++p8fnniLjz+Jpk/WILAQ4lMtIzubCYo7TG0Zhbjqt9Px5AaWz7Fh1uZrzK/vYM08OxZ1ghgABrOVguX1NLkSA7t6ymLMp2r7XupXzcFuSfIHP8ZS6lblEXf4kekpK86QuSzLt0C4j66d0R+iTTKT774zcX22ZI4DEwrB7ie4904nTmf0tbiWQ9rCaZD6uTBgstiZt+Yx6oqN2sy0Sb2+E2+PezFOp5Olm7q0WUIIIYQQQgghhJjCJAB8NtIGfwGYTsaf53DBuQZmfPAS/r4/cDKWNe5BYDOzVzbQ9tTgjIz25mqc8x7iKa+Xp9bPHig5e/1TeL2PUg5AOY96vXhvuwowcsM3ou/f9RCzAe55FK/3KR7SLA1tvHYRDza3s9cTLf9UG5vKrqOiyRt3bAaO/9T62Zi/VMGjccsaPtXyIM5LEg4LGLlu4YOJyx969tLe/CC32xNLDrTDfjsPtTwVnXE2+Mn2v008zt727Tz4t5qDCCFEmuWuWk6Jw6oGdnoO0qtO/BqWcX49SxwmIIRv93o1+HPnenb7QoAB21wXpdH4ip6yAKV1NcyxGiAcoMfTiLti0UCAqbJ1sFw8V/0SdSbkwR5GqTboLCvODGNZMTkmCB7ewX5tphjWxPVZIdlZgOJn/6anOXZCmz+5hHs2D9w/7ly/m56gApjJK1miLSqEEEIIIYQQQgiRVjfddCN33LFA96u09Ha+8IUbuOYae8Lr4ovHmsKTunNmzZoVmysqNDIzM3nrrbe0yWfE7NmzOXDggDZ5hOBvzB/o/+UbXPSFP+Hd3/434VMGzsv8C674bCbTACIv43/hf/nwtM64kVvWt1D5BTPKm70c6f49b3Mxny24AftFoBgMfPRcA4s2qHWfvf4pqr/wB37ovI82buD2r92A5U//Cue1RgLPPsMLIeADPz/Z+QyBex7Fe9ssjvzzIh6K7RlsL+fRh2/nqmkRAj2/5IWggsFyHX+VZ2HGSQMGw8vRYxMNAN/OrP97GSV7Fm93/4IXQ3Cx/cvceLUR+r2sqGhB3WHYyC1rW6gsMMO7AY489wJ/eB8uvuqvuOEvzBiUl/nhg/fR1qtWQ22HQjAIf/hpAw/vfoHYXB37PY/y8G1XQVx/XPOlG7nqIoXeJ5dS3XFmZ/WI0zeR137KMgpZuW4ZRTYLpugspXCghz3btrDHFxuDLpq8Jdj8Hpzuw5TWrKQ0z6rOogwH6Nm1ldqn++IOqi75u6xocNanEvLT+cR6th1KjBgYHXNxlZWSH/f5SjiI/+AOqrdF55O5mvCW2BLeN5Qfj7OS+BhhsnVISmEdHWvyOO65n56cOhbaTaD48bjd+EtbWF1gBiXIwcZytsSmwRkdlFatpCTPOjADTAkH8O3ZRu0eX/zRYaC+NiyxjogJ97BZM7tuXNsGkFvD9lVGurZuYY8vl7qONeSZwvRsXkytZlqfq8lLiU0hsM/Nim3x5z2Xte0bKDAr9O5YQPUefWXJXUv7hgLMoR4aK2rpSuIWmONqor7ERqSnkYrOItrW5GHye3AOEy3WUzYp0XHp9yyiNVTDytI8rCYAhZC/k2b3Ng7HtSGpsR4vmWszOi617Yi11aAEOdhcyZa4zkxq7Lia8JZk0bO5gk5HdFa4AbVtvR621O5k4PYQpWf8xlu53cs8Sy+7l1aTOJlV530n2ett4Lxpf1RQqI57ovU9A/eduVUNlObHlQ0H6Nu/E/fOw9qiCUbuM5Wec6GnvkP6SJsdR9dxxxrres9FtHy4ZzOL429gxXV0rM7DpO2HT9HYGdFodR7hPjnudRBCCCGEEEIIIcYQfPMdLJfM1CaflszMTP77q08B8MVfrNBmj4uior9iwYLbmDFjujYrZW+/HeLxx9vo739Vm3XaZAbwWcZ0+dUjBH/jzJhF9p9m8snHCh8EXyL0fjTdeBVZf3Kap/yvH6D8C2YU/w95cFk1Dz/eQsvjD1O97EF+2M8Yy3we4YePt9Difxv4iOBzLbQ83kLLzmeiQVktK+Urb+UqQ4gjj93Nig1NtDzeQtOGFdz92H8SGeHDjH96MS8/djf3fVs9/sOra3nmdSD78yy6Plrorx+gvEBtR/WSFTy0NVq2ZilLtx4hZLiKW+9ZSuLigmYMLz3K2rjgL39azop5V8H/eRP64z5XE0feNWC/eQXXJRxDiDTIcdH0vTXMsw8+dAcwWfNY5hpmhtSMbNa21LMsFoQBMFnJW15DTe5gsdKG4Zb8tTFvzfdocmUPJlJIzdpVzNF8vsFkwT5vDW1VI+8RO5bk66BPVn4NJfboQQ02iqoaWFUQ/bWVwUJ+San638Zi6lrqWVYwGFAAMJis5C2rp72ueDARcDXtjdZ3hBtUnLS07egWVpTXxgX9RzIfWzag+OmKD+hm5FJW58JhBjCQ7SjUWRYcc2yYUej1JBf8JaeKmhIbhlA3T9R2Dd5fh6OnrE5ZRS3UL4sFfwEMmG3zqKmLjgXQP9b1XptxBoO/ATq3JAZ/9Y0dEzmrWlgzLxb8RW2bfSFraxI3h9YzfhPMrafICuG+rmEDmZDkfUfn9ZYuevq3tGEvq+ZoypqsOBYuYdTtYsfoMz3nIqn6Fsbtme1dQ54JMOWxRrPHbvwet0kdN+Y0xrpuRoP6782PFD4aSPsUjZ1xNBnqIIQQQgghhBBCnC0uvvhizjnnHH78432sWrV6yGvjxs185zuPJ/V6/PE2jh9/g08+OcVHHw084RhXpxkNFGda+NVjfJDMDF6zlQyjgfMtV2O+IJoWeZnjb5zSFNRn9k3XYCTEkSfbiE6Ojeql7en/HNeH8Rhv4VqbAaX3GR7pTDxypPMRfvl/CUmD/u+XmvK9/Mf/BAETpkw15fY5147QDvXYB/xgsN/A4sQcXj5yJCHFOv9GrjIovPjzlsTjRJ7hV/8TAYuVG+LThRh3udTUlGAzgBL04WmsiC7Pey+NHh/B4S5Kax4FZoVgz27W3+nEucjNPr8CWMiZ4wDAWNrAErsJQr2Dx3Q6afT0EsKArXgVc+MOqURC9HY+weZ77xws2xlAASyOEhwArZUDeZt71IV7/Z64vSedTpxxM6n01kEPk8WC0vsEdzaqSwibrVbwe7j//k6CgMGSQz5QWOMizwyEfOzeGNe30baZ85ZQo3YZxrIG5toMoATobLx3oL4V7s4hP3JJZ9uSY8FoAELH6UOdOTe3qomOJzewMC5AZzLbdZaF/GwLEOS4UkVDW0dccKmDtoaV5Cf8sqaQtevmYFEC7Nu4adSZiPrK6mcym1GCPQPnuaK5hxBgsM+lKi5uk9RYh9SuzajB4K8fj3sFW+OmIKcydkwmkzqG16t1Xh+tr8lWRH7suDrGr1ZZcQ4mghzdPcpCxkncd/Rcb0lL633HRZHdAEovu+PGw72NHnyjneAx+kzPudBX3+TpO26SY13nuRjOlcUraVriwAAEffuJzVH9NI2dUcXVeeC1eaSl8tNUByGEEEIIIYQQYorKyMjg1KmTvPPOu9osAF5//Q+8+GJvUq+33nqbGTNmEIm8RzB4XHuocSEB4LPNe//L/77wv8MHgT+BgeQZmVz6uUKuHNfln+GqS4zwwSu8+Jw2Bzi92PJQX7QyCwj934FhAssRPhrY5DhRJNg7pPwLoTBgxPxn6t8Xmwwjt4MIL78ZAS7GclN8+tv8oTv+b7jKbAIMXHdP4gwar9dL5Q1GYBZWzZ7GQoyrwhJyLeqSoM2Vblq7+tX0E8foanVT7h7mUboSpLv5bsprd3L0BBDxsc2nvs9ozABgbr4NAyG6G6sHjwl0tVaz26eAKZvcWOSIQ2wqX0r11qc5FLeZZNfWo/QDGI2oR9VHXx10Uvx0bX2aE139qF+vQQ42t9LXF1HvHzMMHGY+8xwmIEjnRjc7D8f17dYV7PCF1eBVsRodXJJnx0AYX+sKtnYdG/iofl9kcJZaVFrbpkckTMbKBtrb61k1x4YJ1CDobt/QgIGeslgpWj4He/y0MkxY7PNY11RDbMJncd1yCswK/v1bSVhZehh6yqYi3LubBeW1A+e5f3+tei6wYBuI2ugY66lcm0BOWQN1JTYM4V52uytp1bQ1lbGjBA/SWOFm51G1zke3duFX1HEeW1REz/hNkL2SfLsBpfcgW45qM+OMed/Rd72li77+7ScSBgzZ5M0djC4e62rFXe4eOZA5Rp/pORdJ1/dQLYsHgoKb6QlHl5LWBAtjKwQnfVxSH+vJMuWtGfi31WOr52EzgeL3UD7QeZ+isTOuJkMdhBBCCCGEEEKIs0dmppmPP/6Yt98OabN0u+iiizj//PM5ceIdbda4kQDwWeiTyMvDBIE/5sTv/pswxwke0wyYcQr+DlA+GhJgTSdFeVubNEEUPhq24SF6f+bF++PhX796WVteiHFkN2MCQr79yS23C6D0c3C/Zi/C6KwhdZ/FfHIsBsBMwYahP25Y7lDzLHGzqYz5ZdRtb2dvQtkSRtiJMAn666BLv4/Wwefz4D/M1iFBxejM12AfXUPy4Gm/Gjo2mq8ECsnOAjiOf+iEPo00t00P2zzWzLNjNoAS6mXf5jvVIKhf0ZbUV5ZomUZ33KyyTgIKYMll4VwwFtfhyjOj9O6iUhvl1NBTNlXH+3Zqk+gKBLVJyY/1VK7NrGLqFtoxKX48tdXsHNLU1MZO/+EtmjoEiSScNj3jN1GhqwgrYfq6hvZfgjHvO3qut3TR27/72djaTQgTtnlr8Hr30r69nqr5cWvpD2P0PtNzLvTWN1k6j5vKWD8NwYObWZCwl+2nZ+yMr8lQByGEEEIIIYQQ4uxgNBq54IIL+OCDD3n33eFnAOsxa1YWM2ZM54033tRmjRsJAJ+lhgsCT5s+zMbT4x38PQlcZMX+p9oM4KIZAzOJxoWiqEtq/ukt2hzAijG2tHUK3g4rcP4VXPMFbQ6AUZ3prAR5+VltXqLQ++rM4g8D0f2Mh7zaeWakpaqFGEfK8L9OSNEMDHou5sK1tKxbSJ7VPMY+4HrorENaKfi0SSNRFMb+/ddkaFsIJRYADPvpbHazYGk12w6pATqjI0sN6AR9OsvGBOisqGZb12Dasa6tbDqoLsdvzIbcohxMgMG+LDFYsiZPXVbaVhJNa9JVdjz3rTQbNCM6hbGu69o8fpguv6LuS71svjY3/WMnqfEbx1hGicMEwaMMs5JxinRcb+NOf/9GujaxdJGb5n09+IMKZquDOcs34N3bhGu47c+T7bOkzoX++iYntePqGus6hHs243Q6uXP9bnwhsBStpmnYzp3iYycNJkMdhBBCCCGEEEKIs0FGxkzOP/983nvvPV5//Q8AnHvuudxwQy7nnXeetviYZs6cySefwDvvyAxgMYzEIPB0LvzzQq7+/Jf47JUz1QLjHfwFnnkpAFj4q7tuIWEbR+N1VN56XdIPxMGIebggcrxn/5NXImCw30KFurXkAPPf3sdfXZqYpscPn32RCGZuuLMczaExznmA2TZQ/L/Bq8nTeuE/XiaEgWturhhyHCHOiGBE/aFETrE25zQcov846nKaFdr9DocuFTp/Xh5mQAl00hi3j6DT6cGvOXLy9NUhPaKBT0sOK4dZOXS+LQuA4/1HgRNEIoDBTLambI7LQWLSZGjbHvxBAAV/1xa27k8Mm7jyrIBCsO+wzrLgD6nLrdqKE74lAMgyJv8tMRnMz7EACpHoRGBdYz2lazNCa+UCPH4Fs2M57XXa96Zr7OgZv4Oyy/KxGxR6DzYzzErGOum53gaZsxLXu86Zry4RnJoU+zfiY/+2WirLF+Nc5GaHLwQGG3NdpZqCyfSZnnORYn3HpPO4KY11/U4c3Yn7iR7CGLDNXYVroDM+HWMnbSZDHYQQQgghhBBCiEluuCWbS0pu5R/+YQkPPFDFlVeOFfBKlJGRwcmTJwmFNCvmjSMJAJ/lEoLA55zLdMN0zmG8gr9Wyhv34vW082B0H9vAtqf4VQiMN1TyveaHqPxaBRVVD7G9dROffz+Q3NLQ/hAR4Kq/bqDyaxU89K1qZmvLAOCl5acvoxisOB9up+GbFVR8rYIHt7TT9ncz+MPr2vI67HuYtudCGGy307BrOw9VDR67veoGzKEjtNQ+NXZ7nnuU9udCGP7UmXCciqqHaGhpp33t8C0TYtx09ah7eVrm0NFUxfz8waff+WV1tNWnNh9yf6/6Y4859Q24ikdfP9QSDeopJ/roiu6LemWxi7rtxUOXxY06EVGvLltRPWW5w+8QrKcO6VDIHnx+BbAyr76esljfZuRSVtfGMocJlF56dkUAH77jauCzaG0VhRmD5epLbEN+HDPRbQN4+qgfBQO2uXXUlUWX/MzIpay+nTkWIOzDs0d/2a7DxwhjwL6knpVxe27ml9WzusAMBOjdD4dqFw8JjjidTpybe9Q9hf2eaFqlrrLa+EqyjOZCHNlq0NqYnU9ZfTvzrGrb9j2tltE11k/j2mx1N9MTAnPe6iFB4PSMHX3jV5VLWYEVwn107Rzz2zIJeq43IKSuEmJ2lFLqUM9b8com6pY7MMcdNd6433cK17K9rYGq+YVcGTtcxEdPdz9hwGDQ1iSZPtN3LnTVVwddx01hrCdzLoZ1qJY9veos+eJVsc25Pw1jR1W8tl1d7aCjgbLTnaGbYh2EEEIIIYQQQohPo9iSzW+++dZAWmfnL+jt/R9mzbJQUeGioOCLCe8Zjbqf8Ee8++4ftVnj5pxZs2adVohwKsvMzOSttwZP5pk0e/ZsDhw4oE0e0bSLruaKv7yC888Zr+Av0QDwo9xui/CrR5fy8L9Hk403UlFbzpdzLBinAUqIwHN7efS566j7xg3wXAOLNqh1n73+Kaq/8Ad+6LyPtoHjGrnlgQbKb7Kq7+9/hrUVTbxwz6N4b5vFkX9exEOxzwLsf/sg9912A1az+tgzEuzlF9+t5aO/e4rbbS/HHbucR723Myvu8wfc8yje267i5R85ue+7sUQjN5Y9yNKvXIP1ougjVSVE4LfP0P5P7fwq7tns8O2IMTN75VqWfsmOJTbhTVEIvf6fPPPkI7R3j/SQV0xWE3ntpyLH1TRsYACigbGBKUcumrwl2MI9bF5cyyFN0USFrG1fQ8FIz3/jjpHtaqJppM8nseyA3BraNhRhiU8DwI9nIIiXfB2SVlhHx5o8TAP9Eu0T7d+xY+e4aKovwTZs4xT8HvfgnrQjtSnkJzDDhpX4+qahbcS1T5sex+8ZnIXmatpLybCNC9HTWEFt3Iae41NW02fDGXKORqGn7EhcTXhLhoRvoxLbpnesJ31tDteOnPnUr1uOwwyh7kaWbuqKvlHH2Im2Lf6cqwqp61hDXvyY1DV+wVjWQPtCO5Hu9SzdNPxcVpWO+46e681YSkP7MuxDyoYIhc2YNfWFUdqY6n1n1OtNwe+ppDJus/Gk+2ykeg57LnTUd8Aw538IfcdNeqzHjNTG+HMRHb/hns3RfaKjcqpo+6c5WAjSeX+5un/7FB87qui1FP1r6HU9guHuL/Hp8WUHjFQHIYQQQgghhBDi9AXffAfLJdGVbMdJZmYm//3VpwD44i9WaLNP2223fZUvf/lL7N//M376058n5N16698wZ86XOffcczl48Jf88IdPc+rUqYQy8YxGI6tXfx2DYQbNzU8QDB7XFhkXMgN4ijj57kv87wsvEnr9xXEK/gIEaFu9AGdJXPAXIPIrWmrKWVQSnYG1YCkrvv1DeqOjSTkZ2ywSDmxYhHNI0DTCM4+sGHx/RRMvAHz3PpzOxOAvQO+/PcyKpQsGZnwtKq+mpRtmTEssB23c53QODf4SO3Z88Bcgwq92rmXFksFjOxcsZcWGxOAvI7YjJsSBbdWUL4qblbZgAUtXPSTBX3FG9LVWcvfmffQGwwxefQqhQDc7WncllE3eITZVuNnRHSA0eNBh9bdW0nowsVw42EtnczPd0aVzhzi6hS1PdBMY9eDJ1yFt+lqpdD9BdyAU17dq+/ZtvjsxkHl0C/c3dxMID5Qi0LMDd8Vuhn6FT4K2Aa3u2iF1CAd72bcxMaDLOJRVQur+waMGfydCTyfdvgChgY2OGbx+3Ilt0zvWT+va7Hsa90YPfgXMBatoq4nNBE7T2NE1fqEs345B6aVz6yiBTL30XG+RPdQ2dxKI2yg3HOhhh7uCg8NVmDTcdw7V0uzp0RxPiatvYvAs6T7TdS501FcXfcfVPdaTOhcj6NvKjp7oLOnYMsVTfOyoWvF0Rysd7qXnoDZfp5TqIIQQQgghhBBCfDplZGRw6tRJ3nnnXW0WP/nJT9m5cxfvv/8+X/5yERUV93DhhcP/5Jq4/YTff/+DtAV/kRnAo5vIWYB6ZwBPBjd8s52HbjLS++QCqju0uePMuJSG9kXYQwdYW96gBpCFGCcTee0LIcSkl7uW9g0FzPA1s9i9X5srhiN9JiZKcR0dq/Mw+J5ggTu6nr0QQgghhBBCCDGBzsYZwJWVK7Bas/nud3fS1/c/CXmZmZksXHg7/+//XcMHH3zAgQOH2L//mRFnAV9zjZ3y8jJeeun3PP748NMOx4PMABbjw17O0i+YQfHzmx9rM8ebkVvuvwW7AYK9ByT4K4QQQpxBpUvyMBPCt1sCmcmSPhNngqu+jXpX8cCevhlXFlNV6sCEgr83toy8EEIIIYQQQggh9Dj33HMxmUx88MGHvPtu4gzgefO+wje/+Q3+4i/s/Nd//Y5vf/uf+clPfjpi8Je4/YTffjtuebI0kBnAo5jIWYCTdwZwOQ1P3Yjx/wK8+PIfUICLs6/jumutGKdF6H2ymuqOgPZNKZv9zTbK/yzMK//7orpU3wWzuOZz13LVJQaU4AGayhuYjL0kzm4Tee0LIYQQQqTC1eRl2C3NgwdZX76FMRYfF0IIIYQQQgghzoizbQbwpZfOYuXK5bz33nvU1zcAkJ19OYsW/S1XXvlnvPvuu/zoR16ee+6I9q3DGm0/4fEkM4CFTi/zymtwse0GbvmqE+dXndx4rQWl/wg/fKRiXIO/AC//78uEjVauKVA/yznnBqyGEL2dLdRVSvBXCCGEEEIIgF27duMb3DwalBCB7h24KyX4K4QQQgghhBBCpCojI4MLLrggYcburFkW/uRP/oRf/vIwdXX1PPfcEQoKvsgddywY9jV//q1kZKhLdo22n/B4khnAo5jIWYCTdwawEFPfRF77QgghhBBCCCGEEEIIIcRUdbbNAC4q+isWLLiNX/6ym92790J0WegZM2bw4YcfDpRzu6vJzr487p2D3n47xLZtT/D663/g/vsrmTXLMux+wuNJZgALIYQQQgghhBBCCCGEEEIIIYTGzJkXcc458Mc//nEg7dSpUwnB33PPPZd//ufHWLVqNd/85j/S1LSd73zn8YHXjh1PEgwex2g0csEFFwy7n/B4kwCwEEIIIYQQQgghhBBCCCGEEEJoZGZewqlTp0Zdsjk+IPzHP4bp6/sfXnyxd+D18st+Tp06RUbGTM4//3zee+89Xn/9D9rDjCsJAAshhBBCCCGEEEIIIYQQQgghhMZFF5n4+OOPE/YATtVFF13E+eefz4kT72izxp0EgIUQQgghhBBCCCGEEEIIIYQQIs65556LyWRCURQuvNDENdfYh7xycv6cCy80ad86rFmzspgxY3ral38GOGfWrFmfaBOFKjMzk7feekubfEbMnj2bAwcOaJOFEGfARF77QgghhBBCCCGEEEIIIcRUFXzzHSyXzNQmn5bMzEz++6tPAfDFX6zQZqfs4ovNfP3rFVgsWdqslJ06dYpnnunkxz/er80aVxIAHsVEBoEkACzExJnIa18IIYQQQgghhBBCCCGEmKrOpgAwwGc/exWf+9y1nHvuOdqsMZnNZmbOvCghze//X/bu9XDq1KmE9PEmAeBRTGQQSALAQkycibz2hRBCCK3S+g6WOUyEuhtZuqlLmy2EEEIIIYQQQghx1jjbAsBnK9kDWAghhEgrF01eL96OOgq1WWLiuZrwer00ubQZZ1BhHR1eL94JrcRIdIxfYxkNe714t6/U5ojT4qLIoe4jYy4ooUybLYQQQgghhBBCCCGEhgSAhRBCnHEOVwPteyc46DaVZeQyv6qJdq8Xr7eDulEid4UrG2jr8OL1qq+97dtZOz9HWwx0lgVwzK2ioa2DvdHyYwVajcXRQGgSwVA9ZcWZkeMqwm5Q6D28U5slTksrB31hAELdHqR3hRBCCCGEEEIIIcRYJAAshBDijMvIzsZs0KaK05ZRiKt+Ox1PbmD5HBtmbb7G/PoO1syzY1EnFwJgMFspWF5PkysxsKunLMZ8qrbvpX7VHOwWE0mdamMpdavyiDv8yPSUFWfIXJblWyDcR9fOiDZTnKY97sU4nU5Z/lkIIYQQQgghhBBCJEUCwEIIIcQUkbtqOSUOKyYUgj0H6VUnDQ7LOL+eJQ4TEMK3ez1OpxPnnevZ7QsBBmxzXZQa9ZcFKK2rYY7VAOEAPZ5G3BWL1Pc4nVS2DpaL56pfos4ePdjDKNUGnWXFmWEsKybHBMHDO9ivzRRCCCGEEEIIIYQQQpxR58yaNesTbaJQZWZm8tZbb2mTz4jZs2dz4MABbXIcIzk5aynOmqHNGOpjP13d2+nTpgshhjWR137KMgpZuW4ZRTYLpuh0y3Cghz3btrDHF5uN56LJW4LN78HpPkxpzUpK86zqLMpwgJ5dW6l9OvFOUbiygWVFg7M+lZCfzifWs+3QiYRyRsdcXGWl5Md9vhIO4j+4g+pth9QEVxPeElvC+4by43FWEh8jTLYOSSmso2NNHsc999OTU8dCuwkUPx63G39pC6sLzKAEOdhYzpZotTE6KK1aSUmedWDWshIO4Nuzjdo9vvijw0B9bVhiHRET7mHz4lpih2W82waQW8P2VUa6tm5hjy+Xuo415JnC9GxeTG38BwOuJi8lNoXAPjcrtsWf91zWtm+gwKzQu2MB1Xv0lSV3Le0bCjCHemisqKUricmgOa4m6ktsRHoaqegsom1NHia/B+cw0WI9ZZMSHZd+zyJaQzWsLM3DagJQCPk7aXZv43BcG5Ia6/GSuTaj41LbjlhbDUqQg82VbInrzKTGjqsJb0kWPZsr6HREZ4UbUNvW62FL7U4Gbg9ResZvvJXbvcyz9LJ7aTXDTQCeW9VAaX5cfcMB+vbvxL3zsLZocm1L9n4WG49hH82L3UOC08ayBtoX2qF3NwuqBxdXHtc66DXavXKEsa6nf4UQQgghhBBCCCEmUvDNd7BcMlObfFrOymf6aSYzgM9WGSspveHPueJPrxz7dVUxX/lstvYIZ9hsHtrlxdtUPpj0hWraPF72NpZjjS86RRkLKni0PbpfZfuD3Dju7TeyaMtevJ52HvxrbZ6Y0nJcNH1vDfPsgwEmAJM1j2WuJfElVTOyWdtSz7JYoALAZCVveQ01uYPFShuGW/LXxrw136PJFX9PKaRm7SrmaD7fYLJgn7eGtqqR94gdS/J10Ccrv4YSe/SgBhtFVQ2sKogumGywkF9Sqv63sZi6lnqWFQwGfwEMJit5y+ppryseTARcTXuj9R170eO0tO3oFlaU18YF/UcyH1s2oPjpig/oZuRSVufCYQYwkO0o1FkWHHNsmFHo9SQX/CWnipoSG4ZQN0/UdjHqW/SU1SmrqIX6ZbHgL4ABs20eNXXRsQD6x7reazPOYPA3QOeWxOCvvrFjImdVC2vmxYK/qG2zL2RtTeLm0HrGb4K59RRZIdzXNWzwt7RhL6vmaOprsuJYuATt7s362pbE/ezoJroDgOlKiuYmvhWg1GHDQJi+rsHg77jXIc309K8QQgghhBBCCCGE+HSQAPBZ6c+59fNf5MJz4pI++Yjj//X/8c//Xx3/9l/H+Vgzr/uya8v5XHz5ycBkSG5fyKnAuIi6B5xcZQzyQqeXX/W+nYb2X4wpiQnhYqrJpaamBJsBlKAPT2NFdHnee2n0+AgOE4zBmkeBWSHYs5v1dzpxLnKzz68AFnLmOAAwljawxG6CUO/gMZ1OGj29hDBgK15FfCxFiYTo7XyCzffeOVi2M4ACWBwlOABaKwfyNveoC/f6Perfg6/B2b9666CHyWJB6X2COxvVJYTNViv4Pdx/fydBwGDJIR8orHGRZwZCPnZvjOvbaNvMeUuoUbsMY1kDc20GUAJ0Nt47UN8KdycBzeens23JsWA0AKHj6uoQRgdzq5roeHIDC+OCWCazXWdZyM+2AEGOK1U0tHWoP3rxevF6O2hrWPn/s3f/8VGVZ8L/P5Yy2p1BGaEM2sxahrYZd59IS1IXqKGppLjQgQiGBXnMgsZAgBKwRmgSShKUpGAsEAqJxlTYuDQsGBqZwpomlkJL+NqEVmf3cWLLUDtZ7VB0EGZWOWj9/nEm8+NkEmYCgQSu9+uV15pzrrnn/nWG7ly575sJYVtFQypFa9IxKW4OPLW+x9Wlqnhi42cwGlE87cFxzt3WjhfQWaexMiznF9Nch749mwGh5K+LxoIlbA5bgtyXuWMwGNQ5vFat89pAfQ2WyUzoKjeO+au1YEoiBjwc36NdXwuQw2SrDhQne8L6bPmmRhyaTuhL22L5PNt5zImCgcTJMyNfq88h2apT+yZQ9f6qQ1zCPiuDPxt62u489v4VQgghhBBCCCGEENcPSQAPQp+9fSETTaHfPz51nJcaHuVHv3+JU584+O3vl1LS8FN+f+pCKOjvkrj3y18J/T4QvFpGVoaN2Y/VXvTL5ejGkV1Wy+6KsFXFA9W/TMKqgxMH8ijaXE3Z+mqOXnL7tdzUPjYbW0YWZa9q74lrVmoG403q9qzb8gqoaelUr585SUtNAdkF3bcKRfHQuu0Rsot3cvwM4Hew3aG+Tq8fDsC0CRZ0eGndlB8qE2ipyWePQwFDAuO7MkccYX12FvmbX+bIydD2qC2bj9MJoNejlhqf+OoQJ8VFy+aXOdPSySkAPBzeVkNHh19dVTpUxzFmMj3JAHhofqqAncfC+nbzEnY4fGqCZ4qaHZyfbEWHD0fNEja3nAy+VafDT9inMfR32+Lh9zF8aQV1deUsS7dgADUJusfRPdkUTyxmJi9Kxxq+JBEDJut01lSuomtR5JTSRUw0KrgObiZiZ+ko4ontC59zD7Ozi4Pj3HmwWB0LTFiCGb845npfnk0gcUEFpRkWdD4newryqNG0tS9zR/EcZlNuATuPq3U+vrkFl6LO866/G4pn/kZIWMoEqw7FeZiNx7U3ATrx+wBdAsnTQsnQky01FGQXRGz33pe2xfJ55t/rwKWALnEy4eu59fOTsACe9p10Vb2/6tB/Yu9fIYQQQgghhBBCCHH9kATwoJNK5te/wmcBPvFz4tgW1jeV8dsPYdTthXxv5nbm3Z4EH75EfdMSao6d5Nwn6itHfXUhEwfaKuBLYsT8xcDKtAFu3EgD4MfrktU44jKzGjEAXsfB2LbbBVA6OXxQc8ZsYMXZvOIjwAQSTTrAyMR1Xas3Qz+LktR7prCFbfoJCyitqqMhIjaDHk6xjEH8dYhLp4OaUG4HXMfY3C2pGPh88XTQ0u0evOxSU8d64xgglYRRAKdwRVsEGaGf2xYPy3RWT7di1IHidXJgw0NqEtSlaCPjiyUQs6kgbEViM24FMI1nzjTQTyklJ9mI4txFnjbLqRFPbF+d6ghtAdylxe3RXop9rvfl2Rw1hdI5VgyKi8bifHZ2a2rf5k7nsY2aOnjwRwxbPPM3UmrOZMyaLZQjHeSpmla8GLBMX43d3kBdVTkrZ2r3Ru5b2y7+eQb4d9LS4QOdhQlhGeAF4y2Am/a9XR8G/ViHfhNr/wohhBBCCCGEEEKI64kkgAeZW7/yIF8dBnz4Fi/9xwJq/niEC597gHlTn+d7945n1M2j+Oq9xZRMLeTrn7vAiT8+wfr/+CknPgR0XyH1TvlC8Gowfi58FZwQl59yIdYMUyyGootnO/HUIqrXzCHZbLyM25rHWYd+peDQXuqJouDVXutmILTNi9KVAPS5aN5WwOysfLYfUZNY+qRRavLS44gztoub5tx8treErp1s2cz6wx7AgD4Bxk9OxADorAsjE22rk9VtpS0ZgWuVccVezjNPjTrNjO7DXI/r2Tx1jBaXop5LvVCzXTH0/9yJaf6G0S8gI8kAnuPBLZSj8besJ2tuAdsOtOPyKBjNSaQvWoe9oZKc4LHJ/du2g3sc6hbOExaoFxKWkmQGxXmM7cE/BunfOvSX2PpXCCGEEEIIIYQQQlxPJAE8mNzwAA98dZT63x/7OPsJcFsxJbMf5KujIr+x/Oyo8Tww+3kevg345BTnPlav33pXZvyrgPWTyN1Yy+7GwBfujbup3ZjLpIhzHMH6QCFVdQ2hL+Yb6qh4eFxkUIRsttjt7F6bFrr06Bbs9t2U3GskbekW6hpC71n1fRvGQFja2t3Y7fmk3AxYZgXfc8ujoaK60Y9j7verqNsbljzYXUvhjLCYkWlqW7ve126nYVctFYsnEdncUN2N38xlS1i7d1cXYhsZCLu3hN12O/l36wE9Kd8LxKxNi95+wuoQ7O86qr5nw7Z2d6BvIsPDqf2yhfBNsfUTc6mo3U1D+Ph93xYWIQY1j189ezRxivbOJThC5ynUrY9zNedQhv3kBfYWnTk9GSOguJvZFHYGpc3WiEtTcuziq0P/CCQ+TYksDTsDtstMi/p5fKrzOHAGvx/QGUnQxCbmJBF5aSC0bS8uD4CCq2Ujmw9Gprhzks2AgqfjWJyx4PKqW2Nbpmj+kQBGDYYtG8LMTDQBCv7AQuC45nqfnk0/NXmzaXQpGJMWUVeqfW1/zZ145m9IwoIJWHUKzsPbglso98jv4OD2YvKy52GbW8AOhxd0FqbldC3J7a+2BRxfT6sbdJYkFughITM5ysrlfq5Df7po/wohhBBCCCGEEEKI64kkgAcNPYlfm8lY7XfnNxr4bE8J3RuG8rkbNdc++xXuHZequdgL/VRKqgux/YOB99ubsO+30/SGD+M/2CiszCelK2xeBWUPT8L00Zs07bdj338Up1eHydyVso2P6f5K8u+BN19RyzrxkR7zPbmULTUDcOKoet39EXD6dez77dj32zn0hrakAP1USqrXk3WPGZ2nLVDHJtpO67i1K1lrzWZLdT62fzCi/PGoWmZzGx5MWGcUUr12qiYJDJhmUfm9b8F/q31z9A9+9AmTyH0qFzPACbWco28rgIL712o97UdPaEtS6adSsilQh45AHVo9GCbl8shX+7As6e58KotsWD/3F9oOBNrcqWAyhR0iLQa3lnb1LE9TOvWVK5k5IZSqmbCglNryvq2HPOh0AybSyyvImaLd7zSSKZDUU8500BI4F3XMlBxKq6Z03xY34IxfXRVpmVzOgvHRz8iMpw79IZW9OFwKYGZ6eTkLuvp2+HgWlNayMMkAipP2XX7AgeOUmvicXLSS1OGhuPIMS7fVole7bQAvH3ehoMMyrZTSBYHdIYaPZ0F5HekmwOegcW/8sS3HTuJDh3V+OUsD5yMDTFhQzmMTjYAb50E4UjyvW2LNZrNh29Cuninsagxcy4srtq+5Ob0xlaQE9VNenzCBBeV1TDerbTvwshoT11y/hGezpmAb7V4wJj/WLQncP3MnvvmrGs+CiWbwddCys5dVzqlFVNVWsHJmKmO6HnW/g/bWTnyAThf63wn907aQncecKDoryfMTyUwygdfRbeVyf9cBYEpRnfoHWfUVLLjUFbpx9K8QQgghhBBCCCGEuH7cMHr06E+1F4VqxIgRvPfee9rLV0RaWhqHDh0KXfjsv7J0zkz+fkjg93PHeaGxjI4vPs0P7xkTitP4868z2f6nVOZlrFC3jgb4XwcvNpTyX5rYaNLW7ib/bmjb/AglzaEveK2LqyibYcL14mzy6yF7k51ZX3Zjn7uE6mCYHuNI8J72A2mU7Mon5fQ+bHm1gfvZbLHPYvRrFcxdF2jro1uw3z8WvG1U5pbQ1FWWNY/aiqmYPIcoyq7gdeihzGj0zK2oI8sKJ35WyIrnndoAwEx25RZmWfy0bc6NaCtYya4sY5bFz9F1WZS9RrDuY/Fq4q3k1VQw9TYPh36QTcXv1KvBfvzRXEpe7Sq3e/vVuKHd62nNZkvZLMbq/JoyIqmv/wv7bCuoBSYV1VE4UUfb5rmUNIfijCONeE/HtdHndeVqPvt9kZhT2XOSxtWILbhcLYdKewYWXzsb5hXT+8mUqRTVrWZiT7mDsDISciqp7On9iYwNGr+K2nWT6f6nCC4ag0m82OsQs9RS6lcnYwj2S6BPtL93lZ2YQ2V5BpaojVNwNRaEzqTtqU1eF+6hFsyE17cf2kZY+7TXw7gaQysYcyobyIjaOC/tm3IpDjs49vLEavosmm5j1It4YnuSU4k9o1v6NiCybfHO9ZifzWjtSJxJ+ZpFJBnB27qJrPUtgRfGMXcCbQsfc1UqpfWrSQ6fk3HNX9AvqKBujhV/61qy1vey/rfXOangaswjL3ggdxxt0z6r2tioplFev4xErxuv2YxyIJclof2fA/q7DoHXBH7rPjY9iDZHwq+HxwZp+1cIIYQQQgghhBDi6vOc/gDTyFu0ly/JYPtO/0qQFcCDxccv0dLRywqbOJxzvRpT8hdm8e279PDub6iNSIiC88XX8aDD/BV1+2KPzw+YuPOhcWGrZP2B5G/83L9+OpT8BXD+ijc9wOcM3b+cvhj9PCZZdSjOfRRGTf4Cd8xikkWH4mziaU1bwUntz97Aj5E7vz0p8tbbv9HEO/nVW+oZl4YRYZdjkkaaVQ+n26jT1tNZy8/f0Nbr4txeH6Bn7D2h7bMBSf5eYzpq8nhkwwGcHh9dR7WCgtfdyo6aXRGxsTvC+twCdrS68YYKjaqzJo+aw5FxPo+T5m3baA1sndvN8Y1sfK4Vd6+Fx16HftNRQ17Bc7S6vWF9q7bvwIZHIhOZxzfy+LZW3L5gFO72HRTk7uFUKCpgALQNqCko7lYHn8fJgaciE7pchljFq54f3Gvy92pob6bV4cYbPOiY0PNTENm2eOf6JT2bHS9T8FQjLgWME5dRu6prJXA/zZ245i8smGBFpzhp3txL8hfgSDHbGts1z7oS9gyFJyf7qW1BB9nj8KIzmzEpTo7tjJYY7e861NDYGvg32Oek/bD2fpzi6l8hhBBCCCGEEEIIcb2QFcC9uJp/MdBtBTDqGcA5cx5Ut4HuWgFsfpoffrPnFcAnfpVJjTtsBfDHb9G4u5DWmEa9a5VrL1yB1bfWLCrWzsV6M+D34Gy1U//iPtpOdwVGW63bfQWsugJ4dNRVrtmVdmZZTgRXt0YvM4p7S9j9vRR8rywhe6tbe1d10ZhAX/xhH7bHaqPXvUtgFfOJn9lY8bx6KbYVwOrv5jdqmV24L6xAVfQyImlXAKOfSv7mXNJu08EnXtzth9j3k3qaOuNPJl9PruazL4QQA974IurWTWSoYxvzCjR7KIv+MaWU+seS0TmeY3ZBYE9yIYQQQgghhBBCiEFIVgBfGbICeDD59CVe+r1mHY77CUpf/k9OnIu8zLmTvPryo9Rocpnvv7E3xuRviNIZOIs22s+v1M2YcdaRPz+LkvqjnPAZsKZnU1JbR2F6t1NzrxpFeV97aUC6oFzG5Ky/iYqcLJZstvP6u2C+exZ51XVsedSqjRRCCCFikjk/GSNeHNoDdMVlkVNeS3nOlOCZvsPHTGFlZhIGFFzOrq3AhRBCCCGEEEIIIYTomSSAB5n33/opvz8HDBtP1tRi7r15OB+efZ6axkepOfYW7589Q8exLZQ2PkHT2TN87uZ/5aGpS9XVv8pbHHnzIls1RvBxQQHdEB8/f7aa6mg/L7WFxXtpe7GMFdlzyXr6EJ5PjEx65AnUTaKvIq8PH2D6sk17J+TE+/gA4x1pYVtYh7nXzGjA8054e/uH/gtWzNqLgPGmodpLMfLjbq6mKDeLuYV1OM/qGHv/ErKjNlQIIYTo3d782dhsWfR29K+4BHoTSRmPsfVFO3a7nRe3Pka6WQeeY+zaeRn/SEwIIYQQQgghhBBCXLMkATzoHGHvb9/iY+Czo5KYOvN5ilIfZeyQM5z4YyEbX36UF/54hA+HpDI1dSfFM2fyf0apicNTv98R5+pfO6+7FLjtG2RfZCWvcWT4CbPg/VUVv30XuKkPZ/bGy2hCczJvpN+pq191VhslPbXj7X38thN01qk80S3GSvb9d6HHw5tdK577RRNvdhK1v/V35WG7SxdxLRb6kcaIhLb/jd00veUHDBi/EnZDCCGEEAPCrl17cIQOYwbFi7t1BwV5G5GcuxBCCCGEEEIIIYSIhSSAB6GP39lBqyf0+7A7/pmcf9nJ0qQHGDUkia8nbaboX1Zw7x1hqb//dfDqH94K/R4TP3XP/5wTip6UlXXUbSwkd3EuuYtzKXyyitrdW8gORM5eW8fu2goKA/fznqxk6h3gd/4Gu6bUy+e3uE8DxhSy1uaSu7KCwoeBewups9tp2JQdWEnrpPKZfZxQjJp2FLK+uo6KhwHcVG+OErOyhKpdFcyywImfPU3Fa9o6XE5uqv/jKF70pKz8CVVr89S+XFvFT578Or63Nat+urWzu68vrWR3XRUlK9Vxyf3+FrK/pod3X8f+O220EEIIIa42/7GdFCyZh81mU39mZ7Fk/V4csvhXCCGEEEIIIYQQQsRIEsCD0lv8/Lf/H+fCV/MO0fP34x7kew8W88C4BIYNCbsHvPNGLb+Pa/VvgLOWwpI6jr7tR584CdsMG7YZNlLG6vC2/oLfBMJO/MGNcouVSYH7U+/U4W6uprhwH/33faWf2u27cXp1mO+2YfuWGX3YgpkI0doxPYUvDfXw5n+HYlYUVtP0h7CY9BRu/dBJ0/ZCVjzv1BTaD14tI3e9HacHzHdPxTbDRtqX4fV/W8++sKR/rE68dQLPEBMp6eq42O4ezftv7KZsZSVXoDVCCCGEEEIIIYQQQgghhBDiCrth9OjRfUkLXhdGjBjBe++9p718RaSlpXHo0CHt5TB6EhOLmBLY3rlXH7toaa2iQ3tdDCpTS3aTl6Jw9IdZlP1ae1eVtnY3+Xf/hX22FdRqb4qYXc1nXwghhBBCCCGEEEIIIYS4VnlOf4Bp5C3ay5dEvtPvThLAvbiaE+biCWBxfUmhcEcJk252Ujc7n93a2wHZlXZmJfQeIy7uaj77QgghhBBCCCGEEEIIIcS1ShLAV4ZsAS3EIGB9NIuUkaC4ftvzmcr6LO5MADrf7DlGCCGEEEIIIYQQQgghhBBCXNNkBXAvruZfDMgK4OvUwxXsvkeP++03+aNHAW7F/LVxjEvQg99J3ap8dr8dFn9vIVUz4HUn3PnNSYy92cvRH2VR9mpYjIjb1Xz2hRBCCCGEEEIIIYQQQohrlawAvjJkBbAQA8nbf+Yv3IoleSq2GTZsMyYxbqSC+7V9VCzTJH8BvD6wTMI2YxJjh7hpe2G9JH+FEEIIIYQQQgghhBBCCCGuY7ICuBdX8y8GZAWwEFfP1Xz2hRBCCCGEEEIIIYQQQohrlawAvjJkBbAQQgjRr3KotNux15eSqr0lBpzEmUVU1TVgt9tDPzJ2MZK5LoQQQgghhBBCCCHEQCAJYCGEEFdcUk4FdQ12KnO0d8RlMXw8M1dWUme3Y7fXU3qRbFzStJVU1NbTEJb0jDY2qUsrqK0PxTTUVVE0M1EbBgMkNl76meWULpqI2ajT3hpw5BkSQgghhBBCCCGEEEL0RBLAQgghrrjhCQkMghzb4DM8lZzyKupfXMeidAtG7X0t/QRWVjVQviwdq8lAb0Mys7ye1dOtmAyhazqjmYmLyqnMiUzADoTYvpifnoQBBU/rcyx/yIbNFviZV8wRbfBVJs+QEEIIIYQQQgghhBCiJ5IAFkIIIa4R45ctIiPJrCYx2w/j9GkjImWWriLdrAOfm/bGTRTkzg0mPfNqQnH6meXMTzIAXhx71qoxD61lj8ML6LBMyyFTP3Bi+yaVhFGA4uLg+pc5eUZ7XwghhBBCCCGEEEIIIQaHG0aPHv2p9qJQXc1Do9PS0jh06JD2shDiCriaz36fDU9l6ZqFTLaYMARWBfrc7ezdvpG9Dn8gKIdKewYWVyO2gmNkrlpKZrIZgxpM+67NFL/cEVaout3uwsmhFZeK10Xzc2vZfiQyO6ZPmkbOgkwmhL2/4vPgOryD/O2BtZM5ldgzLBGv685Foy2PsNxjzHWISWop9auTOdX4OO2JpcyxGkBx0VhQgCuzmscmGkHxcHhTNhu7lnzqk8hcuZSMZHNwxaXic+PYu53ivY7w0iFYXwumro7o4mtng2Yl6WVtG8D4VVQt09OyeSN7HeMprV9NssFH+4Z5FGuXsI4vom7dRIzedjblFtPSNU2iyKm0k2FRcB8oYMn28DkynqK6dUw0Kjh3zCZ/78CI7ZtUtb/oPk4hcT5Dsc6dnErsGaNo35BLc1Jg9bYOQMHrbGRj8U4c/n5+hmKtQ5h45roQQgghhBBCCCGEEACe0x9gGnmL9vIlGZTf6fczWQEshBCDXWIOlT9ZzXRrKPkKYDAnszBnfnikamgCRdXlLOxKXAEYzCQvWsWq8aGwzIpo2+1amL76J1TmJIQuksqqomWka95fZzBhnb6a2pV935o39jrEZ9SEVWRYA4XqLExeWcGyiYENk3UmJmRkqv+tn0JpdTkLJ4YSeAA6g5nkheXUlU4JXQRyKhsC9b343rz90rbjG1mSXRyW9O9ZUroFIwrOxt6TvzATS4K6MrYlPPE6fDwLSnNIMgLoSEhKHSCxcUgtpT547vFqkg2AIZnVYWchRz0POZZnKM65AwYSl1WzenpX4hVAh9E6h6JVcbYrTHzzLPY6xDPXhRBCCCGEEEIIIYQQV5YkgIUQYlAbz6pVGVh0oHgcNG7KDWyNu5xNjQ480RJ75mQmGhU87XtY+5AN29wCDrgUwERiehIA+swK5lsN4HWGyrTZ2NToxIsOy5RlTAsrUvF7cTY/x4blD4Vim90ogCkpgySAmrzgvQ3t6t7Ersawc1ZtNmxhKxfjrUM8DCYTivM5HtrUjg8wms3gauTxx5vxADpTIhOA1FU5JBsBr4M9T4X1baBtxuT5rFK7DP2CCqZZdKC4ad60PFjf3IJm3Jr378+2xWpCggnwcEpZSUVtfVjCs57aiqVMCG6nbEKvA7yn6EBd1TptZSX1L65jTlgC1GC0DpDYKyCGZyieudPFYDCo8WvV52htINZgmcwErswzdNE6xDnXhRBCCCGEEEIIIYQQV54kgIUQYjBLzWC8Sd1ydVteATUtner1MydpqSkguyB8I9gAxUPrtkfILt7J8TOA38F2h/o6vX44ANMmWNDhpXVTfqhMoKUmnz0OBQwJjO/KBnGE9dlZ5G9+mSNhB6e2bD5OJ4Bej1pqfOKrQ5wUFy2bX+ZMSyenAPBweFsNHR1+/ABDdRxjJtOTDICH5qcK2HksrG83L2GHw6cm/KaoqyjnJ1vR4cNRs4TNLSeDb9Xp8HMh+JuqX9sWFzOTF6VjDV8eigGTdTprKlcRtiAc/D6GL62grq6cZekWDIDiaWfPHgfdjhoeCLGxOFLMvGDidAPtvsD2xREJ1cjzkCGWZyi+uRMq9jCbcgvYeVx9jo5vbsGlqPNxaERkbPoyz2KpQzxzXQghhBBCCCGEEEIIceVJAlgIIQYzqxED4HUcvMg2vmGUTg4f1JwxG1hZOK/4CDCBRJMOMDJxXeRWuHa7nUVJ6j1T2OpF/YQFlFbV0RARm8HFTivtWfx1iEung5pQPgxcx9gcefxxaNWpp4OWbvfgZZeaOtYbxwCpJIwCOIXroDZSq5/bFifF6+TApoJgsnP5pmbcCmAaz5zw5aGW6ayebsWoC7xmw0PMzi5mp0sJCxpAsf3pos9QPHMnpPPYRs1z7MHf56b1bZ5dvA7xzHUhhBBCCCGEEEIIIcTVIAlgIYS4BigXYs3+xmIouniWG6YWUb1mDslmI5fvNNA469CvFBzaSz1RFLzaa90MpLa5ac7NZ3tLqIUnWzaz/rAHMKBPAPCidCUAfS6atxUwOyuf7UfUBKg+aZT6RwgexwCJHUjimDuXXT/Ps5jmuhBCCCGEEEIIIYQQ4mqQBLAQQgxmHr96zm7iFO2dS3CEzlOo29fmas8X7b4t7szpyRgBxd3MprAzgG22RlyakmMXXx36RyDpaEpkaeROvQDMtIwC4FTnceAMfj+gM5KgiU3MSSLy0kBoG7i86jbElinBw36DRunDU/l7cXkAFFwtG9l8MDKlmZNsBhQ8HccGSOxAEM/c6S/9Nc/imetCCCGEEEIIIYQQQoirQRLAQggxmLW0q+dzmtKpr1zJzAmh9MuEBaXUludEhMfqoNMNmEgvryBnSu97EZsCyULlTActgTOAx0zJobRqSo9bQJ/xqyuWLZPLWTA++gnB8dShP6SyF4dLAcxMLy9nQVffDh/PgtJaFiYZQHHSvssPOHCcUhOqk4tWkjo8FFeeYem2Mvpqtw2g5dhJfOiwzi9nadhZtBMWlPPYRCPgxhnY4vfl4y4UdFimlVK6IHAy8PDxLCivI90E+Bw07h04sVdfPHOnb67eMxTfXBdCCCGEEEIIIYQQQlx5N4wePfpT7UWhGjFiBO+995728hWRlpbGoUOHtJevuJTv1VJyr5ETL61gxQtu7e1Lkl1pZ5blBPtsK6jV3rzs0ijZlU/K6X3Y8vr/3Xr16Bbs94+m7UdzKXlVe1MMBFfz2e+LxJzKnhMvrkZswSV+OVTaM7D42tkwr5gjmtBIqRTVrWaiUXs9IKyMhJxKKnt6fyJjg8avonbdZEzh1wBw0WjLQ61x7HWIWWop9auTMQT7JdAn2t+7yk7MobI8A0vUxim4GgvIqwkc8tpTm7wu3EMtmAmvbz+0jbD2aa+HcTWGVn3mVDaQEbVxmrb1GuulfVMuxWEHxw6E2PilUlq/muSIcdKK4xmKZ+7kVGLPsESMjaqXOvU03/r6DMVTh57eO+pcF0IIIYQQQgghhBAixHP6A0wjb9FeviSD7Tv9K0FWAF8jvnFT+FDewEO3DuH2sCt9ZdBF/eZaCDGAdNTk8ciGAzg9PrqOSQUFr7uVHTW7ImJjd4T1uQXsaHXjDRUaVWdNHjWHI+N8HifN27bR6gmPDHN8Ixufa8Xda+Gx16HfdNSQV/AcrW5vWN+q7Tuw4ZGIBCnHN/L4tlbcvmAU7vYdFOTu4VQoKmAAtA2oKSjuVgfFq56xG9G2HmJ9HicHnuqeeB0IsVddPHOnL67mMxTXXBdCCCGEEEIIIYQQQlxpsgK4F1fzLwbiWQH8z1828gPzh3zj1Y+C19akj+Yez2kecXzMOxHRA8fAXgFsI796Lnf+qZbsH8Y2DjGTFcAD3tV89oUQQgghhBBCCCGEEEKIa5WsAL4yZAXwIPdQ0gh+cM/foes2kkMYkWLixZTPkqi9JWJgwpxgxCALoIUQQgghhBBCCCGEEEIIIcQg0i1tKAaLG3gk+fOsSLkJ3Uf/y3/+JrT6F+CpX5+mww/DkkxUTb6Rb0TcFUIIIYQQQgghhBBCCCGEEEJciyQBPCh9hhUTP8+Su3TgPceL+7z84ENNyEfneeglD7/1fsqwsSPZeO/n+Oe+jPajW7Dbd1Nyb+hS2trd2O1byNaPY+7aKnY32rHb7dgb6qhYMA59+OsB/V1zKdxWR0NX3O5a1i8Yx1BNnErPpMUV1O4OxNrt7K6tIHdiV6kp5NfasdtrybOGv85M9qYG7PZa8u8Ov96d/q65lFTvDpbfULclrHx1a2q7fRZjAf3d+YG4rj7IZovdzu61aVgfKKGqq56NobZHXt9N1dpZRFRVCCGEEEIIIYQQQgghhBBCiH7Sl5SguKpuYM23RvGQdSjKO142vnyWLZGLf0M++ZilL/+F/3z7E3R33MoP0m7i69qYPjNwV3kxc83v85sDduzNr+PBiHVOIYXTw8Ks2ZSVZDEpQYenvQn7fjtN/63wpdnFTE0IiwNAz9S11RTOsGI43UbTfrVc3y1WbEWVgcRuGxX/fhQvJtIenRtMNuvvz2Xql3V4flVFxWuRpUb43F2UrZ2L+a+/UevyOw8Yx2JbWcisQGGv/8qOff/reAHl7aPY99ux77dz9ERYOaZZFP2LmfdbA22/oLb9icUlFP3rnSi/s2Pf38Trp4divjubJ55ICXuxGKxuvPEmAIYM+az2lhBCCCGEEEIIIYQQQgghxIAgCeBB5zPcfusQ+OADNr/yv+z5m/a+xt/+xg9e/Su/Of0pOuPlPA/YhJmfU5hTROWz1VRvLiLv317Hj547750biDGTvfQ7jNV5adv6CEvWVVL9bDWV65bwyNNteLXn6977BNl3G/G3VfLIspJgudlr7LgVE5P+JVDuq1uoe82LzjqbJ+4FSOOJfxmH3nOIqqfbNIVq3GaG/ywk+weBuvwgj7o3/KC/k2/MUEPaXqqm+lkX7wMXPEepfraa6mfraHo7VIz+DgO/Lc6maHOgjtvb8KMnZcZdvL+/mBU/rKb62UqK8vbhVMBkTWNc6OViEBo6VMeIESbuuOPLJCSM4XOf0651F0IIIYQQQgghhBBCCCGEuPokATzo/I133v8EbrmFlff9HXMuNoKf+QxP3vt5vjHyBhTvx3Ro7/eZnzdersUZfuVnb+BWQPc5o7oyV/8dUiw6FGcTTzf7wyLB/+st/DYsoQowK/0u9Hj4zQtNREQ763j9XdDdfidpAPhpeqaOtrN6Uh7Mw/ZEFik3ezj0bAUXSf/C2Tf4+fMRtWbfa39EQcdQQ9jli3n7t9SGF/Pq6/zxI+CjNzkUXr6/gT++CxhHyzbQg9zf/Z2BoUNDf7Wg090YcV8IIYQQQgghhBBCCCGEEGIguFj6UAw4n/LUL0/xovMCutuNrJp5MyvUXWm7G/JZts8czT/fMQTl7fd58tBH/FYb02d/wd2svebB95Ga7Pw6wD+N5lbA+/ahyIQuAH4ufBJ55VaDDjAxdVvo/N+u83dtdwA3GxkbfHkTT//H6/hvm0ruN00X3/q5i/cv/EZ77ewFLgCjb1fTy7Hwe5yaNnm5oADKBbwR1wPt1A0lnvyyEEIIIYQQQgghhBBCCCGEEH0hCeBB6W9saf0rVW8oYBzGQ7OMPPk5TchNN/LiAya+bryBcydOs+rVD/nPi20X3U8U5X3tpZ4pbo4Gztzt/nOI18NC/Wf9KOqLUM76wu704pMLUZLRQgghhBBCCCGEEEIIIYQQQlwbJAE8aH3KT9r/ypa2j1Bu+jv++RuRy4DX3DOSRD2cc3hYcvh891WvV4LXhw8w3TFVewcwo9ckrX2KAjodvv+sDpy7q/3ZF9riWT+VkocnYfQcpckJ5vtWkCt7LAshhBBCCCGEEEIIIYQQQojrnCSAB7kXHe/x5K//F6Xb6t5PeK/Nw0Ntl/Pc3zj9rg33WdBZp3ZLzhofWME3bou8Zv+9CwUT33h4qnqGcI/0TH08ixSjl6P/Xkbl8024MTN1ee5lP2dXbwxuOi2EEEIIIYQQQgghhBBCCCHEgCcJ4GvAf/7By6qj6mbIqhv40/G/8ojjY94Ju3rlHaL2FydQdGZsZXVUfD+X3MW5FG6so/bBofzl3cho/4vP83OXgj4lj7odFRQuVuNzv7+eqtrdbHlUjdOnP0H23Ub8bXVseRVwVrPllx50d0xlxeJACvjeQursdho2ZWOOeJdYncB7FvhyGhUrc8ldu578e7UxQgghhBCiv/3Txtv5fyf+kRPHbmXhF7R3hehZcslejra30/7Kszyo+ePTS9Ff5QohhBBCCCGEEJeLJICvEb/5KHwJ8Ke8+P4nVzn5q3K/sILCF47i9uux3mPDNsPGuBEemp4p5I0PtdFOagtKqfu1G//NVibNUONtKV9C995v+MWvAf0sCnNS0Ptfp/7ppuB5vs6tdRz16i7jVtCHePonh3D7jVjTbdiSb0XxamOE0Pi8mc98ZzFDcp5myJLNDMn+IZ/552xuGCnfVgeNL6LObqe+fJr2zvXlWu6Hwda21FLq7XbslTnaOwPTZenfHCrtduz1paRqb/VB4swiquoasNvtoZ/LVPaVl0ppfVg7BnVbrh0PfNXIjQCfv5Vvf1t79xpXspf29nb2lmhviFjM+D9j1LkzMpG0NO3dvuuvcoUQQgghhBBCiMvlhtGjR3+qvShUI0aM4L333tNeviLS0tI4dOiQ9rIQ4gqI9uzfcsutDB8+Ivj7mTPv8cEH76u/fOYz3PD1aXzmq1PgM1H+ruZvn/C3tlf49Pgv4NMYPnJzKrFnWLRXUXweXId3kL/9SOQNfRKZK5eSkWzCqNOp13wenMf2srPmII6uv5Toi+GpLF2zkMkWE4ZA0T3WI0ZLq+xMNznZk5XPzh7rlkpp/WqSaWfDvGK6vVOgj1yNNvJqtDcHh9j6YXCKrW2BMTZoLite3B3tvLyrhoOXNHljlFpK/epkDK5GbDFOpqScClZNs+I9eHXmX2z925scKu0ZWHw9PF9x0M8sp3ZREtph5DKUHYvLPxZR5uUVaovo2T9tvJ0XHjBy41/f5ckH3mfH/2gjVN/ZeDtP2W7hr/Y3mbpKe3eQKtlL+4wxnNyfTKYkgeOWXLKXrTPGcOPpNioWLuanmh2I+qq/yh1MppbsonBqIqebZG4KIYQQQggh4uM5/QGmkbdoL1+SaN/pX++iZCqEEELE44Z/mMRnvpYePfkL8JkhfCblPm5IvFt7Jy46gwnr9NU0hK9UTMikorachRPNoeQvgMGENX0ZRav6vm5NP6WIuhdXM90aSv4SrMcySvtY9M5jThSdlfSV47W3rivXcj9cUtt0RsxJ6Swrr6Z8ZqL27oAwPCEBY9gzcaVdUv9eZvPTkzCg4Gl9juUP2bDZAj9XKGF6+cfiCMXzutqxgXaf9v71I3FmObW1RUwbrr1z5f1/q97hH8b+N2Mn9Jz8Bfj8F/6Om2/s4d9icV1qL8lkUnIyyfdd3iRtf5U7mIy47XaG3ai9KoQQQgghhBBioJBvSIQQ4lLob+Ez474FN9ygvRPpM0O4YXw66GP/yyZXYyiZMje3gE0HXPgAnSWDyhw9AKk5mVgNoHja2fNUbjD+oeWbaHS48YYfDx6PhBzKl03ECCgeB42blgfLzn3qOZpdXvpatH9nIw4fGJPmcCmb2A5213I/xNU2XzsbupKGNhsFmxpxeBTASNLCZeQkaF8g4urffpVKwihAcXFw/cucPKO9LwazhKQETKaJLKuuYMHA/FsMIYQQQgghhBBCCNED2QK6F1dzybhsAS3E1RPt2e9pC+gbvvQ1PpP+rxdPAKNuBf3JKzvgTw7tnUi9bG88pbSex5IN+No3MK/4CDmVdjIsarJYG3spxhfVsW6iETytPJW3nmMxbjM7fmUVa9LN4Gpkdi8VSlhaRfV0E849WeRH3cO2b1tAT1tZQeYEK6bA9q2Kz03HwZ0U7DwWCgpIXVrBwslhsV4Xzc+tZfuR8CxWYKtcVyO2gmNkrlpKZrJZ3e7W56Z912aKX+4Ii4+vDhfvB5U+aRo5CzKZEONW3DHVoYc+7K3vYyo34OJt6/l90E+htPoxko3gOVxA9sbQMxPbuKliqm8PW0An5lRSnmFBp3g4vC2PjZbyqFuzR3LRaMsjWEpwe3ZzcJWq4nPj2Lud4r1hnwM5ldgzEnDuyGLvqFJygu1T8Lqa2VawvdszePH+DVH7zIIpfCk/0bc2jqd/ex1DjbjKjbL1vM/dzt7tG9nr8Pe4TX4kzVj0SQzti3WMu2JXLSUzyRyxq0JQ+HjEExtz/8b/eTZhZRWr0s2h56Cl97kWqzX//vc88DV99NW6Zz08+bXT7AD+/Xf/yISbo98L2pjAiQcu9sdVH/DS2E7i3hU6sP1yxy4bL414hkWTEhk5DOA8504eYuvyQl7qWv3Z41bND/LsoXxSaKMibTE/DV6fyMKK5TyY0lUmnD/3Dm+9soOF5S+FXh4s18Zz50pY/kAKt98IcJ7Tjv2ULCynNRTdP/5xFt/91hf4n1/+mH3/HXkr7V+/y//hv/jxv/Xx/2+5bSqPFy5iRvKY4GrS8+fewbF/K4ufaQoLLGFv+wzGnNxP8vKjPF6ynBkpt6MOxzu0vVTG4me6eiLQ54F+BeCctv/D3DZVLS+phxWtwdfGUW7JXtpnjKStYhFNSWUsT+tq33nOdeyn7PFymuJdOfzgsxzKT+H0/u/S/pVyMhOHwfmT7H98OR0Ld5CfMhLOv8Mvt84gP1Ch26Z+l8cXziDliyPD+vc0fzr6HPMLw+YZxDYnA/OxdyfZn5xJ+GPwQNmusOcHzp87yaGthRS+9FZYVDxjLIQQQgghhBjMZAvoKyPKty5CCCFiNuILsSV/CawCNt2hvRoXfWCb5wvKBQCcXnV/UsvkcjKT1FXBl24C06xGQMHRGHvyF1LJmGBGB+gskynqZXfazp3HcCo6rJOX0UtYXDIrGliWHkqAAOgMZpLmzCds02wAMivqWT1dE2u0MH31T6iMtuR0aAJF1eUs7EqWABjMJC9axaqwBsRTB2Luh1RWFS0jPepW3KupXRm5NC/eOsQq3nJja1sP/C3UtHsAMI0J7TUez7jFW99woeSvm+aNfUx66adQWt21PXvoss5gJnlhOXWlU8KjAR0JGdWsiWifDqNlOqtKMyND4+jfnMqGQJ9FyyJGiql/U0upt9ux2+3Y7YGzcg3JrA5eU3/Cd6qPqdwuiTlU/qT71vMGczILc+aHR159cY5xTnmp+hly8aGIKzau/iX2zzOAY5uXUPCcA6/OxOTHaqm4DEuBNzZZeXjCsOjJ3wHq9hk/pfC+UPIKbmTYmPt4/JnHIwPj8PiuZ1j+rfAy4cZht5OU+WBE4qzLyIk7KJ/flfwFuJGRSZmUbLVFBg4mtz3Isz8tZ/6kUPKXQD+kzC/n0LMPhkcHbt7GszvKmd+VGAS48XZS5pfQt66YSMnWErW8aMnfSzKMpMXPUXhfePtuZFhiJoUlUdoWo5ETS9TkL8CNY5hY+BzLU0YGfr+db83ompcPUlL4MN9KDCV/AW4cNpLE+wrZXzExdLEPczI2yTy+65Dm+YEbh43hvsId7C1JDg8O3LzcYyyEEEIIIYQQ16fB882LEEJcx/QJE5i5spL5STrAi/OguoLxyMYaWr2AMYmF5bupqyolZ0qUL/zjkoTJCNCJ62Xtvd4cofm4BwVQXIdZf1x7P4x/Jy0dPjCNZ85l2cM2h8lWHShO9ix/KLid8PJNjTg8kck7fWYF860G8Dpp3BTaNntToxMvOixTlnXfVteczESjgqd9D2sfsmGbW8ABlwKYSExPCgTFXoegGPtB8XtxNj/HhrByNzW7UQBTUgZdNehTHWLSh3JjbFtPOts78QEYTaTGPW59qG9AKPnrorFgCZu7/gKiJi9YzobAwbDh27SrP6EVp6mrckg2Al5HaHv2h5YHx82YPJ9VoYEDwGA0RmznnrutHS+gs05jpfaxjqF/9QsqmGbRgeKmOXwb94Jm3NrYuPo3dvGVO55VqzKw6Lq2ng/rt0YHwaGLcyz6S1xjPK2cKRYd+FwcCLRrbu5T7HF4AfC2bgidmxxHbHz9GxDT51lIx8sF5D7VjFsxYJ1TTtXKCdqQ2C0ehW3sEDj7AfYn/x9jx/43k+e/xa7ffQjA2WN/YGzYCt//+7X/ZuxY9efY2YiSQlZ1BmOePHYegBMvhV6n/vRh9W+YYcOGcf50G3uLF5GcnMyiF9o4B9yYmEZFlPzVxZUwMfFGON/B3u8+SHJyMsnJyXx3634c70Q/eHrYyJFwzsHeYjW++JV3ABiZNIMHtMGDxIMli9XVtOccwb5NfvC7bP3lO5wHhqUspGKq5kW3p5Ay8jzvtO2l+MFkkm0FvHLyPDCSr9zXFfxTFqepfZqcXEHbOU0Z4RYuZuqYG+HcSV6pUOtgW1TMXof6onNtFSQHV/jGUW7AjcOGwenu4zYsMa3P4zZs5EjOd+ziwQp1Ho68/XY4uZ/vfveXnAa4/Suhss+dpuOXL1DWNc9si6gI9O/tSfMJdW+Mc7IkM3ivItABJ/d39UnXT2j1722PP84DicPgXAf7A/2bbFtExf4OznEjY6YuZ2GodFVMYyyEEEIIIYQQ4mIkASyEEJfgU8/b8LdPtJej+9snanyMLBmh1XS7q9ewKN2CAQXP4R2h5Kq/hfVZNjYccOLxgdGcTMZj1djrqyhfcAlf0vfRkY3ZzLbZet3+ucvBbYdxYyBxygLtrT7oxO8DdAkkTwslME621FCQXRCRCJo2wYIOL62b8qlp6Qxeb6nJZ49DAUMC47Vdp3ho3fYI2cU7OX4G8DvY7lBfq9cPDwTFXodwF++HI6zPziJ/88scCTtktWXzcToB9Hq6atDXOlxc38q9eNtiF9+49a2+iQsqKM2woPM52VOQR03kbrhxmMn0JAPgofmpAnYeC9T3zElaNi9hh8OnJts0f6zhc+5hdnZxML7zYLHaNkxYumXxLt6/85Ot6PDhqFnC5paTweudDj/qHgIhMffvkWLmBZOsG2j3dT/H2WYLbSsec7kAqRmMN6nlbcsrCMWfOUlLTQHZBT2NXAxyKiNWKAd/6ksJrTGPR5xjnKDHAHgdO9geaJe/8xg7N7TiBowma6joOGLj6t8uMX2eRfIf28ySgj04fTrM6WuoK5+pDYnNWB03An/93V9YsUM9heZ//r8L/OAHp+kEbv78ZV+CeVmc79jL4/ctptzeDkD7jxez13EeuJ0vztBGx+JP+M6rqxqTZ4Q+o1p3lLBwxsLoqy1Pt1Hx4ELK7eqWufbCQ3R9RMWwUDy6f5zFd7/73e4//5qmjewH3+W+pGHAO/yyYGGwb3mrlR35M9jlUBN+iVO1GfbTtG1dyIzF5djfAt5tovC/1KTqjbrQUR0x+6KBG4HTjh0U/lStw7vtdsrLjvIOMGzEpa16P3/6KBULL/O4cZKmZ57hrZ++qyZ8eYejz5TQ2uqjKyetlv1TFs+4j/n5P+al1sBWy++289P8dt4BuFFHqMf6MCdjMD85kRs5zdGK+ZQE+pd32/lpyXz1Gbrxi0zslgm/zGMshBBCCCGEENcpSQALIcSl+Ouf+fTc+9qrUX167n3465+1l2Ok4HW307jhEbI3tmhvcmR7PtnzbORuaqTd7QODmaQ5a7ptQTqgdG7nmFNBZ52MZhfjPjjIUzWteDFgmb4au72BuqpyVs7Ubo47gUSTDjAycV33ZNCiJPWeSbsITunk8EHNWaWBVYjzirtO4Yy1Dhox9IN+wgJKq+poiKhvBt1PQe1jHS6qj+XG0LYehX0zfiTucetDfUdNoXSOFYPiorE4n519Tv4CmNDrAE8HLVHKedl1CgC9MfIcxVMdOyN+B2hxq1thR9Vr/6aSMArgFK6D2nta8fZvrOIs12oMJD4P0pddt6+sOMfYq6irgpPmkzNBTQrrEyaQs2YyZkDxh41zzLFx9m+XmD7PovFyQfuXA/E6q/7B1Oe/9nk2zlaPT/jCPw1l40YTCcD5s5f6Bv3jnbe6n7P70juXcq7QDgq2tnGaYYy5r5D29qMc2r+Diu/2vL/tydbF/DTizNh3OBfDCtSBaySGG4HTf6JJ27nAj/8UWCk77CuRN879iUM7ws+NDa1KTVvc7STeizunADAyaT4lNjXZfFuyjZKSSdwOnPepKda+eqd1+eUft5P/RUkgl6r+3k5+lD4EuO2BAp7de4ij7e20B39m0P0U3/jn5MU9wFduBxjJpNLw91d/Hk66ERjGCO1n1OUeYyGEEEIIIYS4TkkCWAghLoX/Az493nzxVcB/+0SN83+gvdOjyC1NZ5O1pJiaI5ov7TU6W2ooXjKPhwJbxxqTcyiNe3mbB78CkIClj4u8YrWzpQMfJiYsjLK8EUCnx6S9BuiHDtVewt+ynqy5BWw70I7Lo2A0J5G+aB32hkpygsmxoei6v/Syia0O3fXaD6lFVK+ZQ7LZGNNqob7W4WL6Wm6vbevF+AkW9XzSU519Gre463vqGC0uBXQWJi+8XBNfwaG9FCdj4Nzvnly0fxUFdePg3sTfv7HpW7nKhX7I/oZtGx3x07Xtcp/FOMZ782l2AwYrGWuqsQd2dsiwGkBxcXBH2H77Mcf2rX/7Qj9hJVXli0gyKribnyKrIK7zAUKeehd759/g5lt54Ol/4MSJf+Twrq/wwD/o4PwH2Cs/0r5iwLq990fzot796WLusxXwwittnDytMOz2JL71cCntR/dSEnk0a//57338+Mc/7v7zb4e0kf1HOc+lpNIv2TNbeeUdYFgiM0qfo729HftzpcxIHAbnT9L07I+1rxg8HnyWnxZmkjJmGLGsrb/8c/ISHxIhhBBCCCGEEJdEEsBCCHGJPu14jb+1vdJzEvhvn/C3tlf4tOM17Z1+c+ZgMa1uAAPGsJ1FY/MyTpcC6EictlR78/I6WMAxDxgSp7BAr70J6EwkRlm0mWmJlhZWtzI9uL2YvOx52OYWsMPhBZ2FaTmZgYAjdJ5C3bY1N0oySLN9bZ9ctA5R9NIPM6cnYwQUdzObws6ztdkacUWGhsRRB+OoyP1hE2dOx2KIuBQSR7lBvbStR4k5LEw2AgrO9l19H7e46uunJm82jS4FY9KiS1w970VRAFMiS7Vn9wIzLaMAONXZ20HZqpmJJkAhfIFohB779wx+P6AzkqCpQ2JOEpGX+ti/FxVnuR6/eq514qX0/ZUS5xinFjHRDIrPi09dcAgo+Nzt7CguiNxuPObYOPu3jxJnllO9Jh2zzodzTwFLNqtn0PfJwluZnPAZzp/9kLPn/xa4+AlnOz288EQnqw5r4gesZB5IvB04j3aB6MjbIveznfj4fSQOi7gU8m4TPy5cTOZ9aSTbCtjlOAc3jmHG8se1kQPCsM+PjPj978ZM5e9vjrgUh3MoALcn8oB2l2fgu1+8HYDT7/ZzMvrBhUy6Hc6fO8c59Qhp4Dzn3mljV8lySnpYWTsYfPe+JIYB59/5JVvDzvVNTt5P6FAAjcs6J3/Ku6dRt/lepD0nOPST2df9pYUQQgghhBBC9EoSwEIIcak+/ZRP25v420s/4tOTDlACK5iUj/j0pEO93t4En6rnHV4+qRRVVVGaM4WkMaFzG/UJSUzJqWCiGcBDZx++q9/Z6MAH6MzTaagtZUFqaLPAMakzWVlZRVGUlcXjV1bRYLfTUJmjvdWjmsNOFJ2VCQvCsyhHcHQq6tamj5WzYHygfcPHMGVlFRlWHeDG2bW1bWoRVbUVrJyZSrAr/A7aWzvVduiMXQVz0OkGTKSXV5AzRbvv4CWIow7RRO8HMOnVFTTKmQ5aAmcAj5mSQ2nVlO5bQMdTh+A2s5lkJqmZwylLKyldlES3msZTbhQ9tU1Lnbvl1JZnYNEB3nYad6qrQeMat0uob03BNtq9YEx+rMck8Bm/WifL5LC5GWEvDpcCmJleXs6CwDa+DB/PgtJaFiYZQHHSvitypavemEpSgjoW+oQp5FTUMd0M+Bwc6GXBZfT+deA4pZ5DO7loJanDQ+9fnmHpti4rrv6NQ1zltrTjUgBTOvWVK5nZ1W/AhAWl1JZ3/1y5+Fj0l/jGODU9CSM+OvZuZH1xQSA5O5t5S4rZ64icB/HExtW/fZC0tJLyRUkYFQ+HN2WTf2l7o7Pw27dyM+f5fy/9mTVPdDB/8n8zdqyTr33zNE/9XBsdv7+eV/8Qa+y3R/NkYIvpy2HYiAdIS74NgNuSH6RkVxn33Q6cc/BK1wLRwFbCwxIf4PGpt8FtyTxYtpfy+WoSLsKDW9n/yi4qvvsAE7t2OH63iaNtf1LPcNV1e8XVpZznY+Dmv7+bMYGqmcbNYO53vkKf8788g6MD4HbuK9tBQWD7Zb5io+DZV5ifdCPQQfuzEfsnX3YPpiUyjHO8tb+MspLHWWRLJjl5EmkzFvNMU/++d38baVDX/Srv/QnHn9QtlScuLOHZvWndt4Duw5x8T1Ez5mPSdlBg02zVHbD/rXeA2/lW2S5KFqYReIyEEEIIIYQQQlwBN4wePfpyZySuGSNGjOC9967OpmRpaWkcOtTPf/EuhIgq2rN/yy23Mnz4iODvZ868xwcfxHb2b9xyKrFnWHA1XmzlViql9atJ7mm1JuBt30RWcfczg2MxZVUtyyabuiWKVD7aN8wj8rjI8Pp4aV2bxfqLL3AEplFev4wkHGybV0DwuNLEHCq7EoHdKLgaC8jrWgqXWkr96mR1y+BuFFyNeeTVdAZ+T6WobjUTe8oB+trZENwWNodKewaWiGs9iKsO0UTvh4ScSiqjJOyCwusWTx30mVTULcTarWAvXp8RI30sN6pobbvI/PU52RNxFm8c4xZPfbtiXY3Yuh64xJmUr1lEkhG8rZvIWq95hsavonbd5Cjbk7totOVRQ5zzN/DMR+elfVMuxb0eihutf3upp9eFe6gFc/gYx9O/QYExjChHK75yE3MqoyaoAQgfoy49tTF8LOLR61jQ5zFOWlVL+eTutQRA8eJu38OS9WqWP57Y+Po3js8zYEpRHY9NNEZ5FvvuO1VfpHJqD1sBnP+QE8fe5alHPuQwwMYETjxwizYqzAe8NLaTVeGXZhs59vTtfD78GkSPjUXJXtpndEuVBZyjreJBFncd8Hrb4+x6aT6J3fbaPc3pcyMZSRsVaYv5KerWvIfyU7onhgE4z8n9y8nsOuQ1UIeT+7UrJR/k2UP5pISX22++zPTc+7B8Vnv9LGfP3szN/Fffto2eWMLeZ2YwplufEeiHx8kMLsEtYW/7DMaci6G9vY4bwEn2J2dSAkyteIXyb0WubA46f46T7ft5Zvkz6hnQcZTbL+PWNW9O7ic5syTUJ9rfA330VslenuutvuF9Gc+c7GLbyiulk+jee2H9wINsfSWfSd2DVBHjGccYCyGEEEIIIQY1z+kPMI3s7f/nj1+07/Svd7ICWAghBq0jbNrWSLvLE7ZNKOpWoR4nzdsK+pz8BWjZmM0jGw7gcHvVbRoDFK+b9sZtmuQvwBGaj3tQAMV1OMbkL8BBdqh72DIlfA/bjhoKinfQGuX9W3cUh5JnAEeK2dbYjtsbEYnP4+TAhkc0yckjrM8tYEerm4jwSxVXHaKJ3g+dNXnUHI6sqzq+22jVbgscTx38eyne1ow77IBYn7udHQW5HD4VugZxlhtV9LZ1p+DzuGhv3IRtnjbhFMe4XWp9O16m4KlGXAoYJy6jdpVmJfDxjWx8rlVTvkZHDXkFz3Wbv6E6XCybpuB1t7Kj4GLJX3ru3+MbeXxbK25f1wUf7vYdFOTuQTvEcfVvXOIrt6Mmj0c2HMDp8YX1W6AvanZFxEKMY9Ff4hhjx7a9OALjoCiauuqMmCcuor5cPcc5nth4+zcenY5OPJ5WtuVqn8W++/mSP/G7swB/4/z5C5E3b/wcY79poXrvTZHX49HgZdUL73LirKbsy+o8504eZVdBWPIX4N1neHzrLzl5LnTp3Dtt7CpYSKtmm2h+upit+9s4GdpzWC33dAevlC3snmi76v7AgX1H+Z+zHwd+/xj/X/6Ln+/8N9rD2hu31hIyH9/F0ZPnCO+JUD/0//7LTc/sxxFow/nz4bUAbhzGmEnzeWbHwsjrg0R7SSZbf3kybGtrtW9/+cJWjl6OOWlfTsmuo5rXaP2U5QsL2HU0sh5CCCGEEEIIIfqfrADuxdX8iwFZASzE1RPt2b+iK4CvR/oFVNTNweo5gG3Jdu3d68e13A/XctsuVcyr/nsh/Tug5VQ2kGFRcGzLpeCgupV7l/Erq1iTbkYXWJlrjSO229/hDHAbm6w8MPZjfrfxBJnPRv6/ILO3mHnadjOc9fDk106zI+LuVdLjKk5xbUimZO9WZoxRcGxdxMId6jbJXWxl+ym973bNKlUhhBBCCCGEEJdKVgBfGbICWAghxNXn30lLhw/MkymNcrbwdeNa7odruW0DgfTvAJZDUmCf6KGjkkLnUgMJSVOYYDGqW16f6uRIXLGDz1fHDgHgxoTPMvnO0PV/+vZNfPPOwMrfv54fGMlfcR2Ywf8J7D+tuy0pdPYtkJy2kElfCfzh3+l3JfkrhBBCCCGEEGLQkRXAvbiafzEgK4CFuHqiPfuyAlgI0W8uxwpgMYCNZ1XtOno61hcAxcPhTdlsPBJPrPbGwPeTY//IN7sf0Bty3k/Txj+xZKBkgGUF8DXOxtZXSns+nxbg/Gl+ufU+8iUDLIQQQgghhBCXjawAvjJkBbAQQgghhBD95jgbH99AY7sbr/ZMX8WL23GADY90JXTjiR18Hnn4LV46dpaz5z+JvHH+Qzp/52bNAwMo+SuuA3aWLy9jf9tJzmnP/z1/jnccr1C2UJK/QgghhBBCCCEGJ1kB3Iur+RcDsawANn75Jr79LR23coG25z6kLeLuZ5m16O8w8Qknfvm//OIPMsxCxCrasy8rgIUQQgghhBBCCCGEEEKISyMrgK8MWQE8SJkf/gLP/2gMWTO+wHdm3Mpd2gA+R9qML/CdGX9P3o++zJaHb9AGDHBplOyyY6/M1t4YRK5MG9LW7sZu30Jc76KfS8VeO/YdhaRp7wkhhBBCCCGEEEIIIYQQQohBSxLAg9JnmXvPzegAvO/zH0//hX3aEHxs+XEnTi/AECz3DI+SJBbXrZEGhmqvCSGEEEIIIYQQQgghhBBCiEFPEsCD0hD0N6n/5Wk/Td3hT/BqQ/gU1yvnqHzNp/560xCM2hBx/Xq7lhWZNmwLy+h9o3EhhBBCCCGEEEIIIYQQQggxmEgCeJAz3PxZ7aUI5q77n/yNC9qbQgghhBBCCCGEEEIIIYQQQohriiSAB6XzeAJLfofe1PvZviZ9IAHsvcBR7U0hhBBCCCGEEEIIIYQQQgghxDXlhtGjR3+qvShUI0aM4L333tNeviLS0tI4dKjnzXkf2XInsyzAH9zM+F5gm+coHvnRncz6MuDqZMaKc9rbF/foFuz3j6btR4/Q9OVSsu+1YtIDnyh4O9to2FrGPmdY/Mg0cldl8a0vmdDr1Ev+zjbqN5dExgH6u+ayYrGNlAQjuiGBWM9R6rLLsJNGya58Uk7vw5ZX2/UKpq6tJu9uI37nborz63CiZ9ycFeTOTMFsDLyh4uXEK1UUPnsUf/DdwuqWaEI/BPjEi/tXu/m5IYvcu6HtR3MpeTUUbn2gkBX3h8pVvG7afraFspc0DelRtDYA0ercU38C6Mcxd3kuthQzxsDW3/g9HH0xm7L9kLZ2N/l3/4V9thUEeyq9hOqVKRj9TnYX51OnLbOHumnbjOLFub+C/BdeD8YYv5lL0b9+C8tIvTpunyj4T7v45fPFVLeG9Xhw7uRyyFpCdvpYjDrgEz/u1joKf2iPsnX5wBDt2b/lllsZPnxE8PczZ97jgw/ej4gRQgghhBBCCCGEEEIIIUTPPKc/wDTyFu3lSxLtO/3rnawAHmzuuJGsFaNJs6i/uv8QkeLs5hd/CCSHLSN5eoWBb9+hjYiN4Z4y8r9twvs7O/b9do52+NHfMYnsohKm6kNx2WvzsSUaeP/3Tdj322n6nYehCSlkFxWSFlaePr2E6rIsJiXo8LSrsfbmNt7X3YopLC5Ez6TlFeTebUT5w75A8he49wkKF0zC9ImLo/vt2Pcf5cQFI2Nn5FP2sDns5VMp2ZSP7R+MKB1H1fdr9WCYlMsjXx0a9j4q66NbKHs4slz3EDOTHi6jYl5Yg+OmZ2pRNesXTMI8xENbs6Y/y7aQbQ0Pn0pJ9Xqy7jGj87TRtN+OfX8Tbad13DoyLC6MfmIeFUtTMH50gn1Rk7/R6edVqG3+6M3A+xzF6dVhModOj7Y+uoXaJ2xYb1Fwtap1b2r3wEgrtqJqStK7943p/kry74E3XwmMz0d6zPfkUrY0bHxEjxJyKmmw27HXFTGle/cKIcQ1abB99kl9hRBCCCGEEEIIIcRAIgngwcYyjO+kGzHyCZ7DJymq6n0Bt7uqk8rDfhRuwpo+ikmBxHF89FitXqoXZJH/w2qqn62mbFUWha94wJjC3KXjQqGe16ldPZcl6yqpfraayh/kUff/FDCOIy29q7i5lC5NwaicYF9YbPXmEpZk5QdXsYazPlpG/n1mcO2j8LFaNfkLgI8/vlJG1sJ8yp6tpvrZMlYUN+FBx9iU79D1nWba49mkGBVO/KyQrFVl6vv9MJ+sNftwE1jt2uWObJZMHwtv2ykMLzenkrazOqzfXkJYi+Nz7xNkTzSiuPaRP38JJZtD/Zm1uQ2vbizfeTQrUG89c0tzA/XOZ+6yEiqfrab62UpKlmWR/4K2cMCaTdkTUzFzgn1rVlAbY/IXYN4/WdHhpmllUeB9ysjPfoS87b9VAwL9ovO2URk2FyrXLWHu6n2cUIykPLSClIhS9ZiNJ6jMWaEZHzAnz+17P15HpiVZ1BlqTGLyeO3dS5M4s4iqugbsdnvop76UVG3goJBKaX1YOwZ1W64nMm79KqcSu91OZY72xsDXn599/UHqKwbz8yaEEEIIIYQQQohrjySABxvXOX7+67P4GYJp8t9TOE8bEEk/z0TuZD06PuKNejc/eU0bERtPay1NmsXGzq1NOBUwfXFiMNFau75Is4Wxn31vuQE9xi+qV/QPTsKqU3A2FMaUoLQ+sJ6i+8eCy05pQXjyF3i1gqKtmq2enW/gPgsYR/N1ANJIs+rhdBt1z2ve0FnLz9+IbJh55iTG6hTe/EV15Hv5mzj6lh9MZk2SM3az0u9Cj5e2FzXtAPzNT3PIBTprCvMA9POYZNWhOPdRqK13NNZZrC+axVhOYC+JrW/DeXx+wMSdD40Ljif48Z5W+6erX5yvPN1tLuCsZd/v/TDyTqbeE3nL/WtNvPNXvOkBPmfoYbW3CHfQ4UIB8Do4fFx7t+/0M8spXTQxtN23ENegpJwK6hquzYTMYGtbvPXtr8++WA22+sZrsNVXCCGEEEIIIYQQQsRHEsCDzdvnqdvwP+x+42NgCJaU3vft+07KzeoKD9dpiv79Am5t4i4mftxvurUXAQ++j8ITrYDezNR5hazftIWqugYa9jZgv39sxKu+fvtowMufj8RQmZFpFD08Dr3nKNUF1bwe5SXGlFnkrq1gy7Zadu9toKExn5SbwyPGYrwZlHfepC38coDyt8jfxxoNgI5xj2pWpdnt5KXogdGY71Vjsyu7x9grsyMLDHOrQQcf/Zk3oybi/Zw47QduxXQP8E9mRgPetw9FJrijGk1aUTbj9B6Obi+kWpPUjoX93+04z+oYO2M9u3fXUrFyFilh20yr/dLzuB165y+AEdOXw6/68XTbpvx1vH7gZiOyCfTFddbkMdtmw5a1nhZtV16C+elJGFDwtD7H8ods2GyBn3nFHNEGDwpHKJ7X1Y4NtPd8NLoYUPp33IYnJKhnj1+DBlvb4q1vf332xWqw1Tdeg62+QgghhBBCCCGEECI+kgC+xl04H9gieghhqzr7QJMkjfChDy/q9sNbdlaR99AkvnSzDuXdNzj0iyb2tXm0rwAUlNPaa1H4PXj8oDOO5a6J2hbomVpUR11JNravmtApPv7Y1kTTgUOcOKsJBS4o8XzD6cX5inrGbbSfoyfUqIatRRT9QPOztUFb2CVRlPe1l6Lw4VE7irFf+0bfxtpZR/78LErqj3LCZ8Cank1JbR2FUc71FYNdKgmjAMXFwfUvc/KM9r4QQgghhBBCCCGEEEIIIQarG0aPHt37IbLXsREjRvDee+9pL18RaWlpHDp0SHs56JEtdzLLAv7XXMx78rz2dtA3f2Ah/+4b4exfqfi/p/mVNuBiHt2C/f6xnPjZXFY8r0mg3pFH7bapGJ11zM7fTdra3eTfDW2bH6GkORSrX1zF7hlmTvzMxornYdwTtaz/phHni7PJr48oMUwaJbvySTm9D9t22FIW2to4uLpVn82W3bMwv22ncFn4ds1TKdmVRwptVMwv4RDZbLHPYuy7TSzJqUS7lnlWWQPZd12g7UdzKXk1VL/Xn59N0c80wXEJa0OeerKx+l5+jq7LoqzbKmA92ZW7mZXgpG52Pru/lk/tk2nB/u2J2u9/YZ+tCirLmGWBE/tLKXz29V5WDnevm5bxm/lUrEjD9JHajyeW11J1nxFnfRb5L3YvWa2Hj0M/yKbid11zZ3SwX8NlV9qZZTnBPtuKqGc+X23Rnv1bbrmV4cNHBH8/c+Y9PvggluR8X6RSWr+aZEPYJV87G6Ktzs2pxJ4xxCE9BwAA//RJREFUivYNuTQnrWNRuiWwak3B62xkY/FOHN2GK1A+PZTZRZ9E5sqlZCSbgyvhFJ8bx97tFO91aKMBGL+yijXpZnA1MjuvRns7PjmV2DMScO7IYu+oUnImWzEZUNvmamZbwXaOdWsbMbcvdWkFC4NlguJ10fzcWrYficyI65OmkbMgkwkWE4ZgP3hwHd5B/vbupU9bWUHmhLByfW46Du6kYOcxbWjMdYjb8FSWrlnI5LA6+9zt7N2+kb3hEyKWMU4tpX51MqcaH6c9sZQ5VgMoLhoLCnBlVvPYRCMoHg5vymbjkQEwbjmV2DMuduC9i0ZbHuEz9KLl9kHMcydQZ1ejjcjHRtMn8bYtWO5caryrWJqZjNmA+kdDjoNkF+zUvji2foj1cyfe+sbz2dclxrke01j0d31jed6Io3/jFkd9+6MO44uoWzcRo8/BtnkFHNTc1i+ooG6OFZx7mJ0fmJtx9VkMz5AaTKU9A4urEVvBMTJXLSUz2Yz6aLhp37WZ4pc7wguJTY/PW7TPvjjrEEM/zCxvYFGSQvuGeRR3G1BVTqWdDIuHwwXZbAx03+X/NyvOtgkhhBBCCCGEuO54Tn+AaeQt2suXJNp3+tc7WQE8KA3FZFT/y3f2Y+3NCC7vBe2lPhn7T9mMi1gIqmfW4m9gQsHVZldjjHrgff7SGv6NoJXslMiNfl/f/zoedFi/U8LUWBaXOmsp3H4U75Cx2ErKyLYGrn/NxK3Ahb+6Is7T1d//Te6M2AK6iTc7gdu+QbZmNav+rjxsd0Xu8fj6r07gRced386l660ul32/fhM/RlIeyu5Wtj79CdIsoLh+ix3gd3Zefxd0VhslMa3CdVJbUM3R0zrGziim7FHtO/TOODIwqQK8v6rit+8CN6ln9bpf/i1udFjve6L7uFmzmfVVPXje5NDvNPfEFWAgcVk1q6d3fUEPoMNonUPRqlT119RS6oNblQcSAIZkVmu2MA+ed6mfQml1OQsnhr5sBtAZzCQvLKeudEroYlAqGRPM6ACdZTJF47X3+0JHQkY1a6aHvnAGHUbLdFaVZkaGxiGzop7VEWWCzmhh+uqfUJmTEBaZyqqiZaRbQ0kjAJ3BhHX6ampXJobFQmZFA8vSNeUazCTNmY/2KNHY6xCnxBwqf7Ka6Zo6G8zJLMyZH7oQ5xiPmrCKDGugsjoLk1dWsGxi4HNDZ2JCRvh4XO1xi0//lBvf3OlPoyZXU76wKxkFYMCUNIfaVZEPaXz9EMPnTn+Lda4PhLGI83kbEP17uetwfD2tbsCQyOSZ2pswP9mKDh8dLV3J33j7LE5DEyiqLmdhV3ISwGAmedEqNI9GXLo/b7189sVShxj74aTXCxgw9vg//5Iw6gHFiyuQ/O3Xf7NiaZsQQgghhBBCCCH6jSSAB6ULeANbHBv/8Wa+/dUhRKbuAG7A8tWbmHvX59RfP/pE3aa5TxS8N6WxvmYLhYtzyV2cx/qaOrLv0qO4fs7z9WrCt+kPbsDM1G0VgbhCtuyqYNxnNO/srOTpn51AMaaQt7OOiu/nkrs4l9zvr6eqroJoJ+j6m8vI3dqGVzeWWWVb1CTwr9/gz37Qp2RTtTaP3MW55D1ZS91Do/FFbAHtpvo/juJFT8rKn4Ri11bxkye/ju9tzRKW17ZQ95oX3R02KnZVUbIyUL+VJVRU11FXlBYZH48DZdS+5kVnmRVRduHGOupWpmD0tlFdvDuwctdJ5TP7OKEYSVlZR93GQrUeiwtZX11HxcPawgF/E2XLKmnz6hh7fxlbAklg88NbaLDbqft+z3WfvbaO3bVdY5dL3pOVTL0D/M7fqAnpt6vZEmXc8tZWsXuDukJ739MVUc9ZFvGK/1xUg8EAXgd71j6EzWZjbbMbBTBYJjNBGxyD1FU5JBtRy3wqV63LQ8vZFCjXmDyfVUnaVx2h+bgHBVBch1l/XHu/bwxGI4qnPViP3G3teAGddRoro3znfDH6zArmWw3gddK4KdA2m41NjU686LBMWca0sHjF78XZ/Bwblqt9a7PZgv1gSsog1A05TLbqQHGyJyx2+aZGHJ7Iz5l46xC78axalYFFB4rHESr7oeVsanQQXo14x9hgMqE4n+OhTe34AKNZXen9+OPNeACdKTFirl21cavJC97bEHh4XI1h51zbbNjCVv/GXG4fxD53YhRn27oYjMaonw+mpGnBMetLP1z0cyfu+sbz2Rf7XCfWsejH+sb7vBFL/8Yt9vp2udx12HnMiYKOxMkLIm8kLGW8BfAcZ09gaXBf+iwu5mQmGhU87XtY+5AN29wCDrgUwERiet8LjuuzL4Y6xNoPDq866fX6wJskrKTWbqe+vOvJHYVeD/i9dEL//5sVQ9uEEEIIIYQQQgjRfyQBPEj9vP0sCqC7bTR5T45mljYAAyueHMM3bxsCfIzr12d4QxsSswuc2FnK7hMGxk23YZsxlXEj/Lh/XUthXm1w9a17+xZqX3NzwWhl0gwbtul3omurJr+1+za5zucLKd15FPeHeqz32LDNsGG7+0vo3n2T17XBAf7mEtb/7ASKbiyzntpCttVO2WY7J7xDMd89FdsMG9+4/S/sW7e72zbPvFpG7no7Tg/B2LQvw+v/tp593Y4o9tO0Lo+KA048Q8ykpAfqN/kuTJ+coOnV32pfEAc/TetyKdvzOm5MwbInfQk8r+2mLLeEpvDv3Jy1FJbUcfRtP/rESWo9pqfwpaEe3vzvsLhw/iZK1u/jxEeRSeCLOfEHN8otgbGbYWPqnTrczdUUF+4LbiXtfH4FhdubOBE2blOTb8XX0UR14Qpqw5diiytK8RxmU24BO4+r2zAe39yCSwGG6hgKcKSYecEERuCLf187GyISG11bZ85kepIB8ND8VAE7j6lfFXPmJC2bl7DD4VO/wJ2i/SYbjmzMZrbNdunbP4fxOfcwO7s4WI/Og8XscahfIlu6feN8cdMmWNDhpXVTPjUtgbYBLTX5armGBMYHMxtHWJ+dRf7mlzkSdlhyy+bj6hfoej3Dg1c78fsAXQLJ00Jfbp9sqaEguyAiKRdfHeKQmsF4kzq22/IKQmWfOUlLTQHZBV216MMYKy5aNr/MmZZOTgHg4fC2Gjo6/OpnRNdcC7i64xa7/io3vrnTz7ytvX8+9LEfLvq5059inusMgLHow/N2tfs34HLXwb+zhQ4f6CxJLAjbTSQhMxkzCs7D21D/dqhvfRYXxUPrtkfILt7J8TOA38F2h/o+en3fZ0Rcn30XrUMc/eDw4AX0xjHq66dZMAGGMRNQ12tbMBoA7ynUzZ37+d+si7ZNCCGEEEIIIYQQ/UkSwIOU+4X/4dGn/8zR35/B9Yf/pVsOkw85tP9/+HnDnyhf8gdWvHCJRz3/7XXqfpDN3IxAomh2Fkt+uC9i62Vwsm/dklBMRhZLfmTH+/wKbDb1/N8QP6/vKWNJ1uxQ8mn2XLJX1QZWkB6iZL6t2/m0zudXMNtmw5apJhv9rdWsCCtjbnYRdW80qa+dX0L4Kcr+1mrys+cGY2dnLaHsJSe6zwAoKEpYMF4Obc8ne25Ycmz2bLKWlVAXscV1b6K3Afwc3VnEkvnhbc9iybo6jkYp2v/GbsqWZTE72K+zmZudT23gDOFD6+Zi056l66xlRaYNm202K5534n5B7besH/Z8rvShrUvIygxrb2YWKzbbNWMMzgOVEX1uy5hL9qpK7NrA51dgs3U//xegNs/Wvc7iknQe20hLxPzx4I+Y0/EwodcBng5aohzT97JLTf91fcnc3051dD+ntMXd/VMvNhNINOkAIxPXRW5/bbfbWZSk3jOFLU7ST1hAaVUdDRGxGXQ/KfQgT9W04sWAZfpq7PYG6qrKWTlTu9dl/HWImdWIAfA6Dmrmg1YfxrjTQU3oe39wHWNzlNd2udrjFpv+KlcV+9zpX67D6y/y+dC3fri8nztxinmuq67uWPThebva/Rtw+etwkD0OL+isTFjQlbwdz4JkE/g6aNnZ9WZ967O4KJ0cPqg54zuwCnxeT4foxiCuz76L1iGOfjh2Ci9gCOwBPS0xAcXtxmtIJD0VSDKiB3zerv/B1s//Zl20bUIIIYQQQgghhOhPkgAexLyH/ZT/4F1WfM/Lz7U3+Zh9z52l+oUPORr+hb3QSCHli3pQPJz4tfbetWwsxptBUWLY/1FcxxQCxwQOOEadTnspRkPRxbNsLbWI6jVzSDYbieUd/S3ryZpbwLYD7bg8CkZzEumL1mFvqCQneMxonHXoA+VCDBkxuOJjfMXGLWb9VW78c+fq6sd+6GcxzfUBMxZX9nkbqI7vbMUNmJMCBwGPn4bVCF7HHgK7P4e5Nvqs7599XWLpBydeH6A3ksRMki3ganmZTp8By+TxMFyPHjjVGUq+DpR/s4QQQgghhBBCCHH5SQJYXNesj2aRMhIU12/Vc26vE/qH7sQMuJ3XU6tF7LzqinhTIkuj7K450zIKgFOdl+mQ3z6YmWgCFPw9LKrq2RE6T6Fup5kbtuJd89O1g/XM6ckYAcXdzKawMxJttkZcmpKD/A4Obi8mL3setrkF7HB4QWdhWk5mICC+OsTF41fPNE2cor2jcXXG+EqNW+z6q9y+zR3jqMg9VBNnTsdiiLjUT/qvH/pNzHO9b2NxeV2d523A6tzOMacC5mRWJcG0OUkYcdO6M7z9feuzq/cM9a7vn33x9EPgOTYaGZOazBhdJx0HD9J6UsFoSSfJasSAD6920l/Nf7OEEEIIIYQQQgjRbyQBLK4PD1ewu7aKirV55C7OJXdxIeurd1Nx/1h0fie7t+4OnnN7rUr7fhVbvp9L7ve38JM5VnTeo+x7/lpvteibvThcCmBmenk5CyYEvnUePp4FpbUsTDKA4qR9V/f5M35lFQ12Ow2VOdpbfaY3ppKUoB4WqU+YQk5FHdPNgM/BgZe10Rd30OkGTKSXV5AzRbtnZSSTXl21pZzpoCVwduiYKTmUVk3pvnVsahFVtRWsnJnKmK7jDf0O2ls78QE6nTEYGk8d4tLSrp7PaUqnvnIlM7vGDpiwoJTa8q5x6fsYx+pqjluXM361/pbJ5SwYH/3Myb6UG4u45o5XQQGMSZlkJql9NmVpJaWLkgjNmkixtC0e/dUPXS53fWOf63GORcDlrW//P2+Dzc6WDnyYGJ+5lMljDPgcB9kesWNNnH3Wh2eov0R+9k1gQfmlfPbF1w8urw90w0lOT8TgdlLjh5dbO1BM41mQqAf8eLu2kh4I/2aFmVJUp24rXV/BguDq4+j6K1YIIYQQQgghhLiW3DB69OhLPBz22jVixAjee+897eUrIi0tjUOHej6v9Yp5dAv2+0fT9qPoZ7kOGvfmseX/fgPzSD26IYFrH3lxv3GI3dtrOXRaE38NGreyivXpZgD8nW3Uby5hn/bcXgE9PPu33HIrw4ePCP5+5sx7fPDB+xExl01OJfaMntISAC4abXnUEIp1NWpX36RSWr+aZNrZMK+YyNP2ersXkJhDZXkGlqi7Viq4GgvIq9EeSBgo1wDgpXVtFusvZUFbr/3gpX1TLsVdh1P2Gktkn5FKUd1qJvaUFfCF+iUhp5LKDEvP28aGxZJaSv3qZKIvNlNwNeaRFzxEN/Y6xCsxp5LynursasTWNVFiHeOudgVfm0OlPQOL9veuOvc6Fldm3ILGr6J23WRM4dfg0suNQVxzR59JRd1CrN2CvXh9RozRntVY2hbX50Mc/RBXuQFx1Ldn4eMW+1yPayy6XO76xvq80cf+jUU89e2vOgSNp6huXWC++WjfMI9ux8LG02dxPUOazyztS/qq1/7VfPbFU4c4+kG/tIrd09X/redpziV7cyeQSUVDoG8UJztm57OX/vw3K462BQVeE/it+7wL11+xQgghhBBCCCGuFM/pDzCNvEV7+ZJE+07/eicrgEXvnl+BzTbIk78Ar1ayInsuszPCtqvLzGLJuusj+Qvw+uYlwbbPzZXkr7iIjhryCp6j1e1FCbvs8zg5sOGRKMlfgCM0H/egAIrr8KUlf3uk4HW3sqMg/Iv0eB1hfW4BO1rdeMMbF0VnTR41hyPjfB4nzdu20ardyvNIMdsa23FHFKqE9Vn48rbY6xCvjpo8HtlwAKfHFzZ2gX6r2RUe2Icx7qsrO25Bxzey8blWzZho9aHcGMQ1d/x7Kd7WjNsbuuRzt7OjIJfDp8IDw8TUtnj0Tz8EXfb6xj7X4xqLLpe7vlf0eRsMjrOz1a3+p9dBY7QsYTx91pdn6HJrb6bV4carRP4bcMmffXH0g7/zTCDGQ0dL1785eznmCrzSe4pg9AD5N0tVQ2NrYPB8TtoPa++H669YIYQQQgghhBDi2iIrgHtxNf9iYMCsABbiOhTt2b+iK4CFqscVaGJAk3ETQsRgSmk9jyXrNCtNhRBCCCGEEEIIca2TFcBXhqwAFkIIIYQQQlwRXefiPpZsAG87eyT5K4QQQgghhBBCCHHZSQJYCCGEEEII0b9yKrHb7eyuXsOcJCMoLhqfWh/jGbFCCCGEEEIIIYQQIh6SABZCCCGEEEJcIYFzcYsLuO6OPhZCCCGEEEIIIYS4QuQM4F5czT3D5QxgIa6eaM++nAEshBBCCCGEEEIIIYQQQlwaOQP4ypAVwEIIIYQQQgghhBBCCCGEEEIIcY2QBLAQQgghhBBCCCGEEEIIIYQQQlwjJAEshBBCCCGEEEIIIYQQQgghhBDXCEkACyGEEEIIIYQQQgghhBBCCCHENUISwEIIIYQQQgghhBBCCCGEEEIIcY2QBLAQQgghhBBCCCGEEEIIIYQQQlwjJAE8iBm/fBP/suhmchd9jhTtTT7LrEU3k7tIz7e/fIP2phBCCCAhp5IGux17XRFT9Nq715/M8nrsdjt1RVO0t4QQQgghhBBCCCGEEEIMEpIAHqTMD3+B5380hqwZX+A7M27lLm0AnyNtxhf4zoy/J+9HX2bLw4MtCZxGyS479sps7Y0BLeV7tdjtDWx52Ky9JYQYgKYlWdABGJOYPF57dxDKqcRut1OZo70RixwmJxkAME7MYIH2thAXlUOl3Y69vpRU7S0hhBBCCCGEEEIIIcQVIwngQemzzL3nZjVp4X2f/3j6L+zThuBjy487cXoBhmC5Z3iUJLG43Aw6nfaSEH0QSKL09NO37N51ISmngrqG2BOgBx0uFACvg8PHtXevNzUcdvgA8LY2slN7ux/FO25X1fBUllbUUh98JhuoqyoiMynKEvKu2Iaw57ehntqKpUzQhkcpt76qNHq5AUnTVlJRW6+uYg/8DIo+FEIIIYQQQgghhBBC9CtJAA9KQ9DfpP6Xp/00dYc/wasN4VNcr5yj8jX1y3xuGoJRGyIuu0M/zMJmm82KF9zaW0KIK2B4QgLGOP4Oo7Mmj9k2G7as9bT4tXevP3sL5mGz2cha36K91a/iHberJnUVtT9ZzXSrCXWtNIAOo3kiC0vLyUkIi9VnUtEVG942nQGTdTprKlcRXHSekElFdfdyDeZktdzE4EWVfgIrqxooX5aO1WRQ/yBMCCGEEEIIIYQQQgghAiQBPMgZbv6s9lIEc9f9T/7GBe1NIcTA5mtng82GTfuTV6ONFEJcCcfb6fR7cTU/x9qH1Ocxd1MzbgXQWZgwPykYql8wBasOFHczm5Y/FHx+l3fFmxJJD4RPW5aJ1RAZOzf3KfY4vKCzMC0nckPuzNJVpJt14HPT3riJgty5wfLl40EIIYQQQgghhBBCCHHD6NGjP9VeFKoRI0bw3nvvaS9fEWlpaRw6dEh7OSj3x3fynTtAeeMkDxR9pL0dNGv9l3nkrs+Cq5MZK85pbw9gaZTsyifl9D5sebXam0L0q2jP/i233Mrw4SOCv5858x4ffPB+RMzlk0OlPQOLr50N84o5or0dLqcSe8Yo2jfk0py0jkXplsBKSgWvs5GNxTtxdK1szanEnmHB1ahNEqVSWr+aZALvl1pK/epkTjU+TntiKXOsBlBcNBYU4Mqs5rGJRlA8HN6UzcawyqUurWDhZCumwBJGxeui+bm1bD9yJhTU1TZXI7aCY2SuWkpmslld9ehz075rM8UvdwSj9UnTyFmQyQRLaBWl4vPgOryD/O2BNw+0q3cuGm15qM0OtDe01FJNtkfr63j6F0CfpLYpyRy56rNLT+9zMfokMlcuJSPZHFwpq/jcOPZup3ivIxQXHOO51HhXsTQzGbMBtb6uZrYVbOeYZj5E5WqM+ocGsY1xwPBUlq5ZyOSwsfO529m7fSN7Hf7e3z8ofNxU01ZWkDkhrA4+Nx0Hd1Kw81hYVMj4lVWsSTeDq5HZUdp0OSSsrKU63RTRb13XPM2Pk705NKcBVtbaSTd5aM7NZnPnFErrHyNZ52RPVj47I1aij6eobh0TjWH9ML6IunUTMXrb2ZRbfFVXrqvzwYJJO9m18zyu+RvH8xbvnBRCCCGEEEIIIYQQV53n9AeYRt6ivXxJon2nf72TFcCDlPKJ+n91n+t9BbDxIvcv6tEt2O27KblXz6TFFdTuDpwz2NhA3bZCZlk18SPTyN1Yy+6w8w53V5d0jwP0d82lcFsdDY1hsbWF2LSBQXqmrq1T4yqyUIvUM25OIVV1DWHnK9axZfEkup2a2FW3rvdrrKPqezZsa3cH2hgZbn0gstyGuioKH4jSkHDB/gq7pp/UvU+07dSPY+73q6jbG3ZO5N46qr4/K9DOLtlssdvZvTYN4zdz2RJWv93VhdhGRgSL64aBxGXVrJ7elSxB3ZbWOoeiVamRoXEYNWEVGdZAVkVnYfLKCpZNDGwmrzMxISMzGJtZUc/q6aEkDIDOaGH66p9QGbEvbsDQBIqqy1nYlfwFMJhJXrSKVcF9cVNZVbSMdM0WujqDCev01dSu1O6L219i79+c8lK1TdGSv32ln0JpdTkLJ4aSZwA6g5nkheXUlU4JjwZg1ORqyhd2JX9R62uZzqrS0JjFK64xTsyhMsr2xwZzMgtz5odHxiWzooFl6Zo6GMwkzZlP9KNvU8mYYEYH6CyTKQrOrf7h87qC/9259xguBUzpz1BfuZKZ44czfPwCiqrqSTeBt30XmzsBjOh1ABfwdkvmHsfRqQCjSAhMtaR0C0YUnI1XN/mbU9kQmA8Xmexxz9/Yn7e45qQQQgghhBBCCCGEENcRSQAPNnfcSNaK0aQFFk25/9D7t7+/+EPgDGDLSJ5eYeDbd2gjYmO4p4z8b5vw/s6Ofb+dox1+9HdMIruohKlhmdbstfnYEg28//sm7PvtNP3Ow9CEFLKLCkkLK0+fXkJ1WRaTEnR42tVYe3Mb7+tuxRQWF6Jn0vIKcu82ovxhH8X5dTgB7n2CwgWTMH3i4uh+O/b9RzlxwcjYGfmUPWwOe/lUSjblY/sHI0rHUfX9Wj0YJuXyyFeHhr2PyvroFsoejizXPcTMpIfLqJjXLbXcixTyKwuxJRr4y2tq3zW95kYZaQq1Uz+Vwm3rybrHjM7TRlPg/Zw+PeZ7simrzNYkgQHTLCq/9y34b7Xvjv7Bjz5hErlP5RLWajHYGZJZ3fUHAWE/9aXdk7oGgwG8DvasVbePXdvsRgEMlslM0AbHyGAyoTif46FN7fgAo1ldRfn44814AJ0pkQmAPrOC+VYDeJ00bsoNbkW7qdGJFx2WKcuYpi3cnMxEo4KnfY+6le7cAg64FMBEYte+uIDi9+Jsfo4NYVvobgq0zZSUQRJATV7w3oZ29TPP1ajdOjt8FekRiud1Xd9A4CW9iql/p5UzxaIDn4sDgX4IbuMLeFs3YOvD6t/UVTkkG1Hf/6lA/z60PNgPxuT5rAp1GQAGoxHF0x6Mz93WjhfQWaexsisvFtZvwZ8N6lhrxTfG41m1KgOLDhSPIxT/0HI2NTrwdP2zFfe45TDZqgPFyZ6ILZUbcQQL1TpC83EPCqC4DrP+uPb+5ZGZZAJ8nDwWdnZyZw0FxXtw+sBgSWfRuhd5cd0cJprBdWADWcVdsR2c8gK6JOaUL2BCgvpvzPAxU8gprWJ+UmSCdUKCCfBwSllJRW192GdDPbUVS5kQzz9RfaRfUME0iw4UN82blgfHIregGbcmtk/zN4bnLb45KYQQQgghhBBCCCHE9UUSwIONZRjfSTdi5BM8h09SVNX7Dt7uqk4qD/tRuAlr+igmXWy3zaj0WK1eqhdkkf/DaqqfraZsVRaFr3jAmMLcpeNCoZ7XqV09lyXrKql+tprKH+RR9/8UMI4jLb2ruLmULk3BqJxgX1hs9eYSlmTlE23DZ+ujZeTfZwbXPgofq1WTvwD4+OMrZWQtzKfs2Wqqny1jRXETHnSMTflOcBVw2uPZpBgVTvyskKxVZer7/TCfrDX7cKNZvXRHNkumj4W37RSGl5tTSdtZHdZvLyGsxb27ZyrjTOD/XS0rAn1XuW4JWdklNARC0h7PZtJIhRM/y2fushIqA++XvzCLyte86Czf4dGHIr/R199xKye2PhIss+yxYpreBRK+ztyvRYSK64TiOcym3AJ2Hle3PT2+uQWXAgzV0f1PHGKkuGjZ/DJnWjo5BYCHw9tq6Ojw4ydU9rQJFnR4ad2UT01LZ/DlLTX57HEoYEhgvDYLrXho3fYI2cU7OX4G8DvY7lBfq9cPDwQdYX12FvmbX+bIydB2ri2bj9OpBtIV2d9i6t8EPQbA69jB9kA/+DuPsXNDK27AaOr2pxwxmMn0JAPgofmpAnYeC/TvmZO0bF7CDodPTZpPiVzt6HPuYXZ2cTC+82CxOhaYsPQhKxbXGKdmMN6kbgO8La8gFH/mJC01BWQX9HUb5k78PkCXQPK0UMbwZEsNBdkFEdtEhzuyMZvZNlu/bf88pbQusKK3hoKDkff8bheuU9qUuoFRFgtJwY91B9sOOtVkaNIc1lTvxm638+LWx8gIXyEfwczkRelYw5e+YsBknc6aylX080Jn5idb0eHDUbOEzS0ng9c7HX4uRET2bf7G8rzFNSeFEEIIIYQQQgghhLjOSAJ4sHGd4+e/PoufIZgm/z2F87QBkfTzTORO1qPjI96od/OT17QRsfG01tKkWWDl3NqEUwHTFycGE62164vYF8rOAn72veUG9Bi/qF7RPzgJq07B2VBIbURsdNYH1lN0/1hw2SktCE/+Aq9WULT1qJqM6uJ8A/dZwDiarwOQRppVD6fbqHte84bOWn7+RmTDzDMnMVan8OYvqiPfy9/E0bf8YDKTEn69N+738QH6sZMit2c+7UVdEziLb9/VQ93w0/TMIU6gw5qsGei3f8PTzeH1dvKrtzyAAUPomFox2Pna2aBdoWmzMa+4+xrSzmMbNdvBevAr4b/3QaeDmlBeBVzH0BxlyhEmkGjSAUYmruu+WnlRknrPpFnhh9LJ4YOaMzoDK0LD26efsIDSqjoaIsrNoE9/y3IJYupfrxJI4s0nZ4Ka0NInTCBnzWTMgOL3aF4QC5O6PbCngxZN3wO87FJT83rjmIjrpzp2RvwO0OLuy/sD8Y6x1RhIhB+8zFsUH+Spmla8GLBMX43d3kBdVTkrZ/Z3urNnE1ZWsSzZiOJqDFvRG6CfQunW1Uy3GFA87exYu5xNB1z4AIN1DqXloU2r/XvzKXiuFbc3bFIpXtztjbS6AS6gRGZWUbxODmwqCFsJ3YxbAUzjmdOHJH/sUkkYBXAKlybh3V3f5u/Fn7c456QQQgghhBBCCCGEENcZSQAPNm+fp27D/7D7jY+BIVhSet/r8TspN6vrW12nKfr3C7j79GW8H/eb2k0dATz4PgpPtAJ6M1PnFbJ+0xaq6hpo2NuA/f6xEa/6+u2jAS9/PhJDZUamUfTwOPSeo1QXVPN6lJcYU2aRu7aCLdtq2b23gYbGfFJuDo8Yi/FmUN55k7bwywHK3yJ/H2s0ADrGPdr9S+W8FD0wGrPmvOAevV3Hvl95UIwp5O6wU7ethOx0c9j5xLdiuKnnuuE/gfcsMNLEpPDLHmdk0ht43euLSLQLcWUMRdfnJcYXkVpE9Zo5JJuN2nX6A9PefJrdgMFKxppq7HY7u6vXqOcoKy4O7nhZ+4o4KDi0l+Jk1PW1F/s2xsoF7afUpfO3rCdrbgHbDrTj8igYzUmkL1qHvaGSnCt1JHTAtNI61qSbwXWA4iirmqetUbc+VtwHmJ1dzN7jJ2nZnkd2wQHcCugs06gIO5K54+X1LMmaHfpjj9lZLCluB4O6Yr7jWHjpbppz89neEpoVJ1s2s/6w+odA+itx/K2iBP6QKRaXPn8j9W1OCiGEEEIIIYQQQghxvZAE8DXuwvnAFtFDCEs69oEmSRrhQ5/6JbA1my07q8h7aBJfulmH8u4bHPpFE/vaoq06U1BOa69F4ffg8YPOOJa7JmpboGdqUR11JdnYvmpCp/j4Y1sTTQcOceKsJhS4oMSTjPDifEU9szfaz9ET2vie+Gl6Opus3Ersv3NDQgqzVlZRtynKub5CXCHGUZH7oibOnI4l+j6zF5XKETpPoW7xmtt9tXLXT1923505PRkjoLib2RR25qvN1ohLGzwQpBYx0QyKz4svuFpRweduZ0dxATVRVkBenBdFAUyJLI2S1JtpGQXAqc6LH247M9EEKMS/EDnOMfb41TOaE6dEFnO5+B0c3F5MXvY8bHML2OHwgs7CtJywbGp/0iextLKBZclGdavtvO04ovzzkqA3AAqulu0R1/2O7bS4FECH0dJ71joxZ6GaRHYdY2/gmsurbptsmaL9NxFG6fua5I/HGfx+QGckQTMnE3OSiLx0+eZvpDjnpBBCCCGEEEIIIYQQ1xlJAA9SRsNnAbjwwcfaWxHe/+gT9T+MN8a+bXE3eoyW7l80c8ddmG8GxevmdSDtX6Yy9iY/bZvnMjd7CStWqefZ1r8buU+q90P1y+svzYi4HN2Hb5JfvI8TmEhbWkbuXWH10M/jOxONKG/byZ+dxZLHVlD0w2qqn30j6qok/ResmLUXAeNNkcuI1PrpOe9Wz9ft/lNH09sRL7kof2cT1T9YQtb8Iur+nx/dl2ex5FE98D6+j0B3+53Rx0cfWL3sOcFR7T0h4hXcojiTzMABpFOWVlK6KAmjNjYOB51uwER6eQU5Uy7fnqumQDJLOdNBS+AM4DFTciitmtLjFtBn/GomzjK5nAXjr9QJwarU9CSM+OjYu5H1xV1b885m3pJi9kbLEMZkLw6XApiZXl7OgsDW0gwfz4LSWhYmGUBx0r4rsny9MZWkBHWM9QkTWFBex3Qz4HNwoA8LkeMa45Z29bxWUzr1lSuZ2VVnYMKCUmrDtj7uEtO4pRZRVVvBypmpjOkK8Ttob+3EB+h00Wfx+JVVNNjtNFR2f9+4DZ9GUWUp0y06vO3bmJfffavtSDoSJi9lSrDCMGbKUiYn6AAFryvKXwUMH0PSlEyKKut5JsOCTnFxsKYr/Qstx07iQ4d1fjlLw87OnbCgnMcmGgE3zihbM08pqlN3s6grIkruOA4OHKfUf8cnF60kdXhoPpZnWDSr9fs2f2MR15wME+yH+goW9J5/F0IIIYQQQgghhBBi0JIE8KA0FFPge27f2d4TwC6v5tDAPhr7T9mMi/jCWM+sxd/AhIKrza7GGNWE5l9aw7/ItZKdEpl2fX3/63jQYf1OCVNj+RLaWUvh9qN4h4zFVlJGdtfS2a+ZuBW48FdXxFm9+vu/yZ0RW0A38WYncNs3yE6PfEP9XXnY7or8uvr1X53Ai447v5176at09UaM4W/pf53dTW/iBwzGLwH7aH3TDyNTyHpU+256pj6extiwPhbXGUMyqzXbkNvtdux9TWQdPKYm5gxWFpbvxm6389h0Cwa8eH3a4Nh1bt9FqxcwWsl4rLx7fetLSdW+KAYHHS4UwJC0LFjW1scySDb3vFzZ0dyBB8CYxJx1L4bVo5Jgr+VUhl1fTbJB29dhsXFQk5gGkhaWU16u6YeGOqqKZmpfEpOdNQfVcTMmMSewtbT9xXXMSTahQ8F1sIadmvyZafJqyqvVMd5dvYY5SUbAS3vNRrqfIH1xcY2xfy81BwNjZ0lnUVed7XbWzEnGFOVzP6ZxQ4fRZCV90Wq2vhh6762LkjCg4HJEyXqSSsYEMzpAZ5lM0SUeF5z62AImmtR/M4zJoXkZ/tP1eO5qbMcLGCzTeWxrqE1bH1NX3Cuug+R35XVTS6nvKuPFrZQ/tpCJFgMoHg5v06weP1igriA2WJj+WHjfJmFEwdW4me3hZ3cDkESyJfA/HIwTmb8s9oRpNAf3HMcD6MzprH4xbD56Xbg1nyV9mb+xiGtOBuWQMTHQDwYryZO194UQQgghhBBCCCGEuDZIAnhQuqCeCwsY//Fmvv3VIVFW792A5as3Mfeuz6m/fvRJ1FWxsVHw3pTG+potFC7OJXdxHutr6si+S4/i+jnP16vf3Db9wQ2YmbqtIhBXyJZdFYz7jOadnZU8/bMTKMYU8nbWUfH9XHIX55L7/fVU1VWQHRkNgL+5jNytbXh1Y5lVtkVNAv/6Df7sB31KNlVr88hdnEvek7XUPTQaX8QW0G6q/+MoXvSkrPxJKHZtFT958uv43tZ88/zaFupe86K7w0bFripKVgbqt7KEiuo66orSAoFpFNbZse/dQvYdkUUE/dMKKnfVBd8zd3EhWx5JQY+H1/e/DoD9h7W0eXWMvb+C3dtKyAvEVeyoI+9uI97XqikO9LEQl8S/l+JtzbjDHkmfu50dBbkcPhUeGK8jrM8tYEerG2/kgv9L0lmTR83hyDJ9HifN27bR2tM2xsc3svG5VtyXsyIxcmzbiyOQ/FIUzfvrjJgnLqK+fFrk9Vh01JBX8Bytbi/hpfo8Tg5seIS88OxgezOtDjfeiPdX8Lpb2VGQS3FLXz9L4hvjjpo8HtlwAKfHF1bnQD1qdkXEQozjdqSYbY3tmhglrB+6ZT2BIzQf96AAiusw6+PdafgS+FuKyX1qD+2acVN8HpzN26KeG6xSULxuHM3PsfaRbDZGGbOaguJuY6F4XTRvK4icD0EOtu1qpys3a0q4xEz48Y08vq01LNnrw92+g4LcPXT7KIln/sYlvjmpqqGxNfAB6HPSflh7XwghhBBCCCGEEEKIa8MNo0ePDhwSK7RGjBjBe++9p718RaSlpXHo0CHt5SDzw19g8+ybA1stnmXfjP/hJxERw9iyPyGwTerHuBr+yIoX+jDUj27Bfv9o2jaXceKbedjuMqEfAihe3K81sOWH+8JW31qZtXYF85LNaswnXty/2k3h2W9Td/9YTvzMxornu2L1jJuzgtyZKZiNgRW4ih/PH5uoWlVLG2mU7Mon5fQ+bHm1oXd4dAtl949F99EJ9q1ZQb0xl7KlUxkbKMPveR37ll8x9vt5pNBGxfwSunpRPzGX0ke/hTWw/Ezxumn72RaO/mMp+XdD24/mUvJq1zsZSVtaRNY3raHVaoqC9903aHrxaepa/YEEcD6TPneCfY+voPbtsP7qKuuOuZSsnc1dI/XohgCfKPjffRP7zrJAGQH6SWR9PwvbP5rpOsJR8bp5o7mOp3ceJRSZzRb7LEa/VsHcdZr58egW7N36WfRFtGf/lltuZfjwEcHfz5x5jw8+eD8iRlzfciobyLAoOLblUnBQ3bK6y/iVVaxJN6PztbNhXnGfVuFeEVNKqX8sGZ3jOWYX9GGvaDGATaG0/jGSDeBtfYqs9ce0AUIIIYQQQgghhBBC9DvP6Q8wjbxFe/mSRPtO/3onCeBeXM0Jc7EEMIBxsp7cb9/MaP1HNH3Py88j7n6WWYv+DtOFC7zxiw85Gm1hVCy0Cc1r0NSS3eSlKBz9YRZlv9bejdN10F/Xg2jPviSARe9yqLRnYMGHc882tjUeIXBsMQlJU5iZk8N0iwFcjdjyelr5eWXllNdice3iuT0tnDwDw8dMYeGqZaSbwbkni/y+7MsrBiR9wgQyc3LISDahw8PhtdlsvIKroYUQQgghhBBCCCGE6CIJ4CtDtoAexLyH/ZT/4F1WdEv+AnzMvufOUv3CJSR/rwsppHxRD4qHE5ea/AXSbh8N+PD1fb9tIcSg1E6nB8CAdU7kGbXV5Y+pyV/Fw+E9AyP5C4DeRFLGY8G6vrj1MdLNOvAcY5ckf68ZqaX16jnQgTN3PYd3SfJXCCGEEEIIIYQQQohrnCSAxXXN+mgWKSNBcf0Wu/Zm3FKYZNHDWTdtv9PeE0Jc246z8fENNLZrz98NbJnvOMCGR7LZOID2ft61aw+O0CGuaj1bd1CQtxHJD15rQmclZ29s0d4UQgghhBBCCCGEEEJcY2QL6F5czSXjsWwBfUVcK1saP1zB7nv0uN9+kz96FOBWzF8bx7gEPfid1K3KZ/fb2hfFIpv1NRY8bR5MKWmMuw1OvLSCFS+4tYFiEIn27MsW0EIIIYQQQgghhBBCCCHEpZEtoK8MWQEsrg9v/5m/cCuW5KnYZtiwzZjEuJEK7tf2UbGsr8lfAB/cPI6pM6YyboSfE/srKJTkrxBCCCGEEEIIIYQQQgghhLhKZAVwL67mXwwMmBXAQlyHoj37sgJYCCGEEEIIIYQQQgghhLg0sgL4ypAVwEIIIYQQQgghhBBCCCGEEEIIcY2QBLAQQgghhBBCCCGEEEIIIYQQQlwjJAEshBBCCCGEEEIIIYQQQgghhBDXCDkDuBcjRozAYLhVe/mKGDPmC5w8+T/ay0KIK8Dne7/beQFyBrAQQgghhBBCCCGEEEIIcWnkDOArQ1YACyGEuCoScippsNux1xUxRa+9e/3JLK/HbrdTVzRFe0tcp3Iq66haOUF7WQwk+ikU1dVRPjNRe0cIIYQQQgghhBBCiKtGEsBCCCGuimlJFnQAxiQmj9feHYRyKrHb7VTmaG/EIofJSQYAjBMzWKC9LQaEKauqqLfbsdvt2OsqWKDJ+S2tasDeUEnOZcgFLqioJ8NixKC/Rv86Qr+AigY79qql2juDS0ICxqFGkhatoXRA/SVLDpV2O/b6UlK1t4QQQgghhBBCCCHENU+2gO6FbAEtxPVpwGwBPTyVpWsWMtliwqBTLyk+D67DO8jffkQbfdUl5VSwapoV70EbeTXau90l5FRSmWFB521lU+56WvzaiEEmpxJ7hgVXY2zt18osr2dhkgFv6yb+f/buP6yt7D7w/zvJWMmMlBk0nlpOKrWx0hbSVEkK0yye70CmC0kLVWDj4NrrDos7VF4MzxC8Q3EVHBO8dhRTsjjKg3HNkuJl1mUKIYujhe4U0glOB28ycn5o00DbkdOKppEzHnkmUidznR/fP64E0kWArvhhsD+v59HzDPceXd17zrnHmvvR55zqU5Pa3etGb7vddjn5VBw8yN5SO2ai+E/vp22J26GovpODxXlY1Ng6SiSEf+gMpy7NaouuWNZY1cnAwTz1RwsJ4SnctR0EgNymPj5TaiY46qaxd/Hx9VCPZSHi76K6LU1fSIwNeRbU01WIhPyMnj3DcEBzI6UZR1CihINT9Lad5Upy8TTHjYYCDJ/tWHzcOEdZEzVVhdgtpvm6yeQeSNTXzFA1zReSjp3mHDb9teW68HoqsRNk1N3IKpt/jbjw+iqxR/2c3t/GEreIEEIIIYQQQgghxIaTKaA3hmQACyHEJmQsaWXg6aOU5yUFNgCDyUJeeQPtmzClK8dqxZwSHVveXG8je5xOnNV3QPB3DQy79+N0Ojc0+EsW7Xbb5BTh8vQw+PQJDpXaMWv3a1R4BjlavhDQBTCYbew+5MGrSdHNpGxZoR0DUQLdj+Pc52YqDFisFALkNtFSakEJjq86+Et+Cy2lFoj46e9I0xeKWuj7fHxsmN9owGzbzcF2Dy5rUlljFZ2JssltbDBhySvnmLeF+eR7axWd5xYf12QrUI+rzWo2FtLUM4KnoZS8pABpZso4WGiB6CyTycHfrXpts724L86gGOyUNWQ1BYAQQgghhBBCCCGEEGtKAsBCCLHZWF14GnZjBpRwgNGuJ3E6nTidTupOnmciGEHRvkeIO1x+wyEqHTZMKIT9U8xEtSUWGCs8HHCYgAiBoePq/fP4cYYCEcCAvcxFVXy2Xj1lF+xgYWbmXJpaSrEoQcY7tKmh+tUcKMRClMBQR/ofRlz1MxeLEJw4z/HH4+NC1wQhBTDYKTzgmC9qrCkhzwBKaIKuJx+fH0eeTJS35FIaL17WUEWeKbXsvrqTaj0Y7JS5Uicmr2pvodRmgGgI/2gX7rp988dflCGrYawpIdcE4Sv9jCfv2MLXFhtuZjyoYLCX4KlY1GGEEEIIIYQQQgghhNhQMgX0MmQKaCHuTrd7Cuj81gFO7DZDeJqTjadSpzFNx+igqqmeygLbfCanEg0RGD5L23BgodySUxQX0T54lAKSpgp1efFV7sB/uo4JRzzj0oA6HevMKB1tFwjEFo65vCCjzkbUj4x/VlKmJUtNUZrpOSQYHVS11FPlsKVmBCYs9Tkr0V2/++iNtFBfVYDNhHq+wQm63UlT0i5Xb8FRnGmiTIunKA4ycf44Zy/f1BZNOzVuNORfmO52uc+fl9xuqrKmTqoKk84hGmJ2/ALuC1eSSi3Ib+rhWKkNgqPsSXNNuuS30NNgZPJMB8OB/Hg/Sj8FtMvro9KuEBpzc/hsckZuPq0DJ9htVpjp30PzcOZlz+zo4Vy5LWk/KMFROoKFHCs1ExxtpLF3LmW/bo4W+jzFWEJjOA+f1e5dlrWpj3OllpT+k9gWnniK2jOpmclNfT5KLWEm6mo5M1dC++ARCgwzDFU3k5yUu1APSf0hv5WBE7sxR/x01bWlD1Qvo77HR7kl3Welt2WurczDYIMDUxbtt1rq+GDHoh38tOOervFMx/ird4wSQgghhBBCCCHEXUumgN4YkgF8J3ijiTf9UiH3/sZvz7/e8ktW3iCtK8QWVEhZnhlQCIxmEvwtof2ch4O7Fx7mAxhMNgoOehhoL0kurZOJ3IZzHC1PPPhHnY41by+tLRs1B3Xm5+DytHOwYIngb7ayqN8dxefwHEwEf1HP115OS3tVakEdqjrTTVFsp/zo5/GmzIsbX480zdS4JlsBB10HkkvqUtU5QkOp5hxMNhx7D5B+0tsiKgttGACDvZjW+fl4s3S1g8O1bUuu17qgArsVUIJMJgd0c/KpaXfhMAMYsDqKdJWdO3uYoZmF7PtoaJrefiOuUgvKzMXVB38BR1kuFiA8e0m7K2PRSHD+v+eGrxBUwFL6GQa9TVTk55CTX0NrzyDqLNMXOTMHYMZoALhFZFH1XiUwpwA7sMZvOUepHTMKM6M6A6SoQdJiG0RnJzMK/ibb9Nc2PsZsFLDl4drAJGCXdyQ+Pqww+OkezzIff3WNUUIIIYQQQgghhBBi3UmIcCsz/Qb3/c4R3lZzBMsHP0hO/sM88N6HeeA3C3nwg3/I22rc7Ch38mbTPdp3CiE2LQcWM8AcwQxiQEUtLgrMQCTA0Mm6+PS1T9I1EUIBzAUHaFmYNVU3k8mkHvu4Om3q8fhxTfZide3T3sb5qVFP+9U5eYOj6t8Lr+Qs0su07U9sP038Lcta8RxQg0oldgNEg4x1qfUwP8UrEJk+jTOL7N9s6tdkNqOE/fPl67r9RABDXhlNiThIUr3Nv077SVcdxqpODuSZIDLDaPzanE4nXaMzRDBgL2mgbL50Pi0tldgNienDk855NEA4EdDS3W4uivMMoMwwlDLd7iiB+YNqXWbiahgFUIJTnLqq3b9eLGrAL3KdWdSMx7ImL4NPn2BvgW1+DViTOU9nWbjQXK2uW+10sv/wOI6GUizKDBfbhuMlV6fQagEiBK/oDyZXOSxAlGtXktYNnuvF3TbETBRM9lIOnXiap0/sZbcNgmOnqW5LlJ3legQwONjrqaHQqkYvc3aV4Grv4YAjNbConmeY60oTnX2D+Hy++GuQvs56CpcJftaU5GIizNWhlMmfl7VVrg0u47+mAFbs2ljqOjHWdFJmN4ASYiJ5uQD3BCFN2azGswzGX31jlBBCCCGEEEIIIYTYCBIA3pLu4Y2/Vo1l70fIeTu8/p1xwgMe/vV//Ck/+J9/yg8GPHz/f3yOHz7/j/x0+2+yfe8RHvi1h7QHEVvd+w/R2d1FZ91q0+rE1lVBucMEhJk46eZCImh08xqTZw7TH4gCFnJLss++UsJTdNW5uXBVncLz6plJggqwzcA2beF1ktE5WI2YgEign7OTaj3E5q5w4fQ0IcBsUQN4+mRXv9GZIfbUts2XnxtvYyigABbsWURBygrtGIgw3dVMb/zaACZ7m9XjmqzkJyIxRZXkW9RpX7sb3Qvlb15jstdNrTvbaZjniEUBg5WCsoUI0bXJXty17pRpopNd7qhlj9O5+umfsxGLklPfycCAh4ZSOyZQA/NDgcWBdj1l4/JbGii2KMxcbGN4qRi4LoXsMANEuJ5+Ru0llbQPxLNee3Fr4qqxUJDgde1VmNhht+OYD2YG6B6fUYOAjr0cO/cMPp+Ppz93hMqkQHgqG8WHSslLTvnEhCWvnGPeFtL+y2StpzDPgDIzRUeGPwjYMtcWdy2irh1ttGj3rI8DBXkYiBLoPcyZyWvz2+cCMW6llMxuPMtk/NU1RgkhhBBCCCGEEEKIDSEB4C3oje+qZkfRO3hD5Bv88OkuXv7aC/xU+UlqoVs3uTU7xI3/2cPLITAWuTC/Kye1TCbiQcZu7eu/neATtY+xS1v+o82LyyZepw/xW9ryAG/fx4nuLrq7m9lzr3Zn3FLnceZP6TzRTP1H8rlf+x6Sz+cErgyyIO91fowziXOZ35pP/ek0nx1//clHUw4hxAaKZy+GZ5lMXQITgEvB6wAYzYvu1IzNXenQTIMaJqYk/73+MjqHiBIP8BzAVagGMIzWQlzHirEBSiyseUMmsqvf67MXUv4GmAxl8/kAheRaDICZ3ScSmYgLr0MOdZ8lMb7lmeOB8HH909cua5yTvdNEMGEvP4rPN8JAj4emiuVCYbeZvZyj5XmYDaBEZhg7/bgamA9qO4/OsqjrETcUq1M/n4w00DMYb5ORATprcrWlM7QNQxa/qihs6qGhwIwSHE3Keo0zltD+uaOU200oYT/9x5+kayxIFDDl7aXdszB5d2y4Gff5aUKRpGtWIoT8o0yHAG6hpEYU1brqcidlhE8QUgBLPnvT/NihyFWMjSizk4vvkXS20rUlBBbPM72OirDuALhOcMWE6uzGs5XHX51jlBBCCCGEEEIIIYTYEBIA3mpyyniw0AovXeGHl3zcSjywfOOvYNr7Cd5e+wl+4f2/slD+Zy/x44nP8cPZH3NvYTXGLGLAALe+/22+8txX+cpzV/jOi2Fu/Oyt7Myv5GNHK9mpLQy8+vdfjZdPev3ttxdNRwjw7rJ3s/3VH/Eqv8i7K5dPmUk9j38h9PJr3GP+Rd5dWo2n82N8+NeWiiC/ldzHHtVu1HgX+97/jqWzGl8P803tNT33Vb7+99qCQqxG4uG6FXuFdt9SFALaTXeb4WYmQoApj8pj5/D5fDxz7hiVeSZQgoz3ZzCf9pJWX79mwwprcy4pu6Cgcmvtg1CxyVNU73PTPeYnGFYw2xyUHjqBb8SLK9uY57qIoCQCVNEgE91u9lQ3c/aymsFodOxQg+ThgM6yCfm0NBRjiQboPwnHGooX1ns2mMnb20R99kn3upS1D3Cs1AbBMdrSZHeXHVOn/FVCY+ypbWP46jUmzzZS6x4jpIDBXkZn0tLUs5dOcbh6z8I04HuqOdzmJ54SzWxKZnKIibpmzk4u1M21yTOcmgoDJozaOjDWUOkwQfgqmcz+vKWuLYnVuOwc0etDUVAnu8/E6sezVNmNUUIIIYQQQgghhBBifUkAeEsx8ZZH3ofh5z/g5rN/zU9/lrTrIQf3xVNgt+1ykLrq74+59fyX+NG/5fDWRx7lDSn7MvOTG9/iL4e+wF8OPcPZ//Zpjjd/lq98/yds+6UCPpwmAeyVuS/Eyye9Ll3hB9qCPErJu97Ka/80xtfnYKejnHdriyRJPY9OPn3iOE0tn+Z/Toe5de87+N1Df0hJmhjwrdd/wr3vLODDafbNK/ptfmP7T3gtqsmmTrj1Mt/UXtPQF0h6PizEGrjETFABDOSW1Wt3asSDV5bctAGnCvsOAK7Ppc61at6ROhdnbkU59vTzoG4dRa3stoESjRCdz05TiIb89Le56U2T8bay7Oo3nYpcC6CgPxH5MnPXUadtrdOu0bvwmp9hORxDPeV1WoA0FmD8bBuNtftx7nPTH4iAwU6ZKynSdtsNEwwDKAQnOzgznjpIuwpsgEJ49orOsqqi1iMUW6IELp7kUmkhdgNEA904nU7cU2HARt4yGaJLS7S1Gc0tupjRQb13hIYCszrleONZAmli/lajKX5tZ1O2xwJnmYyPM2b78tH7XNdBNdAavEJipeNgRJ0u2F6yONi5w5j+xw7WmkLyDAozU90se8dswWtLlm8xA1EiQe2e9XCTWEz94YFVM0bluhykblq78SyVzjFKCCGEEEIIIYQQQmwICQBvJfcXYXrbPfz0xcv8+DXNvpcC/Nur6n/e+ucAi0KYP/tHfuT/HrztN+cDxavzPf5yJgy8le3Zzy4LRe/hl+59jeDVK4z//b9Azi4e0TtN4Gthnn/60/S+cAPu/VVKD7xLW4IfXLvGa9vewSNp9qnu5cP/bhf3vnaNf341NXwuxEa7MKquO2qwlTPS105N0cJNtquogiZvD61FAMMEggpgo9zjoSY+9TE5+dS093HQYQJlBv/FePRkfprkKqriC2SW1HtpP+TAPP8J2bsZUz/HXuyhJj/L6QayVFTqwEyU2eEOTrUlpm3dw/7DbQynix5lRGf9xhnNRTisav0arYXUeAYotwHRAGNZJCKPz4QAC6WeTlwlKwyQk351fU5LKYPeJioS5wwU1rTTlzQtbkJG7VbUSk9fJ00VRexKFIkF8E/PqX3VkL4H5Tf1MOLzMeJd/Lnr6dLVIAoG7GXttNfEf6WUk0+NR11PlmiA0XjET09Zilo5tNtMNHAR96UYmA0YgFtRNf/Sal4cNNTjylwYMGNPardFcspo9bZTbjcQ8Xezv3ml6ZQNWIvrKZlvONhVUk+x1QAoRIJpfh2RswtHSRWt3kE+U2nHoAQZ701UAkxeuUYUA3kHPNQnrRlbWOPhyG4zEGImJcs3n5rdNojOMnlhmftxS15bsnwcVgNwnbll1nEuaR1Qp0geaCVNnFmHAIHrasC6uLWJopyF8clTaSc1XJ3deJYJXWNUkvl6GOwk65nThRBCCCGEEEIIIURab9i5c+fPtRuFavv27ZhMD2o3b4hdu36Ra9f+JXXjr7t4+24TP/pSFz9Sl2rT540Pk/OfynjjN7p4+VtR7d703n+Izpp3QWCA5nOpWSH37v0TOh/bzuwX/hjvl+MbP9pM97//RUJfPsKnv5BSPI17+XDzCX7X/Hecbf1zvnNvOc2eD7LzxS/Q/LmvphZd5jzmxd+/69WreI8PMEvy+ZznRv4h3vfmf+Avm8/yFe17HX+Ip+49cPU8X99xiBLrvzDZ0MkIxNcArubdfJf+o+f5uva9S4q/7+ZzNI/dw8f2F2K7/x742Wv84JtjfLbvq9x670cXtgOv/vNXecb7Bb6ZEuB/K7+1/wk+/PA72B7PYH71+1f5q6l7+fD+FepEZCUafZkbN26kbHvggQfJydk+//fNmzd45ZWXU8qspZKWPhqKLZoH+AlR/Kf303YZyHXh9VRiT1tQITjqpjGR/mqsonPgIHmLykaIRM2Y8XN6fxuXAVxefJV2gqPazK0i2gePUpBcNiG/hb4TxSyeyD3IqLORXhaOu7TFZTM5B0dLH57ixZ8MxNf6HOLwqSyir3rqd9lri+DvqqNtuYV5i9oZPFqAKTiKM+WCi2gdOMru9DFWiKa2Ra7Lmyb4E7fo2Bm2W+LctEUgXg+NNPbOabbH28kEEGH6eDWnVjNULXsOquS+4vKOUJm24Ra3RWZl4+2wLcD5WjeXYoC1np5z5diS36LM0F/dzPAyTb2k/FYGTuzGHJnmePWptJmyRe2DHFUrdUmJejCWtHPuSMGSP/BQgqPsSVTYUvWrhJnqbqRD03eXrjPNfQEYazoZ2JtHbPo41ct0gq14bSni7WecGWLPksFrBy19HhLDVXjKTW3HKqYSWer+jQQJbbNjSx6rsxjPMhl/9Y5RKhdeXyWJEXPx5wghhBBCCCGEEOJOFX7pFSwPPaDdvCrbt29f9Ez/bicZwFvIPTkm4Ca3tMHfX/wIv/AHf8zO+dd/5C2aIqCuB/yT1+AeY7pVe3W6t5A/zLfAa9f4ViL4q9e9H+Ldu+7h1eAVvgPw2t8wO6dO1fy72rKZeG1MncpzuyXNNNLf5UtX/4Vb9+7it5yL54H+wGO/yv2E+cb4d7W7Vu/Nv8rHqgvgH6/wlee+Tejf7mVnfiX1j+/jY39YyH3ff4GvPPdVvvnPr3H/Lz3KwYYPsnCG9/JI3R9zsOgd3P/69+JrEH+bG/e9h9//6K9qpvoWd5LJjlqeOD1GIBRhfkZjQImE8I92q8FfgNleGt3nmdaUi4ZnGDv9RGqgIjZMW/cEoaTFIqMhP/3uOqa040o2rnbQcX6aUCT5TDZGoHuYQPx3Lcr8oq5xBjO23YcY9GQxL6+e+vVPMB0IEUn5fIVIaJp+9wrB32Vd5lSdm/7pEJlU7WxvI0+cHmMmHE065/h59F5MKQsZttvlNrpH/ZoySlI9aIO/AJeZuBpGAZTg1OqCv1nodbctqrNoeIaxk4vbIpOyRa2H2G2O4u89qQZ/AebOcmZoZuF90RBT3W3ZBX8Brp5iKqiA2cHeilWlhgIQm2yj7uQQfu04Eg0zM9Gddm1dlYISCRGYOM/xJ2oXBUhZos6UiLqOsjZAWlOYh0GZYeLM2nWCzXJtyVwHC9SZCCaXCv4CBOi+6CfxMzyLNc06Gnpc7eCp7mlC87/rixLy9+OuG2LRsK5nPNNF3xil6mV0Ov6PUXQG/5R2vxBCCCGEEEIIIYRYDckAXsZmywC+55Ej7LB9j+vPfHHxFM9v/E0e+I9OjG8BmOPlvj/nx9oywFvKP8GD/A3fH9Nk2C4lnnl7z/e/zfN//ypwDw/ZdmHbZeH+W2Gev/BZ/ue3ktJV4xm36Wizgnfu/xM+UXQf3zx3nN548su9zo/hKbMyN36cTl/ScTPJAAYeqf8Uf/Dulxeyd1Mykh+lsfOj5Eav0PnJZ7iWeNPbK/mTlsd46Noon/jsc5S5u9JnAC9KHQKiy2UFJ973GrNf+K94vxy/nvjn2bbBq4FnOHHuCuqed+E6dYj3Gb/Hl5o+y1+RVP9zz/FZz+jCOfNWPtx8nN/ddQ+vrVAnQr/NkAEs9FEz9hQC3XW4x2+m7Mtv6uFYqQ1D2iy0TaSkncEjBRgC59njziJbWdwZEhmdUT9dtW2kiU9uLfGs2G2Bbva7l5w7ecszVnUycDAPkjOPl1RC++ARCkwQmT5J9all5osWQgghhBBCCCGEuMNIBvDGkAzgrcaUkz7r82c/4meLosJav8K2t8LPlHSh4eVte/t7+MBjj/KBxwp59zstbLv2HJ9u/XRq8DfJq3//Vb7yXOrr63+fXOJX+d1ft8DNazyfNPPha76/Y+7WPezKLyebPOX779um3ZTkq0x+90fwC+/lw0ULW99dVoBt24+Y/fJz8UDsEl4PxzNwk15/+21C2nJa0e/xQiL4C/D9K4RuAtzg/11KBH8Bvst3/uU12PZWduapWx55+B3cy4/4ji85+AvwI770t/+w/PkKcddw4YjPabpth2NhjVrA6iih0G5Wp0O+Prdpgr8uTx8eV8n8uebsKqGpyoEJheDMpLa4uJtc7aB/OgKmAhrSrNm81VQdKMBMhMDQnRv8JdeF50Ceup5wx/LBX6O1kJr2AzhMAGEC4xL8FUIIIYQQQgghhBBrTwLAW8hPbkaBHLbt0O7J0Bt3cs998JOb6abqXN5rgQEaGo7Q0HqeyWuvce87H8P1++/SFpv3ytwX+Muh1Ndk8hJ3jkfJ3c7C9M/z/pr/N/cTsLyLkren7MiAhe2me+D1f+MV7a6474z7Cd26F/u/K49Ps/woJe96K4S/xZdWWoLv1st8U3NNf3npCj/QltO6Geb5lA1hXnsd4Me89v2UHdz6GcB93He/+vfOB+6F139AMN25/VS7QYi7lZ+5MICJvL1H+dzTPnw+9XXOc4Ryu0ld63No+cDMhjJacFQemT/Xpz93hFKbAcJXuHhhq6d8itW6fKqa0aCCwV7JQHuJdveWMty8B6dzles/b2a5FXiOVWI3RPB3u0k7G3pcUfsgz5w7xt4CCwYUwlMX6bhT60UIIYQQQgghhBBC3FYSAN5K5uZQMPHmd1i1ezLyhne/i3vfGOX1f14xZLm0m99lpHOAr9+A7e//KAcd2gKZUdfchfvzD9Hd3ZXy+vCue4Dt/EbZ0gHmtN7+KPZfgFvf/54m4Jrk+6NMv/ga23a9hw+/HXbuf5Tce3/Cta+PrRzIvV1u/UQyfYVY1lU6njrNqF+7/i6gRAgFxjj9RC0dmyX9F7h4cYjAwqKd6nlO9+Nu7EDiQQKgt3EPo8EIkfCilVzFZjIXQyGCv/vJRWtLp7ewdnZth2T7CyGEEEIIIYQQQoj1IQHgreTVy8Sug+HXP8hb3qLduYI3/gZvdeyEyAyxVT9L/i79vm/zKtt5X8VH2aXdvaLHeO+ueyH6PZ7XTqn83Ff5ynNXCb0G97/rt/mA9q1Legd7agrZyWv8/dTYsgHTrzz3D7yKhd8se4wPOyxw8+8YH1/uHbfPv936CZh2sCtdNrTpnvTTgQtxN7p5md62w1Tv2YPT6Vx47anmsPssl1OXBb7tYlcu4D68P/U8Tw0TyCR+JO4avY3VNJ5NNwWE2DRik7RVV9OmWXs8nctt+3E697C/tpmzm21QEkIIIYQQQgghhBB3FAkAbylRXvu/3+DWG6zk/PtHFxrv/kLe+jsf5L77Eht28tbyvbwlPo0w5PCW3/0wpnuj/Ohv/5qfJTavxtcGmfj719j29kL2fcSi3buse53vxf5muDEzxv/UTqk89AX+cmiA6X96De618t6ktXqXlJPP7x89RIn1Hl4NXOLPv6YtoBEY5PlrP+F+x+/x7hz4QWBMMw315vGVa2FgO7/5HwrjU1bH3fur/EHxr7LcisdCCCGEEEIIIYQQQgghhBDi7iMB4K3muo8bV+bgbb/Njg9/kDdtA6L/j9j0F/nhF3r5wVAvPxj6c2589W94PQq80cp9zsM8+LZ7uPV3X+JH4Z9oj5il15gc+r+Ebt2D7QP7+d2U6CQ8YP0ov79X+yrnkbdb+HD+O9jGDWb/zz+kvinJV/7v93iN5LV6Vfdsf2/8WPuo/y/NfOLEp+g+Vc0HfmkbN65+Ac+5K8tm/6pe40v/9xqvbbuHbbe+x9dHw9oC6W17kPctuqaP8vul6lTVOz/SzJnuLjy1+dp3Zu21L3yZb74K9757H/+19RB/sPej/P7jh/jEJ+v5jdfDGVyrEEIIIYQQQgghhBBCCCGEuJtIAHgL+tl3B/jhCz+Ahwqx/MERct77DnjtB/zs1aTXaz/hnl//jzz0B39IjgVe/9Zf8MPpf9QeanW+P8ozX7sB295B6aHHUgK19//ao3zgscWv9/3Go+RagB/+A5PfT3qD1tcuM3sTtu36dcqSDrzt7e+JH6uQd7/zF9lu+gk/mLnCX372OMf7vsqrycdYzuW/YfYmvBp4lr/KNIr6ZgvvS3NNH/itX9OWXENX6T3x53zlxRuw81088tijfOBhK/z9KOcnX9YWFkIIIYQQQgghhBBCCCGEEHe5N+zcufPn2o1CtX37dkymB7WbN8SuXb/ItWv/ot2c4g0P/TYPlBRyn0ldCfbnyo/5+c+AN97DGw3xbbE5XvnKX/Bv//pjzbuFEEuJRl/mxo0bKdseeOBBcnK2z/998+YNXnlFgvBCCCGEEEIIIYQQQgghRKbCL72C5aEHtJtXZfv27Yue6d/tJAC8jM0eAJ5nsGLY9T7e/I5f4E3xTT//0Rw//sdpXr8e1RQWQqxEAsBCCCGEEEIIIYQQQgghxNqTAPDGkADwMrZMAFgIsaYkACyEEEIIIYQQQgghhBBCrD0JAG8MWQNYCCGEuMtZXV5GfD58A62UGLV77x5SD0IIIYQQQgghhBBCiDuBBICFEOKuUUT7oA+fL+k12E6Rtpi465Q57BgAzA6K87V77x5SD0IXlxefz4fXpd2x1bjwyr8HQgghhBBCCCGEEHcUCQALIcSmkiZI6/PhGxmgx9NEmWNj0xIdrk4GRu6EAIdYznggiAIQCTB1Vbv37iH1oM9tHx9yiqjv7GNwJHmsHKSvs57CVQ6Vt/3ahBBCCCGEEEIIIYRYBQkACyHEVmAwY3OU0uA5h6ciV7s3Q5dp2+/E6XTidJ7GH9XuXyzHasVs0G4Vd5q53kb2OJ04q08xGdPuvXtIPehzW8cHYxWdnz9KeZ4FU/I5GExY8so55m1hNUnct/XahBBCCCGEEEIIIYRYJQkACyHEZhT1c9qZCNY6cXeNEggrgBnHwQZcVu0bhBDi7mGsKSHPAEpogq4nH58fK5/smiCkAJZcSh3adwkhhBBCCCGEEEIIcXd4w86dO3+u3ShU27dvx2R6ULt5Q+za9Ytcu/Yv2s1CiA0Qjb7MjRs3UrY98MCD5ORsn//75s0bvPLKyyll1kYR7YNHKcDP6f1tXE7eZSyh/dwRCswQnnJT2xFYeFd9JweL87CY1L+VSJCJ88c5e/nmwvtTLPM5Li++SnvyljSCjDob6Y3/ZXSU4aqpotC+kI2nRMMEp/ppPptydP1yiqg/dpDipGNHQ36Gz3YwHEhK0zQ6qGqqp7LANp+5p0RDBIbP0jYcr6uidgaPFnB99Cn8ue3szTOBEmTU7SZYdY4ju82ghJnqqqXjcqIurMz0VzO8ox3XfB0rRIITdLvPcmX+FFx4fZXYg6M43VeoaqmnqsCGCSAawn/xDG2XZhOFQWe7lTV1UlWYVDYaYnb8Au4LV7RFMywb7wPxMhD/4YG2PyRkUr8k6mwH/tN1TDhOcKjUHi+vEJkZpaPtAsnNlrF4vwyOOmlMdDxYti+veT3ovTajQ+0HDltqlmrCUp+zHD31oKv/ZiiL8SHjvqODtamPc6UWwhNPUXsm9b5q6vNRagkzUVfLmbmUXcvTe23zbbGP3kgL9VUF2NQbnnBgnFr3haT3rd/4oHf8VY9rx6LtlGn6Y2b3kBBCCCGEEEIIIUTmwi+9guWhB7SbV2X79u2Lnunf7SQAvIzb2WEee+wxnnvuOe1mIcQGSHfvb4oAcFLQg9AYzsNnAajqHORgXnL0KkEhONpIY2+6CMgyn6M3CJIugJYkXYAmY7kuvJ5K7OmCZ8FRnIkIWFJwPJ2Iv4vqtsn5ADDhMAaLhcRhI6EQRptt/m9lpp89zcPzdRGNRDCZFx98vhwsBHhCfqZNBexeVDzM1PFaOuJry+ppt6rOEQ7mpa2E1ECbrrJp2i1NAAh01C8L/ScajWIyLb6+qP80+9sWfcLK9AQ+16sedF6byztCZdrOG7fU5yxHTz3o6r8Z0js+6Ok7elhdeL3q2BANTnCxv58pKmlwlbHbZsruuHqvbYX6DU8dpzZxw6/b+JCm/ybRjr/L9klNf8z8HhJCCCGEEEIIIYTInASAN4ZMAS2EEFvInH+OKIDZQhFgrOrkQJ4JIjOMdtXNT4PaNTpDBAP2kgbKtAdZSW/j/HFOxxcKDo4uTEetvlIf/iuxCDMT5zmdNBVr10QIBbA4KsluJtZ8WlrUAI8SDixc3+NP0jUaIJyUuVjU4lIDTJEAQyeTysXPwVxwgJakkzBZLCgz53m8y08UMNtsEBzlqacmCAMGSy6FC8Uxmc0oYf/8seu6/UQAQ14ZTdrpuG0F7DYrhP1DHH/ciXOfm7GgAljIjc9Jq6/dXBTnGUCZYShlqttRAsmVoLts5mtC661fQA2QRgIMHVfP43i8rMlenFK362N96iEho2sr81CiRicZi7fxvrqTDAUiAESmT+PUG/zNkq7+uxKd40M2fScjc72424aYiYLJXsqhE0/z9Im97LZBcOy0/uAv+q8twWQ2p+0PFkfZ4r6+5uND5uOvsaaTMrsBlBATXU/Ol61zTxBKOp5Kzz0khBBCCCGEEEIIITYbCQALIcQWVlZox0CE6a5meicXMkYne5sZCihgspK/KAKx1i5zqraa5jOXuHxtYWrSyTNXmQMwGslJLp6pokryLWpWWneje+H6bl5jstdNrTsRhqmg3GECwkycdHPhSlK5M4fpD0TV4EpJUqRLCTJ55hI3J+e4Dmr2XXcvs7MxYgDbDGxbKE10Zog9tW3zx54bb1PrFwt2bYRdCTPd/QS1bRe4ehOIBTgbUN9nNKo1oa/d5ohFAYOVgrKFSNm1yV7ctW5NMEpP2UxlUb+AEp6iq87Nhatqn7h6ZpKgsrhu18d61MOCjK7NasQERAL9nI23cWzuChdOTxMCzJa8hQOuM139d01l13cyFQsFCV7XRuxN7LDbcRg1m9dTZHrl/pCw5uND5uPvgYI8DEQJ9B7mzOS1+bJzgRi35v+a37qu95AQQgghhBBCCCGEWF8SABZCiK0kaTbOyxSSazEAZnaf8OHzpb4OOdR9lmyy63QyFtbQ3jPASMo5VLLSZKrLyjPHA2jjTC6bcGbBaADCs0ymmWn6UlAN8RrNuxY2zgVImRk7eIXlZqm+Ppu8lqdqMhTWblIpc0yNa9bwjWcWqtMD6223cU72ThPBhL38KD7fCAM9Hpoq8lM/Q3fZTGVRv8DclQ5Nu4WJKcl/r6f1qIcFGV1bRFEzXB0HcBWqAU6jtRDXsWJsgBJbov+sA139d01l13cyYiyh/XNHKbebUMJ++o8/SddYkChgyttLu8elfce6CU6dWrk/JKz5+JDp+FuEdQfAdYLjKTuWsL73kBBCCCGEEEIIIYRYXxIAFkKILSS/0I4J4PocsA3DovSy26ColXPH9lJgMyfHp9eMcmvZ6G8ShYB20zoyG7K9Wv3tFps8RfU+N91jfoJhBbPNQemhE/hGvLhysy+rz8bW72qtXz1kaLiZiRBgyqPy2Dl8Ph/PnDtGZZ4JlCDj/Ze079hQ2fffbKx93yk7pk4trYTG2FPbxvDVa0yebaTWPUZIAYO9jM4q7bu2Ap3jg97xV1FQJyFf2W2/h4QQQgghhBBCCCFE1iQALIQQW0Wui4MFZkBhxn8RuMzcddTpVeu061QuvBrXea7OivICzIASmqAraa1Ip3OUoLawHuGYuoZlbol2j0YERS1IfZqZZCvsOwC4PndVu2tVKnItgIL+RM4s2y0WYPxsG421+3Huc9MfiIDBTpkrTZRLT9kV3Z76XYp5R+qc5rkV5dhNKZsWrGk96FTUym4bKNEI0flsUIVoyE9/m5veNBmxeuiqhzSy7796rF/fsRpNgEJw8mzK9ljgLJNBBTBgtm/FKKW+8SHz8fcmsRhgMGPVtEWuy0Ga5lHdzntICCGEEEIIIYQQQmRNAsBCCLHJGa0OSlwe+jyV2A1AxM/oBTUrdnwmBFgo9XTiKln7uZ5vxtTPsRd7qMlPv5KvxajmnSk3Z5mMr0G5q8RFe0/J6qaAnvSr62haShn0NlERn0YXoLCmnb75KV6HCQQVwEa5x0NNolxOPjXtfRx0mECZwX8x00zixYzmIhxWdVFRo7UEV+cA5TYgGmAsi0ROXe1W1EpPXydNFUXsSjRBLIB/eo4oYDCYsyubsfWv34zMT6lcRVV8gdeSei/thxwsuqp1qQd9ikodmIkyO9zBqTZ3PCi3h/2H2xgOrKKu9NRD3Fr334SVx4f17jsGrMX1lMw3MuwqqafYagAUIsHso+wrX9v60TM+ZD7+BghcV9dcLm5toihnoR08lfbF2cOb4B4SQgghhBBCCCGEENl7w86dO3+u3ShU27dv58aNG9rNG+Kxxx7jueee027WxWh9Ew8X3Ms7b73G58d+qt0thFhCunv/gQceJCdn+/zfN2/e4JVXXk4pszaKaB88SsFSmXzRGYbamrkwH9coonXgKLuXehYf9XN6fxuXAVxefJXLhWSDjDobSUk8zW+h70QxluRtkFLW6vLiTRdASEg+B51yXd70wQmA4CjORBpcrgtvIkC+iEJw1E1j7ywUtTN4tADT/HtdeH2V2LV/J8552TqL4O+qo21+8U/NezWlU+lot8Q5a8tA/NoaaUwsaKyn7LLXRmp/yLR+WThucFSbxRzv22RSP2kYq+gcOEjeonOIEImaMScfd73qQce1OVr68BQvvnMAUCKE/EMcPpVF9FVPPSx7bdr+m4UMxgddfUcHY0k7546o2a/pKMFR9ixKo9chk2vT0R/Wa3zQNf4udU2RIKFtdmzZ3kNCCCGEEEIIIYQQOoRfegXLQw9oN69Kumf6dzvJAL5DGK1v4gOVJp78xE7O9tn5wv96F4M9v0bzH9l4xP4zbXEhxJaiEA0H8Y924dyfHPwFuMypOjf90yEi89PMrqGrHXScnya0zMHnehvpnUr9/Gh4honubqZXOb3sbG8jT5weYyYcZeHwCpHQNP29F5ML0ug+z3QoklROPY+x009kFWBaWvzz3asJnulot8ttdI/6NW2gJF1bUhBGT1k9NrR+lxAbpq17glDSAqbRkJ9+dx1T15MLrmM96BDoHiYQVf9bUTSNbDBj232IQU9Z6vZM6KmHtNai/8ZlMD6sV9+JTbZRd3IIv+a4SjTMzEQ3be5VBH/J8NrWTebjg67x92oHT3VPE4r3S4gS8vfjrhtiUdfZBPeQEEIIIYQQQgghhMieZAAv43b+YkBXBvD7zPz3/7pzcUYHAK/xlU98j85varevofc309f6GObgF/nYkT5C2v13kryP8Mmm/TxsNQIv8kXnx4l2DFCdG+P5z1bzqS9r36Dfw/+lj0/+ezMvfuFjfOzP7+ja3LTS3fsblwEsNpUlM/yEWJ7LO0KlXSHQXYd7XJ2aNyG/qYdjpTYMGWWDroL0XyGEEEIIIYQQQgixyUgG8MaQDOA7gflNS0zRB7wa5evrGfwFMBmWnnrwjvIwzX9cy8NWePGrPp79RogoD2Lapi23OibD3VGbQghx53LhiM95vG2HY2ENVcDqKKHQblb/3bw+t37BXyGEEEIIIYQQQgghxF1LMoCXcTt/MaArA/i3H2Lwv/wCRu12QPn2NT7a+mPt5g3wXmo/1ciHDM+zr7lPu3NrevTjDPzJIxi+1sm+Exm2jdiS0t37kgF8l5IMSpGVfFr6TrDUEsAAKGGmumrpWM8IsPRfIYQQQgghhBBCCLHJSAbwxpAM4DvBO96cNvgLPyX4jz/hg/vvx/3HJt6j3b2uzNjeYcF4JyWzWh/ECPzg+xL8FUIIsZyrdDx1mlF/iIh2/V8lQigwxukn1jn4K4QQQgghhBBCCCGEuGtJBvAybucvBnRlAP/RL/Klyvu1W1PEvhZk/399Xbt5HT3GJy828/BLX8TZeIdkAP/RZ/H9h3fy4v9y8rH/rt0p7iTp7n3JABZCCCGEEEIIIYQQQgghVkcygDeGBICXcTs7zJoGgJVX+eJ/+Rc+/0/aHcurO+fDaQ3hazjMOc17bfU99JRbmBmspvnp/XzW9xF2xqdGfuz4MzS/f3FOckrgNO8jfPzJPTxsNWN4Uzwj6msjfPbTX2RG875UZh6rb6X6UTuW++PpxUqEmS910vzn31L/Nr6XfU/W4XzYhvkt8bf9OELoBe3xF4LU+/57lD+u38PDVvW8lcgMX/zTNga+HQNq+azvI7xz/n1xQTW4rV7vD/ii82MshLqNvHfvx6ireBibWT3PWPhb+D4b4uFPOXln/L1p/dFn8f2Hnbzw3/bxyS/Htxkfoa6tlt/+lYWs6lj4eQZqP4Uv+b1iTaS79yUALIQQQgghhBBCCCGEEEKsjgSAN4ZMAX0H+MDb3qzdlCL2zZd0B38BBr46g4KN36qwafbY+Mhv2iD2XZ57OqbZBy8+78P3pecJ/Rh46Vv4vuTD9yUfz307XiCvls9+qpZH3gbBaXXf8/9kwPZoLZ/q3LfEdNYAedR6+2guz8OsBHk+ftzn/1HBaDGrRYwf4uPdp6h+1IYh/ALPfkk9l5moUT2+t5Y87WHvfQ+fOr4P2w//Ft+XfDz7jTCY89jX+nGcAHyL577kw/ftCACRb6uf6/tKPOCcRt4ffYq2mkewvSnMCxM+fF96lu/++FfY98kPoa3NlT1Ms/fjOHNN/OBr6mc/+7UQykMWllteUgghhBBCCCGEEEIIIYQQQtx9JAB8B7il/AQlEmXmaxHCP9XsVF7l2f+R3dTPsae/TlABy/v28d7kHb+5j/e+DWLf+eu02aehiQHO/dnzhBXg1SDn/uwc5/7sHF/8GoCN2vrf452E8H28muZPq/s+deQJvC/EMOR9iMO/qT2i6uE//mM+YjcQ+ZqX6oPNfCp+3E+11HL402q29GNP1fLIQwov/q9m9jV8Eu+fnePcn32K5oPVeL8WwWD/Pf7ocU2I+W02+KuPU/sJL+f+7BzeTzSqmb/Gd/HYfoAX+OKfneNcUM32fDmofu65L7yQepyEX67lcPk7MURewOs6zCfPnOPcn3n5ZMMTeL8ZQ/eyyI9+iPdaIPaNPj4Wry/vicNU136SEW1ZIYQQQgghhBBCCCGEEEIIcVeTAPAd4PnT/8xH/1OIP/4fP4Y3pe7LNvtX9QzPfScGlvfye+9f2Prw77wXCxG+9VcZTlGd7Jc/wiN2A8rMs5xLmes5xrNf/S4xLNgKkrcnPIbzNy3w0vN89sSzLM47BvgIH3yPEV56gYH/rp1IOsazn3mOFzGQV7A/dder3+Z/p5SP8cVvh1AwYHxg6XzkpRg/+B7eaVCY+T9/yrMpJxrj2c/8LaHkTZkIvUwUML7zEZwPJW1/KYKakyyEEEIIIYQQQgghhBBCCCGESgLAd5LdbyE+EbJqFdm/Cb6/+S4xzLzr3z8c3/IYzveYYe5vGfiapnAm3vkgJsDwnlp8Pl/qq+lhjMDOtz+mfRfwTsz3g/L977JE3i3wIKa3LFMm9iKRV4GHLDySvP2lEM8m/w1wPcot4EHLb2n3rOi33r4TiPDPl9OEqWO3ULTbVvJPA3zxK2EU88PU9fsY6P4ktaW2ZabKFkIIIYQQQgghhBBCCCGEEHcrCQDfQR62Gbh1/UeE43HH1WX/xn3Zx7deAnPeh3gYoPyDvOt+hZmvDujPZE0S+btn59cGXvR6/kVt8Xm3lDRB1U1JQXlJuy1bMZ7901qq67z4vhEC68N8pKmHga406xkLIYQQQgghhBBCCCGEEEKIu5oEgO8gL/zpP7O/9l/41qtrk/2reoEBfxgeei/Ofw8fefRdGGPf5bmnswzERqLqdMY/Cc2vDax9DUykCy1HuaWA0fae1PWIU7xM9MdgePu71GC1ljGeRRx+kee1+9aQ8lMFsGD7oHYP8MtGTNptGYrNPcu5Txym+kArA38Xw/CrH+HwH0kesBCrYXV5GfH58A20UiK3E1WeQXw+HwOtJdpd4i7l8g7Q01So3Sw2E2MJrQMDeCpytXuEEEIIIYQQQgghxF1KAsB3nPv4pe1rlP0bF7r0dUIYedejzfx/eQZi3/lrfNpCSzFrplv+xnO8+BIY8j5Ena70VR9/OxMDyyM88UdLvfGLTH83Bg89TPWiMkY+9NRjvBOF4AsZn31Wnv/GPxPDwLs+WKfJ0DXzkYb/D0vKtgwYzZiTA1Oxb/HMs98lBpjMv5K0QwihV5nDjgHA7KA4X7t3C3J58fl8eF3aHZlwUexQf6Ji3l1JjXa32BRKWnoYTCydMNBJjSbmV98zgm/Ei2sNYoE1nYNU2s2YjHforyOMNXSO+PD11Gv3bC1WK+ZtZhyHjtG+qX7J4sLr8+EbbKdIu0sIIYQQQgghhBBCrCsJAN9pHn0zFtYq+zfunwZ4fkbB+L5HsBsifOuvntOWSOPrhF4CzA9TfbyOuqZOPv6HAC/w2adfIGKw4Tz9DD3HG6n7z3XU/edGPtnRw0D/x1FXAH6Mjw/48A1/ltpfBojxxVN9vBAx8M7/0Mkz3Z+kMfG+rj56/kR9l+/T6cp8nM7+ARrfbybytXO0DWaZvZypsXM8+w8Khl928qn+Tj4+fw59VL/lB4RTCmuvM41/9zG8FweS6urjfPaJhzES5ltf+pa2tLiT5BRR39nH4MjCWtkjg3101suj9LUyHgiq63JHAkxd1e692/QyFYgCEJke5YJ29zpyuDoZGMk2cH0b5ORT0eRlwOfD5xukfZlbsqi+k77BpHt4oIfWJTI1VyprrOqkodi2MJOEOY+9LS044n/mNvVRboPgeDe9s/Nvy0puUx9780xE/F1Un5rU7l4YnxLBaN8IAz2tVDmSA5BFtCddz1KvlHZPc9zBnnbNcZPoaAutXFcxeQaFmSua3p7mHDb1tc1eoLltlKBipqDBsybBfyGEEEIIIYQQQgixtUkA+A5j/PX7MKxh9q8qxsg3gygGA4a5v2Xga9r96cToO/sMMxEDtvc7cf62DaMaVyA28Uka/9THzEtge/+HcH7YibP8Md7zNnjxb57j69pDJcSe5ZNHOvH9XRje9jAf+rAT54c/xHseUnhxJr5ucOxZPln3KZ75RiipzCPY3xTmhaFPUXfiWdY5/AuE6Dvycfq+GiJ2fx6PfNiJs/y9mK8/S6f728SrIXMvfpcXXzJgKUjU1cPsfPVbPHOqEe+MtrC4UxhLWhl4+ijleRZMhoXtBpOFvPKGpQMBQpe53kb2OJ04q08xuf6Dw6Y37N6P0+lMH/BbRzlWK+akfr5p5RTh8vQw+PQJDpXaMWv3a1R4Bjlanoclae5/g9nG7kMevJooXSZlywrtGIgS6H4c5z43U2HAYqUQILeJllILSnCcxtVGf/NbaCm1QMRPf0eavlDUQt/n4+PT/EYDZttuDrZ7cFlTSmfOWkXnucXHNdkK1OMmV5nOtlisjIOFFojOMnkh6ebfqtc224v74gyKwU5Zw1b5JYUQQgghhBBCCCGEWC9v2Llz58+1G4Vq+/bt3LhxQ7t5Qzz22GM891wmmbap3nMoh4f/z801DgCLNWOso+cZJ7Z/+CLOI33avao/+iy+/7CTF/7bPj75Ze1OsRHS3fsPPPAgOTnb5/++efMGr7zyckqZNWN14fVWYjeAEg4wfvE8vZPX1F2FFVQdKMM4dJhTl7VvFHc9lxdfpZ3gqJPGXu3OzauofZCjBaZNf975rQOc2G0GFML+K0Ryi8kzRfGf3k+b5n40VnjoO+TARITAUBfuC1chJ5+ao0fY6zCDMkN/dTPDsczL0j7CwTyFQHcd7qkC2vuOUGAKMursxtj3GUrNQUYbG+mdSz0XvWo6R9ibpxA4X4v7UppfRhhLaD93ELN/iP7+S1y9CdaSJlobSrEZIDzlprYjoH2XRhHtg0cpMCycc5lnkAaHCSU0QXdHP5PXbmK0FlLV0MBehxllZog9zWq2rp62SMdY08nA3jwiE09ReyYpYL7Fr83lHaHSvkzbbSgXXl8l9qif0/vbWOHUhRBCCCGEEEIIcZcIv/QKloce0G5elXTP9O92EgBexu3sMNkGgMXmZny8k4H9eUS+0krtn6afvvmx48/Q/P4oz32ils5vaPeKjZDu3t/IAPD8w//wNCcbT3FlpWf4RgdVTfVUFtjmsyiVaIjA8FnahuOBiqJ2Bo8WcH30Kfy57ezNM4ESZNTtJlh1jiO7zaCEmeqqpeNyIpBoZaa/muEd7biKE5mJCpHgBN3us0nnFX/IHxzF6b5CVUs9VQXxaWqjIfwXz9B2KTUjsai+k4PzxwQlEmTi/HHOXr6ZUg6grKmTqsKkstEQs+MXcF+4oi2aYdl4cCYp05KlAhQuL77KHfhP1zHhiGfjGVDrYWaUjrYLBJLbx+hQr99hS8ncnrfU56wkkzYmOQC8j95IC/VVBdiWard42bSCozjTRGL1tBs5RdQfO0ixfSGLPRryM3y2g+FAbPnPnxdk1NlI8plk1sYL8pt6OFZqg+Aoe9Jcky75LfQ0GJk808FwID/ej9IH5lxeH5V2hdCYm8Nnk/t/Pq0DJ9htVpjp30PzcOZlz+zo4Vy5LWk/KMFROoKFHCs1ExxtpHG10V9HC32eYiyhMZyHz2r3Lsva1Me5UsuS/SdZblMfnym1EPWfZn/bZaCE9sEjFBhmGKpuJjkpd6EekvqDjrZIp77HR7kl3Welt2WurczDYIMDUxbtt1rq+GDHoh38tOOervFMx/ird4wSQgghhBBCCCHEbSEB4I0hU0ALsVGMH+KPfycPA2G++5X0wV94mEfsRng1xAsS/L1LFVKWp2Z+BUYzCf6W0H7Ow8HdCw/SAQwmGwUHPQy0lySXZkdhC5V58SfjBjvFTZ007I5PMGqwUFhZlVTagLXyHMdSpqU1YLaX09KeXC5um5XWcx4OJoK/ACYbBYdaaMlfKFbVmW6qWzvlRz+PVzO/alXnCA2lmrImG469B9BOcqqnrD4mchvOcbQ8EXxArYe8vbS2pM7F7fK0q9efLvibLZ1tDLCj+Byeg4ngL8u3W4b0tBu5LryJaXSTztlkK+Cg60BySV30t3ERlYU2DIDBXkxrUj/MytUODte2qQHsZVVgtwJKkMnkgG5OPjXtLhxm1PvLUaSr7NzZwwzNRNR1q4FoaJrefiOuUgvKzMXVB38BR1kuFiA8e0m7K2PRSFC7KZWxQp1+WZlhvCMRFjRjNADcIrKoeq8SmFOAHVgTt1zGbZFGmYdiG0RnJzMK/ibb9Nc2PsZsFLDl4VpiaeH14PKOxMeHFQY/3eNZ5uOvrjFKCCGEEEIIIYQQ4g4nAWAh1txjfLxvgJ6uU3z8P9dR95/raDz+WQYuNPKwWSH85QE6U9ZRruVU7yka/3Mjp3o/ziMPKbz4131I/vfdyoHFDDBHMIP4S1GLiwIzEAkwdLIOp9OJ8/En6ZoIoQDmggO0OBbKmywWlJnzPN7lJwqYbWpm5FNPTRAGDJZcdT3RRHmzGSXsnz92XbefCGDIK6NJ+zzdVsBus0LYP8Txx50497kZCyqAhdxS9SSMVZ0cyDNBZIbRrvj5Op10jc4QwYC9pIGy+QO6KM4zgDLD0JOPz5d9smuUQFgbGNFT9jJt+9X9Tudp/BkszG0ymdQ6Pq4e+3i8fk324oX6KvNQYjdANMhY/Nr21Z1kKBABIDJ9GmcW2b9625hM2623cb6e5l+n1X6hpa/d8mlpWZjCfL7840/SNRpgvjmSPv90vBGCo5rzScn+1dPGCZeZuBpGAZTgFKeuavevF4sa8ItcZxY147Gsycvg0yfYm/QDCZM5T2dZuNBcra5b7XSy//A4joZSLMoMF9uG4yVXp9BqASIEr+gPJlc5LECUa1fSrBucJL+hEocJIv6LSQHYWa5HAIODvZ4aCq1q9DJnVwmu9h4OOFYILOpQU5KLiTBXh8a1u5a0Va4NLuO/pgBW7NpY6jox1nRSZjeAEmKi68n5e7POPUFIUzar8SyD8VffGCWEEEIIIYQQQghx55MAsBBr7kVeDEYx2d7FIx924vywkw8V2DC8MsOzf9ZO43/ThnajcP97+dCHP8R7t8d48UudfPzPtY9MhUingnKHCQgzcdLNhUTA5uY1Js8cpj8QVYOvJUmRWiXI5JlL3Jyc4zoAYaa6e5mdjRED2GZg20JpojND7Kltmz/23HgbQwE1qGvXPk1Xwkx3P0Ft2wWu3gRiAc4G1PcZjTkAlBXaMRBhuquZ3smFANNkb7N6XJOV/PmI6hyxKGCwUlC2EBG4NtmLu9adMi2wvrL6KeEpuurcXLiqTiN69cwkQUVTX1YjJiAS6Ods/Npic1e4cHqaEGC2qAE8fbJoY73tlgFd7VZUSb5Fnfa1u9G9UP7mNSZ73dS6s22N7Nr4ckcte5zO1U//nI1YlJz6TgYGPDSU2jGBGpgfCiwOtOspG5ff0kCxRWHmYhvDS8XAdSlkhxkgwvX0M2ovqaR9gFILRPy9uJeLqxprOBDPkB09kxyRD9A9PqMGAR17OXbuGXw+H09/7giVybMKrJa1nsI8A8rMFB0Z/iBgy1xb3LVIBDBgtGj3rI8DBXkYiBLoPcyZ+Hr1AHOBGLdSSmY3nmUy/uoao4QQQgghhBBCCCHuAhIAFmLNhXjm1GGqq/YsZLFV7mFfbTPeL31LDbKleIbWffFye6r52J89n6aMEOnEMwfDs0ymLrELwKWgGuI1mnctbJwLkDJLbPAKZ9K8N+H67AXtJiZDYe0mlTLH1LhmncV4lqe6DmYhuRYDYGb3CR8+X+rrkEPdZ5mP7Y1zsneaCCbs5Ufx+UYY6PHQVJFuHl89ZfWbu9LBZMqNGSamJP8NRJR4gOcArkI1gGG0FuI6VowNUGJL1Nuysmhjve22Ip3tlmeOB8LHNXW2WuvbxuvCXs7R8jzMBlAiM4ydflwNzAe1nUdnWdR1YhuK1amfT0Ya6BmMt8nIAJ01udrSGdqGIfkXIBkqbOqhocCMEhylum35DNmiljLyDBC+cnFR0Do23Iz7/DShSNI1KxFC/lGmQwC3UFIjiroVuYqxEWV2cvE9ks5WuraEwOJ5ptdREdYdANcJLhcch6zHs5XHX51jlBBCCCGEEEIIIcRdQALAQgixqSQebFuxV2j3LUUhoN20jsyGbKcr1R9cik2eonqfm+4xP8GwgtnmoPTQCXwjXlyaGJeesutiuJmJEGDKo/LYOXw+H8+cO6auuawEGe/PYE7vJa2+jTey3QCUW2sfhLrtbZyxCEoiQBUNMtHtZk91M2cvqz+QMDp2qEHycEBn2YR8WhqKsUQD9J+EYw3FC+s9G8zk7W2iXjtF+zopax/gWKkNgmO0rZTdbXWx12FS18ftTp9+O3vpFIerk35Ataeaw21+4inRzOrMTE5hrKHSYYLwVTKZ/XlLXVsSq3EDF/9NUBTUye4zsfrxLFV2Y5QQQgghhBBCCCHEnUwCwEIIsalcYiaoAAZyy+q1OzXigSNLbtpgT4V9BwDX59IHI7JVkWsBFPQntF5m7jrq9J912rVeF16LZuqNBRg/20Zj7X6c+9z0ByJgsFPmqtIU1Fl2rRW1stsGSjRCdD47TSEa8tPf5qY3TcbbytaujTes3cIx1FNepwVIb2cbZ2yYYBhAITjZwZnx1HCXq8AGKIRnr+gsqypqPUKxJUrg4kkulRZiN0A00I3T6cQ9FQZs5GUx1fdCW5vZsdJ0uUYH9d4RGgrM6pTjjWcJrBDzr2gowW6A8FTvogzZ5eS6DlJgBiV4hdWsdGytKSTPoDAz1c2yd8wWvLZk+RYzECUS1O5ZDzeJxdQfHlg1Y1Suy0HqprUbz1LpHKOEEEIIIYQQQggh7gISABZCiE3mwqi65qfBVs5IXzs1RQvTYe4qqqDJ20NrEcAwgaAC2Cj3eKiJTztMTj417X0cjGej+S/qiEZoGM1FOKxqNpnRWoKrc4ByGxANMJZFQuv4TAiwUOrpxFWywnycRa309HXSVFHELnUJYYgF8E/PqfVjMGdXdp0UlTowE2V2uINTbe540GEP+w+3MbxS9GhJ2bVxarsVUuPZwHab9Kvrc1pKGfQ2UZE4Z6Cwpp0+jyulOMDNmHr+9mIPNfmJBtTIso3zm3oY8fkY8S7+3PV06WoQBQP2snbaa+LTVOfkU+NR15MlGmA0HvHTU5aiVg7tNhMNXMR9KQZmAwbgVlTNv7SaV5f9eWUuDJixJ7XbIjlltHrbKbcbiPi72d+cwXTKuU1q9m00wGgmv4bI2YWjpIpW7yCfqbRjUIKM964mRJpPzW4bRGeZvLDM/bglry1ZPg6rAbjO3DIZxSWtA+oUyQOtlKyqywQIXFfX7i1ubaIoZ2F88lTaSZ13ILvxLBO6xqgk8/Uw2EnWM6cLIYQQQgghhBBCbEJv2Llz58+1G4Vq+/bt3LhxQ7tZCHGHS3fvP/DAg+TkbJ//++bNG7zyysspZdZSSUsfDcUWzcPzhCj+0/tpuwzkuvB6KrGnLagQHHXT2DsLRe0MHi3AFBzF2dgLuPD6KrFr/476Ob2/jcsuL75Ku/aAcRH8XXW0zS/KqHmvpnSqIloHjrI7fawOko+ROGdtGYhfWyONiQWN9ZRd9toAgow6G+lloWxwVJs9VkT74FEKWDhfR0sfnmJLcqEFSoSQf4jDp7KIvmbaxqx0bdp2S2NRP5nfkXm7Abkub5rgT9yiY6vr2fadKGZx7SW1hZ42nhdvJxNAhOnj1ZzSm1yYbNlzUCX3FZd3hMq0Dbe4LTIrG2+HbQHO17q5FAOs9fScK8eW/BZlhv7qZl2ZqPPyWxk4sRtzZJrj1afSZsoWtQ9yVK3UJWnvmarOEQ7mGQhPPEXtUguPL1W/Spip7kY6kvvuUmWTJJ+DsaaTgb15xKaPU71MJ9iK15Yi3n7GmSH2LBm8dtDS5yExXIWn3NR2rGJS5qXu30iQ0DY7tqRxMpvxbPG1Lh5/9Y5Rqvi/XfG/Fn+OEEIIIYQQQggh1kP4pVewPPSAdvOqpHumf7eTDGAhhNiEJjtqeeL0GIFQhPnZhAElEsI/2q0GfwFme2l0n2daUy4anmHs9BMLD9LXhEIkNE2/e4Ug4rIuc6rOTf90iEjyCadzuY3uUT+hlIJK0rUlBfv0lF0nge5hAlH1v5X5RV3jDGZsuw8x6MliXl49beyfYDoQIpLy+RvcbsBsbyNPnB5jJhxNOuf4efReTCkLwNUOOs5Pa9pPI6s2vszE1TAKoASnVhf8zUKvu21RnUXDM4ydXNwWmZQtaj3EbnMUf+9JNfgLMHeWM0MzC++Lhpjqbssu+Atw9RRTQQXMDvZWrCo1dEF+K5V5hswzZAFQUCIhAhPnOf5EbWqANAs1hXkYlBkmzqxxJ9gE15bMdbBAnYlgcqngL0CA7ot+4sMVFms86zxbVzt4qnuaUOKARAn5+3HXDXE9taS+8UwXfWOUqpfR6fjKxdEZ/FPa/UIIIYQQQgghhBBbl2QAL0N+MSDE3Sndvb/RGcC33ZKZV2IpaganQqC7Dvf4zZR9+U09HCu1YUibhbaJlLQzeKQAQ+A8e9xZZCuLO0MiozPqp6u2jTWMT94e8azYbYFu9rvHtXvvGMaqTgYO5kFwlD0rDtwltA8eocAEkemTVJ9aZr5oIYQQQgghhBBCiDUkGcAbQzKAhRBCiFVz4YjPabpth2NhjVrA6iih0G5Wp0O+Prdpgr8uTx8eV8n8uebsKqGpyoEJheDMpLa4uJtc7aB/OgKmAhrSrNm81VQdKMBMhMDQnRv8JdeF50Ceup5wx/LBX6O1kJr2AzhMAGEC4xL8FUIIIYQQQgghhLjTSAbwMuQXA0LcndLd+5IBLJaXT0vfifk1NdNSwkx11dKxSSLALq+PtMsFh6c4XtuRdu1XcXdJrEsc8XdR3SY/Cti0civwHDuEw7x4bWmt1DWOFcJT3dR2SNsKIYQQQgghhBBi40gG8MaQDGAhhBBi1a7S8dRpRv3a9XcBJUIoMMbpJzZP8Bfg4sUhAguLdqrnOd2Pu1GCv0LV27iH0WCESHjRSq5iM5mLoRDB3/3kssHfBQtrZ0vwVwghhBBCCCGEEOLOJBnAy5BfDAhxd0p37991GcBCCCGEEEIIIYQQQgghxBqTDOCNIRnAQgghhBBCCCGEEEIIIYQQQghxh5AAsBBCCCGEEEIIIYQQQgghhBBC3CEkACyEEEIIIYQQQgghhBBCCCGEEHcICQALIYQQQgghhBBCCCGEEEIIIcQdQgLAQgghhBBCCLEsF16fj8H2Iu0OIYQQQgghhBBCiE1HAsBCCCGEEEIIIYQQQgghhBBCCHGHkACwEELchawuLyM+H76BVkqM2r3ZW6/jblVVnkF8Ph8DrSXaXeIu5fIO0NNUqN0sNhNjCa0DA3gqcrV7xG0i/7aIbEnfEUIIIYQQQghxt5IAsBBC3IXKHHYMAGYHxfnavdlbr+PeNi4vPp8Pr0u7IxMuih0mAMy7K6nR7habQklLD4M+Hz6fD99AJzWamF99zwi+ES+uNYgF1nQOUmk3YzLeoVEIYw2dIz58PfXaPVuL1Yp5mxnHoWO0S8RoU7jj/m0RG2ZD+s6WG/vU6cx9g+3IhOZCCCGEEEIIced6w86dO3+u3ShU27dv58aNG9rNQog7XLp7/4EHHiQnZ/v83zdv3uCVV15OKbMWitoHOVpgIjjqpLFXu1dV4RnhkCPM2L7DnI1p92bG6vLirbRjiEzTVXeKySWO43B10lKWR2R86fNJlulxtwyXF1+lfdn2WE6VZ5CDDhOR6S6qT01qd68bve122+XkU3HwIHtL7ZiJ4j+9n7bL2kKqovpODhbnYVFj6yiREP6hM5y6NKstumJZY1UnAwfz1OBAQngKd20HASC3qY/PlJoJjrpp7F18fD3UY1mI+LuobkvTF3KKqD92kOI8C+rpKkRCfkbPnmE4oLmREmXtFkyJk1eihINT9Lad5Upy8TTHjYYCDJ/tWHzcOEdZEzVVhdgtpvm6yeQeSNTXzFA1zReSjp3mHDb9teW68HoqsRNk1N3IKps/axmfbxaMJe30HSlQ6y44inOZg+opu7Qi2gePUmCCaKCb/e7xhV3GGjoH9pJngKj/NPs1A8CK/7bEx2otJRomONVP89klBhRdXHh9lexIc35Zy2jsUz938dWptP0h0WfyEgPfcvebTiuNqcn0lM3IUv8eJ+5VQwR/Vx1tms6xEX1nybFv04r3qaif0/vbWPkKhRBCCCGEEGJthV96BctDD2g3r0q6Z/p3O8kAFkKITeRmbOUHhxajAbjFrZWLLmmut5E9TifO6jQPQ5PkWK2YU6Jjy8v0uHeLYfd+nE7nhgZ/yaLdbpucIlyeHgafPsGhUjtm7X6NCs8gR8sXAgoABrON3Yc8eDUpupmULSu0YyBKoPtxnPvcTIUBi5VCgNwmWkotKMHxVQd/yW+hpdQCET/9HWn6QlELfZ8/Svl8IBPAgNm2m4PtHlzWpLLGKjoTZZPb2GDCklfOMW8L80lu1io6zy0+rslWoB5Xm9VsLKSpZwRPQyl5SQHHzJRxsNAC0VkmkwMgW/XaZntxX5xBMdgpa8hqCoDV0Xu+ehmraG+IB3RXoqdshky7ClMyD40HCshb5iKz/bfFYLKQV36Uvpb1Sv3Mks6xL3MuXPE+s2CJ+02nTMbUBD1lV6eI1mOV2A0KwdGTi4K/bEjfWWLsE0IIIYQQQgghbjMJAAshxCYSiKgPD7dtW2HaUUUhot0mxBaT33CISocNEwph/xQzUW2JBcYKDwccJiBCYOg4TqcT5+PHGQpEAAP2MhdV8dtGT9kFO1iYmTmXppZSLEqQ8Y5sMh1T1RwoxEKUwFBH+gDEVT9zsQjBifMcf9yJ0+mkrmuCkAIY7BQecMwXNdaUkGcAJTRB15OPq9fmdPJkorwll9J48bKGKvJMqWX31Z1U68Fgp8yVOjF5VXsLpTYDREP4R7tw1+2bP/5KCZ/GmhJyTRC+0k9SXueWvrbYcDPjQQWDvQRPxaIOs66yOV89XJ4D5BkUZqb8LHPbgc6yy8vDbIJoKETUlEtpUgT4gMOOMjNDKLl4FoKjah2p9/yTdE2EULtOKQs97fbTM/bNC44uXFvSS9sflEiQifMn5/fXnRxCHfrsOMpSy2ZKz5iqp+xqlbQfYrcZIv7uVf9QJ9u+s+TYJ4QQQgghhBBC3GYSABZCiE3IbFk648RoBJQYYVhYx83rAqODqvak9UwHe2ivSM60KaJ9ML5vvkya9d/i6976fD6OFqjpO/ZKzft8XhZy4jI8LoljD9JelENRvZeBkcR7RhjorMGhfSicuKb5chl+zkqMDqpae5I+38fIYA/tVUs95jXiqGqnZ/46Rxjw1lOYfL5J9bbotcQiwkX1nfQl1d3IgJf6ohxtMVVOEfWdfSl1MdjTTlWi0nS3m6qsSXMOgz14ago1pRbkN/Uw4vMxssQ16XF1PEAo7KffXU1t2zTpYqMJB0odmFAIjZ3EfeGquvHmVS64u5iOBzcK48GNTMteCYYBE46Gp/E9c4QCEyjBAIGmFkotCsHxDnrnFs4hK44WivMMEJrCfWmJK4xN0lZdTeOZS1y9qW6amzzDqSn1LrdYF9rDbFDTJCOz40xeixcGrk2eYTb+qxAlAlBC4S4TKDOMNp+ZLxubuzJfD4a8goX+kN9KZZ4BIn66ag/T1jtJYG6J802jpjAPgzLDlDYIs8WvrXd8ligmHGUbuIr3Ks43E7kuL2V2AxF/N23T2r2p9JTN2PUA16ImchMRYGs9+fYos5Oz3AJM5rx4QR3/tqRz8xqTZ66y2lt4PegZ+/Tppbm6kTOXrsxvmbtygX6/er9lK9MxVW/Z1ch1eWkoMKMER9NMq79xfWfJsS9O77+x60H9rjGSVB9LTCme6Xcjvd/l9H7fEUIIIYQQQgixJiQALIQQm8lMJDXDylhD54iPEU9FfEMR5jQP1thmpfWch4MFtoVpOk02Cg61sOLshRvORG7DOY6W25OmKTZgzttLa0vq41mXp129pmWmBtXNWEL7OQ8Hd9tSpkk2mGwUHPQw0F6SXBqAHcXn8BwswDZfuQbM9nJa2qtSC+pQ1Zluikw75Uc/j1c7T2euC2+aqXFNtgIOug4kl9SlqnOEhlLNOZhsOPYeWBQoVhVRWWjDABjsxbSutm9d7eBwbVsG61JWYLcCSpDJs0kP2XPyqWl34TADGLA6inSVnTt7mKGZCEq8SDQ0TW+/EVepBWXmIo2rjv6CoywXCxCevaTdlbFoJDj/33PDVwgqYCn9DIPeJiryc8jJr6G1ZxB1lumLnJkDMGM0ANwiPrFAkqsE5hRgB9b4LecotWNGYWa0LX2W8nLKPBTbIDo7id4ZUDf9tY2PMRsFbHm40o2962BV57uS3CZa4uuhnm+bXD7wqKesLgHGZqOYckspAqwVDmzRa0ytcfpkzq4SXJ3F2IHw7AQBbYHbKeOxb/V2lTTRVKxOQT96Ubs3E5mPqfrKrkKui4YyO4aIn273GqTEa2Tcd1YY+/T/G7v2XN6R+HeNFb5I6f5ulPl3OV3fd4QQQgghhBBCrBkJAAshxCZkMFrU/yhzYDeAYdduUhJmrs9xOflvWwG7zQph/5A6zeo+N2NBBbCQm5gzlcu07U9McXga/1JTTvY2zk+DeDpeKGVqRKcTp7ORhUeuGR43iclkgkiAoePq1K3H41MtmuzF6vqrqA9WS+wGiAYZ66rDmTzFKxCZPo1zf1tqPWSgqMVFgRn180+qx02e7tFccIAWTbKLyWxGCfvny9d1+4kAhrwymhLPLpPqbf51Ov2UqcaqTg7kmSAyw2j82pxOJ12jM0QwYC9pSGrvfFpaKrEbQAkHFso//iRdowHCiYfOutvNpWamKjMMpUy3O0pg/qBal5m4GkYBlOAUp+LJXevPogb8IteZRc1SKmvyMvj0CfYm/ehBzRzUUxYuNFer60M6new/PI6joRSLMsPFtuF4ydUptFqACMEr+oPJVQ4LEOXalaTstrle3G1DzETBZC/l0ImnefrEXnbbIDh2OikTbpbrEcDgYK+nhkKrGr3M2VWCq72HA47UYIB6nmGuK0109g0mZYoN0tepyXbXqCnJxUSYq0OZR/C2yrXBZfzXFMCKXRv/WCerO9/lFNF6rBSLEmLs5KkVxk49ZTNUuGN+rdvLE7NETXaK861UFdiIzo6lmT5X/78tybMePP25I1TmbSM4dpLajg0brNaPvXKhL4yMMNDTjmuJDEqXd6EePnekFEt4iq4ns/1BgZ4xVU/ZLG0rof1YJXaCjJ5c6po2pu8sP/Zl82/s2jLWdFJmN4ASYqLryflzqHNPLJpuPavvRhl8l9P3fUcIIYQQQgghxFqSALAQQmwm1yLEAINBfUxeUWCHcJioaReFRSw8XNVSwkx3P0Ft2wV1mtVYgLMBNeBkNKZ/QHw7KeEpuurcXIjPCXv1zCRBBdhmYFuikNWICYgE+jk7qV5LbO4KF05PEwLMlmweIFdQ7jABYSZOurmQCMrdvMbkmcP0B6Jq0LwkNSMlOjPEntq2+fJz420MBdQAuz2LJ5dlhXYMRJjuaqY3fm0Ak73N6nFNVvITT0+LKsm3AFE/3Y3uhfI3rzHZ66Y26+ynOWJRwGCloGzhqe61yV7cte6kQHGqyx217HE62aNdeHIjxKLk1HcyMOChodSOCdTA/FBgcaBdT9m4/JYGii0KMxfbGF6T5/OF7DADRLi+MCNrRkraB+JZr724NbGFWChI8Lr2KkzssNuTpt4M0D0+oz64d+zl2LlnFgIbyTMFpLBRfKiUvOQ0LUxY8so55m0hbcK3tZ7CPAPKzBTLxElSbJlri7sWUdcuTfwuZ2Nkf75LUddLVQiOnyE5OTMdPWUzFh/fY5FrcHmC2agZe2UNuZYosxOXgTAxJbHOwVoxYS9vwJOyHMIdwGDAbCug8ujn8bpWvjaDrZgjn/OwqmrQM6bqKavTjmI1UBm+0ssSsy6vkRX6zopjX3b/xq6lAwV5GIgS6D3Mmclr89vnAjFupZTM7rtRJt/ldH3fEUIIIYQQQgixpiQALIQQm8lcLGmazSIKdhmIBK4wpyTWSzRjMIAS06znp8wxNb6wZiYsZITub1uT3K01NXelQ5O1E3/wnyyixAM8B3AVqg8djdZCXMeKsZGmDjISD6CHZ5lM8+D4UvA6AEbzrpTt12cvpPwNMBnK5vMBCsm1GAAzu08sZBwlXocc6j5L4nlxnjkeCB9fItMpW+Oc7J0mggl7+VF17b4eD00V2YSWNoi9nKPleZgNoERmGDv9uBqYD2o7j86yAPktNBSrUz+fjDQsrPc8MkBnzRIBgBVtwzD/i4bMFTb1LL22pbGE9s8dpdxuQgn76T/+JF1jQaKAKW8v7Z6FiUVjw824z08TiiRdsxIh5B9lOgRwCyU1CqDWVZc7KVttgpACWPLZm+bHDkWuYmxEmZ1cfI+ks5WuLSGweJ7pDZHt+aZjLGnHVWCOT22eZvBLoqdsNmKxOXU2gdkoloLd2CIBRi8DRFAUwGjOfK1WjeRZD/bVneT8RJAoZhwHXdSsZVx5Q/XSmDKTg5MnT59nOqQABuwlBxdlUPY2Jpcdwh9WwOzgUFO9pqQOesZUPWV1uj7Viz8KluIW2kvWrlH19p2Vx77b/W9sEdYdANcJpktQTpHdd6OVv8vp/L4jhBBCCCGEEGJNSQBYCCE2I/MOCh27sZrCzE5eJBBUMFl3k3hGpijqNMh3tOFmJkKAKY/KY+fw+Xw8c+4YlXkmUIKM92e/piooS6/plyGzIV0qdiayCwoqt9Y+CBWbPEX1PjfdY36CYQWzzUHpoRP4RrxkkFS2geKBIYBokIluN3uqmzl7Wf3Rg9GxQw2ShwM6yybk09JQjCUaoP8kHGsoXljv2WAmb28T9Ru0TGFZ+wDHSm0QHKMtTXZ32TE1+00JjbGnto3hq9eYPNtIrXuMkAIGexmdSUtTz146xeHqPQvBoz3VHG7zE0/JYzYlMznERF0zZycX6uba5BlOTYUBE0ZtHRhrqHSYIHyVtDOgamypa0tiXdOM1Exlf77p5BfnYgIMeQdTgzBHC9SM6fnphb26yupaxzT+Y5aEyxOzRIHIzDhpEyhXKTZ3hUtnGrkYUMBgx6GNkm5h1y5f4lRzfBpfk5HlusO1yxdoq+0noMTXstYWWJGeMVVP2SzdmqSj108EMwUNnnX5t2rFvpPh2Lcp/o1VFDL/xrj670apsvu+I4QQQgghhBBibUgAWAghNpUZIlF1+rwdJblYonNMB2IMz86BJZeyMjNG4JY2te1OVNTKbhso0QjR+YwShWjIT3+bO8upH+MPpy25aQN6FfYdAFyfWzkcUZFrART0JyJfZu466lSLdalZXcmv+RmWwzHUU16nBUhjAcbPttFYux/nPjf9gQgY7JS5kiJtt90wwTCAQnCygzPjqY+oXQU2QCE8e0VnWVVR6xGKLVECF09yqbQQuwGigW6cTifuqTBgI08bAMhIoq3N7Fhpikujg3rvCA0FZnXK8cazBNLE/K1GU/zazqZsjwXOMhlUMwLN9uUjC7mug2qgNXiFxErHwYg6xac9TUbdjrTzzoO1ppA8g8LMVPfyAbwteG3J8i1mIEokqN2zPlZ7vlvG5Tb2O51Ub9Bi4rdWn3y6uVgNGMg0wBdbCMzqpmdM1VM2e7HJNk6OBlEMdiqPtZPmVllT2r6T8djH7fw39iaxmPojJqvm+06uy6H50cDafTdKpfP7jhBCCCGEEEKINSUBYCGE2IwMOygrsKBc83MZiI3PEMJCfpkVIxDRu6Bolm7G1CiNvdhDTf7GriVcVOrATJTZ4Q5OtSWmQd3D/sNtDKeLHmVkmEBQAWyUezzUxKeWJiefmvY+DjpMoMzgv5h6fKO5CIdVfcJstBZS4xmg3AZEA4xlkYg8PhMCLJR6OnGVrDD34aRfXVPPUsqgt4mKxDkDhTXt9CVNi5uQUbsVtdLT10lTRRG7EkViAfzTc0ST1qHWym/qYcTnY8S7+HPX06WrQRQM2Mvaaa+JT6GZk0+NR11PlmiA0XjET09Zilo5tNtMNHAR96UYmNWgyq2oGlKxmlcXWbgyFwbM2JPabZGcMlq97ZTbDUT83exvXmpK0QQD1uJ6SuYbDnaV1FNsNQAKkWCaX0fk7MJRUkWrd5DPVNoxKEHGexOVAJNXrhHFQN4BD/VJ6zwW1ng4stsMhJhJyXTLp2a3DaKzTF5Y5n7ckteWLB+H1QBcZ26ZYbekdUDNih1oXXUwKtvznT+HwU60s5Zfbtu/KOjidDpxnvara7IGR+PbGnWVXZe4jclMNiu8L5Kzi5J6LwccBlCCzGhmHN/KCiua8LaXYgGis1PzP3ZIZ5ejhHqviwITKDNTadtsub6DzjFVT9nVmO1tpNsfAXMBDWn+HVyVZftOhmNflv/Grt1YEiBwXf0xSXFrE0U5C991PJV29ccD87L7bpQJXd93kqzUJ4UQQgghhBBCrOwNO3fu/Ll2o1Bt376dGzduaDcLIe5w6e79Bx54kJyc7fN/37x5g1deeTmlzFqp7/GpwUUUZvr30Bx/UNrU51MfnsbXqlMzJlx4fZXYo35O729j2dV+XV58lXbt1iRBRrUP9PNb6DtRTPxjkySV1XPceNmF808oon3wKAUsXIejpQ9P8eJPBuJrfQ5x+FQW0ddcF15PJfa0iXQKwVH3wrqXy15bBH9XHW3LLcxb1M7g0QJMwVGcKRdcROvAUXanf/4LmvbMdXnTPLCNW3TsDNstcW7aIhCvh0Yae+c02+PtZAKIMH28mlUl7y17DqrkvuLyjlCZtuEWt0VmZePtsC3A+Vo3l2KAtZ6ec+XYkt+izNBf3czwMk29pPxWBk7sxhyZ5nj1qbTZYkXtgxxVK3VJiXowlrRz7kgBS3UdJTjKnkSFLVW/Spip7kY6NH136TrT3BeAsaaTgb15xKaPL5vBuRWvLUW8/YwzQ+xZMnjtoKXPQ2K4Ck+5qe1Y3USq+s83/m9B/K/FY+wSlhyj0tBTNo3EmL70uSXGl/g4tez4S9p/W9Jbqs70Uut4h/80+9uW/dd2ZUv13yTz9bRMWSU8RXdj0jqsy9VDZJquulNp1pLPrO8s3SezHX91WuL7Q+K7UcTftbCu+HL1AKvqO5mOfcu129L/xq7xWLLUd4FIkNA2O7ak71zZfDfStkW673J6v++oMuuTQgghhBBCiK0r/NIrWB56QLt5VdI907/bSQawEEJsMrfmZ3eeYzYpy2tyNjHX8MZNRcrVDjrOTxOKZD13ZNYC3cMEoup/K9q5Kw1mbLsPMejJYl7e2V4a3eeZDkVIPmo0PMPY6SdSgwT+CaYDISIpn68QCU3T787yITYAlzlV56Z/OkQmVTvb28gTp8eYCUeTzjl+Hr0XU8pChu12uY3uUb+mjJJUD9oH0wCXmbgaRgGU4NTqgr9Z6HW3LaqzaHiGsZOL2yKTskWth9htjuLvPakGfwHmznJmaGbhfdEQU91t2QV/Aa6eYiqogNnB3opVpXNBfOrTupND+DX9V4mGmZnoTru2rkpBiYQITJzn+BO1iwKkLFFnSkRdx1MbPKspzMOgzDBxZu06wWa5tmSugwXqTASTSwV/AQJ0X4xnxwIWazzrcRX0n28vo9PxiYCjM/intPtvvxyjUf33a0a7JyExXexaUYiE/Ixqx/UtTyEaDjI9dJw9tUnB3yUokRCBsS6c1emCv2Tcd9L1Se2YmqCn7Gqd6RglqIC5oAHvmi2su3TfyXjsy+rf2DUeS6528FT3NKHEAYkS8vfjrhti0a2m57uRLvq+76gy65NCCCGEEEIIIZYnGcDLkF8MCHF3Snfvb2QGsFCpGUQKge463OM3U/blN/VwrNSGIW3myCZS0s7gkQIMgfPscWeRrSzuDIksrKifrtq2JYIwW0g8K3ZboJv97jRzEd8hjFWdDBzMg+TM4yWV0D54hAITRKZPUn1qmfmixRa1hhnAYmvakLFPxhIhhBBCCCHEnU8ygDeGZAALIYTYhFw44vMQbtvhWFg/D7A6Sii0m9XpkK/PbZrgr8vTh8dVMn+uObtKaKpyYEIheCctPin0u9pB/3QETOuwVuVtUHWgADMRAkPrFQDZBHJdeA7kqesJdywf/DVaC6lpP4DDBBAmMC4BGyHuROs99slYIoQQQgghhBBiLUkG8DLkFwNC3J3S3fuSAbzR8mnpOzG/Dl5aSpiprlo6NkkE2OX1kXYZwfAUx2s70q79Ku4uiXUxU9aqFJtPbgWeY4dwmFderzR1jWOF8FQ3tR3StncmyQAW60fGEiGEEEIIIcTdRDKAN4ZkAAshhNiErtLx1GlG/dr1dwElQigwxuknNk/wF+DixSECCwvtqec53Y+7UYK/QtXbuIfRYIRIeNHqi2IzmYuhEMHf/eSywd8FC+t6SsBGCJE9GUuEEEIIIYQQQqwdyQBehvxiQIi7U7p7XzKAhRBCCCGEEEIIIYQQQojVkQzgjSEZwEIIIYQQQgghhBBCCCGEEEIIcYeQALAQQgghhBBCCCGEEEIIIYQQQtwhJAAshBBCCCGEEEIIIYQQQgghhBB3CAkACyGEEEIIIYQQQgghhBBCCCHEHUICwEIIIYQQQgghhBBCCCGEEEIIcYeQALAQQgghhBBCCCGEEEIIIYQQQtwhJAAshBBCbBIu7wA9TYXazWIzMZbQOjCApyJXu0cIkPt4bcn9Ju5iMpasQMYHIYQQQgghhFiWBICFEEKsUhHtgz58vqTXYDtF2mJiWTWdg1TazZiMRu2uJbjwrqqupd2yYrVi3mbGcegY7SWZtpVYndX29Y0j9/Eak/sNitoZ9PnweV3aPUK31d5vGyfTsSS3opWegZE7dwxYjowPQgghhBBCCLEsCQALIcRmknjQu9JrFQ+CHa5OBkZ8rOIQGyeniPrOvqQ6GWGgp5UqR5oHfYmyI0n1NDJIX2c9hdriaY472NOe/rhxjrImOvsGGUlqh7Wqw9ymPvbmmYj4u6g+NandvWnc3r4Tf3C/xGupc1q53XQed/YCzW2jBBUzBQ0eXJJ4tGUU1XfSlxQsHRnooXUNM8fkPs5cxm0h95vYhDLuv1nKdCwxVnhoP7Qbm9mg3bWlZVy/Mj4IIYQQQgghxLIkACyEEHeZHKuVtX1WeJm2/U6cTidO52n8Ue3+LBW10Pf5o5TnWTDNbzRgtu3mYLsHlzWprLGKzkTZ5GszmLDklXPM20J+Ypu1is5zi49rshWox9U+QDQW0tQzgqehlDyLiTWtOoD8FlpKLRDx09+x9IPetae/3da+76yj9Wy32V7cF2dQDHbKGm5jFE1krMIzyNHyPCwLNz0Gs43dhzx4F930WZD7OGO620LuN7GJ6O6/eukYSw6UOjChEJ4+z5OPJ8YBJ879bVzWFt4idNevjA9CCCGEEEIIsSQJAAshxGZyuY39iQd4TifO036iAMHRhW1OJ87GXu077zxX/czFIgQnznM8/mCzrmuCkAIY7BQecMwXNdaUkGcAJTRB15OPz9fTk4nyllxK48XLGqrIM6WW3Vd3kqFABAx2ylw1C+cAVLW3UGozQDSEf7QLd92++eOvRTPUHCjEQpTAUAeTMe1esYj2XliiLXS3W4bHTYgNNzMeVDDYS/BULJ05Lm4/Y4WHAw4TECEwdFxt28ePq/c8BuxlLqpW2YRyH2cm27aQ+01sBtn2Xz0yH0uKsO4AlCDjpy5x7aZ2/9aTbf3K+CCEEEIIIYQQ6b1h586dP9duFKrt27dz48YN7WYhxB0u3b3/wAMPkpOzff7vmzdv8MorL6eUWRdF7QweLcAUHF066Gt0UNVUT2WBbT6rS4mGCAyfpW04oG5wefFV2lPetliQUWcjiU8xOspw1VRRaF/IqlWiYYJT/TSfXSq3pIj2waMU4Of0OmWgWJv6OFdqUQN28TpJbAtPPEXtmdmU8k19PkotYSbqajkzV0L74BEKDDMMVTdzIeXhaj6tAyfYbU6qh/xWBk7sxhzx01XXtsLD2Cw4WujzFGMJjeE8fFa7N0VRfScHi+1YUlKcgejiulbLLmTQKJEgE+ePc/byUk+Il2m3Des7K3Hh9VViX+5eSNDVbjqOq1XmYbDBgSmD9ls7SefrvkJVSz1VBTY1mz0awn/xDG2XUu+BjPpDvJ2Do9qg99J9o6ypk6rCpONGQ8yOX8B94UpSKVVG5xCnp69nwuX1UWlXCI25OXw2uW4S97zCTP8emoeTdukh93HGVtUWt+N+c3nxVVqZ6a9meEc7rvn2UIgEJ+h2n+VK0viiu85yiqg/dpDipPLRkJ/hsx0MB+IHXuJ7QK7Li6fSjkEJM9XdSMfyA10aMpakaZFlrar/ZkLHWLJcfS7Q2caZfJ+M98fro0/hz21nb54JlCCjbjfBqnMc2W0GJcxUVy0d6U9qSauq39sxPgghhBBCCCGyFn7pFSwPPaDdvCrpnunf7SQDWAghtjJjCe3nPBzcvfCwDsBgslFw0MNAe0lyaR2KaGltoFQzpbLBZCGv/Ch9TWmm4dtg0Uhw/r/nhq8QVMBS+hkGvU1U5OeQk19Da88g6kyKFzkzB2DGaAC4RWTRs/KrBOYUYAfWInWLo9SOGYWZ0ZWCiNlxlOViAcKzl7S7Uri8I/EpEVeet7WqM930iXbKj34eb8q82evl9ved9W63eeNjzEYBWx6ujU462mal9ZyHg4mH+QAmGwWHWmiZn+98/fpDVecIDaWa45psOPYeQDsJp55z0NPXM1OB3apmyU0mBxRy8qlpd+EwAxiwOuI3fRbkPs7UKtvitt1vBqyV5ziW0h4GzPZyWtqrksrprLNcF940SxeYbAUcdB1ILrnIQvA3xERHNsHfJDKWZGiV/TcDK44lRe0Mzq9Rf5QCE2Aq4OhKa9dn0sY6v0/uKGyhMi9+NIOd4qZOGnab439bKKxMvjcyscr6vW3jgxBCCCGEEEJsXhIAFkKILayoxUWBGYgEGDpZF58u70m6JkIogLngAC0OoLdxfkrb0/FFIoOj2uluFzK/AJRYhJmJ85xOmlI5cVyLo5KFCZg3VpXDAkS5diVpbby5XtxtQ8xEwWQv5dCJp3n6xF522yA4dprqtkTZWa5HAIODvZ4aCq3qU8KcXSW42ns44Eh9UFxotQBhritNdPYNJj1gHaSvs57CVT5kVI8fIXhlTrtrnrGmkzK7AZQQE11PzrdFnXuCkLZsVScH8kwQmWG0K94fnE66RmeIYMBe0kCZ5j0r2mx9x1650A4jIwz0tOMqykkpklW7ZXDcxS7jv6YAVuzZ/tYiW7YCdpsVwv4hdYr0fW7GggpgITc+3/m69AcAXBTnGUCZYShlyvVRAuHUQJSec9DT1zNnUX/0EbnOLGqGW1mTl8GnT7A3KRhiMuelvk0HuY8ztdq2uH33m8lsRgn75/+drev2EwEMeWU0JcUdM6+zfFpaKrEbQAkHFtr58SfpGg2guY1SLAR/g4y6D3MmOQU5GzKWZGi1/XdlmYwlWcmgjTP+PhlnslhQZs7zeJe6VInZZoPgKE89NUEYMFhyKVwonoHV1u/tGx+EEEIIIYQQYrOSALAQQmxZFZQ7TECYiZNuLiQeGN68xuSZw/QHourDvZJsMnMuc6q2muYzl7ictLDc5JmrzAEYjawUGlsPJe0D8YzeXtzjqftioSDB62pgY4GJHXY7jvmAX4Du8Rn1YaZjL8fOPYPP5+Ppzx2hMjkzJoWN4kOl5CWnHGHCklfOMW8LSQlSOhWywwwQ4friWS7nHSjIw0CUQO9hzkxem98+F4hxK6UklBXaMRBhuquZ3smFB8iTvc0MBRQwWcnX90Q2CxvYdwwGzLYCKo9+Hq9Lm5G4inZb9riprkXUtQmNFu2edaaEme5+gtq2C1y9CcQCnA2obW40qjW8fv1hjlgUMFgpKFuICFyb7MVd604JIuo5Bz19XbdYlJz6TgYGPDSU2jGBGtAbCqjrrGdN7mPdVtEWt+t+i84Msae2bf7f2bnxNrUtsGCfj3zqqLOiSvIt6lTE3Y3uhXa+eY3JXje17vTT0efWdNJeaccQnWHI3Uhv6gzNKpc3JRt0/jXYTtrcSRlL9FlF/11eBmPJ5Tb2z/9g4zT+aHw665Qfcmin3s6kjbP4PqkEmTxziZuTc1wHIMxUdy+zszFiANsMbFsonblV1O/tGh+EEEIIIYQQYrOSALAQQmxZ8WyJ8CyTaR4CXwqqj+SM5l3aXRkxFtbQ3jPASMpD5EpWWkVyvRQ29dBQYEYJjiZl9MYZS2j/3FHK7SaUsJ/+40/SNRYkCpjy9tLuWZgPMTbcjPv8NKGIsvB+JULIP8p0COAWiuYJsRKZYazLnZSdNEFIASz57M0u7QnYhmHFp6NFWHcAXCeoCXgvVkiuxQCY2X1i8cP/Qw51n0V/2p5u69N3emnUPOR+8vR5pkMKYMBecnBRBlpm7ab/uMkCi+cS3xjKHFPjmjUv41me+9sur3N/GOdk7zQRTNjLj+LzjTDQ46GpQhtW13MOevp6FuzlHC3Pw2yI94vTj6sBvWDSOJAVuY91W0Vb3K777frsBe0mJkNh7abM6yzPjAmIBMYzn6Z+Rwnte/MwKUFG25q5kObf/azIWKLPKvrv8jIZS7K0Yhtn8X1yLkDvQhweglc4k+a9uq2ifm/X+CCEEEIIIYQQm5UEgIUQYstTCGg3rVZRK+eO7aXAZsag3XcblLUPcKzUBsEx2tJkRpUdU6cuVEJj7KltY/jqNSbPNlLrHiOkgMFeRmfScnSzl05xuHrPQtBvTzWH2/zEU02YTcm+CTFR18zZyYVavjZ5hlNTYcCEMZsEa70UhYh22yLr+PBYjw3sO9cuX+JUc3xKT5OR1KbIvt2WP24qqzHdfNKbwfr2h9jkKar3ueke8xMMK5htDkoPncA34mUhaTqLc8ior+sRQUnEDaJBJrrd7Klu5uxlNRhidOxQA3HhNR9FF8vo2rKos/WwLvfx6ttiM91vZoOmZrKoM+WWjoDV9StMBhV1vdWDFdq9C5Km+0557W/jsrZsRta3T8pYspmsw/fJjK2+fjfT+CCEEEIIIYQQm4EEgIUQYsuKPyyz5FKfJkJVYd8BwPW5q9pdK6ooL8AMKKEJupLW5XM6RwlqC68no4N67wgNBWZ1Cs7GswTSPC+3Gk2AQnDybMr2WOCs+sAcA2b78lP55roOqkHk4BWG49uCEXXaQ3vJ4oeKO4yZPuJfymXmrgOY2bHk1Jk3icUAgxmrpo1zXQ5NYDJxvDATdWke/sdfi6aGXGMb3nesBjXYkvSwf03aLc1x08m3mIEokXW5uNXIrj+YNZ0xt6Ice/q50SEWYPxsG421+3Huc9MfiIDBTpkr8WsLPeegp6/rMUwwTHx86ODMeGrwwFVgAxTCqb/60EHu48ytvi020/1WkWsBFGLxRGBddRaOqesC5+pZrDRGb+MeRoMKZschBtr1vHc1suuTMpbolclYsl7W7/tk5lZfv5tpfBBCCCGEEEKIzUACwEIIsWUNEwgqgI1yj4eawvhTu5x8atr7OOgwgTKD/2JqxPRmTP3bXuyhJj/9Ko6WeJBMuTnLZHwtw10lLtp7ShZPZblecspo9bZTbjcQ8Xezv3nxFJypDFiL6ynZtXBNu0rqKbYaAIVIMM3chDm7cJRU0eod5DOVdgxKkPHeRPgXJq9cI4qBvAMe6pPWvius8XBktxkIMbOKKSavzIUBM/ZE2y0SIHBdDWYWtzZRlLPQvp5K+6Iss/GZEGCh1NOJqySr+TiXtdn6TmFFE972UixAdHZqPnC/2nZb6riL5eOwGoDrzC39TJqS1gF1qtKBVtLEpNeNrv4QUeJrY1dRFV80u6TeS/shB2Zt2aJWevo6aaooYv52iwXwT88RBQyGhXdkfg76+roel64GUTBgL2unvSY+tWxOPjUedU1xogFGl27kFcl9nLnVtcXtu9+M5iIcVvVgRmsJrs4Bym3q+Y5dUsvoqrNJP0EFsJQy6G2iIqnvFNa005e0bIFWr7sbfwTMBUc2LAisq0/KWJK1lceS9ZLd98m1trr6zWx8EEIIIYQQQoi7yRt27tz5c+1Godq+fTs3btzQbhZC3OHS3fsPPPAgOTnb5/++efMGr7zyckqZdVHUzuDRAkzBUZza9BqAXBdeTyX2tE80FYKjbhp7NYHP/Bb6ThRjSd0KBBl1NtILWF1evMs9KI36OZ2YTtLlxVe56PF2koXj6lHUPsjRgqXShVTBUTXjx1jSzrkjavZVOkpwlD2J+kvU6aJCYaa6G+nQLMjo8o5QmbaCl6hfPfJbGTixG3NkmuPVp0ibW7NUe0WChLbZsZHUFhTROnCU3UtVxGrbbalzybbv6LFUuwFKeIruxo6UtTQzbjedx00Rbz/jzBB7lvyBgoOWPg/F8UoLT7mp7Vh6CsuVufD6KrFnVI86+oOxis6Bg+QtqrIIkagZc3I/W6bO1PptpHF+cUgd57BU/0rb1/VZuj9E8HfV0bZkI2dA7mNdsm6L23G/LVu/qeert85yXd6lA5LJ/+an+x6QW4Hn2CEcZohMd1F9ajLl7ZmRsWT5a04v6/6biUzGknlFtA8epWDZa9HRxpl+n1zUH+Ofof07k89MI+v6zWh8EEIIIYQQQmwW4ZdewfLQA9rNq5Lumf7dTjKAhRBiK5vtpdF9nulQhMTSaQDR8Axjp59IH5y82kHH+WlCkeR3pJrrbaR3KkRykWh4honubqbj011uJrHJNupODuHX1IMSDTMz0Z123WCVghIJEZg4z/EnahcFfwF63W30T6fWhRJR16dLW796XD3FVFABs4O9FUukql3t4KnuaULRxIYoIX8/7rohrqeWBC5zqs696HzXzKbqOwrRcJDpoePsqV0cpM2+3ZY/bjLXwQLMRJmdXO5hc4Dui34SzWexxrOaNoSO/hAbpq17glDSfNfRkJ9+dx1T2o52uY3uUb+mHyhJ404iYIO+c9DV1/VJ1x+i4RnGTi4TUMiU3Me6ZNsWm+d+U4iEpul3p56v3jqb7W3kidNjzISjSf9uxY/dezGl7CKzl3CfHCWogHl3A30t650JrKNPyliSvUzGkvWSzffJdZBt/WY2PgghhBBCCCHE3UUygJchvxgQ4u6U7t6/bRnA4s6XyFSK+umqbVs24Cg2D2NVJwMH8yA5u3xJJbQPHqHABJHpk1Sfkvkp7zhyH6+r23a/xTOAE7NNCLHuZCzRTd/4IIQQQgghhNgMJAN4Y0gGsBBCCHE7Xe2gfzoCpgIalln3UWwiuS48B/LUNaM7ln/YbLQWUtN+AIcJIExgfBXBKLF5yX28fuR+E3cTGUv00TE+CCGEEEIIIcTdRgLAQgghxG12+VQ1o0EFg72Sgfb1nspTrEpuBZ5jldgNEfzdblJmKNUoah/kmXPH2FtgwYBCeOoiHcsv6ii2MLmP14Hcb+IuJGNJhnSMD0IIIYQQQghxN5IAsBBCCLEJ9DbuYTQYIRJe7QqFYl3NxVCI4O9+ctn1CBcsrGdZ2zGp3SnuMHIfrzG538RdSsaSDOgeH4QQQgghhBDi7iJrAC9D5gwX4u6U7t6XNYCFEEIIIYQQQgghhBBCiNWRNYA3hmQACyGEEEIIIYQQQgghhBBCCCHEHUICwEIIIYQQQgghhBBCCCGEEEIIcYeQALAQQgghhBBCCCGEEEIIIYQQQtwhJAAshBBCCCGEEEIIIYQQQgghhBB3iDfs3Lnz59qNG+FN5neQ9+5c3ml9G297q5E33/umlP0/fe11Yj/6V/517kVmvzPD9yI/Tdm/EWTRaCHuTunu/QceeJCcnO3zf9+8eYNXXnk5pYwQQgghhBBCCCGEEEIIIZYWfukVLA89oN28Kume6d/tNjYA/MY387b3llLy8Dt58F7tzhW89jIvvjDJxLf+ldd/pt25PqTDCHF3SnfvSwBYCCGEEEIIIYQQQgghhFgdCQBvjDeZTKZPajeuh/t/9TH2VP0ev2V/kHu3xTf+9HVefWmO783+P2b+8Z/5rv/LfPXrQcKv3uAHN17jZ28ycO9b3sw9bwS23cuDv/xuHn6vnXtf/We+9/Lrmk9Ye/fddx+vvfaadrMQ4g6X7t5/y1vu5S1vuW/+7x//+DVef13GB3FnsLq89J9ooLpsF+FnL3PtlraEEHcel3cAV+6/8r+vzGl3Cb2MJbR+/gTlP/07Jmflf7aEEEIIIYQQQgixtNi/vY7pvrdoN69Kumf6d7v1zwDe9gv8VuUedr/9zfOb/m3u20w/P813fpBZEPfNO9/N7kd28x7rQvDl9e9PMzL6dX64jg+p5RcDQtyd0t37kgEsbp8i2gePUmBK2hT1c3p/G5eTNq2Gy+uj0g4QxX96P21rdeAN4cLrq8SedZ2sf/2KzJS09OAqtmECiMwwdLKZC7ML++t7Rii3zDHqbqQ3aXs2ajoH2ZtnIjLdRfWpSe3uzclYQ+fAXvLCYzgPn9Xuvb1ya+hs30ueKYK/q462yZi2xG2y2vFBCCGEEEIIIYQQa00ygDfG+gaA738PFf/xMd4Rj/3+9IffZuKvLjOb7Xq+97+Tx8pLec+O+AFf/x7P/cUlvv2qtuDakA4jxN0p3b0vAeCVOVydtJTlERl30tir3buJuLz41GhnEoVoOMhU/0nOXr6p2Xe7rX+A0ury4q20Y4hM01V3ik0Tu8nIagM8+ut3y/T1bOTkU3HwIHtL7ZhX+EFAUX0nB4vzsMTrTomE8A+d4dSlxdHZlcoaqzoZOJiHIflN4SnctR0EgNymPj5TaiY46qZxldFf9VgWIv4uqtu0wd94f9JsTQiOpm9zR1kTNVWF2C2m+WtILZvdcZMl6mBmqJrmC4mbNLvjrsv55rrweiqxE1yTIP3aWO34IIQQQgghhBBCiLUmAeCN8UbthjVz33vY8weJ4O9P+eHVEc79xXPZB38BXn2R5wb/O39xJb4O8JvfwWN/sIf3LCQGCyGEuE1yrFbMKdGbrcSAyZJH+dHP0V5i1O68zS7Ttt+J0+nE6TyNP6rdv3pzvY3scTpxVm+14O9a0F+/W7uvLyGnCJenh8GnT3Co1I5Zu1+jwjPI0fKFgC6AwWxj9yEPXlductGMypYV2jEQJdD9OM59bqbCgMVKIUBuEy2lFpTg+KqDv+S30FJqgYif/g5t8DcLxkKaekbwNJSSlxRMXXtlHCy0QHSWyfngbxbW83xne3FfnEEx2ClrcGn3CiGEEEIIIYQQQogNtD4B4Dfm8nvVj2HdBvzsVWb/95/zF1+dI23o941v5sFd7+bRD1VQURl/fehR3r3rQd6c9ux+yg+/NsTA+Cyv/gzYZuWx6t8jN21ZIYQQIr2o/3Q86Ofk8eND+MMKYKag8oC2qBB3vPyGQ1Q6bJhQCPunmFkmEG6s8HDAYQIiBIaOq/fR48cZCkQAA/YyF1Xx31HoKbtgB8b5bbk0tZRiUYKMd2hTTvWrOVCIhSiBoY7lf+wQHJ0fH5Jf2qzXqvYWSm0GiIbwj3bhrtu3ZFnI/LhaxpoSck0QvtLPuHYnmR93vc83NtzMeFDBYC/BU7GoYYUQQgghhBBCCCHEBlmHKaDv4z17/pDHrG+Cn73O974ywKXAv2kLwRvv550f+B1K3/22JQK9wM/+je/97Sj/+xs/TBs8vu+dv8Pvl+Vy/xvhp3PP8ecj3ybNJ2VNUsaFuDulu/c3dgro+JSVwVGc7itUtdRTVRBfFzMawn/xDG2aKVYXT68aZOL88YXpjIvaGTxawPXRp/DntrM3zwRKkFG3m2DVOY7sNoMSZqqrlo7EHJlGB1VN9VQW2OazHZVoiMDwWdqGA+qGtNMpawUZdTaSHC9Y8Xw18pt6OFZqg+Aoe5aKPGQqfs5R/2n2J89tW9LO4JECTGmmCtVzvmVNnVQVJpWNhpgdv4D7wpXUgpnU7yLx6YpZfI7ktzJwYjfmaIDu/e5FQSJjTScDe/NgZog9zRf0TX3s8uKr3IH/dB0TjniGqAFAITIzSkfbBQLJwTSjQ+23DhumdCmGS31OBtS2sGPRHjjNMfW0m2qZ+s2irxsdZbhqqii0W+brQYmGCU7103x28dVn3Hfi1vS+yG+hp8HI5JkOhgP58b6Rfgpodc1ohdCYm8Nnk8eifFoHTrDbrDDTv4fm4czLntnRw7lyW9J+UIKjdAQLOVZqJjjaSGPvXMp+3Rwt9HmKsYSWW0M3afxdqU4T91zET1dd2/IBZT3HTaO+x0e5ZYah6mZSE4B1HHejzrfMw2CDA9Oy9bw+Mh4fMh1/9Y59WY07QgghhBBCCCHE3UWmgN4YS4Ves/Zmx+9SZH0TAK9+59ISwd//n73/j4+yvvP9/wdFppUZkQF00GaqDNtNbBtsCXXBNZQKpQtOQSgcKF/5wBrC8uMYsaawKR6TeMR8oNkFswehxvRA048LhQVDRzhyiIeCx7CW0JXYmmzLoE1aHQoM4gzWQeT7xzUzmbkySWYmPwjwvN9uc5Nc13uuvK/39WPi9ZrX630bEx5ayAPZMcHfTy/x8Ucf8/FHH3Pp00i7gdyZ+z2W/JevMyRBTy+ceIU9x4wATP+MXP4uOzw3sIjItWBABqs3l7EwEvwFsDnJWbySlaNbm80qT1Re1cXUVT+hIj+jdSFw69iVTM8KN7S4GL+inOXjwsVeLQ7GTp9l/Ns6kdLNZSwc1/pwHMBic5KzsIzq0omtC1OUSn8NuUwf68QCWFzjWR2z793KajHKoV4McTFmcSr9nVW+i+WTTG1tTrJnzyOuIGpPjO+xNdQ1A7YRjJ9iXgmzso0Su021W82rkmQjc/lmVk2NBEAALNizZrN6ZW5cy/yyUuO8TRT87YL8il3hY9H5hlM5bj0jl5WrlzMpqzX4C2CxOciauoqqFfFlkpM+d6K6+bo4to6lecXsNEez2piGKwMIeamNDegOHs2C0nyy7QAWMrJzU2rb8txSdjT6CYWbBJrrqNxiJX+Sg1Dji10P/gLZUzJxAL6mPeZVacme5MJOiMaazoKpXTSljPFOCDTVmoK/qem1/u7bS1MAcGaR34tJwEnfH1K+/yZ/77vy9x0REREREREREUOCsGoXfCaTSfdl0B/gVB0//z/vmVsYGcIPzmTU4PCPF//Mb179Vzb+j438uPLH/Ljyx2z8Hxv52f86zp8/Npr0Hz6O7z04ikRT/Z59fRd1pwD6k3HfJJWCFpFrhzOHcfYQvvodPPmQG/ecIvZ6Q4CDzEnZAFhnlTMvywb+RmrWL4mW51xf04gfC66Jy4mNBdocDkKNz/PQ+noCgN1pZA8+/vgBfIDFkclYIHdlPjl2wN/AjqfD233oEdYfaCYE2HPmsTIbqCyI/s614clTvTXmcqExGZEp9tdwmAPHfISAkPcQa46Z13fdiInLqJiXjQXwNewjkm+ZWn/zGZ9lgVAjOx55KNr2kfU1NPjioy1Jj2+Kth5pJISNzPHT4ldY88nJshi/L5oanPrctzabzdjGk8b+PRnur8013pirFSNYNdFlgYCXveExm7Pk6XDJX/DXrcVtzq5NgnVBOVNcFgg1c2D9I9HxXVJ0gGZz25SOW5JSPNcBQkE/jQeeZ23M+RA5xo7s6bQe4uTPnVY9f10k5sBqAfynaMLIpJyyooJtP3uK2TFfVrHZs1JsC1sL5xtzUbvdzF26j+zlk3CEGnmxeGe4ZdeMzXAAfrxHkggmu6bj8XiM165dVG8qJT838serwdiej1OhFZRXbWtt79lGVfkyxiYKfiaxXbMFEzOx4eNY68XbVhLb7a3+wmHqT4aADFzmWGoPSeX+kM79N5l7X4/cd0RERERERERE0tSt4dKBo0czcgDAeY4f/FXCcsyxGcKcb+Llrf9K7VvmEs+XOPufB/nXn+ziN+eNJe1n+F7gVwePcx5gwEhGj04UJhYRuQqFfNRtfJi84q0cOwcEG3iuwQhcWK3GA/gpY11Y8FO3vpDK2tagRm1lITsaQmDLYHQ0MhfOxNuwh3O1LZwCwMehjZU0NQUJAgywcIRpTM22AT4OPF3E1kiw5NxJajcsZUtDwAhCT0w9mynl/oYdXpfHTLe762VuY9hyVkUDG//y2FRcNqPkbN661khaav1tIRgALBnkTGmNHpysraQorygmMNhz4xvc2YA3BJbM8YRzuQGwzsvGBfjqt9KVOGHId4j1S4rYeswoZXpsQy3ekHHeDIg0yrBiA/wNW3guPGbBliNsXVtHM2B3GMG+VM3LycJCgIbKpWyoPRld3tIQjMvYJuXj1lMOsyZvPoUb9nD4ZGvp19oNx2gBsFppDaMle+7E64nrImnBAIOXlVNdXcbySS5sQMhXz44dDbT5LkEqbcNGr1zOeEeIxheL2dleDDwlY7nVDuDnVOKK2u2zWLA7c5i+6idU5MdnboOT8YsnkRWb8okNR9ZUnqhYSYeJ2R1uNyxjGWOzLIQaDxFza+pYh9vt4f6GnfQbczxbHeY1PSP5+0N6999k7n19474jIiIiIiIiImLoxgDwbdzzlVsAuHSyjoPvm9cDZHDf34QzhC+9x8Gfv8KJRFHiiIst1P78IO9dwsjw/Zv7SPg4/P2D1J00Qsi3fOUebjOvFxG5GoVaOLTPNGdgOAvRmLt2LJkOC2Bn3FORTK7W1+JsY50jNpOppYG4SqreI2yIn064NWvP10Rtm3Wwx2uEjq32EeZVnUijv73Id2itKZCWan/38XRlHX5suKauwuPZRfWmMlZMM4dUemp8geBWapsCYHExNiYCvGC0C2imfmcSmY8daDmyzlQ61kcwUrM3wh8ysuiy55E/1vjUtmaMJf+J8TiBUNBnekMycsm4FeAU3g6SIA2pHreeYx27gNJN1eyK68N02s4knOy504e4prJqahZ2C4T8jexd+xAz84rZ6jWfECm2xZiPePl4o/Tz0/7lbNoWHrtd1ZQv6Djw2L4BWKLfUuhIJQVxWd1uHln7PHXNIcCCa+LCNlmcIX8je9cXxWRuH6A5BDhGMzvaOPXtAuTmj8fZYen21Lfbk/2NaPB3S9Q+SancH9K7/3Z+7+s79x0REREREREREbo1ADw8kzsHAXzM748neKIC8IVMRoQTdM++WcvxjoK/EReOU/umMc8vA5381XBzA0PT8d/zMcCgO8lsp42IyLUl2YBGukI0mBd1SU/3NzWB+rW43W4eenIHDX5wjH/MlNWWen+DtWuYP6eIjXvr8fpC2J3ZTFr8FJ5dFbRNmOvu8TXs29FglBsdu8BYkLGMbCeEGo/wXNfiv8nZWciBZsCWxfQnNuPxeNi++Qlj7umQl31bujD/aiiEUUi6I6kftx6Ru5rNT8wmx2k35pbuRGrnzpXkJxQJfAW8HNhYxMz5hTx32PiyijX7ViMD3NeQYtuI0axcPh5HoIEtT8MTy8fjjCSrWuxkzV7BsoTfBuw5Jw/vYU1huJSwzWr6MmIzB5YU8lxt6z6crN3AmkM+wIa1g752vF3AuoDp2TbwHYsp3d65jrfbg/2NkWFNVE+6hyV1f4jo7vtvH7nviIiIiIiIiIiEdVsAeJArg0EAH71D07vmtYZBGbeF5/E9T0tTOKibhLNNLUaJZwYxxEgybuvdJt75CGAQGa5B5rUiItegw7ScwihluSQ+Uyv2lXp12HDQxpGZMNAyzXUrAKdakq1HGtFT/e2ac8e2UvR8PQEsuKYsJz+6z2n2N9jAvueKKcibi3tOEVsa/GBxMSU/kpLbU+MbdmwNdc1gcWWzwAoZs3I6ySDsZrmrGeeEUMBPIJohFyLQXM+W4iIq2/mOWMfOEQwaAcAM05hl5mebAlFpHrduNm1qDnYg1HyA9THz+rrdNXjNjSM6PXf6gp14fQAhvLXr2LAvPoyWn+MEQviajqTY1pC7+jHGOwI0vPg0eyaNxWWBQMNG3G43RYd8gJOsjlJP2xU5L+zcmk4Z3gyLEciPCTJ6/Ua5YNfEtsHOW63JhP0Tbze6asFYsiwhGg9tTL10e4Lt9nR/Y4122IEA/nZP9u6Uyv2hp+6/feO+IyIiIiIiIiIS0W0B4DuHDzH+caqFd8wrw6yfvSH8r/Oc/bNpZUf+fDYcAIaBN7UX3H0n/OAFhgy/07xSROSatK+xGXAwqayc/IndU1syl500eEOAk6llZSwIl/Fl8GgWlFaxMNsGoUbqX4wv8XkuaPzsGl/GgtGts5vGSre/o1dsYpfHw66KfPOq7nG4mJ2NIbC4mLi8NbqUUn9zV7OpqpwV03IZEdn9YAP1dS0EAIvFHl6Y3vimYuuRRkKWLHLmZTIr2wH+hpQyCLsid1I2dgI07VzHmuJImdmZzF1azM6GdPepgYZTRvBq/OoV5A5uHa+y6a42GbYpHbc0JHOuO8IBtdC5JmrDcwCPmJhP6aaJbUtAJ33uxOvx66Ide455CWHBNaWU0gXhMtWDR7OgrJpJDiDQQM3O1NuSu5rF4+wEGl6kaE8Q7Eaw8WLACDVm2NsGLlNxpMUH2HFFrrkkjZ22gorSSTiAQNMhIt2tPXKSABay5pWxLGbO2LELynhsnB1oprGD66697RpGs2CcEwJN1G5N7bppb7s9299Yo8nOsACnaOlgvuWJq6uNEsnVq0kQk05BKveHnrv/pnvfiY7DtnLSrnAuIiIiIiIiImLSb/jw4ZfNC1N3GxMWzmbUIDj/5r+y5ZeJo7u3fXMhs7MHAe9x8H/s4Pin5hbt+MwoZv/XCdwGtPyfCna1U7Ptlm8s5Ht3D4Lzx9mx5SDvmRukaOjQoZw5c8a8WESucYmu/ZtvHsLgwUOjP587d4YPPki+kkFq8qnwTMcVqGft3GIOm1fHyWV19SrGJY4PQWQbuaVsW5WDzVuDu6Cy9XeYf460z8ynomw6LnNkDYxsvpoiCsypnKNXUvXUeBzxSwEvNe4CjMSnJPsbtzCX0m2ryLEB+Kl7cj5rUk3OipVfgWe6i0D92vBcymGZK6j6p0k48HHg8bzw3Mgp9DcyxuY2EB6zAgoiEzCnMr7h/rYvdnwjplC2bTmZ/mb8TiehvUtYaq7/nMp2w229NeYMtvCxoXUcsldWUTa+7VkAQMhPc/0Olq5Jowx0e+eX30vzABfOmD6kdNxSGYeI9voS0zYjv4KKNsGnGOmeO1HdfF102AdD7PHPr9jF9IQnsJ/69UsojpkwNbm24WM2oIHn84rYEzTKl2/aPBVn7FtCjWyZX8jO1ONzMHo11U+Nw+6v48n5axJn1XYwDiHfITYWxM8F2/6+ma7jFLdrXVBO9ewsgnVPMr+jA5vidnuqv3HC42xt3MHMwvYqD2SzsqqMyK3Cd6iIvHXt/IGfjPauyUT3hzTuv8nc+1K670SFP3vDP7X9PSIiIiIiIiLXHt/pD3AMu9m8uEsSPdO/3nVTBvAQBoWfEJ3vILX3PV8kWHIrd/61aWVHnLcRzi/mk0umdTH+fDacJ2wbFG0vInJtO8yaJUVsqWvGHy232w2aKikoep66Zj+xmw34Gtm79uG2wV+AY+tY93wdzR12JJ3+HubAMR8hIOQ91LUgV0eaNrClPpxFFi25m0J/DxezsabetP+hmDGLCeClM74p2ceOBj8WpxNHqJEjW83Bw57TsHEnDQHj36HoBLBhFjvOcYvZVpZGDd9j63h8Yx3N4W1DgOb6LRQt2UG4AEiMFI5bOpI411sqC6g8FP/7A75GDmzcSJ0vtmWK505UL10X7agsKm4zvgFfI3ufjg/+kmTb3NWLGWcPUF/5tBH8BWh5jg07GlvfF2jm0Mbi9IK/GOXRD3lDYM9m9rRkU05DBHxe6nY8ycy8tkHPRPsW8hvzHXd8HXe83QVjs7CEGjmwIdUD2/F2e6q/sfIX5hhVADosO9/AxhfriVzOjoxwdni6Urk/9Nj9N537TiU1deFi2oFG6g+Z14uIiIiIiIiIpKebMoBHMbNgAhmdZOhy42hm593HbZ8BTtXxwrZfccHcpo2BjJr190y4vT98+h6vVe3g2EfmNmHZMyn4ZgbQwsGKXRw3r0+RvjEgcn1KdO33bgawyNXLyDAM0bBxCUX7jNLHEaNXbOKJSU4sCTPhRHpBJFM0UM/6vOIOA5lXTDiDdkDDRuYWdVCTuQ+yziqnemEWeGuY2Wkq60RKtz1Gjg38dU8zf00H9aJFRERERERE5JqhDODe0U0ZwEn66BjH3w2n8N56D3+XPdDcoo2B2X9H7u39Abj07vH2g78iIiJyheWTHa6rOuDW7Nb5bIGM7ImMddmNksinWhT8lSvj2Dq21PnBlsPyst6dOzlZs+blYMdPQ29N3N1dMvMpm5eFJeRl37qOg7/WjLEsKJ1Htg3AR8M+BX9FRERERERERLpTNwWAL/FJkvP5NtUe5r1LAP3J+ObfM/ueWzDCu2b9ueWe2fz9NzOM9RdbOFybZEm2Tz+hg0rRIiIi0iPqafEB2MiavYp/+ZkHj8d4bS57jKkuG4R8HNrRcXBIpCcdXjOfGm8Ii2s61aUTzauvuJ2FM3G7uzinc2/LnEbZE9NxWfzUbywiYdXysNzSbWzf/ASzcxxYCOE79CLrrqZ9FRERERERERG5CnRTAPgs58Nzbg0adpt5ZbwLx3n5fzVx/lOA/tw29nssf3gmE+75MnfeMohBt9zJl+97gIfyl/O9sbcZwd9Pz/ObX9RwvJN60bcMGWT8I3AeFWYVERHpbcdY9/haauqb8Zvn/w35aW7Yy9qH81in9F+5wioLZlLj9eP3tZkhVtLREiSEn/qNj7SZAzqx1jmu89bVmleKiIiIiIiIiEgXddMcwPDl6QVMvAP400EqdnY+++7AkQ/wXx4YSThk275L5/mNp5raSOnoDkT78G4tFTW/Ma9OmWqGi1yfEl37mgNYRERERERERERERKRrNAdw7+imDGBo/nM4EOJwkmleaTJw5AQeuD+J4C9A/0F82T2fB77UWes7ybjV+NfZPzebV4qIiIiIiIiIiIiIiIiIXPO6LQB8/u13jLLL/e8kM8u8NmIgIyctZNEDo7jtxvCiS+f58++OU3f4NV7ZtYUtu17htcPHaGo5y4VI0m//QeH3fZlB7fX4jkzuvBHgLO+8fd68VkRERERERERERERERETkmtffZrOVmBem5S8BBv31KG678TMMtl7kP37zHvFFmwcycvJ/4YG7wpm8n17gndd28v/teZ3jv3+HP73/HmfOf8zH58/w3vt/4MTbxzn2q6N4Q0O54/YhfLY/DBjiIvv2j/jN2z4uxm0bMsf/HZn2z4D/bWr//Q98ZFqfjoEDB/LRR92xJRG5miS69j/3uRv53OcGRn/+y18+4uOPdX8QEREREREREREREUlW8MLH2AZ+zry4SxI907/etZdPm4az/Oo37xn/HD6aCXfErx04ZjoPZIWDvxdOUPvTF9jz6z+bgsRml/jzr19mywu7+E04qbd/xgT+yzdvi29mH8fX7+gPwHu/+ZWRiSwiIiIiIiIiIiIiIiIicp3pxgAwfHzsNY6fBxhI5jcnEA3TDvw608feYvz7YgsHX3w5GtBNysUWan+6I7xtGJT9bSYMj6wcyNe//XWGfAY4f5zXjn0c80YRERERERERERERERERketHtwaA4T0Ovn7CyOodNIpvhzN1M795D7d8BuASJ2p3cfyC6W3J+PQ9Du7/DUYMeBCjxo/ms8Bt3/wvjLsVY9uvHyScgywiIiIiIiIiIiIiIiIict3p5gAw8J8vc+CEUdh5UPZMZt79db48wijPzPt1HPjP+OYp+VMtdSfDRaOHZ/L1MTOZmW2Ulb707sGubVtERKSPy8ivYJfHg6d6NROt5rVyvdH5ICJybdF9XURERERERLpL9weAgaZ9u8LlmvuT8Y1xZISzf985foyuFmhuOv778DZuYfS9GfTHKP286xe/6fK2RUQkLL8Cj8dDRb55hQBgXUD5Lg+eTcvMa9pKpW0npmS7sADYsxk/2rw2RT11jHtqu31ZNx7jePlUeDx4tpWSa17V3efDNS2X0m0ePJ6YVztj2jd0Q3977JwUuV50fP/tKbqvi4iIiIiISHfpkQAwn77HwZ+/wom4Us+neKc7MnTffYf3wknAEJ5T+OcHee/TmGUiIler3FK2xT70b+/VB6Nr2fnlVO9KLvCXStu+KDN/PFmWEI1HtppXtZFK287sa/ASAvA3cOiYeW2rq318rzadHeMF5bvC1+42yqaY16bvajofcpeVUxUT1NxVvYnV0zLNzQyDRzNtRQXV4TEr7c3oyzWizTnZC58t3XuetQbBt5kvmkhw2+NhWxdOju7tb1+R4MsD3XR8e9K1eSzSczXd10VERERERKRv65kAMMCFJl5+8WV+cy6y4DYmLJzG6FvD5aDT0N+eyYS5E7gzsokLJ3hla5pzCouISLcanJGB3WJemlgqbfueKSwc64BAE7Vbg+aVJqm07VxLZQEz3W7c89dQ28Hmru7xvdp0coytC8h2WQh5vfiwkTl+mrlF2q6W82Fa2TZWTc3CYWtdZrE7Gbe4jIr8mCDw4Fzyyzax7WdPsXiSC3vrmi46TPFcN263G7d7LfUB8/q+pqv97eSc7CE9dZ7ZRoyNy8C0zsshqxt+T0/1V1KnY9Hqarmvi4iIiIiISN/XcwFgjABt7c+28PJvzxs/2+7kvrnL+Yf5D/D1EUOM8s1J+OzwLzNh5iKWz/82o279LAAXflfLlp+8TJOCvyJyLTlczFx35MG/G/faegIA3prWZW437oJK8zull1gXTCTTBr4jW9hnXmmSSlu5OnV2jI1gVYimA1vw+sGSOY7uCwH3fdZpZczLtgF+GnY8ady/HnqSHQ1+wIJrSj6zwvNcjl6+mOnZTmyE8NUfojHlwKfQ3jl51X22ZGG3QaC5mYAtk0kxEeB52S5CjY00xzaXeIF61sYe1z53fEVERERERESkp/UbPnz4ZfPCnjBw5AQeuH8Ut90Ys/DTS5w/3cx7LS38OfgxZ1uaOcsQnBlD+Kz1FjIybuO2oYP4bGyk+KP3OP7qyxyMry/dI4YOHcqZM2fMi0XkGpfo2r/55iEMHjw0+vO5c2f44IOzcW16RG4p21blYPPWtP/g1prNrBXLmJ7jjGaDhALNNOx8juKdDebWycmvwDPdhbdmDpX+lSyblYPTBhDA17CPvKJwWdFwu455qXEXUJlKWyLbzqBxy3x23lpK/vhIBmEIv/cAG4ue44gpO2bKinJmjW3NNAwFmmnat5WirUfiG4aNXrGJJyY5wVvDzPbG12TZJg9THY3smF9IZ8l1Hba1ZjNr5TJmZTuxJcriCdSzdm4xh8mldNsqcmKyJ1vXxUhrfJM4xnFt3cQPU7hvxPSn3e22f9xSMjiXZU8sZLzLER23QHM9O59bx86GmA0nc12Er69TNY9Tn1nK7CwbhLzUFBXhnbWZx8bZIeTj0Po81sUNdqsOjzGQX+FhekYjW2YW4ivdxqocCw3Pz6Roj7mlUSZ54XgXDvMJEXe8e+B8GL2a6qfGYQ80sHFuUZtAtnVBOdWzs6BxBzMLjfPCmj2F/AWzGBtzHEIBH95DWyh8rrUn+RUeprtCNO8tYulzTdHlMJrV1U8xzh6icctMCncCo1eyabmV2g3r2NkwOryfAerXzqW4nfFPXYJzNgHjWMTcS/xeDjz/JM8djpa2MSR9HSc/ZvGS62+szs5JSO6zJan+pnKehX9KarvkU+GZzq31ezmZOZURTWuZW3wYMpaxafN4zm2sxbp8Oq7Y/idzzafR36S2C9E+u7w1uIuOGOdFjhPjttpM/YsbKN4Tew2k/pnVuVTOlxT7m+w45FfgmX4r9WuXcCA7nM1vwfgMaKxhXfFWGoJpHotkr81k+xAjuftvipK+P/TAfd28WEREREREpA/xnf4Ax7CbzYu7JNEz/etdz2YAx7hw4iA7Kjfyr68ep+V8eBLfz/Rn0K13kjn6Pu7Lnci07y1k4femMTH3Pu4bncmdt7YGfy+db+H4q//KxsodvRL8FRG5KlgnUrq5jIXjWh/IAlhsTnIWllFdOjG2dcpuHb+ZsoWRAB6ADUf2bKpWjo5v2GMsZEzfzBNx5WMt2F1TWVk6K67lrPJdLJ9kKjNrc5I9ex6Jp8jLZfpYJxbA4hrP6mR2aUoZ450QaKptP7AS0Unb/LJSFua081C4F/XUMW673cTHLSWZ+VT8ZBVTs1oDRwA2Zw4L8+e1Lkjxurh17EqmZ4U7anExfkU5y8eFCxBbHIyd3k6fOznGWPPJdkHI28BO4PCBJgJYyBzXNgc4v2JXuEzyFTghjq2hrhmwZZKoQvW8nCwsBGiqjXwpIJeVq5czyXQcLDYHWVNXUbUiUtZ5Gq4MIOSlNjb4O3g0C0rzybZjXOPZ4fTOY+tYmlccH8i/AmaVJypZ7WLqqp9QkZ8R2zSF6zjZMeuizs7JpPVUf1PdbgN7mwLYMieRC2RMy8YZOMmhNt9SSO2aT1o62x2QwerNZcZ5EVlmc5KzeCWxt9XUP7N6SDL9TXkcbGQu38yqqZHAK8ZnQNZsVq9Mf97mVK7NVPrQU/ff5O8PIiIiIiIiIt2v1wLAhkv8+a2D7NqykY0v7OKVY028c+o8H38UDgjHtvzoY86feoemY6+w64WNbNyyi4Nv/Zm2LUVErl+5K/PJsQP+BnY8vSRcXvUR1h9oJgTYc+axMtv8ruTZ7HZj208+hNvt5snwdh3ZUxgLUFkQLS25NjxRpbfGXHYynImSStsYNrudkK8+un9LNtbjByxZU1gRfd6bz/gsC4Qa2fGI0Ve3280j62to8LUXBTnMgWM+QkDIe4g1x8zr21owMRMbPo7tMEcf2uqw7ZQyJrosEPCyd72xX3OWPB0uiwv+urW4o5k/Sc4H2oXx7fAYpym545aK0axcOR2XBUK+BmrC4+Z+6BHW1zQQe5hTvS5sDgehxud5aL1RFtfuNLLCH3/8AD7A4shMOBYdHmPAOi8bF9DStNNYcPgATQGwZI4nNqRsXVDOFJcFQs0cWP9I9HgtKTqQoMxtz5wPW480EsJC5vgFcZshYxmjXYDvGLG7GQr6aTzwPGtjrrfI+Dqyp2MMrwOrBfCfogkjG27Kigq2/ewpZscEm2z2rNYNX2HWWeXMy7KBv7H1HHO7WV/TiB8LronLmRJpnNJ1nOyYdU1n52QqkupviudZ0tsde2t0DujDB5oI2FyMH53BrBwngaa9bbLUk77mU+xv0tuN5cxhnD2Er34HTz7kxj2niL3eEOAgc1KkcTqfWSmw5bDK48FjelUkiiwn0d90xsFmsyX8bLG5xqf+90Oq12ZYp31I+f6bgpTuDz1zXxcREREREZHrWy8HgFtdutBC02uvsGfbFn5cuZGKioq418bKH7Nl2x5eea2JlgsK+4qItDWNqdk2wMeBp4vYeqTFWHzuJLUblrKlIWA8wJ2YVrTN4K9j/ZIith4zSise21CLNwQMsDDA3LaHBBp3MDOvOLp/LfuK2dFgPJx2RZ/2thAMAJYMcqa0PoU+WVtJUV5Ruw9DD6/LY6bbnVz554xljM2yEGo8xLrOgsWdtc2wYgP8DVt4rtbYr2DLEbauraMZsDt6MSDWQ8c4ueOWgtzpjHYYZTE3FhRRGR43zp2ktrKIvKLIMUzjugh5qd2wh3O1LZwCwMehjZU0NQUJ0s5YdHaMgQWjXYCXhhcjAZ3DHDkZAIuLsTER4EiGbUPlUjbUnowub2kIcrG1WY8Kbq01gtOubBaE5+QFyJiVg5MQjYc20rqbh1mTN5/CDXs4fLK17GrthmO0AFitDI4uBYIBBi8rp7q6jOWTXNjA+HLAjgZjHtp05Ve0CXB5PB4820pJN8dwylgXFvzUrS9sPceA2spC4/y1ZTA6EjlK6TpOcczSkcQ5mbye6m+S2w1fc0H/yfAXJ+y4pi8g0xGg6cBhwEcwZLRP65pPSprbDfmo2/gwecVbOXYOCDbwXIPxXqs1MmrpfWb1iE77m944hHyHuvWzJaVrMyyZPvTY/Tel+4OIiIiIiIhI97tiAWAREemqcHadr4na+GkFAdjjNUJZVvsI86qkeQ+toTYuGSn80L0XnWqKmYs2rLbZZ1qyj6cr6/BjwzV1FR7PLqo3lbFiWtfKGMfKzR+PM64Mbvs6besPGVlT2fPIH2s8NLdmjCX/ifE4gVDQvH89p6eOcXLHLQVZ9vDD9H2m/pqlcV20NFDZGk8A7xE2JHhvrE6PccYysp1AcyOVMf3dV3eSEBZc0QhwLhm3ApzCa05r7FX7jMw0SxZjF0QCOaNZkOOAQBO1pnrC1rELKN1Uza644Ot0Es5O6ZrKqqlZ2C0Q8jeyd+1DxpcDvN1wonWrsWQ6LICdcU+1DSwvzjbWOSLxuhSv45TGLA2dnpMp6qn+prLdYLDFqNbQFMCRMw6nv4GawwB+QiHAak/vmk9KmtsNtXBon2mu6HDm5tzoZNY9/JkVqGdtXFao8Ur4XadO+5veOLQcWdeNny0pXpthnfehB++/Kd4fRERERERERLqbAsAiIle9EA3mRdc4u6XthHrB2jXMn1PExr31eH0h7M5sJi1+Cs+uCvLN00qmyrqA6dm2NmVwE0qm7c5CDjQDtiymP7EZj8fD9s1PGPPQhrzs27LH/I5rQqLjlqrQxQ6jvzF68LpI4hhnTMvGCeCcGh+sWJwdnnd6bFwZaEIhjMKgV86xrUZmmjM7PBHw6Clk2cHfsCO+5G7uajY/MZscp52Oj2g4SAcQ8HJgYxEz5xfy3GEj2GTNvtUI6vvSPFIx5VDjXjFll1MzAEsqqYmpXMdJj1makjgnU9JT/U12u+EvfEQY82eDv3FfTCa6WU9d8z2z3R79zOoRPTMOyUnx2kxVT9x/U7k/iIiIiIiIiPQABYBFRK5a4eCKI5NlCSpbTnPdCsCplvYfl1+tpmU6gBBtEmiCDex7rpiCvLm45xSxpcEPFhdT8uNCbSnLWDCWLIu5DG5iSbXNXc04J4QCfgLRbKQQgeZ6thQXUZkgy6ovsN8aX18zc9pUXLFRmk60e9yS4Qsac4RmTjSvMen56yKZYzwt22leFC9aBvocwSBgsZNh6m9mfjYJdqHntDzHkcYQOHNYmQ1TZmdjp5m6rfF7OW1qDnYg1HyA9THzl7rdNXjjWu7E6wMI4a1dx4Z98eGj/BwnEMLXdCRu+ZVzmJZTGKVulyQILJuzKFO4jpMfs/Qkc06moqf6m/Z2Dxcz1+1mfsLJ2nvqmu+p7cbooc+s7tUL49CpFK/NpPXg/TeF+4OIiIiIiIhIT1AAWETkqrWTBm8IcDK1rIwF4RKDDB7NgtIqFmbbINRIfXT+0Z51Lmj8Htf4MhaM7nh2yFTaWu25ZGcYk5JaMyaSX17NVCcQaGBvJIEmdzWbqspZMS2XEZHNBRuor2shAFgs9uj2Yo1esYldHg+7KvLNq2KMZsE4Z8IyuG0l1zZ3UjZ2AjTtXMea4qLww+uZzF1azM6G9t+XrFTGNynRUpazmJVtHIuJyyooXZxN4pE1H7exLChLcNxiTFxdbWTIbitnQaLst9p6Y+5GxyS2VaxgWuR8B8YuKKWqLHIMe/q6SOIYR8o/+w5RlCBIMWdHY7gM9AKggYZTxhya41evIHdwa1/Lprs6zpJMUirnw9baJgI4GD1rGeNH2Ag07OO52PLYgMNq9Cp0rona8DyuIybmU7ppYpsyvnuOeY19nVJK6YJwedvBo1lQVs0kh3E+1Ow0vekK2tfYDDiYVFZO/kRTPVmTVK7jVMYsdUmckylKp7/JnGfpbLdDNjv5aV7znfc3ve0mJc3PrCujB8chrPNjkdq1mbz077+dfWalcn9IRzJjJiIiIiIiIte3fsOHD79sXiiGoUOHcubMGfNiEbnGJbr2b755CIMHD43+fO7cGT744Gxcmx6RW8q2VTnYvDW4E6W2ZOZTUTYdV8KnlCG8NUUUpJNmkl+BZ7oLb405oyaX0m2ryKGeteYyq6NXUvXUeByxywDwUuMuIG4zybQN9yExP/Xrl1AcmdwvMk7mZhAehwIK4iZ5pXVfbAB+6p6cT6LkMuuCcqpnZxGse7Kd7LNWybbNXllF2fi2ew9AyE9z/Q6WrglHSTscB7o8vkkdY+ssyqsXktXmPPPjD9ixx7btsL+m4xaVT0XMHKBt+2TIzK9o/6F87DWS7HXR5voK98P8c6B1/5I5xhkrqtg8yYG/vTbWfCq2T8cVamTH/EK2ZrZzvPxemge4cCY9vqR/PkSNZnX1U4yzAwSoXzuX6LSlYRn5FVS0dxwIzz8ac3/Ir9jF9IQHI5Xr2NDeudGhlMYsl9XVq8L7n0DMvqVyHac0Zin1N7lzso025368lPobkcR5lux2z4XHtv3jHbl/h7ed7DUfK4n+Jn0vgYT3i3Z1eK6395mVjAT373al0N9UxiGVz5aIZI5FCtdmSn1o73cnuv9Gdf6Zlcr9IdVrHjrod6K2IiIiIiIifYzv9Ac4ht1sXtwliZ7pX++UASwicjVrqqSg6Hnqmv1EKwwCAV8je9c+3PaBd086to51z9fR7I/tSTtSaRsnhL+5ji1FpiDi4WI21tSbtheKGYdED9IPc+CYjxAQ8h5KGPwFWDA2C0uokQMb2mkQI9m2DRt30hAw/h2KTpIaZrHjHLeYbWVT4penIu3xbUdwJ8UbD9AcM0lioLmeLUVLOHQqtiFQf4C6hmb8cfvVznGLqqSmLrzxQCP1h8zrDU2VBTy8di+NvkDM+R7eduWLsQ177LpI5hjPynYAfhr3tdMmWEmD1ygDnT3LCsfW8fjGOprD5wQEaK7fQtGSHZiHNy0pnQ/H2FrXbPzT30BNgqhQS2UBlYeaid1cwNfIgY0bqUtQ3ruyqJgtdW3b7326vfPhSjrMmiVFbfqbSCrXcapjlopkzslUpdXfJM6zZLc72GoFAvgbW5fFi5QEDkvnmk+iv2ltNxlpfWZdQT01DhHJHIsUrs2UpHX/7fwzK5X7Q1qSGjMRERERERG5nikDuAP6xoDI9SnRtX/FMoCvZ+1m8PSi0aupfmocAxo2Mrdon3ltvBTaGhmRIRo2LqFon1EGNWL0ik08McmJJZmsLOldKRzjq9nE0m08lmPpQhbi9aFPXMfXyTkpcrXpE/cHERERERGRPkoZwL1DGcAiIiLtmDUvBzt+GnZ0HlhJvm0+2eE6mgNuzW6d/xHIyJ7IWJfdKI96qkUPhfuY5I/x1SkyV/NjOTbw17NDwd8O9I3r+Fo/J0WuTn3j/iAiIiIiIiLXN2UAd0DfGBC5PiW69pUBfAX0hQzgHjGalVVP0d7UgACEfBxan8c6PRmW3mCefzLkpaaogK5Wdb226TqWnhY/z2xnAvVrmWuesFuuEN0fREREREREOqIM4N6hDGAREZFedYx1j6+lpt48Ty4Q8tPcsJe1D+uhsFwJ4fmUi4sU/O2UrmMRaY/uDyIiIiIiInLlKQO4A/rGgMj1KdG1rwxgEREREREREREREZGuUQZw71AGsIiIiIiIiIiIiIiIiIjINUIBYBERERERERERERERERGRa4QCwCIiIiIiIiIiIiIiIiIi1wgFgEVERERERERERERERERErhEKAIuIiIiIiIiIiIiIiIiIXCMUABYRERERERERERERERERuUb0Gz58+GXzQjEMHTqUM2fOmBeLyDUu0bV/881DGDx4aPTnc+fO8MEHZ+PaXJPyK/BMd8Uv89bgLqiMXyZXqXwqPNOJP8IB6tfOpfhw3EIRERERERERERGRLvOd/gDHsJvNi7sk0TP9650ygEVErhnTKNvloSLfvFzi5Ffg8Vyj43Qt75uIiIiIiIiIiIiIJEUBYBGRa4afUMi8rHt4a9y43eGXsn+vIZUURI6r202N17xe+qrs/HKq9YWPq46Om4iIiIiIiIiI9AYFgEVErmbWWZRXV1E6KxsrFwldDBH0AYNzWbFpG5tWZJrfISLXgMEZGdgt5qVXv8xpZVRVrWbKYPOaa8O1etxERERERERERKRvUQBYRORqNsDLofogroVlVFdNwR4KYc2pYNvPVjHe1kJTkyINInL1yMjOwOEYx/LN5SzQ91dERERERERERETS0m/48OGXzQvFoEmjRa5Pia79m28ewuDBQ6M/nzt3hg8+OBvX5kqbVVbNwmw7hJo5sH4NGw63mJukLr8Cz3QX3ho37VZ+zq/AM/1W6tcu4UD2Uyye5ApnuIXwN9awrngrDcH4t+QuK2fh+CwcNuPnkN/Lgeef5LnD5wCYVraLxdkh6tfOpfhw/Hsj8is8THf5OFSUx7oG89oORPdpDpX+lSyblYPThtFf7wE2Fj3HkWh/86nwTMflrcFddIRZK5cxK8eJDSDQTP2LGyje0xTdtDV7CvkLZjHW5cAWjr2HAj68h7ZQ+FzMjqQxZgzOZdkTCxkfs+1Acz07n1vHzkjjdvctgK9hH3lFW2O32IYxpoEOx/26lVvKtlU5nKp5nPrMUmZn2SDkpaaoCO+szTw2zg4hH4fW57EuPHZJnw9hU1aUM2tszHURaKZp31aKth4xFoSPb8e81LgLiL1cO7veDKmd6z1p7IpNrJzkxBLycWhjAetqzRdDCnTceu24iYiIiIiIiIgkw3f6AxzDbjYv7pJEz/SvdwoAd2Do0NZgj4hcX8wfFn02ADx4NNMWLmT2JBdWXz1esrEH/dhdDoLN9RzaWUllbRcCwUkHgF0EAgFstnCkIkagfi1zY6KJs8q3sTCrbTsI4a0poKCyheyVVZSNd3Twe7NZWVXGeHsjW2YWstO8uiOR/vr92Ox281pCjVuYWRjZYji40lxPnS2HcW2a+zj0ZB7rjgHkUrptFTmJdg3wHXicvA3hQEyKY0ZmPhVl03ElSuj21rTOy9zJvvkOPUme0dmEFADuQDiQiM+HxeEgcij8zc1Ync7oz63nTwrnAzCrfBcLsxIe4NbAYBqBxGSuN0Mq53rPy5xWxhOLs7EToHFHMYVb0wxi6rj16nETEREREREREemMAsC9QwHgDuiEEbk+Jbr2+2wAOCOfirKx+Gs2sG7nYFZuW4W91k3RkVmsWDadjKanWRoTrEhZCgFgAPwN7Fi/lq3HzjF6xSaemOTE4q/j6flrOAJYZ5VTvTALi7+Rmi0bosHpifnlLJyehT3QwMa5RewLb9N3YAl5G1ogYwVVmydhbdjI3KJ9wERKtz1GzsXWbSctpr8hXz01lZVsPdJCxpRSypbnYMfHgSV5bGihNbhitMZXX8PG9Vs5djGbZWWlTHVZ8B0qIm9dA5DL6qrF2Bt2UFNziMMnjSy9iSs2sXySE4vvEEV562gw9aGzMYPRrKx6ivEOCPka2PfiRmPcBo9g4uzFzHN5ySuKDwAnt922FADuQDiQaAMCjc+zZF8Omx8zfg55ayjaaGXlP03CER3jFM6HyHkWamTH40+zNdx2xMR8Fs9z4c0rissMBcgt3caqHFuH12bS1xukeK73DuvYFZSvnITTEqL5wDqWbmjvzO2AjluvHzcRERERERERkY4oANw7NAewiMjVrKWSgvl5FO9sILZIarBhJ2uWzu9a8DdFId8h1i8pYusxIwhybEMt3hAwwMKAcJspY11Y8FO3vjAuM7m2spAdDSGwZTB6LNDgww9Y7SMAsE5x4QBsI8aSC4ALuw3wn2o3mNmZQOMOZuYVs/WI0Y+WfcVGH3DgmmJqHPJRt/Fh8oq3cuwcEGzguQbjfVbr4HCjw6zJm0/hhj3RoBFA7YZjtBgNibSMSGbMyJ3OaAcQqGdjQVHruJ07SW1lUWvwN5a/rvPtSnpCXmo37OFcbQunwMiw3FhJU1PQuAajY5zK+dBCMABYMsiZkh1derK2kqIEQcRkJX29xUrqXE9RfgUej6fta1tp+HpOLHhkA0uLdtAYsOCc9ATVZdPMTZKn4yYiIiIiIiIiItcRBYBFRK4ZdiyJKpH2kpYj64ifqtNHMBT781gyHRbAzrin2gaDFmcb6xzZwJFT+AGbPQuAKZkZhJqb8dsymZQLZNuxAgF/Y+wvSMmpprbz4dY2+8yLDKEWDu2LnXcTqCzA7XbHlWq2jl1A6aZqdsXtWyQ7r63OxwzIsmMD/A37TG3b5z20pvPtSnpaGohW3wXwHqG971kkfz7s4+nKOvzYcE1dhcezi+pNZayYNtrcMAUpXG+xkjzXe4+fixfNy9Kg4yYiIiIiIiIiItcRBYBFRK4Zeyia2X5Z0StvAJak008b8QcAq51sppHjAm/tHloCNlzjR8NgK1bgVEv3BjbsXYmg565m8xOzyXHao/OKdqfQxSSjv9I3pHg+BGvXMH9OERv31uP1hbA7s5m0+Ck8uyrIzzS3TkYq11sPCwci27zmFtPRFWwdu4JNZYvJtodoPvA084v2mJt0Px03ERERERERERG5BigALCIiveQwLacAfBxYkiAYFH4ZAexwW7udEbk5jLC00LRvH3UnQ9hdk8jOsmMjgN9r/h1dMy3TAYQItpMI3JFpU3OwA6HmA6x/5KGYfaqhS930BQkBjsyJ5jXSh6V1PgQb2PdcMQV5c3HPKWJLgx8sLqbkzzK3TEIq11vfkzmtjM1PTMJpCdC4oyi9+X/ToOMmIiIiIiIiIiLXAgWARUSk1+xrbAYcTCorJ3+iuYZpPK8/AJbB5EzKxNbcSGUQ9tQ1EXKMZkGmFQjib6eEazKs9lyyM6zGvzPGsqCsmqlOINDA3jQSDR1WI18wdK6J2vDcoSMm5lO6aWKC0rEpqK035u91TGJbxQqmjc2Irhq7oJSqsvy45tI3pHQ+5K5mU1U5K6blMiIyXWuwgfq6FgKAxWI3vQHOBY2McNf4MhaMTjzHayrXW1+SvayCssXZ2EM+Dq3Po3BrFy70FOm4iYiIiIiIiIjItUABYBER6TUtz71InR+wZzH9sbI281t6tpWSG257xOcHnOTk2PA1hSOye+rxhmxkZTkg5Kcldk7PFDnGr6Js83Y8Hg/bNz/B7Gw74Ke+cl2HZWnbs6/BSwiwZS+P7s+/PDadHKfN3DQ1wZ1U7gtv2zWJxU9sjm7/idk5OIwYtvQxqZ0PFuyOLCYtXsW//Kz1eviXxdnYCOFt2Gd+Aw0HmvAB2LOZ/dTPYq6jCiJfCUjleusrJq6upmyqC0ugkR1FeaxLduLrbqLjJiIiIiIiIiIi1wIFgEVEpBcdZs2SIrbUNeMPmdfFC7acw2jio6k2EundyRFv+I3+U6SVF1h/gLqGZvyh2A6E8DfXsaVoCcVpBpxaKguoPBS/XwFfIwc2bqQujZLSsZoqC3h47V4afYHwmNDa58oX49pK35DS+XC4mI019TTHXRQhAr5G9q59mILKBN90OLaOdc/Xmd5jlvz11le0NLTg89WxcUkhvZj4G6XjJiIiIiIiIiIi14J+w4cPv2xeKIahQ4dy5swZ8+IOWLn3G3fz5i9fJ73wgYj0BYmu/ZtvHsLgwUOjP587d4YPPjgb1+aalF+BZ7oLb43mnLwe5Fd4mO4KUL92LsXppEGLiIiIiIiIiIiIdMB3+gMcw242L+6SRM/0r3fKAO5GjtmlPPqDQip+MBlV5BQRERERERERERERERGR3qYAcDfy7Sim6pd+7N9YoiCwiFxTXNNj5p+siMxUKVe/fCpi5had7jKvFxEREREREREREZGrzRUtAd2vXz9mzJhBRkaGeRUALS0t7N69m8uXr0wX00sZtzL5BxUs+YYd/y83U/Cj/d1QDjqPZz0zGBm3LMjRf55DyasxixY9i+dBo9WJl9w8+kLMuphtBN8oZ85rE9j+/TGdBKmN39H8oIcZLoAT7HY/SpW52f0l0W0F3yhnzlMHgQmUvFjImEFGk9blrfIqzNuNf0+8BPsr0kMSXfvXewnoON4a3KoHfY3Ip8IznfgjrBLQIiIiIiIiIiIi0jNUArp3XNEMYKvVyk033WReHHXTTTdhtXYcoux7guz/UQGbuykTeMKT2/G0Cf4CWBnzfQ/bn5xgXtEnWe9ZSsn95qUi0udVFuB2u+NfCv5eQyopMB9ft4K/IiIiIiIiIiIiIlezXgkAW61WLBaLeTFDhgxh4MCBAHzwwQe8++67vPvuu5w7dw6AgQMHMmTIENO7wGKx9PHAsBEELn/Fh/0bSyh/5N70gsCLnqXwnvA7zx+lPPpwvpyj543F1nsKeXZR3LuS82oJcxJsL/73dGfGrZUxi0pIOlwd14/u7ouIiIiIiIiIiIiIiIjItanHA8AOh4M5c+bw0EMP4XQ649YNGTKEAQMGAPDb3/6WmpoaampqeOONN/j0008ZMGBAmwCw0+nkoYceYu7cudx+++1x6/qWIK//SyHlr/hwfLswjSDwBEruj+T9nmD3vBJaCygfpGTebk6Efxp5fwqB1Stp0BiWXiUZyyIiIiIiIiIiIiIiIiJXox4NAA8bNowHHngAm82GzWZj2rRpfPOb34xmAzscDgA++eQTTp8+HX3fmTNnuHjxYlwbi8XCN7/5TaZNm4bNZsNqtTJlypSrKgj8zN/HB8A7dP8E7orMhes93nbeXao47g3/c9BdTOjL5ZXPH+VouK/We2aQZ14vIiIiIiIiIiIiIiIiIt2ixwLAw4YNiwZrI/r37092djZz587ljjvuwG63A/Dxxx9z9uzZaLtAIEAwGATAbrdzxx13MHfuXLKzs+nfv3+03dURBIZgKARYsN3ctpx1u1z2aMZw8HQk1zfeidPGGF0NDhZEMpZHMqMiiRDwoDEUejx4Iq8Xr5IsZxEREREREREREREREZErqEcCwMOGDeM73/lONPj73nvv8Ytf/CI6t+/gwYP5zne+w7BhwwAIBoNcuHAh+v6PPvooGgCObGvw4MEQDha/+uqrvP3221y+fLmPB4Gt3P0Pz1D8nZEE6yoo2PCmucF1pIpHXwoHsl0z0pu3WEREREREREREREREREQ61O0B4MGDBzN16lRuuukmCAd/X375ZU6ePMm2bds4fvw4ly5d4jOf+Qyf+Yzx6z/88MNoyeeIM2fOAETbXb58mebmZqqrq3nrrbd49dVXeeedd+KCwMOHD4/bxpUVE/x9o4Ila/aTbr6udVhkLuB4I4eZZhX2+tP+Hb3ihUfZHS4FPfLBZxllXh/r/FHK3W7ckVfcHMgiIiIiIiIiIiIiIiIikki3B4AvXLjAxx9/DMCnn37KiRMnotm9oVCIgwcPsnv3bs6fPw/ApUuX+MMf/hC3DcKB408++QSAixcvcvDgQV566aXoti5dukRjYyOffvophDODI9u88kzB36fSCP6+cDxcMhlwjUowb24eo1zhf55/m4Ovxq8dfrupYPL9TiLh8ff/dOVCqVUxpaBHRvovIiIiIm1k5Fewy+PBU72aiabv/XVFT21XRERERERERET6hm4PAIdCIV577TU+/vhjPvOZz/C1r30tWuo54k9/+hMvvvgiL7/8Mi+88AINDQ1x6wF+97vf8eMf/5iXX36ZrVu30tDQwOXLl6PrBw4cyN/8zd/Qv39/PvnkE15//fW4MtJXTjcEfwGoYvcbkXeOZEbcHLh5POuZQSQv+MSr4ezYVw/ydjgGbr1nKSX3R9pPoGTRmPCcwic4/kJk+ZUQUwpaRBLLr8Dj8VCRb15xDeiNfQv/Do9nE8sU2EiOxkyuNrmlbPN48PTkzaQPXBdTsl1YAOzZjB9tXpu+ntpuHOsCynd58GxaZl4jsfrAeSYiIiIiIiIi155uDwAD/PGPf4ybo/e+++6jf//+cW1CoRAnTpyIZgsncunSpbgM4oh+/frxN3/zNwwZMoTLly/z29/+lpMnT8a1uTK6K/hrOPjUnGjJZAaNodDjCT8gag3+Bt8o59FoQPcgJS8cDf9OK2O+H2lfyJhBkfa7qYo0T9lIZkT7YLy2P2nKNE5GTCnodsXtr/HSvMEikpqLXOzKTbgXZOeXU72rhwPiKdGYXUl9Yd/6Qh/6nit3Xexr8BIC8Ddw6Jh5bfp6aruxMvPHk2UJ0Xhkq3lVn9D3zvUrd56JiIiIiIiIyLWnRwLAAG+88UZ0Ht+MjAzuvvtuc5O0jRgxgrvuugvCcwW/8cYbcdnBV4pjbqkR/D26mYIuBn8jqgrcuP85EtSNdYLdbjdznjKVc361hDnuSJnlWEGO/nOC9ldI1UuJ9klEpBt4/QTMy/qowRkZ2C3mpVeAxqxP6Av71hf60Gf0geuipbKAmW437vlrqO3GP5x6arutprBwrAMCTdRu7ZFf0GV95lzvA+eZiIiIiIiIiFx7eiwA/Je//IXXXnuNUCjUbinoWP369eOmm27ipptuol+/fubVUQMHDmTs2LHccMMNhEIh6urq2mQIXym+bcVs/vFmCko8+M0ru+LVEua43bjjXo92kMlbxaNt2s+hxDRPcKuDlMwLt5sXLicdo6rAvK3W15ynDsb1rzXA3PE24/cpsi8x70nwas10FhHpQCj834CfRtMqaYfGTKQtXRdpsy6YSKYNfEe2sM+8UuLpPBMRERERERGRHtBv+PDh3Zo6a7VaycjI4M477+T2229n4MCB0fLPv/nNb6itrY1rb7FYGDduHF/+8pe54YYbAPjkk0/4zW9+Q11dHaFQ5KmIITMzk0mTJtG/f38uXbrEhQsX+NOf/sQ777xDS0sLwWD3ZRkMHTo0msUsItePRNf+zTcPYfDgodGfz507wwcfnI1r023yK/BMd+GtmUOlfyXLZuXgtAGE8HsPsLHoOY5Eb3X5VHim4/LW4C46wqyVy5iV48QGEGim/sUNFO9pim7amj2F/AWzGOtyYAtnPoUCPryHtlD43OFoO6MPt1K/dgkHsp9i8SRXOFMqhL+xhnXFW2kw324H57LsiYWMj9l2oLmenc+tY2ekcbv7FsDXsI+8om4oFZpbyrZVOdgC9aydW0zMXkXXnap5nPrMUmZn2SDkpaaoCO+szTw2zg4hH4fW57Eu/MakxyxsyopyZo3NwmEzfg4Fmmnat5WirUeMBeEx6JiXGncBlTFLcpeVs3B8zHb9Xg48/yTPHT4X0yq18yGqozFLU6fjEKPTfUtzzJISPSfdFMS9OZfSbavIIWZM8ivwTM+gcct8dt5aSn60z4muzSSls2/WbGatWMb0HGc0gzEUaKZh53MU72yIeV+SUu5DaudZqtdQUveSyDnrrcEdc+Ay8ysom+7CEvJxaGMB67qS3prMdZH0sUhlzMLnXvh6AKCzPqxcxqxsZ3S84kTfm8J20/kMiLFsk4epjkZ2zC8kmgCs+2+v3X9FRERERERE+jLf6Q9wDLvZvLhLEj3Tv951Swaw1Wrlu9/9LkuXLiUvL49vf/vbZGZmctNNN0WDvx9//DFvvfVW3PsGDhzId7/7Xe6+++5o8Bfghhtu4O677+a73/0uAwcOjHtPc3MzH374IQD9+/fnpptuIjMzk29/+9vk5eWxdOlSvvvd72K1WuPeJyJytbl1/GbKFkYCpAAW7K6prCydFd8QYEAGqzeXsTDysBnA5iRn8UpWjo4syGXl6uVMymp9kA5gsTnImrqKqhWZrQsBsJG5fDOrpkYe/GP0IWs2q1fmxjfNzKfiJ6uYatq2zZnDwvx5sS0h4b7ZcGTPpqq1s+k7XMxctxt3Bw/Sbx27kulZ4V9ucTF+RTnLx9nDPzsYOz0yxqmN2azyXSyf1BokALDYnGTPnkdXppmcVb6NVVNN27W7mLrqJ1TkZ8Q2NSR1PsRIYsxSkco4pLxvV5yFjOmbeSKuzx1cm93NOpHSzWUsHNcacCQ8vjkLy6gunRjbumcldZ6ldg2lei+J1Rr8bebAui4Gf0niukjnWCQ1ZqnJLys1tpco+NslKXwGxJpSxngnBJpqW4O/MXT/NensPBMRERERERERSUO3BIAHDBjAkCFDGDBgQNzyS5cuce7cOY4fP86+ffs4depU3Pp77rmHW265BYBQKERTUxNNTU3RrN9bbrmFv/3bv417z4ULF9izZw+/+tWveP/997l48WLc+vb6IiJytbHZ7YR89ex4eglut5slG+vxA5asKawwP3N25jDOHsJXv4MnH3LjnlPEXm8IcJA5KTvaLBT003jgedY+8lC0vPr6A82EAEf2dFpbGmw2G/gb2PGk0f7JcFubazxjo61Gs3LldFwWCPkaqFlv9Nf90COsr2nAlyAAYLPbE27XkT0lZrs9x+ZwEGp8nofW1xMA7E4neGt4/PED+ACLIzPaj+THLJ/xWRYINbIjpu0j62toiB2EyoLourX1xsyP3hpz2fvW7DPrrHLmZdnA39g6tm4362sa8WPBNXE5U1q3bkjyfOgZSY5DKvuW4pj1tJSuzc6kuG+5K/PJsWNcP+Hf737okeg5ac+Zx8pUD3GKfYhK8jxL/hpK/V4S0Rr89VJTtJQNKadipy6tY5HUmB2meG5k3NcSPiSJTSljossCAS97w+M1Z8nT7GgwJiPx162NCSymsN2w5D4D4i2YmIkNH8d2JC7+rPuviIiIiIiIiEjP65YAcKyPPvqI119/nZ/+9Kc899xz/PSnP+XgwYP84Q9/4PLl1mrTN910Ey6XUYLtgw8+4MUXX+SVV17hlVdeYefOnQQCxkMZp9PJTTfdFH0fwLlz56irq+PnP/85mzZtoqqqiv3793P69Om4diIiV7NA4w5m5hWz9UgLAC37itnRYDxEdpmfOId81G18mLzirRw7BwQbeK7BeJ/VOjjc6DBr8uZTuGEPh0+2lq2s3XCMFqMhkZYRId8h1i8pYusxo/2xDbV4Q8AAC9Gv2eROZ7TDKCW6saCIylrj93LuJLWVReQVtQkbgb+u8+32pJCX2g17OFfbgvHVJB+HNlbS1BQkSGw/UhmzFoIBwJJBzpTWh/wnayspyitqGzxL0pSxLiz4qVtf2Dq2QFDxjkkAAP/0SURBVG1loXE+2DIYbY7EJHU+9JTkxyGtfesDUro2u9U0pmbbAB8Hni6K/n7OnaR2w1K2NASMINPEVKPQaUrqPEvhGkrnXgJkLiindLoLS6CRHUUFVCaostv90jwWSY1ZCjKs2AB/wxaeC49XsOUIW9fW0QzYHVnmd6Qkqc+AWBnLGJtlIdR4iHXHzCvDdP8VEREREREREelx3R4AvnDhAm+99Rbnzp2LC/ia3XTTTdEs3f/8z//k/Pnz0XWnT5/mnXfeAeBzn/scQ4YMia5LJBgM0tjYyJ/+9CfzKhGRq9apprbz4dY2+8yLDKEWDu2LnYuwNdNpbnFrUUnr2AWUbqpml8eDJ/qaTnszIrYcWUd8FVUfwVDsz0CWPRyA2Gdq2z7voTWdb7cntTRQ2fosH7xH2NBO0Cj5MdvH05V1+LHhmroKj2cX1ZvKWDEtUc3PZI0l02EB7Ix7Kvb3G6/F2cY6hzmpLMnzoWckOw5p7lsfkNK12a0cWC2Ar4naBOfrHq8RTrPaR5hX9Ywkz7Okr6E07iXcOpHS2VnYQl5qigvZmmBcekaaxyLJMUuaP2RkG2fPI3+sEWy2Zowl/4nxOIFQsGvnZVKfATFy88fjJEBTbdtrJEr3XxERERERERGRHtftAeB0dFSu+fLlyx0GkkVErid2SxcmecxdzeYnZpPjtNOFrbQrdDHZiM1VJMUxC9auYf6cIjburcfrC2F3ZjNp8VN4dlWQb55iOSkDsLT/EdlnJTcOV+e+tadL12bKQjSYF/VVKV5DpHovOXWEWm/ImEt24TTz2l5whY/FzkIONAO2LKY/sRmPx8P2zU8Yc+yGvOzbssf8jp5jXcD0bBv4jtFO9efUpHjuJHffScW1dY8SERERERERketLtweAP/e5z/GFL3yBz33uc+ZVcc6fP89f/vIXAO68805jjrGwYcOGceeddwLw8ccf4/cb85i1p3///jgcDux2u3mViMg1ZVqmAwiRTlLXtKk52IFQ8wHWx8yR6HbX4DU3ToUvaMzHmDnRvOaql9aYBRvY91wxBXlzcc8pYkuDHywupuTPMrdMwmFaTmGUmV1inqey9VWQbn3TntTpOPStfbPfGl/HNXPaVFytf5p0qivXZvL8hIyLjWUJqjxPc90KwKmW9mrv9r6UrqG07iVBKgtmUuMNYc9eTHVpKu/tij5yLHJXM84JoYCfQDQzN0SguZ4txUW9VA7bkLFgLFmWEI2HNtIde53SuRPR6X0nFX3rHiUiIiIiIiIikopuDwBbrVb+7u/+jsWLF7N06VLmzZvHhAkT+MIXvkC/fv2i7QKBAO+++y4AgwcP5nvf+x7f/va3+fa3v82sWbOw2WxcvnyZ3//+93z44Ycxv8Fof8899zBz5kwWL17MsmXLmDNnDk6nM66diMjVzGrPJTvDavw7YywLyqqZ6gQCDexNI6nLYTVyqELnmqgNz6c4YmI+pZsmJiinmYLaemNOSMcktlWsYFq4DCnA2AWlVJXlxzW/mqQ0Zrmr2VRVzoppuYyITPMYbKC+roUAYLG0/ZLSuaCR6egaX8aC0YnnhtzX2Aw4mFRWTv5Ec63RPiiFcUhn35IZs5RES+jOYla2cb1NXFZB6eJs2h4xQ/y1OZH88q5dmxGd79tOGrwhwMnUsjIWRK61waNZUFrFwmwbhBqpfzGFDFqTzvuQmpSuoS7cSyqLNlLvB3vOY70UBO75Y5GM3EnZ2AnQtHMda4qLwkHJmcxdWszOhp793fFGs2CcEwJN1G7tnt+b0rmTwn0nIplzPZ17VE+auLraKEG9rZwFaWU1i4iIiIiIiMj1ot/w4cO7XF85EvS99dZb2y3n/PHHH/PSSy/h87WmxgwcOJAHH3yQYcOGxbWNePfdd/F4PFy6dCm6bODAgcyaNYvBgxM/qLl48SKnTp3if/2v/0Uw/GAnXUOHDjUvEpHrxJkzZ+J+vvnmIQwe3HpPOHfuDB98cDauTbfJr8Azvc3j7TA/9euXUBydlDGfCs90XIF61s4tpqPZBTPyK6iY7mq/lGbsNsJ98NaYs5tyKd22ihzif19mfgVl7W3bW4M7spEUt9vtckvZtioHW7RP4fEz/xwei5OpjFlk2+Y2AITw1hRQEDfxJTB6JVVPjccRvxTwUuMuwBiiXFZXr2Jc2/iFIe7YJ38+9JiUxiGVfQtLasxSYJ1FefVCstocZD/+gB177DmZ0rWZhmT2LTOfirLpuNr0l/D4FlHQlbTPZPqQwnmW0n0nlXtJm2sZyJxG2ROLybaDv24989fUxr2926V0LJIfs47PM+KORfbKKsrGtz1aAIT8NNfvYOma8LcSUthuqvdq64JyqmdnEax7kvlr2sn/bXPMdP9NTXj74Z/aHhsRERERERGRq4Pv9Ac4ht1sXtwlQ4cObfNM/3rXLRnAwWCQf/u3f2PTpk1UVVXxyiuv0NTUxIcffhgN3n72s5/lK1/5Stz7Lly4wM6dO3nzzTf55JNPostDoRDHjh1rE/wFcDqd3HTTTQBcunSJDz/8kKamJl555RWqqqrYtGkT//Zv/9bl4G/EmTNn9NJLr+vsdcXVH6CuoRl/KFrPEwjhb65jS1H6AaaWygIqDzXjj9lswNfIgY0bqeti2dqmygIeXruXRl+A1s2H+1z5Ylzbq0lKY3a4mI019TTHNiZEwNfI3rUPtw0+ABxbx7rn60zvMTvMmiVFbKmL70efldI4pLFvSY1ZCoI7Kd54gOaY2SYCzfVsKVrCoVOxDdvT9WszKpl9a6qkoOh56pr9MdeacV4a49uF4C9J9iEFKV1DXb2XNO2h6OkavCGwj1tO1coezgTu6WORhIaNO2kIGP8OxX1mABY7znGL2VY2JX55D1gwNgtLqJEDG9oJ/qYhpXMnpftOWFLnehr3qB5TSU1d+EYVaKT+kHm9iIiIiIiIiEirbskAbs8XvvAFpk6disViIRgMUlNTw+nTp83NAOjXrx82m41PP/20w+BtbNZwKBTilVde4eTJk+Zm3ULfGBC5PiW69ns1A1hE+qZ2syJFroz8il1Md4Vo2LiEon1GmeSI0Ss28cQkJ5Yey0gNG72a6qfGMaBhI3OL9pnXioiIiIiIiIjEUQZw7+iWDOBEPve5z3HfffdhsVj49NNP+fWvf91u8Bfg8uXLfPjhhx0GfwlnDR85coRPPvkEi8XCuHHjGDhwoLmZiIiIiMg1LJ/scP3pAbdmt859C2RkT2Ssy26UTz7V0nPBX2DWvBzs+GnYoeCviIiIiIiIiCTnr//6r7v1JW31WAD4nnvuic6h29LSwptvvmlukraTJ0/y9ttvQziqf88999CvXz9zMxERERGRa1Q9LT4AG1mzV/EvP/Pg8RivzWWPMdVlg5CPQzt6Nl19Z+FM3O75tDf1r4iIiIiIiIiI9L4eCQB//vOf56677qJfv34Eg0Fee+21NnP5WiwWRo4cyWc/+9m45bH69+/PyJEj22T4Xr58mX//93/n7Nmz9OvXjy996UuMGDEiro2IiIiIyLXrGOseX0tNvXnOeCDkp7lhL2sfzmNdT6b/ioiIiIiIiIhIn9TtcwBbLBZmzJiBw+Hg008/5fXXX+fYsfiUgNtvv53JkyczaNAgLl26xKFDh2hoaIhr88UvfpFvfetb3HDDDVy8eJHXXnuNt956i8uXW7v7xS9+kcmTJ9O/f3/Onj3Lrl27uHDhQtx2ukI1w0WuT4mu/QEDLNxyy20MGGCU2zx16k989FHHJetFRERERERERERERKSV7/QH5N77dfPiLjlz5kybZ/rXu24PAA8ePJhp06YxeLAxEdl7773Hyy+/zIULF7BYLNx77718+ctfpn///tH3nDhxgpdffjlmKzB+/Hi++tWvRn++fPkyLS0tvPLKK1y4cIH+/fszdepU7rzzzmim8csvv8z7778ft52uSBQEEpFrn659ERGR7uXxeMyL2uV2u82LREREREREROQaoQBw7+j2EtDnzp1j7969fPjhhwDcdtttPPDAA4wYMYK5c+cyatQo+vfvz6effsqnn34KwE033cSAAQPithOZPzjSrl+/fjidTubPn89XvvIV7r///mjwNxAI4PF4ujX4KyIiIiIiIiIiIiIiIiJyten2ADDA6dOn+cUvfkEgEIBwEPg73/lONCv43Llz/OIXv+D06dMAWK3WuHl+b7zxRqxWa3RbNTU1nDt3DoDPfvaz3H///dE5hgOBAHv27MHn80Xff+VYufcb92L0XERERERERERERERERESkd/VIAJhw4HbPnj3RIDDApUuXaGhoYNu2bbz77rv4/X4IB3WHDBkSbWez2aIBYL/fT3NzMz/72c/49a9/zaVLl6LtPvzwQ/bs2RMNJF9pjtmlPPqDQip+MFlBYBERERERERERERERERHpdT0WACYcBH755ZcJBALRTN3/83/+D6FQCCCatXvDDTcwbNiw6PuGDh0aLQkdafPpp59y+PBhtm3bxunTp/nwww/jsoj7At+OYqp+6cf+jSUKAouIiIiIiIiIiIiIiIhIr+s3fPjwy+aF3c1qtXLx4sVo4DfiC1/4Ag888AADBgzggw8+iJZ5vvnmmxk8eDAXL17k5Zdf5g9/+EPc+z7zmc/Qr1+/uGzgnjB06NA0Jo22MvkHFSz5hh3/LzdT8KP9BM1NkpBX4WGGy7zUxLsbd8EJSl4sZMwg4PxRyueVcDDB+4NvlDPnqYOx74b7S9j+/TGtgero+ye0brONIEf/eQ4ltL434bbj+nCC3e5HqQJY9CyeB0eGW8Qsj4jpU3S7ce8x8e7GXRC3BZEuS+/aFxERkfZ4PB7zona53W7zIhERERERERG5RvhOf0DuvV83L+6SM2fO6Jm+SY9mAEcEg8E2wV+As2fPcuHCBQgHfe+44w7uuOOO6FzBFy5c4OzZs6Z3GdnAPR38TV+Q/T8qYHMfywS2Zk1ggmnZhPvuusJ9G8mMijzzQhERERERERERERERERFJU68EgNsTDAb58MMPzYujPvzwQ4LBdPJnrzQjCFz+ig/7N5ZQ/si9KQdaqwrcuN3h10snostPvBSzPJnM1/NBIwN50F1MuD92xQQmZFmBIMHzsctNzh+lPPL73G7c7jmUvGpu1AWuGTy7yLywfXH7n+wYiPSS22+/na9+9auMGzeOe++9l3HjxvHVr36V22+/3dz0+jV6NdUeD9vKppjXXF+u5XG42vYtt5RtHg+einzzmr6pW8Y3nwqPB8+2UnLNq9KQOW01m6p34fF4Wl/dtO3el0vptpj9uKr3RURERERERERErldXNAB8+fJldu3aRUVFRcLXrl27uHy5xytU95Agr/9LIeWv+HB8uzCtIHD3snLXfTE5wPdP4K5BAO/z/hWeRnnkg8+iPGC5mvXv358vfelL3HnnnQwcOJB+/foB0K9fPwYOHMidd97Jl770Jfr3729+a2L5FfHBh/Br17YqypclCENYs5m1ehPVu2ICMNuqKF8xheyu3ngG57KsvIptu5LoRzKOraGuGWyZE1nQYd/CQZj2Ai/hMbpaYnZtJD0OV6Gk9y1BoM3jwbOrmk1lK5jS5ZO352Tnl1O96wqdf0mPb++wTiujdPE4nHaLeVWvuKLHQkREREREREREpI+6ogHga198EPiZv3eaG/SCt3nba/wrtgx0tPyz9zjHY1r3phNvHA3PjzySyU+aC1SLXD1GjBjBzTffDOHKBidPnuT48eN4vd5oFYObb76ZESNGmN6ZGovNQdbUVeyKjXRkzKK8qoyF45zYLTEBGJuDrEnLWb0yYfg0KdaJq6n+2SqmZjmwxWza6MdyStPc9NYjjYQsWUxaMdq86rpyLY9Dl/bNYseZPYnlZZspm5ZpXtsnDM7I4ArFO6Gr49vN5k3KxkYIX93zPPJQTIWOucUcNjfuAd1/LA5TPDeyH2upD5jXXz8yp5VRVbWaKcbMLCIiIiIiIiIichVRALgXBEMhwILt5iHmVb3i4PFwCeloGehI+Wc4cfwEzmFxzeMNGkNhbGbWiyVt5hJO259K2PSGERyz3rOUkrgS1YmNfDA+UyyV8tEiPeGWW25hyJAh9OvXjw8++IC33nqL9957j0AgwPvvv89bb73FBx98QL9+/RgyZAi33HKLeRPt8ta0BlPmLCli/V4vAcDimk5FvnEN5+bPIssGIV89O55eEm3/0CPrqWloxt92+vXkZORTtnwcdiDka6Bm/SPRbS95+nkOeP2ku+ng1hoaAmDPnk1Xithe7a7lcUhp3wL1rI0p7V+0voYGXwiwk71wOfkZ5jdISuPbo3LJuBUIedm3Zg8nz5nXy9UsIzsDh2McyzeXs6BvfhdDRERERERERETaoQBwj7Jy9z88Q/F3RhKsq6Bgw5vmBr3jheMYIeBwGeho+ecTHH/B3Lh3HXxqE0fPA1gZs6gbg8siveSmm27ihhtu4OLFi/zxj3/k0qVLcesvXbrEH//4Ry5evMgNN9zATTfdFLc+WcGWBmqfK6AynI52a4aR+ZdltwHQcqSYrUdaou3PnaylsmgpS9ekl4M3esF4XBbAV8e6giIqa09G17Uc2cOGgqUk2vToFZvY5fHEZym3cZjKQ81gy2RiN9ewnbKinKqYssK7tm2ibMFYczMAcpeZ2lZXsCzXnOoWniu1It8otV26yZgv1uPBs20TpQkyVJPvQ/LjYM2ewooUSnEn1Yd2y2i3X347qe1CSvtm1lBbSVHBRur9gMXF2HnZceuTO26G5PvbVmZ+Bbs8Hjy7qlg50RpXmn1VjnHduaa3btt4VRA3nNHy7PF9KJ0Vv0/GtndRPsvK2Lj920V1xTLGthnC1MbXGLPYOXqn4zI3CktlfKNCQXzmZSYpbTdB6fltm0qZFSkLns6x6CnJHuNI29JNcfsV94q95lJpm/T4pnY/q10zn6cPNBOyZTG7LHwdiIiIiIiIiIjIVUEB4B4TE/x9o4Ila/aHyx1fCVUcjykDnRdT/rnK1LKN80cpj8nMcs8r4aC5TZccpOSFcCnoQWNY+qDd3CDOiZdi+uJ28+gVDmCL3HjjjQBcvHiRc+cSp7+dO3eOixcvQkz7dFnDZZ4vhoztNfqNgLBrfFlrcKTLxjIlyw6EaKhZw5Gkb165TB/rxAJYXONZ3UF12patR2gMWcgav5wOmqVkVvkulk/KwmHEgwCw2Jxkz57XJhA0q3wbq6aa2tpdTF31EyoSpZwOyGD15jIW5jiJvsXmJGfxSlbG7EAqfSDpcchl5erlTEpYinsVVSvigzap9iFZqW43uX1rR7CWynojpOgY0RrmSuW4pdrfWJn5FZRNd2EJNXNgXQHrapO+CFpZJ1K6OVKevXWxxeYkZ2EZ1aUTY1sDFjKmb+aJuP2zYHdNZWXprPimKYxvfsWu8Jh1Xic5qfHNLW0NGnpWkWMDbDmsMgUoY79YkNR2IzLzqfhJ29LzNmcOC/Pnxba88lI8xvllpcY9pPNDkVLblMaX5O9nAEc2LKXo+Qb8FgfjH6uiXKnAIiIiIiIiItINTkxclvAl3UcB4B5hCv4+dSWDv4aqaBloO6OGRco/dxr+7R2vxpSCdo00gtMiEseaMZZpKyqYl20B/DTuOwLA4XWV1PkBezYLy7ZTvamU/IkJHvinJBuHHaAF7x7zuo4c5sAxHyEg5D3EmmPm9TGCW6ltCoBjNLO7pYZtPuOzLBBqZMcjD0W/JPLI+hoafPF3YOuscuZl2cDfSM361rLZ62sa8WPBNXF527K6zhzG2UP46nfw5ENu3HOK2OsNAQ4yJ0Uy/ZLvQ1SS4xAK+mk88DxrY7a7/kAzIcCRPZ3WXMM0+pCUNLab5L61p6W+hQCA3UFuysctjf6GtQZ/vdQULWVD5BsQlQXR7awNZ+LHlmk3XgVUhreTuzKfHDvgb2gtz/7QI9HjZs+Zx0pTkqjNbo8r575kYz1+wJI1hRXmyzqJ8bUuKGeKywKhZg7ElnEvOkCzuW1K45u81LY7mpUrp+OyRErPx4xbTQPRQ5fisegpKR3jKWVMdFkg4GVveL/mLHmaHQ1+APx1a1vnTU6hbWrjG5bU/axV054iljx9gOaQjazZZWxakVwWvYiIiIiIiIiIXDkKAHe7vhf8BeCF3eFSyyMZ6aJPlH+O1VoKWuTq8tFHHwEwYMAABg82l9s0DB48mAEDBkBM+2TEljTdvvkJFk9yYSOE79CW1uBqsJY1892s3duILwB2Zw7TH9uMJ4VSt93p8Lo8ZrrdzCzoPPSyb+MhmrGROXGBeVUaWggGAEsGOVNaAxgnayspyiuKCwRNGevCgp+69YVU1raWza6tLGRHQwhsGYw2D13IR93Gh8kr3sqxc0CwgecajPdarZHjnnwfYnU+DodZkzefwg17OBwzyWrthmO0AFittJ556fWhc+ltt/N9S15qxy29/mYuKKd0ugtLoJEdRQVUNplbJGsaU7NtgI8DTxe1lmc/d5LaDUvZ0hAwgm2mL2sEGncwM6+1nHvLvmJj33DgahPF63x85+VkYSFAQ+VSNsSWcW8IYtQQaJX0+B4uZm40yLqW+kDbeZzdbjeRW0DS2wXInc5oh7G9jQVFre3PnaS2soi8ovaOXBJiykZ3VEo5eSke4wwrNsDfsIXnwvsVbDnC1rV1NAN2R1brplNom9L4RiR1P4sXPLKBpUU7aAxYcE56guqyaeYmIiIiIiIiIiLShygA3K36aPAXgIMcbIzpTTLlnzHKMheaHpY+uyi+ifWeQtMD1WfJi2+ShJhS0B0Y+aDpwe2LJeYmIr3qww8/5JNPPmHAgAF8/vOfp3///nHr+/fvz+c//3kGDBjAJ598wocffhi3Pnkh/M311Kx9mLx1teaVHH6ukLy5bpasr6G+OQA2J9mzn2hTgrRPaXmOI40hLFnjMVUxTsM+nq6sw48N19RVxtypm8pYMc1cHHcsmQ4LYGfcU22DQYuzjXUOcxJcqIVD+0wlvsNZiHOLI5MhJ9sHkyTGwTp2AaWbqo05aaOvRPO4ptmHTqW53ST2rV0xpW8Pp3zc0ujvrRMpnZ2FLeSlpriQrWkHfwEcWC2Ar4naBNvZ4z0FgNU+Im75qaatcT8D1DZ3MLtuh+ObS8atAKfw7jOvM0t1fJOV4naz7OHA5z7Sqbrdu1I8xv6QkRWcPY/8sUZQ2JoxlvwnxuMEQsGY45x02xTHNyKp+1kifsKzGYiIiIiIiIiISB+nAHA3cswtNYK/RzdT0KeCv4aDr70d7VOfKf8c69US9ofnKha5Wvz5z3/m7NmzXL58mZtvvpmvfOUrDB8+nIEDBzJ8+HC+8pWvcPPNN3P58mXOnj3Ln//8Z/Mm2hVf0nQm85cWU3k48TzDES21lRQvnctD4dKx9px8SlNOb/MRDAFk4OrhJK+ttU0EcDB2YYL0RgCLFYd5GWANZ1THCtauYf6cIjburcfrC2F3ZjNp8VN4dlWQHw2ODcDS9q3dJrk+tNXhOOSuZvMTs8lx2mNjou1Ktw+dSXe7He5bB0aPdRnzk55qSeu4pdzfU0eo9YbA4mL8wu468UM0mBelyB6e97s9nY5vKIRROLgjqY9vctLbbuhiD/wFFVM2Ou4VKbuctiSP8c5CDjQDtiymP7EZT7iyw/QsG4S87NsSU28/6bbpjW86rGNXsKlsMdn2EM0HnmZ+UUrzA4iIiIiIiIiISC9TALgb+bYVs/nHmyko8STxsDUFLzwafVD5aJuyzQcpmRd+iDmvhIPhpVUFbZfxaglz2mwn0ftjliV4PfpC/Lbavh6lKrYP4Z+hs32JfY+bOU+Fex7znjavecoAlivv5MmTfPDBBwBYrVZcLhdf/epXcblcWK3GrNYffPABJ0+2lmDtaef2FVPXDGDDHlNZNDl7aPSGAAuZU5aZV3avfUUc8YEtcyILEk0AbnGQmSBpc5YrUVjYKGW677liCvLm4p5TxJYGP1hcTMmfFW5wmJZTGGVblyS4p4RfSVSwbl+nfUigg3GYNjUHOxBqPsD6mPls3e4a2v3OTAp9sN8aXx82c9pUXLa4Ra1S2G5UB/vWrsx8FubYgRCN9S+mf9xS6m+QyoKZ1HhD2LMXdzF73k8oBDgyWWaeuxeY5roVgFMtHU2UbZiW6QBCxCaIxml3fM8RDAIWOxmmPmTmZxO/KM3x7VSK2/UFjXmtM7sy9r0lxWOcu5pxTggF/ARCkVYhAs31bCkuii83nnTbFMc3TZnTytj8xCSclgCNO4pYusGYg15ERERERERERPouBYC7VZD9v+jm4K+I9HmXLl3it7/9Le+88w4XLlzg8uXLAFy+fJkLFy7wzjvv8Nvf/pZLly6Z39pFuazetInS/Ilkj2idt9Gakc3E/HLGOQF8tKTxrH5rTQMBwOKcyq6qUhbktpaqHZE7jRUVm1idILN49IpN7PJ42FWRb17VrspDjYQsWYxdEBtFOUxDS8gobfpYGQtGh/dv8AgmrtjE9CwL0ExjpLRt7mo2VZWzYlou0aEINlBf12Lsh8Ue2TD7GpsBB5PKysmfaK6N2gUp9CGRxOMADquRARo610RteA7gERPzKd00sW0J6FT6EC0zO4tZ2UbkcOKyCkoXZ9Omp6lsN4H29s3MOHfLqCqbjssC+Oup2Wpkg6Z03LrQ38qijdT7wZ7zWLtB4HNBo0+u8THnZpydNHhDgJOpZWUsCJfxZfBoFpRWsTDbBqFG6l+Mz3S12nPJzjCOhTVjIvnl1Ux1AoEG9naQcJl4fBtoOGXMQzt+9QpyB7f+/rLprjbZ5CmNbwpS2m5tPd4Q4JjEtooVTIuMGzB2QSlVZW3vK50fi56S2jHOnZSNnQBNO9exprgoHJydydylxexsiD8PUmmb0vimIXtZBWWLs7GHfBxan0dh12qji4iIiIiIiIhIL+k3fPhwI1IhbQwdOpQzZ86YF4vINe6KX/v5FXimu/DWdJa5lUvptlXktJetCfjr1zO/uO2cwcmYuLKK5eMdbQJFhgD1a+cSP11kbH/81D05nzWdJzgCUyjbtpxsGtg4t4jodKWZ+VREAoFthPDWFFEQSYXLLWXbqhyjZHAbIbw1BRRUtoR/zmV19SrGtRcDDNSzNloWNp8Kz3RcccvakVIfEkk8Dhn5FVQkCNhFxfYtlT5YZ1FevZCsNhv24w/YsZPmdhNKtG+dnL+BRnbEzcWbwnFLpb+Rtt4a3JELLnMaZU8sJtsO/rr1zF9juoZGr6TqqfEJypN7qXEXUEmK52/4mk/MT/36JRR3OCluovHtoJ9+L80DXDhjj3Eq4xsVPoZx2zFLbbuZ+RUJA9QAxB6jiPb2MfZYpKLDY0Haxzh7ZRVl49v2EoCQn+b6HSxdY0T5U2mb2vimcD8DJq6u5rFx9gTXYno8Ho95Ubvcbrd5kYiIiIiIiIhcI3ynP+D2//Y/zYsBGFn7nHlRUs6cOXNln+n3QcoAFhG5ah1m/cYa6r2+mDKhGKVCfY0c2FiUdvAXoHZdHg+v3UtDs5/YzYf8zdTXbDQFfwEOc+CYjxAQ8h5KMvgLsI8tRg1bJsbWsG2qpKh4C3UJfn/dluLW4BnA4WI21tTT7I9rScDXyN61D5uCk4dZs6SILXXNxDXvqpT6kEjicWipLKDyUHxfjeO7kTpzWeBU+hDcSfHGAzTHlK0INNezpWgJh061LoMUt5tQ4n1rK0TA56W+Zj3uueaAUwrHrav9bdpD0dM1eENgH7ecqpWmTOBj61j3fJ1p+yZNlRQUPd/m/G3tQ2fRtBD+5jq2FHUW/KX98T22jsc31tEciCwI0Fy/haIlOzAf4pTGNyWpbbepsoCH1+6l0ReIGbfwWFS+GNcWkjwWPSWFY9ywcScN4eMQCpn6arHjHLeYbWXGPM6ptE11fFPR0tCCz1fHxiXma1FEREREREREpGvG3Xlrwpd0H2UAd+CKZwGKyBWha/8KsC6gvHo2Wb69uJem9y2va8K1PA7X8r51VdJZ/x3Q+PZp+RW7mO4K0bBxCUX7jFLuEaNXbOKJSU4s4czcrBTatvkeTh+mDGARERERERERIZwB/MiytlN9AfzHf/yHeVFSlAHcljKARUTkygtupbYpAM7xlCaYW/i6cS2Pw7W8b32BxrcPyyc7XCd6wK3ZrfNSAxnZExnrshslr0+1cDiltiIiIiIiIiIiIokpA7gDygIUuT7p2heRXtUdGcDSh41mZdVTtDetLwAhH4fW57HucCptzSv6NmUAi4iIiIiIiAjKAO41ygAWEREREekxx1j3+Fpq6pvxm+f0DflpbtjL2ocjAd1U2oqIiIiIiIiIiCSmDOAOKAtQ5Pqka19ERKR7KQNYRERERERERFAGcK/p9+Uvf1kBYBERERERERERERERERGRa4BKQIuIiIiIiIiIiIiIiIiIXCP68Y9vXTMZwMO3TDIvEhERERERERGRa4zri18yL7pqeX/3W/MiEREREZEuUQawiIiIiIiIiIiIiIiIiMg1QgFgEREREREREREREREREZFrhALAIiIiIiIiIiIiIiIiIiLXCAWA5apgHbeEZ6t34fF48NRsZ9OTM8gyNxIRERERERERERERERG5zvXjH9+6bF7YG0aMzaD8lnN89xcB86q0Dd8yybxIrgV35PHs+hmM/MsJXv/l25y138U37xtJ6I0Kljy1n6C5vVzV7GNmMHPSGEY5hmAbZiF0OkDQf4Jfvb4bz4HmPnS8ncxZXci9vE75mu00m1eLiIiIiIhIj3F98UvmRV10E1/6xkTGj7qDoYMHccPH5/novJ//OPa/OPzGKT4yN+9G3t/91rxIREREuqj1ObPNWHDRz/GXn6Xql37s38jj0QdGYR9grAr4jnP0wC52H/XHbeNKsmbcy+Rpk/nbL9oxunkR/7u/4vWdHva39J2n5BJhxTnJzfxv3IvjFhu2SwH8vrf5v3u3X7Hz6ooEgEeMdVL7wCDsfzjF/ZV/5tfmBmnqUgDY6uTeb01mlCN8xScr1MLB/+mh0bxcuo3zkSo2fdPP9vmFVIfva1krqiifFGC3+1GqzG+Qq5L9G0soWeRmpB34i5/m5rOEACw2ht/mwGoBzp/A8+MSNv/yytww49xfwvbvj8FKkKP/PIeSV80NREREREREpKd0ZwB40OgHWTLzXjKswCcfcebPZ/mo/yAcQ25iwA3Ah++y/6c/wfP7ngkDKwAsIpI6+xcnM/leeH3rflNihpPJC+6FWgXJrl9ZzF9XypwvWc0rgBC+d/3Y73BgMa8Cgr/dTvHK6isb77HezfziQuZ8yQ6Xgvha3icQCj8nz3Bg7Q/B33l49onNvK5TvG8Y5uaHZQ9z722W1thGHzhevR4A7qngL10JAFsnU7K5gDF284rknPg3N4/+T/PSxPIqPMxwAZy4zoKXeTzrmcHwN8qZ89RB88oOTXhyO4VZb1M+r4ToOxc9i+dBrrMxvFZZmfyDCpZ8w8HF33mo+qfqBH+cWXFOmk/hw25GDgpx4hel/PDHb17BbOAsCirLmczrvM693Mt+CvMrruwfBiIiIiIiIteR7goAj3jwUf7rNz7PgOAfObzrJ+w49mHM2htx3PNtFjx4LxkDznJ0x7P89I3uDwIrAJy6CU9up/Ce9/VcSOS61Pos0XL+aPwzYwAmUPJiIWMGhWh+pZzCf3n9Cj5D7ArjeTovuXn0BfO6zoTH4PRu3AXX311yzA+qKPmGAy4FaT7+Jm+2nMD7Drj+ZgKT73GGA78hmt/Yz8F/98KdLkZm3M3do5xY+4PvlyXk/eioebO9I2s+5aVzyOrv4+j2Cn60w/wM3Mrds39AwZwxOC41sr24kGo9lL6yIvHFG5vZv/kZquKqmNoZ89CjLJ05Bsf516lY/gz7e/GG1KsB4J4M/tKVAPDfP4vnuyMBOJHSDTW1m3BehYcZwxJ9KF0P0g8AM3UN25f9Fc3biin8WSNY72bJumLc1qOULHyG6K04az7lq+eQFQ7kB1uOsm1DCbv7xA2wC/vfRdZxSyhd9E2yHOFvPIX8nDhQRclzB7nyebRWJj+5mYJ7rEkGdbOYX17KnKwBnHjphzz6QrIH1xh/4yoHEv5xmDzr3HKqH3Ly9gsP8ww/5CeL7qL5Z/Mp3NZx7zti/M9r67fSUrsXiYiIiIiIXF+6JQD85e9RvOhrDPrj6/x440v8Z3ux3Rvv4f8pfJAxN77DS//9eV5tr12a0gsA9+ZzhgmUvLgUXuhq9SvT/5tHeFMPUKQVAF70LJ5Rx1P+Xd0j0b5fjxXFIoG5Xk6MCVdxe7+9Zy33l7D9+3fx9j/PoYRIxbf2BSPX3aJn8TzY5oxOMfHHdG6kcT10VefXU6Lz13BFnl/dsYRNG93Yjm6moMTTzvNNK/euqKBwUoj9y5ey+V3z+iRFjnESzxIjz/ai50eXpRZ7iHc9B4Aj95kgb77wMKtfin1eG1mX+Pmw9cE1/GTR3VgTrOsVkUAiR6lYUsL+oFHGev70CYy0wUX/2xx8qRrP8SAMc1OyfgljeJ3y+c+k3Ffzs+iI7jt/O7+3dLb+6mBlTnk1813N7P7ho1S1E66wjlpCeYmbIY1VPPzD3Z3EQLrPZ8wLekpPB3+7pH/8j/f+oIpdlYXcG7+4i/IY5YJg48GUL8buMuHJ7XheLGGCeUVft7caTyNkzS1n185d7HpxDe6MIK//7NnW4C8TKHlyDlmWE+x/oZyKf3uTwK1jyPtBIWPiNnZ9sU4qYfNqN65Pf4/nhXJW/0s1r/8enFMLqfjvM3Ca39DLrJN+QN49Vpp/8UMe7TT4C9BIdWExu70wcupS8u4wr0+k9X+K3W43bnc5RxlDYdrXwhiWfisLvPvZ/FKQ4Eub2e+FrG8tTftca/2wcxt9fOkEIx/08Owic0sRERERERHpHrfy4JRshn7yLq/EBX//igcXP8qS7/xVa9OP3uCnP30D34C/4v7/ktW6/HpwfwnbPeGH5V2QV+HBEw5kGP9vHn7989EkngV0XV6Fp51AXS9Y9GzCfd/tNTe8Diya0eVzqce9WsKcmONU/kYwHNBtXRYfHAly9J9N53XSwYxwYNW7u/WZ1bAZffb5bTD6bK31lXpgsht86y6cf3mTXe0GfwGCvL7Bw9t/cXLXt8zr0jBoDDM6fE6Xx4wEwTS5EkZiHwTwPt644G/ngi95eR9gkD3hFx562oTH8xhjPcHuNSXsD2Yxf912qkvymPxlJ06nE1eOmyXPVFP1g8lYT3soWeOh2Xov83+QwlPp+0vY7vEYFVdN17P7pRNYh12JPb+K3fMo7ixo3PXDdoO/AMHjm3n2//iwjprM/KRiGt2jWwPAX8uxM2+oeWkfD/4mEDzdTPMf/b3yB6gko5HqwodZumE/PiwEf1NNxfIlPHMg5gg9+C1GDfLz+j89SsVLB9n/P1dT8P81EnLczeT7Yrd1pVTxaJs/EHuCFeekOSz5hyUs+YdCnskfg9W7mx/mr2bzSwd585XtPLNyPj986QTWr83n0blX8g+TMSz93his7x3k2R+H747We5kwLlGfrNz7jXvD375spOq5g/gsI5m8yG1u2MaEJycz8vxRNkXH/iAlLxwl2Okfbok5F83nXkeQ4y9VhecXaabqpeMEHfcyf1E6IXXjD8QTL8X8z8ELjxpB7vv75h/8IiIiIiIiV73bxnP352/g/Fu17I/L6L2J4V/4PCMcN8UuhHdfYvdbHzIoczy58WuuUXk86/Hg6SQTMhkTntzODJcRQGsTLHq1hDk9mJ024cnteDyR6diuhAmU3D8SvLvb7HtVwXWY/Xu/AguxJjw5mZGcYHf0GujaM6vrSuhiB8HfCD8XQ+Zl6QgSPA8jR+WZV7RaNIqR4XbSlzmwfS78z8/ZcJjWXllzcH/Viv+NaqoaYcLq1cz50gBO/GI1c2bOZOasmcycPp/yAz7s31jCM4uyoHEzVW/4cYyZQedPyTE+278/Bt4ox50ow/mFR3s1Y/zgU3NS+MJM33T3N0ZiD3n51c86jyY2/uR1TuDk69PSiSGkpxsDwLdQ7r6dqgUZbYLAU79kZcSnF9i4r+8HfwF+/79385Nd+/m9eYVcQUGaDxzHF4Kz3u1t54i127AQ4OxvWhcF/QEuYsGSaDb3a1HWDNZs2c6mFfNxT52M+zsTGGltZv8/VbWZm7bxhXIOvmfB9TfzGTnMtLK3TJ3B1x0hGn/Z2r/Jjz9K4Q8qKJwU/7+XWYueofAHj/LD74Q/lhsr8BwPYf3yBObEtTSbwIQsa9vM+1cP8nZnf7gl5GbJt0ZC4y5+9KoV56jw3BCv/ohdjTDyW0uS/LCNsWgUIznBcfP/CB4/AYPuYsL98ctFRERERESkG4z5PEP5iJa3zf/H3L7fvv1HPrpxCCMyzWuuQfc7GR7JbOxKlu79JSw1f+m5F40cZjVK6l6xjFsjEy14+oR5xfVn0QzGcJTdb6R9Nl1zRg6zwnk/cWfHq81GBqL0KW83ngDXZEoSPqczvtwQfONt3u/rGe7XFRtWU6Zl1j9MwBWJFVhcTPgHU1WPO6zY4pf0ngdH4bL4ePOVo2DNY8Y4O8E3KsJVM604v+jEip+DG5byzGtBRk5dxBzg6Gtv47f+FWOSmB01r2KGKVFKusp+ow3+EsBnXpFI8AT+82Cz996XoboxAPxnJv78LG/fdHObIPDGmj+z96MbWb3wTlZnxL6nb/r6wz9kzT/m8XXzijQZ3zY05kmw3lOIx+Nh+5MTot+mfHZRpBSOB09FbEAq/G3LmJfxvhj3l7Dds52S+2O24fHg8TxLdEuRtP57rDBoDIUeD57we+K3E/N+U6mR1vLRpj7F9bdVfF96oZTtq2/TjJO//YEbOxjzBD84Cmuombf/3dy4rbyK8L4sejam35Ex6nyfI98obfveCGMbsccv+jtNY9/mGCfDOpmS1XncbWtm/4/m454+E7fbzfwlz1CdcI6LZo43B7F80c2zWzxs31zCjF6uYjVhzF9hNX07Zv8/Pcv+U3YmLHuGJaOMIHDWomd55sGRBOuqeOYXrbfS3ce9hCwuRj0YXdTW/RO4axC8/yfzh9pBmk8Dw5wpZdhmPTKDu60+Dr6wnSBfJ+8f14TvFUG2v3AQn/VuZjyS2kDmjRrZ9o99AK+fIFbsV+xbyiIiIiIiItew/gAfcqYh/PODj1Kxfh0V67/Hl6xw45e/F/65lCWRyoqfAtzIQFNycF/VpecOr5Ywx931DNUJ992F9fxRdpszfzsS92wm0TOW5FUVuHs1m6mtKo57wXrPjNbndAm1PiM0P2NKdLzMbdobo7btYp4X0vnzQGO+zNj3x/Yn/LwswXOytvJ49sGRnHi1pO3zj+vYidPBtqVmw1++8F+RLyxcHcYMGwKXQnSe3BsidAmGDEuhPG57XjvOCazcdV/b69EobR7k7deMWoFmba/DRM/lt1Nyf+v1lui6h9hrNv5aNv+O7U+2H2Ayt43fVrgP5us6fF+Of8ZvtI30tUufOd3q/3LiPQAHk8s2seYfl7DkH37Ims3VlH/HiYUQPq+PEBac3ymnevMafvgPS1jyj2vYVDbZyAp+7wT/17zZnjbMhuUv73Pi18B37sKJj1/94mB0jtlN6zdRvT4PJ3D0lTfxWZzcdT/wmo+zWLHfad6gmTFF6YlXE2T+dqLjcyZ9xnbD2wqfN4niSHkV5s8nc9yse/qTttPNSY7pr3i/89IF3aobA8DA2+8xOlEQ+MwZHqj0sfeTgTx9FQSBf/WTZ1j9/1bxK/OKNBmp7Ls5ETNXQmwp4OH3b2fU8XCd9cgfpeH5QVrnLTW+cck9hW1vwFgZ831P6zbc5Rw9P5IZkYsiPHdF+RtBY3Jztxt37B/xi57F8/0xvB+di6SdOVIHjaHQM4rjMf0JumaYbuLGjX/GsMjvceN274YHjQB4j3l3M8++dALrmCVU7wrPE+y6SOOuF9ie7BcLXTPwjDoeM4ZWxizaznbPZPyRuTwS7nMeM0w183d7rYz5fhI3HtcMPItgU2yd/XsKE97oOuJcMIMxdh8H1y2l4petdxF/S3P4W7pZ5K3fzq4XnyUvHJ/81U+eYfV/W035tqMEho0h75ly5nS1rlMKRg6zwpk/8HrswuDrVDy+mYN+J+6SZyhYEQ7+vlHBkjX7479xXPcH/FgY4uis04n/aD5xOtkTI8w6h0XfdBA87klcz7+xCs/xII5vLkp9HBN9SOgbnyIiIiIiIj3nEsBNDP1y+OeDO/kfm5/nf2x+hf8Mwke/fyX8czW7I9XGPgPwER/8MbqVvq+bnjukx6jKlfD/edthzNU7PG5O1fI3YMz3Ez8UvhpUFezmBCOZkUQgZPj921nKptZngeHjlc5zqLwKD4X3EDeWcVnQnT4PnEDJi4WMOR2Zn9Z4LpbOs4q8CmOeW3MZ7Ovdwaf2G+dG9FnvBEoWjcHq3d/lL19ck4aNZMJDJSy9x47v+P74Z4oJvc7+4z7s9z3KmocmdLEKYhW73wgm/DJH3qiR0O4xS+56Bbhr0VJ4wWiTcBrB+0vY/n1jur/YsrnGtf5+zDzV5bydlWi+beO5fXxbN7u9I5kRDUof5GBjEFyj4gPMtw8HTNUU75/AXYOCvP1aTF+v6GeOwTrqbxlpD/8wyMnd97lxf+de7s6wAyF8r/2EwoJCfvKajxBgz7ibe7/jxn3f3TgjY2Yfyd+Gk5N6VaS0+Y0DsBAi8J8Af4XTbqQtWwbZGQLwaz+B+Hd2LlymPNFz8vYlc850k3YrdhqB62iFz/tL2G6Kmxn9aXtN9T1BLl4yL+tZ3RsAJtkg8AjK7zK9rw8ZkjWKcV+7y7iYeoH19H7TH0CRshHl8Tf7V0uY81LichPBN8pjtnGQkleTLR+baC6S9uabCHL0n2NK9rxawn4vWLMmtAaKF81gzKAT7I6rIV/Fo10pF5SkxhceZf6a1/FbLPh/U03Fkocp/FmiSF17THNuvHoCBlnhjU2tH+CJ9pkqHjXVzK966ShBhuPsdPxNY/XCbo4mvNF1bPIXnfDem2x/w7yGcPD3GWZ80Ypl0EhmPG0EgYMtb/Lmr9/k4M9KyFt3EJ8li8nL7ja/uWd9FAzPoxsjuJ/ygs0c/ctIJk8aycVfb6bgKVPwF+DdIAFgiKMLufrmb1l2YMwjbrI4wf4f727bFwCC7P7xfk6QhfuRbvhmYdjw2zv+n0MRERERERFJw3+e4gw34nDdavx87o/8Z9Pv+c+ms3wC8PHZ8M+/xxeeI/hLd32eG4On+N17sRvq67rnuUOvuL+Eya4gR/85PvP44FNz2O2Fkfebs1OvFlU8Gg6+xlcGbMt6en/8s8AXHqW8TdApiedQi55lRoKxrCqIPNdL5nmgUb76xPGYDOpXS3g02j9jvzrNsF70rDEHdGftrlpGYk5cdlyb5J32VPGoezcnXDPC7w0H3PvoWEXO3yuWdfdgAYVzx+AIvk71j46a1yZ09EfVvO63c/fcQgo6qiKYhEjAfnLs9Xt/CZNdpuskThLXKwBWaIx5Bm0WG/yNPT+i983YMvsHKZlnJKPFiTy3N825WlUQToR60DiaB197myAjGRWNCxhf5jnhPRFXTdGo8PA2B+P6fGU/c6yTStj8zAxGfg6gmdd/5sHzi/3sP+DB829VPLNkPnn/rwc/fjz/bx7zlzxD1b958BzYz/5fePD87HXjWfXnRjLjmc2UmKYp7FGXgEEOsqzAqyfw4eCvZliBN9n07GY8BzxsfnYTbwLWh+7Cyfs0/3ukbHWIiylHhMPMVTdikwKTPGe6R+IvH0SmT9wf/uzJe3AMVlMZ68gXreKuTYEeCQCTTBD4Rh7/bt8NAju/NoHJ942it6ZibjMPSKJvz0S8kKjcRIK2yZaPDf+uoy+ZPqTC2Ydxwac2N/S2pUqMbzwdbzuvS7dnM9oZ+bW7uTvmNfnv11Dx+L3Y/a9T/cME8wR3xtxvr58gicoHtyP2Zvn9MViTGX/z70yzNDH92wmmRoO/F/H5QvAXH75LrUHgqDf+N2/7wOHsvsBlUvoPINHHaNbffYORg4wPPutd32JmB1WVA/42f84kL1Hp5UTuyGP+PXaC/7GbqoQltcPerWL3fwSx3zOfPNMcE+lK+vwTERERERGR5DXV8ttTMPSrD3L/jbErLnLho0+48PHF2IVw43juz7yJ8797neTCDn1Edz136AWJgwmGquPJJjr0XVUFrVm41oQV/hIHkQ7+6X1oEyzq+DmUMd1U4rGEZJ8HGnMVjnywC1le95ew/cGRV2wO6N4Rnis7JjuuNUBnLlNqDq48iye28qDbTfnpyW1LBPcRkcqWra9ePq4vVVC+7U389nuZ/4PknmGO+cF87rX6OLqtnIqXzGtTFS7pHpMYlHSZ+w6u14j2nwHm8Wyi4G+H903j+o3V7nN7c+AtnIkZjQvcP4G7Bp3g+Et+gjH34ZHDElR4aLP93vzMuZul3xtjTA8JRrbvts1s/nEFFRs2s/nnRxPM0+rj6M83s3lDBRU/3szmbUZWsMHOmO8tpdfSpWKDvu9Wsb8R7MOckJXHM//4MJPvm8zD//gMeVngHGaHxtfZFgTrt0bioJm3f2HeYJJeeLT1/mOaoz3pc6abJPqSRXwf2itjbZzv1mHJpnp1n5H2RNGNjlmvzjmATcJB4JM338zG6TG5tLFB4OnObj1BusvrP8pjZn55EmUkukebm7vLnjAo1iNcdqyJvqkWnrM4NRNwdqmURnJsf11C1c5qnv3va1gT8yr47t1Ymj2UP/ZM0qWFukVkXoMHaS2F0AsZz7FOnA5Cxl3MN5841s8ygCCN24qpfvcihJqpLt5Oo/8iIUtsYzu2GyEUSverQql72+eH2/4Kt2m5fWoJq//+bjheReG8Co5+NJIZpeXMNweBJzkZToj3m9uGveO1/YOKyB8pSXIvmsxIGtn1T52fWQf/aReNjGTyIvOedSDRH0H3OzGKq4iIiIiIiEj3O4WntpGPbvwrHljuZkR0+Vv8dM0PKa1+K6btHTy4/O/46wF/5Oj+VCqNXe9Se/Cfyv+nX82qCoyyqLhmpFcWtdPnUOHnc+bATKykngcepGRepFytsb69zOXEIuWMr+fSz+Es6dhXNDvSmBc5GFt5EDj41KYeyKy7Rpw+wcGfrebZ1/w4Rk3mXvP6Nu5l8igH/jc2UfKzg5w4bV6fuqqXYrPk85hxjzVBMCpGp9drRPuleUc+OIORcZUrY9Ylfd9M5bm9EdyLBLon3HcXVu9xql49yNvnI4lp4UBcgi+tXDljcDrMyyLuprBiE89urqDwa+FFXyukYvOzbKoobD/I63CS3FcNusG7u3ndC1nfXMoYgmwvfoZNv2zk3u9OYOQgC5bPWbAMGsmE795L4y838UzxdoKMYem4kYQaj7Kt7UkVL9mEwahUzpnuYvqShTnDPvy8fOSD5s+uwgQlz3uDE6stxZjKJcBm7bXk054LAGPh8XGDuOszn/D6700DcOYMD1T+kf9fTXOCbw9IJPO0V3j9BBN9Uy38SjjfQLvCf9j3MMeXxmBr9lDxw6XMMfV3/mObOdgLfWjV+sdsr3/rLcbBnxulh2eULeHu2M/94Jtsfmx+fCnsxmoK8wupPt56lmUtmsGoQSG8Rz2t7XrY67/+A0GLi68/1Nph66QSKpaNwfq73az54W4ag/spWVPFm6Es5qwuwR3zoeP+xl1YQ14a/3frsjYSZbJDcv8zFJFVwIyvWfHVbTPNJ238j1DrH+5hwe1sq/Nh/doMCsxB6wTMWfRRLjvWDv74ExERERERka756I1/5cW6U/D58fzXlbMYM9jcAm78q4ks+W//wP2fv4GL5/7IyXPmFtKRVDJ3T5zutadhV17KZVHfp/lVknwOlcTzuRSeB0YylyNzeSbKXE5oUXgO0mh5Y+NVeI8VwnMiJ72trmr3+VCYy441Osa9JBzIaJMYFMmsS/KLE9ejo6fPQn8LxqyoHbFg6Q9nT3dj3YaYeUonPDmZkZzgeLtfcEjmeu3ciZfKOXo+8Rynyd83k7gvxDj4p/fD9+5w+efjVa2B4WEjo2V529/3vsZIfgIbtkiKsN2GDeBGW0zW8JXUTNXPXsfnmMCjT07GGjzK0V+DpX/8mW7pb4FfH+Vo0MrkJx9lgsPHwReqO48ntTvHbntSO2e6S+zfDW0y7MP38hPRuetNrwRfkuhZ9/KFoeB/N/lU0qN/8sHQLyTxBZbu0UMBYAuPPzyC8hGw93+f5IFDrYnzUWc+4MW3zQuvvOHjnuXZ9cm+7u2ZDL1Xm3m/TZnnsPBk3W1KPqero9+VhhOn20n9XzSqbYArJXYm/P23cH4OCDbi+Z/V7D/e3PmN7QqZcN9dvZfFDdBYxQ+fO0rQ5WbNi9VsijtPS8iLfLMJgLvJK2ldv6lqO+UPjuRi425e6PSrQt1o7//m7fMWsqb+IPoHrXO4DX63mx8+VkU0ZN24m9VrdnMCOxm3h0f1jjy+9WUrwd8cpLrDLrctzQKR0iXJfEvNypxFE3AE38TznPmPxfA4luS1+ZbY0ec8vBl0MGHRnE7Pg7bzahg6LdckIiIiIiIiXfQRb/58Iz8+8C6fOO7h/ylex9r/VsjK7z/Kyu8/yuqnnmHt8m/zJet53nz1Dc4Ovof/p/B7jIsrGS0demG3kc24qPP5e1sDDuY11+7/I5unhUv0YN7Y946nsDI/h2r3+VxEOs8Dw/MRJx2YjCkrGvsySoyeMLIhe+1hfTvPh8LaL3Pag9oNShsBt6SSFuQKOEjJqyfANZmlWVaCb+xO+bwxX6+dO0jJvMRB4Hbvm+Fnn7Havy+Ez7nYayA8DaX9vnD553AA7uCf3gfXKEpuH97718z14I1yfvTSCaz3FLD5v8+JT/SKZb2bOf99MwX3WDnx0o+oSKo4SeTcTb76RErnTHcJ/91w1315TMiyEmw8GHMvDE9NkOCz8oqY+3VclmZ+taezCqWt3vzlCfwWF1+fa17TM3ogABwO/o6EV9sL/vZVoRADbnbidCb76qlSzVU8Gv5WXVxplfC8GebSIMlK/IFQxe43gvz/2XvzOMuK8nz8qXNuLzM9OzMMwyK7siiIIu6Ke6K4oEbc0CQIiiCYgBpNoqgx3/wQNyQRjcYdxCUYcYnEIKKCLCogsjMswzIzzN5733tO/f6oeqqeU31u9+2eHhZz3/7cPnWq3nq3et+qOlVnGTji9CTwj8QZZ08/OU+B72k/Wr9n4V9pMns4AMed/SWc/ppDsWDzOmzuOQDH/PN/4GOv2jHWnxn4O2G0I3z+GTjxiIdetuGfnYF3fOBcXHz9JmB51Verr6IfwNLdYtmC5hpc/tW/x1+f/vW46fqQwKX40v/cgYlFh+O4D74YAwBu/sbpOFY3fwk3fwmnHnsqzr1+2PnDaS9zH3//4vRPLPPVLCeGWJrBK4iOOBVHHQDc8T/n4sJJG83ejrvV9APDF+Lc/7kDOOAonHpEWpjAJWfg4tXAvq+SCdzbPoOj9xnGNV+c4hUyXehCF7rQhS50oQtd6EIXutCFOYBR3Pqjf8X7Pvof+P5Vt2MbFmLlziuxcudlaAzdhet+cj7+4e/+BV+66Lv45Hd+j22LDsNru5vADp5/Bi6Y9lull+KMN16IOxYdjtNrnl7D2z4TnwL94qn+dcNVmkd+8IJH8TXycfhMjd7HnX06Dl90By5O37yXLMw73fV7h52tQ7nXCE/eLDrubJ53sh54HD5TeUI33Zj037d9qJ7i3U7g+tDpibzBv9LvIe9wYBucmPj7iTi8o4cW/o9Db08HT20uRc/0jwnPHPwG1cCi6R7S6ixeOwPflyKJa95k87ca637tM5w7aN8vuP6o+oppd9PELgf41z8z+4vX4w7sggPDU8GPJPgWLpU3XlbhUlx6zRpsvvdqXH6lz7ryclx972asuUY3GKswfP2l+FaauYPh5i+eig98+RpMHHwMXvci4I41a+W7xMNYc+sdwIteh2MOnsA1X/4ATv3ipJX09uBv5Nn3VfWv9E9fKT4zn5kr8E+aH3F0zTgZN7FT+eP49lDBAI49fB/0rluDm5cdikMP6/DXvAl3bO7FPocfOylGdwTM8QZwL047fh+3+fvTO/GCR9PmL9bgh8e+Gq9+7Ux+P5ry7rvtgi+eiqM+eQ1wxOmVD8Sv/f5MX8ssEAaEH+KHMkG/9CPH4Kjv35G8O/10LL1+NhPrL+HUozixJ61DcP1RF87aVnu881QcvU8T13z6GBxz3HE49tWn48LVPTj0dfHJ0YcTvnQK78Dy+r4N+Fzttxx2PAxf/0Oc/Y+n4sSKLx+Hs36lWJfjrONj+bHvOB3//J3rHhZ513z5Azj3qs1YesQpOPejR2PaNyYPHIpjz/owjt6niZu/fRa+dHeKUAOXnIFjKrF0Og7fcGEHd5nugePefDiWbrseF36x7i4eb8c23wtf88ULcf22pTj8zcdN+07/L51yFC5cLT70ql1wzSePmdWNHl3oQhe60IUudKELXehCF7rQhVnAlptxyflfwMc++iGc9ncfwGl/9yF8+Mwv4EsX/x7bPMroVefjzEfYJvCArhvx9xBtyLlXM3byVK77DupZV+0Sr3vD9e++lU2EL51yFM66CpVv055+xFpceNSj+RpZrvf97+jl1+CsmlfC3vH9s7D5+ao7cM0nj6rcwN7ZOhS/31vlfTTiRk5H64GV1zd3up7yCIVLzsAxR12IO9JXUh9wE856mPzLtcHaGn+vtvlDA5P9VNePH1HwPzdhTf+BOOrdz5hiA2Upjjrj1Ti0fw1umurzcbMC/5ru1RdP6zedxWun4NfdfVu5mzf06WC224nAF8/CNRy8ArTpF9r0R1+6/g4MLEo3er+E61e7ze9H3mfrhnHhBz6EC26kdffF0ed9Dmf81YuxxwBw6SdPxLHvOAsXs3j4Ypz1jmNx4icvBQb2wIv/6gx87rz4HfThGy/Ahz5w4Szbavvg5u+dgeNO+GdcgWdg4ssX4nq25bab8MNvTeAZuAL/fMJxOON7M9j89XDpR47BUUddiLU184fJN1vNzGfqYeZ9i3tjJuqfMK7bN/vhD/HiDTN/Gn/7YBl6cwArn4HTP/oxfKzj33E4fCmAvBfLUpI7AAz+7gabZs4O/ObvPsAlP1n9sGz+7vKVF6ZZncHbPuM/xO6c9sgPXuC/R+Fg+Kqz2my6HofP/PBo4PsPx6D8fweO/OAFbjKm31pN2qwL00OtHR8RcACO/ue/x3GHLAW23YEf/sdZ+PrP0td7D2CPFx6L0//6KOy7aBg3f+tD1e8a7wg46BR86cwXY2WaP2NYh4vfexzOvjHN70IXutCFLnShC13oQhe60IUuzBb22f+gNOshg3lHvAHv/YvDsNPQDTj/zK/hitEUY2aw+rZH5wXjcWf/EC/e0G7NrAszg+4aYxe60DkM4BnvOgunv2QP9G67pmat80iccd7pOHzRBNb89Cyc/tnLH5ZNvC48XDCAQ//iPTjlmMOxst9nFRMY3rAOt992HdZsbmLdXZuwbK+V6Fm6Bw7dfz+sXD7gNvMAYGwdrrngbHz8YXpgajLQnwHU+nsXHklwzFn/iWMXX4rTjz8bN+NwfOArZ+Dw+7+EV3/gwhT1IYE53ABegC++exX2/t3dD8vmL7ZnA/iI0/GlDx6JlZvX4NJvn4hrDqvZAL5oX5zxlkOSV0sswC77r8Ta7uRsh8Kh7/kSPvb0CfzwAyfiXL/nd/jffR1nHLEOX3/16bggrdCFWtjjhcfiZbutw4++ejHqnmd9eCEZmCeGse6BtRiaANC7ALvsvhIDOTDxwDW44LMfxwVtX+cxlzCAZ/zFsThke2/F2XQ9vv6d7kSzC13oQhe60IUudKELXehCF+YSHs4NYACYd8Rb8PfHPB6Ltt2Ar334a7gmRZgBPDo3gI/DZ354CK7v3pg/R9DdAO5CF2YKA7s/Ay9++gJc8510rXMPvPgvDsfQFRfj8nu7K3L/d2EpjvyrU3HM8w/HHtO/LxzYvAbXXHIBPvPlS7E5LXtYobsB/GiCgReegXPffTgGNqzBOqzEHsuHcfknj8U/T/O2gB0Fc7gB/PDDrDeAASx97jtw+qsOxOZLTvUbwBO45qu/xso3HIVl17bbAAbQXIdL/+OfceEOfhjx/zTseRw+86mjsW9zDa654jps2ukpOPKwlRi+6my84yMXdzfW/qRgKQ5/1avx4icfgpUrlmGPgSGs2TCBoXWX4xffuxgX3/bIGn670IUudKELXehCF7rQhS50oQsPDzzcG8DwTwK/ddfLce73O/k+UXt4dG4Ad2FuobsB3IUudKELOwoGdj8Uz3zW03H4wQdi5QIpGFqHm/54Da741a9x3SP2ZoE9cMzfn45nLAew4XKc9bELHoEPd3VBgXuNC5qbcf2PPoMv/eLh29PobgDXwJEf/BKOvv/jOPWLN+OAt30G79n1QhzXfZ3NwwoDT38H/vmdR2HfpQCKYaz57bfwmY9ciO6+exe60IUudKELXehCF7rQhS50oQv/9+CRsAE8V9DdAO5CdwO4C13oQhe60IUuzDV0N4C70IUudKELXehCF7rQhS50oQtd6EIXuvCogu4GcBe60IUudKELXehCF7rQHrI0owtd6EIXutCFLnShC13oQhe60IUudKELXehCF7rQhS50oQtd6EIXuvDohO4GcBe60IUudKELXehCF7rQhS50oQtd6EIXutCFLnShC13oQhe60IUu/IlAdwO4C13oQhe60IUudKELXehCF7rQhS50oQtd6EIXutCFLnShC13oQhf+RKC7AdyFLnShC13oQhe60IUudKELXehCF7rQhS50oQtd6EIXutCFLnShC38i0N0A7kIXutCFLnShC13oQhe60IUudKELXehCF7rQhS50oQtd6EIXutCFPxEwF3//+9YYA1uWMFkGa20stRYWgAEAYwApY8pIvsky2LJkAay1yLIMtrSxxhT4AaydXOarW1gYk8EYoCxFVgAmMyjL0slE2QCU1oa0AnU1xsAAKMsSWZ5XbUBcALa0MJmnEwzg6lfqeB2t52t9XlmWyIwJuhqRTWnY1O6BrMNRuSGipHipXCke84y0RXosAWSpfnCVrAWyjDJVyzKTwcLlq38JCkqplGVZaDvrKgUbalmwZ0rD12G58XYkT7VZapu6dGq7lAbPma7DnxYSOkqP6bIskYkOtEFRlk5H3z5qn3aylNaGtiQfqK1q6qW4mg+xBdNa3zL+JY8yp/jKwbLMx7/xvgBpU8qsXm0M/SRkVHRLQXUw8LbORV4b/gVfy0L7OBRj3D9b2gpfWFvBB1x/5eKfaL5eZgAYWOv0tRL/Fbm98ejzStta9hfRrsa4PisIVuMTgU8WZXFHF//Wx29d76FlStoEGRA4pG3gTCRtx36HssPAwgI2ykbdtAOotpXnC1/fxv6aNFmnjg7Lg1EsAi3SII9wblChGwhW7EW9SVhhsl0VSlsiM9X7tEyWoSycn7MNHJ6LffpjwPd4sQ2cHLF+LNM2Ae0m7ab5EFswrfVtTfwrpPgK7cooT125kX5wpsC6Wc75ymRoZ4tUFp6n+GxL+pP6opE2o98H3yLQJ2ts73qM6Iusb+nXglMB8gl9hjtyzAXH79q6Ht+nA9APpR9LbYHEZllmUJaRf8fxX1qvrthEdGfsWInVoKfYrFLO/sPzZxOkdg+2FbqUq2IuNol0xQqetbIK6cr47/OM91UGMM9Nlsn4FAVgW4Txn3x8PtuCeAQb7OY8SFUiXmh/zkOYD9c2WZ5V5unKgvhOp4AS+rRobyCQsK5PNzAoqxKFeZBjEmlOZXd4+iYZ/6uUHVTm/wIVWeU8nfPqHI24YY4ghrHSdxBXofRzP6UdDGRcvx5iwMcUUp/wR+frcfxl3If4F31SSaz4U+pv9CUvxqS5kNoMwj/Nt3Xzf/U9sRnz0rppOW2b5rUrJ1R5EA8AKJe/Xp0ULdHaM4XUbvC2KouiIivxjPelcO0MBN/qPP69v4TrNxcfGhU0jaNHu2QovQ3YH2ZZzHM4JsYd+3VXEHAY47b0/lNpCwtjsuDbCuH6n/YmTWuBmrgN6vg2LMsSuc7/EyhLiyzMJ10e2z/6gjsHbAUfIf7d2gXxaPfUl4Pdk7aHlwN+zCRE30Tgn8pVp1bKn0eOx0y3q8sytRnpQfwntQVlI1TG/9LCZIAtnQ+G+Ifx/W9suGizSId6VNur2g+mdq3NS+t5u4drCpmTGFmLqPprbMN2PIKReJS8yhji8zJjUOj8P/N43u5GxmF4n2AbsV2AdvP/UC20H2rin0lTif+od5hn+fYgKJ0Un2AR/TCt4+Sl7BVhnd4y3s0EXN0SWZZLP16FuvZDm/a2dfP/JAaI53BMhW9aV/GDXWpkQUI3tVEKxIt1Mlh/nVK6AHRl2vahspRpsYGnY4Ovpfo4fjouOL48sg+zVtcGlW6VBtV0PCLPOP47mqxTT2dyP0hajkbV7tb6+HeZsTyGRzhHhVIVmK/lTFf6MJ9nTIaijOO/m/f6ebFxc+OKD/tA73z8jzIE/0h0oq6kh2DHaIPS2595zK/FF8M4kaplJGHB+VAsJxi/DsK+JNC0almFIAlMGKOcvLXY4sOhD/MO4Or4Wl5JxQfHf3/tEvFoX+2z47ipcjs7WD8OubEwqkhbxbYyvg0q/pqCR8wSv39Yx39rK2NWOv/XdiMNHimPtifLac/YLlU60d60nrYD510m6OHkdfqSB7z+qT1Yrv5AULunuEVZIvc6sC0zk6EoihAYYd7r5waMZwI14vUraaumddcZNpmHKk0m1TcUR+1ftUWsm+ITHM9qGetY73Op/zi8aAfWc3US+jxKexn2tVPM//X6P+qAELvkwflKul5A/1Y8vf6vjGVeaJVb6QJxHhrqiDzWr2GpXHVqmQduvDFkp06ojVcURTgPDiTSMT90oIaBGAdd5cPFBV1oIHABQoEDNmXMssxtgokM7gIud4OA6KIT82pH4oA6akfj8hwOBzLFJY2ijHZBmEQ63KIovDxuQ4U2ZH2fCPqr7YOuwekzF6xSTjrM1zYoy7JCg3XyRqOiIzsV0svzHGVZBj2yLEPLLzaQRqPH0SjLEg1PjzxYjzxowyCLtcjzPOCq/vB6ZN5WRuzJNMQvC/UTaW/KGvT0tNNyyskyRybSYR5xW61W5FcTL0o/6h+B/sp6ZVkibzQquqXlastUNpU/rcdzlpXeH9SWxIflImxVH9oZs4x/CB7pqDzkoe0PAKXECbwHqWyqu5q4ZPyLbpzYQPjWyY66+Pf51towCCstY0zFLqRP2Rn/LCuKItAhf9ZxcR59JthQ4z/Ji3TcwG8r8V9U8FkntQ9xSC/Pc5RFNf4Zi6TBmC8l/gmsRx7Km3w0/qk/wRiDvMP4V1srD/JtJwPz1PfUnqlNiDtV/Lv2i/RT3hB5WK8snX+obtXydvHv9Ff503o8Z1nZNv6rtqcOmIP4VzzSIR9tS21/tB3/q+1S52NlTfwrb9U7lR118S/llEdpmVnEf5bloT8jHepPvLq08kjl4NG2Gf8JttP4T8b/omhV+O7Y+K/2OWXhNuUUj7YoC983+BGePMi3nQzMU99Te6Y2Ie5U8U8apJ/yNnXxX5TIG7mbqLeJY7VlKpvKn9bjORA3RllH5VMdlT6S+G/NJv7DBc9kPpW27CD+dX4XdJfxEnXxLwsKjkTn8a8L6Na6C0PFJY26+OcYX7RaNfFfP/4HPokvhfwk/jk3UTo2LNjw5i3BT+Jf5wtGFtMbtfFfuD5rjuK/MWX8dz7/Z1nKg3zbycA8yskyzCj+q/FIGqSf8gaA0i/asl7p/VV1S8vVlqlsKn9aL5yLj7GOyqc6RvpOR9oZMxj/zXTjv1/EL/2cV3UgaLtSuna6qwxFGv9JO5rElgRr3XKu0lS7kB/TmCb+iVs//mv8R18hbcqVppVHKoc7xjagHorPOql9iEN69eP/QzT/9+tFWZ6haCXxn7m5AIBwk15ZurlBusZAvu1kYJ76ntrT2rgpQsgmxX/VJ0mD9FPeqBn/6a9qAy1Pban87HTx7zeDWFbOKP7FPjOMf/VTxUv5UG7VgUC9FZQe1+NSG5dliTyvrm8pb9U7lR0PS/xXbUG8urTySOXg0c5J/MfYzmcZ/9rPKm/yaRv/Xg/lSXsqHm2htlYe5NtOBuap76k9U5sQty7+qwvskX7KGzXxX+7I+Bc9SZ91VD7VUeljluO/+qniVfiwLzdt4r8okHkfIbTTXWVw6ykx/sF9AG6YzCD+dbeE/BSXNLY3/nltRtrMT9OOB2WL9uT1Au2itlEapNMu/qmvKy+CHtks4r+ubciHMhCXNiOYR3z8R79UXNIg/ZQ3tiP+uW+Qhf7GwMqNMfA3TGk9npNm2UH8600AmDb+HR0C84lD2ioXgfzJQ9sfHYz/5JPamPZU3ZS34YNzlfh3cmPa8d+1u9IycxD/agvi1aWVRyoHj3YW8Z8ZY4ITKgIAtFotlD7QU8aqGMvVYRS3KNxmBPE1DW94xaeTpsJTKfjGprKkF9LS4XPzkjx4pI5qDHY62uEBQC48IHIynToc67Kjg5elp6encq66pPi0AfXSempv4pIGy7UecSkXZUxpZL7j5bm1cYMY6ohiX+KTL2Whf5AuaRpj0Gq1AMQ7Wuh/5MPAAYBGoxFsT1zy0800M02HQ96qS6vVCnhqY5bzSD1pEyQBR+DFEu1Q+HYgTp5lyKWTyRuNCi+ITa0MlCo38U0yaFjvhxA70w94VDy1V8NvQpMn6Wxv/OvFI+2gdiNN2p51s8QfWEY9UIl/J4dLV+PUzDb+/eIDIaWrOlIutSfrpvHf2yb+izmIf9JgudYjLuWijCmNLHMLLzynzqynNiad7Yl/0p5t/Kt+5hEQ/0yrHRSHtmD75fls49/Vpw9TFp5TV/LnUfGivbJgf/Ikne2Nf6ZnHP/bO/4n/knZlBd1VFu0G/9TujwyXbVnu/jP0NPTK+fRRynL9sS/+oLahnmkx3P+lEZWM/5TJzxc8d8zRfz7TTlejKj9tY2op/Kwj4T4b1QvKtBx/Me4Y7mdIv45D1E8tVe7+G+2WijKsnKjJWVtPBLiX+4wtnMY/3rDIxA3HEg31VFpZG3jf/r5PzdGMZv495sjLNd6xKVcZlL8u2Pmb/YkTdqS9dTGpDOb+G/O0fxf9TOPivjPQ77qkso6V/HPuKcciqf2qsZ/A2Xp2nTHjP+T/Yq2J37aViyjHqgZ/7kpRNoQWxpjwoIyedFWaosdO/5PH/+KTxtQR62n9iau+oLahnmkx3P+lEb2cI///omGolWEsTGM//5mHuabTMf/R0v8V8d/9veprNsd/3LDHPNZh+dqr6nG/3LO4z/ajTRpe+KnbcWysiwrayw2iXlNI41/8UHW55EydePf3ezJc+rMempj0pnT+Pd8/nTH//T6fwfFv9eV/HlUPLVXu/jfIeM/3+xRG//sv9qs/3k6CPHvblIg7bgWSLvEG4nUB1mfR+r+6Ij/LNxIqDqpL7C9WU5cykUZUxrZwz3+d+M/8LIS/5nxT/Z6oEyxzZ1cPKeu5M8jZU799SGNf7EbadL2xE/bimXUA9sx/oenqR+18T+3439+2kknnRGoi3MhaWRVTIVXY7BMBaewFEIFJZ7iE2j0NI+Q8oHIzse4U/nJm7QoO8tIj0EQeIjOmQ9iY/juDw9J50IcPqVqvaNQpvBLGjuSi7LYpFOhXMTTTS7SCGmPlzppwBOnK/0dPaSbZfEOUOWpPAiUnHiRX8RnWSqbgtKE56UdFPNAep6WkY6MtiJQB62n5ZTHSrsRtL3UBioP8xq5H6xQfeIn4Hs7GRNf06A6USa2s9KmXjoAsp7Kx/rEyby/ko+mqQPlJT3SSeOnTnceCcSjPmUZX02b6kU8xXfgO3N5hQemjP9oC/KxcxH//g59jxRkTH2ENJhHPNIlL97xbaXNUIn/KJ/Kgmnin0/oVds52pb1SZNHJINOWZZo9DTinfiJjVQ/x6MaqxA85ZfSIF3SU0hp0gYqs9JTWu3iv109AmnY7Yx/4hLS+Ccw7ei6NidvdBT/1bZQ+VifdbJp4z/6HHZQ/DMv1Yt4ik+gnGkeIeWDHRH/NTrTnswnKC7xSNfxKsMT32gb/9GWKgumjf/24z/xOo7/ZPxXG6l+qIlVCN7s4z/Kg07j3/N6VMY/X/s9o/hPaEwT/1wkYZnKrfKiTfzzFUWZkScKE5sSaCPq00n8887jujZhnq2Lfz/GBRyN/9Iib+SVp5A7jf9M49/PLYxxC1fZTOJf4ta2mf9jruLfb+IqTdqD9UlTeaXx3zNF/OvTydjO+C/pVwmkNGkDlbkik+j56Ij/2CZqG/LGHMZ/Nqv4L8MTwNSHetfpntYnHvWpxL9/usQjBjzFJ1DONI+Q8jFp/NeN/3xtXo0d1F/zHTL+18W/q0tctaXKgmnjv27+P7v4f9jH/zzTNzA6GzRy19f7VQalx0V/86iJ/5i21t24wDRlYjsrLvWaSfxTzzq/YLnKC4khwK0Nqd51uqf1iUd9KvHfZvxXfALlnJTn0ykfdBL/HY7/D138xzYhfaVHWTBt/M/l/N8tUnPsUBupfthR8Z/QpA1UZqWntB6N8a+yUSa2s+JSr4cy/tP4qdM9rU886jOn8S++6upXcUiLY0Ke55VX4z+6479AluXh0x/klc1R/JvK+F/tRymP6kceKRCvG/9zH/9FWYabxvTTVtbGDV7WZ53sTyn+JZ3yQSX+Xd1U/snxH2V55Mf/Dhr/T3vnO89QJB1giFzKHQTaMKocmRIczeg42lmrEFpHDaBBbJN3ggccX593GIT8tDGTARKJo2s+eYa8pFEB/80V30mSl24QkTbvjilL96pfhaBPEgj6K0v3iuSgm8ibdjZ2ik6KDpb7u2nScsXRfG5es0wDiHSsnfx1kCqPSJe8UrxqW1eDIMVlvjHxtaspvtrC+nz1MwLbjnqlPs0yK4MQQdOlf1uww/VPcshEhK880+/LpLpgioFIcahvKot2dpgUP9EvUvuzvjFugWRu498fTXxFsdqW5wRHx9GqyC/fBIpax5icLv7tdsQ/j9a619uZGtsYsa3qV4l/mbxayPcSp4l/limY2viPT9So7JRJ66TligPAfUPAD1hZB/GfQsqDafJK8VJfJbCe4jJfaab45KP46mcE2pd6pT7NMjtF/Fvhl+KmdHiu9Y18Q4TlNm2PSfrasEjL8rRtU5uShtor0op1dkT8K2+1Cc8JKlud/FrO/OwhjH8tY33yqtOvGv/147/WZZo/1SOtOzn+Oxj/O41/n882cGVOD+VXJ5uWocZ3U5mpZ2zrUBzqKS7zlWaKr7ZgvvoZgfalXqlPs8xOEf8QfiluSkc3YoJscjMH8W1Ne6T6prKkbas21XFB7ZXScn5ajf/MX3ha68Yq6pDaCtsZ/yZpy6pP1Pua9d/smRT/hY+bcg7j3/NiHuun8U/7mEnxH8f/lEawxRzGv9E27Cj+J9erxr/fQBN+dbJpGaT9mZ/KnE2K/8nxzPx2NFN8tQXz1TcJD3X8u/OHZv5f+P4Gs4r/iEvZmaaMqa3QSfzDVjbsSIegsgXaU/ga6xdFETbSWJf4lfj33w5jXZWRtSmPlhFfy9Q2Qb+kf5s+/qN9WEd/ncd/jGPWjTw6jf/pxv8YJ5iiTbQM0v7MV3zikQ8g33W26TfOlCZlrfJP+agM6mcE2pd6qU8zZtKYJmia/FJc9YU0VkL9HRT/FZuKX6i9Ulq6wMx1J7WB6qS2Ih21cSo7eatNeE5Q2erk1xhnflY7/4/052z83yHxX20XpvnrPP6rPk+ZVSatk5YrDvv+0lrYWcY/Ywc1vpvKTLra1gTWU1zmK80UX23BfPUzwlTxr7LZKeLfCr8UN6XDc62vurDcPkzxr35KXMrONGVMbYVO498/nJXevImkLd2GZ1V+LXf5JbIsR1HwSU4LwIQnZK11193tPoeiMhLIkzcnskxlTW1T0W+Hxb/X3c8Zdlz8M7/6GQjKo/yibFVIeTBNXile6qsE1lNc5ivNFF9twXz1M8JcxD+EX4qb0tFYqdOF5bamPYyp7ndkRm+Gqm7W4iGJf7dJqjqpjVPZSU9twnOCylYnv5YzP6sd/9vM/yf5k0trPnmq/A6/Wqa2aaff3MZ/te5cxX/+3lNOOYOEWEBQZbShCIqveMy3snHrftFYrK+GJA9teH33dqQblVInDA2UXDjQSVQ25ZU2UOoEbAjSoyzWO1jdXZzGGOR5I2x8q60U9AlWgpWACu9/F3mpL/xki3mQgAu0/DG1eZZl0IsP1tNgJxj/2ga+jkF5KS2V25U7OTVIWMbNZc0jPT3C24PfGgh5iMBvjhCXelAu5sPzUFuq/jyW/k6oQjZEM+Hh8JzNC//UBPWD8KK8gY/vqAmaJl/S0XagPUibeeSn/qB6FPIqA9YjrtreWv8keuKjLCNeCqSNhH7K03KAFNlZf1J7+ad/WT+kwUljXfy7jo24qVzZHMZ/6fXghrZ2xKkMnAhQRwX6r9pYF6dYpj7EPNYhbpblk16HXo2Qql+o/TTfGPdtllRe00H8M43EfrZN/LO9NY/4ga74URr/CkYmcayv9JlPXLUly/XYWfw7OoXHpX4QXpPiP4l5l45yzSz+q76s+vHYWfznkxalCcRlvRQUX/FSnjaM/53Ef/Qfyqm0NF/rKW4qVzaH8a962BnFfyBfuYlFbUwgPcpmpo3/9uM/IbU5baH5ZjvGf6ax3fHvcFUGO038ZyZDUbrvlLLeQxX/xKV+EF7aduzLJse/A/IlnenjP/JTf1A9NP7RNv4n1yVkshBOm+mooviUq2JzWYjlT+VmmfGbzNoupJll1U0gzTd+vOKiUpa5p8dSubIZxL9N49/EDWV4nSiLnVH8V21LoP2NcZuvEP+hbKbT+JcNpRSYF+SeFP++rF38N5sPUfxH21IGO038m4dl/Hc27zT+WaZj/o6M/yx5lTnrEVdtn9blCMUy4qUQ8UWuxOaU3dr4Gl+9kTltL4j/8NpWaTFN+VmPeaRLsDbeJMJXSyqPzM/hdvz4H2VSUBsTSC+bUfxHm9bxYh7lof003zwSxn8ZM7iOY0uLRqPH06n3w7mMf87pp45/R2d28e8gz93b3UhvzuLf9+VFUaAoSxRFEV7naOXVlzxvtlpoFe67j0VRhB9xiadlRYKveMxnXqvVCr/Sv1KS9RWHOrF97FzF/wzGfy0jLtuF9CiLfUTFf+Rbx4t5lIe20HwT/K66FmQeyvgX21I2+4gc/x2doizQaPRUbuQmL207lqXxTyBfMxfx74/FrMd/BywjXgqKr3gpT6vzf97wyvlmaK+44csjN3iVVszPwuuQ4/qfww02QPUmUZVNeT164t/Huqny5Le64fnW8Qo26Sj+q3FmuvEf2oJAOsSlfhBecx3/VuPMxL2NrCaGzSzif2br/1U/U7yUp+3g+p/thUr8R18jnuZrPcVN5cqS8d8GHq6sfNTEv8tjHeIyD55vHS/mUR7awqy96SbLAjJThSlEikMhKIgqSoMWhWscNXBZVt9v7vIifSrCAHB1q0+ugkYSZVSO0j8SH/KlsVqtVlA+1ZNlkZd+dNs3Sl7tCLLMLVAVRYFGo4FmsxmcwhgDmAxF0Qqv02Ed0qAz0paUjQ7b8nSLogibxaRtvDNDOlSWWd9hMK2vtYO/uI56Vh2D+aWf9Pf0uIsv8gj8/LdmCrEHaTncOHjXAeWD2J968dz5kbx/P+komaeg/sBFBNo7k86A+tLXaGe06USYdixjeeojTBsTX1PIumVRhCexkQwSBMcjyqa0IR1Uaoe6I8HFkeuQdGAgGLZZ0uGp7YhDeSkny8iTvGhnnkPiWr93p/SdbvHilHVTfWxZfXVk+jqHmB/twfjn4meq5+T4l0FM/CfIK23RLv6NxDJtpTR47mwZJy2sQ7psM9qctB14m1f0jfagLVRfpZPi6SLMlPEvdlRgHnGpdx2QP+1PvfIsQ7PVQiOJf9ImXh1ttbXqzrLtj39vHylXWZhOZbSJP8OPh2bG8R9jSXnUHQnka2rjv2pX9RO1nZbRfnU6k9dU8T+z8b8m/kVPbW/y13zizXz8n9y2ag+eo+P4d3X4HXilQVtStpnFf/34j9nGv9CI8e8W7LR91I4KzCMuZakD8qf9eWMDz9Pxn7Spv7XWbXzJ1iRxsYPjX8vrbK4ymnbx7zcXSV95aJsRH+JzqR3qjoHmlPFfje00Lji/0zLar05n6li0Zh7/+o0em3w2oaKP6MkNYNLgTUzqM+Q5Vfw328W//24ZzNTx39NoYGJiwi2USNuov7FOSsNa9xoZyjZd/PNpYULpr7WC7NPEPybFv9O1OoeQ+C+K8EQQ5jD+ueiQdTj/J23i1dFWW6vuLJub+K/Gq8rCdCqjtTZ8BoB5Gk9KT2VL9dQ2UB61R1+nnFH8R79Q2ykO7ZfqzOszbbeyLP23W11ZOUX8q27lDMd/KzJqPvHyRmN28S/2V3vwHB2P/ymNyJu2pGzTxT9pE7iAnsqrNlJ9lU6KpzRC/D8U8/+mj//MIMtytJpN5I2GWz+RJ8eph+qpoLZW3VnWSfzrmgLxmFa7Ma/O5qmMtmb8T2/wJ57KluqpbaA8wjFzazJFUWBgYAC9/X1ukyozMHDrY7zdiFTZ/8M/VU31qrxjmcuvUPBp+lHsR3iOoBvCOfMmJpqYGB/H2OgoeuS7j7SXPlXKOpF2bG++bU3ziTfd+L/j5//taVBfyjbz+J+r+b+TnWsrs4l/jgHEpSx1kNqfevH8kTv+i+3lplXWJY7m25r4py6kTzyVLdVT20B51B0J5Gs6Gv+rcUHbaRntV6czedHOPIeXw1r3Wn+C0uf8n28d0vVSlVn11PYmf2tL5Fl8BbSdYfzrwwesTzzKy3NsR/ybmca/twuvk2mRcjvjP11LZb3ZxD/ziEtZ6iC1P23G80de/Eef0PI6m6cy2lnEf1G6TyjyIUMEn0vtENtMjwTyNW3in29iMjVxQdtpGceJOp3Ja8r472D+n9pLZVY9tb3JX/OJl+d5mOM7vGiHbNrx3/FVe/Ac2xH/PKctKVvb+J/j8T8//eSTz6DR1BhEIiMVinhKnHUIjp7vpASfdNXIqoiCW+iO/KkUwUrnUlEe8Y4R5ZOm1VhsEOZlWfV7I9ZWXwFHftxIZSNp45NuLnevqJza8NTDJIHYyN1dolqH+hKoU115O525KW6kfbWcHQ7rEgIvncAnMihunc/keR4ufMiPwcdfnT/qRYAx7m5zvVCjHhpc5MF06hNpPW0/pUPQxZFcNtXTuqpDWZTBXroRX4ZvLkTZaCuek5fakNCQO4/403a30oESbNIxIvE5+PYhrtKua0vSU39EMjlVfNItrb8xI+Rb+TkgTdJgO7rMGP82xH/0qani37qTeN4m/gMr4yZeKg9tSDpTxr+0udqeaf7qNuLStqAMVfmqcrnyqs5M85zyMc1z3fwlTQWed5Jv2viM2oMydBL/qgtlVmAe25J5qkvqE2m96ePfyz2T+E90iflucIfIRlvV1YsyO312SPzX2Ju/urYkPfVHdBD/Kf86IE3SYDsqME91stPEP9OKz7ZmnuqjevKc/PibSfynT2PyR9qpT9XJlcqncml5O50pH9M8V9mVNkF5TZdv2vjM1PGfI5tp/Hu34KYY25J4qW2VDvNZ1mn8Y4bxrxtdIb+ofnO97Dj+HXQa/3qzlZ1B/HO+ZYybF9S1JempPwJxYzvUF99QP9N8+KbkGWmSBttRwVp3A0CWVW9cmvP499//5TltyB/jv8HFKl4f1MS/8lAaNmkL1q2TiwtllIc+xHL1gzqdqTfTPGffZGvi38i55ut5Bb+Nz1TixrrFtkfb+I8Zxr/qovmzG/8dTBf/uoFKsB3F/46f/6f868B0Gv+0q/huffxHHVUG6280Yb6pi/85HP+Vh9Ig7dSn6uRK5eO1Q1pe1X/6+FfZI+0IPO8k37TxmSnH/9zNAcrS3fCOGn8knToZzBzFPzexUtA42d7455PGENloq7p6KjPaxb9fo5poNrF0p2Xom9cfefiR1Rh+T5nnjCPyMnAbua4WfzF+Yj3SU9kcPZZr/JOeK48jvUGeZ+jt60Wj0YPRkRHnC5lfg+sw/p3t3bE+/utjwXYy/j/i4z/KpeXtdKZ8TPOcedOu/3WQb2YT/4+y8Z/rmGld1SHVRfPnPP7FVnbW43/V3vzVtSXpsQ6B9PgjPumGt4EkPqMRnmXxLZXklQIfdFCdrLXoaTTCw2bKtyKD4LOttf0IqifPyY+/2cY/1w/tTOLf2vi0s9hP5U7bkGmeUz6muQHs8hwuaSoor+nyTRufeXTHf6y7veN/2UH867pB+oRuT6MBjQ/yxSzjX3kRV2nHtoxxQHqsQ6CO/BGfdFP+dUCapMF2VGCe6mSnGf/trOK/fv2fv9nGv9Ig7dSn6uRK5VO5tDzVn+eUL/9b+QZwKpQSYlqNoI6NxLnSulHBLBiT9VnPlZNe7BzYOMqLfGhwCH/I9+pUBiTOlCUdE/MFORqq4e5oIB4QByvjg6OOhsl8Jy8yE6gffJnKwiOdlXqwk2C6gpt2dEJL0yFPbEC61stKHPBVRUmgVV6Ll5Q5+WIHp3oGukm7p52UQqoLQe0PsWEIIAnE3N/9wh9q7Moj81gv+p+jT31oK9Uv83dtGOPuZG7Hj7ZSmTSPwDTlUvxUFuMHUqVHmrm/+430Mh9/adtkfiGFuulCI+kRd3bxH9td4z9PXt/COuSTlqleFu7pnDQ2iKdA25Q2vgZR8ylnmpfnOQqxrUI2RfyTf2ob5pGWa9tqH8gj62Ka+NenflKbpe2sdImv8qmOtfEvvNMyla9d/NNOxJ0q/ouyrEx0Cams1IV3zZGvnbP4j75DusRTGdQX2vGjrRRH8whMV+M/9gOqo5lV/Fd9iPjUjfIyzXMzx/GvdLUO+aRlqhdpK53p4p+4qjvz63Bzf0cj8xTMnMV/lEWPqV6aVly1cWoz5ZXSJb7Kpzo+3PGf6kIIsmau78uyHMaPA6TP41zGv9IlHmlmbeLf1MW/X7Tna9FoP9WTacqV0lVZzKziv9o2xLdtxv88c4uyZrr4t+5tOVqGpN21nWgX0rOIG9B17a96aTuk7clzgtqN9kzzK7j+6d+84Z5oJp6CkfjnuMOxmPwrtvGgts/kAl9l0rqYKv7le5jGxDeWKI2Krm3iX+cQhB0Z//Sv7Yp/sSF1If3A52GOf4cXadNWiqN5BKZnE/8543VG8e/amrpRXqZ5btrEP298SOta63eEZhD/lK2u/Wkr9c2ypj1VBhhUruFoTyRtG9Alb8eM/5N9F0mMaF1MFf/Jom1qM9oyzSNf0lUahB0Z/8Stj3+HW5YFdCMxxUtt+MiN/8iPtlIczSMw3XH8N1sobImBgQHMG5jv6lv3mYzSli4G5Bvfnks4unz4CETlSV3VxSSbxi67XnYHDtfVi+3vcHg0aPQ0UBYlms1mZZ6R0qOtdvj4v0Pjv+o3KoseU700rbikbWpsprxSusRX+XSzYabxzxs3tj/+HaS6EFRfPKzxH22RPdzxP4fzf+IRSI+46gOo8XGtyzzOp7M8Cw/GqF1Seo7P5P5f9dJ2IJ2ydGtGKgOSNqQ90/w63B0V/7rpprLoUe1TFkXlDXB6zRBsPMP459OfUb6qD840/rUN/vTiP8Yo+at+2Q6K/4JyKb6prkWaR0P8S7trOyldrUM+aZnqRdpKh3VUBpBG4Ol8gvmURXGZl+fxKVyVg3izjX/SyjqN/zke/83am26yWkgGZbJzrURUCRI0codApOccio5HuqzjaEZ+Mb8+uFLeTDE/0PQlzONr5ExiGOsdPdUzpP13nizct1B4V4HxgUeYxN93kJkPWCdTG13EoUi78HcSlGUZ6lN2fR2G9Y7R9PZlvjHxycrSB3nmO9iUZqUO74RIyrVN2cbwFwDklerPjpJ+lPKh3rzzh7IqX9bhhb0xLnjLogCDuMrTpUOAJH4a5PX57BQJlK/wr4Hg3TkOP9YjDZVNOwBtv7zhdKcd2B7pgKf6kwdp0f6sR98q/Hd6qC/jSOXM/cRF7aM2UF0wRfwbaQ/WJdTJSnrZtPHPwSC+esMEm7eJmQQqOlgA/q5AtWu7+McU8U+ZrbVoNVv+4tS1s8rh+FZ9kXbUvDpdyCfyda+TSGVSPbQdon395CvQi7oTL/Kol8EmN3YoD+KF+K+N+WqadqiLf6Y7iX/KQPrEq+OJZNBVUHoA0PCvBCFQpvr4j0fVgbK1jX+vO9Nsjxj/0s/NKP5jXFNfxpfK2Vn8V32fdFIfTO1HqJOVdaJ/Thf/k/N5rJNbgfnt6lIXprWO2lRtQJ2oTzr+qxx1/GlHzXM4WbiZgXVSvrOL/8n0WId4yiOVm+m6cmeDKJvGF3Hr0qQ3s/iPOKmepM82DDwtKj7MTSU7TfznMxr/41F1oGydxH+jNv7jt3KpF3mQFn2Q9ehbM4l/HZ/UBqoLJP4LL2+4mabGfoQ6WUkvk1d7Uj7WgafZLp/HOrkVUh3SumwHprVOad3nKPgkB9L496+XDuP/NPFvPF+3UFMX//WxB7jXdJsO458bzRnjX26YpRysQ7yKbpNk8HLXLCplWebegDLH8Z8Zg2bySQ7lq3SmjP8krfIpKD1sd/xX7dNJ/Lu8yZ9AolzUizxIizHFemUH8W89jUaeozXt+B/LHO0ou/pgaj+CysoNYNYJ/ulf68snbZVmXfzz2q2d3ArGxIUwJO1lGDeNPLwelnXUpu3iP8/cDbFzN/6rLtF2yreT+CdPZ99mRYa0DvGURyo303Xl9D/KNlfxb+rGf+s3CWS+RBlIn21YxxNzEP+tjuK/2gadx391/LeJn6ayzCb+JyYmsHTFcvT09sSNX4uwz2vAJ4DdmRZW9aKtfMWAl8agGz/i01GxDvUy8s1P1nFQbRPAYGJ8HJs3bUJPT0+Qh7QiXgRtj7q1Q9pebcw6alPyYdrI/H94eBh3rH4AP79sC26+Yz4eHG5hvG8tylYDfROrsPNC4MD9h3Hksxbjsfvvjp6eng7iP8aB8p15/M/1/N/7k/AgXifxr5sSqcwpz0nxn7QN0w9l/Hc2/nvfCvEfN15mEv+kq/qTB2nNNP5Vzryj639pu4fq+l/eUFfJF17uGP2xjrfmp3XhZacuTGsdtWnFBkn875jxv/opF9JuG/+Ffx22vOkon6P4Z6y7clRlnGH8M016f1rxX9WBss12/Cdd1R8iS6sowhzUyrVqnnFe7/eZ5iD+zYzi3ztJYreO419otsvnsU5uBdUBNXWpC9M21IltoXoyTZltiH/3KvRUjjr+tKPm1elCPsq3bfzvgPHfPHDjjVaJqwKKyHwCBVGgEGRqra0YjTg8L32j13UoxG21WuEd9KkBGRSsy8bid3qD3B5fgzSVHaKnMfG7tlnmnjBkHWurT8imujFd+E3KoE9iw0BPbEI7EM/aeDedrzTJRpQT0gEYo6/WdU8hB5t7uhp0acekdoWXhe2tnUz49lrSphywtT7rMSh4wc02STuOYEdfx3q/aviLAngbqy0ItG0YyRII5Uke7aEyOJnj++yhHYxfbLbiBywzmXvFI/vJ1MdpCyu21nbgOfVWGtp2ypO0SXOyHpPjTOWZNv7Jc0bxHydNxIm+4gbaOrmMx50q/smDdWnPPMvCRi3BTBH/xEplhJeNfK11r67hRSuS+NfJnPJSIF+VgfxoB24KUicFtQFkMgT4xaogz+T2DzpME/+27DD+xTaxTaM9tD7rZTLZMx3EP+tYxr98P3u6+K8rQ2J7zaM9UrtlfoKnfkpgnto3pad4ai+nVzXeaVueU2+lwQVaJLqQtp1R/Md2mzb+Re+5if/tG//Jg3XpJ/S1lFa7+FccHlU28lV+xE11Y7o+/r1fJu1GfrQDvD6qU6vVQqsoQr9WlCUgvoFk/Cddpa86EBd18T9p/I8TT9ZT2ZR+andXfybx72xAGqxjp4r/IGq0p7Xx7uoU1PaaR3ukdsvmIP51U1rpal/befzPfPzXTxhomcqj8a8bv7oBTGj4eaICeZdlGfTiEz2pTdU+dXIRd0fFfyo7cXgMsvk5bsqPuMrH+IUUAJPfFuI3k6zH62k0kMtd6WVZVp62Ji/aRvONqX77yxVU49/U6KM6cK6A4HdukaBRG/9+wcL7ENsixuz2xz+fVFWZ0Wn8J0A968og5Wke7ZHaLauNf4fDPLVvSk/xdLylXqwzl/GvG6LKT/E0XVbif7JfE5fQbvwv243/9OMO4p9UzQzinwvxtl38Z5mLSe9/qeyMSyRtpz6u/Iib2onp+vE/2tDRc3nkRzsQj7ooqA0Q4t8RSvVO9VEd1IemH/8fjvl/jCuWlQ9h/NMfyH9y/Dtgnto3pad4aq8siwu7mMP4H58Yx4pVu0Rbys1BACqvf+ZmrWsjXx6+c+hRKrg+x2SVc5/rqFsbniJm25GGkSeH1VYOYv76tWvR19fXcfw7+Rn/1cVT4s9m/m+txR133IuLL92An166MzZtWYGeBbdi3k6/RdHYiPkLl2FiaDcMPfA4tAZXYvnyjXjJc9fhRc/dCfvuu0doM4LqrGn6g+JRJwW1ASrX/3MV//H7y6FVZhj/6bqb1ss6jn93ZB37EMe/5mXTxL8FwvckWab0iMe6Spe2xhzGP2nW6aF4mi4fqut/vy6q66N1cpFeq9lEb28vimnjvwxvLwm+ZgwA9zYiM8P451qn+qXyI25qJ6Y7G//jWoC2D/Goi4K7STTmlaV70hnbEf/pjcm6JoVZxH+dzqFNHvXxX63L9lH7pvQUT+1FvVinXfxzj4fXj3lyI6XDjzFPmnV6qAypPPxUlO0o/mM7EMibOti6+E98BTW2UXqzG/9r5v/ia9xHS+cvqYyoxH+1rYib6sZ0p/HPtLYP8aiLQmqj1MdSeXhkvtIty9I9AcyCYs4/+F1VngJlsmttfPC3ZvHBbysNBO1o5LsARRHvSqbSVt7ZDZFLadjQCMn3bq3bWCRPypXKaH3ghoFSdNFGTTdkUz31dSp68Rrw5DzQLEtk+sFvdSzREZKmw/ICPpPXB6QyWWuDTYypvlM9LHKLPUhfebLteE6/oh48Km3jg1fbUfWmbYuiCKGtsqvtUp2M72z0rp+IG+2gtDP/ijXeMUwI8eLvoFUZCaldiKdHSHzphTnpaSym5VpHY0hpp7boOP4p27TxXwXKnYX4j202VfxzY7WONnEhNqWMeWJf9Zs0/tlCxGNa7c08Y6qvWFQ70ja0u06U2Q6kTzyVzZGIemobaFtNPronC4mb5/5Gi5pJUqpjJvFvyw7jP43TZDBWWUlfeaLD+Ge58tR2VDwj8a955Kc2S3UyU8Z/rKe0aSPNQxIvqYyEaBd3ByTx9Ii28R99grB98e/SHce/APPStq0D2iGbo/GftFQf+gbLOo1/AvGYphxarrIwncpo28a/GzOUnsqmNJrNJoqiQFEUmDd/PhYsXIje3l5YC/T19wc5JwNlrrcZgLBGY+VJtgAu0/uFw62SsdAFPVZJJ9RcEIz0acdoO0yqOzlWHFR5xjpVfMdLfdTJUE37JzVTrLStYT1mBLWTMQZI+msgisUnbVIaihR4qqHV4GkfwvI6WaRc61jrF/P8OBdqsZ19nrX+ydLEFkzTRhWok68tOBxj/FMiPi+ck5a0k7Mf69bQNskNAHW2Y92auIWTgATCzZ4kVzkXW6R0FMcjVvLLssTY6CiMX9QaGhzE6NAQsjxHI8/R19fn+tEkFrUPNjqmCt+oo4PSX8ybKcZ/vSHB9ZOuP0a7+X8ZF5pULx7tLMd/488LTz+lq7SZp/244pmHfPx33yuf2fgfbaR2IZ4e4eXScUTp6Viclhd840BH47/Lc+N/L8rtGP/rbqwAfJxK+7Ub/1vbMf5zE5gypvbNZIEtHf9Jme3CtNqbeSoL06mMtu34r/N/h0+eLFc9tQ2Ux+RjqBL4miniX3WknUiL7antoDIxD3MQ/zwvS//0r3Fjqi5ykzZ50VaahzmOf67LKK6ZFP/bP/9P/V2PmGX8N1tNrNhlF/9pDG9vPx9BZS5nwfHX+reo6CvgySfaIbZdhFTHtFwh+ozzZ5fH8ywz4SnitfffH8ZEbYMUaDsEm8abY9XvXNnM5v8bN27GFVfdhV9dafD7P+yO1XfuB/QBy/b8DgYW/QSDG3owb/Ei9PQvxNa1z8PmNc9HhnHss9dqPPmQNXjWU4GnHr4Xli5dDNTGf/RtypbqSdzUDnVHwtzEf165KUtlUn48Ug/42FFZtR2Ii7r4F3oqM2kzT9tR8cwcxr/y1Hp18d8q4lOEmGH8q38qvso80/hP66jvKO1Uv+Khuv7P/VuB/Cfy8ixDs9X0r1lthT7I0S7c2lbSXgTaDmJTyphn7qYv4qjfTBf/psbvWK6yMF1nW20DtIl/XidQtlTP2AayeV3a+GaMGh8jX9Nh/HOdlLzL0vlk6pdanzR5tHMx/j8q4j/6P220PeN/J/HPuby1emOnxmL1xj0zy/gvZxT/sZ0UV22aAu2QTTH/T+2hstfRJi7EppQxtS/LyhD/rt+mXEqDacpBfXlOnkynMtoO4588KFuqp7aB8qg7EsjXdBD/+WknnXSGZmpjsqKRRlZmqfKpoynjukYl3zpadbJQxjp5tAOb9O3VGsfkeWpEpsO5pxVwPU+1A8tS+2gZ5JUC6ghqC8Wx3klZ1xi/CCMOj0Q3ykC6zCOOlc4TyR001ncuat/AQzp32qgs3d1bvFByeru6xr96gLbgUdNBphq/Ix+dSAJuM1xtpj+1CWo6YdIkD9JQPcmHMrl6VV+nTCqr6sF8vWlA+VB/phWHPFiu+RCZCQzyTAYh1s/9YgfxaA/maZr10nYgL8pPm/C71iovcZhWucmPuKqHto3SUlnsTONf+UtsKPCc+FrPJoO/ykqeLFd6Webu6NZ8lmEu4l9kVXDn8bvG2raUlXW0LI1/6mAqk4tYBvHHOvpqr+niP+Wpfkc+Wo95ajP9UT4C6WkZ67PcdBT/sUz1VFlVD+aTFtNqL+XDBRPVI63L8+grrs7cxH+Mg7QdyJfy0yaar21U1y4ErRv1iLGR0qqThTLWydM2/j2QT3pOfK1na/yZuOSpdkjLNJ9lANBo9AD+rRaqo+I3Gg00m02MjI5i3rx5WLJsGXZZtSsWLl6Mvv4+NHp60dPTSN6y4eIf/KasMckiH8H4RTePb+NmYsTzC/W+T6mW+XLPqx5cedRJcZmu2scYv4lniFMHLj+IJnkAEl3IJt16NXGjjPjWLY46vf0x2bRNqcDfuFQBv3jNRda0vvMLsk2l8oqFjGpa/U9rqn+yzKntn0T1huJTqcRjWgiB43k4Ml/qpfmhnk8H+Yz3oZSH+qnP9tJ4e8lmr0k3z/1TWTAuHezocmlf4vpGSPjUg5GNeqaZr3aiDWjDFGg/tU+Q0Bj09vWhp6cHvX19WLh4MRYvW4ZGTw8mJiYwOjLicHp7Ac9rqvFfLBtwrIxBvEHNdjz+x7v6Td38v4wbtFqu9FlmZjH+800/hLQe87TP1B/1I3B80DLWZ7nZrvG/+go31iF90mKaY22qv+KQR1qX5+lYMdX4z1fFEY/2oL6aZj3mpTpQftpE87WNOK7pj5D5zWjSYpm2jfWxQ51SWShjnTytjsZ/11coX+JrPVvjz8QlT7VDWqb5LMMOnf/HWKQPsm0pK+toWdv5f138ixxarvTVXjONf21r1/0/vPGfrrOQDmUKsiZ6MJ+0mFZ7KR9yUD3SujxPfaVd/Je2xMJFi6LefiOYN6STrg83HxM2PNUbeUS7V+XSow00HA7z+fOYxuFW6yDM5Yzx466fO40MDwfdQvkU8V+d/8d1KIK2pZ6zPo9MW2txwx/vwfd/YvC/v3oCHnhwBUw2hEUrH8Di5ZfDFjfgwTU5imYD8xeOo69vIaxdjPHxEhs3L8e99y9F0dyIVStHsOuuOwE7NP6jLvTBuvhEx/Hv5RL6Kgftn9Jnmdne+E/0Jb55COOfvqVlqqfKqnqov2rddvGvOOSR1uV56ivt4t/M6PrfQV07kBflp000X9uorl0IWjfoITeU6EM21MltRLp5luMV27QsCmTiY3y7h9IwZvbrf7wOUj1oIyt+oPRS+2gZpoh/fVNV+/h3c3rjv6Ec5jEOOdShD6q/8Yc28W8THzbGyUjQ+rRHHX21159u/FfpEJ91mE9aTKu9lI/ikEdaN7xVqm38+888Cf3ZxD/fCpXqQPlpE649qbzEYZo/Qqwr8S82SGmlPsFytmlVnnT8n8xfbU1/Z35az9b4M3HJk+VKX+VRIK928a/47eM/yqi6EJdH+qD6G3+oif/8ve96V9gAVmW1MbUiGSgoceLTSVSB1DA0AtNqvDpDEliHBs/l0fUsc9/s5XldPQWVQQ2sr6xSo5Nf4CVyln7nvSzda1AolzEm3H2sEG3l6Kd6APGuZsBtgGodtUMK3JjNsixezEhbUu6K3ZPgrfupvuGJ5MQ/0MbJKQ8v1jMuVklgs76++pkbv0j8iXx4Th4qjwYYjwQdpOrwuGBheTeZyMQjajq3zPsg5YH4DenzXO1FoC4K7OzTH6Surek0tF2IR56apvxKU8+VTqhv3ATLWrcgmSX+Sbo8N8avyFqAF5qkZaaJf8tqncS/du6BQn2cqAzkSTqKk7ajhVvUUjlLH/9FXfwnAy7zeazqEeNIZQk2TOQOk2RESBd0VU7aiPQ0bYxfBq/xtZQO80iz0/jnYJ1NEf8hjjw/tQd5E09lYTn51sU1Ybr4T22mMvHIMqWj58SxbeO/qgfL62RlfrrAwbp2VvGfQxemlaaeKx2tD2kTtiESG/I81YnyMa321nQKrEM7TxX/dfUUVAZtM8VlHnHoN9rOSMZ/Myn+px//jTEYGR1FlmXYZdUqLN1pJ/T29snNREYW2CD7TLE8AnU3kl9tm0AglMl5bZnxdJWepK3Wc3iTmzBuupoQs6yn+MonEUfB+nlNimBkpzgUqX4IC54qUwVPRDDGbxIav5jKc/8XcOhD3LxMaLD9nNg+JljPc6/Th3j6i6aKfu7kE5voebCH2lVtEvkGsf253mmu+YobZBSIXmiiIQJInxCV98fq2E0gb5WBNLzHCdcqiMUq4HSqbjgHXH/QvoT80iPTbMtQznRi/8wY9PX3Y9GSJejt78f42BjGx8aQZdmkPo20STOrjP+T+zVbWdCp9q36ZE8si/Sn+imdijyzHP/zzN00lz/qxv94Z7fKmcpNHGst8rzh/Nrnu/E/6kugLgrV8T/+sN3jf3XsU5p6rnS0PusCk69PK2XOwaRWlI9pvXlSbZ8C69DOnI+7dplq/I+b9gSVQdtMdWQecWY3/s9k/h/5a9pIe6jcdXrZKeJf5dayTn5Kh3mkSf/ADOKfslBOra9yqj3Im3gqC8vJl7y1DmGq+Kc/1elHeZWX0tFz4tg28399wxuBuijMJP5brRYGFi4M13Eqi634XUzbcEMVz60PV+pf9RMFV7danygxBGNZBBOuf+Jw6xKD27aFxdAU6Au0czVuYr/MY1pPwbSJ/4mJCfzwp/fhimt2w4YtS7BwyTqs2PMm7Hfg7Vi8+HaMDm7Atg0l+ucvw847L8CuuwM7rdwMZNtgigZGRhajVVgsHHgQTzxkRXiyKuXN42Q9ZhL/k/WycxD/fPOa/pQO80jzTyn+MYP4d+urrn4qN3Fsm/hXfQnURWEm8a82UrmJR56aprxKU8+VjtZnXeIQn0eVJdXJZNXxX+2t6QgWrs/IAK+btf6zJUBYNyNPVN4EVR8ntBGS+Fdc5hFnLsd/k/gDeahMwUZZ5q5ZrYUxrh1MG73sdsV/bK/0p3SYR5r0D/wfi3+VM5WbOHYO4j/zfbL7ZWFjmJ9StNsZ/+zvHc2HIP6lXWkTrZfiE1iHdk7jRm1eVy/mTvYtyqE6Mo84cxn/PNbpkabVhip32h7w9Vg3ta3KnZXyznFWpCJakcQYVMSjUKRBHH0NnyqT5hFIS0ENqAobf7cxX73Lux+0HGI8DTTjG4b0jA9a6mlMfB1UWAyj8ZJOUOtR1tJPsl09R8MmHSLlsdJQ8Dhqb8pTlvG7GmlbsR6dqyzdR66D7Xx70GmVX9A3uTBQGfijbMTN8tzZQ9qRE3bqSXmy5M4Y1aslH2EPvOj0nn7Kn3IimRhZ665EMnn0v9FoVPBVR7aJTQLF+nbMMjexADDpNc8qh9oLAEo/GVScLBkIedS7MFVOtifrpvKyzQv/gXfauI4HEnmVLu1KIO2O458xFPzCbZQrzSzPAINwYwaM9x8Byq0wVfxTd0wX/3mOPG9UyqaKf8arAsv44zm/m0eaxNV6PFK/LOmPbKfxn9DUdFkWAYdHtR3bk7xYT/XhOekynz/Kxh9tRz0wh/FP+sRP+VNO1MQ/eW9P/LNcdaOPEVQOpllX6RInaxObD3/8u/oE0u44/hMfIo7SpB3r8gikpTAn8T+L8T8FLVObaL3p4182PWriv9VqYXh4GMtXrMDuj9kT/fPmIy7GBZK1aXdkQTWW3YFtT3k8qpRPD7bCw9mC9R3Ez0JoGwCQjT5jqFbsXyLYZMFQSkJ+VVZ900bIM3HT0/GNOCHFVyPC24V4ykeUq8rpoLKhKOObtW4jkU+0sNwRd/xIukK3HT/jxyQrm6J+vLX+aIyXxutdaWTmJ0BfJi3A02VfIXSsqxD4EQ+eL+ubVPaKnep1BShfNY8+4/LdJi3PnNheNn+MfNyRMjvbsK74ov9zOvnN30QsgvN39ePY5/F8EqgdmA7y+Gx/nL9gAXbdc08sWbECY2NjaDabgZ+OBcqTafbJTGOa8b+kvUJ/FhdRrKdL/UKdHTT+N7vjf8BRObXNs1mM/+FpW9FH6ZMu7Uog7Tkd/2vGRrUtduT4n2fIG40gg3nYxv90/h/xiaf0lGc5x/HPeqoPz0mX+fxRNv5oO23H2cR//fwfyZNfD1388zqWeYQdEf/lDoz/MPfw7lKZi3iIMkefQrgZNIPOVSxvegv+w6OpTDciTqQY9YqZqitow0TAOYn/Wc7/b7n1Pvz0ksfg/i192PfQX+GoY36KU0/eite/fCmesM9jsFP/KuyxGFi1GFi1aAWeuM9uOOali/Huk7fhqNf9FPse+is8sKUXF/98D9x19wOhXVJ5oj0fefHPh0jsDOLfejrML2cV/4+e8d9qeobxb3dk/CcyqSxKl3YlkPacjv/i6yEvj7ZFx+O/O8+MewKYr3Dl2qyOGQBgS7/+1+h8/S+VAWI71TWtN/Px38fHjON/cl/ANmEacxT/ik/Z+KPtNEbmbvx/9MS/pllX6RKHcaH5dobxzyeAS2tRlAWKskRRtIKs7XjgkRj/Ylt0HP/RJ8o5Gf/dkfKSD+HCH/wXTn3PaZUytcnvr7sWLzrqpYEmeRKY/tp538QRz3kmnnbks/G0I5+Npz/vOfjmBecHnC1bt+AfP3IGjnjOM/GCl/0ZvvGt8yo81Rfq6LNNmMZM4v++G26wvGtAladR1KlYrsJZ7wh0UqYdU/eefWVOGqyradIgWL8rzmDWJzD5y2XHHYiLcJl/0nRSuTgqxGAsD68i84+V0zZW9GadTAYQ8nNP+hQAzKRBrgLiSJSPNkAyMMAvJrIs1BNbMT/331Ei1D39qw5F4IIBZVAdgaq8agtXFMvYoaW0aB/4ug35OHioSz9L7qwgD/qBFV/iMZdXnrGc9ZQOZeKR8qqNrHUTB5WhLEs/oXBtDgBFK3bebB/yVVA6AT+RkXlqr5SW6qs0FbRO8CXxcZaTT1mWwceVXjmT+Jd2oexlWSJv5ChaBfJGNf4NZSkt3AVmZ/FfsUu7+Bf9Qt9TlGG9WctRE//kAT+w9MgdVZTf1XHyGmNQFq6Oykkek1vIgbahxoHjXe2oIb7BtLalpwjr74Z0A2L0LeJjivgPNMs28Z/4saaVx1Txz4Hatol/9TOlTx7TxT9lZjnrKR3KxKPGP/EUh3mlxAPzWDetk4LSUXxdeGee2iulFeWc3D8StA7bTn2c5eRTlnGMU3qqr7YLRB/SU3mZLv2kYy7Hf+XDXyfx364cHcQ/bcO6Zorxvy7+I1TbKuhsDEZHRwEY7LLrrujr7wOAmv06O4nGZIgxEcFU6pqavUEHxNEjEp4qw2Sa7qj1qjEayqy+jjDlWa9jpJ3yd8dJejNtwj8W+M1ZtkFZw1twQo51ckuMWCuLqlwgDXYTEEK69RdE9OyjTD5O0oaqGtpXTEDrsFwZ+TT5kOckkDJr/caz0kvsQHmpqmUb+2/6eQtKS3ilNW10Ax6uHdiuFd1dWZB9kl84Wat2dOVsH+pMn2G7hI1g6iU3GKR+rDS03SrlaRsSKvpEHGMMxkdHsfa++5Anr4Rmf9LOP2wZ+0t4jVUuSL8ftfJ15aZFvgqM+AGSfpRp5THb8T/bweN/aYEWgMK6z/o4nnH8n/T0ael8N88MehuAgY7/cXzQOpQthaqtYp7KyDy1V0pL9VWaCqxj4Z/0nnb8r5v/x0WR4C8djP9lu/G/0QjXs9EO1TixdvJrd20y/m9oAveUPfjlWI7fjVs8WFrYrIAxJaxpAbDIsiaWNSbwxAZwZE8DK3p6sYvN0UjeSEa/Lkt3wzTlovyY8/G/CjqHo31pbyT+wXMtU/t5jIq9CMG2SfynoDTb6aB0NL3nOf0Bpw4MgDzP0MiBRp6hJ8/QyA16cuOPGXoamTvPMvQ0fF5u0NNwuK6eq5PnBg1j8JHH3xbkmC7+CdSPx/TV4SnOlvEtOOt3n8Ev1lyGbRODgc6OgJ36l+HP9nox3vH447Gwf2HSvp3H/0RzAjvvuqqijwMDjo+kEXWNfRPruDzyYn14GiYMXdZabB4rcO4NQ/j5hhLjfQN4/k7Aa/fqxT7zS8zvyb1/Kg8ni6fkxl0Tx/91DzyAnp6eGc7/q/1b2/l/WSIfHYF5cB3M2vuQ3XEL8jV3wzy4HnZ0GDbL8Mn7H4fzt7wZCx97L574pPuwz8pdcNvtd2PjptXYsnkbiol+LFm4CxYsXo7+YgQWFkWjgZ7eBg46eB/ctvY+/P73u2Jo7UE45s/vwklvfzIVB5K2nJv4d/lzE/8xljqJ/0zGz9mO/2qHVGZ4PbZn/CdQJh4pb6obcZhX1lz/s+9g38s6KSgd5aEyMi/1cwWVU2kqaB22He3Ceiwr247/O/j6398grPqTl8pvp73+d3sMlI91QP1aLTf3SOZpLEcH1//t1/+2d/z3Oncc/2V8W5t8AxjaK29H/MNaXH/DH3DCu05OS3DVLy4DAHztvPNwzufPxT998EN40fOfH2gaY/D766/DCSefjN/8/NKKb1x/ww244Hvfw89+fgkAYOGChXjqUw7HMa95LQ55/OMr8qmfqczk8ciIf7dpiFnP/yO+ysi81M8VjO9ntb9NQevU+TjLyaeU+OcTxayj8qgdnT5xw1zlZbqcKv4TWZhOdbbTxn86/lfju934byu28dfK0s5/+OMN+I+vfRW/ueoqPO2Ip+IzHz8LnFsYY7Dm3ntx3gXfwn/+4PsAgN9c+svAj3JSBgD4+vnfxAMPrMVLXvQiEFYsX4FdV7k52rtO+xssXLgQ73n332BkZBRvOf6v8dY3vRlvfv0bAz7tw7TaT3FmGv/mgRtvtKwIbwAjnRyJUEGWZdL5kbAVB/A1A3M1MNMQZeoEZGOpEqp05j8eHfjpwFJxVr8IkPCGyiPOnPu7RihHWk4ZA12ZKGdZhlIW9pmvfFhWJpMKlc8FuOfDBQs6f6KX1uWmsDHuqUvqqLN70jG+U6Vumb+LhA6U5TkKDqL+Qpnl9BfSCXw8aD7a2N4VeTvQXpmBte4OBrWb6mh98LMd8ry6+Uu6PLJuNT9DWRbI84bcQeZe3UwaCiq76kZ5VE54W7DzIb7KpudKF9I+ipsuoKR1Kz4pdk2hTnY7Z/Ffus1QufGB/NQulBGA+67FFPEPkZNHwLl2lsZ/guvox1db8Ck8BW03tmPu7xAqy+p371juZKxe6BgzefM06FXjH6RvJ8W/k4s0WY941F/tyn4iq/gYNZzc55KOSb6dkDH+WzEedBBN89Bh/KseKbCMacoy0/gnjah/5J3yUL46YNIupKGgsqe6pXJiRvEfebFc21lxI99Ii0BbpPqlMFl2J9/cxH86/reP/3blGj9qg9SGd5Xz8ItiKba22GZAWVosMS1kYYLoxlG4+0WwSz6BVywZwj+sXlyp48p5XrpzAGXp+o8VfSXeuV8TS3vchFltncqm8sfyaj/DsrIsMTY2hp6eHqzabfeK3SJYxIU7jZ94bibvBSVQrUt8d6zSVxuzvJoX9QUiHZduJwTp14GWqYwunyQn6xjlpo1DvvUVqJOj5Mu9zXyeu5D27eU3fetk1adTdJMw5FkLmIgX7BbkqapJqSIBKVZlJVYSY8d8iIFS/AQoChDrOHMJXWlvEJ/trjQSvwi0Qk3l5+2C6qud0/JqO4vBJhnR8y9tReUqLmKavlzh7uQBLMqJdRjZ+N8wrQfQ7H06lu7yPK+bBcphABlMPjBlPIS4SNuuxi4V28s5oSwKrLv3XrRaLfT39cHWjP/6ikb2L+6mOicX+aV9bpbxNXI6/rt+jTwWrViBnv7+qtWFt09U8yUvxbFlibHBQRQjIy7fA2UH3EIy7TiX4/84ctww3o9fFgtxV7MPYy1v+wKUGiFpgOa2JrZcthbj9wxhz5UNvOZpOZ51cI75fY6ma2fXV1OetH9XuaJ/pONCbG/SRUfjv9jXQ934z2siBaWhdKvjfxzDiDfd+K9vapo0/mfuhupIP/oi5THG9b114/+QzfFfwwO4ttnA6qZB05Qo0QRMCxYtWFPAmAJAgSxrIctb6MnHkWcTWJqXOLwnx4uzZdjD9ld4g3NWsTHbraJbUj7z8T/1j+jP1lpckK/A+WYZtt1TEW1KWPQY4PXlRrwRmzytOI+H+D9qbE7/Mu3m/zIf7mT+/5hz+pNe1YEPJ8AAeeY2dePGr9/YzQx6G5nb4G0Y9PgN4LAxnOA28gx5ZpAb4P898Y7QXqnPUF/aXNuEx6KD+f8/XPFh/HD1j8P5QwGv2f9V+Icj3g/MJv4zg4kJtwGc4sB1xzJeGsDPsfgqZlen2jcZv65W+rE2yuHwHhiawHsvuRf/ffcQSmOw6/77Y2DJEvS2WjhkURNPm9fEsfvzxsbqeO3ZhXGZunIDWPN4JGSV6/9qfbWT+kA2Pob86svRuP5q4N57gG3bkBUFLYHSzwL/8sZX47p5T8KyA36DVbvcATOyCqvv+SPMyEb0NxZjxcrH4TGPOwRLdloOu/FebN24Afdv2oK7163Hfo/dG8W8+3Hv/Xti85rn49DHDOOcT+wb5KCcjH/tS1O5mUc86q96pXikT5hZ/FfjoZP4J23ipPmpbgosY5qyzOX4n/JQvtPFP0Flp25W/E3Xg9B2/I+y6bnSxRyO/9oeBKWhdB/S6/+amypZTj1YBpGTR0KWZWg1m5W3CSquQXV9Ue1DYB7rsd0CftIG1C+tx6PKn9bjOctK7xv8/InKR5rM4wawDbbx7VITG6Sf6kioi39Yi+v/eANOOPkkfOGz5wQaZVniSU98IsqyxNfPPx/nfP5cLFywEBd+63wsXuTWUYwxuPb663H8ySfhykt/AXj5f/bzS/APH/kIXvPKV+GZT3saFixYgOHhYfzqisvxkhe+CIc+4QmBB/lRh0du/Mf2Zn4qJx6C+E8f/tve+G/MOP6rc+QZxb/4Ylo+4/ifbv1f6JO3Wi5dx9+8ZQv+9n3vxZte/3pc9GM37zv7rE+EGy7KssQ/fvTDeNx++2N4ZBhf+cbX8ZtLfxnqZ1mGtx5/HHbbdTd87IwPwxiDU07/Wzz5iYfh2De+KchFeay1ePrznoMvnPO5cEPE18//Jq7+7W9x9lmfjDLvoPHf3P/HP1o6KgmoQbRBlUEKKRMH8VyVABAajnmlDxh45ejgNukMCKRTlv5JQ++cxjdwKk9qsFar5egmejl6bsMzC0/1Rv0jLe8Q4piURYG6GRPv2iDvlGaWZZhoNpH5u8xNJh200kucgOnSWjQaPUEWkzlddSEg84Ec5PK6pbT02zRtcXzHwDT5BlsnnQJtTxzLDo93eeRuIs92Jk3WJbAeafGKgjisT9ncubtLiLKpDQmcmNTpmUJdvspKvsbbn3ZvNNxT8azLdkDiC/B6pL7HctqSfHSwUZ/zFSr4qXxzF/9pbgTWJa1WqxW+RZdlGcrkooJ87BTxb2Sg1fiHxj/FtTZcyJqaGFSb0x5ss7w2/k3YPAu2KmIfRmBbcHO2jjdpZlmGZnOiEit18a+2cWWOtrU23LGoA1tqN41/tkek5Ta9mG6L49OUJ9hA4p9lpKHyUF7411VQJvLEDOKfZSozJsV/vKmEdJWW1q/TM4W6fJWVfCkj7T45/idPTimT2j7VP70Db6r4p6zEr8rn7EL8FDeVQe2loPzqgHVJa7rxn3xsm/g/Y3w/bC6c3GUJlKW7M9Zai7KwKP2mqy1t2Mh9XN8YPrjrRrziup1grctzdC1s6fmWrBvp2RJ44comPvh497oi97RcNjn+RQcC76ZX2zL+m80mSmux+x6PiX5TGc/oC9GuLk8YVMD5BRf1UINfpVmlXQ+KMzmdNrn6h9MZk3BjnuKltFGRUflMpVttuc8wJj7VG6sJgan0FCyXW7+ZaOBfI2zjufpI0DW8bVilqSqgUkwywKT+QDYUyYvlpEODCK7LrubX0p4GlF89eD09LW7c0rqWTwCB5hAbeMQocWwR1ov83f+JsXvR279bwI8W9pvBfowryzGgHIYd+hFGttyAZnMEI63dsHKfv0ZP/0o0R27D6JarYLI+zF/2XOS9KwJNiH3o96mtjMdR23JRyldwR09H+9GyLHHv6tVo5HlYDGef6arEu7at77saPQ3f57k5B2kSOA7xKV/2x3wCGADmL1mCJbvsEuoov7q04tWV8zg0NARs3uz6ZSlv+LcWcZ5FeWnX7Rn/R0uDS7bNx9e37oT70QvbcuOB86fkaAFkFtt+9gCGfrMejb4MPf392HMl8L5XWTznoBwNJ6Jvympbq6y2dvxv1Yz/M5v/lxu+j+a958CWY55rEEbSfchXvBr5bscDphd2yvG/bv5f1aGT8Z9vb5oE7HOlLdFm/NdXRZPPxlaGM7csx+qWQTMDLFooTRMWLQAlStMETNOHfQtZ1kKet5BnE+htTKCRj6AnG8eixgSeb5bhlXZvmJo5OK8Hy5r5f9oGasPUnpPH/zgXo21brab/HrSj+XKzHwDg7t+MV+pOBbs9uQFYix837gSAMBfh0xzkadrEf7D5FHN7dDj/3+Ns95aCAEYGZp/O/dO9jYbfAM64uevO3RPA1Q3fkPYbv43cIM+A3Ov1icPvDHo6VpPjn7ZAMv+vvf6v0f9ZX3k+BhtDAacd9Ga9WLVoFRb1L8JA7wDm985HZjKMt8axdWwr1g2uw4bhDSjcXSdTwiK7EL94888mxR6B8tGn1GettWgVLazYZZfKdMJVN4izAcaYCd/31XI2odpCm1Xhrf91O364egil57dq//2wcNkyX2rRWxZYaZr46EEWBy11fh/6C9+PWitv27DA2vvvR2+v67vq5v983St1b3v978Fai2x0BH3f+jKyP14LOzISbvcrADQqvmBw5LX/gE1Ll2PhnhfDZL/F5vsz5D0PYuFYCyt33g+r9j4Ey/bYC0tXrERjdBs23XcHbl99K268/35MtHIsWdVCWT4ZI2v/HDv3Gfzg2yuCLdO+J8iXZWiG9b+ZXP+7tJ2T+I9jBDqMf6bJNy0jDZWH8uJRev0/+Qk8pw9lJV/KSLtv7/jPcjNF/JNmqgPxU/kmj/878PrfPxxSN/4zJmzb6//Yd8b4dw/xFEUrzFuYnxl/gZHYwNTEIPmpLdlm7df/ZjP+V3nr/D2bNv6t3wSOtqnM/7cj/mEtrrvhDzjBb+JGO0acr513Hq75/e9w77334YXPfx7eefwJoQ2v+8Mf8LaT3okrL/0FrH/y94R3nYx/+uCH8MLnPa+iE/2UNn90xX+7/NiGpE/Z1JdmEv9FWU7yPZYb2nIO41/XqBWH7cK8MLEQUH51wLqkNbv4r/oxZjj+h/JKDFb9QW357ve+B9ZanH3WJ+DmRFV7fu28b+Cccz+HK3/xqyBfnuf43L9/AQsWDODYN7wJWZbhXaf9DQ5/0pNx7BveCFPT9xzxnGfiC+f8Gw479IloNpv45gXfwm9//zucfdYnH4rx32WQCBucTOCFTBlpOeSd0wj4MWj1WPr3vmf+btO0Ey7LsvK0o8pi5F3boHM0vOPD34UsgUiclE7Bu9o8n5IdEoC80UCr1QrypHq7BnHGK4WPMSbKInSbrRasTHhpXzYQZcoyt7FLW7O+8keymRvru/eZA27AcLgBLdAkMKAy6VgDLWOQyXv1IYOm6kp7kl9RuO+QBj1ER/IgDmhPACZ3T0xneQZr42sV9Md6tBWhVRSw0uGX/r3wvLh26M42Wea/TQu4NhEfK8t4Vxp5aLsoMJ86aXvyaK1FqyhQ+vf2q53haWp92p7y8NfT0xPSKgdlpt6Q11Gk8QS4DXbWVzq5z98x8R/r6LGU+DeV+I+DtdpCZVH9wPj3nTVEN9th/JOP8szzfFL820nxb8K3U8nHtIn/lv/GRSfxT37MJ47qoW2u9TlRCPEvQJqEKeNf/DP9qa6Uty7+SZvyk0ca/+Sl9WYS//Rb0ixD/MeJBDwP8oGffNg0/rWfnYP4p12YT3zMSfz78afD+Gecozb+4x2QKq/amjIQhz+F2cR/1mb8V1uoLKrfWOlsV3a4+VtahwPALWzJ5u50m79labF+1MlXFK0wtlnL7xsaGJOF11FZv5ngdG0C0s6078TEBFqtFlbtupt8VqA6bju1mRFlrwO6l7NdWloFtgcX+lIw/kUlrszhuB/bkWn6QvQLY5JFvYo+dbLFOYxH8ukoIwIPrRdjUW0TZFBbeQW4gejq8cdFgqqdeYwbjcxN8q1rM2v52mi3o2RtPEZ7OzDGeFxH0dmA6ShvJg1RocDYFoM4OSTmRGYTGzMeKYf0E7B+ThYwaoB8k8ao6Chy+4x49HFmjMNTeV2T2MTKcRHHVVHp6G8W1hZojd6KkQ3fxsgDZ2FiyyUYXv99jG75DZrNUdx/97XBImwTCwuYHINrv4uhzTdgfGwzJsa2YmTrrShaLcCWaI7dj+EtN2B02y0oJ9YFWzlfjm1bsaX/WetvZPUy8miMQXNiA1rNjcGOTp5q+2RZhlWPeQwmms0wJ9E+n3MmcP5v3GdJgowBL9oZHY7/BOpZ91Mc7bc1HWSRMp6DF6R+ocP6eTPl5W+2439RWtww2MB59w/gpg3AlvsGsWXtILat19+28BvcNIgtt27E8LX3o7e3if7+Fub1jmDzWI7f3plj81DUh3Zjf65HuwPH/7E7/wV2/H6guSn+WpuT9FoU9/8bmre9G2htnWb834Hz//BN+Hh0Y+L043/LAn9szsPpG3fF7WUfWnz9oSnZUaCEe+2zCzf6lUFZuj6jVWSw1gAZMJa18L/5alzUuAkj5Vhl/l9MM/93dD1umP+7OrSnkYU04lJXhHamn1QX3JtjTUyMNnH9U9fg94ffheuOuAfXPuXuyk/zrzviHgxvHsHQ5pHQDpSDfqeg7YcO4z+0ofxUV/pI4a/BK6D8Q/y7Xt21FVy7+ZYsrZuDldbNv6zvN0v/BhdeRxelRVFYNEuLZhG/Adcu/lWfjLHZ7vpf2lmP023+LuhZgCft+iT85eF/iTNedAY+9YpP4fOv+Ty+/sav47w3nYcvH/NlfPrln8b7jnwfXnnQK7HXkr3Qk7mbedrBNjMI0yb+IXFEvaHzfz6AYLxxAWT+QQDWJXCNrvTzYhdLfmyUJjQ6lPtWs7C4acMIXnL+zfjBnXHzN6AEMJjIGlhj5uGt1zXwo3smwrWwkT6C8lrraFMO7YuMMWFtB76NGHOQGKBvMw1r0XPX7eg75/8Drv4VMDwE4xwSsBZ56NOAFgwKWKwt98HwtsdgfGh35OVOWDK/D7sv2ge2NQ82m4cJAKtvuwV3r74Fm0bHcfe6jbjrrjux67Kl6MuB1vgijA3uiqGtu2HthsXBx1z8z/31/8Ma//+Hrv9L6+fIMn6rDpRzR43/mC7+Z3z9vwPH/6TPMf5m907Gf9pCZeE1NsFaG665MSn+ow+kdOgj5KM868Z/103Mxfi/PfHv5w++rciTNzJRju2Jf3b6fLqz7gcAH/rAB/CVb3wDt95+W8XPXV2nx3cuvBBPe8oReMkLXxjq/SnEP/OJr+3JI/WgXdTOmEH8904R/24+9HDF/+S26Cj+ZzD/py1UFtUPIf6nH/9TOjH+HS/lqfGvExmWV+M/FAfZyrLEO952PN78+jcGXQHgnHP/DU997rNw9Otfh//64UWVdv+rY9+C71z4n9iydQtuX30HvnbeN/C6V79mkl+Sr/KkTtR3pvGfkTAR+W0GrUzl1UisxyMZkznz1OFYxvopH74qinIoEJc0ytK/GtlVrsjAADPiMMyHN5YuNABu8zjzAdxoNPyFSdRH9UhlYbpMJkDGy6F4lI28CIV3FmOqi5XEh6+jMsMvPFMfJMFmjEFT7rQwMnEwfvBI28CGi63SbbB6HG1f0iIv6k2aGtQKxLHWImvkYUKgMqf2IR/WA8PSt63K4eSiXWUAFx9P+VjEu9IUiM/OUWWEb6+idE9rFaV7SprHpm/HTF6pV8qdKqk8wV+8D3NBuChcJ2O5KVHjR0yTTzuanLim7aeymO2O/xgTzMumiX9KbLLqjQcdxX/i67Xx7y+I3c0aLp35QY84pEGfI2/qyzqEVBamy9LfyOB9Sv2dkPo3ofSbRZRH+VJOTROY3y7+OdiynUqJf8qstPj0UCkxr2n+VI5S4t92GP+M3bQdU/uQD+sRTNv4j4Mkz3nUuiqLtq3iYIr4VztSfx7Zj2ezjn+XpzYvkwkw8Zkmn3Y0WUZ6tJs++WW2O/5jvDBPbcuyduM/5aUcCtqm7txO3vz1G7jW55Xp5q83T7q569LVuiwPOln4XSr3zW+VhRuAZemeYrLWx3+eyyaNA+rYbDaxctWq8GQf5fdMEIQNbiJxXw2r0A6TwDj9Qj1AFmDjeQrEcTRtSDtcHlGR1fFw49bkjT+C8UUqk+oc6xLPncRigpEN6arN0n7C5ack3JaqcXXSQiDQJC2PWcm31tflhrc88QsvH/Ot3GnKuR08TZZVZA9+537O9KpXXJUlHy13zeDnkpLvCsMjQYAV2wR5I6SmId2A42k7vUKLubxS+LgcQOtX5KJvODvo94jgbeQTck4cg9bYgxheez5ag1dhbPhuNId+i4mtv0Bry39j873fxsYNq7Huvps8trdJ2cT4tt+jYR9A0RpBls9DT98ylGWB5uhdsDDomb83BpYegoElByHv393xTu1J/dknItrSuMKIaAxs2cS2+7+FwXU/kvr+dXUOKeT39vVh5W67YXxiwi/MZDAmCzic/3PeyLf10CdmPP5LP88xJ01Tfz2v+6U4yrfd+M/X4XE8pR6sp7JON/5vahr8dOM8XLcJGN06jLHRCYyPNf1vAhNjExgfb2KCv6KF5h1b0NMq0T/QwLz5OXrnN5ANZPjjpgybRn1MAShLtyhFfp2N/+7uf8pJsDMY/7NyW6g3Hdgtv0Bx76fRag5Nag+1KWUxczn+Z+5TIrMd/28t5+PjW5Zj0OSwKAGUYfPXonB5pkSJFqz/PrOFhbVc+DG+szBuS8cCyIDLem/BBQsux3A5Gngp/3J75/9y/U99HJ7jwzzyAoChLSMY3jIsC0+RttpE08NbRjC8ZSTk181TzSzjnzidzv9pae0V9dwGW0aburmaz3OtC+s3fAs/dytKly5Ki8JatIoSzcKi1SrRKmIfojajjnoejl4e2oxl2rYE0pwSCqBhGljYtxA7LdgJNrMY6BvAbkt2w/ye+ejJezC/dz5K43xq6cBSzGvMg/E3KEwFtk38Eyg/02zjSIA6GD/H9dnWF1bmYqzk7KJ0jJ9W6M+YDDc9OIa3/eguXL12GH4iHn/Wwods5WcavTjzrgYykwFhfknOHC/d39Tz/8njhml3/Z/naNx5OxrnfQm483Yni4Vf/C1RwF8j+Dl/VpYwpUVvzxCaI30Y2/p4wB6AJTsBe/aX6OvrxbqtW3HbbbfhvrtXo5H3YPPWQWwZHEQfSjymt4nFi0qgOBDjW5+AiaEFQCNu2tTFP/WbSfwTmD838R/HqpnEf/l/5PrfSr7akfrz2H78fyRe/++g8T+9/vfXyOhw/J86/t38S+U2JkNRuI29LMv8228y5DKWU5ZsFut/4eGyGlmYZvsHGcTHCMwjL0I5bfx7enIzD+CeIKY+EP+kbjOJfw4Ev7/uWvz+uuvwu2uvxa23346S8Q83WB/6hCfgta86Gh878+OAl13lzvMc/3PJ/+LI5zwn0gZw/R9vwHV/+AOuvf56rF23LsiTtoHah3pQXoJ5GOJfj2pHtjuPD0X8597H8bDEf/xmOI/Txr/49NzEf+fjP+tRlizEf+xDyb+sxD8CqB5B7g7j/9NnnoXfXPpLXHXZr3Hi8Sfg3/798/jfn18S6LziZS/Hb666Ei866qV4y9v+GgcfeBAOOvAg4CEY/83am26yajQSojEyec8285QRcSBGdg3vglPzWIeOkmXVp17VgKxLfOUHeVqT+HrOuswnfTpkIcGY5zngy/LcfUuWThDKtdH94lGWvCaCdzJSHivOStlJLzSE6M48fd1y0FvLg12iDfRpW3ceg9ttfDmaqYNyEzzISKdJApd8kAyeQVcbF/pU59o0N+1rBg63sOUg6ELbJa8I0KO7mIn4pBt0SwLEGL8om/hV5u2YyytRyMeYeLcVgbToV0ovSwYC+o/SrObHducxyC/2i1DtgFmHR+PtoP4G8vd+0ZC74Bg3cxP//gnfDuKfsmYa/xU/r9oibRc+OaL8WZf5xriLysK/zsW9NkbiX2KznCb+DfnmuXvNTKIbdQL8ArjYqigKNKQ9qBd/Oqml/NXyql2IxycKqq/wqNoZNfGvcusxXbgjH0wR/yo36bRLE9K21DLWYR59mbh6TPFJl3UpM/GIm9LPpol/5ae0ti/+qwO36sa8Ot5pn8c6PJop4p+65yH+ne7UBdsd/84e5KU+QzzmU1bKqHmpPuRnjMHp2/bBcGlQFo4WN4R5A4O18E8Dx83gA/vH8OHHbMbLfrvUb7i4err5GzeEHV+WP3FpiXOOmHDylPHNI1nmFrrT8Z9yg7byb7fI/aufszzHrrvtBo7jYRW1AnaacgCwGB0bR29Pw98dLXV8eTxP6aW4U+QDrr6RjUav12QeSARO04S0vI4nQf08LUuhSsv5Upy/RWkEz1af0KxuMDKdMva0pI7f8gMMN0AdFjcwWU7cND9IpvvSanMF5nu7EEelpc2qbea10zITdVE8sI/RPKZFd6VTzWO1qj3dWZDSC0xkUYBEKnbTXIdobYkNay7A2MaLsGjJnjBZjkZjHga33I1s4Bmw/c/ATdf9CE96+puwYNHOrr3KFkYe/E80h67EvIFVGB/bgi0bbsHWoQb2e9IZ6F/4WKdHOe6+DWjczRoTw7eiYQYxPrYVfYufhiyfT0Gj3nD62LIJiwJZPs/Na3xfObrlt4BpYN6iQ6r6J37gwGDtmntQtorwWkyC9XMg9ovWuq8Yhv6zzfifTxr/PSdjMG/xYizaeedKP5byTPPTY1354OAgsq1bQ3k6xuqmP+VnOccy4uoxxS9Ld2Pm1Zt78P5bF2LNaA7bGo/xFGLOAoY0LExmYf9nI/q2tdC3oAeN/hxlfwNlfx/6B3J89IUTeOaeJXoyV9vMavz33CbN/6MdeIxtE8fCsSsPhvWbZp2AMQ2gsRDVR/QAk/mYr2YDFv7byN4d8z5kK16N3secVCtv8CnRqSiKcDMnrz87Gf8LT2tjK8NpD+6KbSZzm7so3Eavafn0uH8V9ETcDAaQZc4qWVagJxtHT2MMPY1R9PUMoa9nEH2NEfQ2RtCbjeKJ5a54zdBzgk+1Opz/U37iprpNHv+dbt+7aRjvu3gjjJtYwMAfbYmBo54Eay1GL7oasCWMLd0TioLjnlgsnZ/aEq0/ezasBXp/8vNIU8o//OqD8PIn7hrsTB0oXyq3HunPCtRJ65HWnuf0RzxM7sF4nofv+mZoZECjwVc9+2/85gY9/M6vT+eZQZ77Y2aQGSDz/eXnnxk/mswYMVPM/63HI67GGG3DfoY0Dv3GEYEHoWEaWDmwEtvGtmGoNQQLi75GH1YtXIV9dtoHh6w6BC953EswXozjpzf/FNfefy3u2HgHNo1sQqtsIbc5Vi1cha3jWzHUdPVT+N0bf1NpE9pfQXUG28gA4+PjWLmba3u3yKl9pYEbL+Ff/QznM8YAiPOkdva01uK2jaN41XduwwMjTVhU/QQAVu2/PxYs2ynNDnDlM8cBv0Ed5kxeRmPc+L9+7drKzZGUj7IwP423LLn+NyPD6DvnTJSrb0Vu3XVB9E/3zd8SQMPbBC7q8KpbTsQtI8+DXVxip90vw/LlP8H89SVuu28dhsZLmLwXvfP6cfjTnoW169Zj7T13wIxtw2N33xmbFzWxZdvLsHXtkbDDi/G4x92K7355j9Cf0KbUi79Ut3blsS2jzlpGfNLoPP6r45kCedbFP3kqnsqZpgmpvlqmuhB3JuM/bYDtvP63IpvyU1rOXlV5s7bjf9V36/J5ZF4db81vV5e6MK11bOX6P8YN7UTZqEe2Pdf/eWfjv/qn6qw6ujUy8ivdK5EDnjsPdW0Z+hnqpm2s4zvTZYfjf6Pj8T/aqi7++ZkW5qU2Ypkrd3zcumLEq87/Zxf/mTG49g/X44STT4LC0444Amd//CxYa/H188/Hb3//O3zq/zsT2wYH8do3vRHvPOHtOPrlL/evjz45fAP4qUc+F1/47DnhO7/WWjz1yOcGuie/4x148zGvr+jLNGp8m21GXD2m+LRF0G074p98WCeOHpP9SullD1H8cw8JNXWpC9Onvud0nH3WJ4LuGv+88bbz+K/6FPnS1tkOXv9TfoqnfJlP+pQr7v/FVzHXxf+7TvtbGGNw9lmfkLek+JjLc3z1m9/Av37+c7ji55cFmVJ5yF95nPvFL+DGm2/Gp888C9sGt+G1b3oDTnr7iXjVUS/HtsFtOPNTn8Tg4CA+feZZQXbaR+1CHmwXlhGfNmD7qH2lneKucpncZcA8OhHzUhyWIXFCpuk0FA5wm3J69ckyKsI6EKOW1sKaeE7FicMGLOROAIiMxlTv4jImPiGR+81ftYVzknj3RNigTJw1b0T7FHzaUpyYv8pgojJZvyAmgWR4F4Q0qpPDhIkqZSFY674B5rLjxTfLKCNtqUDe3PxV2bQt1K70l0KeDkhxAADGv/5DLnUYjOSVvrJDn67lwkBLXt3g8DJHPPE3DWQrd/EEW8gFl+MdOw3WzfwGeWn9BnvSmaiuaZ7x/qF3ktH2k22ZgxNveBkpE2kRV+u5uzUBIL4WXNsN3g7Gd3yUz3i/yHP3/evMx6Hxti69LzrSLm9HxD9lJXAgK0u3SFoX/6TH82wm8V/zGiwerbQ79amP/9h/cPOXdUmL+Na6GzGYJp71NzOQjzEm3I2s8hgf/65c47/qC6wDb0P6HPGDzyfxrzSID7hXSKof2Q7in0eVjzgElR+18V+Vk23BOM5q47/qd6Sv8U9e0PhP7EcZbM3CHnVhHbULaaV5lLuz+K/GeWoP5qvMpMc8jQHKginin3qmddiOBOY9FPHPMm13Au1Pepnvj2ey+eue6iWvms1f68qtlSd/wxPE7hhs4N9cQbnS8Z+y0lb85X7CPTY2hhU77wy9mKhZA6zeEOUX7hxY/OEP1+PMM8/E8ccfj5e97M/xZ3/+5zj++Lfhk5/8FO6//35P2lZ5yNLXJH6hyNcxWpXI3PD1BdaCi4muQP0iJJlTPfV8og+IbJOODlfbsB5coTF+ozL4or9o4VxBahjie3sZI4uSXr+q7b1h/KllVjiJ6fB6Q+WdKBA3fmNOxS6Mf8FwPL1vKU3jb+LzeKRhrd+YlfrBl309aliRztvR2SfKk9qvFkTPmIyrr1z0jUguF9bjqJ1MIp2XobKBnuVYvsdrMNLaHQ+uvRVbHrwVm9bdiN7+pdj8wBW44rKLMDoyittv+t9AtizGMD50M8rSojkxgomxzRgbGUXetwsafTuhLLahOb4ByPpgTA+MsWiN3IDxzf+NvHktWtsuxdb1v4SRPlDjvTV6C0YeOAvrb/kwHrznB2GODWsxb/GT4+YvGI80iNfOmFC+bOeVGBsfD7QJMX4c70bDLZqz70nHVaYn+aEv41hJnHRMUP3qfsRhvfRHSMd/fsLC1owD7GtnMv4PTZT47bYM6yeayMttaGSjaGQj6MmG0JsPoS8fRF++Df35NvQ3tmB+/2b0DW9CY6hA7/weNOb1oJzfi2J+H5rzcmztH8AvN87DtibnCtUxjfaGt+WOGv/HJoDBMWBwpP1vaCzDeDkA9O+KXQ55HfZ+6pux99PfgL2fdgz2fupfYO+nvhp7HX409nryy7HnYS/Dnk/8M+x56Iuw5yEvwJ6HPg97HfYc7HXYs7D3YU/HXgcfgiXZr4IcqmeQL2kHHnnNNJPxf2sLOHPTzhgyfALAAihhyxZa4xNojU+gaJUo/WanXsuVpYG1BrZ0/UMc10uUpUFpgTwbRd4Yx+29t+PO3jVuE2gG838eK+N/u/m/f6LOWov3/XQDjC38Bm8BlAVMWQC2wPDt6zB8+zqYsoCxhd/QLWBKhxvObelxSoyvfgDN1feHc+IZT/eM715f8S+1PWVSUPl1Tmg7mP9XKU2GUO7bo7QWSwcyLJtvsGy+wcI+hDlcYd2Tvxks+hvA/F5gfg+QG6BVWDQLi2ZZolnE6yXUxD/7DUifpn0MwUwz/0/BwOD5+z0f//Tn/4RPHf0pvPTAl2JezzyMt8Zx1+a7cMntl+DcK87F+3/8fvzDT/4B/3H1f+CKu6/A+qH1aJUt7L1sb/zN8/4Gn3rVp/De570XS+ctTVkAcq2ibUZgWzKPevJTItFPMxj/Fhj4dSPjh9is8np293M2DGxCHtdZmkWJS+7cipefdyvuH265p+ytn2dVfr7R2/1CvyGsrB/PrRv/1ecYZ9SX59k01//5+DgaXzkXxe03w5QlWhZAZTxy5+4V0C4NC2QA9un9I/oxDAuLophAszmELRMWWW8f+vtyNPISKJu4+/absf7e1RgdHUKRNbB5HJgYH4TJNyLrGUZf7wT22m1z8C349mI7sR3ZppD2nen1v52L6/9ZxH/oB0Q+4hBUftSM/6mctBHjOJvh+F8X/8qDQN6UT+Ofb0CkvxE/bYs0j3LviPGfaeWnMUBZ8Ei6/pc3ZqV6aj3y45FA+5OeOy/9gw+xbd3roAt5EtjpyLU/1UGPtAd5q97txn+uSbMuy6a7/sf2xL/fhKI8KhPztzf+AeCqX1yGqy/7Ja6+7Jf4zJkfr/qst/XiRYvwzuNPwL9+4fPYvGWLDPJRvvUPrg95xhj85ueX4qpfXIanHXEErLdf6u+UU/0gxONDHP9sS7Yz8YlLWmke5Z5p/G8bHAy4mk9craf8SJN6sI7G/88uuQRXXn1VRc+0Trmj4n8G839tdwLtT3o8z6YZ/9WGKmd6pD3IW+VQvlqP5RA7o8P4nz9/ADfefBOMMbjoxz/C7rvuhqNf/goYY7B40WKc+LYTcOXVV+HOu+4KNPhwF+UlkC/ze2YY/xkFDpMm6aR04KBzkCjzjXcwNZjxDqxMg4FKv7Hn69DwFMhI4zOvVRRAZsJrVdU5kDgIeZMO8ZkmzdLLEWiJ7Cpz5OeejI2mj4YkzTzPw/dWVR+mrf+FxTs2pDQMpKOibJncQaHyURYtY2entrfJhKwubf2FGWXX9p7EVwPR651CCBATv5vBtmZdhM7Z0Q3t5eVQvZAEGvzdoATKab0v57l7shvie67Nfe2aTi/o7f3USPsrDeJrPu/2Mb4NKIfa3iYDNPxTqVqH9KkbedDGxrjFjbBZa9x3qwu+ulvudCr9OduUdLWMk1we6+K/nMP4J15d/NtK/Me4oRz8ljNtA/cMh78LEP4Ct038F9G3KIceVXaVWfmF2PLcaQ/Kmee56wM0/v0msAJ5pfk8p7+QbxoLlI9QFP5Os+2Mf2vd3Zp2BvGP6eJf8NvHf6xD26U6s77qHv2gPv61HVN80qWepKF+YXZ4/EffJi7pp3Jo/Kdy0K7lLOKfF0vkXxf/Khf1YT5lJ13mkSflVbm1jsa/yg3xG8qRyV2IbjPQ+k1cbvBa2GTzN27iujLL/LAYyTxvU9n8dXJ52omvUj7+0C7+ZfwHgIlmE4sWLUZPT6/0JAl4Fw/15AnKBzc8iK989av48Ic/jJ/97H+w+s7VWLRoMRp5jhtvvAnf/s63ccqpp+Ab3/gmRkfHJtGcdMJkEIXMmef4VoFyVdtWwYmeEDdG0sQTG3gdA0I493nG6F5DYr9Y11q/0hmQfb7ge8ldHmWwESdsLIZNxiBw5GvlaVQbNzetdRsT1vrFUDEDN4V1Q5gLn/wD68qTO8aP++lcMZRZp0f0mTjGGENbiszqu3IMbck8XzfQTXAqc1mPazx/V+5Qq/aL8jq9xKah3RHyHG9ubmu5B+M25I3pwz6PfyfMgudiy1ADa9c/iK2DGRat/HP09M7HFZdfgbX33Y4bf38RmhOjMHk/8oEno8BOAAzGx0axdXAME81e5D2LMbzxFxh+8Eew1mJ86BaMPPgjNCauQI/ZjC0b/oCx4QdQTGzAxOjdXgwDoMDY1qsxuPYHsKNXYMGiXbBwYT8GH/gWRgfvQNHcDMtvlwYFqH9sO9BUnm5vXy8GFiwI44yCfs6mKIrgN8SzMxn/ZawIbe7LdQzQNPH0XH/av7NvT8d/6+e0czX+jyDD74ZG0NcziPk9mzDgfwt6N2FBz0Ys6HW/gd4NWNC7EQvnPYjeTWPoyRaip78HZV+OVr9Bc8CinNdA0V/iJ5sG8N37BrBuzG8wznj8Lysb9JjF+D+wx5FYdehbsethb8Wuhx2LXZ/4Zux66Bux66FvwK6HHoNdD/kL7HrIX2D3J74Oex52NObN7weaDwIT64GJB4HmBqC50X8zeAvQ3Aq0tgHFEFAMA8UIUI4CxRhQTsCgwKKddqq0944Y/zkv//HoEtzV6nX2LQpsW78Z629eg7U33If1N6zFg39cj003bsDmGzdh6K4RFKPVvsCRcf2utcb/ANgSGdymVVmUaGXDuHzerzFmxwG4J2Aor8rM+QZmNP676xFI32y4oSubvMzL/rga+R9XJzgs979kk3fhjX/Ewpv+mOAI7eRtQnUxr2ltW/VDtYnSS+mwFUyS1q6qBDCvx+CDf7YQX33TUvzHG5bgC69bgpOfNT98zqMsLfZeluGth/fh5Gf14cSn9+EdT+vFix+bw8C6TeCWO04V/3Xzf94ozTzTwfw/hSft9iSc8LQT8NKDX4pXPv6V+MiffQSnPvtULOpbFHDGWmO49v5rccPaGzDecv5ljMERexyBD73oQzjx6Sfi+Y99Pt7ylLfguKcch/k98Q0ShFSOjub/8l1kjrFluHHRgvMK48eHVmHxzVuHcdyvtuKdl2/GdRsnwvzEtX0ZWtRaiwtu2IATf3gX1o23XKC1/QV2tT8Dg9J/fy/jTRLea8ImsPiZ6yPd3F/jkaBjFmPWGoubb/8Vtq7+AzJr3YYD5/P+VePW+jnL0qXof/aRWHTyaVh2xr9g2Yf+CU97+WIsXDyMLB8HMIxyYgQ98+djl11XYI+9VmG33VdgpyXzsXXT/cjNGJYsnofFSxejZ/58jG8bBuw69PZtxYKBMTzhQPfmIAL9lPoReM64op7pWJj6pZaF8XQ7x/+ZxD99U0Hjh/j0U9SM/6xD/qnOrK+6zzT+FZ9028X/Q7P+N/Pxv06OEP+zuv6vyko+LKdNyY/6MJ+yky7zyJPyqtxah7JTF8qGSfHP6//oQwTVz/UTru3L0r2JpCzarP/LUWVXmdn+qBn/2YeQZhz/21//M2/r1q347n/+Jz792c/i0+d8Fv/x1a9gzb33AlPFf2Yqr60lTJr/zzL+OWmxbeJfr28B4DWvehUOPuBA/PuXvxzoEQ583AH4/XXXA23inze3q021jYLOOyD+r7z6anzzgm/h81/6Ev7tC1/A188/D1ddc3XQm7ja/kqD+mj+XMT/xk2bcPeaNWi1WpPk2N74/9wX/71Cj2WUcar1/9Qf9Cl7yk66zNtx8d/Z+E86xGeaNEmDR5U9yAzAyM1o6qsOYrxA4v+v3nE8/uHDHwLaxP/w8DAOOuDASfk8p78MDQ/BwN24WBSFe927/xnK5+ViflEULkytf7uAT+dZFvCZBoD8tHe+8wx1UA1AKwOGNqoaO/dPtSio0sQrxRmQdjzSiJlXNjgiHSN59z3EqciDx9CA/khelMGY+L3RkhtpibMqbW48qQMpHifNqqPWT1YtA2R+k1LrqL3sJFtKGyX60dEzOr+0YUpf5SlL98SlMfKESDJgqAyBdzLIsR5tArg7Ukvfqdhkgqn4mX8sHz5NPqRNH3TnWbizWu2lcpCe6m9Mcsdpwj/Y299JYn1nzaBP7QGZ+CoPtZPmGYkV6uSaor3fBjvV2BbG2ZdAPYwEN/PqbKQ8qBvTegy2n1H8Z5OekFAZMEX883XdjYaLDZbXTXzceXxKKbURj4GXvxg2/i0CRi4AUhul9uEvyCN4ipvydjp536uayctVraP20jx4WpSHZY5O7gYJiX/ipTLpOWRADnnSxxBUBuZXbJHoH+VyOJ3EP+VQ+qRdjf9qTKX6sa4O+BX9BJS/6vfQxX910pTqQVopD0Iqk/LUvDobKQ/SYVqPczX+qwyYIv6zZPxnear7f48sxnjp3vLE1zZzAVE3f3lelhYrGgVesGwc37i33437+qSvtWF81aOjDayaZ/GKvaJeKpPass6+xsT4Hxsbw/IVK/zr7Sb7JNA+uyha+KePfhQ///kl6O/vx0knnYzTTj8df/mXf4Vjjz0WL3nJS7B40WJccsnP8ctf/hJDQ4N49rOenZIR8EJNYqh5SZnx/4zbdJPMyZDYItJVfzEezW0WpvYDAD9Q+vyQrJFfj6leqYwRx/HyMhnjL07jGxxctnF1jK8rsgZyopsxbrNScUwWbRb8SETlprCr59QOOEGGCGor52PxWMlX+8XKkbUv07QYGYb1BC/kJ3gukW7SBk4xJ9WFOMY4cTNy9fZ0BppUp8rdIu9ZiqUrD8eCxQdjdKyJvQ85HYtWHIr9HvtkHPbUF+OeO2/Cxg2rMTz4AJYt3wsLlj4BY8UeuP2W32LJzkfA5Cuw7+OPR0/fEvTM2w09A/sjz+cha8zD8IM/RmvsXoyNbcL42GY0J0awYe2NWLTiWeidt7OTwhiMD96CoQd/jN4eZ//mxDaU5QhazSaao3egb8HBMCZ3i93lKJpDN6NorkOWL4bJ3Ft/qlaOPrVtyxb09fWFc3CsSeb/7EtLG1+tzHzj23713Xdh7fr12Lh5EzZs2oQNmzZi3fr1sHmO/vnzMTExgfHx8crR/cYxMTGO8XF3zjKVif6t/eX4+DjyZrNSZvzTv1xw5VN6HB/MLMZ/k2W4Y2gMF6zbiNwModcMoa8x4l4BnMdjb2MEffko+hoj6O9rATfPw5ueNB/HPCfHCw8GXvS4Bp6zKMezWg08vchw+EQvVgwtQnZvL1r3zMPouoVobu5FNn8cjb5oX8qfyurGyrgAk+qQ6qG2I87KlduwYKCBgQV9GBjod8cF/RiY34eBAZeeP6+Bvp4JZHYYKMf9O52t+1kL+RCmTyO8XnhyuXtd8VDPUZ2P/97vVG5tJ7QZ/ze1MnxvcCdsRA/Gh8ew5vrbsHXtFkyMlihaBoXNUdoGylaGcsKgNVhgfO0IUGZoLG74scHCGIvMFDCmQJ41kWcTyLMWehqD6DGjyLNRZFkLw2YjDpx4LOYXA5P8SNsgq5n/K57icmGzmmdwzhXu9c/u52xqLF/v7H/+9c0hP8FBKI+vhNY6PHdPGZd4x4vdIpPqlbbDpPm/6ExgPbSZ/3/m6p7QD9M6PDcA4lhi8Lonzce7n7cAey/PsWpRhiXzc3zvujH8cW0LxgDzewxeelAvnrNvD3ZeYLDTQIYVCwy2jVn89t4WWnzriwVeu6/7trXqhynm/1UvjW2jumTJ/P9z130h4C/uXYxjn3wsjj7kaPQ3+pGZDEvnLcXjd3k8dl+yOy6/6/Kw4auQmQzP2PMZ+MALP4Dn7PscLOxbCGMM+hp9OGiXg/DL23+JB4YeqNwS9I5Djq/4mupBSNuITwCXZYmBhY6He9LXhhaJ1Q2+f+coTrtqENdtbuKGjRP4yb0TOGJ5D3Yb4AIvnM8Zgx/fugnvuvgebJ2oLr6msNtAD/bdfSWGjBuj6uBte7bcd4CBuPFr3I1g9LXRkZFK39L++n9yH2OMwebmIL668ecY2boBB6wdjfMErxMAmP55mP+8F2Hpu9+H+S9/LbbtfSgeWLwvhnfZD3s9YU/84vJxrN/Uh6z3fizoX41VS1Zi0aL5WLRwPgbm96G3p4He3h4MDPRhwfz5WLJoAZYvXYx1G9ZjvLUf0NoPe6wYxwl/uQiLFy2gBAF0jONRddE8eD1t7fX/5PU/4pFeSp8wF/GftoPKZR+l1//lQ3L9P9lvlT5ppTwIqUzKU/PqbKQ8SIdpPc7J9X/yemyI7MRTvp1c/7t+KQPCWwra2dHr56/pVRezHet/iqe4Vd7VPMJnzvks/ur447FtcAjNVhMbNm7CHXeuxpmfOAu/v+46HPmc56C3tzfQCbYs/Y0sfLLZ083nKP7XrluHi37yY7ztrX8Z2kfrXf+HG/DA2gfw5y9+SaC97z5742Nnnok9H/MYXPXba3D8X/4VjDEYGJiPf/3C53Hks5+NnVesCDbOsgw/ufhi7LpqFZ5w8MEwD1H837NmDT752c/igx/7J1x40Q9w5113YXBoCA+sXYvLf3MlLvjed/HNb1+Au+65G/vtuw8WL1rUJv5je88k/m+/4w4c89Zj8cDatXjWM55Rif+77r4bS5cswaKFC7F12zYMDg1iyeIlgVbKg5Blbi8GXvcsy7BtcBtuue1WrFu/DkNDQ1ixfDku/t+f4b9+eBEA4ClPfjLWrV+H+fPnYXx8AvesuQfLd1pOJsFmPNbHf5S9o/iv8TvaU+1Fvp3F/+QYS23Eo/IyJu5lGOP8xOkU5bv+hj9g3fr1uPSXl2F8bBz77L03hoaGsWL5clhrcdsdt+Pe++7Fdddfj5tuuRlHHP4UrFu/Dit3dp+WWrt2LXZdtQqHPuEQXPy/P8NXvv51PO6xj8XChQtx4Q/+C//6+c/htFNOxZ6PeQyW77Qc//r5z2H5TjvhwAMOwJatW/CVr38NW7cN4tQTT5pkS9pI9Ztt/BvAfQMY/o4nvge8lDtPyFQJECz8nbO+I4mGduUpQ9LlOdOlvxOAuKXfDDTG3Smo+GljEV/PFZdgvJyhTPLUWIoP+AXgNkEezvmMiDgkdeKFMPN9xUCHvKlHCLzE5vzWQVEUyBvxI9yEsnQvWM5kMUXlUdl1c7QsS2T+9de5fBeBspGGMfEbuFGmqs2sn+wVZVFZkCItlmt7WWth4QKSvNNyhCCOvsly9Tu3cdiYtPgQ/Dls+ru7Yvi6a/X3dkCdSU9tAPFLQlpG/AjuPM9z94Q7c5OYUfl8NSChWaeDAcK3dBUfCQ/KRDtW7JXEv76GgFDXDg4n0lccrcN0WRP//DZG2eZVXxVdJsV/bH+CMbphAfcKGbFN6supzORJnYD4/Q7WYx0r8a80rfV3RwN+jdwtsqndU5uTPvPp42oDxoX1d/o4/6zKo7IrH6Ypb9FqH//tZCJYxr/ElerDcidflA3e16aP/8k+pH6ntmFd2pU01M4qp/KoA+rM+moDiF8S0jK1X8SJfS5B+aAu/j1YuXmknQ5KR9PKw8kU/SC1l+pVp0NdO6T4iqN1mKbvEZf21TSB8py6YU8MF9nkzV//Wud089eWFgfPn8DH9t2Gl1yxSDaKHc1Qz8bXQ2v5YUsLnPvMeEckZU/PKaPqRChaBcbGxrD3fvvJ1pUFuLnlk5WJCsEA37ng2/jq176C/fd/LD78kY9i8eL41InWueWWW3DC29+O0ZERfPBDH8LLXvpSVxBok1HVN9P2UjwAuP3223HppZfimt/+FoDFihU746ADD8Szn/1s7L777tA+P2wCGva7XkDmC92YzfqVolAO+KoVEFrW4sR3vhNHH300XvziFwtK5O1MEJ+6jfIIkxqoNk9MsR0dBRHOx6dLVr/3m+Koj1QYAZPrTdK/SkNjJdg/TddApd1Te+h52gDi87X1pa3jUz4KceE3mtUnNB0gWr9SX84jqKwu/957bsIPv/sJLFg4Hzst3xn77H8E7r7rTixYuBzPeO5rUnRYa9EcvRvF2F3IJ67G0Na7UJYtLFnxeGxcex3uv/8+PObg92Kn3Z4LIIO1E2hu+jZscw2aY1tQFuOYmBjGxPggJorF6Fv6Iuz8mJcib8yHLZsY3XwZNq65EECJZbu/GgPLXwBYI7K7NNt49U03Y9EiF/fa1mU6/mu5bxvSKMsSn//ql3HNtb8PfmN9v9pqtfDyl78Cz3mu+16XwycO50Lk6vJYDljss8++WLBgQcWnSXtoaAi9w8OVPp14uZ+P89tqaflMxv9mWeL7D27Cl9c+iLI55jbSjN8sM6W3ZzzPGxaN8X68a+ETccjuvZjX66w+dm+BsSt7MbixFyMTLRS2Dy30wtoG0NsDmzWwqL8f440NeOyrtqB3QRzHbdvxv2qXmY7/u/R8zj2pay34jVhH0238xTTzBYd1tLxDOg/M+1ylnyEYU3P973+pLmnbMc2x8vej/fh/m3bGxge34f5b7kJpcphGL0yj4Te3MpgMbpMX/qnaYgJojaExYLHgsfPRmAcYlGjk4+jJh9DXGERvYxt6G0OY1zOEnnwQ/b1D6M2H0chGsUdrJd48eEKY66hcKjP1UBvUnSM8eVkd/x931i1hE9dt0Dq7GzfBiMdQzvOkXDaC2577jeCr/7+ja2VnW2ma8k51/a96Wpn/h28A+27LxmSlN955YY4fn7gCey6LT+es3tjCa/9jCyYKoCc3eNLuvXjrEf3Ye6cc7r56993fq+4p8O9XjqHZCkMOvvfn62rjn3JS/rJ0b/XS+W3W4fxfvwH8nL2fg3/+83/GwasOruAAwND4EF77tdfi6jVX+9eTR1jQtwBvf9rb8Z4j34O+xuSN0Yv+cBHeceE7MNIcCXm/f9OVQE38E6gb2yHokGeYmJjAilWrkhaIaQ7LJ/1yC867S94S4+EfnzCAvzpgPpbNyzEyUeLMX9+Lf/vtWkwk3xFX6M8NnrRqAT7+gsfg6xsW4WcPTrYl4arnxk1yzsPCzXF+Hrj+gbXo6+tDWZbhpgp4vVO/dDjxHABuGbobn1j9dYwObsE//PgBHPSA09NYuHWy/nlY+Pq3YN5fvBl3ji7AD34/gWvvKTA4apFlwE7zC4zccBVuuXYAd2+4HfMXfBZb7x5Fns+DyebB2hyFbcFYIM96ANOCLcdRtCzmLd8M23Ms9l3xeLzs2RbHvPbxFb+knNQl9UvmKx7z66//4/hPXzBTrP+1j//43dM6O7eTiWD/RK7/o0YRqDPrqw0AhE0RQrVMx/8Iai+C8sFs4n9W1//Rjqm9bI0vKtS1Q4ofHpCaZvynTLSvpglOntgnOBz3hoCUtrt4d8lKfo1tqCtB9VJ8tQHP3Rwp1rE14z/z337SO3H7HXfgFa98JZYsWRLKAHdz+OW//jXuWL0aP/n+f2HRokWBH+UrWi00Gj1RHl+33M74t2WJP9z4R5xw8kn4wjnn+Kmfq7fXnntiyeLF+Np55+Ga3/0OZ5/lvglMGp/793/Hd//r+xgcHMQ1v/xViKv3f+hDuOqaq/GaV74KT3/qU2GtxV333I1zPv95vPVNb8Jb3vDGYJ9sB8X/5i1b8MWvfgXnf+c7ePITn4iXv/RleNbTn47lO+1Uif9Nmzfj11dcgYt+8mP87tpr8YbXvQ7HveWtWLbUfaKBtuOmobYLeZEvz1l26+234cR3nwoAOPiAA/GZj58VcC76yY9x1mc+jX/71Gdw8IEHoixL3HHnaixfthOWLVsW5EuBbcMH/cqyxDfOPx//+oVzA85Jb38H3vLGN+HVb3g97rv/vkr9/zz/Aty95h78zXvfgwMfdwDe/5734ID9H+todhT/sS/BdPGfxBLPmdZY4Tn9VX0BYmfmpTgpLqGSX4n/OAYT/6nPnfzQxFOfcgQ+8/FPwBiDU07/W1x59VUpCq667NdAEv9btm7B57/4RVx8yc8wODiIAx93AI7/q7/GM5/+jKDLH/54Az51ztm46eabAQAvev4LcOLbTsBuu+4abEj55nr8z/TJy9I/Cg7vWJbG8r/Suif0+P1e4/Egd0NwMGPDMM1jw7/XPvODDZKBufD84ZoGmQzUqgjpaZ4qzMa01i8Ce8VdnqtLh4U8Zk5w9fVugUif9YxxG9R8tRD5siEgTl+W7klb0iMd2o2NFr47K7rwtRfGmPDkbdTFp/lt5MTZiRPSOtGx/kleaT9tC7Wrbv6St6MRdaY9SrE/HZO0SdeBAfydnbQZnZN1yb/wryjgOWnqZDX3G+4qE+CflK2aJNiJfDUNrxfzCv+6AqZRsbGBtXx9nfvGq1+lcMuSJgNMfMIZJoPhk98+5rLkDrNIO/qPZxXKcnnVSK19xVf4Y13qw6ORu3sYB6SpoPFf1w6oxH8cuMjXdBj/xvhFJeteSTxd/LMvYr7aRPUvrYuTQMffSYe28e94UD6Vl31DKd+aUF7qwzwa4xa13ZPbxr1ZIIl/9XPS1HalHSLPyIM8VQ/SUEh9HBr/eRa+cUqdg507iX+5owrTxr+jR/osV9uxvNP4V3mUbx0oX01jRvEf+2C1P8uZVl3Ijzf1ZJ3Gf+Dr7rwjvupZ1278kW41/uPrVagf66Wgsip91Mb/7Md/5pNfXfzbMr6CqXbz14/57jyWA5i0uUscy83fUFfKZUNP27mcQfwXZYEF/skMRwAIq5k0d43dYYD77r0X553/Tey6627467/+ayz2m0BhcibwuMc9DiefdBKGhofx6U9/Gq1Ws4ogi4JBFGkj9pE6aN5www046xOfAACcftppOP200/HKV74CD254EP39fV4INxYCqT48qd/8RVDb1Y/uHxVzdg2nAYIt3UliCn+mOAoGDsfr7OwhtvFHWN7iF2NNKVo4BXg5nj6tGhY50z+xOX/ejAHSTeO0DrxtmFeJW+PtbatU1E+1Lng+yY4e2Dj60/oiC1QWr4+Bu4kM8HXFXsbrWvE7G+k48q4smsfVIpVoONdWo1uvRtHaxpaDhcXOK+bjL449A61mA3euvg3XXnMxbLEB/f2+zZSM16ssRjC84b8xMb4FWd5Alvdj68ZbMD62DQsW74rexmjYHG0O/g492SD6568ATIbRkY2YGN+GsixgW+tx3y1fwqa1bnEfKDA+cg8mxh7AxOhaTIzeB1s2g54O4jhkjMGCxYvQbDYrfQ7T2i8pVHzC4914y82T/CD0ocyrnLvFNJJyG79Fpdxai0H/HSvyTX8cnwj041I2r7XvZPlMxv+WLXHryAMYmLcZAz0bMdAbX//sjhvja6B7NmLx4hE8c7nFU/fpwZKBDD05YMZayO6YQPP2LRhdtx4TG4cxunEYIxuGsW3DCLbcP4wt927DmtvXobhzAe6/PF7XaWwG/WrHf38RPoPxH60hv7DpvifrNm/9uabDj3lSpw5nOjq+PSmnthuS8d+F7czGfxiDX40O4IF7NuCem9agZfphG/Ng8z7ANGDRQGkyWGSwpgFreoBGP2zvANC/EK2xHgzdOoxigjeINL0O7mjQQuFfBWnLFlot54v3525hbObz/6hjJ+N/+P7vpNc7+3Qlr/qK6LpXQFde+ZyeexwCdSFQNvW16a7/1R7qk9bKOpGw0R6M58ceMYAl8w3GWhajzRJjTYv3/2AbhsZLFKVFIwMevyrHHkv8NZH/HvCE//av+waw+/5vs2gf//zRN6lvCtSLOmu7qW0AoL/RjyeueiIOWHmAUIjw5au/jBvX3Thp8xcAhieGccntl+A39/wmLQIAvOTAl2CvJXtV+BHS+Nf2Yn/Btslynf/Dt4BrHQ7d8PNfa938lvMD/Z35x0G841dbcN2GCZz5q3vx+d+uw0TLN0jNb1lPjn86cg+cf/T+OHBFv+8/JtPlj3OfMF/yaSeT3FRnLbIsbiiyTWgDtpn6KevdPXI/No5tw3CvwbefvBRb+jPY0qKAhTUGvc9+Pub9xZvxg9vm4X3fHsH3rpnArWsL3L+lxH2bS/zhPoNbst0wNm8r5veshDUvxoJdD8S8nXfHTnuswJ6P2x37HXAYHnfw4dhj/1VYtvtyzF/5GCzYdU/0LX4uBnr2woF7j+HZz9jZPZQg4x59LKtZ/5v59f/sxn/mR39yryadVfz7H8t4Dq8X06oHQemznPKpDDMZ//VHvnWgfDUNsY3dodf/Mx//WVYb/7O6/q/61aPj+j/a2eVVx2e1yZatW7Fl61bYJGYoA2F7xv/p1v9vvOkmnPa+9+LQpxyO2+9Yjdcdc8ykzV8A6O/vx/Nf8ALstddeOOHkk4C28R/nHOWcxX9cCz3h5JNxwrtOxttPeRdOeNfJuOueuyON5Pvs1lq84XWvw6KFCwGJd2stPvahD+Gdx5+A31x9VaD3/Ysuwmtf+Sq88mVHOXI7MP43btqEd5x6Ci768Y/x8Y/+E774r/+GVx111KRN3SzLsNOyZXjFy16G//jcuTjzY/+MH/zoR3jHqadg46ZN2xX/t99xB05896l40fOej7e+6c2AvH0yyzK88mVH4clPPAzv+8e/x5atW5FlGXZZuQs2bo58FbS9GBPWWlx40Q/wtfO/iY/84wdx1WW/wlWX/QpveeObcPH//mzS5u+rX/FKrNplFzztKUfgu988H7vvthve/8EPYsvWrR3Gv7uBL20HPGTxH+lpntajXOoPncb/lb/4Ja78xS9x1WW/Ckdu/gLAZz/xKfzm0l/iqst+jd9c+ktc8fPLcOUvflXhRdoLFyzEe//2NFz8gx/hyl/8Cl/+/L/jWc94JiDj/6FPOARfPvffceUvfoUrfn4Z/umDZ2D33XYLsjIuKHOqy/bEf0aCBBqVTJUxQRUlvgJx6aRahzTVsZmf53l4cpT5rVYLWZah2WzC8B3XXsHC39nJHxduuYDFzSo6mDHu1c/wG2n67nylba17piAuMLvgpi145LKg0lBbhBvj4fiqI0M6y4KvoZZAIi1jXABQN+oe6Bj/euysuvkb68f3xxehc3YXAW6zp9qulCvL/Gu8jPvgPduvop90eqxPGbUNKQvtBrhlO16gEQ+J8+byfnhulpAW24OdZJDXQ+RTpUudwEVZtrevyw/NczAxEnQ8d684hmubkjdQ5HC3LHMh0S+k+7+84V7tF76xg7gh6dov+hXEbk54/6uJo9w/1aw2Z1lRupsO1F5RB6eX+iNmEP8aa2p3VOK/EdKp3JSVZdSFfJnfbLVg8vr4r9AQHpwgUr9M4z9zNwOYLENR+NvJa+Kf/Ckb5aKdiceY409tqeksGcjcRKqA9TcP0IaT4z9Ofnju6OUg+Ur7+L4PxsWDqY3/+BaAtF0BhO8lkx/9hj8C7aL1tQ7zqAvtpvhpWsur8R/l4XmZxL/SI52ULmloWvXqLP5j21An+lgKrKftynxno+g7ah+VU4H0yg7iX/2U9lIdXPs7PQkpvuqXykBaWh/bOf6TL/Pbjf+lrW7shk1cbv7Kxm8sc2Oeq+tlCpscsvnr6bDcWgD+RgttJ+pNe6a20HSWZWhONDGwYIHrrOBounRIuP4I7O99nrW45rfXoNls4tnPfjYOOeTQWJ9AV/HH1772tTjssMNw33334brr/+AyK81kPfJkH0PY7Hb9FGBxyc8vwUEHHYi3ve1t2G+/fbHffvvi8Cc/GaeccgqWL/evEFI9aoUjz84gyODOfB7LAHDD0NqQ3xYYV+7EkbM+DRtNXZYArBvjU9wgPjdI5elTEzd9K2Z2Unpdqnlp3FhLezsiutVJ4HxG44+0SY82cfT8XNjEzWDj1dC6BGdWL6/QmGRgTwukq+BxTaWe3yiwPlWp42LMGL8QHCzoF4SNm6/Cz9lopIhHsBjd+js0x+5Ba+sPUYzdgonNP8L4+i9hbMP3Mb7+Cxhc+23096zDq495K575vLegp3cp7rv3Ptx71+9w9a++io3r75gUwwbjWLh4JZoTQxhYtDcGFu2J8dGtGB8fwfp1azBvyREwJsfYtutRFE2MjazHyLb70JzYhqzRh0XLDsC8+Tsjz3P09mRojt6D4Y2/hEED8xYdigXLDseCnQ7H/MWHwmTu1W/w9wJEnZ3J5g8smHQdYaR/ZnuyLzIy/rP/t37uFtKhDyzd4pLP43yB7ePaz+PJ5jDbybVR9E1Huzp3UH+j/KGOyI/tGP/HyybuGb0b8806DPRtwkDvRgz0bcL83o0Y6PMbwr0uf0HfJizs2YCnLl6KRhbH/2zEwt6zFY3xYTSaI+hpjaKnqb9h9DRH0GiOwI5vxfDdk7/NDLFF+/E/xiHHFZbX0Qubs/A/WwIofGBx49bGsvDTjV3Xx9XTEfqeprXO3whpe2o7Yhbjv/O3EpetBzY8sBml6YHNetxGLwxKfse3REhbf7PQYxcCx+3bi7fsPx/LigZG72nC2HH3lBCaXtUmygIwmADKJlrN0t+8UKCAm1eYWc7/Ie3nrgsn+zTgNoAnb9jGTV6MDcKObIId2eiOw/7I3/Am2JHNLj26CZgYrt8Y9ueu3aaI/6nm/xJP1Jf1VD/ihfEklEjajz8rFmR4xRPmoSyB0QmLsQngP68bxdX3TKDwfcfjV+V41j49yDKL0g8Ra7aUGJ6wmChKtAqLVsnNYH+NWxThWobXUNbzhfct7Veok6ZVr3T+T9h5YGccsuoQ5HLTMOHXd/4a/3b5v2FwfDAtAjyf6++/Huf97jzcs/metBi9jV68YJ8XIDeRtsqpoO1XhjWzuH5gk+s8N37E8QD+pj9jgLcfPIDd+v1AI7/xlsH/rBnDy3+yAf92w2aMtnx/UfNb0ADOPWov/OVhO2NRv7sB3troU3WQ+hHnQsZ/5o1ldor5P7z/KZCuMQZ3jz4A6/uwW3buxU0r+2BhkVkLLFqCRa94Ne4cHcDXfz2GezcV7pvS3j7Wj4/Zot1Q7jwPe+w9ht2XHA6Do1EUr4bpeTYWrdgf+xy4C/bYbzkGlu0Dmz0TreKVgHk5Vi18Op57KPDcpy/AbrutBOqu/yUeecSMrv+3c/yfw/jX+lqHeZSlfIRf/1sAzYf8+n9m4z/plXN2/T/Zboqv+qUykJbWxyzGf+bP5Pof08Q/ANyx+k68/k1vxOvf9EbcfscdFT2UFn+zHf/5JsDUFtZafO/CC/GyV70SPb29eP/734+/e//fYf/99sduu+3mPwM1GZ797Gfj7rvvxk9/9j9BrvDaXb9+rO2W6sUjbdFp/B/6+Cfgyksvw5WX/gJXXvoL/Obnl+Lqy36JQw5+PKy1ePPrX4/PnPnxgE8aixctwn+edz6uvPQXgSfb5lUvfzm++oV/x29+fil+8/NL8dUv/DtOPP54LF60aJKtMIfxv3nLFrzz3acCFvivC76NFzzveYHPD370I3z805/G2046CceffBI+/ulP439//nPAj/8veO5zcdF3vgsAOPHdp4YbCMhfbUtfyHz833bH7fj7D5+BU99zOk55z2l4+6nvwouf/wK8//T3AIjX9B/86Efws0suAQB86AN/j8GhIVzw3e/AGINFCxciMxlGRke9NhG0/cqyRMPH/ze/9S285Q1vwkEHHIgPfOiDeNdpf4vNW7bg4AMPwrlnn4O/O+30QONNr39DkHmP3XfHe/7mb7BtcBuuuubqSfZV/VIZtD0UiPtwxz/9m22jekRasWy28c/6qS00nXU4/jce6vEfHrQC0zQcK1N5FYRpV56hp6c34BTykWmI0BxcVYHCb1iFBvOTQX3cueArfv1El3JyEFQeSj8a2ASHKrw+rEfnK4oCVp7OoHyT5Db+CU//JJ/1m6rGZOHmSCeP23C23p7Qzs5ftFBnSKfqjq7h+OpiK5OosnQbj3HzyITNYsrIJ4ct+LSjwwGAvOGelqUNqK8x8envXDatTY2TUW93R0gGG54cikEB8ZEsc4uqcWPcAcsJZZgYuQ0KZ+Nqu9IOxrjNdX7EPMjov7taoWvjBIly8pjn7s4Ux5exQJ5OFv4crXiHMS8ai6IA/B1S6iukR75M064BL/MLyn6Qd4uAkYbqrHJSB0inRxtalxlsw/qsS6Cu1FHbFR3EPzfCGz09wSdbRRHahbLZNI7oc35QoPyUMbzSI4l/1iM9Y9xCQ+onlJ1pxn9Z+m9fe3/JJP5Jm6B8lC6XOfSp/LRN6I+2Jv4zTy/L8uDnzgYubokf9As8YvuqbiYZLDLfz1kvo0cKsd0u/klv+viv+hW0b2sT/4pDYDlB25d10nbVWKCcamPVh0C+ajPVNbUBj0ynOrFuJf49/VnFv/AlaBnbPpWTcqAm/hWP/PiL9eK5lmm70t7UgflV2cysx/8yxL+LQ8rRdvxPNn+5aRs3cKvHsnRjWqvZ8mvk9CX4dW5/HtbQ4+av2+hwPqJyE6gXbaA4qc83/J32AHSVNJ5Yn7SCYAzuvsvdhbvvvvtJvQR8PfI6/PDDAQC3335baK+IS9o810Kvn4lP7N54403Y8zF7KpIvJ606oZgX/ax6Xg/RvJGuk9+1Qzz68uDLfBo0qlcLvt0j8MYsNYb1NPzOVyhWHRwR8g5+wVj2f/pES4CwyS7g2FY3fj0bA2drg7jRnPoa8xzvCE4N2cjlL/FjZ1IpMyIJ61vZ+E3z4Z/w9Th1sjm7Uj6W+U1f62wedXTt4uRy9uMcyWe5pnGVAACZaWJk7eeQl2tQjl4PjN8CU25Ac/ByNMwoMHEn5uFabLn3a9hzj8V41evfjz87+m+wZcsI7rjtOvzuyu/gtj/+D6w8Qbd17X9jYmQ9Ws1RDG6+E4Nb7kSzOYqJiQJLdn4KGn3LARg0+nfD+PDdGN56H4YH78H46BYsXLwfFizaA739S5DnPejt60Nm1/snk0v0LzoUK/Z+B1bsfSL6Fj7BPQHsbahPSDlwN7BAxkgdy9hH0u46DqTjorYPN37jOdvN/VxzRryiiDesAbFvdWSrNNIfcRRsJ+N/3vn4/8DERjTmbcBA9iAW9mzCop7NWNzYhCU9m7G0sRnLGpuxU88WLG9swc6927B8eCMOXrh7kMEYg2JoDM0HN8NgBL0YRy/G0JeNoT8bxbxsxP+GMT8bRp8ZQk9ztIPxP7aNG+tmPv7Hjdp0w1ee5A0bujaeQzZ8K5u8+vP44byA9U8A143/VtquLEuYzKCnd2bjP+O3LEus2zKBsTHrN37dNQjHYo7BtrQoC4ty22a8tOcBnHvIBE56rMGpB/Tg/CMX4bl5CTtWILNjMHYcsBMw5Tgyuw22GAfKcZRlC2WrhaJVoNVsAcn1P32AwHaZfvyPN6fxGjrz17yTnvTlU7rcsG2N4r7ybNxrz8G9+FesMZ/DGnMuUBY49V3vxymnfACnnPL3eNep/4h3nfoh2NaYe92z30yGpwnZBJ4q/qmL2c75P/WMvUFytG5MftdzFmJ+LzDatOF39i+GMNGyKAqLJfMMnrpnL5YP+Ha3Fr+9t4m7NrYw1iwx4Td9W+FJ4Ch7o+76X/QhUC/tM1XX1AZad8WCFThol4PCOWHTyCac8T9nYP3Q+kr+obseiifs8oRwXtgCP7rpR/jhTT/EaHPywu7zHvu88F1cBfqb6eD6n/5GfyQ4dOoTf4cub+D/O2IxHjeQs6sPP2sybGsZTCxYDsxbAMB9R5O/3szixXsuwmV//QS8aL9lyP20gRvkrg3rfybz3+T0XhKe/q34o1uHaDf/V/217aj7H7etDjRHGwaX7TuAzf0ZitJi3iFPRONxB+OCqyZw/5b4EImzUvU3f69Dke+3F5506CKs6t8XfUOPw+j6g7Ft065oosRIMYHBLbthfNPj0TP0OOzUeCyedfAivOHo3fHMpx2A3C++2rrrf7l+ZhnHBR5Re/3vx4LtGP/nKv7Jh3kqi+ZpfeIQWE7Q9mUd8uJPYyEd/1lXjxC+M4l/8iMv1Yl1H9rr/8ltRTkg8U8bKh758af1lHeKD68TZVAZU9l6enoCTifjP3mX06z/mRnG/2233YqT3nUyBgcHsW1wECefegpuv/326vqf2HJuxv/q9f+NN92E937g/TjjQx/C81/wAuy0004AgMLPA1esWIGdd945+Cy8HLvssgte9rKX4cMf+xj+/JWvwC233urXZEv/SbwMpb8+KcP6fzf+KQsAfPRf/h8Gh4Zx7tlnhyd+v//Di/DsF78IZ539Gdx73304/LAn4slPPAz33X8fPvwv/w/PecmL8V8/+hGMMVi6ZAk+f/ZnAQt85F/+3yQ7UQ4k8f++f/xHWGtxxOGH4/DDnoSTjn873ve3pzn80q8IWIsFCxbgk+ecHXi96XXH4KKf/DjYYuHChRgaGgp8TJv4L335ffffhyc8/vG49JeX4Wc/vwRXXn0V3v3e07Fh4wbsvdde2HuvvQAAr3nlq7D7brvBSDsvXrQYjz/wIFz0k5/g/gceCGXartX4d2naQWV7pMS/0qc88Df4xM8k0pYmPKw2l/HPMng7pf6v8ZNl7kZK2oBH7ODxP1NFWUF/rKQGZmWeM22TR+QpuNankDznxhE74FarBfhNNFUYXujS4xM0+JU/FWbamMx/RygGDfHVcMY/EaUOQlxr/YJeHjeQmc8G0zrGuAUsyg86Qu6edKbdKDPrWL/hyIsrpZ1lfILRbbpx44gyNBo9gGz0ujulXRntx7qpbpQhlzsGqA99I88bcaNbJhmOnrMzZFOccmRZHu7apsNDgkv9yPGu+pLyMsYv+iJO3I0xyBv8/vD/z957x1tSlOnjT3Wfc+PcyTkwhCHMkDOK5KQgQdYEmEUFlbACxhUQDChgABUVFWUlqGt2XSUnlRyHIcyQJue5OZ3TVb8/qp6qt+v0uXPvzIDs77vv/Zzb3RXeemNVdaUO8teugTSwtBhjeQDgJn0Tx4+tCPgzhscChGN6DMLEr9RxWrKT/JI+0i7BT144GSeuwiGdlDVgyaCsimQk5cdnpmM40ydJAqMUqtp+79nwRUzoy+Kw9iF/FpfU60j93x6BTX1B7LyHsLGc/4uKjfFQQFLKfx8CBf5fzdwRdGKltvQdyoi/LLPfq87cLvt4MjdOT3ky3soy7KiVeXgv6TVC95QbZaaNAcREvI1W0Nr4yXguClHOZmgHpLlUsrZty7TlMs77v7A3WRd6+pw9SxmQ5xgHQaaFsAv5TPzJsPzffQ5A8EqIZcow2gJxMh/xMpz+bO0zyEKCEW0D0zOcuHmV8XDljMz/4w6JBcqlSEZSfnxmOoYzPdNmYgUaaQ/lBR3Ln8UVOoJJkiJNw3dWbD0v/d/6r5WLXVQj81M2fLZ8J64DlvrjiiknqZuc7RlTOPlrXJgdw7ZxHDyGse0m+TfuO8Gc/NV8Jh434Ownhwv9n3k37v9GdFaV8lv8vPw8RI8wdhJXa4M5c+ZEkQ4cf7JvtPXWdsL2pRdf8vSEQkU+eYXAYWDrEAXss8/euPueu7Fs2TJfL7kbBwaAQk9PD2666SZ86rzzccaZZ+Brl12GRYteEHQZPPzII7jssstwxpln4owzz8TXLvsali0LxxQtWrQIZ5x5Bp566ilcdfXVOOPMM/HUU24XM4CHH34EXxP5r7r6aixaZFd4k6K//e0WfPHCi3DGmWfgixdeiPnz5/v8XGDlF1oZS7sNDEHG7Tql/lyM5zXIR8ZTNFI2Lpi2x8FYkc4YN+EnUOXSwYSr86OiqyzX2liYrLVlkDkxiSvSeztnuhDprx4vw0U6Xz5tnxEiv6fD8WhFaOXoJxaNk7NIy3Il1aQZBuhedTPK2SNIVIYNa5/GYP8GdHa8gvZ1z0LrKnq7V6C/vwMd6xdisH89Bgc6sGH9cqxZ8TLSUhueW/AcXnnpJTy/4O+Y/9ifMdDfDaUUGkbtjvYNS5BlGVpGz0SWDWJgoA89vRU0N41BpX8FjDEoNYxHY4PGuCm7orl1JpRK0Ne1DF3tL6G/dx2yrIJUVdC5/kW327cMIIFKx0BX29G3/k70rv0rBtr/iayy3tmZ05tSANwEm2jbZLuqZftP22afNW67Xf3p6zvXr2UdamVPUzG5Xb8WbBifbfmhHxb/mMZspP13JdsFwbL9z4bf/q+uLsfUtk5MStoxOW3HlLQdU9IO/5uctmNy0o7JaQdmtnZj17Y2tJVaArJKhnRtL5p7+5CYXjSqATQl/WhUfWhUfWhK+tCk+tCsetGk+tCa9qOpYTBHS3H7HwZH8u1/Qf/fyStu/8Mxzjyauc4xzjKN/3HiN3rO4bE/o6swugoYeyVdiev/00+pN0sv7CekhD7IE/NTNsrV1eQ7TVO0r+2BQQpjbN+Xbbhsy6EN9PKXMW/t0/jCG8ZibGsDMtf/bysDn99zNFq6+6DQDZh+KN0Do/uhMw2TDdj+ieOJvJImaYdSH7Et12//A78mbv/dzl9O0CK3a5f6qwU1RHh85HPu3g0QG+f/mfN/jrfwSp/Xzvc0B7rE2IxyfclCHAhNFmsGW1MFeOO2jdhndiO0BvorBv0V4PqHevDSugoybZBpg2mjExww2+2IMkDPgMEjSypY36sxUAUGq0BFHAVdjVaR04b4bkn509+Yhr6HYfb/Cc3lZkxotQP4Er5z73fw7Kpnc0c/n7zLyfjLh/+C333gdzhsO7vzCO4o6BsevQGPL3/chxFmjZtVMwFMWyPd0tf4WSvW8zKdBfpceAcL4xysZRXeuk0zfnHkeBw3o5GVff4HBYwaC4wZD5TKgDFohsH5B8zAD07YDtuOb/aaN8Ytste27aj3M34Mz9Gr7Al2fA+ytA7d/yewzqcfUmfLutf4OiMzBo/MasY/t25FJVFo2ms/rK804KmlGaou3lYt8p4/hZ6WrbHDofvg6itK+NAJ12OfGfciWQM8du9MPP3gNiivL2Pf6f/AB4+8HF/5bCdO/8A8zNluFkruuEtJL+1P6pI002blFU4W1K9sNxnOvLrm/d8C43Ltf1R/sSzSx3JJP+u8GAdBpsX/svd/joVKMK/p+//w23/yIuXHZ6ZjONMzbTbk+7/FoQvf//N6TUc0/le//UfU/idDjf+NwP8XLVqEs889F11dXfjSxRfjkosuRldXFz557jl44QV7wo9MT5qkjKU+ZHqmYTzDdMH7/09//nO8653vxLTp0z29MZRKJUybNg0zZszATjvuhD322APbbbcdTjzpJPzwhz/EoYceine+5zQ3MWfnMAD4upK6JQ1bxv8tDikD8hzjIMi0eF34P3D5V76CsWPGwBiDi778ZVzyta/h1He8E3/81a/x7W98Ax//6Mdw5kc+giu/dhn+9Ov/wmnvfBcuuexruPDLl8IYgzGjR+Oiz3/OfbbIAmVFulkuYdnyZXjnySfjtHe9G+895VS87YQTfFyaun6tMTj9Ax/EylWrcOvtt0MphQPf8EasXLUKi5csAQA0Njaiu6fb21QsI8pP0qaicYdnn3sOH/3kJ/DK4nDqyHtPPS3Hg5TjAw89iO/96IfQG/V/Of73+vN/CPnwXjkbTiKbD/7vTn6q6/+WHqaJ/UcX+H/MO4Zo/1VN+w8YowHY9+okUVAKSBIF26eDD4d/F7cT5Ixnh4txVn6Zz6sUkJAICpzOyc6LJJxGQSEzL1yFRGEQX+YaHN57Bj1pzGuZzrIMpXKowKQgWR7zSOFJwUsFkie709bRLvgkvR4X07vyJM2KnQkAxtQaMmng4IxPL4zJuBcs4pXG6mXjGAySDQ0zgDBoyAleYTTkOXUv6OzYkMZqtWq/qSoqU5k/SdwOXZePPGX+mAXrgFyVYZw+jHgRYVlSruxcezm7lSFMS1kFesIqEMrQ8uwGW4VtgPSKiXbJk6ycZR7eK7fKROqaZcLpjJOKEigvre2qLOKEq5QS0cCxLG8HjoZqtVrToJJXTprYiVcLxMVyZSXCeAj9MY58JUliB2gS5X8adgCWZScb9f9gt3HZpB0b8X8M5f+iA8Nwn2eE/p9pO/lP2fJHPkmvxZXXO3GzfOJg2Srn/+7FbCP+z7ze/6tF/h94JFCGhFgmzEf+UtdBZ7lMK1c/SlykmzbLfFwwE/zf5pX+T2AZki7G857PG/f/UPdQhgyXP+KL+ZQy2Rz/Jz7auwQj/V90lLDJ/m9xWV7h/J871K2NsU5gubQbAsuPy5EypdwlXcxj3K7/JElRKpdd3cOJKptG+/bf5VXwtBnXuaUvZVkViePPylfsRBfDhJwYy7IqSuWwgIl9CtaBllSbzw8Km/zkr58Mdr7PyV8/GZw5GbudRfzZIwfdc5SHOqGeKU9pw7RXxqkC/9fGIC0733ErQSH0VhcUMGP6DGitsXjJ4nznQIABB9fs86qVqwAAU6dNtfFGO/nVQUAyGO2fDd58zJsBKFz65S/j5l/ejEWLFrnIAD09Pbjs69/AgmeewamnnILzzzsfkyZOwhVXXoGlS5YCMFi7di1uvfVWHHjggTj/vPPwyU9+Aq2to3DlN7+Jnp4egU3hp9ddh5123AHnn3cettlmGwAKN918E378k59g3ry57lvE52HSxAnum0qW4Hvvuw9LlizG+9/3Ppz1yU+ipaUFP73uOvT29njmlJgbpf2xXC8AUZ/Ugstsjd6FOXtW9ihjGWbgBkUFeuMGZP3krrFp/KSox0FM4c8435O00Y4YZu3MRwZ/VwWT1o4PWTfk0rD+lvV6iPWyYJj1mSAj5i0C7m42xogXWgWAE/qxYYa7wA/QuX4hejoWY7C/HdVKHyZOfyMaGiegOtiPtvE7oNw0AVAJBvu7kZZb8PD99+LX138Rf/3D9zH/8buxauVyPP3E41iyZDGeX/BPPPz3X6C/rxtjpx2LWXtej3LLtsiqg8iqGXp6KujsHkSpZVuUm6ZZ/660w1SWQqkUUAZQKbq7lqNj/UL09qxGtVqBNhprVy+EKo33cz66sgoDnU+iv+tZ9HUuQF/XAlR6nobRA4DTK2WepiVoUe+FY2a/AAC9v0lEQVSYTWz/bR2n7cuhCRO/RrNuChPHnOjV3q6Yn3rWMK794Isy6z7S6O1hGO1/ohTSzWj/e6svYaoKk76TOemb2knfKWkHpqYdmJJ0YEZjB+a2bIWsGtp83V9Bw8pOtKUGZTWARjWARtWPJtWP5qQXTcruAG5yO4FHpQNomRD42bT2vz6vBHvPSVztfJb30eSvD3Np4nQSD5gmc/qTE8HuKuyL/SHyAeQXVmGY/X+f18mkf1DbBZAg6c7GZHvc3Ynsxeew/+yxaCqnyJxNU1at5RTz2gBlemCyfgCDUKYC6AxGDwJ6AKj2wZgM1UoGNRj3gfL9PqkLaaOqTvtft/8vd//G3+zV+W/2SlCoEx4fIy0mfvkcv/9X6vT/KX/aLPORp6o4Zjmr1/8XP0T6PXaXZjSWlNv5C7y8oYqbH+5Bltn+1ahGhcPmNKKtSVk9A3h8WQXL2qsYzAwGqwaVqkFF213AlUyj4vwVgl7yKXnaEv1/AGgsN2JM8xj/DAD/fOWf+NOCP6F7sNuHfWjfD+GHb/8hWhpaMKF1Aq466SoctcNRPn7BqgX44/w/1uwYnjp6ahCeqDckDUrZDQX81i/7/8bJm2ltfQKvBcsy6yH2AZXvvswZW8KX92/DrmPKNkv8gwIamoExEzFtbDOuO3l7nPPGGRjbbPvqPAnPhCJrceTw5cGSamDEhAZ5l3qQ9uZ1X+f9f1APwthOPYwx6C0r/G6PMeguKyTjJ2BND9DVr/1pdAb2HQBs93J1mcGyjjJ233svXHhmgl9/6WY89L1v4KVrvoqFV30VD3336/ivS27Ef7znSey6y3ZoamrK2RHrd9JNW2M9SprJbwz1fFbesxw9zPY/j8uWT9kzH+Wa/T/w/s8TBGSZxEc9STBb6v1fbGoo5FUs5GOY9393KoqNjP0/lEN8Sfz+L957WHbC8b+yGP9z7xnktbD9d+VJfL79z2rbfwnMmw1j/I/A+9j/X3zxRXzynLPR2dWFiy+8EEcedjiOPupIXHzhhejs6sInzjkHCxcu9D4X0yzL25T2X6a/5bZbsfsee3iai6BcLmPG9Bk45JBDsNXsreJovOXYY3HM0Ufjm9/5jg8zRTsw3Xi/3iT/t3QH/7d8/W/2/+9cfjnm7WRPYPjBj3+MO++9B7/48U/wsQ9/GOPHjfP5lfP/MaNH42Mf/jD+89of48577sE1114LpRR2njsPV37tMsRAedEnIHjnKXYMY1na2JbSGIPx48Zhz933wKKXXoTWGrvMmwcDYOWqlTDGoKFcFgu2LBAXy02S4s9e1oJBa0srPvCe92LqlCl+l29Ohu7KSef64/92XI9hBOKSOvH+X9D/l8C8W8L/6deklfk97W5csNb/i+t9PnN8lmWrYfg/8dE+mZd4rRwNkkQ5n7a+HXeS6vmsvA8824leWS7TVquVGlxJEECtgJmZ4Yk4XkK5WXuZh/FGNCQyLTtWkigK0hh7vBlXAEicpIWdsjg/lUtalTMEwB6zmmV2l59xjTN5Jl0Wlz2+UuKFkImBARJrCKSLZRjHV0XQniT2GGvmD4MnwXikvDiALmVEo8rY4Lr9H5nrtbJzQ75tmvBCRD4J/P4h6Za8KrEz0zjjCbK2g/Fwju0NyOWXBg4h48RVUFKWLKuGN2P8LkdZPtOFiQMLxtkL3zqZh6C1nazP7zbN3A7mwAPLl0BbgZCNvPfP7ts7nHymrHkkBHXLsnxY5LjEZ+3ByiDQrMGXN+VsveieZUsZS4jL4rNx9maUm0SxY7E5PyVu2qttmPIrgWQ8+bRp6f+h05Cjz9kd8wzl/8Y4Dxi2/9tr1fkahvJ/BZQbgv/Hg/8x3eSPccZYvcP5YCIahCI8WZYhSe2Kvhx/9Nk6PgJvE8X+z3iJjyB1w3y8qnr+72ybaaXvyDAvt8j/yRuG5f9BZiyfYaSZIPngM+mCkJFspLVYwSjjY5B4Je+8L3om3RiG//Oeefwq/jR1p0O4Fz9lv8cMUddoHRa7UO6ybCljCb4s0i53wkobVfD1KctkvKUvsS8IiULK49lh81h7drp3vOjM0su0lgbbNlq6EmRVtv+pPZLR0WBxWnxsF0jXD2ctxw3bLMdN267AzduvwK92WIn/mrcav5m3Gr/dZTX+sMc6/GG3tfjLvu34817r8D/7t+Mb87qRllLccUg37jq8B3cf0Yu/HzOAf7xlEP94cz8ePL6KB4+v4METKnj4pCoeOqmCR06u4vF3GPz40Hxnqtb/7fdKCPX83zcs1IWSgeJeyADGYKvZs2GMweJXXglJqeK8qj2K+U8/DQDYfvvtXUSUIc7v6wpjf4ZxCjNnzsSll1yCQw4+CA899DCuuPIKfO2yy7B06VKXT+Hvf/871qxZg3PPOQf77LM35syZg9NP/zAmTZqEe++9FwAwceIkfO6zn8VBBx+EOdvPwS4774xTTzkFvb29WLFyhSvf0rDvPvvg6KOPwZw5c9A6qhWLFi3C3Xffg9NOPRUnnnAi5syZgzlztsMpp5yCiRMneBlPmjQJH/6w/VbxzjvvjHe8/e3o7e3Fiy++5HQSWPV6yUEQqFL8x3D+vGjEjdO1tv00O4HLXpu946QuJ3ltToePdYn78+lEGuN8VCnbUNfz9TgMPm8ULoRRJAmZ3tprOMmjpgzWRZIGVybDQV6sYK2E3EuPcn38HEonQ0o3Lw0nQsfDxK0/hgFsg57uDmTVQXSuX4SBvvXITBUd6xaiu+MVZNUK2sZuhXK5AWNaF+PAw07FkcedjuPffjbeftoFOOjIUzF1+q5Yv74Dr7z0HB64+2dYv+YlW3bDrlj80pPo7C1j5rzzsMsbLsSMbd/q/R/pKFSzFnSufx593SsBA4wasxUam8bbSWHHQblhFKBK3rayajuqlXb09yxBb9ciVPpXI6u0w5gBwPXLLNgrn4du/0N9SZDtPydqjRETv6I9sD/tJ3/h9GR/YUEn442zLy6YIcQ4aRdDtf/aDWbJsJG0/2m2DFPU+tyu3ylpJ6Yk7pd2YlLaiSnlTrT1tGNm047eFwEgrWQoLV2FEuwO36akz00A2+cW1Ytm1eOuvWhRPWjdKrwLj7j9j9oU7zuiHxP8SSM/CRxP6Jp8vPz5dPHEMSd5M8C4HbKm6ieCjQkTFYn4fFL+/d++o0kbSwrGCoyoD8gX3//7e6u+OjJGLtJydao2MK88B1XN0FC238pmn4jlGGOwzZgqoAeQoB/Q/dB6EEZ3+53NOqsCehBGV7Gj2dXTUi6Xc3TB6YlXqRfyxzhT9P4v/LLeEdDyuQiU6NNKsLuIo2OkeXVleXk7kLqB4JF8sa9sat7/8/YobTKGUJqtnPffugGzxqSoaIP+KtBbMfjx37uxrMN9LskY7Di5hAO3a7B6hsH6ngyPLhlEe69Gpg0Gqu4bwNWw+7eqnX+x3Fep/09Q7h2c0DPYg+///ftY2r4UAFBOy/j4gR/HZcddlvvMx8yxM/HlN38ZR21/lD8e+YbHbsCjSx9FVQt7UYlo1YJsc/7P/j/1pcMO7dhOcxUaXHNrW2b/bLMYAAYbuvvQv24l0N9HB6z9JSmqoyZj8WADeivBnkIZQkYWbfFPCU45rufySx1C2Cx5jP2QeaT/K2Unpe0nyaxNGWOwsqWEP+w2GgPZIMopZWLThIng8BO1KZoaAKUMjM6gM5fJaJRStokGKgm0x/4f66d2/C//PqbqtJEQNjF0+x/wEV4t/2d5hP8N7/+ZGB+MQeKVvMeykM+kG5vS/vv3f3dK5cbe/937s+ZYAN/Ro/d2D2KRK/HymT/SBGXTSzyMTxJLH/Wdb/9Dm0g+E7b/Sb79j2XI9j8ZzvhfQX7a5AsvvIBPnH0Wurq6cMnFF+PIw4+w4//VDEcfeRQuufAidHd34RPn2klg8kBcm9v+x+//XV1daG5u9mESmpubMW/uXBx++OHYY889MGrUKGy99dbYYYcdavK8+S1vwS233+bek4b2fzPU+P//g/6/Zu1aXPuz63DR5z6PuW5C+P4HH8A5F5yPvQ58I/Z44xvw4Y+fidvvugsAsPPcubjo81/AtT+7Dus3bMjxHstCPpNuiIlD8u/pqpFFPkwBfuyfYVLWqmD8n9+f9hDU7eHJ+fOxw/bb44zTP4In5z+FtevWenr5i0HqivE5nx6J/0f9f8mf2oL+zzRKzv+5RS98LtUb/wfc/F/eNyx/yi+6YDj5YxpT4P9KTOjKq1Kwm2OSBGmSeBsgHskD5RNoGdr/GS/xEaRumC8hMjJEBiEYY2LGUZkUPDuVLFiCgRuwcMJGgbPKBkuJmXMKAg4HaWA48RWCsi+k2tiBZRsU6Ne54xMcncK5JB/saMsJL9KoXUcizuMH7pQd+JLCl0qwvLiVHMK4PG5jJzo13FFNuvaIliyzs/7cbUWgcRtjByFpCqQzV+GL1XKkTWuNLAtyIk4oBeWOojCwdFJvxEucBOqM8mOaAOH7zMoZv9e/kKuVtxg8jezKp3f6kMYOtwoC3kFtPOk3tFdhBx6nsE12kghMw3SknfJVHNh0k2xJ4iaBnV1TTsp9wznGayHombILcRY8H1EDLuXMOJkH9H+345P8kTYD60/UQ97/A26WHwPp4NEiMQ22zDBwTNolj1LGVv8b8X/6njjSTNKvo+NTQPrFABw5I1/km2GSD5sn8YYRdJq3iWL/z9uZtx9du1pJu5cYSRftgnwRcv4vbIDlSP+Xcsr5fzU0nhKnpJ90sGzapyxT8inTSKjn/6QXQu4E6gWRjfBHOomDjbQsJ7ZbPpNexkkeJcR0ev0J/2ca2RkBwuAE3KQOd4V7vO6FDQCyamaPuaf/y5e8TfF/t/MffvJ2iPZfnLDAyVyt3ekHLkssR5tR+H9JtP/M515Gffuf2OM+WbZSln/yyxfSy15sxaefHYXzF7TgvPkt+NRTzTj3sUac+3gjzn60EWc91ICzHm7AmfeX8IkHG3DGP1J8c74t/2P3lXD63Qk+ck+KD9+p8KE7gA/fleADtxt86A7gQ3cqfPB24EN3KHzwDoX336px2SOh3kNd/8/LjuGgvQHIfCfRpbUVkwsTUUb8oLDzzjtDG213ty61xwT5CsowT9DzXXfdhSeffBKtLS3YY489fTggimN6ZvP0+wQ2jXtsbW3FKaeeiksvuQSnn3461qxZgy9/5ctYsmQpoIBnn3sW++y9t//WEREf9KY3YcEzC3xYT08v7r3nHvz42h/jqquvxn988Ys2xk1oWlDYd999vY0AwIsvvoiWlhYcdNBBLo1NF+i25e20444hDsofm718+XK7K8SxarMpKTYHIUDGqTiA4EXk6FBWgdYGHANOj96mfVbZMwt2wzg5KMy8xvXnYmBe+g5g5ZnDGdfLvIns1wPTijilOLKax1UoG4Rw4vd1ng2VyrBmLI3fFWuCJP1TTG9D8xS0jNkNnX1taN/QgTUrn0Zv7zpUBgewfu1CdGxYgp7udix69h4seeU5bL/Lqdh1r6Ow9wHH4Q2HnIzD33wqTj7lHLztlE/hkKPej1XLV+DlFxfgH3ddj/VrXsKA2R4PPD0NOx7wfUyceTSmzDoCSdoIUM5ZF6A70Ng8ETqrYvS47TBh2t5oGT0Ljc1jYQygM4PqYC/6e91iBwMopFBpGWmpFWk6CiptAFTJ243yO6Ft/5WrpFnfbkr7b1zfTrs4+6ytWrWxxzm7nZcA/OCTVTvzuPQCB8GINij+YYj2nzt/U7F4VOp5OO3/eLUWk5MOTE46MTnpxKToNzHpwqSkC7OaezC91IZmNTkcv2oM1PoOqO4OwHSjSfWj0X/zN//t3+akB6PSPphsLZpm211fGGn7H/lq/f6/m6zihC936cpJ3KKjnQufGWYnd40WV/ezO2btRDDcEdDK9YnZDmoxGIh67b/gg/1L5iVI3MGe3FUsTNDta2DWrwJKDXhiWQ9S5wcSunQF/+hbgsR0Q5lOKN0F6E5A90Fng9DZIGCqqFY0WrJROFLbBRyI+n2SD4YP1f7H9afUKYAwMRtP2MpjoQugXjhxFO385S7jofwfdfr/iPv/kb0W9f8lUAIKwJS2FEft2ITmBqBv0KB30GDBikHctXDAnbgCtDYqnLJ3M8Y02e/CDlYN7lg4gIVrKtDaHvncXzUYqNqdv4NVu/u3UrXlJgX+L3+b2/8n9Ff70dHXYeONxu/n/x6PL38cFV1Ba0MrPv6Gj+OLR34R5dQdYy1gh0k74AtHfgGHbncoymkZXQNduP6R67GsI3z2YlXXqhpZkh/ACpT1fMbPFUW+RrqpT4tO2UbGQ209/Zdn1+KM3y3EwlVdQPsaoKfTzogal1X81gxofOHBTpx513osaq/U4IJSMMb2qer9ENujsBubP/g8eZS65T31XgSTym0wWot2zMAYjVt3HIXHBlZg+miNGePciXesX0R7yPvMGKQJsPOMEhrMBmBwJdLEHh9vTIasagDYe60m+/LJH+lnmyCvTCd5kmlZx/CZYeSb+t6U9h9b0P9JB8tm2y7LlHzKNBJei/f/SrUKMwL/J07ikPIl2DTh3Zm0123/o40rxvD93y6GzuGtef8v+eNKOVlB4GJrY8JJV2ECN7xH20lli1T793+7uFvi9LSB7+g2bsTtv9vJKPUk81FGvKeOKTPmiWUp/X/RokX4pJv8/dJFF+PII450vGs/7nDUkUfiSxddjG63E/iFF1/0uLGZ7X+cxxiDtrY2LHCLsAlTpkzBG97wBhxxxBHYdrvtUC7n24u2tjbMmzcPs2bN8vy1traiq6vL9ssz7fs9pKvI/83/+T+UUpg4YQJ+d9PNOPIw+ymG/7jkSzjz3HMxc8ZM/OA7V+EH3/4Odtx+B3z6P76Ai778ZQDA4QcfjN/ddDMmjB/vcbIsabeEmE76XOz/cPMASZJg/YYNePTxxzFnuzkwxuBpNz4yaeJEwJ/Wkuddtv+SLoLW4X1Zwnd/cA3OPv88fONb38R5n/tszZg9XD8KANpGtfk4qUPJH+fB9HD9P/JX5iXkZLeJ/l8ETMt0xFVyfpK6MTnySPptXR5s3u6I59H3GnDHMtvFzxngjly26A1sHyvUCyho/2XZkieZlnLgM8PID+kt8n8M0/+ThJMjFL7o/PgOkWOLExIyjEbNK4/L1W4CQwIZoiJhReUZg1CGVLYRDTbjmFaJysIL0f2MS5u5IwzokBSipcdN8AoaiTtJEvF917BSgfEA3FGZwei1cwqfThg1FWcNydKqbQLPq4xL0gQG/L6o/fairABYnnKrsj3/jj6ms8f8BhplBWKcnign5rXytzKnbGkD7EhwUoCyZNoksTvBEDk3ROMS0qa+QpI0UF7kizpkmaSJaY2zy8zJXw9xJnviOn1e185eSSd1QPyeXtjvo8pyE7HShbyzrMTpBaKyIv8SjDGACmklkGbJBxy9pJH2y6M5WLbEQf0gsj/SxXTEaYwbmjauUVH2xVfD2pPJ+T8AN2AnbYjyJVBG5IXpZFrWLTG/Nf7vJqjJK/Hk0gB+Ul3z6BplV04H/8/T6W2C/i/kU+T/ctUgIv+n9VD+Rf5vhB+Z2P/5IuHsLHWVfOz/0v6kXJlOhqPA/2kb3veMrS+UChNusjziVy5Nkf+TV6Yh1Pq/pZ1hsf+TL+//sl2I/J+88EebYXres0yWC8EPhvJ/oR+Wm2zE/7Wrs9iOyJc/dtaYnmklkGYldME8kmcAKLnjhVm2xEHZAfB1mFJhUpbpJN5YBlLOPg9XFru81sc24v9iwjfmwbj6hjyzLDk5rZTCM50JHt+Q4PENKR7bkOCx9Qke25Dg0fUpHl2v8Mg64JF1CR5ZAzy8Fnh4DfDsBkvnI2sUHlmr8NBq5H+rDB5cDTy0CnhwlcGDq1yYex6p/xMo/1K5hGoWvqdYCMpNFgr7AAx22213HHfcW/HYY4/hxhtuzOexSTz09fXh6u9+F2vWrMGZZ56J1hbxfUsAbhROFOAyC5pzRiqDjX0h3WfvfXDpJZeipaUV9913H2AMFixYgIcfeRhnnPlx97Pf6P3t736PNWvWAADWrluHL154IW659TZMmjQJO+24E8477zxfYpCba3dIqjF49tlnsfXWW4f4Qrp9Bt8pz4nbPRsORhZAsX5Cf5LlGk7Qur4B/IStk60rSEmcKkzmefCTfDUxAGycuwngWQ/+KP1D8kA/kvEyrgYoHNGG+XB5pc4Y7ehhGukDDCOvfkczbJj3K6aNFGfT85l53b2TqYFBy7gDsOP+38LYWe9A8+g90dXXjI6uKjo7+rF+Qy/Wre/H6rWdmLrdaZg060iLx9OsMdDzIrLBddhh3gE49u3noKe3ghXLluLuW36C++/5JZYuFjvwI1lXehagtW0Syg2jUSq3QqVlVKt90HoQOssA943Uwcognrj3S44/g1LjDDQ0TkfTqG0xavwuaGqZjXLzTCRpq+PK2pVyC4TsccuWZrZBvm51tBgTjt2S4XDtvzZh56822k7++uOfDVXl7jWMgT0GWmv7css0vp0IbUPRT7aPlBufWfcrt0AS7j2DL+pmhO3/+FIJ08tdYbI3Db+JqQ2flHRhZlMnpjbvCqjQHiqt0bBqLZqbNFR5AA2pO/rZHfvcrOzEL+/HlQaRTqkA4xs8P8Tl2/9h9P9V1EYTyG+wM7GTt2hXL39yd7APc2ngJn+1djt+edRzmNjwu3/d5DCcTqTcSZ8BJ36G7v/Ld1TyKfWW+gkihpMte69WLYZKSlBJigde7nS4wq4DYwx+3LEA67IewFTcRPeA/d6v7ofS/VCoWvvVGY5TJ2EcJuTo5D11uTn9f4JSKhz3zCOg/QRuuN+68n5sM/g+bDPwXmzbfxq27T8VymT4/hWfwzWXfwbXfOPTuOYbF+Car5/vJn3rfQfYPg/l/wyj7FXh+3+xr8VpYFWWgzQB9t2qATPHphisAr0VjbXdGW5+pBeZGKfce1Yj9prV4Ou5BSsr+NuCPqzutHVUpWowWNUYrNrjn6uZOw6aiwQL/J+/Ldn/7+rvwrINdsJ2Vdcq/HnBn7G8czlaGlpw2l6n4VOHfApNpSafPobdpu2Gc950DvaeuTdKSQm3L7wdDy95GANVe8z/guULct8RJijX78/pQvgNeUb0/k9eHBbHiw2zRw7a5ufGJ9bgrD+9iOc39Fst6gzo2gD0djvnq/1VMoNblvbhfbesw7PrqzZc2b6OrVOcQdT7ybZd8MNniHqP4dQl42zSUM9SFoyb0jQR9vT0YL86Megsp/hdx5NI0gr237aMJDFhp6/49q9kedb4BLvNLCGprETW/SIAu4MU/rh8DaU0Bkrb1/V/PdT7v+C16P2ftvxavf9LmphGlhen+b/3/8RNCAyj/XcbZyTY9GGswPqp/XEyQrnPQdmyA//Gf5pIoVQue1xJGsatPW63QYELuJVK3GQi/Yp+ZGkKMrC0kMciufA6VPtPPUmbID6mJW6pNwzD/3//hz+gkzt/jzhCpLWT6tqN/x195JH4ktsJ/Lvf/76GTkmHtGPUaf8bhmj/jz7ySMyfPx/lchnbbLMNDj/8cOy7775igXR9mDx5MnbddVdMGD8BzyxYgP332w9pqWQXAFRdH8Z/H7TY/3myogzH/4P+v7U7Pe32u+/Gn//6V/zixz/BeWefjX333hv777svzj/nHFx/7Y/x57/+D26/6y6kaYqtZs3y+CW99f3f0jBzxgz86je/wX/efBN+8cub8Zs//N7LyOKx+H56/c8xdcoUHHHooTDG4L5//ANTp0zB1rNnAwAGBgbQ2tKa0wNpgPQbYb9pmtZ2xBzc/+AD+O0ffo+urq5cHSXt+w377Y+Pf+SjHreUMXJyDv5Cmnj9V/k/8cRpVJ35P/luKemUdHDOjcCFN4zHCPr/LFOJXchSdrynfUm+aGfpq9D+JyQw03Zyl8ACpHAZlhdyUCaJpJPzSiYIDE9L+bQxA6RLhksH5FEb2lUWSZL4zhwNkUpXztj5bHHaFYBxmZ736Hu5qZtRT1M7ac5JOJlXuUH1JLETYoyHoEmzsnRH1NK4E7ddXWs7IMPJ9CQJHRJpoAahRpGy9vpIEyCpnQygnlxATT4X4cvLtPv2McKKMvmTBk+apL4pU6YJPNi4UDna8r1RC9mmpdRPXDC/p1eFlekMT0QnT9IadG/TcMcny/Hlu6N5jXGDYn5gzP6oN4mXz3C2oYVDy5+kUcqGYeBAmFhcYeXqjrxydqbd5KC8l7qG4Ik8SpplnNShzJeTg8Sl7OSPv8KtIiylUGkCw8muGv8P9hjXFZQBnPxoRzI89n/yTVyM25j/c/IYQjYsh2JIOIHvQPo/07M85rXxJe+zsk6N/R+uDGuHkf9zwtqloT1J/0ekV4bLMA6QEVTk/zHvErQxyLLwomTT5O3BRP4PwJ68IP1f2JysG4wxUIk9ShyCFuv/qdeDMcZ2fsXKM5vevtDYq92ZSjz8XrmlLeiK+uVLUpKmPj95sP5f67f2Z9MxL5+JT9Js6a7FE2gs9n/lOi2Mo1zklfWwdi+Nxp3EEL9gGuMmVJ2v1vPnWIe8r1dfFF1pV9KniUvaA8PjtJJX3pMuhtP/rS/YH1f4a+0Gi3W414bPBp2Drj6A1SNoF7ZAd6Xu7IMXiRmJ/4e6iPGApYfHXXtwk93+nd8TxnuXCMBbj3srdtpxJ/zxj3/EFy+8EI888ohH46jHf//lLzjzzDPxzDPPYOrUqXjLsccyu4D85FqgJp+QbV69t4rW1lZsvfVsrFlrJ3dnz56NffbeBxecb7/Ne/5559vf+fYeAG699Va0trTg0ksuwYknnoCjjzka48aOjTDD0iKLVQqzZ8/Gyy+/LOghve6aq7+sn/Mn81CsirKPwLjxzFq+g41wEtOmMGBIyGHlplzbHdIFOuKJUE7yAc6eIn3wWcHaS862It+sFy7xe1BuRlyAp5Jx9A8bmLt6LYgXVZ+XuIyVkcxQk9bJNWRyPsY8Cq7P7qQpJiyJywAoldsweauTMHb6W7DzgT/FHkf+NwbMLHT1pNjQodHdo1FqGAelgP7OJ1DtX4Zq79PoW/ML9K69FX0dT8GYCmbPHIVjT/wQOto7sXLFcgz0d2DGzBl+QkyC1hUYKPR2LkFP51IMDHSgq30pOtctRF/3GgwOdCHTVQxWNLLMoKGhEd1rbgWUQlJqRePYA9E8bm80ts1F05j90NC6C4x9PXMysXVRtVoRA4FBxrXtf2hLkiT/SRNbNznZuvoxt9PST+batyke68y6wOS+D8y6N6Qp+knI9yfq9/+Zz7h+tK/7o/4/r8QzuWkPTC11YlZzF6Y3dGJauRNT0g5MSjowOWnH5FIHZjZ3YKwuoa3pALjXYBhjkHV1I132CkzDINBUQdI4iHK5Hw1pH5qSXrQkvWhxxz63JD0YWx5A0/ajkLj+m6SZdBfJgnpQI23/6034+u/3ajeBy3vx8zt9q24wt2KPNNVVt9s3szt+xUQwdwzriHZ/VQDEZ5HiNt3LdRjt/6xRlBGrHHGfaaBjDZCUAJWikhl84y8voOr6y8RVhkKCChT6oUw3Egza3bYw0CaDqWq06DYcro7Ermr32jpXvv9H/dh67b8ReRlPW/Ay09GRzwXf8F1/ytlYd+o5WHfauVj7nk9h7XvOgzIaq8/7Glad/3WsuuAbWHXB5Vj16SugkJ9MRm43sH2W/k/gc+xz0s4Ixvla7K+e78i3be1gf9PHlLDLtDJKqfv276DB7c/144llFX/c7qRRCd63X6vP3z1gcN8LA+jo19h5WhnjW+x7T38F9hjoqkFFa1TczuCcHW7i+z9lBMcfCuofAFjTuQZPL7O7uf7+0t/x7OpnoZTC8XOPx7kHnYu2prBzpgiUUnjj1m/ER/f/KLadsC0quoLfPPUbdPTbXcW3L7gdmfgOdD3/N+7KOC0G3kl3HsiDwGFs+B2LNuDS21/G+v5qXnnaoKFnA+aNyjCuFCnW/bRWWLChgiP/sBo/f6YHPRU3OJ8kUCrIrQjIjzy+kryxT0G+6/X/UWf8j3FbN09zOuf7HwBjoFONR8xqPLx6AY7ZpYQdp5aQKDvpS5CsNpUVjtq5AdtO1tCrfo3EbLALsBxdpVRDa0Brg/7GNwDC//nOTlwcz8u0Xehv5Pu/s8eq+952psP4H08y5FiHce/mlBfxMJxhKrFjSYxjevvOTV+J+w1CDsP0f+qIQL3JZ6bFa9D+U5ax/3PMh+UOx//r/ZiXz8QnaTZ12387ZiE/eRdw2DYmcwuFGR7zy3zcnWbv7bhJgNCWMW/MF+NiHdpbS08N7eK0zhh33KZbXEFnMjxOK3nl/XD9/z2nnYbrf/ZzHHH4EYCbrAHsiVtWXmH876gjj8TPf/JTnHbKKYCgn+UQP22IkBa0/xzfY17GJ0mCD77v/fjn/fdjxowZ2HnnndESL8TeCKRpiq232Rp//etfccB++9nyxAQbItnb8PzYonoN2v/Ydqg3+cy0+Bf6P4zBeWedhXlz50IphRt/9Uvc8MtfQimFnefOxafOOqum/Hq/pI7/f/0Su4v44UcewcOPPIJrrv0RLrvyCl++rYSBru4unHfOuVBKYd369bjhV7/ECcce53XW3tGOtrY2jzvmlzLVrv2fMX0GnnjqSRxx2GE48vAjcMB++2H/fe3vgP3C799Oeht233XXIBMAnV2dmP/MAhz35rdgxvTpgLCvWA62fGtPMV20K9pbsMlX3/+Ji3EbG/+XOLn7mWGSd0s3y7bfRZb+z7TMy3gpNzgMQ47/O/upN/5PXNJ3UOj/gq9h+H/CTDIzM8ZA4TM93IeTIWaVSWSsUDKtlLIrHd3xkzKPxJ24TksqtjEzDUSlQDDGHtdCZlkWeZE/Y0LnSUJMc6VSza0CIA/8VqYSK1Z8fJKfjGM6iV9rbb9REq1syfhdEP+t3tBBIN2JMxg7cRHoZxqluHOYdY3t8BsDJEnqJnQMMm2HHBmu3Coz6iBJE5TKJSQldzSIGOCQPLGTkKYl38GSupZ0034snqBbpmenlrqnrmWHQ4mOlu8QRyvvpF2QTmkXcLLJtPaVCPNygsQmDhMmzGvLSgG/I5wVopjYsrkB4ReMo00konIplewqEikv2ZjJioOduphX5qPead/GvRTIFwfSQSB/Xgbe//P+Uev/oTEv8n9t7HezmY78MY/0eXkPQR/tXKYB/V/sXtSiXES2Ym07L1+XyOeH9H9HM48k4W526afEVeP/glZ25nMvaVElXuj/Lh31YIT/8ztr9B0C05BnCZRrEjUwjGM5LINhpVLJLmZJ7UIJToqqxD5b+1BI0jSsKnV2zTQcrJZp+FKRlmyDar8pSz+z+MIERzh6yO4cDXQYY8LKW9LGVa0KIa874kg+w31fp1qxx5iRduIhhGebl2XBvVwwH/GxXEuwPbbJ0lnP/+3KfcqfOqjv/0GfSoUdvMzHciEmFo3hsU/B16WNMIw4SWMMI/V/4mM68sc8ehj+X7f9z8Jkr41zE77aDsjkJ38BrQ3ayo4eYytI4+pL+Ctlax/IJtNJPyUvQ/t/vv0vlUvo6emxBRGoS6uooDzwPsD222+P884/D3PmzMEtf/sbPnbGx/COd74Dn/7MZ3DO2efg8COOwAUXXIAHH3oIo0aNwsqVK/HpCy5AT0+vReDbiPAiAmvZ4cFybn3GH2umLN0ymQJ6enqwZs1aTJo4CXArbV9ZvBhTp05z3+d1v+3sFUrZ9JMnW/6UnQB9xh8PPTTMmDkDvb29mD+fx2o5RVJW5Ck6Gs0FxgGuX2RtkZmtqoJw8s9OL+xDGFE25RaBT+OMiVO+1gxtDuXkIEH6n7d5Xp3+pG3R7opA+hVB4heGzsgCabk8Vmg+jHdGhBsTdgR5WcGJyYnQhlk+jJvE5R+Y1tMZ5M144xYjenC+y/RJaTRaxu2PUkMrkiTBG97yU+x/xOex/5GXYd9D/gPTZh+CwY77UMqeQ+/Kn0D13onGcg9M5Rkk2csYXP8HdK38I2bMnIm3v+8/YNCAdWvXIi0p3Hf7T9HdaRc9UK6DvS9isG8tOjvXQmeDSNJG9PWsQmf7K+jrWYvBwV5UBjP7qxgM9K1DUxtfxIEkKaPUvBOaRr8RpaatuBxACMxe+/v6US7Zk4BiG6E9DKf9N0bs/HXxxtgdXJVKxU0YmprJ3/g53IeyZF0u4xjOtiHu/zMt6ef7gLRx8kfcMU6lFEY1HYImHIFJTRMxoaEBE1ODCSrDlNIgxusKxusMY9NJ0JUTgd4pSPq6ga4OmFdegr73bpQH25GV+qAaq1CNFajGCtLGQZQaBlAu96Gx1IvGUi9aSv2omnZgx/FANOhF2Hj/f/jtf6btxF74aXcMaYbBSob+/ir6BiroG6iir59XF9ZfQd9ABb399tfXP4jevgp6+wfR119B/0AFlUoVOuMx0PboZ2Ps5DCK2n8VTs8aqv03w2z/37mdctWLrUuMCbt/zUAfFFJXt1u/+OOTq/H08m5A2N0Z43fFOWP2wL4NUzApaUZJZyibDCWtMU1PxElNb8EZjR/CWxqORTmx3xEmxH0W9v+pC/Ig23/5DUlpx5SB16uboOVxz7XPtbYDACiwKQCANnZiOzoCGn6COeSjjKX/UwcMl7bHsJKrZ6TNUj6UEYFPCkBjSWHX6WWMa0ns5G/F4JX1VdzxfD+qmdMtgNP2acW8qfYITG2ABSsrWNqe4QP7t+JzR4/GO/ZsRmuDwkBVo9/t+q34ncCuDivw/+G8/8Ppq+b937+H5GFtz1o8tOQhrOpahUeWPYLlncux76x9ccYbz8DkUZNr2u8iSJMUR+94NN65+zsxoWUC/v7y37GicwWWbFiCuxbdldsB7P0/ifxf6FPySt1JCKwGn/WuqxR+/eRqrOoZjBaSaIwqK1xw4HT85vhpuPKg8ZjYmFgFFfx6BzU+f187zr1zHRZ32t3Adt2Q6w8U/AItrjVnGH/D6f8XjP/R5wBg17Hbo9G9Z6Jq2zXKrbO/G1c//J/YkL2A/zi+Gf+2TyMmtNpFtJlL01gy2G5ygg+8qQkn7a3Ru+rXyFb9l18ok6jMHrMLjSSpIivNRG/ZTiwMZ/yPNHPCF+LzYEzH/Ib1qAtLCt7/OfZGG5agC/yf40GyHJbBsOH6P+lhnKzrJd1MQzwba//5zLIkf6Tz1fZ/+Sx5gWjziJN6lVDb/luek1z7XzT+FxazD/n+L9JJuhnG9DIvNvn9347fGGPfD8FPSG2k/ccw23+PexP8f9q0adhu222FnhO3KF+0wUK+c+bMwYwZM3x+bGL7P9T7/y4774zLv3YZjjnmGFxx+eVYssR9ummY8M9//AMnv+1kdHV14cPv/wCMsRsTksSOcQUdGTfxa3VuNwE4OQl7SV6l9p8yYpzUNXHKNMTzWvv/EYceive82076/+Lmm3HlVVfhiqu+g1/cfBOMMXjPu0/BUYcf7stlPkkHy0Id/99+zhx85aKL8Z3Lr8B3Lr8C3/vWt3HLHbfjsiuv8DiUUvjyhRfj8IMPAQB89fJvoG3UKLzr7e+AUgodnZ2AAVpbWqA24v8lx+uZp38EP7/hF1jwzDOu/Cs9Dd/+xhX41tcvx3cuvxKf/vdPAULGy5Yvxze++U2MbhuN/fbZx8uXPEmg/uQOYNI0XP//xwP346R3vxP7H3oQTnrXO/D8ooU5PT6/aCE+eMZHsf+hB+Ftp7wT9z/0oJf7UP7f3tGOy668HPsfehD2P/Qg/OAn13penpj/FPY/9CDsd8ibcMBhB2O/Q97kn6+/6QbAVmX+e7yJsr25arWKru4uXPGdb+HIt74F+x70RnzwYx/Fs88/5/WYZRkWLlqEcy44H/sfchCOOv443HLbbV4GSin84qYbcfKpp+CAww7B2055N/52262ehyzL8OgTj2Pfg9+EfQ9+Ew447BAccNghOPuC831+ypG2R1+SOmIa8iyBekkK/N9/A5ggI1kAEVP40kGpBKmkhJMAguhSqWTxil0XvJKpJLEr1hRXvIlZcKanEUjmlXLH0IpnSSOvmVtR59zZhxdVRMY1cpSFl4uTBfmmUAHusgqVI/OQZtKi3O40ypVplVL2YC83Kcv0wfHcKjYnXzoZ88Lxlmk3uCqOcGYZSRJ2PcvyKTNO1FSzzH4vo6BxhjeqYFy2w2snko04lkTmseDoEqsaoeTOmTBJ6Z9dR01WMn5SiHwLOplOys3QAVznN9Y3j2jV2k3ia+Pot7rI3wf+JCiVINPG6c6G0Q4pazpglmm/kobpYllL2UlamZ5hLINAmUiQlaWcEOZLpY/TdoGA1ZMK+hq2/1s5S3pVmiAtl5C5hR+x7qT/kx/Kgj7L9JSP59HVJ8b4oeOcTEizcXYRg67r/y6eDZywG1XP/yOfsrIM/i8n31mWTBvKDh0aRP7POL5gUk5eHoJm4iceXTBBznyK/u8alyzL/MtRpsXR/26ehc/8ZVpDpfb74NrYncNMZ1y9xB8SBZWmwf9dnWSgYNzR3gawZSkgy+ygdLVqd6JoY6DSFEbB5nV5sszSWc1surQUyrB5EmSZ9T0oZVfcu3ooKZWCP/BIfbid4q4s4mA60iv5yjINlSb2GDHAp2e7wB0rmXuJIEhdSl0TpH0wPcO8rbufUqqGNrlYguUQrwTaK4R/xnYkfavW/zfS/kd4iY8/8kNc9dp/bWxdY9NtbPLXTma09zs8bL8AwF9DmwYE/yfPpIey2BT/T5MUPd1dpMAWIPoh+fYk3BMfYLD9nO3x05/+FB8+/cOYNGkSnn9+If7yl7/gtttvx8qVK7H99tvjq1/5Ct520kkAgEcefRSXXnopli1bBkT9phwoa6OyPuWA5JKlS3De+efjphtvwvz587HohUWY/9R8XHX1Vejp6cZRRx0JGIOjjjoaPT09uOrqq/Dwww9h0aJFePjhh3DV1Vdj/vz5AIA999gDCxYswC233IpFCxfhb7f8DY89/kRETAxWl/vsvTdmz94K3/3ed23+RS9g/vz5uOmmm4T1ww5k5uTmQMGnU9YIvC6Y1qrbtvXy2aNgOq8/CXbS007mM8jlVfaftTv6tqDP3bpY/0cwsP1RhlFHvN8YyDTWzoNd5zgxYRA20J7fMe7vhT1ZKVp8SonJX/FiwjKleIyjLfhN8B9LiqQu6EXyo5QdvA3PgFIaWaUTRg8CDlfr+IMxacYbMX3bN6Ov8zkMbLgVJdWJUqmCvp4l6O1cAmQDaCh1IsmWIjUr0L/6WozObsAJJx2PwYrG+rXr8MLzj+OOv34fa1e/ZPk2Bo2tO2DUxKOQlidh7KRd0TJqOtJSE8ZPnofxU3ZBU/M49A9k6B8wqFQ11q5di76+Lm8Bxo2pefv0EiWvtk7q7epCQ0ODr2dlvUTw9ax4gWQ4625/5LOrK/kzxmDh88+jvb0D7R0d6OjoQEdHOzra29He3oHOzk50dnaiq7MTHR2d6OiwYR0dHWhvb8eGDRuwbt06rFu3DuvXr8/9OCmlokGc2H7zOrdtbSXq/5OPYCuh7dRmLLLSB1ApnYMsPRfV8vlIGj6G8sARaF4/F41L5wFPzkXzE0DbA3/AqLt+hdG3/RqlP/wXys88jrS5CtNQQdJYgWqqIGmuQDVXkDSJX+MgmkZpDExJgamjPS1SLxiy/z/y9t+uVDeufrOTNVk1Q29/BavW9WPJql4sXt6Pxcv7sHiF+60M96+s6HX3/XhlZR8Wr+zH4pUDWLKyH8vXDGB95yAGBqt2R7CxEx1wu4alHYX23w4Kgz5Y0P7rEbT/+05O0KCyUAWxH+jslHUonWZddxUX/PJ5dA1YuwCABpXi4NbZOHfCwbhs0tvwnUkfwrcmnolvjPt3nD/mwzi04UDMSMLAr6nb/w8+wyvjlWj/02G2/35i1u3aDc/hO8CFUHDaAGC/KTz0EdBhkFryEtuj1AX1EPf/pU0SYhs1VjMAgG0mlLDjFDux2zdod//evXAAG/rscbsAsPO0Mo7ftdnXcRt6Ne57cQDNZYXjd2nGfrMbcOy8ZoxuUqi4Y5+rGqhm/AZw3pYknUO9/0s9Sn1TnzJOwqAZxINLHsT/PPU/WNqxFC0NLfjAPh/ATpN2QprbdTc0tDa04l27vwt7zdgLfZU+LFyzENfdcx2W9y/Pt/cF/i91KX2MOiVQJhKS3KdlBG5T+/v6Mdvg7DfNxNRRDThhuxacvdsoNAraYujTBr99sQfH/XEVHl7pjpIuwMufp0TYnrdFYbN6iP6/5FHKhc8zWqdibNMYmAqglZvsdAuaMq3x9JqFuPLBn6KhZRnOP6YFX337KJxxWDPevGsDTtyrEZ9/6yh8451t+ODBJSxe+ze0v3QVVHUDjDZQSkMpjTS1fqarBn0N+8Ek4wMfBf3/It3JtOSDtsr09exYthlSHrRd4ice5glxYaBfbYb/M00i+hukQeYhsCzmlbSjII8uGP+TfDAP6Szyf7ZD1Icapv/LsuQ94yUwn9RdTt6JQpZVoTex/Ze6lDbEMgixPBGN/7EcFPBB+UDgUZEdcQxUyk3qXdJmjNtMNIz2n/YjZbGp/u915iYGTJ3xP/JA3MRFfFJOjFfR+z8XgTGOtGmtcfJJJ+HPv/s9Xnn5ZRx11FGYMWPGsH/nnHMO3rDffvj1DTfa3aDa+ElgnWV+c4LW+U+HcZewSiibwEPOHuu2/6Ua/3/8ySex78EH+TKMMdj/0ENw8qmn5PRO+Z11/nm4/qYbc3ohsCzKmTQQ4jx6C/g/8wQ9hj6LcZvRWBZtgXi9LW2C/++4/Q645tvfwa133oGf33iDG7cK/v+HP/8ZDz/2KK786mUYN3YsKpUKVq5aifHjxvmyMAz/P+qII/C+U0/D1791JfY/5CDsf8hBOODQg/3vDYcd4sP3P+Qg7Hfwm7D/IQfh5FPehWXLl+OySy/FmNGjvXzID6/5skfo/67//9zC5/Hvn7kAF33+C3jgrnvxthNOxJnnno2ubnssdVd3Fz7+7+fgiMMOw4N334fzzjoH5376fDzx1JO+DOpY2oxSCl//5jfR0dmF2/78F/zupl/htjvvwPU33QBjDLaZPRs/uvp7+OFV38WPrv4efnT19/DlCy8GABx+8KFD+v/Z530KnZ2duO4HP8I/77wbRxx2GD5+7jno7rYLT7u6u/CZL34B++y1F+6/6x5c+bWv4z8uuRhPPPUktNb4/o9+iNvuvBMXfvZzeOCue3DR5z6HL156CR574gkvVwCYu+NO+NHV3/W/s88409NQz45pZ6SbIPUn9cY8Mk4tf+YZI42K9xAGr8QqhFB4GnbIuTAijgsjnizL/IocGaaUOyZPMGjEwJFkVjJkn3n0SRCCxOHTicrJhocKMHMr7zS/O5tlSEop4HZ5pu688ExrlEq2cpQVhmU8TCaRXtnIkx7Lp8vi4rIsQ1qyRpi5QW2vIGmYQkZF8dqEl2TKQBq1Um43YlSJSvkmqW3QSJu8Uk6OeoD0OP7Ir+fVaDfJ6YwX8LuMiVPeE6RBGzE4y3RaVADUGRwt8sr0lnc7qUOZQQWamY5pmZ74pW3kaIvtUZQp5eVlzw6DO5aEeJmHOOuF88owpfK8EgLPxXnJi+QXboWyxEdaLC92FwBpIx9JXf8PtkI8lEci/b9KW8tXcKSV9DKMeYnXl5fl9ZJG/m/5CP5DWi1vGdLI/2lTWbXq9a6d/+si/2e5hf6fr49YAZBelqeUsquK6/g3y2A8j9BivMcf2ZGNC7ZPHNRPTr5RvWWveXuWwDJlPuIinTKdpDO+J8T8yjjmYRh1xrTyGqcnXuYlzUzHtDF+ynFj/k8griyz/iHxpUmCivP/1E00A+EYEu1stygckTyKyg7hlGmwdymHNE2RuLqU8dJnIGhRYqcLaSMfSZIU0ss0Ek/V+RnpTlyY5NG4tNr5ulLum91R+//ufzZjRR+GPfmrNbDPJIPrDlfY578UBjLrhwaw41XGOLfkVdiTNthpvMJvjgXKbnEUV16Sb6Yvue/Wk1+l7FQO7aCnuwfTZsxAc3M4Dsrr1KrL/XM278MCGD9BZFc+PvH4ExjV1oaddtrJf+93Q/sGfP9738cNN9rvBZ988ttw1ifPwpQpU2pwyHu4OjLe0fLwIw/jscce98dOt7S0YN68uTjpxJMwceJE/ya1du1a3HrbbXjooYfR29uDlpZW7LvPPjjqqCNtOij84Q9/wN333IPe3l7ss/feOOWUU3De+efj/PPs7uZFixbhiiuvdM/bBVnA7jr++9/vw733/R1r1qxBS0sz9t13X5xwwglobWnFGWeeiZPfdhKOPvoYQT0Kw2P/UW7eMg/UBW2vOC4PbvrOOmFOn0q5QQllU/kJ3UgXReHuRpjGUP5fW/fGaQiMl2EuAnD263FQSCxDhvHepZflxzS5xC7MPtH/KGcZHpMWh1v6mMhgoOsxrH35erSO2xtjZ56WW2xnDNDX9SLWLPoGxoxuQbXShazaj7TUjGqlFw1N45CkDciqfRgzbgf09qzA+nVr0Dj1s/j9r76J/t4OjB47FhMmTsFOuxyCOTu9CWlawmD/aixbcBnGj5+Igb41qFR6MHXmXhjo68bq5QuwYsVidHUPorc/Q7mhDUe9/QY0Nk90g8r0f9dPBux/FwYo9HZ3Y/Xy5Whpbrb1Sp32n/pKkgSa71dO9uw/feCTH0dPTw+Mq3P5024h1dSpUzB58uRcnK8nfV+N8rQ3xhgcfeghOP7oY3yenA1onbOlHM1CwUVtLGNjOxpe+6+RmEE0dCxEy9JbkK5bBbNBQfX0I+3LgO4qBjo11q41GLXntmiZPB5ZrwKqKUw1BbIEJlNAltgVaVrBGIWWpma07zoHA/vMyxko9VK//1+xuijoN5sh+v8GwLTB88EjoLXW6O6t4qGlrfhu13vxz8q+yEwCcBBHu51v2k4a897YhtHfG63RgEEcNepufHbrm7DjpG40pBqA7YsCGmun3uHp19oOQlYrFSged1rT/3d9SsET5UEdMox51vZpfPSuDA+t4UQQxaqgsgoaFtyJpNQCldrJRRgDZTRK0Ljk5B3xph3GY1yLXchHuVN2stzuvgqSRKGl0e6iIV20pVz/X7z/64L3/9D+W9zF/X9g7y/e4nb5WppJO591XwfWvO/TDleAKT+9BCs/8604GDO+ciZKDS1uItnqSBmrZz7f9cN/z9UNtEvjfDMZdv/fXuv1/7f+XrP3z1GNCQ7bwX7XN1FAVQMvrKnifxb0YUOvnYhTAL5x0lgctF0jAIXBTOOO5wfwvXu6MbktwZeOHYO37tKMp1dU8F+P96KxpPDMygp+90QfBjPX5gB4+ZMDw/R/yztlQZ7IK9NJ2TDN7r/Yz+NqMA3Yc/Ke6NAd2G7ydrjkmEuw7YRtffxwwcDg+oevx1dv/yoOnH4g7n/hfqzMVoY2HsBjpz0AIJx+NpL+f6VSweRpU52kAfZPjF+TZaBUgtsWrsN5//0ClnT0IoXCbtPa8O0TdsSuU3ksN8tSuHtxHz5xxzos7Q393SKY0qQwa/o0rNONcZSHR4/NrP1zLMeFGzifVgorl69AY2Oj1xvtU/IsZUHdMnzAVHDN87/CrSsehOGR+Qq27lb29BAFhemtk/DOnY/F0dschHFN49GgmqGRYSDrxsqe1bjzpX+gsuyn+MjYhWhOMmSZQloy9hPsjvCKGY0N4y9Eb3k/pKVyof/H9RGEb7E+Ia/ki7+Yt3rx0hZMzft/kf/bbxJurv/jdf7+z/HCTfF/yoblFNFmy8uXqeL2n59Jc+PmahPaf14ZFsrOA8Pr5SUvkl9ENsr0iXj/V779t3zlxv/cCWOx3ODqG8qa+GSYpJPhpJX0yrCYH5YXy9CeaJDnQ/JL/KSLcsm17xtp/7Xr07Lceu2/lG2u/JH6fxyf2DFDKReWQZ7Y55cbebyM6EM5/7f2SRoB4ImnnsJHPvkJPHj3Pb6M/Q45GADwyY+dgfefdlrO/886/zzss+deeN+pp3p6iK/ePSHWpYxjHoZRZ0wrr3F64mXeG375Sxijcdq73u3DKRuJX9qG5ruaoE2WxzJV5P+LXngBZ5x7Nt5x0tvw0Q99GEr4/yuLF2Pr2bORZRkWL12KJFHYauYsj4tlyTIZx34BoaOzE68sfiWXLuQFlAK0NkjTBIBCS3Mz5my3HVAw/meE37Ce9Da1CfN/X7viciil8NnzzvdhJ77rHXjvKafi5BNOxONPPoGPnvUJPHj3fZ7+cy44D3vvuRfef9p7auTN52XLl+Ntp7wTv73xl5gxfTqMMbjtzjvw9W9didv+9JccH8bp9xvfuhKApWUo/39lyRJsNWsWtLYLd0ulEvY7+E340Xe/jz122w1/u+1W/ODHP8ZvbrS7yNM0xWVXXoGuri5c8sUL0dXVBQAYN3asp/vs88/DPnvthfedehoA4Oc3/AKPPP4Yrr7imxv3/y3a/idQS59+2khFQRiwLJgZg2JtuKzUmY5peE/cxriOF5mJ8MIZGCGmh0xYusLgsq+BRT7lHCyLHDhzq0PkDtuavOI7iUSuVDgCVNKRsJETvBNYnncQpWBcg8Q4pcKxw8ZNtEiZgU4nysw1Pq4RIJ9kKcgpyI6DdqSfOFiG4Q7YyLiIT8pLyp+4JLAMf3UD64oTbqLSpgyqlfDdi4QdhjSsDNPavkCiwB6Jh+GWVvcsGxWxw4l4tHM62p7lJzic1JXH49M5Gbr7OC07BKSNkyAx3UyjOckonqWsisqXRzKkbrWIBPJLPo0xvgzLd74BJa3adR5sWChf+ujQ/h/si+USN5yElVJ+AgduopQQ02OMnRSSMvC8CpZZTpIkMDn/tzZlec43diKzjzPWWQFHgwwnHZJe8k7I+38YiDWcKIpemDyOguN6yZO0B+pHyjyHJ+f/oSEgLuJgGXxmnsCPqEMcML/EJYHhMp73hf4vFkYY6f9iZaiULdNJvkkzeWQ6RJ1KyQvxskyZByPwf97n04aXB9Im24NYr7yO3P+DXoL/k4egB/Jpavx/U9p/C0P7f9AZyyVugsSLEbT/7/pnM1b2hrpDb2Ty1xiDHccAv34zsN9vEgxUhz/5awDMHafwhxPDEViST4LkF5H/GyfLgYEBNDQ0Yur06a5ukRO/Tm1enTKQIcLf4jwRnmqligsuuAB/u+UWAMC73vUuXHThhS6BhaKJRjkZLOvVHATzqgOSoEA/nGylDcDbga1rmMen42SpsPNAW1ROXZpr6QgQ+iZFQNsDYHWmIr5M6IOGtGH3K6f0lOPdNaZ5PMTh6KAeYlnZ/K4sdyPlohKxvTaCXLqoDmS8sgHMEO4dFNGTyyPSkDsbBs9rkZhjWmyYvcbpJVmCJQEG3Wtuw+oXfoi2ifth8pzzYRBeAOF8qHPtQ+hY/AMkqguto7fCmAk7oWPN0yg3j0dzyyR0t7+Mwf52VAa70T8wiCk7X4MVy1/CL3/+FTQ1N2L06DEYPXY0Zs3eDXvtfzIam1rx7INfxkDPszCmH41NYzB61BhUKv1Yu3YZTDIB7evXw0Bhjzeeg0kz7RFgSgmdqcBUCLKSXLVsOQYH+tHS1AxEbTXrIuqDYdZ9hB25+usDnzgTXW4CmGHGWEvNsiwcmel0U/yz9FGmxhh84F3vxunvyb+s5+xrE9r/NLGfoGG/CMJ+c3xvpP1PTBVtz/4ODSueQqmjF+ipAt0ZTE8VnRs02gdLmHLEHKSqAXowcRPACZClQKZg/AQwUEpKqKZl9Bz/ZlTaRvlTbeK+Qm37bwdNYrqZRm+k/Z/Sf661DGNQqWZYuW4AH1v6GTw0sFuY7NXaH+FdNNkb0oQwThafMvmvuHKX69DaCLjzqGCMxoaZdlDGt3nW6f2xpZQzaWYYJ0ipE8qBIPUIADcuBC56oIpBuNPAwBP9FcrP34dSZqCSsq0ATJhETY3BzjNbsMdWY3H0LpOw+1ZjcnLWWmPJ+j78/oHFmL94A7af1obzT9jZ00Gg7UkbgqNThpO30P7L/rIF2f7v9fn/DhO0EBO17ln3dWD1+z/r8xKm/uQirPjsVXEwZl76UaSNLTWTvmFy2eCOH33Ky5s0S/ox7P5/0BOB+Y0x2OZ7zeDYQjlVGN+aYFQDF6wDnf0a7b3an9JmAOw+vYzGMt/NgdVdGZa2Z2goKWwzoYRtJpSwtjvD6m6NVAG9gware5ztOuAE8HD9n/eSF/JIvcs8iCaAYYCGQXv6wuff+nmc/obT0dY49Ld/68Hza57He65/D5YtW4a+pj6YNPAFNwGslP1cmn/fG2b/f2BgwE0AE2z7YeUCwL1na2Pw1IoevLS+H6VUYZ+ZbZgyquxsmXidLJTCg8v78e/3rMMzayswQkYxTJ48Ba0t4dvOMTx6rF1MDli8bH/so8W7asVKlMt2oYfUK/VVxDuBYY+2P4tvPX0D1g5ucFZHsPKA63elSYqpoyZhq7bpGN3UCl01WNu7AYs6X0Grbsc3Z7yEXZt6kKZ2o36SWjkqBWSZwkDL4Vg/9gKYdFxd/yfNtE3ZTtB+IewRgo+4nfD2UKf9l3hi2bF8Kz+XZjP9n/cSZHlx2pG2/8lmvv+bzfB/M6L3/9q0aSm1E3SJsptQMvtZwZhu4tAbaf+Lypd6Ce//Acgv+TTDfP/P3PeFbX85cX2KYbz/Z679T/K2LHVEkLRhBO//RbwTmC5N7ALIJLUT1NQNea6Xl3EyXhW0/9QhuWEYYTj+n4zU/zO7WQwIm17YN07SxLePcmI4iT4jyXuI9t8v1tfavjNE/v/E/Kfw0U9+Eg/cdbfFrxT2O+Rg/NuJJ+KWO+7A9T+61n8/FgDOPv987LP3Xnjvu0/J6Ur9C/wfW9T/g+yKcNf4f03/v/743ytLlsBoja1nz/bpiYO0xHzA9QsIm+r/qsDf4rKCvC09qOf/ov9PnRljcPKp78aZp38ERx9xpM//hS9dBAC49IsX4YmnnsTHzv4kHrz7Pp/nnAvOwz577433nxreKSVdxhjcesftuObH1+K3N97swxa9+ALe8+EP4hc/uQ47br+Dl2OWZVi6bBn+7bR3+wljCZSHMe50SgfKbRg0xmD/Qw7Cj777Pey68y644tt2ceanP3Wep+13f/wjvn/tD3HHX/5q65/I/8++4Hzst/fefuHBL26+CQ89+giuuvzKGpkh9v8t2v4DCW+YiQmksfCZaQjaNVZ0HIbxShygo4vJX06mMn0afcTZ54kEYgyglO281lbflj46QdGqSXsfDJZ5lLIdhaQUHEhWPoYDI1GjYBCOTqPAGZeThUiTq2g4sSZkwTim4yRr4o5nqVZlBzqsQs7LKSi8Uq368gnUDfFSVlIPkqeYNk5o8QexOoR5pdw5QKJdpwjR5CDLUYn7rqUSq195lI7Ax3Bpe3BHBNJGoMIKGfJAmUj5pmmKcrnsw5WyL17aIvJHynqbU/yWKHddhwaFNiJ5l3pMknAkLMG4Cpl5MnFUiTHG65s0E2/Qp+1ckn9+59kY2GNztd3VkSSpP6bbvgQxn8NS4P/kO9Nu8t35gnGr34f2/2BzUrYQixoybY+FTkuWNptc+mre/2N5e7DsQAn/N05fwW6C7kkHHN98lg1okuS/tS3938siqiOZVtItfULarNQj4wjUNeP5HPs/9YAh/J9HuZB2ppV4GTd8/w+NC/kY0v/dVUcNGGL/j75rxXSSXoKUJUGWS/4R0Sz5Rh3/l3ikTxMX/ZBpGJf3f4tf6jHWPcM3z//ztpSJ7zxWq+HIqUS0Z3E+3pP2WI/UlUyvN+r/Ufsf2YrEO/z2nzLizl8zrMlfow1GlV1+M7LJXxjAIBwtRJDyIi/kT9KtXdtl6/8UPT3dqAxWwHoudGQCbgtB1nA4lbKT3jngoww29tuSl19+OY4++mgAwKOPPiqinS27P4JSbhLVJgqykMj94GB4hreNOjz4IqQPh7QWn0ckLzk68iIReWRQIdRpM2ALsjZcVAbLzscpFabMIdg2xrj7golam5GBAtwOAYlDxkY2JyfrbaDwS2/TNk5epf8VgXJtOztR8p7OIXMTZ9yX4dXkaDdWEj6p7at4tfp6l/GwchG2FtKG+xgsOQqt4w/A9LkXYNzMUwGViHItHUb3Q5lu9Ffb0N9XQWWgC90bXoLOqlBQqFb7bB83bUTa0IYlq0fj5p9diF9f/2V0d3Wgyx2F3NHegZdffBx33fJDLFvyNHbc93OYNe9czN7509hur8swgJlYumQJ+gebMG//i3DEO36Do97xa0yedWiObuP+Aki/NBjoH0B/by+aGptQkf3/qM4FZS/aJdn+swRbV7oJQdHPM9rtaHB6pb0pN8EVPxO8LqM6kWl41ZvQ/mda505GIegRtv8ZUmQts6CrZWBAA/0aqGhUBg16ejTKU5rRMM4APP7ZHQGtmgbttXkQyh0HXRoLVHaYgWxUi3+XRU37b2ndnPZfu/e3kMceJwzY9rVSybBwcCuYLIPJtL1SXlUbphmeOX37NJlIk8FkGRZ2T0O1mvkjoI223xumrvLyz7Z4+/+OOQq7T3LvAaxDNAAY6EnbAtmg8+F8BZABeHJJD2785zJ89LoncNRlf8cxX78HH7zmIZzwjbtx1KV34JRv3Yuf3f0CHli4Dl19wYckXTX9f9Ffivv/tC/+hmr/7cSs+O6vk6t/VgkmX/dlTPnpJZjy0y9h6k8uwtSfXARlNKZ/9ROY8ZUzMeMrZ2Dmlz+KmZd+xNKlxTHS7mhpfy+O7X61+/8GrgIAUMkMVnVmeHFtFS+treKldVWs69HIhLoUgCeXV/DQK4N46JVBPLpkEEvarc0PVg2eXVXBLc/04ZHFg1i8IcNL66pY1WXfY4nGbIL/k2bJNzbS/8+BAgZKAxjsH0R3Vzeq7lSsTYHegV5UN1TRnXTDJFE5BNf2VapVb2/SHiV9MizUQUHPHLi26ZyNAthtWitO3HkijttpAqaManBqpE1b3Mbh3WdqA350xCRMH5UGFyz66YIw+aPvOLyA+FyBjbblDtH/r9GNAyXaj73G7YS3zz4CqSnlujHG6HAFUNUZlnauwD+WPYK/vnAPbnnlXjyyej46B7pwcOsGzGvudrsJM6RpBkCHxTGlNnS1vB2ZssdnUg+SburA6mHLvv8jqnOZXsqpvv9bejfX/8lH8jp8/9eb6f9qs97/nVzEBA4nTyQfZoj237zG7/923FMj0+SD9YejKZL/lm7/JU/MI+2EYTKdBOXH/1zZrg5VKoy1SzqYh8/Dbf+ZjzSRF6aVdFMOTEN5Ma2Mk7iZjjQn7tu/1Urk/25hpNw4Ylx9b4xBpVrxZfg8Q7b/YfzU+4wYc5C8HXPUUdhl7lx8/9of5f0f9j1YyoPlvpb+T75IM8OkfF91/x9m/3/i+PGYNXOmD2fca+n/pF3aLJ/j9HqE/r9s+TJMnjwZEP6/4/Y7oKu7G2maYs/d98DcHXfy3+W95fbb8PSzz+Cwg+xCaSlXyfvKVaswy33PWzn7mbOt3dXc29vr8xDHjb+6GW8/6W1+8lfV8f+0wP8ff9J+rmzihIlQSmHp8uWYOnWql5FSCttuszW6urpysiDtG9rbseDZZzB1ypRAE4D7H3wQ+x1yEI447i245sfXorOrs9j/t2j7b0BrBF/cJbDhStLUdtDcL3OrahJ3z3wUgCSc17DL1TIcN3LSWAhyJZRx3xuyE0aCVjfgEzMn01AYuqDCAGC/3aj57deQhvfETGNgeUnqZBJVcjE9RlQCqTh6QyW2w+uPinQ08gfkv+NFRfp0cBNzvuJyO41ZrjAcSRPDjKuQkpQrumuNp+Q+Nk/j86DsEaA5PrmaRNgAHP8ArM3I3dXK6S8J8rR2ANjBwgSA8pOWdgUdP2JtaiYyjaiowqQf7cGWL2VCm6O8leswyk4jf+QrdatICCwjEZUFKxEjXsYob8+707txOGQFTTzEW3LHjsi8LDuWP/MQUrcCCc7nJO8sgyBxQeCx9ATbl7Rycty4gTril/gk/wQpQ04Eh/3dAKAi/w/Hq1BPPmVUH/A4eFk+albsB1CicyDTaN4ra2PUC3EnrBM34v8AfMef/u8nsoVeSAd/Nl99/zey3hT5CUxL/ZEmhpEHKRNT4/9ln176v1LK0yPzkt4iObMslkGQ8vT8RL5F+QT/z9svcZB/8gDRMLJs0idlSHySNpbJ9GoL+z/xkC/iIB7iHbn/Bz2lafj2zub5f5CFpJV0YWPt/xD+b4bV/uf9v7dq3ORv+I6ln/DVtZO/Wht09LsOuLKNkpUngGFM/hqTlwN5krqS15gXyqRULqGxsRFr16z2cSGtnQS0zyLMgXZHWnn6xR8hP4lkZXjF5ZfjiiuuwLe/FY6SVDxmWMHVbw5k0XCLsNwuQplOoXYi2pbNNHnbCkEF4QQFMiYDHI0uiLKJ5OuFkiOeNzZM2rtSYtell7mLlyh8Fntj87kEkh/FCTtrHyTFuLbR4iF9Lr/QuzFuS4n7+cm/qH8r9et1GEHMp8/rrgyT6WS8p4rxpMvdGxN2mUo7J07mC+USVz5tuA8/CaHNCrIP+YQcvGzhJ61U2oamMfuj1DgVlf4lqPQtgs66PW0qacKoCYcibZmH9q5BtK9fifVrnkNX53J0dSxGx7pFqFb7MHbiThg7cSfMntGMWVvPw4RJszBq1Dh0d/Wip6cX3d096O7qwrq1S/H3O3+Opx79G0aNnYexk/dFQ9MkTNn2Q3ho/iiM2+rjaGnbyvZlk/DdVMDWNV7Wrk6iXmlTa1et8u2vKmj/KXetQy/Khoc6Kqd/8VKqRbvkJ4L508YPChpR14Y02g+2GWEXrO8ksL5kWgJpY7sk6YR7ESd/1c1s/wdHzwSqZaC3CvRr6H6Nvj6gr1+hZdsmJE1V9+3fqv3+r5gETpoqUI2DaGjTGGgYQHXezkDJ7lKTbcGWbP/TJPGfHdDG+MlfOyFhJ251lRO8GfDck8Cdf0Jy938jue9/kP79ryj98xaUHrgN5YduR8PDd6LxsbvR+Pg9aH7yPjQ//Q+UVi/xE8S6qmF0Zgd8TRVwE8GUf6DVDhRuyfZfG4NyAvzmLSnmjXHvga7+NAbIxkyBTuwR1/Wgqg36BjKs6ujHsnX9eOSVdry0pheruwbRNaBRzYDdthqHC07axedRov+vi/r/DrxeNqH9V27St943e9NSA0oNLSg1ttprQytK5WaUyi0oNTTbsHKz/TU0I01L4TvAHo+713YSmD5AGkkTwyQPBNon09d7/1ei/68A204xLlc72+fgqRYYz7RxHu1O2a1pFBywnvHPw/R/KRNZh1L/5J84Y1CpgmpT+NndP8PP7vkZ2nvb4yQbhYdffhgX33wxlg4uRdIUxl4ksOzE+f/I+v9Bn/K9z46ZyHxxwZHNKvt+qpRthZIkwc4Ty/jTSVOx7+QGlFTo5+R+wwD5/m5od7kUQ/f/h5ID0ygovHXGQTh5q0NRNjy9x7Vjoj0zxgBVQGfhXQHGYLu0H2dOWo4GlQGwebTW0FUDnRlUTRs6x5yDgcbdALEgKqYHQie58T+Xnu9lajPe/2V+AsOH8n8Ocss8zGeG6f8yL8uSOAmsa1gGgWVJn2Q485G/bDPbfykTKUNpV7J8/kjD0O//Vre59r+awRidm1Qj/uG0/8kmvf8H2Y9k/E/6JAQeKX/l+mCks7D9d+PJDDfDbP9lPDbb/xP7vgzXv+Yu2QK7VCNs/1lerCt5jXkhns3y/0rFL9rggkjKTeYnMFx+dguR/5MHmYdlGOH/3IxFIO0wwGc+dR5uveMO3PfPf+RkFAPLsmXU6i/5X+//IQ3x0D8k38Qf+39bWxvK5bLHQ7yvlf9LXBjC/3mKUVLP/10+hpN/CVKGEHb80Q9+CN/9wTXY75A34YuXfgn/dsJJmDljBswQ/g8xlANBB8GINnPFypX4zR9+j5NPOMnHM45X0prp8Bk7AHjhxRdx/uc/h0+ecSamT5uWkwvxyKuEJEnQ0dmJf//Mp7HL3Hk46vAjfLrT3vkuPHj3vXjgrntwxVe/hvsffBDXXHutz0d+X432P/E7cbMsN8nLAR9+aDyHkNvc3Y5eIzoNdFAJTMOypKD4M5GRkDmb1nZE+e1En5Z1kDMOn9ffBZpJoyxfGwNw0tdNPjItDYGTsxQ0ZcHJWxnOH/k3xg6UeP7Fd2X9AI+yE11kho5F+iReVixJao9rZn7ipCy9UbgjsEmLETLWPGrETb4xH+PIp3arR4xbiWptIzRmRqw4IQ3Mr91LPZR1eOn0TCtpo8wZT8i0tpOlxviBBzakMj/5p+0SR1oKlSDT89nLzNgBWDqGxE1cUobSGZmOz8xDXgx3ujq7YZyPF2ml7JlO0h7Th6gCkzImn0p04GM5kF6m8zJ0wPJk+kR834L5GVfNMs+rBeVfQmPaZXk+XtlT9ixNeT6rkf9TSibyf8C5k1jxRxqpZ+ZTotKnDOgTkk+rl2APpEs7Gyd+S3fe51h+zv8FHuv/FpLELcgQ+fnz/i/qSUkH2EA7/NJ2iEPaWcmtOvV81/i/DaP/V903H1jmcPyffG6O/0saEuc3Q/l/TiZRJ4jp+cz0zB/bKOknL6RhpP4vy2Oc1KPkm/kZLmmP6cPrzP+Hav9j2mV5jCdImgjS/zsHUGfy19YbOpr81dpgVMnROcLJXzdC5flE5HcM54/885k0M09aKqGnpwf9fX0Wl3y5cgN0MRixc9ZPDop7TuYqudNV2fBSqYRj3/IWbL3N1qHuc8d6kTePQ1zdQ5CLsQupCJZuztw5OSmXScjTPfhyQpzk0+X3YXkaQl5luVb2KhL4uFw+ABywlxA/e4hEH5KRJ4fPnbARkofpb5/F6zHYGHPYCXWGuWewADfp4cKLJn1jGzCOmFj30l5phwRpm9I+lRI7cQpsEYgGcIVfyHuCcnPmtqx8OH9wu30JNh0lyjAd5CcSEzcA9K6/F12r/5vbBjHYswC9a25B9+pb0Lf+TmSVjlCOAmbvdComzTwYpjQZHV09GBgcQE/XKnR1LEVf7wZ0dSxB54bF6O9dgQMPOQ6nn301zvnCdTj/wp/h3e+7EFvN3hU9Pb3o6enBwMAAnnr8Vtz2l+/h2afvxrq1S/GLay/C4ldeRm9PmHyWMlIqGlxR0i6sFfR2d2Ogrw9NTU0wUd9H1kPUsXZ9Et92OLuQeY3rC/Fe7ga2z2Hyl2GaefxPh0U4gifWibIt25z2n/1/LQasN7X9r46ZBpO1IBs00H0ZensNOjYY6NEltO1Ygkndbl9O/DbzWoVqrqDcWkUyWqNvpz1RbWkrpIE8b6n2P9efdhO/MHZgGeAksPtNmg69w+7I5uyGbLtdUN12Z1S3mYfK7LmozN4Jg7N2xMDMHTAwY3v0T5uD/qnbodIyGqaa+V3ARlctfp25BRV2xTn5S5IEmWuLyS/jNrX9p70SrjqkjDltrr4wxjYfSFCZvhO0rtizWEW9ODwwOGinyfjOh/fF6Oaw44N2R5uUtsh+TuZ8ivWetDHyzx/5l3LJT/qKnbtiwjY8iwndOpO89tjnMIEMh4Ph2CL9/3zfu17/31fVGwEmia9KtDcmV+PnQYYboYOcnDfi/0wv/ZE6VwX9/yJQJYX1Detx+S2X49SrT8VND92EnoGeOFkOtNF4dtWz+OJ/fRGn/+h03LfmPlQaKvWZdRD7fxF91J2K+v9w7b9yfcrELbSX8ZYA1t3KtY0K/DKvUmLBm21osfWYEv7zuEk4elYTUuXCxc/qoyYYxgCT1KBt41zJ/CHiSdolIX7/l2lr3v8dJCrF27c+GgdO2QPG2ElerQ3XtvhyMqUBd5ofjMEYVcF50xZjcmkAMBmSpAqV2/nbjM6xZ6O76SgY5Af3Y5+T9oXIv1TR+79oN+RvY+//tGXi35j/l0u2Dtxc/389vv8b12/AZvq/lAPLSYZ6/xc+JsdxZHkYYfsvaY/pwxD+z3LJV5EcyLs97jlff+J1/P4fpy32f/ueRp1IOiH4od2xPJYt+ZT6R+R3EjfzEj/LkOVKHath+79GWirB6CH8383HED/nNCQuaWcjaf/ZQCfC/4l36pQp+MRHP4bLv/1tdHZ1WjwGYRf2v8D/JY4iu+cz0zN/bKNSDlKGdf3f4cIW7P9L2mP6sIX8n+mk/LCF/d8h8fiVcu+6Lv7J+fNx4VcuxY+++308cNe9+N1Nv8Ktd96B/7zpRgDAdf95PQ447GDse/CBOOCwg/1OYRj4T1XGIHk0xuD2u+7E3B13wvZz5vg4rTUOOOxg7HfIm7D/oQdh34MPhHaTv5z/+9ttt+HMc8/G+049De895VTPA/HKn3YbI4wJ83/PL1qID53xMcycMQNf+o8venmoyP/33H0PfOxDH8Zv//iHGrxbuv0vlUpIvIFEE72Jc/QYgfxlVTcJ7AYwWAHFwoknS0m4LljpwryeSZUf7JDlswyGw9qC5ccZrnRCe2/xZ27Sl/kkfrB8sZqD+IyxA20cCPFpBY4kCUdUU7n+6I/EDuBpY7xxsXKDqyjTNA27r6OGTrndyizLOMOQ98wveUvEig0+a/IidCDx+TKcXHlEr5e1SEv82lXiytkUcTCNpIU4eK+E8abuSBDKWeqUtMX8WfmEMuDknYkVa8zPa/xSL+nhik+mJX0SP2lgXv4kr6SS326ACrueiZMDDBwRzVwY5Z+mqZ/Yk2Upl5aykjwwL2knkAfeS9liJP4vGgGIcliu1B3cZCLLIO56/q/cIgdOmjKPLB+uDIbLdORHrka0HXLh/4JniR9F/p8muQF1SYPUcSzL4P+08VCPUH5+d4fwf9oK80HUdZQZ6S3y/zRNfR1k6vi/l2Gh/wefJDBeymAo/0+3gP+zPClX0kQ6iFPikjiH8n/JD58lbZvv/3I3bn4FNfHSD+Jy6JvMK9OwHKaNeaMOWBbv8Rr5v8zDZ9LPtOQRBf4v9Ucgb8YYtKb2qk08+atrJn85mdEx4Mr2E3K8Bj0WTf7Sh1g20/OetGJY/m95aGhowJKlS1GtVOCJAOA7yOQ7sO9fwjgh6CcDld3t4Cr7kF+ghZscZll2AtHxIvAhkrkEOekIuOxKOSJdZ97YlJB4FP+F51BGbhY1MKk4EUbpi4kxn14wGMtL4vQyRT5PDKS/iB4fKOjLYbOZKdFAT0CWkyvLgtWJr6lVCIMJsqHd2FirdxN/J9jRzvB6+iQe3iu22cK2mafI3ovyQpQTl0ew+R0PYlLSPivLWSS2PCorNIrGgsmlMSaDgn0vAQyq/UvR1/0SujfMx2D/Suhqh0vHMlNMmvVmTNzqHegZaENHl0ZnZx96e/rR1bkeq5c/g9UrXoRWW6F51GwABi2tozF56tbYfu7eOPnUz2Duzm9Cb08fenv6MDAwgNWrFuOhf/wW//P7K9A2JsXue++NJa88jL/f9XM89uAfMP+xv+K5BXfhxecfwOKXH8OSlx7DquXPYe2qF7F29Yvo7233MqxUKli1fLmf/FUjaP+DvmxfPBHt/2DFHQun7cQv+8G5iV/X32EY9cWBHTnxy99gpeLr8i3d/qdboP3XSYq+uQdBm1YkAyUMdqeoDqSYffhYpFNLUGMMkrEG6TiD0jigNBYojzMojzUoT1RIxhl0T98RgzPnwqR2AI3lSDnEdGAT2n/2/wGg5Advwu5f7s412n2zWWvoplbocZOQjZuEbOxEZGMmojp6IrLR41Ftc7/Wsf5XaRmNLGkIR0Zz0teESWA72Vyr6ywLk8DkST5L3WGE7f8O4xL87MgEkxu19XVjYAyQtU1GddRYmOoA7E7gfJ00FOw+exwuedduGNdahh5G/185G9ZOn+QHUX0o+3iqTvt/6LypYYJWTPL6CVvNiVs7yYs43k0EM54Tx/6ZE8Vu4cuBe+6Y4432P/z+f9CpxBHLIE1T35QZX0MXN6UyjD+HKP9coFWJ37e9m+D/RvSReSUePieJfZ/jO1khpEBfSx/uX3c/zv3puTjwPw7EV/78FfzxyT/iqeVPoaO/Axt6N+DhxQ/jxgdvxJk/PRPHf+V4/ODeH+AV8wqyhizPcAT0Dcp/pP1/m48FhHYVkdzsPf3O9hwM9S77BNSJsY3v5OYE3z5iPA6b2RQic7/a2V+TDeLSfZysXdlS9pJiqT+C5NvTJXiW6RI3HpIkCUaXW/Gh7U/CkdMOQIOy/UDtJnx9H98YW6UaA1UF3jJmPfZu6nQTvgYKdrFTpg00RqN99NnoaX4zDOyOrbhs0lOv/2/E+1PR+B/bCombvI68/S/2f9r3Zvv/q/j+78fnhE5JUzy+4evpLeD/pK2oXSYPTCPzGmNtimNNdgw0+DBB0kBfj8vZHP+nDlgW71Hn/T9NUregLOhE8ut5cz/9L37/Jx7Js0xn5aG9/I2mTixImcl8fCY99COmleXKtBKHxLvF/V98V5m40pLzf22Qlko2v5ssJiQF/s8ypQ6MMfZ0kQL/R8Q3hJxOOv54KKXw+z/92dKs7OmlEHZBXkgL8UnZ0Ebo/yxPypU0xXRIXBLna+7/BXTgdez/8XeoZX6mlbzxN1L/B4DubrtQjriffe45zJg2HUmS4KfX/wxvP/Ft2GPX3ZAkCWZMn44zT/8Ifn7jLwAA7zv1NNx/5z144K578cBd9+J9p5xmaVZAe4d9ryfuF158EQAweZI9cpo8/e5Pf8SJbz2+xv8fvPs+j/fBu+/z/JfSFL/9w+9xxXe+hcu/8jW8592neHzM29vbmyv75Vde9sdLl0slPP7Uk/j4uefgPaecgq9e/CWMbmvLyS/2/7a2NgDAwhcW5eyHsqzx/01s/51M7A2NTTIWG6UkAmJCK0nsB9+Nq4zgjttVzrCqrlDioXFL5igIuKNx7fG4wUlYjq8YRWVOZSnXASnixwtOKTuxxElrYbSST/aYSRN5SUvhhVCWwXy8J52SHridsAQqieU6hdhdlMIoCNpY+qkzpjeu0gZXvUVGQt5zzix4Iw6mh5usUyqxQ4kq8UeYMD/5lTKI5cHJt5wMRB5wYtM5gqXFrSp0fFDnUr5ZlqHiBpokTnYOya+c4CddxGHEJCDjWYYsSzkamJ/3zCd5kXhYlly9S1rBht59bzpxR2MzP4RN+046GxUXZlyYfxl2eA1sw0v+mJfPKkmQlks2PX3GyZt0k3bqLcgmb+uyk8K8cZjK+X9ij2bZiP9nYrWY5k612P9lXqETaWuSH3acrN87HQl9yR/pgauL+Jwk9hsctIPY3s3G/N/7XJCflC91TP6pBwLLSwr935ZHPcpFInzOtD0ekvZA3oiD6YP/B1nINNIGpAxieUgfkTKQuGv9P98eUeeMN0P4f06WUQNPuoiDeUgj8/Ge6UgD8/Ne8sb0Eo8sgyDvM9fRJ05JByKfgqOlKEyWbSFPG9PxOXFHyiDSq9SdTC9lSly8j33dFPh/IjodxKNH4P+yvET4f+egmNw1YfLX+MGcEM9dam3lIF+4iSSWAQwx+etepFg+dSFlFstnaP+3R0E3NTVg2bKlyNy3e1ztbekxxj0HMLCd3XgC0FVkLpGbNKTdc0iNPAkg3zUTuyzLgbKFysjwLFHKeznJS6EyQS4dJ6WJUJFYR5eYDAdcnNWnDSdOi9/TKlGKrDUBIo2fMM0xF/HOND5JviBiyNNVcytsxvIRynRXJSfUGWTjvG5q+LFAXN6uXULDxQIOD+/p88E3LDA/09YL473EIa8hjwKgvI/WK4/02PsgayVsKp81hLWMPwSjJp8IY2xZSXksyk2T0DRqFtLSaCSl5lz+pNSMptG7Y/z0o7Dbm76KmXNOQldfA9Zu6Mf69ipGTT0F03b6DLbb50KrJ2X9TbkJbKUUDj3mfdhrv2PR1dmJrs4ue+3oRHdnF7q7u6G1RnfXOrz8wuN4bsG9eGb+nXjq0b/isYd+j4f/8Ws8cv9vcP+9v8D99/wcLy2839cZ1SzDyqXL0FAuI3UDAErW2QXtP9OwvqGOtQ4rs40xWL58BdatXYe169Zj3fr1WL9+AzZs2ID1G9Zj/YYNaG9vR/sG9+voQHtHBzo6OtDZ2YGODvv9466urprfilWrvFxkO2S2UPuvnVw40SxxslzyT1yUA+/7t9sDG454L1bP3h0bJm+FhuO2g9ltNgb7J2NATcZgwyQMNIzHQHkMBprG2d+ocehrm4H2bY5E7zYHQjW21PDCcmRZpC++H077n0g87BtirO0bghO/7ju+1QymWrXf+a1mMJm7565ehjONDOe9m0iGm4A0pmq/B1jaytNFGQPw75zJZrb/xsXJ9t/oDLNHKzz8rjKOmw2MalCuBktQmbkbBtsmIDNVQFfdbv/iylBBY+KoRrx176n47of2wYS2Rk8HBE3yx3AU9f83sf0//ci5ue/z+ong3ASuuB9qN7DY+St3D0sZvP/EN3m6pcxJI4Z8/8/bNXlnGskvcSr3M+JKMOLn44LL5NLJK9PWPBs7YTxc/zeOB97L9+HEvSsX6d4YgwlNE1zpBaAA02gwOGEQr6hXcOXfrsQHr/ogDv3coZhz+hxs/9HtccyFx+CsH5+FXz/1a6xtXYtqWxUIGz4KYULjBD9+xvd/2hz5YBhpleD9yre7+fSMh5z4NU47tnEO+V0DzFKs7uzTpNYSfn3iZHx0tzY02Qzi5xJnGqNLGodNGsRvD1PYd7L1nxrao7GOjfX/Aw/5uoZ2IMczAGBK8wScO+9UnL3LezF3zLZoSkrQysBkBqgaqKrtU8MAU5r6ccyYtWhJXN2itT2SXI1DX8vRWDv5m+htPRmZsZ9HkjTyPvZ/2in5QsH7P3XM95+gPwv0SW/XI2r/i/zfnuywuf5P2uU98zCNlIHEPZL237iyi9r/zJXBPpoeov3nlWkYL/llOtLA/NLWiIPpbV47xhXKCPomrRhm+x/TXBQmyyZI2lDAb9H7P3cAm/8l7/8yryxL2prVg7ZHGicJdMbxvyBn0iR/Ml7SzvKpC+pe0sj7V8X/s8yNxUf+7yZ+fZpEQedkHsZckfP/4bf/vGf+mN/RbW248LOfw3d/+AMsXbbMts8Cl5SBxD0S/2d52f+N//kwWTZB0oYCfqX/c1Et+TCvov8fedgR+Pv9/4AW/v/Mc89hz913z/El/R8Aurq6PM4i/3/j/m/AM889ixUrV3qaX3z5JcyYPgPTp03zNC9ZuhTLli/DrvN29jyQN/ljOAA88vhj+P61P8Q1374ae+6+e43/H3bwwbjl9ttz8ln4wgs4YL/9AQAb2jfgvM99Fp/+90/h5BNOHJb/k19+x5ggfYJ64r2sb9Sw2/8M6flnnXUxETGSzNDxqtVqjlgi5jMLVa4Tl2V2slO578fFeOWVhkIcVe8YNh/T0WAMAtNUghaVizQ8KSQgP2Em6ee91naCxIh4v3OXQo2UBcGbUraTwjDSDIRJKqXspJis+DjpqVR+sFPynbjvDZNPxvuy3EuNdAyZBiLOwB2LLL/d5b7xmmV2oigtlWpkJfHxSh2Qt8yttrGTjYE+GijvvbyEEfuBPLFagWmkvGmLsXwhK60k2EAAK3sOiErZUNYE6sOaTKBTVtxSJlIXTKsj+5LppPx8efzeYnSUh88jOi9J4o7vFIstbCTCREESJuF9WWLgUuswSS53yhIXV5ZVcv6fAG4gWeKRfFKOniZWOsoN6btvNysV/JU4pHw9KPvNOvoJ9Urbk2USH9MwnafBo3Q2rZQfaIt9S+ZNYj6F7VEOyvm/KvJ/+r7o1GSZ7aSSVuX831IZJq0T5w/kV9LI8skby4vThDibLhUryiT9mTvCo+S+/UEcxC/DiFPKhf7PMIzI/y2Q15H4P6/kiXKWeGU6RLJRdf0/XEnTcP2feSUepuOV9DBe4pO8yDxKdECJg3HgBGIunQJcuwlRFuVHemUcNrH9N0P4fz0+JI4i/y+i9aYXFAaqBsYf66btvd/Blp/8NcZgRitw8vYJvv24zUe6gI1P/m43RuFtc4IPF8ks5lfaJ+PJM/1Ba42enh60to7K6dTWI26HrxuoUyq/q9dP9PkD+5yq60BuoldZm4jjjHGTr6LvloNgZuJqqUVOz3Jylf0uhjvcJEHIzQInPwPeHA5lqXXVt8siEVocUh+1hMf3ReAJ9I9W7yr0T5X9Z4ty6T1PlEHAYzGR1hAiy/GxuTJkbjdhrNw9+SQqpqHN1ZSV918+S5D2urF00v5jv3V3ef6UDVNiQpe6lGXJ9HkaXLTHC4+f9QnTJOVRSNMyGppnoLF1e6SNM33ZNC+LRaFUakHrmHkYM3FvrFv9IiZvdThmz30fmtpmoVRqCkR6dqxE07SM2dvugklTZmPF8pfQ3dmO/v4+DA4OYnDA/SoDqAxWUK1Wff3or27nxS57Hotd9zwW5YZm6CzDyiVLobVGU2Mjki3S/of6o1Qq4blFC1FOSyiXy2jwvwY0NJTR0NCAhnIDGhsa0NBgr/a+EU0NDWhqbERjYyOa+GtqwlYzZuAL55yDsWPG+Pocjr4t1f4btxvWuEF+8svrsNp/pWAmTILZbU80HvgmJHPfgIG2fdA3ei/0j94b/aP3Qd/YvdA/fm/0jd8TAxP3RN+E3VGZsDMGGicgKTXmZE5eIHTBsiWf9j60B54el49hzJOJRa0MryRzUCnPw2BpH/SX9wVaD8D2k7bG0TNKOGaGwltmJXjLrBTHzi7h2K1KOG52GW/Zuoxjt27AW7dtwFu3bcKx2zbiuO2acdw2DThh+xYcO6cZx+/QguN3aMUR247HVlN3h247EtmoY1BtPQZ9rSdDNUyuodHYm81u/yWOmvZfAUfNKmHvSRqNpQQvbsgwaBLoMVNgWkYDWRXJQDdQHbC1hbG7YE2i0FpOcMobt8K5x+6IdxwwG42lQA9pLaKb8Zx0988Rn0F3eRuwYfn2f+LoZkwf14p7nnzFHrBrNJTh1R4tG57tjkMf559FepEmhs98+Hjsu+u2QI3/h7phS/b/v/2gW1Bs1eWvoeTwLMMIMq/Mn/dcF+/qXAA4a++BYfm/bCGkDKRsaIPGpSOOVb2r8NS6p0O6IlCwk7pNgGkzMKMN9FgNM9bem1EGaASQ1BFABO+a+3a8YfoBflIrljl5IyS5/r89KrW1zR5Pn7gFzzK/VSVtOB/nHqDgBvBp9/QDkYbPB8xoQkMKPLR0ABkURo1qQ6lUxth0AGfOBT6wncH7tk8wrinkYRmK9bGxfVhtDBKl0N3V5dsMVdD/55X65oJn1ide98JPEyhs0zYTe4+fi21Gz0SqSljZtxYV2IUu0ACUweGj23HK+FVoVBoZgKy8NfpGnYyOtg+ht+1tqJZmw5igA+k/hNj/GU/d2fd/jv/l2wqC5Ju/uI5iWfRPaRcyTRwX/N8aBMveFP+X9eKWfP/nCYmxHl+X7//ufcmGh7EqySfvZdmkh/Ee3ya//1tc9dIxnvgTN07JekCW93p+/+eVMmKZxMc0Np2zPe0+YeTeb71O3H3sWyxD0iD59LIt8F3ik/n5S4T/y92XMQ7Jt/30YeIndhnPsigvvzHOiU+p8P4nbWHo9j+r8f+Vq1bhT//zF3zkgx/0Ydf+7DqccNxxmDxpEpRSmDZ1Kl565WXcee89MMZgxrTp2H3XXWE20f+L+v+kPZYvr6++/wdfIG7ywnySJ8mnTMcr6WG8xDdc//ffeHbPki6ZLi5Lu2OOSa+Mw6vg/xMnTMA1P74Wu++2G6ZOmYL/vPlGPPf8c/jCpz8L7dqca6/7KfbYfXdMmTwZy5Yvx7e/910c8qaD8Mb9D/AylVetNcaPG4ennn4aL7/yMnbbZResW78el379qzjz9I9g26238bz988EH8PBjj+LcT5yVoz+mm7RrY/C9H16DGTNmYIftd8CKlSuwavUqrFq9Gh2dnZg4YSKmT5uG/7zpRoxua8PcnXbCE089iW9865v48oUXY1RrK/566y147vmFOO7Nb8aq1auxas1qrF6zBmvWrsWkiROxfMUKnHXBedhm9mxMnTIVT8x/Cp+76EKc+o53Yt+99xH+/+q0/2r5s8+aTHzsmPfKvYBKSFxYmoTvSNUDFpwkKarVihd04s5P9xUgnTRnSLWOC1e5MZwGIDt+Eh+FZdyHzKtZBhRU0tLw5cs2w3K0yEbDGY3Pq+1xEwwjL0kSvqfMMkhbwBEqAyPyMl4l1hj9s6Ax09o5aqgwJcQ8KlasTk7SwIzTg+e3oGJimORd0pqktuMmy0RU+cQVhMfrXkpkmVKPkjfKNsuy8AJJ2t3Aos3jKkfxIqhcpcaVMLbMSOZ+RVqgg+VJoPxkvthyKRdpn7n0vsJOoHWG1B0tJ3mWKwllA6RYkYtGkXxI3LIsKVPeUz+SH+rJInAy9WmDDRQB6U6cv5MePpe8/wc5xHYfQ+pW9EHYNWmkbpIkAQr8n3ojXYDtEJJvRPK2QXn9cKLY0+jKptxlx9VI/xf4JN0xn1IHSrmJaW2gxAB4TCPLVc5eZRyEnOQ9j+4j3UmSiOMV83WvLI9X8iHjiS+nBxePYfo/42WZUo8yHWUr/VHKU8pKhjOu1v/zaZX3fwvJCPw/BvtCOBz/z/uyxCd9MY6XebT7bnbMN+s3s6n+L+iLdVsEpDup4/9x+0/cMd0SmBYAfva8wo+eTdBfsfZk4slf960vTgQbA+w/TeHG4xow7xfBb4GNT/4aY/DeeSkufqOtl2Mardzz/k9eKCumkzJXzr8HBgZgAMycORMNDY1+0nc4YNxiHDf6EEdbICoDuMrER5Efvhj7axFIknwaZnKg4PBH9EsaQksc4nMg8nt6anGyXgwJ60DMk7K65YKqOC7IIR9RaJdGzkLX0shwxYUZKldARJzVjVJhEZDHJ8qlb9FOvA7h5OEmhiX4tJ41i488yfw5XAKK0tYDpgGU/3avDbLPEhfFYvHZdEWoPUohdqZj/jw+ONnb/h1UqRCHTZUXtw+M1MMwGczMSikMDPRj2eJn8c+7f4eFzz1s636VIE3t6SGlUhmlhjJK5ZKdZG1owOxtdsPeB5yEMWOnAAD6enuxatlylNIU5XI51++Q8oerZ0obaf/5bmfYPotvqbEPFLdLVm55e/C44/Zf9I1kO8d4vArtPwfO/nXtv6VFtpcxjYS8XGp1KWnOteUCn2yLh27/N6f/H9p3VfD+z7KShItFhQ9EQLrVRtp/vocSd45uhZxDDmqFDf0GNy/U+O2LGZZ1G1QNkBgNVelHabAbaTaIsWkVH9h3Et42dxTaGhO0NDUU9/+jvjHpIMh3buZlmrxsQz+cYfXa/+eXrcN1//Mk7p3/sp28NXZS11ZWYZKXu5rjNAriOYI37rEDPnDSwdhuK3vsHQp4pB2SfuozqfH/kN/r0l0pK95v8327G56gIKpMWUe7MBOncdcaoLzdo8ynACw+u7JR/0dd/6+gVCpbvEP4f89gD771+NW4/eU70FHt9DheDZjQOAFv3e4tOGuvjyNVoa+JEfp/pVLBlOnTo3Y0SI88WvEEfiH1HckMzC3TirjBzOC/FlVw0wtVdAykOGmbBKfPLWFUg0ICpwcne63thDLfkT1l1BeAFctXoKGhQZRgB7q1sLs0CeN//F4f7VjWcUXv/5nR6KsOYO3ABjy1/nncs/JhPN3+Ivr6BnDd9gux79iJyJp2wEDj/uhrPBA6GQ0kjV5m0qYo9+H4v6RN4kDB+7/UTXwlsFw1RPu/Mf9P3eSSLEPmJ05eyYeMZz7il2VihO2/bPekHmU69S9v/y2w/pQTijHEcmE6eYXwjdi/MUL/Jx8StyxLyjRJEmQ66MvzM4L3/1qOg06TjbT/Uh6x3cfAtBAyJY2xfAOP9lvX1azq6h/pjzo3OSzlzTIkLbyvoXEz/Z8lSh3IMnJXF0fQWruNOqFfL8EYg5Q81vH/JDf+p/wYK/MopfD4U0/io5/8JB66517Px/6HHoIfXnU19thtN49vxcqVeO/ppwMKeP9p78F7330KEG0+oM5Iq6SZuBkW9JjXDWX72vq/tVkJ0l9iGgnmVfb/zL0DGnHyRcy3LEvKNN2k8b9gT/WAdCeR/9925x342hWXo6u7C/vvux/OPuPjmLPddh737//0R/zi5puwdPkytLW14d9OPAmnvvNdGDN6jJcdCvy/q7sLX/jSxXjgoQfR1taGD5z2Xrzn3afAiPb/mh//CM8+/zyuuvzKHA7eS3nD9f/P/fT5uP/BB3wY4YD99sd3Lr8CAPD8ooX47Bf/A8uWL8eM6TNw3tnn4ID99oNSCjf88mZ89wfXxNkBAA/cZRdK/OdNN+H3f/4jli1fjpnTZ+DEtx6P951qvzMs9SavBNqL2sT2Xy179llDocaI5bM0XInAOkZwRN6n/ptFdNSqOzKq1rBpRiHcGkuOBsGXUgqZNrCdWTqf9hNnWnzQng5hIqMJ9IVvvbAs5mW83TWad1DJr3GdlhiUsh1p0FkEfkun9vRDTOZqUeEZY9y3UGsrMvIEIHdEs0ybkzXzCufMy7jW6ZHTS5ARw6ysbQcozk8aZDmB3lDx6OhlRJYj8bBMW66VVbVa9burvQMo+IksY8SkdwHfshztOkL5sNBoIydv+ywrde1WN1EGnl63Cpd5EcnGiIY4pkvyxXiZn+moBxkHsdKDaUqlsp9MZroimefsIvZ/djSG5f/5MEi5+IbNli/5UbH/wyZT7gVWyoF8xJ1guWuXfFKGnj7BP48sIU5ZBq9G+r/Qn9QtgfhQwJukk+GSLqY32g5gSz4leNpF4yjTynJtfMgv7Q2OXn7AXkJMuwyTPPCZQBpkOZJe7Wxe0il5iPEwDcuh/yex/0d5aH+MK/IzRJ0fGUYc2Ij/m3r+rxTY7hGkbMwW8X/qMW8ntf5fqsFRJHNpF4j9f0Ttf33/ZzkEGa6K/N8B43hPWmL/lzjIJ2UY64m4JE5ZhizX+7+QC3FIkLTHvMV0VitV9PX1Yeq06WhraxMTdo62wtds1I+3Jjc0xGniZwe5CWkWY5ieN/XzF4YzrCguhjiNz6vsZCI4Iydo8WDDrPwZJguX4MJksBHhEnyRIo51GIn1UcxbywQnZV0HyF1DHl+Gm9SV+pZ6YRoZBzgbJDnG9oXEqLAP92mjMEK9OIZLHLR1JrNsBfuXkC8myJJ5auSei4PllmJTVqYUJSKxQgx+S/qCXrwAndxrgn05gV8bF4kLALB86fO486834JUX56Ozcx2UUihxErhcxrQZ22L3fY7EPgccBzgZdnd2Ys3KVWgol1Eul305yUbafw7gwOmAaY2xO6p8WpE/ScIgPPOF+lhMvER1l5WDaP8FfbI+Jw2yXfP8bEb7z37dv7b9t23Z8Nt/5g38Ea/ZSPvPnVCMl/mZjvlkHGraf7vKPsYRZB4GK/neTCCdSrb/MFBu8qBe+2820v7LSWYZztOuJA0eXqP2n7TJcObNt/8BhwRJe443R0+sa0kX00va5LPEC6EfmzavW+KP80p7s/ny/kuIaZdhkoc4P2mQ5Uh6tRtMJJ1cRGIi2cW8sJyN+b8dV6D/h8HxJEnFGFGwefv+bwfTWPlRF0mN/w/R/3ef9JD0yryIZGPo/2liT4VyJ4Ax3cj6//a78ZOnTXXpgl3I8mwcrO3CQpC4ozXSARtTu5POPpM/OYZmtJvgLQhzyD1uKRMZvmrFytwuNAnqNfJ/WYYst9b/N7//jy3q/yGtLDfOa/3AfgOS+cizhJh2GSZ5iPOThqH9P9/+x2OxEg/TsJyN+T/zWP/f0u2/8H+3MckMq/23IGVjNtL+j9T/GYdhtv9W5gFXjA/12n9HfzpE+x+HIbInponDlbCtGBjHe9IS+z83rDGeE75aZyilJXvsNWAXzQubI05Zhiw39n9shv+z34zh+n/kn4ynfnzaxI4dGmOQuDYupjFnbzm51tYxT86fj4+e9Uk8ePc9PiyeAGb+3/3xj7jsm1fik2ecife++xRXTrAZWTbpLuKXwHCmYTn/Gv+34XwubP//Bf6fOVsyIg7e/+291hnKBf5fJHPSQSCdgR77nPz/ePyvtv8ffFTyK2UoQTm/QgFvMZ0Yrv9H5fCZdMRpZblx3iRJaieAmVFFCogzM0wJw5TCzdwZ9mFispbwJOHkn3SMsBrVmPwxqDKNfHFkedKBjDHQblI4y+wkYSwk7V5QGSaNnHxANCIMj/HIeOa39Idje0kv+QjKd5VX5JQeCo7mgJBmKC8YKsOk02knS7sjO+wAoHNSPuSRwHSSb8mr/QtlS5uRvBAvy/Txrhxjgh6ZVuKJcXsnFLrS2r5kkPcksXYS65VXdob4HCoo+QH24gqclQ2BMqCsrP4NSuVyDS+yTAibiHWs3EqlssMh41kWaaBceZVlMj1la/PW2luIG6b/u3i5iohyDP4ffCWXV8QZYyc54WjIhQufsxmtS1B2GML/jTF+p7HEy3KIg52qxHXmGOd9J/L/3GBrFE+aWT5frmJdyzySFuYlKNeIxCv/CLI8xvO+qNFNksSfyGCE/yduhRsHVwlMRx0Qj+SR6bAJ/k8wrgEfqf8zrfd/R5u0B0k30+gh/T80zrJ8qZfY/xHJirIJZYQ0skxsUf+3NEk/kLg4CMa8Eg/v+SzpJP4YmE7KmXIcqf8TiI/hpIMyYhrKDhvxf2knkhaJg2GxndTz/yI8sewk/cTBMmKcSinoTCPLMvT19aOhoYyJkyajtbUVmwOyfA9K+UnTmh2kCgBy20bcrBdsWuUmEyXKGtXGCSS4PlFMkwPKzUIRnhBm02qAfJA2kGamjfHYZ2PcDmBPv5w1DOnqgVKUXy7U8RhGVZnO021T2Dvy6uWRL9OyYem0SfN4bIjDwYlJsXAgXhRgrPC9VNjWSVuO0zMs6KUWiCO+hrg4BwA/GWvvA6igBj95W2vHORP15co8EGVYucVmF3AIPVDEOd5tmAv2yRCS1uCGCF+3ZhnWrF6KF55/HC0tbZi19VzM3GoHNDa1+nzdXV1Yu3oNdLWK5uZmV08Iuy6QAaSOIl0p0f5bGm1YkiSoVvLtv/btv+z/h0ExE7X/cjLaGDupLPs5pCPI3t7rLdj+y34d62pZp7767b9dbCyB/JJPk2v/Ay4Ohlk5D93+V0bU/o+k/x/0Eu6t/o0zXIkj5hVwdY97X6ecKccsy6A30v5zkkjGK6X8SVrkl7gB555CdniV2n8uxsZG2/9QJsuV5VN+sa5lHkkL8xKYX+KSIMsLaS1u+r9Ml4gdGaam/78J7/9Cnhix/4c+nXHvalzsEOOJccd1Rez/3A3KRd2km2m01iiVS/a7kMRRiv0/X09JvQzZ/8825v+hTNAmXDsHLxNL78j6/5bParWKSVOnINeXUHCnA8GFk/YwBmOjxESvye++rgGXjrTwmig3kcewOB9sXh8n5ejwrVy+AuWy/cYubS8kefX9nzaFjfp/0GcsB6mvnK5fdf+398Px/9TtavvX+H/gxzhdbSn/f/Xbf+f/QiXkl3yakfh/gY7VJvq/9AOJq177LyeAGSfpJP4YmC5J7EJClkvdSJpikHEy3uOr0/4zDWWHIf1fh/F/Ma8Q4zBGQ5lN93+OzUnZSfqJAwX+Hy+cZF4C8wdc+WNXZHlxWvq/fMdP6rT/ac7/a3fVSr4lr1IOyPlogZ3pYBMyD4T/S59mfC3uf6X/h/LJG4H86teB/+cXcFo7q7rxPy60k3h4z2dJJ/HnIW9TlDPl+Prw/81v/03O/+19EZ5Ydix/S4z/o8A2CLK8OO1w2n+17NlnTVyoRCaRMg3jmS8RLxGMh2eWThF2HfLKEonbxgWDMkYc0yeMo+pWWHo8kTGTNrkrVyXF2/7jDmyW2/af+iONJdAIfNk1inFyEcf+6khRgWbrrKxQghxsOcahjuNlnvrHftpw7WixMs1XON7ZhJHK8hDJlWm0e4GSx+5I3siDBJbnndThKZcbcnhptHwmSJyUQS7cDxaGykKLxkvyLWllGOMJDKMO/bOzzVKa+gUMxOXxiMrCXmsbDDgfqbojUVhmLG82bkwv8VCWzCvTsGzGUafBTkKjInEyDEP5v2jg7QpAuxKL8YgaNtIR4/Xp3aAF8+mowWOeJHFHnYgwlifllgt3cUX+r5RyHSTXKOf8P7+6iaB1OCZ/qIlZ5s0fr5KXt5KNTYH/E0pp6lb05TsslC15lrhlWVKm8nsv0p5seTaOR4pgKP93R2sQR8xjDJIOySM7OHwerv/HNoXIdvmst7D/U46xznhPPCzXXvM+Rki2uP+Hjg7LtnHBXpSwE1kegWEYyv+H3f4HHUh8sY5kmVLGMp2i/wt/lLRLucU8qaH8X+TLt//1/T8R7b+kkRDLhenkFbH/uxW7/f396OruRnNTMyZOmojRY8Za+5A6grHtnLFLsPxkn4omcAkuvGZiUKT3k4nUDx8ley7MGE5MSnzW/sI1htp4yinoKupPFbACEE0RgbXgdSTJrIE6NPtyKF/mj2YCCUbQz3sfFieGfzkPPEcyor24vHZyl3ktbzFfTM+JYMbl7LSenUh5FYRLiO2ZeaRtE0JeG5ZTMeUp4uIwhoPyEmF8zIm6AHI08h8ndqU8Cb5vEMupNmNcZFA95ZOnzxhA6wyd7R1Yu2YNKgMDGDVqFBobGz2Nsi/C9pj4fJ3B9m2I9h+y3RIv08b13ZiedTQApG5Xi4r0rLXd8auj9h+ivpZylmC2YPsvF6rFdhY/s76WfEtaGcZ4mTeuw70c3YLVGJfEw3J5tWXlbSmp0/7zfZHyIK/5urKo/R9J/z+Wg9OJkKHETfzGuPdysQugqP3njj9Tp/0nF5IOAEiiVfAE5d//X932n7loMxtv//N2gzq2I8uRNFPHsRyk7cfxMg9tIPASdM6ygt0G++Q9aSkqDwX+z7Rbrv+/ae//sU1B8iyeOQnM7yOyn0VamY5ysW4Q5Fbs/xvp/7tjwZleyllCQv93k8/W95Ka9zzyGuORsmR4tVrF5GlTI/7g3kFs+0NfNwwQOI2PBRMDRvQOXR7FtCr/Hsx0Xi+i7iA+aR3GpfFxSmHFsuV+Apig/v/e/99i/h9sms/Sbmnnxk0AM31ReYjkyjR6i/p/aP/lwhvGEyROSYsMj8umfKhLhklaGcZ4mTfWoZSj14lYaCjxsFxeWZaEpE77zyv1TF5jPFKWDI9pZdxQ7b8uOPYXQrZMK+OJgzKSnxrB6/H9v1JBqVx77D8nxJSypxsSkmH6Pyd5JEi5UB+SPi+jkfq/07fWdsGS0ZH/u52/pEEp9v9Dn0rqxdOWKy/YCjbZ/4v6RMEfJI+b0v+XtMhwKT8+U1+Sb0krwxgv88Y6lHKMdcZ74mG5vLIsCckW9H/Od/FTCeETCRaffYcMthLTTmAYNur/oZ6hjBiP16P/b2L7b9838jJPRtD+b4nx/zhe5qENxHzLsqRMpV7ST33iExcXEUZDY5gkjAXJe4mDea0A3KqDJBify+jxkjiCx+WOwuHPG5ETvqSNTEkccHmYDsK4IAyVQPoDvaFTyjJ4JR88qgpeZhYXy0yS2u8lexlA1VR2pVJYWa7cC0tILwze66BW8cSlVHgRskbrjjeK6CF9SuXp8XQI+Xu+lR31knYi5cJw4snxkCR+9TdxI6r8jdCrEUZOkDL1ZUaVKFcTyjIIqo5d8xqXp5SbSHd2JumCkLdSyr9o8jlNS34BhJwIJg2SRvKcKzdqMCnnOD3DUCRzkdbSkq+UmZ60Sb0WyYkLM/K0A0rYROIqQCXqBImDeLmDOKZV4lbC/xOVIJHfdq7j/8wjVzxZ/mP/z9tpEb0sg/TacCdPtyCF8SyfafNlBTuDq9gJsf9LvdqbMEhNOhnP8iQuWY60G0T08FmpxNPDchDJUpaJyE4kfikLKUfGyXyMG4n/Mw0iWhiuohWvcV5Vx655jctjepYh6ULs/5E/1uvAEaekUZbBNJIWqcc4PXfwoEDmMq2kWcbxiuH4f3QvcTBvMkz/lzTF9MiflKEsM5YZcTAP0zEv8TCMIMuM6WUZvDJc4mM8CuxFlsW8KPL/chmltISWlhZUqhWsWrkSi195GT09PciqVWRZhv7+fvttUHcMabzTE0DNRC+fi9ISFJS1IfsgIyyYcK+UrYwkL3BhvqLyIDJC5eKJx6cjPoqLj5E9I5fEhtfER/VLMcS08VIQLulTnPxlHUdelE/CQVLbVjq7yAnGhat8jMvlHjhr6CJdOTksnqY8qYEQhotBWycfuPyUVVEYCuTPe3nNyztfJ4S8TG/ZAne5CrDPlkonUpfe5J6HxmGvgS+Gh3svCSkzClFZ/TpWhO7zeWxQoDWUI2wCQJZV0dXZiYGBfnS0t2Pp4lfw4sJF6O/rQ0O5jHHjxiFJknz77xZ9KKHvIpnyXtYxss1Qst0oqo+EnIbT/zcIn7eQ9WToF7367b9C7ad7ZF2rXtX2P7QPsi1lOaSDz/n2//XQ/6/f/lOmUj9FcqIdxbQrxz/flTa9/de+P8Of1uFIaVlmLDPiYB6mwzDafwgdSnpZBq8M54Cgvd8C7f9Q/f8Cm2GY5BGb3P8fnv8zDJGd5OUyXP8PefQI/J9pENHiw4v834DNMFQduwY4pmPzEpieZUi6MCL/r7WRQGOwL1mu5F3qMaaJYVmWoXVUG0LDBt8eMg8iezcuNa3ChynbkDGeyHivxDPTkNZEid1xifv0BGXMsljHELeDrs4ulNwR0PxJGUr+Y5lByGKk/s98wT4tvSyDV8/jlu7/v8b+T00S52vv/4EPOflrNtP/VZH/C1BD+f9G2//I/w2gxcSK1Jsakf/ny2Cakfo/CmQu05IWXpWyE8BMg0ivRXKK75lOve7e/zNfr8KNTQb/12CtphBO2Suil2XwyvDETbKpOrolXQxnHGHk/i/qKXeClZSFxMV8agj/95Dz/+C3yMlyJP4f+rlBjoEvmY959P9W/99i7f+W8X9D2Xj6ZdrgR7xKOkib1E+RnOx9oFviYN7kdeH/tfUa8TCMIMtM3DsMZcjFCyyLfEh8RbrdouP/BbJhmOQRI2n/lz37rJEZZAHxVSJLR/Th4dRPBBv3oeokqgQC8a48McFEPEyjo0qPhibLBKIVyOLI2xxegZthcpUHVH6wkmUxr6SdDY1SbiWO6zgzb7wCIeaD8gQA4xorWR6B8pPlxUC5VDN+oyJvPIHm/G5iiU86ZS4+UcgytwJpBCsQuHM2tg2mLyoPkdFrNwhAZ6HejZEr8Vwej80Cy5bOoYe5Aom6JpAW3hMoH/lM57N8O7uI9CDlIvNK25b0m01agRTkS5BykPoruhK0071SClk1q1kBx8rS3ucbglgexoRvP8mOB8vjlbzBfW/L7niplRHTIuoQ8JjnGC9gO34sU4lKPeZbCf93VFme3Io7KSveA+GlOPb/OK2qswIp5/9u55DfgRzR6JMV2I5MT1tQzo55pKGUA+0bsf/7PCPzf8o0tg2mLyoPBf7PtDX+X8deCZIOxuth+j9G4v/Rs9+BIO1R0Mowxsu8sQ6lHGOdGPrGq+3/I27/h/Z/KQfmIU5eyaeMZz4pI8Yj8v9YV5Jm4maYlLFMp6L2n2EsT8oq5kkNy//t6QaEJLXfVxwcGERvby96e3uRZRm0zjA4WLGng2h3Jn4M2h6xqbMqVJqGdPIKAImCyTIkacnuFtU6fHYi077vkySpjbeNq9tJaMOMO0YRKn+8EPmjjrS231yX/TLaABCO4ofjvUiuOT8tlSx/idsd7WiTA405cGUb7b5h58oslcq+f2i09gvJsAn+zxdp25RZHRvNz2+82v4/VPsv5BkK8LRvef8PL/Lkgbi00XYR12vk/zwFRuKTNBM3w6SMZTq1Cf7P3Imb3C2VSkjTFC0tzWhpbvFyZL6A28owSfInnkDoNVeeiEck9/wKZHf8u6S5sP8vZFbQ/ss8Wue/A0zcocy83Uo90QYQ+dpw2v/yv6z9t3zGNoXIdvlMfQW+g21JWTEeCO+l1CF5lHKs0cmQ/h/kLEHKQakEEPKLrwTt6l4M4f9xHV/U/stFwJ42P8Bp8xM3eaNc1Aj8n2VKfDU6EjxKGct0qq7/y/s8bTLdxtv/YfT/6/h/HoIdSNuR6UmbivryEp+0/The5rG2s6n9/+DnReVhCP8fqv+fb//zPkZ6iafc0OBPW/C27UDSJOUsaZHhUn58V6W+JN85WklbmriD921m0jtS/+cOYCsGaSPBHnknJwDjidz46vMa698KbseyiAPTexk4vbl0sf/m+mwifvXKVWhoaPB4yBvvmT+WEeMxAv+vVCoYGBjwp6UkKrETYlBoamry7YGq6/+1dirDGffa+b+zp2H4f+KOsI9tCXX8kfEyD/0p5luWJe1W6oW0mTrlYRP9fyiZkF7iGXn7H/l/NN4n01E+1CXDJK0MY7zMG+tQyjHWCe+Jh+XyyrIkkNbMfxM9byNF8qSMVJ32HwU6Lmr/SZOUA/MQJ6/kTcYzn5QR41Hj/9aH4n6FTy9sQspYplN1/J91l5RVzJOq4/+yz6w26v92/JPyk/liMMadQFrN/C5/mZ60KWfH+ROGLA5p+7Gt0QZMXf/Pl2Vlmj8Cmvekpag8vO78P9gl42RZcdmUD3XJMEkrwxgv80rblvSbOv7Pnb8Q80RaBznHsyJSDlJ/RVcCZaRy/p/nOdbxv97/67f/xM0wyli+E8CN9bMsgqRdysrfi3RF/p9Lu1H/t0D5yXwxxHJhOnkFALX0mWfyFjEMBcgwCouFSIgLVCo2v6AsIOzglMpiPMtxFHhhSeaUqJi0toN83lnE910kbq54DpBfBZdpDeVWTXi8Ln9YgZ53TsaD44BMLyqTJAnHB9tnUTGp2tVwBGPYTQ3Gb6KGX4bD0U4ai/IodwwB81OfxEVZeVknlnfGSdpScea6DE/SFBX37TEZxwaZ6Ygjlpd/FrbHcG8LaYJcReTvgr7jMsg3ZU/aYvxA2HHAtORf5klLxceXFT3bsGA75IMylLKMy5PhEj/pzodZeqlTmV+mj/MxLcOkTCAmm7TOfxfXYcnRHPPvUxGnr7DzlTXjpW/B2MFGHjst5SL9lM/GHX+RK4/2oE3OUlTBqpwYL+BWN8vvKLtGVtJOUNJ+HUgf5DPLQtQRkXI1xn1byd3Hvsw0Ui7SXkNceBlLkhTVasUP2ms2MJFdSZzEJfk0Q/h/Wtf/a31iKP9nelPk/1EHSoKkWZYxEv9nmJRnHE8bqZVNoJ1pmcZsMf/P+6DEr5TyR3/L/DJ9nI9pGSZlwjDKjrYhQZYdy4Mg81B/0ocYL32LcRtr//lsnF4Q6VXyJGE4/i9p472kMeaVOAjSb+1zoBkIi2wQySh3r92goavH/BGHQ/l/QZ4kSVCtVH1+LlggLsmffOa9TRjsP8vyi4IYviX8P9/+W5tX9JvXgf+X6P/usxxsW3KyErwSz5bx/7w/yzClFFLuGJf+L2Qc52NahkmZMKy+/+dpjvknyDxb0v/5DST9OvB/NSz/j9v/DGnqXha1nWBFJC+WaYz7Dm+d9p87G4yxC+Fk2UmSIK3b/3dpBH/Eidj/bcaczRLMFvR/pjcmHE+t/iXtf97uGE8biWUTnkN9wDAj/L+aZf5bqFva/ykfmT+kzx+bS7wSP9OqJJxqRdl5O/QcBpnLqwTiIPD9zQ7WBp4h/EPiHsr/pd+aIfy/9v1/U/zf0kAaGS+BOAjSB/ks7ZvlIZJRfB/7sg0P+mC5pLcoT1LX//M2JHEyv+TTbHL/P29jw/V/hqsC/89r1X2uwh39bIx9T1fKfg9dyl4pN27jEEh6WaaUZxxf4/8OT5GspCyT1C7or2ZV/93KTfX/SqWC8RMnIi2VcuvhQvlux180HNxfNXh0ZQVn/7UdL7bnBx1HCnMnlnDVMWOxy+QSmtKwwzgGWT7pGxgYwIZ169HQ0OBlLn2LabeE/xtjsGLFCjz2+GPo7u5xZVk6xowZg9133wNTp0zJ4ZX55f3rx//zvirtNc6TukVm/0r/J0eepi3g/zFImmUZm97+C38Un9Sq8X8HRc8MM6L9z17F/j/lI/Mbw/Hk2nxMyzDilmGUHW1DgjxaOeafIPNI+0PkYyyHQB6kTapC/89gtPGLeiQPlidXliCdfodhtv+yfyzjJRAHwctrpP4vcLBM6kb6bJIm7h00gRG7oIvyJIldZBrkvwnv/8L+rW2Jttj7/6DXEyHOz7SxvPjM9OZf5v/5+jSOfz34P60lhFk+OD6iFHL+H4OkVeKXMmEYZeft2abw6SRdzCdBlh/sr8DHNtn/N97+xyD9P4wjWH0U0cZ7SaOXn8NDWgjSB/k8LP+P7iUe6bNSLtJe4zzpeWeddXGcSQqAkLiKgoJmGJ+LDFUSlKZ2wpN5CfJ4XC80MdMut0QT4pfvuFzjXuz4DNhVWnxOxeoS4xRuBxIDPxJXXEaS2O3h9j4Mqkm+tbY7aaTwKQ+7c0byE9JxcpXlSeciHg4MyfyM4zOE8UoaidOni5yMTkUcBOYzQpYyDpFxEozIK+3F/vKNBOOlo0inkKvTKRNCoMnYRt3h9nKNdBDTKldmEHem7YCzEStIgg7DCgyvH6FvppPlS5mSf4ZLnZBHXhkuy5d2JemIyzDCXrSrDKkLiVfyMSz/d9+SVm7XV7H/B9z0OUkfnO/l7NGqGcmQ/u/4jY6Ik7LgjzhlZ1T6P4ytg6wrWF5iXHEZVk5hAtXT5Ab9E1GZax2OoJa2I4HpYj58/hr/TwG/dpu2ZOP4DGEjkkbitJMnzAfAHWso/V9qKuQL8pdxKPApguSDZfJHoHxkOYj8n+WqIv8XNDGNzM94yiKmtcj/pY+RJqlDiZNlxjIP5Qc5QeiCv1i28spwWb6kLdBhO7WyDCP8mSswqQuJV/IxLP/fhPZf8kMo9v+Ntf95H4nLNQX+L+Nz/u/b//q44nBvH7H/C74z5/e8Mh/q+n+t/Gx4Pf+H710qFU4c4TPq+b84Aki5T2wYYwBR5yYuXAJp4b2Un1Ju0JS7il27L+NfPf83AIp3Hsv8zCttUsKW9H8U+n+eXxkmeZY8Sj54jfHKtKRJlmFEe5G5Va01/h+9GPyf/9fqQIZTTryP8SdR+6+U7dPzBZx5CDJdXKaOXnJNgX6U67eQJzWk/+dfUpXTPxxdRf1/4/pPMh93dPEZLM/nCkD+pL34sh1QlkxLIA/E43X4L2//rc3I9KRdDen/QUfy53kusD2ml+VL2iQdTMc8Jtf+1+//a9efl+klcKGQcruEMYT/8/1VynpY/m+XHEK50wGyrIpSqVyjK8m3/ElZ8MfyZDxpIdbN9/98nqTA/0PaEfr/UO2/yM84PqOe/0d+LPNZmdf6P9PKfMzDZxT4FEHywTL5cym8fGQ5GML/KROCpIlpbH7RLnGRnFus5md5AfttSDGmY4zxee197P/123/SZ8uP/d+CD0vsL8t07lui8sr0snxpV5IO5fwPxqCxqRHGffuXMrZRAi8JMgbr+jQuuK0TT64Op9BsKqzt1VjRneGIrZvQ2mDbJwC+7iCw3ZKW093V7Wg1r0n7f+ttt2Hd+vWoVCr+NzA4iK7ubqxdtxZzd9opVwb1zfsYf/J//p8DyQfL9GW7NJSPLAdbxP/zcqUsYlpH3v4L/3cLakk76cNw/L9AJ8Ql+eA1xivTxnpj+MbafxPxHdsXXLlSfwzjc1H/n6cEEKfkh/Dq9f85CZcACrk5A+52tWBQSt1R8+KTkxJXXAblxHtVYJvUj9STtJ2Yn9hOeU9deXp0WBgu8zMfn+F2CiuFIcf/fXk5/w86lmXENirjUOBTBMkHy+SP4GX5v9H/N6f9L9AJcUk+eI3xyrRevgjzLsZY+4abDzJGe11IvJKPzff/vAyIU/JDePX8f/jt//D6/4lbTFfr/zH+5DUZ/8/nZxyfMcz2P2EgC6nHHBEyDk6xTCdxKCFk7SYNByuV8CzyWwZTlMrlHIHEWxVHIkpGWY7ERRqUGyBIhNFyh54xBllmB8KNpyEYjPyFHb61ZRo3cRSXb/FpqDQ/oy9xUAEyD9Nx0pZyYDoaVZLY3Q0yPxBWdBCqWeYHhUljXBZxsJzYCJmH6VSa+NVuDKdMmVfKIzZ06lVrWwkxfSa2uMtw7Y55QO7Y60APeZE2BVf5MT+dm3i97oXtkgbS4eOsg/gw0gcnb5+ff4J3GQ8hJ4nfTlbn5cy0LCcGSbcSfkb8sgx4XJa3JLHfeI31q0bq/26gP6aFeQNdQV6VIf3fHo9IWpgmGZb/2zg+S1r+v/bOJVmW2zjDCVQf3lBQEQqJC/DEXoK8AW+HnFheAGfempfADXAkU1cOyxIldhU8SHzAj2xUv073OfdKzIiOqgIS+UL+hXqg0PxS6v/fXKRvvN3WXozNfugdddalNmQgKaXOMhefWi7fgH/aEAf4kMfWUl1+awf/HM/8UD63py9/hm5tAx+x1HJi2nyVeJA/EP263YF/fFd78AW5SrR/Df6JBWW2h/+QL8ij3swvwrVe9+3p+N/a1/IPwX/wA1toq3bhx/PwL/g7g3/klYD/rU702Sqm46+44nas+0ud1FaqHOoYqxjLy1X4P71hUD76ka22t1fjP47/fayCFxs4ZktMaUu7UvoyoBD9ut2B//3x3+OBXoj29+Hfb5SSTNpAPrG6hP8j9fViHT7qdd/eEP+HN8G/n2fKO+GfF/D84MM+xb/aNPuhN+oss/Ff8pa4EzttR0y0jca4x6GPR8hjq+3tJvx3m5DB/YTq1jbwEUstJ6a01XiQPxBx3u7A/7Zt9Su5bg/XP8hVov19+O99rfrsBvxrvV2JfzxYnoL/c9f/jpMohxUhuOcjztEPbMnZJ0arXfgR8V+kjzL4z27L1mK33IV/tvzgw7d1XX28FhuQGX/ojTrLm+D/vcb/t8Z/72Mt3yL+p+P/Jfwfak5V/B8D/uvLm/V4nIz/D8B/xRB81Jfik+64lwZjztsfikZqdp/B/2FZ7OPHP9hff/xrjyX+ZFamq/FK/sA4pdPV+R5B+Lxu/hywFPlCSXKYvzT68ccf7X/++MeG3WfhX9uV4v/jyq8UX2oVnpnO8neC/+0d8L9u2/BxxdXj/134/3zGf0j7OJLanXbwD59dOf7nh1//d7vA/fnn/4+9/vftUn+53c9iH/dmZn7+5cWYrhDBD71RZ3kP/K++yuW2Pg7/ao/q1jbwEVstJ6a01XiQPxD9up2M/z/jX/uE3JmR2p2uxP9a8b/kXK+Hxv5NT8Q/fsTrf9rTr4/H//Xjv/oVf+jtE0puwz/vj7QdMdE2GmONA3xN3oPH/+V333zzrTIoIwHTuj3S+kGRyMIxP/bg+RIMyba1J8ZM7yadTnnigY/oNRKzlg1+8JXfIL+3j/Ib1Tf/lKfUl8BSXuSmlNpsTsrczipzAsCUkt8sSOxou7CsYp11TgLQTmW1E8fgZz+RwZ+zL/2serqdnZzPvx6JL7hog7380N9iIf3PvtqcK1BJWo2j1b6nrPmn8c6pfuVa2mDPwIEO9GEHsovMqIg2pvoFV+RvMuSrK8ogTg7IizHoNo0nYHTl+jBlqVvNN142wEt9rn231v906Pb0k1U8UXQ7eh5TFvvpHM1kun0hZkF280kGhpleeFPy2W0p1f+czNn8zm3khVRXknxr8iXfm/yJv2qP1/UZ5PBqH7KljL6BP8qDd9a249/rG/5dwOCbnhtmcUS+Xxyn4eFftNMkrxmYypX4Vz+Qq/tqV76Af20zxX+94FC9j8K/Dsjwq4woFzrFf7+A1XILfYVcjjVWuoUv2mAVS1z4dnsOVopfCGp5tEPLYj+do5lMtS/GDNnIvwn/tTw1/He98EIzP+Kx8qp8JeWPejjWPmTbys7i32MT84O2u/gP/R/rZn7Cn+XiWPuix7P3BXJpu4v/nNq6BOpHqeNYqmMVY5ramXO24+pLR2fq0+ns9BH/XQdL/KPvfvyPGH8c/sdzoLYlBpTrMVt0s4Uv2mBn8b8z/kvOtLIJbs7RKHP0RX2PspH/947/aGeUB++s7TX4T/V4hn/qmu6KX+TxNW2000xydoJ/vpjDXr74aHokFupbjD+23DL+l/qiFL63Hf/7jPEoF3oN/vXeTWOlW/RHG2wX//vX/3outtRXU+LlWKurcZ+R1quP7Gvc1S/kb5s/gLXik2ZO9P6M/1Y/wz/HuprazE/488Xx30l10nZ3/JfYqB/I1X21C1vW9TjcjyBL24zjf+d7Ff7rF1WjjUubXBb5VUaUC03xXyewlNKXpO7PpOAf+0RjpVv0RxuoP7y82B9++MH/2zhlX065Tjjvdtb29eglJ/vn3xzsv77/yT7+2ON8D/3Lbw72n//2K/unXy22VB+T1XvWMv5HuKVkf/7zX+zjx4/2w+//27788svmi8Zdbcd3+CIvFGOoseX417/+tf3pT/9rpZh98eEL++KLL+zDhw/21Vdf2b/+9rf2yy9/OfBHPRxrPrLVfoS0z5AH76ztbfg/Hf85Vt05Z38G8Mb412d58Lktt43/2Abfq/B/8/h/J/5D/8YYUK7HGivdwhdtsLvH/xFbUbe2mVGUqTYiS1fXQzbyt/e6/uc8I3FVWZC2j3o41j5kq/0IUa/y4J21dfwfLS99TNK2KmuG/yQ2wp/D+K+rQCnB8xj87/dH/mzwP8qIcqH3xD/P/3PqYztfvfs11ilW2dey2E/naCaTaxn1PcpG/rvhX+yO8s36/Y6/p+x64Vde7UO23KNGO7Wt+qJtkfe88T9b+v677woKU50hoQ1zmI2gHYdBtFnrJ9vH8PYZ2ZCeQHhYxIUwcgGeTV/+juCg3bqu7Q+9+WJE9SVZ/tDMrNQLYOotJg871XReFvOfufiV6zEd5f+R5Hb1E4gAGbma7PWLPo03MYWHr39LPcGtdcaKxrbFpZ5sCy/LpL71jSQEvjQb68l2OfhXTlbjiL8qD53Uw2/hokR16ENCttAmFzDkkhL6zMyK1bjUE1ups85yvcBVHdoemWzxQ+vxRfuBerP+n1Ueq7Ev1GZkp+Qn5KXOyul29DZLfRAOqe0aq+hTOvMn47nmQiKetY36g8yr8F9nymXB/yL4ZyB3G8YB1E7wX30KJ6eO//Eiw+CrX/Rbk+Evt8C/Ypp9XcYQSqkvs2hm1j4pnhD6c87+n7k7+M+S2w0zob8gjbX6Tt2If68rin+NS8RGiBtlxNkv+rutvdz5tnohQdm1+Fc/tQ9Ux2wLKf7JJaXoI3FCVuvvkGPavsXsAv5Vvuq0gB/6LMqlXr+80n5UvlRjy3mdMvRprKJPqeH/xSz0fW/nM8MgtR++q/B/Yfwf8d9lQ/QPddE/dNJG5UQ+lXEJ/yngv4D/nfE/EvrzhfFf7Yp5bxWnUPwyXONNTJFHXbli/Gdf40bZLObRRl8ZwXFIGb4gH3lqW6rjIaR9oDpmWwi96Ur8M/Ygi/7UflCbVB9b98PjHuPh1xevwP9WzN4M/6fjv/M6j8pmSWLlOx6Pw/K6mo+FrxOrbF7qH+v4f1xXezm8vDv+1yvxjyzl1ZhGQn9+Bf7HTL5i/Oe/uS7gH7nIYL8UX8kGKvz3Y4z5Cf79mlbxz0tg5FfGwe5UyyDtgyEOky10Df41d/PD8N99V1uRr3G1+pcZHJ/F/5C/Yz82/bXNM67/tZ3iP2cmMve/A1iP/pUJsjUfzfwlP7JzGP+PV47/3J9RF/3L8h9eFnwhTuhXGeB/O4P/9Sn49y+Vr8F/JHhNcnnA/13j/2nctH4W82hj4f7/1vE/+Kl9oDpmW66M0JvO4F/7izghq9//a37IdZ/EhC9vuadt9XVyrMqPOaLHF/Ff/x7IzJ8beI66HoiX3/pFtMZTY6Xl1EX8b9tm//eXv9i6rvbT3/z/FzX/c32eVfxJWK2v96/1KVVO2TaJHfe2xfpfMNFm3VY7LAdbt7X+v7DgX0a+tWy2pGxb1Vus2MvhxV5eXuwXv/iFLWfwb6/EP/0EpZTsbz/9zY4/HR1b8nQup2wfPnywRV4u2BT/14//keA1yWVs1LzTunIR/+P4H+vVFn1WoeXlCfjnowW1QbcQetOd+Ke/tR/UJtXHFj+0nnbaD9QbvtVna/RZlKuyKdN+VL701Ot/31fZrW9KsVSfv2u+waOYoY64aJv1wviPp/QPddE/dKZX4X+1XJc+Zj/t4H/bVlvyYmZ9dcMZoT8H/C+vwL/ea6nvtof/+vXi4eXF1vp1JHY1GXXVifacdvKR20nMBxu93evw32PV2445HLfQp43/Lktt+BTw/9PxaC86/ldeH8O9j/XaQu1H5vnr/3vw77apn2+D/+vHf+XVmI5oHfvvlvE/3lsrwWuSy9hITOGhrjxw/E/ff/ddwdAYYA2M1c+KCSR8GlwuLlWxKle5ZuYn6FrdDIoDVkiEKqluu0MEh+2yLH0ZPoLcmvmOzkbrsjsQ24vn+uKYAaWI75B2vn4tW0qvS6nfQKMHGb5QRk8I6rj43LiBkJhHORo7y8lK+L8XTawiJ3R+1DcZZlbCMojsK1HetlK21j8zVz5umGmjiU4ubRsROc1H5PSHEdiNX33QUF+a3DqLhzKoyGyLFHKPLTGz5F/VwEtf6X8O4VPLS+lXtoeDn7BUBrY0XaIfX0xmGSnhr/vpsTkcDoMsXoSq7His8YbW4xz/PAjedvHf449ckwGoNmo88HW7YBFf626pA1tuGO34XwP+Y+a2uhorMz8zpIp/9WOMRc3zHfyz3BjtW53INYkftthZ/HesYku3ObW840Wz6vc+GPHvx2ubpaW20NZlj7nHvpLqi7xz/PcBtJzBPwSf+o3N+AifKUajLw3/fZBUf0rAf5QTZUdex3/vpxH/Mad9q9hEBrbM9OML+vXY5L/o8LPUiwWXVbkmvsVjjTd0afzfdvHvpHIt4F/7CL5o1+irE3w9zvv4H9op/nfGf/UjxkL9tYj/ajPtNU9a/jYZrhf9mt+aD8hUWzRmWk97tR8Z6Igy1R9vO+LPbsG/XHe8Ff6Jp92N/9O+GuWMMbOb8Z/NBOdsH4v/MVbExnX0vsvh2mY4lhuNZnela/DPy0XtI0htsyfif70C/7SlTuuRp37EWFAGXYt/feCjMijT/N7W1ZbDwayU9vJVbWltJE4aO/TzAnjbtta/HNNGJ8fRVq/bqpF9v1Ka4D9J3J6Ff72p1nja3fh3+yKmVc4o2786uAX/7n+XsW6bvQj+yVtsmenHF7sZ/6MsjovklNZrvKHjurYHqSqHPrv2/h8+ld36SF68RbtK0dczvV26YfzX9lqncUSe+hFjQVk9uhr/aovKoKznSc8pu3n8H/UTP3Thh7ZRW2gL0V5lKVGu9ezfjv/TB/Xwqd/YjI/wGX4Oudz92i7h/3Cw9Xhs/5VOvcpm/1r8r/UeucWk8mzrZoeXl3Yf5hNueIDbl8lU/dovl/DP86t9/PcYxHqNN3TN+G8X8L+9wfhPX8zwH9tSp/XIUz9iLNRfu2H8V1tizOxh+O94ZB8Z6Ogy+5eZ1NMWor3KUlJ9kRf8l6vxf934r75qHOzNxn/Bf332tIf/aDc825te/8/w34/XyTNT7IYegX97I/wf2vP/bZhkPbaVupBv9Jfaofaqv+kV+OcZImUxT6b4X+tLOvn7AJ45srIE21L6C+AYd5U5Xv+Psdb4s69EudYXmXDcc9r15c8a/93HyPsp4X8d8O/vGLgPdF0j3puuOhlU4w3dh/8RM8i1J+OfvimvHP/7Oxv3XXnwwy7g/3AG/xozuxb/Dxz/l999/fW32kCdakGownMFKER5vPE71D9uRjGkjiEnCVBYzrSUfqMXg+5bTzhs5m04AMyTWdR5ybYe6wMVkcU+thFwQ3cy8xs89wm7YsCbT6n+x0opw+yH5kdI5lRP2trZlGsymfWL5ywg1P4qJHTT78exjZnfCC9hmRATeyyZrau/yE6SYPhR6skSHbQtNW5bPQHFeNJPMT9UrlX7OKaMY2Let/0/57jZm8XSzNpLfPoFGVlyXf1RXuqcv+eayz09mbHNuS95ucdP/+AvOiH24cUOiHhTBv+y9JftlGGLykR3zydOVtZfLi4V/1UtObFt/uUH+u/BPy+R1QdrcRrtxRceNjv+fQYOsteIf2Yo1bxQ29CbZvivFAfbbfOHDLxwHTAm+MNWvlhBr/YTMZnlLDGmTcQy/wdCfc51EkQdvLI8gFCfzcyWww7+kb312UvYQUzKDv7tQfiHYj7QLm47/p13FksTPfiJjHwz/vt5VeXaDv51f8afH4L/rX18Bf+If6+jncpE93bH+E8bbL8H/9F/SPUhj9jAPxv/9/Df8iLEFttivkIz/KsNEZf4AY/6Sz1fXaTX4H8y/rPPcWwDLXvjf0pmMqkE+9SPcg7/9X+K4IG0D4iN1pnkJoQfepxaf3Gs4/89+O+4jrnZeccbOY2ryjXxgS1tGFOtfgWo/PQPPvR+cGIf3i7Tabs4/kvOBB5uckopvmRkJY0JMVS7KScHS/H/GnxP/K9X4l9tQ056Y/xznPbwvyy21RvHdAb/nln7+GfJ55T82oTrt/P479d92Kd+FLA9wf9S7W48lbQPiI3WmcQFwg89TsnvhdJnO/5XvFf+rdQvmp+K/y6vtUs+oRh9+A9pTCwly/U/9aAZ/ssjxn95Tav6UupfAPND3zXj//Fzw//d47/r5ji2gS7jv/vIPn6Uc+P/Hdf/vmpajZvVxy5n8B+35/FfV+sqrNolOVQflPPVCw/XrV6bKS9xjHG1HfzrPT9lqX5p1j9+SO1FBP7woHyIj+RAfgj+x2N0az6hQ/te/aScNuif4b/IdYbGLc3wL36pPuThC/zX4v+zG//vxn/XjwxtAy3Lob0UgLDH3hj/KlcJP/Q43Yz/J47/8h/fEDawpY3yRX76Bx/QCbEPr8q0u/DfeYbr/yfhn/pU3xdojJ+B/+N6tP7c0O1ej8fw/L/LY3JjzFfoHP634hM08cEkFvCov9RznK7G/2bbKnpKxX81q4DFIl//tuv/07F+2R3/3db78e/9AA+Us0wI+Wzx331WXs0VbGCLbOWL/PQpPqATYh9elWm1r7Zy+reEh8n9P+3acX2pjf9e+Cj8dx8oizF+Bv4fNf5jCe//IMUGMcIHk1jw/Fz9pZ7jdDX+T/W0/pLcYJ/j2AZalsVfAKsjMGqHqAObzKBo5TvBNOl0rc+5//8sZTpjk/IY0C57vJCgjvpS/D9GVO+6ru2/hVq56FT/cvYXdtvmL0A3WR4ovsgb7Ks6fTbOeKIpxV/IIEfjS1pFX9Uf9CnF2I4+9BuKmVy1BUopDTMd9ESdwwnHeT0XZmW0gfBD4xK3KfUXyBoTzYPmU30xrRRlcawnHOPrTTlJc0ycu45TMJXis4Sj3Gif8lPe5J7Y5nEG7MjlxIgNUY7qYzBHLmW6jF/sD30piRz3v8/Ecntze3HOgz3q2dIT6iN6tJuGNqG/4n7v9zTMak/Jl6pYDku70EmyvIjaB62rv2RW29r2BDvjwKd5zjb2u+rcNv8Sinrssh38QypL2yE7kvpighs94StPYUDinBaWu8F2dC2LP+BND8V/iP1Ov0PIUT6Nj1KUxfGI/y7DLuCfNlpX5KL2cfg/zbd8F/57nCjb6oWF29Pjpf6pTPzXOHBsO+M/OpFFG/TEetpQvrevspHD9tL4H+0ilmqPbtW/WX+UW/Ef/MGuob30Y5QV26FPSX2xyTmM9ufkKmE7cpb6UJT4RFvP4l+WSLWn4b+xtTq2Ku9Twv+29Uk1KqM8BP9dLmWOf795if2htjefqxyNA8d2Ff77clPoGev/sfHPDbrGF4q+Rn8iDb5cjX9/8djsEcJ25MTr/za7SHi5H9Ky2VLR6NO4xC372g45yqfxUYqyOH48/l9z/d8fHFhdDpll1Z+H//n1f5aHIepzmuK/n/OmfFWutkEP+03XOfzXL4BtB/88rP608D/G7hz+tT3lUPQ1+hNJfbGr8T/KVcJ25ET8R1s1LrGMNhD6sEW3JeRAzlfc/1+Bfy4Qmk/FzOqkfOxG1vC3RtVX7Md2YnBp/N/qsx6NGdfmrg9/UluetJQiXwK/Hv/bRfyPOYwcYs2W+MC7h39I27ieMUe1DeV7+yobOWw/LfzX8+lnh/++yp6Ru0/Af7mAf7bsq6/IUT71QynK4lh9oh67kaVx5rjZfw7/MqFEZSs/5TPb9/ItvxL/lO3jvx+rTPzXOHBsD8C/1Y8h1Na9fZWNHLbX4T8bL6DWo/+Hrtqj22XxCTm8YC034D+9Gf4ljpPY5uxj3Bz/Y+6pLRC2uy7PH9oQk8i7V0YbCH3YO9uyr+2Qo3zqh1KUxfFj8d9fLqvcaF/nP8XtzLbyYPxvfHm6bXbYvf9fzOTvH9R/jQPH2Dvjg7QNemI9bSjf21fZyGF7Hf673nvG/7ZSy7a1DwvLBP+Uo/N5+B9JfbG7xv9iy3988823W32LnORtvCY3BmAsAFAF0ZEkidyUyUC0resQqFxvguFNtVPWCV+Ri3jtCGzQfXhS8hn1JA516EK+xRNGuFDWjtB2KfUbDh6iaUyUnx9+pTCjQ+Xu6bNJAjTaAZRJnNPOCTrnpT3AgS9JXsCLvcQWfo7hM0lsyrjBV/sLoKD/pL7IyRF5DOZDX4pOcho7sdXL+sCmcjmJ0pat2pmSL8ERJxiggwc88JLzxJKLsiyzVGZfJeeQExp75aNusC/MyKFc/bA6SCwV6/Ccx7/PNnsI/usSk+pDj2HEf1+uAr42c5s+TdU+scvE9lQvPE/wX2c/tfhF/EvssQlKyb8AZl9txD4lHvxrfJCJXzNZkJZbyEulwZ+I/7p0TEr+RTd3gMS9xZfz6w3412P4sAFSm6P9GmetLzP8V/3al7o9j//u413457wd/OKnvP0ixdvM8d/95hdzQmOvfNT5fs8rtQnZem6iPt+Ef5f19vg/5UOnxm709RT/yFuWviQZsjQut+CfdrqPPo2J8vDbts1ynWyj8Y2yYnsI2yPt2WUhfiqbWIzx7Xl+M/7rMtDYoHo4jvZrnLW+7OLfX25W5tbGbsJ/H1uei38vPzwV/90+tcknvXWfIWIy4L/+5+y20992Ef/V/k8c/9QhS+PylvhHpsY3yortIWw3Gx8N7dllxE/0QqX4y+kYX9rv4V8f5rVYq8xqg+rhWPftRvwzme99xn9/URP94jfYGfCv4z+rVMWJmGmSExp75aNutC/iv2NCbd62rf3fLjyz8T++zJrhP04EwA6NP7Fged0ZrvuEzjn+eTmHbs2Z6KsF/E+v/yWe0G34H/sOfrVh5O+/R+JfKcnfNsU26EEvRCy0XmOzh398hZ9j+KzaoHq0PqU+eUDjPNRP8I/+PfzrMuOlbO0rXyv+fKY941D81xWRttW/eN/H//nxX+8JO/43S3WlEvKL/+M7vf93uzUnNPadb8w3ZGybv9jDHsrVD2TlOP5P8A8fsmb4p45y7KAdL6RV5xT/P4//J7JiewjbI+3ZZSf4r/0osYjxpf1r8K8zNdXmaL/GWevLHfgnp+HDNi1LEf9Xj/8B/7LiW+Q9N/6/3fV/x0SzWfpx3fp/ST4L/+Xd8O82NHn1vzq9rp+XXX7PHeSiE7lajp9J9uGPMRn4NT6Tvo6yhvZyTBwiaXvfH33R+DYa8O/xhi+9Ev9qo9oc7dc4a335pPDvuYvPEDpG3vfBf1yRtwgmus2e+zn7am2t7cPx3/1/H/z3nETefeP/KWa0ne6jr9TYR35++JVvwX/IOT2G9uyyCf6Xf//6629RosHAQIRA7NOBfMWi7Qi6dpRu0cUM5KXOVICHRDExWOVhBzybzHLCbsDMcUr961L0I0cTOkmH4Bs/wKs2NNkB/NisMo/1T7Ijb/wSiLqTba1XvU1GILUR2RpLCzFQPsqIwcoydCJTSdtim/qOv14mg47oTvXEVeRlqdqDPHzQ2b3O6231U33NI7VjNsP8XL6qv6XmrfoI3yYXUqoz5z6rmLq15oIfjwMRepQfO5SHcngh+tf3T3GJ7dyoaj6onlP8+2whE/w3udIOPT2O4wUFutDLQ3F4TvHfLyRpn1J/wXot/nW5QuQn8F/b6gUZ9vDr+De37Rz+68tpbMh18Jnhn/ZQj9u4hdQn96tVDTxskb3Ul7958aXtiR9y1AZsTg/H/2lbflvFv/oN0ZY8gGL8NXf28d/zXvdVr27VZvyY43/EC3WeT2M/jvjvfqge5ccO5aEcXogcZ592M9uVX/2d+aP7W8C/tkNPjKP6A4/VflJZp/h/0Ph/Dv8SY++vc/jvNsT8i/6pzFP8y4Sn1+B/QmojsjWWdtX47+U341+WqaJO4xHb8rsd//LVTPEXWPfh/3y+dpt7Dt2O/zrxhhnpb47/3vdn8Q9/9pfAFvpb7T2Hf11tI27Rhd5/XPyf+kJbL9u830JuqN4mo9V2HrbI7rHsNsKTgw3YnJLn6qBL8zTowDb1HX815yB4aKexUXto2/Kqlsf434f/W8f/vev/C/gX3eu62suhL8HJ/a/qUX7sUB7K4YXIcfZphy1n8R/6w0J/s38J/+fiWS7hv2IE26I87IDnWvzzIts+G/yPW0j1arnSTLbG0kIMog3YnO4Z/+/APy9cnbee90rHOW3xAYrxJw/KOfzX819eli5fJsY6T883tRk/ZvhvL51rjlPn+dTz08xsXY92OLy0ZxE6EQ09yo8dykM5vFDO/Qvq2A/ddscHPPZE/OvzHNrDYzP8/zz+tzLdQqpXy5VmsjWW1mLgY3+0AZvTG+GfdhobtYe2+ADF+L/N+C/4l/v6iBdkkE+q++2v/7st2j9mZkudCKD+zvzR/e0G/McturDz+fj3/C2lv3OgbaqTctlPObVJ2bTh9wz8p+ALbSnTba31Ffz4z9+QD1C3MbcPYzSWFmKwf/3/SPyf2gsP7TQ2ag/y8AGK8X9z/AtfxAt1+Y3xv0zGf/rXbV/H8b+uYqD+psREuLG/1d7PB/+PGP9d5q34Z2zNO/iPvtCWMt1CqlfLlWayNZZW9fw/bEA8t3w9w50AAAAASUVORK5CYII=</t>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAB4AAAAQ4CAYAAADo08FDAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAP+6SURBVHhe7N19XM73/sDxl1RKkkrlrqQQQm5CwmSTYbk9G9aZdrYYu3HzczLOHGacHNs6DnNszNrObMewDVOTsU0mCZm5iaJaakIhlZQkvz+uq7qu73VVV6ko7+fj8X3Q9/P53l7fz/fu/f18Po1atWp1HyGEEEIIIYQQQgghhBBCCCGEEPWekXKEEEIIIYQQQgghhBBCCCGEEEKI+kkCwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRoICQALIYQQQgghhBBCCCGEEEIIIUQDIQFgIYQQQgghhBBCCCGEEEIIIYRoICQALIQQQgghhBBCCCGEEEIIIYQQDYQEgIUQQgghhBBCCCGEEEIIIYQQooFo1KpVq/vKkUIIIYQQonY1b94cKysrmjZtiqmpqTJZCCGEEEIIoVZYWMjt27fJzs4mJydHmSyEEEIIIRQkACyEEEIIUYfMzc1p3bo1xsbG3Lp1i8LCQgoLCykuLlZmFUIIIYQQ4rFnZGSEqakppqamNGvWjKKiIi5fvkx+fr4yqxBCCCGEUJMAsBBCCCFEHWnevDlOTk7cvHmTmzdvKpOFEEIIIYQQlWjRogUtWrQgNTVVagMLIYQQQpRD+gAWQgghhKgD5ubmtG/fnsuXL0vwVwghhBBCiGq6efMmly9fpn379pibmyuThRBCCCGEBICFEEIIIepG69atuXnzJnfu3FEmCSGEEEIIIargzp073Lx5k9atWyuThBBCCCGEBICFEEIIIWpf8+bNMTExISsrS5kkhBBCCCGEqIasrCxMTExo3ry5MkkIIYQQ4rH30ALAjT3HUjjjY4yfnkkjy5bKZCGEEEKIBsPKyors7GzlaCGEEEIIIcQDyMnJwcrKSjlaCCGEEOKx16hVq1b3lSNrnesArgyeAQV36DzcF4C8fZsojvyS+xnJytxCCCGEEPWam5sb165dk+afhRANQp8+ffDy8sLe3h5TU1Pu379PQUEBFy9eZN++fVy+fFk5iRBCCFErzMzMsLW1JSEhQZlUs1q64jPYhy4OJuoRWST/vJe9F1Qt/Fh3GsGIJ12wVqfevRpPZFQkSddK5yCEEKW6d+/OwIEDady4sTKpSu7du8fx48f59ddflUnV9ris2+HDhzlz5owySYgGpc4DwMXdniTD+2W4dw/u3KGzzzCt9PzjP1K0bTn3s9K1xgshhBBC1Fc9evTg4sWLFBcXK5OEEKLeaNasGc8++yydOnWioKCApKQkbt26BYC9vT3t2rXDyMiIw4cPExERoZxcCCGEqHFGRka0b9+e06dPK5NqhoU3M//xKn6dSkK72rKOhrKdiQT2Lyf9Qjgf/X090XnKFCHE42ro0KG88sorNdZ6QW5uLuvXr+fAgQPKpCp7lNetf//+vPHGG9jY2CiTqiU3N5e1a9cSHR2tTBKiwajTAPDdXmO53vc51R/3iuFOAZ19nlRm4/7RcHJD/085WgghhBCiXurRowe///67crQQQtQbzZo148UXX8TBwYEjR44QERGh81GLtbU1zz33HE5OThw9epRdu3ZppQshhBC1oUOHDrUUAPYkKHQpPg5lYwoLClX/MTLF1LRsvCqxkEL1pdHUTCPxaiRLA0OILRsjhKgj3t7ezJo1C0tLS2WS3uCkvvz379/n2LFjvP/+++Tn55eOr67FixczYMAA5WgtR44cYfny5crROvr06cOCBQs4c+aMQfkrs3jxYrp378677777wDV3H/a6VZS/ptdNiEdV3fQBbGTEHa8/c733s1B8XzXcVw3qf7QG+vkp5/BI+Otf/8qOHTuYNm1a6bjFixezdetW+vTpo5W3IejTpw9bt25l7dq1peP07YOGZNq0aezYsYNx48Ypk2pVz549+eKLL9iwYQNOTk7K5AatcePGrFy5km+++YZnnnlGmSyEqA+6eOLZUjnyEWRqhuZ7GCGEEIYbNmwY9vb27N+/n++//14n+AuQlZXFJ598wvnz5+nTpw8eHh7KLFUTsJItW0JZMESZYJgXVm5hy5YtbNmykheUiXXshZVb2LJxAYOUCUIIIR5ZFi9MwdsBoJC0Hz/g1cl+THx2omqYGMRezR4PLu8laKI67dmJ+E1+lQ9+TKMQwMGbKS9YaGQWQtSFrl278tprr3Ht2jXCw8N1hmvXrjF9+nS6du1aYf7IyEg8PDx49dVXlYsQQohH2oMHgBtX8ia1sQl5g6eT1fVp7fGlEV/0D3Vs7dq1OheBkmHx4sUANGnSRDnZI23atGk621IyfPrpp9UKND5q+6Bx48ZMmTKFjRs3snPnztLt27VrF2+++aYy+yPLzMyMRo0aKUfXOw4ODmzcuJFt27YxePBgZXIpV1dXPv/8cz7//HPc3d0fuN+GR91TTz3FmjVr+Pbbb0uP0R07dvDxxx8zceLER3b79Z1Ddu3axf/+9z9mzpz5yK63qGMt/Vi6aClLQ5YyorUy8RFi6siAEeMYN2IAjpXcugghhNDWpk0b3N3dSU1NrbT5tuLiYiIjI7lz5w59+/ZVJteZF1Zuwc/2BGunTGHKlIV8qcwghBBCVMKvlwumAJcjWbF6L2lazTjHc0pjRF7aKeI1k/PS2Lt6BZGXAUxx6fVoVnYRoiEzNzfHxMSEjIwM1q9frzNkZGRgYmKCubl5hfn3799PUVERFhbyIYcQNcHIyIiAgIByY3IffPABf/3rX+nXr59y0nohPDxcOapCVc1fFdUOAN9vZETBE9O4Mj+Coi66zTgDYGpO9lNzye3gXVbzV6MGsHl6nG7g9yEFgAEKCwvZv3+/zgEXExMDwIoVK5gwYQKffPKJctJH2qlTp3S26ccffyQrK0uZtVL69kGnTp1YvXo1Cxcu1Mpb2xo3bsxbb73Fn//8ZywtLUlISGDfvn2cO3eOzMxMjI2NlZM8dPb29ixfvpz33ntPa/zRo0d54YUXmDFjBqmpqVpp9cnVq1dJSEjA3NycXr16KZNL9erVCysrK1JTUzl16hTz58/n2Wef5fvvv1dmrddatGjBihUrmDNnDo6Ojly5coVffvmFEydOkJWVRatWrfDz86Nt27bKSR8pJeeQH374gcTERJo0acIzzzxT52VePIJa+rH03zPxtM4j/sct2l/AP2oKr3ItKx+au+ItQWAhhKiSDh06YGpqSnx8vN6av0qpqalcunSJli1bYm9vr0yuAy/Q3RnyzkdxSJlUAwbND5XavEII0eA54mClemjISztFmjLZIGmlQWJTKwcclclCCCHEY6i4uJhNmzYxa9Ys/Pz8dIbZs2dz4MABnnnmmXr54YWfn5/BQd3w8HD8/GrvI7FqB4Bvj1nEzYHPw324Nm4Rt4dM164NbNacG0+/RX4rd902nu/fx+b4VqwO/kc5uqwZ6Ifg7t277N+/X+droH379imz1ivJyck627R582Zyc3OVWavF0tKS1q1bY2JiokyqVU8++SS9evUiMTGRmTNnsmDBAtasWcP8+fMJDAxkxYoVykkeOjMzM9q2bVv6ZVlDdOTIEQoKCujSpYve/jUAevfuTXFxMVFRUcqkBqNFixa8/fbbdO/enRMnTvDqq6/y+uuv895777F48WJefvllgoOD60WfoCXnkLVr1zJv3jwWLFjAtWvX6NGjR4WBftHAWYwoC/5ueZugL7W+d38EFZJ0aA+xF2+pgsCjvHGVILAQQhjEysoKgMzMTGVSua5du4aZmRktWrRQJgkhhBD1gCPNzJTjNFng2rLspbRFS1cqfEVt1kwCwEIIIR5r5ubmTJo0CX9//3KHSZMmYW5uTmxsLI0bN37wboUeEkOCwLUd/OVBAsD3i+5qRWxzBk4m67l3ud+sJcXm1mSMWEShZSsoLtaJ7trtWYHp2R/UM9IT/X1YEWBRr7Rv354mTZoQFxfHzZs3lcniIfntt9+4evUqDg4OeoOD3bt3p0OHDly/fp3ffvtNmdxgPPfcc3To0IFjx46xbNkyrl69qszCkSNHWL58eb2r9Z2UlERycjJNmjShffv2ymTxOLAYwdL1s+tR8LeERhDYwhlPCQILIYQQQggh9IrmqrrhPJPmDspE6BKIt4vG3y7eBHbR+FvNobm6skTWVaKViUIIIcRjZNasWaUfF5fHysqKWbNmAXD58uUaq8T4MFQUBK6L4C8PEgC2iHgPy+PhUEzpcKddDzL/8gmZk1ZRfN8ICm5D0d3SILBZZhIOX8+mccb5shkpm35+iE1AV2batGns2LGDcePGKZN0TJ48mc8//5xdu3axa9cuPv/8cyZPnqzM9kgo6UdXc30//vhjXFw072RVlPtg7dq1LFu2DAsLCwYMGEC4um9TQ/bRg8rKyqKoqAhnZ2eD+iLt3bs3//73v0v7Ct62bRsLFiwwqFaCodM6ODiwcOFCtm7dSlhYGGFhYXz11VeMGzeOxYsX8+GHH2Jvb0+HDh1Km+OeNm0aTk5OfPrpp6xdu1ZrfiW/zX//+1++++670v3773//m969e2vlXbx4MVu3bmXIkCH8/e9/Z/v27aXrGhgYaNA+qgm5ubnEx8djZmbGgAEDlMn07dsXS0tLTp06VRoULVn3Pn36aOWtqBzZ29uzYcMGNm3aROfOnUunady4cWl/u76+vlrj165dq5O/Njg4ONC/f3+ys7P55ptvuHfvnjJLuarymz9MRkZGFBUVcePGDQDGjRvHjh07mDZtmjKrzu/bp08ftm7dyuLFixkxYgSfffYZu3bt4rvvvmPt2rV06aLnqVk8Oupt8LeEBIGFEKKq7t69C0CTJk2USeUyMzPj3r17pdNW7gVWbtnCltJhJS8os6gNmh+qkW8LofPLGmNWpfnhDFj0naWTzpAFhGouR29TzoNYsFFzXbawZeULpdPO6msBlr2ZtWULW7aEsmCIcnpDlbMcPXS3+QXVtHryv7BSe54rA1T7Vms/YMC+GLKA0C2hLBhStp5CCPE4iU1TvbMw7TKRNQsnM6K3Bx69RzB5bjCh/xiBA0BhHnmFAA6M+EcowXM18i1cw8QuqoeNq2mxWvPWq8sEJg+vsB4xANajpzJBHpuFqHEnT57k1KlT9OvXr/S9bXh4OMuWLaO4uJiffvpJOYkQogqsra2JiYlh8+bN5Q4xMTFYW1uDxnNofaYvCFxXwV8eJADc6H4xFj+tpsXBT7Vq7hY3seB+y3bQpoNq3J18KLpLi5M7aLHnHzQq0I7YKyv+NoQKwDNnzsTf35+ioiL27dtX2oS0v78/AQEByuwP3fTp03n++ecxMjIiMjKSH374gTt37uDv74+ZWYXt3bB//372799PYWEhv//+O+Hh4ezevZuEhARl1hr3008/8fvvv+Ph4cHq1at1goeavL29efPNN2nXrh0xMTGEh4dz6dIlBg0axFtvvVVhcNTQaV1dXVmxYgXe3t5kZGSwZ88e9uzZw7Vr17CysiImJoYffviB3NxcMjMzS28iyqsF27hxYxYuXIi/vz+NGzfmwIEDhIeHk5iYSIcOHXjzzTfx9vbWmWbq1Kk4Ojry008/ERkZyf379xkzZgzjx4/XyluboqKiyM3NpVOnTlr9vjVu3Jju3btTUFDAiRMntKZRqqwcZWRkkJycjKWlJV27di2drmvXrrRs2ZImTZpoBRK7du2KjY0NqampnD+v8RFKLejcuTMtWrQgLS2Nc+fOKZPLVZ3f/GHw9vamS5cuXL16tdzj1xCOjo68/PLLXLhwgd27d5OSkoKzszNvvPFGuc2H16WSsq9vn7do0YLp06czffp0nQ9BUE+7aNEinnjiCWVS/Vbvg78ltIPAA0YPkSCwEEJU4MqVK6C+3zVE06ZNcXR05NatW3pbQdExZAGhW/ywO76WKVOmqIbd4DfaWZmTF1ZuYVbfTMJL8q07AX1nlQY3D70fyJQp4aQAeer5Bb6v7gk4YCVbXu9N5m71tFPWcoLezNIKfL7Ayi2z6M0J1pYsQz0/Dr5L4JQprD2eB7kl6YG8e7B0YsMNWUDolln0vh5ets1Twklx9tMJxOps85S1nO/sR2+d2yVVoNbPVnvdGa0KiGsxaF+odA54GTap8gkhxOPEwaKZ+n8WuA6eyuzlwQQvn83U4R44mAHkEb/9bd7eHk8egJkDHsM18g0uaxa6mYWeWsQKXTwHMXHWepZWEAS2Hr2UD2aMwLOLNCgtRE27d+8eK1euZNOmTVoB4O+++47g4GCio6Uev6hdmsedoYN49GkGgcPrMPjLgwSAS5gd2Yz19+/p1uC1sAKnztDEnJY/vY/Z6TDlpCrK6R5iDWALCwuWLVumVYD01UqsiJeXFz4+PqSkpPDXv/6VtWvXltaSvXHjBoMGDdIKiNWF8ePH65wYSmrplazvtWvXWLp0KatWrWLdunXMnTuXI0eOYGRU8SGyfft29u/fz927d8nIyGD9+vVs3LiR+PjaDwrcvHmTlStXEhcXR/v27Xn77bcJCQnR+b0sLS157rnnaNSoEf/+979ZuXIl69evJygoiNjYWFxdXXnyySe1pilh6LSNGzdmxowZtGzZkt27dzNr1izWrVvHunXrmDVrFps2bWLfvn1899135Ofnc+vWrdL+mGNj9X8F6ufnh6enJ0lJScyaNYtVq1axfv165s+fz+eff06TJk2YMGGCVvDazMyMvLw8FixYwLp16wgJCWH79u2g/q3ryunTp7l06RJ2dnZatVZ79+6Nk5MTly9f5vDhw1rTaDK0HJUcZ506dSqdtnfv3piYmJCTk0PHjh1L90+3bt1o2rRpnXycYGNjg7GxsWEvPDVU5zevCy4uLsycOZNZs2bxwQcfMH/+fG7fvk1oaOgDNcPRsmVLtm7dyooVK1i/fj1vv/02aWlptG7duk6PV31cXV2ZMWMGTzzxBK+99prWRwYAL7/8MmPHjmXs2LG8/PLLWmldu3bltddeY+DAgcyYMYPu3btrpddbFiN4a11DCP6WKAsC32vqKEFgIYSoQFxcHFevXsXd3V1vK0FKgwcPxtbWlnPnznH79m1lso4XnumNRUp4WaAWYNNCVaBV05AFDHOGlN0L+bJk3MF3+fR4HhZ9x5RbY1hlEAuGOENKOAs3lYw7xLubTpBn2Zsx6u90X1jph3PuCdZOf5eytfmShQtLl1gjSrZ5itZ8v2ThOu31UW1zHifWaWwzh3h3ujoorSlgDL0tUwhXrvu6E6rARCnD9oWKBZz/tHpBbiGEqLe6MPW9rcz2VAViC/Oy1LV81e4VknUxmi/eepmgL+OJ/zKIl9/6guiLWRRqNgBWmEeWekILz9lsfW8qFVXcjf8yiLe/vkrXcoLAquCvK0kbZrNoZ5oyWQhRA+7du8c333xT+t625F33mTNnlFmFqHF+fn5VHkT94KcOAtf1b1ZxdM9AjW7dgBtXdKvxGhlD6w7cN22qnKSMMvD7EAPAhYWF7N+/XytQumfPHi5duqTMWq5+/fphZmbGoUOHtPqlTUpKIiUlhRYtWtCuXTutaWrbqVOndALAJbX2PDw8aNq0Kb/88gtJSUml09y7d4/9+/eTn5+vMadHz9WrV1m4cCHBwcGkpKTQuXNnlixZwpw5c0qDZL169aJdu3YkJiZqfal17949Tp06hZGRUbn9mBo6be/evWnfvj3nz59n48aNWvOorn79+nH//n327Nmj08fxrl27SEtLw9HRkR49epSOv3v3LgcOHNDKHxcXR15eHmZmZnUWOCzZP8bGxlr9AHt5eWFmZsavv/5aYbPIhpajM2fOkJOTg4uLS2mNUTc3N65du8b58+dp2bJlaeDOzc2N/Px8Tp8+XTq/2lZYqPmEqLJ27VqtsqjZZHp1fvO60LNnT/z8/Hj66adp3749hw8f5o033qi0FndlLl26xK5du0r/vnnzJsnJyRgZGWFhofuwKx4u77lT8W4JYEGXKSE61xVDh61LfJSzfmDOQ5/F39+/GsOzDGjfjMYATR3pOUC+ohdCCH2Ki4s5dOgQRkZGjBs3DicnJ2WWUgMHDsTLy4urV68aWEviBbo7Q8pZ3QDroauZWn8P8uqMRe4JwkqDliqqfHa0ragp5iGD6WyZx4nvFcs5eIlMwM5hUOm65J2P0gigGihgpXZTzvqaXC5V/jZzMIrzueDcTRXOHuTVGQsyuaQTgP2dLMV3eC90c4bcLH7XHl26jaUM2hdlMq9WeW8IIUS95jl/PpO7lT2T3o0LZfJEjRfu4yYy9fUVbD1V9nlN3qmtrHh9KhPHaeSbOJnQuLLmKy26TWb+fM/Sv/UpLwhsMbws+Lt0t7pzYiGEEELUC+Hq4G94HdfafuAAcEHXkdzwehluZEDGH1p9ApcM15/7F/l99fd/q4wZP8wmoO/evcv+/fu1vvD57LPPqlSLr0WLFhgbGxMQEKDz0rtfv36Ympri6Fi3L5iTk5O1tkmz1qm9vT137twhOTlZORlFRUXcf1g/RhUdOXKEOXPm8N5773H9+nWGDx/OvHnzQKM2Zq9evXR+k2nTpmFiYkLr1q2Vs4QqTNu2bVtMTU1JTU2tMLBZFVZWVty6dYvff9d5hcO9e/e4du0aTZo0oW3btqXjCwsLSU1N1cqbk5PDnTt3sLCw0Mpb244cOcLNmzfp2LEjDg4OWFpa0qVLF27dusXx48eV2bUYWo6SkpJIS0vD1tYWNzc3OnfujJOTE+fOnePs2bOYm5vTrVs37O3tadeuHZmZmXUSAC4qKgKgVatWyiStj0yUv211fvO6sHPnTvz8/HjrrbdIT0/H29ubZ599VpmtyjIyMnTKy82bNzExMaFly5Za4+taUlISGzZs4JdffuHDDz/Uacr7008/Le2b+tNPP9VKO3fuHB9++CGHDx9mw4YNDeYr0ZNHklC9Zsgj6UA44WHVHKLLPjaqKfk518i6kVW9ISsf1VF4j4Jb2cpZCyGEUGjZsiUvvvgiY8aM0eoGwd7enqlTp/LMM8+Qk5PDjh07uHXrlta0eg1pi51yXDk62Gr2vasx6GkqWkcHayywoPfrimnV/QVD2bpUK+C5aaFGU86qQatGs6aqbrO+oK6OQbS1Ba5fqjx4bci+KJVHVuULF0KIBsQHv94VN9dsMXAyM2dMxlvzu2ULbybPmMnkgRV/zOzQ24/KPomN/zKItzel4qoOAlsMX8r6Wa4krZ0pwV8halnjxo159tlnmTlzZukwffp0nRYnhRDCUOEaNX/rOghc/QCwUWPy+j7PzZ4TVTV9jZtAzg0apZ6jUVGhTkQ3e9DLZP3p39xvouioSBn5fZgR4BpSWFhY2nencqir/nGr4v79+9y5c0c5ul6KiopixYoVXLt2jV69emk1vRoXF6fze5QMMTExWvNRMnRafTU+H1fnz5/n4sWLtGzZEi8vL3r16oWDgwPJyckGBcQMLUcJCQk0adKErl270rVrV0xNTYmPj+fs2bPk5+fj5uaGs7Mz1tbWJCYm6gQca8PFixe5ffs27dq1w8FB+8Fx+/btpR9iZGRkaKU96k6dOsVHH31EXl4eI0eOpGfPnsosDUp0dDTvvfee3tpLN2/eZOPGjWzcuFGntjbqaYODg/nll1+USfVW3o9Lmbk6liwscPXsSN6B9azfUPXhix9rvqmyqyciidgTUfXh5/Pkm5nTmHtkJ0bz04kc5ayFEEIA3bt3Z9y4cRQUFPDll1+SmZnJgAEDePPNN/nHP/7BsmXLmDt3Lq6ursTGxvLRRx+Rnp6unI1+ytqpFfj9umbfu8qhkr54f88ijzxOrFNOpxGsrcK6PJC6Wk55DNkXQgjx2HLFurlynCYPXp02Fb8xU3l1rnfpWO+5rzJ1jB9Tp72Kh1Z+hebWuCrH6RH/7SKCN6XiOmsrW0uCvz8qukYQQtSoxo0b89Zbb/Hiiy9qNbE7btw45s+fz9ChQ5WTCCFqUXFxMVeuXFGOrlfC9TT7XJdB4GoHgHP7v0iuq09ZsLaxMaY5l7CLWELLz1/G6Ha2TrPOd9p04+or31Bkr9HjhbLp54fYBHRNyM/Px8jIiIsXL+rUui3pM6Au+sc1VH5+Pqampjg7637rbWFhUWkfwI+iklqhxsbGmJqacvv2bYqLi7l7967O71Ey7Nu3TzkbAIOnLcnXsWNH5SyqLTs7m2bNmtGhQwdlEo0bN6Zly5bcvn2bixcvKpMfGSU1zXv27MmAAQMwMTEpbX68IlUpRydOnCAvLw83Nzd69uxJdnY2J0+e5MyZM6Snp9OuXTt69OjB/fv3DVp2TThz5gzJycnY29szYcIEZXK56sNvfurUKSIjI2nWrBnjx4/XaVZc2cd5yXqLhqE0CGzRhcnvhDC1og6sHnWmrvg8M4A25vfIOh/JvqNpyCc8Qgihq02bNowaNQojIyMiIiI4d+4c69evJyQkhIiICI4ePcrRo0fZsmUL//znP9m5c2cVPy5VNWVc0uSxphe6aT+jHLqaCZadGVxRU8/lOXiJTCzo7FVes8xUuC41q4LlDBlMZ8uy5qG/PJuif5vV+cocIup8Hjh31+0LOaC7ds1eg/aFEEII/axpZq76n2lj09Kxpf83b4Z16dgHE//tIoI37OCLlRL8FaIueHh40L17d44ePaoVAF6yZAlGRkY88cQTykkaJAsLC5YtW6ZTIaeqw7Jly6SLN/FA9uzZQ2bmQ/109oGE6wn+lqirIHD1o3vF97Rq7Fqe34f1wf9gVJBN41sZtPxyOiaZv0PxfZ3h2nOrye8xFhpgBeDTp09TXFzMoEGDtJpEe1RduHCB+/fv66yvubk5I0eOxNxcfVdrABsbG+WoWuXv788rr7yis46urq44OjpSUFBAdnY2p06d4saNG3Ts2BFv77KvMw1h6LTHjh3j6tWruLq6GhTwa9q0aaXN+J44cQIjIyNGjhypcyyNHTsWR0dHLl26pNM07aMkJiaGa9eu0bFjR7p3705mZiZRUVHKbDqqUo7OnTvHtWvXcHR0xMXFheTk5NKatefPn6dFixb06tWLmzdv1mnt+6+//ppbt27x9NNPM336dJ1AqT715Tf/+uuvuXTpEr169WL06NEA3Lhxg6KiItq1a6e17oMHD6ZNmzYaU4v6Lu/Hpcz+UB0E/scaAutjEFgR/P0p9qoEf4UQQo9mzZoxYcIEzM3N+fHHH7Vacbl58yYHDx5k165dhIeHc+rUqSoGfksc4t2DKeDsp91nbsBK/JTfqG4K40SuBb1fX6kd5ByygJXl9rdb4kvCjudh0XcWKwM0xw9iwcoFqKY+xLubTpDn7MeWlZpLeIGVGn8/UCAaKl7O672xSAlnYUk/x3q3eRALAnqjfJ126P39pOCM38aS7UE1T50msg3ZF0IIIR4F8btD2XpYgr9CCCEeP5cuXVKOqjcqCv6WqIsgcLUDwJbHvqD52e/h/n1sYj7B4uS3NCq+W5puVJCN9bf/R5OLv+pGd+/fJ3vQDLKGL9St+VvPawD/+OOPnDhxAhcXF9auXcu8efOYOXMm8+bN46OPPuKtt95STlLrXFxctPotKOm7oEuXLvz8888kJyfj6urKv/71L2bNmsWsWbNYu3YtdnZ2FBQUKGen49q1a+Tl5dG+fXvefPNNFi5cyMiRI5XZalzTpk0ZO3Ysn3/+OatWrWLOnDm8++67rFixAhsbGw4fPkxSUhJXr15l9+7dmJqaEhQUxDvvvMPMmTN5/fXXef/991m3bh1OTk7K2QMYPO3Nmzf58ssvuXPnDi+++CLvv/8+M2fOZNasWaxbt46AANWblUuXLpGbm0vLli2ZPn06b775JpMmTVIuFtT9rh4/fpyOHTtqHUvvv/8+L774IllZWWzYsKFOmjSurqtXr5KYmIiNjQ02NjYkJiYa1Kd2VcrRvXv3OHPmDDY2NrRo0UKrhn3J/x0dHfnjjz/qtMnlU6dOsWbNGnJzcxk3bhz/+9//CAkJYdasWSxfvpxPP/2Ufv36gUafwfXlN7958yYREREAjBkzBgcHB3777TdSU1NxdHTk3Xff5fXXX2fhwoXMnDmTnBxpVrehydqtDgKbuTKhvgWBJfgrhBAGMTIyYuLEidjb27N//34OHz6szFJzNi1kyu4ULPrOKuuPttsZpuxOUWQ8xLvTpxCe4oyfZt+1r1tzxoBmiw+9H8iU3Sk4j9bs93YW1mffLes39+C7BE4JJ8XZT6tvXNQ1ckEzKLuFLVtCWVCdQHA5y7E7vpYpCzWWxSHenb6WE7ma2/wybFrLiVyNbAB8ycIp4aRo9ZPcnTNTwtHZk4bsCyGEeCzt5dSFip4QIjmXUggUknb+WOnYY+dVLQoVppwjUiu/tsILp9irHCmEEEI8Bg4cOMA777yjU1tcc3jnnXc4cOCActJ6xZDgb4naDgJXOwDM/WKaxoXhsGM2pmmqZl6VjO7m0yLibZqe+0k3wHv/Pnfa9tYzvn4HgO/du0dISAi7d+/G2NiYYcOG4efnx6BBgygsLDSo9mNN69mzp1azFX5+fowePRo3Nzdyc3NZvnw5Bw8exNLSkqeffpphw4aRkZHB5s2bDQo0paamsn37dgoKCnjiiSfo3bt3Nb/+r5qwsDB++OEH8vPzcXV1xdfXl86dO5OZmcm6detYv359ad4dO3awfv16MjMz6dWrF35+fvj6+mJnZ8exY8cq/JrE0Gmjo6NZvXo1v//+Ox07dsTPz4+nnnoKExMTfv/9d1AfH//73/+4ceMGffv2ZeDAgTRq1EixRJV79+6xYsUKduzYAYCPjw9+fn60b9+e2NhYli5dSlJSknKyR050dDQFBQXcuXNHb1+q+lS1HMXHx1NQUEBWVhYnTpwoHZ+QkMDNmze5f/8+p06d0pqmLhw9epT58+ezb98+ioqK6NSpE08//TQ9e/akadOmnDp1iuXLl/P9999DPfvNd+/ezdmzZ2ndujWTJk0iNzeX1atXc+7cORwcHBg1ahQ9e/Zk165dpKQoXzmKhqBeBoE1g7/xPxEhwV8hhNDLyMiIMWPG0LFjR44fP87BgxV1rltDNi3U7ot24Zfqcbp9+365UNlv7UI0Q6aqQGg5fdkqlzNlSllt21Kq6cvPowpEq9J010+fLxdOYcp0ZXBVdzl611lredrLzLuues4oo5xn2b7JvKqYd2X74uC7BBq4fUII0XCkEfr39URfKxtj0XMqS1/wLG3aeetbE/Hzm0jQlrKauXlbgpjo58fEt7aqx1jj+cJSpvbUaK/hWjTr/x5KWtkYIYQQ4rGxZ88eJk6cqBOr0hwmTpzInj17lJPWK34GBn9LVDV/VTRq1apVrYdb7zcy4taAl8jr9aeykcX3oCAPZ/femllLFSxwU44SQgghxCOmy5+CWfSSB9YF8XwxK4itl5U5HhHK4O+vGm906kCPHj1KPwYSQohH3dixY+nfvz/nz5/nyy+/pLi4WJlFPGxDFhD6em8ydyuD03oErGTLaDtOrJNgrhCiYerQoQOnT59Wjn5AXZiwfBGBvTV69L2XRdrxQ+w9sI/IA0lkaWYHwBrXoT74Dh3BoL6OWGv0BJV1IpTgxTsoa7NMCFHbunbtyt/+9jeys7OJi4tTJuPu7o61tTXBwcGcO3eu3PwWFhZ4e3tz6NAhVq1apTWP6li8eDEDBgxQjtZy5MgRli9frhyto0+fPixYsIAzZ84YlL8yhqxbVRm6LZVZvHgx3bt359133+XXX39VJuuoKH9N7zchHlXVrwFcBY3uF2MZE4rl4U+hmLLh/n31vyV/q/4titmmnIUQQgghHkHx3y4ieEs0ez8NfnSDvwCFSZy5eI1rDyH4W8KQvsCFEOJhGzJkCH379iU5OZnt27dL8Pehe4GVWn36qscp+wpGHRTW6lNYPW60M3nHP5XgrxCiQaq9e+x4diyeytT3d3DyD3VN38bWOPb3I3D+Gr4IDyf8m+1sLx3CCQ//gjXzA/HrXxb8zfvjJDven8pUCf4KUefOnTvH+vXrsbGx0all6Ofnh42NDR9++CHnzp2rML+Pjw+//fYba9asUS5CCCEeaXVSA1hTfucRZA+dDfeK4E4ezt37aqUXxkVyL/wfNLr5h9Z4IYQQQoj6ys3NjRs3bpCfn69MEkKIR8qAAQPo0qUL3377Lbdu3VImizo3iAUbZ9HbUnts3vG1epqLfoGVW/xwVoxNMaSWsBBC1FPm5ubY2NiQkJCgTKpR1p4TmDpuBP3cHbE2VaYqFGaRFneMvd99wY5Y3XrCQojHW//+/XnjjTewsbFRJlVLbm4ua9euNbjrvYo8yus2dOhQXnnlFaysrJRJ1ZKbm8v69evrfX+zQlSkzgPAAAWO/bk5bD7cuUX7ngNV445t5/6hTzHKTFRmF0IIIYSo1xwdHbl//z43b95UJgkhhBBCCCGqydpa1URzWlrd9axr0c6Dfp6edHEw0Rp/92o8sbHHymoMCyFEObp3787AgQMfuBWDe/fucfjwYc6cOaNMqrbHZd2OHz+u0zS0EA3NQwkAA9zvMYaCdr1pcvsGjY79j0a35Ys4IYQQQjRMzZs3p127dqSlpXH//kO59RJCCCGEEKJBadSoEY6Ojvzxxx/k5OQok4UQQgghHmsPLQAshBBCCPE4cXFx4e7du2RlyUdvQgghhBBCPCgbGxuMjY1JTk5WJgkhhBBCPPaMlCOEEEIIIUTNu3z5Mi1atKBJkybKJCGEEEIIIUQVNGnSBCsrKy5fvqxMEkIIIYQQEgAWQgghhKgb+fn5XLx4kdatW9OiRQtlshBCCCGEEMIALVq0oHXr1ly8eJH8/HxlshBCCCGEkCaghRBCCCHqlrm5Oa1bt8bY2Jhbt25RWFhIYWEhxcXFyqxCCCGEEEI89oyMjDA1NcXU1JRmzZpRVFTE5cuXJfgrhBBCCFEBCQALIYQQQjwEzZs3x8rKiqZNm2JqaqpMFkIIIYQQQqgVFhZy+/ZtsrOzycnJUSYLIYQQQggFCQALIYQQQgghhBBCCCGEEEIIIUQDIX0ACyGEEEIIIYQQQgghhBBCCCFEAyEBYCGEEEIIIYQQQgghhBBCCCGEaCAkACyEEEIIIYQQQgghhBBCCCGEEA2EBICFEEIIIYQQQgghhBBCCCGEEKKBkACwEEIIIYQQQgghhBBCCCGEEEI0EBIAFkIIIYQQQgghhBBCCCGEEEKIBkICwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRqIRu7u7veVI4UQQgghhBBCCCGEEEIIIYQQQtQ/jVh4pjQA3Oq/w7VTH3O2trZcv35dOVoI0cBJ2RcNiRzPQtQdKW9CNFy2trbEjdmqHC3EY8s9bLJc84SoZXJvKUTFpIwIIUTFJABcAbmICPF4krIvGhI5noWoO1LehGi4bG1tuXXrlnK0EI+tZs2ayTVPiFom95ZCVEzKiBBCVEz6ABZCCCGEEEIIIYQQQgghhBBCiAZCAsBCCCGEEEIIIYQQQgghhBBCCNFASABYCCGEEEIIIYQQQgghhBBCCCEaCAkACyGEEEIIIYQQQgghhBBCCCFEAyEBYCGEEEIIIYQQQgghhBBCCCGEaCAkACyEEEIIIYQQQgghhBBCCCGEEA2EBICFEEIIIYQQQgghhBBCCCGEEKKBkACwEEIIIYQQQgghhBBCCCGEEEI0EBIAFkIIIYQQQgghhBBCCCGEEEKIBkICwEIIIYQQQgghhBBCCCGEEEII0UBIAFgIIYQQQgghhBBCCCGEEEIIIRoICQALIYQQQgghhBBCCCGEEEIIIUQDIQFgIYQQQgghhBBCCCGEEEIIIYRoIBqx8Mz9kj9a/Xe4dupjztbWluvXrytHCyEaOCn7oiGR41mIuiPlTYiGy9bWllu3bilHC/HYatasmVzzhKhlcm8pRMWkjAjxgLr4ETi0HSbK8VWRHc/WLZFkKcc/qEd53eoRCQBXQC4iQjyepOyLhkSOZyHqjpQ3IRquOg0AG1lh6jqAZtZNS0fdyzpNblISxcVaOYV4aCQALETtk3tLISr2SJQRi0b07GuGp+t9oj8rIF6ZLsSjqksga1ZMwNVUmVB1WbHrmb00vOYCrY/yutUzEgCuwCNxERFC1Dkp+6IhkeNZiLoj5U2IhqtOAsBWA7Ad9RyOHawwMoLiwtvcKwKMTDAxM4HiuxSkHSEtbDO52XeVUwtRp+okAGzaDZsRo2hWeJLMXw6QX6Bx3Jt2w8pnODamKaTv3cWdQs0JhWgYav/e0gQT12dp7dmC27/t5kbCRcq+MzLBxHUc9p5tuBv7DRlJ6VpTCvEoqP0yolAS7O1tQddOzXB0MMPCrJEq7fJlXnvlJmnKaYTAh6CNs/GxSCN8w1LWH3g0QpE+S7YS1P8KO/zmEKpMVKupPFVlyDxrKk9D93D6AG42mr9/9QP79++v8vDDV39ndDPlDIUQQgghhBBCiPrIBBOPv9L9tWm07wA5Rzdz5l+v8dv7czj97zmc/tdr/Pr+34jfc5q7DoPp9FoIjh6tlTMRooExwWZyIM0ufMP1693oMHct3UZ4YoQJJu6v0m3m8zS7Hk36xU64vRLwYM0DCvG4cpxGpyfucvXAbxj1D6Jv0F+xbmECpt1oOXUlbp4m5ByIxmj4Ejr0kFImHnfGBH3QheD5zkwYbkeX9uZlwV/g6oVbEvwV5XDFsbUpNHfFb34ooUsm42GhzCNE7XgIAWB3Xv33HJ5qVb3626atnmLORgkCCyEaPseexri0VI4VJTyeX0zw8iBGOSpTxKOoNo9np7FBBAcHMabax4Il7mNnsHh5MMHBwQT0VaaLGmfkgf/iYILnjcJJmSYeXMvG9OzZiNp5pvQiMDiY4EAvZYLhHLwICHqH4OBggoPG0EaZLmqAE2OClL+T6rcLGlu7pc5u+OsEL19MQF8zZZIoR+O+f6WbXxcaZ0YR/68gkn/aT6FmTUeAwmvcPvERF/69hKQLYOe3GOe+tXRhFXVu3CfHSEk5xea/KFOqwpHpixcxTDlar2EsWjydat861YlumOccJjXhInnHP+DseyFcc5xGz3mr6NEnkwv/Wcyl47HcOf0JV+56YGujnP7RYjcwgKB3VPeaQX5y5asKee6rRa3h1s/fcOfKYTK+mMWJ7+/iOHMVveYG0iRqMWe2fkXulViu/HwBq+5DlVM/WizdGTNzser+cnkAnsr0h6m2n31qe/5CrTEW5d7e3iEttkg5ssY9TudD5XWzxp8xHkK5yTsbSexlcOg/leCNa5g51FqZRYgaV+cB4CHLljGpoymk7mbe/HkGDru5qDEPCQILIRqCl9d0JSysK2H/a0nJo5RFTwve/qgjYWFd+TC4E2s+60rYzs58OMdYMfXjzgyT6n1HJGpJfT6e7UYE4j/AibuJUUT8GMvlfGWO2uMVqHqg0RqWv8PC2f54OShzNyBmJjxaR0E9M6wlW8JUZW7NtJKRjRj6ams27exK2GedCQ7uosqzxYFJ2lM/XEYe+M8cg5tFBrE/RhAV/3CavzK282DUi3NZ+Lai/L29GP/eytyiKsyNzZWjREVs/ek4whUu7+Xcp59zu6QZW6MeOLy2kT6LNtLlqR5l+Ysvk/3N34g/cRubEX/FzrYsqSpUAccU7SExgVM/fcYinZ6hFvF9oiJv6XCMzyYq8wN48+4PCaSkpHDqiwBloloQ2+OU8ytZj828+xd35QQqEz/jWMmyn1MmanCezuZf1fP84d2y8aXT6xkSv2eR5jzqSPc2dlCURtx/lSmGG/nBZhYFTmfN7mWVBIGHsWz3GqYHLmLzByOViY+Qphgba7TrXHyRO7dNMDKCoqwL3C1tpzabokJTGlf3qyfHMQQp78XU14OFswMY06/Ng9+z9PTnDT83LDNj2bc7ioS6vPSVt33BwQQHB/IAn3PVEXnuq01GZk25p9G3fFHmTYqNgOJs8jNvlyUU3Aazsn7pq6q8Z57Fi4J4/VkfXB44BmKH70v+eLW9S8LBCPaduEzdPdKpP7oLGlN+EKm2n31qe/6icgV5nNqvHFnTHqPzoZ7rZo0/YzyMcnMrlqXTp7IiLIk8C6kNLOpGnQeATRurz1SFtzgRe8LA4RYlt/2XEy9Q+JgEgX2WbCU8PFx3+CAQCGRNeDjhm5fio5wQH5ZuDic8fA2B5c5nK0uf1JjkyaVsDQ/XeImon755bV2iZw305AvXM//AD3TzaM1TvV7KdNU+EKKBsbBg6dtOeLZTN61UqP56sDHkXa39LwnrlwJiP1/OosUhREgbO4+menM8t8Grpx1kxbD58wii9u9g31llngdljefkuSz8c3nfoWdycncEEbsjiDh4koTLuZjbuTPmjQep1Vw11v0mMXehf919KX87lk3LF7FoVQSpyjRRLZ7z2xM0ugXWjQHuU1h4X5WQV0i8Iu9D1dsDd1NI3rOOHfujiAiPosZ7lOvoy+vz5pbzZbwxLiNfZ/HcSQzuaE1RZgJxR/apyt75BNJzjTGuixcrFa5j/Za6J4RFi5ez6XiBMknosKLFqMFYFKdycdvXFGq8hKf1AGzVL8Sbdh2Adl2H29ze8zlXclvSZtQz1Xqo93a0AxLZ6uyMs7Mzzs7PsODL49xpP4zp721murNG5r+442gMOQeXqPNqDv14abtGXjXHeUGMd2sCQHP78gK57jhaKOf7DC/9YyPRRd2ZvPR7jn2hp5ZqP0fsALCj78TpylS1YbwbGoS3ulZoZlp0WZJ6+sSvlNvijHPHZwguy1lHAnBvBVxJ40HeHe+ZvYRNZ3No3i2ggiCwKvgb0K05OWc3sWT2HmWGR0g2d5u3RfW61wQTr7/han2Ac59+QobTq3TqrzoKoBtm1oXcy9OauMoKkqNU92K79xFzJoGEzHxMbN3wGv867yz0x/MBAlSevd0xLk4m4sMdRB6KIOxQjV/5Kr2XK9s+zSGKJGXGR44899Wm4lwLmrZVP6+ZeuIU0I+879cQty8Pp1dexbzkAtPSDpMCjYBwtSieeRJTyb1rSZvevgQGvcPrI12qH4xp7YWHA2Qd28ymPVFEbt9HnDLPA3PB97Ug5o4sN8xbvuo++xh6v1jd+YsqMsGmuXKcSuHFPJKetmDmAmte7qVMrSnlnA8NPU7qEX3XzRp/xnho5SaP6A1zmLwgVLs28ECJAovaUZ1nxYfq1olXmPf14xMEhiR2+PnhpznMDgVCmbMqlrzmnryqCMD6LHkVz+Z5xK7S7Nxaez4hR8FzniIIXCFVwDmoyzlCtNZnB1f6B5UTiFas+84kXMfrBoHJiVXM04/JyyK1siTt1F5mkssECQKLhmdSC7qYAtwjLew8Y/50gTFjzvHamovsCFNmFuIRV2+OZzssLYGszFq86bektaMdlmblvdLIJfVQFFGHoojas41NH4bw9iexZBlZ4/Vkea/xapZlayfsLM2r/9JFPGQm+PZQfxGdc40PpsTzpz/FM+alC3zweQ6nlNkfImtbGyCLjJp/913G1ok2tsZ6j2ensXMJHNKGoov7WLf8bUI+3MTmXZGqsvf5JtateptNR5RT1YIK1lE8RqyfwaG9CYVx33PzliLt8hGuq2sJ3j5/BJ1XXcWnST8QD+0HlwaKDTcdx9bAjQyNF+RxbF3qT0hUJth4M35qWW7Hno40B9LObyobWaHpvPuXPjTJ+5VfUwA7R/TWAVYHYrXnG8f+/4Yw8+lnCD6cg92QID77p7dGOkx3tgfSSEuB5u7D0BcCHvb+Isa7NiEtJVPVLOPZ70rTVNNnknZMa5KHx7kvjjaQk3YcjTB1Nexnyeg5ZUHgHcrmoIexaEdZ8HfO6CUPFHCuXU0xcfPAwmEg7vPW0uvvoXiOtON2rjNtnhmHRe5NLEb/iwEL19Nn4V9xNMumyKj6tRMB8jPjVPdihyIJ+2oTmz4MYfk7y9nwYypFlu5MmDEJt2q9QbPG2grIziBd8yOPGlbZvVzZ9mkOCWQqM4rHh5kHNi5WtBixll7z1jPgrdnYF93EqKc/Tj0tyC/ypNeSUPq8uR7PMR25k3sTo2qVgRKKZ57PQ1n93tu8vXobJ7OMaTMkkBlDLZUTGcbOEksg62rtPdGBPU5trevmQ8EScr/4iCnr71fJ1M2R4DeceKZnY5J+U6bWsgZ3nNTNdfOhi9+hXRt40ReELplAF2U+IR7QA126H5a4Dx+3IHA5fl7KR0fzsOg/gbJQaCAT+luQd/Qjlv6slVtL5LKPiM2xwHO8IUFUH5ZunoBr8g78/JeiHZoNZY5fCLF4ElRZQPaTOexIBteeleSrVChzdiaBS0+N7RaiAWis+f+yvhvTfrxD9AN+0S5Enas3x7M55o/ik9LF46rmAe1al9+UmBCljDDVKHOmJa1jXSti3y/3yhIeAeV/CFEHHMcwaYA1RclhrP44knSNlkWFeCg6umJBNtdO/KpMgeLTXP1wOr8GTyd+72llqkrcr9wsaknzrlbKlIoN6Ytjc+BKHMqQ7tbMbADsXSeXjpvcQR1w1X4QLNfkT17BuzmkRa7l+G3Axh59dYCDujhWMN80Nv5tK3F5Tej4zBsaQV5v+jo2h5w09idmQvPuDFM8FDrO2Mya5zpC0lZ+vW0HpHFhlWL6vDTi9NRcfiietsMKyEjZqEypBlUQeOOJHJr3nq4RBFYFf6f3bk7OiY2PdPDXqEMg3d5chVsvuJ6Qya3YZfyelEn6/+YR/8Uykr5YRtIXCzmz5yJ3L37D6dib3E06C08tp+cbf8XGXl2bsSYUF5C6fwP/OZAJlh6MGlFS67gqLDGry4CREJUxaoP15LV4vjYO85ST3Lx1gQubosm9FMFvHyxWl7FlJPznAy7l3CT902+4XpzOtcsedJr9L9xGDK3RQFNR5km2rdpGXCG0eXICHtV5U21e/scPQtSdeyTvv84B5WhRRY/TdVNZGziQkM1SG1jUrEYsPKNuHw5a/Vens58a91RwGH/3bgaJ2xg2/SNlcjle5eP9k+gEXIyYxxp1YLP1yPnMf6o1AIVXfuK95//BT9oTPhBbW1uuX7+uHF1nfJZsJaj/FXb4adbkVQpkTbg6ODs7lMAPwpnQMpYQjUBtefMJ/CCcCaim48mlbJ3nyZWdfsz5RCMTwLQ1hI9vReyqyeUHlaetIXw8pcswaJklfyvWV0t566VYnqgfLAZOZs5QV5IOrGHrYWUEqAt+r02kJ6fY/mG4TnOVFgMnM8e3K2n73ucLnWlrVl2V/ZfXdGWCC5CTScifr3HArQWfhLSmtNvPrJvs/TaTL78ronrdRFniPnISo/o5Ya1+4V50PYGwzzcRq7F5dgP9+fNQN+wsjaG4iNzMBCK3bibmakkOJ8YEzcArK4yVh+3wn+CFU1NIOZuKczcnUvcsZ8NBRb2UpoOZ8bdRtDm/jbe/OAmAZbdRTBrphYttybokE7NnGxFnc0sncxobxIwBWYStjMHuzxPxcjSD5DAWhcaU5tHJuyiU0lQHL/wn++BmZ4mxEVCUS+aRbazenaw98WOk4RzPgGkbBv9pEoO72GFpDBRlkRy5nf2WEwkcADHrQwjTaAqpsmPOKzCYMS5l+VWSy44pS3dGTRqFl7O16ngqzCL5SATb9sRRdtQCGNNm0CQmDXLDzkr96qEwi4TdoUS2DmTGAN2qWcm7FhF6pGQdNJZZyokJb87A89Y+ln8YWVbzq2QfdLbDUv1QVJSdScLB/7H5cFkdDr3lQ5VSWp4Xhcao+oWb6YXOGmqWO4P2g2HnmzKK9VBT/WaeOFmblS4rYXcom45V+6ipU3VV3hjWki3z7LAAkr87x5xPYEJwR17uqX7pfe8uaaevsmNDLvv+UE5sOOvuo5g4oqwMFVw9ScQXqXgEjcFFeW42ssNr8p/xKS2fuWTGR/K/rTFkFqv7INRzrGUd2UDILlVtjcqvR2rW7oyaOApPJ2vMjFHnjWHbB1kMCx6DTrHOimFDSBjWU99hUucM9r23jkjtQlwh1X7QOC6LCshKjSViWwRxpfPROKa35zJm8hg826quRUXX4wj7bDOxWQBeBFawjqnqdOsjG/g804cXR7phbZxVdn4zssZ9xETtslaQReoxZZnUV8bK5l2yz8HAMj4gkOCx1sR8/DmZPi8yqqM1xtkl66xQklfznFxyfJScu0p/swjqyxXa1taWW7eU1XQfjNnIELr1vUZy8EpuaiZ0mEaX8T0oC2MlkfrvD1CFZjV1weGNv2Kb+AFn95QTJNZn8fekBLqT+eMc+k0rqxkL4L3uIJufcSTxK2eG/w1gHJ8dW8OwJtEE9/Sn0hDl8DUcXD8Ox9uq/He+OMWyIRC9vCf+Wg9uhs333R9SmOyWyf55JU1NL+L7xOm4J23FeYM9x1YNo/mxENye+49qguHv8uO6yXTMiyZ44n6G7VqE9539zOn3EqotVU//x3cM8ZmDwS3KzttOwuw+pH3tzJy4NayZPY6ONkDRHdIiQ/CfthFeWMP614fh3lrVPmTOqU3MGasdaHUcG8SiaZPxdrOjuaqFbO7cgSZNNLexJmgGfLcSwSgmlwR/JwTXSPC3WbNmNX/NaxlAl0kmpH0SSl4hYBNAt7/0wyhrH2c/24V2RaCOtHrjbzi2uMml9X8l/RrQYihOL4zlXthCLl28q5W7XOrrE8pzoyYjDwLenoTb9UhCPthXdi9byflTdT+mc+XTOKdXcu3UYNx2MJP+NLjsOae4iKzzYYRGtiZQz/W19F7OkO1T07cMfdfi8p/Z0suuPeEQ8OdRuNkaqwLph/5H6J5kihy8NMYXkZUYwedf6G6vJn33tRXdM9qNmMvcoXak713JugNlV0azvgH8baIbWQdWs3pv/aj7XPP3liZYPb+SlvH/IumEqjkWq+fX0r51Ide//iuXlCfFHgvxHNeJ4t+/4tf//Qg0pYnP3+jqeIwzX+zC0I59yn/mKWM3ci5zh1gTt/VtNms0X1Px/WE591Ua96mVPROW0nePlZtJzDeryRqq77mxpCyr77ko574Iyrkvq+g4dtO/XaX3i0r65l/B81mWB/6LJ+F+5ySb3ttGQmn5U8/HIo5F72wuGflIq/kyUgGNZzC9St6FKMdXwmzIDBaPNOzdmvb5sJzjX/M4qcJ1Rke5z1xl9+9Vvm4s3k6u3yTG9HVSrU9hFnHhoWw+rrqyVnjdbKPnGYOy9Sy9Ft/O5OSez0ntFVTJeUdfuamoXD7IOwlV/KbV0RCdVk/LWOA9YwVzRrti0biQq0e/4P1lO3Tej9ek8uI3mgzJ4/HSUmY+2YzYqUHl5qkqQ5ZbU3mqzoAYRoXxjyl4msayZbXutLWhOt9VPVTtR61i1fuqoST4C2DayonOWjkfFyW1YUewdNpSRrhA0s/lBFO1+ODYEvKuVd7ji0+bVpBzjsjygr8An5wiCVd6Kpt31mL4MiujWqesetBfjSjjx1tzp+I92Jup89+hrE6Bise8+cwc7Y336JnMn+ehSJ3MO/On4t3fk8l6pm0wEm4S8lkmV0vu96xbMGJaJzZ9ZscEN0VeA3j8OQj/QW3Ij9uv7mcnjixze1prtI7mNDaIuX7umN2IZd/uCCJ+/o1cK3fGvDEXX+UH7pZeBIw0J+rDRSxatIiNX8WQUAROPbwU/dKBWT8PnIxy+e2wOvg7IJCgPw/GiQSiSvqbMnZh8J+D8O+pmBhLvF4chXnUf1i0aJHe4K9edr7MfWMM7mbpxOxR99+VWoS1nb0yp6gLNXw8Y+TEmNmvM6qbJQXx6j7MDqdjOTiQF3vrNhVmyDGXdCiCiN0nVU3fZZ7U7gvN0ovAef4MbgcJh1R9VUWlGOMyxJ+gP2ueoyzxClzM66PdsSwsWVYEUeeLMLe1JONkJBG7o0i+rbmMCKIqiXhYDvCllxWkno4pC/5aehGwQL0Pzqv3wY8xpGKHu99cgsZWo67w9ZNE7o4gKrlAu1+uQ+orrIH7wZDzTaV6+hP058G0KTjD/j2q3yIuyxz71rq/r9C1Y8VFvr9wR/VHYxMce7Vj9ked+PANk/JfUlTAckAgc58fjItxKjE/qs6pv+W5MGH2KN1a6UZOjJk3lzHdzMg6vo+I3RHsO5mLZbcxzH3DV9VXp9axVkCy+niKPJkBVbketR9D0Dx/Bjsbk65eVsTPsWSaWmNDkqoMnsrUWkbE/pNk4IabkzFcjiOmCsFfJ78ggp4fjItxOrE/q8tAfC7mzoPxnxeIl/LwNHcn8I2JOGXEsG9PBPuOp4OtOxNmTFC/nKloHcsYO08k0COVzcGLWLSoJFDgxJi5QfgPccE4Xb2fdkeRkGuuKpOBXihXp1IGlnEVY1zHBeKRupnlixexSO8LSH3s8H1DdXykH1EtY9+xVIps7ZArNJB9Tbd5598/IX7N19ykKSZNVYP+RgfjuXMTzFrqlMoKBXRWdRKXcVE7+IvzdN4Y4gh34ti/oWSkN452wOW0coO0ZRxZNG8kjsZ3iPt6ARuBTVcygObY67Rnp57vjUwq6oU28UYO0IQmJe8C1f0RZ6ZFw/adnMmEJt2e5A0AJvPZPyfTsUkO0RsWsNFRVdP5zh9x6uCvRn/GaccND/4C3q52NCGHO+1+5KtpdkT/8xmcfeaw50oTHIcHsOhvm/l+sTfZuxczxPkZQo7l0LxnAEGLy+bhPnsz21e9wTCbC+xc6s8QZ2ecfV5ifya1UCN5P8ETSmoCT67x4G+tcXHmXqw6+Atw4yTZQM7PyuAvQCJXjl7EOOcsmdfUo24eIDUsEbsnarhyQ/FJzqcCDk6U3sYacP7Uug+8nay+T4zk5HUDr50lixoQyOLXRuFuVVC6rIhDCRRZ2GFZ2b2cgSwHBPC3mdrL2HcsFezcGfNGEGPa60xR/jObuTuB03zg7D71dcoMpyEv8uIwHwJnjsIyRXW/GJWYj3XnMbzxvPJ6U4lK7hkz924nJgva+Iwpq01q5MZYXzeMr0byv3oS/K0d3Whmlki6OvgLkJ2UiUX2Yd3gL8DpCC7fNiH7zI/qEbe5E7mMVFNf7Fsp8j6gzLgksjCmjXPZNa3y+0PN+yrIPKV9/BvyTAgl5VF5j7WP2ExjrK20nxvL+tNWl+XqqvA4Nux+sSIVPp8Vn2R7eAJFlh6MGl52trEcOgYv6yLidtSP4G+du1vMrYIC0s5mEn+5tD6dWvVr/xYcMvzdmrZKjpMqXGd0VPjMpVL164YZ7i+9wcR2GcTsjSDix1jSscZ94gwmdFTlqPC6qY+lF4GzVeuZeky9jadzcRk/l1HtlJkNUGG5rG3q2sCB64muZ7WBT362lFdrMPj7qHN8bU7lMYwK4x+eeA6fyfz5ymlrR70LAD9+XJkQHk64xqDTh+4nc9iRbIHneE8sknfo1uDVI/CDIDybJ7G33K9Oyri2tIBraQYElSum6ptYzzKbexKktY2V9E385FJe7W9hYKBbiPolfvs1pv0lng+2Z5KWo76hbNmSF6ZbVPEFviceXYwhbR/rtkeq+9nZzOp/ribikjqLuinMrGMbWPlxGJGHoojav4N1q8NILbZj8AjFhcgOkr/YRlzJR2/FJzl5vgja9mKIrWZGa4Z4tIGsOI4nAk29mDTaBS6GEbJqMxGHoog6FMGmkA3EZhnj7uOr+GLdDhI/Z9uZqn1d12aAB3ZGucRu3aReRiRhoSEs/ypWmVXUkZo7nsHJbxJe1kUkh69m9VcRZcf0u9tIUjb4ZeAxlxkfRdShVFUNt9xUjb7QzPCaNAoXo1TCVoWweY+qr6qIz1ey4VgWxt2G4as+5u1GBDLGxZisIxtYvrpkWVFEfLWaDXtSKbgYS9ShODLuaC4jigSt906WOA0azOBBgxk8chKBsxezcKwLucc3s7n0C2DVOrmZZhHzyfKyfbA/jND3VhKWXIT1gImMqvApTo/bqcQeiiIuM1+7X674zNJlVr4fDDjfGMCztzvGpLJv/Q7V+ehQBJs/WM7qPYaFmB57eXdZPy+ZgKUp7D2bj+rduTGOT7dldn9l5kqoy5BxVgwbQkIJ219yTl3JuiNZyhKnLp9ZxH6ykg27VMdA5PZ1rN6dSpHDYHx7Ko+1fDJOq46n2IsFhl+PjDzw/4sX1kXJhL23klD1sqL2hxEasplYMkk4FEVUSq7WMqKOp1KANZZNoSDjsm6wrTyOY5g0UNVk9Mr3SvaDqnwv/ySGLGMXRo1XXCtbO8He1aVlIXL7OjafyAXLXnj1BCpcxzKWtjeIUDRT7eQ3CS/bIpJ3rWRlqHo/HYpg8+rlbDiShbHLKCb01phJpQwt4yUssc6KYMP+dINr/ADQ2gsPB8g9vplN6mVE7golJHgzcoUGrFrqvOwDoDibu5VWYOyBWQu4V3BbmVABR1UTyFpNL7sz7LV32f5VEN5NM4leNZPgFHXSDEdVoN5tMikpKVrDwXXaffM6zltDQLcm8Md+QparIwnxGeQA9u0UPfWq51vVQKyqP+KSPn2/Y+PRNLBw58nZjkz/ahHD7O6Q+PUc/DekgY8jjkDG71sV00PzIcsU25PA9nlai9Li3cYeaI57xwzWvuDPkq/jIOU7jqflAI6M/Isj+1/vh//y70gjjv/sOUMO4NhNvd3D17B+tjfNL25l5mB/lnwVrdrulL7YWwOZaZSt5WPs7G/gtRCrki6+bDywBpp6DlRkBLDDvrcd+cbdsGupHmXaDfsRnhRdvqDI++DSr2t+PWTY+VPrPvBOBnGHoog6FEvqbQOvnag+cg30U1+Tg1eXLitqz2ZWr48gtcJ7uTLWA2YQHBysNZR+PNjUi0mj3TDL1l5G5K5QVr4XRnKRNV4TRimCBRU8s7W2I/frlepzfgSb/hNGcpExLsN9sT4RWnqNjPg8lKhMMO7sTlVegVZ+z5hK2NcxZBm74+un2kYnvzF4WGQS+dW+x7zf47PcyGxPh+Fle9zK1Y58q27Y6+tar9NwbMnGsnvJRxUmmLjPpp3DJfIMjUQa6lKmditLBt0fat5XQW6KxvFv4DMhgMfzgapnTa17LNX7hM3HtZ8by/rTVpXl6qr4ODbsfrF8lT+fFRzfQURyEXaDxuLVVH0eeLINRWe3a9XAFhqibjDtud95bcF1UpWf5uXcYPsnyqCwgQx9t6aj4uPE4OuMUqXPXNW9brTBiX2s/lB9zO/fwbqvTpKLJb0GqM5JFV03damvxcZZxHxStp6Ru0JZ+UksucqHVgNUXC7ryLVwVkyfytIf06C5K37PT1HmeARY4PHcW3z0hTqW891WQpdPxaOqL/pEnaj5AHCz0fz9qx/Yv3+/3uHv3vruKCrzEa8MG8YwfcPXNX9j/2hJYoefH34ag26AV1WztmLageQJLWMJqdGq7/poL/NVPsJP3zJzYgnR2kbdpqZdx2sEiKfBR3r3g3i0hbNi9RdER0Xzxftv67zgOLnqfdbvjiZ693reX6X8sm0rb7//BdFHY9mqZ9r6qrS/xoJ72k3i5t1n32fXeO3PF9h7WZ23fTNGaOap1A1y84DW7nhpRleLiyhSfz7vNqAX1qQTu1dxI5Mbw8lLYNzaSbuWV/ZF4hRPyyeP/EYudrj307its/PC3QEyz8SQCpj164uLcQFxkTHaD3TFqRxPzNX+kh6AXC6eq/pj+Y3sXMAS194uWsGJosIqvaYW1VS7x7MTfbtYQ2YMu44oqu4VniTypPa4qh9zCk296OtiTMHpSJ2agqknksjFDqeOAE549bSDzCg+r6RJvYrZ4TF6FKNGj2LUEA9crG4QGfo2Ids1ml9Vr1PR+X2EXdSeGnKJ2RtLFna4D2ijTKw+g/dD5ecbQ9zIzQXa4K5o8qlI+mnV1bjkhcM9ChUt0mYdz2ftghQCPstSB4HNce2vv+5guTw8cDEuIuGnMFIVv2H6XtW5vYwbXj2s4VIsEYpjM/fISdIVNTn0Mfh61M8Td9MiEnaF6hyThsovzFeOKpdqvTKJ2aU4lwBcDCMqBYw7e+CpOT77N/YpzlMJ51MpwhjLqjwQXzrPSa19r97P+s6DQGp4FMnFxrj11FqbihlcxsukJyrv0QyQnUVuMVh27IuLZn9ehUVVCyQ3QAXXs4GWmLVVphjIyAkzSyi4XpWafpNVNW9xZOQXJcHP71n/Ul84tZEFE/upgqdq3j0daU4O0UudcXbWHoa8Hq0x3+m8+0IfmpBD9Gczy2qZhqaRATRv3R1VvWMV1Xwh7byyF2JNjnRv3RzIJlPd15OqP+IM0tS1ZaO3xJFGEzqO+4xZA5uTcziEl+arlq6q6ZxD2qmy7VFNn8hWxbY4O7sxsbSfYKVxuLdrAmSy/z1/NpYExwErM1U7zmk/LmFOSQU5gI72NAeyL+/RqBmdxv5/LtCugTvRHUcLyLl8pkqB8MppNwG9VadP4EfUrV1c+PQwzSb/i26Tn8dmqAdFR5dx2XgcbTQPIIAegbTJ+Y4zsXex6T8QqxFL6LXwr7S8vIn4H/W+KX8g1hbmZX9U4/ypzfBrp9NAD+yMMon6XPeaXBVltRbLhpJWOFT3zvqv++TGsO9EFti541XWCF/Fz2zZCcSc1/j79m8kXQVIJ/ZHzWt9JnEpuWBsj71W0KNiBt0zXgxj2/EsrPuNwcfFl4n9rMk8+D/2lbPKj4+75IcvJunWKLrPXkLbvgHYt77AhU0pWE8YpXhJ3JFWvnZkbNpMloM3Nh2epcPs9fQZZcIfn/yLbOWx8qCsLdEoZYbfH5bD4GdCIy88uxhTFL+dUD33WLXFoOO42gx5PsslZlsEqbjgM9odjwmjcCmOY/tX1bjXe+w0xUnrnFX92r8lDHm3VjWGX2d0GPDMVd3rxm8/Ksrj+QRSi8BY8xprKKNeuDuX847kYhhR1bixqt1yaShrfF5bwfzhjkAeSacevTLZZdoK3n7RG0fzLNIuJJF0GRx6T+btfwai0+hPA5T24ZrKYxgVxj9iif1xPe+/r5y2dtRwANidV/89h6daPTY9dT8SSmrW7lgVS57LBN0awqAbSC6vz109kq7lQUtHfJQJlSpbZsjRPCz6v1pxzd4KJO1Ur/eqWPKae/LqkqqvjXj48g5vZcXKFXravweIJ/zDFazQ03Y+JdMuW1rr/f/WNgv1y1+Lns3pqb4RKswq5BRAezNmvtQEx5IXxBaNUHcNBvl3UXaBWLFkfvwhjlxjF8YEBbN4tj8+Xey0AqPWVmZAG3wXaX8JHhwcrGqqxdoerVDSzcu6N52Jx4nLArsunqVf9jkNdMeuOJXYX1RP1/ZW5oAZHi/qLmdGP0vAGjutFzpZXK7GjVrBoQgiLxVg3S+Qd94JInCsJ056q9SImlJ3x3MbbKyg4I9k/V/sF2uHEKp+zCnYql4+mPUO0Jk++BVPLAFrByegDfbWFayXwZIJW6RqWn3551GkG7XB58+Typqso2ydMlITNEZqSMskC7C2rcEAsMH7ofLzjSGS90UQl22Mi18QwYvm4j/MDTu5pSxjgbrmfCOeGWqp/n8hV9UXzaF/bs6EvmWB3tKPMoC8vKp9je5kZwlkoPdwK0YRtFPVrKWtL4uVx8nyMTgB1nYVH5eGXo+cHKzLX69KFXG3GKxbVbwumqytzOB2OsnlFPD0zCwwsqe15ouN63qulVm55AKWduW8ZNEjN6OsaUYVdQ3m8s43xelkZAN2rbWv3RUxuIyXyEVntQxxO4qIg+kUWHkSuPgdggLH4OkoF2gAEpPIwwqrLq7KFIMY9e+DjVE22ed1jrryqQOOd078RxX4HLuEPSl3aGJnRfaPIWxV1PoZ1sFRFXD9r/Z4pWHrAvC2Ac7uZIHWF7+JZOQANnaM1Birmm8mGXEaI5Wcp9OxHZCZyM8plAVib6RxvCQIe3ATcX9Ac9eONM/cT/DzG9WBVHVN56I04krXvWT6DCparA7nJ+loB5yNYMnXmgnq+eX9ynevazesHNDOXhV8TkgDAvDu3ASSognWDBIDuNtjB2SkVN7AtuE0g78bmTNhAQtKm4OuD0HgA1wKXUh8NNi52WH5xEo6dWpD++dX4jp1iXpYTs9x3Wji+iy9Btth4eVPy+u7OfPeTM6GH6iFj0vMsLYyhtu5qg8dq3z+VDL82tnGzrrCa5Ghymotlg2xF1V1CVX3zuVfX1OvZgHWWGtdYCp4ZtO5FhZQcEf9r7IWV3ERYIxZFboNMfSeMXVXGCfz2uD7kg92mY9708+a7nInZiVn1n9OjpMHLZt50PWVobRwfZbuL5WUsSW4vhZEB3s72r0yDftmHXEdYcW1bQs5FrKSGxmVNlFRdbbWWAL52aoPEwy9PyyPwc+Ebe2wNqrgOauWGHocV4+Bz2e5MWz+OR1LD38mdYO4HZsVHyAKvfqbYn03n7SScvAgtX9LGPBurWoMv84oGfLMVb3rRiaXlYFassjNBZrbVfhBh16Vld17yhGVq91yWTmLnpNZGhpK0GhXTK7G8sVbLzPnk0etzSQ/pvq6YpoTywcvTuXV/5vDnJmTCfrhKqYuzzDtUaywXOMMiGFUGP9YytI66v+Xmg4AD1m2jEkdTSF1N/Pmz9M7hJ5QVFMQD0bdHHLe0R2E/ryUvcngOn4Ngcp8DyAy/Qo074pPRcHbaT1xJYlT5dTKjVw2WdVM9bSl1Qgka/h5KZN3Jj1QMFmIh6cRL/+7K2Ffd2ZLcFscTVF9KRiruiBY+NryzEQXPtzSlbCvOxG2pRNDW6vz/JKNZh0LQ+Se2MzK5avZdjCBXEt3fKfO5Z15Y3DSPPMXpBKj+BK8bFD3hVpC781TKjFnMsHODU87ABf6drOm6HwMUVoP91nE7VHOv2RQ9udRhJ5OvipXnMq+D5ezfH0EJ6+CU78JzFi0mIABddFXx+Oobo9ngLtFhtfcq9oxp1/WGeV0ZUNJjQmqvF4VKzgfwbodcRSZuTOxqv2h1RJD9oNB55vK5J5k83tvs3prFAm5lrgPD2DuYn19Bz2mhjuwaWdnvt3ZhZm91J9TZGQT+RtAE3xGt+XlpV0I29mZb7/twqYAa0wBsjIJ36Y9K8MUUWBYG3MAFFyM0Tk+SgdD+iE0+HpUtfUqk8TlTKBtZ+2PKx5RVak9/6AMKeMqVavVryl17zqWB28g4mQGOHkxYeZiFr9YjT6LG5qs78m8BBaez9GiCsEPAIwG0HqAE2T+yvUqNLdPP0dVwLGkWeRTm5j5xXFysMPbP0iROQD3VlQeMB3yLoueVn9Z1S2Ag1pNKy/CuznQ3JHuziUTqOdbSb+33vOG4W4MaYc3qvvwVfcbfCWOsnrD0Wz6NQ3uJLL1by9pfGWvrul8JU2jxq16+sw0jekNMFHVXHXa73sUtXTV8/vjAiFa40ua2c4gbQMQqO53OCNRp5bvooHuQCZpxxQJ1TaMZbs1g78lff5q9gk8nTW7lz3aQWDuUpx2lltXD3NmRSCx/wjgWORtrKwzyfjhO/KaNiX7u8Uc+8dMYld8RUZRJlnHYykqqIWgFEBTT9xaQ1FqApqvmQ0/f+pn8LXz7l1q7m6zplTzma0mGHrPWJxPfpHqzWdRQa6BTec+Rgovknspm2t7AoldEciRZR9w3doOowvfkXoqD/O7B/ht5UxiVwTyW3Qmdy/Fknsls9Z+dpfuLpiRSfJZjV/K4PvD8hj+TFhUWMdHiKHHcTUZ+nx291YuRUYAueRna6eJchzNYtqUFP554k6N1P5VMfTdWtUYfJ3RUd1nrrpXo2W3lstl+azxeW0Nn66YimfLuyTtDiEwcClbT+kLID5k7V1oZQF58ZHs1Vi9+F0nuYopjp0fKPIjakGNvv4wbaz+JKLwFidiT+gdLj96d631mA9Lp3likRPLR+p+dUNn7yAJV0bUZA3ZT3YQm2OB5/jywsqBrBnvqgpCK5M0hM7eQVJN1N4t6fP4QYPJQtQ5U2wsADN1tax7d0gO+52lW1R/eppAVoH6q0Ez9beZefmc+jqZtz7RG32tXGEmJ/dsYnXw26zbn06RrReT1P0g5RcUgZkxuSe0vwQvGxL01zJSyPzlN9Kxw32gE3T2pLtlLr8dLmvGIregCDCn6Kpy/iVDef15VE9BWhTbPgzh7VWbics2w81vEl41erUTKnV5PKte3li2cdHbT6K5qXZzQQ98zN0uoAgwv5upZ1rVoKoxoV4vJzdFP9YP6NR2ws4XYdzNlwklDxrXc8kH7J3Kabza0U7Vr/FlzYc4a+y0mlwCjNpgb6UYVx6D94NaBecbwxWReSqCTR8s5+0PI0kvtsbruTHKTI8lCwcTTBs3VtfsvU/eH5l8+l6Wqg+m1kZQcIfCe0DjxpiaNgLuk3XxMuvnXWNfFZ8bVWXIXn/zlU3NFOVQVQ7MjHOJ1XOMRB3S7YdQydDrkWq92uDSXTkHQ2Rx8EQqGLuV9gdYmazsAmjaBhftzqtKtbGzhqJ0UtXN29euLHJvg1k7F0VfWmrqsl10ORWDK+lWtYw/qIJUor5ZR8g7IWw+k4VZ5zFMGqDM9LjJ5sa+KG4budJ+4jOUVty3HkGbKc/RsjRC7kSrF17FqvRi05IW/i/i0CybKxFfU5WQ13Rndc1UjWaRCf2VxDxo4toHrZ56nfviaFNZwNSRRX8bT0fjO/z6wRCdZqKdnZ1ZcjAHsMLuafUkGvNVNotWavi7LHvaEXKi2bRK/dmYut/gtN+1a9tGzx6Cs9twFmjWri1pWjnteNlHZyX9DldY7VjXuG6ONCGHtF8Vn6+p55eZpvysTR18zkzT+uAt+7Ii35B3Gda58kC44VTB34Buzck5u0kj+FtCFQTedDaH5t0C6</t>
+  </si>
+  <si>
+    <t>Brakes</t>
+  </si>
+  <si>
+    <t>Nexon</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>2025-07-10</t>
+  </si>
+  <si>
+    <t>Brake not responsive on downhill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prima </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low </t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Prima 3835</t>
+  </si>
+  <si>
+    <t>2025-07-26</t>
   </si>
 </sst>
 </file>
@@ -598,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
@@ -901,7 +928,7 @@
         <v>51</v>
       </c>
       <c r="M9" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -936,13 +963,13 @@
         <v>45</v>
       </c>
       <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" t="s">
         <v>53</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>54</v>
-      </c>
-      <c r="M10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -959,28 +986,28 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
         <v>57</v>
       </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>58</v>
-      </c>
-      <c r="I11" t="s">
-        <v>59</v>
       </c>
       <c r="J11" t="s">
         <v>45</v>
       </c>
       <c r="K11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" t="s">
         <v>60</v>
-      </c>
-      <c r="L11" t="s">
-        <v>61</v>
       </c>
       <c r="M11" t="s">
         <v>23</v>
@@ -991,7 +1018,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -1003,16 +1030,16 @@
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
       </c>
       <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" t="s">
         <v>63</v>
-      </c>
-      <c r="I12" t="s">
-        <v>64</v>
       </c>
       <c r="J12" t="s">
         <v>45</v>
@@ -1021,10 +1048,86 @@
         <v>46</v>
       </c>
       <c r="L12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" t="s">
         <v>65</v>
       </c>
-      <c r="M12" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>